<commit_message>
Some code refactoring done
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="600" windowWidth="24615" windowHeight="11445" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="18705" windowHeight="6465" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="PaidTillDate" sheetId="1" r:id="rId1"/>
@@ -16,11 +16,12 @@
     <sheet name="Sheet2" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:R20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="130">
   <si>
     <t>Item</t>
   </si>
@@ -407,6 +408,9 @@
   </si>
   <si>
     <t>JP Associates</t>
+  </si>
+  <si>
+    <t>Tata Power</t>
   </si>
 </sst>
 </file>
@@ -12369,7 +12373,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -12517,9 +12521,15 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
+      <c r="A7" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="10">
+        <v>421</v>
+      </c>
+      <c r="C7" s="11">
+        <v>42914</v>
+      </c>
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
       <c r="F7" s="10"/>
@@ -12774,10 +12784,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C14"/>
+    <sheetView topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12792,7 +12802,7 @@
     <col min="10" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="27" customFormat="1">
+    <row r="1" spans="1:16" s="27" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>47</v>
       </c>
@@ -12827,7 +12837,7 @@
         <v>43075</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" s="14" t="s">
         <v>51</v>
       </c>
@@ -12871,8 +12881,11 @@
       <c r="O2">
         <v>40.9</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="P2">
+        <v>42.35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="18" t="s">
         <v>52</v>
       </c>
@@ -12916,8 +12929,11 @@
       <c r="O3">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3">
+        <v>63.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="18" t="s">
         <v>53</v>
       </c>
@@ -12961,8 +12977,11 @@
       <c r="O4">
         <v>244.35</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="P4">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="18" t="s">
         <v>54</v>
       </c>
@@ -13006,8 +13025,11 @@
       <c r="O5">
         <v>62.75</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="P5">
+        <v>64.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="18" t="s">
         <v>55</v>
       </c>
@@ -13051,8 +13073,11 @@
       <c r="O6">
         <v>81.349999999999994</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="P6">
+        <v>83.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="18" t="s">
         <v>56</v>
       </c>
@@ -13096,8 +13121,11 @@
       <c r="O7">
         <v>91.05</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7">
+        <v>92.55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="18" t="s">
         <v>57</v>
       </c>
@@ -13141,8 +13169,11 @@
       <c r="O8">
         <v>104.2</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="P8">
+        <v>106.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="18" t="s">
         <v>58</v>
       </c>
@@ -13186,8 +13217,11 @@
       <c r="O9">
         <v>134.55000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9">
+        <v>136.55000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="18" t="s">
         <v>59</v>
       </c>
@@ -13231,8 +13265,11 @@
       <c r="O10">
         <v>121.55</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="P10">
+        <v>124.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="18" t="s">
         <v>60</v>
       </c>
@@ -13276,8 +13313,11 @@
       <c r="O11">
         <v>643</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="P11">
+        <v>640.04999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="18" t="s">
         <v>61</v>
       </c>
@@ -13321,8 +13361,11 @@
       <c r="O12">
         <v>117</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="P12">
+        <v>119.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="18" t="s">
         <v>62</v>
       </c>
@@ -13366,8 +13409,11 @@
       <c r="O13">
         <v>19.25</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="P13">
+        <v>19.45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="18" t="s">
         <v>63</v>
       </c>
@@ -13411,8 +13457,11 @@
       <c r="O14">
         <v>81.2</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="P14">
+        <v>81.900000000000006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="18" t="s">
         <v>64</v>
       </c>
@@ -13456,8 +13505,11 @@
       <c r="O15">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="P15">
+        <v>49.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" s="18" t="s">
         <v>65</v>
       </c>
@@ -13501,8 +13553,11 @@
       <c r="O16">
         <v>36.299999999999997</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="P16">
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="18" t="s">
         <v>66</v>
       </c>
@@ -13546,8 +13601,11 @@
       <c r="O17">
         <v>56.4</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="P17">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="18" t="s">
         <v>67</v>
       </c>
@@ -13591,8 +13649,11 @@
       <c r="O18">
         <v>23.8</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="P18">
+        <v>23.95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="20" t="s">
         <v>68</v>
       </c>
@@ -13628,8 +13689,11 @@
       <c r="O19">
         <v>18.25</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="P19">
+        <v>19.149999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="20" t="s">
         <v>69</v>
       </c>
@@ -13665,8 +13729,11 @@
       <c r="O20">
         <v>585</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="P20">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="20" t="s">
         <v>70</v>
       </c>
@@ -13700,8 +13767,11 @@
       <c r="O21">
         <v>55.05</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="P21">
+        <v>55.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="20" t="s">
         <v>71</v>
       </c>
@@ -13733,8 +13803,11 @@
       <c r="O22">
         <v>23.2</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="P22">
+        <v>23.95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="20" t="s">
         <v>45</v>
       </c>
@@ -13764,8 +13837,11 @@
       <c r="O23">
         <v>512.20000000000005</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="P23">
+        <v>521.95000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="30" t="s">
         <v>116</v>
       </c>
@@ -13775,13 +13851,19 @@
       <c r="N24">
         <v>311</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="P24">
+        <v>308.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="30" t="s">
         <v>117</v>
       </c>
       <c r="N25">
         <v>500.9</v>
+      </c>
+      <c r="P25">
+        <v>485.3</v>
       </c>
     </row>
   </sheetData>
@@ -13795,7 +13877,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13807,7 +13889,7 @@
     <col min="6" max="6" width="5" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -13817,8 +13899,9 @@
       <c r="C1" s="16" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="16">
         <v>15000</v>
       </c>
@@ -13828,8 +13911,11 @@
       <c r="C2" s="16" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="16">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="16">
         <v>20000</v>
       </c>
@@ -13839,8 +13925,11 @@
       <c r="C3" s="16" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="16">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="16">
         <v>13000</v>
       </c>
@@ -13850,8 +13939,11 @@
       <c r="C4" s="16" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="16">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="16">
         <v>1000</v>
       </c>
@@ -13861,8 +13953,11 @@
       <c r="C5" s="16" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="16">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="16">
         <v>3000</v>
       </c>
@@ -13872,8 +13967,11 @@
       <c r="C6" s="16" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="16">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="16">
         <v>3000</v>
       </c>
@@ -13883,8 +13981,11 @@
       <c r="C7" s="16" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="16">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="16">
         <v>5000</v>
       </c>
@@ -13894,8 +13995,11 @@
       <c r="C8" s="16" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="16">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="16">
         <v>18870</v>
       </c>
@@ -13905,8 +14009,11 @@
       <c r="C9" s="16" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="16">
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="16">
         <v>3000</v>
       </c>
@@ -13916,8 +14023,9 @@
       <c r="C10" s="16" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="16">
         <v>2100</v>
       </c>
@@ -13927,8 +14035,11 @@
       <c r="C11" s="16" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" s="16">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="16">
         <v>5000</v>
       </c>
@@ -13938,8 +14049,9 @@
       <c r="C12" s="16" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="16">
         <v>6000</v>
       </c>
@@ -13949,28 +14061,35 @@
       <c r="C13" s="16" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="16">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" s="16"/>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="16">
         <f>SUM(A2:A17)</f>
         <v>94970</v>
@@ -13982,8 +14101,12 @@
       <c r="C18" s="16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" s="16">
+        <f>SUM(D2:D17)</f>
+        <v>98600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="16">
         <v>112000</v>
       </c>
@@ -13993,8 +14116,9 @@
       <c r="C19" s="16" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="16">
         <f>A19-A18</f>
         <v>17030</v>
@@ -14005,6 +14129,10 @@
       </c>
       <c r="C20" s="16" t="s">
         <v>85</v>
+      </c>
+      <c r="D20" s="16">
+        <f>B19-D18</f>
+        <v>13400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code changes and refactoring
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="18705" windowHeight="6465" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="18705" windowHeight="6465" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="PaidTillDate" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,11 @@
     <sheet name="Sheet2" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:R20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="128">
   <si>
     <t>Item</t>
   </si>
@@ -275,9 +274,6 @@
     <t>SIP</t>
   </si>
   <si>
-    <t>Salary</t>
-  </si>
-  <si>
     <t>Thekedaar</t>
   </si>
   <si>
@@ -353,64 +349,61 @@
     <t>Bhel</t>
   </si>
   <si>
-    <t>407138365676 </t>
-  </si>
-  <si>
-    <t>Reliance Mutual Fund</t>
-  </si>
-  <si>
-    <t>1551643 </t>
-  </si>
-  <si>
-    <t>IDFC</t>
-  </si>
-  <si>
-    <t>ICICI Prudential</t>
-  </si>
-  <si>
-    <t>SBI Mutual Fund</t>
-  </si>
-  <si>
     <t>ITC</t>
   </si>
   <si>
     <t>SCHAND</t>
   </si>
   <si>
-    <t>80C</t>
-  </si>
-  <si>
-    <t>SBIN0003633</t>
-  </si>
-  <si>
-    <t>005801565788</t>
-  </si>
-  <si>
-    <t>30200155294</t>
-  </si>
-  <si>
-    <t>ICIC0000058</t>
-  </si>
-  <si>
-    <t>State Bank Of India</t>
-  </si>
-  <si>
-    <t>059399500001653</t>
-  </si>
-  <si>
-    <t>YESB0000593</t>
-  </si>
-  <si>
-    <t>Yes Bank Ltd</t>
-  </si>
-  <si>
-    <t>ICICI Bank Ltd</t>
-  </si>
-  <si>
     <t>JP Associates</t>
   </si>
   <si>
     <t>Tata Power</t>
+  </si>
+  <si>
+    <t>Monthly Expense (Rent + Kharcha)</t>
+  </si>
+  <si>
+    <t>HomeLoan</t>
+  </si>
+  <si>
+    <t>EMI Marriage</t>
+  </si>
+  <si>
+    <t>EMI Loan</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Estimates</t>
+  </si>
+  <si>
+    <t>Flooring</t>
+  </si>
+  <si>
+    <t>Outside Wall Stone</t>
+  </si>
+  <si>
+    <t>Bathroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kitchen </t>
+  </si>
+  <si>
+    <t>Rooms almirahs</t>
+  </si>
+  <si>
+    <t>Beds</t>
+  </si>
+  <si>
+    <t>Electric Wiring</t>
+  </si>
+  <si>
+    <t>Paint</t>
+  </si>
+  <si>
+    <t>Gate</t>
   </si>
 </sst>
 </file>
@@ -421,11 +414,18 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy"/>
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -551,60 +551,65 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -899,7 +904,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -993,7 +998,7 @@
       </c>
       <c r="H3" s="5">
         <f>H2-B25</f>
-        <v>265990</v>
+        <v>245990</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -1135,8 +1140,12 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:26">
-      <c r="A18" s="5"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="8">
+        <v>42917</v>
+      </c>
+      <c r="B18" s="2">
+        <v>20000</v>
+      </c>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:26">
@@ -1175,7 +1184,7 @@
       </c>
       <c r="B25" s="2">
         <f>SUM(B2:B24)</f>
-        <v>292500</v>
+        <v>312500</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -12465,7 +12474,7 @@
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" s="10">
         <v>410</v>
@@ -12480,8 +12489,8 @@
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="31" t="s">
-        <v>116</v>
+      <c r="A5" s="29" t="s">
+        <v>109</v>
       </c>
       <c r="B5" s="10">
         <v>622</v>
@@ -12496,8 +12505,8 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="31" t="s">
-        <v>128</v>
+      <c r="A6" s="29" t="s">
+        <v>111</v>
       </c>
       <c r="B6" s="10">
         <v>1739</v>
@@ -12521,8 +12530,8 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
-      <c r="A7" s="31" t="s">
-        <v>129</v>
+      <c r="A7" s="29" t="s">
+        <v>112</v>
       </c>
       <c r="B7" s="10">
         <v>421</v>
@@ -12784,10 +12793,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12802,15 +12811,15 @@
     <col min="10" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="27" customFormat="1">
+    <row r="1" spans="1:17" s="27" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>107</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>108</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>48</v>
@@ -12837,12 +12846,12 @@
         <v>43075</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" s="14" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="15">
@@ -12884,13 +12893,16 @@
       <c r="P2">
         <v>42.35</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="18" t="s">
         <v>52</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="19">
@@ -12932,13 +12944,16 @@
       <c r="P3">
         <v>63.25</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="Q3">
+        <v>63.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="18" t="s">
         <v>53</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="19">
@@ -12980,13 +12995,16 @@
       <c r="P4">
         <v>246</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="Q4">
+        <v>244.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="18" t="s">
         <v>54</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="19">
@@ -13028,13 +13046,16 @@
       <c r="P5">
         <v>64.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="Q5">
+        <v>64.650000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="18" t="s">
         <v>55</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="19">
@@ -13076,13 +13097,16 @@
       <c r="P6">
         <v>83.95</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="Q6">
+        <v>85.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="18" t="s">
         <v>56</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="19">
@@ -13124,13 +13148,16 @@
       <c r="P7">
         <v>92.55</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="Q7">
+        <v>93.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="18" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="19">
@@ -13172,13 +13199,16 @@
       <c r="P8">
         <v>106.75</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="Q8">
+        <v>108.35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" s="18" t="s">
         <v>58</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="19">
@@ -13220,8 +13250,11 @@
       <c r="P9">
         <v>136.55000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="Q9">
+        <v>135.30000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" s="18" t="s">
         <v>59</v>
       </c>
@@ -13268,13 +13301,16 @@
       <c r="P10">
         <v>124.6</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="Q10">
+        <v>123.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="18" t="s">
         <v>60</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="19">
@@ -13316,13 +13352,16 @@
       <c r="P11">
         <v>640.04999999999995</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="Q11">
+        <v>648.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="18" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="19">
@@ -13364,13 +13403,16 @@
       <c r="P12">
         <v>119.8</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="Q12">
+        <v>123.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="18" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="19">
@@ -13412,13 +13454,16 @@
       <c r="P13">
         <v>19.45</v>
       </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="Q13">
+        <v>19.850000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="18" t="s">
         <v>63</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="19">
@@ -13460,13 +13505,16 @@
       <c r="P14">
         <v>81.900000000000006</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="Q14">
+        <v>80.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="18" t="s">
         <v>64</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="19">
@@ -13508,13 +13556,16 @@
       <c r="P15">
         <v>49.7</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="Q15">
+        <v>52.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="18" t="s">
         <v>65</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="19">
@@ -13556,13 +13607,16 @@
       <c r="P16">
         <v>36.799999999999997</v>
       </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="Q16">
+        <v>36.35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="18" t="s">
         <v>66</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="19">
@@ -13604,13 +13658,16 @@
       <c r="P17">
         <v>57.1</v>
       </c>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="Q17">
+        <v>58.35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" s="18" t="s">
         <v>67</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="19">
@@ -13652,13 +13709,16 @@
       <c r="P18">
         <v>23.95</v>
       </c>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="Q18">
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" s="20" t="s">
         <v>68</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="16"/>
@@ -13692,13 +13752,16 @@
       <c r="P19">
         <v>19.149999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="Q19">
+        <v>21.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" s="20" t="s">
         <v>69</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="16"/>
@@ -13732,13 +13795,16 @@
       <c r="P20">
         <v>580</v>
       </c>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="Q20">
+        <v>589.70000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" s="20" t="s">
         <v>70</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="16"/>
@@ -13770,13 +13836,16 @@
       <c r="P21">
         <v>55.7</v>
       </c>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="Q21">
+        <v>54.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22" s="20" t="s">
         <v>71</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="16"/>
@@ -13806,13 +13875,16 @@
       <c r="P22">
         <v>23.95</v>
       </c>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="Q22">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" s="20" t="s">
         <v>45</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="10"/>
@@ -13840,10 +13912,13 @@
       <c r="P23">
         <v>521.95000000000005</v>
       </c>
-    </row>
-    <row r="24" spans="1:16">
-      <c r="A24" s="30" t="s">
-        <v>116</v>
+      <c r="Q23">
+        <v>545.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="28" t="s">
+        <v>109</v>
       </c>
       <c r="M24">
         <v>310.55</v>
@@ -13854,16 +13929,22 @@
       <c r="P24">
         <v>308.8</v>
       </c>
-    </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="30" t="s">
-        <v>117</v>
+      <c r="Q24">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="28" t="s">
+        <v>110</v>
       </c>
       <c r="N25">
         <v>500.9</v>
       </c>
       <c r="P25">
         <v>485.3</v>
+      </c>
+      <c r="Q25">
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -13874,10 +13955,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13887,9 +13968,12 @@
     <col min="3" max="3" width="20.42578125" style="21" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" style="21"/>
     <col min="6" max="6" width="5" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:12">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -13900,8 +13984,17 @@
         <v>0</v>
       </c>
       <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="H1" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="36">
+        <v>25000</v>
+      </c>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="16">
         <v>15000</v>
       </c>
@@ -13914,8 +14007,17 @@
       <c r="D2" s="16">
         <v>15000</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="H2" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="36">
+        <v>20000</v>
+      </c>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="16">
         <v>20000</v>
       </c>
@@ -13928,8 +14030,17 @@
       <c r="D3" s="16">
         <v>22000</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="H3" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="36">
+        <v>15000</v>
+      </c>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="16">
         <v>13000</v>
       </c>
@@ -13942,8 +14053,17 @@
       <c r="D4" s="16">
         <v>13000</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="H4" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="I4" s="36">
+        <v>20000</v>
+      </c>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="16">
         <v>1000</v>
       </c>
@@ -13956,8 +14076,17 @@
       <c r="D5" s="16">
         <v>1000</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="H5" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="I5" s="36">
+        <v>20000</v>
+      </c>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="16">
         <v>3000</v>
       </c>
@@ -13970,8 +14099,17 @@
       <c r="D6" s="16">
         <v>2500</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="H6" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="I6" s="36">
+        <v>4139</v>
+      </c>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="16">
         <v>3000</v>
       </c>
@@ -13984,8 +14122,17 @@
       <c r="D7" s="16">
         <v>3000</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="H7" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="36">
+        <v>6000</v>
+      </c>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="16">
         <v>5000</v>
       </c>
@@ -13998,8 +14145,17 @@
       <c r="D8" s="16">
         <v>15000</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="H8" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="36">
+        <v>109004</v>
+      </c>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="16">
         <v>18870</v>
       </c>
@@ -14013,7 +14169,7 @@
         <v>19000</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:12">
       <c r="A10" s="16">
         <v>3000</v>
       </c>
@@ -14025,7 +14181,7 @@
       </c>
       <c r="D10" s="16"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:12">
       <c r="A11" s="16">
         <v>2100</v>
       </c>
@@ -14039,7 +14195,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:12">
       <c r="A12" s="16">
         <v>5000</v>
       </c>
@@ -14051,7 +14207,7 @@
       </c>
       <c r="D12" s="16"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:12">
       <c r="A13" s="16">
         <v>6000</v>
       </c>
@@ -14065,23 +14221,34 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:12">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:12">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+    <row r="16" spans="1:12">
+      <c r="A16" s="16">
+        <f>SUM(A2:A15)</f>
+        <v>94970</v>
+      </c>
+      <c r="B16" s="16">
+        <f>SUM(B2:B15)</f>
+        <v>87968</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="16">
+        <f>SUM(D2:D15)</f>
+        <v>98600</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="16"/>
@@ -14090,50 +14257,10 @@
       <c r="D17" s="16"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="16">
-        <f>SUM(A2:A17)</f>
-        <v>94970</v>
-      </c>
-      <c r="B18" s="16">
-        <f>SUM(B2:B17)</f>
-        <v>87968</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="16">
-        <f>SUM(D2:D17)</f>
-        <v>98600</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="16">
-        <v>112000</v>
-      </c>
-      <c r="B19" s="16">
-        <v>112000</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="16"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="16">
-        <f>A19-A18</f>
-        <v>17030</v>
-      </c>
-      <c r="B20" s="16">
-        <f>B19-B18</f>
-        <v>24032</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="16">
-        <f>B19-D18</f>
-        <v>13400</v>
-      </c>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14142,101 +14269,114 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="B3" s="23" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="B4" s="23" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="C10" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <v>737556</v>
-      </c>
-      <c r="E10" s="33">
-        <v>108403.13</v>
-      </c>
-      <c r="F10">
-        <v>194677</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="C11" s="32" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="D11">
-        <v>244833</v>
-      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="24">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="24"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="24"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="10"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="10"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="10"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="10"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="30"/>
+      <c r="E10" s="31"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="30"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="10"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="B25" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="C25" s="34" t="s">
-        <v>121</v>
-      </c>
+      <c r="A25" s="23"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="32"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="B26" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="C26" s="34" t="s">
-        <v>120</v>
-      </c>
+      <c r="A26" s="23"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="32"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="C27" s="34" t="s">
-        <v>124</v>
-      </c>
+      <c r="A27" s="23"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added the actual price calculator improved
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13965" windowHeight="5625" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13965" windowHeight="5625" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="PaidTillDate" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="155">
   <si>
     <t>Date</t>
   </si>
@@ -471,9 +471,6 @@
   </si>
   <si>
     <t>Stamp Duty Total</t>
-  </si>
-  <si>
-    <t> 0.0002</t>
   </si>
   <si>
     <t>Actual Price Bought</t>
@@ -624,7 +621,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -666,6 +663,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6162,8 +6160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7710,7 +7708,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8153,8 +8151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8170,13 +8168,13 @@
         <v>135</v>
       </c>
       <c r="B2" s="5">
-        <v>287.7</v>
+        <v>36.5</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E2" s="5">
-        <v>300</v>
+        <v>41.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -8199,14 +8197,14 @@
       </c>
       <c r="B4" s="5">
         <f>B2*B3</f>
-        <v>1.4384999999999999</v>
+        <v>0.1825</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>137</v>
       </c>
       <c r="E4" s="5">
         <f>E2*E3</f>
-        <v>1.5</v>
+        <v>0.20750000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -8229,14 +8227,14 @@
       </c>
       <c r="B6" s="5">
         <f>B4*B5</f>
-        <v>1.4384999999999999</v>
+        <v>0.1825</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>139</v>
       </c>
       <c r="E6" s="5">
         <f>E4*E5</f>
-        <v>1.5</v>
+        <v>0.20750000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -8245,14 +8243,14 @@
       </c>
       <c r="B7" s="5">
         <f>B2+B4</f>
-        <v>289.13849999999996</v>
+        <v>36.682499999999997</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>140</v>
       </c>
       <c r="E7" s="5">
         <f>E2-E4</f>
-        <v>298.5</v>
+        <v>41.292499999999997</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -8260,15 +8258,15 @@
         <v>144</v>
       </c>
       <c r="B8" s="5">
-        <f>B7*B5</f>
-        <v>289.13849999999996</v>
+        <f>ROUND(B7*B5,2)</f>
+        <v>36.68</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>144</v>
       </c>
       <c r="E8" s="5">
-        <f>E7*E5</f>
-        <v>298.5</v>
+        <f>ROUND(E7*E5,2)</f>
+        <v>41.29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -8291,14 +8289,14 @@
       </c>
       <c r="B10" s="5">
         <f>B9*B6</f>
-        <v>0.25892999999999999</v>
+        <v>3.2849999999999997E-2</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>143</v>
       </c>
       <c r="E10" s="5">
         <f>E9*E6</f>
-        <v>0.27</v>
+        <v>3.7350000000000001E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -8321,14 +8319,14 @@
       </c>
       <c r="B12" s="5">
         <f>B11*B8</f>
-        <v>0.28913849999999996</v>
+        <v>3.6679999999999997E-2</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>146</v>
       </c>
       <c r="E12" s="5">
         <f>E11*E8</f>
-        <v>0.29849999999999999</v>
+        <v>4.129E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -8351,28 +8349,28 @@
       </c>
       <c r="B14" s="5">
         <f>B13*B8</f>
-        <v>9.3970012499999984E-3</v>
+        <v>1.1921E-3</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>148</v>
       </c>
       <c r="E14" s="5">
         <f>E13*E8</f>
-        <v>9.7012499999999998E-3</v>
+        <v>1.3419249999999999E-3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="B15" s="34" t="s">
-        <v>151</v>
+      <c r="B15" s="35">
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="D15" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="E15" s="34" t="s">
-        <v>151</v>
+      <c r="E15" s="35">
+        <v>2.0000000000000001E-4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -8380,45 +8378,47 @@
         <v>150</v>
       </c>
       <c r="B16" s="5">
-        <v>0.3</v>
+        <f>B8*B15</f>
+        <v>7.3360000000000005E-3</v>
       </c>
       <c r="D16" s="34" t="s">
         <v>150</v>
       </c>
       <c r="E16" s="5">
-        <v>0.3</v>
+        <f>E8*E15</f>
+        <v>8.2579999999999997E-3</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B17" s="5">
         <f>B10+B12+B14+B16</f>
-        <v>0.85746550124999987</v>
+        <v>7.8058099999999991E-2</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E17" s="5">
         <f>E10+E12+E14+E16</f>
-        <v>0.87820125000000004</v>
+        <v>8.8239924999999997E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B18" s="5">
         <f>B8+B17</f>
-        <v>289.99596550124994</v>
+        <v>36.7580581</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E18" s="5">
         <f>E8-E17</f>
-        <v>297.62179874999998</v>
+        <v>41.201760074999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality to read the stocks from properties file
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13965" windowHeight="5625" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13965" windowHeight="5625" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PaidTillDate" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="163">
   <si>
     <t>Date</t>
   </si>
@@ -501,6 +501,12 @@
   </si>
   <si>
     <t>RELIANCE</t>
+  </si>
+  <si>
+    <t>IDEA</t>
+  </si>
+  <si>
+    <t>BHARTIARTL</t>
   </si>
 </sst>
 </file>
@@ -6177,10 +6183,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28:N29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6278,7 +6284,7 @@
         <v>44.35</v>
       </c>
       <c r="N2" s="5">
-        <v>44.15</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -6322,7 +6328,7 @@
         <v>65.599999999999994</v>
       </c>
       <c r="N3" s="5">
-        <v>65.349999999999994</v>
+        <v>66.900000000000006</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -6366,7 +6372,7 @@
         <v>255.4</v>
       </c>
       <c r="N4" s="5">
-        <v>261</v>
+        <v>262.5</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -6410,7 +6416,7 @@
         <v>70</v>
       </c>
       <c r="N5" s="5">
-        <v>70.900000000000006</v>
+        <v>70.75</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -6454,7 +6460,7 @@
         <v>95.15</v>
       </c>
       <c r="N6" s="5">
-        <v>92.85</v>
+        <v>91.65</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -6498,7 +6504,7 @@
         <v>105.85</v>
       </c>
       <c r="N7" s="5">
-        <v>104.3</v>
+        <v>102.9</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -6542,7 +6548,7 @@
         <v>123.7</v>
       </c>
       <c r="N8" s="5">
-        <v>123.55</v>
+        <v>122.8</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -6586,7 +6592,7 @@
         <v>146.30000000000001</v>
       </c>
       <c r="N9" s="5">
-        <v>145.65</v>
+        <v>144.9</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -6630,7 +6636,7 @@
         <v>126.9</v>
       </c>
       <c r="N10" s="5">
-        <v>128.80000000000001</v>
+        <v>128.55000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -6674,7 +6680,7 @@
         <v>744.85</v>
       </c>
       <c r="N11" s="5">
-        <v>743.9</v>
+        <v>719.5</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -6718,7 +6724,7 @@
         <v>140.80000000000001</v>
       </c>
       <c r="N12" s="5">
-        <v>139.65</v>
+        <v>136.75</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -6762,7 +6768,7 @@
         <v>17.850000000000001</v>
       </c>
       <c r="N13" s="5">
-        <v>17.850000000000001</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -6806,7 +6812,7 @@
         <v>83</v>
       </c>
       <c r="N14" s="5">
-        <v>83.1</v>
+        <v>83.3</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -6850,7 +6856,7 @@
         <v>53</v>
       </c>
       <c r="N15" s="5">
-        <v>53.5</v>
+        <v>55.15</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -6894,7 +6900,7 @@
         <v>34.35</v>
       </c>
       <c r="N16" s="5">
-        <v>35.450000000000003</v>
+        <v>33.799999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -6938,7 +6944,7 @@
         <v>62.9</v>
       </c>
       <c r="N17" s="5">
-        <v>62.55</v>
+        <v>62.4</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -6982,7 +6988,7 @@
         <v>26.25</v>
       </c>
       <c r="N18" s="5">
-        <v>27.75</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -7066,7 +7072,7 @@
         <v>621.20000000000005</v>
       </c>
       <c r="N20" s="5">
-        <v>624.54999999999995</v>
+        <v>613</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -7108,7 +7114,7 @@
         <v>59</v>
       </c>
       <c r="N21" s="5">
-        <v>59.25</v>
+        <v>58.35</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -7150,7 +7156,7 @@
         <v>37.6</v>
       </c>
       <c r="N22" s="5">
-        <v>37.25</v>
+        <v>37.450000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -7192,7 +7198,7 @@
         <v>557.35</v>
       </c>
       <c r="N23" s="5">
-        <v>553.25</v>
+        <v>552.20000000000005</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -7234,7 +7240,7 @@
         <v>290</v>
       </c>
       <c r="N24" s="5">
-        <v>289.2</v>
+        <v>288.5</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -7276,7 +7282,7 @@
         <v>536</v>
       </c>
       <c r="N25" s="5">
-        <v>547</v>
+        <v>537</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -7318,7 +7324,7 @@
         <v>177</v>
       </c>
       <c r="N26" s="5">
-        <v>184.7</v>
+        <v>180.5</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -7344,7 +7350,7 @@
         <v>449.4</v>
       </c>
       <c r="N27" s="5">
-        <v>442.85</v>
+        <v>438.5</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -7366,7 +7372,7 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5">
-        <v>748</v>
+        <v>744.65</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -7388,7 +7394,29 @@
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="36">
-        <v>1582.65</v>
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5">
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -7933,8 +7961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7976,7 +8004,7 @@
       </c>
       <c r="I1">
         <f>SUM(H2:H200)</f>
-        <v>126</v>
+        <v>172.20000000000005</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8035,6 +8063,12 @@
         <f t="shared" ref="H3:H5" si="2">G3-D3</f>
         <v>120</v>
       </c>
+      <c r="J3">
+        <v>172</v>
+      </c>
+      <c r="K3" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -8050,13 +8084,20 @@
         <f t="shared" si="0"/>
         <v>374</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="E4" s="5">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="F4" s="5">
+        <v>11</v>
+      </c>
       <c r="G4" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H4" s="5"/>
+        <v>420.20000000000005</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" si="2"/>
+        <v>46.200000000000045</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -8124,7 +8165,9 @@
         <v>184.2</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5">
+        <v>2</v>
+      </c>
       <c r="G7" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8136,14 +8179,14 @@
         <v>156</v>
       </c>
       <c r="B8" s="5">
-        <v>770</v>
+        <v>762</v>
       </c>
       <c r="C8" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" ref="D8:D17" si="3">B8*C8</f>
-        <v>770</v>
+        <v>1524</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -8176,12 +8219,18 @@
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="A10" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="5">
+        <v>90.2</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
       <c r="D10" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>90.2</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -8192,12 +8241,18 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="5">
+        <v>410.1</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
       <c r="D11" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>410.1</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>

</xml_diff>

<commit_message>
Updated the sheet for 31072017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="170">
   <si>
     <t>Date</t>
   </si>
@@ -526,6 +526,9 @@
   </si>
   <si>
     <t>28/07/2017</t>
+  </si>
+  <si>
+    <t>31/07/2017</t>
   </si>
 </sst>
 </file>
@@ -6188,8 +6191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6198,7 +6201,7 @@
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -6226,7 +6229,9 @@
       <c r="H1" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="I1" s="31"/>
+      <c r="I1" s="30" t="s">
+        <v>169</v>
+      </c>
       <c r="J1" s="31"/>
       <c r="K1" s="31"/>
       <c r="L1" s="31"/>
@@ -6256,7 +6261,9 @@
       <c r="H2" s="31">
         <v>45.25</v>
       </c>
-      <c r="I2" s="31"/>
+      <c r="I2" s="31">
+        <v>45.15</v>
+      </c>
       <c r="J2" s="31"/>
       <c r="K2" s="31"/>
       <c r="L2" s="31"/>
@@ -6286,7 +6293,9 @@
       <c r="H3" s="31">
         <v>72</v>
       </c>
-      <c r="I3" s="31"/>
+      <c r="I3" s="31">
+        <v>70</v>
+      </c>
       <c r="J3" s="31"/>
       <c r="K3" s="31"/>
       <c r="L3" s="31"/>
@@ -6316,7 +6325,9 @@
       <c r="H4" s="31">
         <v>251.1</v>
       </c>
-      <c r="I4" s="31"/>
+      <c r="I4" s="31">
+        <v>249.65</v>
+      </c>
       <c r="J4" s="31"/>
       <c r="K4" s="31"/>
       <c r="L4" s="31"/>
@@ -6346,7 +6357,9 @@
       <c r="H5" s="31">
         <v>69.45</v>
       </c>
-      <c r="I5" s="31"/>
+      <c r="I5" s="31">
+        <v>70</v>
+      </c>
       <c r="J5" s="31"/>
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
@@ -6376,7 +6389,9 @@
       <c r="H6" s="31">
         <v>95.4</v>
       </c>
-      <c r="I6" s="31"/>
+      <c r="I6" s="31">
+        <v>92.35</v>
+      </c>
       <c r="J6" s="31"/>
       <c r="K6" s="31"/>
       <c r="L6" s="31"/>
@@ -6406,7 +6421,9 @@
       <c r="H7" s="31">
         <v>109.45</v>
       </c>
-      <c r="I7" s="31"/>
+      <c r="I7" s="31">
+        <v>109.15</v>
+      </c>
       <c r="J7" s="31"/>
       <c r="K7" s="31"/>
       <c r="L7" s="31"/>
@@ -6436,7 +6453,9 @@
       <c r="H8" s="31">
         <v>122.5</v>
       </c>
-      <c r="I8" s="31"/>
+      <c r="I8" s="31">
+        <v>126.6</v>
+      </c>
       <c r="J8" s="31"/>
       <c r="K8" s="31"/>
       <c r="L8" s="31"/>
@@ -6466,7 +6485,9 @@
       <c r="H9" s="31">
         <v>143.75</v>
       </c>
-      <c r="I9" s="31"/>
+      <c r="I9" s="31">
+        <v>144.80000000000001</v>
+      </c>
       <c r="J9" s="31"/>
       <c r="K9" s="31"/>
       <c r="L9" s="31"/>
@@ -6496,7 +6517,9 @@
       <c r="H10" s="31">
         <v>123.75</v>
       </c>
-      <c r="I10" s="31"/>
+      <c r="I10" s="31">
+        <v>124.5</v>
+      </c>
       <c r="J10" s="31"/>
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
@@ -6526,7 +6549,9 @@
       <c r="H11" s="31">
         <v>675</v>
       </c>
-      <c r="I11" s="31"/>
+      <c r="I11" s="31">
+        <v>672.95</v>
+      </c>
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
       <c r="L11" s="31"/>
@@ -6556,7 +6581,9 @@
       <c r="H12" s="31">
         <v>149.80000000000001</v>
       </c>
-      <c r="I12" s="31"/>
+      <c r="I12" s="31">
+        <v>152.94999999999999</v>
+      </c>
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
       <c r="L12" s="31"/>
@@ -6586,7 +6613,9 @@
       <c r="H13" s="31">
         <v>18.95</v>
       </c>
-      <c r="I13" s="31"/>
+      <c r="I13" s="31">
+        <v>18.75</v>
+      </c>
       <c r="J13" s="31"/>
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
@@ -6616,7 +6645,9 @@
       <c r="H14" s="31">
         <v>82.55</v>
       </c>
-      <c r="I14" s="31"/>
+      <c r="I14" s="31">
+        <v>82</v>
+      </c>
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
       <c r="L14" s="31"/>
@@ -6646,7 +6677,9 @@
       <c r="H15" s="31">
         <v>57.15</v>
       </c>
-      <c r="I15" s="31"/>
+      <c r="I15" s="31">
+        <v>55.55</v>
+      </c>
       <c r="J15" s="31"/>
       <c r="K15" s="31"/>
       <c r="L15" s="31"/>
@@ -6676,7 +6709,9 @@
       <c r="H16" s="31">
         <v>33</v>
       </c>
-      <c r="I16" s="31"/>
+      <c r="I16" s="31">
+        <v>32.5</v>
+      </c>
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
       <c r="L16" s="31"/>
@@ -6706,7 +6741,9 @@
       <c r="H17" s="31">
         <v>62.6</v>
       </c>
-      <c r="I17" s="31"/>
+      <c r="I17" s="31">
+        <v>63.3</v>
+      </c>
       <c r="J17" s="31"/>
       <c r="K17" s="31"/>
       <c r="L17" s="31"/>
@@ -6736,7 +6773,9 @@
       <c r="H18" s="31">
         <v>27.05</v>
       </c>
-      <c r="I18" s="31"/>
+      <c r="I18" s="31">
+        <v>27</v>
+      </c>
       <c r="J18" s="31"/>
       <c r="K18" s="31"/>
       <c r="L18" s="31"/>
@@ -6766,7 +6805,9 @@
       <c r="H19" s="31">
         <v>24.85</v>
       </c>
-      <c r="I19" s="31"/>
+      <c r="I19" s="31">
+        <v>24.7</v>
+      </c>
       <c r="J19" s="31"/>
       <c r="K19" s="31"/>
       <c r="L19" s="31"/>
@@ -6796,7 +6837,9 @@
       <c r="H20" s="31">
         <v>595.95000000000005</v>
       </c>
-      <c r="I20" s="31"/>
+      <c r="I20" s="31">
+        <v>599</v>
+      </c>
       <c r="J20" s="31"/>
       <c r="K20" s="31"/>
       <c r="L20" s="31"/>
@@ -6826,7 +6869,9 @@
       <c r="H21" s="31">
         <v>59.5</v>
       </c>
-      <c r="I21" s="31"/>
+      <c r="I21" s="31">
+        <v>58.7</v>
+      </c>
       <c r="J21" s="31"/>
       <c r="K21" s="31"/>
       <c r="L21" s="31"/>
@@ -6856,7 +6901,9 @@
       <c r="H22" s="31">
         <v>36.200000000000003</v>
       </c>
-      <c r="I22" s="31"/>
+      <c r="I22" s="31">
+        <v>37.25</v>
+      </c>
       <c r="J22" s="31"/>
       <c r="K22" s="31"/>
       <c r="L22" s="31"/>
@@ -6886,7 +6933,9 @@
       <c r="H23" s="31">
         <v>552</v>
       </c>
-      <c r="I23" s="31"/>
+      <c r="I23" s="31">
+        <v>567.6</v>
+      </c>
       <c r="J23" s="31"/>
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
@@ -6916,7 +6965,9 @@
       <c r="H24" s="31">
         <v>290.35000000000002</v>
       </c>
-      <c r="I24" s="31"/>
+      <c r="I24" s="31">
+        <v>285.25</v>
+      </c>
       <c r="J24" s="31"/>
       <c r="K24" s="31"/>
       <c r="L24" s="31"/>
@@ -6946,7 +6997,9 @@
       <c r="H25" s="31">
         <v>503.55</v>
       </c>
-      <c r="I25" s="31"/>
+      <c r="I25" s="31">
+        <v>501.4</v>
+      </c>
       <c r="J25" s="31"/>
       <c r="K25" s="31"/>
       <c r="L25" s="31"/>
@@ -6976,7 +7029,9 @@
       <c r="H26" s="31">
         <v>195.2</v>
       </c>
-      <c r="I26" s="31"/>
+      <c r="I26" s="31">
+        <v>190.05</v>
+      </c>
       <c r="J26" s="31"/>
       <c r="K26" s="31"/>
       <c r="L26" s="31"/>
@@ -7004,7 +7059,9 @@
       <c r="H27" s="31">
         <v>453</v>
       </c>
-      <c r="I27" s="31"/>
+      <c r="I27" s="31">
+        <v>440.7</v>
+      </c>
       <c r="J27" s="31"/>
       <c r="K27" s="31"/>
       <c r="L27" s="31"/>
@@ -7032,7 +7089,9 @@
       <c r="H28" s="31">
         <v>724.95</v>
       </c>
-      <c r="I28" s="31"/>
+      <c r="I28" s="31">
+        <v>718.65</v>
+      </c>
       <c r="J28" s="31"/>
       <c r="K28" s="31"/>
       <c r="L28" s="31"/>
@@ -7060,7 +7119,9 @@
       <c r="H29" s="34">
         <v>1594</v>
       </c>
-      <c r="I29" s="31"/>
+      <c r="I29" s="34">
+        <v>1615.45</v>
+      </c>
       <c r="J29" s="31"/>
       <c r="K29" s="31"/>
       <c r="L29" s="31"/>
@@ -7088,7 +7149,9 @@
       <c r="H30" s="31">
         <v>412.95</v>
       </c>
-      <c r="I30" s="31"/>
+      <c r="I30" s="31">
+        <v>420</v>
+      </c>
       <c r="J30" s="31"/>
       <c r="K30" s="31"/>
       <c r="L30" s="31"/>
@@ -7114,7 +7177,9 @@
       <c r="H31" s="31">
         <v>124.3</v>
       </c>
-      <c r="I31" s="31"/>
+      <c r="I31" s="31">
+        <v>123.75</v>
+      </c>
       <c r="J31" s="31"/>
       <c r="K31" s="31"/>
       <c r="L31" s="31"/>
@@ -7662,7 +7727,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:D7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7704,7 +7769,7 @@
       </c>
       <c r="I1">
         <f>SUM(H2:H200)</f>
-        <v>180.10000000000002</v>
+        <v>297.70000000000039</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7715,11 +7780,11 @@
         <v>296</v>
       </c>
       <c r="C2" s="5">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D2" s="5">
         <f t="shared" ref="D2:D7" si="0">B2*C2</f>
-        <v>10064</v>
+        <v>10656</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -7760,7 +7825,7 @@
         <v>2160</v>
       </c>
       <c r="H3" s="5">
-        <f t="shared" ref="H3:H5" si="2">G3-D3</f>
+        <f t="shared" ref="H3:H4" si="2">G3-D3</f>
         <v>120</v>
       </c>
       <c r="J3">
@@ -7830,8 +7895,14 @@
         <v>82</v>
       </c>
       <c r="H5" s="5">
-        <f t="shared" si="2"/>
+        <f>G5-D5</f>
         <v>6</v>
+      </c>
+      <c r="J5">
+        <v>298</v>
+      </c>
+      <c r="K5" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7971,7 +8042,7 @@
         <v>418</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" ref="H11" si="4">G11-D11</f>
+        <f t="shared" ref="H11:H12" si="4">G11-D11</f>
         <v>7.8999999999999773</v>
       </c>
     </row>
@@ -7989,13 +8060,20 @@
         <f t="shared" si="3"/>
         <v>4235</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="E12" s="5">
+        <v>124.36</v>
+      </c>
+      <c r="F12" s="5">
+        <v>35</v>
+      </c>
       <c r="G12" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="5"/>
+        <v>4352.6000000000004</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" si="4"/>
+        <v>117.60000000000036</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -8027,11 +8105,11 @@
         <v>34.25</v>
       </c>
       <c r="C14" s="5">
-        <v>110</v>
+        <v>170</v>
       </c>
       <c r="D14" s="5">
         <f t="shared" si="3"/>
-        <v>3767.5</v>
+        <v>5822.5</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>

</xml_diff>

<commit_message>
Updated the sheet for 01082017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="156">
   <si>
     <t>Date</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Reliance power</t>
   </si>
   <si>
-    <t xml:space="preserve">Jsw energy </t>
-  </si>
-  <si>
     <t xml:space="preserve">Coal India </t>
   </si>
   <si>
@@ -75,24 +72,9 @@
     <t xml:space="preserve">Idea </t>
   </si>
   <si>
-    <t xml:space="preserve">Ashok Leyland </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMDC Ltd </t>
-  </si>
-  <si>
     <t xml:space="preserve">BHEL </t>
   </si>
   <si>
-    <t xml:space="preserve">PFC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Divis Lab </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jindal Steel </t>
-  </si>
-  <si>
     <t xml:space="preserve">GMR </t>
   </si>
   <si>
@@ -108,18 +90,6 @@
     <t xml:space="preserve">Sail </t>
   </si>
   <si>
-    <t xml:space="preserve">IFCI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Videocon Industries </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hindustan Composite </t>
-  </si>
-  <si>
-    <t xml:space="preserve">idfc </t>
-  </si>
-  <si>
     <t>sintex</t>
   </si>
   <si>
@@ -138,9 +108,6 @@
     <t>RPOWER</t>
   </si>
   <si>
-    <t xml:space="preserve">JSWENERGY </t>
-  </si>
-  <si>
     <t xml:space="preserve">COALINDIA </t>
   </si>
   <si>
@@ -150,21 +117,9 @@
     <t xml:space="preserve">IDEA </t>
   </si>
   <si>
-    <t xml:space="preserve">ASHOKLEY </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMDC </t>
-  </si>
-  <si>
     <t>BHEL </t>
   </si>
   <si>
-    <t>DIVISLAB</t>
-  </si>
-  <si>
-    <t>JINDALSTEL </t>
-  </si>
-  <si>
     <t>GMRINFRA </t>
   </si>
   <si>
@@ -180,18 +135,6 @@
     <t>SAIL </t>
   </si>
   <si>
-    <t>IFCI </t>
-  </si>
-  <si>
-    <t>VIDEOIND </t>
-  </si>
-  <si>
-    <t>HINDCOMPOS </t>
-  </si>
-  <si>
-    <t>IDFC </t>
-  </si>
-  <si>
     <t>SINTEX </t>
   </si>
   <si>
@@ -529,6 +472,21 @@
   </si>
   <si>
     <t>31/07/2017</t>
+  </si>
+  <si>
+    <t>CENTRALBK</t>
+  </si>
+  <si>
+    <t>SBI</t>
+  </si>
+  <si>
+    <t>ICICI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICICIBANK </t>
+  </si>
+  <si>
+    <t>SBIN</t>
   </si>
 </sst>
 </file>
@@ -6189,10 +6147,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+      <selection activeCell="J2" sqref="J2:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6202,46 +6160,50 @@
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C1" s="14">
         <v>42921</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="J1" s="31"/>
+        <v>150</v>
+      </c>
+      <c r="J1" s="14">
+        <v>42743</v>
+      </c>
       <c r="K1" s="31"/>
       <c r="L1" s="31"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C2" s="5">
         <v>42.45</v>
@@ -6264,927 +6226,681 @@
       <c r="I2" s="31">
         <v>45.15</v>
       </c>
-      <c r="J2" s="31"/>
+      <c r="J2" s="31">
+        <v>44.25</v>
+      </c>
       <c r="K2" s="31"/>
       <c r="L2" s="31"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C3" s="5">
-        <v>67.599999999999994</v>
+        <v>247.3</v>
       </c>
       <c r="D3" s="5">
-        <v>66.900000000000006</v>
+        <v>262.5</v>
       </c>
       <c r="E3" s="5">
-        <v>66.55</v>
+        <v>258.39999999999998</v>
       </c>
       <c r="F3" s="5">
-        <v>68</v>
+        <v>260.5</v>
       </c>
       <c r="G3" s="31">
-        <v>67.5</v>
+        <v>255.5</v>
       </c>
       <c r="H3" s="31">
-        <v>72</v>
+        <v>251.1</v>
       </c>
       <c r="I3" s="31">
-        <v>70</v>
-      </c>
-      <c r="J3" s="31"/>
+        <v>249.65</v>
+      </c>
+      <c r="J3" s="31">
+        <v>251.8</v>
+      </c>
       <c r="K3" s="31"/>
       <c r="L3" s="31"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C4" s="5">
-        <v>247.3</v>
+        <v>67.3</v>
       </c>
       <c r="D4" s="5">
-        <v>262.5</v>
+        <v>70.75</v>
       </c>
       <c r="E4" s="5">
-        <v>258.39999999999998</v>
+        <v>70.400000000000006</v>
       </c>
       <c r="F4" s="5">
-        <v>260.5</v>
+        <v>70.95</v>
       </c>
       <c r="G4" s="31">
-        <v>255.5</v>
+        <v>70.150000000000006</v>
       </c>
       <c r="H4" s="31">
-        <v>251.1</v>
+        <v>69.45</v>
       </c>
       <c r="I4" s="31">
-        <v>249.65</v>
-      </c>
-      <c r="J4" s="31"/>
+        <v>70</v>
+      </c>
+      <c r="J4" s="31">
+        <v>70</v>
+      </c>
       <c r="K4" s="31"/>
       <c r="L4" s="31"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C5" s="5">
-        <v>67.3</v>
+        <v>83.3</v>
       </c>
       <c r="D5" s="5">
-        <v>70.75</v>
+        <v>91.65</v>
       </c>
       <c r="E5" s="5">
-        <v>70.400000000000006</v>
+        <v>96.9</v>
       </c>
       <c r="F5" s="5">
-        <v>70.95</v>
+        <v>95.5</v>
       </c>
       <c r="G5" s="31">
-        <v>70.150000000000006</v>
+        <v>92.35</v>
       </c>
       <c r="H5" s="31">
-        <v>69.45</v>
+        <v>95.4</v>
       </c>
       <c r="I5" s="31">
-        <v>70</v>
-      </c>
-      <c r="J5" s="31"/>
+        <v>92.35</v>
+      </c>
+      <c r="J5" s="31">
+        <v>92.3</v>
+      </c>
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C6" s="5">
-        <v>83.3</v>
+        <v>134.15</v>
       </c>
       <c r="D6" s="5">
-        <v>91.65</v>
+        <v>144.9</v>
       </c>
       <c r="E6" s="5">
-        <v>96.9</v>
+        <v>145.4</v>
       </c>
       <c r="F6" s="5">
-        <v>95.5</v>
+        <v>143.94999999999999</v>
       </c>
       <c r="G6" s="31">
-        <v>92.35</v>
+        <v>142.5</v>
       </c>
       <c r="H6" s="31">
-        <v>95.4</v>
+        <v>143.75</v>
       </c>
       <c r="I6" s="31">
-        <v>92.35</v>
-      </c>
-      <c r="J6" s="31"/>
+        <v>144.80000000000001</v>
+      </c>
+      <c r="J6" s="31">
+        <v>144.35</v>
+      </c>
       <c r="K6" s="31"/>
       <c r="L6" s="31"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C7" s="5">
-        <v>102.05</v>
+        <v>18.95</v>
       </c>
       <c r="D7" s="5">
-        <v>102.9</v>
+        <v>18</v>
       </c>
       <c r="E7" s="5">
-        <v>105.1</v>
+        <v>18.75</v>
       </c>
       <c r="F7" s="5">
-        <v>106.1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="G7" s="31">
-        <v>105.35</v>
+        <v>19.350000000000001</v>
       </c>
       <c r="H7" s="31">
-        <v>109.45</v>
+        <v>18.95</v>
       </c>
       <c r="I7" s="31">
-        <v>109.15</v>
-      </c>
-      <c r="J7" s="31"/>
+        <v>18.75</v>
+      </c>
+      <c r="J7" s="31">
+        <v>18.7</v>
+      </c>
       <c r="K7" s="31"/>
       <c r="L7" s="31"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C8" s="5">
-        <v>111.1</v>
+        <v>81.650000000000006</v>
       </c>
       <c r="D8" s="5">
-        <v>122.8</v>
+        <v>83.3</v>
       </c>
       <c r="E8" s="5">
-        <v>121.3</v>
+        <v>82.95</v>
       </c>
       <c r="F8" s="5">
-        <v>124</v>
+        <v>82.55</v>
       </c>
       <c r="G8" s="31">
-        <v>122.5</v>
+        <v>82.1</v>
       </c>
       <c r="H8" s="31">
-        <v>122.5</v>
+        <v>82.55</v>
       </c>
       <c r="I8" s="31">
-        <v>126.6</v>
-      </c>
-      <c r="J8" s="31"/>
+        <v>82</v>
+      </c>
+      <c r="J8" s="31">
+        <v>83.25</v>
+      </c>
       <c r="K8" s="31"/>
       <c r="L8" s="31"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C9" s="5">
-        <v>134.15</v>
+        <v>52.8</v>
       </c>
       <c r="D9" s="5">
-        <v>144.9</v>
+        <v>55.15</v>
       </c>
       <c r="E9" s="5">
-        <v>145.4</v>
+        <v>58.1</v>
       </c>
       <c r="F9" s="5">
-        <v>143.94999999999999</v>
+        <v>58.7</v>
       </c>
       <c r="G9" s="31">
-        <v>142.5</v>
+        <v>56.45</v>
       </c>
       <c r="H9" s="31">
-        <v>143.75</v>
+        <v>57.15</v>
       </c>
       <c r="I9" s="31">
-        <v>144.80000000000001</v>
-      </c>
-      <c r="J9" s="31"/>
+        <v>55.55</v>
+      </c>
+      <c r="J9" s="31">
+        <v>55.3</v>
+      </c>
       <c r="K9" s="31"/>
       <c r="L9" s="31"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C10" s="5">
-        <v>124</v>
+        <v>36.35</v>
       </c>
       <c r="D10" s="5">
-        <v>128.55000000000001</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="E10" s="5">
-        <v>124.6</v>
+        <v>32.9</v>
       </c>
       <c r="F10" s="5">
-        <v>123.1</v>
+        <v>34.4</v>
       </c>
       <c r="G10" s="31">
-        <v>121.85</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="H10" s="31">
-        <v>123.75</v>
+        <v>33</v>
       </c>
       <c r="I10" s="31">
-        <v>124.5</v>
-      </c>
-      <c r="J10" s="31"/>
+        <v>32.5</v>
+      </c>
+      <c r="J10" s="31">
+        <v>32.6</v>
+      </c>
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C11" s="5">
-        <v>657.75</v>
+        <v>59.8</v>
       </c>
       <c r="D11" s="5">
-        <v>719.5</v>
+        <v>62.4</v>
       </c>
       <c r="E11" s="5">
-        <v>676.5</v>
+        <v>63.4</v>
       </c>
       <c r="F11" s="5">
-        <v>680.4</v>
+        <v>64</v>
       </c>
       <c r="G11" s="31">
-        <v>660</v>
+        <v>63.3</v>
       </c>
       <c r="H11" s="31">
-        <v>675</v>
+        <v>62.6</v>
       </c>
       <c r="I11" s="31">
-        <v>672.95</v>
-      </c>
-      <c r="J11" s="31"/>
+        <v>63.3</v>
+      </c>
+      <c r="J11" s="31">
+        <v>63.25</v>
+      </c>
       <c r="K11" s="31"/>
       <c r="L11" s="31"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C12" s="5">
-        <v>131.25</v>
+        <v>25.7</v>
       </c>
       <c r="D12" s="5">
-        <v>136.75</v>
+        <v>37.450000000000003</v>
       </c>
       <c r="E12" s="5">
-        <v>140.80000000000001</v>
+        <v>37.049999999999997</v>
       </c>
       <c r="F12" s="5">
-        <v>151.19999999999999</v>
+        <v>36.65</v>
       </c>
       <c r="G12" s="31">
-        <v>152.55000000000001</v>
+        <v>34.85</v>
       </c>
       <c r="H12" s="31">
-        <v>149.80000000000001</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="I12" s="31">
-        <v>152.94999999999999</v>
-      </c>
-      <c r="J12" s="31"/>
+        <v>37.25</v>
+      </c>
+      <c r="J12" s="31">
+        <v>36.25</v>
+      </c>
       <c r="K12" s="31"/>
       <c r="L12" s="31"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>24</v>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C13" s="5">
-        <v>18.95</v>
+        <v>550.29999999999995</v>
       </c>
       <c r="D13" s="5">
-        <v>18</v>
+        <v>552.20000000000005</v>
       </c>
       <c r="E13" s="5">
-        <v>18.75</v>
+        <v>552.79999999999995</v>
       </c>
       <c r="F13" s="5">
-        <v>19.100000000000001</v>
+        <v>566.15</v>
       </c>
       <c r="G13" s="31">
-        <v>19.350000000000001</v>
+        <v>561.04999999999995</v>
       </c>
       <c r="H13" s="31">
-        <v>18.95</v>
+        <v>552</v>
       </c>
       <c r="I13" s="31">
-        <v>18.75</v>
-      </c>
-      <c r="J13" s="31"/>
+        <v>567.6</v>
+      </c>
+      <c r="J13" s="31">
+        <v>570.95000000000005</v>
+      </c>
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>49</v>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C14" s="5">
-        <v>81.650000000000006</v>
+        <v>331.65</v>
       </c>
       <c r="D14" s="5">
-        <v>83.3</v>
+        <v>288.5</v>
       </c>
       <c r="E14" s="5">
-        <v>82.95</v>
+        <v>291.5</v>
       </c>
       <c r="F14" s="5">
-        <v>82.55</v>
+        <v>293.35000000000002</v>
       </c>
       <c r="G14" s="31">
-        <v>82.1</v>
+        <v>291.7</v>
       </c>
       <c r="H14" s="31">
-        <v>82.55</v>
+        <v>290.35000000000002</v>
       </c>
       <c r="I14" s="31">
-        <v>82</v>
-      </c>
-      <c r="J14" s="31"/>
+        <v>285.25</v>
+      </c>
+      <c r="J14" s="31">
+        <v>287.75</v>
+      </c>
       <c r="K14" s="31"/>
       <c r="L14" s="31"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>50</v>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="C15" s="5">
-        <v>52.8</v>
+        <v>483.4</v>
       </c>
       <c r="D15" s="5">
-        <v>55.15</v>
+        <v>537</v>
       </c>
       <c r="E15" s="5">
-        <v>58.1</v>
+        <v>523</v>
       </c>
       <c r="F15" s="5">
-        <v>58.7</v>
+        <v>524.04999999999995</v>
       </c>
       <c r="G15" s="31">
-        <v>56.45</v>
+        <v>515</v>
       </c>
       <c r="H15" s="31">
-        <v>57.15</v>
+        <v>503.55</v>
       </c>
       <c r="I15" s="31">
-        <v>55.55</v>
-      </c>
-      <c r="J15" s="31"/>
+        <v>501.4</v>
+      </c>
+      <c r="J15" s="31">
+        <v>497</v>
+      </c>
       <c r="K15" s="31"/>
       <c r="L15" s="31"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>51</v>
+      <c r="N15" s="11"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="C16" s="5">
-        <v>36.35</v>
+        <v>174.25</v>
       </c>
       <c r="D16" s="5">
-        <v>33.799999999999997</v>
+        <v>180.5</v>
       </c>
       <c r="E16" s="5">
-        <v>32.9</v>
+        <v>189.9</v>
       </c>
       <c r="F16" s="5">
-        <v>34.4</v>
+        <v>196</v>
       </c>
       <c r="G16" s="31">
-        <v>33.200000000000003</v>
+        <v>196.55</v>
       </c>
       <c r="H16" s="31">
-        <v>33</v>
+        <v>195.2</v>
       </c>
       <c r="I16" s="31">
-        <v>32.5</v>
-      </c>
-      <c r="J16" s="31"/>
+        <v>190.05</v>
+      </c>
+      <c r="J16" s="31">
+        <v>195.15</v>
+      </c>
       <c r="K16" s="31"/>
       <c r="L16" s="31"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="5">
-        <v>59.8</v>
-      </c>
+      <c r="A17" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="5"/>
       <c r="D17" s="5">
-        <v>62.4</v>
+        <v>438.5</v>
       </c>
       <c r="E17" s="5">
-        <v>63.4</v>
+        <v>437.4</v>
       </c>
       <c r="F17" s="5">
-        <v>64</v>
+        <v>439</v>
       </c>
       <c r="G17" s="31">
-        <v>63.3</v>
+        <v>450.5</v>
       </c>
       <c r="H17" s="31">
-        <v>62.6</v>
+        <v>453</v>
       </c>
       <c r="I17" s="31">
-        <v>63.3</v>
-      </c>
-      <c r="J17" s="31"/>
+        <v>440.7</v>
+      </c>
+      <c r="J17" s="31">
+        <v>449</v>
+      </c>
       <c r="K17" s="31"/>
       <c r="L17" s="31"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="5">
-        <v>25.55</v>
-      </c>
+      <c r="A18" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="5"/>
       <c r="D18" s="5">
-        <v>27.5</v>
+        <v>744.65</v>
       </c>
       <c r="E18" s="5">
-        <v>27.2</v>
+        <v>751.95</v>
       </c>
       <c r="F18" s="5">
-        <v>26.85</v>
-      </c>
-      <c r="G18" s="31">
-        <v>27.25</v>
+        <v>748.7</v>
+      </c>
+      <c r="G18" s="34">
+        <v>739.1</v>
       </c>
       <c r="H18" s="31">
-        <v>27.05</v>
+        <v>724.95</v>
       </c>
       <c r="I18" s="31">
-        <v>27</v>
-      </c>
-      <c r="J18" s="31"/>
+        <v>718.65</v>
+      </c>
+      <c r="J18" s="31">
+        <v>736</v>
+      </c>
       <c r="K18" s="31"/>
       <c r="L18" s="31"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="5">
-        <v>24.4</v>
-      </c>
-      <c r="D19" s="5">
-        <v>26.55</v>
-      </c>
-      <c r="E19" s="5">
-        <v>24.75</v>
-      </c>
-      <c r="F19" s="5">
-        <v>25.6</v>
-      </c>
-      <c r="G19" s="31">
-        <v>24.9</v>
-      </c>
-      <c r="H19" s="31">
-        <v>24.85</v>
-      </c>
-      <c r="I19" s="31">
-        <v>24.7</v>
-      </c>
-      <c r="J19" s="31"/>
+        <v>138</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="33">
+        <v>1584</v>
+      </c>
+      <c r="E19" s="33">
+        <v>1602.5</v>
+      </c>
+      <c r="F19" s="33">
+        <v>1622.9</v>
+      </c>
+      <c r="G19" s="34">
+        <v>1592.8</v>
+      </c>
+      <c r="H19" s="34">
+        <v>1594</v>
+      </c>
+      <c r="I19" s="34">
+        <v>1615.45</v>
+      </c>
+      <c r="J19" s="34">
+        <v>1605.8</v>
+      </c>
       <c r="K19" s="31"/>
       <c r="L19" s="31"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="5">
-        <v>577.5</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="5"/>
       <c r="D20" s="5">
-        <v>613</v>
+        <v>411</v>
       </c>
       <c r="E20" s="5">
-        <v>611</v>
+        <v>427.5</v>
       </c>
       <c r="F20" s="5">
-        <v>608</v>
+        <v>426.5</v>
       </c>
       <c r="G20" s="31">
-        <v>600</v>
+        <v>414.05</v>
       </c>
       <c r="H20" s="31">
-        <v>595.95000000000005</v>
+        <v>412.95</v>
       </c>
       <c r="I20" s="31">
-        <v>599</v>
-      </c>
-      <c r="J20" s="31"/>
+        <v>420</v>
+      </c>
+      <c r="J20" s="31">
+        <v>419.5</v>
+      </c>
       <c r="K20" s="31"/>
       <c r="L20" s="31"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>32</v>
+      <c r="A21" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="5">
-        <v>60.55</v>
-      </c>
-      <c r="D21" s="5">
-        <v>58.35</v>
-      </c>
-      <c r="E21" s="5">
-        <v>58.4</v>
-      </c>
-      <c r="F21" s="5">
-        <v>58.5</v>
-      </c>
-      <c r="G21" s="31">
-        <v>57.6</v>
-      </c>
-      <c r="H21" s="31">
-        <v>59.5</v>
-      </c>
-      <c r="I21" s="31">
-        <v>58.7</v>
-      </c>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
+        <v>151</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5">
+        <v>89.3</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="5">
-        <v>25.7</v>
-      </c>
-      <c r="D22" s="5">
-        <v>37.450000000000003</v>
-      </c>
-      <c r="E22" s="5">
-        <v>37.049999999999997</v>
-      </c>
-      <c r="F22" s="5">
-        <v>36.65</v>
-      </c>
-      <c r="G22" s="31">
-        <v>34.85</v>
-      </c>
-      <c r="H22" s="31">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="I22" s="31">
-        <v>37.25</v>
-      </c>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
+        <v>152</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5">
+        <v>309.25</v>
+      </c>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="5">
-        <v>550.29999999999995</v>
-      </c>
-      <c r="D23" s="5">
-        <v>552.20000000000005</v>
-      </c>
-      <c r="E23" s="5">
-        <v>552.79999999999995</v>
-      </c>
-      <c r="F23" s="5">
-        <v>566.15</v>
-      </c>
-      <c r="G23" s="31">
-        <v>561.04999999999995</v>
-      </c>
-      <c r="H23" s="31">
-        <v>552</v>
-      </c>
-      <c r="I23" s="31">
-        <v>567.6</v>
-      </c>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="5">
-        <v>331.65</v>
-      </c>
-      <c r="D24" s="5">
-        <v>288.5</v>
-      </c>
-      <c r="E24" s="5">
-        <v>291.5</v>
-      </c>
-      <c r="F24" s="5">
-        <v>293.35000000000002</v>
-      </c>
-      <c r="G24" s="31">
-        <v>291.7</v>
-      </c>
-      <c r="H24" s="31">
-        <v>290.35000000000002</v>
-      </c>
-      <c r="I24" s="31">
-        <v>285.25</v>
-      </c>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="5">
-        <v>483.4</v>
-      </c>
-      <c r="D25" s="5">
-        <v>537</v>
-      </c>
-      <c r="E25" s="5">
-        <v>523</v>
-      </c>
-      <c r="F25" s="5">
-        <v>524.04999999999995</v>
-      </c>
-      <c r="G25" s="31">
-        <v>515</v>
-      </c>
-      <c r="H25" s="31">
-        <v>503.55</v>
-      </c>
-      <c r="I25" s="31">
-        <v>501.4</v>
-      </c>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="5">
-        <v>174.25</v>
-      </c>
-      <c r="D26" s="5">
-        <v>180.5</v>
-      </c>
-      <c r="E26" s="5">
-        <v>189.9</v>
-      </c>
-      <c r="F26" s="5">
-        <v>196</v>
-      </c>
-      <c r="G26" s="31">
-        <v>196.55</v>
-      </c>
-      <c r="H26" s="31">
-        <v>195.2</v>
-      </c>
-      <c r="I26" s="31">
-        <v>190.05</v>
-      </c>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5">
-        <v>438.5</v>
-      </c>
-      <c r="E27" s="5">
-        <v>437.4</v>
-      </c>
-      <c r="F27" s="5">
-        <v>439</v>
-      </c>
-      <c r="G27" s="31">
-        <v>450.5</v>
-      </c>
-      <c r="H27" s="31">
-        <v>453</v>
-      </c>
-      <c r="I27" s="31">
-        <v>440.7</v>
-      </c>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5">
-        <v>744.65</v>
-      </c>
-      <c r="E28" s="5">
-        <v>751.95</v>
-      </c>
-      <c r="F28" s="5">
-        <v>748.7</v>
-      </c>
-      <c r="G28" s="34">
-        <v>739.1</v>
-      </c>
-      <c r="H28" s="31">
-        <v>724.95</v>
-      </c>
-      <c r="I28" s="31">
-        <v>718.65</v>
-      </c>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="33">
-        <v>1584</v>
-      </c>
-      <c r="E29" s="33">
-        <v>1602.5</v>
-      </c>
-      <c r="F29" s="33">
-        <v>1622.9</v>
-      </c>
-      <c r="G29" s="34">
-        <v>1592.8</v>
-      </c>
-      <c r="H29" s="34">
-        <v>1594</v>
-      </c>
-      <c r="I29" s="34">
-        <v>1615.45</v>
-      </c>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5">
-        <v>411</v>
-      </c>
-      <c r="E30" s="5">
-        <v>427.5</v>
-      </c>
-      <c r="F30" s="5">
-        <v>426.5</v>
-      </c>
-      <c r="G30" s="31">
-        <v>414.05</v>
-      </c>
-      <c r="H30" s="31">
-        <v>412.95</v>
-      </c>
-      <c r="I30" s="31">
-        <v>420</v>
-      </c>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5">
-        <v>123.15</v>
-      </c>
-      <c r="F31" s="5">
-        <v>121.05</v>
-      </c>
-      <c r="G31" s="31">
-        <v>122.6</v>
-      </c>
-      <c r="H31" s="31">
-        <v>124.3</v>
-      </c>
-      <c r="I31" s="31">
-        <v>123.75</v>
-      </c>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5">
+        <v>302.7</v>
+      </c>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
     </row>
   </sheetData>
+  <sortState ref="N1:N37">
+    <sortCondition ref="N13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -7221,22 +6937,22 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B1" s="8">
         <v>25000</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="8" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="18"/>
       <c r="G1" s="8" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="J1" s="5">
         <f>SUM(K2:K100)</f>
@@ -7244,51 +6960,51 @@
       </c>
       <c r="K1" s="5"/>
       <c r="M1" s="12" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="N1" s="5">
         <v>112000</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="B2" s="8">
         <v>15000</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="8" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="E2" s="8">
         <v>40000</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="8" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="H2" s="8">
         <v>100000</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="K2" s="5">
         <v>5000</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="N2" s="5">
         <v>3000</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="Q2" s="5">
         <v>5000</v>
@@ -7296,39 +7012,39 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="B3" s="8">
         <v>20000</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="8" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="E3" s="8">
         <v>15000</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="8" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="H3" s="8">
         <v>50000</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="K3" s="5">
         <v>500</v>
       </c>
       <c r="M3" s="28" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="N3" s="29">
         <v>2200</v>
       </c>
       <c r="P3" s="12" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="Q3" s="5">
         <f>Q2/2</f>
@@ -7337,27 +7053,27 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="B4" s="8">
         <v>40000</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="8" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="E4" s="8">
         <v>20000</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="8" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="H4" s="8">
         <v>30000</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="K4" s="5">
         <v>3000</v>
@@ -7370,7 +7086,7 @@
         <v>117200</v>
       </c>
       <c r="P4" s="13" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="Q4" s="5">
         <v>500</v>
@@ -7378,33 +7094,33 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="B5" s="8">
         <v>4139</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="8" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="E5" s="8">
         <v>20000</v>
       </c>
       <c r="F5" s="18"/>
       <c r="G5" s="8" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="H5" s="8">
         <v>50000</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="K5" s="15">
         <v>500</v>
       </c>
       <c r="P5" s="13" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="Q5" s="5">
         <f>Q3*Q4</f>
@@ -7413,40 +7129,40 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B6" s="8">
         <v>6000</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="8" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E6" s="8">
         <v>3000</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="8" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="H6" s="8">
         <v>100000</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="K6" s="15">
         <v>900</v>
       </c>
       <c r="M6" s="21" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="N6" s="17">
         <f>J1-N4</f>
         <v>25150</v>
       </c>
       <c r="P6" s="13" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="Q6" s="5">
         <f>Q5/20</f>
@@ -7455,27 +7171,27 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B7" s="8">
         <v>3000</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="8" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="E7" s="8">
         <v>5000</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="8" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="H7" s="8">
         <v>40000</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="K7" s="15">
         <v>400</v>
@@ -7483,27 +7199,27 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B8" s="8">
         <v>10000</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="8" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="E8" s="8">
         <v>10000</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="8" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="H8" s="8">
         <v>30000</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="K8" s="15">
         <v>400</v>
@@ -7524,13 +7240,13 @@
         <v>113000</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="H9" s="8">
         <v>200000</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="K9" s="15">
         <v>400</v>
@@ -7538,37 +7254,37 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G10" s="8" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="H10" s="8">
         <v>187000</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="K10" s="15">
         <v>3000</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G11" s="8" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="H11" s="8">
         <v>300000</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="K11" s="15">
         <v>1000</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="N11" s="5">
         <v>5000</v>
@@ -7576,19 +7292,19 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G12" s="8" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="H12" s="8">
         <v>250000</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="K12" s="15">
         <v>2000</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="N12" s="5">
         <v>5000</v>
@@ -7602,7 +7318,7 @@
         <v>1337000</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="K13" s="15">
         <v>750</v>
@@ -7611,7 +7327,7 @@
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D14" s="22"/>
       <c r="J14" s="13" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="K14" s="15">
         <v>2000</v>
@@ -7620,7 +7336,7 @@
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D15" s="22"/>
       <c r="J15" s="13" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="K15" s="15">
         <v>13000</v>
@@ -7629,7 +7345,7 @@
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D16" s="22"/>
       <c r="J16" s="13" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="K16" s="15">
         <v>500</v>
@@ -7637,7 +7353,7 @@
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="J17" s="13" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="K17" s="15">
         <v>500</v>
@@ -7645,7 +7361,7 @@
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.25">
       <c r="J18" s="13" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="K18" s="15">
         <v>500</v>
@@ -7653,7 +7369,7 @@
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.25">
       <c r="J19" s="13" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="K19" s="15">
         <v>2000</v>
@@ -7661,7 +7377,7 @@
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.25">
       <c r="J20" s="13" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="K20" s="15">
         <v>6000</v>
@@ -7669,7 +7385,7 @@
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.25">
       <c r="J21" s="13" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="K21" s="15">
         <v>5000</v>
@@ -7677,7 +7393,7 @@
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.25">
       <c r="J22" s="13" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="K22" s="15">
         <v>15000</v>
@@ -7685,7 +7401,7 @@
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.25">
       <c r="J23" s="13" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="K23" s="15">
         <v>20000</v>
@@ -7693,7 +7409,7 @@
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.25">
       <c r="J24" s="13" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="K24" s="15">
         <v>40000</v>
@@ -7701,7 +7417,7 @@
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.25">
       <c r="J25" s="13" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="K25" s="15">
         <v>10000</v>
@@ -7710,7 +7426,7 @@
     <row r="26" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D26" s="21"/>
       <c r="J26" s="13" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K26" s="15">
         <v>10000</v>
@@ -7744,28 +7460,28 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="I1">
         <f>SUM(H2:H200)</f>
@@ -7774,7 +7490,7 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="B2" s="5">
         <v>296</v>
@@ -7797,12 +7513,12 @@
         <v>126</v>
       </c>
       <c r="K2" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="B3" s="5">
         <v>170</v>
@@ -7832,12 +7548,12 @@
         <v>172</v>
       </c>
       <c r="K3" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B4" s="5">
         <v>34</v>
@@ -7867,12 +7583,12 @@
         <v>180</v>
       </c>
       <c r="K4" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="B5" s="5">
         <v>38</v>
@@ -7902,12 +7618,12 @@
         <v>298</v>
       </c>
       <c r="K5" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B6" s="5">
         <v>71.010000000000005</v>
@@ -7929,7 +7645,7 @@
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="B7" s="5">
         <v>92.1</v>
@@ -7953,7 +7669,7 @@
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="B8" s="5">
         <v>762</v>
@@ -7975,7 +7691,7 @@
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="B9" s="5">
         <v>1595</v>
@@ -7997,7 +7713,7 @@
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="B10" s="5">
         <v>90.2</v>
@@ -8019,7 +7735,7 @@
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="B11" s="5">
         <v>410.1</v>
@@ -8048,7 +7764,7 @@
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="B12" s="5">
         <v>121</v>
@@ -8077,7 +7793,7 @@
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="B13" s="5">
         <v>200.25</v>
@@ -8099,7 +7815,7 @@
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="B14" s="5">
         <v>34.25</v>
@@ -8274,13 +7990,13 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="B2" s="5">
         <v>36.5</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="E2" s="5">
         <v>41.5</v>
@@ -8288,13 +8004,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B3" s="5">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="E3" s="5">
         <v>5.0000000000000001E-3</v>
@@ -8302,14 +8018,14 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="B4" s="5">
         <f>B2*B3</f>
         <v>0.1825</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="E4" s="5">
         <f>E2*E3</f>
@@ -8318,13 +8034,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="B5" s="5">
         <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="E5" s="5">
         <v>1</v>
@@ -8332,14 +8048,14 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="B6" s="5">
         <f>B4*B5</f>
         <v>0.1825</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="E6" s="5">
         <f>E4*E5</f>
@@ -8348,14 +8064,14 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="B7" s="5">
         <f>B2+B4</f>
         <v>36.682499999999997</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="E7" s="5">
         <f>E2-E4</f>
@@ -8364,14 +8080,14 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B8" s="5">
         <f>ROUND(B7*B5,2)</f>
         <v>36.68</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="E8" s="5">
         <f>ROUND(E7*E5,2)</f>
@@ -8380,13 +8096,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="B9" s="5">
         <v>0.18</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="E9" s="5">
         <v>0.18</v>
@@ -8394,14 +8110,14 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="B10" s="5">
         <f>B9*B6</f>
         <v>3.2849999999999997E-2</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="E10" s="5">
         <f>E9*E6</f>
@@ -8410,13 +8126,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="B11" s="5">
         <v>1E-3</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="E11" s="5">
         <v>1E-3</v>
@@ -8424,14 +8140,14 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="B12" s="5">
         <f>B11*B8</f>
         <v>3.6679999999999997E-2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="E12" s="5">
         <f>E11*E8</f>
@@ -8440,13 +8156,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="B13" s="5">
         <v>3.2499999999999997E-5</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="E13" s="5">
         <v>3.2499999999999997E-5</v>
@@ -8454,14 +8170,14 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="B14" s="5">
         <f>B13*B8</f>
         <v>1.1921E-3</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="E14" s="5">
         <f>E13*E8</f>
@@ -8470,13 +8186,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="B15" s="32">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="E15" s="32">
         <v>2.0000000000000001E-4</v>
@@ -8484,14 +8200,14 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="B16" s="5">
         <f>B8*B15</f>
         <v>7.3360000000000005E-3</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="E16" s="5">
         <f>E8*E15</f>
@@ -8500,14 +8216,14 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="B17" s="5">
         <f>B10+B12+B14+B16</f>
         <v>7.8058099999999991E-2</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="E17" s="5">
         <f>E10+E12+E14+E16</f>
@@ -8516,14 +8232,14 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B18" s="5">
         <f>B8+B17</f>
         <v>36.7580581</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="E18" s="5">
         <f>E8-E17</f>
@@ -8548,7 +8264,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -8559,7 +8275,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the sheet for 04082017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -13,13 +13,14 @@
     <sheet name="Profit" sheetId="7" r:id="rId4"/>
     <sheet name="Actual Price Calculator" sheetId="8" r:id="rId5"/>
     <sheet name="Spent" sheetId="9" r:id="rId6"/>
+    <sheet name="Papa" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="175">
   <si>
     <t>Date</t>
   </si>
@@ -517,6 +518,33 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>TATAMTRDVR</t>
+  </si>
+  <si>
+    <t>Total Principal</t>
+  </si>
+  <si>
+    <t>Total Paid Till Date</t>
+  </si>
+  <si>
+    <t>Needed to be paid</t>
+  </si>
+  <si>
+    <t>Interest</t>
+  </si>
+  <si>
+    <t>Principal Paid Till Date</t>
+  </si>
+  <si>
+    <t>Interest Paid Till Date</t>
+  </si>
+  <si>
+    <t>To be paid</t>
+  </si>
+  <si>
+    <t>Outstanding Principal</t>
   </si>
 </sst>
 </file>
@@ -526,7 +554,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -578,6 +606,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -643,7 +677,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -690,6 +724,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6188,10 +6226,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H24"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6227,7 +6265,9 @@
       <c r="H1" s="14">
         <v>42802</v>
       </c>
-      <c r="I1" s="31"/>
+      <c r="I1" s="14">
+        <v>42833</v>
+      </c>
       <c r="J1" s="31"/>
       <c r="K1" s="31"/>
       <c r="L1" s="31"/>
@@ -6255,9 +6295,11 @@
         <v>306</v>
       </c>
       <c r="H2" s="5">
-        <v>300.55</v>
-      </c>
-      <c r="I2" s="5"/>
+        <v>300.64999999999998</v>
+      </c>
+      <c r="I2" s="5">
+        <v>305.8</v>
+      </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -6285,9 +6327,11 @@
         <v>301.39999999999998</v>
       </c>
       <c r="H3" s="5">
-        <v>295.95</v>
-      </c>
-      <c r="I3" s="5"/>
+        <v>295.10000000000002</v>
+      </c>
+      <c r="I3" s="5">
+        <v>296.8</v>
+      </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -6321,9 +6365,11 @@
         <v>284.85000000000002</v>
       </c>
       <c r="H4" s="31">
-        <v>281.3</v>
-      </c>
-      <c r="I4" s="31"/>
+        <v>280.89999999999998</v>
+      </c>
+      <c r="I4" s="31">
+        <v>280.8</v>
+      </c>
       <c r="J4" s="31"/>
       <c r="K4" s="31"/>
       <c r="L4" s="31"/>
@@ -6357,9 +6403,11 @@
         <v>1628.55</v>
       </c>
       <c r="H5" s="33">
-        <v>1651.5</v>
-      </c>
-      <c r="I5" s="31"/>
+        <v>1654</v>
+      </c>
+      <c r="I5" s="33">
+        <v>1626.5</v>
+      </c>
       <c r="J5" s="31"/>
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
@@ -6393,9 +6441,11 @@
         <v>251.05</v>
       </c>
       <c r="H6" s="31">
-        <v>241.7</v>
-      </c>
-      <c r="I6" s="31"/>
+        <v>242</v>
+      </c>
+      <c r="I6" s="31">
+        <v>249.2</v>
+      </c>
       <c r="J6" s="31"/>
       <c r="K6" s="31"/>
       <c r="L6" s="31"/>
@@ -6429,9 +6479,11 @@
         <v>18.399999999999999</v>
       </c>
       <c r="H7" s="31">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="I7" s="31"/>
+        <v>17.95</v>
+      </c>
+      <c r="I7" s="31">
+        <v>17.649999999999999</v>
+      </c>
       <c r="J7" s="31"/>
       <c r="K7" s="31"/>
       <c r="L7" s="31"/>
@@ -6465,9 +6517,11 @@
         <v>63.2</v>
       </c>
       <c r="H8" s="31">
-        <v>60.9</v>
-      </c>
-      <c r="I8" s="31"/>
+        <v>60.75</v>
+      </c>
+      <c r="I8" s="31">
+        <v>61.9</v>
+      </c>
       <c r="J8" s="31"/>
       <c r="K8" s="31"/>
       <c r="L8" s="31"/>
@@ -6493,9 +6547,11 @@
         <v>58.2</v>
       </c>
       <c r="H9" s="9">
-        <v>58.05</v>
-      </c>
-      <c r="I9" s="9"/>
+        <v>57.95</v>
+      </c>
+      <c r="I9" s="9">
+        <v>57.25</v>
+      </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
@@ -6529,9 +6585,11 @@
         <v>43.9</v>
       </c>
       <c r="H10" s="31">
-        <v>42.55</v>
-      </c>
-      <c r="I10" s="31"/>
+        <v>42.5</v>
+      </c>
+      <c r="I10" s="31">
+        <v>42.4</v>
+      </c>
       <c r="J10" s="31"/>
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
@@ -6567,7 +6625,9 @@
       <c r="H11" s="31">
         <v>66.5</v>
       </c>
-      <c r="I11" s="31"/>
+      <c r="I11" s="31">
+        <v>69.099999999999994</v>
+      </c>
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
       <c r="L11" s="31"/>
@@ -6601,9 +6661,11 @@
         <v>92.3</v>
       </c>
       <c r="H12" s="31">
-        <v>93.2</v>
-      </c>
-      <c r="I12" s="31"/>
+        <v>93.45</v>
+      </c>
+      <c r="I12" s="31">
+        <v>92.9</v>
+      </c>
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
       <c r="L12" s="31"/>
@@ -6637,9 +6699,11 @@
         <v>140.9</v>
       </c>
       <c r="H13" s="31">
-        <v>138.55000000000001</v>
-      </c>
-      <c r="I13" s="31"/>
+        <v>138.65</v>
+      </c>
+      <c r="I13" s="31">
+        <v>137.1</v>
+      </c>
       <c r="J13" s="31"/>
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
@@ -6673,9 +6737,11 @@
         <v>82.55</v>
       </c>
       <c r="H14" s="31">
-        <v>82.5</v>
-      </c>
-      <c r="I14" s="31"/>
+        <v>82.45</v>
+      </c>
+      <c r="I14" s="31">
+        <v>80.2</v>
+      </c>
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
       <c r="L14" s="31"/>
@@ -6709,9 +6775,11 @@
         <v>54.25</v>
       </c>
       <c r="H15" s="31">
+        <v>53.8</v>
+      </c>
+      <c r="I15" s="31">
         <v>54</v>
       </c>
-      <c r="I15" s="31"/>
       <c r="J15" s="31"/>
       <c r="K15" s="31"/>
       <c r="L15" s="31"/>
@@ -6745,9 +6813,11 @@
         <v>32.799999999999997</v>
       </c>
       <c r="H16" s="31">
-        <v>32</v>
-      </c>
-      <c r="I16" s="31"/>
+        <v>31.95</v>
+      </c>
+      <c r="I16" s="31">
+        <v>32.700000000000003</v>
+      </c>
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
       <c r="L16" s="31"/>
@@ -6775,7 +6845,9 @@
       <c r="H17" s="31">
         <v>34.049999999999997</v>
       </c>
-      <c r="I17" s="31"/>
+      <c r="I17" s="31">
+        <v>33.65</v>
+      </c>
       <c r="J17" s="31"/>
       <c r="K17" s="31"/>
       <c r="L17" s="31"/>
@@ -6809,9 +6881,11 @@
         <v>568.95000000000005</v>
       </c>
       <c r="H18" s="31">
-        <v>559.20000000000005</v>
-      </c>
-      <c r="I18" s="31"/>
+        <v>559.75</v>
+      </c>
+      <c r="I18" s="31">
+        <v>580.79999999999995</v>
+      </c>
       <c r="J18" s="31"/>
       <c r="K18" s="31"/>
       <c r="L18" s="31"/>
@@ -6845,9 +6919,11 @@
         <v>498.05</v>
       </c>
       <c r="H19" s="31">
-        <v>487.25</v>
-      </c>
-      <c r="I19" s="31"/>
+        <v>485.2</v>
+      </c>
+      <c r="I19" s="31">
+        <v>500.5</v>
+      </c>
       <c r="J19" s="31"/>
       <c r="K19" s="31"/>
       <c r="L19" s="31"/>
@@ -6881,9 +6957,11 @@
         <v>195.3</v>
       </c>
       <c r="H20" s="31">
-        <v>196</v>
-      </c>
-      <c r="I20" s="31"/>
+        <v>195.75</v>
+      </c>
+      <c r="I20" s="31">
+        <v>197</v>
+      </c>
       <c r="J20" s="31"/>
       <c r="K20" s="31"/>
       <c r="L20" s="31"/>
@@ -6917,9 +6995,11 @@
         <v>452.75</v>
       </c>
       <c r="H21" s="31">
-        <v>451.2</v>
-      </c>
-      <c r="I21" s="31"/>
+        <v>450</v>
+      </c>
+      <c r="I21" s="31">
+        <v>447.8</v>
+      </c>
       <c r="J21" s="31"/>
       <c r="K21" s="31"/>
       <c r="L21" s="31"/>
@@ -6955,7 +7035,9 @@
       <c r="H22" s="31">
         <v>741.05</v>
       </c>
-      <c r="I22" s="31"/>
+      <c r="I22" s="31">
+        <v>724.7</v>
+      </c>
       <c r="J22" s="31"/>
       <c r="K22" s="31"/>
       <c r="L22" s="31"/>
@@ -6989,9 +7071,11 @@
         <v>415.9</v>
       </c>
       <c r="H23" s="31">
-        <v>424.75</v>
-      </c>
-      <c r="I23" s="31"/>
+        <v>423.4</v>
+      </c>
+      <c r="I23" s="31">
+        <v>421.1</v>
+      </c>
       <c r="J23" s="31"/>
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
@@ -7019,9 +7103,11 @@
         <v>88.85</v>
       </c>
       <c r="H24" s="5">
-        <v>86.9</v>
-      </c>
-      <c r="I24" s="5"/>
+        <v>86.5</v>
+      </c>
+      <c r="I24" s="5">
+        <v>87.25</v>
+      </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -7049,7 +7135,9 @@
       <c r="H25" s="5">
         <v>84.45</v>
       </c>
-      <c r="I25" s="5"/>
+      <c r="I25" s="5">
+        <v>75.7</v>
+      </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
@@ -7059,6 +7147,32 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5">
+        <v>255.75</v>
+      </c>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
     </row>
   </sheetData>
   <sortState ref="J1:J37">
@@ -7607,7 +7721,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q11"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8580,7 +8694,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A2" sqref="A2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8693,4 +8807,460 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="42"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="40">
+        <v>42522</v>
+      </c>
+      <c r="B1">
+        <v>5800</v>
+      </c>
+      <c r="C1" s="41">
+        <v>2185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="40">
+        <v>42552</v>
+      </c>
+      <c r="B2">
+        <v>5800</v>
+      </c>
+      <c r="C2" s="41">
+        <v>2185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="40">
+        <v>42583</v>
+      </c>
+      <c r="B3">
+        <v>5800</v>
+      </c>
+      <c r="C3" s="41">
+        <v>2185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
+      <c r="B4">
+        <v>5800</v>
+      </c>
+      <c r="C4" s="41">
+        <v>2185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="40"/>
+      <c r="B5">
+        <v>5800</v>
+      </c>
+      <c r="C5" s="41">
+        <v>2185</v>
+      </c>
+      <c r="E5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F5">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="40"/>
+      <c r="B6">
+        <v>5800</v>
+      </c>
+      <c r="C6" s="41">
+        <v>2185</v>
+      </c>
+      <c r="E6" t="s">
+        <v>169</v>
+      </c>
+      <c r="F6">
+        <f>SUM(B:B)</f>
+        <v>348000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>5800</v>
+      </c>
+      <c r="C7" s="41">
+        <v>2185</v>
+      </c>
+      <c r="E7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F7">
+        <f>F6-F5</f>
+        <v>98000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="40">
+        <v>42736</v>
+      </c>
+      <c r="B8">
+        <v>5800</v>
+      </c>
+      <c r="C8" s="41">
+        <v>2185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>5800</v>
+      </c>
+      <c r="C9" s="41">
+        <v>2185</v>
+      </c>
+      <c r="E9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F9">
+        <v>87000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>5800</v>
+      </c>
+      <c r="C10" s="41">
+        <v>2185</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="F10">
+        <v>178149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>5800</v>
+      </c>
+      <c r="C11" s="41">
+        <v>2185</v>
+      </c>
+      <c r="E11" t="s">
+        <v>171</v>
+      </c>
+      <c r="F11">
+        <f>F5-F10</f>
+        <v>71851</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>5800</v>
+      </c>
+      <c r="C12" s="41">
+        <v>2185</v>
+      </c>
+      <c r="E12" t="s">
+        <v>172</v>
+      </c>
+      <c r="F12">
+        <f>F9-F11</f>
+        <v>15149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>5800</v>
+      </c>
+      <c r="C13" s="41">
+        <v>2185</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="F13">
+        <v>261000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>5800</v>
+      </c>
+      <c r="C14" s="41">
+        <v>2185</v>
+      </c>
+      <c r="E14" s="43"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="40">
+        <v>42948</v>
+      </c>
+      <c r="B15">
+        <v>5800</v>
+      </c>
+      <c r="C15" s="41">
+        <v>2185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>5800</v>
+      </c>
+      <c r="C16" s="42">
+        <f>SUM(C1:C15)</f>
+        <v>32775</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="40">
+        <v>43101</v>
+      </c>
+      <c r="B20">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="40">
+        <v>43466</v>
+      </c>
+      <c r="B32">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="40">
+        <v>43831</v>
+      </c>
+      <c r="B44">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="40">
+        <v>44197</v>
+      </c>
+      <c r="B56">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>5800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the sheet for 09082017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="179">
   <si>
     <t>Date</t>
   </si>
@@ -6240,8 +6240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6287,7 +6287,9 @@
       <c r="K1" s="14">
         <v>42955</v>
       </c>
-      <c r="L1" s="31"/>
+      <c r="L1" s="14">
+        <v>42986</v>
+      </c>
       <c r="M1" s="31"/>
       <c r="N1" s="31"/>
       <c r="O1" s="31"/>
@@ -6323,7 +6325,9 @@
       <c r="K2" s="5">
         <v>305</v>
       </c>
-      <c r="L2" s="5"/>
+      <c r="L2" s="5">
+        <v>302.95</v>
+      </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
@@ -6359,7 +6363,9 @@
       <c r="K3" s="5">
         <v>295.95</v>
       </c>
-      <c r="L3" s="5"/>
+      <c r="L3" s="5">
+        <v>290.64999999999998</v>
+      </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -6401,7 +6407,9 @@
       <c r="K4" s="31">
         <v>273.85000000000002</v>
       </c>
-      <c r="L4" s="31"/>
+      <c r="L4" s="31">
+        <v>272.8</v>
+      </c>
       <c r="M4" s="31"/>
       <c r="N4" s="31"/>
       <c r="O4" s="31"/>
@@ -6443,7 +6451,9 @@
       <c r="K5" s="33">
         <v>1604.6</v>
       </c>
-      <c r="L5" s="31"/>
+      <c r="L5" s="33">
+        <v>1600.3</v>
+      </c>
       <c r="M5" s="31"/>
       <c r="N5" s="31"/>
       <c r="O5" s="31"/>
@@ -6485,7 +6495,9 @@
       <c r="K6" s="31">
         <v>244.4</v>
       </c>
-      <c r="L6" s="31"/>
+      <c r="L6" s="31">
+        <v>243.1</v>
+      </c>
       <c r="M6" s="31"/>
       <c r="N6" s="31"/>
       <c r="O6" s="31"/>
@@ -6527,7 +6539,9 @@
       <c r="K7" s="31">
         <v>17.649999999999999</v>
       </c>
-      <c r="L7" s="31"/>
+      <c r="L7" s="31">
+        <v>17.05</v>
+      </c>
       <c r="M7" s="31"/>
       <c r="N7" s="31"/>
       <c r="O7" s="31"/>
@@ -6569,7 +6583,9 @@
       <c r="K8" s="31">
         <v>62.95</v>
       </c>
-      <c r="L8" s="31"/>
+      <c r="L8" s="31">
+        <v>61.85</v>
+      </c>
       <c r="M8" s="31"/>
       <c r="N8" s="31"/>
       <c r="O8" s="31"/>
@@ -6603,7 +6619,9 @@
       <c r="K9" s="9">
         <v>56.6</v>
       </c>
-      <c r="L9" s="9"/>
+      <c r="L9" s="9">
+        <v>56.4</v>
+      </c>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -6645,7 +6663,9 @@
       <c r="K10" s="31">
         <v>41.8</v>
       </c>
-      <c r="L10" s="31"/>
+      <c r="L10" s="31">
+        <v>41.35</v>
+      </c>
       <c r="M10" s="31"/>
       <c r="N10" s="31"/>
       <c r="O10" s="31"/>
@@ -6687,7 +6707,9 @@
       <c r="K11" s="31">
         <v>69.849999999999994</v>
       </c>
-      <c r="L11" s="31"/>
+      <c r="L11" s="31">
+        <v>70.75</v>
+      </c>
       <c r="M11" s="31"/>
       <c r="N11" s="31"/>
       <c r="O11" s="31"/>
@@ -6729,7 +6751,9 @@
       <c r="K12" s="31">
         <v>91.65</v>
       </c>
-      <c r="L12" s="31"/>
+      <c r="L12" s="31">
+        <v>91.25</v>
+      </c>
       <c r="M12" s="31"/>
       <c r="N12" s="31"/>
       <c r="O12" s="31"/>
@@ -6771,7 +6795,9 @@
       <c r="K13" s="31">
         <v>134.5</v>
       </c>
-      <c r="L13" s="31"/>
+      <c r="L13" s="31">
+        <v>133</v>
+      </c>
       <c r="M13" s="31"/>
       <c r="N13" s="31"/>
       <c r="O13" s="31"/>
@@ -6813,7 +6839,9 @@
       <c r="K14" s="31">
         <v>78.150000000000006</v>
       </c>
-      <c r="L14" s="31"/>
+      <c r="L14" s="31">
+        <v>77.8</v>
+      </c>
       <c r="M14" s="31"/>
       <c r="N14" s="31"/>
       <c r="O14" s="31"/>
@@ -6855,7 +6883,9 @@
       <c r="K15" s="31">
         <v>53.45</v>
       </c>
-      <c r="L15" s="31"/>
+      <c r="L15" s="31">
+        <v>52.15</v>
+      </c>
       <c r="M15" s="31"/>
       <c r="N15" s="31"/>
       <c r="O15" s="31"/>
@@ -6897,7 +6927,9 @@
       <c r="K16" s="31">
         <v>31.6</v>
       </c>
-      <c r="L16" s="31"/>
+      <c r="L16" s="31">
+        <v>31.5</v>
+      </c>
       <c r="M16" s="31"/>
       <c r="N16" s="31"/>
       <c r="O16" s="31"/>
@@ -6931,7 +6963,9 @@
       <c r="K17" s="31">
         <v>32.299999999999997</v>
       </c>
-      <c r="L17" s="31"/>
+      <c r="L17" s="31">
+        <v>29.5</v>
+      </c>
       <c r="M17" s="31"/>
       <c r="N17" s="31"/>
       <c r="O17" s="31"/>
@@ -6973,7 +7007,9 @@
       <c r="K18" s="31">
         <v>614</v>
       </c>
-      <c r="L18" s="31"/>
+      <c r="L18" s="31">
+        <v>605.25</v>
+      </c>
       <c r="M18" s="31"/>
       <c r="N18" s="31"/>
       <c r="O18" s="31"/>
@@ -7015,7 +7051,9 @@
       <c r="K19" s="31">
         <v>492</v>
       </c>
-      <c r="L19" s="31"/>
+      <c r="L19" s="31">
+        <v>479</v>
+      </c>
       <c r="M19" s="31"/>
       <c r="N19" s="31"/>
       <c r="O19" s="31"/>
@@ -7057,7 +7095,9 @@
       <c r="K20" s="31">
         <v>212.35</v>
       </c>
-      <c r="L20" s="31"/>
+      <c r="L20" s="31">
+        <v>206.05</v>
+      </c>
       <c r="M20" s="31"/>
       <c r="N20" s="31"/>
       <c r="O20" s="31"/>
@@ -7099,7 +7139,9 @@
       <c r="K21" s="31">
         <v>452.6</v>
       </c>
-      <c r="L21" s="31"/>
+      <c r="L21" s="31">
+        <v>450.5</v>
+      </c>
       <c r="M21" s="31"/>
       <c r="N21" s="31"/>
       <c r="O21" s="31"/>
@@ -7141,7 +7183,9 @@
       <c r="K22" s="31">
         <v>726.55</v>
       </c>
-      <c r="L22" s="31"/>
+      <c r="L22" s="31">
+        <v>683.05</v>
+      </c>
       <c r="M22" s="31"/>
       <c r="N22" s="31"/>
       <c r="O22" s="31"/>
@@ -7183,7 +7227,9 @@
       <c r="K23" s="31">
         <v>417.95</v>
       </c>
-      <c r="L23" s="31"/>
+      <c r="L23" s="31">
+        <v>416</v>
+      </c>
       <c r="M23" s="31"/>
       <c r="N23" s="31"/>
       <c r="O23" s="31"/>
@@ -7219,7 +7265,9 @@
       <c r="K24" s="5">
         <v>85.7</v>
       </c>
-      <c r="L24" s="5"/>
+      <c r="L24" s="5">
+        <v>84.9</v>
+      </c>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
@@ -7253,7 +7301,9 @@
       <c r="K25" s="5">
         <v>54.95</v>
       </c>
-      <c r="L25" s="5"/>
+      <c r="L25" s="5">
+        <v>57.45</v>
+      </c>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
@@ -7283,7 +7333,9 @@
       <c r="K26" s="5">
         <v>248.95</v>
       </c>
-      <c r="L26" s="5"/>
+      <c r="L26" s="5">
+        <v>242.3</v>
+      </c>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
@@ -7837,8 +7889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7880,7 +7932,7 @@
       </c>
       <c r="I1">
         <f>SUM(H2:H200)</f>
-        <v>366.45000000000039</v>
+        <v>388.45000000000039</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7941,7 +7993,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="5">
-        <f t="shared" ref="G3:G21" si="1">E3*F3</f>
+        <f t="shared" ref="G3:G23" si="1">E3*F3</f>
         <v>2160</v>
       </c>
       <c r="H3" s="5">
@@ -8165,11 +8217,11 @@
         <v>762</v>
       </c>
       <c r="C8" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" s="5">
-        <f t="shared" ref="D8:D21" si="4">B8*C8</f>
-        <v>3048</v>
+        <f t="shared" ref="D8:D23" si="4">B8*C8</f>
+        <v>3810</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -8178,6 +8230,12 @@
         <v>0</v>
       </c>
       <c r="H8" s="5"/>
+      <c r="J8">
+        <v>388</v>
+      </c>
+      <c r="K8" s="38">
+        <v>42986</v>
+      </c>
       <c r="M8" s="36" t="s">
         <v>154</v>
       </c>
@@ -8552,24 +8610,52 @@
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+      <c r="A22" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B22" s="5">
+        <v>255</v>
+      </c>
+      <c r="C22" s="5">
+        <v>3</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="4"/>
+        <v>765</v>
+      </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
+      <c r="A23" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B23" s="5">
+        <v>48</v>
+      </c>
+      <c r="C23" s="5">
+        <v>2</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="4"/>
+        <v>96</v>
+      </c>
+      <c r="E23" s="5">
+        <v>59</v>
+      </c>
+      <c r="F23" s="5">
+        <v>2</v>
+      </c>
+      <c r="G23" s="5">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" ref="H23" si="7">G23-D23</f>
+        <v>22</v>
+      </c>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>

</xml_diff>

<commit_message>
Updated the sheet for 10082017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="180">
   <si>
     <t>Date</t>
   </si>
@@ -557,6 +557,9 @@
   </si>
   <si>
     <t>TATAPOWER</t>
+  </si>
+  <si>
+    <t>#######</t>
   </si>
 </sst>
 </file>
@@ -6238,10 +6241,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6251,6 +6254,7 @@
     <col min="3" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -6290,7 +6294,9 @@
       <c r="L1" s="14">
         <v>42986</v>
       </c>
-      <c r="M1" s="31"/>
+      <c r="M1" s="14">
+        <v>43016</v>
+      </c>
       <c r="N1" s="31"/>
       <c r="O1" s="31"/>
       <c r="P1" s="31"/>
@@ -6328,7 +6334,9 @@
       <c r="L2" s="5">
         <v>302.95</v>
       </c>
-      <c r="M2" s="5"/>
+      <c r="M2" s="5">
+        <v>298</v>
+      </c>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
@@ -6366,7 +6374,9 @@
       <c r="L3" s="5">
         <v>290.64999999999998</v>
       </c>
-      <c r="M3" s="5"/>
+      <c r="M3" s="5">
+        <v>291</v>
+      </c>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
@@ -6410,7 +6420,9 @@
       <c r="L4" s="31">
         <v>272.8</v>
       </c>
-      <c r="M4" s="31"/>
+      <c r="M4" s="31">
+        <v>273.8</v>
+      </c>
       <c r="N4" s="31"/>
       <c r="O4" s="31"/>
       <c r="P4" s="31"/>
@@ -6454,7 +6466,9 @@
       <c r="L5" s="33">
         <v>1600.3</v>
       </c>
-      <c r="M5" s="31"/>
+      <c r="M5" s="33">
+        <v>1593.75</v>
+      </c>
       <c r="N5" s="31"/>
       <c r="O5" s="31"/>
       <c r="P5" s="31"/>
@@ -6498,7 +6512,9 @@
       <c r="L6" s="31">
         <v>243.1</v>
       </c>
-      <c r="M6" s="31"/>
+      <c r="M6" s="31">
+        <v>239.45</v>
+      </c>
       <c r="N6" s="31"/>
       <c r="O6" s="31"/>
       <c r="P6" s="31"/>
@@ -6542,7 +6558,9 @@
       <c r="L7" s="31">
         <v>17.05</v>
       </c>
-      <c r="M7" s="31"/>
+      <c r="M7" s="31">
+        <v>16.149999999999999</v>
+      </c>
       <c r="N7" s="31"/>
       <c r="O7" s="31"/>
       <c r="P7" s="31"/>
@@ -6586,7 +6604,9 @@
       <c r="L8" s="31">
         <v>61.85</v>
       </c>
-      <c r="M8" s="31"/>
+      <c r="M8" s="31">
+        <v>59.15</v>
+      </c>
       <c r="N8" s="31"/>
       <c r="O8" s="31"/>
       <c r="P8" s="31"/>
@@ -6622,7 +6642,9 @@
       <c r="L9" s="9">
         <v>56.4</v>
       </c>
-      <c r="M9" s="9"/>
+      <c r="M9" s="9">
+        <v>54.45</v>
+      </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
@@ -6666,7 +6688,9 @@
       <c r="L10" s="31">
         <v>41.35</v>
       </c>
-      <c r="M10" s="31"/>
+      <c r="M10" s="31">
+        <v>39.15</v>
+      </c>
       <c r="N10" s="31"/>
       <c r="O10" s="31"/>
       <c r="P10" s="31"/>
@@ -6710,7 +6734,9 @@
       <c r="L11" s="31">
         <v>70.75</v>
       </c>
-      <c r="M11" s="31"/>
+      <c r="M11" s="31">
+        <v>65.45</v>
+      </c>
       <c r="N11" s="31"/>
       <c r="O11" s="31"/>
       <c r="P11" s="31"/>
@@ -6754,7 +6780,9 @@
       <c r="L12" s="31">
         <v>91.25</v>
       </c>
-      <c r="M12" s="31"/>
+      <c r="M12" s="31">
+        <v>88.3</v>
+      </c>
       <c r="N12" s="31"/>
       <c r="O12" s="31"/>
       <c r="P12" s="31"/>
@@ -6798,7 +6826,9 @@
       <c r="L13" s="31">
         <v>133</v>
       </c>
-      <c r="M13" s="31"/>
+      <c r="M13" s="31">
+        <v>128</v>
+      </c>
       <c r="N13" s="31"/>
       <c r="O13" s="31"/>
       <c r="P13" s="31"/>
@@ -6842,7 +6872,9 @@
       <c r="L14" s="31">
         <v>77.8</v>
       </c>
-      <c r="M14" s="31"/>
+      <c r="M14" s="31">
+        <v>77</v>
+      </c>
       <c r="N14" s="31"/>
       <c r="O14" s="31"/>
       <c r="P14" s="31"/>
@@ -6886,7 +6918,9 @@
       <c r="L15" s="31">
         <v>52.15</v>
       </c>
-      <c r="M15" s="31"/>
+      <c r="M15" s="31">
+        <v>51.45</v>
+      </c>
       <c r="N15" s="31"/>
       <c r="O15" s="31"/>
       <c r="P15" s="31"/>
@@ -6930,7 +6964,9 @@
       <c r="L16" s="31">
         <v>31.5</v>
       </c>
-      <c r="M16" s="31"/>
+      <c r="M16" s="31">
+        <v>30.55</v>
+      </c>
       <c r="N16" s="31"/>
       <c r="O16" s="31"/>
       <c r="P16" s="31"/>
@@ -6966,7 +7002,9 @@
       <c r="L17" s="31">
         <v>29.5</v>
       </c>
-      <c r="M17" s="31"/>
+      <c r="M17" s="31">
+        <v>27.75</v>
+      </c>
       <c r="N17" s="31"/>
       <c r="O17" s="31"/>
       <c r="P17" s="31"/>
@@ -7010,7 +7048,9 @@
       <c r="L18" s="31">
         <v>605.25</v>
       </c>
-      <c r="M18" s="31"/>
+      <c r="M18" s="31">
+        <v>606.5</v>
+      </c>
       <c r="N18" s="31"/>
       <c r="O18" s="31"/>
       <c r="P18" s="31"/>
@@ -7054,7 +7094,9 @@
       <c r="L19" s="31">
         <v>479</v>
       </c>
-      <c r="M19" s="31"/>
+      <c r="M19" s="31">
+        <v>453</v>
+      </c>
       <c r="N19" s="31"/>
       <c r="O19" s="31"/>
       <c r="P19" s="31"/>
@@ -7098,7 +7140,9 @@
       <c r="L20" s="31">
         <v>206.05</v>
       </c>
-      <c r="M20" s="31"/>
+      <c r="M20" s="31">
+        <v>191.95</v>
+      </c>
       <c r="N20" s="31"/>
       <c r="O20" s="31"/>
       <c r="P20" s="31"/>
@@ -7142,7 +7186,9 @@
       <c r="L21" s="31">
         <v>450.5</v>
       </c>
-      <c r="M21" s="31"/>
+      <c r="M21" s="31">
+        <v>455</v>
+      </c>
       <c r="N21" s="31"/>
       <c r="O21" s="31"/>
       <c r="P21" s="31"/>
@@ -7186,7 +7232,9 @@
       <c r="L22" s="31">
         <v>683.05</v>
       </c>
-      <c r="M22" s="31"/>
+      <c r="M22" s="31">
+        <v>696</v>
+      </c>
       <c r="N22" s="31"/>
       <c r="O22" s="31"/>
       <c r="P22" s="31"/>
@@ -7230,7 +7278,9 @@
       <c r="L23" s="31">
         <v>416</v>
       </c>
-      <c r="M23" s="31"/>
+      <c r="M23" s="31">
+        <v>416.4</v>
+      </c>
       <c r="N23" s="31"/>
       <c r="O23" s="31"/>
       <c r="P23" s="31"/>
@@ -7268,7 +7318,9 @@
       <c r="L24" s="5">
         <v>84.9</v>
       </c>
-      <c r="M24" s="5"/>
+      <c r="M24" s="5">
+        <v>83</v>
+      </c>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
@@ -7304,7 +7356,9 @@
       <c r="L25" s="5">
         <v>57.45</v>
       </c>
-      <c r="M25" s="5"/>
+      <c r="M25" s="5">
+        <v>57.35</v>
+      </c>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
@@ -7336,12 +7390,19 @@
       <c r="L26" s="5">
         <v>242.3</v>
       </c>
-      <c r="M26" s="5"/>
+      <c r="M26" s="5">
+        <v>223</v>
+      </c>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>179</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="J1:J37">
@@ -7889,8 +7950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8019,7 +8080,9 @@
         <f>N3*O3</f>
         <v>618.5</v>
       </c>
-      <c r="Q3" s="5"/>
+      <c r="Q3" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -8068,7 +8131,9 @@
         <f t="shared" ref="P4:P10" si="3">N4*O4</f>
         <v>605.4</v>
       </c>
-      <c r="Q4" s="5"/>
+      <c r="Q4" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -8285,7 +8350,9 @@
         <f t="shared" si="3"/>
         <v>126</v>
       </c>
-      <c r="Q9" s="5"/>
+      <c r="Q9" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -8321,7 +8388,9 @@
         <f t="shared" si="3"/>
         <v>120</v>
       </c>
-      <c r="Q10" s="5"/>
+      <c r="Q10" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -8434,11 +8503,11 @@
         <v>34.25</v>
       </c>
       <c r="C14" s="5">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="D14" s="5">
         <f t="shared" si="4"/>
-        <v>6165</v>
+        <v>6678.75</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -8507,11 +8576,11 @@
         <v>464</v>
       </c>
       <c r="C17" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D17" s="5">
         <f t="shared" si="4"/>
-        <v>4640</v>
+        <v>5104</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -8617,11 +8686,11 @@
         <v>255</v>
       </c>
       <c r="C22" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D22" s="5">
         <f t="shared" si="4"/>
-        <v>765</v>
+        <v>1020</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>

</xml_diff>

<commit_message>
Added details for 21/08/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -16,13 +16,14 @@
     <sheet name="Papa" sheetId="10" r:id="rId7"/>
     <sheet name="Tiles" sheetId="11" r:id="rId8"/>
     <sheet name="DoorsWindows" sheetId="12" r:id="rId9"/>
+    <sheet name="Electricity" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="284">
   <si>
     <t>Date</t>
   </si>
@@ -567,9 +568,6 @@
     <t>Sand</t>
   </si>
   <si>
-    <t>Frame</t>
-  </si>
-  <si>
     <t>Fatte (10 feet length)</t>
   </si>
   <si>
@@ -640,6 +638,243 @@
   </si>
   <si>
     <t>16/8/2017</t>
+  </si>
+  <si>
+    <t>Wire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wire </t>
+  </si>
+  <si>
+    <t>2.5 mm</t>
+  </si>
+  <si>
+    <t>1.5 mm</t>
+  </si>
+  <si>
+    <t>0.75 mm</t>
+  </si>
+  <si>
+    <t>Fan Sheet</t>
+  </si>
+  <si>
+    <t>Round Sheet</t>
+  </si>
+  <si>
+    <t>Tape Roll</t>
+  </si>
+  <si>
+    <t>Steel Watcher</t>
+  </si>
+  <si>
+    <t>1 kg</t>
+  </si>
+  <si>
+    <t>Batten Holder</t>
+  </si>
+  <si>
+    <t>Angel Holder</t>
+  </si>
+  <si>
+    <t>Ceiling Cell</t>
+  </si>
+  <si>
+    <t>5 Amp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch </t>
+  </si>
+  <si>
+    <t>Socket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicator </t>
+  </si>
+  <si>
+    <t>Two Way</t>
+  </si>
+  <si>
+    <t>Bell Switch</t>
+  </si>
+  <si>
+    <t>15 Amp</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>60 Amp</t>
+  </si>
+  <si>
+    <t>MCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 Amp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 Amp </t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>8 mm</t>
+  </si>
+  <si>
+    <t>3 mm</t>
+  </si>
+  <si>
+    <t>6 mm</t>
+  </si>
+  <si>
+    <t>12 mm</t>
+  </si>
+  <si>
+    <t>Bijli</t>
+  </si>
+  <si>
+    <t>Frames Required</t>
+  </si>
+  <si>
+    <t>Floor Wooden</t>
+  </si>
+  <si>
+    <t>Gallary and Stairs</t>
+  </si>
+  <si>
+    <t>Area Sq Feet</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Ask</t>
+  </si>
+  <si>
+    <t>Area covered per box</t>
+  </si>
+  <si>
+    <t>No of tiles in one box</t>
+  </si>
+  <si>
+    <t>Wooden tiles (preferred dark brown)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiles should be anti-skit </t>
+  </si>
+  <si>
+    <t>should be vitrified</t>
+  </si>
+  <si>
+    <t>Which is better vitrified or porcelain tiles</t>
+  </si>
+  <si>
+    <t>Diff in price of vitrified and porcelain tiles</t>
+  </si>
+  <si>
+    <t>Reddish black granite</t>
+  </si>
+  <si>
+    <t>Carriage to Kullu</t>
+  </si>
+  <si>
+    <t>What if required extra tiles</t>
+  </si>
+  <si>
+    <t>Difference in Kajaria/Cera/Italiano/Somany price</t>
+  </si>
+  <si>
+    <t>Local tiles k rates bhi pta kriyo kinti sasti hai</t>
+  </si>
+  <si>
+    <t>Difference in quality of local and branded quality</t>
+  </si>
+  <si>
+    <t>Stairs and Gallery k liye ask for parking tiles jyada mehngi nahi</t>
+  </si>
+  <si>
+    <t>Stair tiles and floor tiles mein macthing tile leni hein</t>
+  </si>
+  <si>
+    <t>Dono dark color would be preferred.</t>
+  </si>
+  <si>
+    <t>Kitchen Wall</t>
+  </si>
+  <si>
+    <t>Kitchen Floor</t>
+  </si>
+  <si>
+    <t>Bathroom Wall</t>
+  </si>
+  <si>
+    <t>Bathroom Floor</t>
+  </si>
+  <si>
+    <t>Total Square Feet</t>
+  </si>
+  <si>
+    <t>Per Square Feet</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>kabje</t>
+  </si>
+  <si>
+    <t>chitnkami</t>
+  </si>
+  <si>
+    <t>4 inch</t>
+  </si>
+  <si>
+    <t>6 inch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">handle </t>
+  </si>
+  <si>
+    <t>darwaza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Handle </t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>chitkani</t>
+  </si>
+  <si>
+    <t>7 foot</t>
+  </si>
+  <si>
+    <t>6 foot</t>
+  </si>
+  <si>
+    <t>Kabje</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>khidki stopper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">door stopper peeche </t>
+  </si>
+  <si>
+    <t>door stopper neeche</t>
+  </si>
+  <si>
+    <t>door closure</t>
+  </si>
+  <si>
+    <t>21/8/2017</t>
   </si>
 </sst>
 </file>
@@ -764,7 +999,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -810,9 +1045,12 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1116,7 +1354,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -6307,12 +6545,274 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3">
+      <c r="A2" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="C12" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="C13" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C14" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C15" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C19" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="C20" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C21" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="C23" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="C24" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="C25" s="5">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O26"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6365,12 +6865,14 @@
         <v>43047</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O1" s="29" t="s">
-        <v>205</v>
-      </c>
-      <c r="P1" s="29"/>
+        <v>204</v>
+      </c>
+      <c r="P1" s="29" t="s">
+        <v>283</v>
+      </c>
       <c r="Q1" s="29"/>
     </row>
     <row r="2" spans="1:17">
@@ -6413,7 +6915,9 @@
       <c r="O2" s="5">
         <v>283.2</v>
       </c>
-      <c r="P2" s="5"/>
+      <c r="P2" s="5">
+        <v>274.55</v>
+      </c>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17">
@@ -6456,7 +6960,9 @@
       <c r="O3" s="5">
         <v>295.2</v>
       </c>
-      <c r="P3" s="5"/>
+      <c r="P3" s="5">
+        <v>293.35000000000002</v>
+      </c>
       <c r="Q3" s="5"/>
     </row>
     <row r="4" spans="1:17">
@@ -6505,7 +7011,9 @@
       <c r="O4" s="29">
         <v>279.2</v>
       </c>
-      <c r="P4" s="29"/>
+      <c r="P4" s="29">
+        <v>282.45</v>
+      </c>
       <c r="Q4" s="29"/>
     </row>
     <row r="5" spans="1:17">
@@ -6554,7 +7062,9 @@
       <c r="O5" s="31">
         <v>1576</v>
       </c>
-      <c r="P5" s="29"/>
+      <c r="P5" s="31">
+        <v>1564.3</v>
+      </c>
       <c r="Q5" s="29"/>
     </row>
     <row r="6" spans="1:17">
@@ -6603,7 +7113,9 @@
       <c r="O6" s="29">
         <v>238.45</v>
       </c>
-      <c r="P6" s="29"/>
+      <c r="P6" s="29">
+        <v>239.2</v>
+      </c>
       <c r="Q6" s="29"/>
     </row>
     <row r="7" spans="1:17">
@@ -6652,7 +7164,9 @@
       <c r="O7" s="29">
         <v>16.600000000000001</v>
       </c>
-      <c r="P7" s="29"/>
+      <c r="P7" s="29">
+        <v>17.5</v>
+      </c>
       <c r="Q7" s="29"/>
     </row>
     <row r="8" spans="1:17">
@@ -6701,7 +7215,9 @@
       <c r="O8" s="29">
         <v>59.55</v>
       </c>
-      <c r="P8" s="29"/>
+      <c r="P8" s="29">
+        <v>59.2</v>
+      </c>
       <c r="Q8" s="29"/>
     </row>
     <row r="9" spans="1:17">
@@ -6742,7 +7258,9 @@
       <c r="O9" s="7">
         <v>55.85</v>
       </c>
-      <c r="P9" s="7"/>
+      <c r="P9" s="7">
+        <v>54.55</v>
+      </c>
       <c r="Q9" s="7"/>
     </row>
     <row r="10" spans="1:17">
@@ -6791,7 +7309,9 @@
       <c r="O10" s="29">
         <v>40.700000000000003</v>
       </c>
-      <c r="P10" s="29"/>
+      <c r="P10" s="29">
+        <v>39.200000000000003</v>
+      </c>
       <c r="Q10" s="29"/>
     </row>
     <row r="11" spans="1:17">
@@ -6840,7 +7360,9 @@
       <c r="O11" s="29">
         <v>68.849999999999994</v>
       </c>
-      <c r="P11" s="29"/>
+      <c r="P11" s="29">
+        <v>68.900000000000006</v>
+      </c>
       <c r="Q11" s="29"/>
     </row>
     <row r="12" spans="1:17">
@@ -6889,7 +7411,9 @@
       <c r="O12" s="29">
         <v>86.95</v>
       </c>
-      <c r="P12" s="29"/>
+      <c r="P12" s="29">
+        <v>88.75</v>
+      </c>
       <c r="Q12" s="29"/>
     </row>
     <row r="13" spans="1:17">
@@ -6938,7 +7462,9 @@
       <c r="O13" s="29">
         <v>129.75</v>
       </c>
-      <c r="P13" s="29"/>
+      <c r="P13" s="29">
+        <v>124.25</v>
+      </c>
       <c r="Q13" s="29"/>
     </row>
     <row r="14" spans="1:17">
@@ -6987,7 +7513,9 @@
       <c r="O14" s="29">
         <v>82</v>
       </c>
-      <c r="P14" s="29"/>
+      <c r="P14" s="29">
+        <v>80.3</v>
+      </c>
       <c r="Q14" s="29"/>
     </row>
     <row r="15" spans="1:17">
@@ -7036,7 +7564,9 @@
       <c r="O15" s="29">
         <v>53.25</v>
       </c>
-      <c r="P15" s="29"/>
+      <c r="P15" s="29">
+        <v>50.5</v>
+      </c>
       <c r="Q15" s="29"/>
     </row>
     <row r="16" spans="1:17">
@@ -7085,7 +7615,9 @@
       <c r="O16" s="29">
         <v>31.8</v>
       </c>
-      <c r="P16" s="29"/>
+      <c r="P16" s="29">
+        <v>33</v>
+      </c>
       <c r="Q16" s="29"/>
     </row>
     <row r="17" spans="1:17">
@@ -7126,7 +7658,9 @@
       <c r="O17" s="29">
         <v>34</v>
       </c>
-      <c r="P17" s="29"/>
+      <c r="P17" s="29">
+        <v>31.5</v>
+      </c>
       <c r="Q17" s="29"/>
     </row>
     <row r="18" spans="1:17">
@@ -7175,7 +7709,9 @@
       <c r="O18" s="29">
         <v>632.15</v>
       </c>
-      <c r="P18" s="29"/>
+      <c r="P18" s="29">
+        <v>621.45000000000005</v>
+      </c>
       <c r="Q18" s="29"/>
     </row>
     <row r="19" spans="1:17">
@@ -7224,7 +7760,9 @@
       <c r="O19" s="29">
         <v>506</v>
       </c>
-      <c r="P19" s="29"/>
+      <c r="P19" s="29">
+        <v>488.5</v>
+      </c>
       <c r="Q19" s="29"/>
     </row>
     <row r="20" spans="1:17">
@@ -7273,7 +7811,9 @@
       <c r="O20" s="29">
         <v>195</v>
       </c>
-      <c r="P20" s="29"/>
+      <c r="P20" s="29">
+        <v>197.5</v>
+      </c>
       <c r="Q20" s="29"/>
     </row>
     <row r="21" spans="1:17">
@@ -7322,7 +7862,9 @@
       <c r="O21" s="29">
         <v>454.5</v>
       </c>
-      <c r="P21" s="29"/>
+      <c r="P21" s="29">
+        <v>448.95</v>
+      </c>
       <c r="Q21" s="29"/>
     </row>
     <row r="22" spans="1:17">
@@ -7371,7 +7913,9 @@
       <c r="O22" s="29">
         <v>712.95</v>
       </c>
-      <c r="P22" s="29"/>
+      <c r="P22" s="29">
+        <v>695</v>
+      </c>
       <c r="Q22" s="29"/>
     </row>
     <row r="23" spans="1:17">
@@ -7420,7 +7964,9 @@
       <c r="O23" s="29">
         <v>408.35</v>
       </c>
-      <c r="P23" s="29"/>
+      <c r="P23" s="29">
+        <v>419.95</v>
+      </c>
       <c r="Q23" s="29"/>
     </row>
     <row r="24" spans="1:17">
@@ -7463,7 +8009,9 @@
       <c r="O24" s="5">
         <v>73.7</v>
       </c>
-      <c r="P24" s="5"/>
+      <c r="P24" s="5">
+        <v>73.900000000000006</v>
+      </c>
       <c r="Q24" s="5"/>
     </row>
     <row r="25" spans="1:17">
@@ -7504,7 +8052,9 @@
       <c r="O25" s="5">
         <v>62</v>
       </c>
-      <c r="P25" s="5"/>
+      <c r="P25" s="5">
+        <v>57.9</v>
+      </c>
       <c r="Q25" s="5"/>
     </row>
     <row r="26" spans="1:17">
@@ -7541,7 +8091,9 @@
       <c r="O26" s="5">
         <v>232.55</v>
       </c>
-      <c r="P26" s="5"/>
+      <c r="P26" s="5">
+        <v>223</v>
+      </c>
       <c r="Q26" s="5"/>
     </row>
   </sheetData>
@@ -7555,10 +8107,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.85546875" defaultRowHeight="15"/>
@@ -7582,7 +8134,7 @@
     <col min="18" max="16384" width="17.85546875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:20">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -7603,7 +8155,7 @@
       </c>
       <c r="J1" s="5">
         <f>SUM(K2:K100)</f>
-        <v>142350</v>
+        <v>141850</v>
       </c>
       <c r="K1" s="5"/>
       <c r="M1" s="10" t="s">
@@ -7616,8 +8168,13 @@
         <v>81</v>
       </c>
       <c r="Q1" s="5"/>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="S1" s="5">
+        <f>SUM(T2:T100)</f>
+        <v>111775</v>
+      </c>
+      <c r="T1" s="5"/>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" s="6" t="s">
         <v>30</v>
       </c>
@@ -7656,8 +8213,14 @@
       <c r="Q2" s="5">
         <v>5000</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="S2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" s="5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
@@ -7697,8 +8260,14 @@
         <f>Q2/2</f>
         <v>2500</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="S3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="T3" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" s="6" t="s">
         <v>72</v>
       </c>
@@ -7738,8 +8307,14 @@
       <c r="Q4" s="5">
         <v>500</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="S4" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4" s="13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
@@ -7773,8 +8348,14 @@
         <f>Q3*Q4</f>
         <v>1250000</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="S5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="T5" s="13">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
@@ -7806,7 +8387,7 @@
       </c>
       <c r="N6" s="15">
         <f>J1-N4</f>
-        <v>25150</v>
+        <v>24650</v>
       </c>
       <c r="P6" s="11" t="s">
         <v>86</v>
@@ -7815,8 +8396,14 @@
         <f>Q5/20</f>
         <v>62500</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="S6" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="T6" s="13">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
@@ -7843,8 +8430,14 @@
       <c r="K7" s="13">
         <v>400</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="S7" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="T7" s="13">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
@@ -7871,8 +8464,14 @@
       <c r="K8" s="13">
         <v>400</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="S8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="T8" s="13">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9" s="6" t="s">
         <v>5</v>
       </c>
@@ -7898,8 +8497,14 @@
       <c r="K9" s="13">
         <v>400</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="S9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="T9" s="13">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
       <c r="G10" s="6" t="s">
         <v>48</v>
       </c>
@@ -7916,8 +8521,14 @@
         <v>80</v>
       </c>
       <c r="N10" s="5"/>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="S10" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="T10" s="13">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
       <c r="G11" s="6" t="s">
         <v>49</v>
       </c>
@@ -7936,8 +8547,14 @@
       <c r="N11" s="5">
         <v>5000</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="S11" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="T11" s="13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
       <c r="G12" s="6" t="s">
         <v>52</v>
       </c>
@@ -7956,8 +8573,14 @@
       <c r="N12" s="5">
         <v>5000</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="S12" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="T12" s="13">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
       <c r="G13" s="6" t="s">
         <v>5</v>
       </c>
@@ -7970,8 +8593,14 @@
       <c r="K13" s="13">
         <v>750</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="S13" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="T13" s="13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
       <c r="D14" s="20"/>
       <c r="J14" s="11" t="s">
         <v>62</v>
@@ -7980,8 +8609,14 @@
         <v>2000</v>
       </c>
       <c r="P14" s="32"/>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="S14" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="T14" s="13">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
       <c r="D15" s="20"/>
       <c r="J15" s="11" t="s">
         <v>63</v>
@@ -7989,8 +8624,14 @@
       <c r="K15" s="13">
         <v>13000</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="S15" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="T15" s="13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
       <c r="D16" s="20"/>
       <c r="J16" s="11" t="s">
         <v>64</v>
@@ -7998,87 +8639,121 @@
       <c r="K16" s="13">
         <v>500</v>
       </c>
-    </row>
-    <row r="17" spans="4:11">
+      <c r="S16" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="T16" s="13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="4:20">
       <c r="J17" s="11" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="K17" s="13">
         <v>500</v>
       </c>
-    </row>
-    <row r="18" spans="4:11">
+      <c r="S17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="T17" s="13">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="18" spans="4:20">
       <c r="J18" s="11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K18" s="13">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="19" spans="4:11">
+        <v>2000</v>
+      </c>
+      <c r="S18" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="T18" s="13">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="19" spans="4:20">
       <c r="J19" s="11" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="K19" s="13">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="20" spans="4:11">
+        <v>6000</v>
+      </c>
+      <c r="S19" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="T19" s="13">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="20" spans="4:20">
       <c r="J20" s="11" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="K20" s="13">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="21" spans="4:11">
+        <v>5000</v>
+      </c>
+      <c r="S20" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="T20" s="13">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="21" spans="4:20">
       <c r="J21" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K21" s="13">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="22" spans="4:11">
+        <v>15000</v>
+      </c>
+      <c r="S21" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="T21" s="13">
+        <v>38625</v>
+      </c>
+    </row>
+    <row r="22" spans="4:20">
       <c r="J22" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K22" s="13">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="23" spans="4:11">
+        <v>20000</v>
+      </c>
+      <c r="S22" s="41"/>
+      <c r="T22" s="19"/>
+    </row>
+    <row r="23" spans="4:20">
       <c r="J23" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K23" s="13">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="24" spans="4:11">
+        <v>40000</v>
+      </c>
+      <c r="S23" s="41"/>
+      <c r="T23" s="19"/>
+    </row>
+    <row r="24" spans="4:20">
       <c r="J24" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K24" s="13">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="25" spans="4:11">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="25" spans="4:20">
       <c r="J25" s="11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="K25" s="13">
         <v>10000</v>
       </c>
     </row>
-    <row r="26" spans="4:11">
+    <row r="26" spans="4:20">
       <c r="D26" s="19"/>
-      <c r="J26" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="K26" s="13">
-        <v>10000</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8163,12 +8838,12 @@
       <c r="K2" t="s">
         <v>119</v>
       </c>
-      <c r="M2" s="41" t="s">
+      <c r="M2" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
       <c r="Q2" s="5" t="s">
         <v>153</v>
       </c>
@@ -9179,10 +9854,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9226,7 +9901,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(B2:B200)</f>
-        <v>549393</v>
+        <v>572093</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -9244,7 +9919,7 @@
       </c>
       <c r="F3" s="5">
         <f>F1-F2</f>
-        <v>925996</v>
+        <v>903296</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -9315,7 +9990,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B10" s="13">
         <v>1850</v>
@@ -9326,7 +10001,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B11" s="5">
         <v>4250</v>
@@ -9337,7 +10012,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B12" s="5">
         <v>1200</v>
@@ -9348,7 +10023,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B13" s="5">
         <v>3000</v>
@@ -9359,7 +10034,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B14" s="5">
         <v>4000</v>
@@ -9381,13 +10056,24 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B16" s="13">
         <v>6000</v>
       </c>
       <c r="C16" s="33">
         <v>42961</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="B17" s="13">
+        <v>22700</v>
+      </c>
+      <c r="C17" s="33">
+        <v>42966</v>
       </c>
     </row>
   </sheetData>
@@ -9854,10 +10540,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9868,12 +10554,15 @@
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="57.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" s="5"/>
       <c r="B1" s="10" t="s">
         <v>175</v>
@@ -9891,25 +10580,28 @@
         <v>177</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>173</v>
+        <v>241</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>177</v>
       </c>
       <c r="J1" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="M1" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="O1" s="10" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="10" t="s">
         <v>168</v>
       </c>
@@ -9931,28 +10623,30 @@
         <v>200</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I2" s="5">
-        <f>F2+F3+F6+F7+F9</f>
-        <v>1057.4000000000001</v>
+        <v>1157</v>
       </c>
       <c r="J2" s="5">
         <v>16</v>
       </c>
       <c r="K2" s="5">
         <f>I2/J2</f>
-        <v>66.087500000000006</v>
+        <v>72.3125</v>
       </c>
       <c r="L2" s="5">
         <v>700</v>
       </c>
       <c r="M2" s="5">
         <f>K2*L2</f>
-        <v>46261.250000000007</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>50618.75</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="10" t="s">
         <v>167</v>
       </c>
@@ -9974,28 +10668,30 @@
         <v>265</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I3" s="5">
-        <f>F4+F5</f>
-        <v>326.60000000000002</v>
+        <v>330</v>
       </c>
       <c r="J3" s="5">
         <v>9</v>
       </c>
       <c r="K3" s="5">
         <f>I3/J3</f>
-        <v>36.288888888888891</v>
+        <v>36.666666666666664</v>
       </c>
       <c r="L3" s="5">
         <v>330</v>
       </c>
       <c r="M3" s="5">
         <f t="shared" ref="M3:M5" si="2">K3*L3</f>
-        <v>11975.333333333334</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>12100</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="10" t="s">
         <v>35</v>
       </c>
@@ -10017,28 +10713,30 @@
         <v>275</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I4" s="5">
-        <f>F10+F8</f>
-        <v>850</v>
+        <v>740</v>
       </c>
       <c r="J4" s="5">
         <v>16</v>
       </c>
       <c r="K4" s="5">
         <f>I4/J4</f>
-        <v>53.125</v>
+        <v>46.25</v>
       </c>
       <c r="L4" s="5">
         <v>370</v>
       </c>
       <c r="M4" s="5">
         <f t="shared" si="2"/>
-        <v>19656.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>17112.5</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="10" t="s">
         <v>35</v>
       </c>
@@ -10060,28 +10758,30 @@
         <v>51.599999999999994</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I5" s="5">
-        <f>F11</f>
-        <v>88.2</v>
+        <v>150</v>
       </c>
       <c r="J5" s="5">
         <v>16</v>
       </c>
       <c r="K5" s="5">
         <f>I5/J5</f>
-        <v>5.5125000000000002</v>
+        <v>9.375</v>
       </c>
       <c r="L5" s="5">
         <v>370</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" si="2"/>
-        <v>2039.625</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>3468.75</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="10" t="s">
         <v>169</v>
       </c>
@@ -10111,10 +10811,13 @@
       </c>
       <c r="M6" s="10">
         <f>SUM(M2:M5)</f>
-        <v>79932.458333333343</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>83300</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="10" t="s">
         <v>170</v>
       </c>
@@ -10135,8 +10838,11 @@
         <f t="shared" si="1"/>
         <v>269.39999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="O7" s="11" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="10" t="s">
         <v>171</v>
       </c>
@@ -10157,8 +10863,27 @@
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="H8" s="5"/>
+      <c r="I8" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="10" t="s">
         <v>172</v>
       </c>
@@ -10179,8 +10904,31 @@
         <f t="shared" si="1"/>
         <v>188</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="H9" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="I9" s="5">
+        <v>27</v>
+      </c>
+      <c r="J9" s="5">
+        <v>10</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" ref="K9:K20" si="3">I9*J9</f>
+        <v>270</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0</v>
+      </c>
+      <c r="M9" s="5">
+        <f t="shared" ref="M9:M20" si="4">K9+L9</f>
+        <v>270</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="10" t="s">
         <v>179</v>
       </c>
@@ -10201,8 +10949,31 @@
         <f t="shared" si="1"/>
         <v>550</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="H10" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="I10" s="5">
+        <v>10</v>
+      </c>
+      <c r="J10" s="5">
+        <v>6</v>
+      </c>
+      <c r="K10" s="5">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="10" t="s">
         <v>178</v>
       </c>
@@ -10223,8 +10994,31 @@
         <f t="shared" si="1"/>
         <v>88.2</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="H11" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="I11" s="5">
+        <v>20</v>
+      </c>
+      <c r="J11" s="5">
+        <v>3</v>
+      </c>
+      <c r="K11" s="5">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="10" t="s">
         <v>177</v>
       </c>
@@ -10236,10 +11030,33 @@
         <f>SUM(F2:F11)</f>
         <v>2322.1999999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="H12" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="I12" s="5">
+        <v>15</v>
+      </c>
+      <c r="J12" s="5">
+        <v>3</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B13" s="5">
         <v>20</v>
@@ -10258,10 +11075,33 @@
         <f>D13+E13</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="H13" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="I13" s="5">
+        <v>13</v>
+      </c>
+      <c r="J13" s="5">
+        <v>13</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" si="3"/>
+        <v>169</v>
+      </c>
+      <c r="L13" s="5">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5">
+        <f t="shared" si="4"/>
+        <v>169</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B14" s="5">
         <v>13</v>
@@ -10270,20 +11110,43 @@
         <v>13</v>
       </c>
       <c r="D14" s="5">
-        <f t="shared" ref="D14:D24" si="3">B14*C14</f>
+        <f t="shared" ref="D14:D24" si="5">B14*C14</f>
         <v>169</v>
       </c>
       <c r="E14" s="5">
         <v>0</v>
       </c>
       <c r="F14" s="5">
-        <f t="shared" ref="F14:F24" si="4">D14+E14</f>
+        <f t="shared" ref="F14:F24" si="6">D14+E14</f>
         <v>169</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="H14" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="I14" s="5">
+        <v>18</v>
+      </c>
+      <c r="J14" s="5">
+        <v>17</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" si="3"/>
+        <v>306</v>
+      </c>
+      <c r="L14" s="5">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5">
+        <f t="shared" si="4"/>
+        <v>306</v>
+      </c>
+      <c r="O14" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B15" s="5">
         <v>15</v>
@@ -10292,18 +11155,41 @@
         <v>3</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="E15" s="5">
         <v>0</v>
       </c>
       <c r="F15" s="5">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="I15" s="5">
+        <v>13</v>
+      </c>
+      <c r="J15" s="5">
+        <v>16</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" si="3"/>
+        <v>208</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5">
         <f t="shared" si="4"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+        <v>208</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="10" t="s">
         <v>167</v>
       </c>
@@ -10314,20 +11200,43 @@
         <v>17</v>
       </c>
       <c r="D16" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>306</v>
       </c>
       <c r="E16" s="5">
         <v>0</v>
       </c>
       <c r="F16" s="5">
+        <f t="shared" si="6"/>
+        <v>306</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="I16" s="5">
+        <v>15</v>
+      </c>
+      <c r="J16" s="5">
+        <v>16</v>
+      </c>
+      <c r="K16" s="5">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+      <c r="L16" s="5">
+        <v>0</v>
+      </c>
+      <c r="M16" s="5">
         <f t="shared" si="4"/>
-        <v>306</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>240</v>
+      </c>
+      <c r="O16" s="11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B17" s="5">
         <v>27</v>
@@ -10336,20 +11245,43 @@
         <v>10</v>
       </c>
       <c r="D17" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>270</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
       </c>
       <c r="F17" s="5">
+        <f t="shared" si="6"/>
+        <v>270</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="I17" s="5">
+        <v>18</v>
+      </c>
+      <c r="J17" s="5">
+        <v>13</v>
+      </c>
+      <c r="K17" s="5">
+        <f t="shared" si="3"/>
+        <v>234</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0</v>
+      </c>
+      <c r="M17" s="5">
         <f t="shared" si="4"/>
-        <v>270</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>234</v>
+      </c>
+      <c r="O17" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B18" s="5">
         <v>10</v>
@@ -10358,18 +11290,38 @@
         <v>6</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="E18" s="5">
         <v>0</v>
       </c>
       <c r="F18" s="5">
+        <f t="shared" si="6"/>
+        <v>60</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="I18" s="5">
+        <v>102</v>
+      </c>
+      <c r="J18" s="5">
+        <v>4.3</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" si="3"/>
+        <v>438.59999999999997</v>
+      </c>
+      <c r="L18" s="5">
+        <v>0</v>
+      </c>
+      <c r="M18" s="5">
         <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>438.59999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="10" t="s">
         <v>169</v>
       </c>
@@ -10380,18 +11332,38 @@
         <v>16</v>
       </c>
       <c r="D19" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>208</v>
       </c>
       <c r="E19" s="5">
         <v>0</v>
       </c>
       <c r="F19" s="5">
+        <f t="shared" si="6"/>
+        <v>208</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="I19" s="5">
+        <v>30</v>
+      </c>
+      <c r="J19" s="5">
+        <v>5</v>
+      </c>
+      <c r="K19" s="5">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="L19" s="5">
+        <v>0</v>
+      </c>
+      <c r="M19" s="5">
         <f t="shared" si="4"/>
-        <v>208</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="10" t="s">
         <v>170</v>
       </c>
@@ -10402,18 +11374,38 @@
         <v>16</v>
       </c>
       <c r="D20" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>240</v>
       </c>
       <c r="E20" s="5">
         <v>0</v>
       </c>
       <c r="F20" s="5">
+        <f t="shared" si="6"/>
+        <v>240</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="I20" s="5">
+        <v>100</v>
+      </c>
+      <c r="J20" s="5">
+        <v>3</v>
+      </c>
+      <c r="K20" s="5">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="L20" s="5">
+        <v>0</v>
+      </c>
+      <c r="M20" s="5">
         <f t="shared" si="4"/>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="10" t="s">
         <v>171</v>
       </c>
@@ -10424,18 +11416,18 @@
         <v>3</v>
       </c>
       <c r="D21" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>300</v>
       </c>
       <c r="E21" s="5">
         <v>0</v>
       </c>
       <c r="F21" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:15">
       <c r="A22" s="10" t="s">
         <v>172</v>
       </c>
@@ -10446,18 +11438,24 @@
         <v>13</v>
       </c>
       <c r="D22" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>234</v>
       </c>
       <c r="E22" s="5">
         <v>0</v>
       </c>
       <c r="F22" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>234</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="H22" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="10" t="s">
         <v>179</v>
       </c>
@@ -10468,18 +11466,24 @@
         <v>4.3</v>
       </c>
       <c r="D23" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>438.59999999999997</v>
       </c>
       <c r="E23" s="5">
         <v>0</v>
       </c>
       <c r="F23" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>438.59999999999997</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="H23" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="I23" s="5">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="10" t="s">
         <v>178</v>
       </c>
@@ -10490,18 +11494,24 @@
         <v>5</v>
       </c>
       <c r="D24" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="E24" s="5">
         <v>0</v>
       </c>
       <c r="F24" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="H24" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="I24" s="13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="10" t="s">
         <v>177</v>
       </c>
@@ -10513,6 +11523,52 @@
         <f>SUM(F13:F24)</f>
         <v>2480.6</v>
       </c>
+      <c r="H25" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="I25" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="H26" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="I26" s="5">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="H27" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="I27" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="H28" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="I28" s="5">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="H29" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="I29" s="5">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="H30" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="I30" s="13">
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10521,31 +11577,37 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:15">
       <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>176</v>
+      </c>
       <c r="D1" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="E1" s="10" t="s">
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="10" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="B2" s="5">
         <v>1.5</v>
@@ -10559,10 +11621,25 @@
       <c r="E2" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="J2" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B3" s="5">
         <v>1.5</v>
@@ -10576,8 +11653,14 @@
       <c r="E3" s="5">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="J3" s="44" t="s">
+        <v>276</v>
+      </c>
+      <c r="K3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="10" t="s">
         <v>80</v>
       </c>
@@ -10588,7 +11671,163 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="B6" s="5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="B7" s="5">
+        <v>400</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="B8" s="5">
+        <f>B6*B7</f>
+        <v>48000</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="E8" s="5">
+        <v>30</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="D9" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="E9" s="5">
+        <v>20</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="D10" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="E10" s="5">
+        <v>20</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="D11" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="E11" s="5">
+        <v>3</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="D12" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="E12" s="5">
+        <v>7</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="D13" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="E13" s="5">
+        <v>3</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="D14" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="E14" s="5">
+        <v>5</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="D15" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="E15" s="5">
+        <v>2</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="D16" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="4:6">
+      <c r="D17" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="E17" s="5">
+        <v>45</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6">
+      <c r="D18" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="E18" s="5">
+        <v>85</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6">
+      <c r="D19" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="E19" s="5">
+        <v>85</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6">
+      <c r="D20" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="E20" s="5">
+        <v>40</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added details for 23/08/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13965" windowHeight="5625" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13965" windowHeight="5625" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="PaidTillDate" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="Tiles" sheetId="11" r:id="rId8"/>
     <sheet name="DoorsWindows" sheetId="12" r:id="rId9"/>
     <sheet name="Electricity" sheetId="13" r:id="rId10"/>
+    <sheet name="Railings" sheetId="14" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="291">
   <si>
     <t>Date</t>
   </si>
@@ -878,6 +879,24 @@
   </si>
   <si>
     <t>INFY</t>
+  </si>
+  <si>
+    <t>Gate</t>
+  </si>
+  <si>
+    <t>Pillars</t>
+  </si>
+  <si>
+    <t>Length (feet)</t>
+  </si>
+  <si>
+    <t>Breadth (feet)</t>
+  </si>
+  <si>
+    <t>22/08/2017</t>
+  </si>
+  <si>
+    <t>23/08/2017</t>
   </si>
 </sst>
 </file>
@@ -887,7 +906,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -938,6 +957,22 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1015,7 +1050,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1067,6 +1102,22 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6824,25 +6875,98 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="9" customFormat="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:4" s="9" customFormat="1">
+      <c r="A1" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="B2" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="C2" s="5">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="5">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5">
+        <v>118</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Y27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="9" customFormat="1">
+      <c r="A1" s="47" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="28" t="s">
@@ -6884,16 +7008,28 @@
       <c r="N1" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="O1" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="P1" s="28" t="s">
         <v>283</v>
       </c>
-      <c r="Q1" s="29"/>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="8" t="s">
+      <c r="Q1" s="28" t="s">
+        <v>289</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" s="48" t="s">
         <v>139</v>
       </c>
       <c r="B2" s="5"/>
@@ -6938,9 +7074,19 @@
       <c r="Q2" s="5">
         <v>274.05</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="8" t="s">
+      <c r="R2" s="5">
+        <v>278.7</v>
+      </c>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" s="48" t="s">
         <v>138</v>
       </c>
       <c r="B3" s="5"/>
@@ -6985,9 +7131,19 @@
       <c r="Q3" s="5">
         <v>294</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="8" t="s">
+      <c r="R3" s="5">
+        <v>298.60000000000002</v>
+      </c>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" s="48" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="29">
@@ -7038,9 +7194,19 @@
       <c r="Q4" s="29">
         <v>283</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="8" t="s">
+      <c r="R4" s="5">
+        <v>281.95</v>
+      </c>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" s="48" t="s">
         <v>124</v>
       </c>
       <c r="B5" s="31">
@@ -7091,9 +7257,19 @@
       <c r="Q5" s="31">
         <v>1560.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="5" t="s">
+      <c r="R5" s="46">
+        <v>1582.55</v>
+      </c>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" s="49" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="29">
@@ -7144,9 +7320,19 @@
       <c r="Q6" s="29">
         <v>241</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="5" t="s">
+      <c r="R6" s="5">
+        <v>241.35</v>
+      </c>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" s="49" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="29">
@@ -7197,9 +7383,19 @@
       <c r="Q7" s="29">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="5" t="s">
+      <c r="R7" s="5">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="A8" s="49" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="29">
@@ -7250,9 +7446,19 @@
       <c r="Q8" s="29">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="7" t="s">
+      <c r="R8" s="5">
+        <v>60.8</v>
+      </c>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9" s="47" t="s">
         <v>149</v>
       </c>
       <c r="B9" s="7"/>
@@ -7295,9 +7501,19 @@
       <c r="Q9" s="7">
         <v>54.75</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="5" t="s">
+      <c r="R9" s="5">
+        <v>55.65</v>
+      </c>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="A10" s="49" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="29">
@@ -7348,9 +7564,19 @@
       <c r="Q10" s="29">
         <v>38.65</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="5" t="s">
+      <c r="R10" s="5">
+        <v>39.1</v>
+      </c>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="A11" s="49" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="29">
@@ -7401,9 +7627,19 @@
       <c r="Q11" s="29">
         <v>69.599999999999994</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="5" t="s">
+      <c r="R11" s="5">
+        <v>69.8</v>
+      </c>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12" s="49" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="29">
@@ -7454,9 +7690,19 @@
       <c r="Q12" s="29">
         <v>88.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="5" t="s">
+      <c r="R12" s="5">
+        <v>90.35</v>
+      </c>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="A13" s="49" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="29">
@@ -7507,9 +7753,19 @@
       <c r="Q13" s="29">
         <v>125.9</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="5" t="s">
+      <c r="R13" s="5">
+        <v>128.05000000000001</v>
+      </c>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14" s="49" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="29">
@@ -7560,9 +7816,19 @@
       <c r="Q14" s="29">
         <v>80.099999999999994</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15" s="5" t="s">
+      <c r="R14" s="5">
+        <v>78.7</v>
+      </c>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="A15" s="49" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="29">
@@ -7613,9 +7879,19 @@
       <c r="Q15" s="29">
         <v>48.85</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="5" t="s">
+      <c r="R15" s="5">
+        <v>50.65</v>
+      </c>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="A16" s="49" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="29">
@@ -7666,9 +7942,19 @@
       <c r="Q16" s="29">
         <v>32.049999999999997</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17" s="29" t="s">
+      <c r="R16" s="5">
+        <v>32.15</v>
+      </c>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+    </row>
+    <row r="17" spans="1:25">
+      <c r="A17" s="49" t="s">
         <v>150</v>
       </c>
       <c r="B17" s="29"/>
@@ -7711,9 +7997,19 @@
       <c r="Q17" s="29">
         <v>30.35</v>
       </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18" s="5" t="s">
+      <c r="R17" s="5">
+        <v>30.25</v>
+      </c>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+    </row>
+    <row r="18" spans="1:25">
+      <c r="A18" s="49" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="29">
@@ -7764,9 +8060,19 @@
       <c r="Q18" s="29">
         <v>621.6</v>
       </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19" s="8" t="s">
+      <c r="R18" s="5">
+        <v>635.25</v>
+      </c>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+    </row>
+    <row r="19" spans="1:25">
+      <c r="A19" s="48" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="29">
@@ -7817,9 +8123,19 @@
       <c r="Q19" s="29">
         <v>473.7</v>
       </c>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="A20" s="8" t="s">
+      <c r="R19" s="5">
+        <v>460</v>
+      </c>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+    </row>
+    <row r="20" spans="1:25">
+      <c r="A20" s="48" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="29">
@@ -7870,9 +8186,19 @@
       <c r="Q20" s="29">
         <v>198</v>
       </c>
-    </row>
-    <row r="21" spans="1:17">
-      <c r="A21" s="8" t="s">
+      <c r="R20" s="5">
+        <v>201.9</v>
+      </c>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
+    </row>
+    <row r="21" spans="1:25">
+      <c r="A21" s="48" t="s">
         <v>50</v>
       </c>
       <c r="B21" s="29">
@@ -7923,9 +8249,19 @@
       <c r="Q21" s="29">
         <v>446.05</v>
       </c>
-    </row>
-    <row r="22" spans="1:17">
-      <c r="A22" s="8" t="s">
+      <c r="R21" s="5">
+        <v>460.25</v>
+      </c>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
+    </row>
+    <row r="22" spans="1:25">
+      <c r="A22" s="48" t="s">
         <v>121</v>
       </c>
       <c r="B22" s="31">
@@ -7976,9 +8312,19 @@
       <c r="Q22" s="29">
         <v>694.3</v>
       </c>
-    </row>
-    <row r="23" spans="1:17">
-      <c r="A23" s="8" t="s">
+      <c r="R22" s="5">
+        <v>698.85</v>
+      </c>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+    </row>
+    <row r="23" spans="1:25">
+      <c r="A23" s="48" t="s">
         <v>126</v>
       </c>
       <c r="B23" s="29">
@@ -8029,9 +8375,19 @@
       <c r="Q23" s="29">
         <v>424.9</v>
       </c>
-    </row>
-    <row r="24" spans="1:17">
-      <c r="A24" s="5" t="s">
+      <c r="R23" s="5">
+        <v>433.5</v>
+      </c>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="5"/>
+    </row>
+    <row r="24" spans="1:25">
+      <c r="A24" s="49" t="s">
         <v>135</v>
       </c>
       <c r="B24" s="5"/>
@@ -8076,9 +8432,19 @@
       <c r="Q24" s="5">
         <v>73.3</v>
       </c>
-    </row>
-    <row r="25" spans="1:17">
-      <c r="A25" s="5" t="s">
+      <c r="R24" s="5">
+        <v>73.8</v>
+      </c>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5"/>
+    </row>
+    <row r="25" spans="1:25">
+      <c r="A25" s="49" t="s">
         <v>151</v>
       </c>
       <c r="B25" s="5"/>
@@ -8121,9 +8487,19 @@
       <c r="Q25" s="5">
         <v>59.85</v>
       </c>
-    </row>
-    <row r="26" spans="1:17">
-      <c r="A26" s="29" t="s">
+      <c r="R25" s="5">
+        <v>61.45</v>
+      </c>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+    </row>
+    <row r="26" spans="1:25">
+      <c r="A26" s="49" t="s">
         <v>154</v>
       </c>
       <c r="B26" s="5"/>
@@ -8162,9 +8538,19 @@
       <c r="Q26" s="5">
         <v>225.2</v>
       </c>
-    </row>
-    <row r="27" spans="1:17">
-      <c r="A27" s="42" t="s">
+      <c r="R26" s="5">
+        <v>226.2</v>
+      </c>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+    </row>
+    <row r="27" spans="1:25">
+      <c r="A27" s="50" t="s">
         <v>284</v>
       </c>
       <c r="B27" s="5"/>
@@ -8185,6 +8571,16 @@
       <c r="Q27" s="5">
         <v>876</v>
       </c>
+      <c r="R27" s="5">
+        <v>893.4</v>
+      </c>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
     </row>
   </sheetData>
   <sortState ref="I1:I37">
@@ -10646,7 +11042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated the sheet for 29082017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="298">
   <si>
     <t>Date</t>
   </si>
@@ -913,6 +913,12 @@
   </si>
   <si>
     <t>31/08/2017</t>
+  </si>
+  <si>
+    <t>Mimimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
   </si>
 </sst>
 </file>
@@ -6981,1725 +6987,1914 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y27"/>
+  <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V9" sqref="V9"/>
+      <pane xSplit="3" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA17" sqref="AA17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="E1" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="F1" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="E1" s="12">
+      <c r="G1" s="12">
         <v>42743</v>
       </c>
-      <c r="F1" s="12">
+      <c r="H1" s="12">
         <v>42774</v>
       </c>
-      <c r="G1" s="12">
+      <c r="I1" s="12">
         <v>42802</v>
       </c>
-      <c r="H1" s="12">
+      <c r="J1" s="12">
         <v>42833</v>
       </c>
-      <c r="I1" s="12">
+      <c r="K1" s="12">
         <v>42924</v>
       </c>
-      <c r="J1" s="12">
+      <c r="L1" s="12">
         <v>42955</v>
       </c>
-      <c r="K1" s="12">
+      <c r="M1" s="12">
         <v>42986</v>
       </c>
-      <c r="L1" s="12">
+      <c r="N1" s="12">
         <v>43016</v>
       </c>
-      <c r="M1" s="12">
+      <c r="O1" s="12">
         <v>43047</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="Q1" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="R1" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="S1" s="28" t="s">
         <v>288</v>
       </c>
-      <c r="R1" s="28" t="s">
+      <c r="T1" s="28" t="s">
         <v>289</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="U1" s="28" t="s">
         <v>290</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="V1" s="28" t="s">
         <v>292</v>
       </c>
-      <c r="U1" s="28" t="s">
+      <c r="W1" s="28" t="s">
         <v>293</v>
       </c>
-      <c r="V1" s="28" t="s">
+      <c r="X1" s="28" t="s">
         <v>294</v>
       </c>
-      <c r="W1" s="28" t="s">
+      <c r="Y1" s="28" t="s">
         <v>295</v>
       </c>
-      <c r="X1" s="12">
+      <c r="Z1" s="12">
         <v>42744</v>
       </c>
-      <c r="Y1" s="28"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="B2" s="13">
+        <f>MIN(D2:ZZ2)</f>
+        <v>274.05</v>
+      </c>
+      <c r="C2" s="13">
+        <f>MAX(D2:ZZ2)</f>
+        <v>310.60000000000002</v>
+      </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="5">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5">
         <v>309.25</v>
       </c>
-      <c r="F2" s="5">
+      <c r="H2" s="5">
         <v>306</v>
       </c>
-      <c r="G2" s="5">
+      <c r="I2" s="5">
         <v>300.64999999999998</v>
       </c>
-      <c r="H2" s="5">
+      <c r="J2" s="5">
         <v>305.8</v>
       </c>
-      <c r="I2" s="5">
+      <c r="K2" s="5">
         <v>310.60000000000002</v>
       </c>
-      <c r="J2" s="5">
+      <c r="L2" s="5">
         <v>305</v>
       </c>
-      <c r="K2" s="5">
+      <c r="M2" s="5">
         <v>302.95</v>
       </c>
-      <c r="L2" s="5">
+      <c r="N2" s="5">
         <v>298</v>
       </c>
-      <c r="M2" s="5">
+      <c r="O2" s="5">
         <v>280.35000000000002</v>
       </c>
-      <c r="N2" s="5">
+      <c r="P2" s="5">
         <v>280</v>
       </c>
-      <c r="O2" s="5">
+      <c r="Q2" s="5">
         <v>283.2</v>
       </c>
-      <c r="P2" s="5">
+      <c r="R2" s="5">
         <v>274.55</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="S2" s="5">
         <v>274.05</v>
       </c>
-      <c r="R2" s="5">
+      <c r="T2" s="5">
         <v>278.7</v>
       </c>
-      <c r="S2" s="5">
+      <c r="U2" s="5">
         <v>280.10000000000002</v>
       </c>
-      <c r="T2" s="5">
+      <c r="V2" s="5">
         <v>279.3</v>
       </c>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z2" s="5"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="13">
+        <f t="shared" ref="B3:B27" si="0">MIN(D3:ZZ3)</f>
+        <v>285.8</v>
+      </c>
+      <c r="C3" s="13">
+        <f t="shared" ref="C3:C27" si="1">MAX(D3:ZZ3)</f>
+        <v>302.7</v>
+      </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="5">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5">
         <v>302.7</v>
       </c>
-      <c r="F3" s="5">
+      <c r="H3" s="5">
         <v>301.39999999999998</v>
       </c>
-      <c r="G3" s="5">
+      <c r="I3" s="5">
         <v>295.10000000000002</v>
       </c>
-      <c r="H3" s="5">
+      <c r="J3" s="5">
         <v>296.8</v>
       </c>
-      <c r="I3" s="5">
+      <c r="K3" s="5">
         <v>300</v>
       </c>
-      <c r="J3" s="5">
+      <c r="L3" s="5">
         <v>295.95</v>
       </c>
-      <c r="K3" s="5">
+      <c r="M3" s="5">
         <v>290.64999999999998</v>
-      </c>
-      <c r="L3" s="5">
-        <v>291</v>
-      </c>
-      <c r="M3" s="5">
-        <v>285.8</v>
       </c>
       <c r="N3" s="5">
         <v>291</v>
       </c>
       <c r="O3" s="5">
+        <v>285.8</v>
+      </c>
+      <c r="P3" s="5">
+        <v>291</v>
+      </c>
+      <c r="Q3" s="5">
         <v>295.2</v>
       </c>
-      <c r="P3" s="5">
+      <c r="R3" s="5">
         <v>293.35000000000002</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="S3" s="5">
         <v>294</v>
       </c>
-      <c r="R3" s="5">
+      <c r="T3" s="5">
         <v>298.60000000000002</v>
       </c>
-      <c r="S3" s="5">
+      <c r="U3" s="5">
         <v>298.95</v>
       </c>
-      <c r="T3" s="5">
+      <c r="V3" s="5">
         <v>301</v>
       </c>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z3" s="5"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="13">
+        <f t="shared" si="0"/>
+        <v>271.2</v>
+      </c>
+      <c r="C4" s="13">
+        <f t="shared" si="1"/>
         <v>291.7</v>
       </c>
-      <c r="C4" s="29">
+      <c r="D4" s="29">
+        <v>291.7</v>
+      </c>
+      <c r="E4" s="29">
         <v>290.35000000000002</v>
       </c>
-      <c r="D4" s="29">
+      <c r="F4" s="29">
         <v>285.25</v>
       </c>
-      <c r="E4" s="29">
+      <c r="G4" s="29">
         <v>287.75</v>
       </c>
-      <c r="F4" s="29">
+      <c r="H4" s="29">
         <v>284.85000000000002</v>
       </c>
-      <c r="G4" s="29">
+      <c r="I4" s="29">
         <v>280.89999999999998</v>
       </c>
-      <c r="H4" s="29">
+      <c r="J4" s="29">
         <v>280.8</v>
       </c>
-      <c r="I4" s="29">
+      <c r="K4" s="29">
         <v>279.5</v>
       </c>
-      <c r="J4" s="29">
+      <c r="L4" s="29">
         <v>273.85000000000002</v>
       </c>
-      <c r="K4" s="29">
+      <c r="M4" s="29">
         <v>272.8</v>
       </c>
-      <c r="L4" s="29">
+      <c r="N4" s="29">
         <v>273.8</v>
       </c>
-      <c r="M4" s="29">
+      <c r="O4" s="29">
         <v>271.2</v>
       </c>
-      <c r="N4" s="29">
+      <c r="P4" s="29">
         <v>271.3</v>
       </c>
-      <c r="O4" s="29">
+      <c r="Q4" s="29">
         <v>279.2</v>
       </c>
-      <c r="P4" s="29">
+      <c r="R4" s="29">
         <v>282.45</v>
       </c>
-      <c r="Q4" s="29">
+      <c r="S4" s="29">
         <v>283</v>
       </c>
-      <c r="R4" s="5">
+      <c r="T4" s="5">
         <v>281.95</v>
       </c>
-      <c r="S4" s="5">
+      <c r="U4" s="5">
         <v>281.5</v>
       </c>
-      <c r="T4" s="5">
+      <c r="V4" s="5">
         <v>282.89999999999998</v>
       </c>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z4" s="5"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="13">
+        <f t="shared" si="0"/>
+        <v>1545.5</v>
+      </c>
+      <c r="C5" s="13">
+        <f t="shared" si="1"/>
+        <v>1654</v>
+      </c>
+      <c r="D5" s="31">
         <v>1592.8</v>
       </c>
-      <c r="C5" s="31">
+      <c r="E5" s="31">
         <v>1594</v>
       </c>
-      <c r="D5" s="31">
+      <c r="F5" s="31">
         <v>1615.45</v>
       </c>
-      <c r="E5" s="31">
+      <c r="G5" s="31">
         <v>1605.8</v>
       </c>
-      <c r="F5" s="31">
+      <c r="H5" s="31">
         <v>1628.55</v>
       </c>
-      <c r="G5" s="31">
+      <c r="I5" s="31">
         <v>1654</v>
       </c>
-      <c r="H5" s="31">
+      <c r="J5" s="31">
         <v>1626.5</v>
       </c>
-      <c r="I5" s="31">
+      <c r="K5" s="31">
         <v>1618</v>
       </c>
-      <c r="J5" s="31">
+      <c r="L5" s="31">
         <v>1604.6</v>
       </c>
-      <c r="K5" s="31">
+      <c r="M5" s="31">
         <v>1600.3</v>
       </c>
-      <c r="L5" s="31">
+      <c r="N5" s="31">
         <v>1593.75</v>
       </c>
-      <c r="M5" s="31">
+      <c r="O5" s="31">
         <v>1545.5</v>
       </c>
-      <c r="N5" s="31">
+      <c r="P5" s="31">
         <v>1575.05</v>
       </c>
-      <c r="O5" s="31">
+      <c r="Q5" s="31">
         <v>1576</v>
       </c>
-      <c r="P5" s="31">
+      <c r="R5" s="31">
         <v>1564.3</v>
       </c>
-      <c r="Q5" s="31">
+      <c r="S5" s="31">
         <v>1560.1</v>
       </c>
-      <c r="R5" s="45">
+      <c r="T5" s="45">
         <v>1582.55</v>
       </c>
-      <c r="S5" s="45">
+      <c r="U5" s="45">
         <v>1570</v>
       </c>
-      <c r="T5" s="45">
+      <c r="V5" s="45">
         <v>1564.75</v>
       </c>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z5" s="5"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="13">
+        <f t="shared" si="0"/>
+        <v>236.45</v>
+      </c>
+      <c r="C6" s="13">
+        <f t="shared" si="1"/>
         <v>255.5</v>
       </c>
-      <c r="C6" s="29">
+      <c r="D6" s="29">
+        <v>255.5</v>
+      </c>
+      <c r="E6" s="29">
         <v>251.1</v>
       </c>
-      <c r="D6" s="29">
+      <c r="F6" s="29">
         <v>249.65</v>
       </c>
-      <c r="E6" s="29">
+      <c r="G6" s="29">
         <v>251.8</v>
       </c>
-      <c r="F6" s="29">
+      <c r="H6" s="29">
         <v>251.05</v>
       </c>
-      <c r="G6" s="29">
+      <c r="I6" s="29">
         <v>242</v>
       </c>
-      <c r="H6" s="29">
+      <c r="J6" s="29">
         <v>249.2</v>
       </c>
-      <c r="I6" s="29">
+      <c r="K6" s="29">
         <v>251.25</v>
       </c>
-      <c r="J6" s="29">
+      <c r="L6" s="29">
         <v>244.4</v>
       </c>
-      <c r="K6" s="29">
+      <c r="M6" s="29">
         <v>243.1</v>
       </c>
-      <c r="L6" s="29">
+      <c r="N6" s="29">
         <v>239.45</v>
       </c>
-      <c r="M6" s="29">
+      <c r="O6" s="29">
         <v>236.45</v>
       </c>
-      <c r="N6" s="29">
+      <c r="P6" s="29">
         <v>237.9</v>
       </c>
-      <c r="O6" s="29">
+      <c r="Q6" s="29">
         <v>238.45</v>
       </c>
-      <c r="P6" s="29">
+      <c r="R6" s="29">
         <v>239.2</v>
       </c>
-      <c r="Q6" s="29">
+      <c r="S6" s="29">
         <v>241</v>
       </c>
-      <c r="R6" s="5">
+      <c r="T6" s="5">
         <v>241.35</v>
       </c>
-      <c r="S6" s="5">
+      <c r="U6" s="5">
         <v>241.65</v>
       </c>
-      <c r="T6" s="5">
+      <c r="V6" s="5">
         <v>242.8</v>
       </c>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
       <c r="W6" s="5"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z6" s="5"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="13">
+        <f t="shared" si="0"/>
+        <v>15.6</v>
+      </c>
+      <c r="C7" s="13">
+        <f t="shared" si="1"/>
         <v>19.350000000000001</v>
       </c>
-      <c r="C7" s="29">
+      <c r="D7" s="29">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="E7" s="29">
         <v>18.95</v>
       </c>
-      <c r="D7" s="29">
+      <c r="F7" s="29">
         <v>18.75</v>
       </c>
-      <c r="E7" s="29">
+      <c r="G7" s="29">
         <v>18.7</v>
       </c>
-      <c r="F7" s="29">
+      <c r="H7" s="29">
         <v>18.399999999999999</v>
       </c>
-      <c r="G7" s="29">
+      <c r="I7" s="29">
         <v>17.95</v>
-      </c>
-      <c r="H7" s="29">
-        <v>17.649999999999999</v>
-      </c>
-      <c r="I7" s="29">
-        <v>18.55</v>
       </c>
       <c r="J7" s="29">
         <v>17.649999999999999</v>
       </c>
       <c r="K7" s="29">
+        <v>18.55</v>
+      </c>
+      <c r="L7" s="29">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="M7" s="29">
         <v>17.05</v>
       </c>
-      <c r="L7" s="29">
+      <c r="N7" s="29">
         <v>16.149999999999999</v>
       </c>
-      <c r="M7" s="29">
+      <c r="O7" s="29">
         <v>15.6</v>
       </c>
-      <c r="N7" s="29">
+      <c r="P7" s="29">
         <v>16.2</v>
       </c>
-      <c r="O7" s="29">
+      <c r="Q7" s="29">
         <v>16.600000000000001</v>
       </c>
-      <c r="P7" s="29">
+      <c r="R7" s="29">
         <v>17.5</v>
       </c>
-      <c r="Q7" s="29">
+      <c r="S7" s="29">
         <v>17</v>
       </c>
-      <c r="R7" s="5">
+      <c r="T7" s="5">
         <v>17.100000000000001</v>
       </c>
-      <c r="S7" s="5">
+      <c r="U7" s="5">
         <v>17.2</v>
       </c>
-      <c r="T7" s="5">
+      <c r="V7" s="5">
         <v>17.350000000000001</v>
       </c>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
       <c r="W7" s="5"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z7" s="5"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="13">
+        <f t="shared" si="0"/>
+        <v>56.6</v>
+      </c>
+      <c r="C8" s="13">
+        <f t="shared" si="1"/>
         <v>63.3</v>
-      </c>
-      <c r="C8" s="29">
-        <v>62.6</v>
       </c>
       <c r="D8" s="29">
         <v>63.3</v>
       </c>
       <c r="E8" s="29">
+        <v>62.6</v>
+      </c>
+      <c r="F8" s="29">
+        <v>63.3</v>
+      </c>
+      <c r="G8" s="29">
         <v>63.25</v>
       </c>
-      <c r="F8" s="29">
+      <c r="H8" s="29">
         <v>63.2</v>
       </c>
-      <c r="G8" s="29">
+      <c r="I8" s="29">
         <v>60.75</v>
       </c>
-      <c r="H8" s="29">
+      <c r="J8" s="29">
         <v>61.9</v>
       </c>
-      <c r="I8" s="29">
+      <c r="K8" s="29">
         <v>62.15</v>
       </c>
-      <c r="J8" s="29">
+      <c r="L8" s="29">
         <v>62.95</v>
       </c>
-      <c r="K8" s="29">
+      <c r="M8" s="29">
         <v>61.85</v>
       </c>
-      <c r="L8" s="29">
+      <c r="N8" s="29">
         <v>59.15</v>
       </c>
-      <c r="M8" s="29">
+      <c r="O8" s="29">
         <v>56.6</v>
       </c>
-      <c r="N8" s="29">
+      <c r="P8" s="29">
         <v>57.9</v>
       </c>
-      <c r="O8" s="29">
+      <c r="Q8" s="29">
         <v>59.55</v>
       </c>
-      <c r="P8" s="29">
+      <c r="R8" s="29">
         <v>59.2</v>
       </c>
-      <c r="Q8" s="29">
+      <c r="S8" s="29">
         <v>59</v>
       </c>
-      <c r="R8" s="5">
+      <c r="T8" s="5">
         <v>60.8</v>
       </c>
-      <c r="S8" s="5">
+      <c r="U8" s="5">
         <v>60.75</v>
       </c>
-      <c r="T8" s="5">
+      <c r="V8" s="5">
         <v>61.45</v>
       </c>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
       <c r="W8" s="5"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z8" s="5"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="13">
+        <f t="shared" si="0"/>
+        <v>53.5</v>
+      </c>
+      <c r="C9" s="13">
+        <f t="shared" si="1"/>
+        <v>58.2</v>
+      </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="7">
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7">
         <v>58.2</v>
       </c>
-      <c r="G9" s="7">
+      <c r="I9" s="7">
         <v>57.95</v>
       </c>
-      <c r="H9" s="7">
+      <c r="J9" s="7">
         <v>57.25</v>
       </c>
-      <c r="I9" s="7">
+      <c r="K9" s="7">
         <v>57.75</v>
       </c>
-      <c r="J9" s="7">
+      <c r="L9" s="7">
         <v>56.6</v>
       </c>
-      <c r="K9" s="7">
+      <c r="M9" s="7">
         <v>56.4</v>
-      </c>
-      <c r="L9" s="7">
-        <v>54.45</v>
-      </c>
-      <c r="M9" s="7">
-        <v>53.5</v>
       </c>
       <c r="N9" s="7">
         <v>54.45</v>
       </c>
       <c r="O9" s="7">
+        <v>53.5</v>
+      </c>
+      <c r="P9" s="7">
+        <v>54.45</v>
+      </c>
+      <c r="Q9" s="7">
         <v>55.85</v>
       </c>
-      <c r="P9" s="7">
+      <c r="R9" s="7">
         <v>54.55</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="S9" s="7">
         <v>54.75</v>
       </c>
-      <c r="R9" s="5">
+      <c r="T9" s="5">
         <v>55.65</v>
       </c>
-      <c r="S9" s="5">
+      <c r="U9" s="5">
         <v>55.15</v>
       </c>
-      <c r="T9" s="5">
+      <c r="V9" s="5">
         <v>56</v>
       </c>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
       <c r="W9" s="5"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="5"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z9" s="5"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="13">
+        <f t="shared" si="0"/>
+        <v>38.6</v>
+      </c>
+      <c r="C10" s="13">
+        <f t="shared" si="1"/>
+        <v>45.25</v>
+      </c>
+      <c r="D10" s="29">
         <v>45.1</v>
       </c>
-      <c r="C10" s="29">
+      <c r="E10" s="29">
         <v>45.25</v>
       </c>
-      <c r="D10" s="29">
+      <c r="F10" s="29">
         <v>45.15</v>
       </c>
-      <c r="E10" s="29">
+      <c r="G10" s="29">
         <v>44.25</v>
       </c>
-      <c r="F10" s="29">
+      <c r="H10" s="29">
         <v>43.9</v>
       </c>
-      <c r="G10" s="29">
+      <c r="I10" s="29">
         <v>42.5</v>
       </c>
-      <c r="H10" s="29">
+      <c r="J10" s="29">
         <v>42.4</v>
       </c>
-      <c r="I10" s="29">
+      <c r="K10" s="29">
         <v>42.95</v>
       </c>
-      <c r="J10" s="29">
+      <c r="L10" s="29">
         <v>41.8</v>
       </c>
-      <c r="K10" s="29">
+      <c r="M10" s="29">
         <v>41.35</v>
       </c>
-      <c r="L10" s="29">
+      <c r="N10" s="29">
         <v>39.15</v>
       </c>
-      <c r="M10" s="29">
+      <c r="O10" s="29">
         <v>38.6</v>
       </c>
-      <c r="N10" s="29">
+      <c r="P10" s="29">
         <v>40</v>
       </c>
-      <c r="O10" s="29">
+      <c r="Q10" s="29">
         <v>40.700000000000003</v>
       </c>
-      <c r="P10" s="29">
+      <c r="R10" s="29">
         <v>39.200000000000003</v>
       </c>
-      <c r="Q10" s="29">
+      <c r="S10" s="29">
         <v>38.65</v>
       </c>
-      <c r="R10" s="5">
+      <c r="T10" s="5">
         <v>39.1</v>
       </c>
-      <c r="S10" s="5">
+      <c r="U10" s="5">
         <v>39.549999999999997</v>
       </c>
-      <c r="T10" s="5">
+      <c r="V10" s="5">
         <v>40.25</v>
       </c>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
       <c r="W10" s="5"/>
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z10" s="5"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="13">
+        <f t="shared" si="0"/>
+        <v>62.6</v>
+      </c>
+      <c r="C11" s="13">
+        <f t="shared" si="1"/>
+        <v>70.75</v>
+      </c>
+      <c r="D11" s="29">
         <v>70.150000000000006</v>
       </c>
-      <c r="C11" s="29">
+      <c r="E11" s="29">
         <v>69.45</v>
       </c>
-      <c r="D11" s="29">
+      <c r="F11" s="29">
         <v>70</v>
       </c>
-      <c r="E11" s="29">
+      <c r="G11" s="29">
         <v>70</v>
       </c>
-      <c r="F11" s="29">
+      <c r="H11" s="29">
         <v>69.3</v>
       </c>
-      <c r="G11" s="29">
+      <c r="I11" s="29">
         <v>66.5</v>
       </c>
-      <c r="H11" s="29">
+      <c r="J11" s="29">
         <v>69.099999999999994</v>
       </c>
-      <c r="I11" s="29">
+      <c r="K11" s="29">
         <v>69.099999999999994</v>
       </c>
-      <c r="J11" s="29">
+      <c r="L11" s="29">
         <v>69.849999999999994</v>
       </c>
-      <c r="K11" s="29">
+      <c r="M11" s="29">
         <v>70.75</v>
       </c>
-      <c r="L11" s="29">
+      <c r="N11" s="29">
         <v>65.45</v>
       </c>
-      <c r="M11" s="29">
+      <c r="O11" s="29">
         <v>62.6</v>
       </c>
-      <c r="N11" s="29">
+      <c r="P11" s="29">
         <v>66.25</v>
       </c>
-      <c r="O11" s="29">
+      <c r="Q11" s="29">
         <v>68.849999999999994</v>
       </c>
-      <c r="P11" s="29">
+      <c r="R11" s="29">
         <v>68.900000000000006</v>
       </c>
-      <c r="Q11" s="29">
+      <c r="S11" s="29">
         <v>69.599999999999994</v>
       </c>
-      <c r="R11" s="5">
+      <c r="T11" s="5">
         <v>69.8</v>
       </c>
-      <c r="S11" s="5">
+      <c r="U11" s="5">
         <v>69.900000000000006</v>
       </c>
-      <c r="T11" s="5">
+      <c r="V11" s="5">
         <v>69.5</v>
       </c>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
       <c r="W11" s="5"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="5"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z11" s="5"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="29">
-        <v>92.35</v>
-      </c>
-      <c r="C12" s="29">
+      <c r="B12" s="13">
+        <f t="shared" si="0"/>
+        <v>86.5</v>
+      </c>
+      <c r="C12" s="13">
+        <f t="shared" si="1"/>
         <v>95.4</v>
       </c>
       <c r="D12" s="29">
         <v>92.35</v>
       </c>
       <c r="E12" s="29">
+        <v>95.4</v>
+      </c>
+      <c r="F12" s="29">
+        <v>92.35</v>
+      </c>
+      <c r="G12" s="29">
         <v>92.3</v>
       </c>
-      <c r="F12" s="29">
+      <c r="H12" s="29">
         <v>92.3</v>
       </c>
-      <c r="G12" s="29">
+      <c r="I12" s="29">
         <v>93.45</v>
       </c>
-      <c r="H12" s="29">
+      <c r="J12" s="29">
         <v>92.9</v>
       </c>
-      <c r="I12" s="29">
+      <c r="K12" s="29">
         <v>93.1</v>
       </c>
-      <c r="J12" s="29">
+      <c r="L12" s="29">
         <v>91.65</v>
       </c>
-      <c r="K12" s="29">
+      <c r="M12" s="29">
         <v>91.25</v>
       </c>
-      <c r="L12" s="29">
+      <c r="N12" s="29">
         <v>88.3</v>
       </c>
-      <c r="M12" s="29">
+      <c r="O12" s="29">
         <v>86.5</v>
       </c>
-      <c r="N12" s="29">
+      <c r="P12" s="29">
         <v>86.8</v>
       </c>
-      <c r="O12" s="29">
+      <c r="Q12" s="29">
         <v>86.95</v>
       </c>
-      <c r="P12" s="29">
+      <c r="R12" s="29">
         <v>88.75</v>
       </c>
-      <c r="Q12" s="29">
+      <c r="S12" s="29">
         <v>88.5</v>
       </c>
-      <c r="R12" s="5">
+      <c r="T12" s="5">
         <v>90.35</v>
       </c>
-      <c r="S12" s="5">
+      <c r="U12" s="5">
         <v>89.85</v>
       </c>
-      <c r="T12" s="5">
+      <c r="V12" s="5">
         <v>89.8</v>
       </c>
-      <c r="U12" s="5"/>
-      <c r="V12" s="5"/>
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z12" s="5"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="13">
+        <f t="shared" si="0"/>
+        <v>124.25</v>
+      </c>
+      <c r="C13" s="13">
+        <f t="shared" si="1"/>
+        <v>144.80000000000001</v>
+      </c>
+      <c r="D13" s="29">
         <v>142.5</v>
       </c>
-      <c r="C13" s="29">
+      <c r="E13" s="29">
         <v>143.75</v>
       </c>
-      <c r="D13" s="29">
+      <c r="F13" s="29">
         <v>144.80000000000001</v>
       </c>
-      <c r="E13" s="29">
+      <c r="G13" s="29">
         <v>144.35</v>
       </c>
-      <c r="F13" s="29">
+      <c r="H13" s="29">
         <v>140.9</v>
       </c>
-      <c r="G13" s="29">
+      <c r="I13" s="29">
         <v>138.65</v>
       </c>
-      <c r="H13" s="29">
+      <c r="J13" s="29">
         <v>137.1</v>
       </c>
-      <c r="I13" s="29">
+      <c r="K13" s="29">
         <v>138.35</v>
       </c>
-      <c r="J13" s="29">
+      <c r="L13" s="29">
         <v>134.5</v>
       </c>
-      <c r="K13" s="29">
+      <c r="M13" s="29">
         <v>133</v>
       </c>
-      <c r="L13" s="29">
+      <c r="N13" s="29">
         <v>128</v>
       </c>
-      <c r="M13" s="29">
+      <c r="O13" s="29">
         <v>125</v>
       </c>
-      <c r="N13" s="29">
+      <c r="P13" s="29">
         <v>126.95</v>
       </c>
-      <c r="O13" s="29">
+      <c r="Q13" s="29">
         <v>129.75</v>
       </c>
-      <c r="P13" s="29">
+      <c r="R13" s="29">
         <v>124.25</v>
       </c>
-      <c r="Q13" s="29">
+      <c r="S13" s="29">
         <v>125.9</v>
       </c>
-      <c r="R13" s="5">
+      <c r="T13" s="5">
         <v>128.05000000000001</v>
       </c>
-      <c r="S13" s="5">
+      <c r="U13" s="5">
         <v>127.15</v>
       </c>
-      <c r="T13" s="5">
+      <c r="V13" s="5">
         <v>127.7</v>
       </c>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
       <c r="W13" s="5"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z13" s="5"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="29">
+      <c r="B14" s="13">
+        <f t="shared" si="0"/>
+        <v>76.7</v>
+      </c>
+      <c r="C14" s="13">
+        <f t="shared" si="1"/>
+        <v>83.25</v>
+      </c>
+      <c r="D14" s="29">
         <v>82.1</v>
       </c>
-      <c r="C14" s="29">
+      <c r="E14" s="29">
         <v>82.55</v>
       </c>
-      <c r="D14" s="29">
+      <c r="F14" s="29">
         <v>82</v>
       </c>
-      <c r="E14" s="29">
+      <c r="G14" s="29">
         <v>83.25</v>
       </c>
-      <c r="F14" s="29">
+      <c r="H14" s="29">
         <v>82.55</v>
       </c>
-      <c r="G14" s="29">
+      <c r="I14" s="29">
         <v>82.45</v>
       </c>
-      <c r="H14" s="29">
+      <c r="J14" s="29">
         <v>80.2</v>
       </c>
-      <c r="I14" s="29">
+      <c r="K14" s="29">
         <v>80</v>
       </c>
-      <c r="J14" s="29">
+      <c r="L14" s="29">
         <v>78.150000000000006</v>
       </c>
-      <c r="K14" s="29">
+      <c r="M14" s="29">
         <v>77.8</v>
       </c>
-      <c r="L14" s="29">
+      <c r="N14" s="29">
         <v>77</v>
       </c>
-      <c r="M14" s="29">
+      <c r="O14" s="29">
         <v>76.7</v>
       </c>
-      <c r="N14" s="29">
+      <c r="P14" s="29">
         <v>80.05</v>
       </c>
-      <c r="O14" s="29">
+      <c r="Q14" s="29">
         <v>82</v>
       </c>
-      <c r="P14" s="29">
+      <c r="R14" s="29">
         <v>80.3</v>
       </c>
-      <c r="Q14" s="29">
+      <c r="S14" s="29">
         <v>80.099999999999994</v>
       </c>
-      <c r="R14" s="5">
+      <c r="T14" s="5">
         <v>78.7</v>
       </c>
-      <c r="S14" s="5">
+      <c r="U14" s="5">
         <v>79.05</v>
       </c>
-      <c r="T14" s="5">
+      <c r="V14" s="5">
         <v>79</v>
       </c>
-      <c r="U14" s="5"/>
-      <c r="V14" s="5"/>
       <c r="W14" s="5"/>
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z14" s="5"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="13">
+        <f t="shared" si="0"/>
+        <v>48.85</v>
+      </c>
+      <c r="C15" s="13">
+        <f t="shared" si="1"/>
+        <v>57.15</v>
+      </c>
+      <c r="D15" s="29">
         <v>56.45</v>
       </c>
-      <c r="C15" s="29">
+      <c r="E15" s="29">
         <v>57.15</v>
       </c>
-      <c r="D15" s="29">
+      <c r="F15" s="29">
         <v>55.55</v>
       </c>
-      <c r="E15" s="29">
+      <c r="G15" s="29">
         <v>55.3</v>
       </c>
-      <c r="F15" s="29">
+      <c r="H15" s="29">
         <v>54.25</v>
       </c>
-      <c r="G15" s="29">
+      <c r="I15" s="29">
         <v>53.8</v>
       </c>
-      <c r="H15" s="29">
+      <c r="J15" s="29">
         <v>54</v>
       </c>
-      <c r="I15" s="29">
+      <c r="K15" s="29">
         <v>54.75</v>
       </c>
-      <c r="J15" s="29">
+      <c r="L15" s="29">
         <v>53.45</v>
       </c>
-      <c r="K15" s="29">
+      <c r="M15" s="29">
         <v>52.15</v>
       </c>
-      <c r="L15" s="29">
+      <c r="N15" s="29">
         <v>51.45</v>
       </c>
-      <c r="M15" s="29">
+      <c r="O15" s="29">
         <v>51</v>
       </c>
-      <c r="N15" s="29">
+      <c r="P15" s="29">
         <v>51.85</v>
       </c>
-      <c r="O15" s="29">
+      <c r="Q15" s="29">
         <v>53.25</v>
       </c>
-      <c r="P15" s="29">
+      <c r="R15" s="29">
         <v>50.5</v>
       </c>
-      <c r="Q15" s="29">
+      <c r="S15" s="29">
         <v>48.85</v>
       </c>
-      <c r="R15" s="5">
+      <c r="T15" s="5">
         <v>50.65</v>
       </c>
-      <c r="S15" s="5">
+      <c r="U15" s="5">
         <v>49.9</v>
       </c>
-      <c r="T15" s="5">
+      <c r="V15" s="5">
         <v>50.3</v>
       </c>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z15" s="5"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="29">
+      <c r="B16" s="13">
+        <f t="shared" si="0"/>
+        <v>30.55</v>
+      </c>
+      <c r="C16" s="13">
+        <f t="shared" si="1"/>
         <v>33.200000000000003</v>
       </c>
-      <c r="C16" s="29">
+      <c r="D16" s="29">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="E16" s="29">
         <v>33</v>
       </c>
-      <c r="D16" s="29">
+      <c r="F16" s="29">
         <v>32.5</v>
       </c>
-      <c r="E16" s="29">
+      <c r="G16" s="29">
         <v>32.6</v>
       </c>
-      <c r="F16" s="29">
+      <c r="H16" s="29">
         <v>32.799999999999997</v>
       </c>
-      <c r="G16" s="29">
+      <c r="I16" s="29">
         <v>31.95</v>
       </c>
-      <c r="H16" s="29">
+      <c r="J16" s="29">
         <v>32.700000000000003</v>
       </c>
-      <c r="I16" s="29">
+      <c r="K16" s="29">
         <v>32.4</v>
       </c>
-      <c r="J16" s="29">
+      <c r="L16" s="29">
         <v>31.6</v>
       </c>
-      <c r="K16" s="29">
+      <c r="M16" s="29">
         <v>31.5</v>
       </c>
-      <c r="L16" s="29">
+      <c r="N16" s="29">
         <v>30.55</v>
       </c>
-      <c r="M16" s="29">
+      <c r="O16" s="29">
         <v>31.4</v>
       </c>
-      <c r="N16" s="29">
+      <c r="P16" s="29">
         <v>31.5</v>
       </c>
-      <c r="O16" s="29">
+      <c r="Q16" s="29">
         <v>31.8</v>
       </c>
-      <c r="P16" s="29">
+      <c r="R16" s="29">
         <v>33</v>
       </c>
-      <c r="Q16" s="29">
+      <c r="S16" s="29">
         <v>32.049999999999997</v>
       </c>
-      <c r="R16" s="5">
+      <c r="T16" s="5">
         <v>32.15</v>
       </c>
-      <c r="S16" s="5">
+      <c r="U16" s="5">
         <v>32.5</v>
       </c>
-      <c r="T16" s="5">
+      <c r="V16" s="5">
         <v>33</v>
       </c>
-      <c r="U16" s="5"/>
-      <c r="V16" s="5"/>
       <c r="W16" s="5"/>
       <c r="X16" s="5"/>
       <c r="Y16" s="5"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z16" s="5"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
+      <c r="B17" s="13">
+        <f t="shared" si="0"/>
+        <v>27.75</v>
+      </c>
+      <c r="C17" s="13">
+        <f t="shared" si="1"/>
+        <v>36.4</v>
+      </c>
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
-      <c r="F17" s="29">
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29">
         <v>35.35</v>
       </c>
-      <c r="G17" s="29">
+      <c r="I17" s="29">
         <v>34.049999999999997</v>
       </c>
-      <c r="H17" s="29">
+      <c r="J17" s="29">
         <v>33.65</v>
       </c>
-      <c r="I17" s="29">
+      <c r="K17" s="29">
         <v>36.4</v>
       </c>
-      <c r="J17" s="29">
+      <c r="L17" s="29">
         <v>32.299999999999997</v>
       </c>
-      <c r="K17" s="29">
+      <c r="M17" s="29">
         <v>29.5</v>
       </c>
-      <c r="L17" s="29">
+      <c r="N17" s="29">
         <v>27.75</v>
       </c>
-      <c r="M17" s="29">
+      <c r="O17" s="29">
         <v>28.5</v>
       </c>
-      <c r="N17" s="29">
+      <c r="P17" s="29">
         <v>31.8</v>
       </c>
-      <c r="O17" s="29">
+      <c r="Q17" s="29">
         <v>34</v>
       </c>
-      <c r="P17" s="29">
+      <c r="R17" s="29">
         <v>31.5</v>
       </c>
-      <c r="Q17" s="29">
+      <c r="S17" s="29">
         <v>30.35</v>
       </c>
-      <c r="R17" s="5">
+      <c r="T17" s="5">
         <v>30.25</v>
       </c>
-      <c r="S17" s="5">
+      <c r="U17" s="5">
         <v>29.95</v>
       </c>
-      <c r="T17" s="5">
+      <c r="V17" s="5">
         <v>30.65</v>
       </c>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
       <c r="W17" s="5"/>
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z17" s="5"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="13">
+        <f t="shared" si="0"/>
+        <v>552</v>
+      </c>
+      <c r="C18" s="13">
+        <f t="shared" si="1"/>
+        <v>638.79999999999995</v>
+      </c>
+      <c r="D18" s="29">
         <v>561.04999999999995</v>
       </c>
-      <c r="C18" s="29">
+      <c r="E18" s="29">
         <v>552</v>
       </c>
-      <c r="D18" s="29">
+      <c r="F18" s="29">
         <v>567.6</v>
       </c>
-      <c r="E18" s="29">
+      <c r="G18" s="29">
         <v>570.95000000000005</v>
       </c>
-      <c r="F18" s="29">
+      <c r="H18" s="29">
         <v>568.95000000000005</v>
       </c>
-      <c r="G18" s="29">
+      <c r="I18" s="29">
         <v>559.75</v>
       </c>
-      <c r="H18" s="29">
+      <c r="J18" s="29">
         <v>580.79999999999995</v>
       </c>
-      <c r="I18" s="29">
+      <c r="K18" s="29">
         <v>600.79999999999995</v>
       </c>
-      <c r="J18" s="29">
+      <c r="L18" s="29">
         <v>614</v>
       </c>
-      <c r="K18" s="29">
+      <c r="M18" s="29">
         <v>605.25</v>
       </c>
-      <c r="L18" s="29">
+      <c r="N18" s="29">
         <v>606.5</v>
       </c>
-      <c r="M18" s="29">
+      <c r="O18" s="29">
         <v>601</v>
       </c>
-      <c r="N18" s="29">
+      <c r="P18" s="29">
         <v>620.4</v>
       </c>
-      <c r="O18" s="29">
+      <c r="Q18" s="29">
         <v>632.15</v>
       </c>
-      <c r="P18" s="29">
+      <c r="R18" s="29">
         <v>621.45000000000005</v>
       </c>
-      <c r="Q18" s="29">
+      <c r="S18" s="29">
         <v>621.6</v>
       </c>
-      <c r="R18" s="5">
+      <c r="T18" s="5">
         <v>635.25</v>
       </c>
-      <c r="S18" s="5">
+      <c r="U18" s="5">
         <v>638.79999999999995</v>
       </c>
-      <c r="T18" s="5">
+      <c r="V18" s="5">
         <v>634.75</v>
       </c>
-      <c r="U18" s="5"/>
-      <c r="V18" s="5"/>
       <c r="W18" s="5"/>
       <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z18" s="5"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="13">
+        <f t="shared" si="0"/>
+        <v>453</v>
+      </c>
+      <c r="C19" s="13">
+        <f t="shared" si="1"/>
         <v>515</v>
       </c>
-      <c r="C19" s="29">
+      <c r="D19" s="29">
+        <v>515</v>
+      </c>
+      <c r="E19" s="29">
         <v>503.55</v>
       </c>
-      <c r="D19" s="29">
+      <c r="F19" s="29">
         <v>501.4</v>
       </c>
-      <c r="E19" s="29">
+      <c r="G19" s="29">
         <v>497</v>
       </c>
-      <c r="F19" s="29">
+      <c r="H19" s="29">
         <v>498.05</v>
       </c>
-      <c r="G19" s="29">
+      <c r="I19" s="29">
         <v>485.2</v>
       </c>
-      <c r="H19" s="29">
+      <c r="J19" s="29">
         <v>500.5</v>
       </c>
-      <c r="I19" s="29">
+      <c r="K19" s="29">
         <v>493</v>
       </c>
-      <c r="J19" s="29">
+      <c r="L19" s="29">
         <v>492</v>
       </c>
-      <c r="K19" s="29">
+      <c r="M19" s="29">
         <v>479</v>
       </c>
-      <c r="L19" s="29">
+      <c r="N19" s="29">
         <v>453</v>
       </c>
-      <c r="M19" s="29">
+      <c r="O19" s="29">
         <v>468.25</v>
       </c>
-      <c r="N19" s="29">
+      <c r="P19" s="29">
         <v>479</v>
       </c>
-      <c r="O19" s="29">
+      <c r="Q19" s="29">
         <v>506</v>
       </c>
-      <c r="P19" s="29">
+      <c r="R19" s="29">
         <v>488.5</v>
       </c>
-      <c r="Q19" s="29">
+      <c r="S19" s="29">
         <v>473.7</v>
       </c>
-      <c r="R19" s="5">
+      <c r="T19" s="5">
         <v>460</v>
       </c>
-      <c r="S19" s="5">
+      <c r="U19" s="5">
         <v>471.85</v>
       </c>
-      <c r="T19" s="5">
+      <c r="V19" s="5">
         <v>484.5</v>
       </c>
-      <c r="U19" s="5"/>
-      <c r="V19" s="5"/>
       <c r="W19" s="5"/>
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z19" s="5"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="29">
+      <c r="B20" s="13">
+        <f t="shared" si="0"/>
+        <v>178.8</v>
+      </c>
+      <c r="C20" s="13">
+        <f t="shared" si="1"/>
+        <v>212.35</v>
+      </c>
+      <c r="D20" s="29">
         <v>196.55</v>
       </c>
-      <c r="C20" s="29">
+      <c r="E20" s="29">
         <v>195.2</v>
       </c>
-      <c r="D20" s="29">
+      <c r="F20" s="29">
         <v>190.05</v>
       </c>
-      <c r="E20" s="29">
+      <c r="G20" s="29">
         <v>195.15</v>
       </c>
-      <c r="F20" s="29">
+      <c r="H20" s="29">
         <v>195.3</v>
       </c>
-      <c r="G20" s="29">
+      <c r="I20" s="29">
         <v>195.75</v>
       </c>
-      <c r="H20" s="29">
+      <c r="J20" s="29">
         <v>197</v>
       </c>
-      <c r="I20" s="29">
+      <c r="K20" s="29">
         <v>210.7</v>
       </c>
-      <c r="J20" s="29">
+      <c r="L20" s="29">
         <v>212.35</v>
       </c>
-      <c r="K20" s="29">
+      <c r="M20" s="29">
         <v>206.05</v>
       </c>
-      <c r="L20" s="29">
+      <c r="N20" s="29">
         <v>191.95</v>
       </c>
-      <c r="M20" s="29">
+      <c r="O20" s="29">
         <v>178.8</v>
       </c>
-      <c r="N20" s="29">
+      <c r="P20" s="29">
         <v>189.1</v>
       </c>
-      <c r="O20" s="29">
+      <c r="Q20" s="29">
         <v>195</v>
       </c>
-      <c r="P20" s="29">
+      <c r="R20" s="29">
         <v>197.5</v>
       </c>
-      <c r="Q20" s="29">
+      <c r="S20" s="29">
         <v>198</v>
       </c>
-      <c r="R20" s="5">
+      <c r="T20" s="5">
         <v>201.9</v>
       </c>
-      <c r="S20" s="5">
+      <c r="U20" s="5">
         <v>202.9</v>
       </c>
-      <c r="T20" s="5">
+      <c r="V20" s="5">
         <v>212</v>
       </c>
-      <c r="U20" s="5"/>
-      <c r="V20" s="5"/>
       <c r="W20" s="5"/>
       <c r="X20" s="5"/>
       <c r="Y20" s="5"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z20" s="5"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="29">
+      <c r="B21" s="13">
+        <f t="shared" si="0"/>
+        <v>440.7</v>
+      </c>
+      <c r="C21" s="13">
+        <f t="shared" si="1"/>
+        <v>475.45</v>
+      </c>
+      <c r="D21" s="29">
         <v>450.5</v>
       </c>
-      <c r="C21" s="29">
+      <c r="E21" s="29">
         <v>453</v>
       </c>
-      <c r="D21" s="29">
+      <c r="F21" s="29">
         <v>440.7</v>
       </c>
-      <c r="E21" s="29">
+      <c r="G21" s="29">
         <v>449</v>
       </c>
-      <c r="F21" s="29">
+      <c r="H21" s="29">
         <v>452.75</v>
       </c>
-      <c r="G21" s="29">
+      <c r="I21" s="29">
         <v>450</v>
       </c>
-      <c r="H21" s="29">
+      <c r="J21" s="29">
         <v>447.8</v>
       </c>
-      <c r="I21" s="29">
+      <c r="K21" s="29">
         <v>464.55</v>
       </c>
-      <c r="J21" s="29">
+      <c r="L21" s="29">
         <v>452.6</v>
       </c>
-      <c r="K21" s="29">
+      <c r="M21" s="29">
         <v>450.5</v>
       </c>
-      <c r="L21" s="29">
+      <c r="N21" s="29">
         <v>455</v>
       </c>
-      <c r="M21" s="29">
+      <c r="O21" s="29">
         <v>443.85</v>
       </c>
-      <c r="N21" s="29">
+      <c r="P21" s="29">
         <v>451.15</v>
       </c>
-      <c r="O21" s="29">
+      <c r="Q21" s="29">
         <v>454.5</v>
       </c>
-      <c r="P21" s="29">
+      <c r="R21" s="29">
         <v>448.95</v>
       </c>
-      <c r="Q21" s="29">
+      <c r="S21" s="29">
         <v>446.05</v>
       </c>
-      <c r="R21" s="5">
+      <c r="T21" s="5">
         <v>460.25</v>
       </c>
-      <c r="S21" s="5">
+      <c r="U21" s="5">
         <v>470.45</v>
       </c>
-      <c r="T21" s="5">
+      <c r="V21" s="5">
         <v>475.45</v>
       </c>
-      <c r="U21" s="5"/>
-      <c r="V21" s="5"/>
       <c r="W21" s="5"/>
       <c r="X21" s="5"/>
       <c r="Y21" s="5"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z21" s="5"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="B22" s="31">
+      <c r="B22" s="13">
+        <f t="shared" si="0"/>
+        <v>683.05</v>
+      </c>
+      <c r="C22" s="13">
+        <f t="shared" si="1"/>
+        <v>744</v>
+      </c>
+      <c r="D22" s="31">
         <v>739.1</v>
       </c>
-      <c r="C22" s="29">
+      <c r="E22" s="29">
         <v>724.95</v>
       </c>
-      <c r="D22" s="29">
+      <c r="F22" s="29">
         <v>718.65</v>
       </c>
-      <c r="E22" s="29">
+      <c r="G22" s="29">
         <v>736</v>
       </c>
-      <c r="F22" s="29">
+      <c r="H22" s="29">
         <v>729.9</v>
       </c>
-      <c r="G22" s="29">
+      <c r="I22" s="29">
         <v>741.05</v>
       </c>
-      <c r="H22" s="29">
+      <c r="J22" s="29">
         <v>724.7</v>
       </c>
-      <c r="I22" s="29">
+      <c r="K22" s="29">
         <v>726</v>
       </c>
-      <c r="J22" s="29">
+      <c r="L22" s="29">
         <v>726.55</v>
       </c>
-      <c r="K22" s="29">
+      <c r="M22" s="29">
         <v>683.05</v>
       </c>
-      <c r="L22" s="29">
+      <c r="N22" s="29">
         <v>696</v>
       </c>
-      <c r="M22" s="29">
+      <c r="O22" s="29">
         <v>706.8</v>
       </c>
-      <c r="N22" s="29">
+      <c r="P22" s="29">
         <v>714.55</v>
       </c>
-      <c r="O22" s="29">
+      <c r="Q22" s="29">
         <v>712.95</v>
       </c>
-      <c r="P22" s="29">
+      <c r="R22" s="29">
         <v>695</v>
       </c>
-      <c r="Q22" s="29">
+      <c r="S22" s="29">
         <v>694.3</v>
       </c>
-      <c r="R22" s="5">
+      <c r="T22" s="5">
         <v>698.85</v>
       </c>
-      <c r="S22" s="5">
+      <c r="U22" s="5">
         <v>732.2</v>
       </c>
-      <c r="T22" s="5">
+      <c r="V22" s="5">
         <v>744</v>
       </c>
-      <c r="U22" s="5"/>
-      <c r="V22" s="5"/>
       <c r="W22" s="5"/>
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
-    </row>
-    <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z22" s="5"/>
+    </row>
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="29">
+      <c r="B23" s="13">
+        <f t="shared" si="0"/>
+        <v>408.35</v>
+      </c>
+      <c r="C23" s="13">
+        <f t="shared" si="1"/>
+        <v>434.65</v>
+      </c>
+      <c r="D23" s="29">
         <v>414.05</v>
       </c>
-      <c r="C23" s="29">
+      <c r="E23" s="29">
         <v>412.95</v>
       </c>
-      <c r="D23" s="29">
+      <c r="F23" s="29">
         <v>420</v>
       </c>
-      <c r="E23" s="29">
+      <c r="G23" s="29">
         <v>419.5</v>
       </c>
-      <c r="F23" s="29">
+      <c r="H23" s="29">
         <v>415.9</v>
       </c>
-      <c r="G23" s="29">
+      <c r="I23" s="29">
         <v>423.4</v>
       </c>
-      <c r="H23" s="29">
+      <c r="J23" s="29">
         <v>421.1</v>
       </c>
-      <c r="I23" s="29">
+      <c r="K23" s="29">
         <v>417.5</v>
       </c>
-      <c r="J23" s="29">
+      <c r="L23" s="29">
         <v>417.95</v>
       </c>
-      <c r="K23" s="29">
+      <c r="M23" s="29">
         <v>416</v>
       </c>
-      <c r="L23" s="29">
+      <c r="N23" s="29">
         <v>416.4</v>
       </c>
-      <c r="M23" s="29">
+      <c r="O23" s="29">
         <v>414.8</v>
       </c>
-      <c r="N23" s="29">
+      <c r="P23" s="29">
         <v>411</v>
       </c>
-      <c r="O23" s="29">
+      <c r="Q23" s="29">
         <v>408.35</v>
       </c>
-      <c r="P23" s="29">
+      <c r="R23" s="29">
         <v>419.95</v>
       </c>
-      <c r="Q23" s="29">
+      <c r="S23" s="29">
         <v>424.9</v>
       </c>
-      <c r="R23" s="5">
+      <c r="T23" s="5">
         <v>433.5</v>
       </c>
-      <c r="S23" s="5">
+      <c r="U23" s="5">
         <v>433.35</v>
       </c>
-      <c r="T23" s="5">
+      <c r="V23" s="5">
         <v>434.65</v>
       </c>
-      <c r="U23" s="5"/>
-      <c r="V23" s="5"/>
       <c r="W23" s="5"/>
       <c r="X23" s="5"/>
       <c r="Y23" s="5"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z23" s="5"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="B24" s="13">
+        <f t="shared" si="0"/>
+        <v>72.8</v>
+      </c>
+      <c r="C24" s="13">
+        <f t="shared" si="1"/>
+        <v>89.3</v>
+      </c>
       <c r="D24" s="5"/>
-      <c r="E24" s="5">
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5">
         <v>89.3</v>
       </c>
-      <c r="F24" s="5">
+      <c r="H24" s="5">
         <v>88.85</v>
       </c>
-      <c r="G24" s="5">
+      <c r="I24" s="5">
         <v>86.5</v>
       </c>
-      <c r="H24" s="5">
+      <c r="J24" s="5">
         <v>87.25</v>
       </c>
-      <c r="I24" s="5">
+      <c r="K24" s="5">
         <v>86.4</v>
       </c>
-      <c r="J24" s="5">
+      <c r="L24" s="5">
         <v>85.7</v>
       </c>
-      <c r="K24" s="5">
+      <c r="M24" s="5">
         <v>84.9</v>
       </c>
-      <c r="L24" s="5">
+      <c r="N24" s="5">
         <v>83</v>
       </c>
-      <c r="M24" s="5">
+      <c r="O24" s="5">
         <v>72.8</v>
       </c>
-      <c r="N24" s="5">
+      <c r="P24" s="5">
         <v>76.400000000000006</v>
       </c>
-      <c r="O24" s="5">
+      <c r="Q24" s="5">
         <v>73.7</v>
       </c>
-      <c r="P24" s="5">
+      <c r="R24" s="5">
         <v>73.900000000000006</v>
       </c>
-      <c r="Q24" s="5">
+      <c r="S24" s="5">
         <v>73.3</v>
       </c>
-      <c r="R24" s="5">
+      <c r="T24" s="5">
         <v>73.8</v>
       </c>
-      <c r="S24" s="5">
+      <c r="U24" s="5">
         <v>73.400000000000006</v>
       </c>
-      <c r="T24" s="5">
+      <c r="V24" s="5">
         <v>80</v>
       </c>
-      <c r="U24" s="5"/>
-      <c r="V24" s="5"/>
       <c r="W24" s="5"/>
       <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z24" s="5"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="B25" s="13">
+        <f t="shared" si="0"/>
+        <v>54.95</v>
+      </c>
+      <c r="C25" s="13">
+        <f t="shared" si="1"/>
+        <v>85.65</v>
+      </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="5">
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5">
         <v>85.65</v>
       </c>
-      <c r="G25" s="5">
+      <c r="I25" s="5">
         <v>84.45</v>
       </c>
-      <c r="H25" s="5">
+      <c r="J25" s="5">
         <v>75.7</v>
       </c>
-      <c r="I25" s="5">
+      <c r="K25" s="5">
         <v>68.75</v>
       </c>
-      <c r="J25" s="5">
+      <c r="L25" s="5">
         <v>54.95</v>
       </c>
-      <c r="K25" s="5">
+      <c r="M25" s="5">
         <v>57.45</v>
       </c>
-      <c r="L25" s="5">
+      <c r="N25" s="5">
         <v>57.35</v>
       </c>
-      <c r="M25" s="5">
+      <c r="O25" s="5">
         <v>58.1</v>
       </c>
-      <c r="N25" s="5">
+      <c r="P25" s="5">
         <v>57.05</v>
       </c>
-      <c r="O25" s="5">
+      <c r="Q25" s="5">
         <v>62</v>
       </c>
-      <c r="P25" s="5">
+      <c r="R25" s="5">
         <v>57.9</v>
       </c>
-      <c r="Q25" s="5">
+      <c r="S25" s="5">
         <v>59.85</v>
       </c>
-      <c r="R25" s="5">
+      <c r="T25" s="5">
         <v>61.45</v>
       </c>
-      <c r="S25" s="5">
+      <c r="U25" s="5">
         <v>61.55</v>
       </c>
-      <c r="T25" s="5">
+      <c r="V25" s="5">
         <v>62.1</v>
       </c>
-      <c r="U25" s="5"/>
-      <c r="V25" s="5"/>
       <c r="W25" s="5"/>
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
-    </row>
-    <row r="26" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z25" s="5"/>
+    </row>
+    <row r="26" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="B26" s="13">
+        <f t="shared" si="0"/>
+        <v>222.65</v>
+      </c>
+      <c r="C26" s="13">
+        <f t="shared" si="1"/>
+        <v>255.75</v>
+      </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="5">
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5">
         <v>255.75</v>
       </c>
-      <c r="I26" s="5">
+      <c r="K26" s="5">
         <v>250.45</v>
       </c>
-      <c r="J26" s="5">
+      <c r="L26" s="5">
         <v>248.95</v>
       </c>
-      <c r="K26" s="5">
+      <c r="M26" s="5">
         <v>242.3</v>
       </c>
-      <c r="L26" s="5">
+      <c r="N26" s="5">
         <v>223</v>
       </c>
-      <c r="M26" s="5">
+      <c r="O26" s="5">
         <v>222.65</v>
       </c>
-      <c r="N26" s="5">
+      <c r="P26" s="5">
         <v>227.25</v>
       </c>
-      <c r="O26" s="5">
+      <c r="Q26" s="5">
         <v>232.55</v>
       </c>
-      <c r="P26" s="5">
+      <c r="R26" s="5">
         <v>223</v>
       </c>
-      <c r="Q26" s="5">
+      <c r="S26" s="5">
         <v>225.2</v>
       </c>
-      <c r="R26" s="5">
+      <c r="T26" s="5">
         <v>226.2</v>
       </c>
-      <c r="S26" s="5">
+      <c r="U26" s="5">
         <v>227.65</v>
       </c>
-      <c r="T26" s="5">
+      <c r="V26" s="5">
         <v>225.6</v>
       </c>
-      <c r="U26" s="5"/>
-      <c r="V26" s="5"/>
       <c r="W26" s="5"/>
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z26" s="5"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="49" t="s">
         <v>283</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="B27" s="13">
+        <f t="shared" si="0"/>
+        <v>876</v>
+      </c>
+      <c r="C27" s="13">
+        <f t="shared" si="1"/>
+        <v>940.3</v>
+      </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -8713,27 +8908,28 @@
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
-      <c r="Q27" s="5">
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5">
         <v>876</v>
       </c>
-      <c r="R27" s="5">
+      <c r="T27" s="5">
         <v>893.4</v>
       </c>
-      <c r="S27" s="5">
+      <c r="U27" s="5">
         <v>911.5</v>
       </c>
-      <c r="T27" s="5">
+      <c r="V27" s="5">
         <v>940.3</v>
       </c>
-      <c r="U27" s="5"/>
-      <c r="V27" s="5"/>
       <c r="W27" s="5"/>
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="I1:I37">
-    <sortCondition ref="I13"/>
+  <sortState ref="K1:K37">
+    <sortCondition ref="K13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated the sheet for 04092017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="296">
   <si>
     <t>Date</t>
   </si>
@@ -883,6 +883,36 @@
   </si>
   <si>
     <t xml:space="preserve">ANDHRACEMT </t>
+  </si>
+  <si>
+    <t>Tiles</t>
+  </si>
+  <si>
+    <t>Bricks</t>
+  </si>
+  <si>
+    <t>13/9/2017</t>
+  </si>
+  <si>
+    <t>14/9/2017</t>
+  </si>
+  <si>
+    <t>15/9/2017</t>
+  </si>
+  <si>
+    <t>18/9/2017</t>
+  </si>
+  <si>
+    <t>19/9/2017</t>
+  </si>
+  <si>
+    <t>20/9/2017</t>
+  </si>
+  <si>
+    <t>21/9/2017</t>
+  </si>
+  <si>
+    <t>22/9/2017</t>
   </si>
 </sst>
 </file>
@@ -7090,26 +7120,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z41"/>
+  <dimension ref="A1:AX41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A38" sqref="A38:XFD38"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA26" sqref="AA26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" style="49" customWidth="1"/>
-    <col min="4" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="25" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="24" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="30" width="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12" customWidth="1"/>
+    <col min="32" max="32" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="35" width="13" bestFit="1" customWidth="1"/>
+    <col min="36" max="43" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>268</v>
       </c>
@@ -7188,8 +7228,62 @@
       <c r="Z1" s="12">
         <v>42744</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" s="12">
+        <v>42834</v>
+      </c>
+      <c r="AB1" s="12">
+        <v>42864</v>
+      </c>
+      <c r="AC1" s="12">
+        <v>42895</v>
+      </c>
+      <c r="AD1" s="12">
+        <v>42925</v>
+      </c>
+      <c r="AE1" s="12">
+        <v>42956</v>
+      </c>
+      <c r="AF1" s="12">
+        <v>43048</v>
+      </c>
+      <c r="AG1" s="12">
+        <v>43078</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="AI1" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="AJ1" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="AK1" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="AL1" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="AM1" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="AN1" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO1" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="28"/>
+      <c r="AS1" s="28"/>
+      <c r="AT1" s="28"/>
+      <c r="AU1" s="28"/>
+      <c r="AV1" s="28"/>
+      <c r="AW1" s="28"/>
+      <c r="AX1" s="28"/>
+    </row>
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <f t="shared" ref="A2:A27" si="0">MIN(D2:ZZ2)</f>
         <v>274.05</v>
@@ -7264,8 +7358,34 @@
       <c r="Z2" s="5">
         <v>278</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA2" s="5">
+        <v>277.45</v>
+      </c>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5"/>
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="5"/>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="5"/>
+      <c r="AU2" s="5"/>
+      <c r="AV2" s="5"/>
+      <c r="AW2" s="5"/>
+      <c r="AX2" s="5"/>
+    </row>
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <f t="shared" si="0"/>
         <v>285.8</v>
@@ -7340,8 +7460,34 @@
       <c r="Z3" s="5">
         <v>298.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA3" s="5">
+        <v>297.10000000000002</v>
+      </c>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="5"/>
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="5"/>
+      <c r="AM3" s="5"/>
+      <c r="AN3" s="5"/>
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="5"/>
+      <c r="AQ3" s="5"/>
+      <c r="AR3" s="5"/>
+      <c r="AS3" s="5"/>
+      <c r="AT3" s="5"/>
+      <c r="AU3" s="5"/>
+      <c r="AV3" s="5"/>
+      <c r="AW3" s="5"/>
+      <c r="AX3" s="5"/>
+    </row>
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <f t="shared" si="0"/>
         <v>271.2</v>
@@ -7422,8 +7568,34 @@
       <c r="Z4" s="5">
         <v>283.89999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA4" s="5">
+        <v>282.8</v>
+      </c>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="5"/>
+      <c r="AN4" s="5"/>
+      <c r="AO4" s="5"/>
+      <c r="AP4" s="5"/>
+      <c r="AQ4" s="5"/>
+      <c r="AR4" s="5"/>
+      <c r="AS4" s="5"/>
+      <c r="AT4" s="5"/>
+      <c r="AU4" s="5"/>
+      <c r="AV4" s="5"/>
+      <c r="AW4" s="5"/>
+      <c r="AX4" s="5"/>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <f t="shared" si="0"/>
         <v>1532.05</v>
@@ -7504,8 +7676,34 @@
       <c r="Z5" s="44">
         <v>1611.95</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA5" s="44">
+        <v>1615</v>
+      </c>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="5"/>
+      <c r="AQ5" s="5"/>
+      <c r="AR5" s="5"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="5"/>
+      <c r="AU5" s="5"/>
+      <c r="AV5" s="5"/>
+      <c r="AW5" s="5"/>
+      <c r="AX5" s="5"/>
+    </row>
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <f t="shared" si="0"/>
         <v>236.45</v>
@@ -7586,8 +7784,34 @@
       <c r="Z6" s="5">
         <v>239</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA6" s="5">
+        <v>246.25</v>
+      </c>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="5"/>
+      <c r="AM6" s="5"/>
+      <c r="AN6" s="5"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="5"/>
+      <c r="AQ6" s="5"/>
+      <c r="AR6" s="5"/>
+      <c r="AS6" s="5"/>
+      <c r="AT6" s="5"/>
+      <c r="AU6" s="5"/>
+      <c r="AV6" s="5"/>
+      <c r="AW6" s="5"/>
+      <c r="AX6" s="5"/>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <f t="shared" si="0"/>
         <v>15.6</v>
@@ -7668,8 +7892,34 @@
       <c r="Z7" s="5">
         <v>17.75</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA7" s="5">
+        <v>17.2</v>
+      </c>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="5"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="5"/>
+      <c r="AM7" s="5"/>
+      <c r="AN7" s="5"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="5"/>
+      <c r="AQ7" s="5"/>
+      <c r="AR7" s="5"/>
+      <c r="AS7" s="5"/>
+      <c r="AT7" s="5"/>
+      <c r="AU7" s="5"/>
+      <c r="AV7" s="5"/>
+      <c r="AW7" s="5"/>
+      <c r="AX7" s="5"/>
+    </row>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <f t="shared" si="0"/>
         <v>56.6</v>
@@ -7750,8 +8000,34 @@
       <c r="Z8" s="5">
         <v>62.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA8" s="5">
+        <v>62.55</v>
+      </c>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="5"/>
+      <c r="AE8" s="5"/>
+      <c r="AF8" s="5"/>
+      <c r="AG8" s="5"/>
+      <c r="AH8" s="5"/>
+      <c r="AI8" s="5"/>
+      <c r="AJ8" s="5"/>
+      <c r="AK8" s="5"/>
+      <c r="AL8" s="5"/>
+      <c r="AM8" s="5"/>
+      <c r="AN8" s="5"/>
+      <c r="AO8" s="5"/>
+      <c r="AP8" s="5"/>
+      <c r="AQ8" s="5"/>
+      <c r="AR8" s="5"/>
+      <c r="AS8" s="5"/>
+      <c r="AT8" s="5"/>
+      <c r="AU8" s="5"/>
+      <c r="AV8" s="5"/>
+      <c r="AW8" s="5"/>
+      <c r="AX8" s="5"/>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <f t="shared" si="0"/>
         <v>53.5</v>
@@ -7824,8 +8100,34 @@
       <c r="Z9" s="5">
         <v>57.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA9" s="5">
+        <v>57.1</v>
+      </c>
+      <c r="AB9" s="5"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="5"/>
+      <c r="AE9" s="5"/>
+      <c r="AF9" s="5"/>
+      <c r="AG9" s="5"/>
+      <c r="AH9" s="5"/>
+      <c r="AI9" s="5"/>
+      <c r="AJ9" s="5"/>
+      <c r="AK9" s="5"/>
+      <c r="AL9" s="5"/>
+      <c r="AM9" s="5"/>
+      <c r="AN9" s="5"/>
+      <c r="AO9" s="5"/>
+      <c r="AP9" s="5"/>
+      <c r="AQ9" s="5"/>
+      <c r="AR9" s="5"/>
+      <c r="AS9" s="5"/>
+      <c r="AT9" s="5"/>
+      <c r="AU9" s="5"/>
+      <c r="AV9" s="5"/>
+      <c r="AW9" s="5"/>
+      <c r="AX9" s="5"/>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <f t="shared" si="0"/>
         <v>38.6</v>
@@ -7906,8 +8208,34 @@
       <c r="Z10" s="5">
         <v>41.15</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA10" s="5">
+        <v>40.1</v>
+      </c>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="5"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="5"/>
+      <c r="AI10" s="5"/>
+      <c r="AJ10" s="5"/>
+      <c r="AK10" s="5"/>
+      <c r="AL10" s="5"/>
+      <c r="AM10" s="5"/>
+      <c r="AN10" s="5"/>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="5"/>
+      <c r="AQ10" s="5"/>
+      <c r="AR10" s="5"/>
+      <c r="AS10" s="5"/>
+      <c r="AT10" s="5"/>
+      <c r="AU10" s="5"/>
+      <c r="AV10" s="5"/>
+      <c r="AW10" s="5"/>
+      <c r="AX10" s="5"/>
+    </row>
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <f t="shared" si="0"/>
         <v>62.6</v>
@@ -7988,8 +8316,34 @@
       <c r="Z11" s="5">
         <v>75.05</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA11" s="5">
+        <v>73.45</v>
+      </c>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="5"/>
+      <c r="AE11" s="5"/>
+      <c r="AF11" s="5"/>
+      <c r="AG11" s="5"/>
+      <c r="AH11" s="5"/>
+      <c r="AI11" s="5"/>
+      <c r="AJ11" s="5"/>
+      <c r="AK11" s="5"/>
+      <c r="AL11" s="5"/>
+      <c r="AM11" s="5"/>
+      <c r="AN11" s="5"/>
+      <c r="AO11" s="5"/>
+      <c r="AP11" s="5"/>
+      <c r="AQ11" s="5"/>
+      <c r="AR11" s="5"/>
+      <c r="AS11" s="5"/>
+      <c r="AT11" s="5"/>
+      <c r="AU11" s="5"/>
+      <c r="AV11" s="5"/>
+      <c r="AW11" s="5"/>
+      <c r="AX11" s="5"/>
+    </row>
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <f t="shared" si="0"/>
         <v>86.5</v>
@@ -8070,8 +8424,34 @@
       <c r="Z12" s="5">
         <v>88.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA12" s="5">
+        <v>86.7</v>
+      </c>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="5"/>
+      <c r="AE12" s="5"/>
+      <c r="AF12" s="5"/>
+      <c r="AG12" s="5"/>
+      <c r="AH12" s="5"/>
+      <c r="AI12" s="5"/>
+      <c r="AJ12" s="5"/>
+      <c r="AK12" s="5"/>
+      <c r="AL12" s="5"/>
+      <c r="AM12" s="5"/>
+      <c r="AN12" s="5"/>
+      <c r="AO12" s="5"/>
+      <c r="AP12" s="5"/>
+      <c r="AQ12" s="5"/>
+      <c r="AR12" s="5"/>
+      <c r="AS12" s="5"/>
+      <c r="AT12" s="5"/>
+      <c r="AU12" s="5"/>
+      <c r="AV12" s="5"/>
+      <c r="AW12" s="5"/>
+      <c r="AX12" s="5"/>
+    </row>
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <f t="shared" si="0"/>
         <v>124.25</v>
@@ -8152,8 +8532,34 @@
       <c r="Z13" s="5">
         <v>130</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA13" s="5">
+        <v>131.1</v>
+      </c>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="5"/>
+      <c r="AE13" s="5"/>
+      <c r="AF13" s="5"/>
+      <c r="AG13" s="5"/>
+      <c r="AH13" s="5"/>
+      <c r="AI13" s="5"/>
+      <c r="AJ13" s="5"/>
+      <c r="AK13" s="5"/>
+      <c r="AL13" s="5"/>
+      <c r="AM13" s="5"/>
+      <c r="AN13" s="5"/>
+      <c r="AO13" s="5"/>
+      <c r="AP13" s="5"/>
+      <c r="AQ13" s="5"/>
+      <c r="AR13" s="5"/>
+      <c r="AS13" s="5"/>
+      <c r="AT13" s="5"/>
+      <c r="AU13" s="5"/>
+      <c r="AV13" s="5"/>
+      <c r="AW13" s="5"/>
+      <c r="AX13" s="5"/>
+    </row>
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <f t="shared" si="0"/>
         <v>76.7</v>
@@ -8234,8 +8640,34 @@
       <c r="Z14" s="5">
         <v>79.900000000000006</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA14" s="5">
+        <v>78.5</v>
+      </c>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="5"/>
+      <c r="AF14" s="5"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="5"/>
+      <c r="AI14" s="5"/>
+      <c r="AJ14" s="5"/>
+      <c r="AK14" s="5"/>
+      <c r="AL14" s="5"/>
+      <c r="AM14" s="5"/>
+      <c r="AN14" s="5"/>
+      <c r="AO14" s="5"/>
+      <c r="AP14" s="5"/>
+      <c r="AQ14" s="5"/>
+      <c r="AR14" s="5"/>
+      <c r="AS14" s="5"/>
+      <c r="AT14" s="5"/>
+      <c r="AU14" s="5"/>
+      <c r="AV14" s="5"/>
+      <c r="AW14" s="5"/>
+      <c r="AX14" s="5"/>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <f t="shared" si="0"/>
         <v>48.8</v>
@@ -8316,8 +8748,34 @@
       <c r="Z15" s="5">
         <v>49.55</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA15" s="5">
+        <v>51</v>
+      </c>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="5"/>
+      <c r="AE15" s="5"/>
+      <c r="AF15" s="5"/>
+      <c r="AG15" s="5"/>
+      <c r="AH15" s="5"/>
+      <c r="AI15" s="5"/>
+      <c r="AJ15" s="5"/>
+      <c r="AK15" s="5"/>
+      <c r="AL15" s="5"/>
+      <c r="AM15" s="5"/>
+      <c r="AN15" s="5"/>
+      <c r="AO15" s="5"/>
+      <c r="AP15" s="5"/>
+      <c r="AQ15" s="5"/>
+      <c r="AR15" s="5"/>
+      <c r="AS15" s="5"/>
+      <c r="AT15" s="5"/>
+      <c r="AU15" s="5"/>
+      <c r="AV15" s="5"/>
+      <c r="AW15" s="5"/>
+      <c r="AX15" s="5"/>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <f t="shared" si="0"/>
         <v>30.55</v>
@@ -8398,8 +8856,34 @@
       <c r="Z16" s="5">
         <v>32.75</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA16" s="5">
+        <v>31.8</v>
+      </c>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="5"/>
+      <c r="AD16" s="5"/>
+      <c r="AE16" s="5"/>
+      <c r="AF16" s="5"/>
+      <c r="AG16" s="5"/>
+      <c r="AH16" s="5"/>
+      <c r="AI16" s="5"/>
+      <c r="AJ16" s="5"/>
+      <c r="AK16" s="5"/>
+      <c r="AL16" s="5"/>
+      <c r="AM16" s="5"/>
+      <c r="AN16" s="5"/>
+      <c r="AO16" s="5"/>
+      <c r="AP16" s="5"/>
+      <c r="AQ16" s="5"/>
+      <c r="AR16" s="5"/>
+      <c r="AS16" s="5"/>
+      <c r="AT16" s="5"/>
+      <c r="AU16" s="5"/>
+      <c r="AV16" s="5"/>
+      <c r="AW16" s="5"/>
+      <c r="AX16" s="5"/>
+    </row>
+    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <f t="shared" si="0"/>
         <v>27.75</v>
@@ -8472,8 +8956,34 @@
       <c r="Z17" s="5">
         <v>30.6</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA17" s="5">
+        <v>30.15</v>
+      </c>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="5"/>
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="5"/>
+      <c r="AG17" s="5"/>
+      <c r="AH17" s="5"/>
+      <c r="AI17" s="5"/>
+      <c r="AJ17" s="5"/>
+      <c r="AK17" s="5"/>
+      <c r="AL17" s="5"/>
+      <c r="AM17" s="5"/>
+      <c r="AN17" s="5"/>
+      <c r="AO17" s="5"/>
+      <c r="AP17" s="5"/>
+      <c r="AQ17" s="5"/>
+      <c r="AR17" s="5"/>
+      <c r="AS17" s="5"/>
+      <c r="AT17" s="5"/>
+      <c r="AU17" s="5"/>
+      <c r="AV17" s="5"/>
+      <c r="AW17" s="5"/>
+      <c r="AX17" s="5"/>
+    </row>
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <f t="shared" si="0"/>
         <v>552</v>
@@ -8554,8 +9064,34 @@
       <c r="Z18" s="5">
         <v>650.9</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA18" s="5">
+        <v>646.75</v>
+      </c>
+      <c r="AB18" s="5"/>
+      <c r="AC18" s="5"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="5"/>
+      <c r="AF18" s="5"/>
+      <c r="AG18" s="5"/>
+      <c r="AH18" s="5"/>
+      <c r="AI18" s="5"/>
+      <c r="AJ18" s="5"/>
+      <c r="AK18" s="5"/>
+      <c r="AL18" s="5"/>
+      <c r="AM18" s="5"/>
+      <c r="AN18" s="5"/>
+      <c r="AO18" s="5"/>
+      <c r="AP18" s="5"/>
+      <c r="AQ18" s="5"/>
+      <c r="AR18" s="5"/>
+      <c r="AS18" s="5"/>
+      <c r="AT18" s="5"/>
+      <c r="AU18" s="5"/>
+      <c r="AV18" s="5"/>
+      <c r="AW18" s="5"/>
+      <c r="AX18" s="5"/>
+    </row>
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <f t="shared" si="0"/>
         <v>453</v>
@@ -8636,15 +9172,41 @@
       <c r="Z19" s="5">
         <v>483.15</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA19" s="5">
+        <v>479</v>
+      </c>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="5"/>
+      <c r="AF19" s="5"/>
+      <c r="AG19" s="5"/>
+      <c r="AH19" s="5"/>
+      <c r="AI19" s="5"/>
+      <c r="AJ19" s="5"/>
+      <c r="AK19" s="5"/>
+      <c r="AL19" s="5"/>
+      <c r="AM19" s="5"/>
+      <c r="AN19" s="5"/>
+      <c r="AO19" s="5"/>
+      <c r="AP19" s="5"/>
+      <c r="AQ19" s="5"/>
+      <c r="AR19" s="5"/>
+      <c r="AS19" s="5"/>
+      <c r="AT19" s="5"/>
+      <c r="AU19" s="5"/>
+      <c r="AV19" s="5"/>
+      <c r="AW19" s="5"/>
+      <c r="AX19" s="5"/>
+    </row>
+    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <f t="shared" si="0"/>
         <v>178.8</v>
       </c>
       <c r="B20" s="13">
         <f t="shared" si="1"/>
-        <v>228.7</v>
+        <v>228.85</v>
       </c>
       <c r="C20" s="46" t="s">
         <v>41</v>
@@ -8718,8 +9280,34 @@
       <c r="Z20" s="5">
         <v>228.7</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA20" s="5">
+        <v>228.85</v>
+      </c>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="5"/>
+      <c r="AD20" s="5"/>
+      <c r="AE20" s="5"/>
+      <c r="AF20" s="5"/>
+      <c r="AG20" s="5"/>
+      <c r="AH20" s="5"/>
+      <c r="AI20" s="5"/>
+      <c r="AJ20" s="5"/>
+      <c r="AK20" s="5"/>
+      <c r="AL20" s="5"/>
+      <c r="AM20" s="5"/>
+      <c r="AN20" s="5"/>
+      <c r="AO20" s="5"/>
+      <c r="AP20" s="5"/>
+      <c r="AQ20" s="5"/>
+      <c r="AR20" s="5"/>
+      <c r="AS20" s="5"/>
+      <c r="AT20" s="5"/>
+      <c r="AU20" s="5"/>
+      <c r="AV20" s="5"/>
+      <c r="AW20" s="5"/>
+      <c r="AX20" s="5"/>
+    </row>
+    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <f t="shared" si="0"/>
         <v>440.7</v>
@@ -8800,8 +9388,34 @@
       <c r="Z21" s="5">
         <v>507</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA21" s="5">
+        <v>495.8</v>
+      </c>
+      <c r="AB21" s="5"/>
+      <c r="AC21" s="5"/>
+      <c r="AD21" s="5"/>
+      <c r="AE21" s="5"/>
+      <c r="AF21" s="5"/>
+      <c r="AG21" s="5"/>
+      <c r="AH21" s="5"/>
+      <c r="AI21" s="5"/>
+      <c r="AJ21" s="5"/>
+      <c r="AK21" s="5"/>
+      <c r="AL21" s="5"/>
+      <c r="AM21" s="5"/>
+      <c r="AN21" s="5"/>
+      <c r="AO21" s="5"/>
+      <c r="AP21" s="5"/>
+      <c r="AQ21" s="5"/>
+      <c r="AR21" s="5"/>
+      <c r="AS21" s="5"/>
+      <c r="AT21" s="5"/>
+      <c r="AU21" s="5"/>
+      <c r="AV21" s="5"/>
+      <c r="AW21" s="5"/>
+      <c r="AX21" s="5"/>
+    </row>
+    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <f t="shared" si="0"/>
         <v>683.05</v>
@@ -8882,8 +9496,34 @@
       <c r="Z22" s="5">
         <v>757.3</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA22" s="5">
+        <v>748.4</v>
+      </c>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="5"/>
+      <c r="AE22" s="5"/>
+      <c r="AF22" s="5"/>
+      <c r="AG22" s="5"/>
+      <c r="AH22" s="5"/>
+      <c r="AI22" s="5"/>
+      <c r="AJ22" s="5"/>
+      <c r="AK22" s="5"/>
+      <c r="AL22" s="5"/>
+      <c r="AM22" s="5"/>
+      <c r="AN22" s="5"/>
+      <c r="AO22" s="5"/>
+      <c r="AP22" s="5"/>
+      <c r="AQ22" s="5"/>
+      <c r="AR22" s="5"/>
+      <c r="AS22" s="5"/>
+      <c r="AT22" s="5"/>
+      <c r="AU22" s="5"/>
+      <c r="AV22" s="5"/>
+      <c r="AW22" s="5"/>
+      <c r="AX22" s="5"/>
+    </row>
+    <row r="23" spans="1:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <f t="shared" si="0"/>
         <v>408.35</v>
@@ -8964,11 +9604,37 @@
       <c r="Z23" s="5">
         <v>423</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA23" s="5">
+        <v>414.45</v>
+      </c>
+      <c r="AB23" s="5"/>
+      <c r="AC23" s="5"/>
+      <c r="AD23" s="5"/>
+      <c r="AE23" s="5"/>
+      <c r="AF23" s="5"/>
+      <c r="AG23" s="5"/>
+      <c r="AH23" s="5"/>
+      <c r="AI23" s="5"/>
+      <c r="AJ23" s="5"/>
+      <c r="AK23" s="5"/>
+      <c r="AL23" s="5"/>
+      <c r="AM23" s="5"/>
+      <c r="AN23" s="5"/>
+      <c r="AO23" s="5"/>
+      <c r="AP23" s="5"/>
+      <c r="AQ23" s="5"/>
+      <c r="AR23" s="5"/>
+      <c r="AS23" s="5"/>
+      <c r="AT23" s="5"/>
+      <c r="AU23" s="5"/>
+      <c r="AV23" s="5"/>
+      <c r="AW23" s="5"/>
+      <c r="AX23" s="5"/>
+    </row>
+    <row r="24" spans="1:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <f t="shared" si="0"/>
-        <v>12.2</v>
+        <v>12.05</v>
       </c>
       <c r="B24" s="13">
         <f t="shared" si="1"/>
@@ -9002,8 +9668,34 @@
       <c r="Z24" s="5">
         <v>12.2</v>
       </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA24" s="5">
+        <v>12.05</v>
+      </c>
+      <c r="AB24" s="5"/>
+      <c r="AC24" s="5"/>
+      <c r="AD24" s="5"/>
+      <c r="AE24" s="5"/>
+      <c r="AF24" s="5"/>
+      <c r="AG24" s="5"/>
+      <c r="AH24" s="5"/>
+      <c r="AI24" s="5"/>
+      <c r="AJ24" s="5"/>
+      <c r="AK24" s="5"/>
+      <c r="AL24" s="5"/>
+      <c r="AM24" s="5"/>
+      <c r="AN24" s="5"/>
+      <c r="AO24" s="5"/>
+      <c r="AP24" s="5"/>
+      <c r="AQ24" s="5"/>
+      <c r="AR24" s="5"/>
+      <c r="AS24" s="5"/>
+      <c r="AT24" s="5"/>
+      <c r="AU24" s="5"/>
+      <c r="AV24" s="5"/>
+      <c r="AW24" s="5"/>
+      <c r="AX24" s="5"/>
+    </row>
+    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <f t="shared" si="0"/>
         <v>54.95</v>
@@ -9076,8 +9768,34 @@
       <c r="Z25" s="5">
         <v>64.099999999999994</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA25" s="5">
+        <v>62.25</v>
+      </c>
+      <c r="AB25" s="5"/>
+      <c r="AC25" s="5"/>
+      <c r="AD25" s="5"/>
+      <c r="AE25" s="5"/>
+      <c r="AF25" s="5"/>
+      <c r="AG25" s="5"/>
+      <c r="AH25" s="5"/>
+      <c r="AI25" s="5"/>
+      <c r="AJ25" s="5"/>
+      <c r="AK25" s="5"/>
+      <c r="AL25" s="5"/>
+      <c r="AM25" s="5"/>
+      <c r="AN25" s="5"/>
+      <c r="AO25" s="5"/>
+      <c r="AP25" s="5"/>
+      <c r="AQ25" s="5"/>
+      <c r="AR25" s="5"/>
+      <c r="AS25" s="5"/>
+      <c r="AT25" s="5"/>
+      <c r="AU25" s="5"/>
+      <c r="AV25" s="5"/>
+      <c r="AW25" s="5"/>
+      <c r="AX25" s="5"/>
+    </row>
+    <row r="26" spans="1:50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <f t="shared" si="0"/>
         <v>218.8</v>
@@ -9146,8 +9864,34 @@
       <c r="Z26" s="5">
         <v>224.35</v>
       </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA26" s="5">
+        <v>219.5</v>
+      </c>
+      <c r="AB26" s="5"/>
+      <c r="AC26" s="5"/>
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="5"/>
+      <c r="AF26" s="5"/>
+      <c r="AG26" s="5"/>
+      <c r="AH26" s="5"/>
+      <c r="AI26" s="5"/>
+      <c r="AJ26" s="5"/>
+      <c r="AK26" s="5"/>
+      <c r="AL26" s="5"/>
+      <c r="AM26" s="5"/>
+      <c r="AN26" s="5"/>
+      <c r="AO26" s="5"/>
+      <c r="AP26" s="5"/>
+      <c r="AQ26" s="5"/>
+      <c r="AR26" s="5"/>
+      <c r="AS26" s="5"/>
+      <c r="AT26" s="5"/>
+      <c r="AU26" s="5"/>
+      <c r="AV26" s="5"/>
+      <c r="AW26" s="5"/>
+      <c r="AX26" s="5"/>
+    </row>
+    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <f t="shared" si="0"/>
         <v>876</v>
@@ -9198,8 +9942,34 @@
       <c r="Z27" s="5">
         <v>919.85</v>
       </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA27" s="5">
+        <v>899.95</v>
+      </c>
+      <c r="AB27" s="5"/>
+      <c r="AC27" s="5"/>
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="5"/>
+      <c r="AF27" s="5"/>
+      <c r="AG27" s="5"/>
+      <c r="AH27" s="5"/>
+      <c r="AI27" s="5"/>
+      <c r="AJ27" s="5"/>
+      <c r="AK27" s="5"/>
+      <c r="AL27" s="5"/>
+      <c r="AM27" s="5"/>
+      <c r="AN27" s="5"/>
+      <c r="AO27" s="5"/>
+      <c r="AP27" s="5"/>
+      <c r="AQ27" s="5"/>
+      <c r="AR27" s="5"/>
+      <c r="AS27" s="5"/>
+      <c r="AT27" s="5"/>
+      <c r="AU27" s="5"/>
+      <c r="AV27" s="5"/>
+      <c r="AW27" s="5"/>
+      <c r="AX27" s="5"/>
+    </row>
+    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <f t="shared" ref="A28:A41" si="2">MIN(D28:ZZ28)</f>
         <v>85.9</v>
@@ -9238,11 +10008,37 @@
       <c r="Z28" s="5">
         <v>87.95</v>
       </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA28" s="5">
+        <v>87.8</v>
+      </c>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="5"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="5"/>
+      <c r="AF28" s="5"/>
+      <c r="AG28" s="5"/>
+      <c r="AH28" s="5"/>
+      <c r="AI28" s="5"/>
+      <c r="AJ28" s="5"/>
+      <c r="AK28" s="5"/>
+      <c r="AL28" s="5"/>
+      <c r="AM28" s="5"/>
+      <c r="AN28" s="5"/>
+      <c r="AO28" s="5"/>
+      <c r="AP28" s="5"/>
+      <c r="AQ28" s="5"/>
+      <c r="AR28" s="5"/>
+      <c r="AS28" s="5"/>
+      <c r="AT28" s="5"/>
+      <c r="AU28" s="5"/>
+      <c r="AV28" s="5"/>
+      <c r="AW28" s="5"/>
+      <c r="AX28" s="5"/>
+    </row>
+    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <f t="shared" si="2"/>
-        <v>38.1</v>
+        <v>37.65</v>
       </c>
       <c r="B29" s="13">
         <f t="shared" si="3"/>
@@ -9278,11 +10074,37 @@
       <c r="Z29" s="5">
         <v>38.15</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA29" s="5">
+        <v>37.65</v>
+      </c>
+      <c r="AB29" s="5"/>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29" s="5"/>
+      <c r="AF29" s="5"/>
+      <c r="AG29" s="5"/>
+      <c r="AH29" s="5"/>
+      <c r="AI29" s="5"/>
+      <c r="AJ29" s="5"/>
+      <c r="AK29" s="5"/>
+      <c r="AL29" s="5"/>
+      <c r="AM29" s="5"/>
+      <c r="AN29" s="5"/>
+      <c r="AO29" s="5"/>
+      <c r="AP29" s="5"/>
+      <c r="AQ29" s="5"/>
+      <c r="AR29" s="5"/>
+      <c r="AS29" s="5"/>
+      <c r="AT29" s="5"/>
+      <c r="AU29" s="5"/>
+      <c r="AV29" s="5"/>
+      <c r="AW29" s="5"/>
+      <c r="AX29" s="5"/>
+    </row>
+    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <f t="shared" si="2"/>
-        <v>55.4</v>
+        <v>55.1</v>
       </c>
       <c r="B30" s="13">
         <f t="shared" si="3"/>
@@ -9318,11 +10140,37 @@
       <c r="Z30" s="5">
         <v>55.4</v>
       </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA30" s="5">
+        <v>55.1</v>
+      </c>
+      <c r="AB30" s="5"/>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30" s="5"/>
+      <c r="AF30" s="5"/>
+      <c r="AG30" s="5"/>
+      <c r="AH30" s="5"/>
+      <c r="AI30" s="5"/>
+      <c r="AJ30" s="5"/>
+      <c r="AK30" s="5"/>
+      <c r="AL30" s="5"/>
+      <c r="AM30" s="5"/>
+      <c r="AN30" s="5"/>
+      <c r="AO30" s="5"/>
+      <c r="AP30" s="5"/>
+      <c r="AQ30" s="5"/>
+      <c r="AR30" s="5"/>
+      <c r="AS30" s="5"/>
+      <c r="AT30" s="5"/>
+      <c r="AU30" s="5"/>
+      <c r="AV30" s="5"/>
+      <c r="AW30" s="5"/>
+      <c r="AX30" s="5"/>
+    </row>
+    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <f t="shared" si="2"/>
-        <v>127.65</v>
+        <v>127.05</v>
       </c>
       <c r="B31" s="13">
         <f t="shared" si="3"/>
@@ -9358,8 +10206,34 @@
       <c r="Z31" s="5">
         <v>129.35</v>
       </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA31" s="5">
+        <v>127.05</v>
+      </c>
+      <c r="AB31" s="5"/>
+      <c r="AC31" s="5"/>
+      <c r="AD31" s="5"/>
+      <c r="AE31" s="5"/>
+      <c r="AF31" s="5"/>
+      <c r="AG31" s="5"/>
+      <c r="AH31" s="5"/>
+      <c r="AI31" s="5"/>
+      <c r="AJ31" s="5"/>
+      <c r="AK31" s="5"/>
+      <c r="AL31" s="5"/>
+      <c r="AM31" s="5"/>
+      <c r="AN31" s="5"/>
+      <c r="AO31" s="5"/>
+      <c r="AP31" s="5"/>
+      <c r="AQ31" s="5"/>
+      <c r="AR31" s="5"/>
+      <c r="AS31" s="5"/>
+      <c r="AT31" s="5"/>
+      <c r="AU31" s="5"/>
+      <c r="AV31" s="5"/>
+      <c r="AW31" s="5"/>
+      <c r="AX31" s="5"/>
+    </row>
+    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <f t="shared" si="2"/>
         <v>190.05</v>
@@ -9398,11 +10272,37 @@
       <c r="Z32" s="5">
         <v>193.9</v>
       </c>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA32" s="5">
+        <v>191.85</v>
+      </c>
+      <c r="AB32" s="5"/>
+      <c r="AC32" s="5"/>
+      <c r="AD32" s="5"/>
+      <c r="AE32" s="5"/>
+      <c r="AF32" s="5"/>
+      <c r="AG32" s="5"/>
+      <c r="AH32" s="5"/>
+      <c r="AI32" s="5"/>
+      <c r="AJ32" s="5"/>
+      <c r="AK32" s="5"/>
+      <c r="AL32" s="5"/>
+      <c r="AM32" s="5"/>
+      <c r="AN32" s="5"/>
+      <c r="AO32" s="5"/>
+      <c r="AP32" s="5"/>
+      <c r="AQ32" s="5"/>
+      <c r="AR32" s="5"/>
+      <c r="AS32" s="5"/>
+      <c r="AT32" s="5"/>
+      <c r="AU32" s="5"/>
+      <c r="AV32" s="5"/>
+      <c r="AW32" s="5"/>
+      <c r="AX32" s="5"/>
+    </row>
+    <row r="33" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <f t="shared" si="2"/>
-        <v>77</v>
+        <v>76.849999999999994</v>
       </c>
       <c r="B33" s="13">
         <f t="shared" si="3"/>
@@ -9438,11 +10338,37 @@
       <c r="Z33" s="5">
         <v>77</v>
       </c>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA33" s="5">
+        <v>76.849999999999994</v>
+      </c>
+      <c r="AB33" s="5"/>
+      <c r="AC33" s="5"/>
+      <c r="AD33" s="5"/>
+      <c r="AE33" s="5"/>
+      <c r="AF33" s="5"/>
+      <c r="AG33" s="5"/>
+      <c r="AH33" s="5"/>
+      <c r="AI33" s="5"/>
+      <c r="AJ33" s="5"/>
+      <c r="AK33" s="5"/>
+      <c r="AL33" s="5"/>
+      <c r="AM33" s="5"/>
+      <c r="AN33" s="5"/>
+      <c r="AO33" s="5"/>
+      <c r="AP33" s="5"/>
+      <c r="AQ33" s="5"/>
+      <c r="AR33" s="5"/>
+      <c r="AS33" s="5"/>
+      <c r="AT33" s="5"/>
+      <c r="AU33" s="5"/>
+      <c r="AV33" s="5"/>
+      <c r="AW33" s="5"/>
+      <c r="AX33" s="5"/>
+    </row>
+    <row r="34" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <f t="shared" si="2"/>
-        <v>39.799999999999997</v>
+        <v>39.25</v>
       </c>
       <c r="B34" s="13">
         <f t="shared" si="3"/>
@@ -9478,11 +10404,37 @@
       <c r="Z34" s="5">
         <v>40.1</v>
       </c>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA34" s="5">
+        <v>39.25</v>
+      </c>
+      <c r="AB34" s="5"/>
+      <c r="AC34" s="5"/>
+      <c r="AD34" s="5"/>
+      <c r="AE34" s="5"/>
+      <c r="AF34" s="5"/>
+      <c r="AG34" s="5"/>
+      <c r="AH34" s="5"/>
+      <c r="AI34" s="5"/>
+      <c r="AJ34" s="5"/>
+      <c r="AK34" s="5"/>
+      <c r="AL34" s="5"/>
+      <c r="AM34" s="5"/>
+      <c r="AN34" s="5"/>
+      <c r="AO34" s="5"/>
+      <c r="AP34" s="5"/>
+      <c r="AQ34" s="5"/>
+      <c r="AR34" s="5"/>
+      <c r="AS34" s="5"/>
+      <c r="AT34" s="5"/>
+      <c r="AU34" s="5"/>
+      <c r="AV34" s="5"/>
+      <c r="AW34" s="5"/>
+      <c r="AX34" s="5"/>
+    </row>
+    <row r="35" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <f t="shared" si="2"/>
-        <v>64.5</v>
+        <v>64</v>
       </c>
       <c r="B35" s="13">
         <f t="shared" si="3"/>
@@ -9518,11 +10470,37 @@
       <c r="Z35" s="5">
         <v>65</v>
       </c>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA35" s="5">
+        <v>64</v>
+      </c>
+      <c r="AB35" s="5"/>
+      <c r="AC35" s="5"/>
+      <c r="AD35" s="5"/>
+      <c r="AE35" s="5"/>
+      <c r="AF35" s="5"/>
+      <c r="AG35" s="5"/>
+      <c r="AH35" s="5"/>
+      <c r="AI35" s="5"/>
+      <c r="AJ35" s="5"/>
+      <c r="AK35" s="5"/>
+      <c r="AL35" s="5"/>
+      <c r="AM35" s="5"/>
+      <c r="AN35" s="5"/>
+      <c r="AO35" s="5"/>
+      <c r="AP35" s="5"/>
+      <c r="AQ35" s="5"/>
+      <c r="AR35" s="5"/>
+      <c r="AS35" s="5"/>
+      <c r="AT35" s="5"/>
+      <c r="AU35" s="5"/>
+      <c r="AV35" s="5"/>
+      <c r="AW35" s="5"/>
+      <c r="AX35" s="5"/>
+    </row>
+    <row r="36" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <f t="shared" si="2"/>
-        <v>31.05</v>
+        <v>31</v>
       </c>
       <c r="B36" s="13">
         <f t="shared" si="3"/>
@@ -9558,11 +10536,37 @@
       <c r="Z36" s="5">
         <v>31.15</v>
       </c>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA36" s="5">
+        <v>31</v>
+      </c>
+      <c r="AB36" s="5"/>
+      <c r="AC36" s="5"/>
+      <c r="AD36" s="5"/>
+      <c r="AE36" s="5"/>
+      <c r="AF36" s="5"/>
+      <c r="AG36" s="5"/>
+      <c r="AH36" s="5"/>
+      <c r="AI36" s="5"/>
+      <c r="AJ36" s="5"/>
+      <c r="AK36" s="5"/>
+      <c r="AL36" s="5"/>
+      <c r="AM36" s="5"/>
+      <c r="AN36" s="5"/>
+      <c r="AO36" s="5"/>
+      <c r="AP36" s="5"/>
+      <c r="AQ36" s="5"/>
+      <c r="AR36" s="5"/>
+      <c r="AS36" s="5"/>
+      <c r="AT36" s="5"/>
+      <c r="AU36" s="5"/>
+      <c r="AV36" s="5"/>
+      <c r="AW36" s="5"/>
+      <c r="AX36" s="5"/>
+    </row>
+    <row r="37" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <f t="shared" si="2"/>
-        <v>44.8</v>
+        <v>44.2</v>
       </c>
       <c r="B37" s="13">
         <f t="shared" si="3"/>
@@ -9598,8 +10602,34 @@
       <c r="Z37" s="5">
         <v>44.85</v>
       </c>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA37" s="5">
+        <v>44.2</v>
+      </c>
+      <c r="AB37" s="5"/>
+      <c r="AC37" s="5"/>
+      <c r="AD37" s="5"/>
+      <c r="AE37" s="5"/>
+      <c r="AF37" s="5"/>
+      <c r="AG37" s="5"/>
+      <c r="AH37" s="5"/>
+      <c r="AI37" s="5"/>
+      <c r="AJ37" s="5"/>
+      <c r="AK37" s="5"/>
+      <c r="AL37" s="5"/>
+      <c r="AM37" s="5"/>
+      <c r="AN37" s="5"/>
+      <c r="AO37" s="5"/>
+      <c r="AP37" s="5"/>
+      <c r="AQ37" s="5"/>
+      <c r="AR37" s="5"/>
+      <c r="AS37" s="5"/>
+      <c r="AT37" s="5"/>
+      <c r="AU37" s="5"/>
+      <c r="AV37" s="5"/>
+      <c r="AW37" s="5"/>
+      <c r="AX37" s="5"/>
+    </row>
+    <row r="38" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <f t="shared" si="2"/>
         <v>84.25</v>
@@ -9638,11 +10668,37 @@
       <c r="Z38" s="5">
         <v>87.4</v>
       </c>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA38" s="5">
+        <v>85.5</v>
+      </c>
+      <c r="AB38" s="5"/>
+      <c r="AC38" s="5"/>
+      <c r="AD38" s="5"/>
+      <c r="AE38" s="5"/>
+      <c r="AF38" s="5"/>
+      <c r="AG38" s="5"/>
+      <c r="AH38" s="5"/>
+      <c r="AI38" s="5"/>
+      <c r="AJ38" s="5"/>
+      <c r="AK38" s="5"/>
+      <c r="AL38" s="5"/>
+      <c r="AM38" s="5"/>
+      <c r="AN38" s="5"/>
+      <c r="AO38" s="5"/>
+      <c r="AP38" s="5"/>
+      <c r="AQ38" s="5"/>
+      <c r="AR38" s="5"/>
+      <c r="AS38" s="5"/>
+      <c r="AT38" s="5"/>
+      <c r="AU38" s="5"/>
+      <c r="AV38" s="5"/>
+      <c r="AW38" s="5"/>
+      <c r="AX38" s="5"/>
+    </row>
+    <row r="39" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <f t="shared" si="2"/>
-        <v>122.2</v>
+        <v>122.05</v>
       </c>
       <c r="B39" s="13">
         <f t="shared" si="3"/>
@@ -9678,11 +10734,37 @@
       <c r="Z39" s="5">
         <v>123.5</v>
       </c>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA39" s="5">
+        <v>122.05</v>
+      </c>
+      <c r="AB39" s="5"/>
+      <c r="AC39" s="5"/>
+      <c r="AD39" s="5"/>
+      <c r="AE39" s="5"/>
+      <c r="AF39" s="5"/>
+      <c r="AG39" s="5"/>
+      <c r="AH39" s="5"/>
+      <c r="AI39" s="5"/>
+      <c r="AJ39" s="5"/>
+      <c r="AK39" s="5"/>
+      <c r="AL39" s="5"/>
+      <c r="AM39" s="5"/>
+      <c r="AN39" s="5"/>
+      <c r="AO39" s="5"/>
+      <c r="AP39" s="5"/>
+      <c r="AQ39" s="5"/>
+      <c r="AR39" s="5"/>
+      <c r="AS39" s="5"/>
+      <c r="AT39" s="5"/>
+      <c r="AU39" s="5"/>
+      <c r="AV39" s="5"/>
+      <c r="AW39" s="5"/>
+      <c r="AX39" s="5"/>
+    </row>
+    <row r="40" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <f t="shared" si="2"/>
-        <v>138.30000000000001</v>
+        <v>136.9</v>
       </c>
       <c r="B40" s="13">
         <f t="shared" si="3"/>
@@ -9718,8 +10800,34 @@
       <c r="Z40" s="5">
         <v>138.35</v>
       </c>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA40" s="5">
+        <v>136.9</v>
+      </c>
+      <c r="AB40" s="5"/>
+      <c r="AC40" s="5"/>
+      <c r="AD40" s="5"/>
+      <c r="AE40" s="5"/>
+      <c r="AF40" s="5"/>
+      <c r="AG40" s="5"/>
+      <c r="AH40" s="5"/>
+      <c r="AI40" s="5"/>
+      <c r="AJ40" s="5"/>
+      <c r="AK40" s="5"/>
+      <c r="AL40" s="5"/>
+      <c r="AM40" s="5"/>
+      <c r="AN40" s="5"/>
+      <c r="AO40" s="5"/>
+      <c r="AP40" s="5"/>
+      <c r="AQ40" s="5"/>
+      <c r="AR40" s="5"/>
+      <c r="AS40" s="5"/>
+      <c r="AT40" s="5"/>
+      <c r="AU40" s="5"/>
+      <c r="AV40" s="5"/>
+      <c r="AW40" s="5"/>
+      <c r="AX40" s="5"/>
+    </row>
+    <row r="41" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <f t="shared" si="2"/>
         <v>146</v>
@@ -9758,6 +10866,32 @@
       <c r="Z41" s="5">
         <v>149.05000000000001</v>
       </c>
+      <c r="AA41" s="5">
+        <v>147.4</v>
+      </c>
+      <c r="AB41" s="5"/>
+      <c r="AC41" s="5"/>
+      <c r="AD41" s="5"/>
+      <c r="AE41" s="5"/>
+      <c r="AF41" s="5"/>
+      <c r="AG41" s="5"/>
+      <c r="AH41" s="5"/>
+      <c r="AI41" s="5"/>
+      <c r="AJ41" s="5"/>
+      <c r="AK41" s="5"/>
+      <c r="AL41" s="5"/>
+      <c r="AM41" s="5"/>
+      <c r="AN41" s="5"/>
+      <c r="AO41" s="5"/>
+      <c r="AP41" s="5"/>
+      <c r="AQ41" s="5"/>
+      <c r="AR41" s="5"/>
+      <c r="AS41" s="5"/>
+      <c r="AT41" s="5"/>
+      <c r="AU41" s="5"/>
+      <c r="AV41" s="5"/>
+      <c r="AW41" s="5"/>
+      <c r="AX41" s="5"/>
     </row>
   </sheetData>
   <sortState ref="K1:K37">
@@ -10880,10 +12014,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A2" sqref="A2:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10927,7 +12061,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(B2:B200)</f>
-        <v>619693</v>
+        <v>728193</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -10945,7 +12079,7 @@
       </c>
       <c r="F3" s="5">
         <f>F1-F2</f>
-        <v>855696</v>
+        <v>747196</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -11122,6 +12256,28 @@
       </c>
       <c r="C19" s="33">
         <v>42974</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="B20" s="13">
+        <v>100000</v>
+      </c>
+      <c r="C20" s="33">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="B21" s="13">
+        <v>8500</v>
+      </c>
+      <c r="C21" s="33">
+        <v>42982</v>
       </c>
     </row>
   </sheetData>
@@ -11590,8 +12746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:I30"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29:I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added new google finance URL on 07/09/2017 after old stopped working
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="298">
   <si>
     <t>Date</t>
   </si>
@@ -916,6 +916,9 @@
   </si>
   <si>
     <t>JSL</t>
+  </si>
+  <si>
+    <t>Ret</t>
   </si>
 </sst>
 </file>
@@ -7135,7 +7138,7 @@
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="3" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB45" sqref="AB45"/>
+      <selection pane="topRight" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7375,8 +7378,12 @@
       <c r="AB2" s="43">
         <v>276.60000000000002</v>
       </c>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
+      <c r="AC2" s="5">
+        <v>274.85000000000002</v>
+      </c>
+      <c r="AD2" s="5">
+        <v>274.85000000000002</v>
+      </c>
       <c r="AE2" s="5"/>
       <c r="AF2" s="5"/>
       <c r="AG2" s="5"/>
@@ -7479,8 +7486,12 @@
       <c r="AB3" s="5">
         <v>297.3</v>
       </c>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="5"/>
+      <c r="AC3" s="5">
+        <v>293.5</v>
+      </c>
+      <c r="AD3" s="5">
+        <v>293.5</v>
+      </c>
       <c r="AE3" s="5"/>
       <c r="AF3" s="5"/>
       <c r="AG3" s="5"/>
@@ -7505,7 +7516,7 @@
     <row r="4" spans="1:50">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
-        <v>271.2</v>
+        <v>270.35000000000002</v>
       </c>
       <c r="B4" s="12">
         <f t="shared" si="1"/>
@@ -7589,8 +7600,12 @@
       <c r="AB4" s="5">
         <v>282</v>
       </c>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
+      <c r="AC4" s="5">
+        <v>270.35000000000002</v>
+      </c>
+      <c r="AD4" s="5">
+        <v>270.35000000000002</v>
+      </c>
       <c r="AE4" s="5"/>
       <c r="AF4" s="5"/>
       <c r="AG4" s="5"/>
@@ -7615,7 +7630,7 @@
     <row r="5" spans="1:50">
       <c r="A5" s="12">
         <f t="shared" si="0"/>
-        <v>1532.05</v>
+        <v>820.7</v>
       </c>
       <c r="B5" s="12">
         <f t="shared" si="1"/>
@@ -7699,8 +7714,12 @@
       <c r="AB5" s="43">
         <v>1632.15</v>
       </c>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
+      <c r="AC5" s="5">
+        <v>820.7</v>
+      </c>
+      <c r="AD5" s="5">
+        <v>820.7</v>
+      </c>
       <c r="AE5" s="5"/>
       <c r="AF5" s="5"/>
       <c r="AG5" s="5"/>
@@ -7809,8 +7828,12 @@
       <c r="AB6" s="5">
         <v>253.7</v>
       </c>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="5"/>
+      <c r="AC6" s="5">
+        <v>252.6</v>
+      </c>
+      <c r="AD6" s="5">
+        <v>252.6</v>
+      </c>
       <c r="AE6" s="5"/>
       <c r="AF6" s="5"/>
       <c r="AG6" s="5"/>
@@ -7919,8 +7942,12 @@
       <c r="AB7" s="5">
         <v>17.05</v>
       </c>
-      <c r="AC7" s="5"/>
-      <c r="AD7" s="5"/>
+      <c r="AC7" s="5">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="AD7" s="5">
+        <v>17.600000000000001</v>
+      </c>
       <c r="AE7" s="5"/>
       <c r="AF7" s="5"/>
       <c r="AG7" s="5"/>
@@ -8029,8 +8056,12 @@
       <c r="AB8" s="5">
         <v>62.15</v>
       </c>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
+      <c r="AC8" s="5">
+        <v>62.9</v>
+      </c>
+      <c r="AD8" s="5">
+        <v>62.9</v>
+      </c>
       <c r="AE8" s="5"/>
       <c r="AF8" s="5"/>
       <c r="AG8" s="5"/>
@@ -8131,8 +8162,12 @@
       <c r="AB9" s="28">
         <v>57.55</v>
       </c>
-      <c r="AC9" s="28"/>
-      <c r="AD9" s="28"/>
+      <c r="AC9" s="28">
+        <v>57.4</v>
+      </c>
+      <c r="AD9" s="28">
+        <v>57.4</v>
+      </c>
       <c r="AE9" s="28"/>
       <c r="AF9" s="28"/>
       <c r="AG9" s="28"/>
@@ -8241,8 +8276,12 @@
       <c r="AB10" s="5">
         <v>40.25</v>
       </c>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="5"/>
+      <c r="AC10" s="5">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="AD10" s="5">
+        <v>39.950000000000003</v>
+      </c>
       <c r="AE10" s="5"/>
       <c r="AF10" s="5"/>
       <c r="AG10" s="5"/>
@@ -8271,7 +8310,7 @@
       </c>
       <c r="B11" s="12">
         <f t="shared" si="1"/>
-        <v>75.05</v>
+        <v>83</v>
       </c>
       <c r="C11" s="46" t="s">
         <v>17</v>
@@ -8351,8 +8390,12 @@
       <c r="AB11" s="5">
         <v>73.8</v>
       </c>
-      <c r="AC11" s="5"/>
-      <c r="AD11" s="5"/>
+      <c r="AC11" s="5">
+        <v>83</v>
+      </c>
+      <c r="AD11" s="5">
+        <v>83</v>
+      </c>
       <c r="AE11" s="5"/>
       <c r="AF11" s="5"/>
       <c r="AG11" s="5"/>
@@ -8377,7 +8420,7 @@
     <row r="12" spans="1:50">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
-        <v>84.5</v>
+        <v>81.2</v>
       </c>
       <c r="B12" s="12">
         <f t="shared" si="1"/>
@@ -8461,8 +8504,12 @@
       <c r="AB12" s="5">
         <v>84.5</v>
       </c>
-      <c r="AC12" s="5"/>
-      <c r="AD12" s="5"/>
+      <c r="AC12" s="5">
+        <v>81.2</v>
+      </c>
+      <c r="AD12" s="5">
+        <v>81.2</v>
+      </c>
       <c r="AE12" s="5"/>
       <c r="AF12" s="5"/>
       <c r="AG12" s="5"/>
@@ -8571,8 +8618,12 @@
       <c r="AB13" s="5">
         <v>131.1</v>
       </c>
-      <c r="AC13" s="5"/>
-      <c r="AD13" s="5"/>
+      <c r="AC13" s="5">
+        <v>130.15</v>
+      </c>
+      <c r="AD13" s="5">
+        <v>130.15</v>
+      </c>
       <c r="AE13" s="5"/>
       <c r="AF13" s="5"/>
       <c r="AG13" s="5"/>
@@ -8681,8 +8732,12 @@
       <c r="AB14" s="5">
         <v>78.3</v>
       </c>
-      <c r="AC14" s="5"/>
-      <c r="AD14" s="5"/>
+      <c r="AC14" s="5">
+        <v>77.349999999999994</v>
+      </c>
+      <c r="AD14" s="5">
+        <v>77.349999999999994</v>
+      </c>
       <c r="AE14" s="5"/>
       <c r="AF14" s="5"/>
       <c r="AG14" s="5"/>
@@ -8791,8 +8846,12 @@
       <c r="AB15" s="5">
         <v>50.9</v>
       </c>
-      <c r="AC15" s="5"/>
-      <c r="AD15" s="5"/>
+      <c r="AC15" s="5">
+        <v>51.75</v>
+      </c>
+      <c r="AD15" s="5">
+        <v>51.75</v>
+      </c>
       <c r="AE15" s="5"/>
       <c r="AF15" s="5"/>
       <c r="AG15" s="5"/>
@@ -8901,8 +8960,12 @@
       <c r="AB16" s="5">
         <v>32.5</v>
       </c>
-      <c r="AC16" s="5"/>
-      <c r="AD16" s="5"/>
+      <c r="AC16" s="5">
+        <v>32.950000000000003</v>
+      </c>
+      <c r="AD16" s="5">
+        <v>32.950000000000003</v>
+      </c>
       <c r="AE16" s="5"/>
       <c r="AF16" s="5"/>
       <c r="AG16" s="5"/>
@@ -9003,8 +9066,12 @@
       <c r="AB17" s="5">
         <v>30.35</v>
       </c>
-      <c r="AC17" s="5"/>
-      <c r="AD17" s="5"/>
+      <c r="AC17" s="5">
+        <v>30.2</v>
+      </c>
+      <c r="AD17" s="5">
+        <v>30.2</v>
+      </c>
       <c r="AE17" s="5"/>
       <c r="AF17" s="5"/>
       <c r="AG17" s="5"/>
@@ -9033,7 +9100,7 @@
       </c>
       <c r="B18" s="12">
         <f t="shared" si="1"/>
-        <v>652.04999999999995</v>
+        <v>654.79999999999995</v>
       </c>
       <c r="C18" s="46" t="s">
         <v>25</v>
@@ -9113,8 +9180,12 @@
       <c r="AB18" s="5">
         <v>652.04999999999995</v>
       </c>
-      <c r="AC18" s="5"/>
-      <c r="AD18" s="5"/>
+      <c r="AC18" s="5">
+        <v>654.79999999999995</v>
+      </c>
+      <c r="AD18" s="5">
+        <v>654.79999999999995</v>
+      </c>
       <c r="AE18" s="5"/>
       <c r="AF18" s="5"/>
       <c r="AG18" s="5"/>
@@ -9223,8 +9294,12 @@
       <c r="AB19" s="5">
         <v>491</v>
       </c>
-      <c r="AC19" s="5"/>
-      <c r="AD19" s="5"/>
+      <c r="AC19" s="5">
+        <v>472.95</v>
+      </c>
+      <c r="AD19" s="5">
+        <v>472.95</v>
+      </c>
       <c r="AE19" s="5"/>
       <c r="AF19" s="5"/>
       <c r="AG19" s="5"/>
@@ -9253,7 +9328,7 @@
       </c>
       <c r="B20" s="12">
         <f t="shared" si="1"/>
-        <v>228.85</v>
+        <v>240.55</v>
       </c>
       <c r="C20" s="45" t="s">
         <v>41</v>
@@ -9333,8 +9408,12 @@
       <c r="AB20" s="5">
         <v>227.6</v>
       </c>
-      <c r="AC20" s="5"/>
-      <c r="AD20" s="5"/>
+      <c r="AC20" s="5">
+        <v>240.55</v>
+      </c>
+      <c r="AD20" s="5">
+        <v>240.55</v>
+      </c>
       <c r="AE20" s="5"/>
       <c r="AF20" s="5"/>
       <c r="AG20" s="5"/>
@@ -9443,8 +9522,12 @@
       <c r="AB21" s="5">
         <v>491.1</v>
       </c>
-      <c r="AC21" s="5"/>
-      <c r="AD21" s="5"/>
+      <c r="AC21" s="5">
+        <v>487.85</v>
+      </c>
+      <c r="AD21" s="5">
+        <v>487.85</v>
+      </c>
       <c r="AE21" s="5"/>
       <c r="AF21" s="5"/>
       <c r="AG21" s="5"/>
@@ -9553,8 +9636,12 @@
       <c r="AB22" s="5">
         <v>743</v>
       </c>
-      <c r="AC22" s="5"/>
-      <c r="AD22" s="5"/>
+      <c r="AC22" s="5">
+        <v>742.1</v>
+      </c>
+      <c r="AD22" s="5">
+        <v>742.1</v>
+      </c>
       <c r="AE22" s="5"/>
       <c r="AF22" s="5"/>
       <c r="AG22" s="5"/>
@@ -9579,7 +9666,7 @@
     <row r="23" spans="1:50" ht="15.75" customHeight="1">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
-        <v>405.85</v>
+        <v>399.5</v>
       </c>
       <c r="B23" s="12">
         <f t="shared" si="1"/>
@@ -9663,8 +9750,12 @@
       <c r="AB23" s="5">
         <v>405.85</v>
       </c>
-      <c r="AC23" s="5"/>
-      <c r="AD23" s="5"/>
+      <c r="AC23" s="5">
+        <v>399.5</v>
+      </c>
+      <c r="AD23" s="5">
+        <v>399.5</v>
+      </c>
       <c r="AE23" s="5"/>
       <c r="AF23" s="5"/>
       <c r="AG23" s="5"/>
@@ -9693,7 +9784,7 @@
       </c>
       <c r="B24" s="12">
         <f t="shared" si="1"/>
-        <v>12.2</v>
+        <v>14.5</v>
       </c>
       <c r="C24" s="45" t="s">
         <v>285</v>
@@ -9729,8 +9820,12 @@
       <c r="AB24" s="5">
         <v>12.15</v>
       </c>
-      <c r="AC24" s="5"/>
-      <c r="AD24" s="5"/>
+      <c r="AC24" s="5">
+        <v>14.5</v>
+      </c>
+      <c r="AD24" s="5">
+        <v>14.5</v>
+      </c>
       <c r="AE24" s="5"/>
       <c r="AF24" s="5"/>
       <c r="AG24" s="5"/>
@@ -9831,8 +9926,12 @@
       <c r="AB25" s="5">
         <v>62.7</v>
       </c>
-      <c r="AC25" s="5"/>
-      <c r="AD25" s="5"/>
+      <c r="AC25" s="5">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="AD25" s="5">
+        <v>66.900000000000006</v>
+      </c>
       <c r="AE25" s="5"/>
       <c r="AF25" s="5"/>
       <c r="AG25" s="5"/>
@@ -9857,7 +9956,7 @@
     <row r="26" spans="1:50" ht="14.25" customHeight="1">
       <c r="A26" s="12">
         <f t="shared" si="0"/>
-        <v>218.8</v>
+        <v>211.4</v>
       </c>
       <c r="B26" s="12">
         <f t="shared" si="1"/>
@@ -9929,8 +10028,12 @@
       <c r="AB26" s="5">
         <v>219</v>
       </c>
-      <c r="AC26" s="5"/>
-      <c r="AD26" s="5"/>
+      <c r="AC26" s="5">
+        <v>211.4</v>
+      </c>
+      <c r="AD26" s="5">
+        <v>211.4</v>
+      </c>
       <c r="AE26" s="5"/>
       <c r="AF26" s="5"/>
       <c r="AG26" s="5"/>
@@ -10009,8 +10112,12 @@
       <c r="AB27" s="5">
         <v>901</v>
       </c>
-      <c r="AC27" s="5"/>
-      <c r="AD27" s="5"/>
+      <c r="AC27" s="5">
+        <v>894.65</v>
+      </c>
+      <c r="AD27" s="5">
+        <v>894.65</v>
+      </c>
       <c r="AE27" s="5"/>
       <c r="AF27" s="5"/>
       <c r="AG27" s="5"/>
@@ -10035,7 +10142,7 @@
     <row r="28" spans="1:50">
       <c r="A28" s="12">
         <f t="shared" ref="A28:A41" si="2">MIN(D28:ZZ28)</f>
-        <v>85.9</v>
+        <v>85.6</v>
       </c>
       <c r="B28" s="12">
         <f t="shared" ref="B28:B41" si="3">MAX(D28:ZZ28)</f>
@@ -10077,8 +10184,12 @@
       <c r="AB28" s="5">
         <v>87.1</v>
       </c>
-      <c r="AC28" s="5"/>
-      <c r="AD28" s="5"/>
+      <c r="AC28" s="5">
+        <v>85.6</v>
+      </c>
+      <c r="AD28" s="5">
+        <v>85.6</v>
+      </c>
       <c r="AE28" s="5"/>
       <c r="AF28" s="5"/>
       <c r="AG28" s="5"/>
@@ -10107,7 +10218,7 @@
       </c>
       <c r="B29" s="12">
         <f t="shared" si="3"/>
-        <v>38.15</v>
+        <v>40.6</v>
       </c>
       <c r="C29" s="46" t="s">
         <v>272</v>
@@ -10145,8 +10256,12 @@
       <c r="AB29" s="5">
         <v>37.6</v>
       </c>
-      <c r="AC29" s="5"/>
-      <c r="AD29" s="5"/>
+      <c r="AC29" s="5">
+        <v>40.6</v>
+      </c>
+      <c r="AD29" s="5">
+        <v>40.6</v>
+      </c>
       <c r="AE29" s="5"/>
       <c r="AF29" s="5"/>
       <c r="AG29" s="5"/>
@@ -10213,8 +10328,12 @@
       <c r="AB30" s="5">
         <v>55.7</v>
       </c>
-      <c r="AC30" s="5"/>
-      <c r="AD30" s="5"/>
+      <c r="AC30" s="5">
+        <v>55.6</v>
+      </c>
+      <c r="AD30" s="5">
+        <v>55.6</v>
+      </c>
       <c r="AE30" s="5"/>
       <c r="AF30" s="5"/>
       <c r="AG30" s="5"/>
@@ -10281,8 +10400,12 @@
       <c r="AB31" s="5">
         <v>129.6</v>
       </c>
-      <c r="AC31" s="5"/>
-      <c r="AD31" s="5"/>
+      <c r="AC31" s="5">
+        <v>127.55</v>
+      </c>
+      <c r="AD31" s="5">
+        <v>127.55</v>
+      </c>
       <c r="AE31" s="5"/>
       <c r="AF31" s="5"/>
       <c r="AG31" s="5"/>
@@ -10311,7 +10434,7 @@
       </c>
       <c r="B32" s="12">
         <f t="shared" si="3"/>
-        <v>193.9</v>
+        <v>194.3</v>
       </c>
       <c r="C32" s="46" t="s">
         <v>275</v>
@@ -10349,8 +10472,12 @@
       <c r="AB32" s="5">
         <v>192.1</v>
       </c>
-      <c r="AC32" s="5"/>
-      <c r="AD32" s="5"/>
+      <c r="AC32" s="5">
+        <v>194.3</v>
+      </c>
+      <c r="AD32" s="5">
+        <v>194.3</v>
+      </c>
       <c r="AE32" s="5"/>
       <c r="AF32" s="5"/>
       <c r="AG32" s="5"/>
@@ -10379,7 +10506,7 @@
       </c>
       <c r="B33" s="12">
         <f t="shared" si="3"/>
-        <v>77.349999999999994</v>
+        <v>78.849999999999994</v>
       </c>
       <c r="C33" s="46" t="s">
         <v>276</v>
@@ -10417,8 +10544,12 @@
       <c r="AB33" s="5">
         <v>77.349999999999994</v>
       </c>
-      <c r="AC33" s="5"/>
-      <c r="AD33" s="5"/>
+      <c r="AC33" s="5">
+        <v>78.849999999999994</v>
+      </c>
+      <c r="AD33" s="5">
+        <v>78.849999999999994</v>
+      </c>
       <c r="AE33" s="5"/>
       <c r="AF33" s="5"/>
       <c r="AG33" s="5"/>
@@ -10447,7 +10578,7 @@
       </c>
       <c r="B34" s="12">
         <f t="shared" si="3"/>
-        <v>40.1</v>
+        <v>40.4</v>
       </c>
       <c r="C34" s="46" t="s">
         <v>277</v>
@@ -10485,8 +10616,12 @@
       <c r="AB34" s="5">
         <v>39.35</v>
       </c>
-      <c r="AC34" s="5"/>
-      <c r="AD34" s="5"/>
+      <c r="AC34" s="5">
+        <v>40.4</v>
+      </c>
+      <c r="AD34" s="5">
+        <v>40.4</v>
+      </c>
       <c r="AE34" s="5"/>
       <c r="AF34" s="5"/>
       <c r="AG34" s="5"/>
@@ -10553,8 +10688,12 @@
       <c r="AB35" s="5">
         <v>65.099999999999994</v>
       </c>
-      <c r="AC35" s="5"/>
-      <c r="AD35" s="5"/>
+      <c r="AC35" s="5">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="AD35" s="5">
+        <v>64.599999999999994</v>
+      </c>
       <c r="AE35" s="5"/>
       <c r="AF35" s="5"/>
       <c r="AG35" s="5"/>
@@ -10583,7 +10722,7 @@
       </c>
       <c r="B36" s="12">
         <f t="shared" si="3"/>
-        <v>31.15</v>
+        <v>32.549999999999997</v>
       </c>
       <c r="C36" s="46" t="s">
         <v>279</v>
@@ -10621,8 +10760,12 @@
       <c r="AB36" s="5">
         <v>31.15</v>
       </c>
-      <c r="AC36" s="5"/>
-      <c r="AD36" s="5"/>
+      <c r="AC36" s="5">
+        <v>32.549999999999997</v>
+      </c>
+      <c r="AD36" s="5">
+        <v>32.549999999999997</v>
+      </c>
       <c r="AE36" s="5"/>
       <c r="AF36" s="5"/>
       <c r="AG36" s="5"/>
@@ -10689,8 +10832,12 @@
       <c r="AB37" s="5">
         <v>44.4</v>
       </c>
-      <c r="AC37" s="5"/>
-      <c r="AD37" s="5"/>
+      <c r="AC37" s="5">
+        <v>44.65</v>
+      </c>
+      <c r="AD37" s="5">
+        <v>44.65</v>
+      </c>
       <c r="AE37" s="5"/>
       <c r="AF37" s="5"/>
       <c r="AG37" s="5"/>
@@ -10757,8 +10904,12 @@
       <c r="AB38" s="5">
         <v>86.5</v>
       </c>
-      <c r="AC38" s="5"/>
-      <c r="AD38" s="5"/>
+      <c r="AC38" s="5">
+        <v>85.6</v>
+      </c>
+      <c r="AD38" s="5">
+        <v>85.6</v>
+      </c>
       <c r="AE38" s="5"/>
       <c r="AF38" s="5"/>
       <c r="AG38" s="5"/>
@@ -10825,8 +10976,12 @@
       <c r="AB39" s="5">
         <v>122.6</v>
       </c>
-      <c r="AC39" s="5"/>
-      <c r="AD39" s="5"/>
+      <c r="AC39" s="5">
+        <v>123.1</v>
+      </c>
+      <c r="AD39" s="5">
+        <v>123.1</v>
+      </c>
       <c r="AE39" s="5"/>
       <c r="AF39" s="5"/>
       <c r="AG39" s="5"/>
@@ -10850,12 +11005,12 @@
     </row>
     <row r="40" spans="1:50">
       <c r="A40" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A40:A42" si="4">MIN(D40:ZZ40)</f>
         <v>136.9</v>
       </c>
       <c r="B40" s="12">
-        <f t="shared" si="3"/>
-        <v>138.6</v>
+        <f t="shared" ref="B40:B42" si="5">MAX(D40:ZZ40)</f>
+        <v>140.15</v>
       </c>
       <c r="C40" s="46" t="s">
         <v>283</v>
@@ -10893,8 +11048,12 @@
       <c r="AB40" s="5">
         <v>138.6</v>
       </c>
-      <c r="AC40" s="5"/>
-      <c r="AD40" s="5"/>
+      <c r="AC40" s="5">
+        <v>140.15</v>
+      </c>
+      <c r="AD40" s="5">
+        <v>140.15</v>
+      </c>
       <c r="AE40" s="5"/>
       <c r="AF40" s="5"/>
       <c r="AG40" s="5"/>
@@ -10918,12 +11077,12 @@
     </row>
     <row r="41" spans="1:50">
       <c r="A41" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>146</v>
       </c>
       <c r="B41" s="12">
-        <f t="shared" si="3"/>
-        <v>152.30000000000001</v>
+        <f t="shared" si="5"/>
+        <v>154.05000000000001</v>
       </c>
       <c r="C41" s="46" t="s">
         <v>284</v>
@@ -10961,8 +11120,12 @@
       <c r="AB41" s="5">
         <v>152.30000000000001</v>
       </c>
-      <c r="AC41" s="5"/>
-      <c r="AD41" s="5"/>
+      <c r="AC41" s="5">
+        <v>154.05000000000001</v>
+      </c>
+      <c r="AD41" s="5">
+        <v>154.05000000000001</v>
+      </c>
       <c r="AE41" s="5"/>
       <c r="AF41" s="5"/>
       <c r="AG41" s="5"/>
@@ -10985,8 +11148,14 @@
       <c r="AX41" s="5"/>
     </row>
     <row r="42" spans="1:50">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="12">
+        <f t="shared" si="4"/>
+        <v>100.4</v>
+      </c>
+      <c r="B42" s="12">
+        <f t="shared" si="5"/>
+        <v>106.7</v>
+      </c>
       <c r="C42" s="46" t="s">
         <v>296</v>
       </c>
@@ -11017,8 +11186,12 @@
       <c r="AB42" s="5">
         <v>100.4</v>
       </c>
-      <c r="AC42" s="5"/>
-      <c r="AD42" s="5"/>
+      <c r="AC42" s="5">
+        <v>106.7</v>
+      </c>
+      <c r="AD42" s="5">
+        <v>106.7</v>
+      </c>
       <c r="AE42" s="5"/>
       <c r="AF42" s="5"/>
       <c r="AG42" s="5"/>
@@ -12161,10 +12334,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C23" sqref="A23:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12208,7 +12381,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(B2:B200)</f>
-        <v>778193</v>
+        <v>782693</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -12226,7 +12399,7 @@
       </c>
       <c r="F3" s="5">
         <f>F1-F2</f>
-        <v>697196</v>
+        <v>692696</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -12436,6 +12609,17 @@
       </c>
       <c r="C22" s="32">
         <v>42983</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="B23" s="12">
+        <v>4500</v>
+      </c>
+      <c r="C23" s="32">
+        <v>42985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the sheet for 12092017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -7143,7 +7143,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="3" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF2" sqref="AF2:AF41"/>
+      <selection pane="topRight" activeCell="AG41" sqref="AG41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7395,7 +7395,9 @@
       <c r="AF2" s="5">
         <v>270.60000000000002</v>
       </c>
-      <c r="AG2" s="5"/>
+      <c r="AG2" s="5">
+        <v>273.60000000000002</v>
+      </c>
       <c r="AH2" s="5"/>
       <c r="AI2" s="5"/>
       <c r="AJ2" s="5"/>
@@ -7507,7 +7509,9 @@
       <c r="AF3" s="5">
         <v>291.5</v>
       </c>
-      <c r="AG3" s="5"/>
+      <c r="AG3" s="5">
+        <v>291.55</v>
+      </c>
       <c r="AH3" s="5"/>
       <c r="AI3" s="5"/>
       <c r="AJ3" s="5"/>
@@ -7625,7 +7629,9 @@
       <c r="AF4" s="5">
         <v>273.8</v>
       </c>
-      <c r="AG4" s="5"/>
+      <c r="AG4" s="5">
+        <v>277.39999999999998</v>
+      </c>
       <c r="AH4" s="5"/>
       <c r="AI4" s="5"/>
       <c r="AJ4" s="5"/>
@@ -7743,7 +7749,9 @@
       <c r="AF5" s="5">
         <v>819.5</v>
       </c>
-      <c r="AG5" s="5"/>
+      <c r="AG5" s="5">
+        <v>824.5</v>
+      </c>
       <c r="AH5" s="5"/>
       <c r="AI5" s="5"/>
       <c r="AJ5" s="5"/>
@@ -7769,7 +7777,7 @@
       </c>
       <c r="B6" s="12">
         <f t="shared" si="1"/>
-        <v>256.75</v>
+        <v>257</v>
       </c>
       <c r="C6" s="45" t="s">
         <v>16</v>
@@ -7861,7 +7869,9 @@
       <c r="AF6" s="5">
         <v>256.75</v>
       </c>
-      <c r="AG6" s="5"/>
+      <c r="AG6" s="5">
+        <v>257</v>
+      </c>
       <c r="AH6" s="5"/>
       <c r="AI6" s="5"/>
       <c r="AJ6" s="5"/>
@@ -7979,7 +7989,9 @@
       <c r="AF7" s="5">
         <v>17.3</v>
       </c>
-      <c r="AG7" s="5"/>
+      <c r="AG7" s="5">
+        <v>17.350000000000001</v>
+      </c>
       <c r="AH7" s="5"/>
       <c r="AI7" s="5"/>
       <c r="AJ7" s="5"/>
@@ -8097,7 +8109,9 @@
       <c r="AF8" s="5">
         <v>63.15</v>
       </c>
-      <c r="AG8" s="5"/>
+      <c r="AG8" s="5">
+        <v>63.25</v>
+      </c>
       <c r="AH8" s="5"/>
       <c r="AI8" s="5"/>
       <c r="AJ8" s="5"/>
@@ -8207,7 +8221,9 @@
       <c r="AF9" s="28">
         <v>56.2</v>
       </c>
-      <c r="AG9" s="28"/>
+      <c r="AG9" s="28">
+        <v>57.3</v>
+      </c>
       <c r="AH9" s="28"/>
       <c r="AI9" s="28"/>
       <c r="AJ9" s="28"/>
@@ -8325,7 +8341,9 @@
       <c r="AF10" s="5">
         <v>39.75</v>
       </c>
-      <c r="AG10" s="5"/>
+      <c r="AG10" s="5">
+        <v>40.4</v>
+      </c>
       <c r="AH10" s="5"/>
       <c r="AI10" s="5"/>
       <c r="AJ10" s="5"/>
@@ -8443,7 +8461,9 @@
       <c r="AF11" s="5">
         <v>83</v>
       </c>
-      <c r="AG11" s="5"/>
+      <c r="AG11" s="5">
+        <v>81.75</v>
+      </c>
       <c r="AH11" s="5"/>
       <c r="AI11" s="5"/>
       <c r="AJ11" s="5"/>
@@ -8465,7 +8485,7 @@
     <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
-        <v>78.599999999999994</v>
+        <v>78.55</v>
       </c>
       <c r="B12" s="12">
         <f t="shared" si="1"/>
@@ -8561,7 +8581,9 @@
       <c r="AF12" s="5">
         <v>78.599999999999994</v>
       </c>
-      <c r="AG12" s="5"/>
+      <c r="AG12" s="5">
+        <v>78.55</v>
+      </c>
       <c r="AH12" s="5"/>
       <c r="AI12" s="5"/>
       <c r="AJ12" s="5"/>
@@ -8679,7 +8701,9 @@
       <c r="AF13" s="5">
         <v>130.5</v>
       </c>
-      <c r="AG13" s="5"/>
+      <c r="AG13" s="5">
+        <v>131.80000000000001</v>
+      </c>
       <c r="AH13" s="5"/>
       <c r="AI13" s="5"/>
       <c r="AJ13" s="5"/>
@@ -8797,7 +8821,9 @@
       <c r="AF14" s="5">
         <v>80.900000000000006</v>
       </c>
-      <c r="AG14" s="5"/>
+      <c r="AG14" s="5">
+        <v>80.8</v>
+      </c>
       <c r="AH14" s="5"/>
       <c r="AI14" s="5"/>
       <c r="AJ14" s="5"/>
@@ -8915,7 +8941,9 @@
       <c r="AF15" s="5">
         <v>49.3</v>
       </c>
-      <c r="AG15" s="5"/>
+      <c r="AG15" s="5">
+        <v>49.35</v>
+      </c>
       <c r="AH15" s="5"/>
       <c r="AI15" s="5"/>
       <c r="AJ15" s="5"/>
@@ -9033,7 +9061,9 @@
       <c r="AF16" s="5">
         <v>32.950000000000003</v>
       </c>
-      <c r="AG16" s="5"/>
+      <c r="AG16" s="5">
+        <v>32.450000000000003</v>
+      </c>
       <c r="AH16" s="5"/>
       <c r="AI16" s="5"/>
       <c r="AJ16" s="5"/>
@@ -9143,7 +9173,9 @@
       <c r="AF17" s="5">
         <v>29.45</v>
       </c>
-      <c r="AG17" s="5"/>
+      <c r="AG17" s="5">
+        <v>29</v>
+      </c>
       <c r="AH17" s="5"/>
       <c r="AI17" s="5"/>
       <c r="AJ17" s="5"/>
@@ -9169,7 +9201,7 @@
       </c>
       <c r="B18" s="12">
         <f t="shared" si="1"/>
-        <v>663</v>
+        <v>680.9</v>
       </c>
       <c r="C18" s="45" t="s">
         <v>25</v>
@@ -9261,7 +9293,9 @@
       <c r="AF18" s="5">
         <v>663</v>
       </c>
-      <c r="AG18" s="5"/>
+      <c r="AG18" s="5">
+        <v>680.9</v>
+      </c>
       <c r="AH18" s="5"/>
       <c r="AI18" s="5"/>
       <c r="AJ18" s="5"/>
@@ -9379,7 +9413,9 @@
       <c r="AF19" s="5">
         <v>477.85</v>
       </c>
-      <c r="AG19" s="5"/>
+      <c r="AG19" s="5">
+        <v>479</v>
+      </c>
       <c r="AH19" s="5"/>
       <c r="AI19" s="5"/>
       <c r="AJ19" s="5"/>
@@ -9497,7 +9533,9 @@
       <c r="AF20" s="5">
         <v>252.7</v>
       </c>
-      <c r="AG20" s="5"/>
+      <c r="AG20" s="5">
+        <v>251.75</v>
+      </c>
       <c r="AH20" s="5"/>
       <c r="AI20" s="5"/>
       <c r="AJ20" s="5"/>
@@ -9615,7 +9653,9 @@
       <c r="AF21" s="5">
         <v>458.05</v>
       </c>
-      <c r="AG21" s="5"/>
+      <c r="AG21" s="5">
+        <v>459.55</v>
+      </c>
       <c r="AH21" s="5"/>
       <c r="AI21" s="5"/>
       <c r="AJ21" s="5"/>
@@ -9733,7 +9773,9 @@
       <c r="AF22" s="5">
         <v>741.05</v>
       </c>
-      <c r="AG22" s="5"/>
+      <c r="AG22" s="5">
+        <v>756.1</v>
+      </c>
       <c r="AH22" s="5"/>
       <c r="AI22" s="5"/>
       <c r="AJ22" s="5"/>
@@ -9851,7 +9893,9 @@
       <c r="AF23" s="5">
         <v>401.95</v>
       </c>
-      <c r="AG23" s="5"/>
+      <c r="AG23" s="5">
+        <v>404.1</v>
+      </c>
       <c r="AH23" s="5"/>
       <c r="AI23" s="5"/>
       <c r="AJ23" s="5"/>
@@ -9915,7 +9959,9 @@
       <c r="AF24" s="5">
         <v>372.55</v>
       </c>
-      <c r="AG24" s="5"/>
+      <c r="AG24" s="5">
+        <v>369.6</v>
+      </c>
       <c r="AH24" s="5"/>
       <c r="AI24" s="5"/>
       <c r="AJ24" s="5"/>
@@ -10025,7 +10071,9 @@
       <c r="AF25" s="5">
         <v>65.3</v>
       </c>
-      <c r="AG25" s="5"/>
+      <c r="AG25" s="5">
+        <v>65.95</v>
+      </c>
       <c r="AH25" s="5"/>
       <c r="AI25" s="5"/>
       <c r="AJ25" s="5"/>
@@ -10131,7 +10179,9 @@
       <c r="AF26" s="5">
         <v>215</v>
       </c>
-      <c r="AG26" s="5"/>
+      <c r="AG26" s="5">
+        <v>221.95</v>
+      </c>
       <c r="AH26" s="5"/>
       <c r="AI26" s="5"/>
       <c r="AJ26" s="5"/>
@@ -10219,7 +10269,9 @@
       <c r="AF27" s="5">
         <v>879.95</v>
       </c>
-      <c r="AG27" s="5"/>
+      <c r="AG27" s="5">
+        <v>883.25</v>
+      </c>
       <c r="AH27" s="5"/>
       <c r="AI27" s="5"/>
       <c r="AJ27" s="5"/>
@@ -10245,7 +10297,7 @@
       </c>
       <c r="B28" s="12">
         <f t="shared" ref="B28:B38" si="3">MAX(D28:ZZ28)</f>
-        <v>87.95</v>
+        <v>88.4</v>
       </c>
       <c r="C28" s="45" t="s">
         <v>271</v>
@@ -10295,7 +10347,9 @@
       <c r="AF28" s="5">
         <v>84.8</v>
       </c>
-      <c r="AG28" s="5"/>
+      <c r="AG28" s="5">
+        <v>88.4</v>
+      </c>
       <c r="AH28" s="5"/>
       <c r="AI28" s="5"/>
       <c r="AJ28" s="5"/>
@@ -10371,7 +10425,9 @@
       <c r="AF29" s="5">
         <v>40.799999999999997</v>
       </c>
-      <c r="AG29" s="5"/>
+      <c r="AG29" s="5">
+        <v>40.299999999999997</v>
+      </c>
       <c r="AH29" s="5"/>
       <c r="AI29" s="5"/>
       <c r="AJ29" s="5"/>
@@ -10397,7 +10453,7 @@
       </c>
       <c r="B30" s="12">
         <f t="shared" si="3"/>
-        <v>56.25</v>
+        <v>56.55</v>
       </c>
       <c r="C30" s="45" t="s">
         <v>273</v>
@@ -10447,7 +10503,9 @@
       <c r="AF30" s="5">
         <v>56.25</v>
       </c>
-      <c r="AG30" s="5"/>
+      <c r="AG30" s="5">
+        <v>56.55</v>
+      </c>
       <c r="AH30" s="5"/>
       <c r="AI30" s="5"/>
       <c r="AJ30" s="5"/>
@@ -10523,7 +10581,9 @@
       <c r="AF31" s="5">
         <v>123.25</v>
       </c>
-      <c r="AG31" s="5"/>
+      <c r="AG31" s="5">
+        <v>124.85</v>
+      </c>
       <c r="AH31" s="5"/>
       <c r="AI31" s="5"/>
       <c r="AJ31" s="5"/>
@@ -10549,7 +10609,7 @@
       </c>
       <c r="B32" s="12">
         <f t="shared" si="3"/>
-        <v>194.3</v>
+        <v>198</v>
       </c>
       <c r="C32" s="45" t="s">
         <v>275</v>
@@ -10599,7 +10659,9 @@
       <c r="AF32" s="5">
         <v>192.05</v>
       </c>
-      <c r="AG32" s="5"/>
+      <c r="AG32" s="5">
+        <v>198</v>
+      </c>
       <c r="AH32" s="5"/>
       <c r="AI32" s="5"/>
       <c r="AJ32" s="5"/>
@@ -10675,7 +10737,9 @@
       <c r="AF33" s="5">
         <v>76.099999999999994</v>
       </c>
-      <c r="AG33" s="5"/>
+      <c r="AG33" s="5">
+        <v>76.5</v>
+      </c>
       <c r="AH33" s="5"/>
       <c r="AI33" s="5"/>
       <c r="AJ33" s="5"/>
@@ -10751,7 +10815,9 @@
       <c r="AF34" s="5">
         <v>39.85</v>
       </c>
-      <c r="AG34" s="5"/>
+      <c r="AG34" s="5">
+        <v>39.75</v>
+      </c>
       <c r="AH34" s="5"/>
       <c r="AI34" s="5"/>
       <c r="AJ34" s="5"/>
@@ -10827,7 +10893,9 @@
       <c r="AF35" s="5">
         <v>63.25</v>
       </c>
-      <c r="AG35" s="5"/>
+      <c r="AG35" s="5">
+        <v>64.8</v>
+      </c>
       <c r="AH35" s="5"/>
       <c r="AI35" s="5"/>
       <c r="AJ35" s="5"/>
@@ -10903,7 +10971,9 @@
       <c r="AF36" s="5">
         <v>31.2</v>
       </c>
-      <c r="AG36" s="5"/>
+      <c r="AG36" s="5">
+        <v>31.15</v>
+      </c>
       <c r="AH36" s="5"/>
       <c r="AI36" s="5"/>
       <c r="AJ36" s="5"/>
@@ -10929,7 +10999,7 @@
       </c>
       <c r="B37" s="12">
         <f t="shared" si="3"/>
-        <v>87.4</v>
+        <v>90.35</v>
       </c>
       <c r="C37" s="45" t="s">
         <v>280</v>
@@ -10979,7 +11049,9 @@
       <c r="AF37" s="5">
         <v>85.4</v>
       </c>
-      <c r="AG37" s="5"/>
+      <c r="AG37" s="5">
+        <v>90.35</v>
+      </c>
       <c r="AH37" s="5"/>
       <c r="AI37" s="5"/>
       <c r="AJ37" s="5"/>
@@ -11005,7 +11077,7 @@
       </c>
       <c r="B38" s="12">
         <f t="shared" si="3"/>
-        <v>127.05</v>
+        <v>127.2</v>
       </c>
       <c r="C38" s="45" t="s">
         <v>281</v>
@@ -11055,7 +11127,9 @@
       <c r="AF38" s="5">
         <v>127.05</v>
       </c>
-      <c r="AG38" s="5"/>
+      <c r="AG38" s="5">
+        <v>127.2</v>
+      </c>
       <c r="AH38" s="5"/>
       <c r="AI38" s="5"/>
       <c r="AJ38" s="5"/>
@@ -11081,7 +11155,7 @@
       </c>
       <c r="B39" s="12">
         <f t="shared" ref="B39:B41" si="5">MAX(D39:ZZ39)</f>
-        <v>140.15</v>
+        <v>142.19999999999999</v>
       </c>
       <c r="C39" s="45" t="s">
         <v>282</v>
@@ -11131,7 +11205,9 @@
       <c r="AF39" s="5">
         <v>137.4</v>
       </c>
-      <c r="AG39" s="5"/>
+      <c r="AG39" s="5">
+        <v>142.19999999999999</v>
+      </c>
       <c r="AH39" s="5"/>
       <c r="AI39" s="5"/>
       <c r="AJ39" s="5"/>
@@ -11207,7 +11283,9 @@
       <c r="AF40" s="5">
         <v>154.44999999999999</v>
       </c>
-      <c r="AG40" s="5"/>
+      <c r="AG40" s="5">
+        <v>153.05000000000001</v>
+      </c>
       <c r="AH40" s="5"/>
       <c r="AI40" s="5"/>
       <c r="AJ40" s="5"/>
@@ -11271,7 +11349,9 @@
       <c r="AF41" s="5">
         <v>113.05</v>
       </c>
-      <c r="AG41" s="5"/>
+      <c r="AG41" s="5">
+        <v>113.2</v>
+      </c>
       <c r="AH41" s="5"/>
       <c r="AI41" s="5"/>
       <c r="AJ41" s="5"/>

</xml_diff>

<commit_message>
Updated the sheet for 13092017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -1454,7 +1454,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7143,7 +7143,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="3" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AG41" sqref="AG41"/>
+      <selection pane="topRight" activeCell="AK26" sqref="AK26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7398,7 +7398,9 @@
       <c r="AG2" s="5">
         <v>273.60000000000002</v>
       </c>
-      <c r="AH2" s="5"/>
+      <c r="AH2" s="5">
+        <v>272.95</v>
+      </c>
       <c r="AI2" s="5"/>
       <c r="AJ2" s="5"/>
       <c r="AK2" s="5"/>
@@ -7512,7 +7514,9 @@
       <c r="AG3" s="5">
         <v>291.55</v>
       </c>
-      <c r="AH3" s="5"/>
+      <c r="AH3" s="5">
+        <v>291.85000000000002</v>
+      </c>
       <c r="AI3" s="5"/>
       <c r="AJ3" s="5"/>
       <c r="AK3" s="5"/>
@@ -7632,7 +7636,9 @@
       <c r="AG4" s="5">
         <v>277.39999999999998</v>
       </c>
-      <c r="AH4" s="5"/>
+      <c r="AH4" s="5">
+        <v>271.60000000000002</v>
+      </c>
       <c r="AI4" s="5"/>
       <c r="AJ4" s="5"/>
       <c r="AK4" s="5"/>
@@ -7752,7 +7758,9 @@
       <c r="AG5" s="5">
         <v>824.5</v>
       </c>
-      <c r="AH5" s="5"/>
+      <c r="AH5" s="5">
+        <v>853.4</v>
+      </c>
       <c r="AI5" s="5"/>
       <c r="AJ5" s="5"/>
       <c r="AK5" s="5"/>
@@ -7872,7 +7880,9 @@
       <c r="AG6" s="5">
         <v>257</v>
       </c>
-      <c r="AH6" s="5"/>
+      <c r="AH6" s="5">
+        <v>256.85000000000002</v>
+      </c>
       <c r="AI6" s="5"/>
       <c r="AJ6" s="5"/>
       <c r="AK6" s="5"/>
@@ -7992,7 +8002,9 @@
       <c r="AG7" s="5">
         <v>17.350000000000001</v>
       </c>
-      <c r="AH7" s="5"/>
+      <c r="AH7" s="5">
+        <v>17.850000000000001</v>
+      </c>
       <c r="AI7" s="5"/>
       <c r="AJ7" s="5"/>
       <c r="AK7" s="5"/>
@@ -8112,7 +8124,9 @@
       <c r="AG8" s="5">
         <v>63.25</v>
       </c>
-      <c r="AH8" s="5"/>
+      <c r="AH8" s="5">
+        <v>61.95</v>
+      </c>
       <c r="AI8" s="5"/>
       <c r="AJ8" s="5"/>
       <c r="AK8" s="5"/>
@@ -8137,7 +8151,7 @@
       </c>
       <c r="B9" s="39">
         <f t="shared" si="1"/>
-        <v>58.2</v>
+        <v>58.9</v>
       </c>
       <c r="C9" s="43" t="s">
         <v>127</v>
@@ -8224,7 +8238,9 @@
       <c r="AG9" s="28">
         <v>57.3</v>
       </c>
-      <c r="AH9" s="28"/>
+      <c r="AH9" s="28">
+        <v>58.9</v>
+      </c>
       <c r="AI9" s="28"/>
       <c r="AJ9" s="28"/>
       <c r="AK9" s="28"/>
@@ -8344,7 +8360,9 @@
       <c r="AG10" s="5">
         <v>40.4</v>
       </c>
-      <c r="AH10" s="5"/>
+      <c r="AH10" s="5">
+        <v>40.35</v>
+      </c>
       <c r="AI10" s="5"/>
       <c r="AJ10" s="5"/>
       <c r="AK10" s="5"/>
@@ -8464,7 +8482,9 @@
       <c r="AG11" s="5">
         <v>81.75</v>
       </c>
-      <c r="AH11" s="5"/>
+      <c r="AH11" s="5">
+        <v>82.4</v>
+      </c>
       <c r="AI11" s="5"/>
       <c r="AJ11" s="5"/>
       <c r="AK11" s="5"/>
@@ -8584,7 +8604,9 @@
       <c r="AG12" s="5">
         <v>78.55</v>
       </c>
-      <c r="AH12" s="5"/>
+      <c r="AH12" s="5">
+        <v>82.55</v>
+      </c>
       <c r="AI12" s="5"/>
       <c r="AJ12" s="5"/>
       <c r="AK12" s="5"/>
@@ -8704,7 +8726,9 @@
       <c r="AG13" s="5">
         <v>131.80000000000001</v>
       </c>
-      <c r="AH13" s="5"/>
+      <c r="AH13" s="5">
+        <v>132.4</v>
+      </c>
       <c r="AI13" s="5"/>
       <c r="AJ13" s="5"/>
       <c r="AK13" s="5"/>
@@ -8729,7 +8753,7 @@
       </c>
       <c r="B14" s="12">
         <f t="shared" si="1"/>
-        <v>83.25</v>
+        <v>85.05</v>
       </c>
       <c r="C14" s="45" t="s">
         <v>21</v>
@@ -8824,7 +8848,9 @@
       <c r="AG14" s="5">
         <v>80.8</v>
       </c>
-      <c r="AH14" s="5"/>
+      <c r="AH14" s="5">
+        <v>85.05</v>
+      </c>
       <c r="AI14" s="5"/>
       <c r="AJ14" s="5"/>
       <c r="AK14" s="5"/>
@@ -8944,7 +8970,9 @@
       <c r="AG15" s="5">
         <v>49.35</v>
       </c>
-      <c r="AH15" s="5"/>
+      <c r="AH15" s="5">
+        <v>49.35</v>
+      </c>
       <c r="AI15" s="5"/>
       <c r="AJ15" s="5"/>
       <c r="AK15" s="5"/>
@@ -9064,7 +9092,9 @@
       <c r="AG16" s="5">
         <v>32.450000000000003</v>
       </c>
-      <c r="AH16" s="5"/>
+      <c r="AH16" s="5">
+        <v>32.450000000000003</v>
+      </c>
       <c r="AI16" s="5"/>
       <c r="AJ16" s="5"/>
       <c r="AK16" s="5"/>
@@ -9176,7 +9206,9 @@
       <c r="AG17" s="5">
         <v>29</v>
       </c>
-      <c r="AH17" s="5"/>
+      <c r="AH17" s="5">
+        <v>29</v>
+      </c>
       <c r="AI17" s="5"/>
       <c r="AJ17" s="5"/>
       <c r="AK17" s="5"/>
@@ -9201,7 +9233,7 @@
       </c>
       <c r="B18" s="12">
         <f t="shared" si="1"/>
-        <v>680.9</v>
+        <v>681.25</v>
       </c>
       <c r="C18" s="45" t="s">
         <v>25</v>
@@ -9296,7 +9328,9 @@
       <c r="AG18" s="5">
         <v>680.9</v>
       </c>
-      <c r="AH18" s="5"/>
+      <c r="AH18" s="5">
+        <v>681.25</v>
+      </c>
       <c r="AI18" s="5"/>
       <c r="AJ18" s="5"/>
       <c r="AK18" s="5"/>
@@ -9416,7 +9450,9 @@
       <c r="AG19" s="5">
         <v>479</v>
       </c>
-      <c r="AH19" s="5"/>
+      <c r="AH19" s="5">
+        <v>471.1</v>
+      </c>
       <c r="AI19" s="5"/>
       <c r="AJ19" s="5"/>
       <c r="AK19" s="5"/>
@@ -9441,7 +9477,7 @@
       </c>
       <c r="B20" s="12">
         <f t="shared" si="1"/>
-        <v>252.7</v>
+        <v>266.64999999999998</v>
       </c>
       <c r="C20" s="44" t="s">
         <v>41</v>
@@ -9536,7 +9572,9 @@
       <c r="AG20" s="5">
         <v>251.75</v>
       </c>
-      <c r="AH20" s="5"/>
+      <c r="AH20" s="5">
+        <v>266.64999999999998</v>
+      </c>
       <c r="AI20" s="5"/>
       <c r="AJ20" s="5"/>
       <c r="AK20" s="5"/>
@@ -9656,7 +9694,9 @@
       <c r="AG21" s="5">
         <v>459.55</v>
       </c>
-      <c r="AH21" s="5"/>
+      <c r="AH21" s="5">
+        <v>479.3</v>
+      </c>
       <c r="AI21" s="5"/>
       <c r="AJ21" s="5"/>
       <c r="AK21" s="5"/>
@@ -9681,7 +9721,7 @@
       </c>
       <c r="B22" s="12">
         <f t="shared" si="1"/>
-        <v>757.3</v>
+        <v>764.95</v>
       </c>
       <c r="C22" s="44" t="s">
         <v>106</v>
@@ -9776,7 +9816,9 @@
       <c r="AG22" s="5">
         <v>756.1</v>
       </c>
-      <c r="AH22" s="5"/>
+      <c r="AH22" s="5">
+        <v>764.95</v>
+      </c>
       <c r="AI22" s="5"/>
       <c r="AJ22" s="5"/>
       <c r="AK22" s="5"/>
@@ -9896,7 +9938,9 @@
       <c r="AG23" s="5">
         <v>404.1</v>
       </c>
-      <c r="AH23" s="5"/>
+      <c r="AH23" s="5">
+        <v>403.5</v>
+      </c>
       <c r="AI23" s="5"/>
       <c r="AJ23" s="5"/>
       <c r="AK23" s="5"/>
@@ -9917,7 +9961,7 @@
     <row r="24" spans="1:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <f t="shared" si="0"/>
-        <v>367.55</v>
+        <v>359.65</v>
       </c>
       <c r="B24" s="12">
         <f t="shared" si="1"/>
@@ -9962,7 +10006,9 @@
       <c r="AG24" s="5">
         <v>369.6</v>
       </c>
-      <c r="AH24" s="5"/>
+      <c r="AH24" s="5">
+        <v>359.65</v>
+      </c>
       <c r="AI24" s="5"/>
       <c r="AJ24" s="5"/>
       <c r="AK24" s="5"/>
@@ -10074,7 +10120,9 @@
       <c r="AG25" s="5">
         <v>65.95</v>
       </c>
-      <c r="AH25" s="5"/>
+      <c r="AH25" s="5">
+        <v>65</v>
+      </c>
       <c r="AI25" s="5"/>
       <c r="AJ25" s="5"/>
       <c r="AK25" s="5"/>
@@ -10182,7 +10230,9 @@
       <c r="AG26" s="5">
         <v>221.95</v>
       </c>
-      <c r="AH26" s="5"/>
+      <c r="AH26" s="5">
+        <v>220.25</v>
+      </c>
       <c r="AI26" s="5"/>
       <c r="AJ26" s="5"/>
       <c r="AK26" s="5"/>
@@ -10272,7 +10322,9 @@
       <c r="AG27" s="5">
         <v>883.25</v>
       </c>
-      <c r="AH27" s="5"/>
+      <c r="AH27" s="5">
+        <v>884.5</v>
+      </c>
       <c r="AI27" s="5"/>
       <c r="AJ27" s="5"/>
       <c r="AK27" s="5"/>
@@ -10297,7 +10349,7 @@
       </c>
       <c r="B28" s="12">
         <f t="shared" ref="B28:B38" si="3">MAX(D28:ZZ28)</f>
-        <v>88.4</v>
+        <v>89.9</v>
       </c>
       <c r="C28" s="45" t="s">
         <v>271</v>
@@ -10350,7 +10402,9 @@
       <c r="AG28" s="5">
         <v>88.4</v>
       </c>
-      <c r="AH28" s="5"/>
+      <c r="AH28" s="5">
+        <v>89.9</v>
+      </c>
       <c r="AI28" s="5"/>
       <c r="AJ28" s="5"/>
       <c r="AK28" s="5"/>
@@ -10428,7 +10482,9 @@
       <c r="AG29" s="5">
         <v>40.299999999999997</v>
       </c>
-      <c r="AH29" s="5"/>
+      <c r="AH29" s="5">
+        <v>40.049999999999997</v>
+      </c>
       <c r="AI29" s="5"/>
       <c r="AJ29" s="5"/>
       <c r="AK29" s="5"/>
@@ -10506,7 +10562,9 @@
       <c r="AG30" s="5">
         <v>56.55</v>
       </c>
-      <c r="AH30" s="5"/>
+      <c r="AH30" s="5">
+        <v>55.8</v>
+      </c>
       <c r="AI30" s="5"/>
       <c r="AJ30" s="5"/>
       <c r="AK30" s="5"/>
@@ -10584,7 +10642,9 @@
       <c r="AG31" s="5">
         <v>124.85</v>
       </c>
-      <c r="AH31" s="5"/>
+      <c r="AH31" s="5">
+        <v>125</v>
+      </c>
       <c r="AI31" s="5"/>
       <c r="AJ31" s="5"/>
       <c r="AK31" s="5"/>
@@ -10662,7 +10722,9 @@
       <c r="AG32" s="5">
         <v>198</v>
       </c>
-      <c r="AH32" s="5"/>
+      <c r="AH32" s="5">
+        <v>194.6</v>
+      </c>
       <c r="AI32" s="5"/>
       <c r="AJ32" s="5"/>
       <c r="AK32" s="5"/>
@@ -10683,7 +10745,7 @@
     <row r="33" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <f t="shared" si="2"/>
-        <v>76.099999999999994</v>
+        <v>75.5</v>
       </c>
       <c r="B33" s="12">
         <f t="shared" si="3"/>
@@ -10740,7 +10802,9 @@
       <c r="AG33" s="5">
         <v>76.5</v>
       </c>
-      <c r="AH33" s="5"/>
+      <c r="AH33" s="5">
+        <v>75.5</v>
+      </c>
       <c r="AI33" s="5"/>
       <c r="AJ33" s="5"/>
       <c r="AK33" s="5"/>
@@ -10765,7 +10829,7 @@
       </c>
       <c r="B34" s="12">
         <f t="shared" si="3"/>
-        <v>40.4</v>
+        <v>42</v>
       </c>
       <c r="C34" s="45" t="s">
         <v>277</v>
@@ -10818,7 +10882,9 @@
       <c r="AG34" s="5">
         <v>39.75</v>
       </c>
-      <c r="AH34" s="5"/>
+      <c r="AH34" s="5">
+        <v>42</v>
+      </c>
       <c r="AI34" s="5"/>
       <c r="AJ34" s="5"/>
       <c r="AK34" s="5"/>
@@ -10843,7 +10909,7 @@
       </c>
       <c r="B35" s="12">
         <f t="shared" si="3"/>
-        <v>65.099999999999994</v>
+        <v>66.5</v>
       </c>
       <c r="C35" s="45" t="s">
         <v>278</v>
@@ -10896,7 +10962,9 @@
       <c r="AG35" s="5">
         <v>64.8</v>
       </c>
-      <c r="AH35" s="5"/>
+      <c r="AH35" s="5">
+        <v>66.5</v>
+      </c>
       <c r="AI35" s="5"/>
       <c r="AJ35" s="5"/>
       <c r="AK35" s="5"/>
@@ -10974,7 +11042,9 @@
       <c r="AG36" s="5">
         <v>31.15</v>
       </c>
-      <c r="AH36" s="5"/>
+      <c r="AH36" s="5">
+        <v>31.3</v>
+      </c>
       <c r="AI36" s="5"/>
       <c r="AJ36" s="5"/>
       <c r="AK36" s="5"/>
@@ -11052,7 +11122,9 @@
       <c r="AG37" s="5">
         <v>90.35</v>
       </c>
-      <c r="AH37" s="5"/>
+      <c r="AH37" s="5">
+        <v>88.9</v>
+      </c>
       <c r="AI37" s="5"/>
       <c r="AJ37" s="5"/>
       <c r="AK37" s="5"/>
@@ -11077,7 +11149,7 @@
       </c>
       <c r="B38" s="12">
         <f t="shared" si="3"/>
-        <v>127.2</v>
+        <v>128.5</v>
       </c>
       <c r="C38" s="45" t="s">
         <v>281</v>
@@ -11130,7 +11202,9 @@
       <c r="AG38" s="5">
         <v>127.2</v>
       </c>
-      <c r="AH38" s="5"/>
+      <c r="AH38" s="5">
+        <v>128.5</v>
+      </c>
       <c r="AI38" s="5"/>
       <c r="AJ38" s="5"/>
       <c r="AK38" s="5"/>
@@ -11155,7 +11229,7 @@
       </c>
       <c r="B39" s="12">
         <f t="shared" ref="B39:B41" si="5">MAX(D39:ZZ39)</f>
-        <v>142.19999999999999</v>
+        <v>143.94999999999999</v>
       </c>
       <c r="C39" s="45" t="s">
         <v>282</v>
@@ -11208,7 +11282,9 @@
       <c r="AG39" s="5">
         <v>142.19999999999999</v>
       </c>
-      <c r="AH39" s="5"/>
+      <c r="AH39" s="5">
+        <v>143.94999999999999</v>
+      </c>
       <c r="AI39" s="5"/>
       <c r="AJ39" s="5"/>
       <c r="AK39" s="5"/>
@@ -11286,7 +11362,9 @@
       <c r="AG40" s="5">
         <v>153.05000000000001</v>
       </c>
-      <c r="AH40" s="5"/>
+      <c r="AH40" s="5">
+        <v>151.85</v>
+      </c>
       <c r="AI40" s="5"/>
       <c r="AJ40" s="5"/>
       <c r="AK40" s="5"/>
@@ -11307,7 +11385,7 @@
     <row r="41" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <f t="shared" si="4"/>
-        <v>113.05</v>
+        <v>111.8</v>
       </c>
       <c r="B41" s="12">
         <f t="shared" si="5"/>
@@ -11352,7 +11430,9 @@
       <c r="AG41" s="5">
         <v>113.2</v>
       </c>
-      <c r="AH41" s="5"/>
+      <c r="AH41" s="5">
+        <v>111.8</v>
+      </c>
       <c r="AI41" s="5"/>
       <c r="AJ41" s="5"/>
       <c r="AK41" s="5"/>

</xml_diff>

<commit_message>
Added stock movement for 18/09/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13965" windowHeight="5625" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13530" windowHeight="8175" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PaidTillDate" sheetId="1" r:id="rId1"/>
@@ -7138,7 +7138,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="3" topLeftCell="AE1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ47" sqref="AJ47"/>
+      <selection pane="topRight" activeCell="AK39" sqref="AK39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7300,7 +7300,7 @@
     <row r="2" spans="1:50">
       <c r="A2" s="12">
         <f t="shared" ref="A2:A26" si="0">MIN(D2:ZZ2)</f>
-        <v>270.60000000000002</v>
+        <v>270</v>
       </c>
       <c r="B2" s="12">
         <f t="shared" ref="B2:B26" si="1">MAX(D2:ZZ2)</f>
@@ -7402,7 +7402,9 @@
       <c r="AJ2" s="5">
         <v>271.5</v>
       </c>
-      <c r="AK2" s="5"/>
+      <c r="AK2" s="5">
+        <v>270</v>
+      </c>
       <c r="AL2" s="5"/>
       <c r="AM2" s="5"/>
       <c r="AN2" s="5"/>
@@ -7522,7 +7524,9 @@
       <c r="AJ3" s="5">
         <v>291.35000000000002</v>
       </c>
-      <c r="AK3" s="5"/>
+      <c r="AK3" s="5">
+        <v>293.14999999999998</v>
+      </c>
       <c r="AL3" s="5"/>
       <c r="AM3" s="5"/>
       <c r="AN3" s="5"/>
@@ -7540,7 +7544,7 @@
     <row r="4" spans="1:50">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
-        <v>269</v>
+        <v>267.39999999999998</v>
       </c>
       <c r="B4" s="12">
         <f t="shared" si="1"/>
@@ -7648,7 +7652,9 @@
       <c r="AJ4" s="5">
         <v>269</v>
       </c>
-      <c r="AK4" s="5"/>
+      <c r="AK4" s="5">
+        <v>267.39999999999998</v>
+      </c>
       <c r="AL4" s="5"/>
       <c r="AM4" s="5"/>
       <c r="AN4" s="5"/>
@@ -7774,7 +7780,9 @@
       <c r="AJ5" s="5">
         <v>842</v>
       </c>
-      <c r="AK5" s="5"/>
+      <c r="AK5" s="5">
+        <v>845.2</v>
+      </c>
       <c r="AL5" s="5"/>
       <c r="AM5" s="5"/>
       <c r="AN5" s="5"/>
@@ -7796,7 +7804,7 @@
       </c>
       <c r="B6" s="12">
         <f t="shared" si="1"/>
-        <v>260.8</v>
+        <v>264.25</v>
       </c>
       <c r="C6" s="45" t="s">
         <v>16</v>
@@ -7900,7 +7908,9 @@
       <c r="AJ6" s="5">
         <v>260.8</v>
       </c>
-      <c r="AK6" s="5"/>
+      <c r="AK6" s="5">
+        <v>264.25</v>
+      </c>
       <c r="AL6" s="5"/>
       <c r="AM6" s="5"/>
       <c r="AN6" s="5"/>
@@ -8026,7 +8036,9 @@
       <c r="AJ7" s="5">
         <v>17.899999999999999</v>
       </c>
-      <c r="AK7" s="5"/>
+      <c r="AK7" s="5">
+        <v>18.149999999999999</v>
+      </c>
       <c r="AL7" s="5"/>
       <c r="AM7" s="5"/>
       <c r="AN7" s="5"/>
@@ -8152,7 +8164,9 @@
       <c r="AJ8" s="5">
         <v>62.25</v>
       </c>
-      <c r="AK8" s="5"/>
+      <c r="AK8" s="5">
+        <v>61.65</v>
+      </c>
       <c r="AL8" s="5"/>
       <c r="AM8" s="5"/>
       <c r="AN8" s="5"/>
@@ -8270,7 +8284,9 @@
       <c r="AJ9" s="28">
         <v>60.35</v>
       </c>
-      <c r="AK9" s="28"/>
+      <c r="AK9" s="28">
+        <v>60.7</v>
+      </c>
       <c r="AL9" s="28"/>
       <c r="AM9" s="28"/>
       <c r="AN9" s="28"/>
@@ -8396,7 +8412,9 @@
       <c r="AJ10" s="5">
         <v>41.75</v>
       </c>
-      <c r="AK10" s="5"/>
+      <c r="AK10" s="5">
+        <v>43.5</v>
+      </c>
       <c r="AL10" s="5"/>
       <c r="AM10" s="5"/>
       <c r="AN10" s="5"/>
@@ -8522,7 +8540,9 @@
       <c r="AJ11" s="5">
         <v>80.3</v>
       </c>
-      <c r="AK11" s="5"/>
+      <c r="AK11" s="5">
+        <v>81.95</v>
+      </c>
       <c r="AL11" s="5"/>
       <c r="AM11" s="5"/>
       <c r="AN11" s="5"/>
@@ -8648,7 +8668,9 @@
       <c r="AJ12" s="5">
         <v>80.349999999999994</v>
       </c>
-      <c r="AK12" s="5"/>
+      <c r="AK12" s="5">
+        <v>82.35</v>
+      </c>
       <c r="AL12" s="5"/>
       <c r="AM12" s="5"/>
       <c r="AN12" s="5"/>
@@ -8774,7 +8796,9 @@
       <c r="AJ13" s="5">
         <v>131.9</v>
       </c>
-      <c r="AK13" s="5"/>
+      <c r="AK13" s="5">
+        <v>133.15</v>
+      </c>
       <c r="AL13" s="5"/>
       <c r="AM13" s="5"/>
       <c r="AN13" s="5"/>
@@ -8900,7 +8924,9 @@
       <c r="AJ14" s="5">
         <v>49.05</v>
       </c>
-      <c r="AK14" s="5"/>
+      <c r="AK14" s="5">
+        <v>49.7</v>
+      </c>
       <c r="AL14" s="5"/>
       <c r="AM14" s="5"/>
       <c r="AN14" s="5"/>
@@ -9026,7 +9052,9 @@
       <c r="AJ15" s="5">
         <v>32</v>
       </c>
-      <c r="AK15" s="5"/>
+      <c r="AK15" s="5">
+        <v>31.95</v>
+      </c>
       <c r="AL15" s="5"/>
       <c r="AM15" s="5"/>
       <c r="AN15" s="5"/>
@@ -9144,7 +9172,9 @@
       <c r="AJ16" s="5">
         <v>28.75</v>
       </c>
-      <c r="AK16" s="5"/>
+      <c r="AK16" s="5">
+        <v>28.65</v>
+      </c>
       <c r="AL16" s="5"/>
       <c r="AM16" s="5"/>
       <c r="AN16" s="5"/>
@@ -9270,7 +9300,9 @@
       <c r="AJ17" s="5">
         <v>677</v>
       </c>
-      <c r="AK17" s="5"/>
+      <c r="AK17" s="5">
+        <v>671.55</v>
+      </c>
       <c r="AL17" s="5"/>
       <c r="AM17" s="5"/>
       <c r="AN17" s="5"/>
@@ -9396,7 +9428,9 @@
       <c r="AJ18" s="5">
         <v>468.55</v>
       </c>
-      <c r="AK18" s="5"/>
+      <c r="AK18" s="5">
+        <v>474.55</v>
+      </c>
       <c r="AL18" s="5"/>
       <c r="AM18" s="5"/>
       <c r="AN18" s="5"/>
@@ -9522,7 +9556,9 @@
       <c r="AJ19" s="5">
         <v>277.8</v>
       </c>
-      <c r="AK19" s="5"/>
+      <c r="AK19" s="5">
+        <v>275.95</v>
+      </c>
       <c r="AL19" s="5"/>
       <c r="AM19" s="5"/>
       <c r="AN19" s="5"/>
@@ -9648,7 +9684,9 @@
       <c r="AJ20" s="5">
         <v>500.7</v>
       </c>
-      <c r="AK20" s="5"/>
+      <c r="AK20" s="5">
+        <v>510</v>
+      </c>
       <c r="AL20" s="5"/>
       <c r="AM20" s="5"/>
       <c r="AN20" s="5"/>
@@ -9774,7 +9812,9 @@
       <c r="AJ21" s="5">
         <v>756</v>
       </c>
-      <c r="AK21" s="5"/>
+      <c r="AK21" s="5">
+        <v>758.4</v>
+      </c>
       <c r="AL21" s="5"/>
       <c r="AM21" s="5"/>
       <c r="AN21" s="5"/>
@@ -9792,7 +9832,7 @@
     <row r="22" spans="1:50" ht="15.75" customHeight="1">
       <c r="A22" s="12">
         <f t="shared" si="0"/>
-        <v>398.75</v>
+        <v>397.3</v>
       </c>
       <c r="B22" s="12">
         <f t="shared" si="1"/>
@@ -9900,7 +9940,9 @@
       <c r="AJ22" s="5">
         <v>398.75</v>
       </c>
-      <c r="AK22" s="5"/>
+      <c r="AK22" s="5">
+        <v>397.3</v>
+      </c>
       <c r="AL22" s="5"/>
       <c r="AM22" s="5"/>
       <c r="AN22" s="5"/>
@@ -9918,7 +9960,7 @@
     <row r="23" spans="1:50" ht="15.75" customHeight="1">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
-        <v>351.2</v>
+        <v>351.1</v>
       </c>
       <c r="B23" s="12">
         <f t="shared" si="1"/>
@@ -9972,7 +10014,9 @@
       <c r="AJ23" s="5">
         <v>351.2</v>
       </c>
-      <c r="AK23" s="5"/>
+      <c r="AK23" s="5">
+        <v>351.1</v>
+      </c>
       <c r="AL23" s="5"/>
       <c r="AM23" s="5"/>
       <c r="AN23" s="5"/>
@@ -10090,7 +10134,9 @@
       <c r="AJ24" s="5">
         <v>62</v>
       </c>
-      <c r="AK24" s="5"/>
+      <c r="AK24" s="5">
+        <v>62.6</v>
+      </c>
       <c r="AL24" s="5"/>
       <c r="AM24" s="5"/>
       <c r="AN24" s="5"/>
@@ -10204,7 +10250,9 @@
       <c r="AJ25" s="5">
         <v>228.85</v>
       </c>
-      <c r="AK25" s="5"/>
+      <c r="AK25" s="5">
+        <v>233.4</v>
+      </c>
       <c r="AL25" s="5"/>
       <c r="AM25" s="5"/>
       <c r="AN25" s="5"/>
@@ -10300,7 +10348,9 @@
       <c r="AJ26" s="5">
         <v>908.6</v>
       </c>
-      <c r="AK26" s="5"/>
+      <c r="AK26" s="5">
+        <v>908.8</v>
+      </c>
       <c r="AL26" s="5"/>
       <c r="AM26" s="5"/>
       <c r="AN26" s="5"/>
@@ -10322,7 +10372,7 @@
       </c>
       <c r="B27" s="12">
         <f t="shared" ref="B27:B37" si="3">MAX(D27:ZZ27)</f>
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C27" s="45" t="s">
         <v>270</v>
@@ -10384,7 +10434,9 @@
       <c r="AJ27" s="5">
         <v>94</v>
       </c>
-      <c r="AK27" s="5"/>
+      <c r="AK27" s="5">
+        <v>96</v>
+      </c>
       <c r="AL27" s="5"/>
       <c r="AM27" s="5"/>
       <c r="AN27" s="5"/>
@@ -10406,7 +10458,7 @@
       </c>
       <c r="B28" s="12">
         <f t="shared" si="3"/>
-        <v>41.1</v>
+        <v>41.4</v>
       </c>
       <c r="C28" s="45" t="s">
         <v>271</v>
@@ -10468,7 +10520,9 @@
       <c r="AJ28" s="5">
         <v>40.200000000000003</v>
       </c>
-      <c r="AK28" s="5"/>
+      <c r="AK28" s="5">
+        <v>41.4</v>
+      </c>
       <c r="AL28" s="5"/>
       <c r="AM28" s="5"/>
       <c r="AN28" s="5"/>
@@ -10490,7 +10544,7 @@
       </c>
       <c r="B29" s="12">
         <f t="shared" si="3"/>
-        <v>56.75</v>
+        <v>57.05</v>
       </c>
       <c r="C29" s="45" t="s">
         <v>272</v>
@@ -10552,7 +10606,9 @@
       <c r="AJ29" s="5">
         <v>56.4</v>
       </c>
-      <c r="AK29" s="5"/>
+      <c r="AK29" s="5">
+        <v>57.05</v>
+      </c>
       <c r="AL29" s="5"/>
       <c r="AM29" s="5"/>
       <c r="AN29" s="5"/>
@@ -10574,7 +10630,7 @@
       </c>
       <c r="B30" s="12">
         <f t="shared" si="3"/>
-        <v>129.6</v>
+        <v>134.5</v>
       </c>
       <c r="C30" s="45" t="s">
         <v>273</v>
@@ -10636,7 +10692,9 @@
       <c r="AJ30" s="5">
         <v>127.1</v>
       </c>
-      <c r="AK30" s="5"/>
+      <c r="AK30" s="5">
+        <v>134.5</v>
+      </c>
       <c r="AL30" s="5"/>
       <c r="AM30" s="5"/>
       <c r="AN30" s="5"/>
@@ -10720,7 +10778,9 @@
       <c r="AJ31" s="5">
         <v>12.7</v>
       </c>
-      <c r="AK31" s="5"/>
+      <c r="AK31" s="5">
+        <v>192.9</v>
+      </c>
       <c r="AL31" s="5"/>
       <c r="AM31" s="5"/>
       <c r="AN31" s="5"/>
@@ -10804,7 +10864,9 @@
       <c r="AJ32" s="5">
         <v>77.5</v>
       </c>
-      <c r="AK32" s="5"/>
+      <c r="AK32" s="5">
+        <v>76.25</v>
+      </c>
       <c r="AL32" s="5"/>
       <c r="AM32" s="5"/>
       <c r="AN32" s="5"/>
@@ -10826,7 +10888,7 @@
       </c>
       <c r="B33" s="12">
         <f t="shared" si="3"/>
-        <v>44.4</v>
+        <v>44.9</v>
       </c>
       <c r="C33" s="45" t="s">
         <v>276</v>
@@ -10888,7 +10950,9 @@
       <c r="AJ33" s="5">
         <v>44.4</v>
       </c>
-      <c r="AK33" s="5"/>
+      <c r="AK33" s="5">
+        <v>44.9</v>
+      </c>
       <c r="AL33" s="5"/>
       <c r="AM33" s="5"/>
       <c r="AN33" s="5"/>
@@ -10972,7 +11036,9 @@
       <c r="AJ34" s="5">
         <v>69.650000000000006</v>
       </c>
-      <c r="AK34" s="5"/>
+      <c r="AK34" s="5">
+        <v>69.599999999999994</v>
+      </c>
       <c r="AL34" s="5"/>
       <c r="AM34" s="5"/>
       <c r="AN34" s="5"/>
@@ -11056,7 +11122,9 @@
       <c r="AJ35" s="5">
         <v>31</v>
       </c>
-      <c r="AK35" s="5"/>
+      <c r="AK35" s="5">
+        <v>31.1</v>
+      </c>
       <c r="AL35" s="5"/>
       <c r="AM35" s="5"/>
       <c r="AN35" s="5"/>
@@ -11140,7 +11208,9 @@
       <c r="AJ36" s="5">
         <v>215</v>
       </c>
-      <c r="AK36" s="5"/>
+      <c r="AK36" s="5">
+        <v>90.8</v>
+      </c>
       <c r="AL36" s="5"/>
       <c r="AM36" s="5"/>
       <c r="AN36" s="5"/>
@@ -11162,7 +11232,7 @@
       </c>
       <c r="B37" s="12">
         <f t="shared" si="3"/>
-        <v>131.30000000000001</v>
+        <v>131.4</v>
       </c>
       <c r="C37" s="45" t="s">
         <v>280</v>
@@ -11224,7 +11294,9 @@
       <c r="AJ37" s="5">
         <v>0.1</v>
       </c>
-      <c r="AK37" s="5"/>
+      <c r="AK37" s="5">
+        <v>131.4</v>
+      </c>
       <c r="AL37" s="5"/>
       <c r="AM37" s="5"/>
       <c r="AN37" s="5"/>
@@ -11308,7 +11380,9 @@
       <c r="AJ38" s="5">
         <v>145.30000000000001</v>
       </c>
-      <c r="AK38" s="5"/>
+      <c r="AK38" s="5">
+        <v>145.19999999999999</v>
+      </c>
       <c r="AL38" s="5"/>
       <c r="AM38" s="5"/>
       <c r="AN38" s="5"/>
@@ -11392,7 +11466,9 @@
       <c r="AJ39" s="5">
         <v>149.44999999999999</v>
       </c>
-      <c r="AK39" s="5"/>
+      <c r="AK39" s="5">
+        <v>150.9</v>
+      </c>
       <c r="AL39" s="5"/>
       <c r="AM39" s="5"/>
       <c r="AN39" s="5"/>
@@ -11464,7 +11540,9 @@
       <c r="AJ40" s="5">
         <v>109.6</v>
       </c>
-      <c r="AK40" s="5"/>
+      <c r="AK40" s="5">
+        <v>112</v>
+      </c>
       <c r="AL40" s="5"/>
       <c r="AM40" s="5"/>
       <c r="AN40" s="5"/>

</xml_diff>

<commit_message>
Added details for 22/09/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="309">
   <si>
     <t>Date</t>
   </si>
@@ -949,6 +949,9 @@
   </si>
   <si>
     <t>20/10/2017</t>
+  </si>
+  <si>
+    <t>BOMDYEING</t>
   </si>
 </sst>
 </file>
@@ -7168,11 +7171,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BH41"/>
+  <dimension ref="A1:BH42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="AM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AN36" sqref="AN36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="AL1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AO42" sqref="AO42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7393,7 +7396,7 @@
     <row r="2" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <f t="shared" ref="A2:A41" si="0">MIN(E2:ZZ2)</f>
-        <v>267.64999999999998</v>
+        <v>262.10000000000002</v>
       </c>
       <c r="B2" s="12">
         <f t="shared" ref="B2:B37" si="1">MAX(E2:ZZ2)</f>
@@ -7401,7 +7404,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2-A2</f>
-        <v>42.950000000000045</v>
+        <v>48.5</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>116</v>
@@ -7508,7 +7511,9 @@
       <c r="AN2" s="5">
         <v>268.64999999999998</v>
       </c>
-      <c r="AO2" s="5"/>
+      <c r="AO2" s="5">
+        <v>262.10000000000002</v>
+      </c>
       <c r="AP2" s="5"/>
       <c r="AQ2" s="5"/>
       <c r="AR2" s="5"/>
@@ -7532,7 +7537,7 @@
     <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <f t="shared" si="0"/>
-        <v>285.10000000000002</v>
+        <v>277.7</v>
       </c>
       <c r="B3" s="12">
         <f t="shared" si="1"/>
@@ -7540,7 +7545,7 @@
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C41" si="2">B3-A3</f>
-        <v>17.599999999999966</v>
+        <v>25</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>115</v>
@@ -7647,7 +7652,9 @@
       <c r="AN3" s="5">
         <v>285.10000000000002</v>
       </c>
-      <c r="AO3" s="5"/>
+      <c r="AO3" s="5">
+        <v>277.7</v>
+      </c>
       <c r="AP3" s="5"/>
       <c r="AQ3" s="5"/>
       <c r="AR3" s="5"/>
@@ -7792,7 +7799,9 @@
       <c r="AN4" s="5">
         <v>269</v>
       </c>
-      <c r="AO4" s="5"/>
+      <c r="AO4" s="5">
+        <v>267.85000000000002</v>
+      </c>
       <c r="AP4" s="5"/>
       <c r="AQ4" s="5"/>
       <c r="AR4" s="5"/>
@@ -7937,7 +7946,9 @@
       <c r="AN5" s="5">
         <v>842.95</v>
       </c>
-      <c r="AO5" s="5"/>
+      <c r="AO5" s="5">
+        <v>816.95</v>
+      </c>
       <c r="AP5" s="5"/>
       <c r="AQ5" s="5"/>
       <c r="AR5" s="5"/>
@@ -8082,7 +8093,9 @@
       <c r="AN6" s="5">
         <v>254.4</v>
       </c>
-      <c r="AO6" s="5"/>
+      <c r="AO6" s="5">
+        <v>253.8</v>
+      </c>
       <c r="AP6" s="5"/>
       <c r="AQ6" s="5"/>
       <c r="AR6" s="5"/>
@@ -8227,7 +8240,9 @@
       <c r="AN7" s="5">
         <v>17.600000000000001</v>
       </c>
-      <c r="AO7" s="5"/>
+      <c r="AO7" s="5">
+        <v>16.75</v>
+      </c>
       <c r="AP7" s="5"/>
       <c r="AQ7" s="5"/>
       <c r="AR7" s="5"/>
@@ -8372,7 +8387,9 @@
       <c r="AN8" s="5">
         <v>61</v>
       </c>
-      <c r="AO8" s="5"/>
+      <c r="AO8" s="5">
+        <v>57.8</v>
+      </c>
       <c r="AP8" s="5"/>
       <c r="AQ8" s="5"/>
       <c r="AR8" s="5"/>
@@ -8509,7 +8526,9 @@
       <c r="AN9" s="28">
         <v>59.3</v>
       </c>
-      <c r="AO9" s="28"/>
+      <c r="AO9" s="28">
+        <v>57.5</v>
+      </c>
       <c r="AP9" s="28"/>
       <c r="AQ9" s="28"/>
       <c r="AR9" s="28"/>
@@ -8654,7 +8673,9 @@
       <c r="AN10" s="5">
         <v>44.75</v>
       </c>
-      <c r="AO10" s="5"/>
+      <c r="AO10" s="5">
+        <v>42.2</v>
+      </c>
       <c r="AP10" s="5"/>
       <c r="AQ10" s="5"/>
       <c r="AR10" s="5"/>
@@ -8799,7 +8820,9 @@
       <c r="AN11" s="5">
         <v>82</v>
       </c>
-      <c r="AO11" s="5"/>
+      <c r="AO11" s="5">
+        <v>75.8</v>
+      </c>
       <c r="AP11" s="5"/>
       <c r="AQ11" s="5"/>
       <c r="AR11" s="5"/>
@@ -8823,7 +8846,7 @@
     <row r="12" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
-        <v>78.55</v>
+        <v>78.05</v>
       </c>
       <c r="B12" s="12">
         <f t="shared" si="1"/>
@@ -8831,7 +8854,7 @@
       </c>
       <c r="C12" s="12">
         <f t="shared" si="2"/>
-        <v>16.850000000000009</v>
+        <v>17.350000000000009</v>
       </c>
       <c r="D12" s="45" t="s">
         <v>18</v>
@@ -8944,7 +8967,9 @@
       <c r="AN12" s="5">
         <v>80.05</v>
       </c>
-      <c r="AO12" s="5"/>
+      <c r="AO12" s="5">
+        <v>78.05</v>
+      </c>
       <c r="AP12" s="5"/>
       <c r="AQ12" s="5"/>
       <c r="AR12" s="5"/>
@@ -9089,7 +9114,9 @@
       <c r="AN13" s="5">
         <v>132.65</v>
       </c>
-      <c r="AO13" s="5"/>
+      <c r="AO13" s="5">
+        <v>129.4</v>
+      </c>
       <c r="AP13" s="5"/>
       <c r="AQ13" s="5"/>
       <c r="AR13" s="5"/>
@@ -9113,7 +9140,7 @@
     <row r="14" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <f t="shared" si="0"/>
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="B14" s="12">
         <f t="shared" si="1"/>
@@ -9121,7 +9148,7 @@
       </c>
       <c r="C14" s="12">
         <f t="shared" si="2"/>
-        <v>8.3500000000000014</v>
+        <v>9.4499999999999957</v>
       </c>
       <c r="D14" s="45" t="s">
         <v>21</v>
@@ -9234,7 +9261,9 @@
       <c r="AN14" s="5">
         <v>49.05</v>
       </c>
-      <c r="AO14" s="5"/>
+      <c r="AO14" s="5">
+        <v>47.7</v>
+      </c>
       <c r="AP14" s="5"/>
       <c r="AQ14" s="5"/>
       <c r="AR14" s="5"/>
@@ -9258,7 +9287,7 @@
     <row r="15" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
-        <v>30.55</v>
+        <v>30.5</v>
       </c>
       <c r="B15" s="12">
         <f t="shared" si="1"/>
@@ -9266,7 +9295,7 @@
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
-        <v>2.6500000000000021</v>
+        <v>2.7000000000000028</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>22</v>
@@ -9379,7 +9408,9 @@
       <c r="AN15" s="5">
         <v>31</v>
       </c>
-      <c r="AO15" s="5"/>
+      <c r="AO15" s="5">
+        <v>30.5</v>
+      </c>
       <c r="AP15" s="5"/>
       <c r="AQ15" s="5"/>
       <c r="AR15" s="5"/>
@@ -9516,7 +9547,9 @@
       <c r="AN16" s="5">
         <v>28.75</v>
       </c>
-      <c r="AO16" s="5"/>
+      <c r="AO16" s="5">
+        <v>28.05</v>
+      </c>
       <c r="AP16" s="5"/>
       <c r="AQ16" s="5"/>
       <c r="AR16" s="5"/>
@@ -9661,7 +9694,9 @@
       <c r="AN17" s="5">
         <v>686.35</v>
       </c>
-      <c r="AO17" s="5"/>
+      <c r="AO17" s="5">
+        <v>654.4</v>
+      </c>
       <c r="AP17" s="5"/>
       <c r="AQ17" s="5"/>
       <c r="AR17" s="5"/>
@@ -9685,7 +9720,7 @@
     <row r="18" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <f t="shared" si="0"/>
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B18" s="12">
         <f t="shared" si="1"/>
@@ -9693,7 +9728,7 @@
       </c>
       <c r="C18" s="12">
         <f t="shared" si="2"/>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D18" s="44" t="s">
         <v>27</v>
@@ -9806,7 +9841,9 @@
       <c r="AN18" s="5">
         <v>466</v>
       </c>
-      <c r="AO18" s="5"/>
+      <c r="AO18" s="5">
+        <v>452</v>
+      </c>
       <c r="AP18" s="5"/>
       <c r="AQ18" s="5"/>
       <c r="AR18" s="5"/>
@@ -9951,7 +9988,9 @@
       <c r="AN19" s="5">
         <v>252.2</v>
       </c>
-      <c r="AO19" s="5"/>
+      <c r="AO19" s="5">
+        <v>240.7</v>
+      </c>
       <c r="AP19" s="5"/>
       <c r="AQ19" s="5"/>
       <c r="AR19" s="5"/>
@@ -9979,11 +10018,11 @@
       </c>
       <c r="B20" s="12">
         <f t="shared" si="1"/>
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C20" s="12">
         <f t="shared" si="2"/>
-        <v>73.300000000000011</v>
+        <v>75.300000000000011</v>
       </c>
       <c r="D20" s="44" t="s">
         <v>49</v>
@@ -10096,7 +10135,9 @@
       <c r="AN20" s="5">
         <v>511.05</v>
       </c>
-      <c r="AO20" s="5"/>
+      <c r="AO20" s="5">
+        <v>516</v>
+      </c>
       <c r="AP20" s="5"/>
       <c r="AQ20" s="5"/>
       <c r="AR20" s="5"/>
@@ -10241,7 +10282,9 @@
       <c r="AN21" s="5">
         <v>751.5</v>
       </c>
-      <c r="AO21" s="5"/>
+      <c r="AO21" s="5">
+        <v>724</v>
+      </c>
       <c r="AP21" s="5"/>
       <c r="AQ21" s="5"/>
       <c r="AR21" s="5"/>
@@ -10386,7 +10429,9 @@
       <c r="AN22" s="5">
         <v>401.8</v>
       </c>
-      <c r="AO22" s="5"/>
+      <c r="AO22" s="5">
+        <v>395.8</v>
+      </c>
       <c r="AP22" s="5"/>
       <c r="AQ22" s="5"/>
       <c r="AR22" s="5"/>
@@ -10410,7 +10455,7 @@
     <row r="23" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
-        <v>351.1</v>
+        <v>338.95</v>
       </c>
       <c r="B23" s="12">
         <f t="shared" si="1"/>
@@ -10418,7 +10463,7 @@
       </c>
       <c r="C23" s="12">
         <f t="shared" si="2"/>
-        <v>21.449999999999989</v>
+        <v>33.600000000000023</v>
       </c>
       <c r="D23" s="44" t="s">
         <v>294</v>
@@ -10477,7 +10522,9 @@
       <c r="AN23" s="5">
         <v>352</v>
       </c>
-      <c r="AO23" s="5"/>
+      <c r="AO23" s="5">
+        <v>338.95</v>
+      </c>
       <c r="AP23" s="5"/>
       <c r="AQ23" s="5"/>
       <c r="AR23" s="5"/>
@@ -10614,7 +10661,9 @@
       <c r="AN24" s="5">
         <v>60.95</v>
       </c>
-      <c r="AO24" s="5"/>
+      <c r="AO24" s="5">
+        <v>58.5</v>
+      </c>
       <c r="AP24" s="5"/>
       <c r="AQ24" s="5"/>
       <c r="AR24" s="5"/>
@@ -10747,7 +10796,9 @@
       <c r="AN25" s="5">
         <v>234</v>
       </c>
-      <c r="AO25" s="5"/>
+      <c r="AO25" s="5">
+        <v>231.85</v>
+      </c>
       <c r="AP25" s="5"/>
       <c r="AQ25" s="5"/>
       <c r="AR25" s="5"/>
@@ -10862,7 +10913,9 @@
       <c r="AN26" s="5">
         <v>911</v>
       </c>
-      <c r="AO26" s="5"/>
+      <c r="AO26" s="5">
+        <v>899</v>
+      </c>
       <c r="AP26" s="5"/>
       <c r="AQ26" s="5"/>
       <c r="AR26" s="5"/>
@@ -10965,7 +11018,9 @@
       <c r="AN27" s="5">
         <v>94.15</v>
       </c>
-      <c r="AO27" s="5"/>
+      <c r="AO27" s="5">
+        <v>88.3</v>
+      </c>
       <c r="AP27" s="5"/>
       <c r="AQ27" s="5"/>
       <c r="AR27" s="5"/>
@@ -11068,7 +11123,9 @@
       <c r="AN28" s="5">
         <v>44.75</v>
       </c>
-      <c r="AO28" s="5"/>
+      <c r="AO28" s="5">
+        <v>42.85</v>
+      </c>
       <c r="AP28" s="5"/>
       <c r="AQ28" s="5"/>
       <c r="AR28" s="5"/>
@@ -11092,7 +11149,7 @@
     <row r="29" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <f t="shared" si="0"/>
-        <v>55.1</v>
+        <v>54.2</v>
       </c>
       <c r="B29" s="12">
         <f t="shared" si="1"/>
@@ -11100,7 +11157,7 @@
       </c>
       <c r="C29" s="12">
         <f t="shared" si="2"/>
-        <v>1.9499999999999957</v>
+        <v>2.8499999999999943</v>
       </c>
       <c r="D29" s="45" t="s">
         <v>272</v>
@@ -11171,7 +11228,9 @@
       <c r="AN29" s="5">
         <v>55.95</v>
       </c>
-      <c r="AO29" s="5"/>
+      <c r="AO29" s="5">
+        <v>54.2</v>
+      </c>
       <c r="AP29" s="5"/>
       <c r="AQ29" s="5"/>
       <c r="AR29" s="5"/>
@@ -11195,7 +11254,7 @@
     <row r="30" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <f t="shared" si="0"/>
-        <v>123.05</v>
+        <v>122.3</v>
       </c>
       <c r="B30" s="12">
         <f t="shared" si="1"/>
@@ -11203,7 +11262,7 @@
       </c>
       <c r="C30" s="12">
         <f t="shared" si="2"/>
-        <v>11.450000000000003</v>
+        <v>12.200000000000003</v>
       </c>
       <c r="D30" s="45" t="s">
         <v>273</v>
@@ -11274,7 +11333,9 @@
       <c r="AN30" s="5">
         <v>128.94999999999999</v>
       </c>
-      <c r="AO30" s="5"/>
+      <c r="AO30" s="5">
+        <v>122.3</v>
+      </c>
       <c r="AP30" s="5"/>
       <c r="AQ30" s="5"/>
       <c r="AR30" s="5"/>
@@ -11298,7 +11359,7 @@
     <row r="31" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B31" s="12">
         <f t="shared" si="1"/>
@@ -11306,7 +11367,7 @@
       </c>
       <c r="C31" s="12">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D31" s="45" t="s">
         <v>274</v>
@@ -11377,7 +11438,9 @@
       <c r="AN31" s="5">
         <v>188</v>
       </c>
-      <c r="AO31" s="5"/>
+      <c r="AO31" s="5">
+        <v>182</v>
+      </c>
       <c r="AP31" s="5"/>
       <c r="AQ31" s="5"/>
       <c r="AR31" s="5"/>
@@ -11401,7 +11464,7 @@
     <row r="32" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <f t="shared" si="0"/>
-        <v>73.400000000000006</v>
+        <v>70.7</v>
       </c>
       <c r="B32" s="12">
         <f t="shared" si="1"/>
@@ -11409,7 +11472,7 @@
       </c>
       <c r="C32" s="12">
         <f t="shared" si="2"/>
-        <v>5.4499999999999886</v>
+        <v>8.1499999999999915</v>
       </c>
       <c r="D32" s="45" t="s">
         <v>275</v>
@@ -11480,7 +11543,9 @@
       <c r="AN32" s="5">
         <v>73.400000000000006</v>
       </c>
-      <c r="AO32" s="5"/>
+      <c r="AO32" s="5">
+        <v>70.7</v>
+      </c>
       <c r="AP32" s="5"/>
       <c r="AQ32" s="5"/>
       <c r="AR32" s="5"/>
@@ -11583,7 +11648,9 @@
       <c r="AN33" s="5">
         <v>47.5</v>
       </c>
-      <c r="AO33" s="5"/>
+      <c r="AO33" s="5">
+        <v>44.95</v>
+      </c>
       <c r="AP33" s="5"/>
       <c r="AQ33" s="5"/>
       <c r="AR33" s="5"/>
@@ -11686,7 +11753,9 @@
       <c r="AN34" s="5">
         <v>68.45</v>
       </c>
-      <c r="AO34" s="5"/>
+      <c r="AO34" s="5">
+        <v>66.3</v>
+      </c>
       <c r="AP34" s="5"/>
       <c r="AQ34" s="5"/>
       <c r="AR34" s="5"/>
@@ -11789,7 +11858,9 @@
       <c r="AN35" s="5">
         <v>30.7</v>
       </c>
-      <c r="AO35" s="5"/>
+      <c r="AO35" s="5">
+        <v>31.05</v>
+      </c>
       <c r="AP35" s="5"/>
       <c r="AQ35" s="5"/>
       <c r="AR35" s="5"/>
@@ -11892,7 +11963,9 @@
       <c r="AN36" s="5">
         <v>88.55</v>
       </c>
-      <c r="AO36" s="5"/>
+      <c r="AO36" s="5">
+        <v>84.85</v>
+      </c>
       <c r="AP36" s="5"/>
       <c r="AQ36" s="5"/>
       <c r="AR36" s="5"/>
@@ -11995,7 +12068,9 @@
       <c r="AN37" s="5">
         <v>132</v>
       </c>
-      <c r="AO37" s="5"/>
+      <c r="AO37" s="5">
+        <v>126.05</v>
+      </c>
       <c r="AP37" s="5"/>
       <c r="AQ37" s="5"/>
       <c r="AR37" s="5"/>
@@ -12098,7 +12173,9 @@
       <c r="AN38" s="5">
         <v>145.4</v>
       </c>
-      <c r="AO38" s="5"/>
+      <c r="AO38" s="5">
+        <v>142.30000000000001</v>
+      </c>
       <c r="AP38" s="5"/>
       <c r="AQ38" s="5"/>
       <c r="AR38" s="5"/>
@@ -12201,7 +12278,9 @@
       <c r="AN39" s="5">
         <v>152</v>
       </c>
-      <c r="AO39" s="5"/>
+      <c r="AO39" s="5">
+        <v>150.75</v>
+      </c>
       <c r="AP39" s="5"/>
       <c r="AQ39" s="5"/>
       <c r="AR39" s="5"/>
@@ -12225,7 +12304,7 @@
     <row r="40" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>101.7</v>
       </c>
       <c r="B40" s="12">
         <f t="shared" si="3"/>
@@ -12233,7 +12312,7 @@
       </c>
       <c r="C40" s="12">
         <f t="shared" si="2"/>
-        <v>12.150000000000006</v>
+        <v>15.450000000000003</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>293</v>
@@ -12292,7 +12371,9 @@
       <c r="AN40" s="5">
         <v>105</v>
       </c>
-      <c r="AO40" s="5"/>
+      <c r="AO40" s="5">
+        <v>101.7</v>
+      </c>
       <c r="AP40" s="5"/>
       <c r="AQ40" s="5"/>
       <c r="AR40" s="5"/>
@@ -12371,7 +12452,9 @@
       <c r="AN41" s="5">
         <v>63.5</v>
       </c>
-      <c r="AO41" s="5"/>
+      <c r="AO41" s="5">
+        <v>60.5</v>
+      </c>
       <c r="AP41" s="5"/>
       <c r="AQ41" s="5"/>
       <c r="AR41" s="5"/>
@@ -12391,6 +12474,81 @@
       <c r="BF41" s="5"/>
       <c r="BG41" s="5"/>
       <c r="BH41" s="5"/>
+    </row>
+    <row r="42" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A42" s="12">
+        <f t="shared" ref="A42" si="5">MIN(E42:ZZ42)</f>
+        <v>202.3</v>
+      </c>
+      <c r="B42" s="12">
+        <f t="shared" ref="B42" si="6">MAX(E42:ZZ42)</f>
+        <v>202.3</v>
+      </c>
+      <c r="C42" s="12">
+        <f t="shared" ref="C42" si="7">B42-A42</f>
+        <v>0</v>
+      </c>
+      <c r="D42" s="45" t="s">
+        <v>308</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="5"/>
+      <c r="U42" s="5"/>
+      <c r="V42" s="5"/>
+      <c r="W42" s="5"/>
+      <c r="X42" s="5"/>
+      <c r="Y42" s="5"/>
+      <c r="Z42" s="5"/>
+      <c r="AA42" s="5"/>
+      <c r="AB42" s="5"/>
+      <c r="AC42" s="5"/>
+      <c r="AD42" s="5"/>
+      <c r="AE42" s="5"/>
+      <c r="AF42" s="5"/>
+      <c r="AG42" s="5"/>
+      <c r="AH42" s="5"/>
+      <c r="AI42" s="5"/>
+      <c r="AJ42" s="5"/>
+      <c r="AK42" s="5"/>
+      <c r="AL42" s="5"/>
+      <c r="AM42" s="5"/>
+      <c r="AN42" s="5"/>
+      <c r="AO42" s="5">
+        <v>202.3</v>
+      </c>
+      <c r="AP42" s="5"/>
+      <c r="AQ42" s="5"/>
+      <c r="AR42" s="5"/>
+      <c r="AS42" s="5"/>
+      <c r="AT42" s="5"/>
+      <c r="AU42" s="5"/>
+      <c r="AV42" s="5"/>
+      <c r="AW42" s="5"/>
+      <c r="AX42" s="5"/>
+      <c r="AY42" s="5"/>
+      <c r="AZ42" s="5"/>
+      <c r="BA42" s="5"/>
+      <c r="BB42" s="5"/>
+      <c r="BC42" s="5"/>
+      <c r="BD42" s="5"/>
+      <c r="BE42" s="5"/>
+      <c r="BF42" s="5"/>
+      <c r="BG42" s="5"/>
+      <c r="BH42" s="5"/>
     </row>
   </sheetData>
   <sortState ref="L1:L37">

</xml_diff>

<commit_message>
Added details for 25/09/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -7173,16 +7173,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="AL1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AO42" sqref="AO42"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="AN1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BE42" sqref="BE42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" style="47" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -7396,7 +7396,7 @@
     <row r="2" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <f t="shared" ref="A2:A41" si="0">MIN(E2:ZZ2)</f>
-        <v>262.10000000000002</v>
+        <v>258.5</v>
       </c>
       <c r="B2" s="12">
         <f t="shared" ref="B2:B37" si="1">MAX(E2:ZZ2)</f>
@@ -7404,7 +7404,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2-A2</f>
-        <v>48.5</v>
+        <v>52.100000000000023</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>116</v>
@@ -7514,7 +7514,9 @@
       <c r="AO2" s="5">
         <v>262.10000000000002</v>
       </c>
-      <c r="AP2" s="5"/>
+      <c r="AP2" s="5">
+        <v>258.5</v>
+      </c>
       <c r="AQ2" s="5"/>
       <c r="AR2" s="5"/>
       <c r="AS2" s="5"/>
@@ -7655,7 +7657,9 @@
       <c r="AO3" s="5">
         <v>277.7</v>
       </c>
-      <c r="AP3" s="5"/>
+      <c r="AP3" s="5">
+        <v>279.25</v>
+      </c>
       <c r="AQ3" s="5"/>
       <c r="AR3" s="5"/>
       <c r="AS3" s="5"/>
@@ -7678,7 +7682,7 @@
     <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
-        <v>267.39999999999998</v>
+        <v>262.25</v>
       </c>
       <c r="B4" s="12">
         <f t="shared" si="1"/>
@@ -7686,7 +7690,7 @@
       </c>
       <c r="C4" s="12">
         <f t="shared" si="2"/>
-        <v>24.300000000000011</v>
+        <v>29.449999999999989</v>
       </c>
       <c r="D4" s="44" t="s">
         <v>26</v>
@@ -7802,7 +7806,9 @@
       <c r="AO4" s="5">
         <v>267.85000000000002</v>
       </c>
-      <c r="AP4" s="5"/>
+      <c r="AP4" s="5">
+        <v>262.25</v>
+      </c>
       <c r="AQ4" s="5"/>
       <c r="AR4" s="5"/>
       <c r="AS4" s="5"/>
@@ -7949,7 +7955,9 @@
       <c r="AO5" s="5">
         <v>816.95</v>
       </c>
-      <c r="AP5" s="5"/>
+      <c r="AP5" s="5">
+        <v>821</v>
+      </c>
       <c r="AQ5" s="5"/>
       <c r="AR5" s="5"/>
       <c r="AS5" s="5"/>
@@ -8096,7 +8104,9 @@
       <c r="AO6" s="5">
         <v>253.8</v>
       </c>
-      <c r="AP6" s="5"/>
+      <c r="AP6" s="5">
+        <v>257.5</v>
+      </c>
       <c r="AQ6" s="5"/>
       <c r="AR6" s="5"/>
       <c r="AS6" s="5"/>
@@ -8243,7 +8253,9 @@
       <c r="AO7" s="5">
         <v>16.75</v>
       </c>
-      <c r="AP7" s="5"/>
+      <c r="AP7" s="5">
+        <v>16.45</v>
+      </c>
       <c r="AQ7" s="5"/>
       <c r="AR7" s="5"/>
       <c r="AS7" s="5"/>
@@ -8390,7 +8402,9 @@
       <c r="AO8" s="5">
         <v>57.8</v>
       </c>
-      <c r="AP8" s="5"/>
+      <c r="AP8" s="5">
+        <v>56.7</v>
+      </c>
       <c r="AQ8" s="5"/>
       <c r="AR8" s="5"/>
       <c r="AS8" s="5"/>
@@ -8529,7 +8543,9 @@
       <c r="AO9" s="28">
         <v>57.5</v>
       </c>
-      <c r="AP9" s="28"/>
+      <c r="AP9" s="28">
+        <v>56.65</v>
+      </c>
       <c r="AQ9" s="28"/>
       <c r="AR9" s="28"/>
       <c r="AS9" s="28"/>
@@ -8676,7 +8692,9 @@
       <c r="AO10" s="5">
         <v>42.2</v>
       </c>
-      <c r="AP10" s="5"/>
+      <c r="AP10" s="5">
+        <v>42.25</v>
+      </c>
       <c r="AQ10" s="5"/>
       <c r="AR10" s="5"/>
       <c r="AS10" s="5"/>
@@ -8823,7 +8841,9 @@
       <c r="AO11" s="5">
         <v>75.8</v>
       </c>
-      <c r="AP11" s="5"/>
+      <c r="AP11" s="5">
+        <v>74.349999999999994</v>
+      </c>
       <c r="AQ11" s="5"/>
       <c r="AR11" s="5"/>
       <c r="AS11" s="5"/>
@@ -8846,7 +8866,7 @@
     <row r="12" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
-        <v>78.05</v>
+        <v>75.900000000000006</v>
       </c>
       <c r="B12" s="12">
         <f t="shared" si="1"/>
@@ -8854,7 +8874,7 @@
       </c>
       <c r="C12" s="12">
         <f t="shared" si="2"/>
-        <v>17.350000000000009</v>
+        <v>19.5</v>
       </c>
       <c r="D12" s="45" t="s">
         <v>18</v>
@@ -8970,7 +8990,9 @@
       <c r="AO12" s="5">
         <v>78.05</v>
       </c>
-      <c r="AP12" s="5"/>
+      <c r="AP12" s="5">
+        <v>75.900000000000006</v>
+      </c>
       <c r="AQ12" s="5"/>
       <c r="AR12" s="5"/>
       <c r="AS12" s="5"/>
@@ -9117,7 +9139,9 @@
       <c r="AO13" s="5">
         <v>129.4</v>
       </c>
-      <c r="AP13" s="5"/>
+      <c r="AP13" s="5">
+        <v>127.2</v>
+      </c>
       <c r="AQ13" s="5"/>
       <c r="AR13" s="5"/>
       <c r="AS13" s="5"/>
@@ -9140,7 +9164,7 @@
     <row r="14" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <f t="shared" si="0"/>
-        <v>47.7</v>
+        <v>44.75</v>
       </c>
       <c r="B14" s="12">
         <f t="shared" si="1"/>
@@ -9148,7 +9172,7 @@
       </c>
       <c r="C14" s="12">
         <f t="shared" si="2"/>
-        <v>9.4499999999999957</v>
+        <v>12.399999999999999</v>
       </c>
       <c r="D14" s="45" t="s">
         <v>21</v>
@@ -9264,7 +9288,9 @@
       <c r="AO14" s="5">
         <v>47.7</v>
       </c>
-      <c r="AP14" s="5"/>
+      <c r="AP14" s="5">
+        <v>44.75</v>
+      </c>
       <c r="AQ14" s="5"/>
       <c r="AR14" s="5"/>
       <c r="AS14" s="5"/>
@@ -9411,7 +9437,9 @@
       <c r="AO15" s="5">
         <v>30.5</v>
       </c>
-      <c r="AP15" s="5"/>
+      <c r="AP15" s="5">
+        <v>30.8</v>
+      </c>
       <c r="AQ15" s="5"/>
       <c r="AR15" s="5"/>
       <c r="AS15" s="5"/>
@@ -9434,7 +9462,7 @@
     <row r="16" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <f t="shared" si="0"/>
-        <v>27.75</v>
+        <v>27</v>
       </c>
       <c r="B16" s="12">
         <f t="shared" si="1"/>
@@ -9442,7 +9470,7 @@
       </c>
       <c r="C16" s="12">
         <f t="shared" si="2"/>
-        <v>8.6499999999999986</v>
+        <v>9.3999999999999986</v>
       </c>
       <c r="D16" s="45" t="s">
         <v>127</v>
@@ -9550,7 +9578,9 @@
       <c r="AO16" s="5">
         <v>28.05</v>
       </c>
-      <c r="AP16" s="5"/>
+      <c r="AP16" s="5">
+        <v>27</v>
+      </c>
       <c r="AQ16" s="5"/>
       <c r="AR16" s="5"/>
       <c r="AS16" s="5"/>
@@ -9697,7 +9727,9 @@
       <c r="AO17" s="5">
         <v>654.4</v>
       </c>
-      <c r="AP17" s="5"/>
+      <c r="AP17" s="5">
+        <v>642.29999999999995</v>
+      </c>
       <c r="AQ17" s="5"/>
       <c r="AR17" s="5"/>
       <c r="AS17" s="5"/>
@@ -9720,7 +9752,7 @@
     <row r="18" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <f t="shared" si="0"/>
-        <v>452</v>
+        <v>441.05</v>
       </c>
       <c r="B18" s="12">
         <f t="shared" si="1"/>
@@ -9728,7 +9760,7 @@
       </c>
       <c r="C18" s="12">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>73.949999999999989</v>
       </c>
       <c r="D18" s="44" t="s">
         <v>27</v>
@@ -9844,7 +9876,9 @@
       <c r="AO18" s="5">
         <v>452</v>
       </c>
-      <c r="AP18" s="5"/>
+      <c r="AP18" s="5">
+        <v>441.05</v>
+      </c>
       <c r="AQ18" s="5"/>
       <c r="AR18" s="5"/>
       <c r="AS18" s="5"/>
@@ -9991,7 +10025,9 @@
       <c r="AO19" s="5">
         <v>240.7</v>
       </c>
-      <c r="AP19" s="5"/>
+      <c r="AP19" s="5">
+        <v>219.7</v>
+      </c>
       <c r="AQ19" s="5"/>
       <c r="AR19" s="5"/>
       <c r="AS19" s="5"/>
@@ -10138,7 +10174,9 @@
       <c r="AO20" s="5">
         <v>516</v>
       </c>
-      <c r="AP20" s="5"/>
+      <c r="AP20" s="5">
+        <v>499</v>
+      </c>
       <c r="AQ20" s="5"/>
       <c r="AR20" s="5"/>
       <c r="AS20" s="5"/>
@@ -10285,7 +10323,9 @@
       <c r="AO21" s="5">
         <v>724</v>
       </c>
-      <c r="AP21" s="5"/>
+      <c r="AP21" s="5">
+        <v>699.5</v>
+      </c>
       <c r="AQ21" s="5"/>
       <c r="AR21" s="5"/>
       <c r="AS21" s="5"/>
@@ -10308,7 +10348,7 @@
     <row r="22" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <f t="shared" si="0"/>
-        <v>395.1</v>
+        <v>388.35</v>
       </c>
       <c r="B22" s="12">
         <f t="shared" si="1"/>
@@ -10316,7 +10356,7 @@
       </c>
       <c r="C22" s="12">
         <f t="shared" si="2"/>
-        <v>39.549999999999955</v>
+        <v>46.299999999999955</v>
       </c>
       <c r="D22" s="44" t="s">
         <v>107</v>
@@ -10432,7 +10472,9 @@
       <c r="AO22" s="5">
         <v>395.8</v>
       </c>
-      <c r="AP22" s="5"/>
+      <c r="AP22" s="5">
+        <v>388.35</v>
+      </c>
       <c r="AQ22" s="5"/>
       <c r="AR22" s="5"/>
       <c r="AS22" s="5"/>
@@ -10455,7 +10497,7 @@
     <row r="23" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
-        <v>338.95</v>
+        <v>325</v>
       </c>
       <c r="B23" s="12">
         <f t="shared" si="1"/>
@@ -10463,7 +10505,7 @@
       </c>
       <c r="C23" s="12">
         <f t="shared" si="2"/>
-        <v>33.600000000000023</v>
+        <v>47.550000000000011</v>
       </c>
       <c r="D23" s="44" t="s">
         <v>294</v>
@@ -10525,7 +10567,9 @@
       <c r="AO23" s="5">
         <v>338.95</v>
       </c>
-      <c r="AP23" s="5"/>
+      <c r="AP23" s="5">
+        <v>325</v>
+      </c>
       <c r="AQ23" s="5"/>
       <c r="AR23" s="5"/>
       <c r="AS23" s="5"/>
@@ -10664,7 +10708,9 @@
       <c r="AO24" s="5">
         <v>58.5</v>
       </c>
-      <c r="AP24" s="5"/>
+      <c r="AP24" s="5">
+        <v>55.6</v>
+      </c>
       <c r="AQ24" s="5"/>
       <c r="AR24" s="5"/>
       <c r="AS24" s="5"/>
@@ -10799,7 +10845,9 @@
       <c r="AO25" s="5">
         <v>231.85</v>
       </c>
-      <c r="AP25" s="5"/>
+      <c r="AP25" s="5">
+        <v>228.65</v>
+      </c>
       <c r="AQ25" s="5"/>
       <c r="AR25" s="5"/>
       <c r="AS25" s="5"/>
@@ -10916,7 +10964,9 @@
       <c r="AO26" s="5">
         <v>899</v>
       </c>
-      <c r="AP26" s="5"/>
+      <c r="AP26" s="5">
+        <v>901</v>
+      </c>
       <c r="AQ26" s="5"/>
       <c r="AR26" s="5"/>
       <c r="AS26" s="5"/>
@@ -11021,7 +11071,9 @@
       <c r="AO27" s="5">
         <v>88.3</v>
       </c>
-      <c r="AP27" s="5"/>
+      <c r="AP27" s="5">
+        <v>85</v>
+      </c>
       <c r="AQ27" s="5"/>
       <c r="AR27" s="5"/>
       <c r="AS27" s="5"/>
@@ -11126,7 +11178,9 @@
       <c r="AO28" s="5">
         <v>42.85</v>
       </c>
-      <c r="AP28" s="5"/>
+      <c r="AP28" s="5">
+        <v>42.5</v>
+      </c>
       <c r="AQ28" s="5"/>
       <c r="AR28" s="5"/>
       <c r="AS28" s="5"/>
@@ -11149,7 +11203,7 @@
     <row r="29" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <f t="shared" si="0"/>
-        <v>54.2</v>
+        <v>53.15</v>
       </c>
       <c r="B29" s="12">
         <f t="shared" si="1"/>
@@ -11157,7 +11211,7 @@
       </c>
       <c r="C29" s="12">
         <f t="shared" si="2"/>
-        <v>2.8499999999999943</v>
+        <v>3.8999999999999986</v>
       </c>
       <c r="D29" s="45" t="s">
         <v>272</v>
@@ -11231,7 +11285,9 @@
       <c r="AO29" s="5">
         <v>54.2</v>
       </c>
-      <c r="AP29" s="5"/>
+      <c r="AP29" s="5">
+        <v>53.15</v>
+      </c>
       <c r="AQ29" s="5"/>
       <c r="AR29" s="5"/>
       <c r="AS29" s="5"/>
@@ -11254,7 +11310,7 @@
     <row r="30" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <f t="shared" si="0"/>
-        <v>122.3</v>
+        <v>119.6</v>
       </c>
       <c r="B30" s="12">
         <f t="shared" si="1"/>
@@ -11262,7 +11318,7 @@
       </c>
       <c r="C30" s="12">
         <f t="shared" si="2"/>
-        <v>12.200000000000003</v>
+        <v>14.900000000000006</v>
       </c>
       <c r="D30" s="45" t="s">
         <v>273</v>
@@ -11336,7 +11392,9 @@
       <c r="AO30" s="5">
         <v>122.3</v>
       </c>
-      <c r="AP30" s="5"/>
+      <c r="AP30" s="5">
+        <v>119.6</v>
+      </c>
       <c r="AQ30" s="5"/>
       <c r="AR30" s="5"/>
       <c r="AS30" s="5"/>
@@ -11359,7 +11417,7 @@
     <row r="31" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
-        <v>182</v>
+        <v>181.2</v>
       </c>
       <c r="B31" s="12">
         <f t="shared" si="1"/>
@@ -11367,7 +11425,7 @@
       </c>
       <c r="C31" s="12">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>16.800000000000011</v>
       </c>
       <c r="D31" s="45" t="s">
         <v>274</v>
@@ -11441,7 +11499,9 @@
       <c r="AO31" s="5">
         <v>182</v>
       </c>
-      <c r="AP31" s="5"/>
+      <c r="AP31" s="5">
+        <v>181.2</v>
+      </c>
       <c r="AQ31" s="5"/>
       <c r="AR31" s="5"/>
       <c r="AS31" s="5"/>
@@ -11464,7 +11524,7 @@
     <row r="32" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <f t="shared" si="0"/>
-        <v>70.7</v>
+        <v>67.25</v>
       </c>
       <c r="B32" s="12">
         <f t="shared" si="1"/>
@@ -11472,7 +11532,7 @@
       </c>
       <c r="C32" s="12">
         <f t="shared" si="2"/>
-        <v>8.1499999999999915</v>
+        <v>11.599999999999994</v>
       </c>
       <c r="D32" s="45" t="s">
         <v>275</v>
@@ -11546,7 +11606,9 @@
       <c r="AO32" s="5">
         <v>70.7</v>
       </c>
-      <c r="AP32" s="5"/>
+      <c r="AP32" s="5">
+        <v>67.25</v>
+      </c>
       <c r="AQ32" s="5"/>
       <c r="AR32" s="5"/>
       <c r="AS32" s="5"/>
@@ -11651,7 +11713,9 @@
       <c r="AO33" s="5">
         <v>44.95</v>
       </c>
-      <c r="AP33" s="5"/>
+      <c r="AP33" s="5">
+        <v>43.25</v>
+      </c>
       <c r="AQ33" s="5"/>
       <c r="AR33" s="5"/>
       <c r="AS33" s="5"/>
@@ -11756,7 +11820,9 @@
       <c r="AO34" s="5">
         <v>66.3</v>
       </c>
-      <c r="AP34" s="5"/>
+      <c r="AP34" s="5">
+        <v>64.5</v>
+      </c>
       <c r="AQ34" s="5"/>
       <c r="AR34" s="5"/>
       <c r="AS34" s="5"/>
@@ -11779,7 +11845,7 @@
     <row r="35" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <f t="shared" si="0"/>
-        <v>30.7</v>
+        <v>30.6</v>
       </c>
       <c r="B35" s="12">
         <f t="shared" si="1"/>
@@ -11787,7 +11853,7 @@
       </c>
       <c r="C35" s="12">
         <f t="shared" si="2"/>
-        <v>1.8499999999999979</v>
+        <v>1.9499999999999957</v>
       </c>
       <c r="D35" s="45" t="s">
         <v>278</v>
@@ -11861,7 +11927,9 @@
       <c r="AO35" s="5">
         <v>31.05</v>
       </c>
-      <c r="AP35" s="5"/>
+      <c r="AP35" s="5">
+        <v>30.6</v>
+      </c>
       <c r="AQ35" s="5"/>
       <c r="AR35" s="5"/>
       <c r="AS35" s="5"/>
@@ -11884,7 +11952,7 @@
     <row r="36" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <f t="shared" si="0"/>
-        <v>84.25</v>
+        <v>83.2</v>
       </c>
       <c r="B36" s="12">
         <f t="shared" si="1"/>
@@ -11892,7 +11960,7 @@
       </c>
       <c r="C36" s="12">
         <f t="shared" si="2"/>
-        <v>6.75</v>
+        <v>7.7999999999999972</v>
       </c>
       <c r="D36" s="45" t="s">
         <v>279</v>
@@ -11966,7 +12034,9 @@
       <c r="AO36" s="5">
         <v>84.85</v>
       </c>
-      <c r="AP36" s="5"/>
+      <c r="AP36" s="5">
+        <v>83.2</v>
+      </c>
       <c r="AQ36" s="5"/>
       <c r="AR36" s="5"/>
       <c r="AS36" s="5"/>
@@ -12071,7 +12141,9 @@
       <c r="AO37" s="5">
         <v>126.05</v>
       </c>
-      <c r="AP37" s="5"/>
+      <c r="AP37" s="5">
+        <v>128.9</v>
+      </c>
       <c r="AQ37" s="5"/>
       <c r="AR37" s="5"/>
       <c r="AS37" s="5"/>
@@ -12176,7 +12248,9 @@
       <c r="AO38" s="5">
         <v>142.30000000000001</v>
       </c>
-      <c r="AP38" s="5"/>
+      <c r="AP38" s="5">
+        <v>142.65</v>
+      </c>
       <c r="AQ38" s="5"/>
       <c r="AR38" s="5"/>
       <c r="AS38" s="5"/>
@@ -12281,7 +12355,9 @@
       <c r="AO39" s="5">
         <v>150.75</v>
       </c>
-      <c r="AP39" s="5"/>
+      <c r="AP39" s="5">
+        <v>147.30000000000001</v>
+      </c>
       <c r="AQ39" s="5"/>
       <c r="AR39" s="5"/>
       <c r="AS39" s="5"/>
@@ -12374,7 +12450,9 @@
       <c r="AO40" s="5">
         <v>101.7</v>
       </c>
-      <c r="AP40" s="5"/>
+      <c r="AP40" s="5">
+        <v>104</v>
+      </c>
       <c r="AQ40" s="5"/>
       <c r="AR40" s="5"/>
       <c r="AS40" s="5"/>
@@ -12397,7 +12475,7 @@
     <row r="41" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <f t="shared" si="0"/>
-        <v>60.5</v>
+        <v>57.9</v>
       </c>
       <c r="B41" s="12">
         <f t="shared" ref="B41" si="4">MAX(E41:ZZ41)</f>
@@ -12405,7 +12483,7 @@
       </c>
       <c r="C41" s="12">
         <f t="shared" si="2"/>
-        <v>3.9000000000000057</v>
+        <v>6.5000000000000071</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>296</v>
@@ -12455,7 +12533,9 @@
       <c r="AO41" s="5">
         <v>60.5</v>
       </c>
-      <c r="AP41" s="5"/>
+      <c r="AP41" s="5">
+        <v>57.9</v>
+      </c>
       <c r="AQ41" s="5"/>
       <c r="AR41" s="5"/>
       <c r="AS41" s="5"/>
@@ -12478,7 +12558,7 @@
     <row r="42" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <f t="shared" ref="A42" si="5">MIN(E42:ZZ42)</f>
-        <v>202.3</v>
+        <v>193</v>
       </c>
       <c r="B42" s="12">
         <f t="shared" ref="B42" si="6">MAX(E42:ZZ42)</f>
@@ -12486,7 +12566,7 @@
       </c>
       <c r="C42" s="12">
         <f t="shared" ref="C42" si="7">B42-A42</f>
-        <v>0</v>
+        <v>9.3000000000000114</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>308</v>
@@ -12530,7 +12610,9 @@
       <c r="AO42" s="5">
         <v>202.3</v>
       </c>
-      <c r="AP42" s="5"/>
+      <c r="AP42" s="5">
+        <v>193</v>
+      </c>
       <c r="AQ42" s="5"/>
       <c r="AR42" s="5"/>
       <c r="AS42" s="5"/>

</xml_diff>

<commit_message>
Added details for 27/09/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="310">
   <si>
     <t>Date</t>
   </si>
@@ -952,6 +952,9 @@
   </si>
   <si>
     <t>BOMDYEING</t>
+  </si>
+  <si>
+    <t>ICICIGI</t>
   </si>
 </sst>
 </file>
@@ -7171,11 +7174,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BH42"/>
+  <dimension ref="A1:BH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="AN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BE42" sqref="BE42"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="AO1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AR2" sqref="AR2:AR43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7396,7 +7399,7 @@
     <row r="2" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <f t="shared" ref="A2:A41" si="0">MIN(E2:ZZ2)</f>
-        <v>258.5</v>
+        <v>250.25</v>
       </c>
       <c r="B2" s="12">
         <f t="shared" ref="B2:B37" si="1">MAX(E2:ZZ2)</f>
@@ -7404,7 +7407,7 @@
       </c>
       <c r="C2" s="12">
         <f>B2-A2</f>
-        <v>52.100000000000023</v>
+        <v>60.350000000000023</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>116</v>
@@ -7517,8 +7520,12 @@
       <c r="AP2" s="5">
         <v>258.5</v>
       </c>
-      <c r="AQ2" s="5"/>
-      <c r="AR2" s="5"/>
+      <c r="AQ2" s="5">
+        <v>258.8</v>
+      </c>
+      <c r="AR2" s="5">
+        <v>250.25</v>
+      </c>
       <c r="AS2" s="5"/>
       <c r="AT2" s="5"/>
       <c r="AU2" s="5"/>
@@ -7539,7 +7546,7 @@
     <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <f t="shared" si="0"/>
-        <v>277.7</v>
+        <v>276.10000000000002</v>
       </c>
       <c r="B3" s="12">
         <f t="shared" si="1"/>
@@ -7547,7 +7554,7 @@
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C41" si="2">B3-A3</f>
-        <v>25</v>
+        <v>26.599999999999966</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>115</v>
@@ -7660,8 +7667,12 @@
       <c r="AP3" s="5">
         <v>279.25</v>
       </c>
-      <c r="AQ3" s="5"/>
-      <c r="AR3" s="5"/>
+      <c r="AQ3" s="5">
+        <v>282.3</v>
+      </c>
+      <c r="AR3" s="5">
+        <v>276.10000000000002</v>
+      </c>
       <c r="AS3" s="5"/>
       <c r="AT3" s="5"/>
       <c r="AU3" s="5"/>
@@ -7682,7 +7693,7 @@
     <row r="4" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
-        <v>262.25</v>
+        <v>259.45</v>
       </c>
       <c r="B4" s="12">
         <f t="shared" si="1"/>
@@ -7690,7 +7701,7 @@
       </c>
       <c r="C4" s="12">
         <f t="shared" si="2"/>
-        <v>29.449999999999989</v>
+        <v>32.25</v>
       </c>
       <c r="D4" s="44" t="s">
         <v>26</v>
@@ -7809,8 +7820,12 @@
       <c r="AP4" s="5">
         <v>262.25</v>
       </c>
-      <c r="AQ4" s="5"/>
-      <c r="AR4" s="5"/>
+      <c r="AQ4" s="5">
+        <v>262.75</v>
+      </c>
+      <c r="AR4" s="5">
+        <v>259.45</v>
+      </c>
       <c r="AS4" s="5"/>
       <c r="AT4" s="5"/>
       <c r="AU4" s="5"/>
@@ -7831,7 +7846,7 @@
     <row r="5" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <f t="shared" si="0"/>
-        <v>816.95</v>
+        <v>798.4</v>
       </c>
       <c r="B5" s="12">
         <f t="shared" si="1"/>
@@ -7839,7 +7854,7 @@
       </c>
       <c r="C5" s="12">
         <f t="shared" si="2"/>
-        <v>837.05</v>
+        <v>855.6</v>
       </c>
       <c r="D5" s="44" t="s">
         <v>106</v>
@@ -7958,8 +7973,12 @@
       <c r="AP5" s="5">
         <v>821</v>
       </c>
-      <c r="AQ5" s="5"/>
-      <c r="AR5" s="5"/>
+      <c r="AQ5" s="5">
+        <v>821.2</v>
+      </c>
+      <c r="AR5" s="5">
+        <v>798.4</v>
+      </c>
       <c r="AS5" s="5"/>
       <c r="AT5" s="5"/>
       <c r="AU5" s="5"/>
@@ -8107,8 +8126,12 @@
       <c r="AP6" s="5">
         <v>257.5</v>
       </c>
-      <c r="AQ6" s="5"/>
-      <c r="AR6" s="5"/>
+      <c r="AQ6" s="5">
+        <v>260.75</v>
+      </c>
+      <c r="AR6" s="5">
+        <v>260.2</v>
+      </c>
       <c r="AS6" s="5"/>
       <c r="AT6" s="5"/>
       <c r="AU6" s="5"/>
@@ -8256,8 +8279,12 @@
       <c r="AP7" s="5">
         <v>16.45</v>
       </c>
-      <c r="AQ7" s="5"/>
-      <c r="AR7" s="5"/>
+      <c r="AQ7" s="5">
+        <v>16.75</v>
+      </c>
+      <c r="AR7" s="5">
+        <v>15.9</v>
+      </c>
       <c r="AS7" s="5"/>
       <c r="AT7" s="5"/>
       <c r="AU7" s="5"/>
@@ -8278,7 +8305,7 @@
     <row r="8" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <f t="shared" si="0"/>
-        <v>56.6</v>
+        <v>54.1</v>
       </c>
       <c r="B8" s="12">
         <f t="shared" si="1"/>
@@ -8286,7 +8313,7 @@
       </c>
       <c r="C8" s="12">
         <f t="shared" si="2"/>
-        <v>6.6999999999999957</v>
+        <v>9.1999999999999957</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>23</v>
@@ -8405,8 +8432,12 @@
       <c r="AP8" s="5">
         <v>56.7</v>
       </c>
-      <c r="AQ8" s="5"/>
-      <c r="AR8" s="5"/>
+      <c r="AQ8" s="5">
+        <v>57</v>
+      </c>
+      <c r="AR8" s="5">
+        <v>54.1</v>
+      </c>
       <c r="AS8" s="5"/>
       <c r="AT8" s="5"/>
       <c r="AU8" s="5"/>
@@ -8546,8 +8577,12 @@
       <c r="AP9" s="28">
         <v>56.65</v>
       </c>
-      <c r="AQ9" s="28"/>
-      <c r="AR9" s="28"/>
+      <c r="AQ9" s="28">
+        <v>57.45</v>
+      </c>
+      <c r="AR9" s="28">
+        <v>56.15</v>
+      </c>
       <c r="AS9" s="28"/>
       <c r="AT9" s="28"/>
       <c r="AU9" s="28"/>
@@ -8695,8 +8730,12 @@
       <c r="AP10" s="5">
         <v>42.25</v>
       </c>
-      <c r="AQ10" s="5"/>
-      <c r="AR10" s="5"/>
+      <c r="AQ10" s="5">
+        <v>42.8</v>
+      </c>
+      <c r="AR10" s="5">
+        <v>41.05</v>
+      </c>
       <c r="AS10" s="5"/>
       <c r="AT10" s="5"/>
       <c r="AU10" s="5"/>
@@ -8844,8 +8883,12 @@
       <c r="AP11" s="5">
         <v>74.349999999999994</v>
       </c>
-      <c r="AQ11" s="5"/>
-      <c r="AR11" s="5"/>
+      <c r="AQ11" s="5">
+        <v>76.95</v>
+      </c>
+      <c r="AR11" s="5">
+        <v>74.900000000000006</v>
+      </c>
       <c r="AS11" s="5"/>
       <c r="AT11" s="5"/>
       <c r="AU11" s="5"/>
@@ -8866,7 +8909,7 @@
     <row r="12" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
-        <v>75.900000000000006</v>
+        <v>75.55</v>
       </c>
       <c r="B12" s="12">
         <f t="shared" si="1"/>
@@ -8874,7 +8917,7 @@
       </c>
       <c r="C12" s="12">
         <f t="shared" si="2"/>
-        <v>19.5</v>
+        <v>19.850000000000009</v>
       </c>
       <c r="D12" s="45" t="s">
         <v>18</v>
@@ -8993,8 +9036,12 @@
       <c r="AP12" s="5">
         <v>75.900000000000006</v>
       </c>
-      <c r="AQ12" s="5"/>
-      <c r="AR12" s="5"/>
+      <c r="AQ12" s="5">
+        <v>76.55</v>
+      </c>
+      <c r="AR12" s="5">
+        <v>75.55</v>
+      </c>
       <c r="AS12" s="5"/>
       <c r="AT12" s="5"/>
       <c r="AU12" s="5"/>
@@ -9142,8 +9189,12 @@
       <c r="AP13" s="5">
         <v>127.2</v>
       </c>
-      <c r="AQ13" s="5"/>
-      <c r="AR13" s="5"/>
+      <c r="AQ13" s="5">
+        <v>128.5</v>
+      </c>
+      <c r="AR13" s="5">
+        <v>124.45</v>
+      </c>
       <c r="AS13" s="5"/>
       <c r="AT13" s="5"/>
       <c r="AU13" s="5"/>
@@ -9164,7 +9215,7 @@
     <row r="14" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <f t="shared" si="0"/>
-        <v>44.75</v>
+        <v>44.1</v>
       </c>
       <c r="B14" s="12">
         <f t="shared" si="1"/>
@@ -9172,7 +9223,7 @@
       </c>
       <c r="C14" s="12">
         <f t="shared" si="2"/>
-        <v>12.399999999999999</v>
+        <v>13.049999999999997</v>
       </c>
       <c r="D14" s="45" t="s">
         <v>21</v>
@@ -9291,8 +9342,12 @@
       <c r="AP14" s="5">
         <v>44.75</v>
       </c>
-      <c r="AQ14" s="5"/>
-      <c r="AR14" s="5"/>
+      <c r="AQ14" s="5">
+        <v>44.6</v>
+      </c>
+      <c r="AR14" s="5">
+        <v>44.1</v>
+      </c>
       <c r="AS14" s="5"/>
       <c r="AT14" s="5"/>
       <c r="AU14" s="5"/>
@@ -9313,7 +9368,7 @@
     <row r="15" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
-        <v>30.5</v>
+        <v>30</v>
       </c>
       <c r="B15" s="12">
         <f t="shared" si="1"/>
@@ -9321,7 +9376,7 @@
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
-        <v>2.7000000000000028</v>
+        <v>3.2000000000000028</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>22</v>
@@ -9440,8 +9495,12 @@
       <c r="AP15" s="5">
         <v>30.8</v>
       </c>
-      <c r="AQ15" s="5"/>
-      <c r="AR15" s="5"/>
+      <c r="AQ15" s="5">
+        <v>30</v>
+      </c>
+      <c r="AR15" s="5">
+        <v>30.65</v>
+      </c>
       <c r="AS15" s="5"/>
       <c r="AT15" s="5"/>
       <c r="AU15" s="5"/>
@@ -9462,7 +9521,7 @@
     <row r="16" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>26.8</v>
       </c>
       <c r="B16" s="12">
         <f t="shared" si="1"/>
@@ -9470,7 +9529,7 @@
       </c>
       <c r="C16" s="12">
         <f t="shared" si="2"/>
-        <v>9.3999999999999986</v>
+        <v>9.5999999999999979</v>
       </c>
       <c r="D16" s="45" t="s">
         <v>127</v>
@@ -9581,8 +9640,12 @@
       <c r="AP16" s="5">
         <v>27</v>
       </c>
-      <c r="AQ16" s="5"/>
-      <c r="AR16" s="5"/>
+      <c r="AQ16" s="5">
+        <v>27.55</v>
+      </c>
+      <c r="AR16" s="5">
+        <v>26.8</v>
+      </c>
       <c r="AS16" s="5"/>
       <c r="AT16" s="5"/>
       <c r="AU16" s="5"/>
@@ -9730,8 +9793,12 @@
       <c r="AP17" s="5">
         <v>642.29999999999995</v>
       </c>
-      <c r="AQ17" s="5"/>
-      <c r="AR17" s="5"/>
+      <c r="AQ17" s="5">
+        <v>656.5</v>
+      </c>
+      <c r="AR17" s="5">
+        <v>650</v>
+      </c>
       <c r="AS17" s="5"/>
       <c r="AT17" s="5"/>
       <c r="AU17" s="5"/>
@@ -9752,7 +9819,7 @@
     <row r="18" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <f t="shared" si="0"/>
-        <v>441.05</v>
+        <v>433</v>
       </c>
       <c r="B18" s="12">
         <f t="shared" si="1"/>
@@ -9760,7 +9827,7 @@
       </c>
       <c r="C18" s="12">
         <f t="shared" si="2"/>
-        <v>73.949999999999989</v>
+        <v>82</v>
       </c>
       <c r="D18" s="44" t="s">
         <v>27</v>
@@ -9879,8 +9946,12 @@
       <c r="AP18" s="5">
         <v>441.05</v>
       </c>
-      <c r="AQ18" s="5"/>
-      <c r="AR18" s="5"/>
+      <c r="AQ18" s="5">
+        <v>433</v>
+      </c>
+      <c r="AR18" s="5">
+        <v>439</v>
+      </c>
       <c r="AS18" s="5"/>
       <c r="AT18" s="5"/>
       <c r="AU18" s="5"/>
@@ -10028,8 +10099,12 @@
       <c r="AP19" s="5">
         <v>219.7</v>
       </c>
-      <c r="AQ19" s="5"/>
-      <c r="AR19" s="5"/>
+      <c r="AQ19" s="5">
+        <v>247.5</v>
+      </c>
+      <c r="AR19" s="5">
+        <v>235</v>
+      </c>
       <c r="AS19" s="5"/>
       <c r="AT19" s="5"/>
       <c r="AU19" s="5"/>
@@ -10177,8 +10252,12 @@
       <c r="AP20" s="5">
         <v>499</v>
       </c>
-      <c r="AQ20" s="5"/>
-      <c r="AR20" s="5"/>
+      <c r="AQ20" s="5">
+        <v>495.5</v>
+      </c>
+      <c r="AR20" s="5">
+        <v>489</v>
+      </c>
       <c r="AS20" s="5"/>
       <c r="AT20" s="5"/>
       <c r="AU20" s="5"/>
@@ -10326,8 +10405,12 @@
       <c r="AP21" s="5">
         <v>699.5</v>
       </c>
-      <c r="AQ21" s="5"/>
-      <c r="AR21" s="5"/>
+      <c r="AQ21" s="5">
+        <v>714</v>
+      </c>
+      <c r="AR21" s="5">
+        <v>689.8</v>
+      </c>
       <c r="AS21" s="5"/>
       <c r="AT21" s="5"/>
       <c r="AU21" s="5"/>
@@ -10348,7 +10431,7 @@
     <row r="22" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <f t="shared" si="0"/>
-        <v>388.35</v>
+        <v>384.85</v>
       </c>
       <c r="B22" s="12">
         <f t="shared" si="1"/>
@@ -10356,7 +10439,7 @@
       </c>
       <c r="C22" s="12">
         <f t="shared" si="2"/>
-        <v>46.299999999999955</v>
+        <v>49.799999999999955</v>
       </c>
       <c r="D22" s="44" t="s">
         <v>107</v>
@@ -10475,8 +10558,12 @@
       <c r="AP22" s="5">
         <v>388.35</v>
       </c>
-      <c r="AQ22" s="5"/>
-      <c r="AR22" s="5"/>
+      <c r="AQ22" s="5">
+        <v>384.85</v>
+      </c>
+      <c r="AR22" s="5">
+        <v>387.3</v>
+      </c>
       <c r="AS22" s="5"/>
       <c r="AT22" s="5"/>
       <c r="AU22" s="5"/>
@@ -10497,7 +10584,7 @@
     <row r="23" spans="1:60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="B23" s="12">
         <f t="shared" si="1"/>
@@ -10505,7 +10592,7 @@
       </c>
       <c r="C23" s="12">
         <f t="shared" si="2"/>
-        <v>47.550000000000011</v>
+        <v>54.550000000000011</v>
       </c>
       <c r="D23" s="44" t="s">
         <v>294</v>
@@ -10570,8 +10657,12 @@
       <c r="AP23" s="5">
         <v>325</v>
       </c>
-      <c r="AQ23" s="5"/>
-      <c r="AR23" s="5"/>
+      <c r="AQ23" s="5">
+        <v>332.1</v>
+      </c>
+      <c r="AR23" s="5">
+        <v>318</v>
+      </c>
       <c r="AS23" s="5"/>
       <c r="AT23" s="5"/>
       <c r="AU23" s="5"/>
@@ -10592,7 +10683,7 @@
     <row r="24" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <f t="shared" si="0"/>
-        <v>54.95</v>
+        <v>54.45</v>
       </c>
       <c r="B24" s="12">
         <f t="shared" si="1"/>
@@ -10600,7 +10691,7 @@
       </c>
       <c r="C24" s="12">
         <f t="shared" si="2"/>
-        <v>30.700000000000003</v>
+        <v>31.200000000000003</v>
       </c>
       <c r="D24" s="45" t="s">
         <v>128</v>
@@ -10711,8 +10802,12 @@
       <c r="AP24" s="5">
         <v>55.6</v>
       </c>
-      <c r="AQ24" s="5"/>
-      <c r="AR24" s="5"/>
+      <c r="AQ24" s="5">
+        <v>56.7</v>
+      </c>
+      <c r="AR24" s="5">
+        <v>54.45</v>
+      </c>
       <c r="AS24" s="5"/>
       <c r="AT24" s="5"/>
       <c r="AU24" s="5"/>
@@ -10848,8 +10943,12 @@
       <c r="AP25" s="5">
         <v>228.65</v>
       </c>
-      <c r="AQ25" s="5"/>
-      <c r="AR25" s="5"/>
+      <c r="AQ25" s="5">
+        <v>229.4</v>
+      </c>
+      <c r="AR25" s="5">
+        <v>223.85</v>
+      </c>
       <c r="AS25" s="5"/>
       <c r="AT25" s="5"/>
       <c r="AU25" s="5"/>
@@ -10967,8 +11066,12 @@
       <c r="AP26" s="5">
         <v>901</v>
       </c>
-      <c r="AQ26" s="5"/>
-      <c r="AR26" s="5"/>
+      <c r="AQ26" s="5">
+        <v>902.15</v>
+      </c>
+      <c r="AR26" s="5">
+        <v>895.9</v>
+      </c>
       <c r="AS26" s="5"/>
       <c r="AT26" s="5"/>
       <c r="AU26" s="5"/>
@@ -11074,8 +11177,12 @@
       <c r="AP27" s="5">
         <v>85</v>
       </c>
-      <c r="AQ27" s="5"/>
-      <c r="AR27" s="5"/>
+      <c r="AQ27" s="5">
+        <v>88.05</v>
+      </c>
+      <c r="AR27" s="5">
+        <v>89.5</v>
+      </c>
       <c r="AS27" s="5"/>
       <c r="AT27" s="5"/>
       <c r="AU27" s="5"/>
@@ -11181,8 +11288,12 @@
       <c r="AP28" s="5">
         <v>42.5</v>
       </c>
-      <c r="AQ28" s="5"/>
-      <c r="AR28" s="5"/>
+      <c r="AQ28" s="5">
+        <v>43.2</v>
+      </c>
+      <c r="AR28" s="5">
+        <v>40.549999999999997</v>
+      </c>
       <c r="AS28" s="5"/>
       <c r="AT28" s="5"/>
       <c r="AU28" s="5"/>
@@ -11203,7 +11314,7 @@
     <row r="29" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <f t="shared" si="0"/>
-        <v>53.15</v>
+        <v>52.15</v>
       </c>
       <c r="B29" s="12">
         <f t="shared" si="1"/>
@@ -11211,7 +11322,7 @@
       </c>
       <c r="C29" s="12">
         <f t="shared" si="2"/>
-        <v>3.8999999999999986</v>
+        <v>4.8999999999999986</v>
       </c>
       <c r="D29" s="45" t="s">
         <v>272</v>
@@ -11288,8 +11399,12 @@
       <c r="AP29" s="5">
         <v>53.15</v>
       </c>
-      <c r="AQ29" s="5"/>
-      <c r="AR29" s="5"/>
+      <c r="AQ29" s="5">
+        <v>53.5</v>
+      </c>
+      <c r="AR29" s="5">
+        <v>52.15</v>
+      </c>
       <c r="AS29" s="5"/>
       <c r="AT29" s="5"/>
       <c r="AU29" s="5"/>
@@ -11310,7 +11425,7 @@
     <row r="30" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <f t="shared" si="0"/>
-        <v>119.6</v>
+        <v>114.8</v>
       </c>
       <c r="B30" s="12">
         <f t="shared" si="1"/>
@@ -11318,7 +11433,7 @@
       </c>
       <c r="C30" s="12">
         <f t="shared" si="2"/>
-        <v>14.900000000000006</v>
+        <v>19.700000000000003</v>
       </c>
       <c r="D30" s="45" t="s">
         <v>273</v>
@@ -11395,8 +11510,12 @@
       <c r="AP30" s="5">
         <v>119.6</v>
       </c>
-      <c r="AQ30" s="5"/>
-      <c r="AR30" s="5"/>
+      <c r="AQ30" s="5">
+        <v>118.7</v>
+      </c>
+      <c r="AR30" s="5">
+        <v>114.8</v>
+      </c>
       <c r="AS30" s="5"/>
       <c r="AT30" s="5"/>
       <c r="AU30" s="5"/>
@@ -11417,7 +11536,7 @@
     <row r="31" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
-        <v>181.2</v>
+        <v>176.9</v>
       </c>
       <c r="B31" s="12">
         <f t="shared" si="1"/>
@@ -11425,7 +11544,7 @@
       </c>
       <c r="C31" s="12">
         <f t="shared" si="2"/>
-        <v>16.800000000000011</v>
+        <v>21.099999999999994</v>
       </c>
       <c r="D31" s="45" t="s">
         <v>274</v>
@@ -11502,8 +11621,12 @@
       <c r="AP31" s="5">
         <v>181.2</v>
       </c>
-      <c r="AQ31" s="5"/>
-      <c r="AR31" s="5"/>
+      <c r="AQ31" s="5">
+        <v>182.6</v>
+      </c>
+      <c r="AR31" s="5">
+        <v>176.9</v>
+      </c>
       <c r="AS31" s="5"/>
       <c r="AT31" s="5"/>
       <c r="AU31" s="5"/>
@@ -11524,7 +11647,7 @@
     <row r="32" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <f t="shared" si="0"/>
-        <v>67.25</v>
+        <v>66.400000000000006</v>
       </c>
       <c r="B32" s="12">
         <f t="shared" si="1"/>
@@ -11532,7 +11655,7 @@
       </c>
       <c r="C32" s="12">
         <f t="shared" si="2"/>
-        <v>11.599999999999994</v>
+        <v>12.449999999999989</v>
       </c>
       <c r="D32" s="45" t="s">
         <v>275</v>
@@ -11609,8 +11732,12 @@
       <c r="AP32" s="5">
         <v>67.25</v>
       </c>
-      <c r="AQ32" s="5"/>
-      <c r="AR32" s="5"/>
+      <c r="AQ32" s="5">
+        <v>66.650000000000006</v>
+      </c>
+      <c r="AR32" s="5">
+        <v>66.400000000000006</v>
+      </c>
       <c r="AS32" s="5"/>
       <c r="AT32" s="5"/>
       <c r="AU32" s="5"/>
@@ -11716,8 +11843,12 @@
       <c r="AP33" s="5">
         <v>43.25</v>
       </c>
-      <c r="AQ33" s="5"/>
-      <c r="AR33" s="5"/>
+      <c r="AQ33" s="5">
+        <v>43.8</v>
+      </c>
+      <c r="AR33" s="5">
+        <v>40.799999999999997</v>
+      </c>
       <c r="AS33" s="5"/>
       <c r="AT33" s="5"/>
       <c r="AU33" s="5"/>
@@ -11738,7 +11869,7 @@
     <row r="34" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <f t="shared" si="0"/>
-        <v>62.95</v>
+        <v>62.65</v>
       </c>
       <c r="B34" s="12">
         <f t="shared" si="1"/>
@@ -11746,7 +11877,7 @@
       </c>
       <c r="C34" s="12">
         <f t="shared" si="2"/>
-        <v>7.1499999999999915</v>
+        <v>7.4499999999999957</v>
       </c>
       <c r="D34" s="45" t="s">
         <v>277</v>
@@ -11823,8 +11954,12 @@
       <c r="AP34" s="5">
         <v>64.5</v>
       </c>
-      <c r="AQ34" s="5"/>
-      <c r="AR34" s="5"/>
+      <c r="AQ34" s="5">
+        <v>65</v>
+      </c>
+      <c r="AR34" s="5">
+        <v>62.65</v>
+      </c>
       <c r="AS34" s="5"/>
       <c r="AT34" s="5"/>
       <c r="AU34" s="5"/>
@@ -11845,7 +11980,7 @@
     <row r="35" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <f t="shared" si="0"/>
-        <v>30.6</v>
+        <v>30.05</v>
       </c>
       <c r="B35" s="12">
         <f t="shared" si="1"/>
@@ -11853,7 +11988,7 @@
       </c>
       <c r="C35" s="12">
         <f t="shared" si="2"/>
-        <v>1.9499999999999957</v>
+        <v>2.4999999999999964</v>
       </c>
       <c r="D35" s="45" t="s">
         <v>278</v>
@@ -11930,8 +12065,12 @@
       <c r="AP35" s="5">
         <v>30.6</v>
       </c>
-      <c r="AQ35" s="5"/>
-      <c r="AR35" s="5"/>
+      <c r="AQ35" s="5">
+        <v>30.9</v>
+      </c>
+      <c r="AR35" s="5">
+        <v>30.05</v>
+      </c>
       <c r="AS35" s="5"/>
       <c r="AT35" s="5"/>
       <c r="AU35" s="5"/>
@@ -11952,7 +12091,7 @@
     <row r="36" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <f t="shared" si="0"/>
-        <v>83.2</v>
+        <v>81.75</v>
       </c>
       <c r="B36" s="12">
         <f t="shared" si="1"/>
@@ -11960,7 +12099,7 @@
       </c>
       <c r="C36" s="12">
         <f t="shared" si="2"/>
-        <v>7.7999999999999972</v>
+        <v>9.25</v>
       </c>
       <c r="D36" s="45" t="s">
         <v>279</v>
@@ -12037,8 +12176,12 @@
       <c r="AP36" s="5">
         <v>83.2</v>
       </c>
-      <c r="AQ36" s="5"/>
-      <c r="AR36" s="5"/>
+      <c r="AQ36" s="5">
+        <v>84.25</v>
+      </c>
+      <c r="AR36" s="5">
+        <v>81.75</v>
+      </c>
       <c r="AS36" s="5"/>
       <c r="AT36" s="5"/>
       <c r="AU36" s="5"/>
@@ -12059,7 +12202,7 @@
     <row r="37" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <f t="shared" si="0"/>
-        <v>122.05</v>
+        <v>121</v>
       </c>
       <c r="B37" s="12">
         <f t="shared" si="1"/>
@@ -12067,7 +12210,7 @@
       </c>
       <c r="C37" s="12">
         <f t="shared" si="2"/>
-        <v>12.950000000000003</v>
+        <v>14</v>
       </c>
       <c r="D37" s="45" t="s">
         <v>280</v>
@@ -12144,8 +12287,12 @@
       <c r="AP37" s="5">
         <v>128.9</v>
       </c>
-      <c r="AQ37" s="5"/>
-      <c r="AR37" s="5"/>
+      <c r="AQ37" s="5">
+        <v>126.9</v>
+      </c>
+      <c r="AR37" s="5">
+        <v>121</v>
+      </c>
       <c r="AS37" s="5"/>
       <c r="AT37" s="5"/>
       <c r="AU37" s="5"/>
@@ -12251,8 +12398,12 @@
       <c r="AP38" s="5">
         <v>142.65</v>
       </c>
-      <c r="AQ38" s="5"/>
-      <c r="AR38" s="5"/>
+      <c r="AQ38" s="5">
+        <v>143.94999999999999</v>
+      </c>
+      <c r="AR38" s="5">
+        <v>138.30000000000001</v>
+      </c>
       <c r="AS38" s="5"/>
       <c r="AT38" s="5"/>
       <c r="AU38" s="5"/>
@@ -12273,7 +12424,7 @@
     <row r="39" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <f t="shared" si="0"/>
-        <v>146</v>
+        <v>144.5</v>
       </c>
       <c r="B39" s="12">
         <f t="shared" si="3"/>
@@ -12281,7 +12432,7 @@
       </c>
       <c r="C39" s="12">
         <f t="shared" si="2"/>
-        <v>8.4499999999999886</v>
+        <v>9.9499999999999886</v>
       </c>
       <c r="D39" s="45" t="s">
         <v>282</v>
@@ -12358,8 +12509,12 @@
       <c r="AP39" s="5">
         <v>147.30000000000001</v>
       </c>
-      <c r="AQ39" s="5"/>
-      <c r="AR39" s="5"/>
+      <c r="AQ39" s="5">
+        <v>148.5</v>
+      </c>
+      <c r="AR39" s="5">
+        <v>144.5</v>
+      </c>
       <c r="AS39" s="5"/>
       <c r="AT39" s="5"/>
       <c r="AU39" s="5"/>
@@ -12380,7 +12535,7 @@
     <row r="40" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <f t="shared" si="0"/>
-        <v>101.7</v>
+        <v>101.6</v>
       </c>
       <c r="B40" s="12">
         <f t="shared" si="3"/>
@@ -12388,7 +12543,7 @@
       </c>
       <c r="C40" s="12">
         <f t="shared" si="2"/>
-        <v>15.450000000000003</v>
+        <v>15.550000000000011</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>293</v>
@@ -12453,8 +12608,12 @@
       <c r="AP40" s="5">
         <v>104</v>
       </c>
-      <c r="AQ40" s="5"/>
-      <c r="AR40" s="5"/>
+      <c r="AQ40" s="5">
+        <v>105.85</v>
+      </c>
+      <c r="AR40" s="5">
+        <v>101.6</v>
+      </c>
       <c r="AS40" s="5"/>
       <c r="AT40" s="5"/>
       <c r="AU40" s="5"/>
@@ -12536,8 +12695,12 @@
       <c r="AP41" s="5">
         <v>57.9</v>
       </c>
-      <c r="AQ41" s="5"/>
-      <c r="AR41" s="5"/>
+      <c r="AQ41" s="5">
+        <v>61.35</v>
+      </c>
+      <c r="AR41" s="5">
+        <v>57.95</v>
+      </c>
       <c r="AS41" s="5"/>
       <c r="AT41" s="5"/>
       <c r="AU41" s="5"/>
@@ -12558,7 +12721,7 @@
     <row r="42" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <f t="shared" ref="A42" si="5">MIN(E42:ZZ42)</f>
-        <v>193</v>
+        <v>176.7</v>
       </c>
       <c r="B42" s="12">
         <f t="shared" ref="B42" si="6">MAX(E42:ZZ42)</f>
@@ -12566,7 +12729,7 @@
       </c>
       <c r="C42" s="12">
         <f t="shared" ref="C42" si="7">B42-A42</f>
-        <v>9.3000000000000114</v>
+        <v>25.600000000000023</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>308</v>
@@ -12613,8 +12776,12 @@
       <c r="AP42" s="5">
         <v>193</v>
       </c>
-      <c r="AQ42" s="5"/>
-      <c r="AR42" s="5"/>
+      <c r="AQ42" s="5">
+        <v>183.35</v>
+      </c>
+      <c r="AR42" s="5">
+        <v>176.7</v>
+      </c>
       <c r="AS42" s="5"/>
       <c r="AT42" s="5"/>
       <c r="AU42" s="5"/>
@@ -12631,6 +12798,81 @@
       <c r="BF42" s="5"/>
       <c r="BG42" s="5"/>
       <c r="BH42" s="5"/>
+    </row>
+    <row r="43" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A43" s="12">
+        <f t="shared" ref="A43" si="8">MIN(E43:ZZ43)</f>
+        <v>680.1</v>
+      </c>
+      <c r="B43" s="12">
+        <f t="shared" ref="B43" si="9">MAX(E43:ZZ43)</f>
+        <v>680.1</v>
+      </c>
+      <c r="C43" s="12">
+        <f t="shared" ref="C43" si="10">B43-A43</f>
+        <v>0</v>
+      </c>
+      <c r="D43" s="45" t="s">
+        <v>309</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="5"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="5"/>
+      <c r="U43" s="5"/>
+      <c r="V43" s="5"/>
+      <c r="W43" s="5"/>
+      <c r="X43" s="5"/>
+      <c r="Y43" s="5"/>
+      <c r="Z43" s="5"/>
+      <c r="AA43" s="5"/>
+      <c r="AB43" s="5"/>
+      <c r="AC43" s="5"/>
+      <c r="AD43" s="5"/>
+      <c r="AE43" s="5"/>
+      <c r="AF43" s="5"/>
+      <c r="AG43" s="5"/>
+      <c r="AH43" s="5"/>
+      <c r="AI43" s="5"/>
+      <c r="AJ43" s="5"/>
+      <c r="AK43" s="5"/>
+      <c r="AL43" s="5"/>
+      <c r="AM43" s="5"/>
+      <c r="AN43" s="5"/>
+      <c r="AO43" s="5"/>
+      <c r="AP43" s="5"/>
+      <c r="AQ43" s="5"/>
+      <c r="AR43" s="5">
+        <v>680.1</v>
+      </c>
+      <c r="AS43" s="5"/>
+      <c r="AT43" s="5"/>
+      <c r="AU43" s="5"/>
+      <c r="AV43" s="5"/>
+      <c r="AW43" s="5"/>
+      <c r="AX43" s="5"/>
+      <c r="AY43" s="5"/>
+      <c r="AZ43" s="5"/>
+      <c r="BA43" s="5"/>
+      <c r="BB43" s="5"/>
+      <c r="BC43" s="5"/>
+      <c r="BD43" s="5"/>
+      <c r="BE43" s="5"/>
+      <c r="BF43" s="5"/>
+      <c r="BG43" s="5"/>
+      <c r="BH43" s="5"/>
     </row>
   </sheetData>
   <sortState ref="L1:L37">

</xml_diff>

<commit_message>
Added share price on 03/10/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13530" windowHeight="8175"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13530" windowHeight="8175" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PaidTillDate" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="312">
   <si>
     <t>Date</t>
   </si>
@@ -958,6 +958,9 @@
   </si>
   <si>
     <t>Wires</t>
+  </si>
+  <si>
+    <t>Electrician</t>
   </si>
 </sst>
 </file>
@@ -1490,7 +1493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -7178,9 +7181,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BH43"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="AL1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AS2" sqref="AS2:AS43"/>
+      <selection pane="topRight" activeCell="AU33" sqref="AU33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7532,7 +7535,9 @@
         <v>252.95</v>
       </c>
       <c r="AT2" s="5"/>
-      <c r="AU2" s="5"/>
+      <c r="AU2" s="5">
+        <v>251.35</v>
+      </c>
       <c r="AV2" s="5"/>
       <c r="AW2" s="5"/>
       <c r="AX2" s="5"/>
@@ -7681,7 +7686,9 @@
         <v>276</v>
       </c>
       <c r="AT3" s="5"/>
-      <c r="AU3" s="5"/>
+      <c r="AU3" s="5">
+        <v>277.35000000000002</v>
+      </c>
       <c r="AV3" s="5"/>
       <c r="AW3" s="5"/>
       <c r="AX3" s="5"/>
@@ -7836,7 +7843,9 @@
         <v>260.3</v>
       </c>
       <c r="AT4" s="5"/>
-      <c r="AU4" s="5"/>
+      <c r="AU4" s="5">
+        <v>261.95</v>
+      </c>
       <c r="AV4" s="5"/>
       <c r="AW4" s="5"/>
       <c r="AX4" s="5"/>
@@ -7991,7 +8000,9 @@
         <v>786.25</v>
       </c>
       <c r="AT5" s="5"/>
-      <c r="AU5" s="5"/>
+      <c r="AU5" s="5">
+        <v>797.75</v>
+      </c>
       <c r="AV5" s="5"/>
       <c r="AW5" s="5"/>
       <c r="AX5" s="5"/>
@@ -8013,11 +8024,11 @@
       </c>
       <c r="B6" s="12">
         <f t="shared" si="1"/>
-        <v>266.35000000000002</v>
+        <v>269.5</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="2"/>
-        <v>29.900000000000034</v>
+        <v>33.050000000000011</v>
       </c>
       <c r="D6" s="45" t="s">
         <v>16</v>
@@ -8146,7 +8157,9 @@
         <v>266.35000000000002</v>
       </c>
       <c r="AT6" s="5"/>
-      <c r="AU6" s="5"/>
+      <c r="AU6" s="5">
+        <v>269.5</v>
+      </c>
       <c r="AV6" s="5"/>
       <c r="AW6" s="5"/>
       <c r="AX6" s="5"/>
@@ -8301,7 +8314,9 @@
         <v>15.9</v>
       </c>
       <c r="AT7" s="5"/>
-      <c r="AU7" s="5"/>
+      <c r="AU7" s="5">
+        <v>16.649999999999999</v>
+      </c>
       <c r="AV7" s="5"/>
       <c r="AW7" s="5"/>
       <c r="AX7" s="5"/>
@@ -8456,7 +8471,9 @@
         <v>53.4</v>
       </c>
       <c r="AT8" s="5"/>
-      <c r="AU8" s="5"/>
+      <c r="AU8" s="5">
+        <v>54.15</v>
+      </c>
       <c r="AV8" s="5"/>
       <c r="AW8" s="5"/>
       <c r="AX8" s="5"/>
@@ -8603,7 +8620,9 @@
         <v>56.3</v>
       </c>
       <c r="AT9" s="28"/>
-      <c r="AU9" s="28"/>
+      <c r="AU9" s="28">
+        <v>56.6</v>
+      </c>
       <c r="AV9" s="28"/>
       <c r="AW9" s="28"/>
       <c r="AX9" s="28"/>
@@ -8758,7 +8777,9 @@
         <v>41</v>
       </c>
       <c r="AT10" s="5"/>
-      <c r="AU10" s="5"/>
+      <c r="AU10" s="5">
+        <v>40.85</v>
+      </c>
       <c r="AV10" s="5"/>
       <c r="AW10" s="5"/>
       <c r="AX10" s="5"/>
@@ -8913,7 +8934,9 @@
         <v>76.400000000000006</v>
       </c>
       <c r="AT11" s="5"/>
-      <c r="AU11" s="5"/>
+      <c r="AU11" s="5">
+        <v>80</v>
+      </c>
       <c r="AV11" s="5"/>
       <c r="AW11" s="5"/>
       <c r="AX11" s="5"/>
@@ -9068,7 +9091,9 @@
         <v>75.400000000000006</v>
       </c>
       <c r="AT12" s="5"/>
-      <c r="AU12" s="5"/>
+      <c r="AU12" s="5">
+        <v>76.55</v>
+      </c>
       <c r="AV12" s="5"/>
       <c r="AW12" s="5"/>
       <c r="AX12" s="5"/>
@@ -9223,7 +9248,9 @@
         <v>82.65</v>
       </c>
       <c r="AT13" s="5"/>
-      <c r="AU13" s="5"/>
+      <c r="AU13" s="5">
+        <v>83.75</v>
+      </c>
       <c r="AV13" s="5"/>
       <c r="AW13" s="5"/>
       <c r="AX13" s="5"/>
@@ -9378,7 +9405,9 @@
         <v>44.45</v>
       </c>
       <c r="AT14" s="5"/>
-      <c r="AU14" s="5"/>
+      <c r="AU14" s="5">
+        <v>44.85</v>
+      </c>
       <c r="AV14" s="5"/>
       <c r="AW14" s="5"/>
       <c r="AX14" s="5"/>
@@ -9533,7 +9562,9 @@
         <v>30.2</v>
       </c>
       <c r="AT15" s="5"/>
-      <c r="AU15" s="5"/>
+      <c r="AU15" s="5">
+        <v>30.2</v>
+      </c>
       <c r="AV15" s="5"/>
       <c r="AW15" s="5"/>
       <c r="AX15" s="5"/>
@@ -9680,7 +9711,9 @@
         <v>26.6</v>
       </c>
       <c r="AT16" s="5"/>
-      <c r="AU16" s="5"/>
+      <c r="AU16" s="5">
+        <v>26.7</v>
+      </c>
       <c r="AV16" s="5"/>
       <c r="AW16" s="5"/>
       <c r="AX16" s="5"/>
@@ -9835,7 +9868,9 @@
         <v>648.25</v>
       </c>
       <c r="AT17" s="5"/>
-      <c r="AU17" s="5"/>
+      <c r="AU17" s="5">
+        <v>660.7</v>
+      </c>
       <c r="AV17" s="5"/>
       <c r="AW17" s="5"/>
       <c r="AX17" s="5"/>
@@ -9990,7 +10025,9 @@
         <v>450</v>
       </c>
       <c r="AT18" s="5"/>
-      <c r="AU18" s="5"/>
+      <c r="AU18" s="5">
+        <v>466.15</v>
+      </c>
       <c r="AV18" s="5"/>
       <c r="AW18" s="5"/>
       <c r="AX18" s="5"/>
@@ -10145,7 +10182,9 @@
         <v>237.6</v>
       </c>
       <c r="AT19" s="5"/>
-      <c r="AU19" s="5"/>
+      <c r="AU19" s="5">
+        <v>265.60000000000002</v>
+      </c>
       <c r="AV19" s="5"/>
       <c r="AW19" s="5"/>
       <c r="AX19" s="5"/>
@@ -10300,7 +10339,9 @@
         <v>500.6</v>
       </c>
       <c r="AT20" s="5"/>
-      <c r="AU20" s="5"/>
+      <c r="AU20" s="5">
+        <v>497.5</v>
+      </c>
       <c r="AV20" s="5"/>
       <c r="AW20" s="5"/>
       <c r="AX20" s="5"/>
@@ -10455,7 +10496,9 @@
         <v>677</v>
       </c>
       <c r="AT21" s="5"/>
-      <c r="AU21" s="5"/>
+      <c r="AU21" s="5">
+        <v>708.7</v>
+      </c>
       <c r="AV21" s="5"/>
       <c r="AW21" s="5"/>
       <c r="AX21" s="5"/>
@@ -10610,7 +10653,9 @@
         <v>378.95</v>
       </c>
       <c r="AT22" s="5"/>
-      <c r="AU22" s="5"/>
+      <c r="AU22" s="5">
+        <v>391</v>
+      </c>
       <c r="AV22" s="5"/>
       <c r="AW22" s="5"/>
       <c r="AX22" s="5"/>
@@ -10711,7 +10756,9 @@
         <v>315.2</v>
       </c>
       <c r="AT23" s="5"/>
-      <c r="AU23" s="5"/>
+      <c r="AU23" s="5">
+        <v>323.45</v>
+      </c>
       <c r="AV23" s="5"/>
       <c r="AW23" s="5"/>
       <c r="AX23" s="5"/>
@@ -10858,7 +10905,9 @@
         <v>55.8</v>
       </c>
       <c r="AT24" s="5"/>
-      <c r="AU24" s="5"/>
+      <c r="AU24" s="5">
+        <v>56.55</v>
+      </c>
       <c r="AV24" s="5"/>
       <c r="AW24" s="5"/>
       <c r="AX24" s="5"/>
@@ -11001,7 +11050,9 @@
         <v>222.85</v>
       </c>
       <c r="AT25" s="5"/>
-      <c r="AU25" s="5"/>
+      <c r="AU25" s="5">
+        <v>234.4</v>
+      </c>
       <c r="AV25" s="5"/>
       <c r="AW25" s="5"/>
       <c r="AX25" s="5"/>
@@ -11126,7 +11177,9 @@
         <v>896</v>
       </c>
       <c r="AT26" s="5"/>
-      <c r="AU26" s="5"/>
+      <c r="AU26" s="5">
+        <v>906.7</v>
+      </c>
       <c r="AV26" s="5"/>
       <c r="AW26" s="5"/>
       <c r="AX26" s="5"/>
@@ -11239,7 +11292,9 @@
         <v>90.05</v>
       </c>
       <c r="AT27" s="5"/>
-      <c r="AU27" s="5"/>
+      <c r="AU27" s="5">
+        <v>89.35</v>
+      </c>
       <c r="AV27" s="5"/>
       <c r="AW27" s="5"/>
       <c r="AX27" s="5"/>
@@ -11352,7 +11407,9 @@
         <v>41.75</v>
       </c>
       <c r="AT28" s="5"/>
-      <c r="AU28" s="5"/>
+      <c r="AU28" s="5">
+        <v>41.75</v>
+      </c>
       <c r="AV28" s="5"/>
       <c r="AW28" s="5"/>
       <c r="AX28" s="5"/>
@@ -11465,7 +11522,9 @@
         <v>52.55</v>
       </c>
       <c r="AT29" s="5"/>
-      <c r="AU29" s="5"/>
+      <c r="AU29" s="5">
+        <v>52.55</v>
+      </c>
       <c r="AV29" s="5"/>
       <c r="AW29" s="5"/>
       <c r="AX29" s="5"/>
@@ -11578,7 +11637,9 @@
         <v>111.95</v>
       </c>
       <c r="AT30" s="5"/>
-      <c r="AU30" s="5"/>
+      <c r="AU30" s="5">
+        <v>115.1</v>
+      </c>
       <c r="AV30" s="5"/>
       <c r="AW30" s="5"/>
       <c r="AX30" s="5"/>
@@ -11691,7 +11752,9 @@
         <v>162.4</v>
       </c>
       <c r="AT31" s="5"/>
-      <c r="AU31" s="5"/>
+      <c r="AU31" s="5">
+        <v>163.19999999999999</v>
+      </c>
       <c r="AV31" s="5"/>
       <c r="AW31" s="5"/>
       <c r="AX31" s="5"/>
@@ -11804,7 +11867,9 @@
         <v>69.05</v>
       </c>
       <c r="AT32" s="5"/>
-      <c r="AU32" s="5"/>
+      <c r="AU32" s="5">
+        <v>68.7</v>
+      </c>
       <c r="AV32" s="5"/>
       <c r="AW32" s="5"/>
       <c r="AX32" s="5"/>
@@ -11917,7 +11982,9 @@
         <v>42.2</v>
       </c>
       <c r="AT33" s="5"/>
-      <c r="AU33" s="5"/>
+      <c r="AU33" s="5">
+        <v>43.05</v>
+      </c>
       <c r="AV33" s="5"/>
       <c r="AW33" s="5"/>
       <c r="AX33" s="5"/>
@@ -12030,7 +12097,9 @@
         <v>62.55</v>
       </c>
       <c r="AT34" s="5"/>
-      <c r="AU34" s="5"/>
+      <c r="AU34" s="5">
+        <v>62.85</v>
+      </c>
       <c r="AV34" s="5"/>
       <c r="AW34" s="5"/>
       <c r="AX34" s="5"/>
@@ -12143,7 +12212,9 @@
         <v>29.9</v>
       </c>
       <c r="AT35" s="5"/>
-      <c r="AU35" s="5"/>
+      <c r="AU35" s="5">
+        <v>30.05</v>
+      </c>
       <c r="AV35" s="5"/>
       <c r="AW35" s="5"/>
       <c r="AX35" s="5"/>
@@ -12256,7 +12327,9 @@
         <v>81.55</v>
       </c>
       <c r="AT36" s="5"/>
-      <c r="AU36" s="5"/>
+      <c r="AU36" s="5">
+        <v>84.1</v>
+      </c>
       <c r="AV36" s="5"/>
       <c r="AW36" s="5"/>
       <c r="AX36" s="5"/>
@@ -12369,7 +12442,9 @@
         <v>122.65</v>
       </c>
       <c r="AT37" s="5"/>
-      <c r="AU37" s="5"/>
+      <c r="AU37" s="5">
+        <v>123.75</v>
+      </c>
       <c r="AV37" s="5"/>
       <c r="AW37" s="5"/>
       <c r="AX37" s="5"/>
@@ -12482,7 +12557,9 @@
         <v>138.85</v>
       </c>
       <c r="AT38" s="5"/>
-      <c r="AU38" s="5"/>
+      <c r="AU38" s="5">
+        <v>137.65</v>
+      </c>
       <c r="AV38" s="5"/>
       <c r="AW38" s="5"/>
       <c r="AX38" s="5"/>
@@ -12595,7 +12672,9 @@
         <v>147.9</v>
       </c>
       <c r="AT39" s="5"/>
-      <c r="AU39" s="5"/>
+      <c r="AU39" s="5">
+        <v>146</v>
+      </c>
       <c r="AV39" s="5"/>
       <c r="AW39" s="5"/>
       <c r="AX39" s="5"/>
@@ -12696,7 +12775,9 @@
         <v>103.05</v>
       </c>
       <c r="AT40" s="5"/>
-      <c r="AU40" s="5"/>
+      <c r="AU40" s="5">
+        <v>104.15</v>
+      </c>
       <c r="AV40" s="5"/>
       <c r="AW40" s="5"/>
       <c r="AX40" s="5"/>
@@ -12785,7 +12866,9 @@
         <v>57.85</v>
       </c>
       <c r="AT41" s="5"/>
-      <c r="AU41" s="5"/>
+      <c r="AU41" s="5">
+        <v>60.45</v>
+      </c>
       <c r="AV41" s="5"/>
       <c r="AW41" s="5"/>
       <c r="AX41" s="5"/>
@@ -12868,7 +12951,9 @@
         <v>167.9</v>
       </c>
       <c r="AT42" s="5"/>
-      <c r="AU42" s="5"/>
+      <c r="AU42" s="5">
+        <v>181.75</v>
+      </c>
       <c r="AV42" s="5"/>
       <c r="AW42" s="5"/>
       <c r="AX42" s="5"/>
@@ -12945,7 +13030,9 @@
         <v>686.3</v>
       </c>
       <c r="AT43" s="5"/>
-      <c r="AU43" s="5"/>
+      <c r="AU43" s="5">
+        <v>685</v>
+      </c>
       <c r="AV43" s="5"/>
       <c r="AW43" s="5"/>
       <c r="AX43" s="5"/>
@@ -14110,10 +14197,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14157,7 +14244,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(B2:B200)</f>
-        <v>816243</v>
+        <v>831643</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -14175,7 +14262,7 @@
       </c>
       <c r="F3" s="5">
         <f>F1-F2</f>
-        <v>659146</v>
+        <v>643746</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -14451,6 +14538,28 @@
       </c>
       <c r="C28" s="31">
         <v>43006</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="12">
+        <v>11400</v>
+      </c>
+      <c r="C29" s="31">
+        <v>43011</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="B30" s="12">
+        <v>4000</v>
+      </c>
+      <c r="C30" s="31">
+        <v>43009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added details for 05/10/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13530" windowHeight="8175" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13530" windowHeight="8175" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="PaidTillDate" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="297">
   <si>
     <t>Date</t>
   </si>
@@ -913,6 +913,9 @@
   </si>
   <si>
     <t>Bhai Clothes</t>
+  </si>
+  <si>
+    <t>Papa (Tiles + POP)</t>
   </si>
 </sst>
 </file>
@@ -7140,9 +7143,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="AV1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AV42" sqref="AV42"/>
+      <selection pane="topRight" activeCell="AW2" sqref="AW2:AW42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7501,7 +7504,7 @@
         <v>253.35</v>
       </c>
       <c r="AW2" s="5">
-        <v>251.55</v>
+        <v>252.1</v>
       </c>
       <c r="AX2" s="5"/>
       <c r="AY2" s="5"/>
@@ -7518,7 +7521,7 @@
     <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <f t="shared" si="0"/>
-        <v>272.35000000000002</v>
+        <v>272</v>
       </c>
       <c r="B3" s="12">
         <f t="shared" si="1"/>
@@ -7526,7 +7529,7 @@
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C40" si="2">B3-A3</f>
-        <v>30.349999999999966</v>
+        <v>30.699999999999989</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>114</v>
@@ -7656,7 +7659,7 @@
         <v>276</v>
       </c>
       <c r="AW3" s="5">
-        <v>272.35000000000002</v>
+        <v>272</v>
       </c>
       <c r="AX3" s="5"/>
       <c r="AY3" s="5"/>
@@ -7817,7 +7820,7 @@
         <v>267</v>
       </c>
       <c r="AW4" s="5">
-        <v>268</v>
+        <v>264.7</v>
       </c>
       <c r="AX4" s="5"/>
       <c r="AY4" s="5"/>
@@ -7978,7 +7981,7 @@
         <v>824</v>
       </c>
       <c r="AW5" s="5">
-        <v>827.5</v>
+        <v>824</v>
       </c>
       <c r="AX5" s="5"/>
       <c r="AY5" s="5"/>
@@ -7999,11 +8002,11 @@
       </c>
       <c r="B6" s="12">
         <f t="shared" si="1"/>
-        <v>272.35000000000002</v>
+        <v>273.10000000000002</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="2"/>
-        <v>35.900000000000034</v>
+        <v>36.650000000000034</v>
       </c>
       <c r="D6" s="45" t="s">
         <v>16</v>
@@ -8139,7 +8142,7 @@
         <v>270</v>
       </c>
       <c r="AW6" s="5">
-        <v>272.35000000000002</v>
+        <v>273.10000000000002</v>
       </c>
       <c r="AX6" s="5"/>
       <c r="AY6" s="5"/>
@@ -8461,7 +8464,7 @@
         <v>53.9</v>
       </c>
       <c r="AW8" s="5">
-        <v>54.1</v>
+        <v>54</v>
       </c>
       <c r="AX8" s="5"/>
       <c r="AY8" s="5"/>
@@ -8614,7 +8617,7 @@
         <v>56.05</v>
       </c>
       <c r="AW9" s="28">
-        <v>56.25</v>
+        <v>57.1</v>
       </c>
       <c r="AX9" s="28"/>
       <c r="AY9" s="28"/>
@@ -8775,7 +8778,7 @@
         <v>40.549999999999997</v>
       </c>
       <c r="AW10" s="5">
-        <v>40.6</v>
+        <v>40.65</v>
       </c>
       <c r="AX10" s="5"/>
       <c r="AY10" s="5"/>
@@ -8792,7 +8795,7 @@
     <row r="11" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <f t="shared" si="0"/>
-        <v>74.2</v>
+        <v>73.7</v>
       </c>
       <c r="B11" s="12">
         <f t="shared" si="1"/>
@@ -8800,7 +8803,7 @@
       </c>
       <c r="C11" s="12">
         <f t="shared" si="2"/>
-        <v>21.200000000000003</v>
+        <v>21.700000000000003</v>
       </c>
       <c r="D11" s="45" t="s">
         <v>17</v>
@@ -8936,7 +8939,7 @@
         <v>74.3</v>
       </c>
       <c r="AW11" s="5">
-        <v>74.2</v>
+        <v>73.7</v>
       </c>
       <c r="AX11" s="5"/>
       <c r="AY11" s="5"/>
@@ -8957,11 +8960,11 @@
       </c>
       <c r="B12" s="12">
         <f t="shared" si="1"/>
-        <v>83.8</v>
+        <v>83.75</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" si="2"/>
-        <v>1.1499999999999915</v>
+        <v>1.0999999999999943</v>
       </c>
       <c r="D12" s="45" t="s">
         <v>18</v>
@@ -9097,7 +9100,7 @@
         <v>83.2</v>
       </c>
       <c r="AW12" s="5">
-        <v>83.8</v>
+        <v>83.65</v>
       </c>
       <c r="AX12" s="5"/>
       <c r="AY12" s="5"/>
@@ -9258,7 +9261,7 @@
         <v>45.05</v>
       </c>
       <c r="AW13" s="5">
-        <v>46.35</v>
+        <v>46.75</v>
       </c>
       <c r="AX13" s="5"/>
       <c r="AY13" s="5"/>
@@ -9419,7 +9422,7 @@
         <v>30.25</v>
       </c>
       <c r="AW14" s="5">
-        <v>30.25</v>
+        <v>30.15</v>
       </c>
       <c r="AX14" s="5"/>
       <c r="AY14" s="5"/>
@@ -9572,7 +9575,7 @@
         <v>26.5</v>
       </c>
       <c r="AW15" s="5">
-        <v>26.7</v>
+        <v>26.6</v>
       </c>
       <c r="AX15" s="5"/>
       <c r="AY15" s="5"/>
@@ -9733,7 +9736,7 @@
         <v>659.7</v>
       </c>
       <c r="AW16" s="5">
-        <v>663.5</v>
+        <v>660.7</v>
       </c>
       <c r="AX16" s="5"/>
       <c r="AY16" s="5"/>
@@ -9894,7 +9897,7 @@
         <v>461.4</v>
       </c>
       <c r="AW17" s="5">
-        <v>456.6</v>
+        <v>457</v>
       </c>
       <c r="AX17" s="5"/>
       <c r="AY17" s="5"/>
@@ -10055,7 +10058,7 @@
         <v>266.7</v>
       </c>
       <c r="AW18" s="5">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="AX18" s="5"/>
       <c r="AY18" s="5"/>
@@ -10216,7 +10219,7 @@
         <v>491</v>
       </c>
       <c r="AW19" s="5">
-        <v>490.05</v>
+        <v>493.9</v>
       </c>
       <c r="AX19" s="5"/>
       <c r="AY19" s="5"/>
@@ -10377,7 +10380,7 @@
         <v>728.2</v>
       </c>
       <c r="AW20" s="5">
-        <v>747.1</v>
+        <v>744.25</v>
       </c>
       <c r="AX20" s="5"/>
       <c r="AY20" s="5"/>
@@ -10538,7 +10541,7 @@
         <v>376.7</v>
       </c>
       <c r="AW21" s="5">
-        <v>379.45</v>
+        <v>378.8</v>
       </c>
       <c r="AX21" s="5"/>
       <c r="AY21" s="5"/>
@@ -10645,7 +10648,7 @@
         <v>322.45</v>
       </c>
       <c r="AW22" s="5">
-        <v>329</v>
+        <v>328.5</v>
       </c>
       <c r="AX22" s="5"/>
       <c r="AY22" s="5"/>
@@ -10798,7 +10801,7 @@
         <v>55.35</v>
       </c>
       <c r="AW23" s="5">
-        <v>56.85</v>
+        <v>56.75</v>
       </c>
       <c r="AX23" s="5"/>
       <c r="AY23" s="5"/>
@@ -10947,7 +10950,7 @@
         <v>240.6</v>
       </c>
       <c r="AW24" s="5">
-        <v>240.35</v>
+        <v>242.45</v>
       </c>
       <c r="AX24" s="5"/>
       <c r="AY24" s="5"/>
@@ -11078,7 +11081,7 @@
         <v>901.45</v>
       </c>
       <c r="AW25" s="5">
-        <v>903.3</v>
+        <v>903</v>
       </c>
       <c r="AX25" s="5"/>
       <c r="AY25" s="5"/>
@@ -11197,7 +11200,7 @@
         <v>86.3</v>
       </c>
       <c r="AW26" s="5">
-        <v>88.9</v>
+        <v>88.25</v>
       </c>
       <c r="AX26" s="5"/>
       <c r="AY26" s="5"/>
@@ -11316,7 +11319,7 @@
         <v>41.1</v>
       </c>
       <c r="AW27" s="5">
-        <v>41.8</v>
+        <v>41.7</v>
       </c>
       <c r="AX27" s="5"/>
       <c r="AY27" s="5"/>
@@ -11333,7 +11336,7 @@
     <row r="28" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <f t="shared" si="0"/>
-        <v>52.15</v>
+        <v>52</v>
       </c>
       <c r="B28" s="12">
         <f t="shared" si="1"/>
@@ -11341,7 +11344,7 @@
       </c>
       <c r="C28" s="12">
         <f t="shared" si="2"/>
-        <v>4.8999999999999986</v>
+        <v>5.0499999999999972</v>
       </c>
       <c r="D28" s="45" t="s">
         <v>254</v>
@@ -11435,7 +11438,7 @@
         <v>52.2</v>
       </c>
       <c r="AW28" s="5">
-        <v>52.2</v>
+        <v>52</v>
       </c>
       <c r="AX28" s="5"/>
       <c r="AY28" s="5"/>
@@ -11554,7 +11557,7 @@
         <v>116.35</v>
       </c>
       <c r="AW29" s="5">
-        <v>115.5</v>
+        <v>114.75</v>
       </c>
       <c r="AX29" s="5"/>
       <c r="AY29" s="5"/>
@@ -11673,7 +11676,7 @@
         <v>165</v>
       </c>
       <c r="AW30" s="5">
-        <v>164.45</v>
+        <v>164.05</v>
       </c>
       <c r="AX30" s="5"/>
       <c r="AY30" s="5"/>
@@ -11690,7 +11693,7 @@
     <row r="31" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
-        <v>66.099999999999994</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="B31" s="12">
         <f t="shared" si="1"/>
@@ -11698,7 +11701,7 @@
       </c>
       <c r="C31" s="12">
         <f t="shared" si="2"/>
-        <v>12.75</v>
+        <v>12.949999999999989</v>
       </c>
       <c r="D31" s="45" t="s">
         <v>257</v>
@@ -11792,7 +11795,7 @@
         <v>66.45</v>
       </c>
       <c r="AW31" s="5">
-        <v>66.099999999999994</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="AX31" s="5"/>
       <c r="AY31" s="5"/>
@@ -11911,7 +11914,7 @@
         <v>46.6</v>
       </c>
       <c r="AW32" s="5">
-        <v>46.4</v>
+        <v>46</v>
       </c>
       <c r="AX32" s="5"/>
       <c r="AY32" s="5"/>
@@ -12030,7 +12033,7 @@
         <v>63.3</v>
       </c>
       <c r="AW33" s="5">
-        <v>64.349999999999994</v>
+        <v>64.3</v>
       </c>
       <c r="AX33" s="5"/>
       <c r="AY33" s="5"/>
@@ -12149,7 +12152,7 @@
         <v>29.95</v>
       </c>
       <c r="AW34" s="5">
-        <v>30.05</v>
+        <v>29.9</v>
       </c>
       <c r="AX34" s="5"/>
       <c r="AY34" s="5"/>
@@ -12268,7 +12271,7 @@
         <v>82.6</v>
       </c>
       <c r="AW35" s="5">
-        <v>83.15</v>
+        <v>82.75</v>
       </c>
       <c r="AX35" s="5"/>
       <c r="AY35" s="5"/>
@@ -12387,7 +12390,7 @@
         <v>124.2</v>
       </c>
       <c r="AW36" s="5">
-        <v>125.2</v>
+        <v>124.75</v>
       </c>
       <c r="AX36" s="5"/>
       <c r="AY36" s="5"/>
@@ -12506,7 +12509,7 @@
         <v>137.55000000000001</v>
       </c>
       <c r="AW37" s="5">
-        <v>139.80000000000001</v>
+        <v>140</v>
       </c>
       <c r="AX37" s="5"/>
       <c r="AY37" s="5"/>
@@ -12625,7 +12628,7 @@
         <v>146.94999999999999</v>
       </c>
       <c r="AW38" s="5">
-        <v>148.80000000000001</v>
+        <v>150.4</v>
       </c>
       <c r="AX38" s="5"/>
       <c r="AY38" s="5"/>
@@ -12732,7 +12735,7 @@
         <v>105.2</v>
       </c>
       <c r="AW39" s="5">
-        <v>104.7</v>
+        <v>103.7</v>
       </c>
       <c r="AX39" s="5"/>
       <c r="AY39" s="5"/>
@@ -12753,11 +12756,11 @@
       </c>
       <c r="B40" s="12">
         <f t="shared" ref="B40" si="4">MAX(E40:ZZ40)</f>
-        <v>65.150000000000006</v>
+        <v>64.849999999999994</v>
       </c>
       <c r="C40" s="12">
         <f t="shared" si="2"/>
-        <v>7.3000000000000043</v>
+        <v>6.9999999999999929</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>278</v>
@@ -12827,7 +12830,7 @@
         <v>61.4</v>
       </c>
       <c r="AW40" s="5">
-        <v>65.150000000000006</v>
+        <v>64.849999999999994</v>
       </c>
       <c r="AX40" s="5"/>
       <c r="AY40" s="5"/>
@@ -12933,7 +12936,7 @@
     <row r="42" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <f t="shared" ref="A42" si="8">MIN(E42:ZZ42)</f>
-        <v>670.25</v>
+        <v>666.1</v>
       </c>
       <c r="B42" s="12">
         <f t="shared" ref="B42" si="9">MAX(E42:ZZ42)</f>
@@ -12941,7 +12944,7 @@
       </c>
       <c r="C42" s="12">
         <f t="shared" ref="C42" si="10">B42-A42</f>
-        <v>16.049999999999955</v>
+        <v>20.199999999999932</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>291</v>
@@ -12999,7 +13002,7 @@
         <v>680.3</v>
       </c>
       <c r="AW42" s="5">
-        <v>670.25</v>
+        <v>666.1</v>
       </c>
       <c r="AX42" s="5"/>
       <c r="AY42" s="5"/>
@@ -14136,10 +14139,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14183,7 +14186,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(B2:B200)</f>
-        <v>885143</v>
+        <v>915143</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -14201,7 +14204,7 @@
       </c>
       <c r="F3" s="5">
         <f>F1-F2</f>
-        <v>590246</v>
+        <v>560246</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -14532,6 +14535,17 @@
       </c>
       <c r="C33" s="31">
         <v>43011</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="39" t="s">
+        <v>296</v>
+      </c>
+      <c r="B34" s="12">
+        <v>30000</v>
+      </c>
+      <c r="C34" s="31">
+        <v>43013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added details for 06/10/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13530" windowHeight="8175" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13530" windowHeight="8175" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PaidTillDate" sheetId="1" r:id="rId1"/>
@@ -7143,9 +7143,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH42"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="AV1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AW2" sqref="AW2:AW42"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="AU1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AX18" sqref="AX18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7506,7 +7506,9 @@
       <c r="AW2" s="5">
         <v>252.1</v>
       </c>
-      <c r="AX2" s="5"/>
+      <c r="AX2" s="5">
+        <v>257.2</v>
+      </c>
       <c r="AY2" s="5"/>
       <c r="AZ2" s="5"/>
       <c r="BA2" s="5"/>
@@ -7661,7 +7663,9 @@
       <c r="AW3" s="5">
         <v>272</v>
       </c>
-      <c r="AX3" s="5"/>
+      <c r="AX3" s="5">
+        <v>272.5</v>
+      </c>
       <c r="AY3" s="5"/>
       <c r="AZ3" s="5"/>
       <c r="BA3" s="5"/>
@@ -7822,7 +7826,9 @@
       <c r="AW4" s="5">
         <v>264.7</v>
       </c>
-      <c r="AX4" s="5"/>
+      <c r="AX4" s="5">
+        <v>266.39999999999998</v>
+      </c>
       <c r="AY4" s="5"/>
       <c r="AZ4" s="5"/>
       <c r="BA4" s="5"/>
@@ -7983,7 +7989,9 @@
       <c r="AW5" s="5">
         <v>824</v>
       </c>
-      <c r="AX5" s="5"/>
+      <c r="AX5" s="5">
+        <v>838.2</v>
+      </c>
       <c r="AY5" s="5"/>
       <c r="AZ5" s="5"/>
       <c r="BA5" s="5"/>
@@ -8002,11 +8010,11 @@
       </c>
       <c r="B6" s="12">
         <f t="shared" si="1"/>
-        <v>273.10000000000002</v>
+        <v>277.45</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="2"/>
-        <v>36.650000000000034</v>
+        <v>41</v>
       </c>
       <c r="D6" s="45" t="s">
         <v>16</v>
@@ -8144,7 +8152,9 @@
       <c r="AW6" s="5">
         <v>273.10000000000002</v>
       </c>
-      <c r="AX6" s="5"/>
+      <c r="AX6" s="5">
+        <v>277.45</v>
+      </c>
       <c r="AY6" s="5"/>
       <c r="AZ6" s="5"/>
       <c r="BA6" s="5"/>
@@ -8305,7 +8315,9 @@
       <c r="AW7" s="5">
         <v>16.3</v>
       </c>
-      <c r="AX7" s="5"/>
+      <c r="AX7" s="5">
+        <v>16.5</v>
+      </c>
       <c r="AY7" s="5"/>
       <c r="AZ7" s="5"/>
       <c r="BA7" s="5"/>
@@ -8466,7 +8478,9 @@
       <c r="AW8" s="5">
         <v>54</v>
       </c>
-      <c r="AX8" s="5"/>
+      <c r="AX8" s="5">
+        <v>56.45</v>
+      </c>
       <c r="AY8" s="5"/>
       <c r="AZ8" s="5"/>
       <c r="BA8" s="5"/>
@@ -8619,7 +8633,9 @@
       <c r="AW9" s="28">
         <v>57.1</v>
       </c>
-      <c r="AX9" s="28"/>
+      <c r="AX9" s="28">
+        <v>57.35</v>
+      </c>
       <c r="AY9" s="28"/>
       <c r="AZ9" s="28"/>
       <c r="BA9" s="28"/>
@@ -8780,7 +8796,9 @@
       <c r="AW10" s="5">
         <v>40.65</v>
       </c>
-      <c r="AX10" s="5"/>
+      <c r="AX10" s="5">
+        <v>41</v>
+      </c>
       <c r="AY10" s="5"/>
       <c r="AZ10" s="5"/>
       <c r="BA10" s="5"/>
@@ -8941,7 +8959,9 @@
       <c r="AW11" s="5">
         <v>73.7</v>
       </c>
-      <c r="AX11" s="5"/>
+      <c r="AX11" s="5">
+        <v>73.900000000000006</v>
+      </c>
       <c r="AY11" s="5"/>
       <c r="AZ11" s="5"/>
       <c r="BA11" s="5"/>
@@ -8960,11 +8980,11 @@
       </c>
       <c r="B12" s="12">
         <f t="shared" si="1"/>
-        <v>83.75</v>
+        <v>85.25</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" si="2"/>
-        <v>1.0999999999999943</v>
+        <v>2.5999999999999943</v>
       </c>
       <c r="D12" s="45" t="s">
         <v>18</v>
@@ -9102,7 +9122,9 @@
       <c r="AW12" s="5">
         <v>83.65</v>
       </c>
-      <c r="AX12" s="5"/>
+      <c r="AX12" s="5">
+        <v>85.25</v>
+      </c>
       <c r="AY12" s="5"/>
       <c r="AZ12" s="5"/>
       <c r="BA12" s="5"/>
@@ -9263,7 +9285,9 @@
       <c r="AW13" s="5">
         <v>46.75</v>
       </c>
-      <c r="AX13" s="5"/>
+      <c r="AX13" s="5">
+        <v>46.4</v>
+      </c>
       <c r="AY13" s="5"/>
       <c r="AZ13" s="5"/>
       <c r="BA13" s="5"/>
@@ -9424,7 +9448,9 @@
       <c r="AW14" s="5">
         <v>30.15</v>
       </c>
-      <c r="AX14" s="5"/>
+      <c r="AX14" s="5">
+        <v>30.05</v>
+      </c>
       <c r="AY14" s="5"/>
       <c r="AZ14" s="5"/>
       <c r="BA14" s="5"/>
@@ -9577,7 +9603,9 @@
       <c r="AW15" s="5">
         <v>26.6</v>
       </c>
-      <c r="AX15" s="5"/>
+      <c r="AX15" s="5">
+        <v>28.9</v>
+      </c>
       <c r="AY15" s="5"/>
       <c r="AZ15" s="5"/>
       <c r="BA15" s="5"/>
@@ -9596,11 +9624,11 @@
       </c>
       <c r="B16" s="12">
         <f t="shared" si="1"/>
-        <v>687.45</v>
+        <v>693.55</v>
       </c>
       <c r="C16" s="12">
         <f t="shared" si="2"/>
-        <v>135.45000000000005</v>
+        <v>141.54999999999995</v>
       </c>
       <c r="D16" s="45" t="s">
         <v>23</v>
@@ -9738,7 +9766,9 @@
       <c r="AW16" s="5">
         <v>660.7</v>
       </c>
-      <c r="AX16" s="5"/>
+      <c r="AX16" s="5">
+        <v>693.55</v>
+      </c>
       <c r="AY16" s="5"/>
       <c r="AZ16" s="5"/>
       <c r="BA16" s="5"/>
@@ -9899,7 +9929,9 @@
       <c r="AW17" s="5">
         <v>457</v>
       </c>
-      <c r="AX17" s="5"/>
+      <c r="AX17" s="5">
+        <v>476</v>
+      </c>
       <c r="AY17" s="5"/>
       <c r="AZ17" s="5"/>
       <c r="BA17" s="5"/>
@@ -10060,7 +10092,9 @@
       <c r="AW18" s="5">
         <v>264</v>
       </c>
-      <c r="AX18" s="5"/>
+      <c r="AX18" s="5">
+        <v>265</v>
+      </c>
       <c r="AY18" s="5"/>
       <c r="AZ18" s="5"/>
       <c r="BA18" s="5"/>
@@ -10221,7 +10255,9 @@
       <c r="AW19" s="5">
         <v>493.9</v>
       </c>
-      <c r="AX19" s="5"/>
+      <c r="AX19" s="5">
+        <v>487.5</v>
+      </c>
       <c r="AY19" s="5"/>
       <c r="AZ19" s="5"/>
       <c r="BA19" s="5"/>
@@ -10382,7 +10418,9 @@
       <c r="AW20" s="5">
         <v>744.25</v>
       </c>
-      <c r="AX20" s="5"/>
+      <c r="AX20" s="5">
+        <v>745.55</v>
+      </c>
       <c r="AY20" s="5"/>
       <c r="AZ20" s="5"/>
       <c r="BA20" s="5"/>
@@ -10543,7 +10581,9 @@
       <c r="AW21" s="5">
         <v>378.8</v>
       </c>
-      <c r="AX21" s="5"/>
+      <c r="AX21" s="5">
+        <v>383.5</v>
+      </c>
       <c r="AY21" s="5"/>
       <c r="AZ21" s="5"/>
       <c r="BA21" s="5"/>
@@ -10650,7 +10690,9 @@
       <c r="AW22" s="5">
         <v>328.5</v>
       </c>
-      <c r="AX22" s="5"/>
+      <c r="AX22" s="5">
+        <v>333.9</v>
+      </c>
       <c r="AY22" s="5"/>
       <c r="AZ22" s="5"/>
       <c r="BA22" s="5"/>
@@ -10803,7 +10845,9 @@
       <c r="AW23" s="5">
         <v>56.75</v>
       </c>
-      <c r="AX23" s="5"/>
+      <c r="AX23" s="5">
+        <v>56.6</v>
+      </c>
       <c r="AY23" s="5"/>
       <c r="AZ23" s="5"/>
       <c r="BA23" s="5"/>
@@ -10952,7 +10996,9 @@
       <c r="AW24" s="5">
         <v>242.45</v>
       </c>
-      <c r="AX24" s="5"/>
+      <c r="AX24" s="5">
+        <v>238.7</v>
+      </c>
       <c r="AY24" s="5"/>
       <c r="AZ24" s="5"/>
       <c r="BA24" s="5"/>
@@ -11083,7 +11129,9 @@
       <c r="AW25" s="5">
         <v>903</v>
       </c>
-      <c r="AX25" s="5"/>
+      <c r="AX25" s="5">
+        <v>920.5</v>
+      </c>
       <c r="AY25" s="5"/>
       <c r="AZ25" s="5"/>
       <c r="BA25" s="5"/>
@@ -11202,7 +11250,9 @@
       <c r="AW26" s="5">
         <v>88.25</v>
       </c>
-      <c r="AX26" s="5"/>
+      <c r="AX26" s="5">
+        <v>86.2</v>
+      </c>
       <c r="AY26" s="5"/>
       <c r="AZ26" s="5"/>
       <c r="BA26" s="5"/>
@@ -11321,7 +11371,9 @@
       <c r="AW27" s="5">
         <v>41.7</v>
       </c>
-      <c r="AX27" s="5"/>
+      <c r="AX27" s="5">
+        <v>42.25</v>
+      </c>
       <c r="AY27" s="5"/>
       <c r="AZ27" s="5"/>
       <c r="BA27" s="5"/>
@@ -11440,7 +11492,9 @@
       <c r="AW28" s="5">
         <v>52</v>
       </c>
-      <c r="AX28" s="5"/>
+      <c r="AX28" s="5">
+        <v>53.55</v>
+      </c>
       <c r="AY28" s="5"/>
       <c r="AZ28" s="5"/>
       <c r="BA28" s="5"/>
@@ -11559,7 +11613,9 @@
       <c r="AW29" s="5">
         <v>114.75</v>
       </c>
-      <c r="AX29" s="5"/>
+      <c r="AX29" s="5">
+        <v>121.7</v>
+      </c>
       <c r="AY29" s="5"/>
       <c r="AZ29" s="5"/>
       <c r="BA29" s="5"/>
@@ -11678,7 +11734,9 @@
       <c r="AW30" s="5">
         <v>164.05</v>
       </c>
-      <c r="AX30" s="5"/>
+      <c r="AX30" s="5">
+        <v>166.3</v>
+      </c>
       <c r="AY30" s="5"/>
       <c r="AZ30" s="5"/>
       <c r="BA30" s="5"/>
@@ -11797,7 +11855,9 @@
       <c r="AW31" s="5">
         <v>65.900000000000006</v>
       </c>
-      <c r="AX31" s="5"/>
+      <c r="AX31" s="5">
+        <v>70.349999999999994</v>
+      </c>
       <c r="AY31" s="5"/>
       <c r="AZ31" s="5"/>
       <c r="BA31" s="5"/>
@@ -11816,11 +11876,11 @@
       </c>
       <c r="B32" s="12">
         <f t="shared" si="1"/>
-        <v>47.5</v>
+        <v>47.9</v>
       </c>
       <c r="C32" s="12">
         <f t="shared" si="2"/>
-        <v>8.25</v>
+        <v>8.6499999999999986</v>
       </c>
       <c r="D32" s="45" t="s">
         <v>258</v>
@@ -11916,7 +11976,9 @@
       <c r="AW32" s="5">
         <v>46</v>
       </c>
-      <c r="AX32" s="5"/>
+      <c r="AX32" s="5">
+        <v>47.9</v>
+      </c>
       <c r="AY32" s="5"/>
       <c r="AZ32" s="5"/>
       <c r="BA32" s="5"/>
@@ -12035,7 +12097,9 @@
       <c r="AW33" s="5">
         <v>64.3</v>
       </c>
-      <c r="AX33" s="5"/>
+      <c r="AX33" s="5">
+        <v>65.05</v>
+      </c>
       <c r="AY33" s="5"/>
       <c r="AZ33" s="5"/>
       <c r="BA33" s="5"/>
@@ -12154,7 +12218,9 @@
       <c r="AW34" s="5">
         <v>29.9</v>
       </c>
-      <c r="AX34" s="5"/>
+      <c r="AX34" s="5">
+        <v>30.2</v>
+      </c>
       <c r="AY34" s="5"/>
       <c r="AZ34" s="5"/>
       <c r="BA34" s="5"/>
@@ -12273,7 +12339,9 @@
       <c r="AW35" s="5">
         <v>82.75</v>
       </c>
-      <c r="AX35" s="5"/>
+      <c r="AX35" s="5">
+        <v>85.85</v>
+      </c>
       <c r="AY35" s="5"/>
       <c r="AZ35" s="5"/>
       <c r="BA35" s="5"/>
@@ -12392,7 +12460,9 @@
       <c r="AW36" s="5">
         <v>124.75</v>
       </c>
-      <c r="AX36" s="5"/>
+      <c r="AX36" s="5">
+        <v>125.25</v>
+      </c>
       <c r="AY36" s="5"/>
       <c r="AZ36" s="5"/>
       <c r="BA36" s="5"/>
@@ -12511,7 +12581,9 @@
       <c r="AW37" s="5">
         <v>140</v>
       </c>
-      <c r="AX37" s="5"/>
+      <c r="AX37" s="5">
+        <v>141.5</v>
+      </c>
       <c r="AY37" s="5"/>
       <c r="AZ37" s="5"/>
       <c r="BA37" s="5"/>
@@ -12530,11 +12602,11 @@
       </c>
       <c r="B38" s="12">
         <f t="shared" si="3"/>
-        <v>154.44999999999999</v>
+        <v>156.85</v>
       </c>
       <c r="C38" s="12">
         <f t="shared" si="2"/>
-        <v>9.9499999999999886</v>
+        <v>12.349999999999994</v>
       </c>
       <c r="D38" s="45" t="s">
         <v>264</v>
@@ -12630,7 +12702,9 @@
       <c r="AW38" s="5">
         <v>150.4</v>
       </c>
-      <c r="AX38" s="5"/>
+      <c r="AX38" s="5">
+        <v>156.85</v>
+      </c>
       <c r="AY38" s="5"/>
       <c r="AZ38" s="5"/>
       <c r="BA38" s="5"/>
@@ -12737,7 +12811,9 @@
       <c r="AW39" s="5">
         <v>103.7</v>
       </c>
-      <c r="AX39" s="5"/>
+      <c r="AX39" s="5">
+        <v>105.95</v>
+      </c>
       <c r="AY39" s="5"/>
       <c r="AZ39" s="5"/>
       <c r="BA39" s="5"/>
@@ -12756,11 +12832,11 @@
       </c>
       <c r="B40" s="12">
         <f t="shared" ref="B40" si="4">MAX(E40:ZZ40)</f>
-        <v>64.849999999999994</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="C40" s="12">
         <f t="shared" si="2"/>
-        <v>6.9999999999999929</v>
+        <v>8.0500000000000043</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>278</v>
@@ -12832,7 +12908,9 @@
       <c r="AW40" s="5">
         <v>64.849999999999994</v>
       </c>
-      <c r="AX40" s="5"/>
+      <c r="AX40" s="5">
+        <v>65.900000000000006</v>
+      </c>
       <c r="AY40" s="5"/>
       <c r="AZ40" s="5"/>
       <c r="BA40" s="5"/>
@@ -12851,11 +12929,11 @@
       </c>
       <c r="B41" s="12">
         <f t="shared" ref="B41" si="6">MAX(E41:ZZ41)</f>
-        <v>204</v>
+        <v>214.2</v>
       </c>
       <c r="C41" s="12">
         <f t="shared" ref="C41" si="7">B41-A41</f>
-        <v>36.099999999999994</v>
+        <v>46.299999999999983</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>290</v>
@@ -12921,7 +12999,9 @@
       <c r="AW41" s="5">
         <v>204</v>
       </c>
-      <c r="AX41" s="5"/>
+      <c r="AX41" s="5">
+        <v>214.2</v>
+      </c>
       <c r="AY41" s="5"/>
       <c r="AZ41" s="5"/>
       <c r="BA41" s="5"/>
@@ -13004,7 +13084,9 @@
       <c r="AW42" s="5">
         <v>666.1</v>
       </c>
-      <c r="AX42" s="5"/>
+      <c r="AX42" s="5">
+        <v>680</v>
+      </c>
       <c r="AY42" s="5"/>
       <c r="AZ42" s="5"/>
       <c r="BA42" s="5"/>
@@ -14141,7 +14223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A34" sqref="A34:C34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added details for 09/10/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="299">
   <si>
     <t>Date</t>
   </si>
@@ -916,6 +916,12 @@
   </si>
   <si>
     <t>Papa (Tiles + POP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sariya </t>
+  </si>
+  <si>
+    <t>Shutter</t>
   </si>
 </sst>
 </file>
@@ -7143,9 +7149,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="AU1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AX18" sqref="AX18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="AX1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AY41" sqref="AY41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7509,7 +7515,9 @@
       <c r="AX2" s="5">
         <v>257.2</v>
       </c>
-      <c r="AY2" s="5"/>
+      <c r="AY2" s="5">
+        <v>256.8</v>
+      </c>
       <c r="AZ2" s="5"/>
       <c r="BA2" s="5"/>
       <c r="BB2" s="5"/>
@@ -7523,7 +7531,7 @@
     <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <f t="shared" si="0"/>
-        <v>272</v>
+        <v>271.55</v>
       </c>
       <c r="B3" s="12">
         <f t="shared" si="1"/>
@@ -7531,7 +7539,7 @@
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C40" si="2">B3-A3</f>
-        <v>30.699999999999989</v>
+        <v>31.149999999999977</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>114</v>
@@ -7666,7 +7674,9 @@
       <c r="AX3" s="5">
         <v>272.5</v>
       </c>
-      <c r="AY3" s="5"/>
+      <c r="AY3" s="5">
+        <v>271.55</v>
+      </c>
       <c r="AZ3" s="5"/>
       <c r="BA3" s="5"/>
       <c r="BB3" s="5"/>
@@ -7829,7 +7839,9 @@
       <c r="AX4" s="5">
         <v>266.39999999999998</v>
       </c>
-      <c r="AY4" s="5"/>
+      <c r="AY4" s="5">
+        <v>268.10000000000002</v>
+      </c>
       <c r="AZ4" s="5"/>
       <c r="BA4" s="5"/>
       <c r="BB4" s="5"/>
@@ -7992,7 +8004,9 @@
       <c r="AX5" s="5">
         <v>838.2</v>
       </c>
-      <c r="AY5" s="5"/>
+      <c r="AY5" s="5">
+        <v>829.25</v>
+      </c>
       <c r="AZ5" s="5"/>
       <c r="BA5" s="5"/>
       <c r="BB5" s="5"/>
@@ -8010,11 +8024,11 @@
       </c>
       <c r="B6" s="12">
         <f t="shared" si="1"/>
-        <v>277.45</v>
+        <v>280.75</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="2"/>
-        <v>41</v>
+        <v>44.300000000000011</v>
       </c>
       <c r="D6" s="45" t="s">
         <v>16</v>
@@ -8155,7 +8169,9 @@
       <c r="AX6" s="5">
         <v>277.45</v>
       </c>
-      <c r="AY6" s="5"/>
+      <c r="AY6" s="5">
+        <v>280.75</v>
+      </c>
       <c r="AZ6" s="5"/>
       <c r="BA6" s="5"/>
       <c r="BB6" s="5"/>
@@ -8318,7 +8334,9 @@
       <c r="AX7" s="5">
         <v>16.5</v>
       </c>
-      <c r="AY7" s="5"/>
+      <c r="AY7" s="5">
+        <v>16.25</v>
+      </c>
       <c r="AZ7" s="5"/>
       <c r="BA7" s="5"/>
       <c r="BB7" s="5"/>
@@ -8481,7 +8499,9 @@
       <c r="AX8" s="5">
         <v>56.45</v>
       </c>
-      <c r="AY8" s="5"/>
+      <c r="AY8" s="5">
+        <v>56.7</v>
+      </c>
       <c r="AZ8" s="5"/>
       <c r="BA8" s="5"/>
       <c r="BB8" s="5"/>
@@ -8636,7 +8656,9 @@
       <c r="AX9" s="28">
         <v>57.35</v>
       </c>
-      <c r="AY9" s="28"/>
+      <c r="AY9" s="28">
+        <v>59.7</v>
+      </c>
       <c r="AZ9" s="28"/>
       <c r="BA9" s="28"/>
       <c r="BB9" s="28"/>
@@ -8799,7 +8821,9 @@
       <c r="AX10" s="5">
         <v>41</v>
       </c>
-      <c r="AY10" s="5"/>
+      <c r="AY10" s="5">
+        <v>41.05</v>
+      </c>
       <c r="AZ10" s="5"/>
       <c r="BA10" s="5"/>
       <c r="BB10" s="5"/>
@@ -8962,7 +8986,9 @@
       <c r="AX11" s="5">
         <v>73.900000000000006</v>
       </c>
-      <c r="AY11" s="5"/>
+      <c r="AY11" s="5">
+        <v>74.5</v>
+      </c>
       <c r="AZ11" s="5"/>
       <c r="BA11" s="5"/>
       <c r="BB11" s="5"/>
@@ -8980,11 +9006,11 @@
       </c>
       <c r="B12" s="12">
         <f t="shared" si="1"/>
-        <v>85.25</v>
+        <v>86.2</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" si="2"/>
-        <v>2.5999999999999943</v>
+        <v>3.5499999999999972</v>
       </c>
       <c r="D12" s="45" t="s">
         <v>18</v>
@@ -9125,7 +9151,9 @@
       <c r="AX12" s="5">
         <v>85.25</v>
       </c>
-      <c r="AY12" s="5"/>
+      <c r="AY12" s="5">
+        <v>86.2</v>
+      </c>
       <c r="AZ12" s="5"/>
       <c r="BA12" s="5"/>
       <c r="BB12" s="5"/>
@@ -9288,7 +9316,9 @@
       <c r="AX13" s="5">
         <v>46.4</v>
       </c>
-      <c r="AY13" s="5"/>
+      <c r="AY13" s="5">
+        <v>46.25</v>
+      </c>
       <c r="AZ13" s="5"/>
       <c r="BA13" s="5"/>
       <c r="BB13" s="5"/>
@@ -9302,7 +9332,7 @@
     <row r="14" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29.75</v>
       </c>
       <c r="B14" s="12">
         <f t="shared" si="1"/>
@@ -9310,7 +9340,7 @@
       </c>
       <c r="C14" s="12">
         <f t="shared" si="2"/>
-        <v>3.2000000000000028</v>
+        <v>3.4500000000000028</v>
       </c>
       <c r="D14" s="45" t="s">
         <v>21</v>
@@ -9451,7 +9481,9 @@
       <c r="AX14" s="5">
         <v>30.05</v>
       </c>
-      <c r="AY14" s="5"/>
+      <c r="AY14" s="5">
+        <v>29.75</v>
+      </c>
       <c r="AZ14" s="5"/>
       <c r="BA14" s="5"/>
       <c r="BB14" s="5"/>
@@ -9606,7 +9638,9 @@
       <c r="AX15" s="5">
         <v>28.9</v>
       </c>
-      <c r="AY15" s="5"/>
+      <c r="AY15" s="5">
+        <v>28.5</v>
+      </c>
       <c r="AZ15" s="5"/>
       <c r="BA15" s="5"/>
       <c r="BB15" s="5"/>
@@ -9624,11 +9658,11 @@
       </c>
       <c r="B16" s="12">
         <f t="shared" si="1"/>
-        <v>693.55</v>
+        <v>696.55</v>
       </c>
       <c r="C16" s="12">
         <f t="shared" si="2"/>
-        <v>141.54999999999995</v>
+        <v>144.54999999999995</v>
       </c>
       <c r="D16" s="45" t="s">
         <v>23</v>
@@ -9769,7 +9803,9 @@
       <c r="AX16" s="5">
         <v>693.55</v>
       </c>
-      <c r="AY16" s="5"/>
+      <c r="AY16" s="5">
+        <v>696.55</v>
+      </c>
       <c r="AZ16" s="5"/>
       <c r="BA16" s="5"/>
       <c r="BB16" s="5"/>
@@ -9932,7 +9968,9 @@
       <c r="AX17" s="5">
         <v>476</v>
       </c>
-      <c r="AY17" s="5"/>
+      <c r="AY17" s="5">
+        <v>474.5</v>
+      </c>
       <c r="AZ17" s="5"/>
       <c r="BA17" s="5"/>
       <c r="BB17" s="5"/>
@@ -10095,7 +10133,9 @@
       <c r="AX18" s="5">
         <v>265</v>
       </c>
-      <c r="AY18" s="5"/>
+      <c r="AY18" s="5">
+        <v>284</v>
+      </c>
       <c r="AZ18" s="5"/>
       <c r="BA18" s="5"/>
       <c r="BB18" s="5"/>
@@ -10258,7 +10298,9 @@
       <c r="AX19" s="5">
         <v>487.5</v>
       </c>
-      <c r="AY19" s="5"/>
+      <c r="AY19" s="5">
+        <v>494.7</v>
+      </c>
       <c r="AZ19" s="5"/>
       <c r="BA19" s="5"/>
       <c r="BB19" s="5"/>
@@ -10421,7 +10463,9 @@
       <c r="AX20" s="5">
         <v>745.55</v>
       </c>
-      <c r="AY20" s="5"/>
+      <c r="AY20" s="5">
+        <v>729.55</v>
+      </c>
       <c r="AZ20" s="5"/>
       <c r="BA20" s="5"/>
       <c r="BB20" s="5"/>
@@ -10584,7 +10628,9 @@
       <c r="AX21" s="5">
         <v>383.5</v>
       </c>
-      <c r="AY21" s="5"/>
+      <c r="AY21" s="5">
+        <v>379.8</v>
+      </c>
       <c r="AZ21" s="5"/>
       <c r="BA21" s="5"/>
       <c r="BB21" s="5"/>
@@ -10693,7 +10739,9 @@
       <c r="AX22" s="5">
         <v>333.9</v>
       </c>
-      <c r="AY22" s="5"/>
+      <c r="AY22" s="5">
+        <v>341</v>
+      </c>
       <c r="AZ22" s="5"/>
       <c r="BA22" s="5"/>
       <c r="BB22" s="5"/>
@@ -10848,7 +10896,9 @@
       <c r="AX23" s="5">
         <v>56.6</v>
       </c>
-      <c r="AY23" s="5"/>
+      <c r="AY23" s="5">
+        <v>57.35</v>
+      </c>
       <c r="AZ23" s="5"/>
       <c r="BA23" s="5"/>
       <c r="BB23" s="5"/>
@@ -10999,7 +11049,9 @@
       <c r="AX24" s="5">
         <v>238.7</v>
       </c>
-      <c r="AY24" s="5"/>
+      <c r="AY24" s="5">
+        <v>238.8</v>
+      </c>
       <c r="AZ24" s="5"/>
       <c r="BA24" s="5"/>
       <c r="BB24" s="5"/>
@@ -11132,7 +11184,9 @@
       <c r="AX25" s="5">
         <v>920.5</v>
       </c>
-      <c r="AY25" s="5"/>
+      <c r="AY25" s="5">
+        <v>924.25</v>
+      </c>
       <c r="AZ25" s="5"/>
       <c r="BA25" s="5"/>
       <c r="BB25" s="5"/>
@@ -11253,7 +11307,9 @@
       <c r="AX26" s="5">
         <v>86.2</v>
       </c>
-      <c r="AY26" s="5"/>
+      <c r="AY26" s="5">
+        <v>86.1</v>
+      </c>
       <c r="AZ26" s="5"/>
       <c r="BA26" s="5"/>
       <c r="BB26" s="5"/>
@@ -11374,7 +11430,9 @@
       <c r="AX27" s="5">
         <v>42.25</v>
       </c>
-      <c r="AY27" s="5"/>
+      <c r="AY27" s="5">
+        <v>44.35</v>
+      </c>
       <c r="AZ27" s="5"/>
       <c r="BA27" s="5"/>
       <c r="BB27" s="5"/>
@@ -11495,7 +11553,9 @@
       <c r="AX28" s="5">
         <v>53.55</v>
       </c>
-      <c r="AY28" s="5"/>
+      <c r="AY28" s="5">
+        <v>53.1</v>
+      </c>
       <c r="AZ28" s="5"/>
       <c r="BA28" s="5"/>
       <c r="BB28" s="5"/>
@@ -11616,7 +11676,9 @@
       <c r="AX29" s="5">
         <v>121.7</v>
       </c>
-      <c r="AY29" s="5"/>
+      <c r="AY29" s="5">
+        <v>125.65</v>
+      </c>
       <c r="AZ29" s="5"/>
       <c r="BA29" s="5"/>
       <c r="BB29" s="5"/>
@@ -11737,7 +11799,9 @@
       <c r="AX30" s="5">
         <v>166.3</v>
       </c>
-      <c r="AY30" s="5"/>
+      <c r="AY30" s="5">
+        <v>166.2</v>
+      </c>
       <c r="AZ30" s="5"/>
       <c r="BA30" s="5"/>
       <c r="BB30" s="5"/>
@@ -11858,7 +11922,9 @@
       <c r="AX31" s="5">
         <v>70.349999999999994</v>
       </c>
-      <c r="AY31" s="5"/>
+      <c r="AY31" s="5">
+        <v>70.900000000000006</v>
+      </c>
       <c r="AZ31" s="5"/>
       <c r="BA31" s="5"/>
       <c r="BB31" s="5"/>
@@ -11876,11 +11942,11 @@
       </c>
       <c r="B32" s="12">
         <f t="shared" si="1"/>
-        <v>47.9</v>
+        <v>48.75</v>
       </c>
       <c r="C32" s="12">
         <f t="shared" si="2"/>
-        <v>8.6499999999999986</v>
+        <v>9.5</v>
       </c>
       <c r="D32" s="45" t="s">
         <v>258</v>
@@ -11979,7 +12045,9 @@
       <c r="AX32" s="5">
         <v>47.9</v>
       </c>
-      <c r="AY32" s="5"/>
+      <c r="AY32" s="5">
+        <v>48.75</v>
+      </c>
       <c r="AZ32" s="5"/>
       <c r="BA32" s="5"/>
       <c r="BB32" s="5"/>
@@ -12100,7 +12168,9 @@
       <c r="AX33" s="5">
         <v>65.05</v>
       </c>
-      <c r="AY33" s="5"/>
+      <c r="AY33" s="5">
+        <v>65.900000000000006</v>
+      </c>
       <c r="AZ33" s="5"/>
       <c r="BA33" s="5"/>
       <c r="BB33" s="5"/>
@@ -12221,7 +12291,9 @@
       <c r="AX34" s="5">
         <v>30.2</v>
       </c>
-      <c r="AY34" s="5"/>
+      <c r="AY34" s="5">
+        <v>30.05</v>
+      </c>
       <c r="AZ34" s="5"/>
       <c r="BA34" s="5"/>
       <c r="BB34" s="5"/>
@@ -12342,7 +12414,9 @@
       <c r="AX35" s="5">
         <v>85.85</v>
       </c>
-      <c r="AY35" s="5"/>
+      <c r="AY35" s="5">
+        <v>85.7</v>
+      </c>
       <c r="AZ35" s="5"/>
       <c r="BA35" s="5"/>
       <c r="BB35" s="5"/>
@@ -12463,7 +12537,9 @@
       <c r="AX36" s="5">
         <v>125.25</v>
       </c>
-      <c r="AY36" s="5"/>
+      <c r="AY36" s="5">
+        <v>123.45</v>
+      </c>
       <c r="AZ36" s="5"/>
       <c r="BA36" s="5"/>
       <c r="BB36" s="5"/>
@@ -12584,7 +12660,9 @@
       <c r="AX37" s="5">
         <v>141.5</v>
       </c>
-      <c r="AY37" s="5"/>
+      <c r="AY37" s="5">
+        <v>141.9</v>
+      </c>
       <c r="AZ37" s="5"/>
       <c r="BA37" s="5"/>
       <c r="BB37" s="5"/>
@@ -12705,7 +12783,9 @@
       <c r="AX38" s="5">
         <v>156.85</v>
       </c>
-      <c r="AY38" s="5"/>
+      <c r="AY38" s="5">
+        <v>150.44999999999999</v>
+      </c>
       <c r="AZ38" s="5"/>
       <c r="BA38" s="5"/>
       <c r="BB38" s="5"/>
@@ -12814,7 +12894,9 @@
       <c r="AX39" s="5">
         <v>105.95</v>
       </c>
-      <c r="AY39" s="5"/>
+      <c r="AY39" s="5">
+        <v>107.8</v>
+      </c>
       <c r="AZ39" s="5"/>
       <c r="BA39" s="5"/>
       <c r="BB39" s="5"/>
@@ -12911,7 +12993,9 @@
       <c r="AX40" s="5">
         <v>65.900000000000006</v>
       </c>
-      <c r="AY40" s="5"/>
+      <c r="AY40" s="5">
+        <v>65.3</v>
+      </c>
       <c r="AZ40" s="5"/>
       <c r="BA40" s="5"/>
       <c r="BB40" s="5"/>
@@ -12929,11 +13013,11 @@
       </c>
       <c r="B41" s="12">
         <f t="shared" ref="B41" si="6">MAX(E41:ZZ41)</f>
-        <v>214.2</v>
+        <v>224.9</v>
       </c>
       <c r="C41" s="12">
         <f t="shared" ref="C41" si="7">B41-A41</f>
-        <v>46.299999999999983</v>
+        <v>57</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>290</v>
@@ -13002,7 +13086,9 @@
       <c r="AX41" s="5">
         <v>214.2</v>
       </c>
-      <c r="AY41" s="5"/>
+      <c r="AY41" s="5">
+        <v>224.9</v>
+      </c>
       <c r="AZ41" s="5"/>
       <c r="BA41" s="5"/>
       <c r="BB41" s="5"/>
@@ -13087,7 +13173,9 @@
       <c r="AX42" s="5">
         <v>680</v>
       </c>
-      <c r="AY42" s="5"/>
+      <c r="AY42" s="5">
+        <v>685</v>
+      </c>
       <c r="AZ42" s="5"/>
       <c r="BA42" s="5"/>
       <c r="BB42" s="5"/>
@@ -14221,10 +14309,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:C34"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14268,7 +14356,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(B2:B200)</f>
-        <v>915143</v>
+        <v>951943</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -14286,7 +14374,7 @@
       </c>
       <c r="F3" s="5">
         <f>F1-F2</f>
-        <v>560246</v>
+        <v>523446</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -14432,7 +14520,7 @@
         <v>42961</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>205</v>
       </c>
@@ -14443,7 +14531,7 @@
         <v>42966</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>107</v>
       </c>
@@ -14454,7 +14542,7 @@
         <v>42969</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>244</v>
       </c>
@@ -14464,8 +14552,17 @@
       <c r="C19" s="31">
         <v>42974</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I19" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="J19" s="12">
+        <v>5000</v>
+      </c>
+      <c r="K19" s="31">
+        <v>42998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>265</v>
       </c>
@@ -14475,8 +14572,17 @@
       <c r="C20" s="31">
         <v>42982</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I20" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="J20" s="12">
+        <v>7600</v>
+      </c>
+      <c r="K20" s="31">
+        <v>42999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>266</v>
       </c>
@@ -14486,8 +14592,17 @@
       <c r="C21" s="31">
         <v>42982</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I21" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="J21" s="12">
+        <v>10000</v>
+      </c>
+      <c r="K21" s="31">
+        <v>43006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>50</v>
       </c>
@@ -14497,8 +14612,17 @@
       <c r="C22" s="31">
         <v>42983</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I22" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="J22" s="12">
+        <v>2500</v>
+      </c>
+      <c r="K22" s="31">
+        <v>43006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>274</v>
       </c>
@@ -14508,8 +14632,17 @@
       <c r="C23" s="31">
         <v>42985</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I23" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="J23" s="12">
+        <v>11400</v>
+      </c>
+      <c r="K23" s="31">
+        <v>43011</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>107</v>
       </c>
@@ -14519,8 +14652,17 @@
       <c r="C24" s="31">
         <v>42987</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I24" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="J24" s="12">
+        <v>4000</v>
+      </c>
+      <c r="K24" s="31">
+        <v>43009</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>205</v>
       </c>
@@ -14530,8 +14672,17 @@
       <c r="C25" s="31">
         <v>42987</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I25" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="J25" s="12">
+        <v>50000</v>
+      </c>
+      <c r="K25" s="31">
+        <v>43010</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>107</v>
       </c>
@@ -14541,8 +14692,17 @@
       <c r="C26" s="31">
         <v>42999</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I26" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="J26" s="12">
+        <v>1000</v>
+      </c>
+      <c r="K26" s="31">
+        <v>43011</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>265</v>
       </c>
@@ -14552,8 +14712,17 @@
       <c r="C27" s="31">
         <v>43006</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I27" s="39" t="s">
+        <v>295</v>
+      </c>
+      <c r="J27" s="12">
+        <v>2500</v>
+      </c>
+      <c r="K27" s="31">
+        <v>43011</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>292</v>
       </c>
@@ -14563,8 +14732,17 @@
       <c r="C28" s="31">
         <v>43006</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I28" s="39" t="s">
+        <v>296</v>
+      </c>
+      <c r="J28" s="12">
+        <v>30000</v>
+      </c>
+      <c r="K28" s="31">
+        <v>43013</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>107</v>
       </c>
@@ -14574,8 +14752,17 @@
       <c r="C29" s="31">
         <v>43011</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I29" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="J29" s="12">
+        <v>7600</v>
+      </c>
+      <c r="K29" s="31">
+        <v>43017</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>293</v>
       </c>
@@ -14585,8 +14772,17 @@
       <c r="C30" s="31">
         <v>43009</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I30" s="39" t="s">
+        <v>297</v>
+      </c>
+      <c r="J30" s="12">
+        <v>19700</v>
+      </c>
+      <c r="K30" s="31">
+        <v>43017</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>50</v>
       </c>
@@ -14596,8 +14792,17 @@
       <c r="C31" s="31">
         <v>43010</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I31" s="39" t="s">
+        <v>274</v>
+      </c>
+      <c r="J31" s="12">
+        <v>4500</v>
+      </c>
+      <c r="K31" s="31">
+        <v>43017</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>294</v>
       </c>
@@ -14607,8 +14812,17 @@
       <c r="C32" s="31">
         <v>43011</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I32" s="39" t="s">
+        <v>298</v>
+      </c>
+      <c r="J32" s="12">
+        <v>5000</v>
+      </c>
+      <c r="K32" s="31">
+        <v>43017</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="39" t="s">
         <v>295</v>
       </c>
@@ -14618,8 +14832,11 @@
       <c r="C33" s="31">
         <v>43011</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="39" t="s">
         <v>296</v>
       </c>
@@ -14628,6 +14845,64 @@
       </c>
       <c r="C34" s="31">
         <v>43013</v>
+      </c>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="12">
+        <v>7600</v>
+      </c>
+      <c r="C35" s="31">
+        <v>43017</v>
+      </c>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="39" t="s">
+        <v>297</v>
+      </c>
+      <c r="B36" s="12">
+        <v>19700</v>
+      </c>
+      <c r="C36" s="31">
+        <v>43017</v>
+      </c>
+      <c r="I36" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="J36" s="5">
+        <f>SUM(J19:J35)</f>
+        <v>160800</v>
+      </c>
+      <c r="K36" s="5"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="39" t="s">
+        <v>274</v>
+      </c>
+      <c r="B37" s="12">
+        <v>4500</v>
+      </c>
+      <c r="C37" s="31">
+        <v>43017</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="39" t="s">
+        <v>298</v>
+      </c>
+      <c r="B38" s="12">
+        <v>5000</v>
+      </c>
+      <c r="C38" s="31">
+        <v>43017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added details for 10/10/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -7149,9 +7149,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BH42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="AX1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AY41" sqref="AY41"/>
+      <selection pane="topRight" activeCell="AZ2" sqref="AZ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7518,7 +7518,9 @@
       <c r="AY2" s="5">
         <v>256.8</v>
       </c>
-      <c r="AZ2" s="5"/>
+      <c r="AZ2" s="5">
+        <v>257</v>
+      </c>
       <c r="BA2" s="5"/>
       <c r="BB2" s="5"/>
       <c r="BC2" s="5"/>
@@ -7531,7 +7533,7 @@
     <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <f t="shared" si="0"/>
-        <v>271.55</v>
+        <v>270</v>
       </c>
       <c r="B3" s="12">
         <f t="shared" si="1"/>
@@ -7539,7 +7541,7 @@
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C40" si="2">B3-A3</f>
-        <v>31.149999999999977</v>
+        <v>32.699999999999989</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>114</v>
@@ -7677,7 +7679,9 @@
       <c r="AY3" s="5">
         <v>271.55</v>
       </c>
-      <c r="AZ3" s="5"/>
+      <c r="AZ3" s="5">
+        <v>270</v>
+      </c>
       <c r="BA3" s="5"/>
       <c r="BB3" s="5"/>
       <c r="BC3" s="5"/>
@@ -7842,7 +7846,9 @@
       <c r="AY4" s="5">
         <v>268.10000000000002</v>
       </c>
-      <c r="AZ4" s="5"/>
+      <c r="AZ4" s="5">
+        <v>265.95</v>
+      </c>
       <c r="BA4" s="5"/>
       <c r="BB4" s="5"/>
       <c r="BC4" s="5"/>
@@ -8007,7 +8013,9 @@
       <c r="AY5" s="5">
         <v>829.25</v>
       </c>
-      <c r="AZ5" s="5"/>
+      <c r="AZ5" s="5">
+        <v>842.25</v>
+      </c>
       <c r="BA5" s="5"/>
       <c r="BB5" s="5"/>
       <c r="BC5" s="5"/>
@@ -8024,11 +8032,11 @@
       </c>
       <c r="B6" s="12">
         <f t="shared" si="1"/>
-        <v>280.75</v>
+        <v>285.60000000000002</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="2"/>
-        <v>44.300000000000011</v>
+        <v>49.150000000000034</v>
       </c>
       <c r="D6" s="45" t="s">
         <v>16</v>
@@ -8172,7 +8180,9 @@
       <c r="AY6" s="5">
         <v>280.75</v>
       </c>
-      <c r="AZ6" s="5"/>
+      <c r="AZ6" s="5">
+        <v>285.60000000000002</v>
+      </c>
       <c r="BA6" s="5"/>
       <c r="BB6" s="5"/>
       <c r="BC6" s="5"/>
@@ -8337,7 +8347,9 @@
       <c r="AY7" s="5">
         <v>16.25</v>
       </c>
-      <c r="AZ7" s="5"/>
+      <c r="AZ7" s="5">
+        <v>16.5</v>
+      </c>
       <c r="BA7" s="5"/>
       <c r="BB7" s="5"/>
       <c r="BC7" s="5"/>
@@ -8502,7 +8514,9 @@
       <c r="AY8" s="5">
         <v>56.7</v>
       </c>
-      <c r="AZ8" s="5"/>
+      <c r="AZ8" s="5">
+        <v>56.8</v>
+      </c>
       <c r="BA8" s="5"/>
       <c r="BB8" s="5"/>
       <c r="BC8" s="5"/>
@@ -8659,7 +8673,9 @@
       <c r="AY9" s="28">
         <v>59.7</v>
       </c>
-      <c r="AZ9" s="28"/>
+      <c r="AZ9" s="28">
+        <v>58.95</v>
+      </c>
       <c r="BA9" s="28"/>
       <c r="BB9" s="28"/>
       <c r="BC9" s="28"/>
@@ -8824,7 +8840,9 @@
       <c r="AY10" s="5">
         <v>41.05</v>
       </c>
-      <c r="AZ10" s="5"/>
+      <c r="AZ10" s="5">
+        <v>40.9</v>
+      </c>
       <c r="BA10" s="5"/>
       <c r="BB10" s="5"/>
       <c r="BC10" s="5"/>
@@ -8837,7 +8855,7 @@
     <row r="11" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <f t="shared" si="0"/>
-        <v>73.7</v>
+        <v>73.150000000000006</v>
       </c>
       <c r="B11" s="12">
         <f t="shared" si="1"/>
@@ -8845,7 +8863,7 @@
       </c>
       <c r="C11" s="12">
         <f t="shared" si="2"/>
-        <v>21.700000000000003</v>
+        <v>22.25</v>
       </c>
       <c r="D11" s="45" t="s">
         <v>17</v>
@@ -8989,7 +9007,9 @@
       <c r="AY11" s="5">
         <v>74.5</v>
       </c>
-      <c r="AZ11" s="5"/>
+      <c r="AZ11" s="5">
+        <v>73.150000000000006</v>
+      </c>
       <c r="BA11" s="5"/>
       <c r="BB11" s="5"/>
       <c r="BC11" s="5"/>
@@ -9006,11 +9026,11 @@
       </c>
       <c r="B12" s="12">
         <f t="shared" si="1"/>
-        <v>86.2</v>
+        <v>86.65</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" si="2"/>
-        <v>3.5499999999999972</v>
+        <v>4</v>
       </c>
       <c r="D12" s="45" t="s">
         <v>18</v>
@@ -9154,7 +9174,9 @@
       <c r="AY12" s="5">
         <v>86.2</v>
       </c>
-      <c r="AZ12" s="5"/>
+      <c r="AZ12" s="5">
+        <v>86.65</v>
+      </c>
       <c r="BA12" s="5"/>
       <c r="BB12" s="5"/>
       <c r="BC12" s="5"/>
@@ -9319,7 +9341,9 @@
       <c r="AY13" s="5">
         <v>46.25</v>
       </c>
-      <c r="AZ13" s="5"/>
+      <c r="AZ13" s="5">
+        <v>47.5</v>
+      </c>
       <c r="BA13" s="5"/>
       <c r="BB13" s="5"/>
       <c r="BC13" s="5"/>
@@ -9484,7 +9508,9 @@
       <c r="AY14" s="5">
         <v>29.75</v>
       </c>
-      <c r="AZ14" s="5"/>
+      <c r="AZ14" s="5">
+        <v>30.2</v>
+      </c>
       <c r="BA14" s="5"/>
       <c r="BB14" s="5"/>
       <c r="BC14" s="5"/>
@@ -9641,7 +9667,9 @@
       <c r="AY15" s="5">
         <v>28.5</v>
       </c>
-      <c r="AZ15" s="5"/>
+      <c r="AZ15" s="5">
+        <v>27.9</v>
+      </c>
       <c r="BA15" s="5"/>
       <c r="BB15" s="5"/>
       <c r="BC15" s="5"/>
@@ -9806,7 +9834,9 @@
       <c r="AY16" s="5">
         <v>696.55</v>
       </c>
-      <c r="AZ16" s="5"/>
+      <c r="AZ16" s="5">
+        <v>691.5</v>
+      </c>
       <c r="BA16" s="5"/>
       <c r="BB16" s="5"/>
       <c r="BC16" s="5"/>
@@ -9971,7 +10001,9 @@
       <c r="AY17" s="5">
         <v>474.5</v>
       </c>
-      <c r="AZ17" s="5"/>
+      <c r="AZ17" s="5">
+        <v>472</v>
+      </c>
       <c r="BA17" s="5"/>
       <c r="BB17" s="5"/>
       <c r="BC17" s="5"/>
@@ -9988,11 +10020,11 @@
       </c>
       <c r="B18" s="12">
         <f t="shared" si="1"/>
-        <v>285.89999999999998</v>
+        <v>288.3</v>
       </c>
       <c r="C18" s="12">
         <f t="shared" si="2"/>
-        <v>107.09999999999997</v>
+        <v>109.5</v>
       </c>
       <c r="D18" s="44" t="s">
         <v>39</v>
@@ -10136,7 +10168,9 @@
       <c r="AY18" s="5">
         <v>284</v>
       </c>
-      <c r="AZ18" s="5"/>
+      <c r="AZ18" s="5">
+        <v>288.3</v>
+      </c>
       <c r="BA18" s="5"/>
       <c r="BB18" s="5"/>
       <c r="BC18" s="5"/>
@@ -10301,7 +10335,9 @@
       <c r="AY19" s="5">
         <v>494.7</v>
       </c>
-      <c r="AZ19" s="5"/>
+      <c r="AZ19" s="5">
+        <v>504.85</v>
+      </c>
       <c r="BA19" s="5"/>
       <c r="BB19" s="5"/>
       <c r="BC19" s="5"/>
@@ -10466,7 +10502,9 @@
       <c r="AY20" s="5">
         <v>729.55</v>
       </c>
-      <c r="AZ20" s="5"/>
+      <c r="AZ20" s="5">
+        <v>737</v>
+      </c>
       <c r="BA20" s="5"/>
       <c r="BB20" s="5"/>
       <c r="BC20" s="5"/>
@@ -10631,7 +10669,9 @@
       <c r="AY21" s="5">
         <v>379.8</v>
       </c>
-      <c r="AZ21" s="5"/>
+      <c r="AZ21" s="5">
+        <v>386.5</v>
+      </c>
       <c r="BA21" s="5"/>
       <c r="BB21" s="5"/>
       <c r="BC21" s="5"/>
@@ -10742,7 +10782,9 @@
       <c r="AY22" s="5">
         <v>341</v>
       </c>
-      <c r="AZ22" s="5"/>
+      <c r="AZ22" s="5">
+        <v>345</v>
+      </c>
       <c r="BA22" s="5"/>
       <c r="BB22" s="5"/>
       <c r="BC22" s="5"/>
@@ -10899,7 +10941,9 @@
       <c r="AY23" s="5">
         <v>57.35</v>
       </c>
-      <c r="AZ23" s="5"/>
+      <c r="AZ23" s="5">
+        <v>57.4</v>
+      </c>
       <c r="BA23" s="5"/>
       <c r="BB23" s="5"/>
       <c r="BC23" s="5"/>
@@ -11052,7 +11096,9 @@
       <c r="AY24" s="5">
         <v>238.8</v>
       </c>
-      <c r="AZ24" s="5"/>
+      <c r="AZ24" s="5">
+        <v>237.4</v>
+      </c>
       <c r="BA24" s="5"/>
       <c r="BB24" s="5"/>
       <c r="BC24" s="5"/>
@@ -11187,7 +11233,9 @@
       <c r="AY25" s="5">
         <v>924.25</v>
       </c>
-      <c r="AZ25" s="5"/>
+      <c r="AZ25" s="5">
+        <v>935.15</v>
+      </c>
       <c r="BA25" s="5"/>
       <c r="BB25" s="5"/>
       <c r="BC25" s="5"/>
@@ -11310,7 +11358,9 @@
       <c r="AY26" s="5">
         <v>86.1</v>
       </c>
-      <c r="AZ26" s="5"/>
+      <c r="AZ26" s="5">
+        <v>88.2</v>
+      </c>
       <c r="BA26" s="5"/>
       <c r="BB26" s="5"/>
       <c r="BC26" s="5"/>
@@ -11433,7 +11483,9 @@
       <c r="AY27" s="5">
         <v>44.35</v>
       </c>
-      <c r="AZ27" s="5"/>
+      <c r="AZ27" s="5">
+        <v>44.1</v>
+      </c>
       <c r="BA27" s="5"/>
       <c r="BB27" s="5"/>
       <c r="BC27" s="5"/>
@@ -11556,7 +11608,9 @@
       <c r="AY28" s="5">
         <v>53.1</v>
       </c>
-      <c r="AZ28" s="5"/>
+      <c r="AZ28" s="5">
+        <v>53.2</v>
+      </c>
       <c r="BA28" s="5"/>
       <c r="BB28" s="5"/>
       <c r="BC28" s="5"/>
@@ -11679,7 +11733,9 @@
       <c r="AY29" s="5">
         <v>125.65</v>
       </c>
-      <c r="AZ29" s="5"/>
+      <c r="AZ29" s="5">
+        <v>127</v>
+      </c>
       <c r="BA29" s="5"/>
       <c r="BB29" s="5"/>
       <c r="BC29" s="5"/>
@@ -11802,7 +11858,9 @@
       <c r="AY30" s="5">
         <v>166.2</v>
       </c>
-      <c r="AZ30" s="5"/>
+      <c r="AZ30" s="5">
+        <v>165.5</v>
+      </c>
       <c r="BA30" s="5"/>
       <c r="BB30" s="5"/>
       <c r="BC30" s="5"/>
@@ -11925,7 +11983,9 @@
       <c r="AY31" s="5">
         <v>70.900000000000006</v>
       </c>
-      <c r="AZ31" s="5"/>
+      <c r="AZ31" s="5">
+        <v>67.95</v>
+      </c>
       <c r="BA31" s="5"/>
       <c r="BB31" s="5"/>
       <c r="BC31" s="5"/>
@@ -12048,7 +12108,9 @@
       <c r="AY32" s="5">
         <v>48.75</v>
       </c>
-      <c r="AZ32" s="5"/>
+      <c r="AZ32" s="5">
+        <v>48.1</v>
+      </c>
       <c r="BA32" s="5"/>
       <c r="BB32" s="5"/>
       <c r="BC32" s="5"/>
@@ -12171,7 +12233,9 @@
       <c r="AY33" s="5">
         <v>65.900000000000006</v>
       </c>
-      <c r="AZ33" s="5"/>
+      <c r="AZ33" s="5">
+        <v>68.8</v>
+      </c>
       <c r="BA33" s="5"/>
       <c r="BB33" s="5"/>
       <c r="BC33" s="5"/>
@@ -12294,7 +12358,9 @@
       <c r="AY34" s="5">
         <v>30.05</v>
       </c>
-      <c r="AZ34" s="5"/>
+      <c r="AZ34" s="5">
+        <v>30</v>
+      </c>
       <c r="BA34" s="5"/>
       <c r="BB34" s="5"/>
       <c r="BC34" s="5"/>
@@ -12417,7 +12483,9 @@
       <c r="AY35" s="5">
         <v>85.7</v>
       </c>
-      <c r="AZ35" s="5"/>
+      <c r="AZ35" s="5">
+        <v>88.8</v>
+      </c>
       <c r="BA35" s="5"/>
       <c r="BB35" s="5"/>
       <c r="BC35" s="5"/>
@@ -12540,7 +12608,9 @@
       <c r="AY36" s="5">
         <v>123.45</v>
       </c>
-      <c r="AZ36" s="5"/>
+      <c r="AZ36" s="5">
+        <v>123.35</v>
+      </c>
       <c r="BA36" s="5"/>
       <c r="BB36" s="5"/>
       <c r="BC36" s="5"/>
@@ -12663,7 +12733,9 @@
       <c r="AY37" s="5">
         <v>141.9</v>
       </c>
-      <c r="AZ37" s="5"/>
+      <c r="AZ37" s="5">
+        <v>141.6</v>
+      </c>
       <c r="BA37" s="5"/>
       <c r="BB37" s="5"/>
       <c r="BC37" s="5"/>
@@ -12786,7 +12858,9 @@
       <c r="AY38" s="5">
         <v>150.44999999999999</v>
       </c>
-      <c r="AZ38" s="5"/>
+      <c r="AZ38" s="5">
+        <v>153.35</v>
+      </c>
       <c r="BA38" s="5"/>
       <c r="BB38" s="5"/>
       <c r="BC38" s="5"/>
@@ -12897,7 +12971,9 @@
       <c r="AY39" s="5">
         <v>107.8</v>
       </c>
-      <c r="AZ39" s="5"/>
+      <c r="AZ39" s="5">
+        <v>113.15</v>
+      </c>
       <c r="BA39" s="5"/>
       <c r="BB39" s="5"/>
       <c r="BC39" s="5"/>
@@ -12914,11 +12990,11 @@
       </c>
       <c r="B40" s="12">
         <f t="shared" ref="B40" si="4">MAX(E40:ZZ40)</f>
-        <v>65.900000000000006</v>
+        <v>67.099999999999994</v>
       </c>
       <c r="C40" s="12">
         <f t="shared" si="2"/>
-        <v>8.0500000000000043</v>
+        <v>9.2499999999999929</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>278</v>
@@ -12996,7 +13072,9 @@
       <c r="AY40" s="5">
         <v>65.3</v>
       </c>
-      <c r="AZ40" s="5"/>
+      <c r="AZ40" s="5">
+        <v>67.099999999999994</v>
+      </c>
       <c r="BA40" s="5"/>
       <c r="BB40" s="5"/>
       <c r="BC40" s="5"/>
@@ -13013,11 +13091,11 @@
       </c>
       <c r="B41" s="12">
         <f t="shared" ref="B41" si="6">MAX(E41:ZZ41)</f>
-        <v>224.9</v>
+        <v>236.1</v>
       </c>
       <c r="C41" s="12">
         <f t="shared" ref="C41" si="7">B41-A41</f>
-        <v>57</v>
+        <v>68.199999999999989</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>290</v>
@@ -13089,7 +13167,9 @@
       <c r="AY41" s="5">
         <v>224.9</v>
       </c>
-      <c r="AZ41" s="5"/>
+      <c r="AZ41" s="5">
+        <v>236.1</v>
+      </c>
       <c r="BA41" s="5"/>
       <c r="BB41" s="5"/>
       <c r="BC41" s="5"/>
@@ -13106,11 +13186,11 @@
       </c>
       <c r="B42" s="12">
         <f t="shared" ref="B42" si="9">MAX(E42:ZZ42)</f>
-        <v>686.3</v>
+        <v>687</v>
       </c>
       <c r="C42" s="12">
         <f t="shared" ref="C42" si="10">B42-A42</f>
-        <v>20.199999999999932</v>
+        <v>20.899999999999977</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>291</v>
@@ -13176,7 +13256,9 @@
       <c r="AY42" s="5">
         <v>685</v>
       </c>
-      <c r="AZ42" s="5"/>
+      <c r="AZ42" s="5">
+        <v>687</v>
+      </c>
       <c r="BA42" s="5"/>
       <c r="BB42" s="5"/>
       <c r="BC42" s="5"/>

</xml_diff>

<commit_message>
Added details for 11/10/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="300">
   <si>
     <t>Date</t>
   </si>
@@ -922,6 +922,9 @@
   </si>
   <si>
     <t>Shutter</t>
+  </si>
+  <si>
+    <t>POP Inder Bhai</t>
   </si>
 </sst>
 </file>
@@ -7151,7 +7154,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="AX1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AZ2" sqref="AZ2"/>
+      <selection pane="topRight" activeCell="BA2" sqref="BA2:BA42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7521,7 +7524,9 @@
       <c r="AZ2" s="5">
         <v>257</v>
       </c>
-      <c r="BA2" s="5"/>
+      <c r="BA2" s="5">
+        <v>251.2</v>
+      </c>
       <c r="BB2" s="5"/>
       <c r="BC2" s="5"/>
       <c r="BD2" s="5"/>
@@ -7533,7 +7538,7 @@
     <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <f t="shared" si="0"/>
-        <v>270</v>
+        <v>267.10000000000002</v>
       </c>
       <c r="B3" s="12">
         <f t="shared" si="1"/>
@@ -7541,7 +7546,7 @@
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C40" si="2">B3-A3</f>
-        <v>32.699999999999989</v>
+        <v>35.599999999999966</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>114</v>
@@ -7682,7 +7687,9 @@
       <c r="AZ3" s="5">
         <v>270</v>
       </c>
-      <c r="BA3" s="5"/>
+      <c r="BA3" s="5">
+        <v>267.10000000000002</v>
+      </c>
       <c r="BB3" s="5"/>
       <c r="BC3" s="5"/>
       <c r="BD3" s="5"/>
@@ -7849,7 +7856,9 @@
       <c r="AZ4" s="5">
         <v>265.95</v>
       </c>
-      <c r="BA4" s="5"/>
+      <c r="BA4" s="5">
+        <v>265.05</v>
+      </c>
       <c r="BB4" s="5"/>
       <c r="BC4" s="5"/>
       <c r="BD4" s="5"/>
@@ -8016,7 +8025,9 @@
       <c r="AZ5" s="5">
         <v>842.25</v>
       </c>
-      <c r="BA5" s="5"/>
+      <c r="BA5" s="5">
+        <v>839</v>
+      </c>
       <c r="BB5" s="5"/>
       <c r="BC5" s="5"/>
       <c r="BD5" s="5"/>
@@ -8183,7 +8194,9 @@
       <c r="AZ6" s="5">
         <v>285.60000000000002</v>
       </c>
-      <c r="BA6" s="5"/>
+      <c r="BA6" s="5">
+        <v>281</v>
+      </c>
       <c r="BB6" s="5"/>
       <c r="BC6" s="5"/>
       <c r="BD6" s="5"/>
@@ -8350,7 +8363,9 @@
       <c r="AZ7" s="5">
         <v>16.5</v>
       </c>
-      <c r="BA7" s="5"/>
+      <c r="BA7" s="5">
+        <v>15.65</v>
+      </c>
       <c r="BB7" s="5"/>
       <c r="BC7" s="5"/>
       <c r="BD7" s="5"/>
@@ -8517,7 +8532,9 @@
       <c r="AZ8" s="5">
         <v>56.8</v>
       </c>
-      <c r="BA8" s="5"/>
+      <c r="BA8" s="5">
+        <v>54.75</v>
+      </c>
       <c r="BB8" s="5"/>
       <c r="BC8" s="5"/>
       <c r="BD8" s="5"/>
@@ -8676,7 +8693,9 @@
       <c r="AZ9" s="28">
         <v>58.95</v>
       </c>
-      <c r="BA9" s="28"/>
+      <c r="BA9" s="28">
+        <v>57.6</v>
+      </c>
       <c r="BB9" s="28"/>
       <c r="BC9" s="28"/>
       <c r="BD9" s="28"/>
@@ -8843,7 +8862,9 @@
       <c r="AZ10" s="5">
         <v>40.9</v>
       </c>
-      <c r="BA10" s="5"/>
+      <c r="BA10" s="5">
+        <v>40</v>
+      </c>
       <c r="BB10" s="5"/>
       <c r="BC10" s="5"/>
       <c r="BD10" s="5"/>
@@ -8855,7 +8876,7 @@
     <row r="11" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <f t="shared" si="0"/>
-        <v>73.150000000000006</v>
+        <v>72.650000000000006</v>
       </c>
       <c r="B11" s="12">
         <f t="shared" si="1"/>
@@ -8863,7 +8884,7 @@
       </c>
       <c r="C11" s="12">
         <f t="shared" si="2"/>
-        <v>22.25</v>
+        <v>22.75</v>
       </c>
       <c r="D11" s="45" t="s">
         <v>17</v>
@@ -9010,7 +9031,9 @@
       <c r="AZ11" s="5">
         <v>73.150000000000006</v>
       </c>
-      <c r="BA11" s="5"/>
+      <c r="BA11" s="5">
+        <v>72.650000000000006</v>
+      </c>
       <c r="BB11" s="5"/>
       <c r="BC11" s="5"/>
       <c r="BD11" s="5"/>
@@ -9177,7 +9200,9 @@
       <c r="AZ12" s="5">
         <v>86.65</v>
       </c>
-      <c r="BA12" s="5"/>
+      <c r="BA12" s="5">
+        <v>85</v>
+      </c>
       <c r="BB12" s="5"/>
       <c r="BC12" s="5"/>
       <c r="BD12" s="5"/>
@@ -9344,7 +9369,9 @@
       <c r="AZ13" s="5">
         <v>47.5</v>
       </c>
-      <c r="BA13" s="5"/>
+      <c r="BA13" s="5">
+        <v>47.5</v>
+      </c>
       <c r="BB13" s="5"/>
       <c r="BC13" s="5"/>
       <c r="BD13" s="5"/>
@@ -9511,7 +9538,9 @@
       <c r="AZ14" s="5">
         <v>30.2</v>
       </c>
-      <c r="BA14" s="5"/>
+      <c r="BA14" s="5">
+        <v>30.25</v>
+      </c>
       <c r="BB14" s="5"/>
       <c r="BC14" s="5"/>
       <c r="BD14" s="5"/>
@@ -9670,7 +9699,9 @@
       <c r="AZ15" s="5">
         <v>27.9</v>
       </c>
-      <c r="BA15" s="5"/>
+      <c r="BA15" s="5">
+        <v>27.05</v>
+      </c>
       <c r="BB15" s="5"/>
       <c r="BC15" s="5"/>
       <c r="BD15" s="5"/>
@@ -9837,7 +9868,9 @@
       <c r="AZ16" s="5">
         <v>691.5</v>
       </c>
-      <c r="BA16" s="5"/>
+      <c r="BA16" s="5">
+        <v>682.5</v>
+      </c>
       <c r="BB16" s="5"/>
       <c r="BC16" s="5"/>
       <c r="BD16" s="5"/>
@@ -10004,7 +10037,9 @@
       <c r="AZ17" s="5">
         <v>472</v>
       </c>
-      <c r="BA17" s="5"/>
+      <c r="BA17" s="5">
+        <v>465.55</v>
+      </c>
       <c r="BB17" s="5"/>
       <c r="BC17" s="5"/>
       <c r="BD17" s="5"/>
@@ -10171,7 +10206,9 @@
       <c r="AZ18" s="5">
         <v>288.3</v>
       </c>
-      <c r="BA18" s="5"/>
+      <c r="BA18" s="5">
+        <v>285</v>
+      </c>
       <c r="BB18" s="5"/>
       <c r="BC18" s="5"/>
       <c r="BD18" s="5"/>
@@ -10338,7 +10375,9 @@
       <c r="AZ19" s="5">
         <v>504.85</v>
       </c>
-      <c r="BA19" s="5"/>
+      <c r="BA19" s="5">
+        <v>504.75</v>
+      </c>
       <c r="BB19" s="5"/>
       <c r="BC19" s="5"/>
       <c r="BD19" s="5"/>
@@ -10505,7 +10544,9 @@
       <c r="AZ20" s="5">
         <v>737</v>
       </c>
-      <c r="BA20" s="5"/>
+      <c r="BA20" s="5">
+        <v>732.5</v>
+      </c>
       <c r="BB20" s="5"/>
       <c r="BC20" s="5"/>
       <c r="BD20" s="5"/>
@@ -10672,7 +10713,9 @@
       <c r="AZ21" s="5">
         <v>386.5</v>
       </c>
-      <c r="BA21" s="5"/>
+      <c r="BA21" s="5">
+        <v>405.95</v>
+      </c>
       <c r="BB21" s="5"/>
       <c r="BC21" s="5"/>
       <c r="BD21" s="5"/>
@@ -10785,7 +10828,9 @@
       <c r="AZ22" s="5">
         <v>345</v>
       </c>
-      <c r="BA22" s="5"/>
+      <c r="BA22" s="5">
+        <v>330.1</v>
+      </c>
       <c r="BB22" s="5"/>
       <c r="BC22" s="5"/>
       <c r="BD22" s="5"/>
@@ -10944,7 +10989,9 @@
       <c r="AZ23" s="5">
         <v>57.4</v>
       </c>
-      <c r="BA23" s="5"/>
+      <c r="BA23" s="5">
+        <v>55.05</v>
+      </c>
       <c r="BB23" s="5"/>
       <c r="BC23" s="5"/>
       <c r="BD23" s="5"/>
@@ -11099,7 +11146,9 @@
       <c r="AZ24" s="5">
         <v>237.4</v>
       </c>
-      <c r="BA24" s="5"/>
+      <c r="BA24" s="5">
+        <v>234.4</v>
+      </c>
       <c r="BB24" s="5"/>
       <c r="BC24" s="5"/>
       <c r="BD24" s="5"/>
@@ -11236,7 +11285,9 @@
       <c r="AZ25" s="5">
         <v>935.15</v>
       </c>
-      <c r="BA25" s="5"/>
+      <c r="BA25" s="5">
+        <v>930.6</v>
+      </c>
       <c r="BB25" s="5"/>
       <c r="BC25" s="5"/>
       <c r="BD25" s="5"/>
@@ -11361,7 +11412,9 @@
       <c r="AZ26" s="5">
         <v>88.2</v>
       </c>
-      <c r="BA26" s="5"/>
+      <c r="BA26" s="5">
+        <v>86.05</v>
+      </c>
       <c r="BB26" s="5"/>
       <c r="BC26" s="5"/>
       <c r="BD26" s="5"/>
@@ -11486,7 +11539,9 @@
       <c r="AZ27" s="5">
         <v>44.1</v>
       </c>
-      <c r="BA27" s="5"/>
+      <c r="BA27" s="5">
+        <v>41.6</v>
+      </c>
       <c r="BB27" s="5"/>
       <c r="BC27" s="5"/>
       <c r="BD27" s="5"/>
@@ -11498,7 +11553,7 @@
     <row r="28" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>51.75</v>
       </c>
       <c r="B28" s="12">
         <f t="shared" si="1"/>
@@ -11506,7 +11561,7 @@
       </c>
       <c r="C28" s="12">
         <f t="shared" si="2"/>
-        <v>5.0499999999999972</v>
+        <v>5.2999999999999972</v>
       </c>
       <c r="D28" s="45" t="s">
         <v>254</v>
@@ -11611,7 +11666,9 @@
       <c r="AZ28" s="5">
         <v>53.2</v>
       </c>
-      <c r="BA28" s="5"/>
+      <c r="BA28" s="5">
+        <v>51.75</v>
+      </c>
       <c r="BB28" s="5"/>
       <c r="BC28" s="5"/>
       <c r="BD28" s="5"/>
@@ -11736,7 +11793,9 @@
       <c r="AZ29" s="5">
         <v>127</v>
       </c>
-      <c r="BA29" s="5"/>
+      <c r="BA29" s="5">
+        <v>128.80000000000001</v>
+      </c>
       <c r="BB29" s="5"/>
       <c r="BC29" s="5"/>
       <c r="BD29" s="5"/>
@@ -11861,7 +11920,9 @@
       <c r="AZ30" s="5">
         <v>165.5</v>
       </c>
-      <c r="BA30" s="5"/>
+      <c r="BA30" s="5">
+        <v>166.1</v>
+      </c>
       <c r="BB30" s="5"/>
       <c r="BC30" s="5"/>
       <c r="BD30" s="5"/>
@@ -11986,7 +12047,9 @@
       <c r="AZ31" s="5">
         <v>67.95</v>
       </c>
-      <c r="BA31" s="5"/>
+      <c r="BA31" s="5">
+        <v>67.45</v>
+      </c>
       <c r="BB31" s="5"/>
       <c r="BC31" s="5"/>
       <c r="BD31" s="5"/>
@@ -12111,7 +12174,9 @@
       <c r="AZ32" s="5">
         <v>48.1</v>
       </c>
-      <c r="BA32" s="5"/>
+      <c r="BA32" s="5">
+        <v>45.6</v>
+      </c>
       <c r="BB32" s="5"/>
       <c r="BC32" s="5"/>
       <c r="BD32" s="5"/>
@@ -12236,7 +12301,9 @@
       <c r="AZ33" s="5">
         <v>68.8</v>
       </c>
-      <c r="BA33" s="5"/>
+      <c r="BA33" s="5">
+        <v>65.2</v>
+      </c>
       <c r="BB33" s="5"/>
       <c r="BC33" s="5"/>
       <c r="BD33" s="5"/>
@@ -12248,7 +12315,7 @@
     <row r="34" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <f t="shared" si="0"/>
-        <v>29.9</v>
+        <v>29.85</v>
       </c>
       <c r="B34" s="12">
         <f t="shared" si="1"/>
@@ -12256,7 +12323,7 @@
       </c>
       <c r="C34" s="12">
         <f t="shared" si="2"/>
-        <v>2.6499999999999986</v>
+        <v>2.6999999999999957</v>
       </c>
       <c r="D34" s="45" t="s">
         <v>260</v>
@@ -12361,7 +12428,9 @@
       <c r="AZ34" s="5">
         <v>30</v>
       </c>
-      <c r="BA34" s="5"/>
+      <c r="BA34" s="5">
+        <v>29.85</v>
+      </c>
       <c r="BB34" s="5"/>
       <c r="BC34" s="5"/>
       <c r="BD34" s="5"/>
@@ -12486,7 +12555,9 @@
       <c r="AZ35" s="5">
         <v>88.8</v>
       </c>
-      <c r="BA35" s="5"/>
+      <c r="BA35" s="5">
+        <v>86.3</v>
+      </c>
       <c r="BB35" s="5"/>
       <c r="BC35" s="5"/>
       <c r="BD35" s="5"/>
@@ -12498,7 +12569,7 @@
     <row r="36" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <f t="shared" si="0"/>
-        <v>121</v>
+        <v>120.85</v>
       </c>
       <c r="B36" s="12">
         <f t="shared" si="1"/>
@@ -12506,7 +12577,7 @@
       </c>
       <c r="C36" s="12">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>14.150000000000006</v>
       </c>
       <c r="D36" s="45" t="s">
         <v>262</v>
@@ -12611,7 +12682,9 @@
       <c r="AZ36" s="5">
         <v>123.35</v>
       </c>
-      <c r="BA36" s="5"/>
+      <c r="BA36" s="5">
+        <v>120.85</v>
+      </c>
       <c r="BB36" s="5"/>
       <c r="BC36" s="5"/>
       <c r="BD36" s="5"/>
@@ -12736,7 +12809,9 @@
       <c r="AZ37" s="5">
         <v>141.6</v>
       </c>
-      <c r="BA37" s="5"/>
+      <c r="BA37" s="5">
+        <v>138.80000000000001</v>
+      </c>
       <c r="BB37" s="5"/>
       <c r="BC37" s="5"/>
       <c r="BD37" s="5"/>
@@ -12861,7 +12936,9 @@
       <c r="AZ38" s="5">
         <v>153.35</v>
       </c>
-      <c r="BA38" s="5"/>
+      <c r="BA38" s="5">
+        <v>149.55000000000001</v>
+      </c>
       <c r="BB38" s="5"/>
       <c r="BC38" s="5"/>
       <c r="BD38" s="5"/>
@@ -12974,7 +13051,9 @@
       <c r="AZ39" s="5">
         <v>113.15</v>
       </c>
-      <c r="BA39" s="5"/>
+      <c r="BA39" s="5">
+        <v>114.3</v>
+      </c>
       <c r="BB39" s="5"/>
       <c r="BC39" s="5"/>
       <c r="BD39" s="5"/>
@@ -13075,7 +13154,9 @@
       <c r="AZ40" s="5">
         <v>67.099999999999994</v>
       </c>
-      <c r="BA40" s="5"/>
+      <c r="BA40" s="5">
+        <v>64.8</v>
+      </c>
       <c r="BB40" s="5"/>
       <c r="BC40" s="5"/>
       <c r="BD40" s="5"/>
@@ -13170,7 +13251,9 @@
       <c r="AZ41" s="5">
         <v>236.1</v>
       </c>
-      <c r="BA41" s="5"/>
+      <c r="BA41" s="5">
+        <v>224.3</v>
+      </c>
       <c r="BB41" s="5"/>
       <c r="BC41" s="5"/>
       <c r="BD41" s="5"/>
@@ -13186,11 +13269,11 @@
       </c>
       <c r="B42" s="12">
         <f t="shared" ref="B42" si="9">MAX(E42:ZZ42)</f>
-        <v>687</v>
+        <v>687.5</v>
       </c>
       <c r="C42" s="12">
         <f t="shared" ref="C42" si="10">B42-A42</f>
-        <v>20.899999999999977</v>
+        <v>21.399999999999977</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>291</v>
@@ -13259,7 +13342,9 @@
       <c r="AZ42" s="5">
         <v>687</v>
       </c>
-      <c r="BA42" s="5"/>
+      <c r="BA42" s="5">
+        <v>687.5</v>
+      </c>
       <c r="BB42" s="5"/>
       <c r="BC42" s="5"/>
       <c r="BD42" s="5"/>
@@ -14391,10 +14476,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="I19" sqref="I19:K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14404,6 +14489,7 @@
     <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -14438,7 +14524,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(B2:B200)</f>
-        <v>951943</v>
+        <v>956943</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -14456,7 +14542,7 @@
       </c>
       <c r="F3" s="5">
         <f>F1-F2</f>
-        <v>523446</v>
+        <v>518446</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -14914,9 +15000,15 @@
       <c r="C33" s="31">
         <v>43011</v>
       </c>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
+      <c r="I33" s="39" t="s">
+        <v>299</v>
+      </c>
+      <c r="J33" s="12">
+        <v>5000</v>
+      </c>
+      <c r="K33" s="31">
+        <v>43019</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="39" t="s">
@@ -14961,7 +15053,7 @@
       </c>
       <c r="J36" s="5">
         <f>SUM(J19:J35)</f>
-        <v>160800</v>
+        <v>165800</v>
       </c>
       <c r="K36" s="5"/>
     </row>
@@ -14985,6 +15077,17 @@
       </c>
       <c r="C38" s="31">
         <v>43017</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="39" t="s">
+        <v>299</v>
+      </c>
+      <c r="B39" s="12">
+        <v>5000</v>
+      </c>
+      <c r="C39" s="31">
+        <v>43019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added details for 24/10/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -21,11 +21,12 @@
     <sheet name="Bathroom" sheetId="15" r:id="rId12"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="312">
   <si>
     <t>Date</t>
   </si>
@@ -940,6 +941,27 @@
   </si>
   <si>
     <t>SOBHA</t>
+  </si>
+  <si>
+    <t>RECLTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAVELLS </t>
+  </si>
+  <si>
+    <t>25/10/2017</t>
+  </si>
+  <si>
+    <t>26/102017</t>
+  </si>
+  <si>
+    <t>27/10/2017</t>
+  </si>
+  <si>
+    <t>30/10/2017</t>
+  </si>
+  <si>
+    <t>31/10/2017</t>
   </si>
 </sst>
 </file>
@@ -1176,13 +1198,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -7178,11 +7200,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BG44"/>
+  <dimension ref="A1:BO46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="AQ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BF1" sqref="BF1"/>
+      <pane xSplit="4" topLeftCell="BF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BG1" sqref="BG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7214,11 +7236,17 @@
     <col min="51" max="51" width="13" customWidth="1"/>
     <col min="52" max="52" width="14" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="54" max="58" width="14" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="54" max="57" width="14" bestFit="1" customWidth="1"/>
+    <col min="58" max="60" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.42578125" customWidth="1"/>
+    <col min="63" max="63" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="14" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12" bestFit="1" customWidth="1"/>
+    <col min="66" max="67" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:67" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>249</v>
       </c>
@@ -7390,14 +7418,38 @@
       <c r="BE1" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="BF1" s="53" t="s">
+      <c r="BF1" s="51" t="s">
         <v>301</v>
       </c>
-      <c r="BG1" s="53" t="s">
+      <c r="BG1" s="51" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BH1" s="51" t="s">
+        <v>307</v>
+      </c>
+      <c r="BI1" s="51" t="s">
+        <v>308</v>
+      </c>
+      <c r="BJ1" s="51" t="s">
+        <v>309</v>
+      </c>
+      <c r="BK1" s="51" t="s">
+        <v>310</v>
+      </c>
+      <c r="BL1" s="51" t="s">
+        <v>311</v>
+      </c>
+      <c r="BM1" s="51">
+        <v>42746</v>
+      </c>
+      <c r="BN1" s="51">
+        <v>42777</v>
+      </c>
+      <c r="BO1" s="51">
+        <v>42805</v>
+      </c>
+    </row>
+    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <f t="shared" ref="A2:A39" si="0">MIN(E2:ZY2)</f>
         <v>243.6</v>
@@ -7567,9 +7619,19 @@
       <c r="BF2" s="5">
         <v>246</v>
       </c>
-      <c r="BG2" s="5"/>
-    </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG2" s="5">
+        <v>254.9</v>
+      </c>
+      <c r="BH2" s="5"/>
+      <c r="BI2" s="5"/>
+      <c r="BJ2" s="5"/>
+      <c r="BK2" s="5"/>
+      <c r="BL2" s="5"/>
+      <c r="BM2" s="5"/>
+      <c r="BN2" s="5"/>
+      <c r="BO2" s="5"/>
+    </row>
+    <row r="3" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <f t="shared" si="0"/>
         <v>262.7</v>
@@ -7739,9 +7801,19 @@
       <c r="BF3" s="5">
         <v>263.45</v>
       </c>
-      <c r="BG3" s="5"/>
-    </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG3" s="5">
+        <v>266.14999999999998</v>
+      </c>
+      <c r="BH3" s="5"/>
+      <c r="BI3" s="5"/>
+      <c r="BJ3" s="5"/>
+      <c r="BK3" s="5"/>
+      <c r="BL3" s="5"/>
+      <c r="BM3" s="5"/>
+      <c r="BN3" s="5"/>
+      <c r="BO3" s="5"/>
+    </row>
+    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
         <v>259.45</v>
@@ -7917,9 +7989,19 @@
       <c r="BF4" s="5">
         <v>266.89999999999998</v>
       </c>
-      <c r="BG4" s="5"/>
-    </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG4" s="5">
+        <v>267.10000000000002</v>
+      </c>
+      <c r="BH4" s="5"/>
+      <c r="BI4" s="5"/>
+      <c r="BJ4" s="5"/>
+      <c r="BK4" s="5"/>
+      <c r="BL4" s="5"/>
+      <c r="BM4" s="5"/>
+      <c r="BN4" s="5"/>
+      <c r="BO4" s="5"/>
+    </row>
+    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <f t="shared" si="0"/>
         <v>786.25</v>
@@ -8095,9 +8177,19 @@
       <c r="BF5" s="5">
         <v>943.4</v>
       </c>
-      <c r="BG5" s="5"/>
-    </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG5" s="5">
+        <v>936.2</v>
+      </c>
+      <c r="BH5" s="5"/>
+      <c r="BI5" s="5"/>
+      <c r="BJ5" s="5"/>
+      <c r="BK5" s="5"/>
+      <c r="BL5" s="5"/>
+      <c r="BM5" s="5"/>
+      <c r="BN5" s="5"/>
+      <c r="BO5" s="5"/>
+    </row>
+    <row r="6" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <f t="shared" si="0"/>
         <v>236.45</v>
@@ -8273,9 +8365,19 @@
       <c r="BF6" s="5">
         <v>290.89999999999998</v>
       </c>
-      <c r="BG6" s="5"/>
-    </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG6" s="5">
+        <v>289.5</v>
+      </c>
+      <c r="BH6" s="5"/>
+      <c r="BI6" s="5"/>
+      <c r="BJ6" s="5"/>
+      <c r="BK6" s="5"/>
+      <c r="BL6" s="5"/>
+      <c r="BM6" s="5"/>
+      <c r="BN6" s="5"/>
+      <c r="BO6" s="5"/>
+    </row>
+    <row r="7" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <f t="shared" si="0"/>
         <v>15.6</v>
@@ -8451,9 +8553,19 @@
       <c r="BF7" s="5">
         <v>16.95</v>
       </c>
-      <c r="BG7" s="5"/>
-    </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG7" s="5">
+        <v>17.350000000000001</v>
+      </c>
+      <c r="BH7" s="5"/>
+      <c r="BI7" s="5"/>
+      <c r="BJ7" s="5"/>
+      <c r="BK7" s="5"/>
+      <c r="BL7" s="5"/>
+      <c r="BM7" s="5"/>
+      <c r="BN7" s="5"/>
+      <c r="BO7" s="5"/>
+    </row>
+    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <f t="shared" si="0"/>
         <v>53.4</v>
@@ -8629,9 +8741,19 @@
       <c r="BF8" s="5">
         <v>59</v>
       </c>
-      <c r="BG8" s="5"/>
-    </row>
-    <row r="9" spans="1:59" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BG8" s="5">
+        <v>61.6</v>
+      </c>
+      <c r="BH8" s="5"/>
+      <c r="BI8" s="5"/>
+      <c r="BJ8" s="5"/>
+      <c r="BK8" s="5"/>
+      <c r="BL8" s="5"/>
+      <c r="BM8" s="5"/>
+      <c r="BN8" s="5"/>
+      <c r="BO8" s="5"/>
+    </row>
+    <row r="9" spans="1:67" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <f t="shared" si="0"/>
         <v>53.5</v>
@@ -8799,9 +8921,19 @@
       <c r="BF9" s="28">
         <v>56.3</v>
       </c>
-      <c r="BG9" s="28"/>
-    </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG9" s="28">
+        <v>56.9</v>
+      </c>
+      <c r="BH9" s="28"/>
+      <c r="BI9" s="28"/>
+      <c r="BJ9" s="28"/>
+      <c r="BK9" s="28"/>
+      <c r="BL9" s="28"/>
+      <c r="BM9" s="28"/>
+      <c r="BN9" s="28"/>
+      <c r="BO9" s="28"/>
+    </row>
+    <row r="10" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <f t="shared" si="0"/>
         <v>38.6</v>
@@ -8977,20 +9109,30 @@
       <c r="BF10" s="5">
         <v>39.049999999999997</v>
       </c>
-      <c r="BG10" s="5"/>
-    </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG10" s="5">
+        <v>39.5</v>
+      </c>
+      <c r="BH10" s="5"/>
+      <c r="BI10" s="5"/>
+      <c r="BJ10" s="5"/>
+      <c r="BK10" s="5"/>
+      <c r="BL10" s="5"/>
+      <c r="BM10" s="5"/>
+      <c r="BN10" s="5"/>
+      <c r="BO10" s="5"/>
+    </row>
+    <row r="11" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <f t="shared" si="0"/>
         <v>72.650000000000006</v>
       </c>
       <c r="B11" s="12">
         <f t="shared" si="1"/>
-        <v>98</v>
+        <v>98.4</v>
       </c>
       <c r="C11" s="12">
         <f t="shared" si="2"/>
-        <v>25.349999999999994</v>
+        <v>25.75</v>
       </c>
       <c r="D11" s="45" t="s">
         <v>17</v>
@@ -9155,20 +9297,30 @@
       <c r="BF11" s="5">
         <v>98</v>
       </c>
-      <c r="BG11" s="5"/>
-    </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG11" s="5">
+        <v>98.4</v>
+      </c>
+      <c r="BH11" s="5"/>
+      <c r="BI11" s="5"/>
+      <c r="BJ11" s="5"/>
+      <c r="BK11" s="5"/>
+      <c r="BL11" s="5"/>
+      <c r="BM11" s="5"/>
+      <c r="BN11" s="5"/>
+      <c r="BO11" s="5"/>
+    </row>
+    <row r="12" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
         <v>82.65</v>
       </c>
       <c r="B12" s="12">
         <f t="shared" si="1"/>
-        <v>86.95</v>
+        <v>88.15</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" si="2"/>
-        <v>4.2999999999999972</v>
+        <v>5.5</v>
       </c>
       <c r="D12" s="45" t="s">
         <v>18</v>
@@ -9333,9 +9485,19 @@
       <c r="BF12" s="5">
         <v>86.95</v>
       </c>
-      <c r="BG12" s="5"/>
-    </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG12" s="5">
+        <v>88.15</v>
+      </c>
+      <c r="BH12" s="5"/>
+      <c r="BI12" s="5"/>
+      <c r="BJ12" s="5"/>
+      <c r="BK12" s="5"/>
+      <c r="BL12" s="5"/>
+      <c r="BM12" s="5"/>
+      <c r="BN12" s="5"/>
+      <c r="BO12" s="5"/>
+    </row>
+    <row r="13" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <f t="shared" si="0"/>
         <v>44.1</v>
@@ -9511,9 +9673,19 @@
       <c r="BF13" s="5">
         <v>49.25</v>
       </c>
-      <c r="BG13" s="5"/>
-    </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG13" s="5">
+        <v>50.9</v>
+      </c>
+      <c r="BH13" s="5"/>
+      <c r="BI13" s="5"/>
+      <c r="BJ13" s="5"/>
+      <c r="BK13" s="5"/>
+      <c r="BL13" s="5"/>
+      <c r="BM13" s="5"/>
+      <c r="BN13" s="5"/>
+      <c r="BO13" s="5"/>
+    </row>
+    <row r="14" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <f t="shared" si="0"/>
         <v>29.75</v>
@@ -9689,9 +9861,19 @@
       <c r="BF14" s="5">
         <v>29.75</v>
       </c>
-      <c r="BG14" s="5"/>
-    </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG14" s="5">
+        <v>30.65</v>
+      </c>
+      <c r="BH14" s="5"/>
+      <c r="BI14" s="5"/>
+      <c r="BJ14" s="5"/>
+      <c r="BK14" s="5"/>
+      <c r="BL14" s="5"/>
+      <c r="BM14" s="5"/>
+      <c r="BN14" s="5"/>
+      <c r="BO14" s="5"/>
+    </row>
+    <row r="15" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
         <v>26.5</v>
@@ -9859,20 +10041,30 @@
       <c r="BF15" s="5">
         <v>26.9</v>
       </c>
-      <c r="BG15" s="5"/>
-    </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG15" s="5">
+        <v>26.95</v>
+      </c>
+      <c r="BH15" s="5"/>
+      <c r="BI15" s="5"/>
+      <c r="BJ15" s="5"/>
+      <c r="BK15" s="5"/>
+      <c r="BL15" s="5"/>
+      <c r="BM15" s="5"/>
+      <c r="BN15" s="5"/>
+      <c r="BO15" s="5"/>
+    </row>
+    <row r="16" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <f t="shared" si="0"/>
         <v>552</v>
       </c>
       <c r="B16" s="12">
         <f t="shared" si="1"/>
-        <v>714.45</v>
+        <v>718.95</v>
       </c>
       <c r="C16" s="12">
         <f t="shared" si="2"/>
-        <v>162.45000000000005</v>
+        <v>166.95000000000005</v>
       </c>
       <c r="D16" s="45" t="s">
         <v>23</v>
@@ -10037,9 +10229,19 @@
       <c r="BF16" s="5">
         <v>712.2</v>
       </c>
-      <c r="BG16" s="5"/>
-    </row>
-    <row r="17" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG16" s="5">
+        <v>718.95</v>
+      </c>
+      <c r="BH16" s="5"/>
+      <c r="BI16" s="5"/>
+      <c r="BJ16" s="5"/>
+      <c r="BK16" s="5"/>
+      <c r="BL16" s="5"/>
+      <c r="BM16" s="5"/>
+      <c r="BN16" s="5"/>
+      <c r="BO16" s="5"/>
+    </row>
+    <row r="17" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <f t="shared" si="0"/>
         <v>433</v>
@@ -10215,9 +10417,19 @@
       <c r="BF17" s="5">
         <v>455.25</v>
       </c>
-      <c r="BG17" s="5"/>
-    </row>
-    <row r="18" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG17" s="5">
+        <v>469</v>
+      </c>
+      <c r="BH17" s="5"/>
+      <c r="BI17" s="5"/>
+      <c r="BJ17" s="5"/>
+      <c r="BK17" s="5"/>
+      <c r="BL17" s="5"/>
+      <c r="BM17" s="5"/>
+      <c r="BN17" s="5"/>
+      <c r="BO17" s="5"/>
+    </row>
+    <row r="18" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <f t="shared" si="0"/>
         <v>178.8</v>
@@ -10393,20 +10605,30 @@
       <c r="BF18" s="5">
         <v>282.89999999999998</v>
       </c>
-      <c r="BG18" s="5"/>
-    </row>
-    <row r="19" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG18" s="5">
+        <v>281.25</v>
+      </c>
+      <c r="BH18" s="5"/>
+      <c r="BI18" s="5"/>
+      <c r="BJ18" s="5"/>
+      <c r="BK18" s="5"/>
+      <c r="BL18" s="5"/>
+      <c r="BM18" s="5"/>
+      <c r="BN18" s="5"/>
+      <c r="BO18" s="5"/>
+    </row>
+    <row r="19" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <f t="shared" si="0"/>
         <v>440.7</v>
       </c>
       <c r="B19" s="12">
         <f t="shared" si="1"/>
-        <v>544.95000000000005</v>
+        <v>546.25</v>
       </c>
       <c r="C19" s="12">
         <f t="shared" si="2"/>
-        <v>104.25000000000006</v>
+        <v>105.55000000000001</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -10571,9 +10793,19 @@
       <c r="BF19" s="5">
         <v>544.95000000000005</v>
       </c>
-      <c r="BG19" s="5"/>
-    </row>
-    <row r="20" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG19" s="5">
+        <v>546.25</v>
+      </c>
+      <c r="BH19" s="5"/>
+      <c r="BI19" s="5"/>
+      <c r="BJ19" s="5"/>
+      <c r="BK19" s="5"/>
+      <c r="BL19" s="5"/>
+      <c r="BM19" s="5"/>
+      <c r="BN19" s="5"/>
+      <c r="BO19" s="5"/>
+    </row>
+    <row r="20" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <f t="shared" si="0"/>
         <v>677</v>
@@ -10749,20 +10981,30 @@
       <c r="BF20" s="5">
         <v>750.35</v>
       </c>
-      <c r="BG20" s="5"/>
-    </row>
-    <row r="21" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BG20" s="5">
+        <v>742.5</v>
+      </c>
+      <c r="BH20" s="5"/>
+      <c r="BI20" s="5"/>
+      <c r="BJ20" s="5"/>
+      <c r="BK20" s="5"/>
+      <c r="BL20" s="5"/>
+      <c r="BM20" s="5"/>
+      <c r="BN20" s="5"/>
+      <c r="BO20" s="5"/>
+    </row>
+    <row r="21" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <f t="shared" si="0"/>
         <v>376.7</v>
       </c>
       <c r="B21" s="12">
         <f t="shared" si="1"/>
-        <v>497.15</v>
+        <v>500.15</v>
       </c>
       <c r="C21" s="12">
         <f t="shared" si="2"/>
-        <v>120.44999999999999</v>
+        <v>123.44999999999999</v>
       </c>
       <c r="D21" s="44" t="s">
         <v>106</v>
@@ -10927,9 +11169,19 @@
       <c r="BF21" s="5">
         <v>497.15</v>
       </c>
-      <c r="BG21" s="5"/>
-    </row>
-    <row r="22" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BG21" s="5">
+        <v>500.15</v>
+      </c>
+      <c r="BH21" s="5"/>
+      <c r="BI21" s="5"/>
+      <c r="BJ21" s="5"/>
+      <c r="BK21" s="5"/>
+      <c r="BL21" s="5"/>
+      <c r="BM21" s="5"/>
+      <c r="BN21" s="5"/>
+      <c r="BO21" s="5"/>
+    </row>
+    <row r="22" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <f t="shared" si="0"/>
         <v>315.2</v>
@@ -11051,9 +11303,19 @@
       <c r="BF22" s="5">
         <v>338</v>
       </c>
-      <c r="BG22" s="5"/>
-    </row>
-    <row r="23" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG22" s="5">
+        <v>335.6</v>
+      </c>
+      <c r="BH22" s="5"/>
+      <c r="BI22" s="5"/>
+      <c r="BJ22" s="5"/>
+      <c r="BK22" s="5"/>
+      <c r="BL22" s="5"/>
+      <c r="BM22" s="5"/>
+      <c r="BN22" s="5"/>
+      <c r="BO22" s="5"/>
+    </row>
+    <row r="23" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
         <v>54.45</v>
@@ -11221,9 +11483,19 @@
       <c r="BF23" s="5">
         <v>54.45</v>
       </c>
-      <c r="BG23" s="5"/>
-    </row>
-    <row r="24" spans="1:59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BG23" s="5">
+        <v>55.2</v>
+      </c>
+      <c r="BH23" s="5"/>
+      <c r="BI23" s="5"/>
+      <c r="BJ23" s="5"/>
+      <c r="BK23" s="5"/>
+      <c r="BL23" s="5"/>
+      <c r="BM23" s="5"/>
+      <c r="BN23" s="5"/>
+      <c r="BO23" s="5"/>
+    </row>
+    <row r="24" spans="1:67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <f t="shared" si="0"/>
         <v>210.65</v>
@@ -11387,9 +11659,19 @@
       <c r="BF24" s="5">
         <v>235.55</v>
       </c>
-      <c r="BG24" s="5"/>
-    </row>
-    <row r="25" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG24" s="5">
+        <v>231.1</v>
+      </c>
+      <c r="BH24" s="5"/>
+      <c r="BI24" s="5"/>
+      <c r="BJ24" s="5"/>
+      <c r="BK24" s="5"/>
+      <c r="BL24" s="5"/>
+      <c r="BM24" s="5"/>
+      <c r="BN24" s="5"/>
+      <c r="BO24" s="5"/>
+    </row>
+    <row r="25" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <f t="shared" si="0"/>
         <v>876</v>
@@ -11535,9 +11817,19 @@
       <c r="BF25" s="5">
         <v>937.45</v>
       </c>
-      <c r="BG25" s="5"/>
-    </row>
-    <row r="26" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG25" s="5">
+        <v>924.35</v>
+      </c>
+      <c r="BH25" s="5"/>
+      <c r="BI25" s="5"/>
+      <c r="BJ25" s="5"/>
+      <c r="BK25" s="5"/>
+      <c r="BL25" s="5"/>
+      <c r="BM25" s="5"/>
+      <c r="BN25" s="5"/>
+      <c r="BO25" s="5"/>
+    </row>
+    <row r="26" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <f t="shared" si="0"/>
         <v>83.5</v>
@@ -11671,9 +11963,19 @@
       <c r="BF26" s="5">
         <v>83.5</v>
       </c>
-      <c r="BG26" s="5"/>
-    </row>
-    <row r="27" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG26" s="5">
+        <v>84.05</v>
+      </c>
+      <c r="BH26" s="5"/>
+      <c r="BI26" s="5"/>
+      <c r="BJ26" s="5"/>
+      <c r="BK26" s="5"/>
+      <c r="BL26" s="5"/>
+      <c r="BM26" s="5"/>
+      <c r="BN26" s="5"/>
+      <c r="BO26" s="5"/>
+    </row>
+    <row r="27" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <f t="shared" si="0"/>
         <v>37.6</v>
@@ -11807,9 +12109,19 @@
       <c r="BF27" s="5">
         <v>41.1</v>
       </c>
-      <c r="BG27" s="5"/>
-    </row>
-    <row r="28" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG27" s="5">
+        <v>40.9</v>
+      </c>
+      <c r="BH27" s="5"/>
+      <c r="BI27" s="5"/>
+      <c r="BJ27" s="5"/>
+      <c r="BK27" s="5"/>
+      <c r="BL27" s="5"/>
+      <c r="BM27" s="5"/>
+      <c r="BN27" s="5"/>
+      <c r="BO27" s="5"/>
+    </row>
+    <row r="28" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <f t="shared" si="0"/>
         <v>51.75</v>
@@ -11943,9 +12255,19 @@
       <c r="BF28" s="5">
         <v>51.95</v>
       </c>
-      <c r="BG28" s="5"/>
-    </row>
-    <row r="29" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG28" s="5">
+        <v>54.05</v>
+      </c>
+      <c r="BH28" s="5"/>
+      <c r="BI28" s="5"/>
+      <c r="BJ28" s="5"/>
+      <c r="BK28" s="5"/>
+      <c r="BL28" s="5"/>
+      <c r="BM28" s="5"/>
+      <c r="BN28" s="5"/>
+      <c r="BO28" s="5"/>
+    </row>
+    <row r="29" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <f t="shared" si="0"/>
         <v>111.95</v>
@@ -12079,9 +12401,19 @@
       <c r="BF29" s="5">
         <v>141.65</v>
       </c>
-      <c r="BG29" s="5"/>
-    </row>
-    <row r="30" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG29" s="5">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="BH29" s="5"/>
+      <c r="BI29" s="5"/>
+      <c r="BJ29" s="5"/>
+      <c r="BK29" s="5"/>
+      <c r="BL29" s="5"/>
+      <c r="BM29" s="5"/>
+      <c r="BN29" s="5"/>
+      <c r="BO29" s="5"/>
+    </row>
+    <row r="30" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <f t="shared" si="0"/>
         <v>62.3</v>
@@ -12215,9 +12547,19 @@
       <c r="BF30" s="5">
         <v>67</v>
       </c>
-      <c r="BG30" s="5"/>
-    </row>
-    <row r="31" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG30" s="5">
+        <v>66.45</v>
+      </c>
+      <c r="BH30" s="5"/>
+      <c r="BI30" s="5"/>
+      <c r="BJ30" s="5"/>
+      <c r="BK30" s="5"/>
+      <c r="BL30" s="5"/>
+      <c r="BM30" s="5"/>
+      <c r="BN30" s="5"/>
+      <c r="BO30" s="5"/>
+    </row>
+    <row r="31" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
         <v>39.25</v>
@@ -12351,20 +12693,30 @@
       <c r="BF31" s="5">
         <v>43.7</v>
       </c>
-      <c r="BG31" s="5"/>
-    </row>
-    <row r="32" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG31" s="5">
+        <v>43.25</v>
+      </c>
+      <c r="BH31" s="5"/>
+      <c r="BI31" s="5"/>
+      <c r="BJ31" s="5"/>
+      <c r="BK31" s="5"/>
+      <c r="BL31" s="5"/>
+      <c r="BM31" s="5"/>
+      <c r="BN31" s="5"/>
+      <c r="BO31" s="5"/>
+    </row>
+    <row r="32" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <f t="shared" si="0"/>
         <v>62.55</v>
       </c>
       <c r="B32" s="12">
         <f t="shared" si="1"/>
-        <v>70.099999999999994</v>
+        <v>72.2</v>
       </c>
       <c r="C32" s="12">
         <f t="shared" si="2"/>
-        <v>7.5499999999999972</v>
+        <v>9.6500000000000057</v>
       </c>
       <c r="D32" s="45" t="s">
         <v>258</v>
@@ -12487,9 +12839,19 @@
       <c r="BF32" s="5">
         <v>67.8</v>
       </c>
-      <c r="BG32" s="5"/>
-    </row>
-    <row r="33" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG32" s="5">
+        <v>72.2</v>
+      </c>
+      <c r="BH32" s="5"/>
+      <c r="BI32" s="5"/>
+      <c r="BJ32" s="5"/>
+      <c r="BK32" s="5"/>
+      <c r="BL32" s="5"/>
+      <c r="BM32" s="5"/>
+      <c r="BN32" s="5"/>
+      <c r="BO32" s="5"/>
+    </row>
+    <row r="33" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <f t="shared" si="0"/>
         <v>29.15</v>
@@ -12623,20 +12985,30 @@
       <c r="BF33" s="5">
         <v>29.15</v>
       </c>
-      <c r="BG33" s="5"/>
-    </row>
-    <row r="34" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG33" s="5">
+        <v>30.4</v>
+      </c>
+      <c r="BH33" s="5"/>
+      <c r="BI33" s="5"/>
+      <c r="BJ33" s="5"/>
+      <c r="BK33" s="5"/>
+      <c r="BL33" s="5"/>
+      <c r="BM33" s="5"/>
+      <c r="BN33" s="5"/>
+      <c r="BO33" s="5"/>
+    </row>
+    <row r="34" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <f t="shared" si="0"/>
         <v>81.55</v>
       </c>
       <c r="B34" s="12">
         <f t="shared" si="1"/>
-        <v>95.25</v>
+        <v>101.75</v>
       </c>
       <c r="C34" s="12">
         <f t="shared" si="2"/>
-        <v>13.700000000000003</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="D34" s="45" t="s">
         <v>260</v>
@@ -12759,9 +13131,19 @@
       <c r="BF34" s="5">
         <v>95.25</v>
       </c>
-      <c r="BG34" s="5"/>
-    </row>
-    <row r="35" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG34" s="5">
+        <v>101.75</v>
+      </c>
+      <c r="BH34" s="5"/>
+      <c r="BI34" s="5"/>
+      <c r="BJ34" s="5"/>
+      <c r="BK34" s="5"/>
+      <c r="BL34" s="5"/>
+      <c r="BM34" s="5"/>
+      <c r="BN34" s="5"/>
+      <c r="BO34" s="5"/>
+    </row>
+    <row r="35" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <f t="shared" si="0"/>
         <v>119.95</v>
@@ -12895,9 +13277,19 @@
       <c r="BF35" s="5">
         <v>131.19999999999999</v>
       </c>
-      <c r="BG35" s="5"/>
-    </row>
-    <row r="36" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG35" s="5">
+        <v>132.6</v>
+      </c>
+      <c r="BH35" s="5"/>
+      <c r="BI35" s="5"/>
+      <c r="BJ35" s="5"/>
+      <c r="BK35" s="5"/>
+      <c r="BL35" s="5"/>
+      <c r="BM35" s="5"/>
+      <c r="BN35" s="5"/>
+      <c r="BO35" s="5"/>
+    </row>
+    <row r="36" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <f t="shared" si="0"/>
         <v>136.69999999999999</v>
@@ -13031,9 +13423,19 @@
       <c r="BF36" s="5">
         <v>137.44999999999999</v>
       </c>
-      <c r="BG36" s="5"/>
-    </row>
-    <row r="37" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG36" s="5">
+        <v>143.19999999999999</v>
+      </c>
+      <c r="BH36" s="5"/>
+      <c r="BI36" s="5"/>
+      <c r="BJ36" s="5"/>
+      <c r="BK36" s="5"/>
+      <c r="BL36" s="5"/>
+      <c r="BM36" s="5"/>
+      <c r="BN36" s="5"/>
+      <c r="BO36" s="5"/>
+    </row>
+    <row r="37" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <f t="shared" si="0"/>
         <v>144.5</v>
@@ -13167,20 +13569,30 @@
       <c r="BF37" s="5">
         <v>145.30000000000001</v>
       </c>
-      <c r="BG37" s="5"/>
-    </row>
-    <row r="38" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG37" s="5">
+        <v>145.9</v>
+      </c>
+      <c r="BH37" s="5"/>
+      <c r="BI37" s="5"/>
+      <c r="BJ37" s="5"/>
+      <c r="BK37" s="5"/>
+      <c r="BL37" s="5"/>
+      <c r="BM37" s="5"/>
+      <c r="BN37" s="5"/>
+      <c r="BO37" s="5"/>
+    </row>
+    <row r="38" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <f t="shared" si="0"/>
         <v>101.6</v>
       </c>
       <c r="B38" s="12">
         <f t="shared" si="3"/>
-        <v>117.15</v>
+        <v>121.8</v>
       </c>
       <c r="C38" s="12">
         <f t="shared" si="2"/>
-        <v>15.550000000000011</v>
+        <v>20.200000000000003</v>
       </c>
       <c r="D38" s="45" t="s">
         <v>274</v>
@@ -13291,9 +13703,19 @@
       <c r="BF38" s="5">
         <v>115.6</v>
       </c>
-      <c r="BG38" s="5"/>
-    </row>
-    <row r="39" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG38" s="5">
+        <v>121.8</v>
+      </c>
+      <c r="BH38" s="5"/>
+      <c r="BI38" s="5"/>
+      <c r="BJ38" s="5"/>
+      <c r="BK38" s="5"/>
+      <c r="BL38" s="5"/>
+      <c r="BM38" s="5"/>
+      <c r="BN38" s="5"/>
+      <c r="BO38" s="5"/>
+    </row>
+    <row r="39" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <f t="shared" si="0"/>
         <v>57.85</v>
@@ -13403,9 +13825,19 @@
       <c r="BF39" s="5">
         <v>60.3</v>
       </c>
-      <c r="BG39" s="5"/>
-    </row>
-    <row r="40" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG39" s="5">
+        <v>58.4</v>
+      </c>
+      <c r="BH39" s="5"/>
+      <c r="BI39" s="5"/>
+      <c r="BJ39" s="5"/>
+      <c r="BK39" s="5"/>
+      <c r="BL39" s="5"/>
+      <c r="BM39" s="5"/>
+      <c r="BN39" s="5"/>
+      <c r="BO39" s="5"/>
+    </row>
+    <row r="40" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <f t="shared" ref="A40" si="5">MIN(E40:ZY40)</f>
         <v>167.9</v>
@@ -13509,9 +13941,19 @@
       <c r="BF40" s="5">
         <v>208.5</v>
       </c>
-      <c r="BG40" s="5"/>
-    </row>
-    <row r="41" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG40" s="5">
+        <v>203.5</v>
+      </c>
+      <c r="BH40" s="5"/>
+      <c r="BI40" s="5"/>
+      <c r="BJ40" s="5"/>
+      <c r="BK40" s="5"/>
+      <c r="BL40" s="5"/>
+      <c r="BM40" s="5"/>
+      <c r="BN40" s="5"/>
+      <c r="BO40" s="5"/>
+    </row>
+    <row r="41" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <f t="shared" ref="A41:A42" si="8">MIN(E41:ZY41)</f>
         <v>661</v>
@@ -13611,12 +14053,22 @@
       <c r="BF41" s="5">
         <v>692.5</v>
       </c>
-      <c r="BG41" s="5"/>
-    </row>
-    <row r="42" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG41" s="5">
+        <v>704.95</v>
+      </c>
+      <c r="BH41" s="5"/>
+      <c r="BI41" s="5"/>
+      <c r="BJ41" s="5"/>
+      <c r="BK41" s="5"/>
+      <c r="BL41" s="5"/>
+      <c r="BM41" s="5"/>
+      <c r="BN41" s="5"/>
+      <c r="BO41" s="5"/>
+    </row>
+    <row r="42" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <f t="shared" si="8"/>
-        <v>425.95</v>
+        <v>421.65</v>
       </c>
       <c r="B42" s="12">
         <f t="shared" ref="B42" si="11">MAX(E42:ZY42)</f>
@@ -13624,7 +14076,7 @@
       </c>
       <c r="C42" s="12">
         <f t="shared" ref="C42" si="12">B42-A42</f>
-        <v>94.050000000000011</v>
+        <v>98.350000000000023</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>296</v>
@@ -13695,20 +14147,30 @@
       <c r="BF42" s="5">
         <v>425.95</v>
       </c>
-      <c r="BG42" s="5"/>
-    </row>
-    <row r="43" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG42" s="5">
+        <v>421.65</v>
+      </c>
+      <c r="BH42" s="5"/>
+      <c r="BI42" s="5"/>
+      <c r="BJ42" s="5"/>
+      <c r="BK42" s="5"/>
+      <c r="BL42" s="5"/>
+      <c r="BM42" s="5"/>
+      <c r="BN42" s="5"/>
+      <c r="BO42" s="5"/>
+    </row>
+    <row r="43" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <f t="shared" ref="A43" si="13">MIN(E43:ZY43)</f>
         <v>226</v>
       </c>
       <c r="B43" s="12">
         <f t="shared" ref="B43" si="14">MAX(E43:ZY43)</f>
-        <v>226</v>
+        <v>245</v>
       </c>
       <c r="C43" s="12">
         <f t="shared" ref="C43" si="15">B43-A43</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D43" s="45" t="s">
         <v>303</v>
@@ -13769,20 +14231,30 @@
       <c r="BF43" s="5">
         <v>226</v>
       </c>
-      <c r="BG43" s="5"/>
-    </row>
-    <row r="44" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="BG43" s="5">
+        <v>245</v>
+      </c>
+      <c r="BH43" s="5"/>
+      <c r="BI43" s="5"/>
+      <c r="BJ43" s="5"/>
+      <c r="BK43" s="5"/>
+      <c r="BL43" s="5"/>
+      <c r="BM43" s="5"/>
+      <c r="BN43" s="5"/>
+      <c r="BO43" s="5"/>
+    </row>
+    <row r="44" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <f t="shared" ref="A44" si="16">MIN(E44:ZY44)</f>
         <v>512</v>
       </c>
       <c r="B44" s="12">
         <f t="shared" ref="B44" si="17">MAX(E44:ZY44)</f>
-        <v>512</v>
+        <v>532.54999999999995</v>
       </c>
       <c r="C44" s="12">
         <f t="shared" ref="C44" si="18">B44-A44</f>
-        <v>0</v>
+        <v>20.549999999999955</v>
       </c>
       <c r="D44" s="45" t="s">
         <v>304</v>
@@ -13843,7 +14315,163 @@
       <c r="BF44" s="5">
         <v>512</v>
       </c>
-      <c r="BG44" s="5"/>
+      <c r="BG44" s="5">
+        <v>532.54999999999995</v>
+      </c>
+      <c r="BH44" s="5"/>
+      <c r="BI44" s="5"/>
+      <c r="BJ44" s="5"/>
+      <c r="BK44" s="5"/>
+      <c r="BL44" s="5"/>
+      <c r="BM44" s="5"/>
+      <c r="BN44" s="5"/>
+      <c r="BO44" s="5"/>
+    </row>
+    <row r="45" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="45" t="s">
+        <v>305</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="5"/>
+      <c r="U45" s="5"/>
+      <c r="V45" s="5"/>
+      <c r="W45" s="5"/>
+      <c r="X45" s="5"/>
+      <c r="Y45" s="5"/>
+      <c r="Z45" s="5"/>
+      <c r="AA45" s="5"/>
+      <c r="AB45" s="5"/>
+      <c r="AC45" s="5"/>
+      <c r="AD45" s="5"/>
+      <c r="AE45" s="5"/>
+      <c r="AF45" s="5"/>
+      <c r="AG45" s="5"/>
+      <c r="AH45" s="5"/>
+      <c r="AI45" s="5"/>
+      <c r="AJ45" s="5"/>
+      <c r="AK45" s="5"/>
+      <c r="AL45" s="5"/>
+      <c r="AM45" s="5"/>
+      <c r="AN45" s="5"/>
+      <c r="AO45" s="5"/>
+      <c r="AP45" s="5"/>
+      <c r="AQ45" s="5"/>
+      <c r="AR45" s="5"/>
+      <c r="AS45" s="5"/>
+      <c r="AT45" s="5"/>
+      <c r="AU45" s="5"/>
+      <c r="AV45" s="5"/>
+      <c r="AW45" s="5"/>
+      <c r="AX45" s="5"/>
+      <c r="AY45" s="5"/>
+      <c r="AZ45" s="5"/>
+      <c r="BA45" s="5"/>
+      <c r="BB45" s="5"/>
+      <c r="BC45" s="5"/>
+      <c r="BD45" s="5"/>
+      <c r="BE45" s="5"/>
+      <c r="BF45" s="5"/>
+      <c r="BG45" s="5">
+        <v>156.05000000000001</v>
+      </c>
+      <c r="BH45" s="5"/>
+      <c r="BI45" s="5"/>
+      <c r="BJ45" s="5"/>
+      <c r="BK45" s="5"/>
+      <c r="BL45" s="5"/>
+      <c r="BM45" s="5"/>
+      <c r="BN45" s="5"/>
+      <c r="BO45" s="5"/>
+    </row>
+    <row r="46" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="45" t="s">
+        <v>306</v>
+      </c>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="5"/>
+      <c r="V46" s="5"/>
+      <c r="W46" s="5"/>
+      <c r="X46" s="5"/>
+      <c r="Y46" s="5"/>
+      <c r="Z46" s="5"/>
+      <c r="AA46" s="5"/>
+      <c r="AB46" s="5"/>
+      <c r="AC46" s="5"/>
+      <c r="AD46" s="5"/>
+      <c r="AE46" s="5"/>
+      <c r="AF46" s="5"/>
+      <c r="AG46" s="5"/>
+      <c r="AH46" s="5"/>
+      <c r="AI46" s="5"/>
+      <c r="AJ46" s="5"/>
+      <c r="AK46" s="5"/>
+      <c r="AL46" s="5"/>
+      <c r="AM46" s="5"/>
+      <c r="AN46" s="5"/>
+      <c r="AO46" s="5"/>
+      <c r="AP46" s="5"/>
+      <c r="AQ46" s="5"/>
+      <c r="AR46" s="5"/>
+      <c r="AS46" s="5"/>
+      <c r="AT46" s="5"/>
+      <c r="AU46" s="5"/>
+      <c r="AV46" s="5"/>
+      <c r="AW46" s="5"/>
+      <c r="AX46" s="5"/>
+      <c r="AY46" s="5"/>
+      <c r="AZ46" s="5"/>
+      <c r="BA46" s="5"/>
+      <c r="BB46" s="5"/>
+      <c r="BC46" s="5"/>
+      <c r="BD46" s="5"/>
+      <c r="BE46" s="5"/>
+      <c r="BF46" s="5"/>
+      <c r="BG46" s="5">
+        <v>515</v>
+      </c>
+      <c r="BH46" s="5"/>
+      <c r="BI46" s="5"/>
+      <c r="BJ46" s="5"/>
+      <c r="BK46" s="5"/>
+      <c r="BL46" s="5"/>
+      <c r="BM46" s="5"/>
+      <c r="BN46" s="5"/>
+      <c r="BO46" s="5"/>
     </row>
   </sheetData>
   <sortState ref="L1:L37">
@@ -13865,12 +14493,12 @@
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
     </row>
     <row r="3" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
@@ -14360,10 +14988,10 @@
       <c r="K8" s="12">
         <v>400</v>
       </c>
-      <c r="P8" s="52" t="s">
+      <c r="P8" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="52"/>
+      <c r="Q8" s="53"/>
       <c r="S8" s="10" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Added details for 25/10/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -21,7 +21,6 @@
     <sheet name="Bathroom" sheetId="15" r:id="rId12"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -7202,9 +7201,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BO46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="BF1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BG1" sqref="BG1"/>
+      <selection pane="topRight" activeCell="BM26" sqref="BM26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7456,11 +7455,11 @@
       </c>
       <c r="B2" s="12">
         <f t="shared" ref="B2:B35" si="1">MAX(E2:ZY2)</f>
-        <v>310.60000000000002</v>
+        <v>322.95</v>
       </c>
       <c r="C2" s="12">
         <f>B2-A2</f>
-        <v>67.000000000000028</v>
+        <v>79.349999999999994</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>115</v>
@@ -7622,7 +7621,9 @@
       <c r="BG2" s="5">
         <v>254.9</v>
       </c>
-      <c r="BH2" s="5"/>
+      <c r="BH2" s="5">
+        <v>322.95</v>
+      </c>
       <c r="BI2" s="5"/>
       <c r="BJ2" s="5"/>
       <c r="BK2" s="5"/>
@@ -7638,11 +7639,11 @@
       </c>
       <c r="B3" s="12">
         <f t="shared" si="1"/>
-        <v>302.7</v>
+        <v>305.35000000000002</v>
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C39" si="2">B3-A3</f>
-        <v>40</v>
+        <v>42.650000000000034</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>114</v>
@@ -7804,7 +7805,9 @@
       <c r="BG3" s="5">
         <v>266.14999999999998</v>
       </c>
-      <c r="BH3" s="5"/>
+      <c r="BH3" s="5">
+        <v>305.35000000000002</v>
+      </c>
       <c r="BI3" s="5"/>
       <c r="BJ3" s="5"/>
       <c r="BK3" s="5"/>
@@ -7992,7 +7995,9 @@
       <c r="BG4" s="5">
         <v>267.10000000000002</v>
       </c>
-      <c r="BH4" s="5"/>
+      <c r="BH4" s="5">
+        <v>269.10000000000002</v>
+      </c>
       <c r="BI4" s="5"/>
       <c r="BJ4" s="5"/>
       <c r="BK4" s="5"/>
@@ -8180,7 +8185,9 @@
       <c r="BG5" s="5">
         <v>936.2</v>
       </c>
-      <c r="BH5" s="5"/>
+      <c r="BH5" s="5">
+        <v>939.3</v>
+      </c>
       <c r="BI5" s="5"/>
       <c r="BJ5" s="5"/>
       <c r="BK5" s="5"/>
@@ -8368,7 +8375,9 @@
       <c r="BG6" s="5">
         <v>289.5</v>
       </c>
-      <c r="BH6" s="5"/>
+      <c r="BH6" s="5">
+        <v>288.55</v>
+      </c>
       <c r="BI6" s="5"/>
       <c r="BJ6" s="5"/>
       <c r="BK6" s="5"/>
@@ -8556,7 +8565,9 @@
       <c r="BG7" s="5">
         <v>17.350000000000001</v>
       </c>
-      <c r="BH7" s="5"/>
+      <c r="BH7" s="5">
+        <v>18.600000000000001</v>
+      </c>
       <c r="BI7" s="5"/>
       <c r="BJ7" s="5"/>
       <c r="BK7" s="5"/>
@@ -8572,11 +8583,11 @@
       </c>
       <c r="B8" s="12">
         <f t="shared" si="1"/>
-        <v>63.3</v>
+        <v>67</v>
       </c>
       <c r="C8" s="12">
         <f t="shared" si="2"/>
-        <v>9.8999999999999986</v>
+        <v>13.600000000000001</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>22</v>
@@ -8744,7 +8755,9 @@
       <c r="BG8" s="5">
         <v>61.6</v>
       </c>
-      <c r="BH8" s="5"/>
+      <c r="BH8" s="5">
+        <v>67</v>
+      </c>
       <c r="BI8" s="5"/>
       <c r="BJ8" s="5"/>
       <c r="BK8" s="5"/>
@@ -8924,7 +8937,9 @@
       <c r="BG9" s="28">
         <v>56.9</v>
       </c>
-      <c r="BH9" s="28"/>
+      <c r="BH9" s="28">
+        <v>57.35</v>
+      </c>
       <c r="BI9" s="28"/>
       <c r="BJ9" s="28"/>
       <c r="BK9" s="28"/>
@@ -9112,7 +9127,9 @@
       <c r="BG10" s="5">
         <v>39.5</v>
       </c>
-      <c r="BH10" s="5"/>
+      <c r="BH10" s="5">
+        <v>40.5</v>
+      </c>
       <c r="BI10" s="5"/>
       <c r="BJ10" s="5"/>
       <c r="BK10" s="5"/>
@@ -9128,11 +9145,11 @@
       </c>
       <c r="B11" s="12">
         <f t="shared" si="1"/>
-        <v>98.4</v>
+        <v>99.1</v>
       </c>
       <c r="C11" s="12">
         <f t="shared" si="2"/>
-        <v>25.75</v>
+        <v>26.449999999999989</v>
       </c>
       <c r="D11" s="45" t="s">
         <v>17</v>
@@ -9300,7 +9317,9 @@
       <c r="BG11" s="5">
         <v>98.4</v>
       </c>
-      <c r="BH11" s="5"/>
+      <c r="BH11" s="5">
+        <v>99.1</v>
+      </c>
       <c r="BI11" s="5"/>
       <c r="BJ11" s="5"/>
       <c r="BK11" s="5"/>
@@ -9316,11 +9335,11 @@
       </c>
       <c r="B12" s="12">
         <f t="shared" si="1"/>
-        <v>88.15</v>
+        <v>90.9</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" si="2"/>
-        <v>5.5</v>
+        <v>8.25</v>
       </c>
       <c r="D12" s="45" t="s">
         <v>18</v>
@@ -9488,7 +9507,9 @@
       <c r="BG12" s="5">
         <v>88.15</v>
       </c>
-      <c r="BH12" s="5"/>
+      <c r="BH12" s="5">
+        <v>90.9</v>
+      </c>
       <c r="BI12" s="5"/>
       <c r="BJ12" s="5"/>
       <c r="BK12" s="5"/>
@@ -9676,7 +9697,9 @@
       <c r="BG13" s="5">
         <v>50.9</v>
       </c>
-      <c r="BH13" s="5"/>
+      <c r="BH13" s="5">
+        <v>50.3</v>
+      </c>
       <c r="BI13" s="5"/>
       <c r="BJ13" s="5"/>
       <c r="BK13" s="5"/>
@@ -9864,7 +9887,9 @@
       <c r="BG14" s="5">
         <v>30.65</v>
       </c>
-      <c r="BH14" s="5"/>
+      <c r="BH14" s="5">
+        <v>31.1</v>
+      </c>
       <c r="BI14" s="5"/>
       <c r="BJ14" s="5"/>
       <c r="BK14" s="5"/>
@@ -10044,7 +10069,9 @@
       <c r="BG15" s="5">
         <v>26.95</v>
       </c>
-      <c r="BH15" s="5"/>
+      <c r="BH15" s="5">
+        <v>27</v>
+      </c>
       <c r="BI15" s="5"/>
       <c r="BJ15" s="5"/>
       <c r="BK15" s="5"/>
@@ -10232,7 +10259,9 @@
       <c r="BG16" s="5">
         <v>718.95</v>
       </c>
-      <c r="BH16" s="5"/>
+      <c r="BH16" s="5">
+        <v>717.1</v>
+      </c>
       <c r="BI16" s="5"/>
       <c r="BJ16" s="5"/>
       <c r="BK16" s="5"/>
@@ -10420,7 +10449,9 @@
       <c r="BG17" s="5">
         <v>469</v>
       </c>
-      <c r="BH17" s="5"/>
+      <c r="BH17" s="5">
+        <v>474</v>
+      </c>
       <c r="BI17" s="5"/>
       <c r="BJ17" s="5"/>
       <c r="BK17" s="5"/>
@@ -10608,7 +10639,9 @@
       <c r="BG18" s="5">
         <v>281.25</v>
       </c>
-      <c r="BH18" s="5"/>
+      <c r="BH18" s="5">
+        <v>274.5</v>
+      </c>
       <c r="BI18" s="5"/>
       <c r="BJ18" s="5"/>
       <c r="BK18" s="5"/>
@@ -10624,11 +10657,11 @@
       </c>
       <c r="B19" s="12">
         <f t="shared" si="1"/>
-        <v>546.25</v>
+        <v>547.95000000000005</v>
       </c>
       <c r="C19" s="12">
         <f t="shared" si="2"/>
-        <v>105.55000000000001</v>
+        <v>107.25000000000006</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -10796,7 +10829,9 @@
       <c r="BG19" s="5">
         <v>546.25</v>
       </c>
-      <c r="BH19" s="5"/>
+      <c r="BH19" s="5">
+        <v>547.95000000000005</v>
+      </c>
       <c r="BI19" s="5"/>
       <c r="BJ19" s="5"/>
       <c r="BK19" s="5"/>
@@ -10984,7 +11019,9 @@
       <c r="BG20" s="5">
         <v>742.5</v>
       </c>
-      <c r="BH20" s="5"/>
+      <c r="BH20" s="5">
+        <v>734.5</v>
+      </c>
       <c r="BI20" s="5"/>
       <c r="BJ20" s="5"/>
       <c r="BK20" s="5"/>
@@ -11000,11 +11037,11 @@
       </c>
       <c r="B21" s="12">
         <f t="shared" si="1"/>
-        <v>500.15</v>
+        <v>514.79999999999995</v>
       </c>
       <c r="C21" s="12">
         <f t="shared" si="2"/>
-        <v>123.44999999999999</v>
+        <v>138.09999999999997</v>
       </c>
       <c r="D21" s="44" t="s">
         <v>106</v>
@@ -11172,7 +11209,9 @@
       <c r="BG21" s="5">
         <v>500.15</v>
       </c>
-      <c r="BH21" s="5"/>
+      <c r="BH21" s="5">
+        <v>514.79999999999995</v>
+      </c>
       <c r="BI21" s="5"/>
       <c r="BJ21" s="5"/>
       <c r="BK21" s="5"/>
@@ -11306,7 +11345,9 @@
       <c r="BG22" s="5">
         <v>335.6</v>
       </c>
-      <c r="BH22" s="5"/>
+      <c r="BH22" s="5">
+        <v>325.14999999999998</v>
+      </c>
       <c r="BI22" s="5"/>
       <c r="BJ22" s="5"/>
       <c r="BK22" s="5"/>
@@ -11486,7 +11527,9 @@
       <c r="BG23" s="5">
         <v>55.2</v>
       </c>
-      <c r="BH23" s="5"/>
+      <c r="BH23" s="5">
+        <v>56.25</v>
+      </c>
       <c r="BI23" s="5"/>
       <c r="BJ23" s="5"/>
       <c r="BK23" s="5"/>
@@ -11662,7 +11705,9 @@
       <c r="BG24" s="5">
         <v>231.1</v>
       </c>
-      <c r="BH24" s="5"/>
+      <c r="BH24" s="5">
+        <v>234.75</v>
+      </c>
       <c r="BI24" s="5"/>
       <c r="BJ24" s="5"/>
       <c r="BK24" s="5"/>
@@ -11820,7 +11865,9 @@
       <c r="BG25" s="5">
         <v>924.35</v>
       </c>
-      <c r="BH25" s="5"/>
+      <c r="BH25" s="5">
+        <v>934.25</v>
+      </c>
       <c r="BI25" s="5"/>
       <c r="BJ25" s="5"/>
       <c r="BK25" s="5"/>
@@ -11832,7 +11879,7 @@
     <row r="26" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <f t="shared" si="0"/>
-        <v>83.5</v>
+        <v>83.1</v>
       </c>
       <c r="B26" s="12">
         <f t="shared" si="1"/>
@@ -11840,7 +11887,7 @@
       </c>
       <c r="C26" s="12">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>12.900000000000006</v>
       </c>
       <c r="D26" s="45" t="s">
         <v>252</v>
@@ -11966,7 +12013,9 @@
       <c r="BG26" s="5">
         <v>84.05</v>
       </c>
-      <c r="BH26" s="5"/>
+      <c r="BH26" s="5">
+        <v>83.1</v>
+      </c>
       <c r="BI26" s="5"/>
       <c r="BJ26" s="5"/>
       <c r="BK26" s="5"/>
@@ -12112,7 +12161,9 @@
       <c r="BG27" s="5">
         <v>40.9</v>
       </c>
-      <c r="BH27" s="5"/>
+      <c r="BH27" s="5">
+        <v>40.65</v>
+      </c>
       <c r="BI27" s="5"/>
       <c r="BJ27" s="5"/>
       <c r="BK27" s="5"/>
@@ -12128,11 +12179,11 @@
       </c>
       <c r="B28" s="12">
         <f t="shared" si="1"/>
-        <v>57.05</v>
+        <v>64.8</v>
       </c>
       <c r="C28" s="12">
         <f t="shared" si="2"/>
-        <v>5.2999999999999972</v>
+        <v>13.049999999999997</v>
       </c>
       <c r="D28" s="45" t="s">
         <v>254</v>
@@ -12258,7 +12309,9 @@
       <c r="BG28" s="5">
         <v>54.05</v>
       </c>
-      <c r="BH28" s="5"/>
+      <c r="BH28" s="5">
+        <v>64.8</v>
+      </c>
       <c r="BI28" s="5"/>
       <c r="BJ28" s="5"/>
       <c r="BK28" s="5"/>
@@ -12404,7 +12457,9 @@
       <c r="BG29" s="5">
         <v>139.69999999999999</v>
       </c>
-      <c r="BH29" s="5"/>
+      <c r="BH29" s="5">
+        <v>140.25</v>
+      </c>
       <c r="BI29" s="5"/>
       <c r="BJ29" s="5"/>
       <c r="BK29" s="5"/>
@@ -12550,7 +12605,9 @@
       <c r="BG30" s="5">
         <v>66.45</v>
       </c>
-      <c r="BH30" s="5"/>
+      <c r="BH30" s="5">
+        <v>65.25</v>
+      </c>
       <c r="BI30" s="5"/>
       <c r="BJ30" s="5"/>
       <c r="BK30" s="5"/>
@@ -12696,7 +12753,9 @@
       <c r="BG31" s="5">
         <v>43.25</v>
       </c>
-      <c r="BH31" s="5"/>
+      <c r="BH31" s="5">
+        <v>43.1</v>
+      </c>
       <c r="BI31" s="5"/>
       <c r="BJ31" s="5"/>
       <c r="BK31" s="5"/>
@@ -12712,11 +12771,11 @@
       </c>
       <c r="B32" s="12">
         <f t="shared" si="1"/>
-        <v>72.2</v>
+        <v>84.5</v>
       </c>
       <c r="C32" s="12">
         <f t="shared" si="2"/>
-        <v>9.6500000000000057</v>
+        <v>21.950000000000003</v>
       </c>
       <c r="D32" s="45" t="s">
         <v>258</v>
@@ -12842,7 +12901,9 @@
       <c r="BG32" s="5">
         <v>72.2</v>
       </c>
-      <c r="BH32" s="5"/>
+      <c r="BH32" s="5">
+        <v>84.5</v>
+      </c>
       <c r="BI32" s="5"/>
       <c r="BJ32" s="5"/>
       <c r="BK32" s="5"/>
@@ -12858,11 +12919,11 @@
       </c>
       <c r="B33" s="12">
         <f t="shared" si="1"/>
-        <v>32.549999999999997</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="C33" s="12">
         <f t="shared" si="2"/>
-        <v>3.3999999999999986</v>
+        <v>7.1499999999999986</v>
       </c>
       <c r="D33" s="45" t="s">
         <v>259</v>
@@ -12988,7 +13049,9 @@
       <c r="BG33" s="5">
         <v>30.4</v>
       </c>
-      <c r="BH33" s="5"/>
+      <c r="BH33" s="5">
+        <v>36.299999999999997</v>
+      </c>
       <c r="BI33" s="5"/>
       <c r="BJ33" s="5"/>
       <c r="BK33" s="5"/>
@@ -13004,11 +13067,11 @@
       </c>
       <c r="B34" s="12">
         <f t="shared" si="1"/>
-        <v>101.75</v>
+        <v>107.4</v>
       </c>
       <c r="C34" s="12">
         <f t="shared" si="2"/>
-        <v>20.200000000000003</v>
+        <v>25.850000000000009</v>
       </c>
       <c r="D34" s="45" t="s">
         <v>260</v>
@@ -13134,7 +13197,9 @@
       <c r="BG34" s="5">
         <v>101.75</v>
       </c>
-      <c r="BH34" s="5"/>
+      <c r="BH34" s="5">
+        <v>107.4</v>
+      </c>
       <c r="BI34" s="5"/>
       <c r="BJ34" s="5"/>
       <c r="BK34" s="5"/>
@@ -13150,11 +13215,11 @@
       </c>
       <c r="B35" s="12">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>141.94999999999999</v>
       </c>
       <c r="C35" s="12">
         <f t="shared" si="2"/>
-        <v>15.049999999999997</v>
+        <v>21.999999999999986</v>
       </c>
       <c r="D35" s="45" t="s">
         <v>261</v>
@@ -13280,7 +13345,9 @@
       <c r="BG35" s="5">
         <v>132.6</v>
       </c>
-      <c r="BH35" s="5"/>
+      <c r="BH35" s="5">
+        <v>141.94999999999999</v>
+      </c>
       <c r="BI35" s="5"/>
       <c r="BJ35" s="5"/>
       <c r="BK35" s="5"/>
@@ -13296,11 +13363,11 @@
       </c>
       <c r="B36" s="12">
         <f t="shared" ref="B36:B38" si="3">MAX(E36:ZY36)</f>
-        <v>148.1</v>
+        <v>184</v>
       </c>
       <c r="C36" s="12">
         <f t="shared" si="2"/>
-        <v>11.400000000000006</v>
+        <v>47.300000000000011</v>
       </c>
       <c r="D36" s="45" t="s">
         <v>262</v>
@@ -13426,7 +13493,9 @@
       <c r="BG36" s="5">
         <v>143.19999999999999</v>
       </c>
-      <c r="BH36" s="5"/>
+      <c r="BH36" s="5">
+        <v>184</v>
+      </c>
       <c r="BI36" s="5"/>
       <c r="BJ36" s="5"/>
       <c r="BK36" s="5"/>
@@ -13572,7 +13641,9 @@
       <c r="BG37" s="5">
         <v>145.9</v>
       </c>
-      <c r="BH37" s="5"/>
+      <c r="BH37" s="5">
+        <v>145.5</v>
+      </c>
       <c r="BI37" s="5"/>
       <c r="BJ37" s="5"/>
       <c r="BK37" s="5"/>
@@ -13706,7 +13777,9 @@
       <c r="BG38" s="5">
         <v>121.8</v>
       </c>
-      <c r="BH38" s="5"/>
+      <c r="BH38" s="5">
+        <v>121.05</v>
+      </c>
       <c r="BI38" s="5"/>
       <c r="BJ38" s="5"/>
       <c r="BK38" s="5"/>
@@ -13718,7 +13791,7 @@
     <row r="39" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <f t="shared" si="0"/>
-        <v>57.85</v>
+        <v>57.65</v>
       </c>
       <c r="B39" s="12">
         <f t="shared" ref="B39" si="4">MAX(E39:ZY39)</f>
@@ -13726,7 +13799,7 @@
       </c>
       <c r="C39" s="12">
         <f t="shared" si="2"/>
-        <v>9.2499999999999929</v>
+        <v>9.4499999999999957</v>
       </c>
       <c r="D39" s="45" t="s">
         <v>277</v>
@@ -13828,7 +13901,9 @@
       <c r="BG39" s="5">
         <v>58.4</v>
       </c>
-      <c r="BH39" s="5"/>
+      <c r="BH39" s="5">
+        <v>57.65</v>
+      </c>
       <c r="BI39" s="5"/>
       <c r="BJ39" s="5"/>
       <c r="BK39" s="5"/>
@@ -13944,7 +14019,9 @@
       <c r="BG40" s="5">
         <v>203.5</v>
       </c>
-      <c r="BH40" s="5"/>
+      <c r="BH40" s="5">
+        <v>198.6</v>
+      </c>
       <c r="BI40" s="5"/>
       <c r="BJ40" s="5"/>
       <c r="BK40" s="5"/>
@@ -14056,7 +14133,9 @@
       <c r="BG41" s="5">
         <v>704.95</v>
       </c>
-      <c r="BH41" s="5"/>
+      <c r="BH41" s="5">
+        <v>678.55</v>
+      </c>
       <c r="BI41" s="5"/>
       <c r="BJ41" s="5"/>
       <c r="BK41" s="5"/>
@@ -14068,7 +14147,7 @@
     <row r="42" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <f t="shared" si="8"/>
-        <v>421.65</v>
+        <v>402.9</v>
       </c>
       <c r="B42" s="12">
         <f t="shared" ref="B42" si="11">MAX(E42:ZY42)</f>
@@ -14076,7 +14155,7 @@
       </c>
       <c r="C42" s="12">
         <f t="shared" ref="C42" si="12">B42-A42</f>
-        <v>98.350000000000023</v>
+        <v>117.10000000000002</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>296</v>
@@ -14150,7 +14229,9 @@
       <c r="BG42" s="5">
         <v>421.65</v>
       </c>
-      <c r="BH42" s="5"/>
+      <c r="BH42" s="5">
+        <v>402.9</v>
+      </c>
       <c r="BI42" s="5"/>
       <c r="BJ42" s="5"/>
       <c r="BK42" s="5"/>
@@ -14166,11 +14247,11 @@
       </c>
       <c r="B43" s="12">
         <f t="shared" ref="B43" si="14">MAX(E43:ZY43)</f>
-        <v>245</v>
+        <v>251.5</v>
       </c>
       <c r="C43" s="12">
         <f t="shared" ref="C43" si="15">B43-A43</f>
-        <v>19</v>
+        <v>25.5</v>
       </c>
       <c r="D43" s="45" t="s">
         <v>303</v>
@@ -14234,7 +14315,9 @@
       <c r="BG43" s="5">
         <v>245</v>
       </c>
-      <c r="BH43" s="5"/>
+      <c r="BH43" s="5">
+        <v>251.5</v>
+      </c>
       <c r="BI43" s="5"/>
       <c r="BJ43" s="5"/>
       <c r="BK43" s="5"/>
@@ -14250,11 +14333,11 @@
       </c>
       <c r="B44" s="12">
         <f t="shared" ref="B44" si="17">MAX(E44:ZY44)</f>
-        <v>532.54999999999995</v>
+        <v>538.9</v>
       </c>
       <c r="C44" s="12">
         <f t="shared" ref="C44" si="18">B44-A44</f>
-        <v>20.549999999999955</v>
+        <v>26.899999999999977</v>
       </c>
       <c r="D44" s="45" t="s">
         <v>304</v>
@@ -14318,7 +14401,9 @@
       <c r="BG44" s="5">
         <v>532.54999999999995</v>
       </c>
-      <c r="BH44" s="5"/>
+      <c r="BH44" s="5">
+        <v>538.9</v>
+      </c>
       <c r="BI44" s="5"/>
       <c r="BJ44" s="5"/>
       <c r="BK44" s="5"/>
@@ -14328,9 +14413,18 @@
       <c r="BO44" s="5"/>
     </row>
     <row r="45" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
+      <c r="A45" s="12">
+        <f t="shared" ref="A45:A46" si="19">MIN(E45:ZY45)</f>
+        <v>156.05000000000001</v>
+      </c>
+      <c r="B45" s="12">
+        <f t="shared" ref="B45:B46" si="20">MAX(E45:ZY45)</f>
+        <v>163.69999999999999</v>
+      </c>
+      <c r="C45" s="12">
+        <f t="shared" ref="C45:C46" si="21">B45-A45</f>
+        <v>7.6499999999999773</v>
+      </c>
       <c r="D45" s="45" t="s">
         <v>305</v>
       </c>
@@ -14391,7 +14485,9 @@
       <c r="BG45" s="5">
         <v>156.05000000000001</v>
       </c>
-      <c r="BH45" s="5"/>
+      <c r="BH45" s="5">
+        <v>163.69999999999999</v>
+      </c>
       <c r="BI45" s="5"/>
       <c r="BJ45" s="5"/>
       <c r="BK45" s="5"/>
@@ -14401,9 +14497,18 @@
       <c r="BO45" s="5"/>
     </row>
     <row r="46" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
+      <c r="A46" s="12">
+        <f t="shared" si="19"/>
+        <v>495.25</v>
+      </c>
+      <c r="B46" s="12">
+        <f t="shared" si="20"/>
+        <v>515</v>
+      </c>
+      <c r="C46" s="12">
+        <f t="shared" si="21"/>
+        <v>19.75</v>
+      </c>
       <c r="D46" s="45" t="s">
         <v>306</v>
       </c>
@@ -14464,7 +14569,9 @@
       <c r="BG46" s="5">
         <v>515</v>
       </c>
-      <c r="BH46" s="5"/>
+      <c r="BH46" s="5">
+        <v>495.25</v>
+      </c>
       <c r="BI46" s="5"/>
       <c r="BJ46" s="5"/>
       <c r="BK46" s="5"/>

</xml_diff>

<commit_message>
Added details for 26/10/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -7202,8 +7202,8 @@
   <dimension ref="A1:BO46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="BF1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BM26" sqref="BM26"/>
+      <pane xSplit="4" topLeftCell="BH1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BI46" sqref="BI46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7624,7 +7624,9 @@
       <c r="BH2" s="5">
         <v>322.95</v>
       </c>
-      <c r="BI2" s="5"/>
+      <c r="BI2" s="5">
+        <v>317.8</v>
+      </c>
       <c r="BJ2" s="5"/>
       <c r="BK2" s="5"/>
       <c r="BL2" s="5"/>
@@ -7808,7 +7810,9 @@
       <c r="BH3" s="5">
         <v>305.35000000000002</v>
       </c>
-      <c r="BI3" s="5"/>
+      <c r="BI3" s="5">
+        <v>298.3</v>
+      </c>
       <c r="BJ3" s="5"/>
       <c r="BK3" s="5"/>
       <c r="BL3" s="5"/>
@@ -7998,7 +8002,9 @@
       <c r="BH4" s="5">
         <v>269.10000000000002</v>
       </c>
-      <c r="BI4" s="5"/>
+      <c r="BI4" s="5">
+        <v>268.25</v>
+      </c>
       <c r="BJ4" s="5"/>
       <c r="BK4" s="5"/>
       <c r="BL4" s="5"/>
@@ -8013,11 +8019,11 @@
       </c>
       <c r="B5" s="12">
         <f t="shared" si="1"/>
-        <v>943.4</v>
+        <v>944.95</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" si="2"/>
-        <v>157.14999999999998</v>
+        <v>158.70000000000005</v>
       </c>
       <c r="D5" s="44" t="s">
         <v>105</v>
@@ -8188,7 +8194,9 @@
       <c r="BH5" s="5">
         <v>939.3</v>
       </c>
-      <c r="BI5" s="5"/>
+      <c r="BI5" s="5">
+        <v>944.95</v>
+      </c>
       <c r="BJ5" s="5"/>
       <c r="BK5" s="5"/>
       <c r="BL5" s="5"/>
@@ -8203,11 +8211,11 @@
       </c>
       <c r="B6" s="12">
         <f t="shared" si="1"/>
-        <v>290.89999999999998</v>
+        <v>293.95</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="2"/>
-        <v>54.449999999999989</v>
+        <v>57.5</v>
       </c>
       <c r="D6" s="45" t="s">
         <v>16</v>
@@ -8378,7 +8386,9 @@
       <c r="BH6" s="5">
         <v>288.55</v>
       </c>
-      <c r="BI6" s="5"/>
+      <c r="BI6" s="5">
+        <v>293.95</v>
+      </c>
       <c r="BJ6" s="5"/>
       <c r="BK6" s="5"/>
       <c r="BL6" s="5"/>
@@ -8568,7 +8578,9 @@
       <c r="BH7" s="5">
         <v>18.600000000000001</v>
       </c>
-      <c r="BI7" s="5"/>
+      <c r="BI7" s="5">
+        <v>18.399999999999999</v>
+      </c>
       <c r="BJ7" s="5"/>
       <c r="BK7" s="5"/>
       <c r="BL7" s="5"/>
@@ -8583,11 +8595,11 @@
       </c>
       <c r="B8" s="12">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>76.849999999999994</v>
       </c>
       <c r="C8" s="12">
         <f t="shared" si="2"/>
-        <v>13.600000000000001</v>
+        <v>23.449999999999996</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>22</v>
@@ -8758,7 +8770,9 @@
       <c r="BH8" s="5">
         <v>67</v>
       </c>
-      <c r="BI8" s="5"/>
+      <c r="BI8" s="5">
+        <v>76.849999999999994</v>
+      </c>
       <c r="BJ8" s="5"/>
       <c r="BK8" s="5"/>
       <c r="BL8" s="5"/>
@@ -8940,7 +8954,9 @@
       <c r="BH9" s="28">
         <v>57.35</v>
       </c>
-      <c r="BI9" s="28"/>
+      <c r="BI9" s="28">
+        <v>57.25</v>
+      </c>
       <c r="BJ9" s="28"/>
       <c r="BK9" s="28"/>
       <c r="BL9" s="28"/>
@@ -9130,7 +9146,9 @@
       <c r="BH10" s="5">
         <v>40.5</v>
       </c>
-      <c r="BI10" s="5"/>
+      <c r="BI10" s="5">
+        <v>39.9</v>
+      </c>
       <c r="BJ10" s="5"/>
       <c r="BK10" s="5"/>
       <c r="BL10" s="5"/>
@@ -9320,7 +9338,9 @@
       <c r="BH11" s="5">
         <v>99.1</v>
       </c>
-      <c r="BI11" s="5"/>
+      <c r="BI11" s="5">
+        <v>96.55</v>
+      </c>
       <c r="BJ11" s="5"/>
       <c r="BK11" s="5"/>
       <c r="BL11" s="5"/>
@@ -9335,11 +9355,11 @@
       </c>
       <c r="B12" s="12">
         <f t="shared" si="1"/>
-        <v>90.9</v>
+        <v>96</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" si="2"/>
-        <v>8.25</v>
+        <v>13.349999999999994</v>
       </c>
       <c r="D12" s="45" t="s">
         <v>18</v>
@@ -9510,7 +9530,9 @@
       <c r="BH12" s="5">
         <v>90.9</v>
       </c>
-      <c r="BI12" s="5"/>
+      <c r="BI12" s="5">
+        <v>96</v>
+      </c>
       <c r="BJ12" s="5"/>
       <c r="BK12" s="5"/>
       <c r="BL12" s="5"/>
@@ -9700,7 +9722,9 @@
       <c r="BH13" s="5">
         <v>50.3</v>
       </c>
-      <c r="BI13" s="5"/>
+      <c r="BI13" s="5">
+        <v>51.2</v>
+      </c>
       <c r="BJ13" s="5"/>
       <c r="BK13" s="5"/>
       <c r="BL13" s="5"/>
@@ -9890,7 +9914,9 @@
       <c r="BH14" s="5">
         <v>31.1</v>
       </c>
-      <c r="BI14" s="5"/>
+      <c r="BI14" s="5">
+        <v>30.85</v>
+      </c>
       <c r="BJ14" s="5"/>
       <c r="BK14" s="5"/>
       <c r="BL14" s="5"/>
@@ -10072,7 +10098,9 @@
       <c r="BH15" s="5">
         <v>27</v>
       </c>
-      <c r="BI15" s="5"/>
+      <c r="BI15" s="5">
+        <v>27.05</v>
+      </c>
       <c r="BJ15" s="5"/>
       <c r="BK15" s="5"/>
       <c r="BL15" s="5"/>
@@ -10087,11 +10115,11 @@
       </c>
       <c r="B16" s="12">
         <f t="shared" si="1"/>
-        <v>718.95</v>
+        <v>729.5</v>
       </c>
       <c r="C16" s="12">
         <f t="shared" si="2"/>
-        <v>166.95000000000005</v>
+        <v>177.5</v>
       </c>
       <c r="D16" s="45" t="s">
         <v>23</v>
@@ -10262,7 +10290,9 @@
       <c r="BH16" s="5">
         <v>717.1</v>
       </c>
-      <c r="BI16" s="5"/>
+      <c r="BI16" s="5">
+        <v>729.5</v>
+      </c>
       <c r="BJ16" s="5"/>
       <c r="BK16" s="5"/>
       <c r="BL16" s="5"/>
@@ -10452,7 +10482,9 @@
       <c r="BH17" s="5">
         <v>474</v>
       </c>
-      <c r="BI17" s="5"/>
+      <c r="BI17" s="5">
+        <v>471</v>
+      </c>
       <c r="BJ17" s="5"/>
       <c r="BK17" s="5"/>
       <c r="BL17" s="5"/>
@@ -10642,7 +10674,9 @@
       <c r="BH18" s="5">
         <v>274.5</v>
       </c>
-      <c r="BI18" s="5"/>
+      <c r="BI18" s="5">
+        <v>279.10000000000002</v>
+      </c>
       <c r="BJ18" s="5"/>
       <c r="BK18" s="5"/>
       <c r="BL18" s="5"/>
@@ -10832,7 +10866,9 @@
       <c r="BH19" s="5">
         <v>547.95000000000005</v>
       </c>
-      <c r="BI19" s="5"/>
+      <c r="BI19" s="5">
+        <v>546.79999999999995</v>
+      </c>
       <c r="BJ19" s="5"/>
       <c r="BK19" s="5"/>
       <c r="BL19" s="5"/>
@@ -11022,7 +11058,9 @@
       <c r="BH20" s="5">
         <v>734.5</v>
       </c>
-      <c r="BI20" s="5"/>
+      <c r="BI20" s="5">
+        <v>753.4</v>
+      </c>
       <c r="BJ20" s="5"/>
       <c r="BK20" s="5"/>
       <c r="BL20" s="5"/>
@@ -11212,7 +11250,9 @@
       <c r="BH21" s="5">
         <v>514.79999999999995</v>
       </c>
-      <c r="BI21" s="5"/>
+      <c r="BI21" s="5">
+        <v>514.04999999999995</v>
+      </c>
       <c r="BJ21" s="5"/>
       <c r="BK21" s="5"/>
       <c r="BL21" s="5"/>
@@ -11348,7 +11388,9 @@
       <c r="BH22" s="5">
         <v>325.14999999999998</v>
       </c>
-      <c r="BI22" s="5"/>
+      <c r="BI22" s="5">
+        <v>322.3</v>
+      </c>
       <c r="BJ22" s="5"/>
       <c r="BK22" s="5"/>
       <c r="BL22" s="5"/>
@@ -11530,7 +11572,9 @@
       <c r="BH23" s="5">
         <v>56.25</v>
       </c>
-      <c r="BI23" s="5"/>
+      <c r="BI23" s="5">
+        <v>57.8</v>
+      </c>
       <c r="BJ23" s="5"/>
       <c r="BK23" s="5"/>
       <c r="BL23" s="5"/>
@@ -11708,7 +11752,9 @@
       <c r="BH24" s="5">
         <v>234.75</v>
       </c>
-      <c r="BI24" s="5"/>
+      <c r="BI24" s="5">
+        <v>230.95</v>
+      </c>
       <c r="BJ24" s="5"/>
       <c r="BK24" s="5"/>
       <c r="BL24" s="5"/>
@@ -11723,11 +11769,11 @@
       </c>
       <c r="B25" s="12">
         <f t="shared" si="1"/>
-        <v>940.3</v>
+        <v>950</v>
       </c>
       <c r="C25" s="12">
         <f t="shared" si="2"/>
-        <v>64.299999999999955</v>
+        <v>74</v>
       </c>
       <c r="D25" s="46" t="s">
         <v>236</v>
@@ -11868,7 +11914,9 @@
       <c r="BH25" s="5">
         <v>934.25</v>
       </c>
-      <c r="BI25" s="5"/>
+      <c r="BI25" s="5">
+        <v>950</v>
+      </c>
       <c r="BJ25" s="5"/>
       <c r="BK25" s="5"/>
       <c r="BL25" s="5"/>
@@ -12016,7 +12064,9 @@
       <c r="BH26" s="5">
         <v>83.1</v>
       </c>
-      <c r="BI26" s="5"/>
+      <c r="BI26" s="5">
+        <v>83.85</v>
+      </c>
       <c r="BJ26" s="5"/>
       <c r="BK26" s="5"/>
       <c r="BL26" s="5"/>
@@ -12164,7 +12214,9 @@
       <c r="BH27" s="5">
         <v>40.65</v>
       </c>
-      <c r="BI27" s="5"/>
+      <c r="BI27" s="5">
+        <v>40.799999999999997</v>
+      </c>
       <c r="BJ27" s="5"/>
       <c r="BK27" s="5"/>
       <c r="BL27" s="5"/>
@@ -12179,11 +12231,11 @@
       </c>
       <c r="B28" s="12">
         <f t="shared" si="1"/>
-        <v>64.8</v>
+        <v>67.599999999999994</v>
       </c>
       <c r="C28" s="12">
         <f t="shared" si="2"/>
-        <v>13.049999999999997</v>
+        <v>15.849999999999994</v>
       </c>
       <c r="D28" s="45" t="s">
         <v>254</v>
@@ -12312,7 +12364,9 @@
       <c r="BH28" s="5">
         <v>64.8</v>
       </c>
-      <c r="BI28" s="5"/>
+      <c r="BI28" s="5">
+        <v>67.599999999999994</v>
+      </c>
       <c r="BJ28" s="5"/>
       <c r="BK28" s="5"/>
       <c r="BL28" s="5"/>
@@ -12460,7 +12514,9 @@
       <c r="BH29" s="5">
         <v>140.25</v>
       </c>
-      <c r="BI29" s="5"/>
+      <c r="BI29" s="5">
+        <v>137.75</v>
+      </c>
       <c r="BJ29" s="5"/>
       <c r="BK29" s="5"/>
       <c r="BL29" s="5"/>
@@ -12608,7 +12664,9 @@
       <c r="BH30" s="5">
         <v>65.25</v>
       </c>
-      <c r="BI30" s="5"/>
+      <c r="BI30" s="5">
+        <v>66.05</v>
+      </c>
       <c r="BJ30" s="5"/>
       <c r="BK30" s="5"/>
       <c r="BL30" s="5"/>
@@ -12756,7 +12814,9 @@
       <c r="BH31" s="5">
         <v>43.1</v>
       </c>
-      <c r="BI31" s="5"/>
+      <c r="BI31" s="5">
+        <v>43.25</v>
+      </c>
       <c r="BJ31" s="5"/>
       <c r="BK31" s="5"/>
       <c r="BL31" s="5"/>
@@ -12904,7 +12964,9 @@
       <c r="BH32" s="5">
         <v>84.5</v>
       </c>
-      <c r="BI32" s="5"/>
+      <c r="BI32" s="5">
+        <v>81.150000000000006</v>
+      </c>
       <c r="BJ32" s="5"/>
       <c r="BK32" s="5"/>
       <c r="BL32" s="5"/>
@@ -13052,7 +13114,9 @@
       <c r="BH33" s="5">
         <v>36.299999999999997</v>
       </c>
-      <c r="BI33" s="5"/>
+      <c r="BI33" s="5">
+        <v>34.25</v>
+      </c>
       <c r="BJ33" s="5"/>
       <c r="BK33" s="5"/>
       <c r="BL33" s="5"/>
@@ -13067,11 +13131,11 @@
       </c>
       <c r="B34" s="12">
         <f t="shared" si="1"/>
-        <v>107.4</v>
+        <v>109.55</v>
       </c>
       <c r="C34" s="12">
         <f t="shared" si="2"/>
-        <v>25.850000000000009</v>
+        <v>28</v>
       </c>
       <c r="D34" s="45" t="s">
         <v>260</v>
@@ -13200,7 +13264,9 @@
       <c r="BH34" s="5">
         <v>107.4</v>
       </c>
-      <c r="BI34" s="5"/>
+      <c r="BI34" s="5">
+        <v>109.55</v>
+      </c>
       <c r="BJ34" s="5"/>
       <c r="BK34" s="5"/>
       <c r="BL34" s="5"/>
@@ -13215,11 +13281,11 @@
       </c>
       <c r="B35" s="12">
         <f t="shared" si="1"/>
-        <v>141.94999999999999</v>
+        <v>143.75</v>
       </c>
       <c r="C35" s="12">
         <f t="shared" si="2"/>
-        <v>21.999999999999986</v>
+        <v>23.799999999999997</v>
       </c>
       <c r="D35" s="45" t="s">
         <v>261</v>
@@ -13348,7 +13414,9 @@
       <c r="BH35" s="5">
         <v>141.94999999999999</v>
       </c>
-      <c r="BI35" s="5"/>
+      <c r="BI35" s="5">
+        <v>143.75</v>
+      </c>
       <c r="BJ35" s="5"/>
       <c r="BK35" s="5"/>
       <c r="BL35" s="5"/>
@@ -13363,11 +13431,11 @@
       </c>
       <c r="B36" s="12">
         <f t="shared" ref="B36:B38" si="3">MAX(E36:ZY36)</f>
-        <v>184</v>
+        <v>184.6</v>
       </c>
       <c r="C36" s="12">
         <f t="shared" si="2"/>
-        <v>47.300000000000011</v>
+        <v>47.900000000000006</v>
       </c>
       <c r="D36" s="45" t="s">
         <v>262</v>
@@ -13496,7 +13564,9 @@
       <c r="BH36" s="5">
         <v>184</v>
       </c>
-      <c r="BI36" s="5"/>
+      <c r="BI36" s="5">
+        <v>184.6</v>
+      </c>
       <c r="BJ36" s="5"/>
       <c r="BK36" s="5"/>
       <c r="BL36" s="5"/>
@@ -13644,7 +13714,9 @@
       <c r="BH37" s="5">
         <v>145.5</v>
       </c>
-      <c r="BI37" s="5"/>
+      <c r="BI37" s="5">
+        <v>145.85</v>
+      </c>
       <c r="BJ37" s="5"/>
       <c r="BK37" s="5"/>
       <c r="BL37" s="5"/>
@@ -13780,7 +13852,9 @@
       <c r="BH38" s="5">
         <v>121.05</v>
       </c>
-      <c r="BI38" s="5"/>
+      <c r="BI38" s="5">
+        <v>116.75</v>
+      </c>
       <c r="BJ38" s="5"/>
       <c r="BK38" s="5"/>
       <c r="BL38" s="5"/>
@@ -13791,7 +13865,7 @@
     <row r="39" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <f t="shared" si="0"/>
-        <v>57.65</v>
+        <v>56.75</v>
       </c>
       <c r="B39" s="12">
         <f t="shared" ref="B39" si="4">MAX(E39:ZY39)</f>
@@ -13799,7 +13873,7 @@
       </c>
       <c r="C39" s="12">
         <f t="shared" si="2"/>
-        <v>9.4499999999999957</v>
+        <v>10.349999999999994</v>
       </c>
       <c r="D39" s="45" t="s">
         <v>277</v>
@@ -13904,7 +13978,9 @@
       <c r="BH39" s="5">
         <v>57.65</v>
       </c>
-      <c r="BI39" s="5"/>
+      <c r="BI39" s="5">
+        <v>56.75</v>
+      </c>
       <c r="BJ39" s="5"/>
       <c r="BK39" s="5"/>
       <c r="BL39" s="5"/>
@@ -14022,7 +14098,9 @@
       <c r="BH40" s="5">
         <v>198.6</v>
       </c>
-      <c r="BI40" s="5"/>
+      <c r="BI40" s="5">
+        <v>202</v>
+      </c>
       <c r="BJ40" s="5"/>
       <c r="BK40" s="5"/>
       <c r="BL40" s="5"/>
@@ -14136,7 +14214,9 @@
       <c r="BH41" s="5">
         <v>678.55</v>
       </c>
-      <c r="BI41" s="5"/>
+      <c r="BI41" s="5">
+        <v>683.7</v>
+      </c>
       <c r="BJ41" s="5"/>
       <c r="BK41" s="5"/>
       <c r="BL41" s="5"/>
@@ -14232,7 +14312,9 @@
       <c r="BH42" s="5">
         <v>402.9</v>
       </c>
-      <c r="BI42" s="5"/>
+      <c r="BI42" s="5">
+        <v>411.1</v>
+      </c>
       <c r="BJ42" s="5"/>
       <c r="BK42" s="5"/>
       <c r="BL42" s="5"/>
@@ -14318,7 +14400,9 @@
       <c r="BH43" s="5">
         <v>251.5</v>
       </c>
-      <c r="BI43" s="5"/>
+      <c r="BI43" s="5">
+        <v>242</v>
+      </c>
       <c r="BJ43" s="5"/>
       <c r="BK43" s="5"/>
       <c r="BL43" s="5"/>
@@ -14404,7 +14488,9 @@
       <c r="BH44" s="5">
         <v>538.9</v>
       </c>
-      <c r="BI44" s="5"/>
+      <c r="BI44" s="5">
+        <v>515.35</v>
+      </c>
       <c r="BJ44" s="5"/>
       <c r="BK44" s="5"/>
       <c r="BL44" s="5"/>
@@ -14419,11 +14505,11 @@
       </c>
       <c r="B45" s="12">
         <f t="shared" ref="B45:B46" si="20">MAX(E45:ZY45)</f>
-        <v>163.69999999999999</v>
+        <v>167.15</v>
       </c>
       <c r="C45" s="12">
         <f t="shared" ref="C45:C46" si="21">B45-A45</f>
-        <v>7.6499999999999773</v>
+        <v>11.099999999999994</v>
       </c>
       <c r="D45" s="45" t="s">
         <v>305</v>
@@ -14488,7 +14574,9 @@
       <c r="BH45" s="5">
         <v>163.69999999999999</v>
       </c>
-      <c r="BI45" s="5"/>
+      <c r="BI45" s="5">
+        <v>167.15</v>
+      </c>
       <c r="BJ45" s="5"/>
       <c r="BK45" s="5"/>
       <c r="BL45" s="5"/>
@@ -14499,7 +14587,7 @@
     <row r="46" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <f t="shared" si="19"/>
-        <v>495.25</v>
+        <v>485.45</v>
       </c>
       <c r="B46" s="12">
         <f t="shared" si="20"/>
@@ -14507,7 +14595,7 @@
       </c>
       <c r="C46" s="12">
         <f t="shared" si="21"/>
-        <v>19.75</v>
+        <v>29.550000000000011</v>
       </c>
       <c r="D46" s="45" t="s">
         <v>306</v>
@@ -14572,7 +14660,9 @@
       <c r="BH46" s="5">
         <v>495.25</v>
       </c>
-      <c r="BI46" s="5"/>
+      <c r="BI46" s="5">
+        <v>485.45</v>
+      </c>
       <c r="BJ46" s="5"/>
       <c r="BK46" s="5"/>
       <c r="BL46" s="5"/>

</xml_diff>

<commit_message>
Added details for 27/10/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="312">
   <si>
     <t>Date</t>
   </si>
@@ -7202,8 +7202,8 @@
   <dimension ref="A1:BO46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="BH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BI46" sqref="BI46"/>
+      <pane xSplit="4" topLeftCell="BI1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BJ46" sqref="BJ46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7627,7 +7627,9 @@
       <c r="BI2" s="5">
         <v>317.8</v>
       </c>
-      <c r="BJ2" s="5"/>
+      <c r="BJ2" s="5">
+        <v>310.60000000000002</v>
+      </c>
       <c r="BK2" s="5"/>
       <c r="BL2" s="5"/>
       <c r="BM2" s="5"/>
@@ -7813,7 +7815,9 @@
       <c r="BI3" s="5">
         <v>298.3</v>
       </c>
-      <c r="BJ3" s="5"/>
+      <c r="BJ3" s="5">
+        <v>302.25</v>
+      </c>
       <c r="BK3" s="5"/>
       <c r="BL3" s="5"/>
       <c r="BM3" s="5"/>
@@ -8005,7 +8009,9 @@
       <c r="BI4" s="5">
         <v>268.25</v>
       </c>
-      <c r="BJ4" s="5"/>
+      <c r="BJ4" s="5">
+        <v>269.3</v>
+      </c>
       <c r="BK4" s="5"/>
       <c r="BL4" s="5"/>
       <c r="BM4" s="5"/>
@@ -8197,7 +8203,9 @@
       <c r="BI5" s="5">
         <v>944.95</v>
       </c>
-      <c r="BJ5" s="5"/>
+      <c r="BJ5" s="5">
+        <v>930.95</v>
+      </c>
       <c r="BK5" s="5"/>
       <c r="BL5" s="5"/>
       <c r="BM5" s="5"/>
@@ -8389,7 +8397,9 @@
       <c r="BI6" s="5">
         <v>293.95</v>
       </c>
-      <c r="BJ6" s="5"/>
+      <c r="BJ6" s="5">
+        <v>288.75</v>
+      </c>
       <c r="BK6" s="5"/>
       <c r="BL6" s="5"/>
       <c r="BM6" s="5"/>
@@ -8581,7 +8591,9 @@
       <c r="BI7" s="5">
         <v>18.399999999999999</v>
       </c>
-      <c r="BJ7" s="5"/>
+      <c r="BJ7" s="5">
+        <v>18.05</v>
+      </c>
       <c r="BK7" s="5"/>
       <c r="BL7" s="5"/>
       <c r="BM7" s="5"/>
@@ -8595,11 +8607,11 @@
       </c>
       <c r="B8" s="12">
         <f t="shared" si="1"/>
-        <v>76.849999999999994</v>
+        <v>79.95</v>
       </c>
       <c r="C8" s="12">
         <f t="shared" si="2"/>
-        <v>23.449999999999996</v>
+        <v>26.550000000000004</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>22</v>
@@ -8773,7 +8785,9 @@
       <c r="BI8" s="5">
         <v>76.849999999999994</v>
       </c>
-      <c r="BJ8" s="5"/>
+      <c r="BJ8" s="5">
+        <v>79.95</v>
+      </c>
       <c r="BK8" s="5"/>
       <c r="BL8" s="5"/>
       <c r="BM8" s="5"/>
@@ -8957,7 +8971,9 @@
       <c r="BI9" s="28">
         <v>57.25</v>
       </c>
-      <c r="BJ9" s="28"/>
+      <c r="BJ9" s="28">
+        <v>56.9</v>
+      </c>
       <c r="BK9" s="28"/>
       <c r="BL9" s="28"/>
       <c r="BM9" s="28"/>
@@ -9149,7 +9165,9 @@
       <c r="BI10" s="5">
         <v>39.9</v>
       </c>
-      <c r="BJ10" s="5"/>
+      <c r="BJ10" s="5">
+        <v>40.65</v>
+      </c>
       <c r="BK10" s="5"/>
       <c r="BL10" s="5"/>
       <c r="BM10" s="5"/>
@@ -9341,7 +9359,9 @@
       <c r="BI11" s="5">
         <v>96.55</v>
       </c>
-      <c r="BJ11" s="5"/>
+      <c r="BJ11" s="5">
+        <v>93.15</v>
+      </c>
       <c r="BK11" s="5"/>
       <c r="BL11" s="5"/>
       <c r="BM11" s="5"/>
@@ -9533,7 +9553,9 @@
       <c r="BI12" s="5">
         <v>96</v>
       </c>
-      <c r="BJ12" s="5"/>
+      <c r="BJ12" s="5">
+        <v>95.1</v>
+      </c>
       <c r="BK12" s="5"/>
       <c r="BL12" s="5"/>
       <c r="BM12" s="5"/>
@@ -9725,7 +9747,9 @@
       <c r="BI13" s="5">
         <v>51.2</v>
       </c>
-      <c r="BJ13" s="5"/>
+      <c r="BJ13" s="5">
+        <v>50.5</v>
+      </c>
       <c r="BK13" s="5"/>
       <c r="BL13" s="5"/>
       <c r="BM13" s="5"/>
@@ -9917,7 +9941,9 @@
       <c r="BI14" s="5">
         <v>30.85</v>
       </c>
-      <c r="BJ14" s="5"/>
+      <c r="BJ14" s="5">
+        <v>30.75</v>
+      </c>
       <c r="BK14" s="5"/>
       <c r="BL14" s="5"/>
       <c r="BM14" s="5"/>
@@ -10101,7 +10127,9 @@
       <c r="BI15" s="5">
         <v>27.05</v>
       </c>
-      <c r="BJ15" s="5"/>
+      <c r="BJ15" s="5">
+        <v>27.05</v>
+      </c>
       <c r="BK15" s="5"/>
       <c r="BL15" s="5"/>
       <c r="BM15" s="5"/>
@@ -10293,7 +10321,9 @@
       <c r="BI16" s="5">
         <v>729.5</v>
       </c>
-      <c r="BJ16" s="5"/>
+      <c r="BJ16" s="5">
+        <v>727.5</v>
+      </c>
       <c r="BK16" s="5"/>
       <c r="BL16" s="5"/>
       <c r="BM16" s="5"/>
@@ -10485,7 +10515,9 @@
       <c r="BI17" s="5">
         <v>471</v>
       </c>
-      <c r="BJ17" s="5"/>
+      <c r="BJ17" s="5">
+        <v>476.2</v>
+      </c>
       <c r="BK17" s="5"/>
       <c r="BL17" s="5"/>
       <c r="BM17" s="5"/>
@@ -10677,7 +10709,9 @@
       <c r="BI18" s="5">
         <v>279.10000000000002</v>
       </c>
-      <c r="BJ18" s="5"/>
+      <c r="BJ18" s="5">
+        <v>280.64999999999998</v>
+      </c>
       <c r="BK18" s="5"/>
       <c r="BL18" s="5"/>
       <c r="BM18" s="5"/>
@@ -10869,7 +10903,9 @@
       <c r="BI19" s="5">
         <v>546.79999999999995</v>
       </c>
-      <c r="BJ19" s="5"/>
+      <c r="BJ19" s="5">
+        <v>538</v>
+      </c>
       <c r="BK19" s="5"/>
       <c r="BL19" s="5"/>
       <c r="BM19" s="5"/>
@@ -11061,7 +11097,9 @@
       <c r="BI20" s="5">
         <v>753.4</v>
       </c>
-      <c r="BJ20" s="5"/>
+      <c r="BJ20" s="5">
+        <v>762.05</v>
+      </c>
       <c r="BK20" s="5"/>
       <c r="BL20" s="5"/>
       <c r="BM20" s="5"/>
@@ -11253,7 +11291,9 @@
       <c r="BI21" s="5">
         <v>514.04999999999995</v>
       </c>
-      <c r="BJ21" s="5"/>
+      <c r="BJ21" s="5">
+        <v>487.45</v>
+      </c>
       <c r="BK21" s="5"/>
       <c r="BL21" s="5"/>
       <c r="BM21" s="5"/>
@@ -11391,7 +11431,9 @@
       <c r="BI22" s="5">
         <v>322.3</v>
       </c>
-      <c r="BJ22" s="5"/>
+      <c r="BJ22" s="5">
+        <v>323.10000000000002</v>
+      </c>
       <c r="BK22" s="5"/>
       <c r="BL22" s="5"/>
       <c r="BM22" s="5"/>
@@ -11575,7 +11617,9 @@
       <c r="BI23" s="5">
         <v>57.8</v>
       </c>
-      <c r="BJ23" s="5"/>
+      <c r="BJ23" s="5">
+        <v>56.7</v>
+      </c>
       <c r="BK23" s="5"/>
       <c r="BL23" s="5"/>
       <c r="BM23" s="5"/>
@@ -11755,7 +11799,9 @@
       <c r="BI24" s="5">
         <v>230.95</v>
       </c>
-      <c r="BJ24" s="5"/>
+      <c r="BJ24" s="5">
+        <v>238</v>
+      </c>
       <c r="BK24" s="5"/>
       <c r="BL24" s="5"/>
       <c r="BM24" s="5"/>
@@ -11917,7 +11963,9 @@
       <c r="BI25" s="5">
         <v>950</v>
       </c>
-      <c r="BJ25" s="5"/>
+      <c r="BJ25" s="5">
+        <v>947</v>
+      </c>
       <c r="BK25" s="5"/>
       <c r="BL25" s="5"/>
       <c r="BM25" s="5"/>
@@ -12067,7 +12115,9 @@
       <c r="BI26" s="5">
         <v>83.85</v>
       </c>
-      <c r="BJ26" s="5"/>
+      <c r="BJ26" s="5">
+        <v>84.2</v>
+      </c>
       <c r="BK26" s="5"/>
       <c r="BL26" s="5"/>
       <c r="BM26" s="5"/>
@@ -12217,7 +12267,9 @@
       <c r="BI27" s="5">
         <v>40.799999999999997</v>
       </c>
-      <c r="BJ27" s="5"/>
+      <c r="BJ27" s="5">
+        <v>40.75</v>
+      </c>
       <c r="BK27" s="5"/>
       <c r="BL27" s="5"/>
       <c r="BM27" s="5"/>
@@ -12367,7 +12419,9 @@
       <c r="BI28" s="5">
         <v>67.599999999999994</v>
       </c>
-      <c r="BJ28" s="5"/>
+      <c r="BJ28" s="5">
+        <v>62.55</v>
+      </c>
       <c r="BK28" s="5"/>
       <c r="BL28" s="5"/>
       <c r="BM28" s="5"/>
@@ -12517,7 +12571,9 @@
       <c r="BI29" s="5">
         <v>137.75</v>
       </c>
-      <c r="BJ29" s="5"/>
+      <c r="BJ29" s="5">
+        <v>136.5</v>
+      </c>
       <c r="BK29" s="5"/>
       <c r="BL29" s="5"/>
       <c r="BM29" s="5"/>
@@ -12667,7 +12723,9 @@
       <c r="BI30" s="5">
         <v>66.05</v>
       </c>
-      <c r="BJ30" s="5"/>
+      <c r="BJ30" s="5">
+        <v>65.3</v>
+      </c>
       <c r="BK30" s="5"/>
       <c r="BL30" s="5"/>
       <c r="BM30" s="5"/>
@@ -12817,7 +12875,9 @@
       <c r="BI31" s="5">
         <v>43.25</v>
       </c>
-      <c r="BJ31" s="5"/>
+      <c r="BJ31" s="5">
+        <v>44.3</v>
+      </c>
       <c r="BK31" s="5"/>
       <c r="BL31" s="5"/>
       <c r="BM31" s="5"/>
@@ -12967,7 +13027,9 @@
       <c r="BI32" s="5">
         <v>81.150000000000006</v>
       </c>
-      <c r="BJ32" s="5"/>
+      <c r="BJ32" s="5">
+        <v>77.150000000000006</v>
+      </c>
       <c r="BK32" s="5"/>
       <c r="BL32" s="5"/>
       <c r="BM32" s="5"/>
@@ -13117,7 +13179,9 @@
       <c r="BI33" s="5">
         <v>34.25</v>
       </c>
-      <c r="BJ33" s="5"/>
+      <c r="BJ33" s="5">
+        <v>32.65</v>
+      </c>
       <c r="BK33" s="5"/>
       <c r="BL33" s="5"/>
       <c r="BM33" s="5"/>
@@ -13267,7 +13331,9 @@
       <c r="BI34" s="5">
         <v>109.55</v>
       </c>
-      <c r="BJ34" s="5"/>
+      <c r="BJ34" s="5">
+        <v>107.8</v>
+      </c>
       <c r="BK34" s="5"/>
       <c r="BL34" s="5"/>
       <c r="BM34" s="5"/>
@@ -13281,11 +13347,11 @@
       </c>
       <c r="B35" s="12">
         <f t="shared" si="1"/>
-        <v>143.75</v>
+        <v>145.69999999999999</v>
       </c>
       <c r="C35" s="12">
         <f t="shared" si="2"/>
-        <v>23.799999999999997</v>
+        <v>25.749999999999986</v>
       </c>
       <c r="D35" s="45" t="s">
         <v>261</v>
@@ -13417,7 +13483,9 @@
       <c r="BI35" s="5">
         <v>143.75</v>
       </c>
-      <c r="BJ35" s="5"/>
+      <c r="BJ35" s="5">
+        <v>145.69999999999999</v>
+      </c>
       <c r="BK35" s="5"/>
       <c r="BL35" s="5"/>
       <c r="BM35" s="5"/>
@@ -13567,7 +13635,9 @@
       <c r="BI36" s="5">
         <v>184.6</v>
       </c>
-      <c r="BJ36" s="5"/>
+      <c r="BJ36" s="5">
+        <v>174.2</v>
+      </c>
       <c r="BK36" s="5"/>
       <c r="BL36" s="5"/>
       <c r="BM36" s="5"/>
@@ -13717,7 +13787,9 @@
       <c r="BI37" s="5">
         <v>145.85</v>
       </c>
-      <c r="BJ37" s="5"/>
+      <c r="BJ37" s="5">
+        <v>145.65</v>
+      </c>
       <c r="BK37" s="5"/>
       <c r="BL37" s="5"/>
       <c r="BM37" s="5"/>
@@ -13855,7 +13927,9 @@
       <c r="BI38" s="5">
         <v>116.75</v>
       </c>
-      <c r="BJ38" s="5"/>
+      <c r="BJ38" s="5">
+        <v>114.8</v>
+      </c>
       <c r="BK38" s="5"/>
       <c r="BL38" s="5"/>
       <c r="BM38" s="5"/>
@@ -13981,7 +14055,9 @@
       <c r="BI39" s="5">
         <v>56.75</v>
       </c>
-      <c r="BJ39" s="5"/>
+      <c r="BJ39" s="5">
+        <v>61.35</v>
+      </c>
       <c r="BK39" s="5"/>
       <c r="BL39" s="5"/>
       <c r="BM39" s="5"/>
@@ -14101,7 +14177,9 @@
       <c r="BI40" s="5">
         <v>202</v>
       </c>
-      <c r="BJ40" s="5"/>
+      <c r="BJ40" s="5">
+        <v>199.05</v>
+      </c>
       <c r="BK40" s="5"/>
       <c r="BL40" s="5"/>
       <c r="BM40" s="5"/>
@@ -14217,7 +14295,9 @@
       <c r="BI41" s="5">
         <v>683.7</v>
       </c>
-      <c r="BJ41" s="5"/>
+      <c r="BJ41" s="5">
+        <v>683</v>
+      </c>
       <c r="BK41" s="5"/>
       <c r="BL41" s="5"/>
       <c r="BM41" s="5"/>
@@ -14315,7 +14395,9 @@
       <c r="BI42" s="5">
         <v>411.1</v>
       </c>
-      <c r="BJ42" s="5"/>
+      <c r="BJ42" s="5">
+        <v>412.1</v>
+      </c>
       <c r="BK42" s="5"/>
       <c r="BL42" s="5"/>
       <c r="BM42" s="5"/>
@@ -14403,7 +14485,9 @@
       <c r="BI43" s="5">
         <v>242</v>
       </c>
-      <c r="BJ43" s="5"/>
+      <c r="BJ43" s="5">
+        <v>245.7</v>
+      </c>
       <c r="BK43" s="5"/>
       <c r="BL43" s="5"/>
       <c r="BM43" s="5"/>
@@ -14413,7 +14497,7 @@
     <row r="44" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <f t="shared" ref="A44" si="16">MIN(E44:ZY44)</f>
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B44" s="12">
         <f t="shared" ref="B44" si="17">MAX(E44:ZY44)</f>
@@ -14421,7 +14505,7 @@
       </c>
       <c r="C44" s="12">
         <f t="shared" ref="C44" si="18">B44-A44</f>
-        <v>26.899999999999977</v>
+        <v>28.899999999999977</v>
       </c>
       <c r="D44" s="45" t="s">
         <v>304</v>
@@ -14491,7 +14575,9 @@
       <c r="BI44" s="5">
         <v>515.35</v>
       </c>
-      <c r="BJ44" s="5"/>
+      <c r="BJ44" s="5">
+        <v>510</v>
+      </c>
       <c r="BK44" s="5"/>
       <c r="BL44" s="5"/>
       <c r="BM44" s="5"/>
@@ -14505,11 +14591,11 @@
       </c>
       <c r="B45" s="12">
         <f t="shared" ref="B45:B46" si="20">MAX(E45:ZY45)</f>
-        <v>167.15</v>
+        <v>173.75</v>
       </c>
       <c r="C45" s="12">
         <f t="shared" ref="C45:C46" si="21">B45-A45</f>
-        <v>11.099999999999994</v>
+        <v>17.699999999999989</v>
       </c>
       <c r="D45" s="45" t="s">
         <v>305</v>
@@ -14577,7 +14663,9 @@
       <c r="BI45" s="5">
         <v>167.15</v>
       </c>
-      <c r="BJ45" s="5"/>
+      <c r="BJ45" s="5">
+        <v>173.75</v>
+      </c>
       <c r="BK45" s="5"/>
       <c r="BL45" s="5"/>
       <c r="BM45" s="5"/>
@@ -14587,7 +14675,7 @@
     <row r="46" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <f t="shared" si="19"/>
-        <v>485.45</v>
+        <v>485.3</v>
       </c>
       <c r="B46" s="12">
         <f t="shared" si="20"/>
@@ -14595,7 +14683,7 @@
       </c>
       <c r="C46" s="12">
         <f t="shared" si="21"/>
-        <v>29.550000000000011</v>
+        <v>29.699999999999989</v>
       </c>
       <c r="D46" s="45" t="s">
         <v>306</v>
@@ -14663,7 +14751,9 @@
       <c r="BI46" s="5">
         <v>485.45</v>
       </c>
-      <c r="BJ46" s="5"/>
+      <c r="BJ46" s="5">
+        <v>485.3</v>
+      </c>
       <c r="BK46" s="5"/>
       <c r="BL46" s="5"/>
       <c r="BM46" s="5"/>
@@ -14825,10 +14915,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14855,7 +14945,7 @@
     <col min="22" max="16384" width="17.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>27</v>
       </c>
@@ -14894,8 +14984,13 @@
         <v>119225</v>
       </c>
       <c r="T1" s="5"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V1" s="5">
+        <f>SUM(W2:W100)</f>
+        <v>121325</v>
+      </c>
+      <c r="W1" s="5"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
@@ -14940,8 +15035,14 @@
       <c r="T2" s="5">
         <v>500</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="W2" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>28</v>
       </c>
@@ -14987,8 +15088,14 @@
       <c r="T3" s="12">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="W3" s="12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>70</v>
       </c>
@@ -15034,8 +15141,14 @@
       <c r="T4" s="12">
         <v>900</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="W4" s="12">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>29</v>
       </c>
@@ -15075,8 +15188,14 @@
       <c r="T5" s="12">
         <v>400</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V5" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="W5" s="12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
@@ -15123,8 +15242,14 @@
       <c r="T6" s="12">
         <v>400</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V6" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="W6" s="12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
@@ -15157,8 +15282,14 @@
       <c r="T7" s="12">
         <v>400</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V7" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="W7" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
@@ -15195,8 +15326,14 @@
       <c r="T8" s="12">
         <v>3000</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W8" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>5</v>
       </c>
@@ -15234,8 +15371,14 @@
       <c r="T9" s="12">
         <v>13000</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V9" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="W9" s="12">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G10" s="6" t="s">
         <v>46</v>
       </c>
@@ -15264,8 +15407,14 @@
       <c r="T10" s="12">
         <v>500</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V10" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="W10" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G11" s="6" t="s">
         <v>47</v>
       </c>
@@ -15296,8 +15445,14 @@
       <c r="T11" s="12">
         <v>12000</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="W11" s="12">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G12" s="6" t="s">
         <v>50</v>
       </c>
@@ -15328,8 +15483,14 @@
       <c r="T12" s="12">
         <v>4300</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V12" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="W12" s="12">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G13" s="6" t="s">
         <v>5</v>
       </c>
@@ -15354,8 +15515,14 @@
       <c r="T13" s="12">
         <v>15000</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V13" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="W13" s="12">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D14" s="19"/>
       <c r="J14" s="10" t="s">
         <v>60</v>
@@ -15375,8 +15542,14 @@
       <c r="T14" s="12">
         <v>20000</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V14" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="W14" s="12">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D15" s="19"/>
       <c r="J15" s="10" t="s">
         <v>61</v>
@@ -15397,8 +15570,14 @@
       <c r="T15" s="12">
         <v>38625</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V15" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="W15" s="12">
+        <v>38625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D16" s="19"/>
       <c r="J16" s="10" t="s">
         <v>62</v>
@@ -15410,6 +15589,12 @@
         <v>13</v>
       </c>
       <c r="T16" s="12">
+        <v>10000</v>
+      </c>
+      <c r="V16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="W16" s="12">
         <v>10000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added share price on 29/10/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="307">
   <si>
     <t>Date</t>
   </si>
@@ -943,6 +943,9 @@
   </si>
   <si>
     <t>DISHTV</t>
+  </si>
+  <si>
+    <t>CHENNPETRO</t>
   </si>
 </sst>
 </file>
@@ -1180,14 +1183,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -7181,11 +7184,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BO39"/>
+  <dimension ref="A1:BO40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="BI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A38" sqref="A38:C39"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="AS1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BI52" sqref="BI52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13734,6 +13737,88 @@
       <c r="BN39" s="5"/>
       <c r="BO39" s="5"/>
     </row>
+    <row r="40" spans="1:67">
+      <c r="A40" s="12">
+        <f t="shared" ref="A40" si="22">MIN(E40:ZY40)</f>
+        <v>446</v>
+      </c>
+      <c r="B40" s="12">
+        <f t="shared" ref="B40" si="23">MAX(E40:ZY40)</f>
+        <v>446</v>
+      </c>
+      <c r="C40" s="12">
+        <f t="shared" ref="C40" si="24">B40-A40</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="45" t="s">
+        <v>306</v>
+      </c>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
+      <c r="S40" s="5"/>
+      <c r="T40" s="5"/>
+      <c r="U40" s="5"/>
+      <c r="V40" s="5"/>
+      <c r="W40" s="5"/>
+      <c r="X40" s="5"/>
+      <c r="Y40" s="5"/>
+      <c r="Z40" s="5"/>
+      <c r="AA40" s="5"/>
+      <c r="AB40" s="5"/>
+      <c r="AC40" s="5"/>
+      <c r="AD40" s="5"/>
+      <c r="AE40" s="5"/>
+      <c r="AF40" s="5"/>
+      <c r="AG40" s="5"/>
+      <c r="AH40" s="5"/>
+      <c r="AI40" s="5"/>
+      <c r="AJ40" s="5"/>
+      <c r="AK40" s="5"/>
+      <c r="AL40" s="5"/>
+      <c r="AM40" s="5"/>
+      <c r="AN40" s="5"/>
+      <c r="AO40" s="5"/>
+      <c r="AP40" s="5"/>
+      <c r="AQ40" s="5"/>
+      <c r="AR40" s="5"/>
+      <c r="AS40" s="5"/>
+      <c r="AT40" s="5"/>
+      <c r="AU40" s="5"/>
+      <c r="AV40" s="5"/>
+      <c r="AW40" s="5"/>
+      <c r="AX40" s="5"/>
+      <c r="AY40" s="5"/>
+      <c r="AZ40" s="5"/>
+      <c r="BA40" s="5"/>
+      <c r="BB40" s="5"/>
+      <c r="BC40" s="5"/>
+      <c r="BD40" s="5"/>
+      <c r="BE40" s="5"/>
+      <c r="BF40" s="5"/>
+      <c r="BG40" s="5"/>
+      <c r="BH40" s="5"/>
+      <c r="BI40" s="5"/>
+      <c r="BJ40" s="5">
+        <v>446</v>
+      </c>
+      <c r="BK40" s="5"/>
+      <c r="BL40" s="5"/>
+      <c r="BM40" s="5"/>
+      <c r="BN40" s="5"/>
+      <c r="BO40" s="5"/>
+    </row>
   </sheetData>
   <sortState ref="L1:L37">
     <sortCondition ref="L13"/>
@@ -13754,12 +13839,12 @@
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="2" spans="2:5" ht="15" customHeight="1">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
     </row>
     <row r="3" spans="2:5" ht="15" customHeight="1">
       <c r="B3" s="7" t="s">
@@ -14290,10 +14375,10 @@
       <c r="K8" s="12">
         <v>400</v>
       </c>
-      <c r="P8" s="53" t="s">
+      <c r="P8" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="53"/>
+      <c r="Q8" s="55"/>
       <c r="S8" s="10" t="s">
         <v>12</v>
       </c>
@@ -15541,13 +15626,13 @@
       <c r="C36" s="31">
         <v>43017</v>
       </c>
-      <c r="I36" s="55" t="s">
+      <c r="I36" s="53" t="s">
         <v>304</v>
       </c>
       <c r="J36" s="26">
         <v>13790</v>
       </c>
-      <c r="K36" s="54">
+      <c r="K36" s="52">
         <v>43037</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added details for 31/10/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="308">
   <si>
     <t>Date</t>
   </si>
@@ -946,6 +946,9 @@
   </si>
   <si>
     <t>CHENNPETRO</t>
+  </si>
+  <si>
+    <t>ADANITRANS</t>
   </si>
 </sst>
 </file>
@@ -7186,11 +7189,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BO40"/>
+  <dimension ref="A1:BO41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="BI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BK40" sqref="BK40"/>
+      <pane xSplit="4" topLeftCell="BL1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CJ41" sqref="CJ41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7620,7 +7623,9 @@
       <c r="BK2" s="5">
         <v>313</v>
       </c>
-      <c r="BL2" s="5"/>
+      <c r="BL2" s="5">
+        <v>305.75</v>
+      </c>
       <c r="BM2" s="5"/>
       <c r="BN2" s="5"/>
       <c r="BO2" s="5"/>
@@ -7810,7 +7815,9 @@
       <c r="BK3" s="5">
         <v>300.64999999999998</v>
       </c>
-      <c r="BL3" s="5"/>
+      <c r="BL3" s="5">
+        <v>300.14999999999998</v>
+      </c>
       <c r="BM3" s="5"/>
       <c r="BN3" s="5"/>
       <c r="BO3" s="5"/>
@@ -8006,7 +8013,9 @@
       <c r="BK4" s="5">
         <v>265.2</v>
       </c>
-      <c r="BL4" s="5"/>
+      <c r="BL4" s="5">
+        <v>266.39999999999998</v>
+      </c>
       <c r="BM4" s="5"/>
       <c r="BN4" s="5"/>
       <c r="BO4" s="5"/>
@@ -8202,7 +8211,9 @@
       <c r="BK5" s="5">
         <v>945.35</v>
       </c>
-      <c r="BL5" s="5"/>
+      <c r="BL5" s="5">
+        <v>939.8</v>
+      </c>
       <c r="BM5" s="5"/>
       <c r="BN5" s="5"/>
       <c r="BO5" s="5"/>
@@ -8398,7 +8409,9 @@
       <c r="BK6" s="5">
         <v>289</v>
       </c>
-      <c r="BL6" s="5"/>
+      <c r="BL6" s="5">
+        <v>286.14999999999998</v>
+      </c>
       <c r="BM6" s="5"/>
       <c r="BN6" s="5"/>
       <c r="BO6" s="5"/>
@@ -8594,7 +8607,9 @@
       <c r="BK7" s="5">
         <v>18.25</v>
       </c>
-      <c r="BL7" s="5"/>
+      <c r="BL7" s="5">
+        <v>19.149999999999999</v>
+      </c>
       <c r="BM7" s="5"/>
       <c r="BN7" s="5"/>
       <c r="BO7" s="5"/>
@@ -8790,7 +8805,9 @@
       <c r="BK8" s="5">
         <v>80</v>
       </c>
-      <c r="BL8" s="5"/>
+      <c r="BL8" s="5">
+        <v>77.8</v>
+      </c>
       <c r="BM8" s="5"/>
       <c r="BN8" s="5"/>
       <c r="BO8" s="5"/>
@@ -8978,7 +8995,9 @@
       <c r="BK9" s="28">
         <v>56</v>
       </c>
-      <c r="BL9" s="28"/>
+      <c r="BL9" s="28">
+        <v>56.65</v>
+      </c>
       <c r="BM9" s="28"/>
       <c r="BN9" s="28"/>
       <c r="BO9" s="28"/>
@@ -9174,7 +9193,9 @@
       <c r="BK10" s="5">
         <v>40.950000000000003</v>
       </c>
-      <c r="BL10" s="5"/>
+      <c r="BL10" s="5">
+        <v>40.85</v>
+      </c>
       <c r="BM10" s="5"/>
       <c r="BN10" s="5"/>
       <c r="BO10" s="5"/>
@@ -9370,7 +9391,9 @@
       <c r="BK11" s="5">
         <v>94.8</v>
       </c>
-      <c r="BL11" s="5"/>
+      <c r="BL11" s="5">
+        <v>93.05</v>
+      </c>
       <c r="BM11" s="5"/>
       <c r="BN11" s="5"/>
       <c r="BO11" s="5"/>
@@ -9382,11 +9405,11 @@
       </c>
       <c r="B12" s="12">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>97.75</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" si="2"/>
-        <v>13.349999999999994</v>
+        <v>15.099999999999994</v>
       </c>
       <c r="D12" s="45" t="s">
         <v>18</v>
@@ -9566,7 +9589,9 @@
       <c r="BK12" s="5">
         <v>95.55</v>
       </c>
-      <c r="BL12" s="5"/>
+      <c r="BL12" s="5">
+        <v>97.75</v>
+      </c>
       <c r="BM12" s="5"/>
       <c r="BN12" s="5"/>
       <c r="BO12" s="5"/>
@@ -9762,7 +9787,9 @@
       <c r="BK13" s="5">
         <v>48.95</v>
       </c>
-      <c r="BL13" s="5"/>
+      <c r="BL13" s="5">
+        <v>51.25</v>
+      </c>
       <c r="BM13" s="5"/>
       <c r="BN13" s="5"/>
       <c r="BO13" s="5"/>
@@ -9958,7 +9985,9 @@
       <c r="BK14" s="5">
         <v>30.85</v>
       </c>
-      <c r="BL14" s="5"/>
+      <c r="BL14" s="5">
+        <v>30.5</v>
+      </c>
       <c r="BM14" s="5"/>
       <c r="BN14" s="5"/>
       <c r="BO14" s="5"/>
@@ -10146,7 +10175,9 @@
       <c r="BK15" s="5">
         <v>27.15</v>
       </c>
-      <c r="BL15" s="5"/>
+      <c r="BL15" s="5">
+        <v>26.6</v>
+      </c>
       <c r="BM15" s="5"/>
       <c r="BN15" s="5"/>
       <c r="BO15" s="5"/>
@@ -10342,7 +10373,9 @@
       <c r="BK16" s="5">
         <v>719.7</v>
       </c>
-      <c r="BL16" s="5"/>
+      <c r="BL16" s="5">
+        <v>703.65</v>
+      </c>
       <c r="BM16" s="5"/>
       <c r="BN16" s="5"/>
       <c r="BO16" s="5"/>
@@ -10538,7 +10571,9 @@
       <c r="BK17" s="5">
         <v>486</v>
       </c>
-      <c r="BL17" s="5"/>
+      <c r="BL17" s="5">
+        <v>481</v>
+      </c>
       <c r="BM17" s="5"/>
       <c r="BN17" s="5"/>
       <c r="BO17" s="5"/>
@@ -10734,7 +10769,9 @@
       <c r="BK18" s="5">
         <v>278.39999999999998</v>
       </c>
-      <c r="BL18" s="5"/>
+      <c r="BL18" s="5">
+        <v>286.2</v>
+      </c>
       <c r="BM18" s="5"/>
       <c r="BN18" s="5"/>
       <c r="BO18" s="5"/>
@@ -10746,11 +10783,11 @@
       </c>
       <c r="B19" s="12">
         <f t="shared" si="1"/>
-        <v>547.95000000000005</v>
+        <v>562.79999999999995</v>
       </c>
       <c r="C19" s="12">
         <f t="shared" si="2"/>
-        <v>107.25000000000006</v>
+        <v>122.09999999999997</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -10930,7 +10967,9 @@
       <c r="BK19" s="5">
         <v>537</v>
       </c>
-      <c r="BL19" s="5"/>
+      <c r="BL19" s="5">
+        <v>562.79999999999995</v>
+      </c>
       <c r="BM19" s="5"/>
       <c r="BN19" s="5"/>
       <c r="BO19" s="5"/>
@@ -11126,7 +11165,9 @@
       <c r="BK20" s="5">
         <v>767.1</v>
       </c>
-      <c r="BL20" s="5"/>
+      <c r="BL20" s="5">
+        <v>759.55</v>
+      </c>
       <c r="BM20" s="5"/>
       <c r="BN20" s="5"/>
       <c r="BO20" s="5"/>
@@ -11322,7 +11363,9 @@
       <c r="BK21" s="5">
         <v>492</v>
       </c>
-      <c r="BL21" s="5"/>
+      <c r="BL21" s="5">
+        <v>497.4</v>
+      </c>
       <c r="BM21" s="5"/>
       <c r="BN21" s="5"/>
       <c r="BO21" s="5"/>
@@ -11464,7 +11507,9 @@
       <c r="BK22" s="5">
         <v>330.4</v>
       </c>
-      <c r="BL22" s="5"/>
+      <c r="BL22" s="5">
+        <v>339.1</v>
+      </c>
       <c r="BM22" s="5"/>
       <c r="BN22" s="5"/>
       <c r="BO22" s="5"/>
@@ -11652,7 +11697,9 @@
       <c r="BK23" s="5">
         <v>59.25</v>
       </c>
-      <c r="BL23" s="5"/>
+      <c r="BL23" s="5">
+        <v>59.1</v>
+      </c>
       <c r="BM23" s="5"/>
       <c r="BN23" s="5"/>
       <c r="BO23" s="5"/>
@@ -11836,7 +11883,9 @@
       <c r="BK24" s="5">
         <v>244.7</v>
       </c>
-      <c r="BL24" s="5"/>
+      <c r="BL24" s="5">
+        <v>240.2</v>
+      </c>
       <c r="BM24" s="5"/>
       <c r="BN24" s="5"/>
       <c r="BO24" s="5"/>
@@ -12002,7 +12051,9 @@
       <c r="BK25" s="5">
         <v>943.9</v>
       </c>
-      <c r="BL25" s="5"/>
+      <c r="BL25" s="5">
+        <v>921.25</v>
+      </c>
       <c r="BM25" s="5"/>
       <c r="BN25" s="5"/>
       <c r="BO25" s="5"/>
@@ -12156,7 +12207,9 @@
       <c r="BK26" s="5">
         <v>86.5</v>
       </c>
-      <c r="BL26" s="5"/>
+      <c r="BL26" s="5">
+        <v>85.55</v>
+      </c>
       <c r="BM26" s="5"/>
       <c r="BN26" s="5"/>
       <c r="BO26" s="5"/>
@@ -12310,7 +12363,9 @@
       <c r="BK27" s="5">
         <v>41.95</v>
       </c>
-      <c r="BL27" s="5"/>
+      <c r="BL27" s="5">
+        <v>43.6</v>
+      </c>
       <c r="BM27" s="5"/>
       <c r="BN27" s="5"/>
       <c r="BO27" s="5"/>
@@ -12464,7 +12519,9 @@
       <c r="BK28" s="5">
         <v>139.5</v>
       </c>
-      <c r="BL28" s="5"/>
+      <c r="BL28" s="5">
+        <v>139.9</v>
+      </c>
       <c r="BM28" s="5"/>
       <c r="BN28" s="5"/>
       <c r="BO28" s="5"/>
@@ -12618,7 +12675,9 @@
       <c r="BK29" s="5">
         <v>67.099999999999994</v>
       </c>
-      <c r="BL29" s="5"/>
+      <c r="BL29" s="5">
+        <v>67.2</v>
+      </c>
       <c r="BM29" s="5"/>
       <c r="BN29" s="5"/>
       <c r="BO29" s="5"/>
@@ -12772,7 +12831,9 @@
       <c r="BK30" s="5">
         <v>44.3</v>
       </c>
-      <c r="BL30" s="5"/>
+      <c r="BL30" s="5">
+        <v>44.8</v>
+      </c>
       <c r="BM30" s="5"/>
       <c r="BN30" s="5"/>
       <c r="BO30" s="5"/>
@@ -12780,7 +12841,7 @@
     <row r="31" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
-        <v>144</v>
+        <v>143.9</v>
       </c>
       <c r="B31" s="12">
         <f t="shared" ref="B31:B32" si="3">MAX(E31:ZY31)</f>
@@ -12788,7 +12849,7 @@
       </c>
       <c r="C31" s="12">
         <f t="shared" si="2"/>
-        <v>12.849999999999994</v>
+        <v>12.949999999999989</v>
       </c>
       <c r="D31" s="45" t="s">
         <v>257</v>
@@ -12926,7 +12987,9 @@
       <c r="BK31" s="5">
         <v>144</v>
       </c>
-      <c r="BL31" s="5"/>
+      <c r="BL31" s="5">
+        <v>143.9</v>
+      </c>
       <c r="BM31" s="5"/>
       <c r="BN31" s="5"/>
       <c r="BO31" s="5"/>
@@ -13068,7 +13131,9 @@
       <c r="BK32" s="5">
         <v>114.8</v>
       </c>
-      <c r="BL32" s="5"/>
+      <c r="BL32" s="5">
+        <v>114.85</v>
+      </c>
       <c r="BM32" s="5"/>
       <c r="BN32" s="5"/>
       <c r="BO32" s="5"/>
@@ -13198,7 +13263,9 @@
       <c r="BK33" s="5">
         <v>61.85</v>
       </c>
-      <c r="BL33" s="5"/>
+      <c r="BL33" s="5">
+        <v>61.25</v>
+      </c>
       <c r="BM33" s="5"/>
       <c r="BN33" s="5"/>
       <c r="BO33" s="5"/>
@@ -13322,7 +13389,9 @@
       <c r="BK34" s="5">
         <v>198</v>
       </c>
-      <c r="BL34" s="5"/>
+      <c r="BL34" s="5">
+        <v>194.75</v>
+      </c>
       <c r="BM34" s="5"/>
       <c r="BN34" s="5"/>
       <c r="BO34" s="5"/>
@@ -13442,7 +13511,9 @@
       <c r="BK35" s="5">
         <v>681</v>
       </c>
-      <c r="BL35" s="5"/>
+      <c r="BL35" s="5">
+        <v>677</v>
+      </c>
       <c r="BM35" s="5"/>
       <c r="BN35" s="5"/>
       <c r="BO35" s="5"/>
@@ -13544,7 +13615,9 @@
       <c r="BK36" s="5">
         <v>411.95</v>
       </c>
-      <c r="BL36" s="5"/>
+      <c r="BL36" s="5">
+        <v>416.7</v>
+      </c>
       <c r="BM36" s="5"/>
       <c r="BN36" s="5"/>
       <c r="BO36" s="5"/>
@@ -13556,11 +13629,11 @@
       </c>
       <c r="B37" s="12">
         <f t="shared" ref="B37" si="14">MAX(E37:ZY37)</f>
-        <v>262.35000000000002</v>
+        <v>270.60000000000002</v>
       </c>
       <c r="C37" s="12">
         <f t="shared" ref="C37" si="15">B37-A37</f>
-        <v>36.350000000000023</v>
+        <v>44.600000000000023</v>
       </c>
       <c r="D37" s="45" t="s">
         <v>297</v>
@@ -13636,7 +13709,9 @@
       <c r="BK37" s="5">
         <v>262.35000000000002</v>
       </c>
-      <c r="BL37" s="5"/>
+      <c r="BL37" s="5">
+        <v>270.60000000000002</v>
+      </c>
       <c r="BM37" s="5"/>
       <c r="BN37" s="5"/>
       <c r="BO37" s="5"/>
@@ -13644,7 +13719,7 @@
     <row r="38" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <f t="shared" ref="A38" si="16">MIN(E38:ZY38)</f>
-        <v>485.3</v>
+        <v>485</v>
       </c>
       <c r="B38" s="12">
         <f t="shared" ref="B38" si="17">MAX(E38:ZY38)</f>
@@ -13652,7 +13727,7 @@
       </c>
       <c r="C38" s="12">
         <f t="shared" ref="C38" si="18">B38-A38</f>
-        <v>29.699999999999989</v>
+        <v>30</v>
       </c>
       <c r="D38" s="45" t="s">
         <v>298</v>
@@ -13726,7 +13801,9 @@
       <c r="BK38" s="5">
         <v>489.65</v>
       </c>
-      <c r="BL38" s="5"/>
+      <c r="BL38" s="5">
+        <v>485</v>
+      </c>
       <c r="BM38" s="5"/>
       <c r="BN38" s="5"/>
       <c r="BO38" s="5"/>
@@ -13810,7 +13887,9 @@
       <c r="BK39" s="5">
         <v>77.900000000000006</v>
       </c>
-      <c r="BL39" s="5"/>
+      <c r="BL39" s="5">
+        <v>77.95</v>
+      </c>
       <c r="BM39" s="5"/>
       <c r="BN39" s="5"/>
       <c r="BO39" s="5"/>
@@ -13822,11 +13901,11 @@
       </c>
       <c r="B40" s="12">
         <f t="shared" ref="B40" si="23">MAX(E40:ZY40)</f>
-        <v>465.55</v>
+        <v>469.15</v>
       </c>
       <c r="C40" s="12">
         <f t="shared" ref="C40" si="24">B40-A40</f>
-        <v>4.5500000000000114</v>
+        <v>8.1499999999999773</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>306</v>
@@ -13894,10 +13973,94 @@
       <c r="BK40" s="5">
         <v>461</v>
       </c>
-      <c r="BL40" s="5"/>
+      <c r="BL40" s="5">
+        <v>469.15</v>
+      </c>
       <c r="BM40" s="5"/>
       <c r="BN40" s="5"/>
       <c r="BO40" s="5"/>
+    </row>
+    <row r="41" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A41" s="12">
+        <f t="shared" ref="A41" si="25">MIN(E41:ZY41)</f>
+        <v>208</v>
+      </c>
+      <c r="B41" s="12">
+        <f t="shared" ref="B41" si="26">MAX(E41:ZY41)</f>
+        <v>208</v>
+      </c>
+      <c r="C41" s="12">
+        <f t="shared" ref="C41" si="27">B41-A41</f>
+        <v>0</v>
+      </c>
+      <c r="D41" s="45" t="s">
+        <v>307</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="5"/>
+      <c r="U41" s="5"/>
+      <c r="V41" s="5"/>
+      <c r="W41" s="5"/>
+      <c r="X41" s="5"/>
+      <c r="Y41" s="5"/>
+      <c r="Z41" s="5"/>
+      <c r="AA41" s="5"/>
+      <c r="AB41" s="5"/>
+      <c r="AC41" s="5"/>
+      <c r="AD41" s="5"/>
+      <c r="AE41" s="5"/>
+      <c r="AF41" s="5"/>
+      <c r="AG41" s="5"/>
+      <c r="AH41" s="5"/>
+      <c r="AI41" s="5"/>
+      <c r="AJ41" s="5"/>
+      <c r="AK41" s="5"/>
+      <c r="AL41" s="5"/>
+      <c r="AM41" s="5"/>
+      <c r="AN41" s="5"/>
+      <c r="AO41" s="5"/>
+      <c r="AP41" s="5"/>
+      <c r="AQ41" s="5"/>
+      <c r="AR41" s="5"/>
+      <c r="AS41" s="5"/>
+      <c r="AT41" s="5"/>
+      <c r="AU41" s="5"/>
+      <c r="AV41" s="5"/>
+      <c r="AW41" s="5"/>
+      <c r="AX41" s="5"/>
+      <c r="AY41" s="5"/>
+      <c r="AZ41" s="5"/>
+      <c r="BA41" s="5"/>
+      <c r="BB41" s="5"/>
+      <c r="BC41" s="5"/>
+      <c r="BD41" s="5"/>
+      <c r="BE41" s="5"/>
+      <c r="BF41" s="5"/>
+      <c r="BG41" s="5"/>
+      <c r="BH41" s="5"/>
+      <c r="BI41" s="5"/>
+      <c r="BJ41" s="5"/>
+      <c r="BK41" s="5"/>
+      <c r="BL41" s="5">
+        <v>208</v>
+      </c>
+      <c r="BM41" s="5"/>
+      <c r="BN41" s="5"/>
+      <c r="BO41" s="5"/>
     </row>
   </sheetData>
   <sortState ref="L1:L37">

</xml_diff>

<commit_message>
Added details for 2/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -1500,7 +1500,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1594,7 +1594,7 @@
       </c>
       <c r="H3" s="4">
         <f>H2-B25</f>
-        <v>95990</v>
+        <v>45990</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1772,8 +1772,12 @@
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="20"/>
+      <c r="A22" s="23">
+        <v>43040</v>
+      </c>
+      <c r="B22" s="20">
+        <v>50000</v>
+      </c>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1792,7 +1796,7 @@
       </c>
       <c r="B25" s="20">
         <f>SUM(B2:B24)</f>
-        <v>462500</v>
+        <v>512500</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -7189,11 +7193,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BO41"/>
+  <dimension ref="A1:BN41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="BL1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CJ41" sqref="CJ41"/>
+      <selection pane="topRight" activeCell="BM9" sqref="BM9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7231,11 +7235,10 @@
     <col min="62" max="62" width="14.42578125" customWidth="1"/>
     <col min="63" max="63" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="14" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12" bestFit="1" customWidth="1"/>
-    <col min="66" max="67" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="65" max="66" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>249</v>
       </c>
@@ -7429,22 +7432,19 @@
         <v>303</v>
       </c>
       <c r="BM1" s="51">
-        <v>42746</v>
+        <v>42777</v>
       </c>
       <c r="BN1" s="51">
-        <v>42777</v>
-      </c>
-      <c r="BO1" s="51">
         <v>42805</v>
       </c>
     </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
-        <f t="shared" ref="A2:A33" si="0">MIN(E2:ZY2)</f>
+        <f>MIN(E2:ZX2)</f>
         <v>243.6</v>
       </c>
       <c r="B2" s="12">
-        <f t="shared" ref="B2:B30" si="1">MAX(E2:ZY2)</f>
+        <f>MAX(E2:ZX2)</f>
         <v>322.95</v>
       </c>
       <c r="C2" s="12">
@@ -7626,22 +7626,23 @@
       <c r="BL2" s="5">
         <v>305.75</v>
       </c>
-      <c r="BM2" s="5"/>
+      <c r="BM2" s="5">
+        <v>314.2</v>
+      </c>
       <c r="BN2" s="5"/>
-      <c r="BO2" s="5"/>
-    </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E3:ZX3)</f>
         <v>262.7</v>
       </c>
       <c r="B3" s="12">
-        <f t="shared" si="1"/>
-        <v>305.35000000000002</v>
+        <f>MAX(E3:ZX3)</f>
+        <v>316.14999999999998</v>
       </c>
       <c r="C3" s="12">
-        <f t="shared" ref="C3:C33" si="2">B3-A3</f>
-        <v>42.650000000000034</v>
+        <f t="shared" ref="C3:C33" si="0">B3-A3</f>
+        <v>53.449999999999989</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>114</v>
@@ -7818,21 +7819,22 @@
       <c r="BL3" s="5">
         <v>300.14999999999998</v>
       </c>
-      <c r="BM3" s="5"/>
+      <c r="BM3" s="5">
+        <v>316.14999999999998</v>
+      </c>
       <c r="BN3" s="5"/>
-      <c r="BO3" s="5"/>
-    </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
+        <f>MIN(E4:ZX4)</f>
+        <v>259.45</v>
+      </c>
+      <c r="B4" s="12">
+        <f>MAX(E4:ZX4)</f>
+        <v>291.7</v>
+      </c>
+      <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>259.45</v>
-      </c>
-      <c r="B4" s="12">
-        <f t="shared" si="1"/>
-        <v>291.7</v>
-      </c>
-      <c r="C4" s="12">
-        <f t="shared" si="2"/>
         <v>32.25</v>
       </c>
       <c r="D4" s="44" t="s">
@@ -8016,22 +8018,23 @@
       <c r="BL4" s="5">
         <v>266.39999999999998</v>
       </c>
-      <c r="BM4" s="5"/>
+      <c r="BM4" s="5">
+        <v>265.8</v>
+      </c>
       <c r="BN4" s="5"/>
-      <c r="BO4" s="5"/>
-    </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
+        <f>MIN(E5:ZX5)</f>
+        <v>786.25</v>
+      </c>
+      <c r="B5" s="12">
+        <f>MAX(E5:ZX5)</f>
+        <v>946.8</v>
+      </c>
+      <c r="C5" s="12">
         <f t="shared" si="0"/>
-        <v>786.25</v>
-      </c>
-      <c r="B5" s="12">
-        <f t="shared" si="1"/>
-        <v>945.35</v>
-      </c>
-      <c r="C5" s="12">
-        <f t="shared" si="2"/>
-        <v>159.10000000000002</v>
+        <v>160.54999999999995</v>
       </c>
       <c r="D5" s="44" t="s">
         <v>105</v>
@@ -8214,21 +8217,22 @@
       <c r="BL5" s="5">
         <v>939.8</v>
       </c>
-      <c r="BM5" s="5"/>
+      <c r="BM5" s="5">
+        <v>946.8</v>
+      </c>
       <c r="BN5" s="5"/>
-      <c r="BO5" s="5"/>
-    </row>
-    <row r="6" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
+        <f>MIN(E6:ZX6)</f>
+        <v>236.45</v>
+      </c>
+      <c r="B6" s="12">
+        <f>MAX(E6:ZX6)</f>
+        <v>293.95</v>
+      </c>
+      <c r="C6" s="12">
         <f t="shared" si="0"/>
-        <v>236.45</v>
-      </c>
-      <c r="B6" s="12">
-        <f t="shared" si="1"/>
-        <v>293.95</v>
-      </c>
-      <c r="C6" s="12">
-        <f t="shared" si="2"/>
         <v>57.5</v>
       </c>
       <c r="D6" s="45" t="s">
@@ -8412,21 +8416,22 @@
       <c r="BL6" s="5">
         <v>286.14999999999998</v>
       </c>
-      <c r="BM6" s="5"/>
+      <c r="BM6" s="5">
+        <v>290.8</v>
+      </c>
       <c r="BN6" s="5"/>
-      <c r="BO6" s="5"/>
-    </row>
-    <row r="7" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
+        <f>MIN(E7:ZX7)</f>
+        <v>15.6</v>
+      </c>
+      <c r="B7" s="12">
+        <f>MAX(E7:ZX7)</f>
+        <v>19.350000000000001</v>
+      </c>
+      <c r="C7" s="12">
         <f t="shared" si="0"/>
-        <v>15.6</v>
-      </c>
-      <c r="B7" s="12">
-        <f t="shared" si="1"/>
-        <v>19.350000000000001</v>
-      </c>
-      <c r="C7" s="12">
-        <f t="shared" si="2"/>
         <v>3.7500000000000018</v>
       </c>
       <c r="D7" s="45" t="s">
@@ -8610,22 +8615,23 @@
       <c r="BL7" s="5">
         <v>19.149999999999999</v>
       </c>
-      <c r="BM7" s="5"/>
+      <c r="BM7" s="5">
+        <v>18.899999999999999</v>
+      </c>
       <c r="BN7" s="5"/>
-      <c r="BO7" s="5"/>
-    </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
+        <f>MIN(E8:ZX8)</f>
+        <v>53.4</v>
+      </c>
+      <c r="B8" s="12">
+        <f>MAX(E8:ZX8)</f>
+        <v>80.150000000000006</v>
+      </c>
+      <c r="C8" s="12">
         <f t="shared" si="0"/>
-        <v>53.4</v>
-      </c>
-      <c r="B8" s="12">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="C8" s="12">
-        <f t="shared" si="2"/>
-        <v>26.6</v>
+        <v>26.750000000000007</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>22</v>
@@ -8808,21 +8814,22 @@
       <c r="BL8" s="5">
         <v>77.8</v>
       </c>
-      <c r="BM8" s="5"/>
+      <c r="BM8" s="5">
+        <v>80.150000000000006</v>
+      </c>
       <c r="BN8" s="5"/>
-      <c r="BO8" s="5"/>
-    </row>
-    <row r="9" spans="1:67" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:66" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
+        <f>MIN(E9:ZX9)</f>
+        <v>53.5</v>
+      </c>
+      <c r="B9" s="39">
+        <f>MAX(E9:ZX9)</f>
+        <v>61</v>
+      </c>
+      <c r="C9" s="12">
         <f t="shared" si="0"/>
-        <v>53.5</v>
-      </c>
-      <c r="B9" s="39">
-        <f t="shared" si="1"/>
-        <v>61</v>
-      </c>
-      <c r="C9" s="12">
-        <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
       <c r="D9" s="43" t="s">
@@ -8998,21 +9005,22 @@
       <c r="BL9" s="28">
         <v>56.65</v>
       </c>
-      <c r="BM9" s="28"/>
+      <c r="BM9" s="28">
+        <v>59.45</v>
+      </c>
       <c r="BN9" s="28"/>
-      <c r="BO9" s="28"/>
-    </row>
-    <row r="10" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
+        <f>MIN(E10:ZX10)</f>
+        <v>38.6</v>
+      </c>
+      <c r="B10" s="12">
+        <f>MAX(E10:ZX10)</f>
+        <v>45.35</v>
+      </c>
+      <c r="C10" s="12">
         <f t="shared" si="0"/>
-        <v>38.6</v>
-      </c>
-      <c r="B10" s="12">
-        <f t="shared" si="1"/>
-        <v>45.35</v>
-      </c>
-      <c r="C10" s="12">
-        <f t="shared" si="2"/>
         <v>6.75</v>
       </c>
       <c r="D10" s="45" t="s">
@@ -9196,22 +9204,23 @@
       <c r="BL10" s="5">
         <v>40.85</v>
       </c>
-      <c r="BM10" s="5"/>
+      <c r="BM10" s="5">
+        <v>41.3</v>
+      </c>
       <c r="BN10" s="5"/>
-      <c r="BO10" s="5"/>
-    </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
+        <f>MIN(E11:ZX11)</f>
+        <v>72.650000000000006</v>
+      </c>
+      <c r="B11" s="12">
+        <f>MAX(E11:ZX11)</f>
+        <v>106.1</v>
+      </c>
+      <c r="C11" s="12">
         <f t="shared" si="0"/>
-        <v>72.650000000000006</v>
-      </c>
-      <c r="B11" s="12">
-        <f t="shared" si="1"/>
-        <v>99.1</v>
-      </c>
-      <c r="C11" s="12">
-        <f t="shared" si="2"/>
-        <v>26.449999999999989</v>
+        <v>33.449999999999989</v>
       </c>
       <c r="D11" s="45" t="s">
         <v>17</v>
@@ -9394,21 +9403,22 @@
       <c r="BL11" s="5">
         <v>93.05</v>
       </c>
-      <c r="BM11" s="5"/>
+      <c r="BM11" s="5">
+        <v>106.1</v>
+      </c>
       <c r="BN11" s="5"/>
-      <c r="BO11" s="5"/>
-    </row>
-    <row r="12" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
+        <f>MIN(E12:ZX12)</f>
+        <v>82.65</v>
+      </c>
+      <c r="B12" s="12">
+        <f>MAX(E12:ZX12)</f>
+        <v>97.75</v>
+      </c>
+      <c r="C12" s="12">
         <f t="shared" si="0"/>
-        <v>82.65</v>
-      </c>
-      <c r="B12" s="12">
-        <f t="shared" si="1"/>
-        <v>97.75</v>
-      </c>
-      <c r="C12" s="12">
-        <f t="shared" si="2"/>
         <v>15.099999999999994</v>
       </c>
       <c r="D12" s="45" t="s">
@@ -9592,21 +9602,22 @@
       <c r="BL12" s="5">
         <v>97.75</v>
       </c>
-      <c r="BM12" s="5"/>
+      <c r="BM12" s="5">
+        <v>97.55</v>
+      </c>
       <c r="BN12" s="5"/>
-      <c r="BO12" s="5"/>
-    </row>
-    <row r="13" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
+        <f>MIN(E13:ZX13)</f>
+        <v>44.1</v>
+      </c>
+      <c r="B13" s="12">
+        <f>MAX(E13:ZX13)</f>
+        <v>57.15</v>
+      </c>
+      <c r="C13" s="12">
         <f t="shared" si="0"/>
-        <v>44.1</v>
-      </c>
-      <c r="B13" s="12">
-        <f t="shared" si="1"/>
-        <v>57.15</v>
-      </c>
-      <c r="C13" s="12">
-        <f t="shared" si="2"/>
         <v>13.049999999999997</v>
       </c>
       <c r="D13" s="45" t="s">
@@ -9790,21 +9801,22 @@
       <c r="BL13" s="5">
         <v>51.25</v>
       </c>
-      <c r="BM13" s="5"/>
+      <c r="BM13" s="5">
+        <v>49.65</v>
+      </c>
       <c r="BN13" s="5"/>
-      <c r="BO13" s="5"/>
-    </row>
-    <row r="14" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
+        <f>MIN(E14:ZX14)</f>
+        <v>29.75</v>
+      </c>
+      <c r="B14" s="12">
+        <f>MAX(E14:ZX14)</f>
+        <v>33.200000000000003</v>
+      </c>
+      <c r="C14" s="12">
         <f t="shared" si="0"/>
-        <v>29.75</v>
-      </c>
-      <c r="B14" s="12">
-        <f t="shared" si="1"/>
-        <v>33.200000000000003</v>
-      </c>
-      <c r="C14" s="12">
-        <f t="shared" si="2"/>
         <v>3.4500000000000028</v>
       </c>
       <c r="D14" s="45" t="s">
@@ -9988,21 +10000,22 @@
       <c r="BL14" s="5">
         <v>30.5</v>
       </c>
-      <c r="BM14" s="5"/>
+      <c r="BM14" s="5">
+        <v>31.8</v>
+      </c>
       <c r="BN14" s="5"/>
-      <c r="BO14" s="5"/>
-    </row>
-    <row r="15" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
+        <f>MIN(E15:ZX15)</f>
+        <v>26.5</v>
+      </c>
+      <c r="B15" s="12">
+        <f>MAX(E15:ZX15)</f>
+        <v>36.4</v>
+      </c>
+      <c r="C15" s="12">
         <f t="shared" si="0"/>
-        <v>26.5</v>
-      </c>
-      <c r="B15" s="12">
-        <f t="shared" si="1"/>
-        <v>36.4</v>
-      </c>
-      <c r="C15" s="12">
-        <f t="shared" si="2"/>
         <v>9.8999999999999986</v>
       </c>
       <c r="D15" s="45" t="s">
@@ -10178,21 +10191,22 @@
       <c r="BL15" s="5">
         <v>26.6</v>
       </c>
-      <c r="BM15" s="5"/>
+      <c r="BM15" s="5">
+        <v>26.5</v>
+      </c>
       <c r="BN15" s="5"/>
-      <c r="BO15" s="5"/>
-    </row>
-    <row r="16" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
+        <f>MIN(E16:ZX16)</f>
+        <v>552</v>
+      </c>
+      <c r="B16" s="12">
+        <f>MAX(E16:ZX16)</f>
+        <v>729.5</v>
+      </c>
+      <c r="C16" s="12">
         <f t="shared" si="0"/>
-        <v>552</v>
-      </c>
-      <c r="B16" s="12">
-        <f t="shared" si="1"/>
-        <v>729.5</v>
-      </c>
-      <c r="C16" s="12">
-        <f t="shared" si="2"/>
         <v>177.5</v>
       </c>
       <c r="D16" s="45" t="s">
@@ -10376,21 +10390,22 @@
       <c r="BL16" s="5">
         <v>703.65</v>
       </c>
-      <c r="BM16" s="5"/>
+      <c r="BM16" s="5">
+        <v>706</v>
+      </c>
       <c r="BN16" s="5"/>
-      <c r="BO16" s="5"/>
-    </row>
-    <row r="17" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
+        <f>MIN(E17:ZX17)</f>
+        <v>433</v>
+      </c>
+      <c r="B17" s="12">
+        <f>MAX(E17:ZX17)</f>
+        <v>515</v>
+      </c>
+      <c r="C17" s="12">
         <f t="shared" si="0"/>
-        <v>433</v>
-      </c>
-      <c r="B17" s="12">
-        <f t="shared" si="1"/>
-        <v>515</v>
-      </c>
-      <c r="C17" s="12">
-        <f t="shared" si="2"/>
         <v>82</v>
       </c>
       <c r="D17" s="44" t="s">
@@ -10574,21 +10589,22 @@
       <c r="BL17" s="5">
         <v>481</v>
       </c>
-      <c r="BM17" s="5"/>
+      <c r="BM17" s="5">
+        <v>488.95</v>
+      </c>
       <c r="BN17" s="5"/>
-      <c r="BO17" s="5"/>
-    </row>
-    <row r="18" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
+        <f>MIN(E18:ZX18)</f>
+        <v>178.8</v>
+      </c>
+      <c r="B18" s="12">
+        <f>MAX(E18:ZX18)</f>
+        <v>297.25</v>
+      </c>
+      <c r="C18" s="12">
         <f t="shared" si="0"/>
-        <v>178.8</v>
-      </c>
-      <c r="B18" s="12">
-        <f t="shared" si="1"/>
-        <v>297.25</v>
-      </c>
-      <c r="C18" s="12">
-        <f t="shared" si="2"/>
         <v>118.44999999999999</v>
       </c>
       <c r="D18" s="44" t="s">
@@ -10772,21 +10788,22 @@
       <c r="BL18" s="5">
         <v>286.2</v>
       </c>
-      <c r="BM18" s="5"/>
+      <c r="BM18" s="5">
+        <v>295.75</v>
+      </c>
       <c r="BN18" s="5"/>
-      <c r="BO18" s="5"/>
-    </row>
-    <row r="19" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
+        <f>MIN(E19:ZX19)</f>
+        <v>440.7</v>
+      </c>
+      <c r="B19" s="12">
+        <f>MAX(E19:ZX19)</f>
+        <v>562.79999999999995</v>
+      </c>
+      <c r="C19" s="12">
         <f t="shared" si="0"/>
-        <v>440.7</v>
-      </c>
-      <c r="B19" s="12">
-        <f t="shared" si="1"/>
-        <v>562.79999999999995</v>
-      </c>
-      <c r="C19" s="12">
-        <f t="shared" si="2"/>
         <v>122.09999999999997</v>
       </c>
       <c r="D19" s="44" t="s">
@@ -10970,22 +10987,23 @@
       <c r="BL19" s="5">
         <v>562.79999999999995</v>
       </c>
-      <c r="BM19" s="5"/>
+      <c r="BM19" s="5">
+        <v>543</v>
+      </c>
       <c r="BN19" s="5"/>
-      <c r="BO19" s="5"/>
-    </row>
-    <row r="20" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
+        <f>MIN(E20:ZX20)</f>
+        <v>677</v>
+      </c>
+      <c r="B20" s="12">
+        <f>MAX(E20:ZX20)</f>
+        <v>790</v>
+      </c>
+      <c r="C20" s="12">
         <f t="shared" si="0"/>
-        <v>677</v>
-      </c>
-      <c r="B20" s="12">
-        <f t="shared" si="1"/>
-        <v>768.55</v>
-      </c>
-      <c r="C20" s="12">
-        <f t="shared" si="2"/>
-        <v>91.549999999999955</v>
+        <v>113</v>
       </c>
       <c r="D20" s="44" t="s">
         <v>104</v>
@@ -11168,22 +11186,23 @@
       <c r="BL20" s="5">
         <v>759.55</v>
       </c>
-      <c r="BM20" s="5"/>
+      <c r="BM20" s="5">
+        <v>790</v>
+      </c>
       <c r="BN20" s="5"/>
-      <c r="BO20" s="5"/>
-    </row>
-    <row r="21" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
+        <f>MIN(E21:ZX21)</f>
+        <v>376.7</v>
+      </c>
+      <c r="B21" s="12">
+        <f>MAX(E21:ZX21)</f>
+        <v>547.5</v>
+      </c>
+      <c r="C21" s="12">
         <f t="shared" si="0"/>
-        <v>376.7</v>
-      </c>
-      <c r="B21" s="12">
-        <f t="shared" si="1"/>
-        <v>514.79999999999995</v>
-      </c>
-      <c r="C21" s="12">
-        <f t="shared" si="2"/>
-        <v>138.09999999999997</v>
+        <v>170.8</v>
       </c>
       <c r="D21" s="44" t="s">
         <v>106</v>
@@ -11366,21 +11385,22 @@
       <c r="BL21" s="5">
         <v>497.4</v>
       </c>
-      <c r="BM21" s="5"/>
+      <c r="BM21" s="5">
+        <v>547.5</v>
+      </c>
       <c r="BN21" s="5"/>
-      <c r="BO21" s="5"/>
-    </row>
-    <row r="22" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
+        <f>MIN(E22:ZX22)</f>
+        <v>315.2</v>
+      </c>
+      <c r="B22" s="12">
+        <f>MAX(E22:ZX22)</f>
+        <v>372.55</v>
+      </c>
+      <c r="C22" s="12">
         <f t="shared" si="0"/>
-        <v>315.2</v>
-      </c>
-      <c r="B22" s="12">
-        <f t="shared" si="1"/>
-        <v>372.55</v>
-      </c>
-      <c r="C22" s="12">
-        <f t="shared" si="2"/>
         <v>57.350000000000023</v>
       </c>
       <c r="D22" s="44" t="s">
@@ -11510,21 +11530,22 @@
       <c r="BL22" s="5">
         <v>339.1</v>
       </c>
-      <c r="BM22" s="5"/>
+      <c r="BM22" s="5">
+        <v>342.55</v>
+      </c>
       <c r="BN22" s="5"/>
-      <c r="BO22" s="5"/>
-    </row>
-    <row r="23" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
+        <f>MIN(E23:ZX23)</f>
+        <v>54.45</v>
+      </c>
+      <c r="B23" s="12">
+        <f>MAX(E23:ZX23)</f>
+        <v>85.65</v>
+      </c>
+      <c r="C23" s="12">
         <f t="shared" si="0"/>
-        <v>54.45</v>
-      </c>
-      <c r="B23" s="12">
-        <f t="shared" si="1"/>
-        <v>85.65</v>
-      </c>
-      <c r="C23" s="12">
-        <f t="shared" si="2"/>
         <v>31.200000000000003</v>
       </c>
       <c r="D23" s="45" t="s">
@@ -11700,21 +11721,22 @@
       <c r="BL23" s="5">
         <v>59.1</v>
       </c>
-      <c r="BM23" s="5"/>
+      <c r="BM23" s="5">
+        <v>58.4</v>
+      </c>
       <c r="BN23" s="5"/>
-      <c r="BO23" s="5"/>
-    </row>
-    <row r="24" spans="1:67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
+        <f>MIN(E24:ZX24)</f>
+        <v>210.65</v>
+      </c>
+      <c r="B24" s="12">
+        <f>MAX(E24:ZX24)</f>
+        <v>255.75</v>
+      </c>
+      <c r="C24" s="12">
         <f t="shared" si="0"/>
-        <v>210.65</v>
-      </c>
-      <c r="B24" s="12">
-        <f t="shared" si="1"/>
-        <v>255.75</v>
-      </c>
-      <c r="C24" s="12">
-        <f t="shared" si="2"/>
         <v>45.099999999999994</v>
       </c>
       <c r="D24" s="45" t="s">
@@ -11886,21 +11908,22 @@
       <c r="BL24" s="5">
         <v>240.2</v>
       </c>
-      <c r="BM24" s="5"/>
+      <c r="BM24" s="5">
+        <v>241.85</v>
+      </c>
       <c r="BN24" s="5"/>
-      <c r="BO24" s="5"/>
-    </row>
-    <row r="25" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
+        <f>MIN(E25:ZX25)</f>
+        <v>876</v>
+      </c>
+      <c r="B25" s="12">
+        <f>MAX(E25:ZX25)</f>
+        <v>950</v>
+      </c>
+      <c r="C25" s="12">
         <f t="shared" si="0"/>
-        <v>876</v>
-      </c>
-      <c r="B25" s="12">
-        <f t="shared" si="1"/>
-        <v>950</v>
-      </c>
-      <c r="C25" s="12">
-        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="D25" s="46" t="s">
@@ -12054,21 +12077,22 @@
       <c r="BL25" s="5">
         <v>921.25</v>
       </c>
-      <c r="BM25" s="5"/>
+      <c r="BM25" s="5">
+        <v>923.1</v>
+      </c>
       <c r="BN25" s="5"/>
-      <c r="BO25" s="5"/>
-    </row>
-    <row r="26" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
+        <f>MIN(E26:ZX26)</f>
+        <v>83.1</v>
+      </c>
+      <c r="B26" s="12">
+        <f>MAX(E26:ZX26)</f>
+        <v>96</v>
+      </c>
+      <c r="C26" s="12">
         <f t="shared" si="0"/>
-        <v>83.1</v>
-      </c>
-      <c r="B26" s="12">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="C26" s="12">
-        <f t="shared" si="2"/>
         <v>12.900000000000006</v>
       </c>
       <c r="D26" s="45" t="s">
@@ -12210,21 +12234,22 @@
       <c r="BL26" s="5">
         <v>85.55</v>
       </c>
-      <c r="BM26" s="5"/>
+      <c r="BM26" s="5">
+        <v>84.1</v>
+      </c>
       <c r="BN26" s="5"/>
-      <c r="BO26" s="5"/>
-    </row>
-    <row r="27" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
+        <f>MIN(E27:ZX27)</f>
+        <v>37.6</v>
+      </c>
+      <c r="B27" s="12">
+        <f>MAX(E27:ZX27)</f>
+        <v>44.75</v>
+      </c>
+      <c r="C27" s="12">
         <f t="shared" si="0"/>
-        <v>37.6</v>
-      </c>
-      <c r="B27" s="12">
-        <f t="shared" si="1"/>
-        <v>44.75</v>
-      </c>
-      <c r="C27" s="12">
-        <f t="shared" si="2"/>
         <v>7.1499999999999986</v>
       </c>
       <c r="D27" s="45" t="s">
@@ -12366,21 +12391,22 @@
       <c r="BL27" s="5">
         <v>43.6</v>
       </c>
-      <c r="BM27" s="5"/>
+      <c r="BM27" s="5">
+        <v>41.65</v>
+      </c>
       <c r="BN27" s="5"/>
-      <c r="BO27" s="5"/>
-    </row>
-    <row r="28" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
+        <f>MIN(E28:ZX28)</f>
+        <v>111.95</v>
+      </c>
+      <c r="B28" s="12">
+        <f>MAX(E28:ZX28)</f>
+        <v>141.65</v>
+      </c>
+      <c r="C28" s="12">
         <f t="shared" si="0"/>
-        <v>111.95</v>
-      </c>
-      <c r="B28" s="12">
-        <f t="shared" si="1"/>
-        <v>141.65</v>
-      </c>
-      <c r="C28" s="12">
-        <f t="shared" si="2"/>
         <v>29.700000000000003</v>
       </c>
       <c r="D28" s="45" t="s">
@@ -12522,21 +12548,22 @@
       <c r="BL28" s="5">
         <v>139.9</v>
       </c>
-      <c r="BM28" s="5"/>
+      <c r="BM28" s="5">
+        <v>141.1</v>
+      </c>
       <c r="BN28" s="5"/>
-      <c r="BO28" s="5"/>
-    </row>
-    <row r="29" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
+        <f>MIN(E29:ZX29)</f>
+        <v>62.3</v>
+      </c>
+      <c r="B29" s="12">
+        <f>MAX(E29:ZX29)</f>
+        <v>78.849999999999994</v>
+      </c>
+      <c r="C29" s="12">
         <f t="shared" si="0"/>
-        <v>62.3</v>
-      </c>
-      <c r="B29" s="12">
-        <f t="shared" si="1"/>
-        <v>78.849999999999994</v>
-      </c>
-      <c r="C29" s="12">
-        <f t="shared" si="2"/>
         <v>16.549999999999997</v>
       </c>
       <c r="D29" s="45" t="s">
@@ -12678,21 +12705,22 @@
       <c r="BL29" s="5">
         <v>67.2</v>
       </c>
-      <c r="BM29" s="5"/>
+      <c r="BM29" s="5">
+        <v>72.650000000000006</v>
+      </c>
       <c r="BN29" s="5"/>
-      <c r="BO29" s="5"/>
-    </row>
-    <row r="30" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
+        <f>MIN(E30:ZX30)</f>
+        <v>39.25</v>
+      </c>
+      <c r="B30" s="12">
+        <f>MAX(E30:ZX30)</f>
+        <v>48.75</v>
+      </c>
+      <c r="C30" s="12">
         <f t="shared" si="0"/>
-        <v>39.25</v>
-      </c>
-      <c r="B30" s="12">
-        <f t="shared" si="1"/>
-        <v>48.75</v>
-      </c>
-      <c r="C30" s="12">
-        <f t="shared" si="2"/>
         <v>9.5</v>
       </c>
       <c r="D30" s="45" t="s">
@@ -12834,22 +12862,23 @@
       <c r="BL30" s="5">
         <v>44.8</v>
       </c>
-      <c r="BM30" s="5"/>
+      <c r="BM30" s="5">
+        <v>47.7</v>
+      </c>
       <c r="BN30" s="5"/>
-      <c r="BO30" s="5"/>
-    </row>
-    <row r="31" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
+        <f>MIN(E31:ZX31)</f>
+        <v>143.30000000000001</v>
+      </c>
+      <c r="B31" s="12">
+        <f>MAX(E31:ZX31)</f>
+        <v>156.85</v>
+      </c>
+      <c r="C31" s="12">
         <f t="shared" si="0"/>
-        <v>143.9</v>
-      </c>
-      <c r="B31" s="12">
-        <f t="shared" ref="B31:B32" si="3">MAX(E31:ZY31)</f>
-        <v>156.85</v>
-      </c>
-      <c r="C31" s="12">
-        <f t="shared" si="2"/>
-        <v>12.949999999999989</v>
+        <v>13.549999999999983</v>
       </c>
       <c r="D31" s="45" t="s">
         <v>257</v>
@@ -12990,21 +13019,22 @@
       <c r="BL31" s="5">
         <v>143.9</v>
       </c>
-      <c r="BM31" s="5"/>
+      <c r="BM31" s="5">
+        <v>143.30000000000001</v>
+      </c>
       <c r="BN31" s="5"/>
-      <c r="BO31" s="5"/>
-    </row>
-    <row r="32" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
+        <f>MIN(E32:ZX32)</f>
+        <v>101.6</v>
+      </c>
+      <c r="B32" s="12">
+        <f>MAX(E32:ZX32)</f>
+        <v>121.8</v>
+      </c>
+      <c r="C32" s="12">
         <f t="shared" si="0"/>
-        <v>101.6</v>
-      </c>
-      <c r="B32" s="12">
-        <f t="shared" si="3"/>
-        <v>121.8</v>
-      </c>
-      <c r="C32" s="12">
-        <f t="shared" si="2"/>
         <v>20.200000000000003</v>
       </c>
       <c r="D32" s="45" t="s">
@@ -13134,21 +13164,22 @@
       <c r="BL32" s="5">
         <v>114.85</v>
       </c>
-      <c r="BM32" s="5"/>
+      <c r="BM32" s="5">
+        <v>115.6</v>
+      </c>
       <c r="BN32" s="5"/>
-      <c r="BO32" s="5"/>
-    </row>
-    <row r="33" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
+        <f>MIN(E33:ZX33)</f>
+        <v>56.75</v>
+      </c>
+      <c r="B33" s="12">
+        <f>MAX(E33:ZX33)</f>
+        <v>67.099999999999994</v>
+      </c>
+      <c r="C33" s="12">
         <f t="shared" si="0"/>
-        <v>56.75</v>
-      </c>
-      <c r="B33" s="12">
-        <f t="shared" ref="B33" si="4">MAX(E33:ZY33)</f>
-        <v>67.099999999999994</v>
-      </c>
-      <c r="C33" s="12">
-        <f t="shared" si="2"/>
         <v>10.349999999999994</v>
       </c>
       <c r="D33" s="45" t="s">
@@ -13266,21 +13297,22 @@
       <c r="BL33" s="5">
         <v>61.25</v>
       </c>
-      <c r="BM33" s="5"/>
+      <c r="BM33" s="5">
+        <v>60.6</v>
+      </c>
       <c r="BN33" s="5"/>
-      <c r="BO33" s="5"/>
-    </row>
-    <row r="34" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
-        <f t="shared" ref="A34" si="5">MIN(E34:ZY34)</f>
+        <f>MIN(E34:ZX34)</f>
         <v>167.9</v>
       </c>
       <c r="B34" s="12">
-        <f t="shared" ref="B34" si="6">MAX(E34:ZY34)</f>
+        <f>MAX(E34:ZX34)</f>
         <v>236.1</v>
       </c>
       <c r="C34" s="12">
-        <f t="shared" ref="C34" si="7">B34-A34</f>
+        <f t="shared" ref="C34" si="1">B34-A34</f>
         <v>68.199999999999989</v>
       </c>
       <c r="D34" s="45" t="s">
@@ -13392,21 +13424,22 @@
       <c r="BL34" s="5">
         <v>194.75</v>
       </c>
-      <c r="BM34" s="5"/>
+      <c r="BM34" s="5">
+        <v>192.9</v>
+      </c>
       <c r="BN34" s="5"/>
-      <c r="BO34" s="5"/>
-    </row>
-    <row r="35" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
-        <f t="shared" ref="A35:A36" si="8">MIN(E35:ZY35)</f>
+        <f>MIN(E35:ZX35)</f>
         <v>661</v>
       </c>
       <c r="B35" s="12">
-        <f t="shared" ref="B35" si="9">MAX(E35:ZY35)</f>
+        <f>MAX(E35:ZX35)</f>
         <v>714.65</v>
       </c>
       <c r="C35" s="12">
-        <f t="shared" ref="C35" si="10">B35-A35</f>
+        <f t="shared" ref="C35" si="2">B35-A35</f>
         <v>53.649999999999977</v>
       </c>
       <c r="D35" s="45" t="s">
@@ -13514,21 +13547,22 @@
       <c r="BL35" s="5">
         <v>677</v>
       </c>
-      <c r="BM35" s="5"/>
+      <c r="BM35" s="5">
+        <v>677</v>
+      </c>
       <c r="BN35" s="5"/>
-      <c r="BO35" s="5"/>
-    </row>
-    <row r="36" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
-        <f t="shared" si="8"/>
+        <f>MIN(E36:ZX36)</f>
         <v>402.9</v>
       </c>
       <c r="B36" s="12">
-        <f t="shared" ref="B36" si="11">MAX(E36:ZY36)</f>
+        <f>MAX(E36:ZX36)</f>
         <v>520</v>
       </c>
       <c r="C36" s="12">
-        <f t="shared" ref="C36" si="12">B36-A36</f>
+        <f t="shared" ref="C36" si="3">B36-A36</f>
         <v>117.10000000000002</v>
       </c>
       <c r="D36" s="45" t="s">
@@ -13618,22 +13652,23 @@
       <c r="BL36" s="5">
         <v>416.7</v>
       </c>
-      <c r="BM36" s="5"/>
+      <c r="BM36" s="5">
+        <v>405.05</v>
+      </c>
       <c r="BN36" s="5"/>
-      <c r="BO36" s="5"/>
-    </row>
-    <row r="37" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
-        <f t="shared" ref="A37" si="13">MIN(E37:ZY37)</f>
+        <f>MIN(E37:ZX37)</f>
         <v>226</v>
       </c>
       <c r="B37" s="12">
-        <f t="shared" ref="B37" si="14">MAX(E37:ZY37)</f>
-        <v>270.60000000000002</v>
+        <f>MAX(E37:ZX37)</f>
+        <v>281</v>
       </c>
       <c r="C37" s="12">
-        <f t="shared" ref="C37" si="15">B37-A37</f>
-        <v>44.600000000000023</v>
+        <f t="shared" ref="C37" si="4">B37-A37</f>
+        <v>55</v>
       </c>
       <c r="D37" s="45" t="s">
         <v>297</v>
@@ -13712,21 +13747,22 @@
       <c r="BL37" s="5">
         <v>270.60000000000002</v>
       </c>
-      <c r="BM37" s="5"/>
+      <c r="BM37" s="5">
+        <v>281</v>
+      </c>
       <c r="BN37" s="5"/>
-      <c r="BO37" s="5"/>
-    </row>
-    <row r="38" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
-        <f t="shared" ref="A38" si="16">MIN(E38:ZY38)</f>
+        <f>MIN(E38:ZX38)</f>
         <v>485</v>
       </c>
       <c r="B38" s="12">
-        <f t="shared" ref="B38" si="17">MAX(E38:ZY38)</f>
+        <f>MAX(E38:ZX38)</f>
         <v>515</v>
       </c>
       <c r="C38" s="12">
-        <f t="shared" ref="C38" si="18">B38-A38</f>
+        <f t="shared" ref="C38" si="5">B38-A38</f>
         <v>30</v>
       </c>
       <c r="D38" s="45" t="s">
@@ -13804,22 +13840,23 @@
       <c r="BL38" s="5">
         <v>485</v>
       </c>
-      <c r="BM38" s="5"/>
+      <c r="BM38" s="5">
+        <v>496.6</v>
+      </c>
       <c r="BN38" s="5"/>
-      <c r="BO38" s="5"/>
-    </row>
-    <row r="39" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
-        <f t="shared" ref="A39" si="19">MIN(E39:ZY39)</f>
-        <v>77.900000000000006</v>
+        <f>MIN(E39:ZX39)</f>
+        <v>76</v>
       </c>
       <c r="B39" s="12">
-        <f t="shared" ref="B39" si="20">MAX(E39:ZY39)</f>
+        <f>MAX(E39:ZX39)</f>
         <v>78</v>
       </c>
       <c r="C39" s="12">
-        <f t="shared" ref="C39" si="21">B39-A39</f>
-        <v>9.9999999999994316E-2</v>
+        <f t="shared" ref="C39" si="6">B39-A39</f>
+        <v>2</v>
       </c>
       <c r="D39" s="45" t="s">
         <v>305</v>
@@ -13890,21 +13927,22 @@
       <c r="BL39" s="5">
         <v>77.95</v>
       </c>
-      <c r="BM39" s="5"/>
+      <c r="BM39" s="5">
+        <v>76</v>
+      </c>
       <c r="BN39" s="5"/>
-      <c r="BO39" s="5"/>
-    </row>
-    <row r="40" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
-        <f t="shared" ref="A40" si="22">MIN(E40:ZY40)</f>
+        <f>MIN(E40:ZX40)</f>
         <v>461</v>
       </c>
       <c r="B40" s="12">
-        <f t="shared" ref="B40" si="23">MAX(E40:ZY40)</f>
+        <f>MAX(E40:ZX40)</f>
         <v>469.15</v>
       </c>
       <c r="C40" s="12">
-        <f t="shared" ref="C40" si="24">B40-A40</f>
+        <f t="shared" ref="C40" si="7">B40-A40</f>
         <v>8.1499999999999773</v>
       </c>
       <c r="D40" s="45" t="s">
@@ -13976,22 +14014,23 @@
       <c r="BL40" s="5">
         <v>469.15</v>
       </c>
-      <c r="BM40" s="5"/>
+      <c r="BM40" s="5">
+        <v>466</v>
+      </c>
       <c r="BN40" s="5"/>
-      <c r="BO40" s="5"/>
-    </row>
-    <row r="41" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
-        <f t="shared" ref="A41" si="25">MIN(E41:ZY41)</f>
+        <f>MIN(E41:ZX41)</f>
         <v>208</v>
       </c>
       <c r="B41" s="12">
-        <f t="shared" ref="B41" si="26">MAX(E41:ZY41)</f>
-        <v>208</v>
+        <f>MAX(E41:ZX41)</f>
+        <v>209.8</v>
       </c>
       <c r="C41" s="12">
-        <f t="shared" ref="C41" si="27">B41-A41</f>
-        <v>0</v>
+        <f t="shared" ref="C41" si="8">B41-A41</f>
+        <v>1.8000000000000114</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>307</v>
@@ -14058,9 +14097,10 @@
       <c r="BL41" s="5">
         <v>208</v>
       </c>
-      <c r="BM41" s="5"/>
+      <c r="BM41" s="5">
+        <v>209.8</v>
+      </c>
       <c r="BN41" s="5"/>
-      <c r="BO41" s="5"/>
     </row>
   </sheetData>
   <sortState ref="L1:L37">
@@ -14220,7 +14260,7 @@
   <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added details for 3/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="311">
   <si>
     <t>Date</t>
   </si>
@@ -949,6 +949,15 @@
   </si>
   <si>
     <t>ADANITRANS</t>
+  </si>
+  <si>
+    <t>MANINFRA</t>
+  </si>
+  <si>
+    <t>ANANTRAJ</t>
+  </si>
+  <si>
+    <t>HCC</t>
   </si>
 </sst>
 </file>
@@ -7193,11 +7202,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BN41"/>
+  <dimension ref="A1:BS44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="BL1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BM9" sqref="BM9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="BK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BR27" sqref="BR27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7235,10 +7244,11 @@
     <col min="62" max="62" width="14.42578125" customWidth="1"/>
     <col min="63" max="63" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="14" bestFit="1" customWidth="1"/>
-    <col min="65" max="66" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="65" max="70" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:71" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>249</v>
       </c>
@@ -7437,19 +7447,34 @@
       <c r="BN1" s="51">
         <v>42805</v>
       </c>
-    </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BO1" s="51">
+        <v>42897</v>
+      </c>
+      <c r="BP1" s="51">
+        <v>42927</v>
+      </c>
+      <c r="BQ1" s="51">
+        <v>42958</v>
+      </c>
+      <c r="BR1" s="51">
+        <v>42989</v>
+      </c>
+      <c r="BS1" s="51">
+        <v>43019</v>
+      </c>
+    </row>
+    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
-        <f>MIN(E2:ZX2)</f>
+        <f t="shared" ref="A2:A41" si="0">MIN(E2:ZX2)</f>
         <v>243.6</v>
       </c>
       <c r="B2" s="12">
-        <f>MAX(E2:ZX2)</f>
-        <v>322.95</v>
+        <f t="shared" ref="B2:B41" si="1">MAX(E2:ZX2)</f>
+        <v>326</v>
       </c>
       <c r="C2" s="12">
         <f>B2-A2</f>
-        <v>79.349999999999994</v>
+        <v>82.4</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>115</v>
@@ -7629,19 +7654,26 @@
       <c r="BM2" s="5">
         <v>314.2</v>
       </c>
-      <c r="BN2" s="5"/>
-    </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN2" s="5">
+        <v>326</v>
+      </c>
+      <c r="BO2" s="5"/>
+      <c r="BP2" s="5"/>
+      <c r="BQ2" s="5"/>
+      <c r="BR2" s="5"/>
+      <c r="BS2" s="5"/>
+    </row>
+    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
-        <f>MIN(E3:ZX3)</f>
+        <f t="shared" si="0"/>
         <v>262.7</v>
       </c>
       <c r="B3" s="12">
-        <f>MAX(E3:ZX3)</f>
+        <f t="shared" si="1"/>
         <v>316.14999999999998</v>
       </c>
       <c r="C3" s="12">
-        <f t="shared" ref="C3:C33" si="0">B3-A3</f>
+        <f t="shared" ref="C3:C33" si="2">B3-A3</f>
         <v>53.449999999999989</v>
       </c>
       <c r="D3" s="44" t="s">
@@ -7822,19 +7854,26 @@
       <c r="BM3" s="5">
         <v>316.14999999999998</v>
       </c>
-      <c r="BN3" s="5"/>
-    </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN3" s="5">
+        <v>315.2</v>
+      </c>
+      <c r="BO3" s="5"/>
+      <c r="BP3" s="5"/>
+      <c r="BQ3" s="5"/>
+      <c r="BR3" s="5"/>
+      <c r="BS3" s="5"/>
+    </row>
+    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
-        <f>MIN(E4:ZX4)</f>
+        <f t="shared" si="0"/>
         <v>259.45</v>
       </c>
       <c r="B4" s="12">
-        <f>MAX(E4:ZX4)</f>
+        <f t="shared" si="1"/>
         <v>291.7</v>
       </c>
       <c r="C4" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>32.25</v>
       </c>
       <c r="D4" s="44" t="s">
@@ -8021,19 +8060,26 @@
       <c r="BM4" s="5">
         <v>265.8</v>
       </c>
-      <c r="BN4" s="5"/>
-    </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN4" s="5">
+        <v>265.64999999999998</v>
+      </c>
+      <c r="BO4" s="5"/>
+      <c r="BP4" s="5"/>
+      <c r="BQ4" s="5"/>
+      <c r="BR4" s="5"/>
+      <c r="BS4" s="5"/>
+    </row>
+    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
-        <f>MIN(E5:ZX5)</f>
+        <f t="shared" si="0"/>
         <v>786.25</v>
       </c>
       <c r="B5" s="12">
-        <f>MAX(E5:ZX5)</f>
+        <f t="shared" si="1"/>
         <v>946.8</v>
       </c>
       <c r="C5" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>160.54999999999995</v>
       </c>
       <c r="D5" s="44" t="s">
@@ -8220,19 +8266,26 @@
       <c r="BM5" s="5">
         <v>946.8</v>
       </c>
-      <c r="BN5" s="5"/>
-    </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN5" s="5">
+        <v>945.95</v>
+      </c>
+      <c r="BO5" s="5"/>
+      <c r="BP5" s="5"/>
+      <c r="BQ5" s="5"/>
+      <c r="BR5" s="5"/>
+      <c r="BS5" s="5"/>
+    </row>
+    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
-        <f>MIN(E6:ZX6)</f>
+        <f t="shared" si="0"/>
         <v>236.45</v>
       </c>
       <c r="B6" s="12">
-        <f>MAX(E6:ZX6)</f>
+        <f t="shared" si="1"/>
         <v>293.95</v>
       </c>
       <c r="C6" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>57.5</v>
       </c>
       <c r="D6" s="45" t="s">
@@ -8419,19 +8472,26 @@
       <c r="BM6" s="5">
         <v>290.8</v>
       </c>
-      <c r="BN6" s="5"/>
-    </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN6" s="5">
+        <v>286.5</v>
+      </c>
+      <c r="BO6" s="5"/>
+      <c r="BP6" s="5"/>
+      <c r="BQ6" s="5"/>
+      <c r="BR6" s="5"/>
+      <c r="BS6" s="5"/>
+    </row>
+    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
-        <f>MIN(E7:ZX7)</f>
+        <f t="shared" si="0"/>
         <v>15.6</v>
       </c>
       <c r="B7" s="12">
-        <f>MAX(E7:ZX7)</f>
+        <f t="shared" si="1"/>
         <v>19.350000000000001</v>
       </c>
       <c r="C7" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.7500000000000018</v>
       </c>
       <c r="D7" s="45" t="s">
@@ -8618,20 +8678,27 @@
       <c r="BM7" s="5">
         <v>18.899999999999999</v>
       </c>
-      <c r="BN7" s="5"/>
-    </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN7" s="5">
+        <v>19.05</v>
+      </c>
+      <c r="BO7" s="5"/>
+      <c r="BP7" s="5"/>
+      <c r="BQ7" s="5"/>
+      <c r="BR7" s="5"/>
+      <c r="BS7" s="5"/>
+    </row>
+    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
-        <f>MIN(E8:ZX8)</f>
+        <f t="shared" si="0"/>
         <v>53.4</v>
       </c>
       <c r="B8" s="12">
-        <f>MAX(E8:ZX8)</f>
-        <v>80.150000000000006</v>
+        <f t="shared" si="1"/>
+        <v>86.75</v>
       </c>
       <c r="C8" s="12">
-        <f t="shared" si="0"/>
-        <v>26.750000000000007</v>
+        <f t="shared" si="2"/>
+        <v>33.35</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>22</v>
@@ -8817,19 +8884,26 @@
       <c r="BM8" s="5">
         <v>80.150000000000006</v>
       </c>
-      <c r="BN8" s="5"/>
-    </row>
-    <row r="9" spans="1:66" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BN8" s="5">
+        <v>86.75</v>
+      </c>
+      <c r="BO8" s="5"/>
+      <c r="BP8" s="5"/>
+      <c r="BQ8" s="5"/>
+      <c r="BR8" s="5"/>
+      <c r="BS8" s="5"/>
+    </row>
+    <row r="9" spans="1:71" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
-        <f>MIN(E9:ZX9)</f>
+        <f t="shared" si="0"/>
         <v>53.5</v>
       </c>
       <c r="B9" s="39">
-        <f>MAX(E9:ZX9)</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="C9" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
       <c r="D9" s="43" t="s">
@@ -9008,19 +9082,26 @@
       <c r="BM9" s="28">
         <v>59.45</v>
       </c>
-      <c r="BN9" s="28"/>
-    </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN9" s="28">
+        <v>58.9</v>
+      </c>
+      <c r="BO9" s="28"/>
+      <c r="BP9" s="28"/>
+      <c r="BQ9" s="28"/>
+      <c r="BR9" s="28"/>
+      <c r="BS9" s="28"/>
+    </row>
+    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
-        <f>MIN(E10:ZX10)</f>
+        <f t="shared" si="0"/>
         <v>38.6</v>
       </c>
       <c r="B10" s="12">
-        <f>MAX(E10:ZX10)</f>
+        <f t="shared" si="1"/>
         <v>45.35</v>
       </c>
       <c r="C10" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.75</v>
       </c>
       <c r="D10" s="45" t="s">
@@ -9207,20 +9288,27 @@
       <c r="BM10" s="5">
         <v>41.3</v>
       </c>
-      <c r="BN10" s="5"/>
-    </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN10" s="5">
+        <v>41.05</v>
+      </c>
+      <c r="BO10" s="5"/>
+      <c r="BP10" s="5"/>
+      <c r="BQ10" s="5"/>
+      <c r="BR10" s="5"/>
+      <c r="BS10" s="5"/>
+    </row>
+    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
-        <f>MIN(E11:ZX11)</f>
+        <f t="shared" si="0"/>
         <v>72.650000000000006</v>
       </c>
       <c r="B11" s="12">
-        <f>MAX(E11:ZX11)</f>
-        <v>106.1</v>
+        <f t="shared" si="1"/>
+        <v>106.5</v>
       </c>
       <c r="C11" s="12">
-        <f t="shared" si="0"/>
-        <v>33.449999999999989</v>
+        <f t="shared" si="2"/>
+        <v>33.849999999999994</v>
       </c>
       <c r="D11" s="45" t="s">
         <v>17</v>
@@ -9406,20 +9494,27 @@
       <c r="BM11" s="5">
         <v>106.1</v>
       </c>
-      <c r="BN11" s="5"/>
-    </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN11" s="5">
+        <v>106.5</v>
+      </c>
+      <c r="BO11" s="5"/>
+      <c r="BP11" s="5"/>
+      <c r="BQ11" s="5"/>
+      <c r="BR11" s="5"/>
+      <c r="BS11" s="5"/>
+    </row>
+    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
-        <f>MIN(E12:ZX12)</f>
+        <f t="shared" si="0"/>
         <v>82.65</v>
       </c>
       <c r="B12" s="12">
-        <f>MAX(E12:ZX12)</f>
-        <v>97.75</v>
+        <f t="shared" si="1"/>
+        <v>99.6</v>
       </c>
       <c r="C12" s="12">
-        <f t="shared" si="0"/>
-        <v>15.099999999999994</v>
+        <f t="shared" si="2"/>
+        <v>16.949999999999989</v>
       </c>
       <c r="D12" s="45" t="s">
         <v>18</v>
@@ -9605,19 +9700,26 @@
       <c r="BM12" s="5">
         <v>97.55</v>
       </c>
-      <c r="BN12" s="5"/>
-    </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN12" s="5">
+        <v>99.6</v>
+      </c>
+      <c r="BO12" s="5"/>
+      <c r="BP12" s="5"/>
+      <c r="BQ12" s="5"/>
+      <c r="BR12" s="5"/>
+      <c r="BS12" s="5"/>
+    </row>
+    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
-        <f>MIN(E13:ZX13)</f>
+        <f t="shared" si="0"/>
         <v>44.1</v>
       </c>
       <c r="B13" s="12">
-        <f>MAX(E13:ZX13)</f>
+        <f t="shared" si="1"/>
         <v>57.15</v>
       </c>
       <c r="C13" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13.049999999999997</v>
       </c>
       <c r="D13" s="45" t="s">
@@ -9804,20 +9906,27 @@
       <c r="BM13" s="5">
         <v>49.65</v>
       </c>
-      <c r="BN13" s="5"/>
-    </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN13" s="5">
+        <v>50.45</v>
+      </c>
+      <c r="BO13" s="5"/>
+      <c r="BP13" s="5"/>
+      <c r="BQ13" s="5"/>
+      <c r="BR13" s="5"/>
+      <c r="BS13" s="5"/>
+    </row>
+    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
-        <f>MIN(E14:ZX14)</f>
+        <f t="shared" si="0"/>
         <v>29.75</v>
       </c>
       <c r="B14" s="12">
-        <f>MAX(E14:ZX14)</f>
-        <v>33.200000000000003</v>
+        <f t="shared" si="1"/>
+        <v>38.15</v>
       </c>
       <c r="C14" s="12">
-        <f t="shared" si="0"/>
-        <v>3.4500000000000028</v>
+        <f t="shared" si="2"/>
+        <v>8.3999999999999986</v>
       </c>
       <c r="D14" s="45" t="s">
         <v>21</v>
@@ -10003,20 +10112,27 @@
       <c r="BM14" s="5">
         <v>31.8</v>
       </c>
-      <c r="BN14" s="5"/>
-    </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN14" s="5">
+        <v>38.15</v>
+      </c>
+      <c r="BO14" s="5"/>
+      <c r="BP14" s="5"/>
+      <c r="BQ14" s="5"/>
+      <c r="BR14" s="5"/>
+      <c r="BS14" s="5"/>
+    </row>
+    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
-        <f>MIN(E15:ZX15)</f>
-        <v>26.5</v>
+        <f t="shared" si="0"/>
+        <v>26.3</v>
       </c>
       <c r="B15" s="12">
-        <f>MAX(E15:ZX15)</f>
+        <f t="shared" si="1"/>
         <v>36.4</v>
       </c>
       <c r="C15" s="12">
-        <f t="shared" si="0"/>
-        <v>9.8999999999999986</v>
+        <f t="shared" si="2"/>
+        <v>10.099999999999998</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>126</v>
@@ -10194,19 +10310,26 @@
       <c r="BM15" s="5">
         <v>26.5</v>
       </c>
-      <c r="BN15" s="5"/>
-    </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN15" s="5">
+        <v>26.3</v>
+      </c>
+      <c r="BO15" s="5"/>
+      <c r="BP15" s="5"/>
+      <c r="BQ15" s="5"/>
+      <c r="BR15" s="5"/>
+      <c r="BS15" s="5"/>
+    </row>
+    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
-        <f>MIN(E16:ZX16)</f>
+        <f t="shared" si="0"/>
         <v>552</v>
       </c>
       <c r="B16" s="12">
-        <f>MAX(E16:ZX16)</f>
+        <f t="shared" si="1"/>
         <v>729.5</v>
       </c>
       <c r="C16" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>177.5</v>
       </c>
       <c r="D16" s="45" t="s">
@@ -10393,19 +10516,26 @@
       <c r="BM16" s="5">
         <v>706</v>
       </c>
-      <c r="BN16" s="5"/>
-    </row>
-    <row r="17" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN16" s="5">
+        <v>708.55</v>
+      </c>
+      <c r="BO16" s="5"/>
+      <c r="BP16" s="5"/>
+      <c r="BQ16" s="5"/>
+      <c r="BR16" s="5"/>
+      <c r="BS16" s="5"/>
+    </row>
+    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
-        <f>MIN(E17:ZX17)</f>
+        <f t="shared" si="0"/>
         <v>433</v>
       </c>
       <c r="B17" s="12">
-        <f>MAX(E17:ZX17)</f>
+        <f t="shared" si="1"/>
         <v>515</v>
       </c>
       <c r="C17" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>82</v>
       </c>
       <c r="D17" s="44" t="s">
@@ -10592,20 +10722,27 @@
       <c r="BM17" s="5">
         <v>488.95</v>
       </c>
-      <c r="BN17" s="5"/>
-    </row>
-    <row r="18" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN17" s="5">
+        <v>482.25</v>
+      </c>
+      <c r="BO17" s="5"/>
+      <c r="BP17" s="5"/>
+      <c r="BQ17" s="5"/>
+      <c r="BR17" s="5"/>
+      <c r="BS17" s="5"/>
+    </row>
+    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
-        <f>MIN(E18:ZX18)</f>
+        <f t="shared" si="0"/>
         <v>178.8</v>
       </c>
       <c r="B18" s="12">
-        <f>MAX(E18:ZX18)</f>
-        <v>297.25</v>
+        <f t="shared" si="1"/>
+        <v>302.2</v>
       </c>
       <c r="C18" s="12">
-        <f t="shared" si="0"/>
-        <v>118.44999999999999</v>
+        <f t="shared" si="2"/>
+        <v>123.39999999999998</v>
       </c>
       <c r="D18" s="44" t="s">
         <v>39</v>
@@ -10791,19 +10928,26 @@
       <c r="BM18" s="5">
         <v>295.75</v>
       </c>
-      <c r="BN18" s="5"/>
-    </row>
-    <row r="19" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN18" s="5">
+        <v>302.2</v>
+      </c>
+      <c r="BO18" s="5"/>
+      <c r="BP18" s="5"/>
+      <c r="BQ18" s="5"/>
+      <c r="BR18" s="5"/>
+      <c r="BS18" s="5"/>
+    </row>
+    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
-        <f>MIN(E19:ZX19)</f>
+        <f t="shared" si="0"/>
         <v>440.7</v>
       </c>
       <c r="B19" s="12">
-        <f>MAX(E19:ZX19)</f>
+        <f t="shared" si="1"/>
         <v>562.79999999999995</v>
       </c>
       <c r="C19" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>122.09999999999997</v>
       </c>
       <c r="D19" s="44" t="s">
@@ -10990,19 +11134,26 @@
       <c r="BM19" s="5">
         <v>543</v>
       </c>
-      <c r="BN19" s="5"/>
-    </row>
-    <row r="20" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN19" s="5">
+        <v>526.1</v>
+      </c>
+      <c r="BO19" s="5"/>
+      <c r="BP19" s="5"/>
+      <c r="BQ19" s="5"/>
+      <c r="BR19" s="5"/>
+      <c r="BS19" s="5"/>
+    </row>
+    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
-        <f>MIN(E20:ZX20)</f>
+        <f t="shared" si="0"/>
         <v>677</v>
       </c>
       <c r="B20" s="12">
-        <f>MAX(E20:ZX20)</f>
+        <f t="shared" si="1"/>
         <v>790</v>
       </c>
       <c r="C20" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>113</v>
       </c>
       <c r="D20" s="44" t="s">
@@ -11189,19 +11340,26 @@
       <c r="BM20" s="5">
         <v>790</v>
       </c>
-      <c r="BN20" s="5"/>
-    </row>
-    <row r="21" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BN20" s="5">
+        <v>788.1</v>
+      </c>
+      <c r="BO20" s="5"/>
+      <c r="BP20" s="5"/>
+      <c r="BQ20" s="5"/>
+      <c r="BR20" s="5"/>
+      <c r="BS20" s="5"/>
+    </row>
+    <row r="21" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
-        <f>MIN(E21:ZX21)</f>
+        <f t="shared" si="0"/>
         <v>376.7</v>
       </c>
       <c r="B21" s="12">
-        <f>MAX(E21:ZX21)</f>
+        <f t="shared" si="1"/>
         <v>547.5</v>
       </c>
       <c r="C21" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>170.8</v>
       </c>
       <c r="D21" s="44" t="s">
@@ -11388,20 +11546,27 @@
       <c r="BM21" s="5">
         <v>547.5</v>
       </c>
-      <c r="BN21" s="5"/>
-    </row>
-    <row r="22" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BN21" s="5">
+        <v>539.79999999999995</v>
+      </c>
+      <c r="BO21" s="5"/>
+      <c r="BP21" s="5"/>
+      <c r="BQ21" s="5"/>
+      <c r="BR21" s="5"/>
+      <c r="BS21" s="5"/>
+    </row>
+    <row r="22" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
-        <f>MIN(E22:ZX22)</f>
+        <f t="shared" si="0"/>
         <v>315.2</v>
       </c>
       <c r="B22" s="12">
-        <f>MAX(E22:ZX22)</f>
-        <v>372.55</v>
+        <f t="shared" si="1"/>
+        <v>373</v>
       </c>
       <c r="C22" s="12">
-        <f t="shared" si="0"/>
-        <v>57.350000000000023</v>
+        <f t="shared" si="2"/>
+        <v>57.800000000000011</v>
       </c>
       <c r="D22" s="44" t="s">
         <v>269</v>
@@ -11533,19 +11698,26 @@
       <c r="BM22" s="5">
         <v>342.55</v>
       </c>
-      <c r="BN22" s="5"/>
-    </row>
-    <row r="23" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN22" s="5">
+        <v>373</v>
+      </c>
+      <c r="BO22" s="5"/>
+      <c r="BP22" s="5"/>
+      <c r="BQ22" s="5"/>
+      <c r="BR22" s="5"/>
+      <c r="BS22" s="5"/>
+    </row>
+    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
-        <f>MIN(E23:ZX23)</f>
+        <f t="shared" si="0"/>
         <v>54.45</v>
       </c>
       <c r="B23" s="12">
-        <f>MAX(E23:ZX23)</f>
+        <f t="shared" si="1"/>
         <v>85.65</v>
       </c>
       <c r="C23" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>31.200000000000003</v>
       </c>
       <c r="D23" s="45" t="s">
@@ -11724,19 +11896,26 @@
       <c r="BM23" s="5">
         <v>58.4</v>
       </c>
-      <c r="BN23" s="5"/>
-    </row>
-    <row r="24" spans="1:66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BN23" s="5">
+        <v>59</v>
+      </c>
+      <c r="BO23" s="5"/>
+      <c r="BP23" s="5"/>
+      <c r="BQ23" s="5"/>
+      <c r="BR23" s="5"/>
+      <c r="BS23" s="5"/>
+    </row>
+    <row r="24" spans="1:71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
-        <f>MIN(E24:ZX24)</f>
+        <f t="shared" si="0"/>
         <v>210.65</v>
       </c>
       <c r="B24" s="12">
-        <f>MAX(E24:ZX24)</f>
+        <f t="shared" si="1"/>
         <v>255.75</v>
       </c>
       <c r="C24" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>45.099999999999994</v>
       </c>
       <c r="D24" s="45" t="s">
@@ -11911,19 +12090,26 @@
       <c r="BM24" s="5">
         <v>241.85</v>
       </c>
-      <c r="BN24" s="5"/>
-    </row>
-    <row r="25" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN24" s="5">
+        <v>247.6</v>
+      </c>
+      <c r="BO24" s="5"/>
+      <c r="BP24" s="5"/>
+      <c r="BQ24" s="5"/>
+      <c r="BR24" s="5"/>
+      <c r="BS24" s="5"/>
+    </row>
+    <row r="25" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
-        <f>MIN(E25:ZX25)</f>
+        <f t="shared" si="0"/>
         <v>876</v>
       </c>
       <c r="B25" s="12">
-        <f>MAX(E25:ZX25)</f>
+        <f t="shared" si="1"/>
         <v>950</v>
       </c>
       <c r="C25" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="D25" s="46" t="s">
@@ -12080,19 +12266,26 @@
       <c r="BM25" s="5">
         <v>923.1</v>
       </c>
-      <c r="BN25" s="5"/>
-    </row>
-    <row r="26" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN25" s="5">
+        <v>926.8</v>
+      </c>
+      <c r="BO25" s="5"/>
+      <c r="BP25" s="5"/>
+      <c r="BQ25" s="5"/>
+      <c r="BR25" s="5"/>
+      <c r="BS25" s="5"/>
+    </row>
+    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
-        <f>MIN(E26:ZX26)</f>
+        <f t="shared" si="0"/>
         <v>83.1</v>
       </c>
       <c r="B26" s="12">
-        <f>MAX(E26:ZX26)</f>
+        <f t="shared" si="1"/>
         <v>96</v>
       </c>
       <c r="C26" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12.900000000000006</v>
       </c>
       <c r="D26" s="45" t="s">
@@ -12237,19 +12430,26 @@
       <c r="BM26" s="5">
         <v>84.1</v>
       </c>
-      <c r="BN26" s="5"/>
-    </row>
-    <row r="27" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN26" s="5">
+        <v>92.5</v>
+      </c>
+      <c r="BO26" s="5"/>
+      <c r="BP26" s="5"/>
+      <c r="BQ26" s="5"/>
+      <c r="BR26" s="5"/>
+      <c r="BS26" s="5"/>
+    </row>
+    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
-        <f>MIN(E27:ZX27)</f>
+        <f t="shared" si="0"/>
         <v>37.6</v>
       </c>
       <c r="B27" s="12">
-        <f>MAX(E27:ZX27)</f>
+        <f t="shared" si="1"/>
         <v>44.75</v>
       </c>
       <c r="C27" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.1499999999999986</v>
       </c>
       <c r="D27" s="45" t="s">
@@ -12394,19 +12594,26 @@
       <c r="BM27" s="5">
         <v>41.65</v>
       </c>
-      <c r="BN27" s="5"/>
-    </row>
-    <row r="28" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN27" s="5">
+        <v>41.2</v>
+      </c>
+      <c r="BO27" s="5"/>
+      <c r="BP27" s="5"/>
+      <c r="BQ27" s="5"/>
+      <c r="BR27" s="5"/>
+      <c r="BS27" s="5"/>
+    </row>
+    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
-        <f>MIN(E28:ZX28)</f>
+        <f t="shared" si="0"/>
         <v>111.95</v>
       </c>
       <c r="B28" s="12">
-        <f>MAX(E28:ZX28)</f>
+        <f t="shared" si="1"/>
         <v>141.65</v>
       </c>
       <c r="C28" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>29.700000000000003</v>
       </c>
       <c r="D28" s="45" t="s">
@@ -12551,19 +12758,26 @@
       <c r="BM28" s="5">
         <v>141.1</v>
       </c>
-      <c r="BN28" s="5"/>
-    </row>
-    <row r="29" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN28" s="5">
+        <v>140.44999999999999</v>
+      </c>
+      <c r="BO28" s="5"/>
+      <c r="BP28" s="5"/>
+      <c r="BQ28" s="5"/>
+      <c r="BR28" s="5"/>
+      <c r="BS28" s="5"/>
+    </row>
+    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
-        <f>MIN(E29:ZX29)</f>
+        <f t="shared" si="0"/>
         <v>62.3</v>
       </c>
       <c r="B29" s="12">
-        <f>MAX(E29:ZX29)</f>
+        <f t="shared" si="1"/>
         <v>78.849999999999994</v>
       </c>
       <c r="C29" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16.549999999999997</v>
       </c>
       <c r="D29" s="45" t="s">
@@ -12708,20 +12922,27 @@
       <c r="BM29" s="5">
         <v>72.650000000000006</v>
       </c>
-      <c r="BN29" s="5"/>
-    </row>
-    <row r="30" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN29" s="5">
+        <v>72.95</v>
+      </c>
+      <c r="BO29" s="5"/>
+      <c r="BP29" s="5"/>
+      <c r="BQ29" s="5"/>
+      <c r="BR29" s="5"/>
+      <c r="BS29" s="5"/>
+    </row>
+    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
-        <f>MIN(E30:ZX30)</f>
+        <f t="shared" si="0"/>
         <v>39.25</v>
       </c>
       <c r="B30" s="12">
-        <f>MAX(E30:ZX30)</f>
-        <v>48.75</v>
+        <f t="shared" si="1"/>
+        <v>50.3</v>
       </c>
       <c r="C30" s="12">
-        <f t="shared" si="0"/>
-        <v>9.5</v>
+        <f t="shared" si="2"/>
+        <v>11.049999999999997</v>
       </c>
       <c r="D30" s="45" t="s">
         <v>256</v>
@@ -12865,20 +13086,27 @@
       <c r="BM30" s="5">
         <v>47.7</v>
       </c>
-      <c r="BN30" s="5"/>
-    </row>
-    <row r="31" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN30" s="5">
+        <v>50.3</v>
+      </c>
+      <c r="BO30" s="5"/>
+      <c r="BP30" s="5"/>
+      <c r="BQ30" s="5"/>
+      <c r="BR30" s="5"/>
+      <c r="BS30" s="5"/>
+    </row>
+    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
-        <f>MIN(E31:ZX31)</f>
-        <v>143.30000000000001</v>
+        <f t="shared" si="0"/>
+        <v>142.6</v>
       </c>
       <c r="B31" s="12">
-        <f>MAX(E31:ZX31)</f>
+        <f t="shared" si="1"/>
         <v>156.85</v>
       </c>
       <c r="C31" s="12">
-        <f t="shared" si="0"/>
-        <v>13.549999999999983</v>
+        <f t="shared" si="2"/>
+        <v>14.25</v>
       </c>
       <c r="D31" s="45" t="s">
         <v>257</v>
@@ -13022,19 +13250,26 @@
       <c r="BM31" s="5">
         <v>143.30000000000001</v>
       </c>
-      <c r="BN31" s="5"/>
-    </row>
-    <row r="32" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN31" s="5">
+        <v>142.6</v>
+      </c>
+      <c r="BO31" s="5"/>
+      <c r="BP31" s="5"/>
+      <c r="BQ31" s="5"/>
+      <c r="BR31" s="5"/>
+      <c r="BS31" s="5"/>
+    </row>
+    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
-        <f>MIN(E32:ZX32)</f>
+        <f t="shared" si="0"/>
         <v>101.6</v>
       </c>
       <c r="B32" s="12">
-        <f>MAX(E32:ZX32)</f>
+        <f t="shared" si="1"/>
         <v>121.8</v>
       </c>
       <c r="C32" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20.200000000000003</v>
       </c>
       <c r="D32" s="45" t="s">
@@ -13167,19 +13402,26 @@
       <c r="BM32" s="5">
         <v>115.6</v>
       </c>
-      <c r="BN32" s="5"/>
-    </row>
-    <row r="33" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN32" s="5">
+        <v>115.5</v>
+      </c>
+      <c r="BO32" s="5"/>
+      <c r="BP32" s="5"/>
+      <c r="BQ32" s="5"/>
+      <c r="BR32" s="5"/>
+      <c r="BS32" s="5"/>
+    </row>
+    <row r="33" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
-        <f>MIN(E33:ZX33)</f>
+        <f t="shared" si="0"/>
         <v>56.75</v>
       </c>
       <c r="B33" s="12">
-        <f>MAX(E33:ZX33)</f>
+        <f t="shared" si="1"/>
         <v>67.099999999999994</v>
       </c>
       <c r="C33" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10.349999999999994</v>
       </c>
       <c r="D33" s="45" t="s">
@@ -13300,19 +13542,26 @@
       <c r="BM33" s="5">
         <v>60.6</v>
       </c>
-      <c r="BN33" s="5"/>
-    </row>
-    <row r="34" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN33" s="5">
+        <v>59.65</v>
+      </c>
+      <c r="BO33" s="5"/>
+      <c r="BP33" s="5"/>
+      <c r="BQ33" s="5"/>
+      <c r="BR33" s="5"/>
+      <c r="BS33" s="5"/>
+    </row>
+    <row r="34" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
-        <f>MIN(E34:ZX34)</f>
+        <f t="shared" si="0"/>
         <v>167.9</v>
       </c>
       <c r="B34" s="12">
-        <f>MAX(E34:ZX34)</f>
+        <f t="shared" si="1"/>
         <v>236.1</v>
       </c>
       <c r="C34" s="12">
-        <f t="shared" ref="C34" si="1">B34-A34</f>
+        <f t="shared" ref="C34" si="3">B34-A34</f>
         <v>68.199999999999989</v>
       </c>
       <c r="D34" s="45" t="s">
@@ -13427,19 +13676,26 @@
       <c r="BM34" s="5">
         <v>192.9</v>
       </c>
-      <c r="BN34" s="5"/>
-    </row>
-    <row r="35" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN34" s="5">
+        <v>194.3</v>
+      </c>
+      <c r="BO34" s="5"/>
+      <c r="BP34" s="5"/>
+      <c r="BQ34" s="5"/>
+      <c r="BR34" s="5"/>
+      <c r="BS34" s="5"/>
+    </row>
+    <row r="35" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
-        <f>MIN(E35:ZX35)</f>
+        <f t="shared" si="0"/>
         <v>661</v>
       </c>
       <c r="B35" s="12">
-        <f>MAX(E35:ZX35)</f>
+        <f t="shared" si="1"/>
         <v>714.65</v>
       </c>
       <c r="C35" s="12">
-        <f t="shared" ref="C35" si="2">B35-A35</f>
+        <f t="shared" ref="C35" si="4">B35-A35</f>
         <v>53.649999999999977</v>
       </c>
       <c r="D35" s="45" t="s">
@@ -13550,19 +13806,26 @@
       <c r="BM35" s="5">
         <v>677</v>
       </c>
-      <c r="BN35" s="5"/>
-    </row>
-    <row r="36" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN35" s="5">
+        <v>677</v>
+      </c>
+      <c r="BO35" s="5"/>
+      <c r="BP35" s="5"/>
+      <c r="BQ35" s="5"/>
+      <c r="BR35" s="5"/>
+      <c r="BS35" s="5"/>
+    </row>
+    <row r="36" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
-        <f>MIN(E36:ZX36)</f>
+        <f t="shared" si="0"/>
         <v>402.9</v>
       </c>
       <c r="B36" s="12">
-        <f>MAX(E36:ZX36)</f>
+        <f t="shared" si="1"/>
         <v>520</v>
       </c>
       <c r="C36" s="12">
-        <f t="shared" ref="C36" si="3">B36-A36</f>
+        <f t="shared" ref="C36" si="5">B36-A36</f>
         <v>117.10000000000002</v>
       </c>
       <c r="D36" s="45" t="s">
@@ -13655,20 +13918,27 @@
       <c r="BM36" s="5">
         <v>405.05</v>
       </c>
-      <c r="BN36" s="5"/>
-    </row>
-    <row r="37" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN36" s="5">
+        <v>446.3</v>
+      </c>
+      <c r="BO36" s="5"/>
+      <c r="BP36" s="5"/>
+      <c r="BQ36" s="5"/>
+      <c r="BR36" s="5"/>
+      <c r="BS36" s="5"/>
+    </row>
+    <row r="37" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
-        <f>MIN(E37:ZX37)</f>
+        <f t="shared" si="0"/>
         <v>226</v>
       </c>
       <c r="B37" s="12">
-        <f>MAX(E37:ZX37)</f>
-        <v>281</v>
+        <f t="shared" si="1"/>
+        <v>309.95</v>
       </c>
       <c r="C37" s="12">
-        <f t="shared" ref="C37" si="4">B37-A37</f>
-        <v>55</v>
+        <f t="shared" ref="C37" si="6">B37-A37</f>
+        <v>83.949999999999989</v>
       </c>
       <c r="D37" s="45" t="s">
         <v>297</v>
@@ -13750,19 +14020,26 @@
       <c r="BM37" s="5">
         <v>281</v>
       </c>
-      <c r="BN37" s="5"/>
-    </row>
-    <row r="38" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN37" s="5">
+        <v>309.95</v>
+      </c>
+      <c r="BO37" s="5"/>
+      <c r="BP37" s="5"/>
+      <c r="BQ37" s="5"/>
+      <c r="BR37" s="5"/>
+      <c r="BS37" s="5"/>
+    </row>
+    <row r="38" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
-        <f>MIN(E38:ZX38)</f>
+        <f t="shared" si="0"/>
         <v>485</v>
       </c>
       <c r="B38" s="12">
-        <f>MAX(E38:ZX38)</f>
+        <f t="shared" si="1"/>
         <v>515</v>
       </c>
       <c r="C38" s="12">
-        <f t="shared" ref="C38" si="5">B38-A38</f>
+        <f t="shared" ref="C38" si="7">B38-A38</f>
         <v>30</v>
       </c>
       <c r="D38" s="45" t="s">
@@ -13843,19 +14120,26 @@
       <c r="BM38" s="5">
         <v>496.6</v>
       </c>
-      <c r="BN38" s="5"/>
-    </row>
-    <row r="39" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN38" s="5">
+        <v>494</v>
+      </c>
+      <c r="BO38" s="5"/>
+      <c r="BP38" s="5"/>
+      <c r="BQ38" s="5"/>
+      <c r="BR38" s="5"/>
+      <c r="BS38" s="5"/>
+    </row>
+    <row r="39" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
-        <f>MIN(E39:ZX39)</f>
+        <f t="shared" si="0"/>
         <v>76</v>
       </c>
       <c r="B39" s="12">
-        <f>MAX(E39:ZX39)</f>
+        <f t="shared" si="1"/>
         <v>78</v>
       </c>
       <c r="C39" s="12">
-        <f t="shared" ref="C39" si="6">B39-A39</f>
+        <f t="shared" ref="C39" si="8">B39-A39</f>
         <v>2</v>
       </c>
       <c r="D39" s="45" t="s">
@@ -13930,20 +14214,27 @@
       <c r="BM39" s="5">
         <v>76</v>
       </c>
-      <c r="BN39" s="5"/>
-    </row>
-    <row r="40" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN39" s="5">
+        <v>76.849999999999994</v>
+      </c>
+      <c r="BO39" s="5"/>
+      <c r="BP39" s="5"/>
+      <c r="BQ39" s="5"/>
+      <c r="BR39" s="5"/>
+      <c r="BS39" s="5"/>
+    </row>
+    <row r="40" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
-        <f>MIN(E40:ZX40)</f>
+        <f t="shared" si="0"/>
         <v>461</v>
       </c>
       <c r="B40" s="12">
-        <f>MAX(E40:ZX40)</f>
-        <v>469.15</v>
+        <f t="shared" si="1"/>
+        <v>472</v>
       </c>
       <c r="C40" s="12">
-        <f t="shared" ref="C40" si="7">B40-A40</f>
-        <v>8.1499999999999773</v>
+        <f t="shared" ref="C40" si="9">B40-A40</f>
+        <v>11</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>306</v>
@@ -14017,20 +14308,27 @@
       <c r="BM40" s="5">
         <v>466</v>
       </c>
-      <c r="BN40" s="5"/>
-    </row>
-    <row r="41" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BN40" s="5">
+        <v>472</v>
+      </c>
+      <c r="BO40" s="5"/>
+      <c r="BP40" s="5"/>
+      <c r="BQ40" s="5"/>
+      <c r="BR40" s="5"/>
+      <c r="BS40" s="5"/>
+    </row>
+    <row r="41" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
-        <f>MIN(E41:ZX41)</f>
-        <v>208</v>
+        <f t="shared" si="0"/>
+        <v>203.65</v>
       </c>
       <c r="B41" s="12">
-        <f>MAX(E41:ZX41)</f>
+        <f t="shared" si="1"/>
         <v>209.8</v>
       </c>
       <c r="C41" s="12">
-        <f t="shared" ref="C41" si="8">B41-A41</f>
-        <v>1.8000000000000114</v>
+        <f t="shared" ref="C41" si="10">B41-A41</f>
+        <v>6.1500000000000057</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>307</v>
@@ -14100,7 +14398,272 @@
       <c r="BM41" s="5">
         <v>209.8</v>
       </c>
-      <c r="BN41" s="5"/>
+      <c r="BN41" s="5">
+        <v>203.65</v>
+      </c>
+      <c r="BO41" s="5"/>
+      <c r="BP41" s="5"/>
+      <c r="BQ41" s="5"/>
+      <c r="BR41" s="5"/>
+      <c r="BS41" s="5"/>
+    </row>
+    <row r="42" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A42" s="12">
+        <f t="shared" ref="A42:A43" si="11">MIN(E42:ZX42)</f>
+        <v>63.5</v>
+      </c>
+      <c r="B42" s="12">
+        <f t="shared" ref="B42:B43" si="12">MAX(E42:ZX42)</f>
+        <v>63.5</v>
+      </c>
+      <c r="C42" s="12">
+        <f t="shared" ref="C42:C43" si="13">B42-A42</f>
+        <v>0</v>
+      </c>
+      <c r="D42" s="45" t="s">
+        <v>308</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="5"/>
+      <c r="U42" s="5"/>
+      <c r="V42" s="5"/>
+      <c r="W42" s="5"/>
+      <c r="X42" s="5"/>
+      <c r="Y42" s="5"/>
+      <c r="Z42" s="5"/>
+      <c r="AA42" s="5"/>
+      <c r="AB42" s="5"/>
+      <c r="AC42" s="5"/>
+      <c r="AD42" s="5"/>
+      <c r="AE42" s="5"/>
+      <c r="AF42" s="5"/>
+      <c r="AG42" s="5"/>
+      <c r="AH42" s="5"/>
+      <c r="AI42" s="5"/>
+      <c r="AJ42" s="5"/>
+      <c r="AK42" s="5"/>
+      <c r="AL42" s="5"/>
+      <c r="AM42" s="5"/>
+      <c r="AN42" s="5"/>
+      <c r="AO42" s="5"/>
+      <c r="AP42" s="5"/>
+      <c r="AQ42" s="5"/>
+      <c r="AR42" s="5"/>
+      <c r="AS42" s="5"/>
+      <c r="AT42" s="5"/>
+      <c r="AU42" s="5"/>
+      <c r="AV42" s="5"/>
+      <c r="AW42" s="5"/>
+      <c r="AX42" s="5"/>
+      <c r="AY42" s="5"/>
+      <c r="AZ42" s="5"/>
+      <c r="BA42" s="5"/>
+      <c r="BB42" s="5"/>
+      <c r="BC42" s="5"/>
+      <c r="BD42" s="5"/>
+      <c r="BE42" s="5"/>
+      <c r="BF42" s="5"/>
+      <c r="BG42" s="5"/>
+      <c r="BH42" s="5"/>
+      <c r="BI42" s="5"/>
+      <c r="BJ42" s="5"/>
+      <c r="BK42" s="5"/>
+      <c r="BL42" s="5"/>
+      <c r="BM42" s="5"/>
+      <c r="BN42" s="5">
+        <v>63.5</v>
+      </c>
+      <c r="BO42" s="5"/>
+      <c r="BP42" s="5"/>
+      <c r="BQ42" s="5"/>
+      <c r="BR42" s="5"/>
+      <c r="BS42" s="5"/>
+    </row>
+    <row r="43" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A43" s="12">
+        <f t="shared" si="11"/>
+        <v>60.75</v>
+      </c>
+      <c r="B43" s="12">
+        <f t="shared" si="12"/>
+        <v>60.75</v>
+      </c>
+      <c r="C43" s="12">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="D43" s="45" t="s">
+        <v>309</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="5"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="5"/>
+      <c r="U43" s="5"/>
+      <c r="V43" s="5"/>
+      <c r="W43" s="5"/>
+      <c r="X43" s="5"/>
+      <c r="Y43" s="5"/>
+      <c r="Z43" s="5"/>
+      <c r="AA43" s="5"/>
+      <c r="AB43" s="5"/>
+      <c r="AC43" s="5"/>
+      <c r="AD43" s="5"/>
+      <c r="AE43" s="5"/>
+      <c r="AF43" s="5"/>
+      <c r="AG43" s="5"/>
+      <c r="AH43" s="5"/>
+      <c r="AI43" s="5"/>
+      <c r="AJ43" s="5"/>
+      <c r="AK43" s="5"/>
+      <c r="AL43" s="5"/>
+      <c r="AM43" s="5"/>
+      <c r="AN43" s="5"/>
+      <c r="AO43" s="5"/>
+      <c r="AP43" s="5"/>
+      <c r="AQ43" s="5"/>
+      <c r="AR43" s="5"/>
+      <c r="AS43" s="5"/>
+      <c r="AT43" s="5"/>
+      <c r="AU43" s="5"/>
+      <c r="AV43" s="5"/>
+      <c r="AW43" s="5"/>
+      <c r="AX43" s="5"/>
+      <c r="AY43" s="5"/>
+      <c r="AZ43" s="5"/>
+      <c r="BA43" s="5"/>
+      <c r="BB43" s="5"/>
+      <c r="BC43" s="5"/>
+      <c r="BD43" s="5"/>
+      <c r="BE43" s="5"/>
+      <c r="BF43" s="5"/>
+      <c r="BG43" s="5"/>
+      <c r="BH43" s="5"/>
+      <c r="BI43" s="5"/>
+      <c r="BJ43" s="5"/>
+      <c r="BK43" s="5"/>
+      <c r="BL43" s="5"/>
+      <c r="BM43" s="5"/>
+      <c r="BN43" s="5">
+        <v>60.75</v>
+      </c>
+      <c r="BO43" s="5"/>
+      <c r="BP43" s="5"/>
+      <c r="BQ43" s="5"/>
+      <c r="BR43" s="5"/>
+      <c r="BS43" s="5"/>
+    </row>
+    <row r="44" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A44" s="12">
+        <f t="shared" ref="A44" si="14">MIN(E44:ZX44)</f>
+        <v>38.1</v>
+      </c>
+      <c r="B44" s="12">
+        <f t="shared" ref="B44" si="15">MAX(E44:ZX44)</f>
+        <v>38.1</v>
+      </c>
+      <c r="C44" s="12">
+        <f t="shared" ref="C44" si="16">B44-A44</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="45" t="s">
+        <v>310</v>
+      </c>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5"/>
+      <c r="R44" s="5"/>
+      <c r="S44" s="5"/>
+      <c r="T44" s="5"/>
+      <c r="U44" s="5"/>
+      <c r="V44" s="5"/>
+      <c r="W44" s="5"/>
+      <c r="X44" s="5"/>
+      <c r="Y44" s="5"/>
+      <c r="Z44" s="5"/>
+      <c r="AA44" s="5"/>
+      <c r="AB44" s="5"/>
+      <c r="AC44" s="5"/>
+      <c r="AD44" s="5"/>
+      <c r="AE44" s="5"/>
+      <c r="AF44" s="5"/>
+      <c r="AG44" s="5"/>
+      <c r="AH44" s="5"/>
+      <c r="AI44" s="5"/>
+      <c r="AJ44" s="5"/>
+      <c r="AK44" s="5"/>
+      <c r="AL44" s="5"/>
+      <c r="AM44" s="5"/>
+      <c r="AN44" s="5"/>
+      <c r="AO44" s="5"/>
+      <c r="AP44" s="5"/>
+      <c r="AQ44" s="5"/>
+      <c r="AR44" s="5"/>
+      <c r="AS44" s="5"/>
+      <c r="AT44" s="5"/>
+      <c r="AU44" s="5"/>
+      <c r="AV44" s="5"/>
+      <c r="AW44" s="5"/>
+      <c r="AX44" s="5"/>
+      <c r="AY44" s="5"/>
+      <c r="AZ44" s="5"/>
+      <c r="BA44" s="5"/>
+      <c r="BB44" s="5"/>
+      <c r="BC44" s="5"/>
+      <c r="BD44" s="5"/>
+      <c r="BE44" s="5"/>
+      <c r="BF44" s="5"/>
+      <c r="BG44" s="5"/>
+      <c r="BH44" s="5"/>
+      <c r="BI44" s="5"/>
+      <c r="BJ44" s="5"/>
+      <c r="BK44" s="5"/>
+      <c r="BL44" s="5"/>
+      <c r="BM44" s="5"/>
+      <c r="BN44" s="5">
+        <v>38.1</v>
+      </c>
+      <c r="BO44" s="5"/>
+      <c r="BP44" s="5"/>
+      <c r="BQ44" s="5"/>
+      <c r="BR44" s="5"/>
+      <c r="BS44" s="5"/>
     </row>
   </sheetData>
   <sortState ref="L1:L37">

</xml_diff>

<commit_message>
Added details for 6/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -1047,6 +1047,7 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -7206,7 +7207,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="BK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BR27" sqref="BR27"/>
+      <selection pane="topRight" activeCell="BO24" sqref="BO24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7470,11 +7471,11 @@
       </c>
       <c r="B2" s="12">
         <f t="shared" ref="B2:B41" si="1">MAX(E2:ZX2)</f>
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C2" s="12">
         <f>B2-A2</f>
-        <v>82.4</v>
+        <v>84.4</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>115</v>
@@ -7657,7 +7658,9 @@
       <c r="BN2" s="5">
         <v>326</v>
       </c>
-      <c r="BO2" s="5"/>
+      <c r="BO2" s="5">
+        <v>328</v>
+      </c>
       <c r="BP2" s="5"/>
       <c r="BQ2" s="5"/>
       <c r="BR2" s="5"/>
@@ -7857,7 +7860,9 @@
       <c r="BN3" s="5">
         <v>315.2</v>
       </c>
-      <c r="BO3" s="5"/>
+      <c r="BO3" s="5">
+        <v>315.5</v>
+      </c>
       <c r="BP3" s="5"/>
       <c r="BQ3" s="5"/>
       <c r="BR3" s="5"/>
@@ -8063,7 +8068,9 @@
       <c r="BN4" s="5">
         <v>265.64999999999998</v>
       </c>
-      <c r="BO4" s="5"/>
+      <c r="BO4" s="5">
+        <v>265</v>
+      </c>
       <c r="BP4" s="5"/>
       <c r="BQ4" s="5"/>
       <c r="BR4" s="5"/>
@@ -8269,7 +8276,9 @@
       <c r="BN5" s="5">
         <v>945.95</v>
       </c>
-      <c r="BO5" s="5"/>
+      <c r="BO5" s="5">
+        <v>931.35</v>
+      </c>
       <c r="BP5" s="5"/>
       <c r="BQ5" s="5"/>
       <c r="BR5" s="5"/>
@@ -8475,7 +8484,9 @@
       <c r="BN6" s="5">
         <v>286.5</v>
       </c>
-      <c r="BO6" s="5"/>
+      <c r="BO6" s="5">
+        <v>286.14999999999998</v>
+      </c>
       <c r="BP6" s="5"/>
       <c r="BQ6" s="5"/>
       <c r="BR6" s="5"/>
@@ -8681,7 +8692,9 @@
       <c r="BN7" s="5">
         <v>19.05</v>
       </c>
-      <c r="BO7" s="5"/>
+      <c r="BO7" s="5">
+        <v>18.350000000000001</v>
+      </c>
       <c r="BP7" s="5"/>
       <c r="BQ7" s="5"/>
       <c r="BR7" s="5"/>
@@ -8887,7 +8900,9 @@
       <c r="BN8" s="5">
         <v>86.75</v>
       </c>
-      <c r="BO8" s="5"/>
+      <c r="BO8" s="5">
+        <v>83.85</v>
+      </c>
       <c r="BP8" s="5"/>
       <c r="BQ8" s="5"/>
       <c r="BR8" s="5"/>
@@ -9085,7 +9100,9 @@
       <c r="BN9" s="28">
         <v>58.9</v>
       </c>
-      <c r="BO9" s="28"/>
+      <c r="BO9" s="28">
+        <v>57.3</v>
+      </c>
       <c r="BP9" s="28"/>
       <c r="BQ9" s="28"/>
       <c r="BR9" s="28"/>
@@ -9291,7 +9308,9 @@
       <c r="BN10" s="5">
         <v>41.05</v>
       </c>
-      <c r="BO10" s="5"/>
+      <c r="BO10" s="5">
+        <v>40.75</v>
+      </c>
       <c r="BP10" s="5"/>
       <c r="BQ10" s="5"/>
       <c r="BR10" s="5"/>
@@ -9497,7 +9516,9 @@
       <c r="BN11" s="5">
         <v>106.5</v>
       </c>
-      <c r="BO11" s="5"/>
+      <c r="BO11" s="5">
+        <v>100.2</v>
+      </c>
       <c r="BP11" s="5"/>
       <c r="BQ11" s="5"/>
       <c r="BR11" s="5"/>
@@ -9703,7 +9724,9 @@
       <c r="BN12" s="5">
         <v>99.6</v>
       </c>
-      <c r="BO12" s="5"/>
+      <c r="BO12" s="5">
+        <v>98.8</v>
+      </c>
       <c r="BP12" s="5"/>
       <c r="BQ12" s="5"/>
       <c r="BR12" s="5"/>
@@ -9909,7 +9932,9 @@
       <c r="BN13" s="5">
         <v>50.45</v>
       </c>
-      <c r="BO13" s="5"/>
+      <c r="BO13" s="5">
+        <v>49.85</v>
+      </c>
       <c r="BP13" s="5"/>
       <c r="BQ13" s="5"/>
       <c r="BR13" s="5"/>
@@ -9922,11 +9947,11 @@
       </c>
       <c r="B14" s="12">
         <f t="shared" si="1"/>
-        <v>38.15</v>
+        <v>41.85</v>
       </c>
       <c r="C14" s="12">
         <f t="shared" si="2"/>
-        <v>8.3999999999999986</v>
+        <v>12.100000000000001</v>
       </c>
       <c r="D14" s="45" t="s">
         <v>21</v>
@@ -10115,7 +10140,9 @@
       <c r="BN14" s="5">
         <v>38.15</v>
       </c>
-      <c r="BO14" s="5"/>
+      <c r="BO14" s="5">
+        <v>41.85</v>
+      </c>
       <c r="BP14" s="5"/>
       <c r="BQ14" s="5"/>
       <c r="BR14" s="5"/>
@@ -10124,7 +10151,7 @@
     <row r="15" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
-        <v>26.3</v>
+        <v>26.05</v>
       </c>
       <c r="B15" s="12">
         <f t="shared" si="1"/>
@@ -10132,7 +10159,7 @@
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
-        <v>10.099999999999998</v>
+        <v>10.349999999999998</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>126</v>
@@ -10313,7 +10340,9 @@
       <c r="BN15" s="5">
         <v>26.3</v>
       </c>
-      <c r="BO15" s="5"/>
+      <c r="BO15" s="5">
+        <v>26.05</v>
+      </c>
       <c r="BP15" s="5"/>
       <c r="BQ15" s="5"/>
       <c r="BR15" s="5"/>
@@ -10519,7 +10548,9 @@
       <c r="BN16" s="5">
         <v>708.55</v>
       </c>
-      <c r="BO16" s="5"/>
+      <c r="BO16" s="5">
+        <v>704.5</v>
+      </c>
       <c r="BP16" s="5"/>
       <c r="BQ16" s="5"/>
       <c r="BR16" s="5"/>
@@ -10725,7 +10756,9 @@
       <c r="BN17" s="5">
         <v>482.25</v>
       </c>
-      <c r="BO17" s="5"/>
+      <c r="BO17" s="5">
+        <v>485</v>
+      </c>
       <c r="BP17" s="5"/>
       <c r="BQ17" s="5"/>
       <c r="BR17" s="5"/>
@@ -10931,7 +10964,9 @@
       <c r="BN18" s="5">
         <v>302.2</v>
       </c>
-      <c r="BO18" s="5"/>
+      <c r="BO18" s="5">
+        <v>295</v>
+      </c>
       <c r="BP18" s="5"/>
       <c r="BQ18" s="5"/>
       <c r="BR18" s="5"/>
@@ -11137,7 +11172,9 @@
       <c r="BN19" s="5">
         <v>526.1</v>
       </c>
-      <c r="BO19" s="5"/>
+      <c r="BO19" s="5">
+        <v>553</v>
+      </c>
       <c r="BP19" s="5"/>
       <c r="BQ19" s="5"/>
       <c r="BR19" s="5"/>
@@ -11150,11 +11187,11 @@
       </c>
       <c r="B20" s="12">
         <f t="shared" si="1"/>
-        <v>790</v>
+        <v>795.95</v>
       </c>
       <c r="C20" s="12">
         <f t="shared" si="2"/>
-        <v>113</v>
+        <v>118.95000000000005</v>
       </c>
       <c r="D20" s="44" t="s">
         <v>104</v>
@@ -11343,7 +11380,9 @@
       <c r="BN20" s="5">
         <v>788.1</v>
       </c>
-      <c r="BO20" s="5"/>
+      <c r="BO20" s="5">
+        <v>795.95</v>
+      </c>
       <c r="BP20" s="5"/>
       <c r="BQ20" s="5"/>
       <c r="BR20" s="5"/>
@@ -11549,7 +11588,9 @@
       <c r="BN21" s="5">
         <v>539.79999999999995</v>
       </c>
-      <c r="BO21" s="5"/>
+      <c r="BO21" s="5">
+        <v>532.9</v>
+      </c>
       <c r="BP21" s="5"/>
       <c r="BQ21" s="5"/>
       <c r="BR21" s="5"/>
@@ -11701,7 +11742,9 @@
       <c r="BN22" s="5">
         <v>373</v>
       </c>
-      <c r="BO22" s="5"/>
+      <c r="BO22" s="5">
+        <v>372.25</v>
+      </c>
       <c r="BP22" s="5"/>
       <c r="BQ22" s="5"/>
       <c r="BR22" s="5"/>
@@ -11899,7 +11942,9 @@
       <c r="BN23" s="5">
         <v>59</v>
       </c>
-      <c r="BO23" s="5"/>
+      <c r="BO23" s="5">
+        <v>61.3</v>
+      </c>
       <c r="BP23" s="5"/>
       <c r="BQ23" s="5"/>
       <c r="BR23" s="5"/>
@@ -11912,11 +11957,11 @@
       </c>
       <c r="B24" s="12">
         <f t="shared" si="1"/>
-        <v>255.75</v>
+        <v>257.39999999999998</v>
       </c>
       <c r="C24" s="12">
         <f t="shared" si="2"/>
-        <v>45.099999999999994</v>
+        <v>46.749999999999972</v>
       </c>
       <c r="D24" s="45" t="s">
         <v>128</v>
@@ -12093,7 +12138,9 @@
       <c r="BN24" s="5">
         <v>247.6</v>
       </c>
-      <c r="BO24" s="5"/>
+      <c r="BO24" s="5">
+        <v>257.39999999999998</v>
+      </c>
       <c r="BP24" s="5"/>
       <c r="BQ24" s="5"/>
       <c r="BR24" s="5"/>
@@ -12269,7 +12316,9 @@
       <c r="BN25" s="5">
         <v>926.8</v>
       </c>
-      <c r="BO25" s="5"/>
+      <c r="BO25" s="5">
+        <v>928.8</v>
+      </c>
       <c r="BP25" s="5"/>
       <c r="BQ25" s="5"/>
       <c r="BR25" s="5"/>
@@ -12433,7 +12482,9 @@
       <c r="BN26" s="5">
         <v>92.5</v>
       </c>
-      <c r="BO26" s="5"/>
+      <c r="BO26" s="5">
+        <v>91.3</v>
+      </c>
       <c r="BP26" s="5"/>
       <c r="BQ26" s="5"/>
       <c r="BR26" s="5"/>
@@ -12597,7 +12648,9 @@
       <c r="BN27" s="5">
         <v>41.2</v>
       </c>
-      <c r="BO27" s="5"/>
+      <c r="BO27" s="5">
+        <v>39.700000000000003</v>
+      </c>
       <c r="BP27" s="5"/>
       <c r="BQ27" s="5"/>
       <c r="BR27" s="5"/>
@@ -12761,7 +12814,9 @@
       <c r="BN28" s="5">
         <v>140.44999999999999</v>
       </c>
-      <c r="BO28" s="5"/>
+      <c r="BO28" s="5">
+        <v>138.80000000000001</v>
+      </c>
       <c r="BP28" s="5"/>
       <c r="BQ28" s="5"/>
       <c r="BR28" s="5"/>
@@ -12925,7 +12980,9 @@
       <c r="BN29" s="5">
         <v>72.95</v>
       </c>
-      <c r="BO29" s="5"/>
+      <c r="BO29" s="5">
+        <v>71</v>
+      </c>
       <c r="BP29" s="5"/>
       <c r="BQ29" s="5"/>
       <c r="BR29" s="5"/>
@@ -12938,11 +12995,11 @@
       </c>
       <c r="B30" s="12">
         <f t="shared" si="1"/>
-        <v>50.3</v>
+        <v>50.95</v>
       </c>
       <c r="C30" s="12">
         <f t="shared" si="2"/>
-        <v>11.049999999999997</v>
+        <v>11.700000000000003</v>
       </c>
       <c r="D30" s="45" t="s">
         <v>256</v>
@@ -13089,7 +13146,9 @@
       <c r="BN30" s="5">
         <v>50.3</v>
       </c>
-      <c r="BO30" s="5"/>
+      <c r="BO30" s="5">
+        <v>50.95</v>
+      </c>
       <c r="BP30" s="5"/>
       <c r="BQ30" s="5"/>
       <c r="BR30" s="5"/>
@@ -13253,7 +13312,9 @@
       <c r="BN31" s="5">
         <v>142.6</v>
       </c>
-      <c r="BO31" s="5"/>
+      <c r="BO31" s="5">
+        <v>143.19999999999999</v>
+      </c>
       <c r="BP31" s="5"/>
       <c r="BQ31" s="5"/>
       <c r="BR31" s="5"/>
@@ -13405,7 +13466,9 @@
       <c r="BN32" s="5">
         <v>115.5</v>
       </c>
-      <c r="BO32" s="5"/>
+      <c r="BO32" s="5">
+        <v>117</v>
+      </c>
       <c r="BP32" s="5"/>
       <c r="BQ32" s="5"/>
       <c r="BR32" s="5"/>
@@ -13545,7 +13608,9 @@
       <c r="BN33" s="5">
         <v>59.65</v>
       </c>
-      <c r="BO33" s="5"/>
+      <c r="BO33" s="5">
+        <v>60.1</v>
+      </c>
       <c r="BP33" s="5"/>
       <c r="BQ33" s="5"/>
       <c r="BR33" s="5"/>
@@ -13679,7 +13744,9 @@
       <c r="BN34" s="5">
         <v>194.3</v>
       </c>
-      <c r="BO34" s="5"/>
+      <c r="BO34" s="5">
+        <v>203.8</v>
+      </c>
       <c r="BP34" s="5"/>
       <c r="BQ34" s="5"/>
       <c r="BR34" s="5"/>
@@ -13809,7 +13876,9 @@
       <c r="BN35" s="5">
         <v>677</v>
       </c>
-      <c r="BO35" s="5"/>
+      <c r="BO35" s="5">
+        <v>680.5</v>
+      </c>
       <c r="BP35" s="5"/>
       <c r="BQ35" s="5"/>
       <c r="BR35" s="5"/>
@@ -13921,7 +13990,9 @@
       <c r="BN36" s="5">
         <v>446.3</v>
       </c>
-      <c r="BO36" s="5"/>
+      <c r="BO36" s="5">
+        <v>470.4</v>
+      </c>
       <c r="BP36" s="5"/>
       <c r="BQ36" s="5"/>
       <c r="BR36" s="5"/>
@@ -13934,11 +14005,11 @@
       </c>
       <c r="B37" s="12">
         <f t="shared" si="1"/>
-        <v>309.95</v>
+        <v>332</v>
       </c>
       <c r="C37" s="12">
         <f t="shared" ref="C37" si="6">B37-A37</f>
-        <v>83.949999999999989</v>
+        <v>106</v>
       </c>
       <c r="D37" s="45" t="s">
         <v>297</v>
@@ -14023,7 +14094,9 @@
       <c r="BN37" s="5">
         <v>309.95</v>
       </c>
-      <c r="BO37" s="5"/>
+      <c r="BO37" s="5">
+        <v>332</v>
+      </c>
       <c r="BP37" s="5"/>
       <c r="BQ37" s="5"/>
       <c r="BR37" s="5"/>
@@ -14123,7 +14196,9 @@
       <c r="BN38" s="5">
         <v>494</v>
       </c>
-      <c r="BO38" s="5"/>
+      <c r="BO38" s="5">
+        <v>500.1</v>
+      </c>
       <c r="BP38" s="5"/>
       <c r="BQ38" s="5"/>
       <c r="BR38" s="5"/>
@@ -14136,11 +14211,11 @@
       </c>
       <c r="B39" s="12">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>78.5</v>
       </c>
       <c r="C39" s="12">
         <f t="shared" ref="C39" si="8">B39-A39</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="D39" s="45" t="s">
         <v>305</v>
@@ -14217,7 +14292,9 @@
       <c r="BN39" s="5">
         <v>76.849999999999994</v>
       </c>
-      <c r="BO39" s="5"/>
+      <c r="BO39" s="5">
+        <v>78.5</v>
+      </c>
       <c r="BP39" s="5"/>
       <c r="BQ39" s="5"/>
       <c r="BR39" s="5"/>
@@ -14311,7 +14388,9 @@
       <c r="BN40" s="5">
         <v>472</v>
       </c>
-      <c r="BO40" s="5"/>
+      <c r="BO40" s="5">
+        <v>467</v>
+      </c>
       <c r="BP40" s="5"/>
       <c r="BQ40" s="5"/>
       <c r="BR40" s="5"/>
@@ -14320,7 +14399,7 @@
     <row r="41" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <f t="shared" si="0"/>
-        <v>203.65</v>
+        <v>201.7</v>
       </c>
       <c r="B41" s="12">
         <f t="shared" si="1"/>
@@ -14328,7 +14407,7 @@
       </c>
       <c r="C41" s="12">
         <f t="shared" ref="C41" si="10">B41-A41</f>
-        <v>6.1500000000000057</v>
+        <v>8.1000000000000227</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>307</v>
@@ -14401,7 +14480,9 @@
       <c r="BN41" s="5">
         <v>203.65</v>
       </c>
-      <c r="BO41" s="5"/>
+      <c r="BO41" s="5">
+        <v>201.7</v>
+      </c>
       <c r="BP41" s="5"/>
       <c r="BQ41" s="5"/>
       <c r="BR41" s="5"/>
@@ -14414,11 +14495,11 @@
       </c>
       <c r="B42" s="12">
         <f t="shared" ref="B42:B43" si="12">MAX(E42:ZX42)</f>
-        <v>63.5</v>
+        <v>63.7</v>
       </c>
       <c r="C42" s="12">
         <f t="shared" ref="C42:C43" si="13">B42-A42</f>
-        <v>0</v>
+        <v>0.20000000000000284</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>308</v>
@@ -14487,7 +14568,9 @@
       <c r="BN42" s="5">
         <v>63.5</v>
       </c>
-      <c r="BO42" s="5"/>
+      <c r="BO42" s="5">
+        <v>63.7</v>
+      </c>
       <c r="BP42" s="5"/>
       <c r="BQ42" s="5"/>
       <c r="BR42" s="5"/>
@@ -14573,7 +14656,9 @@
       <c r="BN43" s="5">
         <v>60.75</v>
       </c>
-      <c r="BO43" s="5"/>
+      <c r="BO43" s="5">
+        <v>60.75</v>
+      </c>
       <c r="BP43" s="5"/>
       <c r="BQ43" s="5"/>
       <c r="BR43" s="5"/>
@@ -14582,7 +14667,7 @@
     <row r="44" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <f t="shared" ref="A44" si="14">MIN(E44:ZX44)</f>
-        <v>38.1</v>
+        <v>36.950000000000003</v>
       </c>
       <c r="B44" s="12">
         <f t="shared" ref="B44" si="15">MAX(E44:ZX44)</f>
@@ -14590,7 +14675,7 @@
       </c>
       <c r="C44" s="12">
         <f t="shared" ref="C44" si="16">B44-A44</f>
-        <v>0</v>
+        <v>1.1499999999999986</v>
       </c>
       <c r="D44" s="45" t="s">
         <v>310</v>
@@ -14659,7 +14744,9 @@
       <c r="BN44" s="5">
         <v>38.1</v>
       </c>
-      <c r="BO44" s="5"/>
+      <c r="BO44" s="5">
+        <v>36.950000000000003</v>
+      </c>
       <c r="BP44" s="5"/>
       <c r="BQ44" s="5"/>
       <c r="BR44" s="5"/>

</xml_diff>

<commit_message>
Added details for 7/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -7205,9 +7205,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="BK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BO24" sqref="BO24"/>
+      <selection pane="topRight" activeCell="BP2" sqref="BP2:BP44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7661,7 +7661,9 @@
       <c r="BO2" s="5">
         <v>328</v>
       </c>
-      <c r="BP2" s="5"/>
+      <c r="BP2" s="5">
+        <v>317.25</v>
+      </c>
       <c r="BQ2" s="5"/>
       <c r="BR2" s="5"/>
       <c r="BS2" s="5"/>
@@ -7863,7 +7865,9 @@
       <c r="BO3" s="5">
         <v>315.5</v>
       </c>
-      <c r="BP3" s="5"/>
+      <c r="BP3" s="5">
+        <v>312.45</v>
+      </c>
       <c r="BQ3" s="5"/>
       <c r="BR3" s="5"/>
       <c r="BS3" s="5"/>
@@ -8071,7 +8075,9 @@
       <c r="BO4" s="5">
         <v>265</v>
       </c>
-      <c r="BP4" s="5"/>
+      <c r="BP4" s="5">
+        <v>265.10000000000002</v>
+      </c>
       <c r="BQ4" s="5"/>
       <c r="BR4" s="5"/>
       <c r="BS4" s="5"/>
@@ -8279,7 +8285,9 @@
       <c r="BO5" s="5">
         <v>931.35</v>
       </c>
-      <c r="BP5" s="5"/>
+      <c r="BP5" s="5">
+        <v>906.5</v>
+      </c>
       <c r="BQ5" s="5"/>
       <c r="BR5" s="5"/>
       <c r="BS5" s="5"/>
@@ -8487,7 +8495,9 @@
       <c r="BO6" s="5">
         <v>286.14999999999998</v>
       </c>
-      <c r="BP6" s="5"/>
+      <c r="BP6" s="5">
+        <v>285</v>
+      </c>
       <c r="BQ6" s="5"/>
       <c r="BR6" s="5"/>
       <c r="BS6" s="5"/>
@@ -8695,7 +8705,9 @@
       <c r="BO7" s="5">
         <v>18.350000000000001</v>
       </c>
-      <c r="BP7" s="5"/>
+      <c r="BP7" s="5">
+        <v>17.600000000000001</v>
+      </c>
       <c r="BQ7" s="5"/>
       <c r="BR7" s="5"/>
       <c r="BS7" s="5"/>
@@ -8903,7 +8915,9 @@
       <c r="BO8" s="5">
         <v>83.85</v>
       </c>
-      <c r="BP8" s="5"/>
+      <c r="BP8" s="5">
+        <v>78.400000000000006</v>
+      </c>
       <c r="BQ8" s="5"/>
       <c r="BR8" s="5"/>
       <c r="BS8" s="5"/>
@@ -9103,7 +9117,9 @@
       <c r="BO9" s="28">
         <v>57.3</v>
       </c>
-      <c r="BP9" s="28"/>
+      <c r="BP9" s="28">
+        <v>56.35</v>
+      </c>
       <c r="BQ9" s="28"/>
       <c r="BR9" s="28"/>
       <c r="BS9" s="28"/>
@@ -9311,7 +9327,9 @@
       <c r="BO10" s="5">
         <v>40.75</v>
       </c>
-      <c r="BP10" s="5"/>
+      <c r="BP10" s="5">
+        <v>39.6</v>
+      </c>
       <c r="BQ10" s="5"/>
       <c r="BR10" s="5"/>
       <c r="BS10" s="5"/>
@@ -9519,7 +9537,9 @@
       <c r="BO11" s="5">
         <v>100.2</v>
       </c>
-      <c r="BP11" s="5"/>
+      <c r="BP11" s="5">
+        <v>97.75</v>
+      </c>
       <c r="BQ11" s="5"/>
       <c r="BR11" s="5"/>
       <c r="BS11" s="5"/>
@@ -9727,7 +9747,9 @@
       <c r="BO12" s="5">
         <v>98.8</v>
       </c>
-      <c r="BP12" s="5"/>
+      <c r="BP12" s="5">
+        <v>93.55</v>
+      </c>
       <c r="BQ12" s="5"/>
       <c r="BR12" s="5"/>
       <c r="BS12" s="5"/>
@@ -9935,7 +9957,9 @@
       <c r="BO13" s="5">
         <v>49.85</v>
       </c>
-      <c r="BP13" s="5"/>
+      <c r="BP13" s="5">
+        <v>48.9</v>
+      </c>
       <c r="BQ13" s="5"/>
       <c r="BR13" s="5"/>
       <c r="BS13" s="5"/>
@@ -10143,7 +10167,9 @@
       <c r="BO14" s="5">
         <v>41.85</v>
       </c>
-      <c r="BP14" s="5"/>
+      <c r="BP14" s="5">
+        <v>39.950000000000003</v>
+      </c>
       <c r="BQ14" s="5"/>
       <c r="BR14" s="5"/>
       <c r="BS14" s="5"/>
@@ -10151,7 +10177,7 @@
     <row r="15" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
-        <v>26.05</v>
+        <v>25.65</v>
       </c>
       <c r="B15" s="12">
         <f t="shared" si="1"/>
@@ -10159,7 +10185,7 @@
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
-        <v>10.349999999999998</v>
+        <v>10.75</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>126</v>
@@ -10343,7 +10369,9 @@
       <c r="BO15" s="5">
         <v>26.05</v>
       </c>
-      <c r="BP15" s="5"/>
+      <c r="BP15" s="5">
+        <v>25.65</v>
+      </c>
       <c r="BQ15" s="5"/>
       <c r="BR15" s="5"/>
       <c r="BS15" s="5"/>
@@ -10551,7 +10579,9 @@
       <c r="BO16" s="5">
         <v>704.5</v>
       </c>
-      <c r="BP16" s="5"/>
+      <c r="BP16" s="5">
+        <v>696.6</v>
+      </c>
       <c r="BQ16" s="5"/>
       <c r="BR16" s="5"/>
       <c r="BS16" s="5"/>
@@ -10759,7 +10789,9 @@
       <c r="BO17" s="5">
         <v>485</v>
       </c>
-      <c r="BP17" s="5"/>
+      <c r="BP17" s="5">
+        <v>474.1</v>
+      </c>
       <c r="BQ17" s="5"/>
       <c r="BR17" s="5"/>
       <c r="BS17" s="5"/>
@@ -10967,7 +10999,9 @@
       <c r="BO18" s="5">
         <v>295</v>
       </c>
-      <c r="BP18" s="5"/>
+      <c r="BP18" s="5">
+        <v>292.10000000000002</v>
+      </c>
       <c r="BQ18" s="5"/>
       <c r="BR18" s="5"/>
       <c r="BS18" s="5"/>
@@ -11175,7 +11209,9 @@
       <c r="BO19" s="5">
         <v>553</v>
       </c>
-      <c r="BP19" s="5"/>
+      <c r="BP19" s="5">
+        <v>556.54999999999995</v>
+      </c>
       <c r="BQ19" s="5"/>
       <c r="BR19" s="5"/>
       <c r="BS19" s="5"/>
@@ -11383,7 +11419,9 @@
       <c r="BO20" s="5">
         <v>795.95</v>
       </c>
-      <c r="BP20" s="5"/>
+      <c r="BP20" s="5">
+        <v>781</v>
+      </c>
       <c r="BQ20" s="5"/>
       <c r="BR20" s="5"/>
       <c r="BS20" s="5"/>
@@ -11591,7 +11629,9 @@
       <c r="BO21" s="5">
         <v>532.9</v>
       </c>
-      <c r="BP21" s="5"/>
+      <c r="BP21" s="5">
+        <v>514.6</v>
+      </c>
       <c r="BQ21" s="5"/>
       <c r="BR21" s="5"/>
       <c r="BS21" s="5"/>
@@ -11745,7 +11785,9 @@
       <c r="BO22" s="5">
         <v>372.25</v>
       </c>
-      <c r="BP22" s="5"/>
+      <c r="BP22" s="5">
+        <v>360.15</v>
+      </c>
       <c r="BQ22" s="5"/>
       <c r="BR22" s="5"/>
       <c r="BS22" s="5"/>
@@ -11945,7 +11987,9 @@
       <c r="BO23" s="5">
         <v>61.3</v>
       </c>
-      <c r="BP23" s="5"/>
+      <c r="BP23" s="5">
+        <v>60.35</v>
+      </c>
       <c r="BQ23" s="5"/>
       <c r="BR23" s="5"/>
       <c r="BS23" s="5"/>
@@ -12141,7 +12185,9 @@
       <c r="BO24" s="5">
         <v>257.39999999999998</v>
       </c>
-      <c r="BP24" s="5"/>
+      <c r="BP24" s="5">
+        <v>249.9</v>
+      </c>
       <c r="BQ24" s="5"/>
       <c r="BR24" s="5"/>
       <c r="BS24" s="5"/>
@@ -12153,11 +12199,11 @@
       </c>
       <c r="B25" s="12">
         <f t="shared" si="1"/>
-        <v>950</v>
+        <v>955.35</v>
       </c>
       <c r="C25" s="12">
         <f t="shared" si="2"/>
-        <v>74</v>
+        <v>79.350000000000023</v>
       </c>
       <c r="D25" s="46" t="s">
         <v>236</v>
@@ -12319,7 +12365,9 @@
       <c r="BO25" s="5">
         <v>928.8</v>
       </c>
-      <c r="BP25" s="5"/>
+      <c r="BP25" s="5">
+        <v>955.35</v>
+      </c>
       <c r="BQ25" s="5"/>
       <c r="BR25" s="5"/>
       <c r="BS25" s="5"/>
@@ -12485,7 +12533,9 @@
       <c r="BO26" s="5">
         <v>91.3</v>
       </c>
-      <c r="BP26" s="5"/>
+      <c r="BP26" s="5">
+        <v>90.6</v>
+      </c>
       <c r="BQ26" s="5"/>
       <c r="BR26" s="5"/>
       <c r="BS26" s="5"/>
@@ -12651,7 +12701,9 @@
       <c r="BO27" s="5">
         <v>39.700000000000003</v>
       </c>
-      <c r="BP27" s="5"/>
+      <c r="BP27" s="5">
+        <v>39.9</v>
+      </c>
       <c r="BQ27" s="5"/>
       <c r="BR27" s="5"/>
       <c r="BS27" s="5"/>
@@ -12817,7 +12869,9 @@
       <c r="BO28" s="5">
         <v>138.80000000000001</v>
       </c>
-      <c r="BP28" s="5"/>
+      <c r="BP28" s="5">
+        <v>135.15</v>
+      </c>
       <c r="BQ28" s="5"/>
       <c r="BR28" s="5"/>
       <c r="BS28" s="5"/>
@@ -12983,7 +13037,9 @@
       <c r="BO29" s="5">
         <v>71</v>
       </c>
-      <c r="BP29" s="5"/>
+      <c r="BP29" s="5">
+        <v>70.8</v>
+      </c>
       <c r="BQ29" s="5"/>
       <c r="BR29" s="5"/>
       <c r="BS29" s="5"/>
@@ -13149,7 +13205,9 @@
       <c r="BO30" s="5">
         <v>50.95</v>
       </c>
-      <c r="BP30" s="5"/>
+      <c r="BP30" s="5">
+        <v>48</v>
+      </c>
       <c r="BQ30" s="5"/>
       <c r="BR30" s="5"/>
       <c r="BS30" s="5"/>
@@ -13157,7 +13215,7 @@
     <row r="31" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
-        <v>142.6</v>
+        <v>140.19999999999999</v>
       </c>
       <c r="B31" s="12">
         <f t="shared" si="1"/>
@@ -13165,7 +13223,7 @@
       </c>
       <c r="C31" s="12">
         <f t="shared" si="2"/>
-        <v>14.25</v>
+        <v>16.650000000000006</v>
       </c>
       <c r="D31" s="45" t="s">
         <v>257</v>
@@ -13315,7 +13373,9 @@
       <c r="BO31" s="5">
         <v>143.19999999999999</v>
       </c>
-      <c r="BP31" s="5"/>
+      <c r="BP31" s="5">
+        <v>140.19999999999999</v>
+      </c>
       <c r="BQ31" s="5"/>
       <c r="BR31" s="5"/>
       <c r="BS31" s="5"/>
@@ -13469,7 +13529,9 @@
       <c r="BO32" s="5">
         <v>117</v>
       </c>
-      <c r="BP32" s="5"/>
+      <c r="BP32" s="5">
+        <v>110</v>
+      </c>
       <c r="BQ32" s="5"/>
       <c r="BR32" s="5"/>
       <c r="BS32" s="5"/>
@@ -13611,7 +13673,9 @@
       <c r="BO33" s="5">
         <v>60.1</v>
       </c>
-      <c r="BP33" s="5"/>
+      <c r="BP33" s="5">
+        <v>61.8</v>
+      </c>
       <c r="BQ33" s="5"/>
       <c r="BR33" s="5"/>
       <c r="BS33" s="5"/>
@@ -13747,7 +13811,9 @@
       <c r="BO34" s="5">
         <v>203.8</v>
       </c>
-      <c r="BP34" s="5"/>
+      <c r="BP34" s="5">
+        <v>206</v>
+      </c>
       <c r="BQ34" s="5"/>
       <c r="BR34" s="5"/>
       <c r="BS34" s="5"/>
@@ -13879,7 +13945,9 @@
       <c r="BO35" s="5">
         <v>680.5</v>
       </c>
-      <c r="BP35" s="5"/>
+      <c r="BP35" s="5">
+        <v>680.1</v>
+      </c>
       <c r="BQ35" s="5"/>
       <c r="BR35" s="5"/>
       <c r="BS35" s="5"/>
@@ -13993,7 +14061,9 @@
       <c r="BO36" s="5">
         <v>470.4</v>
       </c>
-      <c r="BP36" s="5"/>
+      <c r="BP36" s="5">
+        <v>445</v>
+      </c>
       <c r="BQ36" s="5"/>
       <c r="BR36" s="5"/>
       <c r="BS36" s="5"/>
@@ -14097,7 +14167,9 @@
       <c r="BO37" s="5">
         <v>332</v>
       </c>
-      <c r="BP37" s="5"/>
+      <c r="BP37" s="5">
+        <v>323</v>
+      </c>
       <c r="BQ37" s="5"/>
       <c r="BR37" s="5"/>
       <c r="BS37" s="5"/>
@@ -14199,7 +14271,9 @@
       <c r="BO38" s="5">
         <v>500.1</v>
       </c>
-      <c r="BP38" s="5"/>
+      <c r="BP38" s="5">
+        <v>501.05</v>
+      </c>
       <c r="BQ38" s="5"/>
       <c r="BR38" s="5"/>
       <c r="BS38" s="5"/>
@@ -14295,7 +14369,9 @@
       <c r="BO39" s="5">
         <v>78.5</v>
       </c>
-      <c r="BP39" s="5"/>
+      <c r="BP39" s="5">
+        <v>76</v>
+      </c>
       <c r="BQ39" s="5"/>
       <c r="BR39" s="5"/>
       <c r="BS39" s="5"/>
@@ -14303,7 +14379,7 @@
     <row r="40" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <f t="shared" si="0"/>
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="B40" s="12">
         <f t="shared" si="1"/>
@@ -14311,7 +14387,7 @@
       </c>
       <c r="C40" s="12">
         <f t="shared" ref="C40" si="9">B40-A40</f>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>306</v>
@@ -14391,7 +14467,9 @@
       <c r="BO40" s="5">
         <v>467</v>
       </c>
-      <c r="BP40" s="5"/>
+      <c r="BP40" s="5">
+        <v>454</v>
+      </c>
       <c r="BQ40" s="5"/>
       <c r="BR40" s="5"/>
       <c r="BS40" s="5"/>
@@ -14399,7 +14477,7 @@
     <row r="41" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <f t="shared" si="0"/>
-        <v>201.7</v>
+        <v>199.5</v>
       </c>
       <c r="B41" s="12">
         <f t="shared" si="1"/>
@@ -14407,7 +14485,7 @@
       </c>
       <c r="C41" s="12">
         <f t="shared" ref="C41" si="10">B41-A41</f>
-        <v>8.1000000000000227</v>
+        <v>10.300000000000011</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>307</v>
@@ -14483,7 +14561,9 @@
       <c r="BO41" s="5">
         <v>201.7</v>
       </c>
-      <c r="BP41" s="5"/>
+      <c r="BP41" s="5">
+        <v>199.5</v>
+      </c>
       <c r="BQ41" s="5"/>
       <c r="BR41" s="5"/>
       <c r="BS41" s="5"/>
@@ -14571,7 +14651,9 @@
       <c r="BO42" s="5">
         <v>63.7</v>
       </c>
-      <c r="BP42" s="5"/>
+      <c r="BP42" s="5">
+        <v>63.6</v>
+      </c>
       <c r="BQ42" s="5"/>
       <c r="BR42" s="5"/>
       <c r="BS42" s="5"/>
@@ -14579,7 +14661,7 @@
     <row r="43" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <f t="shared" si="11"/>
-        <v>60.75</v>
+        <v>58.85</v>
       </c>
       <c r="B43" s="12">
         <f t="shared" si="12"/>
@@ -14587,7 +14669,7 @@
       </c>
       <c r="C43" s="12">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1.8999999999999986</v>
       </c>
       <c r="D43" s="45" t="s">
         <v>309</v>
@@ -14659,7 +14741,9 @@
       <c r="BO43" s="5">
         <v>60.75</v>
       </c>
-      <c r="BP43" s="5"/>
+      <c r="BP43" s="5">
+        <v>58.85</v>
+      </c>
       <c r="BQ43" s="5"/>
       <c r="BR43" s="5"/>
       <c r="BS43" s="5"/>
@@ -14747,7 +14831,9 @@
       <c r="BO44" s="5">
         <v>36.950000000000003</v>
       </c>
-      <c r="BP44" s="5"/>
+      <c r="BP44" s="5">
+        <v>37.450000000000003</v>
+      </c>
       <c r="BQ44" s="5"/>
       <c r="BR44" s="5"/>
       <c r="BS44" s="5"/>

</xml_diff>

<commit_message>
Added details for 8/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="313">
   <si>
     <t>Date</t>
   </si>
@@ -958,6 +958,12 @@
   </si>
   <si>
     <t>HCC</t>
+  </si>
+  <si>
+    <t>GRAPHITE</t>
+  </si>
+  <si>
+    <t>LUPIN</t>
   </si>
 </sst>
 </file>
@@ -7203,11 +7209,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BS44"/>
+  <dimension ref="A1:BS46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="BK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BP2" sqref="BP2:BP44"/>
+      <pane xSplit="4" topLeftCell="BH1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BP2" sqref="BP2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7662,7 +7668,7 @@
         <v>328</v>
       </c>
       <c r="BP2" s="5">
-        <v>317.25</v>
+        <v>312.55</v>
       </c>
       <c r="BQ2" s="5"/>
       <c r="BR2" s="5"/>
@@ -7866,7 +7872,7 @@
         <v>315.5</v>
       </c>
       <c r="BP3" s="5">
-        <v>312.45</v>
+        <v>306.39999999999998</v>
       </c>
       <c r="BQ3" s="5"/>
       <c r="BR3" s="5"/>
@@ -8076,7 +8082,7 @@
         <v>265</v>
       </c>
       <c r="BP4" s="5">
-        <v>265.10000000000002</v>
+        <v>265.3</v>
       </c>
       <c r="BQ4" s="5"/>
       <c r="BR4" s="5"/>
@@ -8286,7 +8292,7 @@
         <v>931.35</v>
       </c>
       <c r="BP5" s="5">
-        <v>906.5</v>
+        <v>889.5</v>
       </c>
       <c r="BQ5" s="5"/>
       <c r="BR5" s="5"/>
@@ -8496,7 +8502,7 @@
         <v>286.14999999999998</v>
       </c>
       <c r="BP6" s="5">
-        <v>285</v>
+        <v>286.45</v>
       </c>
       <c r="BQ6" s="5"/>
       <c r="BR6" s="5"/>
@@ -8706,7 +8712,7 @@
         <v>18.350000000000001</v>
       </c>
       <c r="BP7" s="5">
-        <v>17.600000000000001</v>
+        <v>17.55</v>
       </c>
       <c r="BQ7" s="5"/>
       <c r="BR7" s="5"/>
@@ -8916,7 +8922,7 @@
         <v>83.85</v>
       </c>
       <c r="BP8" s="5">
-        <v>78.400000000000006</v>
+        <v>77.75</v>
       </c>
       <c r="BQ8" s="5"/>
       <c r="BR8" s="5"/>
@@ -9118,7 +9124,7 @@
         <v>57.3</v>
       </c>
       <c r="BP9" s="28">
-        <v>56.35</v>
+        <v>56.2</v>
       </c>
       <c r="BQ9" s="28"/>
       <c r="BR9" s="28"/>
@@ -9328,7 +9334,7 @@
         <v>40.75</v>
       </c>
       <c r="BP10" s="5">
-        <v>39.6</v>
+        <v>39.15</v>
       </c>
       <c r="BQ10" s="5"/>
       <c r="BR10" s="5"/>
@@ -9538,7 +9544,7 @@
         <v>100.2</v>
       </c>
       <c r="BP11" s="5">
-        <v>97.75</v>
+        <v>101.3</v>
       </c>
       <c r="BQ11" s="5"/>
       <c r="BR11" s="5"/>
@@ -9748,7 +9754,7 @@
         <v>98.8</v>
       </c>
       <c r="BP12" s="5">
-        <v>93.55</v>
+        <v>90</v>
       </c>
       <c r="BQ12" s="5"/>
       <c r="BR12" s="5"/>
@@ -9958,7 +9964,7 @@
         <v>49.85</v>
       </c>
       <c r="BP13" s="5">
-        <v>48.9</v>
+        <v>48.3</v>
       </c>
       <c r="BQ13" s="5"/>
       <c r="BR13" s="5"/>
@@ -10168,7 +10174,7 @@
         <v>41.85</v>
       </c>
       <c r="BP14" s="5">
-        <v>39.950000000000003</v>
+        <v>39.4</v>
       </c>
       <c r="BQ14" s="5"/>
       <c r="BR14" s="5"/>
@@ -10177,7 +10183,7 @@
     <row r="15" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
-        <v>25.65</v>
+        <v>25.15</v>
       </c>
       <c r="B15" s="12">
         <f t="shared" si="1"/>
@@ -10185,7 +10191,7 @@
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
-        <v>10.75</v>
+        <v>11.25</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>126</v>
@@ -10370,7 +10376,7 @@
         <v>26.05</v>
       </c>
       <c r="BP15" s="5">
-        <v>25.65</v>
+        <v>25.15</v>
       </c>
       <c r="BQ15" s="5"/>
       <c r="BR15" s="5"/>
@@ -10580,7 +10586,7 @@
         <v>704.5</v>
       </c>
       <c r="BP16" s="5">
-        <v>696.6</v>
+        <v>698</v>
       </c>
       <c r="BQ16" s="5"/>
       <c r="BR16" s="5"/>
@@ -10790,7 +10796,7 @@
         <v>485</v>
       </c>
       <c r="BP17" s="5">
-        <v>474.1</v>
+        <v>474.85</v>
       </c>
       <c r="BQ17" s="5"/>
       <c r="BR17" s="5"/>
@@ -11000,7 +11006,7 @@
         <v>295</v>
       </c>
       <c r="BP18" s="5">
-        <v>292.10000000000002</v>
+        <v>294.2</v>
       </c>
       <c r="BQ18" s="5"/>
       <c r="BR18" s="5"/>
@@ -11210,7 +11216,7 @@
         <v>553</v>
       </c>
       <c r="BP19" s="5">
-        <v>556.54999999999995</v>
+        <v>554</v>
       </c>
       <c r="BQ19" s="5"/>
       <c r="BR19" s="5"/>
@@ -11420,7 +11426,7 @@
         <v>795.95</v>
       </c>
       <c r="BP20" s="5">
-        <v>781</v>
+        <v>791.5</v>
       </c>
       <c r="BQ20" s="5"/>
       <c r="BR20" s="5"/>
@@ -11630,7 +11636,7 @@
         <v>532.9</v>
       </c>
       <c r="BP21" s="5">
-        <v>514.6</v>
+        <v>496.3</v>
       </c>
       <c r="BQ21" s="5"/>
       <c r="BR21" s="5"/>
@@ -11786,7 +11792,7 @@
         <v>372.25</v>
       </c>
       <c r="BP22" s="5">
-        <v>360.15</v>
+        <v>369</v>
       </c>
       <c r="BQ22" s="5"/>
       <c r="BR22" s="5"/>
@@ -11988,7 +11994,7 @@
         <v>61.3</v>
       </c>
       <c r="BP23" s="5">
-        <v>60.35</v>
+        <v>59.1</v>
       </c>
       <c r="BQ23" s="5"/>
       <c r="BR23" s="5"/>
@@ -12186,7 +12192,7 @@
         <v>257.39999999999998</v>
       </c>
       <c r="BP24" s="5">
-        <v>249.9</v>
+        <v>245.7</v>
       </c>
       <c r="BQ24" s="5"/>
       <c r="BR24" s="5"/>
@@ -12199,11 +12205,11 @@
       </c>
       <c r="B25" s="12">
         <f t="shared" si="1"/>
-        <v>955.35</v>
+        <v>951.95</v>
       </c>
       <c r="C25" s="12">
         <f t="shared" si="2"/>
-        <v>79.350000000000023</v>
+        <v>75.950000000000045</v>
       </c>
       <c r="D25" s="46" t="s">
         <v>236</v>
@@ -12366,7 +12372,7 @@
         <v>928.8</v>
       </c>
       <c r="BP25" s="5">
-        <v>955.35</v>
+        <v>951.95</v>
       </c>
       <c r="BQ25" s="5"/>
       <c r="BR25" s="5"/>
@@ -12534,7 +12540,7 @@
         <v>91.3</v>
       </c>
       <c r="BP26" s="5">
-        <v>90.6</v>
+        <v>93</v>
       </c>
       <c r="BQ26" s="5"/>
       <c r="BR26" s="5"/>
@@ -12702,7 +12708,7 @@
         <v>39.700000000000003</v>
       </c>
       <c r="BP27" s="5">
-        <v>39.9</v>
+        <v>39</v>
       </c>
       <c r="BQ27" s="5"/>
       <c r="BR27" s="5"/>
@@ -12870,7 +12876,7 @@
         <v>138.80000000000001</v>
       </c>
       <c r="BP28" s="5">
-        <v>135.15</v>
+        <v>135.19999999999999</v>
       </c>
       <c r="BQ28" s="5"/>
       <c r="BR28" s="5"/>
@@ -13038,7 +13044,7 @@
         <v>71</v>
       </c>
       <c r="BP29" s="5">
-        <v>70.8</v>
+        <v>68</v>
       </c>
       <c r="BQ29" s="5"/>
       <c r="BR29" s="5"/>
@@ -13206,7 +13212,7 @@
         <v>50.95</v>
       </c>
       <c r="BP30" s="5">
-        <v>48</v>
+        <v>47.25</v>
       </c>
       <c r="BQ30" s="5"/>
       <c r="BR30" s="5"/>
@@ -13215,7 +13221,7 @@
     <row r="31" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
-        <v>140.19999999999999</v>
+        <v>138.19999999999999</v>
       </c>
       <c r="B31" s="12">
         <f t="shared" si="1"/>
@@ -13223,7 +13229,7 @@
       </c>
       <c r="C31" s="12">
         <f t="shared" si="2"/>
-        <v>16.650000000000006</v>
+        <v>18.650000000000006</v>
       </c>
       <c r="D31" s="45" t="s">
         <v>257</v>
@@ -13374,7 +13380,7 @@
         <v>143.19999999999999</v>
       </c>
       <c r="BP31" s="5">
-        <v>140.19999999999999</v>
+        <v>138.19999999999999</v>
       </c>
       <c r="BQ31" s="5"/>
       <c r="BR31" s="5"/>
@@ -13530,7 +13536,7 @@
         <v>117</v>
       </c>
       <c r="BP32" s="5">
-        <v>110</v>
+        <v>106.35</v>
       </c>
       <c r="BQ32" s="5"/>
       <c r="BR32" s="5"/>
@@ -13674,7 +13680,7 @@
         <v>60.1</v>
       </c>
       <c r="BP33" s="5">
-        <v>61.8</v>
+        <v>61</v>
       </c>
       <c r="BQ33" s="5"/>
       <c r="BR33" s="5"/>
@@ -13812,7 +13818,7 @@
         <v>203.8</v>
       </c>
       <c r="BP34" s="5">
-        <v>206</v>
+        <v>196.95</v>
       </c>
       <c r="BQ34" s="5"/>
       <c r="BR34" s="5"/>
@@ -13946,7 +13952,7 @@
         <v>680.5</v>
       </c>
       <c r="BP35" s="5">
-        <v>680.1</v>
+        <v>681</v>
       </c>
       <c r="BQ35" s="5"/>
       <c r="BR35" s="5"/>
@@ -14062,7 +14068,7 @@
         <v>470.4</v>
       </c>
       <c r="BP36" s="5">
-        <v>445</v>
+        <v>477</v>
       </c>
       <c r="BQ36" s="5"/>
       <c r="BR36" s="5"/>
@@ -14075,11 +14081,11 @@
       </c>
       <c r="B37" s="12">
         <f t="shared" si="1"/>
-        <v>332</v>
+        <v>349</v>
       </c>
       <c r="C37" s="12">
         <f t="shared" ref="C37" si="6">B37-A37</f>
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="D37" s="45" t="s">
         <v>297</v>
@@ -14168,7 +14174,7 @@
         <v>332</v>
       </c>
       <c r="BP37" s="5">
-        <v>323</v>
+        <v>349</v>
       </c>
       <c r="BQ37" s="5"/>
       <c r="BR37" s="5"/>
@@ -14272,7 +14278,7 @@
         <v>500.1</v>
       </c>
       <c r="BP38" s="5">
-        <v>501.05</v>
+        <v>503.15</v>
       </c>
       <c r="BQ38" s="5"/>
       <c r="BR38" s="5"/>
@@ -14281,7 +14287,7 @@
     <row r="39" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <f t="shared" si="0"/>
-        <v>76</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="B39" s="12">
         <f t="shared" si="1"/>
@@ -14289,7 +14295,7 @@
       </c>
       <c r="C39" s="12">
         <f t="shared" ref="C39" si="8">B39-A39</f>
-        <v>2.5</v>
+        <v>2.9000000000000057</v>
       </c>
       <c r="D39" s="45" t="s">
         <v>305</v>
@@ -14370,7 +14376,7 @@
         <v>78.5</v>
       </c>
       <c r="BP39" s="5">
-        <v>76</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="BQ39" s="5"/>
       <c r="BR39" s="5"/>
@@ -14379,7 +14385,7 @@
     <row r="40" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <f t="shared" si="0"/>
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B40" s="12">
         <f t="shared" si="1"/>
@@ -14387,7 +14393,7 @@
       </c>
       <c r="C40" s="12">
         <f t="shared" ref="C40" si="9">B40-A40</f>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>306</v>
@@ -14468,7 +14474,7 @@
         <v>467</v>
       </c>
       <c r="BP40" s="5">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="BQ40" s="5"/>
       <c r="BR40" s="5"/>
@@ -14477,7 +14483,7 @@
     <row r="41" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <f t="shared" si="0"/>
-        <v>199.5</v>
+        <v>197.05</v>
       </c>
       <c r="B41" s="12">
         <f t="shared" si="1"/>
@@ -14485,7 +14491,7 @@
       </c>
       <c r="C41" s="12">
         <f t="shared" ref="C41" si="10">B41-A41</f>
-        <v>10.300000000000011</v>
+        <v>12.75</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>307</v>
@@ -14562,7 +14568,7 @@
         <v>201.7</v>
       </c>
       <c r="BP41" s="5">
-        <v>199.5</v>
+        <v>197.05</v>
       </c>
       <c r="BQ41" s="5"/>
       <c r="BR41" s="5"/>
@@ -14652,7 +14658,7 @@
         <v>63.7</v>
       </c>
       <c r="BP42" s="5">
-        <v>63.6</v>
+        <v>63.7</v>
       </c>
       <c r="BQ42" s="5"/>
       <c r="BR42" s="5"/>
@@ -14661,7 +14667,7 @@
     <row r="43" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <f t="shared" si="11"/>
-        <v>58.85</v>
+        <v>57.15</v>
       </c>
       <c r="B43" s="12">
         <f t="shared" si="12"/>
@@ -14669,7 +14675,7 @@
       </c>
       <c r="C43" s="12">
         <f t="shared" si="13"/>
-        <v>1.8999999999999986</v>
+        <v>3.6000000000000014</v>
       </c>
       <c r="D43" s="45" t="s">
         <v>309</v>
@@ -14742,7 +14748,7 @@
         <v>60.75</v>
       </c>
       <c r="BP43" s="5">
-        <v>58.85</v>
+        <v>57.15</v>
       </c>
       <c r="BQ43" s="5"/>
       <c r="BR43" s="5"/>
@@ -14755,11 +14761,11 @@
       </c>
       <c r="B44" s="12">
         <f t="shared" ref="B44" si="15">MAX(E44:ZX44)</f>
-        <v>38.1</v>
+        <v>38.9</v>
       </c>
       <c r="C44" s="12">
         <f t="shared" ref="C44" si="16">B44-A44</f>
-        <v>1.1499999999999986</v>
+        <v>1.9499999999999957</v>
       </c>
       <c r="D44" s="45" t="s">
         <v>310</v>
@@ -14832,11 +14838,183 @@
         <v>36.950000000000003</v>
       </c>
       <c r="BP44" s="5">
-        <v>37.450000000000003</v>
+        <v>38.9</v>
       </c>
       <c r="BQ44" s="5"/>
       <c r="BR44" s="5"/>
       <c r="BS44" s="5"/>
+    </row>
+    <row r="45" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A45" s="12">
+        <f t="shared" ref="A45:A46" si="17">MIN(E45:ZX45)</f>
+        <v>583.75</v>
+      </c>
+      <c r="B45" s="12">
+        <f t="shared" ref="B45:B46" si="18">MAX(E45:ZX45)</f>
+        <v>583.75</v>
+      </c>
+      <c r="C45" s="12">
+        <f t="shared" ref="C45:C46" si="19">B45-A45</f>
+        <v>0</v>
+      </c>
+      <c r="D45" s="45" t="s">
+        <v>311</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="5"/>
+      <c r="U45" s="5"/>
+      <c r="V45" s="5"/>
+      <c r="W45" s="5"/>
+      <c r="X45" s="5"/>
+      <c r="Y45" s="5"/>
+      <c r="Z45" s="5"/>
+      <c r="AA45" s="5"/>
+      <c r="AB45" s="5"/>
+      <c r="AC45" s="5"/>
+      <c r="AD45" s="5"/>
+      <c r="AE45" s="5"/>
+      <c r="AF45" s="5"/>
+      <c r="AG45" s="5"/>
+      <c r="AH45" s="5"/>
+      <c r="AI45" s="5"/>
+      <c r="AJ45" s="5"/>
+      <c r="AK45" s="5"/>
+      <c r="AL45" s="5"/>
+      <c r="AM45" s="5"/>
+      <c r="AN45" s="5"/>
+      <c r="AO45" s="5"/>
+      <c r="AP45" s="5"/>
+      <c r="AQ45" s="5"/>
+      <c r="AR45" s="5"/>
+      <c r="AS45" s="5"/>
+      <c r="AT45" s="5"/>
+      <c r="AU45" s="5"/>
+      <c r="AV45" s="5"/>
+      <c r="AW45" s="5"/>
+      <c r="AX45" s="5"/>
+      <c r="AY45" s="5"/>
+      <c r="AZ45" s="5"/>
+      <c r="BA45" s="5"/>
+      <c r="BB45" s="5"/>
+      <c r="BC45" s="5"/>
+      <c r="BD45" s="5"/>
+      <c r="BE45" s="5"/>
+      <c r="BF45" s="5"/>
+      <c r="BG45" s="5"/>
+      <c r="BH45" s="5"/>
+      <c r="BI45" s="5"/>
+      <c r="BJ45" s="5"/>
+      <c r="BK45" s="5"/>
+      <c r="BL45" s="5"/>
+      <c r="BM45" s="5"/>
+      <c r="BN45" s="5"/>
+      <c r="BO45" s="5"/>
+      <c r="BP45" s="5">
+        <v>583.75</v>
+      </c>
+      <c r="BQ45" s="5"/>
+      <c r="BR45" s="5"/>
+      <c r="BS45" s="5"/>
+    </row>
+    <row r="46" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A46" s="12">
+        <f t="shared" si="17"/>
+        <v>839.5</v>
+      </c>
+      <c r="B46" s="12">
+        <f t="shared" si="18"/>
+        <v>839.5</v>
+      </c>
+      <c r="C46" s="12">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="D46" s="45" t="s">
+        <v>312</v>
+      </c>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="5"/>
+      <c r="V46" s="5"/>
+      <c r="W46" s="5"/>
+      <c r="X46" s="5"/>
+      <c r="Y46" s="5"/>
+      <c r="Z46" s="5"/>
+      <c r="AA46" s="5"/>
+      <c r="AB46" s="5"/>
+      <c r="AC46" s="5"/>
+      <c r="AD46" s="5"/>
+      <c r="AE46" s="5"/>
+      <c r="AF46" s="5"/>
+      <c r="AG46" s="5"/>
+      <c r="AH46" s="5"/>
+      <c r="AI46" s="5"/>
+      <c r="AJ46" s="5"/>
+      <c r="AK46" s="5"/>
+      <c r="AL46" s="5"/>
+      <c r="AM46" s="5"/>
+      <c r="AN46" s="5"/>
+      <c r="AO46" s="5"/>
+      <c r="AP46" s="5"/>
+      <c r="AQ46" s="5"/>
+      <c r="AR46" s="5"/>
+      <c r="AS46" s="5"/>
+      <c r="AT46" s="5"/>
+      <c r="AU46" s="5"/>
+      <c r="AV46" s="5"/>
+      <c r="AW46" s="5"/>
+      <c r="AX46" s="5"/>
+      <c r="AY46" s="5"/>
+      <c r="AZ46" s="5"/>
+      <c r="BA46" s="5"/>
+      <c r="BB46" s="5"/>
+      <c r="BC46" s="5"/>
+      <c r="BD46" s="5"/>
+      <c r="BE46" s="5"/>
+      <c r="BF46" s="5"/>
+      <c r="BG46" s="5"/>
+      <c r="BH46" s="5"/>
+      <c r="BI46" s="5"/>
+      <c r="BJ46" s="5"/>
+      <c r="BK46" s="5"/>
+      <c r="BL46" s="5"/>
+      <c r="BM46" s="5"/>
+      <c r="BN46" s="5"/>
+      <c r="BO46" s="5"/>
+      <c r="BP46" s="5">
+        <v>839.5</v>
+      </c>
+      <c r="BQ46" s="5"/>
+      <c r="BR46" s="5"/>
+      <c r="BS46" s="5"/>
     </row>
   </sheetData>
   <sortState ref="L1:L37">

</xml_diff>

<commit_message>
Added details for 9/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="314">
   <si>
     <t>Date</t>
   </si>
@@ -964,6 +964,9 @@
   </si>
   <si>
     <t>LUPIN</t>
+  </si>
+  <si>
+    <t>GSFC</t>
   </si>
 </sst>
 </file>
@@ -7209,11 +7212,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BS46"/>
+  <dimension ref="A1:BR47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="BH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BP2" sqref="BP2"/>
+      <pane xSplit="4" topLeftCell="BO1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CM34" sqref="CM34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7251,11 +7254,11 @@
     <col min="62" max="62" width="14.42578125" customWidth="1"/>
     <col min="63" max="63" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="14" bestFit="1" customWidth="1"/>
-    <col min="65" max="70" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="65" max="69" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>249</v>
       </c>
@@ -7461,22 +7464,19 @@
         <v>42927</v>
       </c>
       <c r="BQ1" s="51">
-        <v>42958</v>
+        <v>42989</v>
       </c>
       <c r="BR1" s="51">
-        <v>42989</v>
-      </c>
-      <c r="BS1" s="51">
         <v>43019</v>
       </c>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
-        <f t="shared" ref="A2:A41" si="0">MIN(E2:ZX2)</f>
+        <f>MIN(E2:ZW2)</f>
         <v>243.6</v>
       </c>
       <c r="B2" s="12">
-        <f t="shared" ref="B2:B41" si="1">MAX(E2:ZX2)</f>
+        <f>MAX(E2:ZW2)</f>
         <v>328</v>
       </c>
       <c r="C2" s="12">
@@ -7668,23 +7668,24 @@
         <v>328</v>
       </c>
       <c r="BP2" s="5">
-        <v>312.55</v>
-      </c>
-      <c r="BQ2" s="5"/>
+        <v>311.8</v>
+      </c>
+      <c r="BQ2" s="5">
+        <v>314.8</v>
+      </c>
       <c r="BR2" s="5"/>
-      <c r="BS2" s="5"/>
-    </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E3:ZW3)</f>
         <v>262.7</v>
       </c>
       <c r="B3" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E3:ZW3)</f>
         <v>316.14999999999998</v>
       </c>
       <c r="C3" s="12">
-        <f t="shared" ref="C3:C33" si="2">B3-A3</f>
+        <f t="shared" ref="C3:C33" si="0">B3-A3</f>
         <v>53.449999999999989</v>
       </c>
       <c r="D3" s="44" t="s">
@@ -7872,23 +7873,24 @@
         <v>315.5</v>
       </c>
       <c r="BP3" s="5">
-        <v>306.39999999999998</v>
-      </c>
-      <c r="BQ3" s="5"/>
+        <v>310.7</v>
+      </c>
+      <c r="BQ3" s="5">
+        <v>312</v>
+      </c>
       <c r="BR3" s="5"/>
-      <c r="BS3" s="5"/>
-    </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
+        <f>MIN(E4:ZW4)</f>
+        <v>259.45</v>
+      </c>
+      <c r="B4" s="12">
+        <f>MAX(E4:ZW4)</f>
+        <v>291.7</v>
+      </c>
+      <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>259.45</v>
-      </c>
-      <c r="B4" s="12">
-        <f t="shared" si="1"/>
-        <v>291.7</v>
-      </c>
-      <c r="C4" s="12">
-        <f t="shared" si="2"/>
         <v>32.25</v>
       </c>
       <c r="D4" s="44" t="s">
@@ -8082,23 +8084,24 @@
         <v>265</v>
       </c>
       <c r="BP4" s="5">
-        <v>265.3</v>
-      </c>
-      <c r="BQ4" s="5"/>
+        <v>262.60000000000002</v>
+      </c>
+      <c r="BQ4" s="5">
+        <v>260.35000000000002</v>
+      </c>
       <c r="BR4" s="5"/>
-      <c r="BS4" s="5"/>
-    </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
+        <f>MIN(E5:ZW5)</f>
+        <v>786.25</v>
+      </c>
+      <c r="B5" s="12">
+        <f>MAX(E5:ZW5)</f>
+        <v>946.8</v>
+      </c>
+      <c r="C5" s="12">
         <f t="shared" si="0"/>
-        <v>786.25</v>
-      </c>
-      <c r="B5" s="12">
-        <f t="shared" si="1"/>
-        <v>946.8</v>
-      </c>
-      <c r="C5" s="12">
-        <f t="shared" si="2"/>
         <v>160.54999999999995</v>
       </c>
       <c r="D5" s="44" t="s">
@@ -8292,23 +8295,24 @@
         <v>931.35</v>
       </c>
       <c r="BP5" s="5">
-        <v>889.5</v>
-      </c>
-      <c r="BQ5" s="5"/>
+        <v>906.1</v>
+      </c>
+      <c r="BQ5" s="5">
+        <v>902.4</v>
+      </c>
       <c r="BR5" s="5"/>
-      <c r="BS5" s="5"/>
-    </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
+        <f>MIN(E6:ZW6)</f>
+        <v>236.45</v>
+      </c>
+      <c r="B6" s="12">
+        <f>MAX(E6:ZW6)</f>
+        <v>293.95</v>
+      </c>
+      <c r="C6" s="12">
         <f t="shared" si="0"/>
-        <v>236.45</v>
-      </c>
-      <c r="B6" s="12">
-        <f t="shared" si="1"/>
-        <v>293.95</v>
-      </c>
-      <c r="C6" s="12">
-        <f t="shared" si="2"/>
         <v>57.5</v>
       </c>
       <c r="D6" s="45" t="s">
@@ -8502,23 +8506,24 @@
         <v>286.14999999999998</v>
       </c>
       <c r="BP6" s="5">
-        <v>286.45</v>
-      </c>
-      <c r="BQ6" s="5"/>
+        <v>282.3</v>
+      </c>
+      <c r="BQ6" s="5">
+        <v>283.25</v>
+      </c>
       <c r="BR6" s="5"/>
-      <c r="BS6" s="5"/>
-    </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
+        <f>MIN(E7:ZW7)</f>
+        <v>15.6</v>
+      </c>
+      <c r="B7" s="12">
+        <f>MAX(E7:ZW7)</f>
+        <v>19.350000000000001</v>
+      </c>
+      <c r="C7" s="12">
         <f t="shared" si="0"/>
-        <v>15.6</v>
-      </c>
-      <c r="B7" s="12">
-        <f t="shared" si="1"/>
-        <v>19.350000000000001</v>
-      </c>
-      <c r="C7" s="12">
-        <f t="shared" si="2"/>
         <v>3.7500000000000018</v>
       </c>
       <c r="D7" s="45" t="s">
@@ -8712,23 +8717,24 @@
         <v>18.350000000000001</v>
       </c>
       <c r="BP7" s="5">
-        <v>17.55</v>
-      </c>
-      <c r="BQ7" s="5"/>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="BQ7" s="5">
+        <v>17.8</v>
+      </c>
       <c r="BR7" s="5"/>
-      <c r="BS7" s="5"/>
-    </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
+        <f>MIN(E8:ZW8)</f>
+        <v>53.4</v>
+      </c>
+      <c r="B8" s="12">
+        <f>MAX(E8:ZW8)</f>
+        <v>86.75</v>
+      </c>
+      <c r="C8" s="12">
         <f t="shared" si="0"/>
-        <v>53.4</v>
-      </c>
-      <c r="B8" s="12">
-        <f t="shared" si="1"/>
-        <v>86.75</v>
-      </c>
-      <c r="C8" s="12">
-        <f t="shared" si="2"/>
         <v>33.35</v>
       </c>
       <c r="D8" s="45" t="s">
@@ -8922,23 +8928,24 @@
         <v>83.85</v>
       </c>
       <c r="BP8" s="5">
-        <v>77.75</v>
-      </c>
-      <c r="BQ8" s="5"/>
+        <v>77.95</v>
+      </c>
+      <c r="BQ8" s="5">
+        <v>78.75</v>
+      </c>
       <c r="BR8" s="5"/>
-      <c r="BS8" s="5"/>
-    </row>
-    <row r="9" spans="1:71" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:70" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
+        <f>MIN(E9:ZW9)</f>
+        <v>53.5</v>
+      </c>
+      <c r="B9" s="39">
+        <f>MAX(E9:ZW9)</f>
+        <v>61</v>
+      </c>
+      <c r="C9" s="12">
         <f t="shared" si="0"/>
-        <v>53.5</v>
-      </c>
-      <c r="B9" s="39">
-        <f t="shared" si="1"/>
-        <v>61</v>
-      </c>
-      <c r="C9" s="12">
-        <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
       <c r="D9" s="43" t="s">
@@ -9124,23 +9131,24 @@
         <v>57.3</v>
       </c>
       <c r="BP9" s="28">
-        <v>56.2</v>
-      </c>
-      <c r="BQ9" s="28"/>
+        <v>56.15</v>
+      </c>
+      <c r="BQ9" s="28">
+        <v>56.35</v>
+      </c>
       <c r="BR9" s="28"/>
-      <c r="BS9" s="28"/>
-    </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
+        <f>MIN(E10:ZW10)</f>
+        <v>38.6</v>
+      </c>
+      <c r="B10" s="12">
+        <f>MAX(E10:ZW10)</f>
+        <v>45.35</v>
+      </c>
+      <c r="C10" s="12">
         <f t="shared" si="0"/>
-        <v>38.6</v>
-      </c>
-      <c r="B10" s="12">
-        <f t="shared" si="1"/>
-        <v>45.35</v>
-      </c>
-      <c r="C10" s="12">
-        <f t="shared" si="2"/>
         <v>6.75</v>
       </c>
       <c r="D10" s="45" t="s">
@@ -9336,21 +9344,22 @@
       <c r="BP10" s="5">
         <v>39.15</v>
       </c>
-      <c r="BQ10" s="5"/>
+      <c r="BQ10" s="5">
+        <v>39.299999999999997</v>
+      </c>
       <c r="BR10" s="5"/>
-      <c r="BS10" s="5"/>
-    </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
+        <f>MIN(E11:ZW11)</f>
+        <v>72.650000000000006</v>
+      </c>
+      <c r="B11" s="12">
+        <f>MAX(E11:ZW11)</f>
+        <v>106.5</v>
+      </c>
+      <c r="C11" s="12">
         <f t="shared" si="0"/>
-        <v>72.650000000000006</v>
-      </c>
-      <c r="B11" s="12">
-        <f t="shared" si="1"/>
-        <v>106.5</v>
-      </c>
-      <c r="C11" s="12">
-        <f t="shared" si="2"/>
         <v>33.849999999999994</v>
       </c>
       <c r="D11" s="45" t="s">
@@ -9544,23 +9553,24 @@
         <v>100.2</v>
       </c>
       <c r="BP11" s="5">
-        <v>101.3</v>
-      </c>
-      <c r="BQ11" s="5"/>
+        <v>97.1</v>
+      </c>
+      <c r="BQ11" s="5">
+        <v>96.2</v>
+      </c>
       <c r="BR11" s="5"/>
-      <c r="BS11" s="5"/>
-    </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
+        <f>MIN(E12:ZW12)</f>
+        <v>82.65</v>
+      </c>
+      <c r="B12" s="12">
+        <f>MAX(E12:ZW12)</f>
+        <v>99.6</v>
+      </c>
+      <c r="C12" s="12">
         <f t="shared" si="0"/>
-        <v>82.65</v>
-      </c>
-      <c r="B12" s="12">
-        <f t="shared" si="1"/>
-        <v>99.6</v>
-      </c>
-      <c r="C12" s="12">
-        <f t="shared" si="2"/>
         <v>16.949999999999989</v>
       </c>
       <c r="D12" s="45" t="s">
@@ -9754,23 +9764,24 @@
         <v>98.8</v>
       </c>
       <c r="BP12" s="5">
-        <v>90</v>
-      </c>
-      <c r="BQ12" s="5"/>
+        <v>90.9</v>
+      </c>
+      <c r="BQ12" s="5">
+        <v>92.2</v>
+      </c>
       <c r="BR12" s="5"/>
-      <c r="BS12" s="5"/>
-    </row>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
+        <f>MIN(E13:ZW13)</f>
+        <v>44.1</v>
+      </c>
+      <c r="B13" s="12">
+        <f>MAX(E13:ZW13)</f>
+        <v>57.15</v>
+      </c>
+      <c r="C13" s="12">
         <f t="shared" si="0"/>
-        <v>44.1</v>
-      </c>
-      <c r="B13" s="12">
-        <f t="shared" si="1"/>
-        <v>57.15</v>
-      </c>
-      <c r="C13" s="12">
-        <f t="shared" si="2"/>
         <v>13.049999999999997</v>
       </c>
       <c r="D13" s="45" t="s">
@@ -9964,23 +9975,24 @@
         <v>49.85</v>
       </c>
       <c r="BP13" s="5">
-        <v>48.3</v>
-      </c>
-      <c r="BQ13" s="5"/>
+        <v>48.55</v>
+      </c>
+      <c r="BQ13" s="5">
+        <v>48.35</v>
+      </c>
       <c r="BR13" s="5"/>
-      <c r="BS13" s="5"/>
-    </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
+        <f>MIN(E14:ZW14)</f>
+        <v>29.75</v>
+      </c>
+      <c r="B14" s="12">
+        <f>MAX(E14:ZW14)</f>
+        <v>41.85</v>
+      </c>
+      <c r="C14" s="12">
         <f t="shared" si="0"/>
-        <v>29.75</v>
-      </c>
-      <c r="B14" s="12">
-        <f t="shared" si="1"/>
-        <v>41.85</v>
-      </c>
-      <c r="C14" s="12">
-        <f t="shared" si="2"/>
         <v>12.100000000000001</v>
       </c>
       <c r="D14" s="45" t="s">
@@ -10174,24 +10186,25 @@
         <v>41.85</v>
       </c>
       <c r="BP14" s="5">
-        <v>39.4</v>
-      </c>
-      <c r="BQ14" s="5"/>
+        <v>39.299999999999997</v>
+      </c>
+      <c r="BQ14" s="5">
+        <v>39.1</v>
+      </c>
       <c r="BR14" s="5"/>
-      <c r="BS14" s="5"/>
-    </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
+        <f>MIN(E15:ZW15)</f>
+        <v>25.25</v>
+      </c>
+      <c r="B15" s="12">
+        <f>MAX(E15:ZW15)</f>
+        <v>36.4</v>
+      </c>
+      <c r="C15" s="12">
         <f t="shared" si="0"/>
-        <v>25.15</v>
-      </c>
-      <c r="B15" s="12">
-        <f t="shared" si="1"/>
-        <v>36.4</v>
-      </c>
-      <c r="C15" s="12">
-        <f t="shared" si="2"/>
-        <v>11.25</v>
+        <v>11.149999999999999</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>126</v>
@@ -10376,23 +10389,24 @@
         <v>26.05</v>
       </c>
       <c r="BP15" s="5">
-        <v>25.15</v>
-      </c>
-      <c r="BQ15" s="5"/>
+        <v>25.25</v>
+      </c>
+      <c r="BQ15" s="5">
+        <v>26.25</v>
+      </c>
       <c r="BR15" s="5"/>
-      <c r="BS15" s="5"/>
-    </row>
-    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
+        <f>MIN(E16:ZW16)</f>
+        <v>552</v>
+      </c>
+      <c r="B16" s="12">
+        <f>MAX(E16:ZW16)</f>
+        <v>729.5</v>
+      </c>
+      <c r="C16" s="12">
         <f t="shared" si="0"/>
-        <v>552</v>
-      </c>
-      <c r="B16" s="12">
-        <f t="shared" si="1"/>
-        <v>729.5</v>
-      </c>
-      <c r="C16" s="12">
-        <f t="shared" si="2"/>
         <v>177.5</v>
       </c>
       <c r="D16" s="45" t="s">
@@ -10586,23 +10600,24 @@
         <v>704.5</v>
       </c>
       <c r="BP16" s="5">
-        <v>698</v>
-      </c>
-      <c r="BQ16" s="5"/>
+        <v>696.85</v>
+      </c>
+      <c r="BQ16" s="5">
+        <v>704.9</v>
+      </c>
       <c r="BR16" s="5"/>
-      <c r="BS16" s="5"/>
-    </row>
-    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
+        <f>MIN(E17:ZW17)</f>
+        <v>433</v>
+      </c>
+      <c r="B17" s="12">
+        <f>MAX(E17:ZW17)</f>
+        <v>515</v>
+      </c>
+      <c r="C17" s="12">
         <f t="shared" si="0"/>
-        <v>433</v>
-      </c>
-      <c r="B17" s="12">
-        <f t="shared" si="1"/>
-        <v>515</v>
-      </c>
-      <c r="C17" s="12">
-        <f t="shared" si="2"/>
         <v>82</v>
       </c>
       <c r="D17" s="44" t="s">
@@ -10796,23 +10811,24 @@
         <v>485</v>
       </c>
       <c r="BP17" s="5">
-        <v>474.85</v>
-      </c>
-      <c r="BQ17" s="5"/>
+        <v>475.85</v>
+      </c>
+      <c r="BQ17" s="5">
+        <v>474.5</v>
+      </c>
       <c r="BR17" s="5"/>
-      <c r="BS17" s="5"/>
-    </row>
-    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
+        <f>MIN(E18:ZW18)</f>
+        <v>178.8</v>
+      </c>
+      <c r="B18" s="12">
+        <f>MAX(E18:ZW18)</f>
+        <v>302.2</v>
+      </c>
+      <c r="C18" s="12">
         <f t="shared" si="0"/>
-        <v>178.8</v>
-      </c>
-      <c r="B18" s="12">
-        <f t="shared" si="1"/>
-        <v>302.2</v>
-      </c>
-      <c r="C18" s="12">
-        <f t="shared" si="2"/>
         <v>123.39999999999998</v>
       </c>
       <c r="D18" s="44" t="s">
@@ -11006,24 +11022,25 @@
         <v>295</v>
       </c>
       <c r="BP18" s="5">
-        <v>294.2</v>
-      </c>
-      <c r="BQ18" s="5"/>
+        <v>295.5</v>
+      </c>
+      <c r="BQ18" s="5">
+        <v>294</v>
+      </c>
       <c r="BR18" s="5"/>
-      <c r="BS18" s="5"/>
-    </row>
-    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
+        <f>MIN(E19:ZW19)</f>
+        <v>440.7</v>
+      </c>
+      <c r="B19" s="12">
+        <f>MAX(E19:ZW19)</f>
+        <v>588.75</v>
+      </c>
+      <c r="C19" s="12">
         <f t="shared" si="0"/>
-        <v>440.7</v>
-      </c>
-      <c r="B19" s="12">
-        <f t="shared" si="1"/>
-        <v>562.79999999999995</v>
-      </c>
-      <c r="C19" s="12">
-        <f t="shared" si="2"/>
-        <v>122.09999999999997</v>
+        <v>148.05000000000001</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -11216,23 +11233,24 @@
         <v>553</v>
       </c>
       <c r="BP19" s="5">
-        <v>554</v>
-      </c>
-      <c r="BQ19" s="5"/>
+        <v>572.29999999999995</v>
+      </c>
+      <c r="BQ19" s="5">
+        <v>588.75</v>
+      </c>
       <c r="BR19" s="5"/>
-      <c r="BS19" s="5"/>
-    </row>
-    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
+        <f>MIN(E20:ZW20)</f>
+        <v>677</v>
+      </c>
+      <c r="B20" s="12">
+        <f>MAX(E20:ZW20)</f>
+        <v>795.95</v>
+      </c>
+      <c r="C20" s="12">
         <f t="shared" si="0"/>
-        <v>677</v>
-      </c>
-      <c r="B20" s="12">
-        <f t="shared" si="1"/>
-        <v>795.95</v>
-      </c>
-      <c r="C20" s="12">
-        <f t="shared" si="2"/>
         <v>118.95000000000005</v>
       </c>
       <c r="D20" s="44" t="s">
@@ -11426,23 +11444,24 @@
         <v>795.95</v>
       </c>
       <c r="BP20" s="5">
-        <v>791.5</v>
-      </c>
-      <c r="BQ20" s="5"/>
+        <v>776.25</v>
+      </c>
+      <c r="BQ20" s="5">
+        <v>788.15</v>
+      </c>
       <c r="BR20" s="5"/>
-      <c r="BS20" s="5"/>
-    </row>
-    <row r="21" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
+        <f>MIN(E21:ZW21)</f>
+        <v>376.7</v>
+      </c>
+      <c r="B21" s="12">
+        <f>MAX(E21:ZW21)</f>
+        <v>547.5</v>
+      </c>
+      <c r="C21" s="12">
         <f t="shared" si="0"/>
-        <v>376.7</v>
-      </c>
-      <c r="B21" s="12">
-        <f t="shared" si="1"/>
-        <v>547.5</v>
-      </c>
-      <c r="C21" s="12">
-        <f t="shared" si="2"/>
         <v>170.8</v>
       </c>
       <c r="D21" s="44" t="s">
@@ -11636,24 +11655,25 @@
         <v>532.9</v>
       </c>
       <c r="BP21" s="5">
-        <v>496.3</v>
-      </c>
-      <c r="BQ21" s="5"/>
+        <v>497.85</v>
+      </c>
+      <c r="BQ21" s="5">
+        <v>506.7</v>
+      </c>
       <c r="BR21" s="5"/>
-      <c r="BS21" s="5"/>
-    </row>
-    <row r="22" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
+        <f>MIN(E22:ZW22)</f>
+        <v>315.2</v>
+      </c>
+      <c r="B22" s="12">
+        <f>MAX(E22:ZW22)</f>
+        <v>379.5</v>
+      </c>
+      <c r="C22" s="12">
         <f t="shared" si="0"/>
-        <v>315.2</v>
-      </c>
-      <c r="B22" s="12">
-        <f t="shared" si="1"/>
-        <v>373</v>
-      </c>
-      <c r="C22" s="12">
-        <f t="shared" si="2"/>
-        <v>57.800000000000011</v>
+        <v>64.300000000000011</v>
       </c>
       <c r="D22" s="44" t="s">
         <v>269</v>
@@ -11792,23 +11812,24 @@
         <v>372.25</v>
       </c>
       <c r="BP22" s="5">
-        <v>369</v>
-      </c>
-      <c r="BQ22" s="5"/>
+        <v>365.35</v>
+      </c>
+      <c r="BQ22" s="5">
+        <v>379.5</v>
+      </c>
       <c r="BR22" s="5"/>
-      <c r="BS22" s="5"/>
-    </row>
-    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
+        <f>MIN(E23:ZW23)</f>
+        <v>54.45</v>
+      </c>
+      <c r="B23" s="12">
+        <f>MAX(E23:ZW23)</f>
+        <v>85.65</v>
+      </c>
+      <c r="C23" s="12">
         <f t="shared" si="0"/>
-        <v>54.45</v>
-      </c>
-      <c r="B23" s="12">
-        <f t="shared" si="1"/>
-        <v>85.65</v>
-      </c>
-      <c r="C23" s="12">
-        <f t="shared" si="2"/>
         <v>31.200000000000003</v>
       </c>
       <c r="D23" s="45" t="s">
@@ -11994,23 +12015,24 @@
         <v>61.3</v>
       </c>
       <c r="BP23" s="5">
-        <v>59.1</v>
-      </c>
-      <c r="BQ23" s="5"/>
+        <v>60.95</v>
+      </c>
+      <c r="BQ23" s="5">
+        <v>61.5</v>
+      </c>
       <c r="BR23" s="5"/>
-      <c r="BS23" s="5"/>
-    </row>
-    <row r="24" spans="1:71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
+        <f>MIN(E24:ZW24)</f>
+        <v>210.65</v>
+      </c>
+      <c r="B24" s="12">
+        <f>MAX(E24:ZW24)</f>
+        <v>257.39999999999998</v>
+      </c>
+      <c r="C24" s="12">
         <f t="shared" si="0"/>
-        <v>210.65</v>
-      </c>
-      <c r="B24" s="12">
-        <f t="shared" si="1"/>
-        <v>257.39999999999998</v>
-      </c>
-      <c r="C24" s="12">
-        <f t="shared" si="2"/>
         <v>46.749999999999972</v>
       </c>
       <c r="D24" s="45" t="s">
@@ -12192,24 +12214,25 @@
         <v>257.39999999999998</v>
       </c>
       <c r="BP24" s="5">
-        <v>245.7</v>
-      </c>
-      <c r="BQ24" s="5"/>
+        <v>245.25</v>
+      </c>
+      <c r="BQ24" s="5">
+        <v>246.3</v>
+      </c>
       <c r="BR24" s="5"/>
-      <c r="BS24" s="5"/>
-    </row>
-    <row r="25" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
+        <f>MIN(E25:ZW25)</f>
+        <v>876</v>
+      </c>
+      <c r="B25" s="12">
+        <f>MAX(E25:ZW25)</f>
+        <v>956.2</v>
+      </c>
+      <c r="C25" s="12">
         <f t="shared" si="0"/>
-        <v>876</v>
-      </c>
-      <c r="B25" s="12">
-        <f t="shared" si="1"/>
-        <v>951.95</v>
-      </c>
-      <c r="C25" s="12">
-        <f t="shared" si="2"/>
-        <v>75.950000000000045</v>
+        <v>80.200000000000045</v>
       </c>
       <c r="D25" s="46" t="s">
         <v>236</v>
@@ -12372,23 +12395,24 @@
         <v>928.8</v>
       </c>
       <c r="BP25" s="5">
-        <v>951.95</v>
-      </c>
-      <c r="BQ25" s="5"/>
+        <v>955.75</v>
+      </c>
+      <c r="BQ25" s="5">
+        <v>956.2</v>
+      </c>
       <c r="BR25" s="5"/>
-      <c r="BS25" s="5"/>
-    </row>
-    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
+        <f>MIN(E26:ZW26)</f>
+        <v>83.1</v>
+      </c>
+      <c r="B26" s="12">
+        <f>MAX(E26:ZW26)</f>
+        <v>96</v>
+      </c>
+      <c r="C26" s="12">
         <f t="shared" si="0"/>
-        <v>83.1</v>
-      </c>
-      <c r="B26" s="12">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="C26" s="12">
-        <f t="shared" si="2"/>
         <v>12.900000000000006</v>
       </c>
       <c r="D26" s="45" t="s">
@@ -12540,23 +12564,24 @@
         <v>91.3</v>
       </c>
       <c r="BP26" s="5">
-        <v>93</v>
-      </c>
-      <c r="BQ26" s="5"/>
+        <v>93.5</v>
+      </c>
+      <c r="BQ26" s="5">
+        <v>95.85</v>
+      </c>
       <c r="BR26" s="5"/>
-      <c r="BS26" s="5"/>
-    </row>
-    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
+        <f>MIN(E27:ZW27)</f>
+        <v>37.6</v>
+      </c>
+      <c r="B27" s="12">
+        <f>MAX(E27:ZW27)</f>
+        <v>44.75</v>
+      </c>
+      <c r="C27" s="12">
         <f t="shared" si="0"/>
-        <v>37.6</v>
-      </c>
-      <c r="B27" s="12">
-        <f t="shared" si="1"/>
-        <v>44.75</v>
-      </c>
-      <c r="C27" s="12">
-        <f t="shared" si="2"/>
         <v>7.1499999999999986</v>
       </c>
       <c r="D27" s="45" t="s">
@@ -12708,23 +12733,24 @@
         <v>39.700000000000003</v>
       </c>
       <c r="BP27" s="5">
-        <v>39</v>
-      </c>
-      <c r="BQ27" s="5"/>
+        <v>38.700000000000003</v>
+      </c>
+      <c r="BQ27" s="5">
+        <v>38.25</v>
+      </c>
       <c r="BR27" s="5"/>
-      <c r="BS27" s="5"/>
-    </row>
-    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
+        <f>MIN(E28:ZW28)</f>
+        <v>111.95</v>
+      </c>
+      <c r="B28" s="12">
+        <f>MAX(E28:ZW28)</f>
+        <v>141.65</v>
+      </c>
+      <c r="C28" s="12">
         <f t="shared" si="0"/>
-        <v>111.95</v>
-      </c>
-      <c r="B28" s="12">
-        <f t="shared" si="1"/>
-        <v>141.65</v>
-      </c>
-      <c r="C28" s="12">
-        <f t="shared" si="2"/>
         <v>29.700000000000003</v>
       </c>
       <c r="D28" s="45" t="s">
@@ -12876,23 +12902,24 @@
         <v>138.80000000000001</v>
       </c>
       <c r="BP28" s="5">
-        <v>135.19999999999999</v>
-      </c>
-      <c r="BQ28" s="5"/>
+        <v>134.1</v>
+      </c>
+      <c r="BQ28" s="5">
+        <v>131.44999999999999</v>
+      </c>
       <c r="BR28" s="5"/>
-      <c r="BS28" s="5"/>
-    </row>
-    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
+        <f>MIN(E29:ZW29)</f>
+        <v>62.3</v>
+      </c>
+      <c r="B29" s="12">
+        <f>MAX(E29:ZW29)</f>
+        <v>78.849999999999994</v>
+      </c>
+      <c r="C29" s="12">
         <f t="shared" si="0"/>
-        <v>62.3</v>
-      </c>
-      <c r="B29" s="12">
-        <f t="shared" si="1"/>
-        <v>78.849999999999994</v>
-      </c>
-      <c r="C29" s="12">
-        <f t="shared" si="2"/>
         <v>16.549999999999997</v>
       </c>
       <c r="D29" s="45" t="s">
@@ -13044,23 +13071,24 @@
         <v>71</v>
       </c>
       <c r="BP29" s="5">
-        <v>68</v>
-      </c>
-      <c r="BQ29" s="5"/>
+        <v>69.400000000000006</v>
+      </c>
+      <c r="BQ29" s="5">
+        <v>69.650000000000006</v>
+      </c>
       <c r="BR29" s="5"/>
-      <c r="BS29" s="5"/>
-    </row>
-    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
+        <f>MIN(E30:ZW30)</f>
+        <v>39.25</v>
+      </c>
+      <c r="B30" s="12">
+        <f>MAX(E30:ZW30)</f>
+        <v>50.95</v>
+      </c>
+      <c r="C30" s="12">
         <f t="shared" si="0"/>
-        <v>39.25</v>
-      </c>
-      <c r="B30" s="12">
-        <f t="shared" si="1"/>
-        <v>50.95</v>
-      </c>
-      <c r="C30" s="12">
-        <f t="shared" si="2"/>
         <v>11.700000000000003</v>
       </c>
       <c r="D30" s="45" t="s">
@@ -13212,24 +13240,25 @@
         <v>50.95</v>
       </c>
       <c r="BP30" s="5">
-        <v>47.25</v>
-      </c>
-      <c r="BQ30" s="5"/>
+        <v>47.6</v>
+      </c>
+      <c r="BQ30" s="5">
+        <v>48.2</v>
+      </c>
       <c r="BR30" s="5"/>
-      <c r="BS30" s="5"/>
-    </row>
-    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
+        <f>MIN(E31:ZW31)</f>
+        <v>136.5</v>
+      </c>
+      <c r="B31" s="12">
+        <f>MAX(E31:ZW31)</f>
+        <v>156.85</v>
+      </c>
+      <c r="C31" s="12">
         <f t="shared" si="0"/>
-        <v>138.19999999999999</v>
-      </c>
-      <c r="B31" s="12">
-        <f t="shared" si="1"/>
-        <v>156.85</v>
-      </c>
-      <c r="C31" s="12">
-        <f t="shared" si="2"/>
-        <v>18.650000000000006</v>
+        <v>20.349999999999994</v>
       </c>
       <c r="D31" s="45" t="s">
         <v>257</v>
@@ -13380,23 +13409,24 @@
         <v>143.19999999999999</v>
       </c>
       <c r="BP31" s="5">
-        <v>138.19999999999999</v>
-      </c>
-      <c r="BQ31" s="5"/>
+        <v>136.5</v>
+      </c>
+      <c r="BQ31" s="5">
+        <v>138.9</v>
+      </c>
       <c r="BR31" s="5"/>
-      <c r="BS31" s="5"/>
-    </row>
-    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
+        <f>MIN(E32:ZW32)</f>
+        <v>101.6</v>
+      </c>
+      <c r="B32" s="12">
+        <f>MAX(E32:ZW32)</f>
+        <v>121.8</v>
+      </c>
+      <c r="C32" s="12">
         <f t="shared" si="0"/>
-        <v>101.6</v>
-      </c>
-      <c r="B32" s="12">
-        <f t="shared" si="1"/>
-        <v>121.8</v>
-      </c>
-      <c r="C32" s="12">
-        <f t="shared" si="2"/>
         <v>20.200000000000003</v>
       </c>
       <c r="D32" s="45" t="s">
@@ -13536,23 +13566,24 @@
         <v>117</v>
       </c>
       <c r="BP32" s="5">
-        <v>106.35</v>
-      </c>
-      <c r="BQ32" s="5"/>
+        <v>104.9</v>
+      </c>
+      <c r="BQ32" s="5">
+        <v>106.15</v>
+      </c>
       <c r="BR32" s="5"/>
-      <c r="BS32" s="5"/>
-    </row>
-    <row r="33" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
+        <f>MIN(E33:ZW33)</f>
+        <v>56.75</v>
+      </c>
+      <c r="B33" s="12">
+        <f>MAX(E33:ZW33)</f>
+        <v>67.099999999999994</v>
+      </c>
+      <c r="C33" s="12">
         <f t="shared" si="0"/>
-        <v>56.75</v>
-      </c>
-      <c r="B33" s="12">
-        <f t="shared" si="1"/>
-        <v>67.099999999999994</v>
-      </c>
-      <c r="C33" s="12">
-        <f t="shared" si="2"/>
         <v>10.349999999999994</v>
       </c>
       <c r="D33" s="45" t="s">
@@ -13680,23 +13711,24 @@
         <v>60.1</v>
       </c>
       <c r="BP33" s="5">
-        <v>61</v>
-      </c>
-      <c r="BQ33" s="5"/>
+        <v>60.35</v>
+      </c>
+      <c r="BQ33" s="5">
+        <v>60.25</v>
+      </c>
       <c r="BR33" s="5"/>
-      <c r="BS33" s="5"/>
-    </row>
-    <row r="34" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E34:ZW34)</f>
         <v>167.9</v>
       </c>
       <c r="B34" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E34:ZW34)</f>
         <v>236.1</v>
       </c>
       <c r="C34" s="12">
-        <f t="shared" ref="C34" si="3">B34-A34</f>
+        <f t="shared" ref="C34" si="1">B34-A34</f>
         <v>68.199999999999989</v>
       </c>
       <c r="D34" s="45" t="s">
@@ -13818,23 +13850,24 @@
         <v>203.8</v>
       </c>
       <c r="BP34" s="5">
-        <v>196.95</v>
-      </c>
-      <c r="BQ34" s="5"/>
+        <v>204.55</v>
+      </c>
+      <c r="BQ34" s="5">
+        <v>206.05</v>
+      </c>
       <c r="BR34" s="5"/>
-      <c r="BS34" s="5"/>
-    </row>
-    <row r="35" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E35:ZW35)</f>
         <v>661</v>
       </c>
       <c r="B35" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E35:ZW35)</f>
         <v>714.65</v>
       </c>
       <c r="C35" s="12">
-        <f t="shared" ref="C35" si="4">B35-A35</f>
+        <f t="shared" ref="C35" si="2">B35-A35</f>
         <v>53.649999999999977</v>
       </c>
       <c r="D35" s="45" t="s">
@@ -13952,23 +13985,24 @@
         <v>680.5</v>
       </c>
       <c r="BP35" s="5">
-        <v>681</v>
-      </c>
-      <c r="BQ35" s="5"/>
+        <v>675.7</v>
+      </c>
+      <c r="BQ35" s="5">
+        <v>679</v>
+      </c>
       <c r="BR35" s="5"/>
-      <c r="BS35" s="5"/>
-    </row>
-    <row r="36" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E36:ZW36)</f>
         <v>402.9</v>
       </c>
       <c r="B36" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E36:ZW36)</f>
         <v>520</v>
       </c>
       <c r="C36" s="12">
-        <f t="shared" ref="C36" si="5">B36-A36</f>
+        <f t="shared" ref="C36" si="3">B36-A36</f>
         <v>117.10000000000002</v>
       </c>
       <c r="D36" s="45" t="s">
@@ -14068,24 +14102,25 @@
         <v>470.4</v>
       </c>
       <c r="BP36" s="5">
-        <v>477</v>
-      </c>
-      <c r="BQ36" s="5"/>
+        <v>487.5</v>
+      </c>
+      <c r="BQ36" s="5">
+        <v>491.7</v>
+      </c>
       <c r="BR36" s="5"/>
-      <c r="BS36" s="5"/>
-    </row>
-    <row r="37" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E37:ZW37)</f>
         <v>226</v>
       </c>
       <c r="B37" s="12">
-        <f t="shared" si="1"/>
-        <v>349</v>
+        <f>MAX(E37:ZW37)</f>
+        <v>374.25</v>
       </c>
       <c r="C37" s="12">
-        <f t="shared" ref="C37" si="6">B37-A37</f>
-        <v>123</v>
+        <f t="shared" ref="C37" si="4">B37-A37</f>
+        <v>148.25</v>
       </c>
       <c r="D37" s="45" t="s">
         <v>297</v>
@@ -14174,24 +14209,25 @@
         <v>332</v>
       </c>
       <c r="BP37" s="5">
-        <v>349</v>
-      </c>
-      <c r="BQ37" s="5"/>
+        <v>361</v>
+      </c>
+      <c r="BQ37" s="5">
+        <v>374.25</v>
+      </c>
       <c r="BR37" s="5"/>
-      <c r="BS37" s="5"/>
-    </row>
-    <row r="38" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E38:ZW38)</f>
         <v>485</v>
       </c>
       <c r="B38" s="12">
-        <f t="shared" si="1"/>
-        <v>515</v>
+        <f>MAX(E38:ZW38)</f>
+        <v>515.4</v>
       </c>
       <c r="C38" s="12">
-        <f t="shared" ref="C38" si="7">B38-A38</f>
-        <v>30</v>
+        <f t="shared" ref="C38" si="5">B38-A38</f>
+        <v>30.399999999999977</v>
       </c>
       <c r="D38" s="45" t="s">
         <v>298</v>
@@ -14278,24 +14314,25 @@
         <v>500.1</v>
       </c>
       <c r="BP38" s="5">
-        <v>503.15</v>
-      </c>
-      <c r="BQ38" s="5"/>
+        <v>508.6</v>
+      </c>
+      <c r="BQ38" s="5">
+        <v>515.4</v>
+      </c>
       <c r="BR38" s="5"/>
-      <c r="BS38" s="5"/>
-    </row>
-    <row r="39" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
-        <f t="shared" si="0"/>
-        <v>75.599999999999994</v>
+        <f>MIN(E39:ZW39)</f>
+        <v>75.2</v>
       </c>
       <c r="B39" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E39:ZW39)</f>
         <v>78.5</v>
       </c>
       <c r="C39" s="12">
-        <f t="shared" ref="C39" si="8">B39-A39</f>
-        <v>2.9000000000000057</v>
+        <f t="shared" ref="C39" si="6">B39-A39</f>
+        <v>3.2999999999999972</v>
       </c>
       <c r="D39" s="45" t="s">
         <v>305</v>
@@ -14376,24 +14413,25 @@
         <v>78.5</v>
       </c>
       <c r="BP39" s="5">
-        <v>75.599999999999994</v>
-      </c>
-      <c r="BQ39" s="5"/>
+        <v>75.2</v>
+      </c>
+      <c r="BQ39" s="5">
+        <v>75.900000000000006</v>
+      </c>
       <c r="BR39" s="5"/>
-      <c r="BS39" s="5"/>
-    </row>
-    <row r="40" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
-        <f t="shared" si="0"/>
-        <v>461</v>
+        <f>MIN(E40:ZW40)</f>
+        <v>444.05</v>
       </c>
       <c r="B40" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E40:ZW40)</f>
         <v>472</v>
       </c>
       <c r="C40" s="12">
-        <f t="shared" ref="C40" si="9">B40-A40</f>
-        <v>11</v>
+        <f t="shared" ref="C40" si="7">B40-A40</f>
+        <v>27.949999999999989</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>306</v>
@@ -14474,24 +14512,25 @@
         <v>467</v>
       </c>
       <c r="BP40" s="5">
-        <v>461</v>
-      </c>
-      <c r="BQ40" s="5"/>
+        <v>450.55</v>
+      </c>
+      <c r="BQ40" s="5">
+        <v>444.05</v>
+      </c>
       <c r="BR40" s="5"/>
-      <c r="BS40" s="5"/>
-    </row>
-    <row r="41" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
-        <f t="shared" si="0"/>
-        <v>197.05</v>
+        <f>MIN(E41:ZW41)</f>
+        <v>192.65</v>
       </c>
       <c r="B41" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E41:ZW41)</f>
         <v>209.8</v>
       </c>
       <c r="C41" s="12">
-        <f t="shared" ref="C41" si="10">B41-A41</f>
-        <v>12.75</v>
+        <f t="shared" ref="C41" si="8">B41-A41</f>
+        <v>17.150000000000006</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>307</v>
@@ -14568,24 +14607,25 @@
         <v>201.7</v>
       </c>
       <c r="BP41" s="5">
-        <v>197.05</v>
-      </c>
-      <c r="BQ41" s="5"/>
+        <v>192.65</v>
+      </c>
+      <c r="BQ41" s="5">
+        <v>196.9</v>
+      </c>
       <c r="BR41" s="5"/>
-      <c r="BS41" s="5"/>
-    </row>
-    <row r="42" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
-        <f t="shared" ref="A42:A43" si="11">MIN(E42:ZX42)</f>
+        <f>MIN(E42:ZW42)</f>
         <v>63.5</v>
       </c>
       <c r="B42" s="12">
-        <f t="shared" ref="B42:B43" si="12">MAX(E42:ZX42)</f>
-        <v>63.7</v>
+        <f>MAX(E42:ZW42)</f>
+        <v>65.75</v>
       </c>
       <c r="C42" s="12">
-        <f t="shared" ref="C42:C43" si="13">B42-A42</f>
-        <v>0.20000000000000284</v>
+        <f t="shared" ref="C42:C43" si="9">B42-A42</f>
+        <v>2.25</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>308</v>
@@ -14658,24 +14698,25 @@
         <v>63.7</v>
       </c>
       <c r="BP42" s="5">
-        <v>63.7</v>
-      </c>
-      <c r="BQ42" s="5"/>
+        <v>64.8</v>
+      </c>
+      <c r="BQ42" s="5">
+        <v>65.75</v>
+      </c>
       <c r="BR42" s="5"/>
-      <c r="BS42" s="5"/>
-    </row>
-    <row r="43" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
-        <f t="shared" si="11"/>
-        <v>57.15</v>
+        <f>MIN(E43:ZW43)</f>
+        <v>57.3</v>
       </c>
       <c r="B43" s="12">
-        <f t="shared" si="12"/>
+        <f>MAX(E43:ZW43)</f>
         <v>60.75</v>
       </c>
       <c r="C43" s="12">
-        <f t="shared" si="13"/>
-        <v>3.6000000000000014</v>
+        <f t="shared" si="9"/>
+        <v>3.4500000000000028</v>
       </c>
       <c r="D43" s="45" t="s">
         <v>309</v>
@@ -14748,24 +14789,25 @@
         <v>60.75</v>
       </c>
       <c r="BP43" s="5">
-        <v>57.15</v>
-      </c>
-      <c r="BQ43" s="5"/>
+        <v>57.3</v>
+      </c>
+      <c r="BQ43" s="5">
+        <v>58.3</v>
+      </c>
       <c r="BR43" s="5"/>
-      <c r="BS43" s="5"/>
-    </row>
-    <row r="44" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
-        <f t="shared" ref="A44" si="14">MIN(E44:ZX44)</f>
+        <f>MIN(E44:ZW44)</f>
         <v>36.950000000000003</v>
       </c>
       <c r="B44" s="12">
-        <f t="shared" ref="B44" si="15">MAX(E44:ZX44)</f>
-        <v>38.9</v>
+        <f>MAX(E44:ZW44)</f>
+        <v>38.65</v>
       </c>
       <c r="C44" s="12">
-        <f t="shared" ref="C44" si="16">B44-A44</f>
-        <v>1.9499999999999957</v>
+        <f t="shared" ref="C44:C47" si="10">B44-A44</f>
+        <v>1.6999999999999957</v>
       </c>
       <c r="D44" s="45" t="s">
         <v>310</v>
@@ -14838,24 +14880,25 @@
         <v>36.950000000000003</v>
       </c>
       <c r="BP44" s="5">
-        <v>38.9</v>
-      </c>
-      <c r="BQ44" s="5"/>
+        <v>38.65</v>
+      </c>
+      <c r="BQ44" s="5">
+        <v>38.35</v>
+      </c>
       <c r="BR44" s="5"/>
-      <c r="BS44" s="5"/>
-    </row>
-    <row r="45" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
-        <f t="shared" ref="A45:A46" si="17">MIN(E45:ZX45)</f>
-        <v>583.75</v>
+        <f>MIN(E45:ZW45)</f>
+        <v>577.45000000000005</v>
       </c>
       <c r="B45" s="12">
-        <f t="shared" ref="B45:B46" si="18">MAX(E45:ZX45)</f>
-        <v>583.75</v>
+        <f t="shared" ref="B45:B46" si="11">MAX(E45:ZW45)</f>
+        <v>597.20000000000005</v>
       </c>
       <c r="C45" s="12">
-        <f t="shared" ref="C45:C46" si="19">B45-A45</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>19.75</v>
       </c>
       <c r="D45" s="45" t="s">
         <v>311</v>
@@ -14922,26 +14965,29 @@
       <c r="BL45" s="5"/>
       <c r="BM45" s="5"/>
       <c r="BN45" s="5"/>
-      <c r="BO45" s="5"/>
+      <c r="BO45" s="5">
+        <v>585</v>
+      </c>
       <c r="BP45" s="5">
-        <v>583.75</v>
-      </c>
-      <c r="BQ45" s="5"/>
+        <v>577.45000000000005</v>
+      </c>
+      <c r="BQ45" s="5">
+        <v>597.20000000000005</v>
+      </c>
       <c r="BR45" s="5"/>
-      <c r="BS45" s="5"/>
-    </row>
-    <row r="46" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
-        <f t="shared" si="17"/>
-        <v>839.5</v>
+        <f>MIN(E46:ZW46)</f>
+        <v>830.25</v>
       </c>
       <c r="B46" s="12">
-        <f t="shared" si="18"/>
-        <v>839.5</v>
+        <f t="shared" si="11"/>
+        <v>856</v>
       </c>
       <c r="C46" s="12">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>25.75</v>
       </c>
       <c r="D46" s="45" t="s">
         <v>312</v>
@@ -15008,13 +15054,103 @@
       <c r="BL46" s="5"/>
       <c r="BM46" s="5"/>
       <c r="BN46" s="5"/>
-      <c r="BO46" s="5"/>
+      <c r="BO46" s="5">
+        <v>856</v>
+      </c>
       <c r="BP46" s="5">
-        <v>839.5</v>
-      </c>
-      <c r="BQ46" s="5"/>
+        <v>832.8</v>
+      </c>
+      <c r="BQ46" s="5">
+        <v>830.25</v>
+      </c>
       <c r="BR46" s="5"/>
-      <c r="BS46" s="5"/>
+    </row>
+    <row r="47" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A47" s="12">
+        <f>MIN(E47:ZW47)</f>
+        <v>141.80000000000001</v>
+      </c>
+      <c r="B47" s="12">
+        <f>MAX(E47:ZW47)</f>
+        <v>146</v>
+      </c>
+      <c r="C47" s="12">
+        <f t="shared" si="10"/>
+        <v>4.1999999999999886</v>
+      </c>
+      <c r="D47" s="45" t="s">
+        <v>313</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="5"/>
+      <c r="V47" s="5"/>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5"/>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5"/>
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="5"/>
+      <c r="AC47" s="5"/>
+      <c r="AD47" s="5"/>
+      <c r="AE47" s="5"/>
+      <c r="AF47" s="5"/>
+      <c r="AG47" s="5"/>
+      <c r="AH47" s="5"/>
+      <c r="AI47" s="5"/>
+      <c r="AJ47" s="5"/>
+      <c r="AK47" s="5"/>
+      <c r="AL47" s="5"/>
+      <c r="AM47" s="5"/>
+      <c r="AN47" s="5"/>
+      <c r="AO47" s="5"/>
+      <c r="AP47" s="5"/>
+      <c r="AQ47" s="5"/>
+      <c r="AR47" s="5"/>
+      <c r="AS47" s="5"/>
+      <c r="AT47" s="5"/>
+      <c r="AU47" s="5"/>
+      <c r="AV47" s="5"/>
+      <c r="AW47" s="5"/>
+      <c r="AX47" s="5"/>
+      <c r="AY47" s="5"/>
+      <c r="AZ47" s="5"/>
+      <c r="BA47" s="5"/>
+      <c r="BB47" s="5"/>
+      <c r="BC47" s="5"/>
+      <c r="BD47" s="5"/>
+      <c r="BE47" s="5"/>
+      <c r="BF47" s="5"/>
+      <c r="BG47" s="5"/>
+      <c r="BH47" s="5"/>
+      <c r="BI47" s="5"/>
+      <c r="BJ47" s="5"/>
+      <c r="BK47" s="5"/>
+      <c r="BL47" s="5"/>
+      <c r="BM47" s="5"/>
+      <c r="BN47" s="5"/>
+      <c r="BO47" s="5"/>
+      <c r="BP47" s="5">
+        <v>146</v>
+      </c>
+      <c r="BQ47" s="5">
+        <v>141.80000000000001</v>
+      </c>
+      <c r="BR47" s="5"/>
     </row>
   </sheetData>
   <sortState ref="L1:L37">

</xml_diff>

<commit_message>
Added details for 10/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -7214,9 +7214,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="BO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CM34" sqref="CM34"/>
+      <selection pane="topRight" activeCell="BR48" sqref="BR48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7472,16 +7472,16 @@
     </row>
     <row r="2" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
-        <f>MIN(E2:ZW2)</f>
+        <f t="shared" ref="A2:A47" si="0">MIN(E2:ZW2)</f>
         <v>243.6</v>
       </c>
       <c r="B2" s="12">
-        <f>MAX(E2:ZW2)</f>
-        <v>328</v>
+        <f t="shared" ref="B2:B44" si="1">MAX(E2:ZW2)</f>
+        <v>333.8</v>
       </c>
       <c r="C2" s="12">
         <f>B2-A2</f>
-        <v>84.4</v>
+        <v>90.200000000000017</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>115</v>
@@ -7673,20 +7673,22 @@
       <c r="BQ2" s="5">
         <v>314.8</v>
       </c>
-      <c r="BR2" s="5"/>
+      <c r="BR2" s="5">
+        <v>333.8</v>
+      </c>
     </row>
     <row r="3" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
-        <f>MIN(E3:ZW3)</f>
+        <f t="shared" si="0"/>
         <v>262.7</v>
       </c>
       <c r="B3" s="12">
-        <f>MAX(E3:ZW3)</f>
-        <v>316.14999999999998</v>
+        <f t="shared" si="1"/>
+        <v>318.3</v>
       </c>
       <c r="C3" s="12">
-        <f t="shared" ref="C3:C33" si="0">B3-A3</f>
-        <v>53.449999999999989</v>
+        <f t="shared" ref="C3:C33" si="2">B3-A3</f>
+        <v>55.600000000000023</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>114</v>
@@ -7878,19 +7880,21 @@
       <c r="BQ3" s="5">
         <v>312</v>
       </c>
-      <c r="BR3" s="5"/>
+      <c r="BR3" s="5">
+        <v>318.3</v>
+      </c>
     </row>
     <row r="4" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
-        <f>MIN(E4:ZW4)</f>
+        <f t="shared" si="0"/>
         <v>259.45</v>
       </c>
       <c r="B4" s="12">
-        <f>MAX(E4:ZW4)</f>
+        <f t="shared" si="1"/>
         <v>291.7</v>
       </c>
       <c r="C4" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>32.25</v>
       </c>
       <c r="D4" s="44" t="s">
@@ -8089,19 +8093,21 @@
       <c r="BQ4" s="5">
         <v>260.35000000000002</v>
       </c>
-      <c r="BR4" s="5"/>
+      <c r="BR4" s="5">
+        <v>262.2</v>
+      </c>
     </row>
     <row r="5" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
-        <f>MIN(E5:ZW5)</f>
+        <f t="shared" si="0"/>
         <v>786.25</v>
       </c>
       <c r="B5" s="12">
-        <f>MAX(E5:ZW5)</f>
+        <f t="shared" si="1"/>
         <v>946.8</v>
       </c>
       <c r="C5" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>160.54999999999995</v>
       </c>
       <c r="D5" s="44" t="s">
@@ -8300,19 +8306,21 @@
       <c r="BQ5" s="5">
         <v>902.4</v>
       </c>
-      <c r="BR5" s="5"/>
+      <c r="BR5" s="5">
+        <v>884.9</v>
+      </c>
     </row>
     <row r="6" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
-        <f>MIN(E6:ZW6)</f>
+        <f t="shared" si="0"/>
         <v>236.45</v>
       </c>
       <c r="B6" s="12">
-        <f>MAX(E6:ZW6)</f>
+        <f t="shared" si="1"/>
         <v>293.95</v>
       </c>
       <c r="C6" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>57.5</v>
       </c>
       <c r="D6" s="45" t="s">
@@ -8511,19 +8519,21 @@
       <c r="BQ6" s="5">
         <v>283.25</v>
       </c>
-      <c r="BR6" s="5"/>
+      <c r="BR6" s="5">
+        <v>285.7</v>
+      </c>
     </row>
     <row r="7" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
-        <f>MIN(E7:ZW7)</f>
+        <f t="shared" si="0"/>
         <v>15.6</v>
       </c>
       <c r="B7" s="12">
-        <f>MAX(E7:ZW7)</f>
+        <f t="shared" si="1"/>
         <v>19.350000000000001</v>
       </c>
       <c r="C7" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.7500000000000018</v>
       </c>
       <c r="D7" s="45" t="s">
@@ -8722,19 +8732,21 @@
       <c r="BQ7" s="5">
         <v>17.8</v>
       </c>
-      <c r="BR7" s="5"/>
+      <c r="BR7" s="5">
+        <v>17.7</v>
+      </c>
     </row>
     <row r="8" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
-        <f>MIN(E8:ZW8)</f>
+        <f t="shared" si="0"/>
         <v>53.4</v>
       </c>
       <c r="B8" s="12">
-        <f>MAX(E8:ZW8)</f>
+        <f t="shared" si="1"/>
         <v>86.75</v>
       </c>
       <c r="C8" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>33.35</v>
       </c>
       <c r="D8" s="45" t="s">
@@ -8933,19 +8945,21 @@
       <c r="BQ8" s="5">
         <v>78.75</v>
       </c>
-      <c r="BR8" s="5"/>
+      <c r="BR8" s="5">
+        <v>81.55</v>
+      </c>
     </row>
     <row r="9" spans="1:70" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
-        <f>MIN(E9:ZW9)</f>
+        <f t="shared" si="0"/>
         <v>53.5</v>
       </c>
       <c r="B9" s="39">
-        <f>MAX(E9:ZW9)</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="C9" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
       <c r="D9" s="43" t="s">
@@ -9136,19 +9150,21 @@
       <c r="BQ9" s="28">
         <v>56.35</v>
       </c>
-      <c r="BR9" s="28"/>
+      <c r="BR9" s="28">
+        <v>55.9</v>
+      </c>
     </row>
     <row r="10" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
-        <f>MIN(E10:ZW10)</f>
+        <f t="shared" si="0"/>
         <v>38.6</v>
       </c>
       <c r="B10" s="12">
-        <f>MAX(E10:ZW10)</f>
+        <f t="shared" si="1"/>
         <v>45.35</v>
       </c>
       <c r="C10" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.75</v>
       </c>
       <c r="D10" s="45" t="s">
@@ -9347,19 +9363,21 @@
       <c r="BQ10" s="5">
         <v>39.299999999999997</v>
       </c>
-      <c r="BR10" s="5"/>
+      <c r="BR10" s="5">
+        <v>39.5</v>
+      </c>
     </row>
     <row r="11" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
-        <f>MIN(E11:ZW11)</f>
+        <f t="shared" si="0"/>
         <v>72.650000000000006</v>
       </c>
       <c r="B11" s="12">
-        <f>MAX(E11:ZW11)</f>
+        <f t="shared" si="1"/>
         <v>106.5</v>
       </c>
       <c r="C11" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>33.849999999999994</v>
       </c>
       <c r="D11" s="45" t="s">
@@ -9558,19 +9576,21 @@
       <c r="BQ11" s="5">
         <v>96.2</v>
       </c>
-      <c r="BR11" s="5"/>
+      <c r="BR11" s="5">
+        <v>96.65</v>
+      </c>
     </row>
     <row r="12" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
-        <f>MIN(E12:ZW12)</f>
+        <f t="shared" si="0"/>
         <v>82.65</v>
       </c>
       <c r="B12" s="12">
-        <f>MAX(E12:ZW12)</f>
+        <f t="shared" si="1"/>
         <v>99.6</v>
       </c>
       <c r="C12" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16.949999999999989</v>
       </c>
       <c r="D12" s="45" t="s">
@@ -9769,19 +9789,21 @@
       <c r="BQ12" s="5">
         <v>92.2</v>
       </c>
-      <c r="BR12" s="5"/>
+      <c r="BR12" s="5">
+        <v>92.05</v>
+      </c>
     </row>
     <row r="13" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
-        <f>MIN(E13:ZW13)</f>
+        <f t="shared" si="0"/>
         <v>44.1</v>
       </c>
       <c r="B13" s="12">
-        <f>MAX(E13:ZW13)</f>
+        <f t="shared" si="1"/>
         <v>57.15</v>
       </c>
       <c r="C13" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13.049999999999997</v>
       </c>
       <c r="D13" s="45" t="s">
@@ -9980,19 +10002,21 @@
       <c r="BQ13" s="5">
         <v>48.35</v>
       </c>
-      <c r="BR13" s="5"/>
+      <c r="BR13" s="5">
+        <v>48.75</v>
+      </c>
     </row>
     <row r="14" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
-        <f>MIN(E14:ZW14)</f>
+        <f t="shared" si="0"/>
         <v>29.75</v>
       </c>
       <c r="B14" s="12">
-        <f>MAX(E14:ZW14)</f>
+        <f t="shared" si="1"/>
         <v>41.85</v>
       </c>
       <c r="C14" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12.100000000000001</v>
       </c>
       <c r="D14" s="45" t="s">
@@ -10191,19 +10215,21 @@
       <c r="BQ14" s="5">
         <v>39.1</v>
       </c>
-      <c r="BR14" s="5"/>
+      <c r="BR14" s="5">
+        <v>38.75</v>
+      </c>
     </row>
     <row r="15" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
-        <f>MIN(E15:ZW15)</f>
+        <f t="shared" si="0"/>
         <v>25.25</v>
       </c>
       <c r="B15" s="12">
-        <f>MAX(E15:ZW15)</f>
+        <f t="shared" si="1"/>
         <v>36.4</v>
       </c>
       <c r="C15" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11.149999999999999</v>
       </c>
       <c r="D15" s="45" t="s">
@@ -10394,19 +10420,21 @@
       <c r="BQ15" s="5">
         <v>26.25</v>
       </c>
-      <c r="BR15" s="5"/>
+      <c r="BR15" s="5">
+        <v>25.8</v>
+      </c>
     </row>
     <row r="16" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
-        <f>MIN(E16:ZW16)</f>
+        <f t="shared" si="0"/>
         <v>552</v>
       </c>
       <c r="B16" s="12">
-        <f>MAX(E16:ZW16)</f>
+        <f t="shared" si="1"/>
         <v>729.5</v>
       </c>
       <c r="C16" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>177.5</v>
       </c>
       <c r="D16" s="45" t="s">
@@ -10605,19 +10633,21 @@
       <c r="BQ16" s="5">
         <v>704.9</v>
       </c>
-      <c r="BR16" s="5"/>
+      <c r="BR16" s="5">
+        <v>703.5</v>
+      </c>
     </row>
     <row r="17" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
-        <f>MIN(E17:ZW17)</f>
+        <f t="shared" si="0"/>
         <v>433</v>
       </c>
       <c r="B17" s="12">
-        <f>MAX(E17:ZW17)</f>
+        <f t="shared" si="1"/>
         <v>515</v>
       </c>
       <c r="C17" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>82</v>
       </c>
       <c r="D17" s="44" t="s">
@@ -10816,19 +10846,21 @@
       <c r="BQ17" s="5">
         <v>474.5</v>
       </c>
-      <c r="BR17" s="5"/>
+      <c r="BR17" s="5">
+        <v>477</v>
+      </c>
     </row>
     <row r="18" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
-        <f>MIN(E18:ZW18)</f>
+        <f t="shared" si="0"/>
         <v>178.8</v>
       </c>
       <c r="B18" s="12">
-        <f>MAX(E18:ZW18)</f>
+        <f t="shared" si="1"/>
         <v>302.2</v>
       </c>
       <c r="C18" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>123.39999999999998</v>
       </c>
       <c r="D18" s="44" t="s">
@@ -11027,20 +11059,22 @@
       <c r="BQ18" s="5">
         <v>294</v>
       </c>
-      <c r="BR18" s="5"/>
+      <c r="BR18" s="5">
+        <v>296</v>
+      </c>
     </row>
     <row r="19" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
-        <f>MIN(E19:ZW19)</f>
+        <f t="shared" si="0"/>
         <v>440.7</v>
       </c>
       <c r="B19" s="12">
-        <f>MAX(E19:ZW19)</f>
-        <v>588.75</v>
+        <f t="shared" si="1"/>
+        <v>592</v>
       </c>
       <c r="C19" s="12">
-        <f t="shared" si="0"/>
-        <v>148.05000000000001</v>
+        <f t="shared" si="2"/>
+        <v>151.30000000000001</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -11238,19 +11272,21 @@
       <c r="BQ19" s="5">
         <v>588.75</v>
       </c>
-      <c r="BR19" s="5"/>
+      <c r="BR19" s="5">
+        <v>592</v>
+      </c>
     </row>
     <row r="20" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
-        <f>MIN(E20:ZW20)</f>
+        <f t="shared" si="0"/>
         <v>677</v>
       </c>
       <c r="B20" s="12">
-        <f>MAX(E20:ZW20)</f>
+        <f t="shared" si="1"/>
         <v>795.95</v>
       </c>
       <c r="C20" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118.95000000000005</v>
       </c>
       <c r="D20" s="44" t="s">
@@ -11449,19 +11485,21 @@
       <c r="BQ20" s="5">
         <v>788.15</v>
       </c>
-      <c r="BR20" s="5"/>
+      <c r="BR20" s="5">
+        <v>743.1</v>
+      </c>
     </row>
     <row r="21" spans="1:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
-        <f>MIN(E21:ZW21)</f>
+        <f t="shared" si="0"/>
         <v>376.7</v>
       </c>
       <c r="B21" s="12">
-        <f>MAX(E21:ZW21)</f>
+        <f t="shared" si="1"/>
         <v>547.5</v>
       </c>
       <c r="C21" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>170.8</v>
       </c>
       <c r="D21" s="44" t="s">
@@ -11660,20 +11698,22 @@
       <c r="BQ21" s="5">
         <v>506.7</v>
       </c>
-      <c r="BR21" s="5"/>
+      <c r="BR21" s="5">
+        <v>503.4</v>
+      </c>
     </row>
     <row r="22" spans="1:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
-        <f>MIN(E22:ZW22)</f>
+        <f t="shared" si="0"/>
         <v>315.2</v>
       </c>
       <c r="B22" s="12">
-        <f>MAX(E22:ZW22)</f>
-        <v>379.5</v>
+        <f t="shared" si="1"/>
+        <v>383</v>
       </c>
       <c r="C22" s="12">
-        <f t="shared" si="0"/>
-        <v>64.300000000000011</v>
+        <f t="shared" si="2"/>
+        <v>67.800000000000011</v>
       </c>
       <c r="D22" s="44" t="s">
         <v>269</v>
@@ -11817,19 +11857,21 @@
       <c r="BQ22" s="5">
         <v>379.5</v>
       </c>
-      <c r="BR22" s="5"/>
+      <c r="BR22" s="5">
+        <v>383</v>
+      </c>
     </row>
     <row r="23" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
-        <f>MIN(E23:ZW23)</f>
+        <f t="shared" si="0"/>
         <v>54.45</v>
       </c>
       <c r="B23" s="12">
-        <f>MAX(E23:ZW23)</f>
+        <f t="shared" si="1"/>
         <v>85.65</v>
       </c>
       <c r="C23" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>31.200000000000003</v>
       </c>
       <c r="D23" s="45" t="s">
@@ -12020,19 +12062,21 @@
       <c r="BQ23" s="5">
         <v>61.5</v>
       </c>
-      <c r="BR23" s="5"/>
+      <c r="BR23" s="5">
+        <v>60.45</v>
+      </c>
     </row>
     <row r="24" spans="1:70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
-        <f>MIN(E24:ZW24)</f>
+        <f t="shared" si="0"/>
         <v>210.65</v>
       </c>
       <c r="B24" s="12">
-        <f>MAX(E24:ZW24)</f>
+        <f t="shared" si="1"/>
         <v>257.39999999999998</v>
       </c>
       <c r="C24" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>46.749999999999972</v>
       </c>
       <c r="D24" s="45" t="s">
@@ -12219,20 +12263,22 @@
       <c r="BQ24" s="5">
         <v>246.3</v>
       </c>
-      <c r="BR24" s="5"/>
+      <c r="BR24" s="5">
+        <v>241.6</v>
+      </c>
     </row>
     <row r="25" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
-        <f>MIN(E25:ZW25)</f>
+        <f t="shared" si="0"/>
         <v>876</v>
       </c>
       <c r="B25" s="12">
-        <f>MAX(E25:ZW25)</f>
-        <v>956.2</v>
+        <f t="shared" si="1"/>
+        <v>963.5</v>
       </c>
       <c r="C25" s="12">
-        <f t="shared" si="0"/>
-        <v>80.200000000000045</v>
+        <f t="shared" si="2"/>
+        <v>87.5</v>
       </c>
       <c r="D25" s="46" t="s">
         <v>236</v>
@@ -12400,19 +12446,21 @@
       <c r="BQ25" s="5">
         <v>956.2</v>
       </c>
-      <c r="BR25" s="5"/>
+      <c r="BR25" s="5">
+        <v>963.5</v>
+      </c>
     </row>
     <row r="26" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
-        <f>MIN(E26:ZW26)</f>
+        <f t="shared" si="0"/>
         <v>83.1</v>
       </c>
       <c r="B26" s="12">
-        <f>MAX(E26:ZW26)</f>
+        <f t="shared" si="1"/>
         <v>96</v>
       </c>
       <c r="C26" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12.900000000000006</v>
       </c>
       <c r="D26" s="45" t="s">
@@ -12569,19 +12617,21 @@
       <c r="BQ26" s="5">
         <v>95.85</v>
       </c>
-      <c r="BR26" s="5"/>
+      <c r="BR26" s="5">
+        <v>94.95</v>
+      </c>
     </row>
     <row r="27" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
-        <f>MIN(E27:ZW27)</f>
+        <f t="shared" si="0"/>
         <v>37.6</v>
       </c>
       <c r="B27" s="12">
-        <f>MAX(E27:ZW27)</f>
+        <f t="shared" si="1"/>
         <v>44.75</v>
       </c>
       <c r="C27" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.1499999999999986</v>
       </c>
       <c r="D27" s="45" t="s">
@@ -12738,19 +12788,21 @@
       <c r="BQ27" s="5">
         <v>38.25</v>
       </c>
-      <c r="BR27" s="5"/>
+      <c r="BR27" s="5">
+        <v>38.85</v>
+      </c>
     </row>
     <row r="28" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
-        <f>MIN(E28:ZW28)</f>
+        <f t="shared" si="0"/>
         <v>111.95</v>
       </c>
       <c r="B28" s="12">
-        <f>MAX(E28:ZW28)</f>
+        <f t="shared" si="1"/>
         <v>141.65</v>
       </c>
       <c r="C28" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>29.700000000000003</v>
       </c>
       <c r="D28" s="45" t="s">
@@ -12907,19 +12959,21 @@
       <c r="BQ28" s="5">
         <v>131.44999999999999</v>
       </c>
-      <c r="BR28" s="5"/>
+      <c r="BR28" s="5">
+        <v>127</v>
+      </c>
     </row>
     <row r="29" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
-        <f>MIN(E29:ZW29)</f>
+        <f t="shared" si="0"/>
         <v>62.3</v>
       </c>
       <c r="B29" s="12">
-        <f>MAX(E29:ZW29)</f>
+        <f t="shared" si="1"/>
         <v>78.849999999999994</v>
       </c>
       <c r="C29" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16.549999999999997</v>
       </c>
       <c r="D29" s="45" t="s">
@@ -13076,19 +13130,21 @@
       <c r="BQ29" s="5">
         <v>69.650000000000006</v>
       </c>
-      <c r="BR29" s="5"/>
+      <c r="BR29" s="5">
+        <v>67.95</v>
+      </c>
     </row>
     <row r="30" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
-        <f>MIN(E30:ZW30)</f>
+        <f t="shared" si="0"/>
         <v>39.25</v>
       </c>
       <c r="B30" s="12">
-        <f>MAX(E30:ZW30)</f>
+        <f t="shared" si="1"/>
         <v>50.95</v>
       </c>
       <c r="C30" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11.700000000000003</v>
       </c>
       <c r="D30" s="45" t="s">
@@ -13245,20 +13301,22 @@
       <c r="BQ30" s="5">
         <v>48.2</v>
       </c>
-      <c r="BR30" s="5"/>
+      <c r="BR30" s="5">
+        <v>48.75</v>
+      </c>
     </row>
     <row r="31" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
-        <f>MIN(E31:ZW31)</f>
-        <v>136.5</v>
+        <f t="shared" si="0"/>
+        <v>134.19999999999999</v>
       </c>
       <c r="B31" s="12">
-        <f>MAX(E31:ZW31)</f>
+        <f t="shared" si="1"/>
         <v>156.85</v>
       </c>
       <c r="C31" s="12">
-        <f t="shared" si="0"/>
-        <v>20.349999999999994</v>
+        <f t="shared" si="2"/>
+        <v>22.650000000000006</v>
       </c>
       <c r="D31" s="45" t="s">
         <v>257</v>
@@ -13414,19 +13472,21 @@
       <c r="BQ31" s="5">
         <v>138.9</v>
       </c>
-      <c r="BR31" s="5"/>
+      <c r="BR31" s="5">
+        <v>134.19999999999999</v>
+      </c>
     </row>
     <row r="32" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
-        <f>MIN(E32:ZW32)</f>
+        <f t="shared" si="0"/>
         <v>101.6</v>
       </c>
       <c r="B32" s="12">
-        <f>MAX(E32:ZW32)</f>
+        <f t="shared" si="1"/>
         <v>121.8</v>
       </c>
       <c r="C32" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20.200000000000003</v>
       </c>
       <c r="D32" s="45" t="s">
@@ -13571,19 +13631,21 @@
       <c r="BQ32" s="5">
         <v>106.15</v>
       </c>
-      <c r="BR32" s="5"/>
+      <c r="BR32" s="5">
+        <v>104.5</v>
+      </c>
     </row>
     <row r="33" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
-        <f>MIN(E33:ZW33)</f>
+        <f t="shared" si="0"/>
         <v>56.75</v>
       </c>
       <c r="B33" s="12">
-        <f>MAX(E33:ZW33)</f>
+        <f t="shared" si="1"/>
         <v>67.099999999999994</v>
       </c>
       <c r="C33" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10.349999999999994</v>
       </c>
       <c r="D33" s="45" t="s">
@@ -13716,19 +13778,21 @@
       <c r="BQ33" s="5">
         <v>60.25</v>
       </c>
-      <c r="BR33" s="5"/>
+      <c r="BR33" s="5">
+        <v>59.45</v>
+      </c>
     </row>
     <row r="34" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
-        <f>MIN(E34:ZW34)</f>
+        <f t="shared" si="0"/>
         <v>167.9</v>
       </c>
       <c r="B34" s="12">
-        <f>MAX(E34:ZW34)</f>
+        <f t="shared" si="1"/>
         <v>236.1</v>
       </c>
       <c r="C34" s="12">
-        <f t="shared" ref="C34" si="1">B34-A34</f>
+        <f t="shared" ref="C34" si="3">B34-A34</f>
         <v>68.199999999999989</v>
       </c>
       <c r="D34" s="45" t="s">
@@ -13855,19 +13919,21 @@
       <c r="BQ34" s="5">
         <v>206.05</v>
       </c>
-      <c r="BR34" s="5"/>
+      <c r="BR34" s="5">
+        <v>204</v>
+      </c>
     </row>
     <row r="35" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
-        <f>MIN(E35:ZW35)</f>
+        <f t="shared" si="0"/>
         <v>661</v>
       </c>
       <c r="B35" s="12">
-        <f>MAX(E35:ZW35)</f>
+        <f t="shared" si="1"/>
         <v>714.65</v>
       </c>
       <c r="C35" s="12">
-        <f t="shared" ref="C35" si="2">B35-A35</f>
+        <f t="shared" ref="C35" si="4">B35-A35</f>
         <v>53.649999999999977</v>
       </c>
       <c r="D35" s="45" t="s">
@@ -13990,19 +14056,21 @@
       <c r="BQ35" s="5">
         <v>679</v>
       </c>
-      <c r="BR35" s="5"/>
+      <c r="BR35" s="5">
+        <v>680.5</v>
+      </c>
     </row>
     <row r="36" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
-        <f>MIN(E36:ZW36)</f>
+        <f t="shared" si="0"/>
         <v>402.9</v>
       </c>
       <c r="B36" s="12">
-        <f>MAX(E36:ZW36)</f>
+        <f t="shared" si="1"/>
         <v>520</v>
       </c>
       <c r="C36" s="12">
-        <f t="shared" ref="C36" si="3">B36-A36</f>
+        <f t="shared" ref="C36" si="5">B36-A36</f>
         <v>117.10000000000002</v>
       </c>
       <c r="D36" s="45" t="s">
@@ -14107,20 +14175,22 @@
       <c r="BQ36" s="5">
         <v>491.7</v>
       </c>
-      <c r="BR36" s="5"/>
+      <c r="BR36" s="5">
+        <v>469.85</v>
+      </c>
     </row>
     <row r="37" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
-        <f>MIN(E37:ZW37)</f>
+        <f t="shared" si="0"/>
         <v>226</v>
       </c>
       <c r="B37" s="12">
-        <f>MAX(E37:ZW37)</f>
-        <v>374.25</v>
+        <f t="shared" si="1"/>
+        <v>384</v>
       </c>
       <c r="C37" s="12">
-        <f t="shared" ref="C37" si="4">B37-A37</f>
-        <v>148.25</v>
+        <f t="shared" ref="C37" si="6">B37-A37</f>
+        <v>158</v>
       </c>
       <c r="D37" s="45" t="s">
         <v>297</v>
@@ -14214,19 +14284,21 @@
       <c r="BQ37" s="5">
         <v>374.25</v>
       </c>
-      <c r="BR37" s="5"/>
+      <c r="BR37" s="5">
+        <v>384</v>
+      </c>
     </row>
     <row r="38" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
-        <f>MIN(E38:ZW38)</f>
+        <f t="shared" si="0"/>
         <v>485</v>
       </c>
       <c r="B38" s="12">
-        <f>MAX(E38:ZW38)</f>
+        <f t="shared" si="1"/>
         <v>515.4</v>
       </c>
       <c r="C38" s="12">
-        <f t="shared" ref="C38" si="5">B38-A38</f>
+        <f t="shared" ref="C38" si="7">B38-A38</f>
         <v>30.399999999999977</v>
       </c>
       <c r="D38" s="45" t="s">
@@ -14319,19 +14391,21 @@
       <c r="BQ38" s="5">
         <v>515.4</v>
       </c>
-      <c r="BR38" s="5"/>
+      <c r="BR38" s="5">
+        <v>501.3</v>
+      </c>
     </row>
     <row r="39" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
-        <f>MIN(E39:ZW39)</f>
+        <f t="shared" si="0"/>
         <v>75.2</v>
       </c>
       <c r="B39" s="12">
-        <f>MAX(E39:ZW39)</f>
+        <f t="shared" si="1"/>
         <v>78.5</v>
       </c>
       <c r="C39" s="12">
-        <f t="shared" ref="C39" si="6">B39-A39</f>
+        <f t="shared" ref="C39" si="8">B39-A39</f>
         <v>3.2999999999999972</v>
       </c>
       <c r="D39" s="45" t="s">
@@ -14418,20 +14492,22 @@
       <c r="BQ39" s="5">
         <v>75.900000000000006</v>
       </c>
-      <c r="BR39" s="5"/>
+      <c r="BR39" s="5">
+        <v>77.099999999999994</v>
+      </c>
     </row>
     <row r="40" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
-        <f>MIN(E40:ZW40)</f>
-        <v>444.05</v>
+        <f t="shared" si="0"/>
+        <v>428</v>
       </c>
       <c r="B40" s="12">
-        <f>MAX(E40:ZW40)</f>
+        <f t="shared" si="1"/>
         <v>472</v>
       </c>
       <c r="C40" s="12">
-        <f t="shared" ref="C40" si="7">B40-A40</f>
-        <v>27.949999999999989</v>
+        <f t="shared" ref="C40" si="9">B40-A40</f>
+        <v>44</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>306</v>
@@ -14517,19 +14593,21 @@
       <c r="BQ40" s="5">
         <v>444.05</v>
       </c>
-      <c r="BR40" s="5"/>
+      <c r="BR40" s="5">
+        <v>428</v>
+      </c>
     </row>
     <row r="41" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
-        <f>MIN(E41:ZW41)</f>
+        <f t="shared" si="0"/>
         <v>192.65</v>
       </c>
       <c r="B41" s="12">
-        <f>MAX(E41:ZW41)</f>
+        <f t="shared" si="1"/>
         <v>209.8</v>
       </c>
       <c r="C41" s="12">
-        <f t="shared" ref="C41" si="8">B41-A41</f>
+        <f t="shared" ref="C41" si="10">B41-A41</f>
         <v>17.150000000000006</v>
       </c>
       <c r="D41" s="45" t="s">
@@ -14612,19 +14690,21 @@
       <c r="BQ41" s="5">
         <v>196.9</v>
       </c>
-      <c r="BR41" s="5"/>
+      <c r="BR41" s="5">
+        <v>204.8</v>
+      </c>
     </row>
     <row r="42" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
-        <f>MIN(E42:ZW42)</f>
+        <f t="shared" si="0"/>
         <v>63.5</v>
       </c>
       <c r="B42" s="12">
-        <f>MAX(E42:ZW42)</f>
+        <f t="shared" si="1"/>
         <v>65.75</v>
       </c>
       <c r="C42" s="12">
-        <f t="shared" ref="C42:C43" si="9">B42-A42</f>
+        <f t="shared" ref="C42:C43" si="11">B42-A42</f>
         <v>2.25</v>
       </c>
       <c r="D42" s="45" t="s">
@@ -14703,19 +14783,21 @@
       <c r="BQ42" s="5">
         <v>65.75</v>
       </c>
-      <c r="BR42" s="5"/>
+      <c r="BR42" s="5">
+        <v>65.349999999999994</v>
+      </c>
     </row>
     <row r="43" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
-        <f>MIN(E43:ZW43)</f>
+        <f t="shared" si="0"/>
         <v>57.3</v>
       </c>
       <c r="B43" s="12">
-        <f>MAX(E43:ZW43)</f>
+        <f t="shared" si="1"/>
         <v>60.75</v>
       </c>
       <c r="C43" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3.4500000000000028</v>
       </c>
       <c r="D43" s="45" t="s">
@@ -14794,19 +14876,21 @@
       <c r="BQ43" s="5">
         <v>58.3</v>
       </c>
-      <c r="BR43" s="5"/>
+      <c r="BR43" s="5">
+        <v>57.9</v>
+      </c>
     </row>
     <row r="44" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
-        <f>MIN(E44:ZW44)</f>
+        <f t="shared" si="0"/>
         <v>36.950000000000003</v>
       </c>
       <c r="B44" s="12">
-        <f>MAX(E44:ZW44)</f>
+        <f t="shared" si="1"/>
         <v>38.65</v>
       </c>
       <c r="C44" s="12">
-        <f t="shared" ref="C44:C47" si="10">B44-A44</f>
+        <f t="shared" ref="C44:C47" si="12">B44-A44</f>
         <v>1.6999999999999957</v>
       </c>
       <c r="D44" s="45" t="s">
@@ -14885,19 +14969,21 @@
       <c r="BQ44" s="5">
         <v>38.35</v>
       </c>
-      <c r="BR44" s="5"/>
+      <c r="BR44" s="5">
+        <v>38.450000000000003</v>
+      </c>
     </row>
     <row r="45" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
-        <f>MIN(E45:ZW45)</f>
+        <f t="shared" si="0"/>
         <v>577.45000000000005</v>
       </c>
       <c r="B45" s="12">
-        <f t="shared" ref="B45:B46" si="11">MAX(E45:ZW45)</f>
+        <f t="shared" ref="B45:B46" si="13">MAX(E45:ZW45)</f>
         <v>597.20000000000005</v>
       </c>
       <c r="C45" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>19.75</v>
       </c>
       <c r="D45" s="45" t="s">
@@ -14974,19 +15060,21 @@
       <c r="BQ45" s="5">
         <v>597.20000000000005</v>
       </c>
-      <c r="BR45" s="5"/>
+      <c r="BR45" s="5">
+        <v>584</v>
+      </c>
     </row>
     <row r="46" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
-        <f>MIN(E46:ZW46)</f>
+        <f t="shared" si="0"/>
         <v>830.25</v>
       </c>
       <c r="B46" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>856</v>
       </c>
       <c r="C46" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>25.75</v>
       </c>
       <c r="D46" s="45" t="s">
@@ -15063,20 +15151,22 @@
       <c r="BQ46" s="5">
         <v>830.25</v>
       </c>
-      <c r="BR46" s="5"/>
+      <c r="BR46" s="5">
+        <v>832.95</v>
+      </c>
     </row>
     <row r="47" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
-        <f>MIN(E47:ZW47)</f>
-        <v>141.80000000000001</v>
+        <f t="shared" si="0"/>
+        <v>140.30000000000001</v>
       </c>
       <c r="B47" s="12">
         <f>MAX(E47:ZW47)</f>
         <v>146</v>
       </c>
       <c r="C47" s="12">
-        <f t="shared" si="10"/>
-        <v>4.1999999999999886</v>
+        <f t="shared" si="12"/>
+        <v>5.6999999999999886</v>
       </c>
       <c r="D47" s="45" t="s">
         <v>313</v>
@@ -15150,7 +15240,9 @@
       <c r="BQ47" s="5">
         <v>141.80000000000001</v>
       </c>
-      <c r="BR47" s="5"/>
+      <c r="BR47" s="5">
+        <v>140.30000000000001</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="L1:L37">

</xml_diff>

<commit_message>
Added details for 13/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -951,12 +951,6 @@
     <t>ADANITRANS</t>
   </si>
   <si>
-    <t>MANINFRA</t>
-  </si>
-  <si>
-    <t>ANANTRAJ</t>
-  </si>
-  <si>
     <t>HCC</t>
   </si>
   <si>
@@ -967,6 +961,12 @@
   </si>
   <si>
     <t>GSFC</t>
+  </si>
+  <si>
+    <t>13/11/2017</t>
+  </si>
+  <si>
+    <t>NIACL</t>
   </si>
 </sst>
 </file>
@@ -7212,11 +7212,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BR47"/>
+  <dimension ref="A1:BS46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="BO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BR48" sqref="BR48"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="BP1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BS46" sqref="BS46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7256,9 +7256,10 @@
     <col min="64" max="64" width="14" bestFit="1" customWidth="1"/>
     <col min="65" max="69" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:71" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>249</v>
       </c>
@@ -7469,14 +7470,17 @@
       <c r="BR1" s="51">
         <v>43019</v>
       </c>
-    </row>
-    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS1" s="49" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
-        <f t="shared" ref="A2:A47" si="0">MIN(E2:ZW2)</f>
+        <f t="shared" ref="A2:A45" si="0">MIN(E2:ZW2)</f>
         <v>243.6</v>
       </c>
       <c r="B2" s="12">
-        <f t="shared" ref="B2:B44" si="1">MAX(E2:ZW2)</f>
+        <f t="shared" ref="B2:B42" si="1">MAX(E2:ZW2)</f>
         <v>333.8</v>
       </c>
       <c r="C2" s="12">
@@ -7676,8 +7680,11 @@
       <c r="BR2" s="5">
         <v>333.8</v>
       </c>
-    </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS2" s="5">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <f t="shared" si="0"/>
         <v>262.7</v>
@@ -7883,11 +7890,14 @@
       <c r="BR3" s="5">
         <v>318.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS3" s="5">
+        <v>314.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
-        <v>259.45</v>
+        <v>258.60000000000002</v>
       </c>
       <c r="B4" s="12">
         <f t="shared" si="1"/>
@@ -7895,7 +7905,7 @@
       </c>
       <c r="C4" s="12">
         <f t="shared" si="2"/>
-        <v>32.25</v>
+        <v>33.099999999999966</v>
       </c>
       <c r="D4" s="44" t="s">
         <v>25</v>
@@ -8096,8 +8106,11 @@
       <c r="BR4" s="5">
         <v>262.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS4" s="5">
+        <v>258.60000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <f t="shared" si="0"/>
         <v>786.25</v>
@@ -8309,8 +8322,11 @@
       <c r="BR5" s="5">
         <v>884.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS5" s="5">
+        <v>874.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <f t="shared" si="0"/>
         <v>236.45</v>
@@ -8522,8 +8538,11 @@
       <c r="BR6" s="5">
         <v>285.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS6" s="5">
+        <v>274.35000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <f t="shared" si="0"/>
         <v>15.6</v>
@@ -8735,8 +8754,11 @@
       <c r="BR7" s="5">
         <v>17.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS7" s="5">
+        <v>17.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <f t="shared" si="0"/>
         <v>53.4</v>
@@ -8948,8 +8970,11 @@
       <c r="BR8" s="5">
         <v>81.55</v>
       </c>
-    </row>
-    <row r="9" spans="1:70" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BS8" s="5">
+        <v>78.900000000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:71" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <f t="shared" si="0"/>
         <v>53.5</v>
@@ -9153,8 +9178,11 @@
       <c r="BR9" s="28">
         <v>55.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS9" s="28">
+        <v>55.55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <f t="shared" si="0"/>
         <v>38.6</v>
@@ -9366,8 +9394,11 @@
       <c r="BR10" s="5">
         <v>39.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS10" s="5">
+        <v>38.65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <f t="shared" si="0"/>
         <v>72.650000000000006</v>
@@ -9579,8 +9610,11 @@
       <c r="BR11" s="5">
         <v>96.65</v>
       </c>
-    </row>
-    <row r="12" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS11" s="5">
+        <v>92.95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
         <v>82.65</v>
@@ -9792,8 +9826,11 @@
       <c r="BR12" s="5">
         <v>92.05</v>
       </c>
-    </row>
-    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS12" s="5">
+        <v>89.15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <f t="shared" si="0"/>
         <v>44.1</v>
@@ -10005,8 +10042,11 @@
       <c r="BR13" s="5">
         <v>48.75</v>
       </c>
-    </row>
-    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS13" s="5">
+        <v>49.35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <f t="shared" si="0"/>
         <v>29.75</v>
@@ -10218,8 +10258,11 @@
       <c r="BR14" s="5">
         <v>38.75</v>
       </c>
-    </row>
-    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS14" s="5">
+        <v>36.85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
         <v>25.25</v>
@@ -10423,8 +10466,11 @@
       <c r="BR15" s="5">
         <v>25.8</v>
       </c>
-    </row>
-    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS15" s="5">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <f t="shared" si="0"/>
         <v>552</v>
@@ -10636,8 +10682,11 @@
       <c r="BR16" s="5">
         <v>703.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS16" s="5">
+        <v>690.55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <f t="shared" si="0"/>
         <v>433</v>
@@ -10849,8 +10898,11 @@
       <c r="BR17" s="5">
         <v>477</v>
       </c>
-    </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS17" s="5">
+        <v>473.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <f t="shared" si="0"/>
         <v>178.8</v>
@@ -11062,19 +11114,22 @@
       <c r="BR18" s="5">
         <v>296</v>
       </c>
-    </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS18" s="5">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <f t="shared" si="0"/>
         <v>440.7</v>
       </c>
       <c r="B19" s="12">
         <f t="shared" si="1"/>
-        <v>592</v>
+        <v>619.75</v>
       </c>
       <c r="C19" s="12">
         <f t="shared" si="2"/>
-        <v>151.30000000000001</v>
+        <v>179.05</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -11275,8 +11330,11 @@
       <c r="BR19" s="5">
         <v>592</v>
       </c>
-    </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS19" s="5">
+        <v>619.75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <f t="shared" si="0"/>
         <v>677</v>
@@ -11488,8 +11546,11 @@
       <c r="BR20" s="5">
         <v>743.1</v>
       </c>
-    </row>
-    <row r="21" spans="1:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BS20" s="5">
+        <v>708.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <f t="shared" si="0"/>
         <v>376.7</v>
@@ -11701,8 +11762,11 @@
       <c r="BR21" s="5">
         <v>503.4</v>
       </c>
-    </row>
-    <row r="22" spans="1:70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BS21" s="5">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="22" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <f t="shared" si="0"/>
         <v>315.2</v>
@@ -11860,8 +11924,11 @@
       <c r="BR22" s="5">
         <v>383</v>
       </c>
-    </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS22" s="5">
+        <v>371.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
         <v>54.45</v>
@@ -12065,8 +12132,11 @@
       <c r="BR23" s="5">
         <v>60.45</v>
       </c>
-    </row>
-    <row r="24" spans="1:70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BS23" s="5">
+        <v>57.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <f t="shared" si="0"/>
         <v>210.65</v>
@@ -12266,8 +12336,11 @@
       <c r="BR24" s="5">
         <v>241.6</v>
       </c>
-    </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS24" s="5">
+        <v>238.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <f t="shared" si="0"/>
         <v>876</v>
@@ -12449,8 +12522,11 @@
       <c r="BR25" s="5">
         <v>963.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS25" s="5">
+        <v>952.55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <f t="shared" si="0"/>
         <v>83.1</v>
@@ -12620,8 +12696,11 @@
       <c r="BR26" s="5">
         <v>94.95</v>
       </c>
-    </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS26" s="5">
+        <v>92.65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <f t="shared" si="0"/>
         <v>37.6</v>
@@ -12791,8 +12870,11 @@
       <c r="BR27" s="5">
         <v>38.85</v>
       </c>
-    </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS27" s="5">
+        <v>38.200000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <f t="shared" si="0"/>
         <v>111.95</v>
@@ -12962,8 +13044,11 @@
       <c r="BR28" s="5">
         <v>127</v>
       </c>
-    </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS28" s="5">
+        <v>122.65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <f t="shared" si="0"/>
         <v>62.3</v>
@@ -13133,8 +13218,11 @@
       <c r="BR29" s="5">
         <v>67.95</v>
       </c>
-    </row>
-    <row r="30" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS29" s="5">
+        <v>66.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <f t="shared" si="0"/>
         <v>39.25</v>
@@ -13304,11 +13392,14 @@
       <c r="BR30" s="5">
         <v>48.75</v>
       </c>
-    </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS30" s="5">
+        <v>41.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
-        <v>134.19999999999999</v>
+        <v>132.15</v>
       </c>
       <c r="B31" s="12">
         <f t="shared" si="1"/>
@@ -13316,7 +13407,7 @@
       </c>
       <c r="C31" s="12">
         <f t="shared" si="2"/>
-        <v>22.650000000000006</v>
+        <v>24.699999999999989</v>
       </c>
       <c r="D31" s="45" t="s">
         <v>257</v>
@@ -13475,8 +13566,11 @@
       <c r="BR31" s="5">
         <v>134.19999999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS31" s="5">
+        <v>132.15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <f t="shared" si="0"/>
         <v>101.6</v>
@@ -13634,8 +13728,11 @@
       <c r="BR32" s="5">
         <v>104.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS32" s="5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <f t="shared" si="0"/>
         <v>56.75</v>
@@ -13781,8 +13878,11 @@
       <c r="BR33" s="5">
         <v>59.45</v>
       </c>
-    </row>
-    <row r="34" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS33" s="5">
+        <v>60.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <f t="shared" si="0"/>
         <v>167.9</v>
@@ -13922,8 +14022,11 @@
       <c r="BR34" s="5">
         <v>204</v>
       </c>
-    </row>
-    <row r="35" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS34" s="5">
+        <v>197.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <f t="shared" si="0"/>
         <v>661</v>
@@ -14059,8 +14162,11 @@
       <c r="BR35" s="5">
         <v>680.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS35" s="5">
+        <v>686.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <f t="shared" si="0"/>
         <v>402.9</v>
@@ -14178,19 +14284,22 @@
       <c r="BR36" s="5">
         <v>469.85</v>
       </c>
-    </row>
-    <row r="37" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS36" s="5">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="37" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <f t="shared" si="0"/>
         <v>226</v>
       </c>
       <c r="B37" s="12">
         <f t="shared" si="1"/>
-        <v>384</v>
+        <v>396.85</v>
       </c>
       <c r="C37" s="12">
         <f t="shared" ref="C37" si="6">B37-A37</f>
-        <v>158</v>
+        <v>170.85000000000002</v>
       </c>
       <c r="D37" s="45" t="s">
         <v>297</v>
@@ -14287,8 +14396,11 @@
       <c r="BR37" s="5">
         <v>384</v>
       </c>
-    </row>
-    <row r="38" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS37" s="5">
+        <v>396.85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <f t="shared" si="0"/>
         <v>485</v>
@@ -14394,8 +14506,11 @@
       <c r="BR38" s="5">
         <v>501.3</v>
       </c>
-    </row>
-    <row r="39" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS38" s="5">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="39" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <f t="shared" si="0"/>
         <v>75.2</v>
@@ -14495,11 +14610,14 @@
       <c r="BR39" s="5">
         <v>77.099999999999994</v>
       </c>
-    </row>
-    <row r="40" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS39" s="5">
+        <v>77.25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <f t="shared" si="0"/>
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B40" s="12">
         <f t="shared" si="1"/>
@@ -14507,7 +14625,7 @@
       </c>
       <c r="C40" s="12">
         <f t="shared" ref="C40" si="9">B40-A40</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>306</v>
@@ -14596,19 +14714,22 @@
       <c r="BR40" s="5">
         <v>428</v>
       </c>
-    </row>
-    <row r="41" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS40" s="5">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="41" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <f t="shared" si="0"/>
         <v>192.65</v>
       </c>
       <c r="B41" s="12">
         <f t="shared" si="1"/>
-        <v>209.8</v>
+        <v>215.25</v>
       </c>
       <c r="C41" s="12">
         <f t="shared" ref="C41" si="10">B41-A41</f>
-        <v>17.150000000000006</v>
+        <v>22.599999999999994</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>307</v>
@@ -14693,18 +14814,21 @@
       <c r="BR41" s="5">
         <v>204.8</v>
       </c>
-    </row>
-    <row r="42" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS41" s="5">
+        <v>215.25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>36.4</v>
       </c>
       <c r="B42" s="12">
         <f t="shared" si="1"/>
-        <v>65.75</v>
+        <v>38.65</v>
       </c>
       <c r="C42" s="12">
-        <f t="shared" ref="C42:C43" si="11">B42-A42</f>
+        <f t="shared" ref="C42:C45" si="11">B42-A42</f>
         <v>2.25</v>
       </c>
       <c r="D42" s="45" t="s">
@@ -14772,33 +14896,36 @@
       <c r="BL42" s="5"/>
       <c r="BM42" s="5"/>
       <c r="BN42" s="5">
-        <v>63.5</v>
+        <v>38.1</v>
       </c>
       <c r="BO42" s="5">
-        <v>63.7</v>
+        <v>36.950000000000003</v>
       </c>
       <c r="BP42" s="5">
-        <v>64.8</v>
+        <v>38.65</v>
       </c>
       <c r="BQ42" s="5">
-        <v>65.75</v>
+        <v>38.35</v>
       </c>
       <c r="BR42" s="5">
-        <v>65.349999999999994</v>
-      </c>
-    </row>
-    <row r="43" spans="1:70" x14ac:dyDescent="0.25">
+        <v>38.450000000000003</v>
+      </c>
+      <c r="BS42" s="5">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <f t="shared" si="0"/>
-        <v>57.3</v>
+        <v>577.45000000000005</v>
       </c>
       <c r="B43" s="12">
-        <f t="shared" si="1"/>
-        <v>60.75</v>
+        <f t="shared" ref="B43:B44" si="12">MAX(E43:ZW43)</f>
+        <v>616.15</v>
       </c>
       <c r="C43" s="12">
         <f t="shared" si="11"/>
-        <v>3.4500000000000028</v>
+        <v>38.699999999999932</v>
       </c>
       <c r="D43" s="45" t="s">
         <v>309</v>
@@ -14864,34 +14991,35 @@
       <c r="BK43" s="5"/>
       <c r="BL43" s="5"/>
       <c r="BM43" s="5"/>
-      <c r="BN43" s="5">
-        <v>60.75</v>
-      </c>
+      <c r="BN43" s="5"/>
       <c r="BO43" s="5">
-        <v>60.75</v>
+        <v>585</v>
       </c>
       <c r="BP43" s="5">
-        <v>57.3</v>
+        <v>577.45000000000005</v>
       </c>
       <c r="BQ43" s="5">
-        <v>58.3</v>
+        <v>597.20000000000005</v>
       </c>
       <c r="BR43" s="5">
-        <v>57.9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:70" x14ac:dyDescent="0.25">
+        <v>584</v>
+      </c>
+      <c r="BS43" s="5">
+        <v>616.15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <f t="shared" si="0"/>
-        <v>36.950000000000003</v>
+        <v>826</v>
       </c>
       <c r="B44" s="12">
-        <f t="shared" si="1"/>
-        <v>38.65</v>
+        <f t="shared" si="12"/>
+        <v>856</v>
       </c>
       <c r="C44" s="12">
-        <f t="shared" ref="C44:C47" si="12">B44-A44</f>
-        <v>1.6999999999999957</v>
+        <f t="shared" si="11"/>
+        <v>30</v>
       </c>
       <c r="D44" s="45" t="s">
         <v>310</v>
@@ -14957,34 +15085,35 @@
       <c r="BK44" s="5"/>
       <c r="BL44" s="5"/>
       <c r="BM44" s="5"/>
-      <c r="BN44" s="5">
-        <v>38.1</v>
-      </c>
+      <c r="BN44" s="5"/>
       <c r="BO44" s="5">
-        <v>36.950000000000003</v>
+        <v>856</v>
       </c>
       <c r="BP44" s="5">
-        <v>38.65</v>
+        <v>832.8</v>
       </c>
       <c r="BQ44" s="5">
-        <v>38.35</v>
+        <v>830.25</v>
       </c>
       <c r="BR44" s="5">
-        <v>38.450000000000003</v>
-      </c>
-    </row>
-    <row r="45" spans="1:70" x14ac:dyDescent="0.25">
+        <v>832.95</v>
+      </c>
+      <c r="BS44" s="5">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="45" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <f t="shared" si="0"/>
-        <v>577.45000000000005</v>
+        <v>137.9</v>
       </c>
       <c r="B45" s="12">
-        <f t="shared" ref="B45:B46" si="13">MAX(E45:ZW45)</f>
-        <v>597.20000000000005</v>
+        <f>MAX(E45:ZW45)</f>
+        <v>146</v>
       </c>
       <c r="C45" s="12">
-        <f t="shared" si="12"/>
-        <v>19.75</v>
+        <f t="shared" si="11"/>
+        <v>8.0999999999999943</v>
       </c>
       <c r="D45" s="45" t="s">
         <v>311</v>
@@ -15051,34 +15180,35 @@
       <c r="BL45" s="5"/>
       <c r="BM45" s="5"/>
       <c r="BN45" s="5"/>
-      <c r="BO45" s="5">
-        <v>585</v>
-      </c>
+      <c r="BO45" s="5"/>
       <c r="BP45" s="5">
-        <v>577.45000000000005</v>
+        <v>146</v>
       </c>
       <c r="BQ45" s="5">
-        <v>597.20000000000005</v>
+        <v>141.80000000000001</v>
       </c>
       <c r="BR45" s="5">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="46" spans="1:70" x14ac:dyDescent="0.25">
+        <v>140.30000000000001</v>
+      </c>
+      <c r="BS45" s="5">
+        <v>137.9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
-        <f t="shared" si="0"/>
-        <v>830.25</v>
+        <f t="shared" ref="A46" si="13">MIN(E46:ZW46)</f>
+        <v>723.2</v>
       </c>
       <c r="B46" s="12">
-        <f t="shared" si="13"/>
-        <v>856</v>
+        <f>MAX(E46:ZW46)</f>
+        <v>723.2</v>
       </c>
       <c r="C46" s="12">
-        <f t="shared" si="12"/>
-        <v>25.75</v>
+        <f t="shared" ref="C46" si="14">B46-A46</f>
+        <v>0</v>
       </c>
       <c r="D46" s="45" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -15142,106 +15272,12 @@
       <c r="BL46" s="5"/>
       <c r="BM46" s="5"/>
       <c r="BN46" s="5"/>
-      <c r="BO46" s="5">
-        <v>856</v>
-      </c>
-      <c r="BP46" s="5">
-        <v>832.8</v>
-      </c>
-      <c r="BQ46" s="5">
-        <v>830.25</v>
-      </c>
-      <c r="BR46" s="5">
-        <v>832.95</v>
-      </c>
-    </row>
-    <row r="47" spans="1:70" x14ac:dyDescent="0.25">
-      <c r="A47" s="12">
-        <f t="shared" si="0"/>
-        <v>140.30000000000001</v>
-      </c>
-      <c r="B47" s="12">
-        <f>MAX(E47:ZW47)</f>
-        <v>146</v>
-      </c>
-      <c r="C47" s="12">
-        <f t="shared" si="12"/>
-        <v>5.6999999999999886</v>
-      </c>
-      <c r="D47" s="45" t="s">
-        <v>313</v>
-      </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="5"/>
-      <c r="U47" s="5"/>
-      <c r="V47" s="5"/>
-      <c r="W47" s="5"/>
-      <c r="X47" s="5"/>
-      <c r="Y47" s="5"/>
-      <c r="Z47" s="5"/>
-      <c r="AA47" s="5"/>
-      <c r="AB47" s="5"/>
-      <c r="AC47" s="5"/>
-      <c r="AD47" s="5"/>
-      <c r="AE47" s="5"/>
-      <c r="AF47" s="5"/>
-      <c r="AG47" s="5"/>
-      <c r="AH47" s="5"/>
-      <c r="AI47" s="5"/>
-      <c r="AJ47" s="5"/>
-      <c r="AK47" s="5"/>
-      <c r="AL47" s="5"/>
-      <c r="AM47" s="5"/>
-      <c r="AN47" s="5"/>
-      <c r="AO47" s="5"/>
-      <c r="AP47" s="5"/>
-      <c r="AQ47" s="5"/>
-      <c r="AR47" s="5"/>
-      <c r="AS47" s="5"/>
-      <c r="AT47" s="5"/>
-      <c r="AU47" s="5"/>
-      <c r="AV47" s="5"/>
-      <c r="AW47" s="5"/>
-      <c r="AX47" s="5"/>
-      <c r="AY47" s="5"/>
-      <c r="AZ47" s="5"/>
-      <c r="BA47" s="5"/>
-      <c r="BB47" s="5"/>
-      <c r="BC47" s="5"/>
-      <c r="BD47" s="5"/>
-      <c r="BE47" s="5"/>
-      <c r="BF47" s="5"/>
-      <c r="BG47" s="5"/>
-      <c r="BH47" s="5"/>
-      <c r="BI47" s="5"/>
-      <c r="BJ47" s="5"/>
-      <c r="BK47" s="5"/>
-      <c r="BL47" s="5"/>
-      <c r="BM47" s="5"/>
-      <c r="BN47" s="5"/>
-      <c r="BO47" s="5"/>
-      <c r="BP47" s="5">
-        <v>146</v>
-      </c>
-      <c r="BQ47" s="5">
-        <v>141.80000000000001</v>
-      </c>
-      <c r="BR47" s="5">
-        <v>140.30000000000001</v>
+      <c r="BO46" s="5"/>
+      <c r="BP46" s="5"/>
+      <c r="BQ46" s="5"/>
+      <c r="BR46" s="5"/>
+      <c r="BS46" s="5">
+        <v>723.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added details for 14/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="329">
   <si>
     <t>Date</t>
   </si>
@@ -967,6 +967,51 @@
   </si>
   <si>
     <t>NIACL</t>
+  </si>
+  <si>
+    <t>Painter</t>
+  </si>
+  <si>
+    <t>14/11/2017</t>
+  </si>
+  <si>
+    <t>15/11/2017</t>
+  </si>
+  <si>
+    <t>16/11/2018</t>
+  </si>
+  <si>
+    <t>17/11/2019</t>
+  </si>
+  <si>
+    <t>20/11/2020</t>
+  </si>
+  <si>
+    <t>21/11/2021</t>
+  </si>
+  <si>
+    <t>22/11/2022</t>
+  </si>
+  <si>
+    <t>23/11/2023</t>
+  </si>
+  <si>
+    <t>24/11/2024</t>
+  </si>
+  <si>
+    <t>27/11/2025</t>
+  </si>
+  <si>
+    <t>28/11/2026</t>
+  </si>
+  <si>
+    <t>29/11/2027</t>
+  </si>
+  <si>
+    <t>30/11/2028</t>
+  </si>
+  <si>
+    <t>TIMKEN</t>
   </si>
 </sst>
 </file>
@@ -1518,8 +1563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1613,7 +1658,7 @@
       </c>
       <c r="H3" s="4">
         <f>H2-B25</f>
-        <v>45990</v>
+        <v>55990</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1795,7 +1840,7 @@
         <v>43040</v>
       </c>
       <c r="B22" s="20">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="E22" s="3"/>
     </row>
@@ -1815,7 +1860,7 @@
       </c>
       <c r="B25" s="20">
         <f>SUM(B2:B24)</f>
-        <v>512500</v>
+        <v>502500</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -7212,11 +7257,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BS46"/>
+  <dimension ref="A1:CJ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="BP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BS46" sqref="BS46"/>
+      <selection pane="topRight" activeCell="BT1" sqref="BT1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7257,9 +7302,18 @@
     <col min="65" max="69" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="13.42578125" customWidth="1"/>
+    <col min="72" max="72" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="13.42578125" customWidth="1"/>
+    <col min="74" max="74" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="13.42578125" customWidth="1"/>
+    <col min="76" max="76" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="78" max="79" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="14.42578125" customWidth="1"/>
+    <col min="81" max="84" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:88" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>249</v>
       </c>
@@ -7473,8 +7527,51 @@
       <c r="BS1" s="49" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT1" s="49" t="s">
+        <v>315</v>
+      </c>
+      <c r="BU1" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="BV1" s="49" t="s">
+        <v>317</v>
+      </c>
+      <c r="BW1" s="49" t="s">
+        <v>318</v>
+      </c>
+      <c r="BX1" s="49" t="s">
+        <v>319</v>
+      </c>
+      <c r="BY1" s="49" t="s">
+        <v>320</v>
+      </c>
+      <c r="BZ1" s="49" t="s">
+        <v>321</v>
+      </c>
+      <c r="CA1" s="49" t="s">
+        <v>322</v>
+      </c>
+      <c r="CB1" s="49" t="s">
+        <v>323</v>
+      </c>
+      <c r="CC1" s="49" t="s">
+        <v>324</v>
+      </c>
+      <c r="CD1" s="49" t="s">
+        <v>325</v>
+      </c>
+      <c r="CE1" s="49" t="s">
+        <v>326</v>
+      </c>
+      <c r="CF1" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="CG1" s="27"/>
+      <c r="CH1" s="27"/>
+      <c r="CI1" s="27"/>
+      <c r="CJ1" s="27"/>
+    </row>
+    <row r="2" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <f t="shared" ref="A2:A45" si="0">MIN(E2:ZW2)</f>
         <v>243.6</v>
@@ -7683,8 +7780,27 @@
       <c r="BS2" s="5">
         <v>331</v>
       </c>
-    </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT2" s="5">
+        <v>329.05</v>
+      </c>
+      <c r="BU2" s="5"/>
+      <c r="BV2" s="5"/>
+      <c r="BW2" s="5"/>
+      <c r="BX2" s="5"/>
+      <c r="BY2" s="5"/>
+      <c r="BZ2" s="5"/>
+      <c r="CA2" s="5"/>
+      <c r="CB2" s="5"/>
+      <c r="CC2" s="5"/>
+      <c r="CD2" s="5"/>
+      <c r="CE2" s="5"/>
+      <c r="CF2" s="5"/>
+      <c r="CG2" s="5"/>
+      <c r="CH2" s="5"/>
+      <c r="CI2" s="5"/>
+      <c r="CJ2" s="5"/>
+    </row>
+    <row r="3" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <f t="shared" si="0"/>
         <v>262.7</v>
@@ -7893,11 +8009,30 @@
       <c r="BS3" s="5">
         <v>314.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT3" s="5">
+        <v>313.55</v>
+      </c>
+      <c r="BU3" s="5"/>
+      <c r="BV3" s="5"/>
+      <c r="BW3" s="5"/>
+      <c r="BX3" s="5"/>
+      <c r="BY3" s="5"/>
+      <c r="BZ3" s="5"/>
+      <c r="CA3" s="5"/>
+      <c r="CB3" s="5"/>
+      <c r="CC3" s="5"/>
+      <c r="CD3" s="5"/>
+      <c r="CE3" s="5"/>
+      <c r="CF3" s="5"/>
+      <c r="CG3" s="5"/>
+      <c r="CH3" s="5"/>
+      <c r="CI3" s="5"/>
+      <c r="CJ3" s="5"/>
+    </row>
+    <row r="4" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
-        <v>258.60000000000002</v>
+        <v>256.25</v>
       </c>
       <c r="B4" s="12">
         <f t="shared" si="1"/>
@@ -7905,7 +8040,7 @@
       </c>
       <c r="C4" s="12">
         <f t="shared" si="2"/>
-        <v>33.099999999999966</v>
+        <v>35.449999999999989</v>
       </c>
       <c r="D4" s="44" t="s">
         <v>25</v>
@@ -8109,8 +8244,27 @@
       <c r="BS4" s="5">
         <v>258.60000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT4" s="5">
+        <v>256.25</v>
+      </c>
+      <c r="BU4" s="5"/>
+      <c r="BV4" s="5"/>
+      <c r="BW4" s="5"/>
+      <c r="BX4" s="5"/>
+      <c r="BY4" s="5"/>
+      <c r="BZ4" s="5"/>
+      <c r="CA4" s="5"/>
+      <c r="CB4" s="5"/>
+      <c r="CC4" s="5"/>
+      <c r="CD4" s="5"/>
+      <c r="CE4" s="5"/>
+      <c r="CF4" s="5"/>
+      <c r="CG4" s="5"/>
+      <c r="CH4" s="5"/>
+      <c r="CI4" s="5"/>
+      <c r="CJ4" s="5"/>
+    </row>
+    <row r="5" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <f t="shared" si="0"/>
         <v>786.25</v>
@@ -8325,8 +8479,27 @@
       <c r="BS5" s="5">
         <v>874.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT5" s="5">
+        <v>887.5</v>
+      </c>
+      <c r="BU5" s="5"/>
+      <c r="BV5" s="5"/>
+      <c r="BW5" s="5"/>
+      <c r="BX5" s="5"/>
+      <c r="BY5" s="5"/>
+      <c r="BZ5" s="5"/>
+      <c r="CA5" s="5"/>
+      <c r="CB5" s="5"/>
+      <c r="CC5" s="5"/>
+      <c r="CD5" s="5"/>
+      <c r="CE5" s="5"/>
+      <c r="CF5" s="5"/>
+      <c r="CG5" s="5"/>
+      <c r="CH5" s="5"/>
+      <c r="CI5" s="5"/>
+      <c r="CJ5" s="5"/>
+    </row>
+    <row r="6" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <f t="shared" si="0"/>
         <v>236.45</v>
@@ -8541,8 +8714,27 @@
       <c r="BS6" s="5">
         <v>274.35000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT6" s="5">
+        <v>275.2</v>
+      </c>
+      <c r="BU6" s="5"/>
+      <c r="BV6" s="5"/>
+      <c r="BW6" s="5"/>
+      <c r="BX6" s="5"/>
+      <c r="BY6" s="5"/>
+      <c r="BZ6" s="5"/>
+      <c r="CA6" s="5"/>
+      <c r="CB6" s="5"/>
+      <c r="CC6" s="5"/>
+      <c r="CD6" s="5"/>
+      <c r="CE6" s="5"/>
+      <c r="CF6" s="5"/>
+      <c r="CG6" s="5"/>
+      <c r="CH6" s="5"/>
+      <c r="CI6" s="5"/>
+      <c r="CJ6" s="5"/>
+    </row>
+    <row r="7" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <f t="shared" si="0"/>
         <v>15.6</v>
@@ -8757,8 +8949,27 @@
       <c r="BS7" s="5">
         <v>17.75</v>
       </c>
-    </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT7" s="5">
+        <v>17.8</v>
+      </c>
+      <c r="BU7" s="5"/>
+      <c r="BV7" s="5"/>
+      <c r="BW7" s="5"/>
+      <c r="BX7" s="5"/>
+      <c r="BY7" s="5"/>
+      <c r="BZ7" s="5"/>
+      <c r="CA7" s="5"/>
+      <c r="CB7" s="5"/>
+      <c r="CC7" s="5"/>
+      <c r="CD7" s="5"/>
+      <c r="CE7" s="5"/>
+      <c r="CF7" s="5"/>
+      <c r="CG7" s="5"/>
+      <c r="CH7" s="5"/>
+      <c r="CI7" s="5"/>
+      <c r="CJ7" s="5"/>
+    </row>
+    <row r="8" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <f t="shared" si="0"/>
         <v>53.4</v>
@@ -8973,8 +9184,27 @@
       <c r="BS8" s="5">
         <v>78.900000000000006</v>
       </c>
-    </row>
-    <row r="9" spans="1:71" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BT8" s="5">
+        <v>79.849999999999994</v>
+      </c>
+      <c r="BU8" s="5"/>
+      <c r="BV8" s="5"/>
+      <c r="BW8" s="5"/>
+      <c r="BX8" s="5"/>
+      <c r="BY8" s="5"/>
+      <c r="BZ8" s="5"/>
+      <c r="CA8" s="5"/>
+      <c r="CB8" s="5"/>
+      <c r="CC8" s="5"/>
+      <c r="CD8" s="5"/>
+      <c r="CE8" s="5"/>
+      <c r="CF8" s="5"/>
+      <c r="CG8" s="5"/>
+      <c r="CH8" s="5"/>
+      <c r="CI8" s="5"/>
+      <c r="CJ8" s="5"/>
+    </row>
+    <row r="9" spans="1:88" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <f t="shared" si="0"/>
         <v>53.5</v>
@@ -9181,8 +9411,27 @@
       <c r="BS9" s="28">
         <v>55.55</v>
       </c>
-    </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT9" s="28">
+        <v>55.25</v>
+      </c>
+      <c r="BU9" s="28"/>
+      <c r="BV9" s="28"/>
+      <c r="BW9" s="28"/>
+      <c r="BX9" s="28"/>
+      <c r="BY9" s="28"/>
+      <c r="BZ9" s="28"/>
+      <c r="CA9" s="28"/>
+      <c r="CB9" s="28"/>
+      <c r="CC9" s="28"/>
+      <c r="CD9" s="28"/>
+      <c r="CE9" s="28"/>
+      <c r="CF9" s="28"/>
+      <c r="CG9" s="28"/>
+      <c r="CH9" s="28"/>
+      <c r="CI9" s="28"/>
+      <c r="CJ9" s="28"/>
+    </row>
+    <row r="10" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <f t="shared" si="0"/>
         <v>38.6</v>
@@ -9397,8 +9646,27 @@
       <c r="BS10" s="5">
         <v>38.65</v>
       </c>
-    </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT10" s="5">
+        <v>38.6</v>
+      </c>
+      <c r="BU10" s="5"/>
+      <c r="BV10" s="5"/>
+      <c r="BW10" s="5"/>
+      <c r="BX10" s="5"/>
+      <c r="BY10" s="5"/>
+      <c r="BZ10" s="5"/>
+      <c r="CA10" s="5"/>
+      <c r="CB10" s="5"/>
+      <c r="CC10" s="5"/>
+      <c r="CD10" s="5"/>
+      <c r="CE10" s="5"/>
+      <c r="CF10" s="5"/>
+      <c r="CG10" s="5"/>
+      <c r="CH10" s="5"/>
+      <c r="CI10" s="5"/>
+      <c r="CJ10" s="5"/>
+    </row>
+    <row r="11" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <f t="shared" si="0"/>
         <v>72.650000000000006</v>
@@ -9613,8 +9881,27 @@
       <c r="BS11" s="5">
         <v>92.95</v>
       </c>
-    </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT11" s="5">
+        <v>92.55</v>
+      </c>
+      <c r="BU11" s="5"/>
+      <c r="BV11" s="5"/>
+      <c r="BW11" s="5"/>
+      <c r="BX11" s="5"/>
+      <c r="BY11" s="5"/>
+      <c r="BZ11" s="5"/>
+      <c r="CA11" s="5"/>
+      <c r="CB11" s="5"/>
+      <c r="CC11" s="5"/>
+      <c r="CD11" s="5"/>
+      <c r="CE11" s="5"/>
+      <c r="CF11" s="5"/>
+      <c r="CG11" s="5"/>
+      <c r="CH11" s="5"/>
+      <c r="CI11" s="5"/>
+      <c r="CJ11" s="5"/>
+    </row>
+    <row r="12" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
         <v>82.65</v>
@@ -9829,8 +10116,27 @@
       <c r="BS12" s="5">
         <v>89.15</v>
       </c>
-    </row>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT12" s="5">
+        <v>91.4</v>
+      </c>
+      <c r="BU12" s="5"/>
+      <c r="BV12" s="5"/>
+      <c r="BW12" s="5"/>
+      <c r="BX12" s="5"/>
+      <c r="BY12" s="5"/>
+      <c r="BZ12" s="5"/>
+      <c r="CA12" s="5"/>
+      <c r="CB12" s="5"/>
+      <c r="CC12" s="5"/>
+      <c r="CD12" s="5"/>
+      <c r="CE12" s="5"/>
+      <c r="CF12" s="5"/>
+      <c r="CG12" s="5"/>
+      <c r="CH12" s="5"/>
+      <c r="CI12" s="5"/>
+      <c r="CJ12" s="5"/>
+    </row>
+    <row r="13" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <f t="shared" si="0"/>
         <v>44.1</v>
@@ -10045,8 +10351,27 @@
       <c r="BS13" s="5">
         <v>49.35</v>
       </c>
-    </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT13" s="5">
+        <v>48</v>
+      </c>
+      <c r="BU13" s="5"/>
+      <c r="BV13" s="5"/>
+      <c r="BW13" s="5"/>
+      <c r="BX13" s="5"/>
+      <c r="BY13" s="5"/>
+      <c r="BZ13" s="5"/>
+      <c r="CA13" s="5"/>
+      <c r="CB13" s="5"/>
+      <c r="CC13" s="5"/>
+      <c r="CD13" s="5"/>
+      <c r="CE13" s="5"/>
+      <c r="CF13" s="5"/>
+      <c r="CG13" s="5"/>
+      <c r="CH13" s="5"/>
+      <c r="CI13" s="5"/>
+      <c r="CJ13" s="5"/>
+    </row>
+    <row r="14" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <f t="shared" si="0"/>
         <v>29.75</v>
@@ -10261,11 +10586,30 @@
       <c r="BS14" s="5">
         <v>36.85</v>
       </c>
-    </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT14" s="5">
+        <v>36.1</v>
+      </c>
+      <c r="BU14" s="5"/>
+      <c r="BV14" s="5"/>
+      <c r="BW14" s="5"/>
+      <c r="BX14" s="5"/>
+      <c r="BY14" s="5"/>
+      <c r="BZ14" s="5"/>
+      <c r="CA14" s="5"/>
+      <c r="CB14" s="5"/>
+      <c r="CC14" s="5"/>
+      <c r="CD14" s="5"/>
+      <c r="CE14" s="5"/>
+      <c r="CF14" s="5"/>
+      <c r="CG14" s="5"/>
+      <c r="CH14" s="5"/>
+      <c r="CI14" s="5"/>
+      <c r="CJ14" s="5"/>
+    </row>
+    <row r="15" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
-        <v>25.25</v>
+        <v>25.15</v>
       </c>
       <c r="B15" s="12">
         <f t="shared" si="1"/>
@@ -10273,7 +10617,7 @@
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
-        <v>11.149999999999999</v>
+        <v>11.25</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>126</v>
@@ -10469,8 +10813,27 @@
       <c r="BS15" s="5">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT15" s="5">
+        <v>25.15</v>
+      </c>
+      <c r="BU15" s="5"/>
+      <c r="BV15" s="5"/>
+      <c r="BW15" s="5"/>
+      <c r="BX15" s="5"/>
+      <c r="BY15" s="5"/>
+      <c r="BZ15" s="5"/>
+      <c r="CA15" s="5"/>
+      <c r="CB15" s="5"/>
+      <c r="CC15" s="5"/>
+      <c r="CD15" s="5"/>
+      <c r="CE15" s="5"/>
+      <c r="CF15" s="5"/>
+      <c r="CG15" s="5"/>
+      <c r="CH15" s="5"/>
+      <c r="CI15" s="5"/>
+      <c r="CJ15" s="5"/>
+    </row>
+    <row r="16" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <f t="shared" si="0"/>
         <v>552</v>
@@ -10685,25 +11048,44 @@
       <c r="BS16" s="5">
         <v>690.55</v>
       </c>
-    </row>
-    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT16" s="5">
+        <v>682.8</v>
+      </c>
+      <c r="BU16" s="5"/>
+      <c r="BV16" s="5"/>
+      <c r="BW16" s="5"/>
+      <c r="BX16" s="5"/>
+      <c r="BY16" s="5"/>
+      <c r="BZ16" s="5"/>
+      <c r="CA16" s="5"/>
+      <c r="CB16" s="5"/>
+      <c r="CC16" s="5"/>
+      <c r="CD16" s="5"/>
+      <c r="CE16" s="5"/>
+      <c r="CF16" s="5"/>
+      <c r="CG16" s="5"/>
+      <c r="CH16" s="5"/>
+      <c r="CI16" s="5"/>
+      <c r="CJ16" s="5"/>
+    </row>
+    <row r="17" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <f t="shared" si="0"/>
         <v>433</v>
       </c>
       <c r="B17" s="12">
         <f t="shared" si="1"/>
-        <v>515</v>
+        <v>670</v>
       </c>
       <c r="C17" s="12">
         <f t="shared" si="2"/>
-        <v>82</v>
+        <v>237</v>
       </c>
       <c r="D17" s="44" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="28">
-        <v>515</v>
+        <v>670</v>
       </c>
       <c r="F17" s="28">
         <v>503.55</v>
@@ -10901,8 +11283,27 @@
       <c r="BS17" s="5">
         <v>473.1</v>
       </c>
-    </row>
-    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT17" s="5">
+        <v>471.2</v>
+      </c>
+      <c r="BU17" s="5"/>
+      <c r="BV17" s="5"/>
+      <c r="BW17" s="5"/>
+      <c r="BX17" s="5"/>
+      <c r="BY17" s="5"/>
+      <c r="BZ17" s="5"/>
+      <c r="CA17" s="5"/>
+      <c r="CB17" s="5"/>
+      <c r="CC17" s="5"/>
+      <c r="CD17" s="5"/>
+      <c r="CE17" s="5"/>
+      <c r="CF17" s="5"/>
+      <c r="CG17" s="5"/>
+      <c r="CH17" s="5"/>
+      <c r="CI17" s="5"/>
+      <c r="CJ17" s="5"/>
+    </row>
+    <row r="18" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <f t="shared" si="0"/>
         <v>178.8</v>
@@ -11117,19 +11518,38 @@
       <c r="BS18" s="5">
         <v>287</v>
       </c>
-    </row>
-    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT18" s="5">
+        <v>275.2</v>
+      </c>
+      <c r="BU18" s="5"/>
+      <c r="BV18" s="5"/>
+      <c r="BW18" s="5"/>
+      <c r="BX18" s="5"/>
+      <c r="BY18" s="5"/>
+      <c r="BZ18" s="5"/>
+      <c r="CA18" s="5"/>
+      <c r="CB18" s="5"/>
+      <c r="CC18" s="5"/>
+      <c r="CD18" s="5"/>
+      <c r="CE18" s="5"/>
+      <c r="CF18" s="5"/>
+      <c r="CG18" s="5"/>
+      <c r="CH18" s="5"/>
+      <c r="CI18" s="5"/>
+      <c r="CJ18" s="5"/>
+    </row>
+    <row r="19" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <f t="shared" si="0"/>
         <v>440.7</v>
       </c>
       <c r="B19" s="12">
         <f t="shared" si="1"/>
-        <v>619.75</v>
+        <v>648.15</v>
       </c>
       <c r="C19" s="12">
         <f t="shared" si="2"/>
-        <v>179.05</v>
+        <v>207.45</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -11333,8 +11753,27 @@
       <c r="BS19" s="5">
         <v>619.75</v>
       </c>
-    </row>
-    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT19" s="5">
+        <v>648.15</v>
+      </c>
+      <c r="BU19" s="5"/>
+      <c r="BV19" s="5"/>
+      <c r="BW19" s="5"/>
+      <c r="BX19" s="5"/>
+      <c r="BY19" s="5"/>
+      <c r="BZ19" s="5"/>
+      <c r="CA19" s="5"/>
+      <c r="CB19" s="5"/>
+      <c r="CC19" s="5"/>
+      <c r="CD19" s="5"/>
+      <c r="CE19" s="5"/>
+      <c r="CF19" s="5"/>
+      <c r="CG19" s="5"/>
+      <c r="CH19" s="5"/>
+      <c r="CI19" s="5"/>
+      <c r="CJ19" s="5"/>
+    </row>
+    <row r="20" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <f t="shared" si="0"/>
         <v>677</v>
@@ -11549,8 +11988,27 @@
       <c r="BS20" s="5">
         <v>708.1</v>
       </c>
-    </row>
-    <row r="21" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BT20" s="5">
+        <v>699</v>
+      </c>
+      <c r="BU20" s="5"/>
+      <c r="BV20" s="5"/>
+      <c r="BW20" s="5"/>
+      <c r="BX20" s="5"/>
+      <c r="BY20" s="5"/>
+      <c r="BZ20" s="5"/>
+      <c r="CA20" s="5"/>
+      <c r="CB20" s="5"/>
+      <c r="CC20" s="5"/>
+      <c r="CD20" s="5"/>
+      <c r="CE20" s="5"/>
+      <c r="CF20" s="5"/>
+      <c r="CG20" s="5"/>
+      <c r="CH20" s="5"/>
+      <c r="CI20" s="5"/>
+      <c r="CJ20" s="5"/>
+    </row>
+    <row r="21" spans="1:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <f t="shared" si="0"/>
         <v>376.7</v>
@@ -11765,19 +12223,38 @@
       <c r="BS21" s="5">
         <v>498</v>
       </c>
-    </row>
-    <row r="22" spans="1:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BT21" s="5">
+        <v>498</v>
+      </c>
+      <c r="BU21" s="5"/>
+      <c r="BV21" s="5"/>
+      <c r="BW21" s="5"/>
+      <c r="BX21" s="5"/>
+      <c r="BY21" s="5"/>
+      <c r="BZ21" s="5"/>
+      <c r="CA21" s="5"/>
+      <c r="CB21" s="5"/>
+      <c r="CC21" s="5"/>
+      <c r="CD21" s="5"/>
+      <c r="CE21" s="5"/>
+      <c r="CF21" s="5"/>
+      <c r="CG21" s="5"/>
+      <c r="CH21" s="5"/>
+      <c r="CI21" s="5"/>
+      <c r="CJ21" s="5"/>
+    </row>
+    <row r="22" spans="1:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <f t="shared" si="0"/>
         <v>315.2</v>
       </c>
       <c r="B22" s="12">
         <f t="shared" si="1"/>
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="C22" s="12">
         <f t="shared" si="2"/>
-        <v>67.800000000000011</v>
+        <v>72.800000000000011</v>
       </c>
       <c r="D22" s="44" t="s">
         <v>269</v>
@@ -11927,8 +12404,27 @@
       <c r="BS22" s="5">
         <v>371.2</v>
       </c>
-    </row>
-    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT22" s="5">
+        <v>388</v>
+      </c>
+      <c r="BU22" s="5"/>
+      <c r="BV22" s="5"/>
+      <c r="BW22" s="5"/>
+      <c r="BX22" s="5"/>
+      <c r="BY22" s="5"/>
+      <c r="BZ22" s="5"/>
+      <c r="CA22" s="5"/>
+      <c r="CB22" s="5"/>
+      <c r="CC22" s="5"/>
+      <c r="CD22" s="5"/>
+      <c r="CE22" s="5"/>
+      <c r="CF22" s="5"/>
+      <c r="CG22" s="5"/>
+      <c r="CH22" s="5"/>
+      <c r="CI22" s="5"/>
+      <c r="CJ22" s="5"/>
+    </row>
+    <row r="23" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
         <v>54.45</v>
@@ -12135,8 +12631,27 @@
       <c r="BS23" s="5">
         <v>57.95</v>
       </c>
-    </row>
-    <row r="24" spans="1:71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BT23" s="5">
+        <v>58.3</v>
+      </c>
+      <c r="BU23" s="5"/>
+      <c r="BV23" s="5"/>
+      <c r="BW23" s="5"/>
+      <c r="BX23" s="5"/>
+      <c r="BY23" s="5"/>
+      <c r="BZ23" s="5"/>
+      <c r="CA23" s="5"/>
+      <c r="CB23" s="5"/>
+      <c r="CC23" s="5"/>
+      <c r="CD23" s="5"/>
+      <c r="CE23" s="5"/>
+      <c r="CF23" s="5"/>
+      <c r="CG23" s="5"/>
+      <c r="CH23" s="5"/>
+      <c r="CI23" s="5"/>
+      <c r="CJ23" s="5"/>
+    </row>
+    <row r="24" spans="1:88" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <f t="shared" si="0"/>
         <v>210.65</v>
@@ -12339,8 +12854,27 @@
       <c r="BS24" s="5">
         <v>238.6</v>
       </c>
-    </row>
-    <row r="25" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT24" s="5">
+        <v>237.4</v>
+      </c>
+      <c r="BU24" s="5"/>
+      <c r="BV24" s="5"/>
+      <c r="BW24" s="5"/>
+      <c r="BX24" s="5"/>
+      <c r="BY24" s="5"/>
+      <c r="BZ24" s="5"/>
+      <c r="CA24" s="5"/>
+      <c r="CB24" s="5"/>
+      <c r="CC24" s="5"/>
+      <c r="CD24" s="5"/>
+      <c r="CE24" s="5"/>
+      <c r="CF24" s="5"/>
+      <c r="CG24" s="5"/>
+      <c r="CH24" s="5"/>
+      <c r="CI24" s="5"/>
+      <c r="CJ24" s="5"/>
+    </row>
+    <row r="25" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <f t="shared" si="0"/>
         <v>876</v>
@@ -12525,8 +13059,27 @@
       <c r="BS25" s="5">
         <v>952.55</v>
       </c>
-    </row>
-    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT25" s="5">
+        <v>949.1</v>
+      </c>
+      <c r="BU25" s="5"/>
+      <c r="BV25" s="5"/>
+      <c r="BW25" s="5"/>
+      <c r="BX25" s="5"/>
+      <c r="BY25" s="5"/>
+      <c r="BZ25" s="5"/>
+      <c r="CA25" s="5"/>
+      <c r="CB25" s="5"/>
+      <c r="CC25" s="5"/>
+      <c r="CD25" s="5"/>
+      <c r="CE25" s="5"/>
+      <c r="CF25" s="5"/>
+      <c r="CG25" s="5"/>
+      <c r="CH25" s="5"/>
+      <c r="CI25" s="5"/>
+      <c r="CJ25" s="5"/>
+    </row>
+    <row r="26" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <f t="shared" si="0"/>
         <v>83.1</v>
@@ -12699,11 +13252,30 @@
       <c r="BS26" s="5">
         <v>92.65</v>
       </c>
-    </row>
-    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT26" s="5">
+        <v>92.05</v>
+      </c>
+      <c r="BU26" s="5"/>
+      <c r="BV26" s="5"/>
+      <c r="BW26" s="5"/>
+      <c r="BX26" s="5"/>
+      <c r="BY26" s="5"/>
+      <c r="BZ26" s="5"/>
+      <c r="CA26" s="5"/>
+      <c r="CB26" s="5"/>
+      <c r="CC26" s="5"/>
+      <c r="CD26" s="5"/>
+      <c r="CE26" s="5"/>
+      <c r="CF26" s="5"/>
+      <c r="CG26" s="5"/>
+      <c r="CH26" s="5"/>
+      <c r="CI26" s="5"/>
+      <c r="CJ26" s="5"/>
+    </row>
+    <row r="27" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <f t="shared" si="0"/>
-        <v>37.6</v>
+        <v>37.549999999999997</v>
       </c>
       <c r="B27" s="12">
         <f t="shared" si="1"/>
@@ -12711,7 +13283,7 @@
       </c>
       <c r="C27" s="12">
         <f t="shared" si="2"/>
-        <v>7.1499999999999986</v>
+        <v>7.2000000000000028</v>
       </c>
       <c r="D27" s="45" t="s">
         <v>253</v>
@@ -12873,8 +13445,27 @@
       <c r="BS27" s="5">
         <v>38.200000000000003</v>
       </c>
-    </row>
-    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT27" s="5">
+        <v>37.549999999999997</v>
+      </c>
+      <c r="BU27" s="5"/>
+      <c r="BV27" s="5"/>
+      <c r="BW27" s="5"/>
+      <c r="BX27" s="5"/>
+      <c r="BY27" s="5"/>
+      <c r="BZ27" s="5"/>
+      <c r="CA27" s="5"/>
+      <c r="CB27" s="5"/>
+      <c r="CC27" s="5"/>
+      <c r="CD27" s="5"/>
+      <c r="CE27" s="5"/>
+      <c r="CF27" s="5"/>
+      <c r="CG27" s="5"/>
+      <c r="CH27" s="5"/>
+      <c r="CI27" s="5"/>
+      <c r="CJ27" s="5"/>
+    </row>
+    <row r="28" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <f t="shared" si="0"/>
         <v>111.95</v>
@@ -13047,8 +13638,27 @@
       <c r="BS28" s="5">
         <v>122.65</v>
       </c>
-    </row>
-    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT28" s="5">
+        <v>120.3</v>
+      </c>
+      <c r="BU28" s="5"/>
+      <c r="BV28" s="5"/>
+      <c r="BW28" s="5"/>
+      <c r="BX28" s="5"/>
+      <c r="BY28" s="5"/>
+      <c r="BZ28" s="5"/>
+      <c r="CA28" s="5"/>
+      <c r="CB28" s="5"/>
+      <c r="CC28" s="5"/>
+      <c r="CD28" s="5"/>
+      <c r="CE28" s="5"/>
+      <c r="CF28" s="5"/>
+      <c r="CG28" s="5"/>
+      <c r="CH28" s="5"/>
+      <c r="CI28" s="5"/>
+      <c r="CJ28" s="5"/>
+    </row>
+    <row r="29" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <f t="shared" si="0"/>
         <v>62.3</v>
@@ -13221,8 +13831,27 @@
       <c r="BS29" s="5">
         <v>66.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT29" s="5">
+        <v>65.75</v>
+      </c>
+      <c r="BU29" s="5"/>
+      <c r="BV29" s="5"/>
+      <c r="BW29" s="5"/>
+      <c r="BX29" s="5"/>
+      <c r="BY29" s="5"/>
+      <c r="BZ29" s="5"/>
+      <c r="CA29" s="5"/>
+      <c r="CB29" s="5"/>
+      <c r="CC29" s="5"/>
+      <c r="CD29" s="5"/>
+      <c r="CE29" s="5"/>
+      <c r="CF29" s="5"/>
+      <c r="CG29" s="5"/>
+      <c r="CH29" s="5"/>
+      <c r="CI29" s="5"/>
+      <c r="CJ29" s="5"/>
+    </row>
+    <row r="30" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <f t="shared" si="0"/>
         <v>39.25</v>
@@ -13395,11 +14024,30 @@
       <c r="BS30" s="5">
         <v>41.8</v>
       </c>
-    </row>
-    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT30" s="5">
+        <v>41.85</v>
+      </c>
+      <c r="BU30" s="5"/>
+      <c r="BV30" s="5"/>
+      <c r="BW30" s="5"/>
+      <c r="BX30" s="5"/>
+      <c r="BY30" s="5"/>
+      <c r="BZ30" s="5"/>
+      <c r="CA30" s="5"/>
+      <c r="CB30" s="5"/>
+      <c r="CC30" s="5"/>
+      <c r="CD30" s="5"/>
+      <c r="CE30" s="5"/>
+      <c r="CF30" s="5"/>
+      <c r="CG30" s="5"/>
+      <c r="CH30" s="5"/>
+      <c r="CI30" s="5"/>
+      <c r="CJ30" s="5"/>
+    </row>
+    <row r="31" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
-        <v>132.15</v>
+        <v>130.19999999999999</v>
       </c>
       <c r="B31" s="12">
         <f t="shared" si="1"/>
@@ -13407,7 +14055,7 @@
       </c>
       <c r="C31" s="12">
         <f t="shared" si="2"/>
-        <v>24.699999999999989</v>
+        <v>26.650000000000006</v>
       </c>
       <c r="D31" s="45" t="s">
         <v>257</v>
@@ -13569,11 +14217,30 @@
       <c r="BS31" s="5">
         <v>132.15</v>
       </c>
-    </row>
-    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT31" s="5">
+        <v>130.19999999999999</v>
+      </c>
+      <c r="BU31" s="5"/>
+      <c r="BV31" s="5"/>
+      <c r="BW31" s="5"/>
+      <c r="BX31" s="5"/>
+      <c r="BY31" s="5"/>
+      <c r="BZ31" s="5"/>
+      <c r="CA31" s="5"/>
+      <c r="CB31" s="5"/>
+      <c r="CC31" s="5"/>
+      <c r="CD31" s="5"/>
+      <c r="CE31" s="5"/>
+      <c r="CF31" s="5"/>
+      <c r="CG31" s="5"/>
+      <c r="CH31" s="5"/>
+      <c r="CI31" s="5"/>
+      <c r="CJ31" s="5"/>
+    </row>
+    <row r="32" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <f t="shared" si="0"/>
-        <v>101.6</v>
+        <v>101.5</v>
       </c>
       <c r="B32" s="12">
         <f t="shared" si="1"/>
@@ -13581,7 +14248,7 @@
       </c>
       <c r="C32" s="12">
         <f t="shared" si="2"/>
-        <v>20.200000000000003</v>
+        <v>20.299999999999997</v>
       </c>
       <c r="D32" s="45" t="s">
         <v>268</v>
@@ -13731,8 +14398,27 @@
       <c r="BS32" s="5">
         <v>102</v>
       </c>
-    </row>
-    <row r="33" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT32" s="5">
+        <v>101.5</v>
+      </c>
+      <c r="BU32" s="5"/>
+      <c r="BV32" s="5"/>
+      <c r="BW32" s="5"/>
+      <c r="BX32" s="5"/>
+      <c r="BY32" s="5"/>
+      <c r="BZ32" s="5"/>
+      <c r="CA32" s="5"/>
+      <c r="CB32" s="5"/>
+      <c r="CC32" s="5"/>
+      <c r="CD32" s="5"/>
+      <c r="CE32" s="5"/>
+      <c r="CF32" s="5"/>
+      <c r="CG32" s="5"/>
+      <c r="CH32" s="5"/>
+      <c r="CI32" s="5"/>
+      <c r="CJ32" s="5"/>
+    </row>
+    <row r="33" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <f t="shared" si="0"/>
         <v>56.75</v>
@@ -13881,8 +14567,27 @@
       <c r="BS33" s="5">
         <v>60.4</v>
       </c>
-    </row>
-    <row r="34" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT33" s="5">
+        <v>60.85</v>
+      </c>
+      <c r="BU33" s="5"/>
+      <c r="BV33" s="5"/>
+      <c r="BW33" s="5"/>
+      <c r="BX33" s="5"/>
+      <c r="BY33" s="5"/>
+      <c r="BZ33" s="5"/>
+      <c r="CA33" s="5"/>
+      <c r="CB33" s="5"/>
+      <c r="CC33" s="5"/>
+      <c r="CD33" s="5"/>
+      <c r="CE33" s="5"/>
+      <c r="CF33" s="5"/>
+      <c r="CG33" s="5"/>
+      <c r="CH33" s="5"/>
+      <c r="CI33" s="5"/>
+      <c r="CJ33" s="5"/>
+    </row>
+    <row r="34" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <f t="shared" si="0"/>
         <v>167.9</v>
@@ -14025,8 +14730,27 @@
       <c r="BS34" s="5">
         <v>197.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT34" s="5">
+        <v>195.9</v>
+      </c>
+      <c r="BU34" s="5"/>
+      <c r="BV34" s="5"/>
+      <c r="BW34" s="5"/>
+      <c r="BX34" s="5"/>
+      <c r="BY34" s="5"/>
+      <c r="BZ34" s="5"/>
+      <c r="CA34" s="5"/>
+      <c r="CB34" s="5"/>
+      <c r="CC34" s="5"/>
+      <c r="CD34" s="5"/>
+      <c r="CE34" s="5"/>
+      <c r="CF34" s="5"/>
+      <c r="CG34" s="5"/>
+      <c r="CH34" s="5"/>
+      <c r="CI34" s="5"/>
+      <c r="CJ34" s="5"/>
+    </row>
+    <row r="35" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <f t="shared" si="0"/>
         <v>661</v>
@@ -14165,8 +14889,27 @@
       <c r="BS35" s="5">
         <v>686.8</v>
       </c>
-    </row>
-    <row r="36" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT35" s="5">
+        <v>686.8</v>
+      </c>
+      <c r="BU35" s="5"/>
+      <c r="BV35" s="5"/>
+      <c r="BW35" s="5"/>
+      <c r="BX35" s="5"/>
+      <c r="BY35" s="5"/>
+      <c r="BZ35" s="5"/>
+      <c r="CA35" s="5"/>
+      <c r="CB35" s="5"/>
+      <c r="CC35" s="5"/>
+      <c r="CD35" s="5"/>
+      <c r="CE35" s="5"/>
+      <c r="CF35" s="5"/>
+      <c r="CG35" s="5"/>
+      <c r="CH35" s="5"/>
+      <c r="CI35" s="5"/>
+      <c r="CJ35" s="5"/>
+    </row>
+    <row r="36" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <f t="shared" si="0"/>
         <v>402.9</v>
@@ -14287,8 +15030,27 @@
       <c r="BS36" s="5">
         <v>465</v>
       </c>
-    </row>
-    <row r="37" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT36" s="5">
+        <v>438.6</v>
+      </c>
+      <c r="BU36" s="5"/>
+      <c r="BV36" s="5"/>
+      <c r="BW36" s="5"/>
+      <c r="BX36" s="5"/>
+      <c r="BY36" s="5"/>
+      <c r="BZ36" s="5"/>
+      <c r="CA36" s="5"/>
+      <c r="CB36" s="5"/>
+      <c r="CC36" s="5"/>
+      <c r="CD36" s="5"/>
+      <c r="CE36" s="5"/>
+      <c r="CF36" s="5"/>
+      <c r="CG36" s="5"/>
+      <c r="CH36" s="5"/>
+      <c r="CI36" s="5"/>
+      <c r="CJ36" s="5"/>
+    </row>
+    <row r="37" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <f t="shared" si="0"/>
         <v>226</v>
@@ -14399,8 +15161,27 @@
       <c r="BS37" s="5">
         <v>396.85</v>
       </c>
-    </row>
-    <row r="38" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT37" s="5">
+        <v>382.9</v>
+      </c>
+      <c r="BU37" s="5"/>
+      <c r="BV37" s="5"/>
+      <c r="BW37" s="5"/>
+      <c r="BX37" s="5"/>
+      <c r="BY37" s="5"/>
+      <c r="BZ37" s="5"/>
+      <c r="CA37" s="5"/>
+      <c r="CB37" s="5"/>
+      <c r="CC37" s="5"/>
+      <c r="CD37" s="5"/>
+      <c r="CE37" s="5"/>
+      <c r="CF37" s="5"/>
+      <c r="CG37" s="5"/>
+      <c r="CH37" s="5"/>
+      <c r="CI37" s="5"/>
+      <c r="CJ37" s="5"/>
+    </row>
+    <row r="38" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <f t="shared" si="0"/>
         <v>485</v>
@@ -14509,8 +15290,27 @@
       <c r="BS38" s="5">
         <v>512</v>
       </c>
-    </row>
-    <row r="39" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT38" s="5">
+        <v>514</v>
+      </c>
+      <c r="BU38" s="5"/>
+      <c r="BV38" s="5"/>
+      <c r="BW38" s="5"/>
+      <c r="BX38" s="5"/>
+      <c r="BY38" s="5"/>
+      <c r="BZ38" s="5"/>
+      <c r="CA38" s="5"/>
+      <c r="CB38" s="5"/>
+      <c r="CC38" s="5"/>
+      <c r="CD38" s="5"/>
+      <c r="CE38" s="5"/>
+      <c r="CF38" s="5"/>
+      <c r="CG38" s="5"/>
+      <c r="CH38" s="5"/>
+      <c r="CI38" s="5"/>
+      <c r="CJ38" s="5"/>
+    </row>
+    <row r="39" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <f t="shared" si="0"/>
         <v>75.2</v>
@@ -14613,11 +15413,30 @@
       <c r="BS39" s="5">
         <v>77.25</v>
       </c>
-    </row>
-    <row r="40" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT39" s="5">
+        <v>76</v>
+      </c>
+      <c r="BU39" s="5"/>
+      <c r="BV39" s="5"/>
+      <c r="BW39" s="5"/>
+      <c r="BX39" s="5"/>
+      <c r="BY39" s="5"/>
+      <c r="BZ39" s="5"/>
+      <c r="CA39" s="5"/>
+      <c r="CB39" s="5"/>
+      <c r="CC39" s="5"/>
+      <c r="CD39" s="5"/>
+      <c r="CE39" s="5"/>
+      <c r="CF39" s="5"/>
+      <c r="CG39" s="5"/>
+      <c r="CH39" s="5"/>
+      <c r="CI39" s="5"/>
+      <c r="CJ39" s="5"/>
+    </row>
+    <row r="40" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <f t="shared" si="0"/>
-        <v>427</v>
+        <v>417.75</v>
       </c>
       <c r="B40" s="12">
         <f t="shared" si="1"/>
@@ -14625,7 +15444,7 @@
       </c>
       <c r="C40" s="12">
         <f t="shared" ref="C40" si="9">B40-A40</f>
-        <v>45</v>
+        <v>54.25</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>306</v>
@@ -14717,8 +15536,27 @@
       <c r="BS40" s="5">
         <v>427</v>
       </c>
-    </row>
-    <row r="41" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT40" s="5">
+        <v>417.75</v>
+      </c>
+      <c r="BU40" s="5"/>
+      <c r="BV40" s="5"/>
+      <c r="BW40" s="5"/>
+      <c r="BX40" s="5"/>
+      <c r="BY40" s="5"/>
+      <c r="BZ40" s="5"/>
+      <c r="CA40" s="5"/>
+      <c r="CB40" s="5"/>
+      <c r="CC40" s="5"/>
+      <c r="CD40" s="5"/>
+      <c r="CE40" s="5"/>
+      <c r="CF40" s="5"/>
+      <c r="CG40" s="5"/>
+      <c r="CH40" s="5"/>
+      <c r="CI40" s="5"/>
+      <c r="CJ40" s="5"/>
+    </row>
+    <row r="41" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <f t="shared" si="0"/>
         <v>192.65</v>
@@ -14817,11 +15655,30 @@
       <c r="BS41" s="5">
         <v>215.25</v>
       </c>
-    </row>
-    <row r="42" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT41" s="5">
+        <v>208.5</v>
+      </c>
+      <c r="BU41" s="5"/>
+      <c r="BV41" s="5"/>
+      <c r="BW41" s="5"/>
+      <c r="BX41" s="5"/>
+      <c r="BY41" s="5"/>
+      <c r="BZ41" s="5"/>
+      <c r="CA41" s="5"/>
+      <c r="CB41" s="5"/>
+      <c r="CC41" s="5"/>
+      <c r="CD41" s="5"/>
+      <c r="CE41" s="5"/>
+      <c r="CF41" s="5"/>
+      <c r="CG41" s="5"/>
+      <c r="CH41" s="5"/>
+      <c r="CI41" s="5"/>
+      <c r="CJ41" s="5"/>
+    </row>
+    <row r="42" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <f t="shared" si="0"/>
-        <v>36.4</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="B42" s="12">
         <f t="shared" si="1"/>
@@ -14829,7 +15686,7 @@
       </c>
       <c r="C42" s="12">
         <f t="shared" ref="C42:C45" si="11">B42-A42</f>
-        <v>2.25</v>
+        <v>3.3500000000000014</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>308</v>
@@ -14913,19 +15770,38 @@
       <c r="BS42" s="5">
         <v>36.4</v>
       </c>
-    </row>
-    <row r="43" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT42" s="5">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="BU42" s="5"/>
+      <c r="BV42" s="5"/>
+      <c r="BW42" s="5"/>
+      <c r="BX42" s="5"/>
+      <c r="BY42" s="5"/>
+      <c r="BZ42" s="5"/>
+      <c r="CA42" s="5"/>
+      <c r="CB42" s="5"/>
+      <c r="CC42" s="5"/>
+      <c r="CD42" s="5"/>
+      <c r="CE42" s="5"/>
+      <c r="CF42" s="5"/>
+      <c r="CG42" s="5"/>
+      <c r="CH42" s="5"/>
+      <c r="CI42" s="5"/>
+      <c r="CJ42" s="5"/>
+    </row>
+    <row r="43" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <f t="shared" si="0"/>
         <v>577.45000000000005</v>
       </c>
       <c r="B43" s="12">
         <f t="shared" ref="B43:B44" si="12">MAX(E43:ZW43)</f>
-        <v>616.15</v>
+        <v>619</v>
       </c>
       <c r="C43" s="12">
         <f t="shared" si="11"/>
-        <v>38.699999999999932</v>
+        <v>41.549999999999955</v>
       </c>
       <c r="D43" s="45" t="s">
         <v>309</v>
@@ -15007,8 +15883,27 @@
       <c r="BS43" s="5">
         <v>616.15</v>
       </c>
-    </row>
-    <row r="44" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT43" s="5">
+        <v>619</v>
+      </c>
+      <c r="BU43" s="5"/>
+      <c r="BV43" s="5"/>
+      <c r="BW43" s="5"/>
+      <c r="BX43" s="5"/>
+      <c r="BY43" s="5"/>
+      <c r="BZ43" s="5"/>
+      <c r="CA43" s="5"/>
+      <c r="CB43" s="5"/>
+      <c r="CC43" s="5"/>
+      <c r="CD43" s="5"/>
+      <c r="CE43" s="5"/>
+      <c r="CF43" s="5"/>
+      <c r="CG43" s="5"/>
+      <c r="CH43" s="5"/>
+      <c r="CI43" s="5"/>
+      <c r="CJ43" s="5"/>
+    </row>
+    <row r="44" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <f t="shared" si="0"/>
         <v>826</v>
@@ -15101,8 +15996,27 @@
       <c r="BS44" s="5">
         <v>826</v>
       </c>
-    </row>
-    <row r="45" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT44" s="5">
+        <v>835</v>
+      </c>
+      <c r="BU44" s="5"/>
+      <c r="BV44" s="5"/>
+      <c r="BW44" s="5"/>
+      <c r="BX44" s="5"/>
+      <c r="BY44" s="5"/>
+      <c r="BZ44" s="5"/>
+      <c r="CA44" s="5"/>
+      <c r="CB44" s="5"/>
+      <c r="CC44" s="5"/>
+      <c r="CD44" s="5"/>
+      <c r="CE44" s="5"/>
+      <c r="CF44" s="5"/>
+      <c r="CG44" s="5"/>
+      <c r="CH44" s="5"/>
+      <c r="CI44" s="5"/>
+      <c r="CJ44" s="5"/>
+    </row>
+    <row r="45" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <f t="shared" si="0"/>
         <v>137.9</v>
@@ -15193,19 +16107,38 @@
       <c r="BS45" s="5">
         <v>137.9</v>
       </c>
-    </row>
-    <row r="46" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT45" s="5">
+        <v>140.25</v>
+      </c>
+      <c r="BU45" s="5"/>
+      <c r="BV45" s="5"/>
+      <c r="BW45" s="5"/>
+      <c r="BX45" s="5"/>
+      <c r="BY45" s="5"/>
+      <c r="BZ45" s="5"/>
+      <c r="CA45" s="5"/>
+      <c r="CB45" s="5"/>
+      <c r="CC45" s="5"/>
+      <c r="CD45" s="5"/>
+      <c r="CE45" s="5"/>
+      <c r="CF45" s="5"/>
+      <c r="CG45" s="5"/>
+      <c r="CH45" s="5"/>
+      <c r="CI45" s="5"/>
+      <c r="CJ45" s="5"/>
+    </row>
+    <row r="46" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <f t="shared" ref="A46" si="13">MIN(E46:ZW46)</f>
-        <v>723.2</v>
+        <v>696</v>
       </c>
       <c r="B46" s="12">
         <f>MAX(E46:ZW46)</f>
-        <v>723.2</v>
+        <v>770</v>
       </c>
       <c r="C46" s="12">
         <f t="shared" ref="C46" si="14">B46-A46</f>
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="D46" s="45" t="s">
         <v>313</v>
@@ -15277,8 +16210,132 @@
       <c r="BQ46" s="5"/>
       <c r="BR46" s="5"/>
       <c r="BS46" s="5">
-        <v>723.2</v>
-      </c>
+        <v>770</v>
+      </c>
+      <c r="BT46" s="5">
+        <v>696</v>
+      </c>
+      <c r="BU46" s="5"/>
+      <c r="BV46" s="5"/>
+      <c r="BW46" s="5"/>
+      <c r="BX46" s="5"/>
+      <c r="BY46" s="5"/>
+      <c r="BZ46" s="5"/>
+      <c r="CA46" s="5"/>
+      <c r="CB46" s="5"/>
+      <c r="CC46" s="5"/>
+      <c r="CD46" s="5"/>
+      <c r="CE46" s="5"/>
+      <c r="CF46" s="5"/>
+      <c r="CG46" s="5"/>
+      <c r="CH46" s="5"/>
+      <c r="CI46" s="5"/>
+      <c r="CJ46" s="5"/>
+    </row>
+    <row r="47" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A47" s="12">
+        <f t="shared" ref="A47" si="15">MIN(E47:ZW47)</f>
+        <v>783.15</v>
+      </c>
+      <c r="B47" s="12">
+        <f>MAX(E47:ZW47)</f>
+        <v>790</v>
+      </c>
+      <c r="C47" s="12">
+        <f t="shared" ref="C47" si="16">B47-A47</f>
+        <v>6.8500000000000227</v>
+      </c>
+      <c r="D47" s="45" t="s">
+        <v>328</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="5"/>
+      <c r="V47" s="5"/>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5"/>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5"/>
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="5"/>
+      <c r="AC47" s="5"/>
+      <c r="AD47" s="5"/>
+      <c r="AE47" s="5"/>
+      <c r="AF47" s="5"/>
+      <c r="AG47" s="5"/>
+      <c r="AH47" s="5"/>
+      <c r="AI47" s="5"/>
+      <c r="AJ47" s="5"/>
+      <c r="AK47" s="5"/>
+      <c r="AL47" s="5"/>
+      <c r="AM47" s="5"/>
+      <c r="AN47" s="5"/>
+      <c r="AO47" s="5"/>
+      <c r="AP47" s="5"/>
+      <c r="AQ47" s="5"/>
+      <c r="AR47" s="5"/>
+      <c r="AS47" s="5"/>
+      <c r="AT47" s="5"/>
+      <c r="AU47" s="5"/>
+      <c r="AV47" s="5"/>
+      <c r="AW47" s="5"/>
+      <c r="AX47" s="5"/>
+      <c r="AY47" s="5"/>
+      <c r="AZ47" s="5"/>
+      <c r="BA47" s="5"/>
+      <c r="BB47" s="5"/>
+      <c r="BC47" s="5"/>
+      <c r="BD47" s="5"/>
+      <c r="BE47" s="5"/>
+      <c r="BF47" s="5"/>
+      <c r="BG47" s="5"/>
+      <c r="BH47" s="5"/>
+      <c r="BI47" s="5"/>
+      <c r="BJ47" s="5"/>
+      <c r="BK47" s="5"/>
+      <c r="BL47" s="5"/>
+      <c r="BM47" s="5"/>
+      <c r="BN47" s="5"/>
+      <c r="BO47" s="5"/>
+      <c r="BP47" s="5"/>
+      <c r="BQ47" s="5"/>
+      <c r="BR47" s="5"/>
+      <c r="BS47" s="5">
+        <v>790</v>
+      </c>
+      <c r="BT47" s="5">
+        <v>783.15</v>
+      </c>
+      <c r="BU47" s="5"/>
+      <c r="BV47" s="5"/>
+      <c r="BW47" s="5"/>
+      <c r="BX47" s="5"/>
+      <c r="BY47" s="5"/>
+      <c r="BZ47" s="5"/>
+      <c r="CA47" s="5"/>
+      <c r="CB47" s="5"/>
+      <c r="CC47" s="5"/>
+      <c r="CD47" s="5"/>
+      <c r="CE47" s="5"/>
+      <c r="CF47" s="5"/>
+      <c r="CG47" s="5"/>
+      <c r="CH47" s="5"/>
+      <c r="CI47" s="5"/>
+      <c r="CJ47" s="5"/>
     </row>
   </sheetData>
   <sortState ref="L1:L37">
@@ -16503,10 +17560,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R42" sqref="R42"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16551,7 +17608,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(B2:B200)</f>
-        <v>1047233</v>
+        <v>1102233</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -16569,7 +17626,7 @@
       </c>
       <c r="F3" s="5">
         <f>F1-F2</f>
-        <v>428156</v>
+        <v>373156</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -17180,6 +18237,28 @@
       </c>
       <c r="C43" s="31">
         <v>43037</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="39" t="s">
+        <v>314</v>
+      </c>
+      <c r="B44" s="12">
+        <v>15000</v>
+      </c>
+      <c r="C44" s="31">
+        <v>43053</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="12">
+        <v>40000</v>
+      </c>
+      <c r="C45" s="31">
+        <v>43040</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added details for 15/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -7259,9 +7259,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CJ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="BP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BT1" sqref="BT1"/>
+      <selection pane="topRight" activeCell="BU46" sqref="BU46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7783,7 +7783,9 @@
       <c r="BT2" s="5">
         <v>329.05</v>
       </c>
-      <c r="BU2" s="5"/>
+      <c r="BU2" s="5">
+        <v>326.10000000000002</v>
+      </c>
       <c r="BV2" s="5"/>
       <c r="BW2" s="5"/>
       <c r="BX2" s="5"/>
@@ -8012,7 +8014,9 @@
       <c r="BT3" s="5">
         <v>313.55</v>
       </c>
-      <c r="BU3" s="5"/>
+      <c r="BU3" s="5">
+        <v>315.60000000000002</v>
+      </c>
       <c r="BV3" s="5"/>
       <c r="BW3" s="5"/>
       <c r="BX3" s="5"/>
@@ -8032,7 +8036,7 @@
     <row r="4" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
-        <v>256.25</v>
+        <v>253.85</v>
       </c>
       <c r="B4" s="12">
         <f t="shared" si="1"/>
@@ -8040,7 +8044,7 @@
       </c>
       <c r="C4" s="12">
         <f t="shared" si="2"/>
-        <v>35.449999999999989</v>
+        <v>37.849999999999994</v>
       </c>
       <c r="D4" s="44" t="s">
         <v>25</v>
@@ -8247,7 +8251,9 @@
       <c r="BT4" s="5">
         <v>256.25</v>
       </c>
-      <c r="BU4" s="5"/>
+      <c r="BU4" s="5">
+        <v>253.85</v>
+      </c>
       <c r="BV4" s="5"/>
       <c r="BW4" s="5"/>
       <c r="BX4" s="5"/>
@@ -8482,7 +8488,9 @@
       <c r="BT5" s="5">
         <v>887.5</v>
       </c>
-      <c r="BU5" s="5"/>
+      <c r="BU5" s="5">
+        <v>883.25</v>
+      </c>
       <c r="BV5" s="5"/>
       <c r="BW5" s="5"/>
       <c r="BX5" s="5"/>
@@ -8717,7 +8725,9 @@
       <c r="BT6" s="5">
         <v>275.2</v>
       </c>
-      <c r="BU6" s="5"/>
+      <c r="BU6" s="5">
+        <v>272.75</v>
+      </c>
       <c r="BV6" s="5"/>
       <c r="BW6" s="5"/>
       <c r="BX6" s="5"/>
@@ -8952,7 +8962,9 @@
       <c r="BT7" s="5">
         <v>17.8</v>
       </c>
-      <c r="BU7" s="5"/>
+      <c r="BU7" s="5">
+        <v>16.3</v>
+      </c>
       <c r="BV7" s="5"/>
       <c r="BW7" s="5"/>
       <c r="BX7" s="5"/>
@@ -9187,7 +9199,9 @@
       <c r="BT8" s="5">
         <v>79.849999999999994</v>
       </c>
-      <c r="BU8" s="5"/>
+      <c r="BU8" s="5">
+        <v>76.2</v>
+      </c>
       <c r="BV8" s="5"/>
       <c r="BW8" s="5"/>
       <c r="BX8" s="5"/>
@@ -9414,7 +9428,9 @@
       <c r="BT9" s="28">
         <v>55.25</v>
       </c>
-      <c r="BU9" s="28"/>
+      <c r="BU9" s="28">
+        <v>54.7</v>
+      </c>
       <c r="BV9" s="28"/>
       <c r="BW9" s="28"/>
       <c r="BX9" s="28"/>
@@ -9434,7 +9450,7 @@
     <row r="10" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <f t="shared" si="0"/>
-        <v>38.6</v>
+        <v>35.549999999999997</v>
       </c>
       <c r="B10" s="12">
         <f t="shared" si="1"/>
@@ -9442,7 +9458,7 @@
       </c>
       <c r="C10" s="12">
         <f t="shared" si="2"/>
-        <v>6.75</v>
+        <v>9.8000000000000043</v>
       </c>
       <c r="D10" s="45" t="s">
         <v>15</v>
@@ -9649,7 +9665,9 @@
       <c r="BT10" s="5">
         <v>38.6</v>
       </c>
-      <c r="BU10" s="5"/>
+      <c r="BU10" s="5">
+        <v>35.549999999999997</v>
+      </c>
       <c r="BV10" s="5"/>
       <c r="BW10" s="5"/>
       <c r="BX10" s="5"/>
@@ -9884,7 +9902,9 @@
       <c r="BT11" s="5">
         <v>92.55</v>
       </c>
-      <c r="BU11" s="5"/>
+      <c r="BU11" s="5">
+        <v>93.55</v>
+      </c>
       <c r="BV11" s="5"/>
       <c r="BW11" s="5"/>
       <c r="BX11" s="5"/>
@@ -10119,7 +10139,9 @@
       <c r="BT12" s="5">
         <v>91.4</v>
       </c>
-      <c r="BU12" s="5"/>
+      <c r="BU12" s="5">
+        <v>88.2</v>
+      </c>
       <c r="BV12" s="5"/>
       <c r="BW12" s="5"/>
       <c r="BX12" s="5"/>
@@ -10354,7 +10376,9 @@
       <c r="BT13" s="5">
         <v>48</v>
       </c>
-      <c r="BU13" s="5"/>
+      <c r="BU13" s="5">
+        <v>47.4</v>
+      </c>
       <c r="BV13" s="5"/>
       <c r="BW13" s="5"/>
       <c r="BX13" s="5"/>
@@ -10589,7 +10613,9 @@
       <c r="BT14" s="5">
         <v>36.1</v>
       </c>
-      <c r="BU14" s="5"/>
+      <c r="BU14" s="5">
+        <v>34.799999999999997</v>
+      </c>
       <c r="BV14" s="5"/>
       <c r="BW14" s="5"/>
       <c r="BX14" s="5"/>
@@ -10609,7 +10635,7 @@
     <row r="15" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
-        <v>25.15</v>
+        <v>24.85</v>
       </c>
       <c r="B15" s="12">
         <f t="shared" si="1"/>
@@ -10617,7 +10643,7 @@
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
-        <v>11.25</v>
+        <v>11.549999999999997</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>126</v>
@@ -10816,7 +10842,9 @@
       <c r="BT15" s="5">
         <v>25.15</v>
       </c>
-      <c r="BU15" s="5"/>
+      <c r="BU15" s="5">
+        <v>24.85</v>
+      </c>
       <c r="BV15" s="5"/>
       <c r="BW15" s="5"/>
       <c r="BX15" s="5"/>
@@ -11051,7 +11079,9 @@
       <c r="BT16" s="5">
         <v>682.8</v>
       </c>
-      <c r="BU16" s="5"/>
+      <c r="BU16" s="5">
+        <v>679</v>
+      </c>
       <c r="BV16" s="5"/>
       <c r="BW16" s="5"/>
       <c r="BX16" s="5"/>
@@ -11286,7 +11316,9 @@
       <c r="BT17" s="5">
         <v>471.2</v>
       </c>
-      <c r="BU17" s="5"/>
+      <c r="BU17" s="5">
+        <v>467</v>
+      </c>
       <c r="BV17" s="5"/>
       <c r="BW17" s="5"/>
       <c r="BX17" s="5"/>
@@ -11521,7 +11553,9 @@
       <c r="BT18" s="5">
         <v>275.2</v>
       </c>
-      <c r="BU18" s="5"/>
+      <c r="BU18" s="5">
+        <v>261.60000000000002</v>
+      </c>
       <c r="BV18" s="5"/>
       <c r="BW18" s="5"/>
       <c r="BX18" s="5"/>
@@ -11756,7 +11790,9 @@
       <c r="BT19" s="5">
         <v>648.15</v>
       </c>
-      <c r="BU19" s="5"/>
+      <c r="BU19" s="5">
+        <v>646</v>
+      </c>
       <c r="BV19" s="5"/>
       <c r="BW19" s="5"/>
       <c r="BX19" s="5"/>
@@ -11991,7 +12027,9 @@
       <c r="BT20" s="5">
         <v>699</v>
       </c>
-      <c r="BU20" s="5"/>
+      <c r="BU20" s="5">
+        <v>698</v>
+      </c>
       <c r="BV20" s="5"/>
       <c r="BW20" s="5"/>
       <c r="BX20" s="5"/>
@@ -12226,7 +12264,9 @@
       <c r="BT21" s="5">
         <v>498</v>
       </c>
-      <c r="BU21" s="5"/>
+      <c r="BU21" s="5">
+        <v>488.95</v>
+      </c>
       <c r="BV21" s="5"/>
       <c r="BW21" s="5"/>
       <c r="BX21" s="5"/>
@@ -12407,7 +12447,9 @@
       <c r="BT22" s="5">
         <v>388</v>
       </c>
-      <c r="BU22" s="5"/>
+      <c r="BU22" s="5">
+        <v>382.3</v>
+      </c>
       <c r="BV22" s="5"/>
       <c r="BW22" s="5"/>
       <c r="BX22" s="5"/>
@@ -12634,7 +12676,9 @@
       <c r="BT23" s="5">
         <v>58.3</v>
       </c>
-      <c r="BU23" s="5"/>
+      <c r="BU23" s="5">
+        <v>57.35</v>
+      </c>
       <c r="BV23" s="5"/>
       <c r="BW23" s="5"/>
       <c r="BX23" s="5"/>
@@ -12857,7 +12901,9 @@
       <c r="BT24" s="5">
         <v>237.4</v>
       </c>
-      <c r="BU24" s="5"/>
+      <c r="BU24" s="5">
+        <v>237.3</v>
+      </c>
       <c r="BV24" s="5"/>
       <c r="BW24" s="5"/>
       <c r="BX24" s="5"/>
@@ -13062,7 +13108,9 @@
       <c r="BT25" s="5">
         <v>949.1</v>
       </c>
-      <c r="BU25" s="5"/>
+      <c r="BU25" s="5">
+        <v>950.75</v>
+      </c>
       <c r="BV25" s="5"/>
       <c r="BW25" s="5"/>
       <c r="BX25" s="5"/>
@@ -13255,7 +13303,9 @@
       <c r="BT26" s="5">
         <v>92.05</v>
       </c>
-      <c r="BU26" s="5"/>
+      <c r="BU26" s="5">
+        <v>92.25</v>
+      </c>
       <c r="BV26" s="5"/>
       <c r="BW26" s="5"/>
       <c r="BX26" s="5"/>
@@ -13275,7 +13325,7 @@
     <row r="27" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <f t="shared" si="0"/>
-        <v>37.549999999999997</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="B27" s="12">
         <f t="shared" si="1"/>
@@ -13283,7 +13333,7 @@
       </c>
       <c r="C27" s="12">
         <f t="shared" si="2"/>
-        <v>7.2000000000000028</v>
+        <v>8.5499999999999972</v>
       </c>
       <c r="D27" s="45" t="s">
         <v>253</v>
@@ -13448,7 +13498,9 @@
       <c r="BT27" s="5">
         <v>37.549999999999997</v>
       </c>
-      <c r="BU27" s="5"/>
+      <c r="BU27" s="5">
+        <v>36.200000000000003</v>
+      </c>
       <c r="BV27" s="5"/>
       <c r="BW27" s="5"/>
       <c r="BX27" s="5"/>
@@ -13641,7 +13693,9 @@
       <c r="BT28" s="5">
         <v>120.3</v>
       </c>
-      <c r="BU28" s="5"/>
+      <c r="BU28" s="5">
+        <v>121</v>
+      </c>
       <c r="BV28" s="5"/>
       <c r="BW28" s="5"/>
       <c r="BX28" s="5"/>
@@ -13834,7 +13888,9 @@
       <c r="BT29" s="5">
         <v>65.75</v>
       </c>
-      <c r="BU29" s="5"/>
+      <c r="BU29" s="5">
+        <v>64.2</v>
+      </c>
       <c r="BV29" s="5"/>
       <c r="BW29" s="5"/>
       <c r="BX29" s="5"/>
@@ -14027,7 +14083,9 @@
       <c r="BT30" s="5">
         <v>41.85</v>
       </c>
-      <c r="BU30" s="5"/>
+      <c r="BU30" s="5">
+        <v>40.25</v>
+      </c>
       <c r="BV30" s="5"/>
       <c r="BW30" s="5"/>
       <c r="BX30" s="5"/>
@@ -14220,7 +14278,9 @@
       <c r="BT31" s="5">
         <v>130.19999999999999</v>
       </c>
-      <c r="BU31" s="5"/>
+      <c r="BU31" s="5">
+        <v>139.85</v>
+      </c>
       <c r="BV31" s="5"/>
       <c r="BW31" s="5"/>
       <c r="BX31" s="5"/>
@@ -14240,7 +14300,7 @@
     <row r="32" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <f t="shared" si="0"/>
-        <v>101.5</v>
+        <v>96.65</v>
       </c>
       <c r="B32" s="12">
         <f t="shared" si="1"/>
@@ -14248,7 +14308,7 @@
       </c>
       <c r="C32" s="12">
         <f t="shared" si="2"/>
-        <v>20.299999999999997</v>
+        <v>25.149999999999991</v>
       </c>
       <c r="D32" s="45" t="s">
         <v>268</v>
@@ -14401,7 +14461,9 @@
       <c r="BT32" s="5">
         <v>101.5</v>
       </c>
-      <c r="BU32" s="5"/>
+      <c r="BU32" s="5">
+        <v>96.65</v>
+      </c>
       <c r="BV32" s="5"/>
       <c r="BW32" s="5"/>
       <c r="BX32" s="5"/>
@@ -14570,7 +14632,9 @@
       <c r="BT33" s="5">
         <v>60.85</v>
       </c>
-      <c r="BU33" s="5"/>
+      <c r="BU33" s="5">
+        <v>59.75</v>
+      </c>
       <c r="BV33" s="5"/>
       <c r="BW33" s="5"/>
       <c r="BX33" s="5"/>
@@ -14733,7 +14797,9 @@
       <c r="BT34" s="5">
         <v>195.9</v>
       </c>
-      <c r="BU34" s="5"/>
+      <c r="BU34" s="5">
+        <v>185.75</v>
+      </c>
       <c r="BV34" s="5"/>
       <c r="BW34" s="5"/>
       <c r="BX34" s="5"/>
@@ -14892,7 +14958,9 @@
       <c r="BT35" s="5">
         <v>686.8</v>
       </c>
-      <c r="BU35" s="5"/>
+      <c r="BU35" s="5">
+        <v>686</v>
+      </c>
       <c r="BV35" s="5"/>
       <c r="BW35" s="5"/>
       <c r="BX35" s="5"/>
@@ -15033,7 +15101,9 @@
       <c r="BT36" s="5">
         <v>438.6</v>
       </c>
-      <c r="BU36" s="5"/>
+      <c r="BU36" s="5">
+        <v>416.7</v>
+      </c>
       <c r="BV36" s="5"/>
       <c r="BW36" s="5"/>
       <c r="BX36" s="5"/>
@@ -15164,7 +15234,9 @@
       <c r="BT37" s="5">
         <v>382.9</v>
       </c>
-      <c r="BU37" s="5"/>
+      <c r="BU37" s="5">
+        <v>365.7</v>
+      </c>
       <c r="BV37" s="5"/>
       <c r="BW37" s="5"/>
       <c r="BX37" s="5"/>
@@ -15293,7 +15365,9 @@
       <c r="BT38" s="5">
         <v>514</v>
       </c>
-      <c r="BU38" s="5"/>
+      <c r="BU38" s="5">
+        <v>505.35</v>
+      </c>
       <c r="BV38" s="5"/>
       <c r="BW38" s="5"/>
       <c r="BX38" s="5"/>
@@ -15416,7 +15490,9 @@
       <c r="BT39" s="5">
         <v>76</v>
       </c>
-      <c r="BU39" s="5"/>
+      <c r="BU39" s="5">
+        <v>76.400000000000006</v>
+      </c>
       <c r="BV39" s="5"/>
       <c r="BW39" s="5"/>
       <c r="BX39" s="5"/>
@@ -15539,7 +15615,9 @@
       <c r="BT40" s="5">
         <v>417.75</v>
       </c>
-      <c r="BU40" s="5"/>
+      <c r="BU40" s="5">
+        <v>424.9</v>
+      </c>
       <c r="BV40" s="5"/>
       <c r="BW40" s="5"/>
       <c r="BX40" s="5"/>
@@ -15658,7 +15736,9 @@
       <c r="BT41" s="5">
         <v>208.5</v>
       </c>
-      <c r="BU41" s="5"/>
+      <c r="BU41" s="5">
+        <v>198.3</v>
+      </c>
       <c r="BV41" s="5"/>
       <c r="BW41" s="5"/>
       <c r="BX41" s="5"/>
@@ -15678,7 +15758,7 @@
     <row r="42" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <f t="shared" si="0"/>
-        <v>35.299999999999997</v>
+        <v>35</v>
       </c>
       <c r="B42" s="12">
         <f t="shared" si="1"/>
@@ -15686,7 +15766,7 @@
       </c>
       <c r="C42" s="12">
         <f t="shared" ref="C42:C45" si="11">B42-A42</f>
-        <v>3.3500000000000014</v>
+        <v>3.6499999999999986</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>308</v>
@@ -15773,7 +15853,9 @@
       <c r="BT42" s="5">
         <v>35.299999999999997</v>
       </c>
-      <c r="BU42" s="5"/>
+      <c r="BU42" s="5">
+        <v>35</v>
+      </c>
       <c r="BV42" s="5"/>
       <c r="BW42" s="5"/>
       <c r="BX42" s="5"/>
@@ -15886,7 +15968,9 @@
       <c r="BT43" s="5">
         <v>619</v>
       </c>
-      <c r="BU43" s="5"/>
+      <c r="BU43" s="5">
+        <v>610</v>
+      </c>
       <c r="BV43" s="5"/>
       <c r="BW43" s="5"/>
       <c r="BX43" s="5"/>
@@ -15906,7 +15990,7 @@
     <row r="44" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <f t="shared" si="0"/>
-        <v>826</v>
+        <v>822.95</v>
       </c>
       <c r="B44" s="12">
         <f t="shared" si="12"/>
@@ -15914,7 +15998,7 @@
       </c>
       <c r="C44" s="12">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>33.049999999999955</v>
       </c>
       <c r="D44" s="45" t="s">
         <v>310</v>
@@ -15999,7 +16083,9 @@
       <c r="BT44" s="5">
         <v>835</v>
       </c>
-      <c r="BU44" s="5"/>
+      <c r="BU44" s="5">
+        <v>822.95</v>
+      </c>
       <c r="BV44" s="5"/>
       <c r="BW44" s="5"/>
       <c r="BX44" s="5"/>
@@ -16019,7 +16105,7 @@
     <row r="45" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <f t="shared" si="0"/>
-        <v>137.9</v>
+        <v>134.9</v>
       </c>
       <c r="B45" s="12">
         <f>MAX(E45:ZW45)</f>
@@ -16027,7 +16113,7 @@
       </c>
       <c r="C45" s="12">
         <f t="shared" si="11"/>
-        <v>8.0999999999999943</v>
+        <v>11.099999999999994</v>
       </c>
       <c r="D45" s="45" t="s">
         <v>311</v>
@@ -16110,7 +16196,9 @@
       <c r="BT45" s="5">
         <v>140.25</v>
       </c>
-      <c r="BU45" s="5"/>
+      <c r="BU45" s="5">
+        <v>134.9</v>
+      </c>
       <c r="BV45" s="5"/>
       <c r="BW45" s="5"/>
       <c r="BX45" s="5"/>
@@ -16130,7 +16218,7 @@
     <row r="46" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <f t="shared" ref="A46" si="13">MIN(E46:ZW46)</f>
-        <v>696</v>
+        <v>680.25</v>
       </c>
       <c r="B46" s="12">
         <f>MAX(E46:ZW46)</f>
@@ -16138,7 +16226,7 @@
       </c>
       <c r="C46" s="12">
         <f t="shared" ref="C46" si="14">B46-A46</f>
-        <v>74</v>
+        <v>89.75</v>
       </c>
       <c r="D46" s="45" t="s">
         <v>313</v>
@@ -16215,7 +16303,9 @@
       <c r="BT46" s="5">
         <v>696</v>
       </c>
-      <c r="BU46" s="5"/>
+      <c r="BU46" s="5">
+        <v>680.25</v>
+      </c>
       <c r="BV46" s="5"/>
       <c r="BW46" s="5"/>
       <c r="BX46" s="5"/>
@@ -16235,7 +16325,7 @@
     <row r="47" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <f t="shared" ref="A47" si="15">MIN(E47:ZW47)</f>
-        <v>783.15</v>
+        <v>776.5</v>
       </c>
       <c r="B47" s="12">
         <f>MAX(E47:ZW47)</f>
@@ -16243,7 +16333,7 @@
       </c>
       <c r="C47" s="12">
         <f t="shared" ref="C47" si="16">B47-A47</f>
-        <v>6.8500000000000227</v>
+        <v>13.5</v>
       </c>
       <c r="D47" s="45" t="s">
         <v>328</v>
@@ -16320,7 +16410,9 @@
       <c r="BT47" s="5">
         <v>783.15</v>
       </c>
-      <c r="BU47" s="5"/>
+      <c r="BU47" s="5">
+        <v>776.5</v>
+      </c>
       <c r="BV47" s="5"/>
       <c r="BW47" s="5"/>
       <c r="BX47" s="5"/>

</xml_diff>

<commit_message>
Added details for 16/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -7259,9 +7259,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CJ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="BP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BU46" sqref="BU46"/>
+      <selection pane="topRight" activeCell="BV47" sqref="BV47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7578,11 +7578,11 @@
       </c>
       <c r="B2" s="12">
         <f t="shared" ref="B2:B42" si="1">MAX(E2:ZW2)</f>
-        <v>333.8</v>
+        <v>333.95</v>
       </c>
       <c r="C2" s="12">
         <f>B2-A2</f>
-        <v>90.200000000000017</v>
+        <v>90.35</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>115</v>
@@ -7786,7 +7786,9 @@
       <c r="BU2" s="5">
         <v>326.10000000000002</v>
       </c>
-      <c r="BV2" s="5"/>
+      <c r="BV2" s="5">
+        <v>333.95</v>
+      </c>
       <c r="BW2" s="5"/>
       <c r="BX2" s="5"/>
       <c r="BY2" s="5"/>
@@ -7809,11 +7811,11 @@
       </c>
       <c r="B3" s="12">
         <f t="shared" si="1"/>
-        <v>318.3</v>
+        <v>318.55</v>
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C33" si="2">B3-A3</f>
-        <v>55.600000000000023</v>
+        <v>55.850000000000023</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>114</v>
@@ -8017,7 +8019,9 @@
       <c r="BU3" s="5">
         <v>315.60000000000002</v>
       </c>
-      <c r="BV3" s="5"/>
+      <c r="BV3" s="5">
+        <v>318.55</v>
+      </c>
       <c r="BW3" s="5"/>
       <c r="BX3" s="5"/>
       <c r="BY3" s="5"/>
@@ -8254,7 +8258,9 @@
       <c r="BU4" s="5">
         <v>253.85</v>
       </c>
-      <c r="BV4" s="5"/>
+      <c r="BV4" s="5">
+        <v>255</v>
+      </c>
       <c r="BW4" s="5"/>
       <c r="BX4" s="5"/>
       <c r="BY4" s="5"/>
@@ -8491,7 +8497,9 @@
       <c r="BU5" s="5">
         <v>883.25</v>
       </c>
-      <c r="BV5" s="5"/>
+      <c r="BV5" s="5">
+        <v>905.25</v>
+      </c>
       <c r="BW5" s="5"/>
       <c r="BX5" s="5"/>
       <c r="BY5" s="5"/>
@@ -8728,7 +8736,9 @@
       <c r="BU6" s="5">
         <v>272.75</v>
       </c>
-      <c r="BV6" s="5"/>
+      <c r="BV6" s="5">
+        <v>269</v>
+      </c>
       <c r="BW6" s="5"/>
       <c r="BX6" s="5"/>
       <c r="BY6" s="5"/>
@@ -8965,7 +8975,9 @@
       <c r="BU7" s="5">
         <v>16.3</v>
       </c>
-      <c r="BV7" s="5"/>
+      <c r="BV7" s="5">
+        <v>16.95</v>
+      </c>
       <c r="BW7" s="5"/>
       <c r="BX7" s="5"/>
       <c r="BY7" s="5"/>
@@ -9202,7 +9214,9 @@
       <c r="BU8" s="5">
         <v>76.2</v>
       </c>
-      <c r="BV8" s="5"/>
+      <c r="BV8" s="5">
+        <v>77.400000000000006</v>
+      </c>
       <c r="BW8" s="5"/>
       <c r="BX8" s="5"/>
       <c r="BY8" s="5"/>
@@ -9431,7 +9445,9 @@
       <c r="BU9" s="28">
         <v>54.7</v>
       </c>
-      <c r="BV9" s="28"/>
+      <c r="BV9" s="28">
+        <v>54.25</v>
+      </c>
       <c r="BW9" s="28"/>
       <c r="BX9" s="28"/>
       <c r="BY9" s="28"/>
@@ -9668,7 +9684,9 @@
       <c r="BU10" s="5">
         <v>35.549999999999997</v>
       </c>
-      <c r="BV10" s="5"/>
+      <c r="BV10" s="5">
+        <v>36.9</v>
+      </c>
       <c r="BW10" s="5"/>
       <c r="BX10" s="5"/>
       <c r="BY10" s="5"/>
@@ -9905,7 +9923,9 @@
       <c r="BU11" s="5">
         <v>93.55</v>
       </c>
-      <c r="BV11" s="5"/>
+      <c r="BV11" s="5">
+        <v>95.9</v>
+      </c>
       <c r="BW11" s="5"/>
       <c r="BX11" s="5"/>
       <c r="BY11" s="5"/>
@@ -10142,7 +10162,9 @@
       <c r="BU12" s="5">
         <v>88.2</v>
       </c>
-      <c r="BV12" s="5"/>
+      <c r="BV12" s="5">
+        <v>87.75</v>
+      </c>
       <c r="BW12" s="5"/>
       <c r="BX12" s="5"/>
       <c r="BY12" s="5"/>
@@ -10379,7 +10401,9 @@
       <c r="BU13" s="5">
         <v>47.4</v>
       </c>
-      <c r="BV13" s="5"/>
+      <c r="BV13" s="5">
+        <v>47.45</v>
+      </c>
       <c r="BW13" s="5"/>
       <c r="BX13" s="5"/>
       <c r="BY13" s="5"/>
@@ -10616,7 +10640,9 @@
       <c r="BU14" s="5">
         <v>34.799999999999997</v>
       </c>
-      <c r="BV14" s="5"/>
+      <c r="BV14" s="5">
+        <v>34.4</v>
+      </c>
       <c r="BW14" s="5"/>
       <c r="BX14" s="5"/>
       <c r="BY14" s="5"/>
@@ -10635,7 +10661,7 @@
     <row r="15" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
-        <v>24.85</v>
+        <v>24.5</v>
       </c>
       <c r="B15" s="12">
         <f t="shared" si="1"/>
@@ -10643,7 +10669,7 @@
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
-        <v>11.549999999999997</v>
+        <v>11.899999999999999</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>126</v>
@@ -10845,7 +10871,9 @@
       <c r="BU15" s="5">
         <v>24.85</v>
       </c>
-      <c r="BV15" s="5"/>
+      <c r="BV15" s="5">
+        <v>24.5</v>
+      </c>
       <c r="BW15" s="5"/>
       <c r="BX15" s="5"/>
       <c r="BY15" s="5"/>
@@ -11082,7 +11110,9 @@
       <c r="BU16" s="5">
         <v>679</v>
       </c>
-      <c r="BV16" s="5"/>
+      <c r="BV16" s="5">
+        <v>688.25</v>
+      </c>
       <c r="BW16" s="5"/>
       <c r="BX16" s="5"/>
       <c r="BY16" s="5"/>
@@ -11319,7 +11349,9 @@
       <c r="BU17" s="5">
         <v>467</v>
       </c>
-      <c r="BV17" s="5"/>
+      <c r="BV17" s="5">
+        <v>479</v>
+      </c>
       <c r="BW17" s="5"/>
       <c r="BX17" s="5"/>
       <c r="BY17" s="5"/>
@@ -11556,7 +11588,9 @@
       <c r="BU18" s="5">
         <v>261.60000000000002</v>
       </c>
-      <c r="BV18" s="5"/>
+      <c r="BV18" s="5">
+        <v>265</v>
+      </c>
       <c r="BW18" s="5"/>
       <c r="BX18" s="5"/>
       <c r="BY18" s="5"/>
@@ -11579,11 +11613,11 @@
       </c>
       <c r="B19" s="12">
         <f t="shared" si="1"/>
-        <v>648.15</v>
+        <v>652.5</v>
       </c>
       <c r="C19" s="12">
         <f t="shared" si="2"/>
-        <v>207.45</v>
+        <v>211.8</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -11793,7 +11827,9 @@
       <c r="BU19" s="5">
         <v>646</v>
       </c>
-      <c r="BV19" s="5"/>
+      <c r="BV19" s="5">
+        <v>652.5</v>
+      </c>
       <c r="BW19" s="5"/>
       <c r="BX19" s="5"/>
       <c r="BY19" s="5"/>
@@ -12030,7 +12066,9 @@
       <c r="BU20" s="5">
         <v>698</v>
       </c>
-      <c r="BV20" s="5"/>
+      <c r="BV20" s="5">
+        <v>713.75</v>
+      </c>
       <c r="BW20" s="5"/>
       <c r="BX20" s="5"/>
       <c r="BY20" s="5"/>
@@ -12267,7 +12305,9 @@
       <c r="BU21" s="5">
         <v>488.95</v>
       </c>
-      <c r="BV21" s="5"/>
+      <c r="BV21" s="5">
+        <v>489</v>
+      </c>
       <c r="BW21" s="5"/>
       <c r="BX21" s="5"/>
       <c r="BY21" s="5"/>
@@ -12450,7 +12490,9 @@
       <c r="BU22" s="5">
         <v>382.3</v>
       </c>
-      <c r="BV22" s="5"/>
+      <c r="BV22" s="5">
+        <v>384.5</v>
+      </c>
       <c r="BW22" s="5"/>
       <c r="BX22" s="5"/>
       <c r="BY22" s="5"/>
@@ -12679,7 +12721,9 @@
       <c r="BU23" s="5">
         <v>57.35</v>
       </c>
-      <c r="BV23" s="5"/>
+      <c r="BV23" s="5">
+        <v>59.95</v>
+      </c>
       <c r="BW23" s="5"/>
       <c r="BX23" s="5"/>
       <c r="BY23" s="5"/>
@@ -12904,7 +12948,9 @@
       <c r="BU24" s="5">
         <v>237.3</v>
       </c>
-      <c r="BV24" s="5"/>
+      <c r="BV24" s="5">
+        <v>239</v>
+      </c>
       <c r="BW24" s="5"/>
       <c r="BX24" s="5"/>
       <c r="BY24" s="5"/>
@@ -12927,11 +12973,11 @@
       </c>
       <c r="B25" s="12">
         <f t="shared" si="1"/>
-        <v>963.5</v>
+        <v>989.95</v>
       </c>
       <c r="C25" s="12">
         <f t="shared" si="2"/>
-        <v>87.5</v>
+        <v>113.95000000000005</v>
       </c>
       <c r="D25" s="46" t="s">
         <v>236</v>
@@ -13111,7 +13157,9 @@
       <c r="BU25" s="5">
         <v>950.75</v>
       </c>
-      <c r="BV25" s="5"/>
+      <c r="BV25" s="5">
+        <v>989.95</v>
+      </c>
       <c r="BW25" s="5"/>
       <c r="BX25" s="5"/>
       <c r="BY25" s="5"/>
@@ -13306,7 +13354,9 @@
       <c r="BU26" s="5">
         <v>92.25</v>
       </c>
-      <c r="BV26" s="5"/>
+      <c r="BV26" s="5">
+        <v>94.15</v>
+      </c>
       <c r="BW26" s="5"/>
       <c r="BX26" s="5"/>
       <c r="BY26" s="5"/>
@@ -13501,7 +13551,9 @@
       <c r="BU27" s="5">
         <v>36.200000000000003</v>
       </c>
-      <c r="BV27" s="5"/>
+      <c r="BV27" s="5">
+        <v>39.950000000000003</v>
+      </c>
       <c r="BW27" s="5"/>
       <c r="BX27" s="5"/>
       <c r="BY27" s="5"/>
@@ -13696,7 +13748,9 @@
       <c r="BU28" s="5">
         <v>121</v>
       </c>
-      <c r="BV28" s="5"/>
+      <c r="BV28" s="5">
+        <v>121.6</v>
+      </c>
       <c r="BW28" s="5"/>
       <c r="BX28" s="5"/>
       <c r="BY28" s="5"/>
@@ -13891,7 +13945,9 @@
       <c r="BU29" s="5">
         <v>64.2</v>
       </c>
-      <c r="BV29" s="5"/>
+      <c r="BV29" s="5">
+        <v>66</v>
+      </c>
       <c r="BW29" s="5"/>
       <c r="BX29" s="5"/>
       <c r="BY29" s="5"/>
@@ -14086,7 +14142,9 @@
       <c r="BU30" s="5">
         <v>40.25</v>
       </c>
-      <c r="BV30" s="5"/>
+      <c r="BV30" s="5">
+        <v>40.299999999999997</v>
+      </c>
       <c r="BW30" s="5"/>
       <c r="BX30" s="5"/>
       <c r="BY30" s="5"/>
@@ -14281,7 +14339,9 @@
       <c r="BU31" s="5">
         <v>139.85</v>
       </c>
-      <c r="BV31" s="5"/>
+      <c r="BV31" s="5">
+        <v>130.69999999999999</v>
+      </c>
       <c r="BW31" s="5"/>
       <c r="BX31" s="5"/>
       <c r="BY31" s="5"/>
@@ -14464,7 +14524,9 @@
       <c r="BU32" s="5">
         <v>96.65</v>
       </c>
-      <c r="BV32" s="5"/>
+      <c r="BV32" s="5">
+        <v>99</v>
+      </c>
       <c r="BW32" s="5"/>
       <c r="BX32" s="5"/>
       <c r="BY32" s="5"/>
@@ -14635,7 +14697,9 @@
       <c r="BU33" s="5">
         <v>59.75</v>
       </c>
-      <c r="BV33" s="5"/>
+      <c r="BV33" s="5">
+        <v>58.85</v>
+      </c>
       <c r="BW33" s="5"/>
       <c r="BX33" s="5"/>
       <c r="BY33" s="5"/>
@@ -14800,7 +14864,9 @@
       <c r="BU34" s="5">
         <v>185.75</v>
       </c>
-      <c r="BV34" s="5"/>
+      <c r="BV34" s="5">
+        <v>184</v>
+      </c>
       <c r="BW34" s="5"/>
       <c r="BX34" s="5"/>
       <c r="BY34" s="5"/>
@@ -14961,7 +15027,9 @@
       <c r="BU35" s="5">
         <v>686</v>
       </c>
-      <c r="BV35" s="5"/>
+      <c r="BV35" s="5">
+        <v>679.55</v>
+      </c>
       <c r="BW35" s="5"/>
       <c r="BX35" s="5"/>
       <c r="BY35" s="5"/>
@@ -15104,7 +15172,9 @@
       <c r="BU36" s="5">
         <v>416.7</v>
       </c>
-      <c r="BV36" s="5"/>
+      <c r="BV36" s="5">
+        <v>437.5</v>
+      </c>
       <c r="BW36" s="5"/>
       <c r="BX36" s="5"/>
       <c r="BY36" s="5"/>
@@ -15237,7 +15307,9 @@
       <c r="BU37" s="5">
         <v>365.7</v>
       </c>
-      <c r="BV37" s="5"/>
+      <c r="BV37" s="5">
+        <v>347.45</v>
+      </c>
       <c r="BW37" s="5"/>
       <c r="BX37" s="5"/>
       <c r="BY37" s="5"/>
@@ -15368,7 +15440,9 @@
       <c r="BU38" s="5">
         <v>505.35</v>
       </c>
-      <c r="BV38" s="5"/>
+      <c r="BV38" s="5">
+        <v>500</v>
+      </c>
       <c r="BW38" s="5"/>
       <c r="BX38" s="5"/>
       <c r="BY38" s="5"/>
@@ -15493,7 +15567,9 @@
       <c r="BU39" s="5">
         <v>76.400000000000006</v>
       </c>
-      <c r="BV39" s="5"/>
+      <c r="BV39" s="5">
+        <v>76.7</v>
+      </c>
       <c r="BW39" s="5"/>
       <c r="BX39" s="5"/>
       <c r="BY39" s="5"/>
@@ -15618,7 +15694,9 @@
       <c r="BU40" s="5">
         <v>424.9</v>
       </c>
-      <c r="BV40" s="5"/>
+      <c r="BV40" s="5">
+        <v>425</v>
+      </c>
       <c r="BW40" s="5"/>
       <c r="BX40" s="5"/>
       <c r="BY40" s="5"/>
@@ -15739,7 +15817,9 @@
       <c r="BU41" s="5">
         <v>198.3</v>
       </c>
-      <c r="BV41" s="5"/>
+      <c r="BV41" s="5">
+        <v>206</v>
+      </c>
       <c r="BW41" s="5"/>
       <c r="BX41" s="5"/>
       <c r="BY41" s="5"/>
@@ -15856,7 +15936,9 @@
       <c r="BU42" s="5">
         <v>35</v>
       </c>
-      <c r="BV42" s="5"/>
+      <c r="BV42" s="5">
+        <v>36</v>
+      </c>
       <c r="BW42" s="5"/>
       <c r="BX42" s="5"/>
       <c r="BY42" s="5"/>
@@ -15879,11 +15961,11 @@
       </c>
       <c r="B43" s="12">
         <f t="shared" ref="B43:B44" si="12">MAX(E43:ZW43)</f>
-        <v>619</v>
+        <v>626.70000000000005</v>
       </c>
       <c r="C43" s="12">
         <f t="shared" si="11"/>
-        <v>41.549999999999955</v>
+        <v>49.25</v>
       </c>
       <c r="D43" s="45" t="s">
         <v>309</v>
@@ -15971,7 +16053,9 @@
       <c r="BU43" s="5">
         <v>610</v>
       </c>
-      <c r="BV43" s="5"/>
+      <c r="BV43" s="5">
+        <v>626.70000000000005</v>
+      </c>
       <c r="BW43" s="5"/>
       <c r="BX43" s="5"/>
       <c r="BY43" s="5"/>
@@ -16086,7 +16170,9 @@
       <c r="BU44" s="5">
         <v>822.95</v>
       </c>
-      <c r="BV44" s="5"/>
+      <c r="BV44" s="5">
+        <v>828.55</v>
+      </c>
       <c r="BW44" s="5"/>
       <c r="BX44" s="5"/>
       <c r="BY44" s="5"/>
@@ -16199,7 +16285,9 @@
       <c r="BU45" s="5">
         <v>134.9</v>
       </c>
-      <c r="BV45" s="5"/>
+      <c r="BV45" s="5">
+        <v>137</v>
+      </c>
       <c r="BW45" s="5"/>
       <c r="BX45" s="5"/>
       <c r="BY45" s="5"/>
@@ -16218,7 +16306,7 @@
     <row r="46" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <f t="shared" ref="A46" si="13">MIN(E46:ZW46)</f>
-        <v>680.25</v>
+        <v>679.8</v>
       </c>
       <c r="B46" s="12">
         <f>MAX(E46:ZW46)</f>
@@ -16226,7 +16314,7 @@
       </c>
       <c r="C46" s="12">
         <f t="shared" ref="C46" si="14">B46-A46</f>
-        <v>89.75</v>
+        <v>90.200000000000045</v>
       </c>
       <c r="D46" s="45" t="s">
         <v>313</v>
@@ -16306,7 +16394,9 @@
       <c r="BU46" s="5">
         <v>680.25</v>
       </c>
-      <c r="BV46" s="5"/>
+      <c r="BV46" s="5">
+        <v>679.8</v>
+      </c>
       <c r="BW46" s="5"/>
       <c r="BX46" s="5"/>
       <c r="BY46" s="5"/>
@@ -16413,7 +16503,9 @@
       <c r="BU47" s="5">
         <v>776.5</v>
       </c>
-      <c r="BV47" s="5"/>
+      <c r="BV47" s="5">
+        <v>785</v>
+      </c>
       <c r="BW47" s="5"/>
       <c r="BX47" s="5"/>
       <c r="BY47" s="5"/>

</xml_diff>

<commit_message>
Added details for 17/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -7259,9 +7259,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CJ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="BP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BV47" sqref="BV47"/>
+      <selection pane="topRight" activeCell="BW47" sqref="BW47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7578,11 +7578,11 @@
       </c>
       <c r="B2" s="12">
         <f t="shared" ref="B2:B42" si="1">MAX(E2:ZW2)</f>
-        <v>333.95</v>
+        <v>340.8</v>
       </c>
       <c r="C2" s="12">
         <f>B2-A2</f>
-        <v>90.35</v>
+        <v>97.200000000000017</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>115</v>
@@ -7789,7 +7789,9 @@
       <c r="BV2" s="5">
         <v>333.95</v>
       </c>
-      <c r="BW2" s="5"/>
+      <c r="BW2" s="5">
+        <v>340.8</v>
+      </c>
       <c r="BX2" s="5"/>
       <c r="BY2" s="5"/>
       <c r="BZ2" s="5"/>
@@ -7811,11 +7813,11 @@
       </c>
       <c r="B3" s="12">
         <f t="shared" si="1"/>
-        <v>318.55</v>
+        <v>328.85</v>
       </c>
       <c r="C3" s="12">
         <f t="shared" ref="C3:C33" si="2">B3-A3</f>
-        <v>55.850000000000023</v>
+        <v>66.150000000000034</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>114</v>
@@ -8022,7 +8024,9 @@
       <c r="BV3" s="5">
         <v>318.55</v>
       </c>
-      <c r="BW3" s="5"/>
+      <c r="BW3" s="5">
+        <v>328.85</v>
+      </c>
       <c r="BX3" s="5"/>
       <c r="BY3" s="5"/>
       <c r="BZ3" s="5"/>
@@ -8261,7 +8265,9 @@
       <c r="BV4" s="5">
         <v>255</v>
       </c>
-      <c r="BW4" s="5"/>
+      <c r="BW4" s="5">
+        <v>258</v>
+      </c>
       <c r="BX4" s="5"/>
       <c r="BY4" s="5"/>
       <c r="BZ4" s="5"/>
@@ -8500,7 +8506,9 @@
       <c r="BV5" s="5">
         <v>905.25</v>
       </c>
-      <c r="BW5" s="5"/>
+      <c r="BW5" s="5">
+        <v>919.15</v>
+      </c>
       <c r="BX5" s="5"/>
       <c r="BY5" s="5"/>
       <c r="BZ5" s="5"/>
@@ -8739,7 +8747,9 @@
       <c r="BV6" s="5">
         <v>269</v>
       </c>
-      <c r="BW6" s="5"/>
+      <c r="BW6" s="5">
+        <v>272</v>
+      </c>
       <c r="BX6" s="5"/>
       <c r="BY6" s="5"/>
       <c r="BZ6" s="5"/>
@@ -8978,7 +8988,9 @@
       <c r="BV7" s="5">
         <v>16.95</v>
       </c>
-      <c r="BW7" s="5"/>
+      <c r="BW7" s="5">
+        <v>17.100000000000001</v>
+      </c>
       <c r="BX7" s="5"/>
       <c r="BY7" s="5"/>
       <c r="BZ7" s="5"/>
@@ -9217,7 +9229,9 @@
       <c r="BV8" s="5">
         <v>77.400000000000006</v>
       </c>
-      <c r="BW8" s="5"/>
+      <c r="BW8" s="5">
+        <v>79.400000000000006</v>
+      </c>
       <c r="BX8" s="5"/>
       <c r="BY8" s="5"/>
       <c r="BZ8" s="5"/>
@@ -9448,7 +9462,9 @@
       <c r="BV9" s="28">
         <v>54.25</v>
       </c>
-      <c r="BW9" s="28"/>
+      <c r="BW9" s="28">
+        <v>55.35</v>
+      </c>
       <c r="BX9" s="28"/>
       <c r="BY9" s="28"/>
       <c r="BZ9" s="28"/>
@@ -9687,7 +9703,9 @@
       <c r="BV10" s="5">
         <v>36.9</v>
       </c>
-      <c r="BW10" s="5"/>
+      <c r="BW10" s="5">
+        <v>36.9</v>
+      </c>
       <c r="BX10" s="5"/>
       <c r="BY10" s="5"/>
       <c r="BZ10" s="5"/>
@@ -9926,7 +9944,9 @@
       <c r="BV11" s="5">
         <v>95.9</v>
       </c>
-      <c r="BW11" s="5"/>
+      <c r="BW11" s="5">
+        <v>96.45</v>
+      </c>
       <c r="BX11" s="5"/>
       <c r="BY11" s="5"/>
       <c r="BZ11" s="5"/>
@@ -10165,7 +10185,9 @@
       <c r="BV12" s="5">
         <v>87.75</v>
       </c>
-      <c r="BW12" s="5"/>
+      <c r="BW12" s="5">
+        <v>88.2</v>
+      </c>
       <c r="BX12" s="5"/>
       <c r="BY12" s="5"/>
       <c r="BZ12" s="5"/>
@@ -10404,7 +10426,9 @@
       <c r="BV13" s="5">
         <v>47.45</v>
       </c>
-      <c r="BW13" s="5"/>
+      <c r="BW13" s="5">
+        <v>48.4</v>
+      </c>
       <c r="BX13" s="5"/>
       <c r="BY13" s="5"/>
       <c r="BZ13" s="5"/>
@@ -10643,7 +10667,9 @@
       <c r="BV14" s="5">
         <v>34.4</v>
       </c>
-      <c r="BW14" s="5"/>
+      <c r="BW14" s="5">
+        <v>35.4</v>
+      </c>
       <c r="BX14" s="5"/>
       <c r="BY14" s="5"/>
       <c r="BZ14" s="5"/>
@@ -10874,7 +10900,9 @@
       <c r="BV15" s="5">
         <v>24.5</v>
       </c>
-      <c r="BW15" s="5"/>
+      <c r="BW15" s="5">
+        <v>24.9</v>
+      </c>
       <c r="BX15" s="5"/>
       <c r="BY15" s="5"/>
       <c r="BZ15" s="5"/>
@@ -11113,7 +11141,9 @@
       <c r="BV16" s="5">
         <v>688.25</v>
       </c>
-      <c r="BW16" s="5"/>
+      <c r="BW16" s="5">
+        <v>705.2</v>
+      </c>
       <c r="BX16" s="5"/>
       <c r="BY16" s="5"/>
       <c r="BZ16" s="5"/>
@@ -11352,7 +11382,9 @@
       <c r="BV17" s="5">
         <v>479</v>
       </c>
-      <c r="BW17" s="5"/>
+      <c r="BW17" s="5">
+        <v>477</v>
+      </c>
       <c r="BX17" s="5"/>
       <c r="BY17" s="5"/>
       <c r="BZ17" s="5"/>
@@ -11591,7 +11623,9 @@
       <c r="BV18" s="5">
         <v>265</v>
       </c>
-      <c r="BW18" s="5"/>
+      <c r="BW18" s="5">
+        <v>271</v>
+      </c>
       <c r="BX18" s="5"/>
       <c r="BY18" s="5"/>
       <c r="BZ18" s="5"/>
@@ -11613,11 +11647,11 @@
       </c>
       <c r="B19" s="12">
         <f t="shared" si="1"/>
-        <v>652.5</v>
+        <v>657.9</v>
       </c>
       <c r="C19" s="12">
         <f t="shared" si="2"/>
-        <v>211.8</v>
+        <v>217.2</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -11830,7 +11864,9 @@
       <c r="BV19" s="5">
         <v>652.5</v>
       </c>
-      <c r="BW19" s="5"/>
+      <c r="BW19" s="5">
+        <v>657.9</v>
+      </c>
       <c r="BX19" s="5"/>
       <c r="BY19" s="5"/>
       <c r="BZ19" s="5"/>
@@ -12069,7 +12105,9 @@
       <c r="BV20" s="5">
         <v>713.75</v>
       </c>
-      <c r="BW20" s="5"/>
+      <c r="BW20" s="5">
+        <v>715.5</v>
+      </c>
       <c r="BX20" s="5"/>
       <c r="BY20" s="5"/>
       <c r="BZ20" s="5"/>
@@ -12308,7 +12346,9 @@
       <c r="BV21" s="5">
         <v>489</v>
       </c>
-      <c r="BW21" s="5"/>
+      <c r="BW21" s="5">
+        <v>499.85</v>
+      </c>
       <c r="BX21" s="5"/>
       <c r="BY21" s="5"/>
       <c r="BZ21" s="5"/>
@@ -12330,11 +12370,11 @@
       </c>
       <c r="B22" s="12">
         <f t="shared" si="1"/>
-        <v>388</v>
+        <v>392.05</v>
       </c>
       <c r="C22" s="12">
         <f t="shared" si="2"/>
-        <v>72.800000000000011</v>
+        <v>76.850000000000023</v>
       </c>
       <c r="D22" s="44" t="s">
         <v>269</v>
@@ -12493,7 +12533,9 @@
       <c r="BV22" s="5">
         <v>384.5</v>
       </c>
-      <c r="BW22" s="5"/>
+      <c r="BW22" s="5">
+        <v>392.05</v>
+      </c>
       <c r="BX22" s="5"/>
       <c r="BY22" s="5"/>
       <c r="BZ22" s="5"/>
@@ -12724,7 +12766,9 @@
       <c r="BV23" s="5">
         <v>59.95</v>
       </c>
-      <c r="BW23" s="5"/>
+      <c r="BW23" s="5">
+        <v>65.099999999999994</v>
+      </c>
       <c r="BX23" s="5"/>
       <c r="BY23" s="5"/>
       <c r="BZ23" s="5"/>
@@ -12951,7 +12995,9 @@
       <c r="BV24" s="5">
         <v>239</v>
       </c>
-      <c r="BW24" s="5"/>
+      <c r="BW24" s="5">
+        <v>240.8</v>
+      </c>
       <c r="BX24" s="5"/>
       <c r="BY24" s="5"/>
       <c r="BZ24" s="5"/>
@@ -13160,7 +13206,9 @@
       <c r="BV25" s="5">
         <v>989.95</v>
       </c>
-      <c r="BW25" s="5"/>
+      <c r="BW25" s="5">
+        <v>974.35</v>
+      </c>
       <c r="BX25" s="5"/>
       <c r="BY25" s="5"/>
       <c r="BZ25" s="5"/>
@@ -13357,7 +13405,9 @@
       <c r="BV26" s="5">
         <v>94.15</v>
       </c>
-      <c r="BW26" s="5"/>
+      <c r="BW26" s="5">
+        <v>92.3</v>
+      </c>
       <c r="BX26" s="5"/>
       <c r="BY26" s="5"/>
       <c r="BZ26" s="5"/>
@@ -13554,7 +13604,9 @@
       <c r="BV27" s="5">
         <v>39.950000000000003</v>
       </c>
-      <c r="BW27" s="5"/>
+      <c r="BW27" s="5">
+        <v>40.6</v>
+      </c>
       <c r="BX27" s="5"/>
       <c r="BY27" s="5"/>
       <c r="BZ27" s="5"/>
@@ -13751,7 +13803,9 @@
       <c r="BV28" s="5">
         <v>121.6</v>
       </c>
-      <c r="BW28" s="5"/>
+      <c r="BW28" s="5">
+        <v>123.15</v>
+      </c>
       <c r="BX28" s="5"/>
       <c r="BY28" s="5"/>
       <c r="BZ28" s="5"/>
@@ -13948,7 +14002,9 @@
       <c r="BV29" s="5">
         <v>66</v>
       </c>
-      <c r="BW29" s="5"/>
+      <c r="BW29" s="5">
+        <v>70</v>
+      </c>
       <c r="BX29" s="5"/>
       <c r="BY29" s="5"/>
       <c r="BZ29" s="5"/>
@@ -14145,7 +14201,9 @@
       <c r="BV30" s="5">
         <v>40.299999999999997</v>
       </c>
-      <c r="BW30" s="5"/>
+      <c r="BW30" s="5">
+        <v>40.6</v>
+      </c>
       <c r="BX30" s="5"/>
       <c r="BY30" s="5"/>
       <c r="BZ30" s="5"/>
@@ -14342,7 +14400,9 @@
       <c r="BV31" s="5">
         <v>130.69999999999999</v>
       </c>
-      <c r="BW31" s="5"/>
+      <c r="BW31" s="5">
+        <v>130.4</v>
+      </c>
       <c r="BX31" s="5"/>
       <c r="BY31" s="5"/>
       <c r="BZ31" s="5"/>
@@ -14527,7 +14587,9 @@
       <c r="BV32" s="5">
         <v>99</v>
       </c>
-      <c r="BW32" s="5"/>
+      <c r="BW32" s="5">
+        <v>100.35</v>
+      </c>
       <c r="BX32" s="5"/>
       <c r="BY32" s="5"/>
       <c r="BZ32" s="5"/>
@@ -14700,7 +14762,9 @@
       <c r="BV33" s="5">
         <v>58.85</v>
       </c>
-      <c r="BW33" s="5"/>
+      <c r="BW33" s="5">
+        <v>58.4</v>
+      </c>
       <c r="BX33" s="5"/>
       <c r="BY33" s="5"/>
       <c r="BZ33" s="5"/>
@@ -14867,7 +14931,9 @@
       <c r="BV34" s="5">
         <v>184</v>
       </c>
-      <c r="BW34" s="5"/>
+      <c r="BW34" s="5">
+        <v>188.1</v>
+      </c>
       <c r="BX34" s="5"/>
       <c r="BY34" s="5"/>
       <c r="BZ34" s="5"/>
@@ -15030,7 +15096,9 @@
       <c r="BV35" s="5">
         <v>679.55</v>
       </c>
-      <c r="BW35" s="5"/>
+      <c r="BW35" s="5">
+        <v>684.9</v>
+      </c>
       <c r="BX35" s="5"/>
       <c r="BY35" s="5"/>
       <c r="BZ35" s="5"/>
@@ -15175,7 +15243,9 @@
       <c r="BV36" s="5">
         <v>437.5</v>
       </c>
-      <c r="BW36" s="5"/>
+      <c r="BW36" s="5">
+        <v>448.9</v>
+      </c>
       <c r="BX36" s="5"/>
       <c r="BY36" s="5"/>
       <c r="BZ36" s="5"/>
@@ -15310,7 +15380,9 @@
       <c r="BV37" s="5">
         <v>347.45</v>
       </c>
-      <c r="BW37" s="5"/>
+      <c r="BW37" s="5">
+        <v>335.35</v>
+      </c>
       <c r="BX37" s="5"/>
       <c r="BY37" s="5"/>
       <c r="BZ37" s="5"/>
@@ -15443,7 +15515,9 @@
       <c r="BV38" s="5">
         <v>500</v>
       </c>
-      <c r="BW38" s="5"/>
+      <c r="BW38" s="5">
+        <v>507.55</v>
+      </c>
       <c r="BX38" s="5"/>
       <c r="BY38" s="5"/>
       <c r="BZ38" s="5"/>
@@ -15570,7 +15644,9 @@
       <c r="BV39" s="5">
         <v>76.7</v>
       </c>
-      <c r="BW39" s="5"/>
+      <c r="BW39" s="5">
+        <v>76</v>
+      </c>
       <c r="BX39" s="5"/>
       <c r="BY39" s="5"/>
       <c r="BZ39" s="5"/>
@@ -15697,7 +15773,9 @@
       <c r="BV40" s="5">
         <v>425</v>
       </c>
-      <c r="BW40" s="5"/>
+      <c r="BW40" s="5">
+        <v>426.1</v>
+      </c>
       <c r="BX40" s="5"/>
       <c r="BY40" s="5"/>
       <c r="BZ40" s="5"/>
@@ -15820,7 +15898,9 @@
       <c r="BV41" s="5">
         <v>206</v>
       </c>
-      <c r="BW41" s="5"/>
+      <c r="BW41" s="5">
+        <v>211.6</v>
+      </c>
       <c r="BX41" s="5"/>
       <c r="BY41" s="5"/>
       <c r="BZ41" s="5"/>
@@ -15939,7 +16019,9 @@
       <c r="BV42" s="5">
         <v>36</v>
       </c>
-      <c r="BW42" s="5"/>
+      <c r="BW42" s="5">
+        <v>37.200000000000003</v>
+      </c>
       <c r="BX42" s="5"/>
       <c r="BY42" s="5"/>
       <c r="BZ42" s="5"/>
@@ -16056,7 +16138,9 @@
       <c r="BV43" s="5">
         <v>626.70000000000005</v>
       </c>
-      <c r="BW43" s="5"/>
+      <c r="BW43" s="5">
+        <v>607.29999999999995</v>
+      </c>
       <c r="BX43" s="5"/>
       <c r="BY43" s="5"/>
       <c r="BZ43" s="5"/>
@@ -16173,7 +16257,9 @@
       <c r="BV44" s="5">
         <v>828.55</v>
       </c>
-      <c r="BW44" s="5"/>
+      <c r="BW44" s="5">
+        <v>831.85</v>
+      </c>
       <c r="BX44" s="5"/>
       <c r="BY44" s="5"/>
       <c r="BZ44" s="5"/>
@@ -16288,7 +16374,9 @@
       <c r="BV45" s="5">
         <v>137</v>
       </c>
-      <c r="BW45" s="5"/>
+      <c r="BW45" s="5">
+        <v>137.75</v>
+      </c>
       <c r="BX45" s="5"/>
       <c r="BY45" s="5"/>
       <c r="BZ45" s="5"/>
@@ -16306,7 +16394,7 @@
     <row r="46" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <f t="shared" ref="A46" si="13">MIN(E46:ZW46)</f>
-        <v>679.8</v>
+        <v>679</v>
       </c>
       <c r="B46" s="12">
         <f>MAX(E46:ZW46)</f>
@@ -16314,7 +16402,7 @@
       </c>
       <c r="C46" s="12">
         <f t="shared" ref="C46" si="14">B46-A46</f>
-        <v>90.200000000000045</v>
+        <v>91</v>
       </c>
       <c r="D46" s="45" t="s">
         <v>313</v>
@@ -16397,7 +16485,9 @@
       <c r="BV46" s="5">
         <v>679.8</v>
       </c>
-      <c r="BW46" s="5"/>
+      <c r="BW46" s="5">
+        <v>679</v>
+      </c>
       <c r="BX46" s="5"/>
       <c r="BY46" s="5"/>
       <c r="BZ46" s="5"/>
@@ -16506,7 +16596,9 @@
       <c r="BV47" s="5">
         <v>785</v>
       </c>
-      <c r="BW47" s="5"/>
+      <c r="BW47" s="5">
+        <v>786</v>
+      </c>
       <c r="BX47" s="5"/>
       <c r="BY47" s="5"/>
       <c r="BZ47" s="5"/>

</xml_diff>

<commit_message>
Added details for 21/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="330">
   <si>
     <t>Date</t>
   </si>
@@ -1012,6 +1012,9 @@
   </si>
   <si>
     <t>TIMKEN</t>
+  </si>
+  <si>
+    <t>MEGH</t>
   </si>
 </sst>
 </file>
@@ -7257,11 +7260,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CJ47"/>
+  <dimension ref="A1:CJ48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="BP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BW47" sqref="BW47"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="BX1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BY2" sqref="BY2:BY48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7792,8 +7795,12 @@
       <c r="BW2" s="5">
         <v>340.8</v>
       </c>
-      <c r="BX2" s="5"/>
-      <c r="BY2" s="5"/>
+      <c r="BX2" s="5">
+        <v>332.75</v>
+      </c>
+      <c r="BY2" s="5">
+        <v>330.3</v>
+      </c>
       <c r="BZ2" s="5"/>
       <c r="CA2" s="5"/>
       <c r="CB2" s="5"/>
@@ -8027,8 +8034,12 @@
       <c r="BW3" s="5">
         <v>328.85</v>
       </c>
-      <c r="BX3" s="5"/>
-      <c r="BY3" s="5"/>
+      <c r="BX3" s="5">
+        <v>318.89999999999998</v>
+      </c>
+      <c r="BY3" s="5">
+        <v>318.55</v>
+      </c>
       <c r="BZ3" s="5"/>
       <c r="CA3" s="5"/>
       <c r="CB3" s="5"/>
@@ -8268,8 +8279,12 @@
       <c r="BW4" s="5">
         <v>258</v>
       </c>
-      <c r="BX4" s="5"/>
-      <c r="BY4" s="5"/>
+      <c r="BX4" s="5">
+        <v>259.05</v>
+      </c>
+      <c r="BY4" s="5">
+        <v>255.5</v>
+      </c>
       <c r="BZ4" s="5"/>
       <c r="CA4" s="5"/>
       <c r="CB4" s="5"/>
@@ -8509,8 +8524,12 @@
       <c r="BW5" s="5">
         <v>919.15</v>
       </c>
-      <c r="BX5" s="5"/>
-      <c r="BY5" s="5"/>
+      <c r="BX5" s="5">
+        <v>919</v>
+      </c>
+      <c r="BY5" s="5">
+        <v>932.05</v>
+      </c>
       <c r="BZ5" s="5"/>
       <c r="CA5" s="5"/>
       <c r="CB5" s="5"/>
@@ -8750,8 +8769,12 @@
       <c r="BW6" s="5">
         <v>272</v>
       </c>
-      <c r="BX6" s="5"/>
-      <c r="BY6" s="5"/>
+      <c r="BX6" s="5">
+        <v>278.39999999999998</v>
+      </c>
+      <c r="BY6" s="5">
+        <v>273.2</v>
+      </c>
       <c r="BZ6" s="5"/>
       <c r="CA6" s="5"/>
       <c r="CB6" s="5"/>
@@ -8991,8 +9014,12 @@
       <c r="BW7" s="5">
         <v>17.100000000000001</v>
       </c>
-      <c r="BX7" s="5"/>
-      <c r="BY7" s="5"/>
+      <c r="BX7" s="5">
+        <v>17.2</v>
+      </c>
+      <c r="BY7" s="5">
+        <v>17.25</v>
+      </c>
       <c r="BZ7" s="5"/>
       <c r="CA7" s="5"/>
       <c r="CB7" s="5"/>
@@ -9232,8 +9259,12 @@
       <c r="BW8" s="5">
         <v>79.400000000000006</v>
       </c>
-      <c r="BX8" s="5"/>
-      <c r="BY8" s="5"/>
+      <c r="BX8" s="5">
+        <v>81.5</v>
+      </c>
+      <c r="BY8" s="5">
+        <v>82.75</v>
+      </c>
       <c r="BZ8" s="5"/>
       <c r="CA8" s="5"/>
       <c r="CB8" s="5"/>
@@ -9465,8 +9496,12 @@
       <c r="BW9" s="28">
         <v>55.35</v>
       </c>
-      <c r="BX9" s="28"/>
-      <c r="BY9" s="28"/>
+      <c r="BX9" s="28">
+        <v>54.85</v>
+      </c>
+      <c r="BY9" s="28">
+        <v>54.85</v>
+      </c>
       <c r="BZ9" s="28"/>
       <c r="CA9" s="28"/>
       <c r="CB9" s="28"/>
@@ -9706,8 +9741,12 @@
       <c r="BW10" s="5">
         <v>36.9</v>
       </c>
-      <c r="BX10" s="5"/>
-      <c r="BY10" s="5"/>
+      <c r="BX10" s="5">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="BY10" s="5">
+        <v>38.15</v>
+      </c>
       <c r="BZ10" s="5"/>
       <c r="CA10" s="5"/>
       <c r="CB10" s="5"/>
@@ -9947,8 +9986,12 @@
       <c r="BW11" s="5">
         <v>96.45</v>
       </c>
-      <c r="BX11" s="5"/>
-      <c r="BY11" s="5"/>
+      <c r="BX11" s="5">
+        <v>101.9</v>
+      </c>
+      <c r="BY11" s="5">
+        <v>100.9</v>
+      </c>
       <c r="BZ11" s="5"/>
       <c r="CA11" s="5"/>
       <c r="CB11" s="5"/>
@@ -10188,8 +10231,12 @@
       <c r="BW12" s="5">
         <v>88.2</v>
       </c>
-      <c r="BX12" s="5"/>
-      <c r="BY12" s="5"/>
+      <c r="BX12" s="5">
+        <v>87.2</v>
+      </c>
+      <c r="BY12" s="5">
+        <v>87.5</v>
+      </c>
       <c r="BZ12" s="5"/>
       <c r="CA12" s="5"/>
       <c r="CB12" s="5"/>
@@ -10429,8 +10476,12 @@
       <c r="BW13" s="5">
         <v>48.4</v>
       </c>
-      <c r="BX13" s="5"/>
-      <c r="BY13" s="5"/>
+      <c r="BX13" s="5">
+        <v>48.2</v>
+      </c>
+      <c r="BY13" s="5">
+        <v>51</v>
+      </c>
       <c r="BZ13" s="5"/>
       <c r="CA13" s="5"/>
       <c r="CB13" s="5"/>
@@ -10670,8 +10721,12 @@
       <c r="BW14" s="5">
         <v>35.4</v>
       </c>
-      <c r="BX14" s="5"/>
-      <c r="BY14" s="5"/>
+      <c r="BX14" s="5">
+        <v>35.450000000000003</v>
+      </c>
+      <c r="BY14" s="5">
+        <v>35.25</v>
+      </c>
       <c r="BZ14" s="5"/>
       <c r="CA14" s="5"/>
       <c r="CB14" s="5"/>
@@ -10903,8 +10958,12 @@
       <c r="BW15" s="5">
         <v>24.9</v>
       </c>
-      <c r="BX15" s="5"/>
-      <c r="BY15" s="5"/>
+      <c r="BX15" s="5">
+        <v>24.8</v>
+      </c>
+      <c r="BY15" s="5">
+        <v>24.5</v>
+      </c>
       <c r="BZ15" s="5"/>
       <c r="CA15" s="5"/>
       <c r="CB15" s="5"/>
@@ -11144,8 +11203,12 @@
       <c r="BW16" s="5">
         <v>705.2</v>
       </c>
-      <c r="BX16" s="5"/>
-      <c r="BY16" s="5"/>
+      <c r="BX16" s="5">
+        <v>701.6</v>
+      </c>
+      <c r="BY16" s="5">
+        <v>711.25</v>
+      </c>
       <c r="BZ16" s="5"/>
       <c r="CA16" s="5"/>
       <c r="CB16" s="5"/>
@@ -11385,8 +11448,12 @@
       <c r="BW17" s="5">
         <v>477</v>
       </c>
-      <c r="BX17" s="5"/>
-      <c r="BY17" s="5"/>
+      <c r="BX17" s="5">
+        <v>461</v>
+      </c>
+      <c r="BY17" s="5">
+        <v>466.2</v>
+      </c>
       <c r="BZ17" s="5"/>
       <c r="CA17" s="5"/>
       <c r="CB17" s="5"/>
@@ -11626,8 +11693,12 @@
       <c r="BW18" s="5">
         <v>271</v>
       </c>
-      <c r="BX18" s="5"/>
-      <c r="BY18" s="5"/>
+      <c r="BX18" s="5">
+        <v>263.8</v>
+      </c>
+      <c r="BY18" s="5">
+        <v>255.9</v>
+      </c>
       <c r="BZ18" s="5"/>
       <c r="CA18" s="5"/>
       <c r="CB18" s="5"/>
@@ -11647,11 +11718,11 @@
       </c>
       <c r="B19" s="12">
         <f t="shared" si="1"/>
-        <v>657.9</v>
+        <v>703.7</v>
       </c>
       <c r="C19" s="12">
         <f t="shared" si="2"/>
-        <v>217.2</v>
+        <v>263.00000000000006</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -11867,8 +11938,12 @@
       <c r="BW19" s="5">
         <v>657.9</v>
       </c>
-      <c r="BX19" s="5"/>
-      <c r="BY19" s="5"/>
+      <c r="BX19" s="5">
+        <v>692.95</v>
+      </c>
+      <c r="BY19" s="5">
+        <v>703.7</v>
+      </c>
       <c r="BZ19" s="5"/>
       <c r="CA19" s="5"/>
       <c r="CB19" s="5"/>
@@ -12108,8 +12183,12 @@
       <c r="BW20" s="5">
         <v>715.5</v>
       </c>
-      <c r="BX20" s="5"/>
-      <c r="BY20" s="5"/>
+      <c r="BX20" s="5">
+        <v>706.95</v>
+      </c>
+      <c r="BY20" s="5">
+        <v>708.15</v>
+      </c>
       <c r="BZ20" s="5"/>
       <c r="CA20" s="5"/>
       <c r="CB20" s="5"/>
@@ -12349,8 +12428,12 @@
       <c r="BW21" s="5">
         <v>499.85</v>
       </c>
-      <c r="BX21" s="5"/>
-      <c r="BY21" s="5"/>
+      <c r="BX21" s="5">
+        <v>492.7</v>
+      </c>
+      <c r="BY21" s="5">
+        <v>503.9</v>
+      </c>
       <c r="BZ21" s="5"/>
       <c r="CA21" s="5"/>
       <c r="CB21" s="5"/>
@@ -12370,11 +12453,11 @@
       </c>
       <c r="B22" s="12">
         <f t="shared" si="1"/>
-        <v>392.05</v>
+        <v>406.95</v>
       </c>
       <c r="C22" s="12">
         <f t="shared" si="2"/>
-        <v>76.850000000000023</v>
+        <v>91.75</v>
       </c>
       <c r="D22" s="44" t="s">
         <v>269</v>
@@ -12536,8 +12619,12 @@
       <c r="BW22" s="5">
         <v>392.05</v>
       </c>
-      <c r="BX22" s="5"/>
-      <c r="BY22" s="5"/>
+      <c r="BX22" s="5">
+        <v>406.95</v>
+      </c>
+      <c r="BY22" s="5">
+        <v>396.6</v>
+      </c>
       <c r="BZ22" s="5"/>
       <c r="CA22" s="5"/>
       <c r="CB22" s="5"/>
@@ -12769,8 +12856,12 @@
       <c r="BW23" s="5">
         <v>65.099999999999994</v>
       </c>
-      <c r="BX23" s="5"/>
-      <c r="BY23" s="5"/>
+      <c r="BX23" s="5">
+        <v>64.2</v>
+      </c>
+      <c r="BY23" s="5">
+        <v>62.65</v>
+      </c>
       <c r="BZ23" s="5"/>
       <c r="CA23" s="5"/>
       <c r="CB23" s="5"/>
@@ -12998,8 +13089,12 @@
       <c r="BW24" s="5">
         <v>240.8</v>
       </c>
-      <c r="BX24" s="5"/>
-      <c r="BY24" s="5"/>
+      <c r="BX24" s="5">
+        <v>241.5</v>
+      </c>
+      <c r="BY24" s="5">
+        <v>242.55</v>
+      </c>
       <c r="BZ24" s="5"/>
       <c r="CA24" s="5"/>
       <c r="CB24" s="5"/>
@@ -13209,8 +13304,12 @@
       <c r="BW25" s="5">
         <v>974.35</v>
       </c>
-      <c r="BX25" s="5"/>
-      <c r="BY25" s="5"/>
+      <c r="BX25" s="5">
+        <v>960.95</v>
+      </c>
+      <c r="BY25" s="5">
+        <v>965.5</v>
+      </c>
       <c r="BZ25" s="5"/>
       <c r="CA25" s="5"/>
       <c r="CB25" s="5"/>
@@ -13408,8 +13507,12 @@
       <c r="BW26" s="5">
         <v>92.3</v>
       </c>
-      <c r="BX26" s="5"/>
-      <c r="BY26" s="5"/>
+      <c r="BX26" s="5">
+        <v>92</v>
+      </c>
+      <c r="BY26" s="5">
+        <v>92.95</v>
+      </c>
       <c r="BZ26" s="5"/>
       <c r="CA26" s="5"/>
       <c r="CB26" s="5"/>
@@ -13607,8 +13710,12 @@
       <c r="BW27" s="5">
         <v>40.6</v>
       </c>
-      <c r="BX27" s="5"/>
-      <c r="BY27" s="5"/>
+      <c r="BX27" s="5">
+        <v>42.4</v>
+      </c>
+      <c r="BY27" s="5">
+        <v>43.35</v>
+      </c>
       <c r="BZ27" s="5"/>
       <c r="CA27" s="5"/>
       <c r="CB27" s="5"/>
@@ -13806,8 +13913,12 @@
       <c r="BW28" s="5">
         <v>123.15</v>
       </c>
-      <c r="BX28" s="5"/>
-      <c r="BY28" s="5"/>
+      <c r="BX28" s="5">
+        <v>125.6</v>
+      </c>
+      <c r="BY28" s="5">
+        <v>125.95</v>
+      </c>
       <c r="BZ28" s="5"/>
       <c r="CA28" s="5"/>
       <c r="CB28" s="5"/>
@@ -14005,8 +14116,12 @@
       <c r="BW29" s="5">
         <v>70</v>
       </c>
-      <c r="BX29" s="5"/>
-      <c r="BY29" s="5"/>
+      <c r="BX29" s="5">
+        <v>71.75</v>
+      </c>
+      <c r="BY29" s="5">
+        <v>73.599999999999994</v>
+      </c>
       <c r="BZ29" s="5"/>
       <c r="CA29" s="5"/>
       <c r="CB29" s="5"/>
@@ -14204,8 +14319,12 @@
       <c r="BW30" s="5">
         <v>40.6</v>
       </c>
-      <c r="BX30" s="5"/>
-      <c r="BY30" s="5"/>
+      <c r="BX30" s="5">
+        <v>41.35</v>
+      </c>
+      <c r="BY30" s="5">
+        <v>41.35</v>
+      </c>
       <c r="BZ30" s="5"/>
       <c r="CA30" s="5"/>
       <c r="CB30" s="5"/>
@@ -14221,7 +14340,7 @@
     <row r="31" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
-        <v>130.19999999999999</v>
+        <v>128.9</v>
       </c>
       <c r="B31" s="12">
         <f t="shared" si="1"/>
@@ -14229,7 +14348,7 @@
       </c>
       <c r="C31" s="12">
         <f t="shared" si="2"/>
-        <v>26.650000000000006</v>
+        <v>27.949999999999989</v>
       </c>
       <c r="D31" s="45" t="s">
         <v>257</v>
@@ -14403,8 +14522,12 @@
       <c r="BW31" s="5">
         <v>130.4</v>
       </c>
-      <c r="BX31" s="5"/>
-      <c r="BY31" s="5"/>
+      <c r="BX31" s="5">
+        <v>130.6</v>
+      </c>
+      <c r="BY31" s="5">
+        <v>128.9</v>
+      </c>
       <c r="BZ31" s="5"/>
       <c r="CA31" s="5"/>
       <c r="CB31" s="5"/>
@@ -14590,8 +14713,12 @@
       <c r="BW32" s="5">
         <v>100.35</v>
       </c>
-      <c r="BX32" s="5"/>
-      <c r="BY32" s="5"/>
+      <c r="BX32" s="5">
+        <v>101.6</v>
+      </c>
+      <c r="BY32" s="5">
+        <v>101.15</v>
+      </c>
       <c r="BZ32" s="5"/>
       <c r="CA32" s="5"/>
       <c r="CB32" s="5"/>
@@ -14765,8 +14892,12 @@
       <c r="BW33" s="5">
         <v>58.4</v>
       </c>
-      <c r="BX33" s="5"/>
-      <c r="BY33" s="5"/>
+      <c r="BX33" s="5">
+        <v>57.65</v>
+      </c>
+      <c r="BY33" s="5">
+        <v>58.4</v>
+      </c>
       <c r="BZ33" s="5"/>
       <c r="CA33" s="5"/>
       <c r="CB33" s="5"/>
@@ -14934,8 +15065,12 @@
       <c r="BW34" s="5">
         <v>188.1</v>
       </c>
-      <c r="BX34" s="5"/>
-      <c r="BY34" s="5"/>
+      <c r="BX34" s="5">
+        <v>196.15</v>
+      </c>
+      <c r="BY34" s="5">
+        <v>202.5</v>
+      </c>
       <c r="BZ34" s="5"/>
       <c r="CA34" s="5"/>
       <c r="CB34" s="5"/>
@@ -15099,8 +15234,12 @@
       <c r="BW35" s="5">
         <v>684.9</v>
       </c>
-      <c r="BX35" s="5"/>
-      <c r="BY35" s="5"/>
+      <c r="BX35" s="5">
+        <v>684.75</v>
+      </c>
+      <c r="BY35" s="5">
+        <v>695</v>
+      </c>
       <c r="BZ35" s="5"/>
       <c r="CA35" s="5"/>
       <c r="CB35" s="5"/>
@@ -15246,8 +15385,12 @@
       <c r="BW36" s="5">
         <v>448.9</v>
       </c>
-      <c r="BX36" s="5"/>
-      <c r="BY36" s="5"/>
+      <c r="BX36" s="5">
+        <v>432</v>
+      </c>
+      <c r="BY36" s="5">
+        <v>419</v>
+      </c>
       <c r="BZ36" s="5"/>
       <c r="CA36" s="5"/>
       <c r="CB36" s="5"/>
@@ -15383,8 +15526,12 @@
       <c r="BW37" s="5">
         <v>335.35</v>
       </c>
-      <c r="BX37" s="5"/>
-      <c r="BY37" s="5"/>
+      <c r="BX37" s="5">
+        <v>318</v>
+      </c>
+      <c r="BY37" s="5">
+        <v>302.8</v>
+      </c>
       <c r="BZ37" s="5"/>
       <c r="CA37" s="5"/>
       <c r="CB37" s="5"/>
@@ -15518,8 +15665,12 @@
       <c r="BW38" s="5">
         <v>507.55</v>
       </c>
-      <c r="BX38" s="5"/>
-      <c r="BY38" s="5"/>
+      <c r="BX38" s="5">
+        <v>512</v>
+      </c>
+      <c r="BY38" s="5">
+        <v>506</v>
+      </c>
       <c r="BZ38" s="5"/>
       <c r="CA38" s="5"/>
       <c r="CB38" s="5"/>
@@ -15647,8 +15798,12 @@
       <c r="BW39" s="5">
         <v>76</v>
       </c>
-      <c r="BX39" s="5"/>
-      <c r="BY39" s="5"/>
+      <c r="BX39" s="5">
+        <v>76.650000000000006</v>
+      </c>
+      <c r="BY39" s="5">
+        <v>76.599999999999994</v>
+      </c>
       <c r="BZ39" s="5"/>
       <c r="CA39" s="5"/>
       <c r="CB39" s="5"/>
@@ -15664,7 +15819,7 @@
     <row r="40" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <f t="shared" si="0"/>
-        <v>417.75</v>
+        <v>416</v>
       </c>
       <c r="B40" s="12">
         <f t="shared" si="1"/>
@@ -15672,7 +15827,7 @@
       </c>
       <c r="C40" s="12">
         <f t="shared" ref="C40" si="9">B40-A40</f>
-        <v>54.25</v>
+        <v>56</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>306</v>
@@ -15776,8 +15931,12 @@
       <c r="BW40" s="5">
         <v>426.1</v>
       </c>
-      <c r="BX40" s="5"/>
-      <c r="BY40" s="5"/>
+      <c r="BX40" s="5">
+        <v>416</v>
+      </c>
+      <c r="BY40" s="5">
+        <v>417</v>
+      </c>
       <c r="BZ40" s="5"/>
       <c r="CA40" s="5"/>
       <c r="CB40" s="5"/>
@@ -15901,8 +16060,12 @@
       <c r="BW41" s="5">
         <v>211.6</v>
       </c>
-      <c r="BX41" s="5"/>
-      <c r="BY41" s="5"/>
+      <c r="BX41" s="5">
+        <v>210.3</v>
+      </c>
+      <c r="BY41" s="5">
+        <v>204.5</v>
+      </c>
       <c r="BZ41" s="5"/>
       <c r="CA41" s="5"/>
       <c r="CB41" s="5"/>
@@ -16022,8 +16185,12 @@
       <c r="BW42" s="5">
         <v>37.200000000000003</v>
       </c>
-      <c r="BX42" s="5"/>
-      <c r="BY42" s="5"/>
+      <c r="BX42" s="5">
+        <v>37.65</v>
+      </c>
+      <c r="BY42" s="5">
+        <v>37.65</v>
+      </c>
       <c r="BZ42" s="5"/>
       <c r="CA42" s="5"/>
       <c r="CB42" s="5"/>
@@ -16039,7 +16206,7 @@
     <row r="43" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <f t="shared" si="0"/>
-        <v>577.45000000000005</v>
+        <v>552.04999999999995</v>
       </c>
       <c r="B43" s="12">
         <f t="shared" ref="B43:B44" si="12">MAX(E43:ZW43)</f>
@@ -16047,7 +16214,7 @@
       </c>
       <c r="C43" s="12">
         <f t="shared" si="11"/>
-        <v>49.25</v>
+        <v>74.650000000000091</v>
       </c>
       <c r="D43" s="45" t="s">
         <v>309</v>
@@ -16141,8 +16308,12 @@
       <c r="BW43" s="5">
         <v>607.29999999999995</v>
       </c>
-      <c r="BX43" s="5"/>
-      <c r="BY43" s="5"/>
+      <c r="BX43" s="5">
+        <v>580.04999999999995</v>
+      </c>
+      <c r="BY43" s="5">
+        <v>552.04999999999995</v>
+      </c>
       <c r="BZ43" s="5"/>
       <c r="CA43" s="5"/>
       <c r="CB43" s="5"/>
@@ -16260,8 +16431,12 @@
       <c r="BW44" s="5">
         <v>831.85</v>
       </c>
-      <c r="BX44" s="5"/>
-      <c r="BY44" s="5"/>
+      <c r="BX44" s="5">
+        <v>826</v>
+      </c>
+      <c r="BY44" s="5">
+        <v>837.25</v>
+      </c>
       <c r="BZ44" s="5"/>
       <c r="CA44" s="5"/>
       <c r="CB44" s="5"/>
@@ -16377,8 +16552,12 @@
       <c r="BW45" s="5">
         <v>137.75</v>
       </c>
-      <c r="BX45" s="5"/>
-      <c r="BY45" s="5"/>
+      <c r="BX45" s="5">
+        <v>138.25</v>
+      </c>
+      <c r="BY45" s="5">
+        <v>139.35</v>
+      </c>
       <c r="BZ45" s="5"/>
       <c r="CA45" s="5"/>
       <c r="CB45" s="5"/>
@@ -16394,7 +16573,7 @@
     <row r="46" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <f t="shared" ref="A46" si="13">MIN(E46:ZW46)</f>
-        <v>679</v>
+        <v>667.5</v>
       </c>
       <c r="B46" s="12">
         <f>MAX(E46:ZW46)</f>
@@ -16402,7 +16581,7 @@
       </c>
       <c r="C46" s="12">
         <f t="shared" ref="C46" si="14">B46-A46</f>
-        <v>91</v>
+        <v>102.5</v>
       </c>
       <c r="D46" s="45" t="s">
         <v>313</v>
@@ -16488,8 +16667,12 @@
       <c r="BW46" s="5">
         <v>679</v>
       </c>
-      <c r="BX46" s="5"/>
-      <c r="BY46" s="5"/>
+      <c r="BX46" s="5">
+        <v>668</v>
+      </c>
+      <c r="BY46" s="5">
+        <v>667.5</v>
+      </c>
       <c r="BZ46" s="5"/>
       <c r="CA46" s="5"/>
       <c r="CB46" s="5"/>
@@ -16509,11 +16692,11 @@
       </c>
       <c r="B47" s="12">
         <f>MAX(E47:ZW47)</f>
-        <v>790</v>
+        <v>859.9</v>
       </c>
       <c r="C47" s="12">
         <f t="shared" ref="C47" si="16">B47-A47</f>
-        <v>13.5</v>
+        <v>83.399999999999977</v>
       </c>
       <c r="D47" s="45" t="s">
         <v>328</v>
@@ -16599,8 +16782,12 @@
       <c r="BW47" s="5">
         <v>786</v>
       </c>
-      <c r="BX47" s="5"/>
-      <c r="BY47" s="5"/>
+      <c r="BX47" s="5">
+        <v>811.4</v>
+      </c>
+      <c r="BY47" s="5">
+        <v>859.9</v>
+      </c>
       <c r="BZ47" s="5"/>
       <c r="CA47" s="5"/>
       <c r="CB47" s="5"/>
@@ -16612,6 +16799,113 @@
       <c r="CH47" s="5"/>
       <c r="CI47" s="5"/>
       <c r="CJ47" s="5"/>
+    </row>
+    <row r="48" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A48" s="12">
+        <f t="shared" ref="A48" si="17">MIN(E48:ZW48)</f>
+        <v>109</v>
+      </c>
+      <c r="B48" s="12">
+        <f>MAX(E48:ZW48)</f>
+        <v>110.95</v>
+      </c>
+      <c r="C48" s="12">
+        <f t="shared" ref="C48" si="18">B48-A48</f>
+        <v>1.9500000000000028</v>
+      </c>
+      <c r="D48" s="45" t="s">
+        <v>329</v>
+      </c>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5"/>
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="5"/>
+      <c r="AC48" s="5"/>
+      <c r="AD48" s="5"/>
+      <c r="AE48" s="5"/>
+      <c r="AF48" s="5"/>
+      <c r="AG48" s="5"/>
+      <c r="AH48" s="5"/>
+      <c r="AI48" s="5"/>
+      <c r="AJ48" s="5"/>
+      <c r="AK48" s="5"/>
+      <c r="AL48" s="5"/>
+      <c r="AM48" s="5"/>
+      <c r="AN48" s="5"/>
+      <c r="AO48" s="5"/>
+      <c r="AP48" s="5"/>
+      <c r="AQ48" s="5"/>
+      <c r="AR48" s="5"/>
+      <c r="AS48" s="5"/>
+      <c r="AT48" s="5"/>
+      <c r="AU48" s="5"/>
+      <c r="AV48" s="5"/>
+      <c r="AW48" s="5"/>
+      <c r="AX48" s="5"/>
+      <c r="AY48" s="5"/>
+      <c r="AZ48" s="5"/>
+      <c r="BA48" s="5"/>
+      <c r="BB48" s="5"/>
+      <c r="BC48" s="5"/>
+      <c r="BD48" s="5"/>
+      <c r="BE48" s="5"/>
+      <c r="BF48" s="5"/>
+      <c r="BG48" s="5"/>
+      <c r="BH48" s="5"/>
+      <c r="BI48" s="5"/>
+      <c r="BJ48" s="5"/>
+      <c r="BK48" s="5"/>
+      <c r="BL48" s="5"/>
+      <c r="BM48" s="5"/>
+      <c r="BN48" s="5"/>
+      <c r="BO48" s="5"/>
+      <c r="BP48" s="5"/>
+      <c r="BQ48" s="5"/>
+      <c r="BR48" s="5"/>
+      <c r="BS48" s="5"/>
+      <c r="BT48" s="5"/>
+      <c r="BU48" s="5"/>
+      <c r="BV48" s="5"/>
+      <c r="BW48" s="5">
+        <v>109</v>
+      </c>
+      <c r="BX48" s="5">
+        <v>110.95</v>
+      </c>
+      <c r="BY48" s="5">
+        <v>110.7</v>
+      </c>
+      <c r="BZ48" s="5"/>
+      <c r="CA48" s="5"/>
+      <c r="CB48" s="5"/>
+      <c r="CC48" s="5"/>
+      <c r="CD48" s="5"/>
+      <c r="CE48" s="5"/>
+      <c r="CF48" s="5"/>
+      <c r="CG48" s="5"/>
+      <c r="CH48" s="5"/>
+      <c r="CI48" s="5"/>
+      <c r="CJ48" s="5"/>
     </row>
   </sheetData>
   <sortState ref="L1:L37">

</xml_diff>

<commit_message>
Added details for 22/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -7264,7 +7264,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="BX1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BY2" sqref="BY2:BY48"/>
+      <selection pane="topRight" activeCell="BZ2" sqref="BZ2:BZ48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7801,7 +7801,9 @@
       <c r="BY2" s="5">
         <v>330.3</v>
       </c>
-      <c r="BZ2" s="5"/>
+      <c r="BZ2" s="5">
+        <v>335.5</v>
+      </c>
       <c r="CA2" s="5"/>
       <c r="CB2" s="5"/>
       <c r="CC2" s="5"/>
@@ -8040,7 +8042,9 @@
       <c r="BY3" s="5">
         <v>318.55</v>
       </c>
-      <c r="BZ3" s="5"/>
+      <c r="BZ3" s="5">
+        <v>318.35000000000002</v>
+      </c>
       <c r="CA3" s="5"/>
       <c r="CB3" s="5"/>
       <c r="CC3" s="5"/>
@@ -8285,7 +8289,9 @@
       <c r="BY4" s="5">
         <v>255.5</v>
       </c>
-      <c r="BZ4" s="5"/>
+      <c r="BZ4" s="5">
+        <v>258.5</v>
+      </c>
       <c r="CA4" s="5"/>
       <c r="CB4" s="5"/>
       <c r="CC4" s="5"/>
@@ -8530,7 +8536,9 @@
       <c r="BY5" s="5">
         <v>932.05</v>
       </c>
-      <c r="BZ5" s="5"/>
+      <c r="BZ5" s="5">
+        <v>934.1</v>
+      </c>
       <c r="CA5" s="5"/>
       <c r="CB5" s="5"/>
       <c r="CC5" s="5"/>
@@ -8775,7 +8783,9 @@
       <c r="BY6" s="5">
         <v>273.2</v>
       </c>
-      <c r="BZ6" s="5"/>
+      <c r="BZ6" s="5">
+        <v>271.25</v>
+      </c>
       <c r="CA6" s="5"/>
       <c r="CB6" s="5"/>
       <c r="CC6" s="5"/>
@@ -9020,7 +9030,9 @@
       <c r="BY7" s="5">
         <v>17.25</v>
       </c>
-      <c r="BZ7" s="5"/>
+      <c r="BZ7" s="5">
+        <v>16.95</v>
+      </c>
       <c r="CA7" s="5"/>
       <c r="CB7" s="5"/>
       <c r="CC7" s="5"/>
@@ -9265,7 +9277,9 @@
       <c r="BY8" s="5">
         <v>82.75</v>
       </c>
-      <c r="BZ8" s="5"/>
+      <c r="BZ8" s="5">
+        <v>81.7</v>
+      </c>
       <c r="CA8" s="5"/>
       <c r="CB8" s="5"/>
       <c r="CC8" s="5"/>
@@ -9502,7 +9516,9 @@
       <c r="BY9" s="28">
         <v>54.85</v>
       </c>
-      <c r="BZ9" s="28"/>
+      <c r="BZ9" s="28">
+        <v>54.7</v>
+      </c>
       <c r="CA9" s="28"/>
       <c r="CB9" s="28"/>
       <c r="CC9" s="28"/>
@@ -9747,7 +9763,9 @@
       <c r="BY10" s="5">
         <v>38.15</v>
       </c>
-      <c r="BZ10" s="5"/>
+      <c r="BZ10" s="5">
+        <v>38.35</v>
+      </c>
       <c r="CA10" s="5"/>
       <c r="CB10" s="5"/>
       <c r="CC10" s="5"/>
@@ -9992,7 +10010,9 @@
       <c r="BY11" s="5">
         <v>100.9</v>
       </c>
-      <c r="BZ11" s="5"/>
+      <c r="BZ11" s="5">
+        <v>97.6</v>
+      </c>
       <c r="CA11" s="5"/>
       <c r="CB11" s="5"/>
       <c r="CC11" s="5"/>
@@ -10237,7 +10257,9 @@
       <c r="BY12" s="5">
         <v>87.5</v>
       </c>
-      <c r="BZ12" s="5"/>
+      <c r="BZ12" s="5">
+        <v>89.1</v>
+      </c>
       <c r="CA12" s="5"/>
       <c r="CB12" s="5"/>
       <c r="CC12" s="5"/>
@@ -10482,7 +10504,9 @@
       <c r="BY13" s="5">
         <v>51</v>
       </c>
-      <c r="BZ13" s="5"/>
+      <c r="BZ13" s="5">
+        <v>50.4</v>
+      </c>
       <c r="CA13" s="5"/>
       <c r="CB13" s="5"/>
       <c r="CC13" s="5"/>
@@ -10727,7 +10751,9 @@
       <c r="BY14" s="5">
         <v>35.25</v>
       </c>
-      <c r="BZ14" s="5"/>
+      <c r="BZ14" s="5">
+        <v>34.9</v>
+      </c>
       <c r="CA14" s="5"/>
       <c r="CB14" s="5"/>
       <c r="CC14" s="5"/>
@@ -10742,7 +10768,7 @@
     <row r="15" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
-        <v>24.5</v>
+        <v>23.95</v>
       </c>
       <c r="B15" s="12">
         <f t="shared" si="1"/>
@@ -10750,7 +10776,7 @@
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
-        <v>11.899999999999999</v>
+        <v>12.45</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>126</v>
@@ -10964,7 +10990,9 @@
       <c r="BY15" s="5">
         <v>24.5</v>
       </c>
-      <c r="BZ15" s="5"/>
+      <c r="BZ15" s="5">
+        <v>23.95</v>
+      </c>
       <c r="CA15" s="5"/>
       <c r="CB15" s="5"/>
       <c r="CC15" s="5"/>
@@ -11209,7 +11237,9 @@
       <c r="BY16" s="5">
         <v>711.25</v>
       </c>
-      <c r="BZ16" s="5"/>
+      <c r="BZ16" s="5">
+        <v>711</v>
+      </c>
       <c r="CA16" s="5"/>
       <c r="CB16" s="5"/>
       <c r="CC16" s="5"/>
@@ -11454,7 +11484,9 @@
       <c r="BY17" s="5">
         <v>466.2</v>
       </c>
-      <c r="BZ17" s="5"/>
+      <c r="BZ17" s="5">
+        <v>472</v>
+      </c>
       <c r="CA17" s="5"/>
       <c r="CB17" s="5"/>
       <c r="CC17" s="5"/>
@@ -11699,7 +11731,9 @@
       <c r="BY18" s="5">
         <v>255.9</v>
       </c>
-      <c r="BZ18" s="5"/>
+      <c r="BZ18" s="5">
+        <v>246.5</v>
+      </c>
       <c r="CA18" s="5"/>
       <c r="CB18" s="5"/>
       <c r="CC18" s="5"/>
@@ -11718,11 +11752,11 @@
       </c>
       <c r="B19" s="12">
         <f t="shared" si="1"/>
-        <v>703.7</v>
+        <v>704.5</v>
       </c>
       <c r="C19" s="12">
         <f t="shared" si="2"/>
-        <v>263.00000000000006</v>
+        <v>263.8</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -11944,7 +11978,9 @@
       <c r="BY19" s="5">
         <v>703.7</v>
       </c>
-      <c r="BZ19" s="5"/>
+      <c r="BZ19" s="5">
+        <v>704.5</v>
+      </c>
       <c r="CA19" s="5"/>
       <c r="CB19" s="5"/>
       <c r="CC19" s="5"/>
@@ -12189,7 +12225,9 @@
       <c r="BY20" s="5">
         <v>708.15</v>
       </c>
-      <c r="BZ20" s="5"/>
+      <c r="BZ20" s="5">
+        <v>698.55</v>
+      </c>
       <c r="CA20" s="5"/>
       <c r="CB20" s="5"/>
       <c r="CC20" s="5"/>
@@ -12434,7 +12472,9 @@
       <c r="BY21" s="5">
         <v>503.9</v>
       </c>
-      <c r="BZ21" s="5"/>
+      <c r="BZ21" s="5">
+        <v>499.65</v>
+      </c>
       <c r="CA21" s="5"/>
       <c r="CB21" s="5"/>
       <c r="CC21" s="5"/>
@@ -12625,7 +12665,9 @@
       <c r="BY22" s="5">
         <v>396.6</v>
       </c>
-      <c r="BZ22" s="5"/>
+      <c r="BZ22" s="5">
+        <v>401</v>
+      </c>
       <c r="CA22" s="5"/>
       <c r="CB22" s="5"/>
       <c r="CC22" s="5"/>
@@ -12862,7 +12904,9 @@
       <c r="BY23" s="5">
         <v>62.65</v>
       </c>
-      <c r="BZ23" s="5"/>
+      <c r="BZ23" s="5">
+        <v>61.15</v>
+      </c>
       <c r="CA23" s="5"/>
       <c r="CB23" s="5"/>
       <c r="CC23" s="5"/>
@@ -13095,7 +13139,9 @@
       <c r="BY24" s="5">
         <v>242.55</v>
       </c>
-      <c r="BZ24" s="5"/>
+      <c r="BZ24" s="5">
+        <v>243.55</v>
+      </c>
       <c r="CA24" s="5"/>
       <c r="CB24" s="5"/>
       <c r="CC24" s="5"/>
@@ -13310,7 +13356,9 @@
       <c r="BY25" s="5">
         <v>965.5</v>
       </c>
-      <c r="BZ25" s="5"/>
+      <c r="BZ25" s="5">
+        <v>965.3</v>
+      </c>
       <c r="CA25" s="5"/>
       <c r="CB25" s="5"/>
       <c r="CC25" s="5"/>
@@ -13513,7 +13561,9 @@
       <c r="BY26" s="5">
         <v>92.95</v>
       </c>
-      <c r="BZ26" s="5"/>
+      <c r="BZ26" s="5">
+        <v>89.9</v>
+      </c>
       <c r="CA26" s="5"/>
       <c r="CB26" s="5"/>
       <c r="CC26" s="5"/>
@@ -13716,7 +13766,9 @@
       <c r="BY27" s="5">
         <v>43.35</v>
       </c>
-      <c r="BZ27" s="5"/>
+      <c r="BZ27" s="5">
+        <v>42.7</v>
+      </c>
       <c r="CA27" s="5"/>
       <c r="CB27" s="5"/>
       <c r="CC27" s="5"/>
@@ -13919,7 +13971,9 @@
       <c r="BY28" s="5">
         <v>125.95</v>
       </c>
-      <c r="BZ28" s="5"/>
+      <c r="BZ28" s="5">
+        <v>124.6</v>
+      </c>
       <c r="CA28" s="5"/>
       <c r="CB28" s="5"/>
       <c r="CC28" s="5"/>
@@ -14122,7 +14176,9 @@
       <c r="BY29" s="5">
         <v>73.599999999999994</v>
       </c>
-      <c r="BZ29" s="5"/>
+      <c r="BZ29" s="5">
+        <v>74.5</v>
+      </c>
       <c r="CA29" s="5"/>
       <c r="CB29" s="5"/>
       <c r="CC29" s="5"/>
@@ -14325,7 +14381,9 @@
       <c r="BY30" s="5">
         <v>41.35</v>
       </c>
-      <c r="BZ30" s="5"/>
+      <c r="BZ30" s="5">
+        <v>41.1</v>
+      </c>
       <c r="CA30" s="5"/>
       <c r="CB30" s="5"/>
       <c r="CC30" s="5"/>
@@ -14340,7 +14398,7 @@
     <row r="31" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
-        <v>128.9</v>
+        <v>125.3</v>
       </c>
       <c r="B31" s="12">
         <f t="shared" si="1"/>
@@ -14348,7 +14406,7 @@
       </c>
       <c r="C31" s="12">
         <f t="shared" si="2"/>
-        <v>27.949999999999989</v>
+        <v>31.549999999999997</v>
       </c>
       <c r="D31" s="45" t="s">
         <v>257</v>
@@ -14528,7 +14586,9 @@
       <c r="BY31" s="5">
         <v>128.9</v>
       </c>
-      <c r="BZ31" s="5"/>
+      <c r="BZ31" s="5">
+        <v>125.3</v>
+      </c>
       <c r="CA31" s="5"/>
       <c r="CB31" s="5"/>
       <c r="CC31" s="5"/>
@@ -14719,7 +14779,9 @@
       <c r="BY32" s="5">
         <v>101.15</v>
       </c>
-      <c r="BZ32" s="5"/>
+      <c r="BZ32" s="5">
+        <v>101.05</v>
+      </c>
       <c r="CA32" s="5"/>
       <c r="CB32" s="5"/>
       <c r="CC32" s="5"/>
@@ -14898,7 +14960,9 @@
       <c r="BY33" s="5">
         <v>58.4</v>
       </c>
-      <c r="BZ33" s="5"/>
+      <c r="BZ33" s="5">
+        <v>60.2</v>
+      </c>
       <c r="CA33" s="5"/>
       <c r="CB33" s="5"/>
       <c r="CC33" s="5"/>
@@ -15071,7 +15135,9 @@
       <c r="BY34" s="5">
         <v>202.5</v>
       </c>
-      <c r="BZ34" s="5"/>
+      <c r="BZ34" s="5">
+        <v>197.7</v>
+      </c>
       <c r="CA34" s="5"/>
       <c r="CB34" s="5"/>
       <c r="CC34" s="5"/>
@@ -15240,7 +15306,9 @@
       <c r="BY35" s="5">
         <v>695</v>
       </c>
-      <c r="BZ35" s="5"/>
+      <c r="BZ35" s="5">
+        <v>699</v>
+      </c>
       <c r="CA35" s="5"/>
       <c r="CB35" s="5"/>
       <c r="CC35" s="5"/>
@@ -15391,7 +15459,9 @@
       <c r="BY36" s="5">
         <v>419</v>
       </c>
-      <c r="BZ36" s="5"/>
+      <c r="BZ36" s="5">
+        <v>434.5</v>
+      </c>
       <c r="CA36" s="5"/>
       <c r="CB36" s="5"/>
       <c r="CC36" s="5"/>
@@ -15532,7 +15602,9 @@
       <c r="BY37" s="5">
         <v>302.8</v>
       </c>
-      <c r="BZ37" s="5"/>
+      <c r="BZ37" s="5">
+        <v>319.3</v>
+      </c>
       <c r="CA37" s="5"/>
       <c r="CB37" s="5"/>
       <c r="CC37" s="5"/>
@@ -15671,7 +15743,9 @@
       <c r="BY38" s="5">
         <v>506</v>
       </c>
-      <c r="BZ38" s="5"/>
+      <c r="BZ38" s="5">
+        <v>500</v>
+      </c>
       <c r="CA38" s="5"/>
       <c r="CB38" s="5"/>
       <c r="CC38" s="5"/>
@@ -15804,7 +15878,9 @@
       <c r="BY39" s="5">
         <v>76.599999999999994</v>
       </c>
-      <c r="BZ39" s="5"/>
+      <c r="BZ39" s="5">
+        <v>76.599999999999994</v>
+      </c>
       <c r="CA39" s="5"/>
       <c r="CB39" s="5"/>
       <c r="CC39" s="5"/>
@@ -15937,7 +16013,9 @@
       <c r="BY40" s="5">
         <v>417</v>
       </c>
-      <c r="BZ40" s="5"/>
+      <c r="BZ40" s="5">
+        <v>416.8</v>
+      </c>
       <c r="CA40" s="5"/>
       <c r="CB40" s="5"/>
       <c r="CC40" s="5"/>
@@ -16066,7 +16144,9 @@
       <c r="BY41" s="5">
         <v>204.5</v>
       </c>
-      <c r="BZ41" s="5"/>
+      <c r="BZ41" s="5">
+        <v>208</v>
+      </c>
       <c r="CA41" s="5"/>
       <c r="CB41" s="5"/>
       <c r="CC41" s="5"/>
@@ -16191,7 +16271,9 @@
       <c r="BY42" s="5">
         <v>37.65</v>
       </c>
-      <c r="BZ42" s="5"/>
+      <c r="BZ42" s="5">
+        <v>37.15</v>
+      </c>
       <c r="CA42" s="5"/>
       <c r="CB42" s="5"/>
       <c r="CC42" s="5"/>
@@ -16314,7 +16396,9 @@
       <c r="BY43" s="5">
         <v>552.04999999999995</v>
       </c>
-      <c r="BZ43" s="5"/>
+      <c r="BZ43" s="5">
+        <v>580.1</v>
+      </c>
       <c r="CA43" s="5"/>
       <c r="CB43" s="5"/>
       <c r="CC43" s="5"/>
@@ -16437,7 +16521,9 @@
       <c r="BY44" s="5">
         <v>837.25</v>
       </c>
-      <c r="BZ44" s="5"/>
+      <c r="BZ44" s="5">
+        <v>828.3</v>
+      </c>
       <c r="CA44" s="5"/>
       <c r="CB44" s="5"/>
       <c r="CC44" s="5"/>
@@ -16558,7 +16644,9 @@
       <c r="BY45" s="5">
         <v>139.35</v>
       </c>
-      <c r="BZ45" s="5"/>
+      <c r="BZ45" s="5">
+        <v>138.19999999999999</v>
+      </c>
       <c r="CA45" s="5"/>
       <c r="CB45" s="5"/>
       <c r="CC45" s="5"/>
@@ -16573,7 +16661,7 @@
     <row r="46" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <f t="shared" ref="A46" si="13">MIN(E46:ZW46)</f>
-        <v>667.5</v>
+        <v>663.95</v>
       </c>
       <c r="B46" s="12">
         <f>MAX(E46:ZW46)</f>
@@ -16581,7 +16669,7 @@
       </c>
       <c r="C46" s="12">
         <f t="shared" ref="C46" si="14">B46-A46</f>
-        <v>102.5</v>
+        <v>106.04999999999995</v>
       </c>
       <c r="D46" s="45" t="s">
         <v>313</v>
@@ -16673,7 +16761,9 @@
       <c r="BY46" s="5">
         <v>667.5</v>
       </c>
-      <c r="BZ46" s="5"/>
+      <c r="BZ46" s="5">
+        <v>663.95</v>
+      </c>
       <c r="CA46" s="5"/>
       <c r="CB46" s="5"/>
       <c r="CC46" s="5"/>
@@ -16788,7 +16878,9 @@
       <c r="BY47" s="5">
         <v>859.9</v>
       </c>
-      <c r="BZ47" s="5"/>
+      <c r="BZ47" s="5">
+        <v>852</v>
+      </c>
       <c r="CA47" s="5"/>
       <c r="CB47" s="5"/>
       <c r="CC47" s="5"/>
@@ -16895,7 +16987,9 @@
       <c r="BY48" s="5">
         <v>110.7</v>
       </c>
-      <c r="BZ48" s="5"/>
+      <c r="BZ48" s="5">
+        <v>109.5</v>
+      </c>
       <c r="CA48" s="5"/>
       <c r="CB48" s="5"/>
       <c r="CC48" s="5"/>

</xml_diff>

<commit_message>
Added details for 23/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="329">
   <si>
     <t>Date</t>
   </si>
@@ -991,9 +991,6 @@
   </si>
   <si>
     <t>22/11/2022</t>
-  </si>
-  <si>
-    <t>23/11/2023</t>
   </si>
   <si>
     <t>24/11/2024</t>
@@ -7260,11 +7257,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CJ48"/>
+  <dimension ref="A1:CI48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="BX1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BZ2" sqref="BZ2:BZ48"/>
+      <pane xSplit="4" topLeftCell="BT1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CA2" sqref="CA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7311,12 +7308,12 @@
     <col min="75" max="75" width="13.42578125" customWidth="1"/>
     <col min="76" max="76" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="78" max="79" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="14.42578125" customWidth="1"/>
-    <col min="81" max="84" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="14.42578125" customWidth="1"/>
+    <col min="80" max="83" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:87" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>249</v>
       </c>
@@ -7566,21 +7563,18 @@
       <c r="CE1" s="49" t="s">
         <v>326</v>
       </c>
-      <c r="CF1" s="49" t="s">
-        <v>327</v>
-      </c>
+      <c r="CF1" s="27"/>
       <c r="CG1" s="27"/>
       <c r="CH1" s="27"/>
       <c r="CI1" s="27"/>
-      <c r="CJ1" s="27"/>
-    </row>
-    <row r="2" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
-        <f t="shared" ref="A2:A45" si="0">MIN(E2:ZW2)</f>
+        <f>MIN(E2:ZV2)</f>
         <v>243.6</v>
       </c>
       <c r="B2" s="12">
-        <f t="shared" ref="B2:B42" si="1">MAX(E2:ZW2)</f>
+        <f>MAX(E2:ZV2)</f>
         <v>340.8</v>
       </c>
       <c r="C2" s="12">
@@ -7804,7 +7798,9 @@
       <c r="BZ2" s="5">
         <v>335.5</v>
       </c>
-      <c r="CA2" s="5"/>
+      <c r="CA2" s="5">
+        <v>332.1</v>
+      </c>
       <c r="CB2" s="5"/>
       <c r="CC2" s="5"/>
       <c r="CD2" s="5"/>
@@ -7813,19 +7809,18 @@
       <c r="CG2" s="5"/>
       <c r="CH2" s="5"/>
       <c r="CI2" s="5"/>
-      <c r="CJ2" s="5"/>
-    </row>
-    <row r="3" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E3:ZV3)</f>
         <v>262.7</v>
       </c>
       <c r="B3" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E3:ZV3)</f>
         <v>328.85</v>
       </c>
       <c r="C3" s="12">
-        <f t="shared" ref="C3:C33" si="2">B3-A3</f>
+        <f t="shared" ref="C3:C33" si="0">B3-A3</f>
         <v>66.150000000000034</v>
       </c>
       <c r="D3" s="44" t="s">
@@ -8045,7 +8040,9 @@
       <c r="BZ3" s="5">
         <v>318.35000000000002</v>
       </c>
-      <c r="CA3" s="5"/>
+      <c r="CA3" s="5">
+        <v>316.85000000000002</v>
+      </c>
       <c r="CB3" s="5"/>
       <c r="CC3" s="5"/>
       <c r="CD3" s="5"/>
@@ -8054,19 +8051,18 @@
       <c r="CG3" s="5"/>
       <c r="CH3" s="5"/>
       <c r="CI3" s="5"/>
-      <c r="CJ3" s="5"/>
-    </row>
-    <row r="4" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
+        <f>MIN(E4:ZV4)</f>
+        <v>253.85</v>
+      </c>
+      <c r="B4" s="12">
+        <f>MAX(E4:ZV4)</f>
+        <v>291.7</v>
+      </c>
+      <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>253.85</v>
-      </c>
-      <c r="B4" s="12">
-        <f t="shared" si="1"/>
-        <v>291.7</v>
-      </c>
-      <c r="C4" s="12">
-        <f t="shared" si="2"/>
         <v>37.849999999999994</v>
       </c>
       <c r="D4" s="44" t="s">
@@ -8292,7 +8288,9 @@
       <c r="BZ4" s="5">
         <v>258.5</v>
       </c>
-      <c r="CA4" s="5"/>
+      <c r="CA4" s="5">
+        <v>260.64999999999998</v>
+      </c>
       <c r="CB4" s="5"/>
       <c r="CC4" s="5"/>
       <c r="CD4" s="5"/>
@@ -8301,20 +8299,19 @@
       <c r="CG4" s="5"/>
       <c r="CH4" s="5"/>
       <c r="CI4" s="5"/>
-      <c r="CJ4" s="5"/>
-    </row>
-    <row r="5" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
+        <f>MIN(E5:ZV5)</f>
+        <v>786.25</v>
+      </c>
+      <c r="B5" s="12">
+        <f>MAX(E5:ZV5)</f>
+        <v>951.25</v>
+      </c>
+      <c r="C5" s="12">
         <f t="shared" si="0"/>
-        <v>786.25</v>
-      </c>
-      <c r="B5" s="12">
-        <f t="shared" si="1"/>
-        <v>946.8</v>
-      </c>
-      <c r="C5" s="12">
-        <f t="shared" si="2"/>
-        <v>160.54999999999995</v>
+        <v>165</v>
       </c>
       <c r="D5" s="44" t="s">
         <v>105</v>
@@ -8539,7 +8536,9 @@
       <c r="BZ5" s="5">
         <v>934.1</v>
       </c>
-      <c r="CA5" s="5"/>
+      <c r="CA5" s="5">
+        <v>951.25</v>
+      </c>
       <c r="CB5" s="5"/>
       <c r="CC5" s="5"/>
       <c r="CD5" s="5"/>
@@ -8548,19 +8547,18 @@
       <c r="CG5" s="5"/>
       <c r="CH5" s="5"/>
       <c r="CI5" s="5"/>
-      <c r="CJ5" s="5"/>
-    </row>
-    <row r="6" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
+        <f>MIN(E6:ZV6)</f>
+        <v>236.45</v>
+      </c>
+      <c r="B6" s="12">
+        <f>MAX(E6:ZV6)</f>
+        <v>293.95</v>
+      </c>
+      <c r="C6" s="12">
         <f t="shared" si="0"/>
-        <v>236.45</v>
-      </c>
-      <c r="B6" s="12">
-        <f t="shared" si="1"/>
-        <v>293.95</v>
-      </c>
-      <c r="C6" s="12">
-        <f t="shared" si="2"/>
         <v>57.5</v>
       </c>
       <c r="D6" s="45" t="s">
@@ -8786,7 +8784,9 @@
       <c r="BZ6" s="5">
         <v>271.25</v>
       </c>
-      <c r="CA6" s="5"/>
+      <c r="CA6" s="5">
+        <v>271.64999999999998</v>
+      </c>
       <c r="CB6" s="5"/>
       <c r="CC6" s="5"/>
       <c r="CD6" s="5"/>
@@ -8795,19 +8795,18 @@
       <c r="CG6" s="5"/>
       <c r="CH6" s="5"/>
       <c r="CI6" s="5"/>
-      <c r="CJ6" s="5"/>
-    </row>
-    <row r="7" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
+        <f>MIN(E7:ZV7)</f>
+        <v>15.6</v>
+      </c>
+      <c r="B7" s="12">
+        <f>MAX(E7:ZV7)</f>
+        <v>19.350000000000001</v>
+      </c>
+      <c r="C7" s="12">
         <f t="shared" si="0"/>
-        <v>15.6</v>
-      </c>
-      <c r="B7" s="12">
-        <f t="shared" si="1"/>
-        <v>19.350000000000001</v>
-      </c>
-      <c r="C7" s="12">
-        <f t="shared" si="2"/>
         <v>3.7500000000000018</v>
       </c>
       <c r="D7" s="45" t="s">
@@ -9033,7 +9032,9 @@
       <c r="BZ7" s="5">
         <v>16.95</v>
       </c>
-      <c r="CA7" s="5"/>
+      <c r="CA7" s="5">
+        <v>18.649999999999999</v>
+      </c>
       <c r="CB7" s="5"/>
       <c r="CC7" s="5"/>
       <c r="CD7" s="5"/>
@@ -9042,19 +9043,18 @@
       <c r="CG7" s="5"/>
       <c r="CH7" s="5"/>
       <c r="CI7" s="5"/>
-      <c r="CJ7" s="5"/>
-    </row>
-    <row r="8" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
+        <f>MIN(E8:ZV8)</f>
+        <v>53.4</v>
+      </c>
+      <c r="B8" s="12">
+        <f>MAX(E8:ZV8)</f>
+        <v>86.75</v>
+      </c>
+      <c r="C8" s="12">
         <f t="shared" si="0"/>
-        <v>53.4</v>
-      </c>
-      <c r="B8" s="12">
-        <f t="shared" si="1"/>
-        <v>86.75</v>
-      </c>
-      <c r="C8" s="12">
-        <f t="shared" si="2"/>
         <v>33.35</v>
       </c>
       <c r="D8" s="45" t="s">
@@ -9280,7 +9280,9 @@
       <c r="BZ8" s="5">
         <v>81.7</v>
       </c>
-      <c r="CA8" s="5"/>
+      <c r="CA8" s="5">
+        <v>82.3</v>
+      </c>
       <c r="CB8" s="5"/>
       <c r="CC8" s="5"/>
       <c r="CD8" s="5"/>
@@ -9289,19 +9291,18 @@
       <c r="CG8" s="5"/>
       <c r="CH8" s="5"/>
       <c r="CI8" s="5"/>
-      <c r="CJ8" s="5"/>
-    </row>
-    <row r="9" spans="1:88" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:87" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
+        <f>MIN(E9:ZV9)</f>
+        <v>53.5</v>
+      </c>
+      <c r="B9" s="39">
+        <f>MAX(E9:ZV9)</f>
+        <v>61</v>
+      </c>
+      <c r="C9" s="12">
         <f t="shared" si="0"/>
-        <v>53.5</v>
-      </c>
-      <c r="B9" s="39">
-        <f t="shared" si="1"/>
-        <v>61</v>
-      </c>
-      <c r="C9" s="12">
-        <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
       <c r="D9" s="43" t="s">
@@ -9519,7 +9520,9 @@
       <c r="BZ9" s="28">
         <v>54.7</v>
       </c>
-      <c r="CA9" s="28"/>
+      <c r="CA9" s="28">
+        <v>54.65</v>
+      </c>
       <c r="CB9" s="28"/>
       <c r="CC9" s="28"/>
       <c r="CD9" s="28"/>
@@ -9528,19 +9531,18 @@
       <c r="CG9" s="28"/>
       <c r="CH9" s="28"/>
       <c r="CI9" s="28"/>
-      <c r="CJ9" s="28"/>
-    </row>
-    <row r="10" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
+        <f>MIN(E10:ZV10)</f>
+        <v>35.549999999999997</v>
+      </c>
+      <c r="B10" s="12">
+        <f>MAX(E10:ZV10)</f>
+        <v>45.35</v>
+      </c>
+      <c r="C10" s="12">
         <f t="shared" si="0"/>
-        <v>35.549999999999997</v>
-      </c>
-      <c r="B10" s="12">
-        <f t="shared" si="1"/>
-        <v>45.35</v>
-      </c>
-      <c r="C10" s="12">
-        <f t="shared" si="2"/>
         <v>9.8000000000000043</v>
       </c>
       <c r="D10" s="45" t="s">
@@ -9766,7 +9768,9 @@
       <c r="BZ10" s="5">
         <v>38.35</v>
       </c>
-      <c r="CA10" s="5"/>
+      <c r="CA10" s="5">
+        <v>38.35</v>
+      </c>
       <c r="CB10" s="5"/>
       <c r="CC10" s="5"/>
       <c r="CD10" s="5"/>
@@ -9775,19 +9779,18 @@
       <c r="CG10" s="5"/>
       <c r="CH10" s="5"/>
       <c r="CI10" s="5"/>
-      <c r="CJ10" s="5"/>
-    </row>
-    <row r="11" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
+        <f>MIN(E11:ZV11)</f>
+        <v>72.650000000000006</v>
+      </c>
+      <c r="B11" s="12">
+        <f>MAX(E11:ZV11)</f>
+        <v>106.5</v>
+      </c>
+      <c r="C11" s="12">
         <f t="shared" si="0"/>
-        <v>72.650000000000006</v>
-      </c>
-      <c r="B11" s="12">
-        <f t="shared" si="1"/>
-        <v>106.5</v>
-      </c>
-      <c r="C11" s="12">
-        <f t="shared" si="2"/>
         <v>33.849999999999994</v>
       </c>
       <c r="D11" s="45" t="s">
@@ -10013,7 +10016,9 @@
       <c r="BZ11" s="5">
         <v>97.6</v>
       </c>
-      <c r="CA11" s="5"/>
+      <c r="CA11" s="5">
+        <v>94.6</v>
+      </c>
       <c r="CB11" s="5"/>
       <c r="CC11" s="5"/>
       <c r="CD11" s="5"/>
@@ -10022,19 +10027,18 @@
       <c r="CG11" s="5"/>
       <c r="CH11" s="5"/>
       <c r="CI11" s="5"/>
-      <c r="CJ11" s="5"/>
-    </row>
-    <row r="12" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
+        <f>MIN(E12:ZV12)</f>
+        <v>82.65</v>
+      </c>
+      <c r="B12" s="12">
+        <f>MAX(E12:ZV12)</f>
+        <v>99.6</v>
+      </c>
+      <c r="C12" s="12">
         <f t="shared" si="0"/>
-        <v>82.65</v>
-      </c>
-      <c r="B12" s="12">
-        <f t="shared" si="1"/>
-        <v>99.6</v>
-      </c>
-      <c r="C12" s="12">
-        <f t="shared" si="2"/>
         <v>16.949999999999989</v>
       </c>
       <c r="D12" s="45" t="s">
@@ -10260,7 +10264,9 @@
       <c r="BZ12" s="5">
         <v>89.1</v>
       </c>
-      <c r="CA12" s="5"/>
+      <c r="CA12" s="5">
+        <v>92.1</v>
+      </c>
       <c r="CB12" s="5"/>
       <c r="CC12" s="5"/>
       <c r="CD12" s="5"/>
@@ -10269,19 +10275,18 @@
       <c r="CG12" s="5"/>
       <c r="CH12" s="5"/>
       <c r="CI12" s="5"/>
-      <c r="CJ12" s="5"/>
-    </row>
-    <row r="13" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
+        <f>MIN(E13:ZV13)</f>
+        <v>44.1</v>
+      </c>
+      <c r="B13" s="12">
+        <f>MAX(E13:ZV13)</f>
+        <v>57.15</v>
+      </c>
+      <c r="C13" s="12">
         <f t="shared" si="0"/>
-        <v>44.1</v>
-      </c>
-      <c r="B13" s="12">
-        <f t="shared" si="1"/>
-        <v>57.15</v>
-      </c>
-      <c r="C13" s="12">
-        <f t="shared" si="2"/>
         <v>13.049999999999997</v>
       </c>
       <c r="D13" s="45" t="s">
@@ -10507,7 +10512,9 @@
       <c r="BZ13" s="5">
         <v>50.4</v>
       </c>
-      <c r="CA13" s="5"/>
+      <c r="CA13" s="5">
+        <v>52</v>
+      </c>
       <c r="CB13" s="5"/>
       <c r="CC13" s="5"/>
       <c r="CD13" s="5"/>
@@ -10516,19 +10523,18 @@
       <c r="CG13" s="5"/>
       <c r="CH13" s="5"/>
       <c r="CI13" s="5"/>
-      <c r="CJ13" s="5"/>
-    </row>
-    <row r="14" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
+        <f>MIN(E14:ZV14)</f>
+        <v>29.75</v>
+      </c>
+      <c r="B14" s="12">
+        <f>MAX(E14:ZV14)</f>
+        <v>41.85</v>
+      </c>
+      <c r="C14" s="12">
         <f t="shared" si="0"/>
-        <v>29.75</v>
-      </c>
-      <c r="B14" s="12">
-        <f t="shared" si="1"/>
-        <v>41.85</v>
-      </c>
-      <c r="C14" s="12">
-        <f t="shared" si="2"/>
         <v>12.100000000000001</v>
       </c>
       <c r="D14" s="45" t="s">
@@ -10754,7 +10760,9 @@
       <c r="BZ14" s="5">
         <v>34.9</v>
       </c>
-      <c r="CA14" s="5"/>
+      <c r="CA14" s="5">
+        <v>34.9</v>
+      </c>
       <c r="CB14" s="5"/>
       <c r="CC14" s="5"/>
       <c r="CD14" s="5"/>
@@ -10763,19 +10771,18 @@
       <c r="CG14" s="5"/>
       <c r="CH14" s="5"/>
       <c r="CI14" s="5"/>
-      <c r="CJ14" s="5"/>
-    </row>
-    <row r="15" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
+        <f>MIN(E15:ZV15)</f>
+        <v>23.95</v>
+      </c>
+      <c r="B15" s="12">
+        <f>MAX(E15:ZV15)</f>
+        <v>36.4</v>
+      </c>
+      <c r="C15" s="12">
         <f t="shared" si="0"/>
-        <v>23.95</v>
-      </c>
-      <c r="B15" s="12">
-        <f t="shared" si="1"/>
-        <v>36.4</v>
-      </c>
-      <c r="C15" s="12">
-        <f t="shared" si="2"/>
         <v>12.45</v>
       </c>
       <c r="D15" s="45" t="s">
@@ -10993,7 +11000,9 @@
       <c r="BZ15" s="5">
         <v>23.95</v>
       </c>
-      <c r="CA15" s="5"/>
+      <c r="CA15" s="5">
+        <v>25.6</v>
+      </c>
       <c r="CB15" s="5"/>
       <c r="CC15" s="5"/>
       <c r="CD15" s="5"/>
@@ -11002,19 +11011,18 @@
       <c r="CG15" s="5"/>
       <c r="CH15" s="5"/>
       <c r="CI15" s="5"/>
-      <c r="CJ15" s="5"/>
-    </row>
-    <row r="16" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
+        <f>MIN(E16:ZV16)</f>
+        <v>552</v>
+      </c>
+      <c r="B16" s="12">
+        <f>MAX(E16:ZV16)</f>
+        <v>729.5</v>
+      </c>
+      <c r="C16" s="12">
         <f t="shared" si="0"/>
-        <v>552</v>
-      </c>
-      <c r="B16" s="12">
-        <f t="shared" si="1"/>
-        <v>729.5</v>
-      </c>
-      <c r="C16" s="12">
-        <f t="shared" si="2"/>
         <v>177.5</v>
       </c>
       <c r="D16" s="45" t="s">
@@ -11240,7 +11248,9 @@
       <c r="BZ16" s="5">
         <v>711</v>
       </c>
-      <c r="CA16" s="5"/>
+      <c r="CA16" s="5">
+        <v>708.1</v>
+      </c>
       <c r="CB16" s="5"/>
       <c r="CC16" s="5"/>
       <c r="CD16" s="5"/>
@@ -11249,19 +11259,18 @@
       <c r="CG16" s="5"/>
       <c r="CH16" s="5"/>
       <c r="CI16" s="5"/>
-      <c r="CJ16" s="5"/>
-    </row>
-    <row r="17" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
+        <f>MIN(E17:ZV17)</f>
+        <v>433</v>
+      </c>
+      <c r="B17" s="12">
+        <f>MAX(E17:ZV17)</f>
+        <v>670</v>
+      </c>
+      <c r="C17" s="12">
         <f t="shared" si="0"/>
-        <v>433</v>
-      </c>
-      <c r="B17" s="12">
-        <f t="shared" si="1"/>
-        <v>670</v>
-      </c>
-      <c r="C17" s="12">
-        <f t="shared" si="2"/>
         <v>237</v>
       </c>
       <c r="D17" s="44" t="s">
@@ -11487,7 +11496,9 @@
       <c r="BZ17" s="5">
         <v>472</v>
       </c>
-      <c r="CA17" s="5"/>
+      <c r="CA17" s="5">
+        <v>470</v>
+      </c>
       <c r="CB17" s="5"/>
       <c r="CC17" s="5"/>
       <c r="CD17" s="5"/>
@@ -11496,19 +11507,18 @@
       <c r="CG17" s="5"/>
       <c r="CH17" s="5"/>
       <c r="CI17" s="5"/>
-      <c r="CJ17" s="5"/>
-    </row>
-    <row r="18" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
+        <f>MIN(E18:ZV18)</f>
+        <v>178.8</v>
+      </c>
+      <c r="B18" s="12">
+        <f>MAX(E18:ZV18)</f>
+        <v>302.2</v>
+      </c>
+      <c r="C18" s="12">
         <f t="shared" si="0"/>
-        <v>178.8</v>
-      </c>
-      <c r="B18" s="12">
-        <f t="shared" si="1"/>
-        <v>302.2</v>
-      </c>
-      <c r="C18" s="12">
-        <f t="shared" si="2"/>
         <v>123.39999999999998</v>
       </c>
       <c r="D18" s="44" t="s">
@@ -11734,7 +11744,9 @@
       <c r="BZ18" s="5">
         <v>246.5</v>
       </c>
-      <c r="CA18" s="5"/>
+      <c r="CA18" s="5">
+        <v>260.60000000000002</v>
+      </c>
       <c r="CB18" s="5"/>
       <c r="CC18" s="5"/>
       <c r="CD18" s="5"/>
@@ -11743,20 +11755,19 @@
       <c r="CG18" s="5"/>
       <c r="CH18" s="5"/>
       <c r="CI18" s="5"/>
-      <c r="CJ18" s="5"/>
-    </row>
-    <row r="19" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
+        <f>MIN(E19:ZV19)</f>
+        <v>440.7</v>
+      </c>
+      <c r="B19" s="12">
+        <f>MAX(E19:ZV19)</f>
+        <v>710.3</v>
+      </c>
+      <c r="C19" s="12">
         <f t="shared" si="0"/>
-        <v>440.7</v>
-      </c>
-      <c r="B19" s="12">
-        <f t="shared" si="1"/>
-        <v>704.5</v>
-      </c>
-      <c r="C19" s="12">
-        <f t="shared" si="2"/>
-        <v>263.8</v>
+        <v>269.59999999999997</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -11981,7 +11992,9 @@
       <c r="BZ19" s="5">
         <v>704.5</v>
       </c>
-      <c r="CA19" s="5"/>
+      <c r="CA19" s="5">
+        <v>710.3</v>
+      </c>
       <c r="CB19" s="5"/>
       <c r="CC19" s="5"/>
       <c r="CD19" s="5"/>
@@ -11990,19 +12003,18 @@
       <c r="CG19" s="5"/>
       <c r="CH19" s="5"/>
       <c r="CI19" s="5"/>
-      <c r="CJ19" s="5"/>
-    </row>
-    <row r="20" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
+        <f>MIN(E20:ZV20)</f>
+        <v>677</v>
+      </c>
+      <c r="B20" s="12">
+        <f>MAX(E20:ZV20)</f>
+        <v>795.95</v>
+      </c>
+      <c r="C20" s="12">
         <f t="shared" si="0"/>
-        <v>677</v>
-      </c>
-      <c r="B20" s="12">
-        <f t="shared" si="1"/>
-        <v>795.95</v>
-      </c>
-      <c r="C20" s="12">
-        <f t="shared" si="2"/>
         <v>118.95000000000005</v>
       </c>
       <c r="D20" s="44" t="s">
@@ -12228,7 +12240,9 @@
       <c r="BZ20" s="5">
         <v>698.55</v>
       </c>
-      <c r="CA20" s="5"/>
+      <c r="CA20" s="5">
+        <v>717</v>
+      </c>
       <c r="CB20" s="5"/>
       <c r="CC20" s="5"/>
       <c r="CD20" s="5"/>
@@ -12237,19 +12251,18 @@
       <c r="CG20" s="5"/>
       <c r="CH20" s="5"/>
       <c r="CI20" s="5"/>
-      <c r="CJ20" s="5"/>
-    </row>
-    <row r="21" spans="1:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
+        <f>MIN(E21:ZV21)</f>
+        <v>376.7</v>
+      </c>
+      <c r="B21" s="12">
+        <f>MAX(E21:ZV21)</f>
+        <v>547.5</v>
+      </c>
+      <c r="C21" s="12">
         <f t="shared" si="0"/>
-        <v>376.7</v>
-      </c>
-      <c r="B21" s="12">
-        <f t="shared" si="1"/>
-        <v>547.5</v>
-      </c>
-      <c r="C21" s="12">
-        <f t="shared" si="2"/>
         <v>170.8</v>
       </c>
       <c r="D21" s="44" t="s">
@@ -12475,7 +12488,9 @@
       <c r="BZ21" s="5">
         <v>499.65</v>
       </c>
-      <c r="CA21" s="5"/>
+      <c r="CA21" s="5">
+        <v>496.75</v>
+      </c>
       <c r="CB21" s="5"/>
       <c r="CC21" s="5"/>
       <c r="CD21" s="5"/>
@@ -12484,20 +12499,19 @@
       <c r="CG21" s="5"/>
       <c r="CH21" s="5"/>
       <c r="CI21" s="5"/>
-      <c r="CJ21" s="5"/>
-    </row>
-    <row r="22" spans="1:88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
+        <f>MIN(E22:ZV22)</f>
+        <v>315.2</v>
+      </c>
+      <c r="B22" s="12">
+        <f>MAX(E22:ZV22)</f>
+        <v>413.5</v>
+      </c>
+      <c r="C22" s="12">
         <f t="shared" si="0"/>
-        <v>315.2</v>
-      </c>
-      <c r="B22" s="12">
-        <f t="shared" si="1"/>
-        <v>406.95</v>
-      </c>
-      <c r="C22" s="12">
-        <f t="shared" si="2"/>
-        <v>91.75</v>
+        <v>98.300000000000011</v>
       </c>
       <c r="D22" s="44" t="s">
         <v>269</v>
@@ -12668,7 +12682,9 @@
       <c r="BZ22" s="5">
         <v>401</v>
       </c>
-      <c r="CA22" s="5"/>
+      <c r="CA22" s="5">
+        <v>413.5</v>
+      </c>
       <c r="CB22" s="5"/>
       <c r="CC22" s="5"/>
       <c r="CD22" s="5"/>
@@ -12677,19 +12693,18 @@
       <c r="CG22" s="5"/>
       <c r="CH22" s="5"/>
       <c r="CI22" s="5"/>
-      <c r="CJ22" s="5"/>
-    </row>
-    <row r="23" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
+        <f>MIN(E23:ZV23)</f>
+        <v>54.45</v>
+      </c>
+      <c r="B23" s="12">
+        <f>MAX(E23:ZV23)</f>
+        <v>85.65</v>
+      </c>
+      <c r="C23" s="12">
         <f t="shared" si="0"/>
-        <v>54.45</v>
-      </c>
-      <c r="B23" s="12">
-        <f t="shared" si="1"/>
-        <v>85.65</v>
-      </c>
-      <c r="C23" s="12">
-        <f t="shared" si="2"/>
         <v>31.200000000000003</v>
       </c>
       <c r="D23" s="45" t="s">
@@ -12907,7 +12922,9 @@
       <c r="BZ23" s="5">
         <v>61.15</v>
       </c>
-      <c r="CA23" s="5"/>
+      <c r="CA23" s="5">
+        <v>62.25</v>
+      </c>
       <c r="CB23" s="5"/>
       <c r="CC23" s="5"/>
       <c r="CD23" s="5"/>
@@ -12916,19 +12933,18 @@
       <c r="CG23" s="5"/>
       <c r="CH23" s="5"/>
       <c r="CI23" s="5"/>
-      <c r="CJ23" s="5"/>
-    </row>
-    <row r="24" spans="1:88" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
+        <f>MIN(E24:ZV24)</f>
+        <v>210.65</v>
+      </c>
+      <c r="B24" s="12">
+        <f>MAX(E24:ZV24)</f>
+        <v>257.39999999999998</v>
+      </c>
+      <c r="C24" s="12">
         <f t="shared" si="0"/>
-        <v>210.65</v>
-      </c>
-      <c r="B24" s="12">
-        <f t="shared" si="1"/>
-        <v>257.39999999999998</v>
-      </c>
-      <c r="C24" s="12">
-        <f t="shared" si="2"/>
         <v>46.749999999999972</v>
       </c>
       <c r="D24" s="45" t="s">
@@ -13142,7 +13158,9 @@
       <c r="BZ24" s="5">
         <v>243.55</v>
       </c>
-      <c r="CA24" s="5"/>
+      <c r="CA24" s="5">
+        <v>240.7</v>
+      </c>
       <c r="CB24" s="5"/>
       <c r="CC24" s="5"/>
       <c r="CD24" s="5"/>
@@ -13151,20 +13169,19 @@
       <c r="CG24" s="5"/>
       <c r="CH24" s="5"/>
       <c r="CI24" s="5"/>
-      <c r="CJ24" s="5"/>
-    </row>
-    <row r="25" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
+        <f>MIN(E25:ZV25)</f>
+        <v>876</v>
+      </c>
+      <c r="B25" s="12">
+        <f>MAX(E25:ZV25)</f>
+        <v>1008</v>
+      </c>
+      <c r="C25" s="12">
         <f t="shared" si="0"/>
-        <v>876</v>
-      </c>
-      <c r="B25" s="12">
-        <f t="shared" si="1"/>
-        <v>989.95</v>
-      </c>
-      <c r="C25" s="12">
-        <f t="shared" si="2"/>
-        <v>113.95000000000005</v>
+        <v>132</v>
       </c>
       <c r="D25" s="46" t="s">
         <v>236</v>
@@ -13359,7 +13376,9 @@
       <c r="BZ25" s="5">
         <v>965.3</v>
       </c>
-      <c r="CA25" s="5"/>
+      <c r="CA25" s="5">
+        <v>1008</v>
+      </c>
       <c r="CB25" s="5"/>
       <c r="CC25" s="5"/>
       <c r="CD25" s="5"/>
@@ -13368,19 +13387,18 @@
       <c r="CG25" s="5"/>
       <c r="CH25" s="5"/>
       <c r="CI25" s="5"/>
-      <c r="CJ25" s="5"/>
-    </row>
-    <row r="26" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
+        <f>MIN(E26:ZV26)</f>
+        <v>83.1</v>
+      </c>
+      <c r="B26" s="12">
+        <f>MAX(E26:ZV26)</f>
+        <v>96</v>
+      </c>
+      <c r="C26" s="12">
         <f t="shared" si="0"/>
-        <v>83.1</v>
-      </c>
-      <c r="B26" s="12">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="C26" s="12">
-        <f t="shared" si="2"/>
         <v>12.900000000000006</v>
       </c>
       <c r="D26" s="45" t="s">
@@ -13564,7 +13582,9 @@
       <c r="BZ26" s="5">
         <v>89.9</v>
       </c>
-      <c r="CA26" s="5"/>
+      <c r="CA26" s="5">
+        <v>90.1</v>
+      </c>
       <c r="CB26" s="5"/>
       <c r="CC26" s="5"/>
       <c r="CD26" s="5"/>
@@ -13573,19 +13593,18 @@
       <c r="CG26" s="5"/>
       <c r="CH26" s="5"/>
       <c r="CI26" s="5"/>
-      <c r="CJ26" s="5"/>
-    </row>
-    <row r="27" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
+        <f>MIN(E27:ZV27)</f>
+        <v>36.200000000000003</v>
+      </c>
+      <c r="B27" s="12">
+        <f>MAX(E27:ZV27)</f>
+        <v>44.75</v>
+      </c>
+      <c r="C27" s="12">
         <f t="shared" si="0"/>
-        <v>36.200000000000003</v>
-      </c>
-      <c r="B27" s="12">
-        <f t="shared" si="1"/>
-        <v>44.75</v>
-      </c>
-      <c r="C27" s="12">
-        <f t="shared" si="2"/>
         <v>8.5499999999999972</v>
       </c>
       <c r="D27" s="45" t="s">
@@ -13769,7 +13788,9 @@
       <c r="BZ27" s="5">
         <v>42.7</v>
       </c>
-      <c r="CA27" s="5"/>
+      <c r="CA27" s="5">
+        <v>42.55</v>
+      </c>
       <c r="CB27" s="5"/>
       <c r="CC27" s="5"/>
       <c r="CD27" s="5"/>
@@ -13778,19 +13799,18 @@
       <c r="CG27" s="5"/>
       <c r="CH27" s="5"/>
       <c r="CI27" s="5"/>
-      <c r="CJ27" s="5"/>
-    </row>
-    <row r="28" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
+        <f>MIN(E28:ZV28)</f>
+        <v>111.95</v>
+      </c>
+      <c r="B28" s="12">
+        <f>MAX(E28:ZV28)</f>
+        <v>141.65</v>
+      </c>
+      <c r="C28" s="12">
         <f t="shared" si="0"/>
-        <v>111.95</v>
-      </c>
-      <c r="B28" s="12">
-        <f t="shared" si="1"/>
-        <v>141.65</v>
-      </c>
-      <c r="C28" s="12">
-        <f t="shared" si="2"/>
         <v>29.700000000000003</v>
       </c>
       <c r="D28" s="45" t="s">
@@ -13974,7 +13994,9 @@
       <c r="BZ28" s="5">
         <v>124.6</v>
       </c>
-      <c r="CA28" s="5"/>
+      <c r="CA28" s="5">
+        <v>125.1</v>
+      </c>
       <c r="CB28" s="5"/>
       <c r="CC28" s="5"/>
       <c r="CD28" s="5"/>
@@ -13983,19 +14005,18 @@
       <c r="CG28" s="5"/>
       <c r="CH28" s="5"/>
       <c r="CI28" s="5"/>
-      <c r="CJ28" s="5"/>
-    </row>
-    <row r="29" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
+        <f>MIN(E29:ZV29)</f>
+        <v>62.3</v>
+      </c>
+      <c r="B29" s="12">
+        <f>MAX(E29:ZV29)</f>
+        <v>78.849999999999994</v>
+      </c>
+      <c r="C29" s="12">
         <f t="shared" si="0"/>
-        <v>62.3</v>
-      </c>
-      <c r="B29" s="12">
-        <f t="shared" si="1"/>
-        <v>78.849999999999994</v>
-      </c>
-      <c r="C29" s="12">
-        <f t="shared" si="2"/>
         <v>16.549999999999997</v>
       </c>
       <c r="D29" s="45" t="s">
@@ -14179,7 +14200,9 @@
       <c r="BZ29" s="5">
         <v>74.5</v>
       </c>
-      <c r="CA29" s="5"/>
+      <c r="CA29" s="5">
+        <v>73.599999999999994</v>
+      </c>
       <c r="CB29" s="5"/>
       <c r="CC29" s="5"/>
       <c r="CD29" s="5"/>
@@ -14188,19 +14211,18 @@
       <c r="CG29" s="5"/>
       <c r="CH29" s="5"/>
       <c r="CI29" s="5"/>
-      <c r="CJ29" s="5"/>
-    </row>
-    <row r="30" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
+        <f>MIN(E30:ZV30)</f>
+        <v>39.25</v>
+      </c>
+      <c r="B30" s="12">
+        <f>MAX(E30:ZV30)</f>
+        <v>50.95</v>
+      </c>
+      <c r="C30" s="12">
         <f t="shared" si="0"/>
-        <v>39.25</v>
-      </c>
-      <c r="B30" s="12">
-        <f t="shared" si="1"/>
-        <v>50.95</v>
-      </c>
-      <c r="C30" s="12">
-        <f t="shared" si="2"/>
         <v>11.700000000000003</v>
       </c>
       <c r="D30" s="45" t="s">
@@ -14384,7 +14406,9 @@
       <c r="BZ30" s="5">
         <v>41.1</v>
       </c>
-      <c r="CA30" s="5"/>
+      <c r="CA30" s="5">
+        <v>40.65</v>
+      </c>
       <c r="CB30" s="5"/>
       <c r="CC30" s="5"/>
       <c r="CD30" s="5"/>
@@ -14393,19 +14417,18 @@
       <c r="CG30" s="5"/>
       <c r="CH30" s="5"/>
       <c r="CI30" s="5"/>
-      <c r="CJ30" s="5"/>
-    </row>
-    <row r="31" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
+        <f>MIN(E31:ZV31)</f>
+        <v>125.3</v>
+      </c>
+      <c r="B31" s="12">
+        <f>MAX(E31:ZV31)</f>
+        <v>156.85</v>
+      </c>
+      <c r="C31" s="12">
         <f t="shared" si="0"/>
-        <v>125.3</v>
-      </c>
-      <c r="B31" s="12">
-        <f t="shared" si="1"/>
-        <v>156.85</v>
-      </c>
-      <c r="C31" s="12">
-        <f t="shared" si="2"/>
         <v>31.549999999999997</v>
       </c>
       <c r="D31" s="45" t="s">
@@ -14589,7 +14612,9 @@
       <c r="BZ31" s="5">
         <v>125.3</v>
       </c>
-      <c r="CA31" s="5"/>
+      <c r="CA31" s="5">
+        <v>138.55000000000001</v>
+      </c>
       <c r="CB31" s="5"/>
       <c r="CC31" s="5"/>
       <c r="CD31" s="5"/>
@@ -14598,19 +14623,18 @@
       <c r="CG31" s="5"/>
       <c r="CH31" s="5"/>
       <c r="CI31" s="5"/>
-      <c r="CJ31" s="5"/>
-    </row>
-    <row r="32" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
+        <f>MIN(E32:ZV32)</f>
+        <v>96.65</v>
+      </c>
+      <c r="B32" s="12">
+        <f>MAX(E32:ZV32)</f>
+        <v>121.8</v>
+      </c>
+      <c r="C32" s="12">
         <f t="shared" si="0"/>
-        <v>96.65</v>
-      </c>
-      <c r="B32" s="12">
-        <f t="shared" si="1"/>
-        <v>121.8</v>
-      </c>
-      <c r="C32" s="12">
-        <f t="shared" si="2"/>
         <v>25.149999999999991</v>
       </c>
       <c r="D32" s="45" t="s">
@@ -14782,7 +14806,9 @@
       <c r="BZ32" s="5">
         <v>101.05</v>
       </c>
-      <c r="CA32" s="5"/>
+      <c r="CA32" s="5">
+        <v>102.8</v>
+      </c>
       <c r="CB32" s="5"/>
       <c r="CC32" s="5"/>
       <c r="CD32" s="5"/>
@@ -14791,19 +14817,18 @@
       <c r="CG32" s="5"/>
       <c r="CH32" s="5"/>
       <c r="CI32" s="5"/>
-      <c r="CJ32" s="5"/>
-    </row>
-    <row r="33" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
+        <f>MIN(E33:ZV33)</f>
+        <v>56.75</v>
+      </c>
+      <c r="B33" s="12">
+        <f>MAX(E33:ZV33)</f>
+        <v>67.099999999999994</v>
+      </c>
+      <c r="C33" s="12">
         <f t="shared" si="0"/>
-        <v>56.75</v>
-      </c>
-      <c r="B33" s="12">
-        <f t="shared" si="1"/>
-        <v>67.099999999999994</v>
-      </c>
-      <c r="C33" s="12">
-        <f t="shared" si="2"/>
         <v>10.349999999999994</v>
       </c>
       <c r="D33" s="45" t="s">
@@ -14963,7 +14988,9 @@
       <c r="BZ33" s="5">
         <v>60.2</v>
       </c>
-      <c r="CA33" s="5"/>
+      <c r="CA33" s="5">
+        <v>63</v>
+      </c>
       <c r="CB33" s="5"/>
       <c r="CC33" s="5"/>
       <c r="CD33" s="5"/>
@@ -14972,19 +14999,18 @@
       <c r="CG33" s="5"/>
       <c r="CH33" s="5"/>
       <c r="CI33" s="5"/>
-      <c r="CJ33" s="5"/>
-    </row>
-    <row r="34" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E34:ZV34)</f>
         <v>167.9</v>
       </c>
       <c r="B34" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E34:ZV34)</f>
         <v>236.1</v>
       </c>
       <c r="C34" s="12">
-        <f t="shared" ref="C34" si="3">B34-A34</f>
+        <f t="shared" ref="C34" si="1">B34-A34</f>
         <v>68.199999999999989</v>
       </c>
       <c r="D34" s="45" t="s">
@@ -15138,7 +15164,9 @@
       <c r="BZ34" s="5">
         <v>197.7</v>
       </c>
-      <c r="CA34" s="5"/>
+      <c r="CA34" s="5">
+        <v>199.9</v>
+      </c>
       <c r="CB34" s="5"/>
       <c r="CC34" s="5"/>
       <c r="CD34" s="5"/>
@@ -15147,19 +15175,18 @@
       <c r="CG34" s="5"/>
       <c r="CH34" s="5"/>
       <c r="CI34" s="5"/>
-      <c r="CJ34" s="5"/>
-    </row>
-    <row r="35" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E35:ZV35)</f>
         <v>661</v>
       </c>
       <c r="B35" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E35:ZV35)</f>
         <v>714.65</v>
       </c>
       <c r="C35" s="12">
-        <f t="shared" ref="C35" si="4">B35-A35</f>
+        <f t="shared" ref="C35" si="2">B35-A35</f>
         <v>53.649999999999977</v>
       </c>
       <c r="D35" s="45" t="s">
@@ -15309,7 +15336,9 @@
       <c r="BZ35" s="5">
         <v>699</v>
       </c>
-      <c r="CA35" s="5"/>
+      <c r="CA35" s="5">
+        <v>700</v>
+      </c>
       <c r="CB35" s="5"/>
       <c r="CC35" s="5"/>
       <c r="CD35" s="5"/>
@@ -15318,19 +15347,18 @@
       <c r="CG35" s="5"/>
       <c r="CH35" s="5"/>
       <c r="CI35" s="5"/>
-      <c r="CJ35" s="5"/>
-    </row>
-    <row r="36" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E36:ZV36)</f>
         <v>402.9</v>
       </c>
       <c r="B36" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E36:ZV36)</f>
         <v>520</v>
       </c>
       <c r="C36" s="12">
-        <f t="shared" ref="C36" si="5">B36-A36</f>
+        <f t="shared" ref="C36" si="3">B36-A36</f>
         <v>117.10000000000002</v>
       </c>
       <c r="D36" s="45" t="s">
@@ -15462,7 +15490,9 @@
       <c r="BZ36" s="5">
         <v>434.5</v>
       </c>
-      <c r="CA36" s="5"/>
+      <c r="CA36" s="5">
+        <v>423</v>
+      </c>
       <c r="CB36" s="5"/>
       <c r="CC36" s="5"/>
       <c r="CD36" s="5"/>
@@ -15471,19 +15501,18 @@
       <c r="CG36" s="5"/>
       <c r="CH36" s="5"/>
       <c r="CI36" s="5"/>
-      <c r="CJ36" s="5"/>
-    </row>
-    <row r="37" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E37:ZV37)</f>
         <v>226</v>
       </c>
       <c r="B37" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E37:ZV37)</f>
         <v>396.85</v>
       </c>
       <c r="C37" s="12">
-        <f t="shared" ref="C37" si="6">B37-A37</f>
+        <f t="shared" ref="C37" si="4">B37-A37</f>
         <v>170.85000000000002</v>
       </c>
       <c r="D37" s="45" t="s">
@@ -15605,7 +15634,9 @@
       <c r="BZ37" s="5">
         <v>319.3</v>
       </c>
-      <c r="CA37" s="5"/>
+      <c r="CA37" s="5">
+        <v>326.8</v>
+      </c>
       <c r="CB37" s="5"/>
       <c r="CC37" s="5"/>
       <c r="CD37" s="5"/>
@@ -15614,20 +15645,19 @@
       <c r="CG37" s="5"/>
       <c r="CH37" s="5"/>
       <c r="CI37" s="5"/>
-      <c r="CJ37" s="5"/>
-    </row>
-    <row r="38" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E38:ZV38)</f>
         <v>485</v>
       </c>
       <c r="B38" s="12">
-        <f t="shared" si="1"/>
-        <v>515.4</v>
+        <f>MAX(E38:ZV38)</f>
+        <v>519.95000000000005</v>
       </c>
       <c r="C38" s="12">
-        <f t="shared" ref="C38" si="7">B38-A38</f>
-        <v>30.399999999999977</v>
+        <f t="shared" ref="C38" si="5">B38-A38</f>
+        <v>34.950000000000045</v>
       </c>
       <c r="D38" s="45" t="s">
         <v>298</v>
@@ -15746,7 +15776,9 @@
       <c r="BZ38" s="5">
         <v>500</v>
       </c>
-      <c r="CA38" s="5"/>
+      <c r="CA38" s="5">
+        <v>519.95000000000005</v>
+      </c>
       <c r="CB38" s="5"/>
       <c r="CC38" s="5"/>
       <c r="CD38" s="5"/>
@@ -15755,20 +15787,19 @@
       <c r="CG38" s="5"/>
       <c r="CH38" s="5"/>
       <c r="CI38" s="5"/>
-      <c r="CJ38" s="5"/>
-    </row>
-    <row r="39" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E39:ZV39)</f>
         <v>75.2</v>
       </c>
       <c r="B39" s="12">
-        <f t="shared" si="1"/>
-        <v>78.5</v>
+        <f>MAX(E39:ZV39)</f>
+        <v>82</v>
       </c>
       <c r="C39" s="12">
-        <f t="shared" ref="C39" si="8">B39-A39</f>
-        <v>3.2999999999999972</v>
+        <f t="shared" ref="C39" si="6">B39-A39</f>
+        <v>6.7999999999999972</v>
       </c>
       <c r="D39" s="45" t="s">
         <v>305</v>
@@ -15881,7 +15912,9 @@
       <c r="BZ39" s="5">
         <v>76.599999999999994</v>
       </c>
-      <c r="CA39" s="5"/>
+      <c r="CA39" s="5">
+        <v>82</v>
+      </c>
       <c r="CB39" s="5"/>
       <c r="CC39" s="5"/>
       <c r="CD39" s="5"/>
@@ -15890,19 +15923,18 @@
       <c r="CG39" s="5"/>
       <c r="CH39" s="5"/>
       <c r="CI39" s="5"/>
-      <c r="CJ39" s="5"/>
-    </row>
-    <row r="40" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E40:ZV40)</f>
         <v>416</v>
       </c>
       <c r="B40" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E40:ZV40)</f>
         <v>472</v>
       </c>
       <c r="C40" s="12">
-        <f t="shared" ref="C40" si="9">B40-A40</f>
+        <f t="shared" ref="C40" si="7">B40-A40</f>
         <v>56</v>
       </c>
       <c r="D40" s="45" t="s">
@@ -16016,7 +16048,9 @@
       <c r="BZ40" s="5">
         <v>416.8</v>
       </c>
-      <c r="CA40" s="5"/>
+      <c r="CA40" s="5">
+        <v>429.15</v>
+      </c>
       <c r="CB40" s="5"/>
       <c r="CC40" s="5"/>
       <c r="CD40" s="5"/>
@@ -16025,19 +16059,18 @@
       <c r="CG40" s="5"/>
       <c r="CH40" s="5"/>
       <c r="CI40" s="5"/>
-      <c r="CJ40" s="5"/>
-    </row>
-    <row r="41" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E41:ZV41)</f>
         <v>192.65</v>
       </c>
       <c r="B41" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E41:ZV41)</f>
         <v>215.25</v>
       </c>
       <c r="C41" s="12">
-        <f t="shared" ref="C41" si="10">B41-A41</f>
+        <f t="shared" ref="C41" si="8">B41-A41</f>
         <v>22.599999999999994</v>
       </c>
       <c r="D41" s="45" t="s">
@@ -16147,7 +16180,9 @@
       <c r="BZ41" s="5">
         <v>208</v>
       </c>
-      <c r="CA41" s="5"/>
+      <c r="CA41" s="5">
+        <v>201</v>
+      </c>
       <c r="CB41" s="5"/>
       <c r="CC41" s="5"/>
       <c r="CD41" s="5"/>
@@ -16156,19 +16191,18 @@
       <c r="CG41" s="5"/>
       <c r="CH41" s="5"/>
       <c r="CI41" s="5"/>
-      <c r="CJ41" s="5"/>
-    </row>
-    <row r="42" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E42:ZV42)</f>
         <v>35</v>
       </c>
       <c r="B42" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E42:ZV42)</f>
         <v>38.65</v>
       </c>
       <c r="C42" s="12">
-        <f t="shared" ref="C42:C45" si="11">B42-A42</f>
+        <f t="shared" ref="C42:C45" si="9">B42-A42</f>
         <v>3.6499999999999986</v>
       </c>
       <c r="D42" s="45" t="s">
@@ -16274,7 +16308,9 @@
       <c r="BZ42" s="5">
         <v>37.15</v>
       </c>
-      <c r="CA42" s="5"/>
+      <c r="CA42" s="5">
+        <v>37.200000000000003</v>
+      </c>
       <c r="CB42" s="5"/>
       <c r="CC42" s="5"/>
       <c r="CD42" s="5"/>
@@ -16283,19 +16319,18 @@
       <c r="CG42" s="5"/>
       <c r="CH42" s="5"/>
       <c r="CI42" s="5"/>
-      <c r="CJ42" s="5"/>
-    </row>
-    <row r="43" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E43:ZV43)</f>
         <v>552.04999999999995</v>
       </c>
       <c r="B43" s="12">
-        <f t="shared" ref="B43:B44" si="12">MAX(E43:ZW43)</f>
+        <f>MAX(E43:ZV43)</f>
         <v>626.70000000000005</v>
       </c>
       <c r="C43" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>74.650000000000091</v>
       </c>
       <c r="D43" s="45" t="s">
@@ -16399,7 +16434,9 @@
       <c r="BZ43" s="5">
         <v>580.1</v>
       </c>
-      <c r="CA43" s="5"/>
+      <c r="CA43" s="5">
+        <v>581.45000000000005</v>
+      </c>
       <c r="CB43" s="5"/>
       <c r="CC43" s="5"/>
       <c r="CD43" s="5"/>
@@ -16408,19 +16445,18 @@
       <c r="CG43" s="5"/>
       <c r="CH43" s="5"/>
       <c r="CI43" s="5"/>
-      <c r="CJ43" s="5"/>
-    </row>
-    <row r="44" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E44:ZV44)</f>
         <v>822.95</v>
       </c>
       <c r="B44" s="12">
-        <f t="shared" si="12"/>
+        <f>MAX(E44:ZV44)</f>
         <v>856</v>
       </c>
       <c r="C44" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>33.049999999999955</v>
       </c>
       <c r="D44" s="45" t="s">
@@ -16524,7 +16560,9 @@
       <c r="BZ44" s="5">
         <v>828.3</v>
       </c>
-      <c r="CA44" s="5"/>
+      <c r="CA44" s="5">
+        <v>829.4</v>
+      </c>
       <c r="CB44" s="5"/>
       <c r="CC44" s="5"/>
       <c r="CD44" s="5"/>
@@ -16533,19 +16571,18 @@
       <c r="CG44" s="5"/>
       <c r="CH44" s="5"/>
       <c r="CI44" s="5"/>
-      <c r="CJ44" s="5"/>
-    </row>
-    <row r="45" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E45:ZV45)</f>
         <v>134.9</v>
       </c>
       <c r="B45" s="12">
-        <f>MAX(E45:ZW45)</f>
+        <f>MAX(E45:ZV45)</f>
         <v>146</v>
       </c>
       <c r="C45" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>11.099999999999994</v>
       </c>
       <c r="D45" s="45" t="s">
@@ -16647,7 +16684,9 @@
       <c r="BZ45" s="5">
         <v>138.19999999999999</v>
       </c>
-      <c r="CA45" s="5"/>
+      <c r="CA45" s="5">
+        <v>142.9</v>
+      </c>
       <c r="CB45" s="5"/>
       <c r="CC45" s="5"/>
       <c r="CD45" s="5"/>
@@ -16656,20 +16695,19 @@
       <c r="CG45" s="5"/>
       <c r="CH45" s="5"/>
       <c r="CI45" s="5"/>
-      <c r="CJ45" s="5"/>
-    </row>
-    <row r="46" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
-        <f t="shared" ref="A46" si="13">MIN(E46:ZW46)</f>
-        <v>663.95</v>
+        <f>MIN(E46:ZV46)</f>
+        <v>648.4</v>
       </c>
       <c r="B46" s="12">
-        <f>MAX(E46:ZW46)</f>
+        <f>MAX(E46:ZV46)</f>
         <v>770</v>
       </c>
       <c r="C46" s="12">
-        <f t="shared" ref="C46" si="14">B46-A46</f>
-        <v>106.04999999999995</v>
+        <f t="shared" ref="C46" si="10">B46-A46</f>
+        <v>121.60000000000002</v>
       </c>
       <c r="D46" s="45" t="s">
         <v>313</v>
@@ -16764,7 +16802,9 @@
       <c r="BZ46" s="5">
         <v>663.95</v>
       </c>
-      <c r="CA46" s="5"/>
+      <c r="CA46" s="5">
+        <v>648.4</v>
+      </c>
       <c r="CB46" s="5"/>
       <c r="CC46" s="5"/>
       <c r="CD46" s="5"/>
@@ -16773,23 +16813,22 @@
       <c r="CG46" s="5"/>
       <c r="CH46" s="5"/>
       <c r="CI46" s="5"/>
-      <c r="CJ46" s="5"/>
-    </row>
-    <row r="47" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
-        <f t="shared" ref="A47" si="15">MIN(E47:ZW47)</f>
+        <f>MIN(E47:ZV47)</f>
         <v>776.5</v>
       </c>
       <c r="B47" s="12">
-        <f>MAX(E47:ZW47)</f>
+        <f>MAX(E47:ZV47)</f>
         <v>859.9</v>
       </c>
       <c r="C47" s="12">
-        <f t="shared" ref="C47" si="16">B47-A47</f>
+        <f t="shared" ref="C47" si="11">B47-A47</f>
         <v>83.399999999999977</v>
       </c>
       <c r="D47" s="45" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -16881,7 +16920,9 @@
       <c r="BZ47" s="5">
         <v>852</v>
       </c>
-      <c r="CA47" s="5"/>
+      <c r="CA47" s="5">
+        <v>851</v>
+      </c>
       <c r="CB47" s="5"/>
       <c r="CC47" s="5"/>
       <c r="CD47" s="5"/>
@@ -16890,23 +16931,22 @@
       <c r="CG47" s="5"/>
       <c r="CH47" s="5"/>
       <c r="CI47" s="5"/>
-      <c r="CJ47" s="5"/>
-    </row>
-    <row r="48" spans="1:88" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
-        <f t="shared" ref="A48" si="17">MIN(E48:ZW48)</f>
+        <f>MIN(E48:ZV48)</f>
         <v>109</v>
       </c>
       <c r="B48" s="12">
-        <f>MAX(E48:ZW48)</f>
+        <f>MAX(E48:ZV48)</f>
         <v>110.95</v>
       </c>
       <c r="C48" s="12">
-        <f t="shared" ref="C48" si="18">B48-A48</f>
+        <f t="shared" ref="C48" si="12">B48-A48</f>
         <v>1.9500000000000028</v>
       </c>
       <c r="D48" s="45" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -16990,7 +17030,9 @@
       <c r="BZ48" s="5">
         <v>109.5</v>
       </c>
-      <c r="CA48" s="5"/>
+      <c r="CA48" s="5">
+        <v>109.85</v>
+      </c>
       <c r="CB48" s="5"/>
       <c r="CC48" s="5"/>
       <c r="CD48" s="5"/>
@@ -16999,7 +17041,6 @@
       <c r="CG48" s="5"/>
       <c r="CH48" s="5"/>
       <c r="CI48" s="5"/>
-      <c r="CJ48" s="5"/>
     </row>
   </sheetData>
   <sortState ref="L1:L37">
@@ -18224,10 +18265,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18272,7 +18313,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(B2:B200)</f>
-        <v>1102233</v>
+        <v>1108793</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -18290,7 +18331,7 @@
       </c>
       <c r="F3" s="5">
         <f>F1-F2</f>
-        <v>373156</v>
+        <v>366596</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -18923,6 +18964,17 @@
       </c>
       <c r="C45" s="31">
         <v>43040</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="B46" s="26">
+        <v>6560</v>
+      </c>
+      <c r="C46" s="52">
+        <v>43063</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added details for 29/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="330">
   <si>
     <t>Date</t>
   </si>
@@ -1012,6 +1012,9 @@
   </si>
   <si>
     <t>MEGH</t>
+  </si>
+  <si>
+    <t>Di</t>
   </si>
 </sst>
 </file>
@@ -7261,7 +7264,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="BT1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CA2" sqref="CA2"/>
+      <selection pane="topRight" activeCell="CC16" sqref="CC16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7570,11 +7573,11 @@
     </row>
     <row r="2" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
-        <f>MIN(E2:ZV2)</f>
+        <f t="shared" ref="A2:A48" si="0">MIN(E2:ZV2)</f>
         <v>243.6</v>
       </c>
       <c r="B2" s="12">
-        <f>MAX(E2:ZV2)</f>
+        <f t="shared" ref="B2:B48" si="1">MAX(E2:ZV2)</f>
         <v>340.8</v>
       </c>
       <c r="C2" s="12">
@@ -7801,8 +7804,12 @@
       <c r="CA2" s="5">
         <v>332.1</v>
       </c>
-      <c r="CB2" s="5"/>
-      <c r="CC2" s="5"/>
+      <c r="CB2" s="5">
+        <v>329.3</v>
+      </c>
+      <c r="CC2" s="5">
+        <v>331.9</v>
+      </c>
       <c r="CD2" s="5"/>
       <c r="CE2" s="5"/>
       <c r="CF2" s="5"/>
@@ -7812,15 +7819,15 @@
     </row>
     <row r="3" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
-        <f>MIN(E3:ZV3)</f>
+        <f t="shared" si="0"/>
         <v>262.7</v>
       </c>
       <c r="B3" s="12">
-        <f>MAX(E3:ZV3)</f>
+        <f t="shared" si="1"/>
         <v>328.85</v>
       </c>
       <c r="C3" s="12">
-        <f t="shared" ref="C3:C33" si="0">B3-A3</f>
+        <f t="shared" ref="C3:C33" si="2">B3-A3</f>
         <v>66.150000000000034</v>
       </c>
       <c r="D3" s="44" t="s">
@@ -8043,8 +8050,12 @@
       <c r="CA3" s="5">
         <v>316.85000000000002</v>
       </c>
-      <c r="CB3" s="5"/>
-      <c r="CC3" s="5"/>
+      <c r="CB3" s="5">
+        <v>317.5</v>
+      </c>
+      <c r="CC3" s="5">
+        <v>313</v>
+      </c>
       <c r="CD3" s="5"/>
       <c r="CE3" s="5"/>
       <c r="CF3" s="5"/>
@@ -8054,15 +8065,15 @@
     </row>
     <row r="4" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
-        <f>MIN(E4:ZV4)</f>
+        <f t="shared" si="0"/>
         <v>253.85</v>
       </c>
       <c r="B4" s="12">
-        <f>MAX(E4:ZV4)</f>
+        <f t="shared" si="1"/>
         <v>291.7</v>
       </c>
       <c r="C4" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>37.849999999999994</v>
       </c>
       <c r="D4" s="44" t="s">
@@ -8291,8 +8302,12 @@
       <c r="CA4" s="5">
         <v>260.64999999999998</v>
       </c>
-      <c r="CB4" s="5"/>
-      <c r="CC4" s="5"/>
+      <c r="CB4" s="5">
+        <v>259.45</v>
+      </c>
+      <c r="CC4" s="5">
+        <v>257</v>
+      </c>
       <c r="CD4" s="5"/>
       <c r="CE4" s="5"/>
       <c r="CF4" s="5"/>
@@ -8302,15 +8317,15 @@
     </row>
     <row r="5" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
-        <f>MIN(E5:ZV5)</f>
+        <f t="shared" si="0"/>
         <v>786.25</v>
       </c>
       <c r="B5" s="12">
-        <f>MAX(E5:ZV5)</f>
+        <f t="shared" si="1"/>
         <v>951.25</v>
       </c>
       <c r="C5" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>165</v>
       </c>
       <c r="D5" s="44" t="s">
@@ -8539,8 +8554,12 @@
       <c r="CA5" s="5">
         <v>951.25</v>
       </c>
-      <c r="CB5" s="5"/>
-      <c r="CC5" s="5"/>
+      <c r="CB5" s="5">
+        <v>948.35</v>
+      </c>
+      <c r="CC5" s="5">
+        <v>942.4</v>
+      </c>
       <c r="CD5" s="5"/>
       <c r="CE5" s="5"/>
       <c r="CF5" s="5"/>
@@ -8550,15 +8569,15 @@
     </row>
     <row r="6" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
-        <f>MIN(E6:ZV6)</f>
+        <f t="shared" si="0"/>
         <v>236.45</v>
       </c>
       <c r="B6" s="12">
-        <f>MAX(E6:ZV6)</f>
+        <f t="shared" si="1"/>
         <v>293.95</v>
       </c>
       <c r="C6" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>57.5</v>
       </c>
       <c r="D6" s="45" t="s">
@@ -8787,8 +8806,12 @@
       <c r="CA6" s="5">
         <v>271.64999999999998</v>
       </c>
-      <c r="CB6" s="5"/>
-      <c r="CC6" s="5"/>
+      <c r="CB6" s="5">
+        <v>270.8</v>
+      </c>
+      <c r="CC6" s="5">
+        <v>273.8</v>
+      </c>
       <c r="CD6" s="5"/>
       <c r="CE6" s="5"/>
       <c r="CF6" s="5"/>
@@ -8798,15 +8821,15 @@
     </row>
     <row r="7" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
-        <f>MIN(E7:ZV7)</f>
+        <f t="shared" si="0"/>
         <v>15.6</v>
       </c>
       <c r="B7" s="12">
-        <f>MAX(E7:ZV7)</f>
+        <f t="shared" si="1"/>
         <v>19.350000000000001</v>
       </c>
       <c r="C7" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.7500000000000018</v>
       </c>
       <c r="D7" s="45" t="s">
@@ -9035,8 +9058,12 @@
       <c r="CA7" s="5">
         <v>18.649999999999999</v>
       </c>
-      <c r="CB7" s="5"/>
-      <c r="CC7" s="5"/>
+      <c r="CB7" s="5">
+        <v>18.350000000000001</v>
+      </c>
+      <c r="CC7" s="5">
+        <v>18.05</v>
+      </c>
       <c r="CD7" s="5"/>
       <c r="CE7" s="5"/>
       <c r="CF7" s="5"/>
@@ -9046,15 +9073,15 @@
     </row>
     <row r="8" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
-        <f>MIN(E8:ZV8)</f>
+        <f t="shared" si="0"/>
         <v>53.4</v>
       </c>
       <c r="B8" s="12">
-        <f>MAX(E8:ZV8)</f>
+        <f t="shared" si="1"/>
         <v>86.75</v>
       </c>
       <c r="C8" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>33.35</v>
       </c>
       <c r="D8" s="45" t="s">
@@ -9283,8 +9310,12 @@
       <c r="CA8" s="5">
         <v>82.3</v>
       </c>
-      <c r="CB8" s="5"/>
-      <c r="CC8" s="5"/>
+      <c r="CB8" s="5">
+        <v>82</v>
+      </c>
+      <c r="CC8" s="5">
+        <v>80.599999999999994</v>
+      </c>
       <c r="CD8" s="5"/>
       <c r="CE8" s="5"/>
       <c r="CF8" s="5"/>
@@ -9294,15 +9325,15 @@
     </row>
     <row r="9" spans="1:87" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
-        <f>MIN(E9:ZV9)</f>
+        <f t="shared" si="0"/>
         <v>53.5</v>
       </c>
       <c r="B9" s="39">
-        <f>MAX(E9:ZV9)</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="C9" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
       <c r="D9" s="43" t="s">
@@ -9523,8 +9554,12 @@
       <c r="CA9" s="28">
         <v>54.65</v>
       </c>
-      <c r="CB9" s="28"/>
-      <c r="CC9" s="28"/>
+      <c r="CB9" s="28">
+        <v>54.8</v>
+      </c>
+      <c r="CC9" s="28">
+        <v>55.3</v>
+      </c>
       <c r="CD9" s="28"/>
       <c r="CE9" s="28"/>
       <c r="CF9" s="28"/>
@@ -9534,15 +9569,15 @@
     </row>
     <row r="10" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
-        <f>MIN(E10:ZV10)</f>
+        <f t="shared" si="0"/>
         <v>35.549999999999997</v>
       </c>
       <c r="B10" s="12">
-        <f>MAX(E10:ZV10)</f>
+        <f t="shared" si="1"/>
         <v>45.35</v>
       </c>
       <c r="C10" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.8000000000000043</v>
       </c>
       <c r="D10" s="45" t="s">
@@ -9771,8 +9806,12 @@
       <c r="CA10" s="5">
         <v>38.35</v>
       </c>
-      <c r="CB10" s="5"/>
-      <c r="CC10" s="5"/>
+      <c r="CB10" s="5">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="CC10" s="5">
+        <v>38.75</v>
+      </c>
       <c r="CD10" s="5"/>
       <c r="CE10" s="5"/>
       <c r="CF10" s="5"/>
@@ -9782,15 +9821,15 @@
     </row>
     <row r="11" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
-        <f>MIN(E11:ZV11)</f>
+        <f t="shared" si="0"/>
         <v>72.650000000000006</v>
       </c>
       <c r="B11" s="12">
-        <f>MAX(E11:ZV11)</f>
+        <f t="shared" si="1"/>
         <v>106.5</v>
       </c>
       <c r="C11" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>33.849999999999994</v>
       </c>
       <c r="D11" s="45" t="s">
@@ -10019,8 +10058,12 @@
       <c r="CA11" s="5">
         <v>94.6</v>
       </c>
-      <c r="CB11" s="5"/>
-      <c r="CC11" s="5"/>
+      <c r="CB11" s="5">
+        <v>95.1</v>
+      </c>
+      <c r="CC11" s="5">
+        <v>95.1</v>
+      </c>
       <c r="CD11" s="5"/>
       <c r="CE11" s="5"/>
       <c r="CF11" s="5"/>
@@ -10030,15 +10073,15 @@
     </row>
     <row r="12" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
-        <f>MIN(E12:ZV12)</f>
+        <f t="shared" si="0"/>
         <v>82.65</v>
       </c>
       <c r="B12" s="12">
-        <f>MAX(E12:ZV12)</f>
+        <f t="shared" si="1"/>
         <v>99.6</v>
       </c>
       <c r="C12" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16.949999999999989</v>
       </c>
       <c r="D12" s="45" t="s">
@@ -10267,8 +10310,12 @@
       <c r="CA12" s="5">
         <v>92.1</v>
       </c>
-      <c r="CB12" s="5"/>
-      <c r="CC12" s="5"/>
+      <c r="CB12" s="5">
+        <v>91.7</v>
+      </c>
+      <c r="CC12" s="5">
+        <v>93.9</v>
+      </c>
       <c r="CD12" s="5"/>
       <c r="CE12" s="5"/>
       <c r="CF12" s="5"/>
@@ -10278,15 +10325,15 @@
     </row>
     <row r="13" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
-        <f>MIN(E13:ZV13)</f>
+        <f t="shared" si="0"/>
         <v>44.1</v>
       </c>
       <c r="B13" s="12">
-        <f>MAX(E13:ZV13)</f>
+        <f t="shared" si="1"/>
         <v>57.15</v>
       </c>
       <c r="C13" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13.049999999999997</v>
       </c>
       <c r="D13" s="45" t="s">
@@ -10515,8 +10562,12 @@
       <c r="CA13" s="5">
         <v>52</v>
       </c>
-      <c r="CB13" s="5"/>
-      <c r="CC13" s="5"/>
+      <c r="CB13" s="5">
+        <v>52.75</v>
+      </c>
+      <c r="CC13" s="5">
+        <v>53.5</v>
+      </c>
       <c r="CD13" s="5"/>
       <c r="CE13" s="5"/>
       <c r="CF13" s="5"/>
@@ -10526,15 +10577,15 @@
     </row>
     <row r="14" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
-        <f>MIN(E14:ZV14)</f>
+        <f t="shared" si="0"/>
         <v>29.75</v>
       </c>
       <c r="B14" s="12">
-        <f>MAX(E14:ZV14)</f>
+        <f t="shared" si="1"/>
         <v>41.85</v>
       </c>
       <c r="C14" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12.100000000000001</v>
       </c>
       <c r="D14" s="45" t="s">
@@ -10763,8 +10814,12 @@
       <c r="CA14" s="5">
         <v>34.9</v>
       </c>
-      <c r="CB14" s="5"/>
-      <c r="CC14" s="5"/>
+      <c r="CB14" s="5">
+        <v>35</v>
+      </c>
+      <c r="CC14" s="5">
+        <v>38.6</v>
+      </c>
       <c r="CD14" s="5"/>
       <c r="CE14" s="5"/>
       <c r="CF14" s="5"/>
@@ -10774,15 +10829,15 @@
     </row>
     <row r="15" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
-        <f>MIN(E15:ZV15)</f>
+        <f t="shared" si="0"/>
         <v>23.95</v>
       </c>
       <c r="B15" s="12">
-        <f>MAX(E15:ZV15)</f>
+        <f t="shared" si="1"/>
         <v>36.4</v>
       </c>
       <c r="C15" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12.45</v>
       </c>
       <c r="D15" s="45" t="s">
@@ -11003,8 +11058,12 @@
       <c r="CA15" s="5">
         <v>25.6</v>
       </c>
-      <c r="CB15" s="5"/>
-      <c r="CC15" s="5"/>
+      <c r="CB15" s="5">
+        <v>25.45</v>
+      </c>
+      <c r="CC15" s="5">
+        <v>24.9</v>
+      </c>
       <c r="CD15" s="5"/>
       <c r="CE15" s="5"/>
       <c r="CF15" s="5"/>
@@ -11014,15 +11073,15 @@
     </row>
     <row r="16" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
-        <f>MIN(E16:ZV16)</f>
+        <f t="shared" si="0"/>
         <v>552</v>
       </c>
       <c r="B16" s="12">
-        <f>MAX(E16:ZV16)</f>
+        <f t="shared" si="1"/>
         <v>729.5</v>
       </c>
       <c r="C16" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>177.5</v>
       </c>
       <c r="D16" s="45" t="s">
@@ -11251,8 +11310,12 @@
       <c r="CA16" s="5">
         <v>708.1</v>
       </c>
-      <c r="CB16" s="5"/>
-      <c r="CC16" s="5"/>
+      <c r="CB16" s="5">
+        <v>703.4</v>
+      </c>
+      <c r="CC16" s="5">
+        <v>703</v>
+      </c>
       <c r="CD16" s="5"/>
       <c r="CE16" s="5"/>
       <c r="CF16" s="5"/>
@@ -11262,15 +11325,15 @@
     </row>
     <row r="17" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
-        <f>MIN(E17:ZV17)</f>
+        <f t="shared" si="0"/>
         <v>433</v>
       </c>
       <c r="B17" s="12">
-        <f>MAX(E17:ZV17)</f>
+        <f t="shared" si="1"/>
         <v>670</v>
       </c>
       <c r="C17" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>237</v>
       </c>
       <c r="D17" s="44" t="s">
@@ -11499,8 +11562,12 @@
       <c r="CA17" s="5">
         <v>470</v>
       </c>
-      <c r="CB17" s="5"/>
-      <c r="CC17" s="5"/>
+      <c r="CB17" s="5">
+        <v>472</v>
+      </c>
+      <c r="CC17" s="5">
+        <v>469.95</v>
+      </c>
       <c r="CD17" s="5"/>
       <c r="CE17" s="5"/>
       <c r="CF17" s="5"/>
@@ -11510,15 +11577,15 @@
     </row>
     <row r="18" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
-        <f>MIN(E18:ZV18)</f>
+        <f t="shared" si="0"/>
         <v>178.8</v>
       </c>
       <c r="B18" s="12">
-        <f>MAX(E18:ZV18)</f>
+        <f t="shared" si="1"/>
         <v>302.2</v>
       </c>
       <c r="C18" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>123.39999999999998</v>
       </c>
       <c r="D18" s="44" t="s">
@@ -11747,8 +11814,12 @@
       <c r="CA18" s="5">
         <v>260.60000000000002</v>
       </c>
-      <c r="CB18" s="5"/>
-      <c r="CC18" s="5"/>
+      <c r="CB18" s="5">
+        <v>260.10000000000002</v>
+      </c>
+      <c r="CC18" s="5">
+        <v>265.5</v>
+      </c>
       <c r="CD18" s="5"/>
       <c r="CE18" s="5"/>
       <c r="CF18" s="5"/>
@@ -11758,16 +11829,16 @@
     </row>
     <row r="19" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
-        <f>MIN(E19:ZV19)</f>
+        <f t="shared" si="0"/>
         <v>440.7</v>
       </c>
       <c r="B19" s="12">
-        <f>MAX(E19:ZV19)</f>
-        <v>710.3</v>
+        <f t="shared" si="1"/>
+        <v>719.55</v>
       </c>
       <c r="C19" s="12">
-        <f t="shared" si="0"/>
-        <v>269.59999999999997</v>
+        <f t="shared" si="2"/>
+        <v>278.84999999999997</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -11995,8 +12066,12 @@
       <c r="CA19" s="5">
         <v>710.3</v>
       </c>
-      <c r="CB19" s="5"/>
-      <c r="CC19" s="5"/>
+      <c r="CB19" s="5">
+        <v>719.55</v>
+      </c>
+      <c r="CC19" s="5">
+        <v>702</v>
+      </c>
       <c r="CD19" s="5"/>
       <c r="CE19" s="5"/>
       <c r="CF19" s="5"/>
@@ -12006,15 +12081,15 @@
     </row>
     <row r="20" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
-        <f>MIN(E20:ZV20)</f>
+        <f t="shared" si="0"/>
         <v>677</v>
       </c>
       <c r="B20" s="12">
-        <f>MAX(E20:ZV20)</f>
+        <f t="shared" si="1"/>
         <v>795.95</v>
       </c>
       <c r="C20" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118.95000000000005</v>
       </c>
       <c r="D20" s="44" t="s">
@@ -12243,8 +12318,12 @@
       <c r="CA20" s="5">
         <v>717</v>
       </c>
-      <c r="CB20" s="5"/>
-      <c r="CC20" s="5"/>
+      <c r="CB20" s="5">
+        <v>717.65</v>
+      </c>
+      <c r="CC20" s="5">
+        <v>705.1</v>
+      </c>
       <c r="CD20" s="5"/>
       <c r="CE20" s="5"/>
       <c r="CF20" s="5"/>
@@ -12254,15 +12333,15 @@
     </row>
     <row r="21" spans="1:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
-        <f>MIN(E21:ZV21)</f>
+        <f t="shared" si="0"/>
         <v>376.7</v>
       </c>
       <c r="B21" s="12">
-        <f>MAX(E21:ZV21)</f>
+        <f t="shared" si="1"/>
         <v>547.5</v>
       </c>
       <c r="C21" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>170.8</v>
       </c>
       <c r="D21" s="44" t="s">
@@ -12491,8 +12570,12 @@
       <c r="CA21" s="5">
         <v>496.75</v>
       </c>
-      <c r="CB21" s="5"/>
-      <c r="CC21" s="5"/>
+      <c r="CB21" s="5">
+        <v>495</v>
+      </c>
+      <c r="CC21" s="5">
+        <v>490.5</v>
+      </c>
       <c r="CD21" s="5"/>
       <c r="CE21" s="5"/>
       <c r="CF21" s="5"/>
@@ -12502,15 +12585,15 @@
     </row>
     <row r="22" spans="1:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
-        <f>MIN(E22:ZV22)</f>
+        <f t="shared" si="0"/>
         <v>315.2</v>
       </c>
       <c r="B22" s="12">
-        <f>MAX(E22:ZV22)</f>
+        <f t="shared" si="1"/>
         <v>413.5</v>
       </c>
       <c r="C22" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>98.300000000000011</v>
       </c>
       <c r="D22" s="44" t="s">
@@ -12685,8 +12768,12 @@
       <c r="CA22" s="5">
         <v>413.5</v>
       </c>
-      <c r="CB22" s="5"/>
-      <c r="CC22" s="5"/>
+      <c r="CB22" s="5">
+        <v>408.7</v>
+      </c>
+      <c r="CC22" s="5">
+        <v>399</v>
+      </c>
       <c r="CD22" s="5"/>
       <c r="CE22" s="5"/>
       <c r="CF22" s="5"/>
@@ -12696,15 +12783,15 @@
     </row>
     <row r="23" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
-        <f>MIN(E23:ZV23)</f>
+        <f t="shared" si="0"/>
         <v>54.45</v>
       </c>
       <c r="B23" s="12">
-        <f>MAX(E23:ZV23)</f>
+        <f t="shared" si="1"/>
         <v>85.65</v>
       </c>
       <c r="C23" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>31.200000000000003</v>
       </c>
       <c r="D23" s="45" t="s">
@@ -12925,8 +13012,12 @@
       <c r="CA23" s="5">
         <v>62.25</v>
       </c>
-      <c r="CB23" s="5"/>
-      <c r="CC23" s="5"/>
+      <c r="CB23" s="5">
+        <v>62.4</v>
+      </c>
+      <c r="CC23" s="5">
+        <v>61.35</v>
+      </c>
       <c r="CD23" s="5"/>
       <c r="CE23" s="5"/>
       <c r="CF23" s="5"/>
@@ -12936,15 +13027,15 @@
     </row>
     <row r="24" spans="1:87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
-        <f>MIN(E24:ZV24)</f>
+        <f t="shared" si="0"/>
         <v>210.65</v>
       </c>
       <c r="B24" s="12">
-        <f>MAX(E24:ZV24)</f>
+        <f t="shared" si="1"/>
         <v>257.39999999999998</v>
       </c>
       <c r="C24" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>46.749999999999972</v>
       </c>
       <c r="D24" s="45" t="s">
@@ -13161,8 +13252,12 @@
       <c r="CA24" s="5">
         <v>240.7</v>
       </c>
-      <c r="CB24" s="5"/>
-      <c r="CC24" s="5"/>
+      <c r="CB24" s="5">
+        <v>239.15</v>
+      </c>
+      <c r="CC24" s="5">
+        <v>235.75</v>
+      </c>
       <c r="CD24" s="5"/>
       <c r="CE24" s="5"/>
       <c r="CF24" s="5"/>
@@ -13172,15 +13267,15 @@
     </row>
     <row r="25" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
-        <f>MIN(E25:ZV25)</f>
+        <f t="shared" si="0"/>
         <v>876</v>
       </c>
       <c r="B25" s="12">
-        <f>MAX(E25:ZV25)</f>
+        <f t="shared" si="1"/>
         <v>1008</v>
       </c>
       <c r="C25" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>132</v>
       </c>
       <c r="D25" s="46" t="s">
@@ -13379,8 +13474,12 @@
       <c r="CA25" s="5">
         <v>1008</v>
       </c>
-      <c r="CB25" s="5"/>
-      <c r="CC25" s="5"/>
+      <c r="CB25" s="5">
+        <v>996.05</v>
+      </c>
+      <c r="CC25" s="5">
+        <v>982.15</v>
+      </c>
       <c r="CD25" s="5"/>
       <c r="CE25" s="5"/>
       <c r="CF25" s="5"/>
@@ -13390,15 +13489,15 @@
     </row>
     <row r="26" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
-        <f>MIN(E26:ZV26)</f>
+        <f t="shared" si="0"/>
         <v>83.1</v>
       </c>
       <c r="B26" s="12">
-        <f>MAX(E26:ZV26)</f>
+        <f t="shared" si="1"/>
         <v>96</v>
       </c>
       <c r="C26" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12.900000000000006</v>
       </c>
       <c r="D26" s="45" t="s">
@@ -13585,8 +13684,12 @@
       <c r="CA26" s="5">
         <v>90.1</v>
       </c>
-      <c r="CB26" s="5"/>
-      <c r="CC26" s="5"/>
+      <c r="CB26" s="5">
+        <v>90.35</v>
+      </c>
+      <c r="CC26" s="5">
+        <v>93</v>
+      </c>
       <c r="CD26" s="5"/>
       <c r="CE26" s="5"/>
       <c r="CF26" s="5"/>
@@ -13596,15 +13699,15 @@
     </row>
     <row r="27" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
-        <f>MIN(E27:ZV27)</f>
+        <f t="shared" si="0"/>
         <v>36.200000000000003</v>
       </c>
       <c r="B27" s="12">
-        <f>MAX(E27:ZV27)</f>
+        <f t="shared" si="1"/>
         <v>44.75</v>
       </c>
       <c r="C27" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5499999999999972</v>
       </c>
       <c r="D27" s="45" t="s">
@@ -13791,8 +13894,12 @@
       <c r="CA27" s="5">
         <v>42.55</v>
       </c>
-      <c r="CB27" s="5"/>
-      <c r="CC27" s="5"/>
+      <c r="CB27" s="5">
+        <v>43.3</v>
+      </c>
+      <c r="CC27" s="5">
+        <v>43.3</v>
+      </c>
       <c r="CD27" s="5"/>
       <c r="CE27" s="5"/>
       <c r="CF27" s="5"/>
@@ -13802,15 +13909,15 @@
     </row>
     <row r="28" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
-        <f>MIN(E28:ZV28)</f>
+        <f t="shared" si="0"/>
         <v>111.95</v>
       </c>
       <c r="B28" s="12">
-        <f>MAX(E28:ZV28)</f>
+        <f t="shared" si="1"/>
         <v>141.65</v>
       </c>
       <c r="C28" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>29.700000000000003</v>
       </c>
       <c r="D28" s="45" t="s">
@@ -13997,8 +14104,12 @@
       <c r="CA28" s="5">
         <v>125.1</v>
       </c>
-      <c r="CB28" s="5"/>
-      <c r="CC28" s="5"/>
+      <c r="CB28" s="5">
+        <v>124.95</v>
+      </c>
+      <c r="CC28" s="5">
+        <v>124.15</v>
+      </c>
       <c r="CD28" s="5"/>
       <c r="CE28" s="5"/>
       <c r="CF28" s="5"/>
@@ -14008,15 +14119,15 @@
     </row>
     <row r="29" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
-        <f>MIN(E29:ZV29)</f>
+        <f t="shared" si="0"/>
         <v>62.3</v>
       </c>
       <c r="B29" s="12">
-        <f>MAX(E29:ZV29)</f>
+        <f t="shared" si="1"/>
         <v>78.849999999999994</v>
       </c>
       <c r="C29" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16.549999999999997</v>
       </c>
       <c r="D29" s="45" t="s">
@@ -14203,8 +14314,12 @@
       <c r="CA29" s="5">
         <v>73.599999999999994</v>
       </c>
-      <c r="CB29" s="5"/>
-      <c r="CC29" s="5"/>
+      <c r="CB29" s="5">
+        <v>74</v>
+      </c>
+      <c r="CC29" s="5">
+        <v>72.75</v>
+      </c>
       <c r="CD29" s="5"/>
       <c r="CE29" s="5"/>
       <c r="CF29" s="5"/>
@@ -14214,15 +14329,15 @@
     </row>
     <row r="30" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
-        <f>MIN(E30:ZV30)</f>
+        <f t="shared" si="0"/>
         <v>39.25</v>
       </c>
       <c r="B30" s="12">
-        <f>MAX(E30:ZV30)</f>
+        <f t="shared" si="1"/>
         <v>50.95</v>
       </c>
       <c r="C30" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11.700000000000003</v>
       </c>
       <c r="D30" s="45" t="s">
@@ -14409,8 +14524,12 @@
       <c r="CA30" s="5">
         <v>40.65</v>
       </c>
-      <c r="CB30" s="5"/>
-      <c r="CC30" s="5"/>
+      <c r="CB30" s="5">
+        <v>40.65</v>
+      </c>
+      <c r="CC30" s="5">
+        <v>40.6</v>
+      </c>
       <c r="CD30" s="5"/>
       <c r="CE30" s="5"/>
       <c r="CF30" s="5"/>
@@ -14420,15 +14539,15 @@
     </row>
     <row r="31" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
-        <f>MIN(E31:ZV31)</f>
+        <f t="shared" si="0"/>
         <v>125.3</v>
       </c>
       <c r="B31" s="12">
-        <f>MAX(E31:ZV31)</f>
+        <f t="shared" si="1"/>
         <v>156.85</v>
       </c>
       <c r="C31" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>31.549999999999997</v>
       </c>
       <c r="D31" s="45" t="s">
@@ -14615,8 +14734,12 @@
       <c r="CA31" s="5">
         <v>138.55000000000001</v>
       </c>
-      <c r="CB31" s="5"/>
-      <c r="CC31" s="5"/>
+      <c r="CB31" s="5">
+        <v>139.19999999999999</v>
+      </c>
+      <c r="CC31" s="5">
+        <v>140.85</v>
+      </c>
       <c r="CD31" s="5"/>
       <c r="CE31" s="5"/>
       <c r="CF31" s="5"/>
@@ -14626,15 +14749,15 @@
     </row>
     <row r="32" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
-        <f>MIN(E32:ZV32)</f>
+        <f t="shared" si="0"/>
         <v>96.65</v>
       </c>
       <c r="B32" s="12">
-        <f>MAX(E32:ZV32)</f>
+        <f t="shared" si="1"/>
         <v>121.8</v>
       </c>
       <c r="C32" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25.149999999999991</v>
       </c>
       <c r="D32" s="45" t="s">
@@ -14809,8 +14932,12 @@
       <c r="CA32" s="5">
         <v>102.8</v>
       </c>
-      <c r="CB32" s="5"/>
-      <c r="CC32" s="5"/>
+      <c r="CB32" s="5">
+        <v>103.45</v>
+      </c>
+      <c r="CC32" s="5">
+        <v>108.8</v>
+      </c>
       <c r="CD32" s="5"/>
       <c r="CE32" s="5"/>
       <c r="CF32" s="5"/>
@@ -14820,15 +14947,15 @@
     </row>
     <row r="33" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
-        <f>MIN(E33:ZV33)</f>
+        <f t="shared" si="0"/>
         <v>56.75</v>
       </c>
       <c r="B33" s="12">
-        <f>MAX(E33:ZV33)</f>
+        <f t="shared" si="1"/>
         <v>67.099999999999994</v>
       </c>
       <c r="C33" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10.349999999999994</v>
       </c>
       <c r="D33" s="45" t="s">
@@ -14991,8 +15118,12 @@
       <c r="CA33" s="5">
         <v>63</v>
       </c>
-      <c r="CB33" s="5"/>
-      <c r="CC33" s="5"/>
+      <c r="CB33" s="5">
+        <v>62.85</v>
+      </c>
+      <c r="CC33" s="5">
+        <v>60.3</v>
+      </c>
       <c r="CD33" s="5"/>
       <c r="CE33" s="5"/>
       <c r="CF33" s="5"/>
@@ -15002,15 +15133,15 @@
     </row>
     <row r="34" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
-        <f>MIN(E34:ZV34)</f>
+        <f t="shared" si="0"/>
         <v>167.9</v>
       </c>
       <c r="B34" s="12">
-        <f>MAX(E34:ZV34)</f>
+        <f t="shared" si="1"/>
         <v>236.1</v>
       </c>
       <c r="C34" s="12">
-        <f t="shared" ref="C34" si="1">B34-A34</f>
+        <f t="shared" ref="C34" si="3">B34-A34</f>
         <v>68.199999999999989</v>
       </c>
       <c r="D34" s="45" t="s">
@@ -15167,8 +15298,12 @@
       <c r="CA34" s="5">
         <v>199.9</v>
       </c>
-      <c r="CB34" s="5"/>
-      <c r="CC34" s="5"/>
+      <c r="CB34" s="5">
+        <v>203.5</v>
+      </c>
+      <c r="CC34" s="5">
+        <v>207.9</v>
+      </c>
       <c r="CD34" s="5"/>
       <c r="CE34" s="5"/>
       <c r="CF34" s="5"/>
@@ -15178,15 +15313,15 @@
     </row>
     <row r="35" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
-        <f>MIN(E35:ZV35)</f>
+        <f t="shared" si="0"/>
         <v>661</v>
       </c>
       <c r="B35" s="12">
-        <f>MAX(E35:ZV35)</f>
+        <f t="shared" si="1"/>
         <v>714.65</v>
       </c>
       <c r="C35" s="12">
-        <f t="shared" ref="C35" si="2">B35-A35</f>
+        <f t="shared" ref="C35" si="4">B35-A35</f>
         <v>53.649999999999977</v>
       </c>
       <c r="D35" s="45" t="s">
@@ -15339,8 +15474,12 @@
       <c r="CA35" s="5">
         <v>700</v>
       </c>
-      <c r="CB35" s="5"/>
-      <c r="CC35" s="5"/>
+      <c r="CB35" s="5">
+        <v>693.5</v>
+      </c>
+      <c r="CC35" s="5">
+        <v>706</v>
+      </c>
       <c r="CD35" s="5"/>
       <c r="CE35" s="5"/>
       <c r="CF35" s="5"/>
@@ -15350,15 +15489,15 @@
     </row>
     <row r="36" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
-        <f>MIN(E36:ZV36)</f>
+        <f t="shared" si="0"/>
         <v>402.9</v>
       </c>
       <c r="B36" s="12">
-        <f>MAX(E36:ZV36)</f>
+        <f t="shared" si="1"/>
         <v>520</v>
       </c>
       <c r="C36" s="12">
-        <f t="shared" ref="C36" si="3">B36-A36</f>
+        <f t="shared" ref="C36" si="5">B36-A36</f>
         <v>117.10000000000002</v>
       </c>
       <c r="D36" s="45" t="s">
@@ -15493,8 +15632,12 @@
       <c r="CA36" s="5">
         <v>423</v>
       </c>
-      <c r="CB36" s="5"/>
-      <c r="CC36" s="5"/>
+      <c r="CB36" s="5">
+        <v>424</v>
+      </c>
+      <c r="CC36" s="5">
+        <v>419</v>
+      </c>
       <c r="CD36" s="5"/>
       <c r="CE36" s="5"/>
       <c r="CF36" s="5"/>
@@ -15504,15 +15647,15 @@
     </row>
     <row r="37" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
-        <f>MIN(E37:ZV37)</f>
+        <f t="shared" si="0"/>
         <v>226</v>
       </c>
       <c r="B37" s="12">
-        <f>MAX(E37:ZV37)</f>
+        <f t="shared" si="1"/>
         <v>396.85</v>
       </c>
       <c r="C37" s="12">
-        <f t="shared" ref="C37" si="4">B37-A37</f>
+        <f t="shared" ref="C37" si="6">B37-A37</f>
         <v>170.85000000000002</v>
       </c>
       <c r="D37" s="45" t="s">
@@ -15637,8 +15780,12 @@
       <c r="CA37" s="5">
         <v>326.8</v>
       </c>
-      <c r="CB37" s="5"/>
-      <c r="CC37" s="5"/>
+      <c r="CB37" s="5">
+        <v>333.3</v>
+      </c>
+      <c r="CC37" s="5">
+        <v>346</v>
+      </c>
       <c r="CD37" s="5"/>
       <c r="CE37" s="5"/>
       <c r="CF37" s="5"/>
@@ -15648,15 +15795,15 @@
     </row>
     <row r="38" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
-        <f>MIN(E38:ZV38)</f>
+        <f t="shared" si="0"/>
         <v>485</v>
       </c>
       <c r="B38" s="12">
-        <f>MAX(E38:ZV38)</f>
+        <f t="shared" si="1"/>
         <v>519.95000000000005</v>
       </c>
       <c r="C38" s="12">
-        <f t="shared" ref="C38" si="5">B38-A38</f>
+        <f t="shared" ref="C38" si="7">B38-A38</f>
         <v>34.950000000000045</v>
       </c>
       <c r="D38" s="45" t="s">
@@ -15779,8 +15926,12 @@
       <c r="CA38" s="5">
         <v>519.95000000000005</v>
       </c>
-      <c r="CB38" s="5"/>
-      <c r="CC38" s="5"/>
+      <c r="CB38" s="5">
+        <v>512.85</v>
+      </c>
+      <c r="CC38" s="5">
+        <v>518.6</v>
+      </c>
       <c r="CD38" s="5"/>
       <c r="CE38" s="5"/>
       <c r="CF38" s="5"/>
@@ -15790,16 +15941,16 @@
     </row>
     <row r="39" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
-        <f>MIN(E39:ZV39)</f>
+        <f t="shared" si="0"/>
         <v>75.2</v>
       </c>
       <c r="B39" s="12">
-        <f>MAX(E39:ZV39)</f>
-        <v>82</v>
+        <f t="shared" si="1"/>
+        <v>83.85</v>
       </c>
       <c r="C39" s="12">
-        <f t="shared" ref="C39" si="6">B39-A39</f>
-        <v>6.7999999999999972</v>
+        <f t="shared" ref="C39" si="8">B39-A39</f>
+        <v>8.6499999999999915</v>
       </c>
       <c r="D39" s="45" t="s">
         <v>305</v>
@@ -15915,8 +16066,12 @@
       <c r="CA39" s="5">
         <v>82</v>
       </c>
-      <c r="CB39" s="5"/>
-      <c r="CC39" s="5"/>
+      <c r="CB39" s="5">
+        <v>83.85</v>
+      </c>
+      <c r="CC39" s="5">
+        <v>83.8</v>
+      </c>
       <c r="CD39" s="5"/>
       <c r="CE39" s="5"/>
       <c r="CF39" s="5"/>
@@ -15926,15 +16081,15 @@
     </row>
     <row r="40" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
-        <f>MIN(E40:ZV40)</f>
+        <f t="shared" si="0"/>
         <v>416</v>
       </c>
       <c r="B40" s="12">
-        <f>MAX(E40:ZV40)</f>
+        <f t="shared" si="1"/>
         <v>472</v>
       </c>
       <c r="C40" s="12">
-        <f t="shared" ref="C40" si="7">B40-A40</f>
+        <f t="shared" ref="C40" si="9">B40-A40</f>
         <v>56</v>
       </c>
       <c r="D40" s="45" t="s">
@@ -16051,8 +16206,12 @@
       <c r="CA40" s="5">
         <v>429.15</v>
       </c>
-      <c r="CB40" s="5"/>
-      <c r="CC40" s="5"/>
+      <c r="CB40" s="5">
+        <v>430.75</v>
+      </c>
+      <c r="CC40" s="5">
+        <v>420.7</v>
+      </c>
       <c r="CD40" s="5"/>
       <c r="CE40" s="5"/>
       <c r="CF40" s="5"/>
@@ -16062,15 +16221,15 @@
     </row>
     <row r="41" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
-        <f>MIN(E41:ZV41)</f>
+        <f t="shared" si="0"/>
         <v>192.65</v>
       </c>
       <c r="B41" s="12">
-        <f>MAX(E41:ZV41)</f>
+        <f t="shared" si="1"/>
         <v>215.25</v>
       </c>
       <c r="C41" s="12">
-        <f t="shared" ref="C41" si="8">B41-A41</f>
+        <f t="shared" ref="C41" si="10">B41-A41</f>
         <v>22.599999999999994</v>
       </c>
       <c r="D41" s="45" t="s">
@@ -16183,8 +16342,12 @@
       <c r="CA41" s="5">
         <v>201</v>
       </c>
-      <c r="CB41" s="5"/>
-      <c r="CC41" s="5"/>
+      <c r="CB41" s="5">
+        <v>201.4</v>
+      </c>
+      <c r="CC41" s="5">
+        <v>193</v>
+      </c>
       <c r="CD41" s="5"/>
       <c r="CE41" s="5"/>
       <c r="CF41" s="5"/>
@@ -16194,16 +16357,16 @@
     </row>
     <row r="42" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
-        <f>MIN(E42:ZV42)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B42" s="12">
-        <f>MAX(E42:ZV42)</f>
-        <v>38.65</v>
+        <f t="shared" si="1"/>
+        <v>39.799999999999997</v>
       </c>
       <c r="C42" s="12">
-        <f t="shared" ref="C42:C45" si="9">B42-A42</f>
-        <v>3.6499999999999986</v>
+        <f t="shared" ref="C42:C45" si="11">B42-A42</f>
+        <v>4.7999999999999972</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>308</v>
@@ -16311,8 +16474,12 @@
       <c r="CA42" s="5">
         <v>37.200000000000003</v>
       </c>
-      <c r="CB42" s="5"/>
-      <c r="CC42" s="5"/>
+      <c r="CB42" s="5">
+        <v>37</v>
+      </c>
+      <c r="CC42" s="5">
+        <v>39.799999999999997</v>
+      </c>
       <c r="CD42" s="5"/>
       <c r="CE42" s="5"/>
       <c r="CF42" s="5"/>
@@ -16322,15 +16489,15 @@
     </row>
     <row r="43" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
-        <f>MIN(E43:ZV43)</f>
+        <f t="shared" si="0"/>
         <v>552.04999999999995</v>
       </c>
       <c r="B43" s="12">
-        <f>MAX(E43:ZV43)</f>
+        <f t="shared" si="1"/>
         <v>626.70000000000005</v>
       </c>
       <c r="C43" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>74.650000000000091</v>
       </c>
       <c r="D43" s="45" t="s">
@@ -16437,8 +16604,12 @@
       <c r="CA43" s="5">
         <v>581.45000000000005</v>
       </c>
-      <c r="CB43" s="5"/>
-      <c r="CC43" s="5"/>
+      <c r="CB43" s="5">
+        <v>578.15</v>
+      </c>
+      <c r="CC43" s="5">
+        <v>585.65</v>
+      </c>
       <c r="CD43" s="5"/>
       <c r="CE43" s="5"/>
       <c r="CF43" s="5"/>
@@ -16448,15 +16619,15 @@
     </row>
     <row r="44" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
-        <f>MIN(E44:ZV44)</f>
+        <f t="shared" si="0"/>
         <v>822.95</v>
       </c>
       <c r="B44" s="12">
-        <f>MAX(E44:ZV44)</f>
+        <f t="shared" si="1"/>
         <v>856</v>
       </c>
       <c r="C44" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>33.049999999999955</v>
       </c>
       <c r="D44" s="45" t="s">
@@ -16563,8 +16734,12 @@
       <c r="CA44" s="5">
         <v>829.4</v>
       </c>
-      <c r="CB44" s="5"/>
-      <c r="CC44" s="5"/>
+      <c r="CB44" s="5">
+        <v>832.05</v>
+      </c>
+      <c r="CC44" s="5">
+        <v>831.9</v>
+      </c>
       <c r="CD44" s="5"/>
       <c r="CE44" s="5"/>
       <c r="CF44" s="5"/>
@@ -16574,15 +16749,15 @@
     </row>
     <row r="45" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
-        <f>MIN(E45:ZV45)</f>
+        <f t="shared" si="0"/>
         <v>134.9</v>
       </c>
       <c r="B45" s="12">
-        <f>MAX(E45:ZV45)</f>
+        <f t="shared" si="1"/>
         <v>146</v>
       </c>
       <c r="C45" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>11.099999999999994</v>
       </c>
       <c r="D45" s="45" t="s">
@@ -16687,8 +16862,12 @@
       <c r="CA45" s="5">
         <v>142.9</v>
       </c>
-      <c r="CB45" s="5"/>
-      <c r="CC45" s="5"/>
+      <c r="CB45" s="5">
+        <v>143.65</v>
+      </c>
+      <c r="CC45" s="5">
+        <v>142.75</v>
+      </c>
       <c r="CD45" s="5"/>
       <c r="CE45" s="5"/>
       <c r="CF45" s="5"/>
@@ -16698,16 +16877,16 @@
     </row>
     <row r="46" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
-        <f>MIN(E46:ZV46)</f>
-        <v>648.4</v>
+        <f t="shared" si="0"/>
+        <v>638.70000000000005</v>
       </c>
       <c r="B46" s="12">
-        <f>MAX(E46:ZV46)</f>
+        <f t="shared" si="1"/>
         <v>770</v>
       </c>
       <c r="C46" s="12">
-        <f t="shared" ref="C46" si="10">B46-A46</f>
-        <v>121.60000000000002</v>
+        <f t="shared" ref="C46" si="12">B46-A46</f>
+        <v>131.29999999999995</v>
       </c>
       <c r="D46" s="45" t="s">
         <v>313</v>
@@ -16805,8 +16984,12 @@
       <c r="CA46" s="5">
         <v>648.4</v>
       </c>
-      <c r="CB46" s="5"/>
-      <c r="CC46" s="5"/>
+      <c r="CB46" s="5">
+        <v>648.4</v>
+      </c>
+      <c r="CC46" s="5">
+        <v>638.70000000000005</v>
+      </c>
       <c r="CD46" s="5"/>
       <c r="CE46" s="5"/>
       <c r="CF46" s="5"/>
@@ -16816,15 +16999,15 @@
     </row>
     <row r="47" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
-        <f>MIN(E47:ZV47)</f>
+        <f t="shared" si="0"/>
         <v>776.5</v>
       </c>
       <c r="B47" s="12">
-        <f>MAX(E47:ZV47)</f>
+        <f t="shared" si="1"/>
         <v>859.9</v>
       </c>
       <c r="C47" s="12">
-        <f t="shared" ref="C47" si="11">B47-A47</f>
+        <f t="shared" ref="C47" si="13">B47-A47</f>
         <v>83.399999999999977</v>
       </c>
       <c r="D47" s="45" t="s">
@@ -16920,11 +17103,15 @@
       <c r="BZ47" s="5">
         <v>852</v>
       </c>
-      <c r="CA47" s="5">
-        <v>851</v>
-      </c>
-      <c r="CB47" s="5"/>
-      <c r="CC47" s="5"/>
+      <c r="CA47" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="CB47" s="5">
+        <v>842.5</v>
+      </c>
+      <c r="CC47" s="5">
+        <v>853</v>
+      </c>
       <c r="CD47" s="5"/>
       <c r="CE47" s="5"/>
       <c r="CF47" s="5"/>
@@ -16934,16 +17121,16 @@
     </row>
     <row r="48" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
-        <f>MIN(E48:ZV48)</f>
-        <v>109</v>
+        <f t="shared" si="0"/>
+        <v>107.55</v>
       </c>
       <c r="B48" s="12">
-        <f>MAX(E48:ZV48)</f>
+        <f t="shared" si="1"/>
         <v>110.95</v>
       </c>
       <c r="C48" s="12">
-        <f t="shared" ref="C48" si="12">B48-A48</f>
-        <v>1.9500000000000028</v>
+        <f t="shared" ref="C48" si="14">B48-A48</f>
+        <v>3.4000000000000057</v>
       </c>
       <c r="D48" s="45" t="s">
         <v>328</v>
@@ -17033,8 +17220,12 @@
       <c r="CA48" s="5">
         <v>109.85</v>
       </c>
-      <c r="CB48" s="5"/>
-      <c r="CC48" s="5"/>
+      <c r="CB48" s="5">
+        <v>109.9</v>
+      </c>
+      <c r="CC48" s="5">
+        <v>107.55</v>
+      </c>
       <c r="CD48" s="5"/>
       <c r="CE48" s="5"/>
       <c r="CF48" s="5"/>

</xml_diff>

<commit_message>
Added details for 30/11/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13530" windowHeight="8175" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13530" windowHeight="8175" firstSheet="3" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PaidTillDate" sheetId="1" r:id="rId1"/>
@@ -7262,9 +7262,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CI48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="BT1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CC16" sqref="CC16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="CA1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CG28" sqref="CG28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7808,7 +7808,7 @@
         <v>329.3</v>
       </c>
       <c r="CC2" s="5">
-        <v>331.9</v>
+        <v>333</v>
       </c>
       <c r="CD2" s="5"/>
       <c r="CE2" s="5"/>
@@ -8054,7 +8054,7 @@
         <v>317.5</v>
       </c>
       <c r="CC3" s="5">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="CD3" s="5"/>
       <c r="CE3" s="5"/>
@@ -8306,7 +8306,7 @@
         <v>259.45</v>
       </c>
       <c r="CC4" s="5">
-        <v>257</v>
+        <v>257.5</v>
       </c>
       <c r="CD4" s="5"/>
       <c r="CE4" s="5"/>
@@ -8558,7 +8558,7 @@
         <v>948.35</v>
       </c>
       <c r="CC5" s="5">
-        <v>942.4</v>
+        <v>947.4</v>
       </c>
       <c r="CD5" s="5"/>
       <c r="CE5" s="5"/>
@@ -8810,7 +8810,7 @@
         <v>270.8</v>
       </c>
       <c r="CC6" s="5">
-        <v>273.8</v>
+        <v>280.7</v>
       </c>
       <c r="CD6" s="5"/>
       <c r="CE6" s="5"/>
@@ -9062,7 +9062,7 @@
         <v>18.350000000000001</v>
       </c>
       <c r="CC7" s="5">
-        <v>18.05</v>
+        <v>18.149999999999999</v>
       </c>
       <c r="CD7" s="5"/>
       <c r="CE7" s="5"/>
@@ -9314,7 +9314,7 @@
         <v>82</v>
       </c>
       <c r="CC8" s="5">
-        <v>80.599999999999994</v>
+        <v>79.05</v>
       </c>
       <c r="CD8" s="5"/>
       <c r="CE8" s="5"/>
@@ -9558,7 +9558,7 @@
         <v>54.8</v>
       </c>
       <c r="CC9" s="28">
-        <v>55.3</v>
+        <v>56.15</v>
       </c>
       <c r="CD9" s="28"/>
       <c r="CE9" s="28"/>
@@ -9810,7 +9810,7 @@
         <v>38.299999999999997</v>
       </c>
       <c r="CC10" s="5">
-        <v>38.75</v>
+        <v>39</v>
       </c>
       <c r="CD10" s="5"/>
       <c r="CE10" s="5"/>
@@ -10062,7 +10062,7 @@
         <v>95.1</v>
       </c>
       <c r="CC11" s="5">
-        <v>95.1</v>
+        <v>95</v>
       </c>
       <c r="CD11" s="5"/>
       <c r="CE11" s="5"/>
@@ -10314,7 +10314,7 @@
         <v>91.7</v>
       </c>
       <c r="CC12" s="5">
-        <v>93.9</v>
+        <v>94</v>
       </c>
       <c r="CD12" s="5"/>
       <c r="CE12" s="5"/>
@@ -10566,7 +10566,7 @@
         <v>52.75</v>
       </c>
       <c r="CC13" s="5">
-        <v>53.5</v>
+        <v>55.55</v>
       </c>
       <c r="CD13" s="5"/>
       <c r="CE13" s="5"/>
@@ -10818,7 +10818,7 @@
         <v>35</v>
       </c>
       <c r="CC14" s="5">
-        <v>38.6</v>
+        <v>41.55</v>
       </c>
       <c r="CD14" s="5"/>
       <c r="CE14" s="5"/>
@@ -11062,7 +11062,7 @@
         <v>25.45</v>
       </c>
       <c r="CC15" s="5">
-        <v>24.9</v>
+        <v>24.7</v>
       </c>
       <c r="CD15" s="5"/>
       <c r="CE15" s="5"/>
@@ -11314,7 +11314,7 @@
         <v>703.4</v>
       </c>
       <c r="CC16" s="5">
-        <v>703</v>
+        <v>706.65</v>
       </c>
       <c r="CD16" s="5"/>
       <c r="CE16" s="5"/>
@@ -11566,7 +11566,7 @@
         <v>472</v>
       </c>
       <c r="CC17" s="5">
-        <v>469.95</v>
+        <v>474.3</v>
       </c>
       <c r="CD17" s="5"/>
       <c r="CE17" s="5"/>
@@ -11818,7 +11818,7 @@
         <v>260.10000000000002</v>
       </c>
       <c r="CC18" s="5">
-        <v>265.5</v>
+        <v>268.10000000000002</v>
       </c>
       <c r="CD18" s="5"/>
       <c r="CE18" s="5"/>
@@ -12070,7 +12070,7 @@
         <v>719.55</v>
       </c>
       <c r="CC19" s="5">
-        <v>702</v>
+        <v>708</v>
       </c>
       <c r="CD19" s="5"/>
       <c r="CE19" s="5"/>
@@ -12322,7 +12322,7 @@
         <v>717.65</v>
       </c>
       <c r="CC20" s="5">
-        <v>705.1</v>
+        <v>713.55</v>
       </c>
       <c r="CD20" s="5"/>
       <c r="CE20" s="5"/>
@@ -12574,7 +12574,7 @@
         <v>495</v>
       </c>
       <c r="CC21" s="5">
-        <v>490.5</v>
+        <v>494.9</v>
       </c>
       <c r="CD21" s="5"/>
       <c r="CE21" s="5"/>
@@ -12772,7 +12772,7 @@
         <v>408.7</v>
       </c>
       <c r="CC22" s="5">
-        <v>399</v>
+        <v>399.55</v>
       </c>
       <c r="CD22" s="5"/>
       <c r="CE22" s="5"/>
@@ -13016,7 +13016,7 @@
         <v>62.4</v>
       </c>
       <c r="CC23" s="5">
-        <v>61.35</v>
+        <v>62.25</v>
       </c>
       <c r="CD23" s="5"/>
       <c r="CE23" s="5"/>
@@ -13256,7 +13256,7 @@
         <v>239.15</v>
       </c>
       <c r="CC24" s="5">
-        <v>235.75</v>
+        <v>238.3</v>
       </c>
       <c r="CD24" s="5"/>
       <c r="CE24" s="5"/>
@@ -13478,7 +13478,7 @@
         <v>996.05</v>
       </c>
       <c r="CC25" s="5">
-        <v>982.15</v>
+        <v>983.15</v>
       </c>
       <c r="CD25" s="5"/>
       <c r="CE25" s="5"/>
@@ -13688,7 +13688,7 @@
         <v>90.35</v>
       </c>
       <c r="CC26" s="5">
-        <v>93</v>
+        <v>93.95</v>
       </c>
       <c r="CD26" s="5"/>
       <c r="CE26" s="5"/>
@@ -13898,7 +13898,7 @@
         <v>43.3</v>
       </c>
       <c r="CC27" s="5">
-        <v>43.3</v>
+        <v>43.2</v>
       </c>
       <c r="CD27" s="5"/>
       <c r="CE27" s="5"/>
@@ -14108,7 +14108,7 @@
         <v>124.95</v>
       </c>
       <c r="CC28" s="5">
-        <v>124.15</v>
+        <v>130.4</v>
       </c>
       <c r="CD28" s="5"/>
       <c r="CE28" s="5"/>
@@ -14318,7 +14318,7 @@
         <v>74</v>
       </c>
       <c r="CC29" s="5">
-        <v>72.75</v>
+        <v>72.2</v>
       </c>
       <c r="CD29" s="5"/>
       <c r="CE29" s="5"/>
@@ -14528,7 +14528,7 @@
         <v>40.65</v>
       </c>
       <c r="CC30" s="5">
-        <v>40.6</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="CD30" s="5"/>
       <c r="CE30" s="5"/>
@@ -14738,7 +14738,7 @@
         <v>139.19999999999999</v>
       </c>
       <c r="CC31" s="5">
-        <v>140.85</v>
+        <v>141.55000000000001</v>
       </c>
       <c r="CD31" s="5"/>
       <c r="CE31" s="5"/>
@@ -15122,7 +15122,7 @@
         <v>62.85</v>
       </c>
       <c r="CC33" s="5">
-        <v>60.3</v>
+        <v>60.45</v>
       </c>
       <c r="CD33" s="5"/>
       <c r="CE33" s="5"/>
@@ -15302,7 +15302,7 @@
         <v>203.5</v>
       </c>
       <c r="CC34" s="5">
-        <v>207.9</v>
+        <v>207.75</v>
       </c>
       <c r="CD34" s="5"/>
       <c r="CE34" s="5"/>
@@ -15318,11 +15318,11 @@
       </c>
       <c r="B35" s="12">
         <f t="shared" si="1"/>
-        <v>714.65</v>
+        <v>715.7</v>
       </c>
       <c r="C35" s="12">
         <f t="shared" ref="C35" si="4">B35-A35</f>
-        <v>53.649999999999977</v>
+        <v>54.700000000000045</v>
       </c>
       <c r="D35" s="45" t="s">
         <v>281</v>
@@ -15478,7 +15478,7 @@
         <v>693.5</v>
       </c>
       <c r="CC35" s="5">
-        <v>706</v>
+        <v>715.7</v>
       </c>
       <c r="CD35" s="5"/>
       <c r="CE35" s="5"/>
@@ -15636,7 +15636,7 @@
         <v>424</v>
       </c>
       <c r="CC36" s="5">
-        <v>419</v>
+        <v>419.9</v>
       </c>
       <c r="CD36" s="5"/>
       <c r="CE36" s="5"/>
@@ -15784,7 +15784,7 @@
         <v>333.3</v>
       </c>
       <c r="CC37" s="5">
-        <v>346</v>
+        <v>349.9</v>
       </c>
       <c r="CD37" s="5"/>
       <c r="CE37" s="5"/>
@@ -15800,11 +15800,11 @@
       </c>
       <c r="B38" s="12">
         <f t="shared" si="1"/>
-        <v>519.95000000000005</v>
+        <v>520</v>
       </c>
       <c r="C38" s="12">
         <f t="shared" ref="C38" si="7">B38-A38</f>
-        <v>34.950000000000045</v>
+        <v>35</v>
       </c>
       <c r="D38" s="45" t="s">
         <v>298</v>
@@ -15930,7 +15930,7 @@
         <v>512.85</v>
       </c>
       <c r="CC38" s="5">
-        <v>518.6</v>
+        <v>520</v>
       </c>
       <c r="CD38" s="5"/>
       <c r="CE38" s="5"/>
@@ -16070,7 +16070,7 @@
         <v>83.85</v>
       </c>
       <c r="CC39" s="5">
-        <v>83.8</v>
+        <v>83.15</v>
       </c>
       <c r="CD39" s="5"/>
       <c r="CE39" s="5"/>
@@ -16210,7 +16210,7 @@
         <v>430.75</v>
       </c>
       <c r="CC40" s="5">
-        <v>420.7</v>
+        <v>422.1</v>
       </c>
       <c r="CD40" s="5"/>
       <c r="CE40" s="5"/>
@@ -16222,7 +16222,7 @@
     <row r="41" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <f t="shared" si="0"/>
-        <v>192.65</v>
+        <v>191</v>
       </c>
       <c r="B41" s="12">
         <f t="shared" si="1"/>
@@ -16230,7 +16230,7 @@
       </c>
       <c r="C41" s="12">
         <f t="shared" ref="C41" si="10">B41-A41</f>
-        <v>22.599999999999994</v>
+        <v>24.25</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>307</v>
@@ -16346,7 +16346,7 @@
         <v>201.4</v>
       </c>
       <c r="CC41" s="5">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="CD41" s="5"/>
       <c r="CE41" s="5"/>
@@ -16362,11 +16362,11 @@
       </c>
       <c r="B42" s="12">
         <f t="shared" si="1"/>
-        <v>39.799999999999997</v>
+        <v>39.450000000000003</v>
       </c>
       <c r="C42" s="12">
         <f t="shared" ref="C42:C45" si="11">B42-A42</f>
-        <v>4.7999999999999972</v>
+        <v>4.4500000000000028</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>308</v>
@@ -16478,7 +16478,7 @@
         <v>37</v>
       </c>
       <c r="CC42" s="5">
-        <v>39.799999999999997</v>
+        <v>39.450000000000003</v>
       </c>
       <c r="CD42" s="5"/>
       <c r="CE42" s="5"/>
@@ -16608,7 +16608,7 @@
         <v>578.15</v>
       </c>
       <c r="CC43" s="5">
-        <v>585.65</v>
+        <v>607.15</v>
       </c>
       <c r="CD43" s="5"/>
       <c r="CE43" s="5"/>
@@ -16738,7 +16738,7 @@
         <v>832.05</v>
       </c>
       <c r="CC44" s="5">
-        <v>831.9</v>
+        <v>836.65</v>
       </c>
       <c r="CD44" s="5"/>
       <c r="CE44" s="5"/>
@@ -16866,7 +16866,7 @@
         <v>143.65</v>
       </c>
       <c r="CC45" s="5">
-        <v>142.75</v>
+        <v>145.1</v>
       </c>
       <c r="CD45" s="5"/>
       <c r="CE45" s="5"/>
@@ -16878,7 +16878,7 @@
     <row r="46" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <f t="shared" si="0"/>
-        <v>638.70000000000005</v>
+        <v>639.79999999999995</v>
       </c>
       <c r="B46" s="12">
         <f t="shared" si="1"/>
@@ -16886,7 +16886,7 @@
       </c>
       <c r="C46" s="12">
         <f t="shared" ref="C46" si="12">B46-A46</f>
-        <v>131.29999999999995</v>
+        <v>130.20000000000005</v>
       </c>
       <c r="D46" s="45" t="s">
         <v>313</v>
@@ -16988,7 +16988,7 @@
         <v>648.4</v>
       </c>
       <c r="CC46" s="5">
-        <v>638.70000000000005</v>
+        <v>639.79999999999995</v>
       </c>
       <c r="CD46" s="5"/>
       <c r="CE46" s="5"/>
@@ -17004,11 +17004,11 @@
       </c>
       <c r="B47" s="12">
         <f t="shared" si="1"/>
-        <v>859.9</v>
+        <v>868.95</v>
       </c>
       <c r="C47" s="12">
         <f t="shared" ref="C47" si="13">B47-A47</f>
-        <v>83.399999999999977</v>
+        <v>92.450000000000045</v>
       </c>
       <c r="D47" s="45" t="s">
         <v>327</v>
@@ -17110,7 +17110,7 @@
         <v>842.5</v>
       </c>
       <c r="CC47" s="5">
-        <v>853</v>
+        <v>868.95</v>
       </c>
       <c r="CD47" s="5"/>
       <c r="CE47" s="5"/>
@@ -17122,7 +17122,7 @@
     <row r="48" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <f t="shared" si="0"/>
-        <v>107.55</v>
+        <v>107.9</v>
       </c>
       <c r="B48" s="12">
         <f t="shared" si="1"/>
@@ -17130,7 +17130,7 @@
       </c>
       <c r="C48" s="12">
         <f t="shared" ref="C48" si="14">B48-A48</f>
-        <v>3.4000000000000057</v>
+        <v>3.0499999999999972</v>
       </c>
       <c r="D48" s="45" t="s">
         <v>328</v>
@@ -17224,7 +17224,7 @@
         <v>109.9</v>
       </c>
       <c r="CC48" s="5">
-        <v>107.55</v>
+        <v>107.9</v>
       </c>
       <c r="CD48" s="5"/>
       <c r="CE48" s="5"/>

</xml_diff>

<commit_message>
Added details for 1/12/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="326">
   <si>
     <t>Date</t>
   </si>
@@ -921,9 +921,6 @@
     <t xml:space="preserve">RAIN </t>
   </si>
   <si>
-    <t xml:space="preserve">HAVELLS </t>
-  </si>
-  <si>
     <t>25/10/2017</t>
   </si>
   <si>
@@ -1002,19 +999,10 @@
     <t>28/11/2026</t>
   </si>
   <si>
-    <t>29/11/2027</t>
-  </si>
-  <si>
     <t>30/11/2028</t>
   </si>
   <si>
-    <t>TIMKEN</t>
-  </si>
-  <si>
     <t>MEGH</t>
-  </si>
-  <si>
-    <t>Di</t>
   </si>
 </sst>
 </file>
@@ -7260,11 +7248,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CI48"/>
+  <dimension ref="A1:CE46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="CA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CG28" sqref="CG28"/>
+      <selection pane="topRight" activeCell="CD2" sqref="CD2:CD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7313,10 +7301,12 @@
     <col min="77" max="77" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="14.42578125" customWidth="1"/>
-    <col min="80" max="83" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="80" max="81" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:83" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>249</v>
       </c>
@@ -7495,19 +7485,19 @@
         <v>296</v>
       </c>
       <c r="BH1" s="51" t="s">
+        <v>298</v>
+      </c>
+      <c r="BI1" s="51" t="s">
         <v>299</v>
       </c>
-      <c r="BI1" s="51" t="s">
+      <c r="BJ1" s="51" t="s">
         <v>300</v>
       </c>
-      <c r="BJ1" s="51" t="s">
+      <c r="BK1" s="51" t="s">
         <v>301</v>
       </c>
-      <c r="BK1" s="51" t="s">
+      <c r="BL1" s="51" t="s">
         <v>302</v>
-      </c>
-      <c r="BL1" s="51" t="s">
-        <v>303</v>
       </c>
       <c r="BM1" s="51">
         <v>42777</v>
@@ -7528,56 +7518,52 @@
         <v>43019</v>
       </c>
       <c r="BS1" s="49" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="BT1" s="49" t="s">
+        <v>314</v>
+      </c>
+      <c r="BU1" s="49" t="s">
         <v>315</v>
       </c>
-      <c r="BU1" s="49" t="s">
+      <c r="BV1" s="49" t="s">
         <v>316</v>
       </c>
-      <c r="BV1" s="49" t="s">
+      <c r="BW1" s="49" t="s">
         <v>317</v>
       </c>
-      <c r="BW1" s="49" t="s">
+      <c r="BX1" s="49" t="s">
         <v>318</v>
       </c>
-      <c r="BX1" s="49" t="s">
+      <c r="BY1" s="49" t="s">
         <v>319</v>
       </c>
-      <c r="BY1" s="49" t="s">
+      <c r="BZ1" s="49" t="s">
         <v>320</v>
       </c>
-      <c r="BZ1" s="49" t="s">
+      <c r="CA1" s="49" t="s">
         <v>321</v>
       </c>
-      <c r="CA1" s="49" t="s">
+      <c r="CB1" s="49" t="s">
         <v>322</v>
       </c>
-      <c r="CB1" s="49" t="s">
+      <c r="CC1" s="49" t="s">
         <v>323</v>
       </c>
-      <c r="CC1" s="49" t="s">
+      <c r="CD1" s="51">
+        <v>43112</v>
+      </c>
+      <c r="CE1" s="49" t="s">
         <v>324</v>
       </c>
-      <c r="CD1" s="49" t="s">
-        <v>325</v>
-      </c>
-      <c r="CE1" s="49" t="s">
-        <v>326</v>
-      </c>
-      <c r="CF1" s="27"/>
-      <c r="CG1" s="27"/>
-      <c r="CH1" s="27"/>
-      <c r="CI1" s="27"/>
-    </row>
-    <row r="2" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
-        <f t="shared" ref="A2:A48" si="0">MIN(E2:ZV2)</f>
+        <f t="shared" ref="A2:A46" si="0">MIN(E2:ZR2)</f>
         <v>243.6</v>
       </c>
       <c r="B2" s="12">
-        <f t="shared" ref="B2:B48" si="1">MAX(E2:ZV2)</f>
+        <f t="shared" ref="B2:B46" si="1">MAX(E2:ZR2)</f>
         <v>340.8</v>
       </c>
       <c r="C2" s="12">
@@ -7810,14 +7796,12 @@
       <c r="CC2" s="5">
         <v>333</v>
       </c>
-      <c r="CD2" s="5"/>
+      <c r="CD2" s="5">
+        <v>316.95</v>
+      </c>
       <c r="CE2" s="5"/>
-      <c r="CF2" s="5"/>
-      <c r="CG2" s="5"/>
-      <c r="CH2" s="5"/>
-      <c r="CI2" s="5"/>
-    </row>
-    <row r="3" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <f t="shared" si="0"/>
         <v>262.7</v>
@@ -8056,14 +8040,12 @@
       <c r="CC3" s="5">
         <v>315</v>
       </c>
-      <c r="CD3" s="5"/>
+      <c r="CD3" s="5">
+        <v>306.2</v>
+      </c>
       <c r="CE3" s="5"/>
-      <c r="CF3" s="5"/>
-      <c r="CG3" s="5"/>
-      <c r="CH3" s="5"/>
-      <c r="CI3" s="5"/>
-    </row>
-    <row r="4" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
         <v>253.85</v>
@@ -8308,14 +8290,12 @@
       <c r="CC4" s="5">
         <v>257.5</v>
       </c>
-      <c r="CD4" s="5"/>
+      <c r="CD4" s="5">
+        <v>256.45</v>
+      </c>
       <c r="CE4" s="5"/>
-      <c r="CF4" s="5"/>
-      <c r="CG4" s="5"/>
-      <c r="CH4" s="5"/>
-      <c r="CI4" s="5"/>
-    </row>
-    <row r="5" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <f t="shared" si="0"/>
         <v>786.25</v>
@@ -8560,14 +8540,12 @@
       <c r="CC5" s="5">
         <v>947.4</v>
       </c>
-      <c r="CD5" s="5"/>
+      <c r="CD5" s="5">
+        <v>913.5</v>
+      </c>
       <c r="CE5" s="5"/>
-      <c r="CF5" s="5"/>
-      <c r="CG5" s="5"/>
-      <c r="CH5" s="5"/>
-      <c r="CI5" s="5"/>
-    </row>
-    <row r="6" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <f t="shared" si="0"/>
         <v>236.45</v>
@@ -8812,14 +8790,12 @@
       <c r="CC6" s="5">
         <v>280.7</v>
       </c>
-      <c r="CD6" s="5"/>
+      <c r="CD6" s="5">
+        <v>271.39999999999998</v>
+      </c>
       <c r="CE6" s="5"/>
-      <c r="CF6" s="5"/>
-      <c r="CG6" s="5"/>
-      <c r="CH6" s="5"/>
-      <c r="CI6" s="5"/>
-    </row>
-    <row r="7" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <f t="shared" si="0"/>
         <v>15.6</v>
@@ -9064,14 +9040,12 @@
       <c r="CC7" s="5">
         <v>18.149999999999999</v>
       </c>
-      <c r="CD7" s="5"/>
+      <c r="CD7" s="5">
+        <v>17.899999999999999</v>
+      </c>
       <c r="CE7" s="5"/>
-      <c r="CF7" s="5"/>
-      <c r="CG7" s="5"/>
-      <c r="CH7" s="5"/>
-      <c r="CI7" s="5"/>
-    </row>
-    <row r="8" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <f t="shared" si="0"/>
         <v>53.4</v>
@@ -9316,14 +9290,12 @@
       <c r="CC8" s="5">
         <v>79.05</v>
       </c>
-      <c r="CD8" s="5"/>
+      <c r="CD8" s="5">
+        <v>79.45</v>
+      </c>
       <c r="CE8" s="5"/>
-      <c r="CF8" s="5"/>
-      <c r="CG8" s="5"/>
-      <c r="CH8" s="5"/>
-      <c r="CI8" s="5"/>
-    </row>
-    <row r="9" spans="1:87" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:83" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <f t="shared" si="0"/>
         <v>53.5</v>
@@ -9560,14 +9532,12 @@
       <c r="CC9" s="28">
         <v>56.15</v>
       </c>
-      <c r="CD9" s="28"/>
+      <c r="CD9" s="28">
+        <v>54.7</v>
+      </c>
       <c r="CE9" s="28"/>
-      <c r="CF9" s="28"/>
-      <c r="CG9" s="28"/>
-      <c r="CH9" s="28"/>
-      <c r="CI9" s="28"/>
-    </row>
-    <row r="10" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <f t="shared" si="0"/>
         <v>35.549999999999997</v>
@@ -9812,14 +9782,12 @@
       <c r="CC10" s="5">
         <v>39</v>
       </c>
-      <c r="CD10" s="5"/>
+      <c r="CD10" s="5">
+        <v>38.1</v>
+      </c>
       <c r="CE10" s="5"/>
-      <c r="CF10" s="5"/>
-      <c r="CG10" s="5"/>
-      <c r="CH10" s="5"/>
-      <c r="CI10" s="5"/>
-    </row>
-    <row r="11" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <f t="shared" si="0"/>
         <v>72.650000000000006</v>
@@ -10064,14 +10032,12 @@
       <c r="CC11" s="5">
         <v>95</v>
       </c>
-      <c r="CD11" s="5"/>
+      <c r="CD11" s="5">
+        <v>93.6</v>
+      </c>
       <c r="CE11" s="5"/>
-      <c r="CF11" s="5"/>
-      <c r="CG11" s="5"/>
-      <c r="CH11" s="5"/>
-      <c r="CI11" s="5"/>
-    </row>
-    <row r="12" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
         <v>82.65</v>
@@ -10316,14 +10282,12 @@
       <c r="CC12" s="5">
         <v>94</v>
       </c>
-      <c r="CD12" s="5"/>
+      <c r="CD12" s="5">
+        <v>92.05</v>
+      </c>
       <c r="CE12" s="5"/>
-      <c r="CF12" s="5"/>
-      <c r="CG12" s="5"/>
-      <c r="CH12" s="5"/>
-      <c r="CI12" s="5"/>
-    </row>
-    <row r="13" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <f t="shared" si="0"/>
         <v>44.1</v>
@@ -10568,25 +10532,23 @@
       <c r="CC13" s="5">
         <v>55.55</v>
       </c>
-      <c r="CD13" s="5"/>
+      <c r="CD13" s="5">
+        <v>54.25</v>
+      </c>
       <c r="CE13" s="5"/>
-      <c r="CF13" s="5"/>
-      <c r="CG13" s="5"/>
-      <c r="CH13" s="5"/>
-      <c r="CI13" s="5"/>
-    </row>
-    <row r="14" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <f t="shared" si="0"/>
         <v>29.75</v>
       </c>
       <c r="B14" s="12">
         <f t="shared" si="1"/>
-        <v>41.85</v>
+        <v>41.9</v>
       </c>
       <c r="C14" s="12">
         <f t="shared" si="2"/>
-        <v>12.100000000000001</v>
+        <v>12.149999999999999</v>
       </c>
       <c r="D14" s="45" t="s">
         <v>21</v>
@@ -10820,14 +10782,12 @@
       <c r="CC14" s="5">
         <v>41.55</v>
       </c>
-      <c r="CD14" s="5"/>
+      <c r="CD14" s="5">
+        <v>41.9</v>
+      </c>
       <c r="CE14" s="5"/>
-      <c r="CF14" s="5"/>
-      <c r="CG14" s="5"/>
-      <c r="CH14" s="5"/>
-      <c r="CI14" s="5"/>
-    </row>
-    <row r="15" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
         <v>23.95</v>
@@ -11064,14 +11024,12 @@
       <c r="CC15" s="5">
         <v>24.7</v>
       </c>
-      <c r="CD15" s="5"/>
+      <c r="CD15" s="5">
+        <v>24.55</v>
+      </c>
       <c r="CE15" s="5"/>
-      <c r="CF15" s="5"/>
-      <c r="CG15" s="5"/>
-      <c r="CH15" s="5"/>
-      <c r="CI15" s="5"/>
-    </row>
-    <row r="16" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <f t="shared" si="0"/>
         <v>552</v>
@@ -11316,14 +11274,12 @@
       <c r="CC16" s="5">
         <v>706.65</v>
       </c>
-      <c r="CD16" s="5"/>
+      <c r="CD16" s="5">
+        <v>682.55</v>
+      </c>
       <c r="CE16" s="5"/>
-      <c r="CF16" s="5"/>
-      <c r="CG16" s="5"/>
-      <c r="CH16" s="5"/>
-      <c r="CI16" s="5"/>
-    </row>
-    <row r="17" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <f t="shared" si="0"/>
         <v>433</v>
@@ -11568,14 +11524,12 @@
       <c r="CC17" s="5">
         <v>474.3</v>
       </c>
-      <c r="CD17" s="5"/>
+      <c r="CD17" s="5">
+        <v>477.5</v>
+      </c>
       <c r="CE17" s="5"/>
-      <c r="CF17" s="5"/>
-      <c r="CG17" s="5"/>
-      <c r="CH17" s="5"/>
-      <c r="CI17" s="5"/>
-    </row>
-    <row r="18" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <f t="shared" si="0"/>
         <v>178.8</v>
@@ -11820,14 +11774,12 @@
       <c r="CC18" s="5">
         <v>268.10000000000002</v>
       </c>
-      <c r="CD18" s="5"/>
+      <c r="CD18" s="5">
+        <v>273</v>
+      </c>
       <c r="CE18" s="5"/>
-      <c r="CF18" s="5"/>
-      <c r="CG18" s="5"/>
-      <c r="CH18" s="5"/>
-      <c r="CI18" s="5"/>
-    </row>
-    <row r="19" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <f t="shared" si="0"/>
         <v>440.7</v>
@@ -12072,14 +12024,12 @@
       <c r="CC19" s="5">
         <v>708</v>
       </c>
-      <c r="CD19" s="5"/>
+      <c r="CD19" s="5">
+        <v>706.5</v>
+      </c>
       <c r="CE19" s="5"/>
-      <c r="CF19" s="5"/>
-      <c r="CG19" s="5"/>
-      <c r="CH19" s="5"/>
-      <c r="CI19" s="5"/>
-    </row>
-    <row r="20" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <f t="shared" si="0"/>
         <v>677</v>
@@ -12324,14 +12274,12 @@
       <c r="CC20" s="5">
         <v>713.55</v>
       </c>
-      <c r="CD20" s="5"/>
+      <c r="CD20" s="5">
+        <v>684.6</v>
+      </c>
       <c r="CE20" s="5"/>
-      <c r="CF20" s="5"/>
-      <c r="CG20" s="5"/>
-      <c r="CH20" s="5"/>
-      <c r="CI20" s="5"/>
-    </row>
-    <row r="21" spans="1:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <f t="shared" si="0"/>
         <v>376.7</v>
@@ -12576,14 +12524,12 @@
       <c r="CC21" s="5">
         <v>494.9</v>
       </c>
-      <c r="CD21" s="5"/>
+      <c r="CD21" s="5">
+        <v>491.55</v>
+      </c>
       <c r="CE21" s="5"/>
-      <c r="CF21" s="5"/>
-      <c r="CG21" s="5"/>
-      <c r="CH21" s="5"/>
-      <c r="CI21" s="5"/>
-    </row>
-    <row r="22" spans="1:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <f t="shared" si="0"/>
         <v>315.2</v>
@@ -12774,14 +12720,12 @@
       <c r="CC22" s="5">
         <v>399.55</v>
       </c>
-      <c r="CD22" s="5"/>
+      <c r="CD22" s="5">
+        <v>384.8</v>
+      </c>
       <c r="CE22" s="5"/>
-      <c r="CF22" s="5"/>
-      <c r="CG22" s="5"/>
-      <c r="CH22" s="5"/>
-      <c r="CI22" s="5"/>
-    </row>
-    <row r="23" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
         <v>54.45</v>
@@ -13018,14 +12962,12 @@
       <c r="CC23" s="5">
         <v>62.25</v>
       </c>
-      <c r="CD23" s="5"/>
+      <c r="CD23" s="5">
+        <v>60.95</v>
+      </c>
       <c r="CE23" s="5"/>
-      <c r="CF23" s="5"/>
-      <c r="CG23" s="5"/>
-      <c r="CH23" s="5"/>
-      <c r="CI23" s="5"/>
-    </row>
-    <row r="24" spans="1:87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <f t="shared" si="0"/>
         <v>210.65</v>
@@ -13258,14 +13200,12 @@
       <c r="CC24" s="5">
         <v>238.3</v>
       </c>
-      <c r="CD24" s="5"/>
+      <c r="CD24" s="5">
+        <v>231.25</v>
+      </c>
       <c r="CE24" s="5"/>
-      <c r="CF24" s="5"/>
-      <c r="CG24" s="5"/>
-      <c r="CH24" s="5"/>
-      <c r="CI24" s="5"/>
-    </row>
-    <row r="25" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <f t="shared" si="0"/>
         <v>876</v>
@@ -13480,25 +13420,23 @@
       <c r="CC25" s="5">
         <v>983.15</v>
       </c>
-      <c r="CD25" s="5"/>
+      <c r="CD25" s="5">
+        <v>963</v>
+      </c>
       <c r="CE25" s="5"/>
-      <c r="CF25" s="5"/>
-      <c r="CG25" s="5"/>
-      <c r="CH25" s="5"/>
-      <c r="CI25" s="5"/>
-    </row>
-    <row r="26" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <f t="shared" si="0"/>
         <v>83.1</v>
       </c>
       <c r="B26" s="12">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>102.25</v>
       </c>
       <c r="C26" s="12">
         <f t="shared" si="2"/>
-        <v>12.900000000000006</v>
+        <v>19.150000000000006</v>
       </c>
       <c r="D26" s="45" t="s">
         <v>252</v>
@@ -13690,14 +13628,12 @@
       <c r="CC26" s="5">
         <v>93.95</v>
       </c>
-      <c r="CD26" s="5"/>
+      <c r="CD26" s="5">
+        <v>102.25</v>
+      </c>
       <c r="CE26" s="5"/>
-      <c r="CF26" s="5"/>
-      <c r="CG26" s="5"/>
-      <c r="CH26" s="5"/>
-      <c r="CI26" s="5"/>
-    </row>
-    <row r="27" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <f t="shared" si="0"/>
         <v>36.200000000000003</v>
@@ -13900,14 +13836,12 @@
       <c r="CC27" s="5">
         <v>43.2</v>
       </c>
-      <c r="CD27" s="5"/>
+      <c r="CD27" s="5">
+        <v>41.7</v>
+      </c>
       <c r="CE27" s="5"/>
-      <c r="CF27" s="5"/>
-      <c r="CG27" s="5"/>
-      <c r="CH27" s="5"/>
-      <c r="CI27" s="5"/>
-    </row>
-    <row r="28" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <f t="shared" si="0"/>
         <v>111.95</v>
@@ -14110,14 +14044,12 @@
       <c r="CC28" s="5">
         <v>130.4</v>
       </c>
-      <c r="CD28" s="5"/>
+      <c r="CD28" s="5">
+        <v>127.65</v>
+      </c>
       <c r="CE28" s="5"/>
-      <c r="CF28" s="5"/>
-      <c r="CG28" s="5"/>
-      <c r="CH28" s="5"/>
-      <c r="CI28" s="5"/>
-    </row>
-    <row r="29" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <f t="shared" si="0"/>
         <v>62.3</v>
@@ -14320,17 +14252,15 @@
       <c r="CC29" s="5">
         <v>72.2</v>
       </c>
-      <c r="CD29" s="5"/>
+      <c r="CD29" s="5">
+        <v>69.95</v>
+      </c>
       <c r="CE29" s="5"/>
-      <c r="CF29" s="5"/>
-      <c r="CG29" s="5"/>
-      <c r="CH29" s="5"/>
-      <c r="CI29" s="5"/>
-    </row>
-    <row r="30" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <f t="shared" si="0"/>
-        <v>39.25</v>
+        <v>38.6</v>
       </c>
       <c r="B30" s="12">
         <f t="shared" si="1"/>
@@ -14338,7 +14268,7 @@
       </c>
       <c r="C30" s="12">
         <f t="shared" si="2"/>
-        <v>11.700000000000003</v>
+        <v>12.350000000000001</v>
       </c>
       <c r="D30" s="45" t="s">
         <v>256</v>
@@ -14530,14 +14460,12 @@
       <c r="CC30" s="5">
         <v>40.799999999999997</v>
       </c>
-      <c r="CD30" s="5"/>
+      <c r="CD30" s="5">
+        <v>38.6</v>
+      </c>
       <c r="CE30" s="5"/>
-      <c r="CF30" s="5"/>
-      <c r="CG30" s="5"/>
-      <c r="CH30" s="5"/>
-      <c r="CI30" s="5"/>
-    </row>
-    <row r="31" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
         <v>125.3</v>
@@ -14740,14 +14668,12 @@
       <c r="CC31" s="5">
         <v>141.55000000000001</v>
       </c>
-      <c r="CD31" s="5"/>
+      <c r="CD31" s="5">
+        <v>145.44999999999999</v>
+      </c>
       <c r="CE31" s="5"/>
-      <c r="CF31" s="5"/>
-      <c r="CG31" s="5"/>
-      <c r="CH31" s="5"/>
-      <c r="CI31" s="5"/>
-    </row>
-    <row r="32" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <f t="shared" si="0"/>
         <v>96.65</v>
@@ -14938,14 +14864,12 @@
       <c r="CC32" s="5">
         <v>108.8</v>
       </c>
-      <c r="CD32" s="5"/>
+      <c r="CD32" s="5">
+        <v>101.6</v>
+      </c>
       <c r="CE32" s="5"/>
-      <c r="CF32" s="5"/>
-      <c r="CG32" s="5"/>
-      <c r="CH32" s="5"/>
-      <c r="CI32" s="5"/>
-    </row>
-    <row r="33" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <f t="shared" si="0"/>
         <v>56.75</v>
@@ -15124,14 +15048,12 @@
       <c r="CC33" s="5">
         <v>60.45</v>
       </c>
-      <c r="CD33" s="5"/>
+      <c r="CD33" s="5">
+        <v>58.55</v>
+      </c>
       <c r="CE33" s="5"/>
-      <c r="CF33" s="5"/>
-      <c r="CG33" s="5"/>
-      <c r="CH33" s="5"/>
-      <c r="CI33" s="5"/>
-    </row>
-    <row r="34" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <f t="shared" si="0"/>
         <v>167.9</v>
@@ -15304,25 +15226,23 @@
       <c r="CC34" s="5">
         <v>207.75</v>
       </c>
-      <c r="CD34" s="5"/>
+      <c r="CD34" s="5">
+        <v>218.1</v>
+      </c>
       <c r="CE34" s="5"/>
-      <c r="CF34" s="5"/>
-      <c r="CG34" s="5"/>
-      <c r="CH34" s="5"/>
-      <c r="CI34" s="5"/>
-    </row>
-    <row r="35" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <f t="shared" si="0"/>
         <v>661</v>
       </c>
       <c r="B35" s="12">
         <f t="shared" si="1"/>
-        <v>715.7</v>
+        <v>721</v>
       </c>
       <c r="C35" s="12">
         <f t="shared" ref="C35" si="4">B35-A35</f>
-        <v>54.700000000000045</v>
+        <v>60</v>
       </c>
       <c r="D35" s="45" t="s">
         <v>281</v>
@@ -15480,14 +15400,12 @@
       <c r="CC35" s="5">
         <v>715.7</v>
       </c>
-      <c r="CD35" s="5"/>
+      <c r="CD35" s="5">
+        <v>721</v>
+      </c>
       <c r="CE35" s="5"/>
-      <c r="CF35" s="5"/>
-      <c r="CG35" s="5"/>
-      <c r="CH35" s="5"/>
-      <c r="CI35" s="5"/>
-    </row>
-    <row r="36" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <f t="shared" si="0"/>
         <v>402.9</v>
@@ -15638,14 +15556,12 @@
       <c r="CC36" s="5">
         <v>419.9</v>
       </c>
-      <c r="CD36" s="5"/>
+      <c r="CD36" s="5">
+        <v>414.5</v>
+      </c>
       <c r="CE36" s="5"/>
-      <c r="CF36" s="5"/>
-      <c r="CG36" s="5"/>
-      <c r="CH36" s="5"/>
-      <c r="CI36" s="5"/>
-    </row>
-    <row r="37" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <f t="shared" si="0"/>
         <v>226</v>
@@ -15786,28 +15702,26 @@
       <c r="CC37" s="5">
         <v>349.9</v>
       </c>
-      <c r="CD37" s="5"/>
+      <c r="CD37" s="5">
+        <v>357.6</v>
+      </c>
       <c r="CE37" s="5"/>
-      <c r="CF37" s="5"/>
-      <c r="CG37" s="5"/>
-      <c r="CH37" s="5"/>
-      <c r="CI37" s="5"/>
-    </row>
-    <row r="38" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <f t="shared" si="0"/>
-        <v>485</v>
+        <v>75.2</v>
       </c>
       <c r="B38" s="12">
         <f t="shared" si="1"/>
-        <v>520</v>
+        <v>83.85</v>
       </c>
       <c r="C38" s="12">
         <f t="shared" ref="C38" si="7">B38-A38</f>
-        <v>35</v>
+        <v>8.6499999999999915</v>
       </c>
       <c r="D38" s="45" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -15863,94 +15777,86 @@
       <c r="BD38" s="5"/>
       <c r="BE38" s="5"/>
       <c r="BF38" s="5"/>
-      <c r="BG38" s="5">
-        <v>515</v>
-      </c>
-      <c r="BH38" s="5">
-        <v>495.25</v>
-      </c>
-      <c r="BI38" s="5">
-        <v>485.45</v>
-      </c>
+      <c r="BG38" s="5"/>
+      <c r="BH38" s="5"/>
+      <c r="BI38" s="5"/>
       <c r="BJ38" s="5">
-        <v>485.3</v>
+        <v>78</v>
       </c>
       <c r="BK38" s="5">
-        <v>489.65</v>
+        <v>77.900000000000006</v>
       </c>
       <c r="BL38" s="5">
-        <v>485</v>
+        <v>77.95</v>
       </c>
       <c r="BM38" s="5">
-        <v>496.6</v>
+        <v>76</v>
       </c>
       <c r="BN38" s="5">
-        <v>494</v>
+        <v>76.849999999999994</v>
       </c>
       <c r="BO38" s="5">
-        <v>500.1</v>
+        <v>78.5</v>
       </c>
       <c r="BP38" s="5">
-        <v>508.6</v>
+        <v>75.2</v>
       </c>
       <c r="BQ38" s="5">
-        <v>515.4</v>
+        <v>75.900000000000006</v>
       </c>
       <c r="BR38" s="5">
-        <v>501.3</v>
+        <v>77.099999999999994</v>
       </c>
       <c r="BS38" s="5">
-        <v>512</v>
+        <v>77.25</v>
       </c>
       <c r="BT38" s="5">
-        <v>514</v>
+        <v>76</v>
       </c>
       <c r="BU38" s="5">
-        <v>505.35</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="BV38" s="5">
-        <v>500</v>
+        <v>76.7</v>
       </c>
       <c r="BW38" s="5">
-        <v>507.55</v>
+        <v>76</v>
       </c>
       <c r="BX38" s="5">
-        <v>512</v>
+        <v>76.650000000000006</v>
       </c>
       <c r="BY38" s="5">
-        <v>506</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="BZ38" s="5">
-        <v>500</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="CA38" s="5">
-        <v>519.95000000000005</v>
+        <v>82</v>
       </c>
       <c r="CB38" s="5">
-        <v>512.85</v>
+        <v>83.85</v>
       </c>
       <c r="CC38" s="5">
-        <v>520</v>
-      </c>
-      <c r="CD38" s="5"/>
+        <v>83.15</v>
+      </c>
+      <c r="CD38" s="5">
+        <v>82</v>
+      </c>
       <c r="CE38" s="5"/>
-      <c r="CF38" s="5"/>
-      <c r="CG38" s="5"/>
-      <c r="CH38" s="5"/>
-      <c r="CI38" s="5"/>
-    </row>
-    <row r="39" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <f t="shared" si="0"/>
-        <v>75.2</v>
+        <v>416</v>
       </c>
       <c r="B39" s="12">
         <f t="shared" si="1"/>
-        <v>83.85</v>
+        <v>472</v>
       </c>
       <c r="C39" s="12">
         <f t="shared" ref="C39" si="8">B39-A39</f>
-        <v>8.6499999999999915</v>
+        <v>56</v>
       </c>
       <c r="D39" s="45" t="s">
         <v>305</v>
@@ -16013,84 +15919,82 @@
       <c r="BH39" s="5"/>
       <c r="BI39" s="5"/>
       <c r="BJ39" s="5">
-        <v>78</v>
+        <v>465.55</v>
       </c>
       <c r="BK39" s="5">
-        <v>77.900000000000006</v>
+        <v>461</v>
       </c>
       <c r="BL39" s="5">
-        <v>77.95</v>
+        <v>469.15</v>
       </c>
       <c r="BM39" s="5">
-        <v>76</v>
+        <v>466</v>
       </c>
       <c r="BN39" s="5">
-        <v>76.849999999999994</v>
+        <v>472</v>
       </c>
       <c r="BO39" s="5">
-        <v>78.5</v>
+        <v>467</v>
       </c>
       <c r="BP39" s="5">
-        <v>75.2</v>
+        <v>450.55</v>
       </c>
       <c r="BQ39" s="5">
-        <v>75.900000000000006</v>
+        <v>444.05</v>
       </c>
       <c r="BR39" s="5">
-        <v>77.099999999999994</v>
+        <v>428</v>
       </c>
       <c r="BS39" s="5">
-        <v>77.25</v>
+        <v>427</v>
       </c>
       <c r="BT39" s="5">
-        <v>76</v>
+        <v>417.75</v>
       </c>
       <c r="BU39" s="5">
-        <v>76.400000000000006</v>
+        <v>424.9</v>
       </c>
       <c r="BV39" s="5">
-        <v>76.7</v>
+        <v>425</v>
       </c>
       <c r="BW39" s="5">
-        <v>76</v>
+        <v>426.1</v>
       </c>
       <c r="BX39" s="5">
-        <v>76.650000000000006</v>
+        <v>416</v>
       </c>
       <c r="BY39" s="5">
-        <v>76.599999999999994</v>
+        <v>417</v>
       </c>
       <c r="BZ39" s="5">
-        <v>76.599999999999994</v>
+        <v>416.8</v>
       </c>
       <c r="CA39" s="5">
-        <v>82</v>
+        <v>429.15</v>
       </c>
       <c r="CB39" s="5">
-        <v>83.85</v>
+        <v>430.75</v>
       </c>
       <c r="CC39" s="5">
-        <v>83.15</v>
-      </c>
-      <c r="CD39" s="5"/>
+        <v>422.1</v>
+      </c>
+      <c r="CD39" s="5">
+        <v>418.2</v>
+      </c>
       <c r="CE39" s="5"/>
-      <c r="CF39" s="5"/>
-      <c r="CG39" s="5"/>
-      <c r="CH39" s="5"/>
-      <c r="CI39" s="5"/>
-    </row>
-    <row r="40" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <f t="shared" si="0"/>
-        <v>416</v>
+        <v>175.2</v>
       </c>
       <c r="B40" s="12">
         <f t="shared" si="1"/>
-        <v>472</v>
+        <v>215.25</v>
       </c>
       <c r="C40" s="12">
         <f t="shared" ref="C40" si="9">B40-A40</f>
-        <v>56</v>
+        <v>40.050000000000011</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>306</v>
@@ -16152,85 +16056,79 @@
       <c r="BG40" s="5"/>
       <c r="BH40" s="5"/>
       <c r="BI40" s="5"/>
-      <c r="BJ40" s="5">
-        <v>465.55</v>
-      </c>
-      <c r="BK40" s="5">
-        <v>461</v>
-      </c>
+      <c r="BJ40" s="5"/>
+      <c r="BK40" s="5"/>
       <c r="BL40" s="5">
-        <v>469.15</v>
+        <v>208</v>
       </c>
       <c r="BM40" s="5">
-        <v>466</v>
+        <v>209.8</v>
       </c>
       <c r="BN40" s="5">
-        <v>472</v>
+        <v>203.65</v>
       </c>
       <c r="BO40" s="5">
-        <v>467</v>
+        <v>201.7</v>
       </c>
       <c r="BP40" s="5">
-        <v>450.55</v>
+        <v>192.65</v>
       </c>
       <c r="BQ40" s="5">
-        <v>444.05</v>
+        <v>196.9</v>
       </c>
       <c r="BR40" s="5">
-        <v>428</v>
+        <v>204.8</v>
       </c>
       <c r="BS40" s="5">
-        <v>427</v>
+        <v>215.25</v>
       </c>
       <c r="BT40" s="5">
-        <v>417.75</v>
+        <v>208.5</v>
       </c>
       <c r="BU40" s="5">
-        <v>424.9</v>
+        <v>198.3</v>
       </c>
       <c r="BV40" s="5">
-        <v>425</v>
+        <v>206</v>
       </c>
       <c r="BW40" s="5">
-        <v>426.1</v>
+        <v>211.6</v>
       </c>
       <c r="BX40" s="5">
-        <v>416</v>
+        <v>210.3</v>
       </c>
       <c r="BY40" s="5">
-        <v>417</v>
+        <v>204.5</v>
       </c>
       <c r="BZ40" s="5">
-        <v>416.8</v>
+        <v>208</v>
       </c>
       <c r="CA40" s="5">
-        <v>429.15</v>
+        <v>201</v>
       </c>
       <c r="CB40" s="5">
-        <v>430.75</v>
+        <v>201.4</v>
       </c>
       <c r="CC40" s="5">
-        <v>422.1</v>
-      </c>
-      <c r="CD40" s="5"/>
+        <v>191</v>
+      </c>
+      <c r="CD40" s="5">
+        <v>175.2</v>
+      </c>
       <c r="CE40" s="5"/>
-      <c r="CF40" s="5"/>
-      <c r="CG40" s="5"/>
-      <c r="CH40" s="5"/>
-      <c r="CI40" s="5"/>
-    </row>
-    <row r="41" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <f t="shared" si="0"/>
-        <v>191</v>
+        <v>35</v>
       </c>
       <c r="B41" s="12">
         <f t="shared" si="1"/>
-        <v>215.25</v>
+        <v>39.450000000000003</v>
       </c>
       <c r="C41" s="12">
-        <f t="shared" ref="C41" si="10">B41-A41</f>
-        <v>24.25</v>
+        <f t="shared" ref="C41:C44" si="10">B41-A41</f>
+        <v>4.4500000000000028</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>307</v>
@@ -16294,79 +16192,73 @@
       <c r="BI41" s="5"/>
       <c r="BJ41" s="5"/>
       <c r="BK41" s="5"/>
-      <c r="BL41" s="5">
-        <v>208</v>
-      </c>
-      <c r="BM41" s="5">
-        <v>209.8</v>
-      </c>
+      <c r="BL41" s="5"/>
+      <c r="BM41" s="5"/>
       <c r="BN41" s="5">
-        <v>203.65</v>
+        <v>38.1</v>
       </c>
       <c r="BO41" s="5">
-        <v>201.7</v>
+        <v>36.950000000000003</v>
       </c>
       <c r="BP41" s="5">
-        <v>192.65</v>
+        <v>38.65</v>
       </c>
       <c r="BQ41" s="5">
-        <v>196.9</v>
+        <v>38.35</v>
       </c>
       <c r="BR41" s="5">
-        <v>204.8</v>
+        <v>38.450000000000003</v>
       </c>
       <c r="BS41" s="5">
-        <v>215.25</v>
+        <v>36.4</v>
       </c>
       <c r="BT41" s="5">
-        <v>208.5</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="BU41" s="5">
-        <v>198.3</v>
+        <v>35</v>
       </c>
       <c r="BV41" s="5">
-        <v>206</v>
+        <v>36</v>
       </c>
       <c r="BW41" s="5">
-        <v>211.6</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="BX41" s="5">
-        <v>210.3</v>
+        <v>37.65</v>
       </c>
       <c r="BY41" s="5">
-        <v>204.5</v>
+        <v>37.65</v>
       </c>
       <c r="BZ41" s="5">
-        <v>208</v>
+        <v>37.15</v>
       </c>
       <c r="CA41" s="5">
-        <v>201</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="CB41" s="5">
-        <v>201.4</v>
+        <v>37</v>
       </c>
       <c r="CC41" s="5">
-        <v>191</v>
-      </c>
-      <c r="CD41" s="5"/>
+        <v>39.450000000000003</v>
+      </c>
+      <c r="CD41" s="5">
+        <v>38.15</v>
+      </c>
       <c r="CE41" s="5"/>
-      <c r="CF41" s="5"/>
-      <c r="CG41" s="5"/>
-      <c r="CH41" s="5"/>
-      <c r="CI41" s="5"/>
-    </row>
-    <row r="42" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>552.04999999999995</v>
       </c>
       <c r="B42" s="12">
         <f t="shared" si="1"/>
-        <v>39.450000000000003</v>
+        <v>626.70000000000005</v>
       </c>
       <c r="C42" s="12">
-        <f t="shared" ref="C42:C45" si="11">B42-A42</f>
-        <v>4.4500000000000028</v>
+        <f t="shared" si="10"/>
+        <v>74.650000000000091</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>308</v>
@@ -16432,73 +16324,69 @@
       <c r="BK42" s="5"/>
       <c r="BL42" s="5"/>
       <c r="BM42" s="5"/>
-      <c r="BN42" s="5">
-        <v>38.1</v>
-      </c>
+      <c r="BN42" s="5"/>
       <c r="BO42" s="5">
-        <v>36.950000000000003</v>
+        <v>585</v>
       </c>
       <c r="BP42" s="5">
-        <v>38.65</v>
+        <v>577.45000000000005</v>
       </c>
       <c r="BQ42" s="5">
-        <v>38.35</v>
+        <v>597.20000000000005</v>
       </c>
       <c r="BR42" s="5">
-        <v>38.450000000000003</v>
+        <v>584</v>
       </c>
       <c r="BS42" s="5">
-        <v>36.4</v>
+        <v>616.15</v>
       </c>
       <c r="BT42" s="5">
-        <v>35.299999999999997</v>
+        <v>619</v>
       </c>
       <c r="BU42" s="5">
-        <v>35</v>
+        <v>610</v>
       </c>
       <c r="BV42" s="5">
-        <v>36</v>
+        <v>626.70000000000005</v>
       </c>
       <c r="BW42" s="5">
-        <v>37.200000000000003</v>
+        <v>607.29999999999995</v>
       </c>
       <c r="BX42" s="5">
-        <v>37.65</v>
+        <v>580.04999999999995</v>
       </c>
       <c r="BY42" s="5">
-        <v>37.65</v>
+        <v>552.04999999999995</v>
       </c>
       <c r="BZ42" s="5">
-        <v>37.15</v>
+        <v>580.1</v>
       </c>
       <c r="CA42" s="5">
-        <v>37.200000000000003</v>
+        <v>581.45000000000005</v>
       </c>
       <c r="CB42" s="5">
-        <v>37</v>
+        <v>578.15</v>
       </c>
       <c r="CC42" s="5">
-        <v>39.450000000000003</v>
-      </c>
-      <c r="CD42" s="5"/>
+        <v>607.15</v>
+      </c>
+      <c r="CD42" s="5">
+        <v>590</v>
+      </c>
       <c r="CE42" s="5"/>
-      <c r="CF42" s="5"/>
-      <c r="CG42" s="5"/>
-      <c r="CH42" s="5"/>
-      <c r="CI42" s="5"/>
-    </row>
-    <row r="43" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <f t="shared" si="0"/>
-        <v>552.04999999999995</v>
+        <v>814.2</v>
       </c>
       <c r="B43" s="12">
         <f t="shared" si="1"/>
-        <v>626.70000000000005</v>
+        <v>856</v>
       </c>
       <c r="C43" s="12">
-        <f t="shared" si="11"/>
-        <v>74.650000000000091</v>
+        <f t="shared" si="10"/>
+        <v>41.799999999999955</v>
       </c>
       <c r="D43" s="45" t="s">
         <v>309</v>
@@ -16566,69 +16454,67 @@
       <c r="BM43" s="5"/>
       <c r="BN43" s="5"/>
       <c r="BO43" s="5">
-        <v>585</v>
+        <v>856</v>
       </c>
       <c r="BP43" s="5">
-        <v>577.45000000000005</v>
+        <v>832.8</v>
       </c>
       <c r="BQ43" s="5">
-        <v>597.20000000000005</v>
+        <v>830.25</v>
       </c>
       <c r="BR43" s="5">
-        <v>584</v>
+        <v>832.95</v>
       </c>
       <c r="BS43" s="5">
-        <v>616.15</v>
+        <v>826</v>
       </c>
       <c r="BT43" s="5">
-        <v>619</v>
+        <v>835</v>
       </c>
       <c r="BU43" s="5">
-        <v>610</v>
+        <v>822.95</v>
       </c>
       <c r="BV43" s="5">
-        <v>626.70000000000005</v>
+        <v>828.55</v>
       </c>
       <c r="BW43" s="5">
-        <v>607.29999999999995</v>
+        <v>831.85</v>
       </c>
       <c r="BX43" s="5">
-        <v>580.04999999999995</v>
+        <v>826</v>
       </c>
       <c r="BY43" s="5">
-        <v>552.04999999999995</v>
+        <v>837.25</v>
       </c>
       <c r="BZ43" s="5">
-        <v>580.1</v>
+        <v>828.3</v>
       </c>
       <c r="CA43" s="5">
-        <v>581.45000000000005</v>
+        <v>829.4</v>
       </c>
       <c r="CB43" s="5">
-        <v>578.15</v>
+        <v>832.05</v>
       </c>
       <c r="CC43" s="5">
-        <v>607.15</v>
-      </c>
-      <c r="CD43" s="5"/>
+        <v>836.65</v>
+      </c>
+      <c r="CD43" s="5">
+        <v>814.2</v>
+      </c>
       <c r="CE43" s="5"/>
-      <c r="CF43" s="5"/>
-      <c r="CG43" s="5"/>
-      <c r="CH43" s="5"/>
-      <c r="CI43" s="5"/>
-    </row>
-    <row r="44" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <f t="shared" si="0"/>
-        <v>822.95</v>
+        <v>134.9</v>
       </c>
       <c r="B44" s="12">
         <f t="shared" si="1"/>
-        <v>856</v>
+        <v>146</v>
       </c>
       <c r="C44" s="12">
-        <f t="shared" si="11"/>
-        <v>33.049999999999955</v>
+        <f t="shared" si="10"/>
+        <v>11.099999999999994</v>
       </c>
       <c r="D44" s="45" t="s">
         <v>310</v>
@@ -16695,73 +16581,69 @@
       <c r="BL44" s="5"/>
       <c r="BM44" s="5"/>
       <c r="BN44" s="5"/>
-      <c r="BO44" s="5">
-        <v>856</v>
-      </c>
+      <c r="BO44" s="5"/>
       <c r="BP44" s="5">
-        <v>832.8</v>
+        <v>146</v>
       </c>
       <c r="BQ44" s="5">
-        <v>830.25</v>
+        <v>141.80000000000001</v>
       </c>
       <c r="BR44" s="5">
-        <v>832.95</v>
+        <v>140.30000000000001</v>
       </c>
       <c r="BS44" s="5">
-        <v>826</v>
+        <v>137.9</v>
       </c>
       <c r="BT44" s="5">
-        <v>835</v>
+        <v>140.25</v>
       </c>
       <c r="BU44" s="5">
-        <v>822.95</v>
+        <v>134.9</v>
       </c>
       <c r="BV44" s="5">
-        <v>828.55</v>
+        <v>137</v>
       </c>
       <c r="BW44" s="5">
-        <v>831.85</v>
+        <v>137.75</v>
       </c>
       <c r="BX44" s="5">
-        <v>826</v>
+        <v>138.25</v>
       </c>
       <c r="BY44" s="5">
-        <v>837.25</v>
+        <v>139.35</v>
       </c>
       <c r="BZ44" s="5">
-        <v>828.3</v>
+        <v>138.19999999999999</v>
       </c>
       <c r="CA44" s="5">
-        <v>829.4</v>
+        <v>142.9</v>
       </c>
       <c r="CB44" s="5">
-        <v>832.05</v>
+        <v>143.65</v>
       </c>
       <c r="CC44" s="5">
-        <v>836.65</v>
-      </c>
-      <c r="CD44" s="5"/>
+        <v>145.1</v>
+      </c>
+      <c r="CD44" s="5">
+        <v>138.69999999999999</v>
+      </c>
       <c r="CE44" s="5"/>
-      <c r="CF44" s="5"/>
-      <c r="CG44" s="5"/>
-      <c r="CH44" s="5"/>
-      <c r="CI44" s="5"/>
-    </row>
-    <row r="45" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <f t="shared" si="0"/>
-        <v>134.9</v>
+        <v>623</v>
       </c>
       <c r="B45" s="12">
         <f t="shared" si="1"/>
-        <v>146</v>
+        <v>770</v>
       </c>
       <c r="C45" s="12">
-        <f t="shared" si="11"/>
-        <v>11.099999999999994</v>
+        <f t="shared" ref="C45" si="11">B45-A45</f>
+        <v>147</v>
       </c>
       <c r="D45" s="45" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -16826,70 +16708,62 @@
       <c r="BM45" s="5"/>
       <c r="BN45" s="5"/>
       <c r="BO45" s="5"/>
-      <c r="BP45" s="5">
-        <v>146</v>
-      </c>
-      <c r="BQ45" s="5">
-        <v>141.80000000000001</v>
-      </c>
-      <c r="BR45" s="5">
-        <v>140.30000000000001</v>
-      </c>
+      <c r="BP45" s="5"/>
+      <c r="BQ45" s="5"/>
+      <c r="BR45" s="5"/>
       <c r="BS45" s="5">
-        <v>137.9</v>
+        <v>770</v>
       </c>
       <c r="BT45" s="5">
-        <v>140.25</v>
+        <v>696</v>
       </c>
       <c r="BU45" s="5">
-        <v>134.9</v>
+        <v>680.25</v>
       </c>
       <c r="BV45" s="5">
-        <v>137</v>
+        <v>679.8</v>
       </c>
       <c r="BW45" s="5">
-        <v>137.75</v>
+        <v>679</v>
       </c>
       <c r="BX45" s="5">
-        <v>138.25</v>
+        <v>668</v>
       </c>
       <c r="BY45" s="5">
-        <v>139.35</v>
+        <v>667.5</v>
       </c>
       <c r="BZ45" s="5">
-        <v>138.19999999999999</v>
+        <v>663.95</v>
       </c>
       <c r="CA45" s="5">
-        <v>142.9</v>
+        <v>648.4</v>
       </c>
       <c r="CB45" s="5">
-        <v>143.65</v>
+        <v>648.4</v>
       </c>
       <c r="CC45" s="5">
-        <v>145.1</v>
-      </c>
-      <c r="CD45" s="5"/>
+        <v>639.79999999999995</v>
+      </c>
+      <c r="CD45" s="5">
+        <v>623</v>
+      </c>
       <c r="CE45" s="5"/>
-      <c r="CF45" s="5"/>
-      <c r="CG45" s="5"/>
-      <c r="CH45" s="5"/>
-      <c r="CI45" s="5"/>
-    </row>
-    <row r="46" spans="1:87" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <f t="shared" si="0"/>
-        <v>639.79999999999995</v>
+        <v>107.9</v>
       </c>
       <c r="B46" s="12">
         <f t="shared" si="1"/>
-        <v>770</v>
+        <v>110.95</v>
       </c>
       <c r="C46" s="12">
         <f t="shared" ref="C46" si="12">B46-A46</f>
-        <v>130.20000000000005</v>
+        <v>3.0499999999999972</v>
       </c>
       <c r="D46" s="45" t="s">
-        <v>313</v>
+        <v>325</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -16957,281 +16831,35 @@
       <c r="BP46" s="5"/>
       <c r="BQ46" s="5"/>
       <c r="BR46" s="5"/>
-      <c r="BS46" s="5">
-        <v>770</v>
-      </c>
-      <c r="BT46" s="5">
-        <v>696</v>
-      </c>
-      <c r="BU46" s="5">
-        <v>680.25</v>
-      </c>
-      <c r="BV46" s="5">
-        <v>679.8</v>
-      </c>
+      <c r="BS46" s="5"/>
+      <c r="BT46" s="5"/>
+      <c r="BU46" s="5"/>
+      <c r="BV46" s="5"/>
       <c r="BW46" s="5">
-        <v>679</v>
+        <v>109</v>
       </c>
       <c r="BX46" s="5">
-        <v>668</v>
+        <v>110.95</v>
       </c>
       <c r="BY46" s="5">
-        <v>667.5</v>
+        <v>110.7</v>
       </c>
       <c r="BZ46" s="5">
-        <v>663.95</v>
+        <v>109.5</v>
       </c>
       <c r="CA46" s="5">
-        <v>648.4</v>
+        <v>109.85</v>
       </c>
       <c r="CB46" s="5">
-        <v>648.4</v>
+        <v>109.9</v>
       </c>
       <c r="CC46" s="5">
-        <v>639.79999999999995</v>
-      </c>
-      <c r="CD46" s="5"/>
+        <v>107.9</v>
+      </c>
+      <c r="CD46" s="5">
+        <v>107.95</v>
+      </c>
       <c r="CE46" s="5"/>
-      <c r="CF46" s="5"/>
-      <c r="CG46" s="5"/>
-      <c r="CH46" s="5"/>
-      <c r="CI46" s="5"/>
-    </row>
-    <row r="47" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A47" s="12">
-        <f t="shared" si="0"/>
-        <v>776.5</v>
-      </c>
-      <c r="B47" s="12">
-        <f t="shared" si="1"/>
-        <v>868.95</v>
-      </c>
-      <c r="C47" s="12">
-        <f t="shared" ref="C47" si="13">B47-A47</f>
-        <v>92.450000000000045</v>
-      </c>
-      <c r="D47" s="45" t="s">
-        <v>327</v>
-      </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="5"/>
-      <c r="U47" s="5"/>
-      <c r="V47" s="5"/>
-      <c r="W47" s="5"/>
-      <c r="X47" s="5"/>
-      <c r="Y47" s="5"/>
-      <c r="Z47" s="5"/>
-      <c r="AA47" s="5"/>
-      <c r="AB47" s="5"/>
-      <c r="AC47" s="5"/>
-      <c r="AD47" s="5"/>
-      <c r="AE47" s="5"/>
-      <c r="AF47" s="5"/>
-      <c r="AG47" s="5"/>
-      <c r="AH47" s="5"/>
-      <c r="AI47" s="5"/>
-      <c r="AJ47" s="5"/>
-      <c r="AK47" s="5"/>
-      <c r="AL47" s="5"/>
-      <c r="AM47" s="5"/>
-      <c r="AN47" s="5"/>
-      <c r="AO47" s="5"/>
-      <c r="AP47" s="5"/>
-      <c r="AQ47" s="5"/>
-      <c r="AR47" s="5"/>
-      <c r="AS47" s="5"/>
-      <c r="AT47" s="5"/>
-      <c r="AU47" s="5"/>
-      <c r="AV47" s="5"/>
-      <c r="AW47" s="5"/>
-      <c r="AX47" s="5"/>
-      <c r="AY47" s="5"/>
-      <c r="AZ47" s="5"/>
-      <c r="BA47" s="5"/>
-      <c r="BB47" s="5"/>
-      <c r="BC47" s="5"/>
-      <c r="BD47" s="5"/>
-      <c r="BE47" s="5"/>
-      <c r="BF47" s="5"/>
-      <c r="BG47" s="5"/>
-      <c r="BH47" s="5"/>
-      <c r="BI47" s="5"/>
-      <c r="BJ47" s="5"/>
-      <c r="BK47" s="5"/>
-      <c r="BL47" s="5"/>
-      <c r="BM47" s="5"/>
-      <c r="BN47" s="5"/>
-      <c r="BO47" s="5"/>
-      <c r="BP47" s="5"/>
-      <c r="BQ47" s="5"/>
-      <c r="BR47" s="5"/>
-      <c r="BS47" s="5">
-        <v>790</v>
-      </c>
-      <c r="BT47" s="5">
-        <v>783.15</v>
-      </c>
-      <c r="BU47" s="5">
-        <v>776.5</v>
-      </c>
-      <c r="BV47" s="5">
-        <v>785</v>
-      </c>
-      <c r="BW47" s="5">
-        <v>786</v>
-      </c>
-      <c r="BX47" s="5">
-        <v>811.4</v>
-      </c>
-      <c r="BY47" s="5">
-        <v>859.9</v>
-      </c>
-      <c r="BZ47" s="5">
-        <v>852</v>
-      </c>
-      <c r="CA47" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="CB47" s="5">
-        <v>842.5</v>
-      </c>
-      <c r="CC47" s="5">
-        <v>868.95</v>
-      </c>
-      <c r="CD47" s="5"/>
-      <c r="CE47" s="5"/>
-      <c r="CF47" s="5"/>
-      <c r="CG47" s="5"/>
-      <c r="CH47" s="5"/>
-      <c r="CI47" s="5"/>
-    </row>
-    <row r="48" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A48" s="12">
-        <f t="shared" si="0"/>
-        <v>107.9</v>
-      </c>
-      <c r="B48" s="12">
-        <f t="shared" si="1"/>
-        <v>110.95</v>
-      </c>
-      <c r="C48" s="12">
-        <f t="shared" ref="C48" si="14">B48-A48</f>
-        <v>3.0499999999999972</v>
-      </c>
-      <c r="D48" s="45" t="s">
-        <v>328</v>
-      </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5"/>
-      <c r="M48" s="5"/>
-      <c r="N48" s="5"/>
-      <c r="O48" s="5"/>
-      <c r="P48" s="5"/>
-      <c r="Q48" s="5"/>
-      <c r="R48" s="5"/>
-      <c r="S48" s="5"/>
-      <c r="T48" s="5"/>
-      <c r="U48" s="5"/>
-      <c r="V48" s="5"/>
-      <c r="W48" s="5"/>
-      <c r="X48" s="5"/>
-      <c r="Y48" s="5"/>
-      <c r="Z48" s="5"/>
-      <c r="AA48" s="5"/>
-      <c r="AB48" s="5"/>
-      <c r="AC48" s="5"/>
-      <c r="AD48" s="5"/>
-      <c r="AE48" s="5"/>
-      <c r="AF48" s="5"/>
-      <c r="AG48" s="5"/>
-      <c r="AH48" s="5"/>
-      <c r="AI48" s="5"/>
-      <c r="AJ48" s="5"/>
-      <c r="AK48" s="5"/>
-      <c r="AL48" s="5"/>
-      <c r="AM48" s="5"/>
-      <c r="AN48" s="5"/>
-      <c r="AO48" s="5"/>
-      <c r="AP48" s="5"/>
-      <c r="AQ48" s="5"/>
-      <c r="AR48" s="5"/>
-      <c r="AS48" s="5"/>
-      <c r="AT48" s="5"/>
-      <c r="AU48" s="5"/>
-      <c r="AV48" s="5"/>
-      <c r="AW48" s="5"/>
-      <c r="AX48" s="5"/>
-      <c r="AY48" s="5"/>
-      <c r="AZ48" s="5"/>
-      <c r="BA48" s="5"/>
-      <c r="BB48" s="5"/>
-      <c r="BC48" s="5"/>
-      <c r="BD48" s="5"/>
-      <c r="BE48" s="5"/>
-      <c r="BF48" s="5"/>
-      <c r="BG48" s="5"/>
-      <c r="BH48" s="5"/>
-      <c r="BI48" s="5"/>
-      <c r="BJ48" s="5"/>
-      <c r="BK48" s="5"/>
-      <c r="BL48" s="5"/>
-      <c r="BM48" s="5"/>
-      <c r="BN48" s="5"/>
-      <c r="BO48" s="5"/>
-      <c r="BP48" s="5"/>
-      <c r="BQ48" s="5"/>
-      <c r="BR48" s="5"/>
-      <c r="BS48" s="5"/>
-      <c r="BT48" s="5"/>
-      <c r="BU48" s="5"/>
-      <c r="BV48" s="5"/>
-      <c r="BW48" s="5">
-        <v>109</v>
-      </c>
-      <c r="BX48" s="5">
-        <v>110.95</v>
-      </c>
-      <c r="BY48" s="5">
-        <v>110.7</v>
-      </c>
-      <c r="BZ48" s="5">
-        <v>109.5</v>
-      </c>
-      <c r="CA48" s="5">
-        <v>109.85</v>
-      </c>
-      <c r="CB48" s="5">
-        <v>109.9</v>
-      </c>
-      <c r="CC48" s="5">
-        <v>107.9</v>
-      </c>
-      <c r="CD48" s="5"/>
-      <c r="CE48" s="5"/>
-      <c r="CF48" s="5"/>
-      <c r="CG48" s="5"/>
-      <c r="CH48" s="5"/>
-      <c r="CI48" s="5"/>
     </row>
   </sheetData>
   <sortState ref="L1:L37">
@@ -19041,7 +18669,7 @@
         <v>43017</v>
       </c>
       <c r="I36" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J36" s="26">
         <v>13790</v>
@@ -19126,7 +18754,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B43" s="12">
         <v>13790</v>
@@ -19137,7 +18765,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="39" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B44" s="12">
         <v>15000</v>

</xml_diff>

<commit_message>
Added details for 04/12/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13530" windowHeight="8175" firstSheet="3" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13530" windowHeight="8175" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="PaidTillDate" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="325">
   <si>
     <t>Date</t>
   </si>
@@ -870,9 +870,6 @@
     <t>BOMDYEING</t>
   </si>
   <si>
-    <t>ICICIGI</t>
-  </si>
-  <si>
     <t>Wires</t>
   </si>
   <si>
@@ -999,10 +996,10 @@
     <t>28/11/2026</t>
   </si>
   <si>
-    <t>30/11/2028</t>
-  </si>
-  <si>
     <t>MEGH</t>
+  </si>
+  <si>
+    <t>GPPL</t>
   </si>
 </sst>
 </file>
@@ -7248,11 +7245,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CE46"/>
+  <dimension ref="A1:CI46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="CA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CD2" sqref="CD2:CD46"/>
+      <selection pane="topRight" activeCell="CE50" sqref="CE50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7303,10 +7300,12 @@
     <col min="79" max="79" width="14.42578125" customWidth="1"/>
     <col min="80" max="81" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="82" max="82" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="13" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="13" customWidth="1"/>
+    <col min="85" max="87" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:87" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>249</v>
       </c>
@@ -7479,25 +7478,25 @@
         <v>279</v>
       </c>
       <c r="BF1" s="51" t="s">
+        <v>294</v>
+      </c>
+      <c r="BG1" s="51" t="s">
         <v>295</v>
       </c>
-      <c r="BG1" s="51" t="s">
-        <v>296</v>
-      </c>
       <c r="BH1" s="51" t="s">
+        <v>297</v>
+      </c>
+      <c r="BI1" s="51" t="s">
         <v>298</v>
       </c>
-      <c r="BI1" s="51" t="s">
+      <c r="BJ1" s="51" t="s">
         <v>299</v>
       </c>
-      <c r="BJ1" s="51" t="s">
+      <c r="BK1" s="51" t="s">
         <v>300</v>
       </c>
-      <c r="BK1" s="51" t="s">
+      <c r="BL1" s="51" t="s">
         <v>301</v>
-      </c>
-      <c r="BL1" s="51" t="s">
-        <v>302</v>
       </c>
       <c r="BM1" s="51">
         <v>42777</v>
@@ -7518,52 +7517,64 @@
         <v>43019</v>
       </c>
       <c r="BS1" s="49" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="BT1" s="49" t="s">
+        <v>313</v>
+      </c>
+      <c r="BU1" s="49" t="s">
         <v>314</v>
       </c>
-      <c r="BU1" s="49" t="s">
+      <c r="BV1" s="49" t="s">
         <v>315</v>
       </c>
-      <c r="BV1" s="49" t="s">
+      <c r="BW1" s="49" t="s">
         <v>316</v>
       </c>
-      <c r="BW1" s="49" t="s">
+      <c r="BX1" s="49" t="s">
         <v>317</v>
       </c>
-      <c r="BX1" s="49" t="s">
+      <c r="BY1" s="49" t="s">
         <v>318</v>
       </c>
-      <c r="BY1" s="49" t="s">
+      <c r="BZ1" s="49" t="s">
         <v>319</v>
       </c>
-      <c r="BZ1" s="49" t="s">
+      <c r="CA1" s="49" t="s">
         <v>320</v>
       </c>
-      <c r="CA1" s="49" t="s">
+      <c r="CB1" s="49" t="s">
         <v>321</v>
       </c>
-      <c r="CB1" s="49" t="s">
+      <c r="CC1" s="49" t="s">
         <v>322</v>
       </c>
-      <c r="CC1" s="49" t="s">
-        <v>323</v>
-      </c>
       <c r="CD1" s="51">
-        <v>43112</v>
-      </c>
-      <c r="CE1" s="49" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
+        <v>42747</v>
+      </c>
+      <c r="CE1" s="51">
+        <v>42837</v>
+      </c>
+      <c r="CF1" s="51">
+        <v>42867</v>
+      </c>
+      <c r="CG1" s="51">
+        <v>42898</v>
+      </c>
+      <c r="CH1" s="51">
+        <v>42928</v>
+      </c>
+      <c r="CI1" s="51">
+        <v>42959</v>
+      </c>
+    </row>
+    <row r="2" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
-        <f t="shared" ref="A2:A46" si="0">MIN(E2:ZR2)</f>
+        <f t="shared" ref="A2:A45" si="0">MIN(E2:ZR2)</f>
         <v>243.6</v>
       </c>
       <c r="B2" s="12">
-        <f t="shared" ref="B2:B46" si="1">MAX(E2:ZR2)</f>
+        <f t="shared" ref="B2:B45" si="1">MAX(E2:ZR2)</f>
         <v>340.8</v>
       </c>
       <c r="C2" s="12">
@@ -7799,9 +7810,15 @@
       <c r="CD2" s="5">
         <v>316.95</v>
       </c>
-      <c r="CE2" s="5"/>
-    </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE2" s="5">
+        <v>314.25</v>
+      </c>
+      <c r="CF2" s="5"/>
+      <c r="CG2" s="5"/>
+      <c r="CH2" s="5"/>
+      <c r="CI2" s="5"/>
+    </row>
+    <row r="3" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <f t="shared" si="0"/>
         <v>262.7</v>
@@ -8043,9 +8060,15 @@
       <c r="CD3" s="5">
         <v>306.2</v>
       </c>
-      <c r="CE3" s="5"/>
-    </row>
-    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE3" s="5">
+        <v>305.39999999999998</v>
+      </c>
+      <c r="CF3" s="5"/>
+      <c r="CG3" s="5"/>
+      <c r="CH3" s="5"/>
+      <c r="CI3" s="5"/>
+    </row>
+    <row r="4" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
         <v>253.85</v>
@@ -8293,9 +8316,15 @@
       <c r="CD4" s="5">
         <v>256.45</v>
       </c>
-      <c r="CE4" s="5"/>
-    </row>
-    <row r="5" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE4" s="5">
+        <v>254.75</v>
+      </c>
+      <c r="CF4" s="5"/>
+      <c r="CG4" s="5"/>
+      <c r="CH4" s="5"/>
+      <c r="CI4" s="5"/>
+    </row>
+    <row r="5" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <f t="shared" si="0"/>
         <v>786.25</v>
@@ -8543,9 +8572,15 @@
       <c r="CD5" s="5">
         <v>913.5</v>
       </c>
-      <c r="CE5" s="5"/>
-    </row>
-    <row r="6" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE5" s="5">
+        <v>902.6</v>
+      </c>
+      <c r="CF5" s="5"/>
+      <c r="CG5" s="5"/>
+      <c r="CH5" s="5"/>
+      <c r="CI5" s="5"/>
+    </row>
+    <row r="6" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <f t="shared" si="0"/>
         <v>236.45</v>
@@ -8793,9 +8828,15 @@
       <c r="CD6" s="5">
         <v>271.39999999999998</v>
       </c>
-      <c r="CE6" s="5"/>
-    </row>
-    <row r="7" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE6" s="5">
+        <v>265.89999999999998</v>
+      </c>
+      <c r="CF6" s="5"/>
+      <c r="CG6" s="5"/>
+      <c r="CH6" s="5"/>
+      <c r="CI6" s="5"/>
+    </row>
+    <row r="7" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <f t="shared" si="0"/>
         <v>15.6</v>
@@ -9043,9 +9084,15 @@
       <c r="CD7" s="5">
         <v>17.899999999999999</v>
       </c>
-      <c r="CE7" s="5"/>
-    </row>
-    <row r="8" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE7" s="5">
+        <v>17.3</v>
+      </c>
+      <c r="CF7" s="5"/>
+      <c r="CG7" s="5"/>
+      <c r="CH7" s="5"/>
+      <c r="CI7" s="5"/>
+    </row>
+    <row r="8" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <f t="shared" si="0"/>
         <v>53.4</v>
@@ -9293,9 +9340,15 @@
       <c r="CD8" s="5">
         <v>79.45</v>
       </c>
-      <c r="CE8" s="5"/>
-    </row>
-    <row r="9" spans="1:83" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="CE8" s="5">
+        <v>78.3</v>
+      </c>
+      <c r="CF8" s="5"/>
+      <c r="CG8" s="5"/>
+      <c r="CH8" s="5"/>
+      <c r="CI8" s="5"/>
+    </row>
+    <row r="9" spans="1:87" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <f t="shared" si="0"/>
         <v>53.5</v>
@@ -9535,9 +9588,15 @@
       <c r="CD9" s="28">
         <v>54.7</v>
       </c>
-      <c r="CE9" s="28"/>
-    </row>
-    <row r="10" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE9" s="28">
+        <v>54.4</v>
+      </c>
+      <c r="CF9" s="28"/>
+      <c r="CG9" s="28"/>
+      <c r="CH9" s="28"/>
+      <c r="CI9" s="28"/>
+    </row>
+    <row r="10" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <f t="shared" si="0"/>
         <v>35.549999999999997</v>
@@ -9785,9 +9844,15 @@
       <c r="CD10" s="5">
         <v>38.1</v>
       </c>
-      <c r="CE10" s="5"/>
-    </row>
-    <row r="11" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE10" s="5">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="CF10" s="5"/>
+      <c r="CG10" s="5"/>
+      <c r="CH10" s="5"/>
+      <c r="CI10" s="5"/>
+    </row>
+    <row r="11" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <f t="shared" si="0"/>
         <v>72.650000000000006</v>
@@ -10035,9 +10100,15 @@
       <c r="CD11" s="5">
         <v>93.6</v>
       </c>
-      <c r="CE11" s="5"/>
-    </row>
-    <row r="12" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE11" s="5">
+        <v>93.2</v>
+      </c>
+      <c r="CF11" s="5"/>
+      <c r="CG11" s="5"/>
+      <c r="CH11" s="5"/>
+      <c r="CI11" s="5"/>
+    </row>
+    <row r="12" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
         <v>82.65</v>
@@ -10285,9 +10356,15 @@
       <c r="CD12" s="5">
         <v>92.05</v>
       </c>
-      <c r="CE12" s="5"/>
-    </row>
-    <row r="13" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE12" s="5">
+        <v>90.75</v>
+      </c>
+      <c r="CF12" s="5"/>
+      <c r="CG12" s="5"/>
+      <c r="CH12" s="5"/>
+      <c r="CI12" s="5"/>
+    </row>
+    <row r="13" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <f t="shared" si="0"/>
         <v>44.1</v>
@@ -10535,9 +10612,15 @@
       <c r="CD13" s="5">
         <v>54.25</v>
       </c>
-      <c r="CE13" s="5"/>
-    </row>
-    <row r="14" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE13" s="5">
+        <v>54.25</v>
+      </c>
+      <c r="CF13" s="5"/>
+      <c r="CG13" s="5"/>
+      <c r="CH13" s="5"/>
+      <c r="CI13" s="5"/>
+    </row>
+    <row r="14" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <f t="shared" si="0"/>
         <v>29.75</v>
@@ -10785,9 +10868,15 @@
       <c r="CD14" s="5">
         <v>41.9</v>
       </c>
-      <c r="CE14" s="5"/>
-    </row>
-    <row r="15" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE14" s="5">
+        <v>38.950000000000003</v>
+      </c>
+      <c r="CF14" s="5"/>
+      <c r="CG14" s="5"/>
+      <c r="CH14" s="5"/>
+      <c r="CI14" s="5"/>
+    </row>
+    <row r="15" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
         <v>23.95</v>
@@ -11027,9 +11116,15 @@
       <c r="CD15" s="5">
         <v>24.55</v>
       </c>
-      <c r="CE15" s="5"/>
-    </row>
-    <row r="16" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE15" s="5">
+        <v>24.1</v>
+      </c>
+      <c r="CF15" s="5"/>
+      <c r="CG15" s="5"/>
+      <c r="CH15" s="5"/>
+      <c r="CI15" s="5"/>
+    </row>
+    <row r="16" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <f t="shared" si="0"/>
         <v>552</v>
@@ -11277,9 +11372,15 @@
       <c r="CD16" s="5">
         <v>682.55</v>
       </c>
-      <c r="CE16" s="5"/>
-    </row>
-    <row r="17" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE16" s="5">
+        <v>690.2</v>
+      </c>
+      <c r="CF16" s="5"/>
+      <c r="CG16" s="5"/>
+      <c r="CH16" s="5"/>
+      <c r="CI16" s="5"/>
+    </row>
+    <row r="17" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <f t="shared" si="0"/>
         <v>433</v>
@@ -11527,9 +11628,15 @@
       <c r="CD17" s="5">
         <v>477.5</v>
       </c>
-      <c r="CE17" s="5"/>
-    </row>
-    <row r="18" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE17" s="5">
+        <v>474.5</v>
+      </c>
+      <c r="CF17" s="5"/>
+      <c r="CG17" s="5"/>
+      <c r="CH17" s="5"/>
+      <c r="CI17" s="5"/>
+    </row>
+    <row r="18" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <f t="shared" si="0"/>
         <v>178.8</v>
@@ -11777,20 +11884,26 @@
       <c r="CD18" s="5">
         <v>273</v>
       </c>
-      <c r="CE18" s="5"/>
-    </row>
-    <row r="19" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE18" s="5">
+        <v>261.89999999999998</v>
+      </c>
+      <c r="CF18" s="5"/>
+      <c r="CG18" s="5"/>
+      <c r="CH18" s="5"/>
+      <c r="CI18" s="5"/>
+    </row>
+    <row r="19" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <f t="shared" si="0"/>
         <v>440.7</v>
       </c>
       <c r="B19" s="12">
         <f t="shared" si="1"/>
-        <v>719.55</v>
+        <v>740.95</v>
       </c>
       <c r="C19" s="12">
         <f t="shared" si="2"/>
-        <v>278.84999999999997</v>
+        <v>300.25000000000006</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -12027,12 +12140,18 @@
       <c r="CD19" s="5">
         <v>706.5</v>
       </c>
-      <c r="CE19" s="5"/>
-    </row>
-    <row r="20" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE19" s="5">
+        <v>740.95</v>
+      </c>
+      <c r="CF19" s="5"/>
+      <c r="CG19" s="5"/>
+      <c r="CH19" s="5"/>
+      <c r="CI19" s="5"/>
+    </row>
+    <row r="20" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <f t="shared" si="0"/>
-        <v>677</v>
+        <v>674.95</v>
       </c>
       <c r="B20" s="12">
         <f t="shared" si="1"/>
@@ -12040,7 +12159,7 @@
       </c>
       <c r="C20" s="12">
         <f t="shared" si="2"/>
-        <v>118.95000000000005</v>
+        <v>121</v>
       </c>
       <c r="D20" s="44" t="s">
         <v>104</v>
@@ -12277,9 +12396,15 @@
       <c r="CD20" s="5">
         <v>684.6</v>
       </c>
-      <c r="CE20" s="5"/>
-    </row>
-    <row r="21" spans="1:83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CE20" s="5">
+        <v>674.95</v>
+      </c>
+      <c r="CF20" s="5"/>
+      <c r="CG20" s="5"/>
+      <c r="CH20" s="5"/>
+      <c r="CI20" s="5"/>
+    </row>
+    <row r="21" spans="1:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <f t="shared" si="0"/>
         <v>376.7</v>
@@ -12527,9 +12652,15 @@
       <c r="CD21" s="5">
         <v>491.55</v>
       </c>
-      <c r="CE21" s="5"/>
-    </row>
-    <row r="22" spans="1:83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CE21" s="5">
+        <v>485.2</v>
+      </c>
+      <c r="CF21" s="5"/>
+      <c r="CG21" s="5"/>
+      <c r="CH21" s="5"/>
+      <c r="CI21" s="5"/>
+    </row>
+    <row r="22" spans="1:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <f t="shared" si="0"/>
         <v>315.2</v>
@@ -12723,9 +12854,15 @@
       <c r="CD22" s="5">
         <v>384.8</v>
       </c>
-      <c r="CE22" s="5"/>
-    </row>
-    <row r="23" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE22" s="5">
+        <v>379</v>
+      </c>
+      <c r="CF22" s="5"/>
+      <c r="CG22" s="5"/>
+      <c r="CH22" s="5"/>
+      <c r="CI22" s="5"/>
+    </row>
+    <row r="23" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
         <v>54.45</v>
@@ -12965,9 +13102,15 @@
       <c r="CD23" s="5">
         <v>60.95</v>
       </c>
-      <c r="CE23" s="5"/>
-    </row>
-    <row r="24" spans="1:83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CE23" s="5">
+        <v>58.1</v>
+      </c>
+      <c r="CF23" s="5"/>
+      <c r="CG23" s="5"/>
+      <c r="CH23" s="5"/>
+      <c r="CI23" s="5"/>
+    </row>
+    <row r="24" spans="1:87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <f t="shared" si="0"/>
         <v>210.65</v>
@@ -13203,9 +13346,15 @@
       <c r="CD24" s="5">
         <v>231.25</v>
       </c>
-      <c r="CE24" s="5"/>
-    </row>
-    <row r="25" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE24" s="5">
+        <v>230.95</v>
+      </c>
+      <c r="CF24" s="5"/>
+      <c r="CG24" s="5"/>
+      <c r="CH24" s="5"/>
+      <c r="CI24" s="5"/>
+    </row>
+    <row r="25" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <f t="shared" si="0"/>
         <v>876</v>
@@ -13423,9 +13572,15 @@
       <c r="CD25" s="5">
         <v>963</v>
       </c>
-      <c r="CE25" s="5"/>
-    </row>
-    <row r="26" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE25" s="5">
+        <v>984.4</v>
+      </c>
+      <c r="CF25" s="5"/>
+      <c r="CG25" s="5"/>
+      <c r="CH25" s="5"/>
+      <c r="CI25" s="5"/>
+    </row>
+    <row r="26" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <f t="shared" si="0"/>
         <v>83.1</v>
@@ -13631,9 +13786,15 @@
       <c r="CD26" s="5">
         <v>102.25</v>
       </c>
-      <c r="CE26" s="5"/>
-    </row>
-    <row r="27" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE26" s="5">
+        <v>95.25</v>
+      </c>
+      <c r="CF26" s="5"/>
+      <c r="CG26" s="5"/>
+      <c r="CH26" s="5"/>
+      <c r="CI26" s="5"/>
+    </row>
+    <row r="27" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <f t="shared" si="0"/>
         <v>36.200000000000003</v>
@@ -13839,9 +14000,15 @@
       <c r="CD27" s="5">
         <v>41.7</v>
       </c>
-      <c r="CE27" s="5"/>
-    </row>
-    <row r="28" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE27" s="5">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="CF27" s="5"/>
+      <c r="CG27" s="5"/>
+      <c r="CH27" s="5"/>
+      <c r="CI27" s="5"/>
+    </row>
+    <row r="28" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <f t="shared" si="0"/>
         <v>111.95</v>
@@ -14047,9 +14214,15 @@
       <c r="CD28" s="5">
         <v>127.65</v>
       </c>
-      <c r="CE28" s="5"/>
-    </row>
-    <row r="29" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE28" s="5">
+        <v>125.8</v>
+      </c>
+      <c r="CF28" s="5"/>
+      <c r="CG28" s="5"/>
+      <c r="CH28" s="5"/>
+      <c r="CI28" s="5"/>
+    </row>
+    <row r="29" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <f t="shared" si="0"/>
         <v>62.3</v>
@@ -14255,12 +14428,18 @@
       <c r="CD29" s="5">
         <v>69.95</v>
       </c>
-      <c r="CE29" s="5"/>
-    </row>
-    <row r="30" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE29" s="5">
+        <v>67.95</v>
+      </c>
+      <c r="CF29" s="5"/>
+      <c r="CG29" s="5"/>
+      <c r="CH29" s="5"/>
+      <c r="CI29" s="5"/>
+    </row>
+    <row r="30" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <f t="shared" si="0"/>
-        <v>38.6</v>
+        <v>36.950000000000003</v>
       </c>
       <c r="B30" s="12">
         <f t="shared" si="1"/>
@@ -14268,7 +14447,7 @@
       </c>
       <c r="C30" s="12">
         <f t="shared" si="2"/>
-        <v>12.350000000000001</v>
+        <v>14</v>
       </c>
       <c r="D30" s="45" t="s">
         <v>256</v>
@@ -14463,9 +14642,15 @@
       <c r="CD30" s="5">
         <v>38.6</v>
       </c>
-      <c r="CE30" s="5"/>
-    </row>
-    <row r="31" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE30" s="5">
+        <v>36.950000000000003</v>
+      </c>
+      <c r="CF30" s="5"/>
+      <c r="CG30" s="5"/>
+      <c r="CH30" s="5"/>
+      <c r="CI30" s="5"/>
+    </row>
+    <row r="31" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
         <v>125.3</v>
@@ -14671,9 +14856,15 @@
       <c r="CD31" s="5">
         <v>145.44999999999999</v>
       </c>
-      <c r="CE31" s="5"/>
-    </row>
-    <row r="32" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE31" s="5">
+        <v>148</v>
+      </c>
+      <c r="CF31" s="5"/>
+      <c r="CG31" s="5"/>
+      <c r="CH31" s="5"/>
+      <c r="CI31" s="5"/>
+    </row>
+    <row r="32" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <f t="shared" si="0"/>
         <v>96.65</v>
@@ -14867,9 +15058,15 @@
       <c r="CD32" s="5">
         <v>101.6</v>
       </c>
-      <c r="CE32" s="5"/>
-    </row>
-    <row r="33" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE32" s="5">
+        <v>99</v>
+      </c>
+      <c r="CF32" s="5"/>
+      <c r="CG32" s="5"/>
+      <c r="CH32" s="5"/>
+      <c r="CI32" s="5"/>
+    </row>
+    <row r="33" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <f t="shared" si="0"/>
         <v>56.75</v>
@@ -15051,9 +15248,15 @@
       <c r="CD33" s="5">
         <v>58.55</v>
       </c>
-      <c r="CE33" s="5"/>
-    </row>
-    <row r="34" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE33" s="5">
+        <v>58</v>
+      </c>
+      <c r="CF33" s="5"/>
+      <c r="CG33" s="5"/>
+      <c r="CH33" s="5"/>
+      <c r="CI33" s="5"/>
+    </row>
+    <row r="34" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <f t="shared" si="0"/>
         <v>167.9</v>
@@ -15229,23 +15432,29 @@
       <c r="CD34" s="5">
         <v>218.1</v>
       </c>
-      <c r="CE34" s="5"/>
-    </row>
-    <row r="35" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CE34" s="5">
+        <v>201.3</v>
+      </c>
+      <c r="CF34" s="5"/>
+      <c r="CG34" s="5"/>
+      <c r="CH34" s="5"/>
+      <c r="CI34" s="5"/>
+    </row>
+    <row r="35" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <f t="shared" si="0"/>
-        <v>661</v>
+        <v>402.9</v>
       </c>
       <c r="B35" s="12">
         <f t="shared" si="1"/>
-        <v>721</v>
+        <v>520</v>
       </c>
       <c r="C35" s="12">
         <f t="shared" ref="C35" si="4">B35-A35</f>
-        <v>60</v>
+        <v>117.10000000000002</v>
       </c>
       <c r="D35" s="45" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -15285,141 +15494,129 @@
       <c r="AN35" s="5"/>
       <c r="AO35" s="5"/>
       <c r="AP35" s="5"/>
-      <c r="AQ35" s="5">
-        <v>661</v>
-      </c>
-      <c r="AR35" s="5">
-        <v>680.1</v>
-      </c>
-      <c r="AS35" s="5">
-        <v>686.3</v>
-      </c>
+      <c r="AQ35" s="5"/>
+      <c r="AR35" s="5"/>
+      <c r="AS35" s="5"/>
       <c r="AT35" s="5"/>
-      <c r="AU35" s="5">
-        <v>685</v>
-      </c>
-      <c r="AV35" s="5">
-        <v>680.3</v>
-      </c>
-      <c r="AW35" s="5">
-        <v>666.1</v>
-      </c>
-      <c r="AX35" s="5">
-        <v>680</v>
-      </c>
-      <c r="AY35" s="5">
-        <v>685</v>
-      </c>
-      <c r="AZ35" s="5">
-        <v>687</v>
-      </c>
+      <c r="AU35" s="5"/>
+      <c r="AV35" s="5"/>
+      <c r="AW35" s="5"/>
+      <c r="AX35" s="5"/>
+      <c r="AY35" s="5"/>
+      <c r="AZ35" s="5"/>
       <c r="BA35" s="5">
-        <v>687.5</v>
+        <v>520</v>
       </c>
       <c r="BB35" s="5">
-        <v>701</v>
+        <v>452.5</v>
       </c>
       <c r="BC35" s="5">
-        <v>695.45</v>
+        <v>442.95</v>
       </c>
       <c r="BD35" s="5">
-        <v>709.15</v>
+        <v>427.75</v>
       </c>
       <c r="BE35" s="5">
-        <v>714.65</v>
+        <v>443.45</v>
       </c>
       <c r="BF35" s="5">
-        <v>692.5</v>
+        <v>425.95</v>
       </c>
       <c r="BG35" s="5">
-        <v>704.95</v>
+        <v>421.65</v>
       </c>
       <c r="BH35" s="5">
-        <v>678.55</v>
+        <v>402.9</v>
       </c>
       <c r="BI35" s="5">
-        <v>683.7</v>
+        <v>411.1</v>
       </c>
       <c r="BJ35" s="5">
-        <v>683</v>
+        <v>412.1</v>
       </c>
       <c r="BK35" s="5">
-        <v>681</v>
+        <v>411.95</v>
       </c>
       <c r="BL35" s="5">
-        <v>677</v>
+        <v>416.7</v>
       </c>
       <c r="BM35" s="5">
-        <v>677</v>
+        <v>405.05</v>
       </c>
       <c r="BN35" s="5">
-        <v>677</v>
+        <v>446.3</v>
       </c>
       <c r="BO35" s="5">
-        <v>680.5</v>
+        <v>470.4</v>
       </c>
       <c r="BP35" s="5">
-        <v>675.7</v>
+        <v>487.5</v>
       </c>
       <c r="BQ35" s="5">
-        <v>679</v>
+        <v>491.7</v>
       </c>
       <c r="BR35" s="5">
-        <v>680.5</v>
+        <v>469.85</v>
       </c>
       <c r="BS35" s="5">
-        <v>686.8</v>
+        <v>465</v>
       </c>
       <c r="BT35" s="5">
-        <v>686.8</v>
+        <v>438.6</v>
       </c>
       <c r="BU35" s="5">
-        <v>686</v>
+        <v>416.7</v>
       </c>
       <c r="BV35" s="5">
-        <v>679.55</v>
+        <v>437.5</v>
       </c>
       <c r="BW35" s="5">
-        <v>684.9</v>
+        <v>448.9</v>
       </c>
       <c r="BX35" s="5">
-        <v>684.75</v>
+        <v>432</v>
       </c>
       <c r="BY35" s="5">
-        <v>695</v>
+        <v>419</v>
       </c>
       <c r="BZ35" s="5">
-        <v>699</v>
+        <v>434.5</v>
       </c>
       <c r="CA35" s="5">
-        <v>700</v>
+        <v>423</v>
       </c>
       <c r="CB35" s="5">
-        <v>693.5</v>
+        <v>424</v>
       </c>
       <c r="CC35" s="5">
-        <v>715.7</v>
+        <v>419.9</v>
       </c>
       <c r="CD35" s="5">
-        <v>721</v>
-      </c>
-      <c r="CE35" s="5"/>
-    </row>
-    <row r="36" spans="1:83" x14ac:dyDescent="0.25">
+        <v>414.5</v>
+      </c>
+      <c r="CE35" s="5">
+        <v>410</v>
+      </c>
+      <c r="CF35" s="5"/>
+      <c r="CG35" s="5"/>
+      <c r="CH35" s="5"/>
+      <c r="CI35" s="5"/>
+    </row>
+    <row r="36" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <f t="shared" si="0"/>
-        <v>402.9</v>
+        <v>226</v>
       </c>
       <c r="B36" s="12">
         <f t="shared" si="1"/>
-        <v>520</v>
+        <v>396.85</v>
       </c>
       <c r="C36" s="12">
         <f t="shared" ref="C36" si="5">B36-A36</f>
-        <v>117.10000000000002</v>
+        <v>170.85000000000002</v>
       </c>
       <c r="D36" s="45" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -15469,113 +15666,109 @@
       <c r="AX36" s="5"/>
       <c r="AY36" s="5"/>
       <c r="AZ36" s="5"/>
-      <c r="BA36" s="5">
-        <v>520</v>
-      </c>
-      <c r="BB36" s="5">
-        <v>452.5</v>
-      </c>
-      <c r="BC36" s="5">
-        <v>442.95</v>
-      </c>
-      <c r="BD36" s="5">
-        <v>427.75</v>
-      </c>
-      <c r="BE36" s="5">
-        <v>443.45</v>
-      </c>
+      <c r="BA36" s="5"/>
+      <c r="BB36" s="5"/>
+      <c r="BC36" s="5"/>
+      <c r="BD36" s="5"/>
+      <c r="BE36" s="5"/>
       <c r="BF36" s="5">
-        <v>425.95</v>
+        <v>226</v>
       </c>
       <c r="BG36" s="5">
-        <v>421.65</v>
+        <v>245</v>
       </c>
       <c r="BH36" s="5">
-        <v>402.9</v>
+        <v>251.5</v>
       </c>
       <c r="BI36" s="5">
-        <v>411.1</v>
+        <v>242</v>
       </c>
       <c r="BJ36" s="5">
-        <v>412.1</v>
+        <v>245.7</v>
       </c>
       <c r="BK36" s="5">
-        <v>411.95</v>
+        <v>262.35000000000002</v>
       </c>
       <c r="BL36" s="5">
-        <v>416.7</v>
+        <v>270.60000000000002</v>
       </c>
       <c r="BM36" s="5">
-        <v>405.05</v>
+        <v>281</v>
       </c>
       <c r="BN36" s="5">
-        <v>446.3</v>
+        <v>309.95</v>
       </c>
       <c r="BO36" s="5">
-        <v>470.4</v>
+        <v>332</v>
       </c>
       <c r="BP36" s="5">
-        <v>487.5</v>
+        <v>361</v>
       </c>
       <c r="BQ36" s="5">
-        <v>491.7</v>
+        <v>374.25</v>
       </c>
       <c r="BR36" s="5">
-        <v>469.85</v>
+        <v>384</v>
       </c>
       <c r="BS36" s="5">
-        <v>465</v>
+        <v>396.85</v>
       </c>
       <c r="BT36" s="5">
-        <v>438.6</v>
+        <v>382.9</v>
       </c>
       <c r="BU36" s="5">
-        <v>416.7</v>
+        <v>365.7</v>
       </c>
       <c r="BV36" s="5">
-        <v>437.5</v>
+        <v>347.45</v>
       </c>
       <c r="BW36" s="5">
-        <v>448.9</v>
+        <v>335.35</v>
       </c>
       <c r="BX36" s="5">
-        <v>432</v>
+        <v>318</v>
       </c>
       <c r="BY36" s="5">
-        <v>419</v>
+        <v>302.8</v>
       </c>
       <c r="BZ36" s="5">
-        <v>434.5</v>
+        <v>319.3</v>
       </c>
       <c r="CA36" s="5">
-        <v>423</v>
+        <v>326.8</v>
       </c>
       <c r="CB36" s="5">
-        <v>424</v>
+        <v>333.3</v>
       </c>
       <c r="CC36" s="5">
-        <v>419.9</v>
+        <v>349.9</v>
       </c>
       <c r="CD36" s="5">
-        <v>414.5</v>
-      </c>
-      <c r="CE36" s="5"/>
-    </row>
-    <row r="37" spans="1:83" x14ac:dyDescent="0.25">
+        <v>357.6</v>
+      </c>
+      <c r="CE36" s="5">
+        <v>347.9</v>
+      </c>
+      <c r="CF36" s="5"/>
+      <c r="CG36" s="5"/>
+      <c r="CH36" s="5"/>
+      <c r="CI36" s="5"/>
+    </row>
+    <row r="37" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <f t="shared" si="0"/>
-        <v>226</v>
+        <v>75.2</v>
       </c>
       <c r="B37" s="12">
         <f t="shared" si="1"/>
-        <v>396.85</v>
+        <v>83.85</v>
       </c>
       <c r="C37" s="12">
         <f t="shared" ref="C37" si="6">B37-A37</f>
-        <v>170.85000000000002</v>
+        <v>8.6499999999999915</v>
       </c>
       <c r="D37" s="45" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -15630,95 +15823,93 @@
       <c r="BC37" s="5"/>
       <c r="BD37" s="5"/>
       <c r="BE37" s="5"/>
-      <c r="BF37" s="5">
-        <v>226</v>
-      </c>
-      <c r="BG37" s="5">
-        <v>245</v>
-      </c>
-      <c r="BH37" s="5">
-        <v>251.5</v>
-      </c>
-      <c r="BI37" s="5">
-        <v>242</v>
-      </c>
+      <c r="BF37" s="5"/>
+      <c r="BG37" s="5"/>
+      <c r="BH37" s="5"/>
+      <c r="BI37" s="5"/>
       <c r="BJ37" s="5">
-        <v>245.7</v>
+        <v>78</v>
       </c>
       <c r="BK37" s="5">
-        <v>262.35000000000002</v>
+        <v>77.900000000000006</v>
       </c>
       <c r="BL37" s="5">
-        <v>270.60000000000002</v>
+        <v>77.95</v>
       </c>
       <c r="BM37" s="5">
-        <v>281</v>
+        <v>76</v>
       </c>
       <c r="BN37" s="5">
-        <v>309.95</v>
+        <v>76.849999999999994</v>
       </c>
       <c r="BO37" s="5">
-        <v>332</v>
+        <v>78.5</v>
       </c>
       <c r="BP37" s="5">
-        <v>361</v>
+        <v>75.2</v>
       </c>
       <c r="BQ37" s="5">
-        <v>374.25</v>
+        <v>75.900000000000006</v>
       </c>
       <c r="BR37" s="5">
-        <v>384</v>
+        <v>77.099999999999994</v>
       </c>
       <c r="BS37" s="5">
-        <v>396.85</v>
+        <v>77.25</v>
       </c>
       <c r="BT37" s="5">
-        <v>382.9</v>
+        <v>76</v>
       </c>
       <c r="BU37" s="5">
-        <v>365.7</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="BV37" s="5">
-        <v>347.45</v>
+        <v>76.7</v>
       </c>
       <c r="BW37" s="5">
-        <v>335.35</v>
+        <v>76</v>
       </c>
       <c r="BX37" s="5">
-        <v>318</v>
+        <v>76.650000000000006</v>
       </c>
       <c r="BY37" s="5">
-        <v>302.8</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="BZ37" s="5">
-        <v>319.3</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="CA37" s="5">
-        <v>326.8</v>
+        <v>82</v>
       </c>
       <c r="CB37" s="5">
-        <v>333.3</v>
+        <v>83.85</v>
       </c>
       <c r="CC37" s="5">
-        <v>349.9</v>
+        <v>83.15</v>
       </c>
       <c r="CD37" s="5">
-        <v>357.6</v>
-      </c>
-      <c r="CE37" s="5"/>
-    </row>
-    <row r="38" spans="1:83" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="CE37" s="5">
+        <v>80</v>
+      </c>
+      <c r="CF37" s="5"/>
+      <c r="CG37" s="5"/>
+      <c r="CH37" s="5"/>
+      <c r="CI37" s="5"/>
+    </row>
+    <row r="38" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <f t="shared" si="0"/>
-        <v>75.2</v>
+        <v>410.25</v>
       </c>
       <c r="B38" s="12">
         <f t="shared" si="1"/>
-        <v>83.85</v>
+        <v>472</v>
       </c>
       <c r="C38" s="12">
         <f t="shared" ref="C38" si="7">B38-A38</f>
-        <v>8.6499999999999915</v>
+        <v>61.75</v>
       </c>
       <c r="D38" s="45" t="s">
         <v>304</v>
@@ -15781,82 +15972,88 @@
       <c r="BH38" s="5"/>
       <c r="BI38" s="5"/>
       <c r="BJ38" s="5">
-        <v>78</v>
+        <v>465.55</v>
       </c>
       <c r="BK38" s="5">
-        <v>77.900000000000006</v>
+        <v>461</v>
       </c>
       <c r="BL38" s="5">
-        <v>77.95</v>
+        <v>469.15</v>
       </c>
       <c r="BM38" s="5">
-        <v>76</v>
+        <v>466</v>
       </c>
       <c r="BN38" s="5">
-        <v>76.849999999999994</v>
+        <v>472</v>
       </c>
       <c r="BO38" s="5">
-        <v>78.5</v>
+        <v>467</v>
       </c>
       <c r="BP38" s="5">
-        <v>75.2</v>
+        <v>450.55</v>
       </c>
       <c r="BQ38" s="5">
-        <v>75.900000000000006</v>
+        <v>444.05</v>
       </c>
       <c r="BR38" s="5">
-        <v>77.099999999999994</v>
+        <v>428</v>
       </c>
       <c r="BS38" s="5">
-        <v>77.25</v>
+        <v>427</v>
       </c>
       <c r="BT38" s="5">
-        <v>76</v>
+        <v>417.75</v>
       </c>
       <c r="BU38" s="5">
-        <v>76.400000000000006</v>
+        <v>424.9</v>
       </c>
       <c r="BV38" s="5">
-        <v>76.7</v>
+        <v>425</v>
       </c>
       <c r="BW38" s="5">
-        <v>76</v>
+        <v>426.1</v>
       </c>
       <c r="BX38" s="5">
-        <v>76.650000000000006</v>
+        <v>416</v>
       </c>
       <c r="BY38" s="5">
-        <v>76.599999999999994</v>
+        <v>417</v>
       </c>
       <c r="BZ38" s="5">
-        <v>76.599999999999994</v>
+        <v>416.8</v>
       </c>
       <c r="CA38" s="5">
-        <v>82</v>
+        <v>429.15</v>
       </c>
       <c r="CB38" s="5">
-        <v>83.85</v>
+        <v>430.75</v>
       </c>
       <c r="CC38" s="5">
-        <v>83.15</v>
+        <v>422.1</v>
       </c>
       <c r="CD38" s="5">
-        <v>82</v>
-      </c>
-      <c r="CE38" s="5"/>
-    </row>
-    <row r="39" spans="1:83" x14ac:dyDescent="0.25">
+        <v>418.2</v>
+      </c>
+      <c r="CE38" s="5">
+        <v>410.25</v>
+      </c>
+      <c r="CF38" s="5"/>
+      <c r="CG38" s="5"/>
+      <c r="CH38" s="5"/>
+      <c r="CI38" s="5"/>
+    </row>
+    <row r="39" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <f t="shared" si="0"/>
-        <v>416</v>
+        <v>175.2</v>
       </c>
       <c r="B39" s="12">
         <f t="shared" si="1"/>
-        <v>472</v>
+        <v>215.25</v>
       </c>
       <c r="C39" s="12">
         <f t="shared" ref="C39" si="8">B39-A39</f>
-        <v>56</v>
+        <v>40.050000000000011</v>
       </c>
       <c r="D39" s="45" t="s">
         <v>305</v>
@@ -15918,83 +16115,85 @@
       <c r="BG39" s="5"/>
       <c r="BH39" s="5"/>
       <c r="BI39" s="5"/>
-      <c r="BJ39" s="5">
-        <v>465.55</v>
-      </c>
-      <c r="BK39" s="5">
-        <v>461</v>
-      </c>
+      <c r="BJ39" s="5"/>
+      <c r="BK39" s="5"/>
       <c r="BL39" s="5">
-        <v>469.15</v>
+        <v>208</v>
       </c>
       <c r="BM39" s="5">
-        <v>466</v>
+        <v>209.8</v>
       </c>
       <c r="BN39" s="5">
-        <v>472</v>
+        <v>203.65</v>
       </c>
       <c r="BO39" s="5">
-        <v>467</v>
+        <v>201.7</v>
       </c>
       <c r="BP39" s="5">
-        <v>450.55</v>
+        <v>192.65</v>
       </c>
       <c r="BQ39" s="5">
-        <v>444.05</v>
+        <v>196.9</v>
       </c>
       <c r="BR39" s="5">
-        <v>428</v>
+        <v>204.8</v>
       </c>
       <c r="BS39" s="5">
-        <v>427</v>
+        <v>215.25</v>
       </c>
       <c r="BT39" s="5">
-        <v>417.75</v>
+        <v>208.5</v>
       </c>
       <c r="BU39" s="5">
-        <v>424.9</v>
+        <v>198.3</v>
       </c>
       <c r="BV39" s="5">
-        <v>425</v>
+        <v>206</v>
       </c>
       <c r="BW39" s="5">
-        <v>426.1</v>
+        <v>211.6</v>
       </c>
       <c r="BX39" s="5">
-        <v>416</v>
+        <v>210.3</v>
       </c>
       <c r="BY39" s="5">
-        <v>417</v>
+        <v>204.5</v>
       </c>
       <c r="BZ39" s="5">
-        <v>416.8</v>
+        <v>208</v>
       </c>
       <c r="CA39" s="5">
-        <v>429.15</v>
+        <v>201</v>
       </c>
       <c r="CB39" s="5">
-        <v>430.75</v>
+        <v>201.4</v>
       </c>
       <c r="CC39" s="5">
-        <v>422.1</v>
+        <v>191</v>
       </c>
       <c r="CD39" s="5">
-        <v>418.2</v>
-      </c>
-      <c r="CE39" s="5"/>
-    </row>
-    <row r="40" spans="1:83" x14ac:dyDescent="0.25">
+        <v>175.2</v>
+      </c>
+      <c r="CE39" s="5">
+        <v>183.25</v>
+      </c>
+      <c r="CF39" s="5"/>
+      <c r="CG39" s="5"/>
+      <c r="CH39" s="5"/>
+      <c r="CI39" s="5"/>
+    </row>
+    <row r="40" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <f t="shared" si="0"/>
-        <v>175.2</v>
+        <v>35</v>
       </c>
       <c r="B40" s="12">
         <f t="shared" si="1"/>
-        <v>215.25</v>
+        <v>39.450000000000003</v>
       </c>
       <c r="C40" s="12">
-        <f t="shared" ref="C40" si="9">B40-A40</f>
-        <v>40.050000000000011</v>
+        <f t="shared" ref="C40:C43" si="9">B40-A40</f>
+        <v>4.4500000000000028</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>306</v>
@@ -16058,77 +16257,79 @@
       <c r="BI40" s="5"/>
       <c r="BJ40" s="5"/>
       <c r="BK40" s="5"/>
-      <c r="BL40" s="5">
-        <v>208</v>
-      </c>
-      <c r="BM40" s="5">
-        <v>209.8</v>
-      </c>
+      <c r="BL40" s="5"/>
+      <c r="BM40" s="5"/>
       <c r="BN40" s="5">
-        <v>203.65</v>
+        <v>38.1</v>
       </c>
       <c r="BO40" s="5">
-        <v>201.7</v>
+        <v>36.950000000000003</v>
       </c>
       <c r="BP40" s="5">
-        <v>192.65</v>
+        <v>38.65</v>
       </c>
       <c r="BQ40" s="5">
-        <v>196.9</v>
+        <v>38.35</v>
       </c>
       <c r="BR40" s="5">
-        <v>204.8</v>
+        <v>38.450000000000003</v>
       </c>
       <c r="BS40" s="5">
-        <v>215.25</v>
+        <v>36.4</v>
       </c>
       <c r="BT40" s="5">
-        <v>208.5</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="BU40" s="5">
-        <v>198.3</v>
+        <v>35</v>
       </c>
       <c r="BV40" s="5">
-        <v>206</v>
+        <v>36</v>
       </c>
       <c r="BW40" s="5">
-        <v>211.6</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="BX40" s="5">
-        <v>210.3</v>
+        <v>37.65</v>
       </c>
       <c r="BY40" s="5">
-        <v>204.5</v>
+        <v>37.65</v>
       </c>
       <c r="BZ40" s="5">
-        <v>208</v>
+        <v>37.15</v>
       </c>
       <c r="CA40" s="5">
-        <v>201</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="CB40" s="5">
-        <v>201.4</v>
+        <v>37</v>
       </c>
       <c r="CC40" s="5">
-        <v>191</v>
+        <v>39.450000000000003</v>
       </c>
       <c r="CD40" s="5">
-        <v>175.2</v>
-      </c>
-      <c r="CE40" s="5"/>
-    </row>
-    <row r="41" spans="1:83" x14ac:dyDescent="0.25">
+        <v>38.15</v>
+      </c>
+      <c r="CE40" s="5">
+        <v>37</v>
+      </c>
+      <c r="CF40" s="5"/>
+      <c r="CG40" s="5"/>
+      <c r="CH40" s="5"/>
+      <c r="CI40" s="5"/>
+    </row>
+    <row r="41" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>552.04999999999995</v>
       </c>
       <c r="B41" s="12">
         <f t="shared" si="1"/>
-        <v>39.450000000000003</v>
+        <v>626.70000000000005</v>
       </c>
       <c r="C41" s="12">
-        <f t="shared" ref="C41:C44" si="10">B41-A41</f>
-        <v>4.4500000000000028</v>
+        <f t="shared" si="9"/>
+        <v>74.650000000000091</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>307</v>
@@ -16194,71 +16395,75 @@
       <c r="BK41" s="5"/>
       <c r="BL41" s="5"/>
       <c r="BM41" s="5"/>
-      <c r="BN41" s="5">
-        <v>38.1</v>
-      </c>
+      <c r="BN41" s="5"/>
       <c r="BO41" s="5">
-        <v>36.950000000000003</v>
+        <v>585</v>
       </c>
       <c r="BP41" s="5">
-        <v>38.65</v>
+        <v>577.45000000000005</v>
       </c>
       <c r="BQ41" s="5">
-        <v>38.35</v>
+        <v>597.20000000000005</v>
       </c>
       <c r="BR41" s="5">
-        <v>38.450000000000003</v>
+        <v>584</v>
       </c>
       <c r="BS41" s="5">
-        <v>36.4</v>
+        <v>616.15</v>
       </c>
       <c r="BT41" s="5">
-        <v>35.299999999999997</v>
+        <v>619</v>
       </c>
       <c r="BU41" s="5">
-        <v>35</v>
+        <v>610</v>
       </c>
       <c r="BV41" s="5">
-        <v>36</v>
+        <v>626.70000000000005</v>
       </c>
       <c r="BW41" s="5">
-        <v>37.200000000000003</v>
+        <v>607.29999999999995</v>
       </c>
       <c r="BX41" s="5">
-        <v>37.65</v>
+        <v>580.04999999999995</v>
       </c>
       <c r="BY41" s="5">
-        <v>37.65</v>
+        <v>552.04999999999995</v>
       </c>
       <c r="BZ41" s="5">
-        <v>37.15</v>
+        <v>580.1</v>
       </c>
       <c r="CA41" s="5">
-        <v>37.200000000000003</v>
+        <v>581.45000000000005</v>
       </c>
       <c r="CB41" s="5">
-        <v>37</v>
+        <v>578.15</v>
       </c>
       <c r="CC41" s="5">
-        <v>39.450000000000003</v>
+        <v>607.15</v>
       </c>
       <c r="CD41" s="5">
-        <v>38.15</v>
-      </c>
-      <c r="CE41" s="5"/>
-    </row>
-    <row r="42" spans="1:83" x14ac:dyDescent="0.25">
+        <v>590</v>
+      </c>
+      <c r="CE41" s="5">
+        <v>552.75</v>
+      </c>
+      <c r="CF41" s="5"/>
+      <c r="CG41" s="5"/>
+      <c r="CH41" s="5"/>
+      <c r="CI41" s="5"/>
+    </row>
+    <row r="42" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <f t="shared" si="0"/>
-        <v>552.04999999999995</v>
+        <v>814.2</v>
       </c>
       <c r="B42" s="12">
         <f t="shared" si="1"/>
-        <v>626.70000000000005</v>
+        <v>856</v>
       </c>
       <c r="C42" s="12">
-        <f t="shared" si="10"/>
-        <v>74.650000000000091</v>
+        <f t="shared" si="9"/>
+        <v>41.799999999999955</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>308</v>
@@ -16326,67 +16531,73 @@
       <c r="BM42" s="5"/>
       <c r="BN42" s="5"/>
       <c r="BO42" s="5">
-        <v>585</v>
+        <v>856</v>
       </c>
       <c r="BP42" s="5">
-        <v>577.45000000000005</v>
+        <v>832.8</v>
       </c>
       <c r="BQ42" s="5">
-        <v>597.20000000000005</v>
+        <v>830.25</v>
       </c>
       <c r="BR42" s="5">
-        <v>584</v>
+        <v>832.95</v>
       </c>
       <c r="BS42" s="5">
-        <v>616.15</v>
+        <v>826</v>
       </c>
       <c r="BT42" s="5">
-        <v>619</v>
+        <v>835</v>
       </c>
       <c r="BU42" s="5">
-        <v>610</v>
+        <v>822.95</v>
       </c>
       <c r="BV42" s="5">
-        <v>626.70000000000005</v>
+        <v>828.55</v>
       </c>
       <c r="BW42" s="5">
-        <v>607.29999999999995</v>
+        <v>831.85</v>
       </c>
       <c r="BX42" s="5">
-        <v>580.04999999999995</v>
+        <v>826</v>
       </c>
       <c r="BY42" s="5">
-        <v>552.04999999999995</v>
+        <v>837.25</v>
       </c>
       <c r="BZ42" s="5">
-        <v>580.1</v>
+        <v>828.3</v>
       </c>
       <c r="CA42" s="5">
-        <v>581.45000000000005</v>
+        <v>829.4</v>
       </c>
       <c r="CB42" s="5">
-        <v>578.15</v>
+        <v>832.05</v>
       </c>
       <c r="CC42" s="5">
-        <v>607.15</v>
+        <v>836.65</v>
       </c>
       <c r="CD42" s="5">
-        <v>590</v>
-      </c>
-      <c r="CE42" s="5"/>
-    </row>
-    <row r="43" spans="1:83" x14ac:dyDescent="0.25">
+        <v>814.2</v>
+      </c>
+      <c r="CE42" s="5">
+        <v>814.2</v>
+      </c>
+      <c r="CF42" s="5"/>
+      <c r="CG42" s="5"/>
+      <c r="CH42" s="5"/>
+      <c r="CI42" s="5"/>
+    </row>
+    <row r="43" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <f t="shared" si="0"/>
-        <v>814.2</v>
+        <v>134.9</v>
       </c>
       <c r="B43" s="12">
         <f t="shared" si="1"/>
-        <v>856</v>
+        <v>146</v>
       </c>
       <c r="C43" s="12">
-        <f t="shared" si="10"/>
-        <v>41.799999999999955</v>
+        <f t="shared" si="9"/>
+        <v>11.099999999999994</v>
       </c>
       <c r="D43" s="45" t="s">
         <v>309</v>
@@ -16453,71 +16664,75 @@
       <c r="BL43" s="5"/>
       <c r="BM43" s="5"/>
       <c r="BN43" s="5"/>
-      <c r="BO43" s="5">
-        <v>856</v>
-      </c>
+      <c r="BO43" s="5"/>
       <c r="BP43" s="5">
-        <v>832.8</v>
+        <v>146</v>
       </c>
       <c r="BQ43" s="5">
-        <v>830.25</v>
+        <v>141.80000000000001</v>
       </c>
       <c r="BR43" s="5">
-        <v>832.95</v>
+        <v>140.30000000000001</v>
       </c>
       <c r="BS43" s="5">
-        <v>826</v>
+        <v>137.9</v>
       </c>
       <c r="BT43" s="5">
-        <v>835</v>
+        <v>140.25</v>
       </c>
       <c r="BU43" s="5">
-        <v>822.95</v>
+        <v>134.9</v>
       </c>
       <c r="BV43" s="5">
-        <v>828.55</v>
+        <v>137</v>
       </c>
       <c r="BW43" s="5">
-        <v>831.85</v>
+        <v>137.75</v>
       </c>
       <c r="BX43" s="5">
-        <v>826</v>
+        <v>138.25</v>
       </c>
       <c r="BY43" s="5">
-        <v>837.25</v>
+        <v>139.35</v>
       </c>
       <c r="BZ43" s="5">
-        <v>828.3</v>
+        <v>138.19999999999999</v>
       </c>
       <c r="CA43" s="5">
-        <v>829.4</v>
+        <v>142.9</v>
       </c>
       <c r="CB43" s="5">
-        <v>832.05</v>
+        <v>143.65</v>
       </c>
       <c r="CC43" s="5">
-        <v>836.65</v>
+        <v>145.1</v>
       </c>
       <c r="CD43" s="5">
-        <v>814.2</v>
-      </c>
-      <c r="CE43" s="5"/>
-    </row>
-    <row r="44" spans="1:83" x14ac:dyDescent="0.25">
+        <v>138.69999999999999</v>
+      </c>
+      <c r="CE43" s="5">
+        <v>137.65</v>
+      </c>
+      <c r="CF43" s="5"/>
+      <c r="CG43" s="5"/>
+      <c r="CH43" s="5"/>
+      <c r="CI43" s="5"/>
+    </row>
+    <row r="44" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <f t="shared" si="0"/>
-        <v>134.9</v>
+        <v>601.9</v>
       </c>
       <c r="B44" s="12">
         <f t="shared" si="1"/>
-        <v>146</v>
+        <v>770</v>
       </c>
       <c r="C44" s="12">
-        <f t="shared" si="10"/>
-        <v>11.099999999999994</v>
+        <f t="shared" ref="C44" si="10">B44-A44</f>
+        <v>168.10000000000002</v>
       </c>
       <c r="D44" s="45" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -16582,68 +16797,68 @@
       <c r="BM44" s="5"/>
       <c r="BN44" s="5"/>
       <c r="BO44" s="5"/>
-      <c r="BP44" s="5">
-        <v>146</v>
-      </c>
-      <c r="BQ44" s="5">
-        <v>141.80000000000001</v>
-      </c>
-      <c r="BR44" s="5">
-        <v>140.30000000000001</v>
-      </c>
+      <c r="BP44" s="5"/>
+      <c r="BQ44" s="5"/>
+      <c r="BR44" s="5"/>
       <c r="BS44" s="5">
-        <v>137.9</v>
+        <v>770</v>
       </c>
       <c r="BT44" s="5">
-        <v>140.25</v>
+        <v>696</v>
       </c>
       <c r="BU44" s="5">
-        <v>134.9</v>
+        <v>680.25</v>
       </c>
       <c r="BV44" s="5">
-        <v>137</v>
+        <v>679.8</v>
       </c>
       <c r="BW44" s="5">
-        <v>137.75</v>
+        <v>679</v>
       </c>
       <c r="BX44" s="5">
-        <v>138.25</v>
+        <v>668</v>
       </c>
       <c r="BY44" s="5">
-        <v>139.35</v>
+        <v>667.5</v>
       </c>
       <c r="BZ44" s="5">
-        <v>138.19999999999999</v>
+        <v>663.95</v>
       </c>
       <c r="CA44" s="5">
-        <v>142.9</v>
+        <v>648.4</v>
       </c>
       <c r="CB44" s="5">
-        <v>143.65</v>
+        <v>648.4</v>
       </c>
       <c r="CC44" s="5">
-        <v>145.1</v>
+        <v>639.79999999999995</v>
       </c>
       <c r="CD44" s="5">
-        <v>138.69999999999999</v>
-      </c>
-      <c r="CE44" s="5"/>
-    </row>
-    <row r="45" spans="1:83" x14ac:dyDescent="0.25">
+        <v>623</v>
+      </c>
+      <c r="CE44" s="5">
+        <v>601.9</v>
+      </c>
+      <c r="CF44" s="5"/>
+      <c r="CG44" s="5"/>
+      <c r="CH44" s="5"/>
+      <c r="CI44" s="5"/>
+    </row>
+    <row r="45" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <f t="shared" si="0"/>
-        <v>623</v>
+        <v>105.5</v>
       </c>
       <c r="B45" s="12">
         <f t="shared" si="1"/>
-        <v>770</v>
+        <v>110.95</v>
       </c>
       <c r="C45" s="12">
         <f t="shared" ref="C45" si="11">B45-A45</f>
-        <v>147</v>
+        <v>5.4500000000000028</v>
       </c>
       <c r="D45" s="45" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -16711,59 +16926,57 @@
       <c r="BP45" s="5"/>
       <c r="BQ45" s="5"/>
       <c r="BR45" s="5"/>
-      <c r="BS45" s="5">
-        <v>770</v>
-      </c>
-      <c r="BT45" s="5">
-        <v>696</v>
-      </c>
-      <c r="BU45" s="5">
-        <v>680.25</v>
-      </c>
-      <c r="BV45" s="5">
-        <v>679.8</v>
-      </c>
+      <c r="BS45" s="5"/>
+      <c r="BT45" s="5"/>
+      <c r="BU45" s="5"/>
+      <c r="BV45" s="5"/>
       <c r="BW45" s="5">
-        <v>679</v>
+        <v>109</v>
       </c>
       <c r="BX45" s="5">
-        <v>668</v>
+        <v>110.95</v>
       </c>
       <c r="BY45" s="5">
-        <v>667.5</v>
+        <v>110.7</v>
       </c>
       <c r="BZ45" s="5">
-        <v>663.95</v>
+        <v>109.5</v>
       </c>
       <c r="CA45" s="5">
-        <v>648.4</v>
+        <v>109.85</v>
       </c>
       <c r="CB45" s="5">
-        <v>648.4</v>
+        <v>109.9</v>
       </c>
       <c r="CC45" s="5">
-        <v>639.79999999999995</v>
+        <v>107.9</v>
       </c>
       <c r="CD45" s="5">
-        <v>623</v>
-      </c>
-      <c r="CE45" s="5"/>
-    </row>
-    <row r="46" spans="1:83" x14ac:dyDescent="0.25">
+        <v>107.95</v>
+      </c>
+      <c r="CE45" s="5">
+        <v>105.5</v>
+      </c>
+      <c r="CF45" s="5"/>
+      <c r="CG45" s="5"/>
+      <c r="CH45" s="5"/>
+      <c r="CI45" s="5"/>
+    </row>
+    <row r="46" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
-        <f t="shared" si="0"/>
-        <v>107.9</v>
+        <f t="shared" ref="A46" si="12">MIN(E46:ZR46)</f>
+        <v>139</v>
       </c>
       <c r="B46" s="12">
-        <f t="shared" si="1"/>
-        <v>110.95</v>
+        <f t="shared" ref="B46" si="13">MAX(E46:ZR46)</f>
+        <v>145</v>
       </c>
       <c r="C46" s="12">
-        <f t="shared" ref="C46" si="12">B46-A46</f>
-        <v>3.0499999999999972</v>
+        <f t="shared" ref="C46" si="14">B46-A46</f>
+        <v>6</v>
       </c>
       <c r="D46" s="45" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -16835,31 +17048,23 @@
       <c r="BT46" s="5"/>
       <c r="BU46" s="5"/>
       <c r="BV46" s="5"/>
-      <c r="BW46" s="5">
-        <v>109</v>
-      </c>
-      <c r="BX46" s="5">
-        <v>110.95</v>
-      </c>
-      <c r="BY46" s="5">
-        <v>110.7</v>
-      </c>
-      <c r="BZ46" s="5">
-        <v>109.5</v>
-      </c>
-      <c r="CA46" s="5">
-        <v>109.85</v>
-      </c>
-      <c r="CB46" s="5">
-        <v>109.9</v>
-      </c>
-      <c r="CC46" s="5">
-        <v>107.9</v>
-      </c>
+      <c r="BW46" s="5"/>
+      <c r="BX46" s="5"/>
+      <c r="BY46" s="5"/>
+      <c r="BZ46" s="5"/>
+      <c r="CA46" s="5"/>
+      <c r="CB46" s="5"/>
+      <c r="CC46" s="5"/>
       <c r="CD46" s="5">
-        <v>107.95</v>
-      </c>
-      <c r="CE46" s="5"/>
+        <v>145</v>
+      </c>
+      <c r="CE46" s="5">
+        <v>139</v>
+      </c>
+      <c r="CF46" s="5"/>
+      <c r="CG46" s="5"/>
+      <c r="CH46" s="5"/>
+      <c r="CI46" s="5"/>
     </row>
   </sheetData>
   <sortState ref="L1:L37">
@@ -17727,7 +17932,7 @@
         <v>6000</v>
       </c>
       <c r="S19" s="50" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="T19" s="18"/>
     </row>
@@ -18084,10 +18289,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18132,7 +18337,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(B2:B200)</f>
-        <v>1108793</v>
+        <v>1158793</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -18150,7 +18355,7 @@
       </c>
       <c r="F3" s="5">
         <f>F1-F2</f>
-        <v>366596</v>
+        <v>316596</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -18389,7 +18594,7 @@
         <v>42983</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J22" s="12">
         <v>2500</v>
@@ -18429,7 +18634,7 @@
         <v>42987</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J24" s="12">
         <v>4000</v>
@@ -18469,7 +18674,7 @@
         <v>42999</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J26" s="12">
         <v>1000</v>
@@ -18489,7 +18694,7 @@
         <v>43006</v>
       </c>
       <c r="I27" s="39" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J27" s="12">
         <v>2500</v>
@@ -18500,7 +18705,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B28" s="12">
         <v>2500</v>
@@ -18509,7 +18714,7 @@
         <v>43006</v>
       </c>
       <c r="I28" s="39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J28" s="12">
         <v>30000</v>
@@ -18540,7 +18745,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B30" s="12">
         <v>4000</v>
@@ -18549,7 +18754,7 @@
         <v>43009</v>
       </c>
       <c r="I30" s="39" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J30" s="12">
         <v>19700</v>
@@ -18580,7 +18785,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B32" s="12">
         <v>1000</v>
@@ -18589,7 +18794,7 @@
         <v>43011</v>
       </c>
       <c r="I32" s="39" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J32" s="12">
         <v>5000</v>
@@ -18600,7 +18805,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="39" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B33" s="12">
         <v>2500</v>
@@ -18609,7 +18814,7 @@
         <v>43011</v>
       </c>
       <c r="I33" s="39" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J33" s="12">
         <v>5000</v>
@@ -18620,7 +18825,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B34" s="12">
         <v>30000</v>
@@ -18629,7 +18834,7 @@
         <v>43013</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J34" s="5">
         <v>56000</v>
@@ -18649,7 +18854,7 @@
         <v>43017</v>
       </c>
       <c r="I35" s="39" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J35" s="12">
         <v>4000</v>
@@ -18660,7 +18865,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="39" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B36" s="12">
         <v>19700</v>
@@ -18669,7 +18874,7 @@
         <v>43017</v>
       </c>
       <c r="I36" s="53" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J36" s="26">
         <v>13790</v>
@@ -18691,7 +18896,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="39" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B38" s="12">
         <v>5000</v>
@@ -18702,7 +18907,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="39" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B39" s="12">
         <v>5000</v>
@@ -18713,7 +18918,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="39" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B40" s="12">
         <v>56000</v>
@@ -18724,7 +18929,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="39" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B41" s="12">
         <v>16500</v>
@@ -18735,7 +18940,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B42" s="12">
         <v>4000</v>
@@ -18754,7 +18959,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="39" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B43" s="12">
         <v>13790</v>
@@ -18765,7 +18970,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="39" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B44" s="12">
         <v>15000</v>
@@ -18786,14 +18991,25 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="53" t="s">
+      <c r="A46" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="B46" s="26">
+      <c r="B46" s="12">
         <v>6560</v>
       </c>
-      <c r="C46" s="52">
+      <c r="C46" s="31">
         <v>43063</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="12">
+        <v>50000</v>
+      </c>
+      <c r="C47" s="31">
+        <v>43070</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added details for 05/12/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13530" windowHeight="8175" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13530" windowHeight="5625" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PaidTillDate" sheetId="1" r:id="rId1"/>
@@ -7247,9 +7247,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CI46"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="CA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CE50" sqref="CE50"/>
+      <selection pane="topRight" activeCell="CF43" sqref="CF43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7813,7 +7813,9 @@
       <c r="CE2" s="5">
         <v>314.25</v>
       </c>
-      <c r="CF2" s="5"/>
+      <c r="CF2" s="5">
+        <v>312.05</v>
+      </c>
       <c r="CG2" s="5"/>
       <c r="CH2" s="5"/>
       <c r="CI2" s="5"/>
@@ -8063,7 +8065,9 @@
       <c r="CE3" s="5">
         <v>305.39999999999998</v>
       </c>
-      <c r="CF3" s="5"/>
+      <c r="CF3" s="5">
+        <v>305.25</v>
+      </c>
       <c r="CG3" s="5"/>
       <c r="CH3" s="5"/>
       <c r="CI3" s="5"/>
@@ -8319,7 +8323,9 @@
       <c r="CE4" s="5">
         <v>254.75</v>
       </c>
-      <c r="CF4" s="5"/>
+      <c r="CF4" s="5">
+        <v>254.2</v>
+      </c>
       <c r="CG4" s="5"/>
       <c r="CH4" s="5"/>
       <c r="CI4" s="5"/>
@@ -8575,7 +8581,9 @@
       <c r="CE5" s="5">
         <v>902.6</v>
       </c>
-      <c r="CF5" s="5"/>
+      <c r="CF5" s="5">
+        <v>910.75</v>
+      </c>
       <c r="CG5" s="5"/>
       <c r="CH5" s="5"/>
       <c r="CI5" s="5"/>
@@ -8831,7 +8839,9 @@
       <c r="CE6" s="5">
         <v>265.89999999999998</v>
       </c>
-      <c r="CF6" s="5"/>
+      <c r="CF6" s="5">
+        <v>264.60000000000002</v>
+      </c>
       <c r="CG6" s="5"/>
       <c r="CH6" s="5"/>
       <c r="CI6" s="5"/>
@@ -9087,7 +9097,9 @@
       <c r="CE7" s="5">
         <v>17.3</v>
       </c>
-      <c r="CF7" s="5"/>
+      <c r="CF7" s="5">
+        <v>17.100000000000001</v>
+      </c>
       <c r="CG7" s="5"/>
       <c r="CH7" s="5"/>
       <c r="CI7" s="5"/>
@@ -9343,7 +9355,9 @@
       <c r="CE8" s="5">
         <v>78.3</v>
       </c>
-      <c r="CF8" s="5"/>
+      <c r="CF8" s="5">
+        <v>78</v>
+      </c>
       <c r="CG8" s="5"/>
       <c r="CH8" s="5"/>
       <c r="CI8" s="5"/>
@@ -9591,7 +9605,9 @@
       <c r="CE9" s="28">
         <v>54.4</v>
       </c>
-      <c r="CF9" s="28"/>
+      <c r="CF9" s="28">
+        <v>54.1</v>
+      </c>
       <c r="CG9" s="28"/>
       <c r="CH9" s="28"/>
       <c r="CI9" s="28"/>
@@ -9847,7 +9863,9 @@
       <c r="CE10" s="5">
         <v>36.799999999999997</v>
       </c>
-      <c r="CF10" s="5"/>
+      <c r="CF10" s="5">
+        <v>36.450000000000003</v>
+      </c>
       <c r="CG10" s="5"/>
       <c r="CH10" s="5"/>
       <c r="CI10" s="5"/>
@@ -10103,7 +10121,9 @@
       <c r="CE11" s="5">
         <v>93.2</v>
       </c>
-      <c r="CF11" s="5"/>
+      <c r="CF11" s="5">
+        <v>92.85</v>
+      </c>
       <c r="CG11" s="5"/>
       <c r="CH11" s="5"/>
       <c r="CI11" s="5"/>
@@ -10359,7 +10379,9 @@
       <c r="CE12" s="5">
         <v>90.75</v>
       </c>
-      <c r="CF12" s="5"/>
+      <c r="CF12" s="5">
+        <v>89.6</v>
+      </c>
       <c r="CG12" s="5"/>
       <c r="CH12" s="5"/>
       <c r="CI12" s="5"/>
@@ -10615,7 +10637,9 @@
       <c r="CE13" s="5">
         <v>54.25</v>
       </c>
-      <c r="CF13" s="5"/>
+      <c r="CF13" s="5">
+        <v>54.4</v>
+      </c>
       <c r="CG13" s="5"/>
       <c r="CH13" s="5"/>
       <c r="CI13" s="5"/>
@@ -10871,7 +10895,9 @@
       <c r="CE14" s="5">
         <v>38.950000000000003</v>
       </c>
-      <c r="CF14" s="5"/>
+      <c r="CF14" s="5">
+        <v>38.35</v>
+      </c>
       <c r="CG14" s="5"/>
       <c r="CH14" s="5"/>
       <c r="CI14" s="5"/>
@@ -10879,7 +10905,7 @@
     <row r="15" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
-        <v>23.95</v>
+        <v>23.85</v>
       </c>
       <c r="B15" s="12">
         <f t="shared" si="1"/>
@@ -10887,7 +10913,7 @@
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
-        <v>12.45</v>
+        <v>12.549999999999997</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>126</v>
@@ -11119,7 +11145,9 @@
       <c r="CE15" s="5">
         <v>24.1</v>
       </c>
-      <c r="CF15" s="5"/>
+      <c r="CF15" s="5">
+        <v>23.85</v>
+      </c>
       <c r="CG15" s="5"/>
       <c r="CH15" s="5"/>
       <c r="CI15" s="5"/>
@@ -11375,7 +11403,9 @@
       <c r="CE16" s="5">
         <v>690.2</v>
       </c>
-      <c r="CF16" s="5"/>
+      <c r="CF16" s="5">
+        <v>679.8</v>
+      </c>
       <c r="CG16" s="5"/>
       <c r="CH16" s="5"/>
       <c r="CI16" s="5"/>
@@ -11631,7 +11661,9 @@
       <c r="CE17" s="5">
         <v>474.5</v>
       </c>
-      <c r="CF17" s="5"/>
+      <c r="CF17" s="5">
+        <v>470.45</v>
+      </c>
       <c r="CG17" s="5"/>
       <c r="CH17" s="5"/>
       <c r="CI17" s="5"/>
@@ -11887,7 +11919,9 @@
       <c r="CE18" s="5">
         <v>261.89999999999998</v>
       </c>
-      <c r="CF18" s="5"/>
+      <c r="CF18" s="5">
+        <v>260.5</v>
+      </c>
       <c r="CG18" s="5"/>
       <c r="CH18" s="5"/>
       <c r="CI18" s="5"/>
@@ -11899,11 +11933,11 @@
       </c>
       <c r="B19" s="12">
         <f t="shared" si="1"/>
-        <v>740.95</v>
+        <v>749.15</v>
       </c>
       <c r="C19" s="12">
         <f t="shared" si="2"/>
-        <v>300.25000000000006</v>
+        <v>308.45</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -12143,7 +12177,9 @@
       <c r="CE19" s="5">
         <v>740.95</v>
       </c>
-      <c r="CF19" s="5"/>
+      <c r="CF19" s="5">
+        <v>749.15</v>
+      </c>
       <c r="CG19" s="5"/>
       <c r="CH19" s="5"/>
       <c r="CI19" s="5"/>
@@ -12151,7 +12187,7 @@
     <row r="20" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <f t="shared" si="0"/>
-        <v>674.95</v>
+        <v>669.9</v>
       </c>
       <c r="B20" s="12">
         <f t="shared" si="1"/>
@@ -12159,7 +12195,7 @@
       </c>
       <c r="C20" s="12">
         <f t="shared" si="2"/>
-        <v>121</v>
+        <v>126.05000000000007</v>
       </c>
       <c r="D20" s="44" t="s">
         <v>104</v>
@@ -12399,7 +12435,9 @@
       <c r="CE20" s="5">
         <v>674.95</v>
       </c>
-      <c r="CF20" s="5"/>
+      <c r="CF20" s="5">
+        <v>669.9</v>
+      </c>
       <c r="CG20" s="5"/>
       <c r="CH20" s="5"/>
       <c r="CI20" s="5"/>
@@ -12655,7 +12693,9 @@
       <c r="CE21" s="5">
         <v>485.2</v>
       </c>
-      <c r="CF21" s="5"/>
+      <c r="CF21" s="5">
+        <v>488.2</v>
+      </c>
       <c r="CG21" s="5"/>
       <c r="CH21" s="5"/>
       <c r="CI21" s="5"/>
@@ -12857,7 +12897,9 @@
       <c r="CE22" s="5">
         <v>379</v>
       </c>
-      <c r="CF22" s="5"/>
+      <c r="CF22" s="5">
+        <v>371.3</v>
+      </c>
       <c r="CG22" s="5"/>
       <c r="CH22" s="5"/>
       <c r="CI22" s="5"/>
@@ -13105,7 +13147,9 @@
       <c r="CE23" s="5">
         <v>58.1</v>
       </c>
-      <c r="CF23" s="5"/>
+      <c r="CF23" s="5">
+        <v>58.45</v>
+      </c>
       <c r="CG23" s="5"/>
       <c r="CH23" s="5"/>
       <c r="CI23" s="5"/>
@@ -13349,7 +13393,9 @@
       <c r="CE24" s="5">
         <v>230.95</v>
       </c>
-      <c r="CF24" s="5"/>
+      <c r="CF24" s="5">
+        <v>228.95</v>
+      </c>
       <c r="CG24" s="5"/>
       <c r="CH24" s="5"/>
       <c r="CI24" s="5"/>
@@ -13575,7 +13621,9 @@
       <c r="CE25" s="5">
         <v>984.4</v>
       </c>
-      <c r="CF25" s="5"/>
+      <c r="CF25" s="5">
+        <v>996.7</v>
+      </c>
       <c r="CG25" s="5"/>
       <c r="CH25" s="5"/>
       <c r="CI25" s="5"/>
@@ -13789,7 +13837,9 @@
       <c r="CE26" s="5">
         <v>95.25</v>
       </c>
-      <c r="CF26" s="5"/>
+      <c r="CF26" s="5">
+        <v>98.4</v>
+      </c>
       <c r="CG26" s="5"/>
       <c r="CH26" s="5"/>
       <c r="CI26" s="5"/>
@@ -14003,7 +14053,9 @@
       <c r="CE27" s="5">
         <v>39.950000000000003</v>
       </c>
-      <c r="CF27" s="5"/>
+      <c r="CF27" s="5">
+        <v>39</v>
+      </c>
       <c r="CG27" s="5"/>
       <c r="CH27" s="5"/>
       <c r="CI27" s="5"/>
@@ -14217,7 +14269,9 @@
       <c r="CE28" s="5">
         <v>125.8</v>
       </c>
-      <c r="CF28" s="5"/>
+      <c r="CF28" s="5">
+        <v>124.15</v>
+      </c>
       <c r="CG28" s="5"/>
       <c r="CH28" s="5"/>
       <c r="CI28" s="5"/>
@@ -14431,7 +14485,9 @@
       <c r="CE29" s="5">
         <v>67.95</v>
       </c>
-      <c r="CF29" s="5"/>
+      <c r="CF29" s="5">
+        <v>66.8</v>
+      </c>
       <c r="CG29" s="5"/>
       <c r="CH29" s="5"/>
       <c r="CI29" s="5"/>
@@ -14645,7 +14701,9 @@
       <c r="CE30" s="5">
         <v>36.950000000000003</v>
       </c>
-      <c r="CF30" s="5"/>
+      <c r="CF30" s="5">
+        <v>37.299999999999997</v>
+      </c>
       <c r="CG30" s="5"/>
       <c r="CH30" s="5"/>
       <c r="CI30" s="5"/>
@@ -14859,7 +14917,9 @@
       <c r="CE31" s="5">
         <v>148</v>
       </c>
-      <c r="CF31" s="5"/>
+      <c r="CF31" s="5">
+        <v>146.55000000000001</v>
+      </c>
       <c r="CG31" s="5"/>
       <c r="CH31" s="5"/>
       <c r="CI31" s="5"/>
@@ -15061,7 +15121,9 @@
       <c r="CE32" s="5">
         <v>99</v>
       </c>
-      <c r="CF32" s="5"/>
+      <c r="CF32" s="5">
+        <v>98.9</v>
+      </c>
       <c r="CG32" s="5"/>
       <c r="CH32" s="5"/>
       <c r="CI32" s="5"/>
@@ -15251,7 +15313,9 @@
       <c r="CE33" s="5">
         <v>58</v>
       </c>
-      <c r="CF33" s="5"/>
+      <c r="CF33" s="5">
+        <v>57.85</v>
+      </c>
       <c r="CG33" s="5"/>
       <c r="CH33" s="5"/>
       <c r="CI33" s="5"/>
@@ -15435,7 +15499,9 @@
       <c r="CE34" s="5">
         <v>201.3</v>
       </c>
-      <c r="CF34" s="5"/>
+      <c r="CF34" s="5">
+        <v>203.15</v>
+      </c>
       <c r="CG34" s="5"/>
       <c r="CH34" s="5"/>
       <c r="CI34" s="5"/>
@@ -15443,7 +15509,7 @@
     <row r="35" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <f t="shared" si="0"/>
-        <v>402.9</v>
+        <v>400</v>
       </c>
       <c r="B35" s="12">
         <f t="shared" si="1"/>
@@ -15451,7 +15517,7 @@
       </c>
       <c r="C35" s="12">
         <f t="shared" ref="C35" si="4">B35-A35</f>
-        <v>117.10000000000002</v>
+        <v>120</v>
       </c>
       <c r="D35" s="45" t="s">
         <v>289</v>
@@ -15597,7 +15663,9 @@
       <c r="CE35" s="5">
         <v>410</v>
       </c>
-      <c r="CF35" s="5"/>
+      <c r="CF35" s="5">
+        <v>400</v>
+      </c>
       <c r="CG35" s="5"/>
       <c r="CH35" s="5"/>
       <c r="CI35" s="5"/>
@@ -15749,7 +15817,9 @@
       <c r="CE36" s="5">
         <v>347.9</v>
       </c>
-      <c r="CF36" s="5"/>
+      <c r="CF36" s="5">
+        <v>347.55</v>
+      </c>
       <c r="CG36" s="5"/>
       <c r="CH36" s="5"/>
       <c r="CI36" s="5"/>
@@ -15893,7 +15963,9 @@
       <c r="CE37" s="5">
         <v>80</v>
       </c>
-      <c r="CF37" s="5"/>
+      <c r="CF37" s="5">
+        <v>79.3</v>
+      </c>
       <c r="CG37" s="5"/>
       <c r="CH37" s="5"/>
       <c r="CI37" s="5"/>
@@ -16037,7 +16109,9 @@
       <c r="CE38" s="5">
         <v>410.25</v>
       </c>
-      <c r="CF38" s="5"/>
+      <c r="CF38" s="5">
+        <v>411.55</v>
+      </c>
       <c r="CG38" s="5"/>
       <c r="CH38" s="5"/>
       <c r="CI38" s="5"/>
@@ -16177,7 +16251,9 @@
       <c r="CE39" s="5">
         <v>183.25</v>
       </c>
-      <c r="CF39" s="5"/>
+      <c r="CF39" s="5">
+        <v>186.3</v>
+      </c>
       <c r="CG39" s="5"/>
       <c r="CH39" s="5"/>
       <c r="CI39" s="5"/>
@@ -16313,7 +16389,9 @@
       <c r="CE40" s="5">
         <v>37</v>
       </c>
-      <c r="CF40" s="5"/>
+      <c r="CF40" s="5">
+        <v>36.15</v>
+      </c>
       <c r="CG40" s="5"/>
       <c r="CH40" s="5"/>
       <c r="CI40" s="5"/>
@@ -16447,7 +16525,9 @@
       <c r="CE41" s="5">
         <v>552.75</v>
       </c>
-      <c r="CF41" s="5"/>
+      <c r="CF41" s="5">
+        <v>568.20000000000005</v>
+      </c>
       <c r="CG41" s="5"/>
       <c r="CH41" s="5"/>
       <c r="CI41" s="5"/>
@@ -16455,7 +16535,7 @@
     <row r="42" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <f t="shared" si="0"/>
-        <v>814.2</v>
+        <v>811.25</v>
       </c>
       <c r="B42" s="12">
         <f t="shared" si="1"/>
@@ -16463,7 +16543,7 @@
       </c>
       <c r="C42" s="12">
         <f t="shared" si="9"/>
-        <v>41.799999999999955</v>
+        <v>44.75</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>308</v>
@@ -16581,7 +16661,9 @@
       <c r="CE42" s="5">
         <v>814.2</v>
       </c>
-      <c r="CF42" s="5"/>
+      <c r="CF42" s="5">
+        <v>811.25</v>
+      </c>
       <c r="CG42" s="5"/>
       <c r="CH42" s="5"/>
       <c r="CI42" s="5"/>
@@ -16713,7 +16795,9 @@
       <c r="CE43" s="5">
         <v>137.65</v>
       </c>
-      <c r="CF43" s="5"/>
+      <c r="CF43" s="5">
+        <v>135.25</v>
+      </c>
       <c r="CG43" s="5"/>
       <c r="CH43" s="5"/>
       <c r="CI43" s="5"/>
@@ -16721,7 +16805,7 @@
     <row r="44" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <f t="shared" si="0"/>
-        <v>601.9</v>
+        <v>597.04999999999995</v>
       </c>
       <c r="B44" s="12">
         <f t="shared" si="1"/>
@@ -16729,7 +16813,7 @@
       </c>
       <c r="C44" s="12">
         <f t="shared" ref="C44" si="10">B44-A44</f>
-        <v>168.10000000000002</v>
+        <v>172.95000000000005</v>
       </c>
       <c r="D44" s="45" t="s">
         <v>311</v>
@@ -16839,7 +16923,9 @@
       <c r="CE44" s="5">
         <v>601.9</v>
       </c>
-      <c r="CF44" s="5"/>
+      <c r="CF44" s="5">
+        <v>597.04999999999995</v>
+      </c>
       <c r="CG44" s="5"/>
       <c r="CH44" s="5"/>
       <c r="CI44" s="5"/>
@@ -16847,7 +16933,7 @@
     <row r="45" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <f t="shared" si="0"/>
-        <v>105.5</v>
+        <v>103.1</v>
       </c>
       <c r="B45" s="12">
         <f t="shared" si="1"/>
@@ -16855,7 +16941,7 @@
       </c>
       <c r="C45" s="12">
         <f t="shared" ref="C45" si="11">B45-A45</f>
-        <v>5.4500000000000028</v>
+        <v>7.8500000000000085</v>
       </c>
       <c r="D45" s="45" t="s">
         <v>323</v>
@@ -16957,7 +17043,9 @@
       <c r="CE45" s="5">
         <v>105.5</v>
       </c>
-      <c r="CF45" s="5"/>
+      <c r="CF45" s="5">
+        <v>103.1</v>
+      </c>
       <c r="CG45" s="5"/>
       <c r="CH45" s="5"/>
       <c r="CI45" s="5"/>
@@ -17061,7 +17149,9 @@
       <c r="CE46" s="5">
         <v>139</v>
       </c>
-      <c r="CF46" s="5"/>
+      <c r="CF46" s="5">
+        <v>139.30000000000001</v>
+      </c>
       <c r="CG46" s="5"/>
       <c r="CH46" s="5"/>
       <c r="CI46" s="5"/>
@@ -18291,7 +18381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A46" sqref="A46:C47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added details for 08/12/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="326">
   <si>
     <t>Date</t>
   </si>
@@ -1000,6 +1000,9 @@
   </si>
   <si>
     <t>GPPL</t>
+  </si>
+  <si>
+    <t>Batra</t>
   </si>
 </sst>
 </file>
@@ -7245,11 +7248,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CI46"/>
+  <dimension ref="A1:CH46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="CA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CF43" sqref="CF43"/>
+      <selection pane="topRight" activeCell="CH2" sqref="CH2:CH46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7302,10 +7305,10 @@
     <col min="82" max="82" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="13" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="13" customWidth="1"/>
-    <col min="85" max="87" width="13" bestFit="1" customWidth="1"/>
+    <col min="85" max="86" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:86" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>249</v>
       </c>
@@ -7562,19 +7565,16 @@
         <v>42898</v>
       </c>
       <c r="CH1" s="51">
-        <v>42928</v>
-      </c>
-      <c r="CI1" s="51">
         <v>42959</v>
       </c>
     </row>
-    <row r="2" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
-        <f t="shared" ref="A2:A45" si="0">MIN(E2:ZR2)</f>
+        <f>MIN(E2:ZQ2)</f>
         <v>243.6</v>
       </c>
       <c r="B2" s="12">
-        <f t="shared" ref="B2:B45" si="1">MAX(E2:ZR2)</f>
+        <f>MAX(E2:ZQ2)</f>
         <v>340.8</v>
       </c>
       <c r="C2" s="12">
@@ -7816,21 +7816,24 @@
       <c r="CF2" s="5">
         <v>312.05</v>
       </c>
-      <c r="CG2" s="5"/>
-      <c r="CH2" s="5"/>
-      <c r="CI2" s="5"/>
-    </row>
-    <row r="3" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG2" s="5">
+        <v>313.89999999999998</v>
+      </c>
+      <c r="CH2" s="5">
+        <v>313.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E3:ZQ3)</f>
         <v>262.7</v>
       </c>
       <c r="B3" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E3:ZQ3)</f>
         <v>328.85</v>
       </c>
       <c r="C3" s="12">
-        <f t="shared" ref="C3:C33" si="2">B3-A3</f>
+        <f t="shared" ref="C3:C33" si="0">B3-A3</f>
         <v>66.150000000000034</v>
       </c>
       <c r="D3" s="44" t="s">
@@ -8068,22 +8071,25 @@
       <c r="CF3" s="5">
         <v>305.25</v>
       </c>
-      <c r="CG3" s="5"/>
-      <c r="CH3" s="5"/>
-      <c r="CI3" s="5"/>
-    </row>
-    <row r="4" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG3" s="5">
+        <v>302.5</v>
+      </c>
+      <c r="CH3" s="5">
+        <v>310.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
+        <f>MIN(E4:ZQ4)</f>
+        <v>251.25</v>
+      </c>
+      <c r="B4" s="12">
+        <f>MAX(E4:ZQ4)</f>
+        <v>291.7</v>
+      </c>
+      <c r="C4" s="12">
         <f t="shared" si="0"/>
-        <v>253.85</v>
-      </c>
-      <c r="B4" s="12">
-        <f t="shared" si="1"/>
-        <v>291.7</v>
-      </c>
-      <c r="C4" s="12">
-        <f t="shared" si="2"/>
-        <v>37.849999999999994</v>
+        <v>40.449999999999989</v>
       </c>
       <c r="D4" s="44" t="s">
         <v>25</v>
@@ -8326,21 +8332,24 @@
       <c r="CF4" s="5">
         <v>254.2</v>
       </c>
-      <c r="CG4" s="5"/>
-      <c r="CH4" s="5"/>
-      <c r="CI4" s="5"/>
-    </row>
-    <row r="5" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG4" s="5">
+        <v>251.25</v>
+      </c>
+      <c r="CH4" s="5">
+        <v>258.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
+        <f>MIN(E5:ZQ5)</f>
+        <v>786.25</v>
+      </c>
+      <c r="B5" s="12">
+        <f>MAX(E5:ZQ5)</f>
+        <v>951.25</v>
+      </c>
+      <c r="C5" s="12">
         <f t="shared" si="0"/>
-        <v>786.25</v>
-      </c>
-      <c r="B5" s="12">
-        <f t="shared" si="1"/>
-        <v>951.25</v>
-      </c>
-      <c r="C5" s="12">
-        <f t="shared" si="2"/>
         <v>165</v>
       </c>
       <c r="D5" s="44" t="s">
@@ -8584,21 +8593,24 @@
       <c r="CF5" s="5">
         <v>910.75</v>
       </c>
-      <c r="CG5" s="5"/>
-      <c r="CH5" s="5"/>
-      <c r="CI5" s="5"/>
-    </row>
-    <row r="6" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG5" s="5">
+        <v>920.7</v>
+      </c>
+      <c r="CH5" s="5">
+        <v>923.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
+        <f>MIN(E6:ZQ6)</f>
+        <v>236.45</v>
+      </c>
+      <c r="B6" s="12">
+        <f>MAX(E6:ZQ6)</f>
+        <v>293.95</v>
+      </c>
+      <c r="C6" s="12">
         <f t="shared" si="0"/>
-        <v>236.45</v>
-      </c>
-      <c r="B6" s="12">
-        <f t="shared" si="1"/>
-        <v>293.95</v>
-      </c>
-      <c r="C6" s="12">
-        <f t="shared" si="2"/>
         <v>57.5</v>
       </c>
       <c r="D6" s="45" t="s">
@@ -8842,21 +8854,24 @@
       <c r="CF6" s="5">
         <v>264.60000000000002</v>
       </c>
-      <c r="CG6" s="5"/>
-      <c r="CH6" s="5"/>
-      <c r="CI6" s="5"/>
-    </row>
-    <row r="7" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG6" s="5">
+        <v>265.2</v>
+      </c>
+      <c r="CH6" s="5">
+        <v>264.10000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
+        <f>MIN(E7:ZQ7)</f>
+        <v>15.6</v>
+      </c>
+      <c r="B7" s="12">
+        <f>MAX(E7:ZQ7)</f>
+        <v>19.350000000000001</v>
+      </c>
+      <c r="C7" s="12">
         <f t="shared" si="0"/>
-        <v>15.6</v>
-      </c>
-      <c r="B7" s="12">
-        <f t="shared" si="1"/>
-        <v>19.350000000000001</v>
-      </c>
-      <c r="C7" s="12">
-        <f t="shared" si="2"/>
         <v>3.7500000000000018</v>
       </c>
       <c r="D7" s="45" t="s">
@@ -9100,21 +9115,24 @@
       <c r="CF7" s="5">
         <v>17.100000000000001</v>
       </c>
-      <c r="CG7" s="5"/>
-      <c r="CH7" s="5"/>
-      <c r="CI7" s="5"/>
-    </row>
-    <row r="8" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG7" s="5">
+        <v>17.149999999999999</v>
+      </c>
+      <c r="CH7" s="5">
+        <v>17.55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
+        <f>MIN(E8:ZQ8)</f>
+        <v>53.4</v>
+      </c>
+      <c r="B8" s="12">
+        <f>MAX(E8:ZQ8)</f>
+        <v>86.75</v>
+      </c>
+      <c r="C8" s="12">
         <f t="shared" si="0"/>
-        <v>53.4</v>
-      </c>
-      <c r="B8" s="12">
-        <f t="shared" si="1"/>
-        <v>86.75</v>
-      </c>
-      <c r="C8" s="12">
-        <f t="shared" si="2"/>
         <v>33.35</v>
       </c>
       <c r="D8" s="45" t="s">
@@ -9358,21 +9376,24 @@
       <c r="CF8" s="5">
         <v>78</v>
       </c>
-      <c r="CG8" s="5"/>
-      <c r="CH8" s="5"/>
-      <c r="CI8" s="5"/>
-    </row>
-    <row r="9" spans="1:87" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="CG8" s="5">
+        <v>76.650000000000006</v>
+      </c>
+      <c r="CH8" s="5">
+        <v>81.95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:86" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
+        <f>MIN(E9:ZQ9)</f>
+        <v>53.5</v>
+      </c>
+      <c r="B9" s="39">
+        <f>MAX(E9:ZQ9)</f>
+        <v>61</v>
+      </c>
+      <c r="C9" s="12">
         <f t="shared" si="0"/>
-        <v>53.5</v>
-      </c>
-      <c r="B9" s="39">
-        <f t="shared" si="1"/>
-        <v>61</v>
-      </c>
-      <c r="C9" s="12">
-        <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
       <c r="D9" s="43" t="s">
@@ -9608,21 +9629,24 @@
       <c r="CF9" s="28">
         <v>54.1</v>
       </c>
-      <c r="CG9" s="28"/>
-      <c r="CH9" s="28"/>
-      <c r="CI9" s="28"/>
-    </row>
-    <row r="10" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG9" s="28">
+        <v>53.5</v>
+      </c>
+      <c r="CH9" s="28">
+        <v>53.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
+        <f>MIN(E10:ZQ10)</f>
+        <v>35.549999999999997</v>
+      </c>
+      <c r="B10" s="12">
+        <f>MAX(E10:ZQ10)</f>
+        <v>45.35</v>
+      </c>
+      <c r="C10" s="12">
         <f t="shared" si="0"/>
-        <v>35.549999999999997</v>
-      </c>
-      <c r="B10" s="12">
-        <f t="shared" si="1"/>
-        <v>45.35</v>
-      </c>
-      <c r="C10" s="12">
-        <f t="shared" si="2"/>
         <v>9.8000000000000043</v>
       </c>
       <c r="D10" s="45" t="s">
@@ -9866,21 +9890,24 @@
       <c r="CF10" s="5">
         <v>36.450000000000003</v>
       </c>
-      <c r="CG10" s="5"/>
-      <c r="CH10" s="5"/>
-      <c r="CI10" s="5"/>
-    </row>
-    <row r="11" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG10" s="5">
+        <v>36.6</v>
+      </c>
+      <c r="CH10" s="5">
+        <v>37.049999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
+        <f>MIN(E11:ZQ11)</f>
+        <v>72.650000000000006</v>
+      </c>
+      <c r="B11" s="12">
+        <f>MAX(E11:ZQ11)</f>
+        <v>106.5</v>
+      </c>
+      <c r="C11" s="12">
         <f t="shared" si="0"/>
-        <v>72.650000000000006</v>
-      </c>
-      <c r="B11" s="12">
-        <f t="shared" si="1"/>
-        <v>106.5</v>
-      </c>
-      <c r="C11" s="12">
-        <f t="shared" si="2"/>
         <v>33.849999999999994</v>
       </c>
       <c r="D11" s="45" t="s">
@@ -10124,21 +10151,24 @@
       <c r="CF11" s="5">
         <v>92.85</v>
       </c>
-      <c r="CG11" s="5"/>
-      <c r="CH11" s="5"/>
-      <c r="CI11" s="5"/>
-    </row>
-    <row r="12" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG11" s="5">
+        <v>93.25</v>
+      </c>
+      <c r="CH11" s="5">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
+        <f>MIN(E12:ZQ12)</f>
+        <v>82.65</v>
+      </c>
+      <c r="B12" s="12">
+        <f>MAX(E12:ZQ12)</f>
+        <v>99.6</v>
+      </c>
+      <c r="C12" s="12">
         <f t="shared" si="0"/>
-        <v>82.65</v>
-      </c>
-      <c r="B12" s="12">
-        <f t="shared" si="1"/>
-        <v>99.6</v>
-      </c>
-      <c r="C12" s="12">
-        <f t="shared" si="2"/>
         <v>16.949999999999989</v>
       </c>
       <c r="D12" s="45" t="s">
@@ -10382,21 +10412,24 @@
       <c r="CF12" s="5">
         <v>89.6</v>
       </c>
-      <c r="CG12" s="5"/>
-      <c r="CH12" s="5"/>
-      <c r="CI12" s="5"/>
-    </row>
-    <row r="13" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG12" s="5">
+        <v>90.5</v>
+      </c>
+      <c r="CH12" s="5">
+        <v>92.15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
+        <f>MIN(E13:ZQ13)</f>
+        <v>44.1</v>
+      </c>
+      <c r="B13" s="12">
+        <f>MAX(E13:ZQ13)</f>
+        <v>57.15</v>
+      </c>
+      <c r="C13" s="12">
         <f t="shared" si="0"/>
-        <v>44.1</v>
-      </c>
-      <c r="B13" s="12">
-        <f t="shared" si="1"/>
-        <v>57.15</v>
-      </c>
-      <c r="C13" s="12">
-        <f t="shared" si="2"/>
         <v>13.049999999999997</v>
       </c>
       <c r="D13" s="45" t="s">
@@ -10640,22 +10673,25 @@
       <c r="CF13" s="5">
         <v>54.4</v>
       </c>
-      <c r="CG13" s="5"/>
-      <c r="CH13" s="5"/>
-      <c r="CI13" s="5"/>
-    </row>
-    <row r="14" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG13" s="5">
+        <v>53.15</v>
+      </c>
+      <c r="CH13" s="5">
+        <v>53.15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
+        <f>MIN(E14:ZQ14)</f>
+        <v>29.75</v>
+      </c>
+      <c r="B14" s="12">
+        <f>MAX(E14:ZQ14)</f>
+        <v>42.75</v>
+      </c>
+      <c r="C14" s="12">
         <f t="shared" si="0"/>
-        <v>29.75</v>
-      </c>
-      <c r="B14" s="12">
-        <f t="shared" si="1"/>
-        <v>41.9</v>
-      </c>
-      <c r="C14" s="12">
-        <f t="shared" si="2"/>
-        <v>12.149999999999999</v>
+        <v>13</v>
       </c>
       <c r="D14" s="45" t="s">
         <v>21</v>
@@ -10898,22 +10934,25 @@
       <c r="CF14" s="5">
         <v>38.35</v>
       </c>
-      <c r="CG14" s="5"/>
-      <c r="CH14" s="5"/>
-      <c r="CI14" s="5"/>
-    </row>
-    <row r="15" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG14" s="5">
+        <v>42.75</v>
+      </c>
+      <c r="CH14" s="5">
+        <v>42.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
+        <f>MIN(E15:ZQ15)</f>
+        <v>23.5</v>
+      </c>
+      <c r="B15" s="12">
+        <f>MAX(E15:ZQ15)</f>
+        <v>36.4</v>
+      </c>
+      <c r="C15" s="12">
         <f t="shared" si="0"/>
-        <v>23.85</v>
-      </c>
-      <c r="B15" s="12">
-        <f t="shared" si="1"/>
-        <v>36.4</v>
-      </c>
-      <c r="C15" s="12">
-        <f t="shared" si="2"/>
-        <v>12.549999999999997</v>
+        <v>12.899999999999999</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>126</v>
@@ -11148,21 +11187,24 @@
       <c r="CF15" s="5">
         <v>23.85</v>
       </c>
-      <c r="CG15" s="5"/>
-      <c r="CH15" s="5"/>
-      <c r="CI15" s="5"/>
-    </row>
-    <row r="16" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG15" s="5">
+        <v>23.95</v>
+      </c>
+      <c r="CH15" s="5">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
+        <f>MIN(E16:ZQ16)</f>
+        <v>552</v>
+      </c>
+      <c r="B16" s="12">
+        <f>MAX(E16:ZQ16)</f>
+        <v>729.5</v>
+      </c>
+      <c r="C16" s="12">
         <f t="shared" si="0"/>
-        <v>552</v>
-      </c>
-      <c r="B16" s="12">
-        <f t="shared" si="1"/>
-        <v>729.5</v>
-      </c>
-      <c r="C16" s="12">
-        <f t="shared" si="2"/>
         <v>177.5</v>
       </c>
       <c r="D16" s="45" t="s">
@@ -11406,21 +11448,24 @@
       <c r="CF16" s="5">
         <v>679.8</v>
       </c>
-      <c r="CG16" s="5"/>
-      <c r="CH16" s="5"/>
-      <c r="CI16" s="5"/>
-    </row>
-    <row r="17" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG16" s="5">
+        <v>662.95</v>
+      </c>
+      <c r="CH16" s="5">
+        <v>702.85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
+        <f>MIN(E17:ZQ17)</f>
+        <v>433</v>
+      </c>
+      <c r="B17" s="12">
+        <f>MAX(E17:ZQ17)</f>
+        <v>670</v>
+      </c>
+      <c r="C17" s="12">
         <f t="shared" si="0"/>
-        <v>433</v>
-      </c>
-      <c r="B17" s="12">
-        <f t="shared" si="1"/>
-        <v>670</v>
-      </c>
-      <c r="C17" s="12">
-        <f t="shared" si="2"/>
         <v>237</v>
       </c>
       <c r="D17" s="44" t="s">
@@ -11664,21 +11709,24 @@
       <c r="CF17" s="5">
         <v>470.45</v>
       </c>
-      <c r="CG17" s="5"/>
-      <c r="CH17" s="5"/>
-      <c r="CI17" s="5"/>
-    </row>
-    <row r="18" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG17" s="5">
+        <v>474.65</v>
+      </c>
+      <c r="CH17" s="5">
+        <v>484.65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
+        <f>MIN(E18:ZQ18)</f>
+        <v>178.8</v>
+      </c>
+      <c r="B18" s="12">
+        <f>MAX(E18:ZQ18)</f>
+        <v>302.2</v>
+      </c>
+      <c r="C18" s="12">
         <f t="shared" si="0"/>
-        <v>178.8</v>
-      </c>
-      <c r="B18" s="12">
-        <f t="shared" si="1"/>
-        <v>302.2</v>
-      </c>
-      <c r="C18" s="12">
-        <f t="shared" si="2"/>
         <v>123.39999999999998</v>
       </c>
       <c r="D18" s="44" t="s">
@@ -11922,22 +11970,25 @@
       <c r="CF18" s="5">
         <v>260.5</v>
       </c>
-      <c r="CG18" s="5"/>
-      <c r="CH18" s="5"/>
-      <c r="CI18" s="5"/>
-    </row>
-    <row r="19" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG18" s="5">
+        <v>260.64999999999998</v>
+      </c>
+      <c r="CH18" s="5">
+        <v>261.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
+        <f>MIN(E19:ZQ19)</f>
+        <v>440.7</v>
+      </c>
+      <c r="B19" s="12">
+        <f>MAX(E19:ZQ19)</f>
+        <v>759</v>
+      </c>
+      <c r="C19" s="12">
         <f t="shared" si="0"/>
-        <v>440.7</v>
-      </c>
-      <c r="B19" s="12">
-        <f t="shared" si="1"/>
-        <v>749.15</v>
-      </c>
-      <c r="C19" s="12">
-        <f t="shared" si="2"/>
-        <v>308.45</v>
+        <v>318.3</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -12180,22 +12231,25 @@
       <c r="CF19" s="5">
         <v>749.15</v>
       </c>
-      <c r="CG19" s="5"/>
-      <c r="CH19" s="5"/>
-      <c r="CI19" s="5"/>
-    </row>
-    <row r="20" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG19" s="5">
+        <v>733.1</v>
+      </c>
+      <c r="CH19" s="5">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="20" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
+        <f>MIN(E20:ZQ20)</f>
+        <v>660.75</v>
+      </c>
+      <c r="B20" s="12">
+        <f>MAX(E20:ZQ20)</f>
+        <v>795.95</v>
+      </c>
+      <c r="C20" s="12">
         <f t="shared" si="0"/>
-        <v>669.9</v>
-      </c>
-      <c r="B20" s="12">
-        <f t="shared" si="1"/>
-        <v>795.95</v>
-      </c>
-      <c r="C20" s="12">
-        <f t="shared" si="2"/>
-        <v>126.05000000000007</v>
+        <v>135.20000000000005</v>
       </c>
       <c r="D20" s="44" t="s">
         <v>104</v>
@@ -12438,21 +12492,24 @@
       <c r="CF20" s="5">
         <v>669.9</v>
       </c>
-      <c r="CG20" s="5"/>
-      <c r="CH20" s="5"/>
-      <c r="CI20" s="5"/>
-    </row>
-    <row r="21" spans="1:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CG20" s="5">
+        <v>660.75</v>
+      </c>
+      <c r="CH20" s="5">
+        <v>674.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
+        <f>MIN(E21:ZQ21)</f>
+        <v>376.7</v>
+      </c>
+      <c r="B21" s="12">
+        <f>MAX(E21:ZQ21)</f>
+        <v>547.5</v>
+      </c>
+      <c r="C21" s="12">
         <f t="shared" si="0"/>
-        <v>376.7</v>
-      </c>
-      <c r="B21" s="12">
-        <f t="shared" si="1"/>
-        <v>547.5</v>
-      </c>
-      <c r="C21" s="12">
-        <f t="shared" si="2"/>
         <v>170.8</v>
       </c>
       <c r="D21" s="44" t="s">
@@ -12696,21 +12753,24 @@
       <c r="CF21" s="5">
         <v>488.2</v>
       </c>
-      <c r="CG21" s="5"/>
-      <c r="CH21" s="5"/>
-      <c r="CI21" s="5"/>
-    </row>
-    <row r="22" spans="1:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CG21" s="5">
+        <v>485.4</v>
+      </c>
+      <c r="CH21" s="5">
+        <v>525.79999999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
+        <f>MIN(E22:ZQ22)</f>
+        <v>315.2</v>
+      </c>
+      <c r="B22" s="12">
+        <f>MAX(E22:ZQ22)</f>
+        <v>413.5</v>
+      </c>
+      <c r="C22" s="12">
         <f t="shared" si="0"/>
-        <v>315.2</v>
-      </c>
-      <c r="B22" s="12">
-        <f t="shared" si="1"/>
-        <v>413.5</v>
-      </c>
-      <c r="C22" s="12">
-        <f t="shared" si="2"/>
         <v>98.300000000000011</v>
       </c>
       <c r="D22" s="44" t="s">
@@ -12900,21 +12960,24 @@
       <c r="CF22" s="5">
         <v>371.3</v>
       </c>
-      <c r="CG22" s="5"/>
-      <c r="CH22" s="5"/>
-      <c r="CI22" s="5"/>
-    </row>
-    <row r="23" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG22" s="5">
+        <v>371.2</v>
+      </c>
+      <c r="CH22" s="5">
+        <v>382.95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
+        <f>MIN(E23:ZQ23)</f>
+        <v>54.45</v>
+      </c>
+      <c r="B23" s="12">
+        <f>MAX(E23:ZQ23)</f>
+        <v>85.65</v>
+      </c>
+      <c r="C23" s="12">
         <f t="shared" si="0"/>
-        <v>54.45</v>
-      </c>
-      <c r="B23" s="12">
-        <f t="shared" si="1"/>
-        <v>85.65</v>
-      </c>
-      <c r="C23" s="12">
-        <f t="shared" si="2"/>
         <v>31.200000000000003</v>
       </c>
       <c r="D23" s="45" t="s">
@@ -13150,21 +13213,24 @@
       <c r="CF23" s="5">
         <v>58.45</v>
       </c>
-      <c r="CG23" s="5"/>
-      <c r="CH23" s="5"/>
-      <c r="CI23" s="5"/>
-    </row>
-    <row r="24" spans="1:87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CG23" s="5">
+        <v>57</v>
+      </c>
+      <c r="CH23" s="5">
+        <v>57.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:86" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
+        <f>MIN(E24:ZQ24)</f>
+        <v>210.65</v>
+      </c>
+      <c r="B24" s="12">
+        <f>MAX(E24:ZQ24)</f>
+        <v>257.39999999999998</v>
+      </c>
+      <c r="C24" s="12">
         <f t="shared" si="0"/>
-        <v>210.65</v>
-      </c>
-      <c r="B24" s="12">
-        <f t="shared" si="1"/>
-        <v>257.39999999999998</v>
-      </c>
-      <c r="C24" s="12">
-        <f t="shared" si="2"/>
         <v>46.749999999999972</v>
       </c>
       <c r="D24" s="45" t="s">
@@ -13396,21 +13462,24 @@
       <c r="CF24" s="5">
         <v>228.95</v>
       </c>
-      <c r="CG24" s="5"/>
-      <c r="CH24" s="5"/>
-      <c r="CI24" s="5"/>
-    </row>
-    <row r="25" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG24" s="5">
+        <v>227.25</v>
+      </c>
+      <c r="CH24" s="5">
+        <v>233.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
+        <f>MIN(E25:ZQ25)</f>
+        <v>876</v>
+      </c>
+      <c r="B25" s="12">
+        <f>MAX(E25:ZQ25)</f>
+        <v>1008</v>
+      </c>
+      <c r="C25" s="12">
         <f t="shared" si="0"/>
-        <v>876</v>
-      </c>
-      <c r="B25" s="12">
-        <f t="shared" si="1"/>
-        <v>1008</v>
-      </c>
-      <c r="C25" s="12">
-        <f t="shared" si="2"/>
         <v>132</v>
       </c>
       <c r="D25" s="46" t="s">
@@ -13624,22 +13693,25 @@
       <c r="CF25" s="5">
         <v>996.7</v>
       </c>
-      <c r="CG25" s="5"/>
-      <c r="CH25" s="5"/>
-      <c r="CI25" s="5"/>
-    </row>
-    <row r="26" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG25" s="5">
+        <v>986.15</v>
+      </c>
+      <c r="CH25" s="5">
+        <v>1001.45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
+        <f>MIN(E26:ZQ26)</f>
+        <v>83.1</v>
+      </c>
+      <c r="B26" s="12">
+        <f>MAX(E26:ZQ26)</f>
+        <v>107.4</v>
+      </c>
+      <c r="C26" s="12">
         <f t="shared" si="0"/>
-        <v>83.1</v>
-      </c>
-      <c r="B26" s="12">
-        <f t="shared" si="1"/>
-        <v>102.25</v>
-      </c>
-      <c r="C26" s="12">
-        <f t="shared" si="2"/>
-        <v>19.150000000000006</v>
+        <v>24.300000000000011</v>
       </c>
       <c r="D26" s="45" t="s">
         <v>252</v>
@@ -13840,21 +13912,24 @@
       <c r="CF26" s="5">
         <v>98.4</v>
       </c>
-      <c r="CG26" s="5"/>
-      <c r="CH26" s="5"/>
-      <c r="CI26" s="5"/>
-    </row>
-    <row r="27" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG26" s="5">
+        <v>106</v>
+      </c>
+      <c r="CH26" s="5">
+        <v>107.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
+        <f>MIN(E27:ZQ27)</f>
+        <v>36.200000000000003</v>
+      </c>
+      <c r="B27" s="12">
+        <f>MAX(E27:ZQ27)</f>
+        <v>44.75</v>
+      </c>
+      <c r="C27" s="12">
         <f t="shared" si="0"/>
-        <v>36.200000000000003</v>
-      </c>
-      <c r="B27" s="12">
-        <f t="shared" si="1"/>
-        <v>44.75</v>
-      </c>
-      <c r="C27" s="12">
-        <f t="shared" si="2"/>
         <v>8.5499999999999972</v>
       </c>
       <c r="D27" s="45" t="s">
@@ -14056,21 +14131,24 @@
       <c r="CF27" s="5">
         <v>39</v>
       </c>
-      <c r="CG27" s="5"/>
-      <c r="CH27" s="5"/>
-      <c r="CI27" s="5"/>
-    </row>
-    <row r="28" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG27" s="5">
+        <v>39.450000000000003</v>
+      </c>
+      <c r="CH27" s="5">
+        <v>39.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
+        <f>MIN(E28:ZQ28)</f>
+        <v>111.95</v>
+      </c>
+      <c r="B28" s="12">
+        <f>MAX(E28:ZQ28)</f>
+        <v>141.65</v>
+      </c>
+      <c r="C28" s="12">
         <f t="shared" si="0"/>
-        <v>111.95</v>
-      </c>
-      <c r="B28" s="12">
-        <f t="shared" si="1"/>
-        <v>141.65</v>
-      </c>
-      <c r="C28" s="12">
-        <f t="shared" si="2"/>
         <v>29.700000000000003</v>
       </c>
       <c r="D28" s="45" t="s">
@@ -14272,21 +14350,24 @@
       <c r="CF28" s="5">
         <v>124.15</v>
       </c>
-      <c r="CG28" s="5"/>
-      <c r="CH28" s="5"/>
-      <c r="CI28" s="5"/>
-    </row>
-    <row r="29" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG28" s="5">
+        <v>124.95</v>
+      </c>
+      <c r="CH28" s="5">
+        <v>126.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
+        <f>MIN(E29:ZQ29)</f>
+        <v>62.3</v>
+      </c>
+      <c r="B29" s="12">
+        <f>MAX(E29:ZQ29)</f>
+        <v>78.849999999999994</v>
+      </c>
+      <c r="C29" s="12">
         <f t="shared" si="0"/>
-        <v>62.3</v>
-      </c>
-      <c r="B29" s="12">
-        <f t="shared" si="1"/>
-        <v>78.849999999999994</v>
-      </c>
-      <c r="C29" s="12">
-        <f t="shared" si="2"/>
         <v>16.549999999999997</v>
       </c>
       <c r="D29" s="45" t="s">
@@ -14488,21 +14569,24 @@
       <c r="CF29" s="5">
         <v>66.8</v>
       </c>
-      <c r="CG29" s="5"/>
-      <c r="CH29" s="5"/>
-      <c r="CI29" s="5"/>
-    </row>
-    <row r="30" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG29" s="5">
+        <v>68</v>
+      </c>
+      <c r="CH29" s="5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
+        <f>MIN(E30:ZQ30)</f>
+        <v>36.950000000000003</v>
+      </c>
+      <c r="B30" s="12">
+        <f>MAX(E30:ZQ30)</f>
+        <v>50.95</v>
+      </c>
+      <c r="C30" s="12">
         <f t="shared" si="0"/>
-        <v>36.950000000000003</v>
-      </c>
-      <c r="B30" s="12">
-        <f t="shared" si="1"/>
-        <v>50.95</v>
-      </c>
-      <c r="C30" s="12">
-        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="D30" s="45" t="s">
@@ -14704,21 +14788,24 @@
       <c r="CF30" s="5">
         <v>37.299999999999997</v>
       </c>
-      <c r="CG30" s="5"/>
-      <c r="CH30" s="5"/>
-      <c r="CI30" s="5"/>
-    </row>
-    <row r="31" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG30" s="5">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="CH30" s="5">
+        <v>37.950000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
+        <f>MIN(E31:ZQ31)</f>
+        <v>125.3</v>
+      </c>
+      <c r="B31" s="12">
+        <f>MAX(E31:ZQ31)</f>
+        <v>156.85</v>
+      </c>
+      <c r="C31" s="12">
         <f t="shared" si="0"/>
-        <v>125.3</v>
-      </c>
-      <c r="B31" s="12">
-        <f t="shared" si="1"/>
-        <v>156.85</v>
-      </c>
-      <c r="C31" s="12">
-        <f t="shared" si="2"/>
         <v>31.549999999999997</v>
       </c>
       <c r="D31" s="45" t="s">
@@ -14920,21 +15007,24 @@
       <c r="CF31" s="5">
         <v>146.55000000000001</v>
       </c>
-      <c r="CG31" s="5"/>
-      <c r="CH31" s="5"/>
-      <c r="CI31" s="5"/>
-    </row>
-    <row r="32" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG31" s="5">
+        <v>146.1</v>
+      </c>
+      <c r="CH31" s="5">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
+        <f>MIN(E32:ZQ32)</f>
+        <v>96.65</v>
+      </c>
+      <c r="B32" s="12">
+        <f>MAX(E32:ZQ32)</f>
+        <v>121.8</v>
+      </c>
+      <c r="C32" s="12">
         <f t="shared" si="0"/>
-        <v>96.65</v>
-      </c>
-      <c r="B32" s="12">
-        <f t="shared" si="1"/>
-        <v>121.8</v>
-      </c>
-      <c r="C32" s="12">
-        <f t="shared" si="2"/>
         <v>25.149999999999991</v>
       </c>
       <c r="D32" s="45" t="s">
@@ -15124,21 +15214,24 @@
       <c r="CF32" s="5">
         <v>98.9</v>
       </c>
-      <c r="CG32" s="5"/>
-      <c r="CH32" s="5"/>
-      <c r="CI32" s="5"/>
-    </row>
-    <row r="33" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG32" s="5">
+        <v>98.55</v>
+      </c>
+      <c r="CH32" s="5">
+        <v>100.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
+        <f>MIN(E33:ZQ33)</f>
+        <v>56.75</v>
+      </c>
+      <c r="B33" s="12">
+        <f>MAX(E33:ZQ33)</f>
+        <v>67.099999999999994</v>
+      </c>
+      <c r="C33" s="12">
         <f t="shared" si="0"/>
-        <v>56.75</v>
-      </c>
-      <c r="B33" s="12">
-        <f t="shared" si="1"/>
-        <v>67.099999999999994</v>
-      </c>
-      <c r="C33" s="12">
-        <f t="shared" si="2"/>
         <v>10.349999999999994</v>
       </c>
       <c r="D33" s="45" t="s">
@@ -15316,21 +15409,24 @@
       <c r="CF33" s="5">
         <v>57.85</v>
       </c>
-      <c r="CG33" s="5"/>
-      <c r="CH33" s="5"/>
-      <c r="CI33" s="5"/>
-    </row>
-    <row r="34" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG33" s="5">
+        <v>58.25</v>
+      </c>
+      <c r="CH33" s="5">
+        <v>66.099999999999994</v>
+      </c>
+    </row>
+    <row r="34" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E34:ZQ34)</f>
         <v>167.9</v>
       </c>
       <c r="B34" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E34:ZQ34)</f>
         <v>236.1</v>
       </c>
       <c r="C34" s="12">
-        <f t="shared" ref="C34" si="3">B34-A34</f>
+        <f t="shared" ref="C34" si="1">B34-A34</f>
         <v>68.199999999999989</v>
       </c>
       <c r="D34" s="45" t="s">
@@ -15502,22 +15598,25 @@
       <c r="CF34" s="5">
         <v>203.15</v>
       </c>
-      <c r="CG34" s="5"/>
-      <c r="CH34" s="5"/>
-      <c r="CI34" s="5"/>
-    </row>
-    <row r="35" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG34" s="5">
+        <v>203</v>
+      </c>
+      <c r="CH34" s="5">
+        <v>232.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
-        <f t="shared" si="0"/>
-        <v>400</v>
+        <f>MIN(E35:ZQ35)</f>
+        <v>392.1</v>
       </c>
       <c r="B35" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E35:ZQ35)</f>
         <v>520</v>
       </c>
       <c r="C35" s="12">
-        <f t="shared" ref="C35" si="4">B35-A35</f>
-        <v>120</v>
+        <f t="shared" ref="C35" si="2">B35-A35</f>
+        <v>127.89999999999998</v>
       </c>
       <c r="D35" s="45" t="s">
         <v>289</v>
@@ -15666,21 +15765,24 @@
       <c r="CF35" s="5">
         <v>400</v>
       </c>
-      <c r="CG35" s="5"/>
-      <c r="CH35" s="5"/>
-      <c r="CI35" s="5"/>
-    </row>
-    <row r="36" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG35" s="5">
+        <v>392.1</v>
+      </c>
+      <c r="CH35" s="5">
+        <v>417.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E36:ZQ36)</f>
         <v>226</v>
       </c>
       <c r="B36" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E36:ZQ36)</f>
         <v>396.85</v>
       </c>
       <c r="C36" s="12">
-        <f t="shared" ref="C36" si="5">B36-A36</f>
+        <f t="shared" ref="C36" si="3">B36-A36</f>
         <v>170.85000000000002</v>
       </c>
       <c r="D36" s="45" t="s">
@@ -15820,21 +15922,24 @@
       <c r="CF36" s="5">
         <v>347.55</v>
       </c>
-      <c r="CG36" s="5"/>
-      <c r="CH36" s="5"/>
-      <c r="CI36" s="5"/>
-    </row>
-    <row r="37" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG36" s="5">
+        <v>353</v>
+      </c>
+      <c r="CH36" s="5">
+        <v>383.7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E37:ZQ37)</f>
         <v>75.2</v>
       </c>
       <c r="B37" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E37:ZQ37)</f>
         <v>83.85</v>
       </c>
       <c r="C37" s="12">
-        <f t="shared" ref="C37" si="6">B37-A37</f>
+        <f t="shared" ref="C37" si="4">B37-A37</f>
         <v>8.6499999999999915</v>
       </c>
       <c r="D37" s="45" t="s">
@@ -15966,22 +16071,25 @@
       <c r="CF37" s="5">
         <v>79.3</v>
       </c>
-      <c r="CG37" s="5"/>
-      <c r="CH37" s="5"/>
-      <c r="CI37" s="5"/>
-    </row>
-    <row r="38" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG37" s="5">
+        <v>82</v>
+      </c>
+      <c r="CH37" s="5">
+        <v>82.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
-        <f t="shared" si="0"/>
-        <v>410.25</v>
+        <f>MIN(E38:ZQ38)</f>
+        <v>407.05</v>
       </c>
       <c r="B38" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E38:ZQ38)</f>
         <v>472</v>
       </c>
       <c r="C38" s="12">
-        <f t="shared" ref="C38" si="7">B38-A38</f>
-        <v>61.75</v>
+        <f t="shared" ref="C38" si="5">B38-A38</f>
+        <v>64.949999999999989</v>
       </c>
       <c r="D38" s="45" t="s">
         <v>304</v>
@@ -16112,21 +16220,24 @@
       <c r="CF38" s="5">
         <v>411.55</v>
       </c>
-      <c r="CG38" s="5"/>
-      <c r="CH38" s="5"/>
-      <c r="CI38" s="5"/>
-    </row>
-    <row r="39" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG38" s="5">
+        <v>407.05</v>
+      </c>
+      <c r="CH38" s="5">
+        <v>409.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E39:ZQ39)</f>
         <v>175.2</v>
       </c>
       <c r="B39" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E39:ZQ39)</f>
         <v>215.25</v>
       </c>
       <c r="C39" s="12">
-        <f t="shared" ref="C39" si="8">B39-A39</f>
+        <f t="shared" ref="C39" si="6">B39-A39</f>
         <v>40.050000000000011</v>
       </c>
       <c r="D39" s="45" t="s">
@@ -16254,21 +16365,24 @@
       <c r="CF39" s="5">
         <v>186.3</v>
       </c>
-      <c r="CG39" s="5"/>
-      <c r="CH39" s="5"/>
-      <c r="CI39" s="5"/>
-    </row>
-    <row r="40" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG39" s="5">
+        <v>190</v>
+      </c>
+      <c r="CH39" s="5">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="40" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E40:ZQ40)</f>
         <v>35</v>
       </c>
       <c r="B40" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E40:ZQ40)</f>
         <v>39.450000000000003</v>
       </c>
       <c r="C40" s="12">
-        <f t="shared" ref="C40:C43" si="9">B40-A40</f>
+        <f t="shared" ref="C40:C43" si="7">B40-A40</f>
         <v>4.4500000000000028</v>
       </c>
       <c r="D40" s="45" t="s">
@@ -16392,22 +16506,25 @@
       <c r="CF40" s="5">
         <v>36.15</v>
       </c>
-      <c r="CG40" s="5"/>
-      <c r="CH40" s="5"/>
-      <c r="CI40" s="5"/>
-    </row>
-    <row r="41" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG40" s="5">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="CH40" s="5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E41:ZQ41)</f>
         <v>552.04999999999995</v>
       </c>
       <c r="B41" s="12">
-        <f t="shared" si="1"/>
-        <v>626.70000000000005</v>
+        <f>MAX(E41:ZQ41)</f>
+        <v>665.45</v>
       </c>
       <c r="C41" s="12">
-        <f t="shared" si="9"/>
-        <v>74.650000000000091</v>
+        <f t="shared" si="7"/>
+        <v>113.40000000000009</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>307</v>
@@ -16528,22 +16645,25 @@
       <c r="CF41" s="5">
         <v>568.20000000000005</v>
       </c>
-      <c r="CG41" s="5"/>
-      <c r="CH41" s="5"/>
-      <c r="CI41" s="5"/>
-    </row>
-    <row r="42" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG41" s="5">
+        <v>595.25</v>
+      </c>
+      <c r="CH41" s="5">
+        <v>665.45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
-        <f t="shared" si="0"/>
-        <v>811.25</v>
+        <f>MIN(E42:ZQ42)</f>
+        <v>810.6</v>
       </c>
       <c r="B42" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E42:ZQ42)</f>
         <v>856</v>
       </c>
       <c r="C42" s="12">
-        <f t="shared" si="9"/>
-        <v>44.75</v>
+        <f t="shared" si="7"/>
+        <v>45.399999999999977</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>308</v>
@@ -16664,21 +16784,24 @@
       <c r="CF42" s="5">
         <v>811.25</v>
       </c>
-      <c r="CG42" s="5"/>
-      <c r="CH42" s="5"/>
-      <c r="CI42" s="5"/>
-    </row>
-    <row r="43" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG42" s="5">
+        <v>810.6</v>
+      </c>
+      <c r="CH42" s="5">
+        <v>821.35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
-        <f t="shared" si="0"/>
+        <f>MIN(E43:ZQ43)</f>
         <v>134.9</v>
       </c>
       <c r="B43" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E43:ZQ43)</f>
         <v>146</v>
       </c>
       <c r="C43" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>11.099999999999994</v>
       </c>
       <c r="D43" s="45" t="s">
@@ -16798,22 +16921,25 @@
       <c r="CF43" s="5">
         <v>135.25</v>
       </c>
-      <c r="CG43" s="5"/>
-      <c r="CH43" s="5"/>
-      <c r="CI43" s="5"/>
-    </row>
-    <row r="44" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG43" s="5">
+        <v>135</v>
+      </c>
+      <c r="CH43" s="5">
+        <v>140.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
-        <f t="shared" si="0"/>
-        <v>597.04999999999995</v>
+        <f>MIN(E44:ZQ44)</f>
+        <v>583.65</v>
       </c>
       <c r="B44" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E44:ZQ44)</f>
         <v>770</v>
       </c>
       <c r="C44" s="12">
-        <f t="shared" ref="C44" si="10">B44-A44</f>
-        <v>172.95000000000005</v>
+        <f t="shared" ref="C44" si="8">B44-A44</f>
+        <v>186.35000000000002</v>
       </c>
       <c r="D44" s="45" t="s">
         <v>311</v>
@@ -16926,22 +17052,25 @@
       <c r="CF44" s="5">
         <v>597.04999999999995</v>
       </c>
-      <c r="CG44" s="5"/>
-      <c r="CH44" s="5"/>
-      <c r="CI44" s="5"/>
-    </row>
-    <row r="45" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG44" s="5">
+        <v>588</v>
+      </c>
+      <c r="CH44" s="5">
+        <v>583.65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
-        <f t="shared" si="0"/>
-        <v>103.1</v>
+        <f>MIN(E45:ZQ45)</f>
+        <v>101.4</v>
       </c>
       <c r="B45" s="12">
-        <f t="shared" si="1"/>
+        <f>MAX(E45:ZQ45)</f>
         <v>110.95</v>
       </c>
       <c r="C45" s="12">
-        <f t="shared" ref="C45" si="11">B45-A45</f>
-        <v>7.8500000000000085</v>
+        <f t="shared" ref="C45" si="9">B45-A45</f>
+        <v>9.5499999999999972</v>
       </c>
       <c r="D45" s="45" t="s">
         <v>323</v>
@@ -17046,22 +17175,25 @@
       <c r="CF45" s="5">
         <v>103.1</v>
       </c>
-      <c r="CG45" s="5"/>
-      <c r="CH45" s="5"/>
-      <c r="CI45" s="5"/>
-    </row>
-    <row r="46" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CG45" s="5">
+        <v>101.4</v>
+      </c>
+      <c r="CH45" s="5">
+        <v>110.6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
-        <f t="shared" ref="A46" si="12">MIN(E46:ZR46)</f>
-        <v>139</v>
+        <f>MIN(E46:ZQ46)</f>
+        <v>137.65</v>
       </c>
       <c r="B46" s="12">
-        <f t="shared" ref="B46" si="13">MAX(E46:ZR46)</f>
+        <f>MAX(E46:ZQ46)</f>
         <v>145</v>
       </c>
       <c r="C46" s="12">
-        <f t="shared" ref="C46" si="14">B46-A46</f>
-        <v>6</v>
+        <f t="shared" ref="C46" si="10">B46-A46</f>
+        <v>7.3499999999999943</v>
       </c>
       <c r="D46" s="45" t="s">
         <v>324</v>
@@ -17152,9 +17284,12 @@
       <c r="CF46" s="5">
         <v>139.30000000000001</v>
       </c>
-      <c r="CG46" s="5"/>
-      <c r="CH46" s="5"/>
-      <c r="CI46" s="5"/>
+      <c r="CG46" s="5">
+        <v>139.4</v>
+      </c>
+      <c r="CH46" s="5">
+        <v>137.65</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="L1:L37">
@@ -18379,10 +18514,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:C47"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18427,7 +18562,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(B2:B200)</f>
-        <v>1158793</v>
+        <v>1258793</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -18445,7 +18580,7 @@
       </c>
       <c r="F3" s="5">
         <f>F1-F2</f>
-        <v>316596</v>
+        <v>216596</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -19100,6 +19235,17 @@
       </c>
       <c r="C47" s="31">
         <v>43070</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="53" t="s">
+        <v>325</v>
+      </c>
+      <c r="B48" s="26">
+        <v>100000</v>
+      </c>
+      <c r="C48" s="52">
+        <v>43074</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added details for 13/12/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="327">
   <si>
     <t>Date</t>
   </si>
@@ -1003,6 +1003,9 @@
   </si>
   <si>
     <t>Batra</t>
+  </si>
+  <si>
+    <t>13/12/2017</t>
   </si>
 </sst>
 </file>
@@ -1174,7 +1177,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1249,6 +1252,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -7248,11 +7252,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CH46"/>
+  <dimension ref="A1:CI46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="CA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CH2" sqref="CH2:CH46"/>
+      <selection pane="topRight" activeCell="CI2" sqref="CI2:CI46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7306,9 +7310,10 @@
     <col min="83" max="83" width="13" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="13" customWidth="1"/>
     <col min="85" max="86" width="13" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:87" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>249</v>
       </c>
@@ -7567,14 +7572,17 @@
       <c r="CH1" s="51">
         <v>42959</v>
       </c>
-    </row>
-    <row r="2" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI1" s="56" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
-        <f>MIN(E2:ZQ2)</f>
+        <f t="shared" ref="A2:A46" si="0">MIN(E2:ZQ2)</f>
         <v>243.6</v>
       </c>
       <c r="B2" s="12">
-        <f>MAX(E2:ZQ2)</f>
+        <f t="shared" ref="B2:B46" si="1">MAX(E2:ZQ2)</f>
         <v>340.8</v>
       </c>
       <c r="C2" s="12">
@@ -7822,18 +7830,21 @@
       <c r="CH2" s="5">
         <v>313.75</v>
       </c>
-    </row>
-    <row r="3" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI2">
+        <v>313.35000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
-        <f>MIN(E3:ZQ3)</f>
+        <f t="shared" si="0"/>
         <v>262.7</v>
       </c>
       <c r="B3" s="12">
-        <f>MAX(E3:ZQ3)</f>
+        <f t="shared" si="1"/>
         <v>328.85</v>
       </c>
       <c r="C3" s="12">
-        <f t="shared" ref="C3:C33" si="0">B3-A3</f>
+        <f t="shared" ref="C3:C33" si="2">B3-A3</f>
         <v>66.150000000000034</v>
       </c>
       <c r="D3" s="44" t="s">
@@ -8077,18 +8088,21 @@
       <c r="CH3" s="5">
         <v>310.95</v>
       </c>
-    </row>
-    <row r="4" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI3">
+        <v>304.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
-        <f>MIN(E4:ZQ4)</f>
+        <f t="shared" si="0"/>
         <v>251.25</v>
       </c>
       <c r="B4" s="12">
-        <f>MAX(E4:ZQ4)</f>
+        <f t="shared" si="1"/>
         <v>291.7</v>
       </c>
       <c r="C4" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>40.449999999999989</v>
       </c>
       <c r="D4" s="44" t="s">
@@ -8338,18 +8352,21 @@
       <c r="CH4" s="5">
         <v>258.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI4">
+        <v>259.45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
-        <f>MIN(E5:ZQ5)</f>
+        <f t="shared" si="0"/>
         <v>786.25</v>
       </c>
       <c r="B5" s="12">
-        <f>MAX(E5:ZQ5)</f>
+        <f t="shared" si="1"/>
         <v>951.25</v>
       </c>
       <c r="C5" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>165</v>
       </c>
       <c r="D5" s="44" t="s">
@@ -8599,18 +8616,21 @@
       <c r="CH5" s="5">
         <v>923.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI5">
+        <v>914.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
-        <f>MIN(E6:ZQ6)</f>
+        <f t="shared" si="0"/>
         <v>236.45</v>
       </c>
       <c r="B6" s="12">
-        <f>MAX(E6:ZQ6)</f>
+        <f t="shared" si="1"/>
         <v>293.95</v>
       </c>
       <c r="C6" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>57.5</v>
       </c>
       <c r="D6" s="45" t="s">
@@ -8860,18 +8880,21 @@
       <c r="CH6" s="5">
         <v>264.10000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI6">
+        <v>263.10000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
-        <f>MIN(E7:ZQ7)</f>
+        <f t="shared" si="0"/>
         <v>15.6</v>
       </c>
       <c r="B7" s="12">
-        <f>MAX(E7:ZQ7)</f>
+        <f t="shared" si="1"/>
         <v>19.350000000000001</v>
       </c>
       <c r="C7" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.7500000000000018</v>
       </c>
       <c r="D7" s="45" t="s">
@@ -9121,18 +9144,21 @@
       <c r="CH7" s="5">
         <v>17.55</v>
       </c>
-    </row>
-    <row r="8" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
-        <f>MIN(E8:ZQ8)</f>
+        <f t="shared" si="0"/>
         <v>53.4</v>
       </c>
       <c r="B8" s="12">
-        <f>MAX(E8:ZQ8)</f>
+        <f t="shared" si="1"/>
         <v>86.75</v>
       </c>
       <c r="C8" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>33.35</v>
       </c>
       <c r="D8" s="45" t="s">
@@ -9382,19 +9408,22 @@
       <c r="CH8" s="5">
         <v>81.95</v>
       </c>
-    </row>
-    <row r="9" spans="1:86" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="CI8">
+        <v>78.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:87" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
-        <f>MIN(E9:ZQ9)</f>
-        <v>53.5</v>
+        <f t="shared" si="0"/>
+        <v>52.35</v>
       </c>
       <c r="B9" s="39">
-        <f>MAX(E9:ZQ9)</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="C9" s="12">
-        <f t="shared" si="0"/>
-        <v>7.5</v>
+        <f t="shared" si="2"/>
+        <v>8.6499999999999986</v>
       </c>
       <c r="D9" s="43" t="s">
         <v>125</v>
@@ -9635,18 +9664,21 @@
       <c r="CH9" s="28">
         <v>53.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI9" s="37">
+        <v>52.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
-        <f>MIN(E10:ZQ10)</f>
+        <f t="shared" si="0"/>
         <v>35.549999999999997</v>
       </c>
       <c r="B10" s="12">
-        <f>MAX(E10:ZQ10)</f>
+        <f t="shared" si="1"/>
         <v>45.35</v>
       </c>
       <c r="C10" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.8000000000000043</v>
       </c>
       <c r="D10" s="45" t="s">
@@ -9896,18 +9928,21 @@
       <c r="CH10" s="5">
         <v>37.049999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI10">
+        <v>36.15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
-        <f>MIN(E11:ZQ11)</f>
+        <f t="shared" si="0"/>
         <v>72.650000000000006</v>
       </c>
       <c r="B11" s="12">
-        <f>MAX(E11:ZQ11)</f>
+        <f t="shared" si="1"/>
         <v>106.5</v>
       </c>
       <c r="C11" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>33.849999999999994</v>
       </c>
       <c r="D11" s="45" t="s">
@@ -10157,18 +10192,21 @@
       <c r="CH11" s="5">
         <v>97</v>
       </c>
-    </row>
-    <row r="12" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI11">
+        <v>92.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
-        <f>MIN(E12:ZQ12)</f>
+        <f t="shared" si="0"/>
         <v>82.65</v>
       </c>
       <c r="B12" s="12">
-        <f>MAX(E12:ZQ12)</f>
+        <f t="shared" si="1"/>
         <v>99.6</v>
       </c>
       <c r="C12" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16.949999999999989</v>
       </c>
       <c r="D12" s="45" t="s">
@@ -10418,18 +10456,21 @@
       <c r="CH12" s="5">
         <v>92.15</v>
       </c>
-    </row>
-    <row r="13" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI12">
+        <v>89.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
-        <f>MIN(E13:ZQ13)</f>
+        <f t="shared" si="0"/>
         <v>44.1</v>
       </c>
       <c r="B13" s="12">
-        <f>MAX(E13:ZQ13)</f>
+        <f t="shared" si="1"/>
         <v>57.15</v>
       </c>
       <c r="C13" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13.049999999999997</v>
       </c>
       <c r="D13" s="45" t="s">
@@ -10679,18 +10720,21 @@
       <c r="CH13" s="5">
         <v>53.15</v>
       </c>
-    </row>
-    <row r="14" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI13">
+        <v>51.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
-        <f>MIN(E14:ZQ14)</f>
+        <f t="shared" si="0"/>
         <v>29.75</v>
       </c>
       <c r="B14" s="12">
-        <f>MAX(E14:ZQ14)</f>
+        <f t="shared" si="1"/>
         <v>42.75</v>
       </c>
       <c r="C14" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="D14" s="45" t="s">
@@ -10940,19 +10984,22 @@
       <c r="CH14" s="5">
         <v>42.4</v>
       </c>
-    </row>
-    <row r="15" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI14">
+        <v>41.55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
-        <f>MIN(E15:ZQ15)</f>
-        <v>23.5</v>
+        <f t="shared" si="0"/>
+        <v>23.4</v>
       </c>
       <c r="B15" s="12">
-        <f>MAX(E15:ZQ15)</f>
+        <f t="shared" si="1"/>
         <v>36.4</v>
       </c>
       <c r="C15" s="12">
-        <f t="shared" si="0"/>
-        <v>12.899999999999999</v>
+        <f t="shared" si="2"/>
+        <v>13</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>126</v>
@@ -11193,18 +11240,21 @@
       <c r="CH15" s="5">
         <v>23.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI15">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
-        <f>MIN(E16:ZQ16)</f>
+        <f t="shared" si="0"/>
         <v>552</v>
       </c>
       <c r="B16" s="12">
-        <f>MAX(E16:ZQ16)</f>
+        <f t="shared" si="1"/>
         <v>729.5</v>
       </c>
       <c r="C16" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>177.5</v>
       </c>
       <c r="D16" s="45" t="s">
@@ -11454,18 +11504,21 @@
       <c r="CH16" s="5">
         <v>702.85</v>
       </c>
-    </row>
-    <row r="17" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI16">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="17" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
-        <f>MIN(E17:ZQ17)</f>
+        <f t="shared" si="0"/>
         <v>433</v>
       </c>
       <c r="B17" s="12">
-        <f>MAX(E17:ZQ17)</f>
+        <f t="shared" si="1"/>
         <v>670</v>
       </c>
       <c r="C17" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>237</v>
       </c>
       <c r="D17" s="44" t="s">
@@ -11715,18 +11768,21 @@
       <c r="CH17" s="5">
         <v>484.65</v>
       </c>
-    </row>
-    <row r="18" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI17">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="18" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
-        <f>MIN(E18:ZQ18)</f>
+        <f t="shared" si="0"/>
         <v>178.8</v>
       </c>
       <c r="B18" s="12">
-        <f>MAX(E18:ZQ18)</f>
+        <f t="shared" si="1"/>
         <v>302.2</v>
       </c>
       <c r="C18" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>123.39999999999998</v>
       </c>
       <c r="D18" s="44" t="s">
@@ -11976,18 +12032,21 @@
       <c r="CH18" s="5">
         <v>261.75</v>
       </c>
-    </row>
-    <row r="19" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI18">
+        <v>250.15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
-        <f>MIN(E19:ZQ19)</f>
+        <f t="shared" si="0"/>
         <v>440.7</v>
       </c>
       <c r="B19" s="12">
-        <f>MAX(E19:ZQ19)</f>
+        <f t="shared" si="1"/>
         <v>759</v>
       </c>
       <c r="C19" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>318.3</v>
       </c>
       <c r="D19" s="44" t="s">
@@ -12237,18 +12296,21 @@
       <c r="CH19" s="5">
         <v>759</v>
       </c>
-    </row>
-    <row r="20" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI19">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="20" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
-        <f>MIN(E20:ZQ20)</f>
+        <f t="shared" si="0"/>
         <v>660.75</v>
       </c>
       <c r="B20" s="12">
-        <f>MAX(E20:ZQ20)</f>
+        <f t="shared" si="1"/>
         <v>795.95</v>
       </c>
       <c r="C20" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>135.20000000000005</v>
       </c>
       <c r="D20" s="44" t="s">
@@ -12498,18 +12560,21 @@
       <c r="CH20" s="5">
         <v>674.3</v>
       </c>
-    </row>
-    <row r="21" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CI20">
+        <v>670.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
-        <f>MIN(E21:ZQ21)</f>
+        <f t="shared" si="0"/>
         <v>376.7</v>
       </c>
       <c r="B21" s="12">
-        <f>MAX(E21:ZQ21)</f>
+        <f t="shared" si="1"/>
         <v>547.5</v>
       </c>
       <c r="C21" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>170.8</v>
       </c>
       <c r="D21" s="44" t="s">
@@ -12759,18 +12824,21 @@
       <c r="CH21" s="5">
         <v>525.79999999999995</v>
       </c>
-    </row>
-    <row r="22" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CI21">
+        <v>517.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
-        <f>MIN(E22:ZQ22)</f>
+        <f t="shared" si="0"/>
         <v>315.2</v>
       </c>
       <c r="B22" s="12">
-        <f>MAX(E22:ZQ22)</f>
+        <f t="shared" si="1"/>
         <v>413.5</v>
       </c>
       <c r="C22" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>98.300000000000011</v>
       </c>
       <c r="D22" s="44" t="s">
@@ -12966,19 +13034,22 @@
       <c r="CH22" s="5">
         <v>382.95</v>
       </c>
-    </row>
-    <row r="23" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI22">
+        <v>359.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
-        <f>MIN(E23:ZQ23)</f>
-        <v>54.45</v>
+        <f t="shared" si="0"/>
+        <v>52.8</v>
       </c>
       <c r="B23" s="12">
-        <f>MAX(E23:ZQ23)</f>
+        <f t="shared" si="1"/>
         <v>85.65</v>
       </c>
       <c r="C23" s="12">
-        <f t="shared" si="0"/>
-        <v>31.200000000000003</v>
+        <f t="shared" si="2"/>
+        <v>32.850000000000009</v>
       </c>
       <c r="D23" s="45" t="s">
         <v>127</v>
@@ -13219,18 +13290,21 @@
       <c r="CH23" s="5">
         <v>57.25</v>
       </c>
-    </row>
-    <row r="24" spans="1:86" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CI23">
+        <v>52.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
-        <f>MIN(E24:ZQ24)</f>
+        <f t="shared" si="0"/>
         <v>210.65</v>
       </c>
       <c r="B24" s="12">
-        <f>MAX(E24:ZQ24)</f>
+        <f t="shared" si="1"/>
         <v>257.39999999999998</v>
       </c>
       <c r="C24" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>46.749999999999972</v>
       </c>
       <c r="D24" s="45" t="s">
@@ -13468,18 +13542,21 @@
       <c r="CH24" s="5">
         <v>233.4</v>
       </c>
-    </row>
-    <row r="25" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI24">
+        <v>224.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
-        <f>MIN(E25:ZQ25)</f>
+        <f t="shared" si="0"/>
         <v>876</v>
       </c>
       <c r="B25" s="12">
-        <f>MAX(E25:ZQ25)</f>
+        <f t="shared" si="1"/>
         <v>1008</v>
       </c>
       <c r="C25" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>132</v>
       </c>
       <c r="D25" s="46" t="s">
@@ -13699,18 +13776,21 @@
       <c r="CH25" s="5">
         <v>1001.45</v>
       </c>
-    </row>
-    <row r="26" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI25">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
-        <f>MIN(E26:ZQ26)</f>
+        <f t="shared" si="0"/>
         <v>83.1</v>
       </c>
       <c r="B26" s="12">
-        <f>MAX(E26:ZQ26)</f>
+        <f t="shared" si="1"/>
         <v>107.4</v>
       </c>
       <c r="C26" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>24.300000000000011</v>
       </c>
       <c r="D26" s="45" t="s">
@@ -13918,18 +13998,21 @@
       <c r="CH26" s="5">
         <v>107.4</v>
       </c>
-    </row>
-    <row r="27" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI26">
+        <v>106.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
-        <f>MIN(E27:ZQ27)</f>
+        <f t="shared" si="0"/>
         <v>36.200000000000003</v>
       </c>
       <c r="B27" s="12">
-        <f>MAX(E27:ZQ27)</f>
+        <f t="shared" si="1"/>
         <v>44.75</v>
       </c>
       <c r="C27" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5499999999999972</v>
       </c>
       <c r="D27" s="45" t="s">
@@ -14137,18 +14220,21 @@
       <c r="CH27" s="5">
         <v>39.4</v>
       </c>
-    </row>
-    <row r="28" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI27">
+        <v>39.299999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
-        <f>MIN(E28:ZQ28)</f>
+        <f t="shared" si="0"/>
         <v>111.95</v>
       </c>
       <c r="B28" s="12">
-        <f>MAX(E28:ZQ28)</f>
+        <f t="shared" si="1"/>
         <v>141.65</v>
       </c>
       <c r="C28" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>29.700000000000003</v>
       </c>
       <c r="D28" s="45" t="s">
@@ -14356,18 +14442,21 @@
       <c r="CH28" s="5">
         <v>126.9</v>
       </c>
-    </row>
-    <row r="29" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI28">
+        <v>128.35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
-        <f>MIN(E29:ZQ29)</f>
+        <f t="shared" si="0"/>
         <v>62.3</v>
       </c>
       <c r="B29" s="12">
-        <f>MAX(E29:ZQ29)</f>
+        <f t="shared" si="1"/>
         <v>78.849999999999994</v>
       </c>
       <c r="C29" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16.549999999999997</v>
       </c>
       <c r="D29" s="45" t="s">
@@ -14575,19 +14664,22 @@
       <c r="CH29" s="5">
         <v>68</v>
       </c>
-    </row>
-    <row r="30" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI29">
+        <v>68.55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
-        <f>MIN(E30:ZQ30)</f>
-        <v>36.950000000000003</v>
+        <f t="shared" si="0"/>
+        <v>36.049999999999997</v>
       </c>
       <c r="B30" s="12">
-        <f>MAX(E30:ZQ30)</f>
+        <f t="shared" si="1"/>
         <v>50.95</v>
       </c>
       <c r="C30" s="12">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <f t="shared" si="2"/>
+        <v>14.900000000000006</v>
       </c>
       <c r="D30" s="45" t="s">
         <v>256</v>
@@ -14794,18 +14886,21 @@
       <c r="CH30" s="5">
         <v>37.950000000000003</v>
       </c>
-    </row>
-    <row r="31" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI30">
+        <v>36.049999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
-        <f>MIN(E31:ZQ31)</f>
+        <f t="shared" si="0"/>
         <v>125.3</v>
       </c>
       <c r="B31" s="12">
-        <f>MAX(E31:ZQ31)</f>
+        <f t="shared" si="1"/>
         <v>156.85</v>
       </c>
       <c r="C31" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>31.549999999999997</v>
       </c>
       <c r="D31" s="45" t="s">
@@ -15013,19 +15108,22 @@
       <c r="CH31" s="5">
         <v>147</v>
       </c>
-    </row>
-    <row r="32" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI31">
+        <v>130.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
-        <f>MIN(E32:ZQ32)</f>
-        <v>96.65</v>
+        <f t="shared" si="0"/>
+        <v>96</v>
       </c>
       <c r="B32" s="12">
-        <f>MAX(E32:ZQ32)</f>
+        <f t="shared" si="1"/>
         <v>121.8</v>
       </c>
       <c r="C32" s="12">
-        <f t="shared" si="0"/>
-        <v>25.149999999999991</v>
+        <f t="shared" si="2"/>
+        <v>25.799999999999997</v>
       </c>
       <c r="D32" s="45" t="s">
         <v>268</v>
@@ -15220,18 +15318,21 @@
       <c r="CH32" s="5">
         <v>100.6</v>
       </c>
-    </row>
-    <row r="33" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI32">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
-        <f>MIN(E33:ZQ33)</f>
+        <f t="shared" si="0"/>
         <v>56.75</v>
       </c>
       <c r="B33" s="12">
-        <f>MAX(E33:ZQ33)</f>
+        <f t="shared" si="1"/>
         <v>67.099999999999994</v>
       </c>
       <c r="C33" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10.349999999999994</v>
       </c>
       <c r="D33" s="45" t="s">
@@ -15415,18 +15516,21 @@
       <c r="CH33" s="5">
         <v>66.099999999999994</v>
       </c>
-    </row>
-    <row r="34" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI33">
+        <v>63.95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
-        <f>MIN(E34:ZQ34)</f>
+        <f t="shared" si="0"/>
         <v>167.9</v>
       </c>
       <c r="B34" s="12">
-        <f>MAX(E34:ZQ34)</f>
+        <f t="shared" si="1"/>
         <v>236.1</v>
       </c>
       <c r="C34" s="12">
-        <f t="shared" ref="C34" si="1">B34-A34</f>
+        <f t="shared" ref="C34" si="3">B34-A34</f>
         <v>68.199999999999989</v>
       </c>
       <c r="D34" s="45" t="s">
@@ -15604,18 +15708,21 @@
       <c r="CH34" s="5">
         <v>232.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI34">
+        <v>235.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
-        <f>MIN(E35:ZQ35)</f>
+        <f t="shared" si="0"/>
         <v>392.1</v>
       </c>
       <c r="B35" s="12">
-        <f>MAX(E35:ZQ35)</f>
+        <f t="shared" si="1"/>
         <v>520</v>
       </c>
       <c r="C35" s="12">
-        <f t="shared" ref="C35" si="2">B35-A35</f>
+        <f t="shared" ref="C35" si="4">B35-A35</f>
         <v>127.89999999999998</v>
       </c>
       <c r="D35" s="45" t="s">
@@ -15771,18 +15878,21 @@
       <c r="CH35" s="5">
         <v>417.7</v>
       </c>
-    </row>
-    <row r="36" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI35">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="36" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
-        <f>MIN(E36:ZQ36)</f>
+        <f t="shared" si="0"/>
         <v>226</v>
       </c>
       <c r="B36" s="12">
-        <f>MAX(E36:ZQ36)</f>
+        <f t="shared" si="1"/>
         <v>396.85</v>
       </c>
       <c r="C36" s="12">
-        <f t="shared" ref="C36" si="3">B36-A36</f>
+        <f t="shared" ref="C36" si="5">B36-A36</f>
         <v>170.85000000000002</v>
       </c>
       <c r="D36" s="45" t="s">
@@ -15928,18 +16038,21 @@
       <c r="CH36" s="5">
         <v>383.7</v>
       </c>
-    </row>
-    <row r="37" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI36">
+        <v>354.85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
-        <f>MIN(E37:ZQ37)</f>
+        <f t="shared" si="0"/>
         <v>75.2</v>
       </c>
       <c r="B37" s="12">
-        <f>MAX(E37:ZQ37)</f>
+        <f t="shared" si="1"/>
         <v>83.85</v>
       </c>
       <c r="C37" s="12">
-        <f t="shared" ref="C37" si="4">B37-A37</f>
+        <f t="shared" ref="C37" si="6">B37-A37</f>
         <v>8.6499999999999915</v>
       </c>
       <c r="D37" s="45" t="s">
@@ -16077,18 +16190,21 @@
       <c r="CH37" s="5">
         <v>82.1</v>
       </c>
-    </row>
-    <row r="38" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI37">
+        <v>79.900000000000006</v>
+      </c>
+    </row>
+    <row r="38" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
-        <f>MIN(E38:ZQ38)</f>
+        <f t="shared" si="0"/>
         <v>407.05</v>
       </c>
       <c r="B38" s="12">
-        <f>MAX(E38:ZQ38)</f>
+        <f t="shared" si="1"/>
         <v>472</v>
       </c>
       <c r="C38" s="12">
-        <f t="shared" ref="C38" si="5">B38-A38</f>
+        <f t="shared" ref="C38" si="7">B38-A38</f>
         <v>64.949999999999989</v>
       </c>
       <c r="D38" s="45" t="s">
@@ -16226,18 +16342,21 @@
       <c r="CH38" s="5">
         <v>409.9</v>
       </c>
-    </row>
-    <row r="39" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI38">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="39" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
-        <f>MIN(E39:ZQ39)</f>
+        <f t="shared" si="0"/>
         <v>175.2</v>
       </c>
       <c r="B39" s="12">
-        <f>MAX(E39:ZQ39)</f>
+        <f t="shared" si="1"/>
         <v>215.25</v>
       </c>
       <c r="C39" s="12">
-        <f t="shared" ref="C39" si="6">B39-A39</f>
+        <f t="shared" ref="C39" si="8">B39-A39</f>
         <v>40.050000000000011</v>
       </c>
       <c r="D39" s="45" t="s">
@@ -16371,18 +16490,21 @@
       <c r="CH39" s="5">
         <v>195</v>
       </c>
-    </row>
-    <row r="40" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI39">
+        <v>191.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
-        <f>MIN(E40:ZQ40)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B40" s="12">
-        <f>MAX(E40:ZQ40)</f>
+        <f t="shared" si="1"/>
         <v>39.450000000000003</v>
       </c>
       <c r="C40" s="12">
-        <f t="shared" ref="C40:C43" si="7">B40-A40</f>
+        <f t="shared" ref="C40:C43" si="9">B40-A40</f>
         <v>4.4500000000000028</v>
       </c>
       <c r="D40" s="45" t="s">
@@ -16512,18 +16634,21 @@
       <c r="CH40" s="5">
         <v>37</v>
       </c>
-    </row>
-    <row r="41" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI40">
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
-        <f>MIN(E41:ZQ41)</f>
+        <f t="shared" si="0"/>
         <v>552.04999999999995</v>
       </c>
       <c r="B41" s="12">
-        <f>MAX(E41:ZQ41)</f>
+        <f t="shared" si="1"/>
         <v>665.45</v>
       </c>
       <c r="C41" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>113.40000000000009</v>
       </c>
       <c r="D41" s="45" t="s">
@@ -16651,18 +16776,21 @@
       <c r="CH41" s="5">
         <v>665.45</v>
       </c>
-    </row>
-    <row r="42" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI41">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="42" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
-        <f>MIN(E42:ZQ42)</f>
+        <f t="shared" si="0"/>
         <v>810.6</v>
       </c>
       <c r="B42" s="12">
-        <f>MAX(E42:ZQ42)</f>
+        <f t="shared" si="1"/>
         <v>856</v>
       </c>
       <c r="C42" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>45.399999999999977</v>
       </c>
       <c r="D42" s="45" t="s">
@@ -16790,18 +16918,21 @@
       <c r="CH42" s="5">
         <v>821.35</v>
       </c>
-    </row>
-    <row r="43" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI42">
+        <v>845.6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
-        <f>MIN(E43:ZQ43)</f>
+        <f t="shared" si="0"/>
         <v>134.9</v>
       </c>
       <c r="B43" s="12">
-        <f>MAX(E43:ZQ43)</f>
+        <f t="shared" si="1"/>
         <v>146</v>
       </c>
       <c r="C43" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>11.099999999999994</v>
       </c>
       <c r="D43" s="45" t="s">
@@ -16927,19 +17058,22 @@
       <c r="CH43" s="5">
         <v>140.25</v>
       </c>
-    </row>
-    <row r="44" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI43">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
-        <f>MIN(E44:ZQ44)</f>
-        <v>583.65</v>
+        <f t="shared" si="0"/>
+        <v>561.04999999999995</v>
       </c>
       <c r="B44" s="12">
-        <f>MAX(E44:ZQ44)</f>
+        <f t="shared" si="1"/>
         <v>770</v>
       </c>
       <c r="C44" s="12">
-        <f t="shared" ref="C44" si="8">B44-A44</f>
-        <v>186.35000000000002</v>
+        <f t="shared" ref="C44" si="10">B44-A44</f>
+        <v>208.95000000000005</v>
       </c>
       <c r="D44" s="45" t="s">
         <v>311</v>
@@ -17058,18 +17192,21 @@
       <c r="CH44" s="5">
         <v>583.65</v>
       </c>
-    </row>
-    <row r="45" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI44">
+        <v>561.04999999999995</v>
+      </c>
+    </row>
+    <row r="45" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
-        <f>MIN(E45:ZQ45)</f>
+        <f t="shared" si="0"/>
         <v>101.4</v>
       </c>
       <c r="B45" s="12">
-        <f>MAX(E45:ZQ45)</f>
+        <f t="shared" si="1"/>
         <v>110.95</v>
       </c>
       <c r="C45" s="12">
-        <f t="shared" ref="C45" si="9">B45-A45</f>
+        <f t="shared" ref="C45" si="11">B45-A45</f>
         <v>9.5499999999999972</v>
       </c>
       <c r="D45" s="45" t="s">
@@ -17181,18 +17318,21 @@
       <c r="CH45" s="5">
         <v>110.6</v>
       </c>
-    </row>
-    <row r="46" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI45">
+        <v>104.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
-        <f>MIN(E46:ZQ46)</f>
+        <f t="shared" si="0"/>
         <v>137.65</v>
       </c>
       <c r="B46" s="12">
-        <f>MAX(E46:ZQ46)</f>
+        <f t="shared" si="1"/>
         <v>145</v>
       </c>
       <c r="C46" s="12">
-        <f t="shared" ref="C46" si="10">B46-A46</f>
+        <f t="shared" ref="C46" si="12">B46-A46</f>
         <v>7.3499999999999943</v>
       </c>
       <c r="D46" s="45" t="s">
@@ -17290,6 +17430,9 @@
       <c r="CH46" s="5">
         <v>137.65</v>
       </c>
+      <c r="CI46">
+        <v>138.05000000000001</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="L1:L37">

</xml_diff>

<commit_message>
Added details for 15/12/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13530" windowHeight="5625" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13530" windowHeight="5625" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PaidTillDate" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="329">
   <si>
     <t>Date</t>
   </si>
@@ -1006,6 +1006,12 @@
   </si>
   <si>
     <t>13/12/2017</t>
+  </si>
+  <si>
+    <t>14/12/2017</t>
+  </si>
+  <si>
+    <t>15/12/2017</t>
   </si>
 </sst>
 </file>
@@ -1177,7 +1183,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1252,7 +1258,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1558,8 +1563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1652,8 +1657,8 @@
         <v>9</v>
       </c>
       <c r="H3" s="4">
-        <f>H2-B25</f>
-        <v>55990</v>
+        <f>H2-B30</f>
+        <v>35990</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1840,8 +1845,12 @@
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="20"/>
+      <c r="A23" s="23">
+        <v>43070</v>
+      </c>
+      <c r="B23" s="20">
+        <v>20000</v>
+      </c>
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1850,13 +1859,8 @@
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="20">
-        <f>SUM(B2:B24)</f>
-        <v>502500</v>
-      </c>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1883,28 +1887,33 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
       <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="24"/>
       <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
+      <c r="A30" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="20">
+        <f>SUM(B2:B24)</f>
+        <v>522500</v>
+      </c>
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -7252,11 +7261,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CI46"/>
+  <dimension ref="A1:CK46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="CA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CI2" sqref="CI2:CI46"/>
+      <pane xSplit="4" topLeftCell="CG1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CK2" sqref="CK2:CK46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7310,10 +7319,10 @@
     <col min="83" max="83" width="13" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="13" customWidth="1"/>
     <col min="85" max="86" width="13" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="14" bestFit="1" customWidth="1"/>
+    <col min="87" max="89" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:89" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>249</v>
       </c>
@@ -7572,11 +7581,17 @@
       <c r="CH1" s="51">
         <v>42959</v>
       </c>
-      <c r="CI1" s="56" t="s">
+      <c r="CI1" s="49" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="2" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ1" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="CK1" s="49" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <f t="shared" ref="A2:A46" si="0">MIN(E2:ZQ2)</f>
         <v>243.6</v>
@@ -7830,11 +7845,17 @@
       <c r="CH2" s="5">
         <v>313.75</v>
       </c>
-      <c r="CI2">
+      <c r="CI2" s="5">
         <v>313.35000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ2" s="5">
+        <v>313.85000000000002</v>
+      </c>
+      <c r="CK2" s="5">
+        <v>312.35000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <f t="shared" si="0"/>
         <v>262.7</v>
@@ -8088,11 +8109,17 @@
       <c r="CH3" s="5">
         <v>310.95</v>
       </c>
-      <c r="CI3">
+      <c r="CI3" s="5">
         <v>304.05</v>
       </c>
-    </row>
-    <row r="4" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ3" s="5">
+        <v>304.5</v>
+      </c>
+      <c r="CK3" s="5">
+        <v>303.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
         <v>251.25</v>
@@ -8352,11 +8379,17 @@
       <c r="CH4" s="5">
         <v>258.3</v>
       </c>
-      <c r="CI4">
+      <c r="CI4" s="5">
         <v>259.45</v>
       </c>
-    </row>
-    <row r="5" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ4" s="5">
+        <v>264.25</v>
+      </c>
+      <c r="CK4" s="5">
+        <v>264.10000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <f t="shared" si="0"/>
         <v>786.25</v>
@@ -8616,11 +8649,17 @@
       <c r="CH5" s="5">
         <v>923.3</v>
       </c>
-      <c r="CI5">
+      <c r="CI5" s="5">
         <v>914.75</v>
       </c>
-    </row>
-    <row r="6" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ5" s="5">
+        <v>924</v>
+      </c>
+      <c r="CK5" s="5">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="6" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <f t="shared" si="0"/>
         <v>236.45</v>
@@ -8880,11 +8919,17 @@
       <c r="CH6" s="5">
         <v>264.10000000000002</v>
       </c>
-      <c r="CI6">
+      <c r="CI6" s="5">
         <v>263.10000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ6" s="5">
+        <v>262.75</v>
+      </c>
+      <c r="CK6" s="5">
+        <v>271.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <f t="shared" si="0"/>
         <v>15.6</v>
@@ -9144,11 +9189,17 @@
       <c r="CH7" s="5">
         <v>17.55</v>
       </c>
-      <c r="CI7">
+      <c r="CI7" s="5">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ7" s="5">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="CK7" s="5">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <f t="shared" si="0"/>
         <v>53.4</v>
@@ -9408,14 +9459,20 @@
       <c r="CH8" s="5">
         <v>81.95</v>
       </c>
-      <c r="CI8">
+      <c r="CI8" s="5">
         <v>78.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:87" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="CJ8" s="5">
+        <v>77.5</v>
+      </c>
+      <c r="CK8" s="5">
+        <v>78.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:89" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <f t="shared" si="0"/>
-        <v>52.35</v>
+        <v>52.05</v>
       </c>
       <c r="B9" s="39">
         <f t="shared" si="1"/>
@@ -9423,7 +9480,7 @@
       </c>
       <c r="C9" s="12">
         <f t="shared" si="2"/>
-        <v>8.6499999999999986</v>
+        <v>8.9500000000000028</v>
       </c>
       <c r="D9" s="43" t="s">
         <v>125</v>
@@ -9664,11 +9721,17 @@
       <c r="CH9" s="28">
         <v>53.6</v>
       </c>
-      <c r="CI9" s="37">
+      <c r="CI9" s="28">
         <v>52.35</v>
       </c>
-    </row>
-    <row r="10" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ9" s="28">
+        <v>52.05</v>
+      </c>
+      <c r="CK9" s="28">
+        <v>52.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <f t="shared" si="0"/>
         <v>35.549999999999997</v>
@@ -9928,11 +9991,17 @@
       <c r="CH10" s="5">
         <v>37.049999999999997</v>
       </c>
-      <c r="CI10">
+      <c r="CI10" s="5">
         <v>36.15</v>
       </c>
-    </row>
-    <row r="11" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ10" s="5">
+        <v>35.950000000000003</v>
+      </c>
+      <c r="CK10" s="5">
+        <v>36.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <f t="shared" si="0"/>
         <v>72.650000000000006</v>
@@ -10192,11 +10261,17 @@
       <c r="CH11" s="5">
         <v>97</v>
       </c>
-      <c r="CI11">
+      <c r="CI11" s="5">
         <v>92.75</v>
       </c>
-    </row>
-    <row r="12" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ11" s="5">
+        <v>93.95</v>
+      </c>
+      <c r="CK11" s="5">
+        <v>93.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
         <v>82.65</v>
@@ -10456,11 +10531,17 @@
       <c r="CH12" s="5">
         <v>92.15</v>
       </c>
-      <c r="CI12">
+      <c r="CI12" s="5">
         <v>89.8</v>
       </c>
-    </row>
-    <row r="13" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ12" s="5">
+        <v>89.6</v>
+      </c>
+      <c r="CK12" s="5">
+        <v>89.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <f t="shared" si="0"/>
         <v>44.1</v>
@@ -10720,11 +10801,17 @@
       <c r="CH13" s="5">
         <v>53.15</v>
       </c>
-      <c r="CI13">
+      <c r="CI13" s="5">
         <v>51.4</v>
       </c>
-    </row>
-    <row r="14" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ13" s="5">
+        <v>51.15</v>
+      </c>
+      <c r="CK13" s="5">
+        <v>51.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <f t="shared" si="0"/>
         <v>29.75</v>
@@ -10984,14 +11071,20 @@
       <c r="CH14" s="5">
         <v>42.4</v>
       </c>
-      <c r="CI14">
+      <c r="CI14" s="5">
         <v>41.55</v>
       </c>
-    </row>
-    <row r="15" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ14" s="5">
+        <v>40.35</v>
+      </c>
+      <c r="CK14" s="5">
+        <v>40.450000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
-        <v>23.4</v>
+        <v>23.35</v>
       </c>
       <c r="B15" s="12">
         <f t="shared" si="1"/>
@@ -10999,7 +11092,7 @@
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>13.049999999999997</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>126</v>
@@ -11240,11 +11333,17 @@
       <c r="CH15" s="5">
         <v>23.5</v>
       </c>
-      <c r="CI15">
+      <c r="CI15" s="5">
         <v>23.4</v>
       </c>
-    </row>
-    <row r="16" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ15" s="5">
+        <v>23.35</v>
+      </c>
+      <c r="CK15" s="5">
+        <v>23.35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <f t="shared" si="0"/>
         <v>552</v>
@@ -11504,11 +11603,17 @@
       <c r="CH16" s="5">
         <v>702.85</v>
       </c>
-      <c r="CI16">
+      <c r="CI16" s="5">
         <v>683</v>
       </c>
-    </row>
-    <row r="17" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ16" s="5">
+        <v>687</v>
+      </c>
+      <c r="CK16" s="5">
+        <v>696.15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <f t="shared" si="0"/>
         <v>433</v>
@@ -11768,11 +11873,17 @@
       <c r="CH17" s="5">
         <v>484.65</v>
       </c>
-      <c r="CI17">
+      <c r="CI17" s="5">
         <v>482</v>
       </c>
-    </row>
-    <row r="18" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ17" s="5">
+        <v>484.6</v>
+      </c>
+      <c r="CK17" s="5">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="18" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <f t="shared" si="0"/>
         <v>178.8</v>
@@ -12032,11 +12143,17 @@
       <c r="CH18" s="5">
         <v>261.75</v>
       </c>
-      <c r="CI18">
+      <c r="CI18" s="5">
         <v>250.15</v>
       </c>
-    </row>
-    <row r="19" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ18" s="5">
+        <v>247</v>
+      </c>
+      <c r="CK18" s="5">
+        <v>255.55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <f t="shared" si="0"/>
         <v>440.7</v>
@@ -12296,11 +12413,17 @@
       <c r="CH19" s="5">
         <v>759</v>
       </c>
-      <c r="CI19">
+      <c r="CI19" s="5">
         <v>748</v>
       </c>
-    </row>
-    <row r="20" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ19" s="5">
+        <v>739.85</v>
+      </c>
+      <c r="CK19" s="5">
+        <v>747.65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <f t="shared" si="0"/>
         <v>660.75</v>
@@ -12560,11 +12683,17 @@
       <c r="CH20" s="5">
         <v>674.3</v>
       </c>
-      <c r="CI20">
+      <c r="CI20" s="5">
         <v>670.1</v>
       </c>
-    </row>
-    <row r="21" spans="1:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CJ20" s="5">
+        <v>665.4</v>
+      </c>
+      <c r="CK20" s="5">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="21" spans="1:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <f t="shared" si="0"/>
         <v>376.7</v>
@@ -12824,11 +12953,17 @@
       <c r="CH21" s="5">
         <v>525.79999999999995</v>
       </c>
-      <c r="CI21">
+      <c r="CI21" s="5">
         <v>517.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CJ21" s="5">
+        <v>523</v>
+      </c>
+      <c r="CK21" s="5">
+        <v>517.29999999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <f t="shared" si="0"/>
         <v>315.2</v>
@@ -13034,11 +13169,17 @@
       <c r="CH22" s="5">
         <v>382.95</v>
       </c>
-      <c r="CI22">
+      <c r="CI22" s="5">
         <v>359.7</v>
       </c>
-    </row>
-    <row r="23" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ22" s="5">
+        <v>357.75</v>
+      </c>
+      <c r="CK22" s="5">
+        <v>362.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
         <v>52.8</v>
@@ -13290,11 +13431,17 @@
       <c r="CH23" s="5">
         <v>57.25</v>
       </c>
-      <c r="CI23">
+      <c r="CI23" s="5">
         <v>52.8</v>
       </c>
-    </row>
-    <row r="24" spans="1:87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CJ23" s="5">
+        <v>53.85</v>
+      </c>
+      <c r="CK23" s="5">
+        <v>53.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:89" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <f t="shared" si="0"/>
         <v>210.65</v>
@@ -13542,22 +13689,28 @@
       <c r="CH24" s="5">
         <v>233.4</v>
       </c>
-      <c r="CI24">
+      <c r="CI24" s="5">
         <v>224.9</v>
       </c>
-    </row>
-    <row r="25" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ24" s="5">
+        <v>224.75</v>
+      </c>
+      <c r="CK24" s="5">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <f t="shared" si="0"/>
         <v>876</v>
       </c>
       <c r="B25" s="12">
         <f t="shared" si="1"/>
-        <v>1008</v>
+        <v>1019</v>
       </c>
       <c r="C25" s="12">
         <f t="shared" si="2"/>
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="D25" s="46" t="s">
         <v>236</v>
@@ -13776,11 +13929,17 @@
       <c r="CH25" s="5">
         <v>1001.45</v>
       </c>
-      <c r="CI25">
+      <c r="CI25" s="5">
         <v>1005</v>
       </c>
-    </row>
-    <row r="26" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ25" s="5">
+        <v>1012.3</v>
+      </c>
+      <c r="CK25" s="5">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="26" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <f t="shared" si="0"/>
         <v>83.1</v>
@@ -13998,11 +14157,17 @@
       <c r="CH26" s="5">
         <v>107.4</v>
       </c>
-      <c r="CI26">
+      <c r="CI26" s="5">
         <v>106.4</v>
       </c>
-    </row>
-    <row r="27" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ26" s="5">
+        <v>103.3</v>
+      </c>
+      <c r="CK26" s="5">
+        <v>104.35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <f t="shared" si="0"/>
         <v>36.200000000000003</v>
@@ -14220,11 +14385,17 @@
       <c r="CH27" s="5">
         <v>39.4</v>
       </c>
-      <c r="CI27">
+      <c r="CI27" s="5">
         <v>39.299999999999997</v>
       </c>
-    </row>
-    <row r="28" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ27" s="5">
+        <v>38.5</v>
+      </c>
+      <c r="CK27" s="5">
+        <v>39.799999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <f t="shared" si="0"/>
         <v>111.95</v>
@@ -14442,11 +14613,17 @@
       <c r="CH28" s="5">
         <v>126.9</v>
       </c>
-      <c r="CI28">
+      <c r="CI28" s="5">
         <v>128.35</v>
       </c>
-    </row>
-    <row r="29" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ28" s="5">
+        <v>126.8</v>
+      </c>
+      <c r="CK28" s="5">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <f t="shared" si="0"/>
         <v>62.3</v>
@@ -14664,14 +14841,20 @@
       <c r="CH29" s="5">
         <v>68</v>
       </c>
-      <c r="CI29">
+      <c r="CI29" s="5">
         <v>68.55</v>
       </c>
-    </row>
-    <row r="30" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ29" s="5">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="CK29" s="5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <f t="shared" si="0"/>
-        <v>36.049999999999997</v>
+        <v>35.25</v>
       </c>
       <c r="B30" s="12">
         <f t="shared" si="1"/>
@@ -14679,7 +14862,7 @@
       </c>
       <c r="C30" s="12">
         <f t="shared" si="2"/>
-        <v>14.900000000000006</v>
+        <v>15.700000000000003</v>
       </c>
       <c r="D30" s="45" t="s">
         <v>256</v>
@@ -14886,11 +15069,17 @@
       <c r="CH30" s="5">
         <v>37.950000000000003</v>
       </c>
-      <c r="CI30">
+      <c r="CI30" s="5">
         <v>36.049999999999997</v>
       </c>
-    </row>
-    <row r="31" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ30" s="5">
+        <v>35.25</v>
+      </c>
+      <c r="CK30" s="5">
+        <v>35.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
         <v>125.3</v>
@@ -15108,11 +15297,17 @@
       <c r="CH31" s="5">
         <v>147</v>
       </c>
-      <c r="CI31">
+      <c r="CI31" s="5">
         <v>130.4</v>
       </c>
-    </row>
-    <row r="32" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ31" s="5">
+        <v>134</v>
+      </c>
+      <c r="CK31" s="5">
+        <v>136.85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <f t="shared" si="0"/>
         <v>96</v>
@@ -15318,22 +15513,28 @@
       <c r="CH32" s="5">
         <v>100.6</v>
       </c>
-      <c r="CI32">
+      <c r="CI32" s="5">
         <v>96</v>
       </c>
-    </row>
-    <row r="33" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ32" s="5">
+        <v>97.05</v>
+      </c>
+      <c r="CK32" s="5">
+        <v>97.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <f t="shared" si="0"/>
         <v>56.75</v>
       </c>
       <c r="B33" s="12">
         <f t="shared" si="1"/>
-        <v>67.099999999999994</v>
+        <v>67.75</v>
       </c>
       <c r="C33" s="12">
         <f t="shared" si="2"/>
-        <v>10.349999999999994</v>
+        <v>11</v>
       </c>
       <c r="D33" s="45" t="s">
         <v>271</v>
@@ -15516,22 +15717,28 @@
       <c r="CH33" s="5">
         <v>66.099999999999994</v>
       </c>
-      <c r="CI33">
+      <c r="CI33" s="5">
         <v>63.95</v>
       </c>
-    </row>
-    <row r="34" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ33" s="5">
+        <v>63.3</v>
+      </c>
+      <c r="CK33" s="5">
+        <v>67.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <f t="shared" si="0"/>
         <v>167.9</v>
       </c>
       <c r="B34" s="12">
         <f t="shared" si="1"/>
-        <v>236.1</v>
+        <v>264.60000000000002</v>
       </c>
       <c r="C34" s="12">
         <f t="shared" ref="C34" si="3">B34-A34</f>
-        <v>68.199999999999989</v>
+        <v>96.700000000000017</v>
       </c>
       <c r="D34" s="45" t="s">
         <v>280</v>
@@ -15708,11 +15915,17 @@
       <c r="CH34" s="5">
         <v>232.5</v>
       </c>
-      <c r="CI34">
+      <c r="CI34" s="5">
         <v>235.8</v>
       </c>
-    </row>
-    <row r="35" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ34" s="5">
+        <v>228</v>
+      </c>
+      <c r="CK34" s="5">
+        <v>264.60000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <f t="shared" si="0"/>
         <v>392.1</v>
@@ -15878,11 +16091,17 @@
       <c r="CH35" s="5">
         <v>417.7</v>
       </c>
-      <c r="CI35">
+      <c r="CI35" s="5">
         <v>399</v>
       </c>
-    </row>
-    <row r="36" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ35" s="5">
+        <v>397.35</v>
+      </c>
+      <c r="CK35" s="5">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="36" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <f t="shared" si="0"/>
         <v>226</v>
@@ -16038,11 +16257,17 @@
       <c r="CH36" s="5">
         <v>383.7</v>
       </c>
-      <c r="CI36">
+      <c r="CI36" s="5">
         <v>354.85</v>
       </c>
-    </row>
-    <row r="37" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ36" s="5">
+        <v>365.55</v>
+      </c>
+      <c r="CK36" s="5">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="37" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <f t="shared" si="0"/>
         <v>75.2</v>
@@ -16190,11 +16415,17 @@
       <c r="CH37" s="5">
         <v>82.1</v>
       </c>
-      <c r="CI37">
+      <c r="CI37" s="5">
         <v>79.900000000000006</v>
       </c>
-    </row>
-    <row r="38" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ37" s="5">
+        <v>79.25</v>
+      </c>
+      <c r="CK37" s="5">
+        <v>79.95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <f t="shared" si="0"/>
         <v>407.05</v>
@@ -16342,11 +16573,17 @@
       <c r="CH38" s="5">
         <v>409.9</v>
       </c>
-      <c r="CI38">
+      <c r="CI38" s="5">
         <v>418</v>
       </c>
-    </row>
-    <row r="39" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ38" s="5">
+        <v>419.05</v>
+      </c>
+      <c r="CK38" s="5">
+        <v>423.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <f t="shared" si="0"/>
         <v>175.2</v>
@@ -16490,11 +16727,17 @@
       <c r="CH39" s="5">
         <v>195</v>
       </c>
-      <c r="CI39">
+      <c r="CI39" s="5">
         <v>191.8</v>
       </c>
-    </row>
-    <row r="40" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ39" s="5">
+        <v>191.75</v>
+      </c>
+      <c r="CK39" s="5">
+        <v>206.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -16634,11 +16877,17 @@
       <c r="CH40" s="5">
         <v>37</v>
       </c>
-      <c r="CI40">
+      <c r="CI40" s="5">
         <v>35.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ40" s="5">
+        <v>35.9</v>
+      </c>
+      <c r="CK40" s="5">
+        <v>36.1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <f t="shared" si="0"/>
         <v>552.04999999999995</v>
@@ -16776,22 +17025,28 @@
       <c r="CH41" s="5">
         <v>665.45</v>
       </c>
-      <c r="CI41">
+      <c r="CI41" s="5">
         <v>634</v>
       </c>
-    </row>
-    <row r="42" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ41" s="5">
+        <v>632</v>
+      </c>
+      <c r="CK41" s="5">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="42" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <f t="shared" si="0"/>
         <v>810.6</v>
       </c>
       <c r="B42" s="12">
         <f t="shared" si="1"/>
-        <v>856</v>
+        <v>861</v>
       </c>
       <c r="C42" s="12">
         <f t="shared" si="9"/>
-        <v>45.399999999999977</v>
+        <v>50.399999999999977</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>308</v>
@@ -16918,11 +17173,17 @@
       <c r="CH42" s="5">
         <v>821.35</v>
       </c>
-      <c r="CI42">
+      <c r="CI42" s="5">
         <v>845.6</v>
       </c>
-    </row>
-    <row r="43" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ42" s="5">
+        <v>852.5</v>
+      </c>
+      <c r="CK42" s="5">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="43" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <f t="shared" si="0"/>
         <v>134.9</v>
@@ -17058,14 +17319,20 @@
       <c r="CH43" s="5">
         <v>140.25</v>
       </c>
-      <c r="CI43">
+      <c r="CI43" s="5">
         <v>136</v>
       </c>
-    </row>
-    <row r="44" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ43" s="5">
+        <v>135.30000000000001</v>
+      </c>
+      <c r="CK43" s="5">
+        <v>142.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <f t="shared" si="0"/>
-        <v>561.04999999999995</v>
+        <v>545.04999999999995</v>
       </c>
       <c r="B44" s="12">
         <f t="shared" si="1"/>
@@ -17073,7 +17340,7 @@
       </c>
       <c r="C44" s="12">
         <f t="shared" ref="C44" si="10">B44-A44</f>
-        <v>208.95000000000005</v>
+        <v>224.95000000000005</v>
       </c>
       <c r="D44" s="45" t="s">
         <v>311</v>
@@ -17192,11 +17459,17 @@
       <c r="CH44" s="5">
         <v>583.65</v>
       </c>
-      <c r="CI44">
+      <c r="CI44" s="5">
         <v>561.04999999999995</v>
       </c>
-    </row>
-    <row r="45" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ44" s="5">
+        <v>552</v>
+      </c>
+      <c r="CK44" s="5">
+        <v>545.04999999999995</v>
+      </c>
+    </row>
+    <row r="45" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <f t="shared" si="0"/>
         <v>101.4</v>
@@ -17318,14 +17591,20 @@
       <c r="CH45" s="5">
         <v>110.6</v>
       </c>
-      <c r="CI45">
+      <c r="CI45" s="5">
         <v>104.1</v>
       </c>
-    </row>
-    <row r="46" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ45" s="5">
+        <v>104.2</v>
+      </c>
+      <c r="CK45" s="5">
+        <v>106.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <f t="shared" si="0"/>
-        <v>137.65</v>
+        <v>135.1</v>
       </c>
       <c r="B46" s="12">
         <f t="shared" si="1"/>
@@ -17333,7 +17612,7 @@
       </c>
       <c r="C46" s="12">
         <f t="shared" ref="C46" si="12">B46-A46</f>
-        <v>7.3499999999999943</v>
+        <v>9.9000000000000057</v>
       </c>
       <c r="D46" s="45" t="s">
         <v>324</v>
@@ -17430,8 +17709,14 @@
       <c r="CH46" s="5">
         <v>137.65</v>
       </c>
-      <c r="CI46">
+      <c r="CI46" s="5">
         <v>138.05000000000001</v>
+      </c>
+      <c r="CJ46" s="5">
+        <v>135.1</v>
+      </c>
+      <c r="CK46" s="5">
+        <v>135.6</v>
       </c>
     </row>
   </sheetData>
@@ -18657,10 +18942,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19374,7 +19659,7 @@
         <v>74</v>
       </c>
       <c r="B47" s="12">
-        <v>50000</v>
+        <v>30000</v>
       </c>
       <c r="C47" s="31">
         <v>43070</v>
@@ -19389,6 +19674,17 @@
       </c>
       <c r="C48" s="52">
         <v>43074</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="12">
+        <v>20000</v>
+      </c>
+      <c r="C49" s="31">
+        <v>43040</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added details for 19/12/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="331">
   <si>
     <t>Date</t>
   </si>
@@ -1012,6 +1012,12 @@
   </si>
   <si>
     <t>15/12/2017</t>
+  </si>
+  <si>
+    <t>18/12/2017</t>
+  </si>
+  <si>
+    <t>19/12/2017</t>
   </si>
 </sst>
 </file>
@@ -7261,11 +7267,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CK46"/>
+  <dimension ref="A1:CZ46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="CG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CK2" sqref="CK2:CK46"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="CJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CM46" sqref="CM46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7319,10 +7325,10 @@
     <col min="83" max="83" width="13" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="13" customWidth="1"/>
     <col min="85" max="86" width="13" bestFit="1" customWidth="1"/>
-    <col min="87" max="89" width="14" bestFit="1" customWidth="1"/>
+    <col min="87" max="91" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:104" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>249</v>
       </c>
@@ -7590,8 +7596,27 @@
       <c r="CK1" s="49" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="2" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL1" s="49" t="s">
+        <v>329</v>
+      </c>
+      <c r="CM1" s="49" t="s">
+        <v>330</v>
+      </c>
+      <c r="CN1" s="27"/>
+      <c r="CO1" s="27"/>
+      <c r="CP1" s="27"/>
+      <c r="CQ1" s="27"/>
+      <c r="CR1" s="27"/>
+      <c r="CS1" s="27"/>
+      <c r="CT1" s="27"/>
+      <c r="CU1" s="27"/>
+      <c r="CV1" s="27"/>
+      <c r="CW1" s="27"/>
+      <c r="CX1" s="27"/>
+      <c r="CY1" s="27"/>
+      <c r="CZ1" s="27"/>
+    </row>
+    <row r="2" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <f t="shared" ref="A2:A46" si="0">MIN(E2:ZQ2)</f>
         <v>243.6</v>
@@ -7854,8 +7879,27 @@
       <c r="CK2" s="5">
         <v>312.35000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL2" s="5">
+        <v>304.3</v>
+      </c>
+      <c r="CM2" s="5">
+        <v>320</v>
+      </c>
+      <c r="CN2" s="5"/>
+      <c r="CO2" s="5"/>
+      <c r="CP2" s="5"/>
+      <c r="CQ2" s="5"/>
+      <c r="CR2" s="5"/>
+      <c r="CS2" s="5"/>
+      <c r="CT2" s="5"/>
+      <c r="CU2" s="5"/>
+      <c r="CV2" s="5"/>
+      <c r="CW2" s="5"/>
+      <c r="CX2" s="5"/>
+      <c r="CY2" s="5"/>
+      <c r="CZ2" s="5"/>
+    </row>
+    <row r="3" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <f t="shared" si="0"/>
         <v>262.7</v>
@@ -8118,8 +8162,27 @@
       <c r="CK3" s="5">
         <v>303.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL3" s="5">
+        <v>291.95</v>
+      </c>
+      <c r="CM3" s="5">
+        <v>313.2</v>
+      </c>
+      <c r="CN3" s="5"/>
+      <c r="CO3" s="5"/>
+      <c r="CP3" s="5"/>
+      <c r="CQ3" s="5"/>
+      <c r="CR3" s="5"/>
+      <c r="CS3" s="5"/>
+      <c r="CT3" s="5"/>
+      <c r="CU3" s="5"/>
+      <c r="CV3" s="5"/>
+      <c r="CW3" s="5"/>
+      <c r="CX3" s="5"/>
+      <c r="CY3" s="5"/>
+      <c r="CZ3" s="5"/>
+    </row>
+    <row r="4" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
         <v>251.25</v>
@@ -8388,8 +8451,27 @@
       <c r="CK4" s="5">
         <v>264.10000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL4" s="5">
+        <v>259.60000000000002</v>
+      </c>
+      <c r="CM4" s="5">
+        <v>264.2</v>
+      </c>
+      <c r="CN4" s="5"/>
+      <c r="CO4" s="5"/>
+      <c r="CP4" s="5"/>
+      <c r="CQ4" s="5"/>
+      <c r="CR4" s="5"/>
+      <c r="CS4" s="5"/>
+      <c r="CT4" s="5"/>
+      <c r="CU4" s="5"/>
+      <c r="CV4" s="5"/>
+      <c r="CW4" s="5"/>
+      <c r="CX4" s="5"/>
+      <c r="CY4" s="5"/>
+      <c r="CZ4" s="5"/>
+    </row>
+    <row r="5" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <f t="shared" si="0"/>
         <v>786.25</v>
@@ -8658,8 +8740,27 @@
       <c r="CK5" s="5">
         <v>921</v>
       </c>
-    </row>
-    <row r="6" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL5" s="5">
+        <v>893.7</v>
+      </c>
+      <c r="CM5" s="5">
+        <v>926.85</v>
+      </c>
+      <c r="CN5" s="5"/>
+      <c r="CO5" s="5"/>
+      <c r="CP5" s="5"/>
+      <c r="CQ5" s="5"/>
+      <c r="CR5" s="5"/>
+      <c r="CS5" s="5"/>
+      <c r="CT5" s="5"/>
+      <c r="CU5" s="5"/>
+      <c r="CV5" s="5"/>
+      <c r="CW5" s="5"/>
+      <c r="CX5" s="5"/>
+      <c r="CY5" s="5"/>
+      <c r="CZ5" s="5"/>
+    </row>
+    <row r="6" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <f t="shared" si="0"/>
         <v>236.45</v>
@@ -8928,8 +9029,27 @@
       <c r="CK6" s="5">
         <v>271.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL6" s="5">
+        <v>263.3</v>
+      </c>
+      <c r="CM6" s="5">
+        <v>268.35000000000002</v>
+      </c>
+      <c r="CN6" s="5"/>
+      <c r="CO6" s="5"/>
+      <c r="CP6" s="5"/>
+      <c r="CQ6" s="5"/>
+      <c r="CR6" s="5"/>
+      <c r="CS6" s="5"/>
+      <c r="CT6" s="5"/>
+      <c r="CU6" s="5"/>
+      <c r="CV6" s="5"/>
+      <c r="CW6" s="5"/>
+      <c r="CX6" s="5"/>
+      <c r="CY6" s="5"/>
+      <c r="CZ6" s="5"/>
+    </row>
+    <row r="7" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <f t="shared" si="0"/>
         <v>15.6</v>
@@ -9198,8 +9318,27 @@
       <c r="CK7" s="5">
         <v>17.100000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL7" s="5">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="CM7" s="5">
+        <v>17.8</v>
+      </c>
+      <c r="CN7" s="5"/>
+      <c r="CO7" s="5"/>
+      <c r="CP7" s="5"/>
+      <c r="CQ7" s="5"/>
+      <c r="CR7" s="5"/>
+      <c r="CS7" s="5"/>
+      <c r="CT7" s="5"/>
+      <c r="CU7" s="5"/>
+      <c r="CV7" s="5"/>
+      <c r="CW7" s="5"/>
+      <c r="CX7" s="5"/>
+      <c r="CY7" s="5"/>
+      <c r="CZ7" s="5"/>
+    </row>
+    <row r="8" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <f t="shared" si="0"/>
         <v>53.4</v>
@@ -9468,11 +9607,30 @@
       <c r="CK8" s="5">
         <v>78.2</v>
       </c>
-    </row>
-    <row r="9" spans="1:89" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="CL8" s="5">
+        <v>75.95</v>
+      </c>
+      <c r="CM8" s="5">
+        <v>83.4</v>
+      </c>
+      <c r="CN8" s="5"/>
+      <c r="CO8" s="5"/>
+      <c r="CP8" s="5"/>
+      <c r="CQ8" s="5"/>
+      <c r="CR8" s="5"/>
+      <c r="CS8" s="5"/>
+      <c r="CT8" s="5"/>
+      <c r="CU8" s="5"/>
+      <c r="CV8" s="5"/>
+      <c r="CW8" s="5"/>
+      <c r="CX8" s="5"/>
+      <c r="CY8" s="5"/>
+      <c r="CZ8" s="5"/>
+    </row>
+    <row r="9" spans="1:104" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <f t="shared" si="0"/>
-        <v>52.05</v>
+        <v>51.55</v>
       </c>
       <c r="B9" s="39">
         <f t="shared" si="1"/>
@@ -9480,7 +9638,7 @@
       </c>
       <c r="C9" s="12">
         <f t="shared" si="2"/>
-        <v>8.9500000000000028</v>
+        <v>9.4500000000000028</v>
       </c>
       <c r="D9" s="43" t="s">
         <v>125</v>
@@ -9730,11 +9888,30 @@
       <c r="CK9" s="28">
         <v>52.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL9" s="28">
+        <v>51.55</v>
+      </c>
+      <c r="CM9" s="28">
+        <v>53.65</v>
+      </c>
+      <c r="CN9" s="28"/>
+      <c r="CO9" s="28"/>
+      <c r="CP9" s="28"/>
+      <c r="CQ9" s="28"/>
+      <c r="CR9" s="28"/>
+      <c r="CS9" s="28"/>
+      <c r="CT9" s="28"/>
+      <c r="CU9" s="28"/>
+      <c r="CV9" s="28"/>
+      <c r="CW9" s="28"/>
+      <c r="CX9" s="28"/>
+      <c r="CY9" s="28"/>
+      <c r="CZ9" s="28"/>
+    </row>
+    <row r="10" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <f t="shared" si="0"/>
-        <v>35.549999999999997</v>
+        <v>35.15</v>
       </c>
       <c r="B10" s="12">
         <f t="shared" si="1"/>
@@ -9742,7 +9919,7 @@
       </c>
       <c r="C10" s="12">
         <f t="shared" si="2"/>
-        <v>9.8000000000000043</v>
+        <v>10.200000000000003</v>
       </c>
       <c r="D10" s="45" t="s">
         <v>15</v>
@@ -10000,8 +10177,27 @@
       <c r="CK10" s="5">
         <v>36.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL10" s="5">
+        <v>35.15</v>
+      </c>
+      <c r="CM10" s="5">
+        <v>37</v>
+      </c>
+      <c r="CN10" s="5"/>
+      <c r="CO10" s="5"/>
+      <c r="CP10" s="5"/>
+      <c r="CQ10" s="5"/>
+      <c r="CR10" s="5"/>
+      <c r="CS10" s="5"/>
+      <c r="CT10" s="5"/>
+      <c r="CU10" s="5"/>
+      <c r="CV10" s="5"/>
+      <c r="CW10" s="5"/>
+      <c r="CX10" s="5"/>
+      <c r="CY10" s="5"/>
+      <c r="CZ10" s="5"/>
+    </row>
+    <row r="11" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <f t="shared" si="0"/>
         <v>72.650000000000006</v>
@@ -10270,8 +10466,27 @@
       <c r="CK11" s="5">
         <v>93.75</v>
       </c>
-    </row>
-    <row r="12" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL11" s="5">
+        <v>90.7</v>
+      </c>
+      <c r="CM11" s="5">
+        <v>98.55</v>
+      </c>
+      <c r="CN11" s="5"/>
+      <c r="CO11" s="5"/>
+      <c r="CP11" s="5"/>
+      <c r="CQ11" s="5"/>
+      <c r="CR11" s="5"/>
+      <c r="CS11" s="5"/>
+      <c r="CT11" s="5"/>
+      <c r="CU11" s="5"/>
+      <c r="CV11" s="5"/>
+      <c r="CW11" s="5"/>
+      <c r="CX11" s="5"/>
+      <c r="CY11" s="5"/>
+      <c r="CZ11" s="5"/>
+    </row>
+    <row r="12" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
         <v>82.65</v>
@@ -10540,8 +10755,27 @@
       <c r="CK12" s="5">
         <v>89.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL12" s="5">
+        <v>87.35</v>
+      </c>
+      <c r="CM12" s="5">
+        <v>89.95</v>
+      </c>
+      <c r="CN12" s="5"/>
+      <c r="CO12" s="5"/>
+      <c r="CP12" s="5"/>
+      <c r="CQ12" s="5"/>
+      <c r="CR12" s="5"/>
+      <c r="CS12" s="5"/>
+      <c r="CT12" s="5"/>
+      <c r="CU12" s="5"/>
+      <c r="CV12" s="5"/>
+      <c r="CW12" s="5"/>
+      <c r="CX12" s="5"/>
+      <c r="CY12" s="5"/>
+      <c r="CZ12" s="5"/>
+    </row>
+    <row r="13" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <f t="shared" si="0"/>
         <v>44.1</v>
@@ -10810,8 +11044,27 @@
       <c r="CK13" s="5">
         <v>51.75</v>
       </c>
-    </row>
-    <row r="14" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL13" s="5">
+        <v>50.25</v>
+      </c>
+      <c r="CM13" s="5">
+        <v>53.05</v>
+      </c>
+      <c r="CN13" s="5"/>
+      <c r="CO13" s="5"/>
+      <c r="CP13" s="5"/>
+      <c r="CQ13" s="5"/>
+      <c r="CR13" s="5"/>
+      <c r="CS13" s="5"/>
+      <c r="CT13" s="5"/>
+      <c r="CU13" s="5"/>
+      <c r="CV13" s="5"/>
+      <c r="CW13" s="5"/>
+      <c r="CX13" s="5"/>
+      <c r="CY13" s="5"/>
+      <c r="CZ13" s="5"/>
+    </row>
+    <row r="14" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <f t="shared" si="0"/>
         <v>29.75</v>
@@ -11080,11 +11333,30 @@
       <c r="CK14" s="5">
         <v>40.450000000000003</v>
       </c>
-    </row>
-    <row r="15" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL14" s="5">
+        <v>38.049999999999997</v>
+      </c>
+      <c r="CM14" s="5">
+        <v>41.7</v>
+      </c>
+      <c r="CN14" s="5"/>
+      <c r="CO14" s="5"/>
+      <c r="CP14" s="5"/>
+      <c r="CQ14" s="5"/>
+      <c r="CR14" s="5"/>
+      <c r="CS14" s="5"/>
+      <c r="CT14" s="5"/>
+      <c r="CU14" s="5"/>
+      <c r="CV14" s="5"/>
+      <c r="CW14" s="5"/>
+      <c r="CX14" s="5"/>
+      <c r="CY14" s="5"/>
+      <c r="CZ14" s="5"/>
+    </row>
+    <row r="15" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
-        <v>23.35</v>
+        <v>21.35</v>
       </c>
       <c r="B15" s="12">
         <f t="shared" si="1"/>
@@ -11092,7 +11364,7 @@
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
-        <v>13.049999999999997</v>
+        <v>15.049999999999997</v>
       </c>
       <c r="D15" s="45" t="s">
         <v>126</v>
@@ -11342,8 +11614,27 @@
       <c r="CK15" s="5">
         <v>23.35</v>
       </c>
-    </row>
-    <row r="16" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL15" s="5">
+        <v>21.35</v>
+      </c>
+      <c r="CM15" s="5">
+        <v>23.5</v>
+      </c>
+      <c r="CN15" s="5"/>
+      <c r="CO15" s="5"/>
+      <c r="CP15" s="5"/>
+      <c r="CQ15" s="5"/>
+      <c r="CR15" s="5"/>
+      <c r="CS15" s="5"/>
+      <c r="CT15" s="5"/>
+      <c r="CU15" s="5"/>
+      <c r="CV15" s="5"/>
+      <c r="CW15" s="5"/>
+      <c r="CX15" s="5"/>
+      <c r="CY15" s="5"/>
+      <c r="CZ15" s="5"/>
+    </row>
+    <row r="16" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <f t="shared" si="0"/>
         <v>552</v>
@@ -11612,8 +11903,27 @@
       <c r="CK16" s="5">
         <v>696.15</v>
       </c>
-    </row>
-    <row r="17" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL16" s="5">
+        <v>677.3</v>
+      </c>
+      <c r="CM16" s="5">
+        <v>709.55</v>
+      </c>
+      <c r="CN16" s="5"/>
+      <c r="CO16" s="5"/>
+      <c r="CP16" s="5"/>
+      <c r="CQ16" s="5"/>
+      <c r="CR16" s="5"/>
+      <c r="CS16" s="5"/>
+      <c r="CT16" s="5"/>
+      <c r="CU16" s="5"/>
+      <c r="CV16" s="5"/>
+      <c r="CW16" s="5"/>
+      <c r="CX16" s="5"/>
+      <c r="CY16" s="5"/>
+      <c r="CZ16" s="5"/>
+    </row>
+    <row r="17" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <f t="shared" si="0"/>
         <v>433</v>
@@ -11882,8 +12192,27 @@
       <c r="CK17" s="5">
         <v>489</v>
       </c>
-    </row>
-    <row r="18" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL17" s="5">
+        <v>478.7</v>
+      </c>
+      <c r="CM17" s="5">
+        <v>502</v>
+      </c>
+      <c r="CN17" s="5"/>
+      <c r="CO17" s="5"/>
+      <c r="CP17" s="5"/>
+      <c r="CQ17" s="5"/>
+      <c r="CR17" s="5"/>
+      <c r="CS17" s="5"/>
+      <c r="CT17" s="5"/>
+      <c r="CU17" s="5"/>
+      <c r="CV17" s="5"/>
+      <c r="CW17" s="5"/>
+      <c r="CX17" s="5"/>
+      <c r="CY17" s="5"/>
+      <c r="CZ17" s="5"/>
+    </row>
+    <row r="18" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <f t="shared" si="0"/>
         <v>178.8</v>
@@ -12152,19 +12481,38 @@
       <c r="CK18" s="5">
         <v>255.55</v>
       </c>
-    </row>
-    <row r="19" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL18" s="5">
+        <v>249.7</v>
+      </c>
+      <c r="CM18" s="5">
+        <v>255</v>
+      </c>
+      <c r="CN18" s="5"/>
+      <c r="CO18" s="5"/>
+      <c r="CP18" s="5"/>
+      <c r="CQ18" s="5"/>
+      <c r="CR18" s="5"/>
+      <c r="CS18" s="5"/>
+      <c r="CT18" s="5"/>
+      <c r="CU18" s="5"/>
+      <c r="CV18" s="5"/>
+      <c r="CW18" s="5"/>
+      <c r="CX18" s="5"/>
+      <c r="CY18" s="5"/>
+      <c r="CZ18" s="5"/>
+    </row>
+    <row r="19" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <f t="shared" si="0"/>
         <v>440.7</v>
       </c>
       <c r="B19" s="12">
         <f t="shared" si="1"/>
-        <v>759</v>
+        <v>762</v>
       </c>
       <c r="C19" s="12">
         <f t="shared" si="2"/>
-        <v>318.3</v>
+        <v>321.3</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -12422,11 +12770,30 @@
       <c r="CK19" s="5">
         <v>747.65</v>
       </c>
-    </row>
-    <row r="20" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL19" s="5">
+        <v>744.15</v>
+      </c>
+      <c r="CM19" s="5">
+        <v>762</v>
+      </c>
+      <c r="CN19" s="5"/>
+      <c r="CO19" s="5"/>
+      <c r="CP19" s="5"/>
+      <c r="CQ19" s="5"/>
+      <c r="CR19" s="5"/>
+      <c r="CS19" s="5"/>
+      <c r="CT19" s="5"/>
+      <c r="CU19" s="5"/>
+      <c r="CV19" s="5"/>
+      <c r="CW19" s="5"/>
+      <c r="CX19" s="5"/>
+      <c r="CY19" s="5"/>
+      <c r="CZ19" s="5"/>
+    </row>
+    <row r="20" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <f t="shared" si="0"/>
-        <v>660.75</v>
+        <v>653.25</v>
       </c>
       <c r="B20" s="12">
         <f t="shared" si="1"/>
@@ -12434,7 +12801,7 @@
       </c>
       <c r="C20" s="12">
         <f t="shared" si="2"/>
-        <v>135.20000000000005</v>
+        <v>142.70000000000005</v>
       </c>
       <c r="D20" s="44" t="s">
         <v>104</v>
@@ -12692,8 +13059,27 @@
       <c r="CK20" s="5">
         <v>668</v>
       </c>
-    </row>
-    <row r="21" spans="1:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CL20" s="5">
+        <v>653.25</v>
+      </c>
+      <c r="CM20" s="5">
+        <v>685.25</v>
+      </c>
+      <c r="CN20" s="5"/>
+      <c r="CO20" s="5"/>
+      <c r="CP20" s="5"/>
+      <c r="CQ20" s="5"/>
+      <c r="CR20" s="5"/>
+      <c r="CS20" s="5"/>
+      <c r="CT20" s="5"/>
+      <c r="CU20" s="5"/>
+      <c r="CV20" s="5"/>
+      <c r="CW20" s="5"/>
+      <c r="CX20" s="5"/>
+      <c r="CY20" s="5"/>
+      <c r="CZ20" s="5"/>
+    </row>
+    <row r="21" spans="1:104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <f t="shared" si="0"/>
         <v>376.7</v>
@@ -12962,8 +13348,27 @@
       <c r="CK21" s="5">
         <v>517.29999999999995</v>
       </c>
-    </row>
-    <row r="22" spans="1:89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CL21" s="5">
+        <v>497.35</v>
+      </c>
+      <c r="CM21" s="5">
+        <v>540</v>
+      </c>
+      <c r="CN21" s="5"/>
+      <c r="CO21" s="5"/>
+      <c r="CP21" s="5"/>
+      <c r="CQ21" s="5"/>
+      <c r="CR21" s="5"/>
+      <c r="CS21" s="5"/>
+      <c r="CT21" s="5"/>
+      <c r="CU21" s="5"/>
+      <c r="CV21" s="5"/>
+      <c r="CW21" s="5"/>
+      <c r="CX21" s="5"/>
+      <c r="CY21" s="5"/>
+      <c r="CZ21" s="5"/>
+    </row>
+    <row r="22" spans="1:104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <f t="shared" si="0"/>
         <v>315.2</v>
@@ -13178,11 +13583,30 @@
       <c r="CK22" s="5">
         <v>362.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL22" s="5">
+        <v>350.85</v>
+      </c>
+      <c r="CM22" s="5">
+        <v>376.6</v>
+      </c>
+      <c r="CN22" s="5"/>
+      <c r="CO22" s="5"/>
+      <c r="CP22" s="5"/>
+      <c r="CQ22" s="5"/>
+      <c r="CR22" s="5"/>
+      <c r="CS22" s="5"/>
+      <c r="CT22" s="5"/>
+      <c r="CU22" s="5"/>
+      <c r="CV22" s="5"/>
+      <c r="CW22" s="5"/>
+      <c r="CX22" s="5"/>
+      <c r="CY22" s="5"/>
+      <c r="CZ22" s="5"/>
+    </row>
+    <row r="23" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
-        <v>52.8</v>
+        <v>50.85</v>
       </c>
       <c r="B23" s="12">
         <f t="shared" si="1"/>
@@ -13190,7 +13614,7 @@
       </c>
       <c r="C23" s="12">
         <f t="shared" si="2"/>
-        <v>32.850000000000009</v>
+        <v>34.800000000000004</v>
       </c>
       <c r="D23" s="45" t="s">
         <v>127</v>
@@ -13440,8 +13864,27 @@
       <c r="CK23" s="5">
         <v>53.3</v>
       </c>
-    </row>
-    <row r="24" spans="1:89" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CL23" s="5">
+        <v>50.85</v>
+      </c>
+      <c r="CM23" s="5">
+        <v>53</v>
+      </c>
+      <c r="CN23" s="5"/>
+      <c r="CO23" s="5"/>
+      <c r="CP23" s="5"/>
+      <c r="CQ23" s="5"/>
+      <c r="CR23" s="5"/>
+      <c r="CS23" s="5"/>
+      <c r="CT23" s="5"/>
+      <c r="CU23" s="5"/>
+      <c r="CV23" s="5"/>
+      <c r="CW23" s="5"/>
+      <c r="CX23" s="5"/>
+      <c r="CY23" s="5"/>
+      <c r="CZ23" s="5"/>
+    </row>
+    <row r="24" spans="1:104" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <f t="shared" si="0"/>
         <v>210.65</v>
@@ -13698,8 +14141,27 @@
       <c r="CK24" s="5">
         <v>226</v>
       </c>
-    </row>
-    <row r="25" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL24" s="5">
+        <v>220.95</v>
+      </c>
+      <c r="CM24" s="5">
+        <v>232.2</v>
+      </c>
+      <c r="CN24" s="5"/>
+      <c r="CO24" s="5"/>
+      <c r="CP24" s="5"/>
+      <c r="CQ24" s="5"/>
+      <c r="CR24" s="5"/>
+      <c r="CS24" s="5"/>
+      <c r="CT24" s="5"/>
+      <c r="CU24" s="5"/>
+      <c r="CV24" s="5"/>
+      <c r="CW24" s="5"/>
+      <c r="CX24" s="5"/>
+      <c r="CY24" s="5"/>
+      <c r="CZ24" s="5"/>
+    </row>
+    <row r="25" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <f t="shared" si="0"/>
         <v>876</v>
@@ -13938,19 +14400,38 @@
       <c r="CK25" s="5">
         <v>1019</v>
       </c>
-    </row>
-    <row r="26" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL25" s="5">
+        <v>1008.5</v>
+      </c>
+      <c r="CM25" s="5">
+        <v>1006.65</v>
+      </c>
+      <c r="CN25" s="5"/>
+      <c r="CO25" s="5"/>
+      <c r="CP25" s="5"/>
+      <c r="CQ25" s="5"/>
+      <c r="CR25" s="5"/>
+      <c r="CS25" s="5"/>
+      <c r="CT25" s="5"/>
+      <c r="CU25" s="5"/>
+      <c r="CV25" s="5"/>
+      <c r="CW25" s="5"/>
+      <c r="CX25" s="5"/>
+      <c r="CY25" s="5"/>
+      <c r="CZ25" s="5"/>
+    </row>
+    <row r="26" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <f t="shared" si="0"/>
         <v>83.1</v>
       </c>
       <c r="B26" s="12">
         <f t="shared" si="1"/>
-        <v>107.4</v>
+        <v>115.5</v>
       </c>
       <c r="C26" s="12">
         <f t="shared" si="2"/>
-        <v>24.300000000000011</v>
+        <v>32.400000000000006</v>
       </c>
       <c r="D26" s="45" t="s">
         <v>252</v>
@@ -14166,8 +14647,27 @@
       <c r="CK26" s="5">
         <v>104.35</v>
       </c>
-    </row>
-    <row r="27" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL26" s="5">
+        <v>101</v>
+      </c>
+      <c r="CM26" s="5">
+        <v>115.5</v>
+      </c>
+      <c r="CN26" s="5"/>
+      <c r="CO26" s="5"/>
+      <c r="CP26" s="5"/>
+      <c r="CQ26" s="5"/>
+      <c r="CR26" s="5"/>
+      <c r="CS26" s="5"/>
+      <c r="CT26" s="5"/>
+      <c r="CU26" s="5"/>
+      <c r="CV26" s="5"/>
+      <c r="CW26" s="5"/>
+      <c r="CX26" s="5"/>
+      <c r="CY26" s="5"/>
+      <c r="CZ26" s="5"/>
+    </row>
+    <row r="27" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <f t="shared" si="0"/>
         <v>36.200000000000003</v>
@@ -14394,8 +14894,27 @@
       <c r="CK27" s="5">
         <v>39.799999999999997</v>
       </c>
-    </row>
-    <row r="28" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL27" s="5">
+        <v>38.450000000000003</v>
+      </c>
+      <c r="CM27" s="5">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="CN27" s="5"/>
+      <c r="CO27" s="5"/>
+      <c r="CP27" s="5"/>
+      <c r="CQ27" s="5"/>
+      <c r="CR27" s="5"/>
+      <c r="CS27" s="5"/>
+      <c r="CT27" s="5"/>
+      <c r="CU27" s="5"/>
+      <c r="CV27" s="5"/>
+      <c r="CW27" s="5"/>
+      <c r="CX27" s="5"/>
+      <c r="CY27" s="5"/>
+      <c r="CZ27" s="5"/>
+    </row>
+    <row r="28" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <f t="shared" si="0"/>
         <v>111.95</v>
@@ -14622,8 +15141,27 @@
       <c r="CK28" s="5">
         <v>127</v>
       </c>
-    </row>
-    <row r="29" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL28" s="5">
+        <v>123.6</v>
+      </c>
+      <c r="CM28" s="5">
+        <v>128.94999999999999</v>
+      </c>
+      <c r="CN28" s="5"/>
+      <c r="CO28" s="5"/>
+      <c r="CP28" s="5"/>
+      <c r="CQ28" s="5"/>
+      <c r="CR28" s="5"/>
+      <c r="CS28" s="5"/>
+      <c r="CT28" s="5"/>
+      <c r="CU28" s="5"/>
+      <c r="CV28" s="5"/>
+      <c r="CW28" s="5"/>
+      <c r="CX28" s="5"/>
+      <c r="CY28" s="5"/>
+      <c r="CZ28" s="5"/>
+    </row>
+    <row r="29" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <f t="shared" si="0"/>
         <v>62.3</v>
@@ -14850,11 +15388,30 @@
       <c r="CK29" s="5">
         <v>69</v>
       </c>
-    </row>
-    <row r="30" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL29" s="5">
+        <v>66.25</v>
+      </c>
+      <c r="CM29" s="5">
+        <v>71.349999999999994</v>
+      </c>
+      <c r="CN29" s="5"/>
+      <c r="CO29" s="5"/>
+      <c r="CP29" s="5"/>
+      <c r="CQ29" s="5"/>
+      <c r="CR29" s="5"/>
+      <c r="CS29" s="5"/>
+      <c r="CT29" s="5"/>
+      <c r="CU29" s="5"/>
+      <c r="CV29" s="5"/>
+      <c r="CW29" s="5"/>
+      <c r="CX29" s="5"/>
+      <c r="CY29" s="5"/>
+      <c r="CZ29" s="5"/>
+    </row>
+    <row r="30" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <f t="shared" si="0"/>
-        <v>35.25</v>
+        <v>34.450000000000003</v>
       </c>
       <c r="B30" s="12">
         <f t="shared" si="1"/>
@@ -14862,7 +15419,7 @@
       </c>
       <c r="C30" s="12">
         <f t="shared" si="2"/>
-        <v>15.700000000000003</v>
+        <v>16.5</v>
       </c>
       <c r="D30" s="45" t="s">
         <v>256</v>
@@ -15078,8 +15635,27 @@
       <c r="CK30" s="5">
         <v>35.4</v>
       </c>
-    </row>
-    <row r="31" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL30" s="5">
+        <v>34.450000000000003</v>
+      </c>
+      <c r="CM30" s="5">
+        <v>38.1</v>
+      </c>
+      <c r="CN30" s="5"/>
+      <c r="CO30" s="5"/>
+      <c r="CP30" s="5"/>
+      <c r="CQ30" s="5"/>
+      <c r="CR30" s="5"/>
+      <c r="CS30" s="5"/>
+      <c r="CT30" s="5"/>
+      <c r="CU30" s="5"/>
+      <c r="CV30" s="5"/>
+      <c r="CW30" s="5"/>
+      <c r="CX30" s="5"/>
+      <c r="CY30" s="5"/>
+      <c r="CZ30" s="5"/>
+    </row>
+    <row r="31" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
         <v>125.3</v>
@@ -15306,11 +15882,30 @@
       <c r="CK31" s="5">
         <v>136.85</v>
       </c>
-    </row>
-    <row r="32" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL31" s="5">
+        <v>131.30000000000001</v>
+      </c>
+      <c r="CM31" s="5">
+        <v>136.35</v>
+      </c>
+      <c r="CN31" s="5"/>
+      <c r="CO31" s="5"/>
+      <c r="CP31" s="5"/>
+      <c r="CQ31" s="5"/>
+      <c r="CR31" s="5"/>
+      <c r="CS31" s="5"/>
+      <c r="CT31" s="5"/>
+      <c r="CU31" s="5"/>
+      <c r="CV31" s="5"/>
+      <c r="CW31" s="5"/>
+      <c r="CX31" s="5"/>
+      <c r="CY31" s="5"/>
+      <c r="CZ31" s="5"/>
+    </row>
+    <row r="32" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>94.7</v>
       </c>
       <c r="B32" s="12">
         <f t="shared" si="1"/>
@@ -15318,7 +15913,7 @@
       </c>
       <c r="C32" s="12">
         <f t="shared" si="2"/>
-        <v>25.799999999999997</v>
+        <v>27.099999999999994</v>
       </c>
       <c r="D32" s="45" t="s">
         <v>268</v>
@@ -15522,8 +16117,27 @@
       <c r="CK32" s="5">
         <v>97.4</v>
       </c>
-    </row>
-    <row r="33" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL32" s="5">
+        <v>94.7</v>
+      </c>
+      <c r="CM32" s="5">
+        <v>97.5</v>
+      </c>
+      <c r="CN32" s="5"/>
+      <c r="CO32" s="5"/>
+      <c r="CP32" s="5"/>
+      <c r="CQ32" s="5"/>
+      <c r="CR32" s="5"/>
+      <c r="CS32" s="5"/>
+      <c r="CT32" s="5"/>
+      <c r="CU32" s="5"/>
+      <c r="CV32" s="5"/>
+      <c r="CW32" s="5"/>
+      <c r="CX32" s="5"/>
+      <c r="CY32" s="5"/>
+      <c r="CZ32" s="5"/>
+    </row>
+    <row r="33" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <f t="shared" si="0"/>
         <v>56.75</v>
@@ -15726,19 +16340,38 @@
       <c r="CK33" s="5">
         <v>67.75</v>
       </c>
-    </row>
-    <row r="34" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL33" s="5">
+        <v>63.25</v>
+      </c>
+      <c r="CM33" s="5">
+        <v>67.7</v>
+      </c>
+      <c r="CN33" s="5"/>
+      <c r="CO33" s="5"/>
+      <c r="CP33" s="5"/>
+      <c r="CQ33" s="5"/>
+      <c r="CR33" s="5"/>
+      <c r="CS33" s="5"/>
+      <c r="CT33" s="5"/>
+      <c r="CU33" s="5"/>
+      <c r="CV33" s="5"/>
+      <c r="CW33" s="5"/>
+      <c r="CX33" s="5"/>
+      <c r="CY33" s="5"/>
+      <c r="CZ33" s="5"/>
+    </row>
+    <row r="34" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <f t="shared" si="0"/>
         <v>167.9</v>
       </c>
       <c r="B34" s="12">
         <f t="shared" si="1"/>
-        <v>264.60000000000002</v>
+        <v>294.3</v>
       </c>
       <c r="C34" s="12">
         <f t="shared" ref="C34" si="3">B34-A34</f>
-        <v>96.700000000000017</v>
+        <v>126.4</v>
       </c>
       <c r="D34" s="45" t="s">
         <v>280</v>
@@ -15924,11 +16557,30 @@
       <c r="CK34" s="5">
         <v>264.60000000000002</v>
       </c>
-    </row>
-    <row r="35" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL34" s="5">
+        <v>255.7</v>
+      </c>
+      <c r="CM34" s="5">
+        <v>294.3</v>
+      </c>
+      <c r="CN34" s="5"/>
+      <c r="CO34" s="5"/>
+      <c r="CP34" s="5"/>
+      <c r="CQ34" s="5"/>
+      <c r="CR34" s="5"/>
+      <c r="CS34" s="5"/>
+      <c r="CT34" s="5"/>
+      <c r="CU34" s="5"/>
+      <c r="CV34" s="5"/>
+      <c r="CW34" s="5"/>
+      <c r="CX34" s="5"/>
+      <c r="CY34" s="5"/>
+      <c r="CZ34" s="5"/>
+    </row>
+    <row r="35" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <f t="shared" si="0"/>
-        <v>392.1</v>
+        <v>388</v>
       </c>
       <c r="B35" s="12">
         <f t="shared" si="1"/>
@@ -15936,7 +16588,7 @@
       </c>
       <c r="C35" s="12">
         <f t="shared" ref="C35" si="4">B35-A35</f>
-        <v>127.89999999999998</v>
+        <v>132</v>
       </c>
       <c r="D35" s="45" t="s">
         <v>289</v>
@@ -16100,8 +16752,27 @@
       <c r="CK35" s="5">
         <v>394</v>
       </c>
-    </row>
-    <row r="36" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL35" s="5">
+        <v>388</v>
+      </c>
+      <c r="CM35" s="5">
+        <v>397.15</v>
+      </c>
+      <c r="CN35" s="5"/>
+      <c r="CO35" s="5"/>
+      <c r="CP35" s="5"/>
+      <c r="CQ35" s="5"/>
+      <c r="CR35" s="5"/>
+      <c r="CS35" s="5"/>
+      <c r="CT35" s="5"/>
+      <c r="CU35" s="5"/>
+      <c r="CV35" s="5"/>
+      <c r="CW35" s="5"/>
+      <c r="CX35" s="5"/>
+      <c r="CY35" s="5"/>
+      <c r="CZ35" s="5"/>
+    </row>
+    <row r="36" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <f t="shared" si="0"/>
         <v>226</v>
@@ -16266,8 +16937,27 @@
       <c r="CK36" s="5">
         <v>370</v>
       </c>
-    </row>
-    <row r="37" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL36" s="5">
+        <v>351.55</v>
+      </c>
+      <c r="CM36" s="5">
+        <v>367.3</v>
+      </c>
+      <c r="CN36" s="5"/>
+      <c r="CO36" s="5"/>
+      <c r="CP36" s="5"/>
+      <c r="CQ36" s="5"/>
+      <c r="CR36" s="5"/>
+      <c r="CS36" s="5"/>
+      <c r="CT36" s="5"/>
+      <c r="CU36" s="5"/>
+      <c r="CV36" s="5"/>
+      <c r="CW36" s="5"/>
+      <c r="CX36" s="5"/>
+      <c r="CY36" s="5"/>
+      <c r="CZ36" s="5"/>
+    </row>
+    <row r="37" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <f t="shared" si="0"/>
         <v>75.2</v>
@@ -16424,8 +17114,27 @@
       <c r="CK37" s="5">
         <v>79.95</v>
       </c>
-    </row>
-    <row r="38" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL37" s="5">
+        <v>78.8</v>
+      </c>
+      <c r="CM37" s="5">
+        <v>79.7</v>
+      </c>
+      <c r="CN37" s="5"/>
+      <c r="CO37" s="5"/>
+      <c r="CP37" s="5"/>
+      <c r="CQ37" s="5"/>
+      <c r="CR37" s="5"/>
+      <c r="CS37" s="5"/>
+      <c r="CT37" s="5"/>
+      <c r="CU37" s="5"/>
+      <c r="CV37" s="5"/>
+      <c r="CW37" s="5"/>
+      <c r="CX37" s="5"/>
+      <c r="CY37" s="5"/>
+      <c r="CZ37" s="5"/>
+    </row>
+    <row r="38" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <f t="shared" si="0"/>
         <v>407.05</v>
@@ -16582,8 +17291,27 @@
       <c r="CK38" s="5">
         <v>423.75</v>
       </c>
-    </row>
-    <row r="39" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL38" s="5">
+        <v>412.3</v>
+      </c>
+      <c r="CM38" s="5">
+        <v>420</v>
+      </c>
+      <c r="CN38" s="5"/>
+      <c r="CO38" s="5"/>
+      <c r="CP38" s="5"/>
+      <c r="CQ38" s="5"/>
+      <c r="CR38" s="5"/>
+      <c r="CS38" s="5"/>
+      <c r="CT38" s="5"/>
+      <c r="CU38" s="5"/>
+      <c r="CV38" s="5"/>
+      <c r="CW38" s="5"/>
+      <c r="CX38" s="5"/>
+      <c r="CY38" s="5"/>
+      <c r="CZ38" s="5"/>
+    </row>
+    <row r="39" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <f t="shared" si="0"/>
         <v>175.2</v>
@@ -16736,11 +17464,30 @@
       <c r="CK39" s="5">
         <v>206.5</v>
       </c>
-    </row>
-    <row r="40" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL39" s="5">
+        <v>192.2</v>
+      </c>
+      <c r="CM39" s="5">
+        <v>203.55</v>
+      </c>
+      <c r="CN39" s="5"/>
+      <c r="CO39" s="5"/>
+      <c r="CP39" s="5"/>
+      <c r="CQ39" s="5"/>
+      <c r="CR39" s="5"/>
+      <c r="CS39" s="5"/>
+      <c r="CT39" s="5"/>
+      <c r="CU39" s="5"/>
+      <c r="CV39" s="5"/>
+      <c r="CW39" s="5"/>
+      <c r="CX39" s="5"/>
+      <c r="CY39" s="5"/>
+      <c r="CZ39" s="5"/>
+    </row>
+    <row r="40" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>34.5</v>
       </c>
       <c r="B40" s="12">
         <f t="shared" si="1"/>
@@ -16748,7 +17495,7 @@
       </c>
       <c r="C40" s="12">
         <f t="shared" ref="C40:C43" si="9">B40-A40</f>
-        <v>4.4500000000000028</v>
+        <v>4.9500000000000028</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>306</v>
@@ -16886,8 +17633,27 @@
       <c r="CK40" s="5">
         <v>36.1</v>
       </c>
-    </row>
-    <row r="41" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL40" s="5">
+        <v>34.5</v>
+      </c>
+      <c r="CM40" s="5">
+        <v>36.65</v>
+      </c>
+      <c r="CN40" s="5"/>
+      <c r="CO40" s="5"/>
+      <c r="CP40" s="5"/>
+      <c r="CQ40" s="5"/>
+      <c r="CR40" s="5"/>
+      <c r="CS40" s="5"/>
+      <c r="CT40" s="5"/>
+      <c r="CU40" s="5"/>
+      <c r="CV40" s="5"/>
+      <c r="CW40" s="5"/>
+      <c r="CX40" s="5"/>
+      <c r="CY40" s="5"/>
+      <c r="CZ40" s="5"/>
+    </row>
+    <row r="41" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <f t="shared" si="0"/>
         <v>552.04999999999995</v>
@@ -17034,19 +17800,38 @@
       <c r="CK41" s="5">
         <v>665</v>
       </c>
-    </row>
-    <row r="42" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL41" s="5">
+        <v>627.6</v>
+      </c>
+      <c r="CM41" s="5">
+        <v>659.85</v>
+      </c>
+      <c r="CN41" s="5"/>
+      <c r="CO41" s="5"/>
+      <c r="CP41" s="5"/>
+      <c r="CQ41" s="5"/>
+      <c r="CR41" s="5"/>
+      <c r="CS41" s="5"/>
+      <c r="CT41" s="5"/>
+      <c r="CU41" s="5"/>
+      <c r="CV41" s="5"/>
+      <c r="CW41" s="5"/>
+      <c r="CX41" s="5"/>
+      <c r="CY41" s="5"/>
+      <c r="CZ41" s="5"/>
+    </row>
+    <row r="42" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <f t="shared" si="0"/>
         <v>810.6</v>
       </c>
       <c r="B42" s="12">
         <f t="shared" si="1"/>
-        <v>861</v>
+        <v>866.95</v>
       </c>
       <c r="C42" s="12">
         <f t="shared" si="9"/>
-        <v>50.399999999999977</v>
+        <v>56.350000000000023</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>308</v>
@@ -17182,19 +17967,38 @@
       <c r="CK42" s="5">
         <v>861</v>
       </c>
-    </row>
-    <row r="43" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL42" s="5">
+        <v>847.05</v>
+      </c>
+      <c r="CM42" s="5">
+        <v>866.95</v>
+      </c>
+      <c r="CN42" s="5"/>
+      <c r="CO42" s="5"/>
+      <c r="CP42" s="5"/>
+      <c r="CQ42" s="5"/>
+      <c r="CR42" s="5"/>
+      <c r="CS42" s="5"/>
+      <c r="CT42" s="5"/>
+      <c r="CU42" s="5"/>
+      <c r="CV42" s="5"/>
+      <c r="CW42" s="5"/>
+      <c r="CX42" s="5"/>
+      <c r="CY42" s="5"/>
+      <c r="CZ42" s="5"/>
+    </row>
+    <row r="43" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <f t="shared" si="0"/>
-        <v>134.9</v>
+        <v>134</v>
       </c>
       <c r="B43" s="12">
         <f t="shared" si="1"/>
-        <v>146</v>
+        <v>146.1</v>
       </c>
       <c r="C43" s="12">
         <f t="shared" si="9"/>
-        <v>11.099999999999994</v>
+        <v>12.099999999999994</v>
       </c>
       <c r="D43" s="45" t="s">
         <v>309</v>
@@ -17328,11 +18132,30 @@
       <c r="CK43" s="5">
         <v>142.25</v>
       </c>
-    </row>
-    <row r="44" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL43" s="5">
+        <v>134</v>
+      </c>
+      <c r="CM43" s="5">
+        <v>146.1</v>
+      </c>
+      <c r="CN43" s="5"/>
+      <c r="CO43" s="5"/>
+      <c r="CP43" s="5"/>
+      <c r="CQ43" s="5"/>
+      <c r="CR43" s="5"/>
+      <c r="CS43" s="5"/>
+      <c r="CT43" s="5"/>
+      <c r="CU43" s="5"/>
+      <c r="CV43" s="5"/>
+      <c r="CW43" s="5"/>
+      <c r="CX43" s="5"/>
+      <c r="CY43" s="5"/>
+      <c r="CZ43" s="5"/>
+    </row>
+    <row r="44" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <f t="shared" si="0"/>
-        <v>545.04999999999995</v>
+        <v>538.4</v>
       </c>
       <c r="B44" s="12">
         <f t="shared" si="1"/>
@@ -17340,7 +18163,7 @@
       </c>
       <c r="C44" s="12">
         <f t="shared" ref="C44" si="10">B44-A44</f>
-        <v>224.95000000000005</v>
+        <v>231.60000000000002</v>
       </c>
       <c r="D44" s="45" t="s">
         <v>311</v>
@@ -17468,8 +18291,27 @@
       <c r="CK44" s="5">
         <v>545.04999999999995</v>
       </c>
-    </row>
-    <row r="45" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL44" s="5">
+        <v>538.4</v>
+      </c>
+      <c r="CM44" s="5">
+        <v>596.1</v>
+      </c>
+      <c r="CN44" s="5"/>
+      <c r="CO44" s="5"/>
+      <c r="CP44" s="5"/>
+      <c r="CQ44" s="5"/>
+      <c r="CR44" s="5"/>
+      <c r="CS44" s="5"/>
+      <c r="CT44" s="5"/>
+      <c r="CU44" s="5"/>
+      <c r="CV44" s="5"/>
+      <c r="CW44" s="5"/>
+      <c r="CX44" s="5"/>
+      <c r="CY44" s="5"/>
+      <c r="CZ44" s="5"/>
+    </row>
+    <row r="45" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <f t="shared" si="0"/>
         <v>101.4</v>
@@ -17600,11 +18442,30 @@
       <c r="CK45" s="5">
         <v>106.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="CL45" s="5">
+        <v>101.4</v>
+      </c>
+      <c r="CM45" s="5">
+        <v>105.65</v>
+      </c>
+      <c r="CN45" s="5"/>
+      <c r="CO45" s="5"/>
+      <c r="CP45" s="5"/>
+      <c r="CQ45" s="5"/>
+      <c r="CR45" s="5"/>
+      <c r="CS45" s="5"/>
+      <c r="CT45" s="5"/>
+      <c r="CU45" s="5"/>
+      <c r="CV45" s="5"/>
+      <c r="CW45" s="5"/>
+      <c r="CX45" s="5"/>
+      <c r="CY45" s="5"/>
+      <c r="CZ45" s="5"/>
+    </row>
+    <row r="46" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <f t="shared" si="0"/>
-        <v>135.1</v>
+        <v>132.19999999999999</v>
       </c>
       <c r="B46" s="12">
         <f t="shared" si="1"/>
@@ -17612,7 +18473,7 @@
       </c>
       <c r="C46" s="12">
         <f t="shared" ref="C46" si="12">B46-A46</f>
-        <v>9.9000000000000057</v>
+        <v>12.800000000000011</v>
       </c>
       <c r="D46" s="45" t="s">
         <v>324</v>
@@ -17718,6 +18579,25 @@
       <c r="CK46" s="5">
         <v>135.6</v>
       </c>
+      <c r="CL46" s="5">
+        <v>132.19999999999999</v>
+      </c>
+      <c r="CM46" s="5">
+        <v>135.4</v>
+      </c>
+      <c r="CN46" s="5"/>
+      <c r="CO46" s="5"/>
+      <c r="CP46" s="5"/>
+      <c r="CQ46" s="5"/>
+      <c r="CR46" s="5"/>
+      <c r="CS46" s="5"/>
+      <c r="CT46" s="5"/>
+      <c r="CU46" s="5"/>
+      <c r="CV46" s="5"/>
+      <c r="CW46" s="5"/>
+      <c r="CX46" s="5"/>
+      <c r="CY46" s="5"/>
+      <c r="CZ46" s="5"/>
     </row>
   </sheetData>
   <sortState ref="L1:L37">

</xml_diff>

<commit_message>
Added details for 21/12/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="334">
   <si>
     <t>Date</t>
   </si>
@@ -1018,6 +1018,15 @@
   </si>
   <si>
     <t>19/12/2017</t>
+  </si>
+  <si>
+    <t>20/12/2017</t>
+  </si>
+  <si>
+    <t>SCI</t>
+  </si>
+  <si>
+    <t>21/12/2017</t>
   </si>
 </sst>
 </file>
@@ -7267,11 +7276,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CZ46"/>
+  <dimension ref="A1:CZ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="CJ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CM46" sqref="CM46"/>
+      <selection pane="topRight" activeCell="CU24" sqref="CU24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7326,6 +7335,8 @@
     <col min="84" max="84" width="13" customWidth="1"/>
     <col min="85" max="86" width="13" bestFit="1" customWidth="1"/>
     <col min="87" max="91" width="14" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:104" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7602,8 +7613,12 @@
       <c r="CM1" s="49" t="s">
         <v>330</v>
       </c>
-      <c r="CN1" s="27"/>
-      <c r="CO1" s="27"/>
+      <c r="CN1" s="49" t="s">
+        <v>331</v>
+      </c>
+      <c r="CO1" s="49" t="s">
+        <v>333</v>
+      </c>
       <c r="CP1" s="27"/>
       <c r="CQ1" s="27"/>
       <c r="CR1" s="27"/>
@@ -7885,8 +7900,12 @@
       <c r="CM2" s="5">
         <v>320</v>
       </c>
-      <c r="CN2" s="5"/>
-      <c r="CO2" s="5"/>
+      <c r="CN2" s="5">
+        <v>317.35000000000002</v>
+      </c>
+      <c r="CO2" s="5">
+        <v>316.3</v>
+      </c>
       <c r="CP2" s="5"/>
       <c r="CQ2" s="5"/>
       <c r="CR2" s="5"/>
@@ -8168,8 +8187,12 @@
       <c r="CM3" s="5">
         <v>313.2</v>
       </c>
-      <c r="CN3" s="5"/>
-      <c r="CO3" s="5"/>
+      <c r="CN3" s="5">
+        <v>315.7</v>
+      </c>
+      <c r="CO3" s="5">
+        <v>313.95</v>
+      </c>
       <c r="CP3" s="5"/>
       <c r="CQ3" s="5"/>
       <c r="CR3" s="5"/>
@@ -8457,8 +8480,12 @@
       <c r="CM4" s="5">
         <v>264.2</v>
       </c>
-      <c r="CN4" s="5"/>
-      <c r="CO4" s="5"/>
+      <c r="CN4" s="5">
+        <v>263.14999999999998</v>
+      </c>
+      <c r="CO4" s="5">
+        <v>263.05</v>
+      </c>
       <c r="CP4" s="5"/>
       <c r="CQ4" s="5"/>
       <c r="CR4" s="5"/>
@@ -8746,8 +8773,12 @@
       <c r="CM5" s="5">
         <v>926.85</v>
       </c>
-      <c r="CN5" s="5"/>
-      <c r="CO5" s="5"/>
+      <c r="CN5" s="5">
+        <v>918.75</v>
+      </c>
+      <c r="CO5" s="5">
+        <v>913</v>
+      </c>
       <c r="CP5" s="5"/>
       <c r="CQ5" s="5"/>
       <c r="CR5" s="5"/>
@@ -9035,8 +9066,12 @@
       <c r="CM6" s="5">
         <v>268.35000000000002</v>
       </c>
-      <c r="CN6" s="5"/>
-      <c r="CO6" s="5"/>
+      <c r="CN6" s="5">
+        <v>269.3</v>
+      </c>
+      <c r="CO6" s="5">
+        <v>267.60000000000002</v>
+      </c>
       <c r="CP6" s="5"/>
       <c r="CQ6" s="5"/>
       <c r="CR6" s="5"/>
@@ -9056,11 +9091,11 @@
       </c>
       <c r="B7" s="12">
         <f t="shared" si="1"/>
-        <v>19.350000000000001</v>
+        <v>19.95</v>
       </c>
       <c r="C7" s="12">
         <f t="shared" si="2"/>
-        <v>3.7500000000000018</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="D7" s="45" t="s">
         <v>19</v>
@@ -9324,8 +9359,12 @@
       <c r="CM7" s="5">
         <v>17.8</v>
       </c>
-      <c r="CN7" s="5"/>
-      <c r="CO7" s="5"/>
+      <c r="CN7" s="5">
+        <v>18.3</v>
+      </c>
+      <c r="CO7" s="5">
+        <v>19.95</v>
+      </c>
       <c r="CP7" s="5"/>
       <c r="CQ7" s="5"/>
       <c r="CR7" s="5"/>
@@ -9613,8 +9652,12 @@
       <c r="CM8" s="5">
         <v>83.4</v>
       </c>
-      <c r="CN8" s="5"/>
-      <c r="CO8" s="5"/>
+      <c r="CN8" s="5">
+        <v>84.75</v>
+      </c>
+      <c r="CO8" s="5">
+        <v>86.75</v>
+      </c>
       <c r="CP8" s="5"/>
       <c r="CQ8" s="5"/>
       <c r="CR8" s="5"/>
@@ -9894,8 +9937,12 @@
       <c r="CM9" s="28">
         <v>53.65</v>
       </c>
-      <c r="CN9" s="28"/>
-      <c r="CO9" s="28"/>
+      <c r="CN9" s="28">
+        <v>53.85</v>
+      </c>
+      <c r="CO9" s="28">
+        <v>55.15</v>
+      </c>
       <c r="CP9" s="28"/>
       <c r="CQ9" s="28"/>
       <c r="CR9" s="28"/>
@@ -10183,8 +10230,12 @@
       <c r="CM10" s="5">
         <v>37</v>
       </c>
-      <c r="CN10" s="5"/>
-      <c r="CO10" s="5"/>
+      <c r="CN10" s="5">
+        <v>39.15</v>
+      </c>
+      <c r="CO10" s="5">
+        <v>40.200000000000003</v>
+      </c>
       <c r="CP10" s="5"/>
       <c r="CQ10" s="5"/>
       <c r="CR10" s="5"/>
@@ -10472,8 +10523,12 @@
       <c r="CM11" s="5">
         <v>98.55</v>
       </c>
-      <c r="CN11" s="5"/>
-      <c r="CO11" s="5"/>
+      <c r="CN11" s="5">
+        <v>98.05</v>
+      </c>
+      <c r="CO11" s="5">
+        <v>101.05</v>
+      </c>
       <c r="CP11" s="5"/>
       <c r="CQ11" s="5"/>
       <c r="CR11" s="5"/>
@@ -10761,8 +10816,12 @@
       <c r="CM12" s="5">
         <v>89.95</v>
       </c>
-      <c r="CN12" s="5"/>
-      <c r="CO12" s="5"/>
+      <c r="CN12" s="5">
+        <v>90.05</v>
+      </c>
+      <c r="CO12" s="5">
+        <v>91.35</v>
+      </c>
       <c r="CP12" s="5"/>
       <c r="CQ12" s="5"/>
       <c r="CR12" s="5"/>
@@ -11050,8 +11109,12 @@
       <c r="CM13" s="5">
         <v>53.05</v>
       </c>
-      <c r="CN13" s="5"/>
-      <c r="CO13" s="5"/>
+      <c r="CN13" s="5">
+        <v>54</v>
+      </c>
+      <c r="CO13" s="5">
+        <v>54.35</v>
+      </c>
       <c r="CP13" s="5"/>
       <c r="CQ13" s="5"/>
       <c r="CR13" s="5"/>
@@ -11339,8 +11402,12 @@
       <c r="CM14" s="5">
         <v>41.7</v>
       </c>
-      <c r="CN14" s="5"/>
-      <c r="CO14" s="5"/>
+      <c r="CN14" s="5">
+        <v>42.3</v>
+      </c>
+      <c r="CO14" s="5">
+        <v>41.15</v>
+      </c>
       <c r="CP14" s="5"/>
       <c r="CQ14" s="5"/>
       <c r="CR14" s="5"/>
@@ -11620,8 +11687,12 @@
       <c r="CM15" s="5">
         <v>23.5</v>
       </c>
-      <c r="CN15" s="5"/>
-      <c r="CO15" s="5"/>
+      <c r="CN15" s="5">
+        <v>23</v>
+      </c>
+      <c r="CO15" s="5">
+        <v>23</v>
+      </c>
       <c r="CP15" s="5"/>
       <c r="CQ15" s="5"/>
       <c r="CR15" s="5"/>
@@ -11909,8 +11980,12 @@
       <c r="CM16" s="5">
         <v>709.55</v>
       </c>
-      <c r="CN16" s="5"/>
-      <c r="CO16" s="5"/>
+      <c r="CN16" s="5">
+        <v>702.2</v>
+      </c>
+      <c r="CO16" s="5">
+        <v>712</v>
+      </c>
       <c r="CP16" s="5"/>
       <c r="CQ16" s="5"/>
       <c r="CR16" s="5"/>
@@ -12198,8 +12273,12 @@
       <c r="CM17" s="5">
         <v>502</v>
       </c>
-      <c r="CN17" s="5"/>
-      <c r="CO17" s="5"/>
+      <c r="CN17" s="5">
+        <v>522.79999999999995</v>
+      </c>
+      <c r="CO17" s="5">
+        <v>521.25</v>
+      </c>
       <c r="CP17" s="5"/>
       <c r="CQ17" s="5"/>
       <c r="CR17" s="5"/>
@@ -12487,8 +12566,12 @@
       <c r="CM18" s="5">
         <v>255</v>
       </c>
-      <c r="CN18" s="5"/>
-      <c r="CO18" s="5"/>
+      <c r="CN18" s="5">
+        <v>261</v>
+      </c>
+      <c r="CO18" s="5">
+        <v>270.3</v>
+      </c>
       <c r="CP18" s="5"/>
       <c r="CQ18" s="5"/>
       <c r="CR18" s="5"/>
@@ -12504,7 +12587,7 @@
     <row r="19" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <f t="shared" si="0"/>
-        <v>440.7</v>
+        <v>395.5</v>
       </c>
       <c r="B19" s="12">
         <f t="shared" si="1"/>
@@ -12512,7 +12595,7 @@
       </c>
       <c r="C19" s="12">
         <f t="shared" si="2"/>
-        <v>321.3</v>
+        <v>366.5</v>
       </c>
       <c r="D19" s="44" t="s">
         <v>48</v>
@@ -12776,8 +12859,12 @@
       <c r="CM19" s="5">
         <v>762</v>
       </c>
-      <c r="CN19" s="5"/>
-      <c r="CO19" s="5"/>
+      <c r="CN19" s="5">
+        <v>758.1</v>
+      </c>
+      <c r="CO19" s="5">
+        <v>395.5</v>
+      </c>
       <c r="CP19" s="5"/>
       <c r="CQ19" s="5"/>
       <c r="CR19" s="5"/>
@@ -13065,8 +13152,12 @@
       <c r="CM20" s="5">
         <v>685.25</v>
       </c>
-      <c r="CN20" s="5"/>
-      <c r="CO20" s="5"/>
+      <c r="CN20" s="5">
+        <v>687.75</v>
+      </c>
+      <c r="CO20" s="5">
+        <v>684.15</v>
+      </c>
       <c r="CP20" s="5"/>
       <c r="CQ20" s="5"/>
       <c r="CR20" s="5"/>
@@ -13354,8 +13445,12 @@
       <c r="CM21" s="5">
         <v>540</v>
       </c>
-      <c r="CN21" s="5"/>
-      <c r="CO21" s="5"/>
+      <c r="CN21" s="5">
+        <v>528.6</v>
+      </c>
+      <c r="CO21" s="5">
+        <v>524.4</v>
+      </c>
       <c r="CP21" s="5"/>
       <c r="CQ21" s="5"/>
       <c r="CR21" s="5"/>
@@ -13589,8 +13684,12 @@
       <c r="CM22" s="5">
         <v>376.6</v>
       </c>
-      <c r="CN22" s="5"/>
-      <c r="CO22" s="5"/>
+      <c r="CN22" s="5">
+        <v>381</v>
+      </c>
+      <c r="CO22" s="5">
+        <v>392</v>
+      </c>
       <c r="CP22" s="5"/>
       <c r="CQ22" s="5"/>
       <c r="CR22" s="5"/>
@@ -13870,8 +13969,12 @@
       <c r="CM23" s="5">
         <v>53</v>
       </c>
-      <c r="CN23" s="5"/>
-      <c r="CO23" s="5"/>
+      <c r="CN23" s="5">
+        <v>56</v>
+      </c>
+      <c r="CO23" s="5">
+        <v>56.8</v>
+      </c>
       <c r="CP23" s="5"/>
       <c r="CQ23" s="5"/>
       <c r="CR23" s="5"/>
@@ -14147,8 +14250,12 @@
       <c r="CM24" s="5">
         <v>232.2</v>
       </c>
-      <c r="CN24" s="5"/>
-      <c r="CO24" s="5"/>
+      <c r="CN24" s="5">
+        <v>237.55</v>
+      </c>
+      <c r="CO24" s="5">
+        <v>236.8</v>
+      </c>
       <c r="CP24" s="5"/>
       <c r="CQ24" s="5"/>
       <c r="CR24" s="5"/>
@@ -14168,11 +14275,11 @@
       </c>
       <c r="B25" s="12">
         <f t="shared" si="1"/>
-        <v>1019</v>
+        <v>1021.5</v>
       </c>
       <c r="C25" s="12">
         <f t="shared" si="2"/>
-        <v>143</v>
+        <v>145.5</v>
       </c>
       <c r="D25" s="46" t="s">
         <v>236</v>
@@ -14406,8 +14513,12 @@
       <c r="CM25" s="5">
         <v>1006.65</v>
       </c>
-      <c r="CN25" s="5"/>
-      <c r="CO25" s="5"/>
+      <c r="CN25" s="5">
+        <v>1016.35</v>
+      </c>
+      <c r="CO25" s="5">
+        <v>1021.5</v>
+      </c>
       <c r="CP25" s="5"/>
       <c r="CQ25" s="5"/>
       <c r="CR25" s="5"/>
@@ -14653,8 +14764,12 @@
       <c r="CM26" s="5">
         <v>115.5</v>
       </c>
-      <c r="CN26" s="5"/>
-      <c r="CO26" s="5"/>
+      <c r="CN26" s="5">
+        <v>113.5</v>
+      </c>
+      <c r="CO26" s="5">
+        <v>110.25</v>
+      </c>
       <c r="CP26" s="5"/>
       <c r="CQ26" s="5"/>
       <c r="CR26" s="5"/>
@@ -14900,8 +15015,12 @@
       <c r="CM27" s="5">
         <v>39.950000000000003</v>
       </c>
-      <c r="CN27" s="5"/>
-      <c r="CO27" s="5"/>
+      <c r="CN27" s="5">
+        <v>40.35</v>
+      </c>
+      <c r="CO27" s="5">
+        <v>40.450000000000003</v>
+      </c>
       <c r="CP27" s="5"/>
       <c r="CQ27" s="5"/>
       <c r="CR27" s="5"/>
@@ -15147,8 +15266,12 @@
       <c r="CM28" s="5">
         <v>128.94999999999999</v>
       </c>
-      <c r="CN28" s="5"/>
-      <c r="CO28" s="5"/>
+      <c r="CN28" s="5">
+        <v>127.55</v>
+      </c>
+      <c r="CO28" s="5">
+        <v>128.5</v>
+      </c>
       <c r="CP28" s="5"/>
       <c r="CQ28" s="5"/>
       <c r="CR28" s="5"/>
@@ -15394,8 +15517,12 @@
       <c r="CM29" s="5">
         <v>71.349999999999994</v>
       </c>
-      <c r="CN29" s="5"/>
-      <c r="CO29" s="5"/>
+      <c r="CN29" s="5">
+        <v>71.05</v>
+      </c>
+      <c r="CO29" s="5">
+        <v>72.849999999999994</v>
+      </c>
       <c r="CP29" s="5"/>
       <c r="CQ29" s="5"/>
       <c r="CR29" s="5"/>
@@ -15641,8 +15768,12 @@
       <c r="CM30" s="5">
         <v>38.1</v>
       </c>
-      <c r="CN30" s="5"/>
-      <c r="CO30" s="5"/>
+      <c r="CN30" s="5">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="CO30" s="5">
+        <v>40.1</v>
+      </c>
       <c r="CP30" s="5"/>
       <c r="CQ30" s="5"/>
       <c r="CR30" s="5"/>
@@ -15888,8 +16019,12 @@
       <c r="CM31" s="5">
         <v>136.35</v>
       </c>
-      <c r="CN31" s="5"/>
-      <c r="CO31" s="5"/>
+      <c r="CN31" s="5">
+        <v>141.30000000000001</v>
+      </c>
+      <c r="CO31" s="5">
+        <v>143.44999999999999</v>
+      </c>
       <c r="CP31" s="5"/>
       <c r="CQ31" s="5"/>
       <c r="CR31" s="5"/>
@@ -16123,8 +16258,12 @@
       <c r="CM32" s="5">
         <v>97.5</v>
       </c>
-      <c r="CN32" s="5"/>
-      <c r="CO32" s="5"/>
+      <c r="CN32" s="5">
+        <v>97.3</v>
+      </c>
+      <c r="CO32" s="5">
+        <v>100.25</v>
+      </c>
       <c r="CP32" s="5"/>
       <c r="CQ32" s="5"/>
       <c r="CR32" s="5"/>
@@ -16144,11 +16283,11 @@
       </c>
       <c r="B33" s="12">
         <f t="shared" si="1"/>
-        <v>67.75</v>
+        <v>74.150000000000006</v>
       </c>
       <c r="C33" s="12">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>17.400000000000006</v>
       </c>
       <c r="D33" s="45" t="s">
         <v>271</v>
@@ -16346,8 +16485,12 @@
       <c r="CM33" s="5">
         <v>67.7</v>
       </c>
-      <c r="CN33" s="5"/>
-      <c r="CO33" s="5"/>
+      <c r="CN33" s="5">
+        <v>72.2</v>
+      </c>
+      <c r="CO33" s="5">
+        <v>74.150000000000006</v>
+      </c>
       <c r="CP33" s="5"/>
       <c r="CQ33" s="5"/>
       <c r="CR33" s="5"/>
@@ -16367,11 +16510,11 @@
       </c>
       <c r="B34" s="12">
         <f t="shared" si="1"/>
-        <v>294.3</v>
+        <v>294.95</v>
       </c>
       <c r="C34" s="12">
         <f t="shared" ref="C34" si="3">B34-A34</f>
-        <v>126.4</v>
+        <v>127.04999999999998</v>
       </c>
       <c r="D34" s="45" t="s">
         <v>280</v>
@@ -16563,8 +16706,12 @@
       <c r="CM34" s="5">
         <v>294.3</v>
       </c>
-      <c r="CN34" s="5"/>
-      <c r="CO34" s="5"/>
+      <c r="CN34" s="5">
+        <v>289.2</v>
+      </c>
+      <c r="CO34" s="5">
+        <v>294.95</v>
+      </c>
       <c r="CP34" s="5"/>
       <c r="CQ34" s="5"/>
       <c r="CR34" s="5"/>
@@ -16758,8 +16905,12 @@
       <c r="CM35" s="5">
         <v>397.15</v>
       </c>
-      <c r="CN35" s="5"/>
-      <c r="CO35" s="5"/>
+      <c r="CN35" s="5">
+        <v>397</v>
+      </c>
+      <c r="CO35" s="5">
+        <v>396</v>
+      </c>
       <c r="CP35" s="5"/>
       <c r="CQ35" s="5"/>
       <c r="CR35" s="5"/>
@@ -16943,8 +17094,12 @@
       <c r="CM36" s="5">
         <v>367.3</v>
       </c>
-      <c r="CN36" s="5"/>
-      <c r="CO36" s="5"/>
+      <c r="CN36" s="5">
+        <v>360.4</v>
+      </c>
+      <c r="CO36" s="5">
+        <v>356.5</v>
+      </c>
       <c r="CP36" s="5"/>
       <c r="CQ36" s="5"/>
       <c r="CR36" s="5"/>
@@ -17120,8 +17275,12 @@
       <c r="CM37" s="5">
         <v>79.7</v>
       </c>
-      <c r="CN37" s="5"/>
-      <c r="CO37" s="5"/>
+      <c r="CN37" s="5">
+        <v>79.7</v>
+      </c>
+      <c r="CO37" s="5">
+        <v>81.5</v>
+      </c>
       <c r="CP37" s="5"/>
       <c r="CQ37" s="5"/>
       <c r="CR37" s="5"/>
@@ -17297,8 +17456,12 @@
       <c r="CM38" s="5">
         <v>420</v>
       </c>
-      <c r="CN38" s="5"/>
-      <c r="CO38" s="5"/>
+      <c r="CN38" s="5">
+        <v>429</v>
+      </c>
+      <c r="CO38" s="5">
+        <v>429.2</v>
+      </c>
       <c r="CP38" s="5"/>
       <c r="CQ38" s="5"/>
       <c r="CR38" s="5"/>
@@ -17318,11 +17481,11 @@
       </c>
       <c r="B39" s="12">
         <f t="shared" si="1"/>
-        <v>215.25</v>
+        <v>225.55</v>
       </c>
       <c r="C39" s="12">
         <f t="shared" ref="C39" si="8">B39-A39</f>
-        <v>40.050000000000011</v>
+        <v>50.350000000000023</v>
       </c>
       <c r="D39" s="45" t="s">
         <v>305</v>
@@ -17470,8 +17633,12 @@
       <c r="CM39" s="5">
         <v>203.55</v>
       </c>
-      <c r="CN39" s="5"/>
-      <c r="CO39" s="5"/>
+      <c r="CN39" s="5">
+        <v>204.8</v>
+      </c>
+      <c r="CO39" s="5">
+        <v>225.55</v>
+      </c>
       <c r="CP39" s="5"/>
       <c r="CQ39" s="5"/>
       <c r="CR39" s="5"/>
@@ -17491,11 +17658,11 @@
       </c>
       <c r="B40" s="12">
         <f t="shared" si="1"/>
-        <v>39.450000000000003</v>
+        <v>39.6</v>
       </c>
       <c r="C40" s="12">
         <f t="shared" ref="C40:C43" si="9">B40-A40</f>
-        <v>4.9500000000000028</v>
+        <v>5.1000000000000014</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>306</v>
@@ -17639,8 +17806,12 @@
       <c r="CM40" s="5">
         <v>36.65</v>
       </c>
-      <c r="CN40" s="5"/>
-      <c r="CO40" s="5"/>
+      <c r="CN40" s="5">
+        <v>37.450000000000003</v>
+      </c>
+      <c r="CO40" s="5">
+        <v>39.6</v>
+      </c>
       <c r="CP40" s="5"/>
       <c r="CQ40" s="5"/>
       <c r="CR40" s="5"/>
@@ -17806,8 +17977,12 @@
       <c r="CM41" s="5">
         <v>659.85</v>
       </c>
-      <c r="CN41" s="5"/>
-      <c r="CO41" s="5"/>
+      <c r="CN41" s="5">
+        <v>642</v>
+      </c>
+      <c r="CO41" s="5">
+        <v>637.65</v>
+      </c>
       <c r="CP41" s="5"/>
       <c r="CQ41" s="5"/>
       <c r="CR41" s="5"/>
@@ -17827,11 +18002,11 @@
       </c>
       <c r="B42" s="12">
         <f t="shared" si="1"/>
-        <v>866.95</v>
+        <v>880</v>
       </c>
       <c r="C42" s="12">
         <f t="shared" si="9"/>
-        <v>56.350000000000023</v>
+        <v>69.399999999999977</v>
       </c>
       <c r="D42" s="45" t="s">
         <v>308</v>
@@ -17973,8 +18148,12 @@
       <c r="CM42" s="5">
         <v>866.95</v>
       </c>
-      <c r="CN42" s="5"/>
-      <c r="CO42" s="5"/>
+      <c r="CN42" s="5">
+        <v>875</v>
+      </c>
+      <c r="CO42" s="5">
+        <v>880</v>
+      </c>
       <c r="CP42" s="5"/>
       <c r="CQ42" s="5"/>
       <c r="CR42" s="5"/>
@@ -17994,11 +18173,11 @@
       </c>
       <c r="B43" s="12">
         <f t="shared" si="1"/>
-        <v>146.1</v>
+        <v>149.94999999999999</v>
       </c>
       <c r="C43" s="12">
         <f t="shared" si="9"/>
-        <v>12.099999999999994</v>
+        <v>15.949999999999989</v>
       </c>
       <c r="D43" s="45" t="s">
         <v>309</v>
@@ -18138,8 +18317,12 @@
       <c r="CM43" s="5">
         <v>146.1</v>
       </c>
-      <c r="CN43" s="5"/>
-      <c r="CO43" s="5"/>
+      <c r="CN43" s="5">
+        <v>146.80000000000001</v>
+      </c>
+      <c r="CO43" s="5">
+        <v>149.94999999999999</v>
+      </c>
       <c r="CP43" s="5"/>
       <c r="CQ43" s="5"/>
       <c r="CR43" s="5"/>
@@ -18297,8 +18480,12 @@
       <c r="CM44" s="5">
         <v>596.1</v>
       </c>
-      <c r="CN44" s="5"/>
-      <c r="CO44" s="5"/>
+      <c r="CN44" s="5">
+        <v>616</v>
+      </c>
+      <c r="CO44" s="5">
+        <v>616.29999999999995</v>
+      </c>
       <c r="CP44" s="5"/>
       <c r="CQ44" s="5"/>
       <c r="CR44" s="5"/>
@@ -18318,11 +18505,11 @@
       </c>
       <c r="B45" s="12">
         <f t="shared" si="1"/>
-        <v>110.95</v>
+        <v>111.6</v>
       </c>
       <c r="C45" s="12">
         <f t="shared" ref="C45" si="11">B45-A45</f>
-        <v>9.5499999999999972</v>
+        <v>10.199999999999989</v>
       </c>
       <c r="D45" s="45" t="s">
         <v>323</v>
@@ -18448,8 +18635,12 @@
       <c r="CM45" s="5">
         <v>105.65</v>
       </c>
-      <c r="CN45" s="5"/>
-      <c r="CO45" s="5"/>
+      <c r="CN45" s="5">
+        <v>109.5</v>
+      </c>
+      <c r="CO45" s="5">
+        <v>111.6</v>
+      </c>
       <c r="CP45" s="5"/>
       <c r="CQ45" s="5"/>
       <c r="CR45" s="5"/>
@@ -18585,8 +18776,12 @@
       <c r="CM46" s="5">
         <v>135.4</v>
       </c>
-      <c r="CN46" s="5"/>
-      <c r="CO46" s="5"/>
+      <c r="CN46" s="5">
+        <v>135.65</v>
+      </c>
+      <c r="CO46" s="5">
+        <v>138</v>
+      </c>
       <c r="CP46" s="5"/>
       <c r="CQ46" s="5"/>
       <c r="CR46" s="5"/>
@@ -18598,6 +18793,129 @@
       <c r="CX46" s="5"/>
       <c r="CY46" s="5"/>
       <c r="CZ46" s="5"/>
+    </row>
+    <row r="47" spans="1:104" x14ac:dyDescent="0.25">
+      <c r="A47" s="12">
+        <f t="shared" ref="A47" si="13">MIN(E47:ZQ47)</f>
+        <v>93.85</v>
+      </c>
+      <c r="B47" s="12">
+        <f t="shared" ref="B47" si="14">MAX(E47:ZQ47)</f>
+        <v>95</v>
+      </c>
+      <c r="C47" s="12">
+        <f t="shared" ref="C47" si="15">B47-A47</f>
+        <v>1.1500000000000057</v>
+      </c>
+      <c r="D47" s="45" t="s">
+        <v>332</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="5"/>
+      <c r="V47" s="5"/>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5"/>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5"/>
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="5"/>
+      <c r="AC47" s="5"/>
+      <c r="AD47" s="5"/>
+      <c r="AE47" s="5"/>
+      <c r="AF47" s="5"/>
+      <c r="AG47" s="5"/>
+      <c r="AH47" s="5"/>
+      <c r="AI47" s="5"/>
+      <c r="AJ47" s="5"/>
+      <c r="AK47" s="5"/>
+      <c r="AL47" s="5"/>
+      <c r="AM47" s="5"/>
+      <c r="AN47" s="5"/>
+      <c r="AO47" s="5"/>
+      <c r="AP47" s="5"/>
+      <c r="AQ47" s="5"/>
+      <c r="AR47" s="5"/>
+      <c r="AS47" s="5"/>
+      <c r="AT47" s="5"/>
+      <c r="AU47" s="5"/>
+      <c r="AV47" s="5"/>
+      <c r="AW47" s="5"/>
+      <c r="AX47" s="5"/>
+      <c r="AY47" s="5"/>
+      <c r="AZ47" s="5"/>
+      <c r="BA47" s="5"/>
+      <c r="BB47" s="5"/>
+      <c r="BC47" s="5"/>
+      <c r="BD47" s="5"/>
+      <c r="BE47" s="5"/>
+      <c r="BF47" s="5"/>
+      <c r="BG47" s="5"/>
+      <c r="BH47" s="5"/>
+      <c r="BI47" s="5"/>
+      <c r="BJ47" s="5"/>
+      <c r="BK47" s="5"/>
+      <c r="BL47" s="5"/>
+      <c r="BM47" s="5"/>
+      <c r="BN47" s="5"/>
+      <c r="BO47" s="5"/>
+      <c r="BP47" s="5"/>
+      <c r="BQ47" s="5"/>
+      <c r="BR47" s="5"/>
+      <c r="BS47" s="5"/>
+      <c r="BT47" s="5"/>
+      <c r="BU47" s="5"/>
+      <c r="BV47" s="5"/>
+      <c r="BW47" s="5"/>
+      <c r="BX47" s="5"/>
+      <c r="BY47" s="5"/>
+      <c r="BZ47" s="5"/>
+      <c r="CA47" s="5"/>
+      <c r="CB47" s="5"/>
+      <c r="CC47" s="5"/>
+      <c r="CD47" s="5"/>
+      <c r="CE47" s="5"/>
+      <c r="CF47" s="5"/>
+      <c r="CG47" s="5"/>
+      <c r="CH47" s="5"/>
+      <c r="CI47" s="5"/>
+      <c r="CJ47" s="5"/>
+      <c r="CK47" s="5"/>
+      <c r="CL47" s="5"/>
+      <c r="CM47" s="5">
+        <v>95</v>
+      </c>
+      <c r="CN47" s="5">
+        <v>94.85</v>
+      </c>
+      <c r="CO47" s="5">
+        <v>93.85</v>
+      </c>
+      <c r="CP47" s="5"/>
+      <c r="CQ47" s="5"/>
+      <c r="CR47" s="5"/>
+      <c r="CS47" s="5"/>
+      <c r="CT47" s="5"/>
+      <c r="CU47" s="5"/>
+      <c r="CV47" s="5"/>
+      <c r="CW47" s="5"/>
+      <c r="CX47" s="5"/>
+      <c r="CY47" s="5"/>
+      <c r="CZ47" s="5"/>
     </row>
   </sheetData>
   <sortState ref="L1:L37">

</xml_diff>

<commit_message>
Added details for 26/12/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="335">
   <si>
     <t>Date</t>
   </si>
@@ -1027,6 +1027,9 @@
   </si>
   <si>
     <t>21/12/2017</t>
+  </si>
+  <si>
+    <t>26/12/2017</t>
   </si>
 </sst>
 </file>
@@ -7278,9 +7281,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CZ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="CJ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CU24" sqref="CU24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="CK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CP33" sqref="CP33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7337,6 +7340,7 @@
     <col min="87" max="91" width="14" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="14" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:104" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7619,7 +7623,9 @@
       <c r="CO1" s="49" t="s">
         <v>333</v>
       </c>
-      <c r="CP1" s="27"/>
+      <c r="CP1" s="49" t="s">
+        <v>334</v>
+      </c>
       <c r="CQ1" s="27"/>
       <c r="CR1" s="27"/>
       <c r="CS1" s="27"/>
@@ -7906,7 +7912,9 @@
       <c r="CO2" s="5">
         <v>316.3</v>
       </c>
-      <c r="CP2" s="5"/>
+      <c r="CP2" s="5">
+        <v>317</v>
+      </c>
       <c r="CQ2" s="5"/>
       <c r="CR2" s="5"/>
       <c r="CS2" s="5"/>
@@ -8193,7 +8201,9 @@
       <c r="CO3" s="5">
         <v>313.95</v>
       </c>
-      <c r="CP3" s="5"/>
+      <c r="CP3" s="5">
+        <v>317.85000000000002</v>
+      </c>
       <c r="CQ3" s="5"/>
       <c r="CR3" s="5"/>
       <c r="CS3" s="5"/>
@@ -8486,7 +8496,9 @@
       <c r="CO4" s="5">
         <v>263.05</v>
       </c>
-      <c r="CP4" s="5"/>
+      <c r="CP4" s="5">
+        <v>263.75</v>
+      </c>
       <c r="CQ4" s="5"/>
       <c r="CR4" s="5"/>
       <c r="CS4" s="5"/>
@@ -8779,7 +8791,9 @@
       <c r="CO5" s="5">
         <v>913</v>
       </c>
-      <c r="CP5" s="5"/>
+      <c r="CP5" s="5">
+        <v>936</v>
+      </c>
       <c r="CQ5" s="5"/>
       <c r="CR5" s="5"/>
       <c r="CS5" s="5"/>
@@ -9072,7 +9086,9 @@
       <c r="CO6" s="5">
         <v>267.60000000000002</v>
       </c>
-      <c r="CP6" s="5"/>
+      <c r="CP6" s="5">
+        <v>263.3</v>
+      </c>
       <c r="CQ6" s="5"/>
       <c r="CR6" s="5"/>
       <c r="CS6" s="5"/>
@@ -9365,7 +9381,9 @@
       <c r="CO7" s="5">
         <v>19.95</v>
       </c>
-      <c r="CP7" s="5"/>
+      <c r="CP7" s="5">
+        <v>19.350000000000001</v>
+      </c>
       <c r="CQ7" s="5"/>
       <c r="CR7" s="5"/>
       <c r="CS7" s="5"/>
@@ -9384,11 +9402,11 @@
       </c>
       <c r="B8" s="12">
         <f t="shared" si="1"/>
-        <v>86.75</v>
+        <v>90.45</v>
       </c>
       <c r="C8" s="12">
         <f t="shared" si="2"/>
-        <v>33.35</v>
+        <v>37.050000000000004</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>22</v>
@@ -9658,7 +9676,9 @@
       <c r="CO8" s="5">
         <v>86.75</v>
       </c>
-      <c r="CP8" s="5"/>
+      <c r="CP8" s="5">
+        <v>90.45</v>
+      </c>
       <c r="CQ8" s="5"/>
       <c r="CR8" s="5"/>
       <c r="CS8" s="5"/>
@@ -9943,7 +9963,9 @@
       <c r="CO9" s="28">
         <v>55.15</v>
       </c>
-      <c r="CP9" s="28"/>
+      <c r="CP9" s="28">
+        <v>55.1</v>
+      </c>
       <c r="CQ9" s="28"/>
       <c r="CR9" s="28"/>
       <c r="CS9" s="28"/>
@@ -10236,7 +10258,9 @@
       <c r="CO10" s="5">
         <v>40.200000000000003</v>
       </c>
-      <c r="CP10" s="5"/>
+      <c r="CP10" s="5">
+        <v>42.95</v>
+      </c>
       <c r="CQ10" s="5"/>
       <c r="CR10" s="5"/>
       <c r="CS10" s="5"/>
@@ -10529,7 +10553,9 @@
       <c r="CO11" s="5">
         <v>101.05</v>
       </c>
-      <c r="CP11" s="5"/>
+      <c r="CP11" s="5">
+        <v>101.7</v>
+      </c>
       <c r="CQ11" s="5"/>
       <c r="CR11" s="5"/>
       <c r="CS11" s="5"/>
@@ -10822,7 +10848,9 @@
       <c r="CO12" s="5">
         <v>91.35</v>
       </c>
-      <c r="CP12" s="5"/>
+      <c r="CP12" s="5">
+        <v>92.85</v>
+      </c>
       <c r="CQ12" s="5"/>
       <c r="CR12" s="5"/>
       <c r="CS12" s="5"/>
@@ -10841,11 +10869,11 @@
       </c>
       <c r="B13" s="12">
         <f t="shared" si="1"/>
-        <v>57.15</v>
+        <v>59.4</v>
       </c>
       <c r="C13" s="12">
         <f t="shared" si="2"/>
-        <v>13.049999999999997</v>
+        <v>15.299999999999997</v>
       </c>
       <c r="D13" s="45" t="s">
         <v>20</v>
@@ -11115,7 +11143,9 @@
       <c r="CO13" s="5">
         <v>54.35</v>
       </c>
-      <c r="CP13" s="5"/>
+      <c r="CP13" s="5">
+        <v>59.4</v>
+      </c>
       <c r="CQ13" s="5"/>
       <c r="CR13" s="5"/>
       <c r="CS13" s="5"/>
@@ -11408,7 +11438,9 @@
       <c r="CO14" s="5">
         <v>41.15</v>
       </c>
-      <c r="CP14" s="5"/>
+      <c r="CP14" s="5">
+        <v>41.05</v>
+      </c>
       <c r="CQ14" s="5"/>
       <c r="CR14" s="5"/>
       <c r="CS14" s="5"/>
@@ -11693,7 +11725,9 @@
       <c r="CO15" s="5">
         <v>23</v>
       </c>
-      <c r="CP15" s="5"/>
+      <c r="CP15" s="5">
+        <v>24.8</v>
+      </c>
       <c r="CQ15" s="5"/>
       <c r="CR15" s="5"/>
       <c r="CS15" s="5"/>
@@ -11986,7 +12020,9 @@
       <c r="CO16" s="5">
         <v>712</v>
       </c>
-      <c r="CP16" s="5"/>
+      <c r="CP16" s="5">
+        <v>720.45</v>
+      </c>
       <c r="CQ16" s="5"/>
       <c r="CR16" s="5"/>
       <c r="CS16" s="5"/>
@@ -12279,7 +12315,9 @@
       <c r="CO17" s="5">
         <v>521.25</v>
       </c>
-      <c r="CP17" s="5"/>
+      <c r="CP17" s="5">
+        <v>524.45000000000005</v>
+      </c>
       <c r="CQ17" s="5"/>
       <c r="CR17" s="5"/>
       <c r="CS17" s="5"/>
@@ -12572,7 +12610,9 @@
       <c r="CO18" s="5">
         <v>270.3</v>
       </c>
-      <c r="CP18" s="5"/>
+      <c r="CP18" s="5">
+        <v>266.85000000000002</v>
+      </c>
       <c r="CQ18" s="5"/>
       <c r="CR18" s="5"/>
       <c r="CS18" s="5"/>
@@ -12865,7 +12905,9 @@
       <c r="CO19" s="5">
         <v>395.5</v>
       </c>
-      <c r="CP19" s="5"/>
+      <c r="CP19" s="5">
+        <v>431.85</v>
+      </c>
       <c r="CQ19" s="5"/>
       <c r="CR19" s="5"/>
       <c r="CS19" s="5"/>
@@ -13158,7 +13200,9 @@
       <c r="CO20" s="5">
         <v>684.15</v>
       </c>
-      <c r="CP20" s="5"/>
+      <c r="CP20" s="5">
+        <v>683.3</v>
+      </c>
       <c r="CQ20" s="5"/>
       <c r="CR20" s="5"/>
       <c r="CS20" s="5"/>
@@ -13451,7 +13495,9 @@
       <c r="CO21" s="5">
         <v>524.4</v>
       </c>
-      <c r="CP21" s="5"/>
+      <c r="CP21" s="5">
+        <v>544.70000000000005</v>
+      </c>
       <c r="CQ21" s="5"/>
       <c r="CR21" s="5"/>
       <c r="CS21" s="5"/>
@@ -13690,7 +13736,9 @@
       <c r="CO22" s="5">
         <v>392</v>
       </c>
-      <c r="CP22" s="5"/>
+      <c r="CP22" s="5">
+        <v>386.7</v>
+      </c>
       <c r="CQ22" s="5"/>
       <c r="CR22" s="5"/>
       <c r="CS22" s="5"/>
@@ -13975,7 +14023,9 @@
       <c r="CO23" s="5">
         <v>56.8</v>
       </c>
-      <c r="CP23" s="5"/>
+      <c r="CP23" s="5">
+        <v>58.85</v>
+      </c>
       <c r="CQ23" s="5"/>
       <c r="CR23" s="5"/>
       <c r="CS23" s="5"/>
@@ -14256,7 +14306,9 @@
       <c r="CO24" s="5">
         <v>236.8</v>
       </c>
-      <c r="CP24" s="5"/>
+      <c r="CP24" s="5">
+        <v>240.85</v>
+      </c>
       <c r="CQ24" s="5"/>
       <c r="CR24" s="5"/>
       <c r="CS24" s="5"/>
@@ -14275,11 +14327,11 @@
       </c>
       <c r="B25" s="12">
         <f t="shared" si="1"/>
-        <v>1021.5</v>
+        <v>1035</v>
       </c>
       <c r="C25" s="12">
         <f t="shared" si="2"/>
-        <v>145.5</v>
+        <v>159</v>
       </c>
       <c r="D25" s="46" t="s">
         <v>236</v>
@@ -14519,7 +14571,9 @@
       <c r="CO25" s="5">
         <v>1021.5</v>
       </c>
-      <c r="CP25" s="5"/>
+      <c r="CP25" s="5">
+        <v>1035</v>
+      </c>
       <c r="CQ25" s="5"/>
       <c r="CR25" s="5"/>
       <c r="CS25" s="5"/>
@@ -14770,7 +14824,9 @@
       <c r="CO26" s="5">
         <v>110.25</v>
       </c>
-      <c r="CP26" s="5"/>
+      <c r="CP26" s="5">
+        <v>106</v>
+      </c>
       <c r="CQ26" s="5"/>
       <c r="CR26" s="5"/>
       <c r="CS26" s="5"/>
@@ -15021,7 +15077,9 @@
       <c r="CO27" s="5">
         <v>40.450000000000003</v>
       </c>
-      <c r="CP27" s="5"/>
+      <c r="CP27" s="5">
+        <v>40</v>
+      </c>
       <c r="CQ27" s="5"/>
       <c r="CR27" s="5"/>
       <c r="CS27" s="5"/>
@@ -15272,7 +15330,9 @@
       <c r="CO28" s="5">
         <v>128.5</v>
       </c>
-      <c r="CP28" s="5"/>
+      <c r="CP28" s="5">
+        <v>137.4</v>
+      </c>
       <c r="CQ28" s="5"/>
       <c r="CR28" s="5"/>
       <c r="CS28" s="5"/>
@@ -15523,7 +15583,9 @@
       <c r="CO29" s="5">
         <v>72.849999999999994</v>
       </c>
-      <c r="CP29" s="5"/>
+      <c r="CP29" s="5">
+        <v>75.95</v>
+      </c>
       <c r="CQ29" s="5"/>
       <c r="CR29" s="5"/>
       <c r="CS29" s="5"/>
@@ -15774,7 +15836,9 @@
       <c r="CO30" s="5">
         <v>40.1</v>
       </c>
-      <c r="CP30" s="5"/>
+      <c r="CP30" s="5">
+        <v>39.1</v>
+      </c>
       <c r="CQ30" s="5"/>
       <c r="CR30" s="5"/>
       <c r="CS30" s="5"/>
@@ -16025,7 +16089,9 @@
       <c r="CO31" s="5">
         <v>143.44999999999999</v>
       </c>
-      <c r="CP31" s="5"/>
+      <c r="CP31" s="5">
+        <v>150.5</v>
+      </c>
       <c r="CQ31" s="5"/>
       <c r="CR31" s="5"/>
       <c r="CS31" s="5"/>
@@ -16264,7 +16330,9 @@
       <c r="CO32" s="5">
         <v>100.25</v>
       </c>
-      <c r="CP32" s="5"/>
+      <c r="CP32" s="5">
+        <v>100.8</v>
+      </c>
       <c r="CQ32" s="5"/>
       <c r="CR32" s="5"/>
       <c r="CS32" s="5"/>
@@ -16283,11 +16351,11 @@
       </c>
       <c r="B33" s="12">
         <f t="shared" si="1"/>
-        <v>74.150000000000006</v>
+        <v>78.150000000000006</v>
       </c>
       <c r="C33" s="12">
         <f t="shared" si="2"/>
-        <v>17.400000000000006</v>
+        <v>21.400000000000006</v>
       </c>
       <c r="D33" s="45" t="s">
         <v>271</v>
@@ -16491,7 +16559,9 @@
       <c r="CO33" s="5">
         <v>74.150000000000006</v>
       </c>
-      <c r="CP33" s="5"/>
+      <c r="CP33" s="5">
+        <v>78.150000000000006</v>
+      </c>
       <c r="CQ33" s="5"/>
       <c r="CR33" s="5"/>
       <c r="CS33" s="5"/>
@@ -16712,7 +16782,9 @@
       <c r="CO34" s="5">
         <v>294.95</v>
       </c>
-      <c r="CP34" s="5"/>
+      <c r="CP34" s="5">
+        <v>294.60000000000002</v>
+      </c>
       <c r="CQ34" s="5"/>
       <c r="CR34" s="5"/>
       <c r="CS34" s="5"/>
@@ -16911,7 +16983,9 @@
       <c r="CO35" s="5">
         <v>396</v>
       </c>
-      <c r="CP35" s="5"/>
+      <c r="CP35" s="5">
+        <v>398</v>
+      </c>
       <c r="CQ35" s="5"/>
       <c r="CR35" s="5"/>
       <c r="CS35" s="5"/>
@@ -17100,7 +17174,9 @@
       <c r="CO36" s="5">
         <v>356.5</v>
       </c>
-      <c r="CP36" s="5"/>
+      <c r="CP36" s="5">
+        <v>361.45</v>
+      </c>
       <c r="CQ36" s="5"/>
       <c r="CR36" s="5"/>
       <c r="CS36" s="5"/>
@@ -17281,7 +17357,9 @@
       <c r="CO37" s="5">
         <v>81.5</v>
       </c>
-      <c r="CP37" s="5"/>
+      <c r="CP37" s="5">
+        <v>80.150000000000006</v>
+      </c>
       <c r="CQ37" s="5"/>
       <c r="CR37" s="5"/>
       <c r="CS37" s="5"/>
@@ -17462,7 +17540,9 @@
       <c r="CO38" s="5">
         <v>429.2</v>
       </c>
-      <c r="CP38" s="5"/>
+      <c r="CP38" s="5">
+        <v>434</v>
+      </c>
       <c r="CQ38" s="5"/>
       <c r="CR38" s="5"/>
       <c r="CS38" s="5"/>
@@ -17481,11 +17561,11 @@
       </c>
       <c r="B39" s="12">
         <f t="shared" si="1"/>
-        <v>225.55</v>
+        <v>227</v>
       </c>
       <c r="C39" s="12">
         <f t="shared" ref="C39" si="8">B39-A39</f>
-        <v>50.350000000000023</v>
+        <v>51.800000000000011</v>
       </c>
       <c r="D39" s="45" t="s">
         <v>305</v>
@@ -17639,7 +17719,9 @@
       <c r="CO39" s="5">
         <v>225.55</v>
       </c>
-      <c r="CP39" s="5"/>
+      <c r="CP39" s="5">
+        <v>227</v>
+      </c>
       <c r="CQ39" s="5"/>
       <c r="CR39" s="5"/>
       <c r="CS39" s="5"/>
@@ -17658,11 +17740,11 @@
       </c>
       <c r="B40" s="12">
         <f t="shared" si="1"/>
-        <v>39.6</v>
+        <v>41.9</v>
       </c>
       <c r="C40" s="12">
         <f t="shared" ref="C40:C43" si="9">B40-A40</f>
-        <v>5.1000000000000014</v>
+        <v>7.3999999999999986</v>
       </c>
       <c r="D40" s="45" t="s">
         <v>306</v>
@@ -17812,7 +17894,9 @@
       <c r="CO40" s="5">
         <v>39.6</v>
       </c>
-      <c r="CP40" s="5"/>
+      <c r="CP40" s="5">
+        <v>41.9</v>
+      </c>
       <c r="CQ40" s="5"/>
       <c r="CR40" s="5"/>
       <c r="CS40" s="5"/>
@@ -17831,11 +17915,11 @@
       </c>
       <c r="B41" s="12">
         <f t="shared" si="1"/>
-        <v>665.45</v>
+        <v>674</v>
       </c>
       <c r="C41" s="12">
         <f t="shared" si="9"/>
-        <v>113.40000000000009</v>
+        <v>121.95000000000005</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>307</v>
@@ -17983,7 +18067,9 @@
       <c r="CO41" s="5">
         <v>637.65</v>
       </c>
-      <c r="CP41" s="5"/>
+      <c r="CP41" s="5">
+        <v>674</v>
+      </c>
       <c r="CQ41" s="5"/>
       <c r="CR41" s="5"/>
       <c r="CS41" s="5"/>
@@ -18154,7 +18240,9 @@
       <c r="CO42" s="5">
         <v>880</v>
       </c>
-      <c r="CP42" s="5"/>
+      <c r="CP42" s="5">
+        <v>870.7</v>
+      </c>
       <c r="CQ42" s="5"/>
       <c r="CR42" s="5"/>
       <c r="CS42" s="5"/>
@@ -18173,11 +18261,11 @@
       </c>
       <c r="B43" s="12">
         <f t="shared" si="1"/>
-        <v>149.94999999999999</v>
+        <v>153</v>
       </c>
       <c r="C43" s="12">
         <f t="shared" si="9"/>
-        <v>15.949999999999989</v>
+        <v>19</v>
       </c>
       <c r="D43" s="45" t="s">
         <v>309</v>
@@ -18323,7 +18411,9 @@
       <c r="CO43" s="5">
         <v>149.94999999999999</v>
       </c>
-      <c r="CP43" s="5"/>
+      <c r="CP43" s="5">
+        <v>153</v>
+      </c>
       <c r="CQ43" s="5"/>
       <c r="CR43" s="5"/>
       <c r="CS43" s="5"/>
@@ -18486,7 +18576,9 @@
       <c r="CO44" s="5">
         <v>616.29999999999995</v>
       </c>
-      <c r="CP44" s="5"/>
+      <c r="CP44" s="5">
+        <v>612.6</v>
+      </c>
       <c r="CQ44" s="5"/>
       <c r="CR44" s="5"/>
       <c r="CS44" s="5"/>
@@ -18641,7 +18733,9 @@
       <c r="CO45" s="5">
         <v>111.6</v>
       </c>
-      <c r="CP45" s="5"/>
+      <c r="CP45" s="5">
+        <v>109.4</v>
+      </c>
       <c r="CQ45" s="5"/>
       <c r="CR45" s="5"/>
       <c r="CS45" s="5"/>
@@ -18782,7 +18876,9 @@
       <c r="CO46" s="5">
         <v>138</v>
       </c>
-      <c r="CP46" s="5"/>
+      <c r="CP46" s="5">
+        <v>135.9</v>
+      </c>
       <c r="CQ46" s="5"/>
       <c r="CR46" s="5"/>
       <c r="CS46" s="5"/>
@@ -18797,7 +18893,7 @@
     <row r="47" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <f t="shared" ref="A47" si="13">MIN(E47:ZQ47)</f>
-        <v>93.85</v>
+        <v>93.75</v>
       </c>
       <c r="B47" s="12">
         <f t="shared" ref="B47" si="14">MAX(E47:ZQ47)</f>
@@ -18805,7 +18901,7 @@
       </c>
       <c r="C47" s="12">
         <f t="shared" ref="C47" si="15">B47-A47</f>
-        <v>1.1500000000000057</v>
+        <v>1.25</v>
       </c>
       <c r="D47" s="45" t="s">
         <v>332</v>
@@ -18905,7 +19001,9 @@
       <c r="CO47" s="5">
         <v>93.85</v>
       </c>
-      <c r="CP47" s="5"/>
+      <c r="CP47" s="5">
+        <v>93.75</v>
+      </c>
       <c r="CQ47" s="5"/>
       <c r="CR47" s="5"/>
       <c r="CS47" s="5"/>
@@ -18931,7 +19029,7 @@
   <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -21352,7 +21450,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added details for 27/12/2017
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="336">
   <si>
     <t>Date</t>
   </si>
@@ -1030,6 +1030,9 @@
   </si>
   <si>
     <t>26/12/2017</t>
+  </si>
+  <si>
+    <t>27/12/2017</t>
   </si>
 </sst>
 </file>
@@ -7283,7 +7286,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="CK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CP33" sqref="CP33"/>
+      <selection pane="topRight" activeCell="CQ45" sqref="CQ45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7340,7 +7343,7 @@
     <col min="87" max="91" width="14" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="14" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="94" max="95" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:104" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7626,7 +7629,9 @@
       <c r="CP1" s="49" t="s">
         <v>334</v>
       </c>
-      <c r="CQ1" s="27"/>
+      <c r="CQ1" s="49" t="s">
+        <v>335</v>
+      </c>
       <c r="CR1" s="27"/>
       <c r="CS1" s="27"/>
       <c r="CT1" s="27"/>
@@ -7915,7 +7920,9 @@
       <c r="CP2" s="5">
         <v>317</v>
       </c>
-      <c r="CQ2" s="5"/>
+      <c r="CQ2" s="5">
+        <v>313.45</v>
+      </c>
       <c r="CR2" s="5"/>
       <c r="CS2" s="5"/>
       <c r="CT2" s="5"/>
@@ -8204,7 +8211,9 @@
       <c r="CP3" s="5">
         <v>317.85000000000002</v>
       </c>
-      <c r="CQ3" s="5"/>
+      <c r="CQ3" s="5">
+        <v>312.5</v>
+      </c>
       <c r="CR3" s="5"/>
       <c r="CS3" s="5"/>
       <c r="CT3" s="5"/>
@@ -8499,7 +8508,9 @@
       <c r="CP4" s="5">
         <v>263.75</v>
       </c>
-      <c r="CQ4" s="5"/>
+      <c r="CQ4" s="5">
+        <v>262.3</v>
+      </c>
       <c r="CR4" s="5"/>
       <c r="CS4" s="5"/>
       <c r="CT4" s="5"/>
@@ -8794,7 +8805,9 @@
       <c r="CP5" s="5">
         <v>936</v>
       </c>
-      <c r="CQ5" s="5"/>
+      <c r="CQ5" s="5">
+        <v>923.25</v>
+      </c>
       <c r="CR5" s="5"/>
       <c r="CS5" s="5"/>
       <c r="CT5" s="5"/>
@@ -9089,7 +9102,9 @@
       <c r="CP6" s="5">
         <v>263.3</v>
       </c>
-      <c r="CQ6" s="5"/>
+      <c r="CQ6" s="5">
+        <v>262.64999999999998</v>
+      </c>
       <c r="CR6" s="5"/>
       <c r="CS6" s="5"/>
       <c r="CT6" s="5"/>
@@ -9384,7 +9399,9 @@
       <c r="CP7" s="5">
         <v>19.350000000000001</v>
       </c>
-      <c r="CQ7" s="5"/>
+      <c r="CQ7" s="5">
+        <v>18.95</v>
+      </c>
       <c r="CR7" s="5"/>
       <c r="CS7" s="5"/>
       <c r="CT7" s="5"/>
@@ -9402,11 +9419,11 @@
       </c>
       <c r="B8" s="12">
         <f t="shared" si="1"/>
-        <v>90.45</v>
+        <v>90.95</v>
       </c>
       <c r="C8" s="12">
         <f t="shared" si="2"/>
-        <v>37.050000000000004</v>
+        <v>37.550000000000004</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>22</v>
@@ -9679,7 +9696,9 @@
       <c r="CP8" s="5">
         <v>90.45</v>
       </c>
-      <c r="CQ8" s="5"/>
+      <c r="CQ8" s="5">
+        <v>90.95</v>
+      </c>
       <c r="CR8" s="5"/>
       <c r="CS8" s="5"/>
       <c r="CT8" s="5"/>
@@ -9966,7 +9985,9 @@
       <c r="CP9" s="28">
         <v>55.1</v>
       </c>
-      <c r="CQ9" s="28"/>
+      <c r="CQ9" s="28">
+        <v>55.1</v>
+      </c>
       <c r="CR9" s="28"/>
       <c r="CS9" s="28"/>
       <c r="CT9" s="28"/>
@@ -10261,7 +10282,9 @@
       <c r="CP10" s="5">
         <v>42.95</v>
       </c>
-      <c r="CQ10" s="5"/>
+      <c r="CQ10" s="5">
+        <v>44.25</v>
+      </c>
       <c r="CR10" s="5"/>
       <c r="CS10" s="5"/>
       <c r="CT10" s="5"/>
@@ -10556,7 +10579,9 @@
       <c r="CP11" s="5">
         <v>101.7</v>
       </c>
-      <c r="CQ11" s="5"/>
+      <c r="CQ11" s="5">
+        <v>101.3</v>
+      </c>
       <c r="CR11" s="5"/>
       <c r="CS11" s="5"/>
       <c r="CT11" s="5"/>
@@ -10851,7 +10876,9 @@
       <c r="CP12" s="5">
         <v>92.85</v>
       </c>
-      <c r="CQ12" s="5"/>
+      <c r="CQ12" s="5">
+        <v>92.6</v>
+      </c>
       <c r="CR12" s="5"/>
       <c r="CS12" s="5"/>
       <c r="CT12" s="5"/>
@@ -10869,11 +10896,11 @@
       </c>
       <c r="B13" s="12">
         <f t="shared" si="1"/>
-        <v>59.4</v>
+        <v>60.4</v>
       </c>
       <c r="C13" s="12">
         <f t="shared" si="2"/>
-        <v>15.299999999999997</v>
+        <v>16.299999999999997</v>
       </c>
       <c r="D13" s="45" t="s">
         <v>20</v>
@@ -11146,7 +11173,9 @@
       <c r="CP13" s="5">
         <v>59.4</v>
       </c>
-      <c r="CQ13" s="5"/>
+      <c r="CQ13" s="5">
+        <v>60.4</v>
+      </c>
       <c r="CR13" s="5"/>
       <c r="CS13" s="5"/>
       <c r="CT13" s="5"/>
@@ -11441,7 +11470,9 @@
       <c r="CP14" s="5">
         <v>41.05</v>
       </c>
-      <c r="CQ14" s="5"/>
+      <c r="CQ14" s="5">
+        <v>40.6</v>
+      </c>
       <c r="CR14" s="5"/>
       <c r="CS14" s="5"/>
       <c r="CT14" s="5"/>
@@ -11728,7 +11759,9 @@
       <c r="CP15" s="5">
         <v>24.8</v>
       </c>
-      <c r="CQ15" s="5"/>
+      <c r="CQ15" s="5">
+        <v>24.35</v>
+      </c>
       <c r="CR15" s="5"/>
       <c r="CS15" s="5"/>
       <c r="CT15" s="5"/>
@@ -12023,7 +12056,9 @@
       <c r="CP16" s="5">
         <v>720.45</v>
       </c>
-      <c r="CQ16" s="5"/>
+      <c r="CQ16" s="5">
+        <v>722</v>
+      </c>
       <c r="CR16" s="5"/>
       <c r="CS16" s="5"/>
       <c r="CT16" s="5"/>
@@ -12318,7 +12353,9 @@
       <c r="CP17" s="5">
         <v>524.45000000000005</v>
       </c>
-      <c r="CQ17" s="5"/>
+      <c r="CQ17" s="5">
+        <v>527.70000000000005</v>
+      </c>
       <c r="CR17" s="5"/>
       <c r="CS17" s="5"/>
       <c r="CT17" s="5"/>
@@ -12613,7 +12650,9 @@
       <c r="CP18" s="5">
         <v>266.85000000000002</v>
       </c>
-      <c r="CQ18" s="5"/>
+      <c r="CQ18" s="5">
+        <v>261.8</v>
+      </c>
       <c r="CR18" s="5"/>
       <c r="CS18" s="5"/>
       <c r="CT18" s="5"/>
@@ -12908,7 +12947,9 @@
       <c r="CP19" s="5">
         <v>431.85</v>
       </c>
-      <c r="CQ19" s="5"/>
+      <c r="CQ19" s="5">
+        <v>413.15</v>
+      </c>
       <c r="CR19" s="5"/>
       <c r="CS19" s="5"/>
       <c r="CT19" s="5"/>
@@ -13203,7 +13244,9 @@
       <c r="CP20" s="5">
         <v>683.3</v>
       </c>
-      <c r="CQ20" s="5"/>
+      <c r="CQ20" s="5">
+        <v>691</v>
+      </c>
       <c r="CR20" s="5"/>
       <c r="CS20" s="5"/>
       <c r="CT20" s="5"/>
@@ -13498,7 +13541,9 @@
       <c r="CP21" s="5">
         <v>544.70000000000005</v>
       </c>
-      <c r="CQ21" s="5"/>
+      <c r="CQ21" s="5">
+        <v>533.04999999999995</v>
+      </c>
       <c r="CR21" s="5"/>
       <c r="CS21" s="5"/>
       <c r="CT21" s="5"/>
@@ -13739,7 +13784,9 @@
       <c r="CP22" s="5">
         <v>386.7</v>
       </c>
-      <c r="CQ22" s="5"/>
+      <c r="CQ22" s="5">
+        <v>388</v>
+      </c>
       <c r="CR22" s="5"/>
       <c r="CS22" s="5"/>
       <c r="CT22" s="5"/>
@@ -14026,7 +14073,9 @@
       <c r="CP23" s="5">
         <v>58.85</v>
       </c>
-      <c r="CQ23" s="5"/>
+      <c r="CQ23" s="5">
+        <v>56.9</v>
+      </c>
       <c r="CR23" s="5"/>
       <c r="CS23" s="5"/>
       <c r="CT23" s="5"/>
@@ -14309,7 +14358,9 @@
       <c r="CP24" s="5">
         <v>240.85</v>
       </c>
-      <c r="CQ24" s="5"/>
+      <c r="CQ24" s="5">
+        <v>239.1</v>
+      </c>
       <c r="CR24" s="5"/>
       <c r="CS24" s="5"/>
       <c r="CT24" s="5"/>
@@ -14574,7 +14625,9 @@
       <c r="CP25" s="5">
         <v>1035</v>
       </c>
-      <c r="CQ25" s="5"/>
+      <c r="CQ25" s="5">
+        <v>1034</v>
+      </c>
       <c r="CR25" s="5"/>
       <c r="CS25" s="5"/>
       <c r="CT25" s="5"/>
@@ -14827,7 +14880,9 @@
       <c r="CP26" s="5">
         <v>106</v>
       </c>
-      <c r="CQ26" s="5"/>
+      <c r="CQ26" s="5">
+        <v>104.45</v>
+      </c>
       <c r="CR26" s="5"/>
       <c r="CS26" s="5"/>
       <c r="CT26" s="5"/>
@@ -15080,7 +15135,9 @@
       <c r="CP27" s="5">
         <v>40</v>
       </c>
-      <c r="CQ27" s="5"/>
+      <c r="CQ27" s="5">
+        <v>40.35</v>
+      </c>
       <c r="CR27" s="5"/>
       <c r="CS27" s="5"/>
       <c r="CT27" s="5"/>
@@ -15333,7 +15390,9 @@
       <c r="CP28" s="5">
         <v>137.4</v>
       </c>
-      <c r="CQ28" s="5"/>
+      <c r="CQ28" s="5">
+        <v>138.19999999999999</v>
+      </c>
       <c r="CR28" s="5"/>
       <c r="CS28" s="5"/>
       <c r="CT28" s="5"/>
@@ -15586,7 +15645,9 @@
       <c r="CP29" s="5">
         <v>75.95</v>
       </c>
-      <c r="CQ29" s="5"/>
+      <c r="CQ29" s="5">
+        <v>73.3</v>
+      </c>
       <c r="CR29" s="5"/>
       <c r="CS29" s="5"/>
       <c r="CT29" s="5"/>
@@ -15839,7 +15900,9 @@
       <c r="CP30" s="5">
         <v>39.1</v>
       </c>
-      <c r="CQ30" s="5"/>
+      <c r="CQ30" s="5">
+        <v>40.450000000000003</v>
+      </c>
       <c r="CR30" s="5"/>
       <c r="CS30" s="5"/>
       <c r="CT30" s="5"/>
@@ -15857,11 +15920,11 @@
       </c>
       <c r="B31" s="12">
         <f t="shared" si="1"/>
-        <v>156.85</v>
+        <v>159</v>
       </c>
       <c r="C31" s="12">
         <f t="shared" si="2"/>
-        <v>31.549999999999997</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="D31" s="45" t="s">
         <v>257</v>
@@ -16092,7 +16155,9 @@
       <c r="CP31" s="5">
         <v>150.5</v>
       </c>
-      <c r="CQ31" s="5"/>
+      <c r="CQ31" s="5">
+        <v>159</v>
+      </c>
       <c r="CR31" s="5"/>
       <c r="CS31" s="5"/>
       <c r="CT31" s="5"/>
@@ -16333,7 +16398,9 @@
       <c r="CP32" s="5">
         <v>100.8</v>
       </c>
-      <c r="CQ32" s="5"/>
+      <c r="CQ32" s="5">
+        <v>99.4</v>
+      </c>
       <c r="CR32" s="5"/>
       <c r="CS32" s="5"/>
       <c r="CT32" s="5"/>
@@ -16562,7 +16629,9 @@
       <c r="CP33" s="5">
         <v>78.150000000000006</v>
       </c>
-      <c r="CQ33" s="5"/>
+      <c r="CQ33" s="5">
+        <v>76.599999999999994</v>
+      </c>
       <c r="CR33" s="5"/>
       <c r="CS33" s="5"/>
       <c r="CT33" s="5"/>
@@ -16785,7 +16854,9 @@
       <c r="CP34" s="5">
         <v>294.60000000000002</v>
       </c>
-      <c r="CQ34" s="5"/>
+      <c r="CQ34" s="5">
+        <v>284.64999999999998</v>
+      </c>
       <c r="CR34" s="5"/>
       <c r="CS34" s="5"/>
       <c r="CT34" s="5"/>
@@ -16986,7 +17057,9 @@
       <c r="CP35" s="5">
         <v>398</v>
       </c>
-      <c r="CQ35" s="5"/>
+      <c r="CQ35" s="5">
+        <v>390.6</v>
+      </c>
       <c r="CR35" s="5"/>
       <c r="CS35" s="5"/>
       <c r="CT35" s="5"/>
@@ -17177,7 +17250,9 @@
       <c r="CP36" s="5">
         <v>361.45</v>
       </c>
-      <c r="CQ36" s="5"/>
+      <c r="CQ36" s="5">
+        <v>363.75</v>
+      </c>
       <c r="CR36" s="5"/>
       <c r="CS36" s="5"/>
       <c r="CT36" s="5"/>
@@ -17360,7 +17435,9 @@
       <c r="CP37" s="5">
         <v>80.150000000000006</v>
       </c>
-      <c r="CQ37" s="5"/>
+      <c r="CQ37" s="5">
+        <v>80</v>
+      </c>
       <c r="CR37" s="5"/>
       <c r="CS37" s="5"/>
       <c r="CT37" s="5"/>
@@ -17543,7 +17620,9 @@
       <c r="CP38" s="5">
         <v>434</v>
       </c>
-      <c r="CQ38" s="5"/>
+      <c r="CQ38" s="5">
+        <v>432</v>
+      </c>
       <c r="CR38" s="5"/>
       <c r="CS38" s="5"/>
       <c r="CT38" s="5"/>
@@ -17722,7 +17801,9 @@
       <c r="CP39" s="5">
         <v>227</v>
       </c>
-      <c r="CQ39" s="5"/>
+      <c r="CQ39" s="5">
+        <v>223.5</v>
+      </c>
       <c r="CR39" s="5"/>
       <c r="CS39" s="5"/>
       <c r="CT39" s="5"/>
@@ -17897,7 +17978,9 @@
       <c r="CP40" s="5">
         <v>41.9</v>
       </c>
-      <c r="CQ40" s="5"/>
+      <c r="CQ40" s="5">
+        <v>40.950000000000003</v>
+      </c>
       <c r="CR40" s="5"/>
       <c r="CS40" s="5"/>
       <c r="CT40" s="5"/>
@@ -18070,7 +18153,9 @@
       <c r="CP41" s="5">
         <v>674</v>
       </c>
-      <c r="CQ41" s="5"/>
+      <c r="CQ41" s="5">
+        <v>669</v>
+      </c>
       <c r="CR41" s="5"/>
       <c r="CS41" s="5"/>
       <c r="CT41" s="5"/>
@@ -18243,7 +18328,9 @@
       <c r="CP42" s="5">
         <v>870.7</v>
       </c>
-      <c r="CQ42" s="5"/>
+      <c r="CQ42" s="5">
+        <v>876</v>
+      </c>
       <c r="CR42" s="5"/>
       <c r="CS42" s="5"/>
       <c r="CT42" s="5"/>
@@ -18414,7 +18501,9 @@
       <c r="CP43" s="5">
         <v>153</v>
       </c>
-      <c r="CQ43" s="5"/>
+      <c r="CQ43" s="5">
+        <v>148.35</v>
+      </c>
       <c r="CR43" s="5"/>
       <c r="CS43" s="5"/>
       <c r="CT43" s="5"/>
@@ -18579,7 +18668,9 @@
       <c r="CP44" s="5">
         <v>612.6</v>
       </c>
-      <c r="CQ44" s="5"/>
+      <c r="CQ44" s="5">
+        <v>600</v>
+      </c>
       <c r="CR44" s="5"/>
       <c r="CS44" s="5"/>
       <c r="CT44" s="5"/>
@@ -18736,7 +18827,9 @@
       <c r="CP45" s="5">
         <v>109.4</v>
       </c>
-      <c r="CQ45" s="5"/>
+      <c r="CQ45" s="5">
+        <v>107.4</v>
+      </c>
       <c r="CR45" s="5"/>
       <c r="CS45" s="5"/>
       <c r="CT45" s="5"/>
@@ -18879,7 +18972,9 @@
       <c r="CP46" s="5">
         <v>135.9</v>
       </c>
-      <c r="CQ46" s="5"/>
+      <c r="CQ46" s="5">
+        <v>136.35</v>
+      </c>
       <c r="CR46" s="5"/>
       <c r="CS46" s="5"/>
       <c r="CT46" s="5"/>
@@ -18893,7 +18988,7 @@
     <row r="47" spans="1:104" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <f t="shared" ref="A47" si="13">MIN(E47:ZQ47)</f>
-        <v>93.75</v>
+        <v>93.25</v>
       </c>
       <c r="B47" s="12">
         <f t="shared" ref="B47" si="14">MAX(E47:ZQ47)</f>
@@ -18901,7 +18996,7 @@
       </c>
       <c r="C47" s="12">
         <f t="shared" ref="C47" si="15">B47-A47</f>
-        <v>1.25</v>
+        <v>1.75</v>
       </c>
       <c r="D47" s="45" t="s">
         <v>332</v>
@@ -19004,7 +19099,9 @@
       <c r="CP47" s="5">
         <v>93.75</v>
       </c>
-      <c r="CQ47" s="5"/>
+      <c r="CQ47" s="5">
+        <v>93.25</v>
+      </c>
       <c r="CR47" s="5"/>
       <c r="CS47" s="5"/>
       <c r="CT47" s="5"/>

</xml_diff>

<commit_message>
Added details for 02/01/2018
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="337">
   <si>
     <t>Date</t>
   </si>
@@ -1033,6 +1033,9 @@
   </si>
   <si>
     <t>27/12/2017</t>
+  </si>
+  <si>
+    <t>DAAWAT</t>
   </si>
 </sst>
 </file>
@@ -7282,11 +7285,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CZ47"/>
+  <dimension ref="A1:CZ48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" topLeftCell="CK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CQ45" sqref="CQ45"/>
+      <selection pane="topRight" activeCell="CX44" sqref="CX44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7344,6 +7347,7 @@
     <col min="92" max="92" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="14" bestFit="1" customWidth="1"/>
     <col min="94" max="95" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:104" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7632,7 +7636,9 @@
       <c r="CQ1" s="49" t="s">
         <v>335</v>
       </c>
-      <c r="CR1" s="27"/>
+      <c r="CR1" s="11">
+        <v>43132</v>
+      </c>
       <c r="CS1" s="27"/>
       <c r="CT1" s="27"/>
       <c r="CU1" s="27"/>
@@ -7923,7 +7929,9 @@
       <c r="CQ2" s="5">
         <v>313.45</v>
       </c>
-      <c r="CR2" s="5"/>
+      <c r="CR2" s="5">
+        <v>303.60000000000002</v>
+      </c>
       <c r="CS2" s="5"/>
       <c r="CT2" s="5"/>
       <c r="CU2" s="5"/>
@@ -8214,7 +8222,9 @@
       <c r="CQ3" s="5">
         <v>312.5</v>
       </c>
-      <c r="CR3" s="5"/>
+      <c r="CR3" s="5">
+        <v>308.7</v>
+      </c>
       <c r="CS3" s="5"/>
       <c r="CT3" s="5"/>
       <c r="CU3" s="5"/>
@@ -8511,7 +8521,9 @@
       <c r="CQ4" s="5">
         <v>262.3</v>
       </c>
-      <c r="CR4" s="5"/>
+      <c r="CR4" s="5">
+        <v>262.45</v>
+      </c>
       <c r="CS4" s="5"/>
       <c r="CT4" s="5"/>
       <c r="CU4" s="5"/>
@@ -8808,7 +8820,9 @@
       <c r="CQ5" s="5">
         <v>923.25</v>
       </c>
-      <c r="CR5" s="5"/>
+      <c r="CR5" s="5">
+        <v>913.7</v>
+      </c>
       <c r="CS5" s="5"/>
       <c r="CT5" s="5"/>
       <c r="CU5" s="5"/>
@@ -9105,7 +9119,9 @@
       <c r="CQ6" s="5">
         <v>262.64999999999998</v>
       </c>
-      <c r="CR6" s="5"/>
+      <c r="CR6" s="5">
+        <v>268.75</v>
+      </c>
       <c r="CS6" s="5"/>
       <c r="CT6" s="5"/>
       <c r="CU6" s="5"/>
@@ -9122,11 +9138,11 @@
       </c>
       <c r="B7" s="12">
         <f t="shared" si="1"/>
-        <v>19.95</v>
+        <v>21.6</v>
       </c>
       <c r="C7" s="12">
         <f t="shared" si="2"/>
-        <v>4.3499999999999996</v>
+        <v>6.0000000000000018</v>
       </c>
       <c r="D7" s="45" t="s">
         <v>19</v>
@@ -9402,7 +9418,9 @@
       <c r="CQ7" s="5">
         <v>18.95</v>
       </c>
-      <c r="CR7" s="5"/>
+      <c r="CR7" s="5">
+        <v>21.6</v>
+      </c>
       <c r="CS7" s="5"/>
       <c r="CT7" s="5"/>
       <c r="CU7" s="5"/>
@@ -9419,11 +9437,11 @@
       </c>
       <c r="B8" s="12">
         <f t="shared" si="1"/>
-        <v>90.95</v>
+        <v>91.15</v>
       </c>
       <c r="C8" s="12">
         <f t="shared" si="2"/>
-        <v>37.550000000000004</v>
+        <v>37.750000000000007</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>22</v>
@@ -9699,7 +9717,9 @@
       <c r="CQ8" s="5">
         <v>90.95</v>
       </c>
-      <c r="CR8" s="5"/>
+      <c r="CR8" s="5">
+        <v>91.15</v>
+      </c>
       <c r="CS8" s="5"/>
       <c r="CT8" s="5"/>
       <c r="CU8" s="5"/>
@@ -9988,7 +10008,9 @@
       <c r="CQ9" s="28">
         <v>55.1</v>
       </c>
-      <c r="CR9" s="28"/>
+      <c r="CR9" s="28">
+        <v>54.4</v>
+      </c>
       <c r="CS9" s="28"/>
       <c r="CT9" s="28"/>
       <c r="CU9" s="28"/>
@@ -10005,11 +10027,11 @@
       </c>
       <c r="B10" s="12">
         <f t="shared" si="1"/>
-        <v>45.35</v>
+        <v>57.85</v>
       </c>
       <c r="C10" s="12">
         <f t="shared" si="2"/>
-        <v>10.200000000000003</v>
+        <v>22.700000000000003</v>
       </c>
       <c r="D10" s="45" t="s">
         <v>15</v>
@@ -10285,7 +10307,9 @@
       <c r="CQ10" s="5">
         <v>44.25</v>
       </c>
-      <c r="CR10" s="5"/>
+      <c r="CR10" s="5">
+        <v>57.85</v>
+      </c>
       <c r="CS10" s="5"/>
       <c r="CT10" s="5"/>
       <c r="CU10" s="5"/>
@@ -10582,7 +10606,9 @@
       <c r="CQ11" s="5">
         <v>101.3</v>
       </c>
-      <c r="CR11" s="5"/>
+      <c r="CR11" s="5">
+        <v>102.35</v>
+      </c>
       <c r="CS11" s="5"/>
       <c r="CT11" s="5"/>
       <c r="CU11" s="5"/>
@@ -10879,7 +10905,9 @@
       <c r="CQ12" s="5">
         <v>92.6</v>
       </c>
-      <c r="CR12" s="5"/>
+      <c r="CR12" s="5">
+        <v>95.55</v>
+      </c>
       <c r="CS12" s="5"/>
       <c r="CT12" s="5"/>
       <c r="CU12" s="5"/>
@@ -11176,7 +11204,9 @@
       <c r="CQ13" s="5">
         <v>60.4</v>
       </c>
-      <c r="CR13" s="5"/>
+      <c r="CR13" s="5">
+        <v>59.2</v>
+      </c>
       <c r="CS13" s="5"/>
       <c r="CT13" s="5"/>
       <c r="CU13" s="5"/>
@@ -11473,7 +11503,9 @@
       <c r="CQ14" s="5">
         <v>40.6</v>
       </c>
-      <c r="CR14" s="5"/>
+      <c r="CR14" s="5">
+        <v>39.75</v>
+      </c>
       <c r="CS14" s="5"/>
       <c r="CT14" s="5"/>
       <c r="CU14" s="5"/>
@@ -11762,7 +11794,9 @@
       <c r="CQ15" s="5">
         <v>24.35</v>
       </c>
-      <c r="CR15" s="5"/>
+      <c r="CR15" s="5">
+        <v>26.6</v>
+      </c>
       <c r="CS15" s="5"/>
       <c r="CT15" s="5"/>
       <c r="CU15" s="5"/>
@@ -12059,7 +12093,9 @@
       <c r="CQ16" s="5">
         <v>722</v>
       </c>
-      <c r="CR16" s="5"/>
+      <c r="CR16" s="5">
+        <v>720.4</v>
+      </c>
       <c r="CS16" s="5"/>
       <c r="CT16" s="5"/>
       <c r="CU16" s="5"/>
@@ -12356,7 +12392,9 @@
       <c r="CQ17" s="5">
         <v>527.70000000000005</v>
       </c>
-      <c r="CR17" s="5"/>
+      <c r="CR17" s="5">
+        <v>516.29999999999995</v>
+      </c>
       <c r="CS17" s="5"/>
       <c r="CT17" s="5"/>
       <c r="CU17" s="5"/>
@@ -12653,7 +12691,9 @@
       <c r="CQ18" s="5">
         <v>261.8</v>
       </c>
-      <c r="CR18" s="5"/>
+      <c r="CR18" s="5">
+        <v>262.05</v>
+      </c>
       <c r="CS18" s="5"/>
       <c r="CT18" s="5"/>
       <c r="CU18" s="5"/>
@@ -12950,7 +12990,9 @@
       <c r="CQ19" s="5">
         <v>413.15</v>
       </c>
-      <c r="CR19" s="5"/>
+      <c r="CR19" s="5">
+        <v>416.9</v>
+      </c>
       <c r="CS19" s="5"/>
       <c r="CT19" s="5"/>
       <c r="CU19" s="5"/>
@@ -13247,7 +13289,9 @@
       <c r="CQ20" s="5">
         <v>691</v>
       </c>
-      <c r="CR20" s="5"/>
+      <c r="CR20" s="5">
+        <v>677.85</v>
+      </c>
       <c r="CS20" s="5"/>
       <c r="CT20" s="5"/>
       <c r="CU20" s="5"/>
@@ -13544,7 +13588,9 @@
       <c r="CQ21" s="5">
         <v>533.04999999999995</v>
       </c>
-      <c r="CR21" s="5"/>
+      <c r="CR21" s="5">
+        <v>523.70000000000005</v>
+      </c>
       <c r="CS21" s="5"/>
       <c r="CT21" s="5"/>
       <c r="CU21" s="5"/>
@@ -13787,7 +13833,9 @@
       <c r="CQ22" s="5">
         <v>388</v>
       </c>
-      <c r="CR22" s="5"/>
+      <c r="CR22" s="5">
+        <v>381.45</v>
+      </c>
       <c r="CS22" s="5"/>
       <c r="CT22" s="5"/>
       <c r="CU22" s="5"/>
@@ -14076,7 +14124,9 @@
       <c r="CQ23" s="5">
         <v>56.9</v>
       </c>
-      <c r="CR23" s="5"/>
+      <c r="CR23" s="5">
+        <v>62.25</v>
+      </c>
       <c r="CS23" s="5"/>
       <c r="CT23" s="5"/>
       <c r="CU23" s="5"/>
@@ -14361,7 +14411,9 @@
       <c r="CQ24" s="5">
         <v>239.1</v>
       </c>
-      <c r="CR24" s="5"/>
+      <c r="CR24" s="5">
+        <v>245.95</v>
+      </c>
       <c r="CS24" s="5"/>
       <c r="CT24" s="5"/>
       <c r="CU24" s="5"/>
@@ -14628,7 +14680,9 @@
       <c r="CQ25" s="5">
         <v>1034</v>
       </c>
-      <c r="CR25" s="5"/>
+      <c r="CR25" s="5">
+        <v>1034.2</v>
+      </c>
       <c r="CS25" s="5"/>
       <c r="CT25" s="5"/>
       <c r="CU25" s="5"/>
@@ -14883,7 +14937,9 @@
       <c r="CQ26" s="5">
         <v>104.45</v>
       </c>
-      <c r="CR26" s="5"/>
+      <c r="CR26" s="5">
+        <v>106</v>
+      </c>
       <c r="CS26" s="5"/>
       <c r="CT26" s="5"/>
       <c r="CU26" s="5"/>
@@ -15138,7 +15194,9 @@
       <c r="CQ27" s="5">
         <v>40.35</v>
       </c>
-      <c r="CR27" s="5"/>
+      <c r="CR27" s="5">
+        <v>40.700000000000003</v>
+      </c>
       <c r="CS27" s="5"/>
       <c r="CT27" s="5"/>
       <c r="CU27" s="5"/>
@@ -15393,7 +15451,9 @@
       <c r="CQ28" s="5">
         <v>138.19999999999999</v>
       </c>
-      <c r="CR28" s="5"/>
+      <c r="CR28" s="5">
+        <v>134.15</v>
+      </c>
       <c r="CS28" s="5"/>
       <c r="CT28" s="5"/>
       <c r="CU28" s="5"/>
@@ -15648,7 +15708,9 @@
       <c r="CQ29" s="5">
         <v>73.3</v>
       </c>
-      <c r="CR29" s="5"/>
+      <c r="CR29" s="5">
+        <v>72.150000000000006</v>
+      </c>
       <c r="CS29" s="5"/>
       <c r="CT29" s="5"/>
       <c r="CU29" s="5"/>
@@ -15903,7 +15965,9 @@
       <c r="CQ30" s="5">
         <v>40.450000000000003</v>
       </c>
-      <c r="CR30" s="5"/>
+      <c r="CR30" s="5">
+        <v>39.85</v>
+      </c>
       <c r="CS30" s="5"/>
       <c r="CT30" s="5"/>
       <c r="CU30" s="5"/>
@@ -16158,7 +16222,9 @@
       <c r="CQ31" s="5">
         <v>159</v>
       </c>
-      <c r="CR31" s="5"/>
+      <c r="CR31" s="5">
+        <v>156.19999999999999</v>
+      </c>
       <c r="CS31" s="5"/>
       <c r="CT31" s="5"/>
       <c r="CU31" s="5"/>
@@ -16401,7 +16467,9 @@
       <c r="CQ32" s="5">
         <v>99.4</v>
       </c>
-      <c r="CR32" s="5"/>
+      <c r="CR32" s="5">
+        <v>99.3</v>
+      </c>
       <c r="CS32" s="5"/>
       <c r="CT32" s="5"/>
       <c r="CU32" s="5"/>
@@ -16632,7 +16700,9 @@
       <c r="CQ33" s="5">
         <v>76.599999999999994</v>
       </c>
-      <c r="CR33" s="5"/>
+      <c r="CR33" s="5">
+        <v>74.349999999999994</v>
+      </c>
       <c r="CS33" s="5"/>
       <c r="CT33" s="5"/>
       <c r="CU33" s="5"/>
@@ -16857,7 +16927,9 @@
       <c r="CQ34" s="5">
         <v>284.64999999999998</v>
       </c>
-      <c r="CR34" s="5"/>
+      <c r="CR34" s="5">
+        <v>281</v>
+      </c>
       <c r="CS34" s="5"/>
       <c r="CT34" s="5"/>
       <c r="CU34" s="5"/>
@@ -17060,7 +17132,9 @@
       <c r="CQ35" s="5">
         <v>390.6</v>
       </c>
-      <c r="CR35" s="5"/>
+      <c r="CR35" s="5">
+        <v>393</v>
+      </c>
       <c r="CS35" s="5"/>
       <c r="CT35" s="5"/>
       <c r="CU35" s="5"/>
@@ -17253,7 +17327,9 @@
       <c r="CQ36" s="5">
         <v>363.75</v>
       </c>
-      <c r="CR36" s="5"/>
+      <c r="CR36" s="5">
+        <v>369</v>
+      </c>
       <c r="CS36" s="5"/>
       <c r="CT36" s="5"/>
       <c r="CU36" s="5"/>
@@ -17270,11 +17346,11 @@
       </c>
       <c r="B37" s="12">
         <f t="shared" si="1"/>
-        <v>83.85</v>
+        <v>85.1</v>
       </c>
       <c r="C37" s="12">
         <f t="shared" ref="C37" si="6">B37-A37</f>
-        <v>8.6499999999999915</v>
+        <v>9.8999999999999915</v>
       </c>
       <c r="D37" s="45" t="s">
         <v>303</v>
@@ -17438,7 +17514,9 @@
       <c r="CQ37" s="5">
         <v>80</v>
       </c>
-      <c r="CR37" s="5"/>
+      <c r="CR37" s="5">
+        <v>85.1</v>
+      </c>
       <c r="CS37" s="5"/>
       <c r="CT37" s="5"/>
       <c r="CU37" s="5"/>
@@ -17623,7 +17701,9 @@
       <c r="CQ38" s="5">
         <v>432</v>
       </c>
-      <c r="CR38" s="5"/>
+      <c r="CR38" s="5">
+        <v>426.55</v>
+      </c>
       <c r="CS38" s="5"/>
       <c r="CT38" s="5"/>
       <c r="CU38" s="5"/>
@@ -17804,7 +17884,9 @@
       <c r="CQ39" s="5">
         <v>223.5</v>
       </c>
-      <c r="CR39" s="5"/>
+      <c r="CR39" s="5">
+        <v>213.05</v>
+      </c>
       <c r="CS39" s="5"/>
       <c r="CT39" s="5"/>
       <c r="CU39" s="5"/>
@@ -17981,7 +18063,9 @@
       <c r="CQ40" s="5">
         <v>40.950000000000003</v>
       </c>
-      <c r="CR40" s="5"/>
+      <c r="CR40" s="5">
+        <v>41.25</v>
+      </c>
       <c r="CS40" s="5"/>
       <c r="CT40" s="5"/>
       <c r="CU40" s="5"/>
@@ -17998,11 +18082,11 @@
       </c>
       <c r="B41" s="12">
         <f t="shared" si="1"/>
-        <v>674</v>
+        <v>725.05</v>
       </c>
       <c r="C41" s="12">
         <f t="shared" si="9"/>
-        <v>121.95000000000005</v>
+        <v>173</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>307</v>
@@ -18156,7 +18240,9 @@
       <c r="CQ41" s="5">
         <v>669</v>
       </c>
-      <c r="CR41" s="5"/>
+      <c r="CR41" s="5">
+        <v>725.05</v>
+      </c>
       <c r="CS41" s="5"/>
       <c r="CT41" s="5"/>
       <c r="CU41" s="5"/>
@@ -18331,7 +18417,9 @@
       <c r="CQ42" s="5">
         <v>876</v>
       </c>
-      <c r="CR42" s="5"/>
+      <c r="CR42" s="5">
+        <v>877.1</v>
+      </c>
       <c r="CS42" s="5"/>
       <c r="CT42" s="5"/>
       <c r="CU42" s="5"/>
@@ -18504,7 +18592,9 @@
       <c r="CQ43" s="5">
         <v>148.35</v>
       </c>
-      <c r="CR43" s="5"/>
+      <c r="CR43" s="5">
+        <v>149.80000000000001</v>
+      </c>
       <c r="CS43" s="5"/>
       <c r="CT43" s="5"/>
       <c r="CU43" s="5"/>
@@ -18671,7 +18761,9 @@
       <c r="CQ44" s="5">
         <v>600</v>
       </c>
-      <c r="CR44" s="5"/>
+      <c r="CR44" s="5">
+        <v>608</v>
+      </c>
       <c r="CS44" s="5"/>
       <c r="CT44" s="5"/>
       <c r="CU44" s="5"/>
@@ -18830,7 +18922,9 @@
       <c r="CQ45" s="5">
         <v>107.4</v>
       </c>
-      <c r="CR45" s="5"/>
+      <c r="CR45" s="5">
+        <v>106.15</v>
+      </c>
       <c r="CS45" s="5"/>
       <c r="CT45" s="5"/>
       <c r="CU45" s="5"/>
@@ -18975,7 +19069,9 @@
       <c r="CQ46" s="5">
         <v>136.35</v>
       </c>
-      <c r="CR46" s="5"/>
+      <c r="CR46" s="5">
+        <v>135.15</v>
+      </c>
       <c r="CS46" s="5"/>
       <c r="CT46" s="5"/>
       <c r="CU46" s="5"/>
@@ -19102,7 +19198,9 @@
       <c r="CQ47" s="5">
         <v>93.25</v>
       </c>
-      <c r="CR47" s="5"/>
+      <c r="CR47" s="5">
+        <v>93.85</v>
+      </c>
       <c r="CS47" s="5"/>
       <c r="CT47" s="5"/>
       <c r="CU47" s="5"/>
@@ -19111,6 +19209,125 @@
       <c r="CX47" s="5"/>
       <c r="CY47" s="5"/>
       <c r="CZ47" s="5"/>
+    </row>
+    <row r="48" spans="1:104" x14ac:dyDescent="0.25">
+      <c r="A48" s="12">
+        <f t="shared" ref="A48" si="16">MIN(E48:ZQ48)</f>
+        <v>96</v>
+      </c>
+      <c r="B48" s="12">
+        <f t="shared" ref="B48" si="17">MAX(E48:ZQ48)</f>
+        <v>96</v>
+      </c>
+      <c r="C48" s="12">
+        <f t="shared" ref="C48" si="18">B48-A48</f>
+        <v>0</v>
+      </c>
+      <c r="D48" s="45" t="s">
+        <v>336</v>
+      </c>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5"/>
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="5"/>
+      <c r="AC48" s="5"/>
+      <c r="AD48" s="5"/>
+      <c r="AE48" s="5"/>
+      <c r="AF48" s="5"/>
+      <c r="AG48" s="5"/>
+      <c r="AH48" s="5"/>
+      <c r="AI48" s="5"/>
+      <c r="AJ48" s="5"/>
+      <c r="AK48" s="5"/>
+      <c r="AL48" s="5"/>
+      <c r="AM48" s="5"/>
+      <c r="AN48" s="5"/>
+      <c r="AO48" s="5"/>
+      <c r="AP48" s="5"/>
+      <c r="AQ48" s="5"/>
+      <c r="AR48" s="5"/>
+      <c r="AS48" s="5"/>
+      <c r="AT48" s="5"/>
+      <c r="AU48" s="5"/>
+      <c r="AV48" s="5"/>
+      <c r="AW48" s="5"/>
+      <c r="AX48" s="5"/>
+      <c r="AY48" s="5"/>
+      <c r="AZ48" s="5"/>
+      <c r="BA48" s="5"/>
+      <c r="BB48" s="5"/>
+      <c r="BC48" s="5"/>
+      <c r="BD48" s="5"/>
+      <c r="BE48" s="5"/>
+      <c r="BF48" s="5"/>
+      <c r="BG48" s="5"/>
+      <c r="BH48" s="5"/>
+      <c r="BI48" s="5"/>
+      <c r="BJ48" s="5"/>
+      <c r="BK48" s="5"/>
+      <c r="BL48" s="5"/>
+      <c r="BM48" s="5"/>
+      <c r="BN48" s="5"/>
+      <c r="BO48" s="5"/>
+      <c r="BP48" s="5"/>
+      <c r="BQ48" s="5"/>
+      <c r="BR48" s="5"/>
+      <c r="BS48" s="5"/>
+      <c r="BT48" s="5"/>
+      <c r="BU48" s="5"/>
+      <c r="BV48" s="5"/>
+      <c r="BW48" s="5"/>
+      <c r="BX48" s="5"/>
+      <c r="BY48" s="5"/>
+      <c r="BZ48" s="5"/>
+      <c r="CA48" s="5"/>
+      <c r="CB48" s="5"/>
+      <c r="CC48" s="5"/>
+      <c r="CD48" s="5"/>
+      <c r="CE48" s="5"/>
+      <c r="CF48" s="5"/>
+      <c r="CG48" s="5"/>
+      <c r="CH48" s="5"/>
+      <c r="CI48" s="5"/>
+      <c r="CJ48" s="5"/>
+      <c r="CK48" s="5"/>
+      <c r="CL48" s="5"/>
+      <c r="CM48" s="5"/>
+      <c r="CN48" s="5"/>
+      <c r="CO48" s="5"/>
+      <c r="CP48" s="5"/>
+      <c r="CQ48" s="5">
+        <v>96</v>
+      </c>
+      <c r="CR48" s="5"/>
+      <c r="CS48" s="5"/>
+      <c r="CT48" s="5"/>
+      <c r="CU48" s="5"/>
+      <c r="CV48" s="5"/>
+      <c r="CW48" s="5"/>
+      <c r="CX48" s="5"/>
+      <c r="CY48" s="5"/>
+      <c r="CZ48" s="5"/>
     </row>
   </sheetData>
   <sortState ref="L1:L37">

</xml_diff>

<commit_message>
Added details for 09/01/2018
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -7307,9 +7307,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DA48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="5" topLeftCell="CS1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CV1" sqref="CV1:CV48"/>
+      <selection pane="topRight" activeCell="CW48" sqref="CW48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7368,7 +7368,7 @@
     <col min="93" max="93" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="14" bestFit="1" customWidth="1"/>
     <col min="95" max="96" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="97" max="100" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="97" max="101" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:105" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7672,7 +7672,9 @@
       <c r="CV1" s="11">
         <v>43221</v>
       </c>
-      <c r="CW1" s="27"/>
+      <c r="CW1" s="11">
+        <v>43344</v>
+      </c>
       <c r="CX1" s="27"/>
       <c r="CY1" s="27"/>
       <c r="CZ1" s="27"/>
@@ -7972,7 +7974,9 @@
       <c r="CV2" s="5">
         <v>307.25</v>
       </c>
-      <c r="CW2" s="5"/>
+      <c r="CW2" s="5">
+        <v>306.8</v>
+      </c>
       <c r="CX2" s="5"/>
       <c r="CY2" s="5"/>
       <c r="CZ2" s="5"/>
@@ -8272,7 +8276,9 @@
       <c r="CV3" s="5">
         <v>313.39999999999998</v>
       </c>
-      <c r="CW3" s="5"/>
+      <c r="CW3" s="5">
+        <v>313.3</v>
+      </c>
       <c r="CX3" s="5"/>
       <c r="CY3" s="5"/>
       <c r="CZ3" s="5"/>
@@ -8580,7 +8586,9 @@
       <c r="CV4" s="5">
         <v>263</v>
       </c>
-      <c r="CW4" s="5"/>
+      <c r="CW4" s="5">
+        <v>266</v>
+      </c>
       <c r="CX4" s="5"/>
       <c r="CY4" s="5"/>
       <c r="CZ4" s="5"/>
@@ -8886,7 +8894,9 @@
       <c r="CV5" s="5">
         <v>923</v>
       </c>
-      <c r="CW5" s="5"/>
+      <c r="CW5" s="5">
+        <v>927</v>
+      </c>
       <c r="CX5" s="5"/>
       <c r="CY5" s="5"/>
       <c r="CZ5" s="5"/>
@@ -8899,11 +8909,11 @@
       </c>
       <c r="B6" s="12">
         <f t="shared" si="1"/>
-        <v>293.95</v>
+        <v>300.2</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="2"/>
-        <v>57.5</v>
+        <v>63.75</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="45" t="s">
@@ -9192,7 +9202,9 @@
       <c r="CV6" s="5">
         <v>278</v>
       </c>
-      <c r="CW6" s="5"/>
+      <c r="CW6" s="5">
+        <v>300.2</v>
+      </c>
       <c r="CX6" s="5"/>
       <c r="CY6" s="5"/>
       <c r="CZ6" s="5"/>
@@ -9498,7 +9510,9 @@
       <c r="CV7" s="5">
         <v>21.2</v>
       </c>
-      <c r="CW7" s="5"/>
+      <c r="CW7" s="5">
+        <v>22.1</v>
+      </c>
       <c r="CX7" s="5"/>
       <c r="CY7" s="5"/>
       <c r="CZ7" s="5"/>
@@ -9511,11 +9525,11 @@
       </c>
       <c r="B8" s="12">
         <f t="shared" si="1"/>
-        <v>98.15</v>
+        <v>99</v>
       </c>
       <c r="C8" s="12">
         <f t="shared" si="2"/>
-        <v>44.750000000000007</v>
+        <v>45.6</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="45" t="s">
@@ -9804,7 +9818,9 @@
       <c r="CV8" s="5">
         <v>97.6</v>
       </c>
-      <c r="CW8" s="5"/>
+      <c r="CW8" s="5">
+        <v>99</v>
+      </c>
       <c r="CX8" s="5"/>
       <c r="CY8" s="5"/>
       <c r="CZ8" s="5"/>
@@ -9817,11 +9833,11 @@
       </c>
       <c r="B9" s="39">
         <f t="shared" si="1"/>
-        <v>61</v>
+        <v>63.75</v>
       </c>
       <c r="C9" s="12">
         <f t="shared" si="2"/>
-        <v>9.4500000000000028</v>
+        <v>12.200000000000003</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="43" t="s">
@@ -10102,7 +10118,9 @@
       <c r="CV9" s="28">
         <v>58.35</v>
       </c>
-      <c r="CW9" s="28"/>
+      <c r="CW9" s="28">
+        <v>63.75</v>
+      </c>
       <c r="CX9" s="28"/>
       <c r="CY9" s="28"/>
       <c r="CZ9" s="28"/>
@@ -10115,11 +10133,11 @@
       </c>
       <c r="B10" s="12">
         <f t="shared" si="1"/>
-        <v>58.65</v>
+        <v>61.5</v>
       </c>
       <c r="C10" s="12">
         <f t="shared" si="2"/>
-        <v>23.5</v>
+        <v>26.35</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="45" t="s">
@@ -10408,7 +10426,9 @@
       <c r="CV10" s="5">
         <v>58.65</v>
       </c>
-      <c r="CW10" s="5"/>
+      <c r="CW10" s="5">
+        <v>61.5</v>
+      </c>
       <c r="CX10" s="5"/>
       <c r="CY10" s="5"/>
       <c r="CZ10" s="5"/>
@@ -10714,7 +10734,9 @@
       <c r="CV11" s="5">
         <v>115.3</v>
       </c>
-      <c r="CW11" s="5"/>
+      <c r="CW11" s="5">
+        <v>109.95</v>
+      </c>
       <c r="CX11" s="5"/>
       <c r="CY11" s="5"/>
       <c r="CZ11" s="5"/>
@@ -11020,7 +11042,9 @@
       <c r="CV12" s="5">
         <v>102</v>
       </c>
-      <c r="CW12" s="5"/>
+      <c r="CW12" s="5">
+        <v>101.35</v>
+      </c>
       <c r="CX12" s="5"/>
       <c r="CY12" s="5"/>
       <c r="CZ12" s="5"/>
@@ -11033,11 +11057,11 @@
       </c>
       <c r="B13" s="12">
         <f t="shared" si="1"/>
-        <v>60.55</v>
+        <v>60.8</v>
       </c>
       <c r="C13" s="12">
         <f t="shared" si="2"/>
-        <v>16.449999999999996</v>
+        <v>16.699999999999996</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="45" t="s">
@@ -11326,7 +11350,9 @@
       <c r="CV13" s="5">
         <v>60.55</v>
       </c>
-      <c r="CW13" s="5"/>
+      <c r="CW13" s="5">
+        <v>60.8</v>
+      </c>
       <c r="CX13" s="5"/>
       <c r="CY13" s="5"/>
       <c r="CZ13" s="5"/>
@@ -11632,7 +11658,9 @@
       <c r="CV14" s="5">
         <v>40</v>
       </c>
-      <c r="CW14" s="5"/>
+      <c r="CW14" s="5">
+        <v>39.85</v>
+      </c>
       <c r="CX14" s="5"/>
       <c r="CY14" s="5"/>
       <c r="CZ14" s="5"/>
@@ -11930,7 +11958,9 @@
       <c r="CV15" s="5">
         <v>27.1</v>
       </c>
-      <c r="CW15" s="5"/>
+      <c r="CW15" s="5">
+        <v>27.65</v>
+      </c>
       <c r="CX15" s="5"/>
       <c r="CY15" s="5"/>
       <c r="CZ15" s="5"/>
@@ -11943,11 +11973,11 @@
       </c>
       <c r="B16" s="12">
         <f t="shared" si="1"/>
-        <v>770.4</v>
+        <v>771.65</v>
       </c>
       <c r="C16" s="12">
         <f t="shared" si="2"/>
-        <v>218.39999999999998</v>
+        <v>219.64999999999998</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="45" t="s">
@@ -12236,7 +12266,9 @@
       <c r="CV16" s="5">
         <v>770.4</v>
       </c>
-      <c r="CW16" s="5"/>
+      <c r="CW16" s="5">
+        <v>771.65</v>
+      </c>
       <c r="CX16" s="5"/>
       <c r="CY16" s="5"/>
       <c r="CZ16" s="5"/>
@@ -12542,7 +12574,9 @@
       <c r="CV17" s="5">
         <v>526.70000000000005</v>
       </c>
-      <c r="CW17" s="5"/>
+      <c r="CW17" s="5">
+        <v>524</v>
+      </c>
       <c r="CX17" s="5"/>
       <c r="CY17" s="5"/>
       <c r="CZ17" s="5"/>
@@ -12848,7 +12882,9 @@
       <c r="CV18" s="5">
         <v>259</v>
       </c>
-      <c r="CW18" s="5"/>
+      <c r="CW18" s="5">
+        <v>270.55</v>
+      </c>
       <c r="CX18" s="5"/>
       <c r="CY18" s="5"/>
       <c r="CZ18" s="5"/>
@@ -13154,7 +13190,9 @@
       <c r="CV19" s="5">
         <v>405.4</v>
       </c>
-      <c r="CW19" s="5"/>
+      <c r="CW19" s="5">
+        <v>425.95</v>
+      </c>
       <c r="CX19" s="5"/>
       <c r="CY19" s="5"/>
       <c r="CZ19" s="5"/>
@@ -13460,7 +13498,9 @@
       <c r="CV20" s="5">
         <v>670.05</v>
       </c>
-      <c r="CW20" s="5"/>
+      <c r="CW20" s="5">
+        <v>678.8</v>
+      </c>
       <c r="CX20" s="5"/>
       <c r="CY20" s="5"/>
       <c r="CZ20" s="5"/>
@@ -13766,7 +13806,9 @@
       <c r="CV21" s="5">
         <v>539.9</v>
       </c>
-      <c r="CW21" s="5"/>
+      <c r="CW21" s="5">
+        <v>520.1</v>
+      </c>
       <c r="CX21" s="5"/>
       <c r="CY21" s="5"/>
       <c r="CZ21" s="5"/>
@@ -13779,11 +13821,11 @@
       </c>
       <c r="B22" s="12">
         <f t="shared" si="1"/>
-        <v>413.5</v>
+        <v>415.9</v>
       </c>
       <c r="C22" s="12">
         <f t="shared" si="2"/>
-        <v>98.300000000000011</v>
+        <v>100.69999999999999</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="44" t="s">
@@ -14018,7 +14060,9 @@
       <c r="CV22" s="5">
         <v>407.2</v>
       </c>
-      <c r="CW22" s="5"/>
+      <c r="CW22" s="5">
+        <v>415.9</v>
+      </c>
       <c r="CX22" s="5"/>
       <c r="CY22" s="5"/>
       <c r="CZ22" s="5"/>
@@ -14316,7 +14360,9 @@
       <c r="CV23" s="5">
         <v>64</v>
       </c>
-      <c r="CW23" s="5"/>
+      <c r="CW23" s="5">
+        <v>64.900000000000006</v>
+      </c>
       <c r="CX23" s="5"/>
       <c r="CY23" s="5"/>
       <c r="CZ23" s="5"/>
@@ -14610,7 +14656,9 @@
       <c r="CV24" s="5">
         <v>252.45</v>
       </c>
-      <c r="CW24" s="5"/>
+      <c r="CW24" s="5">
+        <v>254.05</v>
+      </c>
       <c r="CX24" s="5"/>
       <c r="CY24" s="5"/>
       <c r="CZ24" s="5"/>
@@ -14623,11 +14671,11 @@
       </c>
       <c r="B25" s="12">
         <f t="shared" si="1"/>
-        <v>1035</v>
+        <v>1038.05</v>
       </c>
       <c r="C25" s="12">
         <f t="shared" si="2"/>
-        <v>159</v>
+        <v>162.04999999999995</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="46" t="s">
@@ -14886,7 +14934,9 @@
       <c r="CV25" s="5">
         <v>1014.25</v>
       </c>
-      <c r="CW25" s="5"/>
+      <c r="CW25" s="5">
+        <v>1038.05</v>
+      </c>
       <c r="CX25" s="5"/>
       <c r="CY25" s="5"/>
       <c r="CZ25" s="5"/>
@@ -15150,7 +15200,9 @@
       <c r="CV26" s="5">
         <v>112.1</v>
       </c>
-      <c r="CW26" s="5"/>
+      <c r="CW26" s="5">
+        <v>110.4</v>
+      </c>
       <c r="CX26" s="5"/>
       <c r="CY26" s="5"/>
       <c r="CZ26" s="5"/>
@@ -15414,7 +15466,9 @@
       <c r="CV27" s="5">
         <v>41.45</v>
       </c>
-      <c r="CW27" s="5"/>
+      <c r="CW27" s="5">
+        <v>41.85</v>
+      </c>
       <c r="CX27" s="5"/>
       <c r="CY27" s="5"/>
       <c r="CZ27" s="5"/>
@@ -15680,7 +15734,9 @@
       <c r="CV28" s="5">
         <v>139.15</v>
       </c>
-      <c r="CW28" s="5"/>
+      <c r="CW28" s="5">
+        <v>140.25</v>
+      </c>
       <c r="CX28" s="5"/>
       <c r="CY28" s="5"/>
       <c r="CZ28" s="5"/>
@@ -15946,7 +16002,9 @@
       <c r="CV29" s="5">
         <v>71.2</v>
       </c>
-      <c r="CW29" s="5"/>
+      <c r="CW29" s="5">
+        <v>72.3</v>
+      </c>
       <c r="CX29" s="5"/>
       <c r="CY29" s="5"/>
       <c r="CZ29" s="5"/>
@@ -16210,7 +16268,9 @@
       <c r="CV30" s="5">
         <v>41.75</v>
       </c>
-      <c r="CW30" s="5"/>
+      <c r="CW30" s="5">
+        <v>44.4</v>
+      </c>
       <c r="CX30" s="5"/>
       <c r="CY30" s="5"/>
       <c r="CZ30" s="5"/>
@@ -16474,7 +16534,9 @@
       <c r="CV31" s="5">
         <v>162.5</v>
       </c>
-      <c r="CW31" s="5"/>
+      <c r="CW31" s="5">
+        <v>163.65</v>
+      </c>
       <c r="CX31" s="5"/>
       <c r="CY31" s="5"/>
       <c r="CZ31" s="5"/>
@@ -16728,7 +16790,9 @@
       <c r="CV32" s="5">
         <v>98.15</v>
       </c>
-      <c r="CW32" s="5"/>
+      <c r="CW32" s="5">
+        <v>105.7</v>
+      </c>
       <c r="CX32" s="5"/>
       <c r="CY32" s="5"/>
       <c r="CZ32" s="5"/>
@@ -16968,7 +17032,9 @@
       <c r="CV33" s="5">
         <v>75.05</v>
       </c>
-      <c r="CW33" s="5"/>
+      <c r="CW33" s="5">
+        <v>74.150000000000006</v>
+      </c>
       <c r="CX33" s="5"/>
       <c r="CY33" s="5"/>
       <c r="CZ33" s="5"/>
@@ -16981,11 +17047,11 @@
       </c>
       <c r="B34" s="12">
         <f t="shared" si="1"/>
-        <v>294.95</v>
+        <v>298.8</v>
       </c>
       <c r="C34" s="12">
         <f t="shared" si="2"/>
-        <v>127.04999999999998</v>
+        <v>130.9</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="45" t="s">
@@ -17202,7 +17268,9 @@
       <c r="CV34" s="5">
         <v>277.7</v>
       </c>
-      <c r="CW34" s="5"/>
+      <c r="CW34" s="5">
+        <v>298.8</v>
+      </c>
       <c r="CX34" s="5"/>
       <c r="CY34" s="5"/>
       <c r="CZ34" s="5"/>
@@ -17414,7 +17482,9 @@
       <c r="CV35" s="5">
         <v>399</v>
       </c>
-      <c r="CW35" s="5"/>
+      <c r="CW35" s="5">
+        <v>433</v>
+      </c>
       <c r="CX35" s="5"/>
       <c r="CY35" s="5"/>
       <c r="CZ35" s="5"/>
@@ -17427,11 +17497,11 @@
       </c>
       <c r="B36" s="12">
         <f t="shared" si="1"/>
-        <v>429.95</v>
+        <v>465.8</v>
       </c>
       <c r="C36" s="12">
         <f t="shared" si="2"/>
-        <v>203.95</v>
+        <v>239.8</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="45" t="s">
@@ -17616,7 +17686,9 @@
       <c r="CV36" s="5">
         <v>420</v>
       </c>
-      <c r="CW36" s="5"/>
+      <c r="CW36" s="5">
+        <v>465.8</v>
+      </c>
       <c r="CX36" s="5"/>
       <c r="CY36" s="5"/>
       <c r="CZ36" s="5"/>
@@ -17629,11 +17701,11 @@
       </c>
       <c r="B37" s="12">
         <f t="shared" si="1"/>
-        <v>85.35</v>
+        <v>85.5</v>
       </c>
       <c r="C37" s="12">
         <f t="shared" si="2"/>
-        <v>10.149999999999991</v>
+        <v>10.299999999999997</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="45" t="s">
@@ -17810,7 +17882,9 @@
       <c r="CV37" s="5">
         <v>84.9</v>
       </c>
-      <c r="CW37" s="5"/>
+      <c r="CW37" s="5">
+        <v>85.5</v>
+      </c>
       <c r="CX37" s="5"/>
       <c r="CY37" s="5"/>
       <c r="CZ37" s="5"/>
@@ -18006,7 +18080,9 @@
       <c r="CV38" s="5">
         <v>422.6</v>
       </c>
-      <c r="CW38" s="5"/>
+      <c r="CW38" s="5">
+        <v>427.85</v>
+      </c>
       <c r="CX38" s="5"/>
       <c r="CY38" s="5"/>
       <c r="CZ38" s="5"/>
@@ -18196,7 +18272,9 @@
       <c r="CV39" s="5">
         <v>209.5</v>
       </c>
-      <c r="CW39" s="5"/>
+      <c r="CW39" s="5">
+        <v>212.25</v>
+      </c>
       <c r="CX39" s="5"/>
       <c r="CY39" s="5"/>
       <c r="CZ39" s="5"/>
@@ -18209,11 +18287,11 @@
       </c>
       <c r="B40" s="12">
         <f t="shared" si="1"/>
-        <v>41.95</v>
+        <v>43</v>
       </c>
       <c r="C40" s="12">
         <f t="shared" si="2"/>
-        <v>7.4500000000000028</v>
+        <v>8.5</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="45" t="s">
@@ -18382,7 +18460,9 @@
       <c r="CV40" s="5">
         <v>41.9</v>
       </c>
-      <c r="CW40" s="5"/>
+      <c r="CW40" s="5">
+        <v>43</v>
+      </c>
       <c r="CX40" s="5"/>
       <c r="CY40" s="5"/>
       <c r="CZ40" s="5"/>
@@ -18395,11 +18475,11 @@
       </c>
       <c r="B41" s="12">
         <f t="shared" si="1"/>
-        <v>856.95</v>
+        <v>866.3</v>
       </c>
       <c r="C41" s="12">
         <f t="shared" si="2"/>
-        <v>304.90000000000009</v>
+        <v>314.25</v>
       </c>
       <c r="D41" s="12"/>
       <c r="E41" s="45" t="s">
@@ -18566,7 +18646,9 @@
       <c r="CV41" s="5">
         <v>809</v>
       </c>
-      <c r="CW41" s="5"/>
+      <c r="CW41" s="5">
+        <v>866.3</v>
+      </c>
       <c r="CX41" s="5"/>
       <c r="CY41" s="5"/>
       <c r="CZ41" s="5"/>
@@ -18579,11 +18661,11 @@
       </c>
       <c r="B42" s="12">
         <f t="shared" si="1"/>
-        <v>900.8</v>
+        <v>922.55</v>
       </c>
       <c r="C42" s="12">
         <f t="shared" si="2"/>
-        <v>90.199999999999932</v>
+        <v>111.94999999999993</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="45" t="s">
@@ -18750,7 +18832,9 @@
       <c r="CV42" s="5">
         <v>900.8</v>
       </c>
-      <c r="CW42" s="5"/>
+      <c r="CW42" s="5">
+        <v>922.55</v>
+      </c>
       <c r="CX42" s="5"/>
       <c r="CY42" s="5"/>
       <c r="CZ42" s="5"/>
@@ -18934,7 +19018,9 @@
       <c r="CV43" s="5">
         <v>154.25</v>
       </c>
-      <c r="CW43" s="5"/>
+      <c r="CW43" s="5">
+        <v>153.65</v>
+      </c>
       <c r="CX43" s="5"/>
       <c r="CY43" s="5"/>
       <c r="CZ43" s="5"/>
@@ -19112,7 +19198,9 @@
       <c r="CV44" s="5">
         <v>625.04999999999995</v>
       </c>
-      <c r="CW44" s="5"/>
+      <c r="CW44" s="5">
+        <v>626.25</v>
+      </c>
       <c r="CX44" s="5"/>
       <c r="CY44" s="5"/>
       <c r="CZ44" s="5"/>
@@ -19280,7 +19368,9 @@
       <c r="CV45" s="5">
         <v>120.45</v>
       </c>
-      <c r="CW45" s="5"/>
+      <c r="CW45" s="5">
+        <v>120.35</v>
+      </c>
       <c r="CX45" s="5"/>
       <c r="CY45" s="5"/>
       <c r="CZ45" s="5"/>
@@ -19436,7 +19526,9 @@
       <c r="CV46" s="5">
         <v>137.30000000000001</v>
       </c>
-      <c r="CW46" s="5"/>
+      <c r="CW46" s="5">
+        <v>137.15</v>
+      </c>
       <c r="CX46" s="5"/>
       <c r="CY46" s="5"/>
       <c r="CZ46" s="5"/>
@@ -19572,7 +19664,9 @@
       <c r="CV47" s="5">
         <v>96.1</v>
       </c>
-      <c r="CW47" s="5"/>
+      <c r="CW47" s="5">
+        <v>95.9</v>
+      </c>
       <c r="CX47" s="5"/>
       <c r="CY47" s="5"/>
       <c r="CZ47" s="5"/>
@@ -19585,11 +19679,11 @@
       </c>
       <c r="B48" s="12">
         <f t="shared" ref="B48" si="6">MAX(F48:ZR48)</f>
-        <v>104.4</v>
+        <v>108</v>
       </c>
       <c r="C48" s="12">
         <f t="shared" ref="C48" si="7">B48-A48</f>
-        <v>8.4000000000000057</v>
+        <v>12</v>
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="45" t="s">
@@ -19698,7 +19792,9 @@
       <c r="CV48" s="5">
         <v>104.4</v>
       </c>
-      <c r="CW48" s="5"/>
+      <c r="CW48" s="5">
+        <v>108</v>
+      </c>
       <c r="CX48" s="5"/>
       <c r="CY48" s="5"/>
       <c r="CZ48" s="5"/>

</xml_diff>

<commit_message>
Added details for 11/01/2018
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -7307,9 +7307,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DA48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="CS1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CW48" sqref="CW48"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="CO1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CX1" sqref="CX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7369,6 +7369,7 @@
     <col min="94" max="94" width="14" bestFit="1" customWidth="1"/>
     <col min="95" max="96" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="97" max="101" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:105" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7675,7 +7676,9 @@
       <c r="CW1" s="11">
         <v>43344</v>
       </c>
-      <c r="CX1" s="27"/>
+      <c r="CX1" s="11">
+        <v>43405</v>
+      </c>
       <c r="CY1" s="27"/>
       <c r="CZ1" s="27"/>
       <c r="DA1" s="27"/>
@@ -7977,7 +7980,9 @@
       <c r="CW2" s="5">
         <v>306.8</v>
       </c>
-      <c r="CX2" s="5"/>
+      <c r="CX2" s="5">
+        <v>302.14999999999998</v>
+      </c>
       <c r="CY2" s="5"/>
       <c r="CZ2" s="5"/>
       <c r="DA2" s="5"/>
@@ -8279,7 +8284,9 @@
       <c r="CW3" s="5">
         <v>313.3</v>
       </c>
-      <c r="CX3" s="5"/>
+      <c r="CX3" s="5">
+        <v>308.85000000000002</v>
+      </c>
       <c r="CY3" s="5"/>
       <c r="CZ3" s="5"/>
       <c r="DA3" s="5"/>
@@ -8589,7 +8596,9 @@
       <c r="CW4" s="5">
         <v>266</v>
       </c>
-      <c r="CX4" s="5"/>
+      <c r="CX4" s="5">
+        <v>269.95</v>
+      </c>
       <c r="CY4" s="5"/>
       <c r="CZ4" s="5"/>
       <c r="DA4" s="5"/>
@@ -8897,7 +8906,9 @@
       <c r="CW5" s="5">
         <v>927</v>
       </c>
-      <c r="CX5" s="5"/>
+      <c r="CX5" s="5">
+        <v>936.9</v>
+      </c>
       <c r="CY5" s="5"/>
       <c r="CZ5" s="5"/>
       <c r="DA5" s="5"/>
@@ -8909,11 +8920,11 @@
       </c>
       <c r="B6" s="12">
         <f t="shared" si="1"/>
-        <v>300.2</v>
+        <v>308.14999999999998</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="2"/>
-        <v>63.75</v>
+        <v>71.699999999999989</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="45" t="s">
@@ -9205,7 +9216,9 @@
       <c r="CW6" s="5">
         <v>300.2</v>
       </c>
-      <c r="CX6" s="5"/>
+      <c r="CX6" s="5">
+        <v>308.14999999999998</v>
+      </c>
       <c r="CY6" s="5"/>
       <c r="CZ6" s="5"/>
       <c r="DA6" s="5"/>
@@ -9513,7 +9526,9 @@
       <c r="CW7" s="5">
         <v>22.1</v>
       </c>
-      <c r="CX7" s="5"/>
+      <c r="CX7" s="5">
+        <v>21.65</v>
+      </c>
       <c r="CY7" s="5"/>
       <c r="CZ7" s="5"/>
       <c r="DA7" s="5"/>
@@ -9821,7 +9836,9 @@
       <c r="CW8" s="5">
         <v>99</v>
       </c>
-      <c r="CX8" s="5"/>
+      <c r="CX8" s="5">
+        <v>98.4</v>
+      </c>
       <c r="CY8" s="5"/>
       <c r="CZ8" s="5"/>
       <c r="DA8" s="5"/>
@@ -9833,11 +9850,11 @@
       </c>
       <c r="B9" s="39">
         <f t="shared" si="1"/>
-        <v>63.75</v>
+        <v>68.25</v>
       </c>
       <c r="C9" s="12">
         <f t="shared" si="2"/>
-        <v>12.200000000000003</v>
+        <v>16.700000000000003</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="43" t="s">
@@ -10121,7 +10138,9 @@
       <c r="CW9" s="28">
         <v>63.75</v>
       </c>
-      <c r="CX9" s="28"/>
+      <c r="CX9" s="28">
+        <v>68.25</v>
+      </c>
       <c r="CY9" s="28"/>
       <c r="CZ9" s="28"/>
       <c r="DA9" s="28"/>
@@ -10429,7 +10448,9 @@
       <c r="CW10" s="5">
         <v>61.5</v>
       </c>
-      <c r="CX10" s="5"/>
+      <c r="CX10" s="5">
+        <v>55.55</v>
+      </c>
       <c r="CY10" s="5"/>
       <c r="CZ10" s="5"/>
       <c r="DA10" s="5"/>
@@ -10737,7 +10758,9 @@
       <c r="CW11" s="5">
         <v>109.95</v>
       </c>
-      <c r="CX11" s="5"/>
+      <c r="CX11" s="5">
+        <v>107.15</v>
+      </c>
       <c r="CY11" s="5"/>
       <c r="CZ11" s="5"/>
       <c r="DA11" s="5"/>
@@ -10749,11 +10772,11 @@
       </c>
       <c r="B12" s="12">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>103.55</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" si="2"/>
-        <v>19.349999999999994</v>
+        <v>20.899999999999991</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="45" t="s">
@@ -11045,7 +11068,9 @@
       <c r="CW12" s="5">
         <v>101.35</v>
       </c>
-      <c r="CX12" s="5"/>
+      <c r="CX12" s="5">
+        <v>103.55</v>
+      </c>
       <c r="CY12" s="5"/>
       <c r="CZ12" s="5"/>
       <c r="DA12" s="5"/>
@@ -11353,7 +11378,9 @@
       <c r="CW13" s="5">
         <v>60.8</v>
       </c>
-      <c r="CX13" s="5"/>
+      <c r="CX13" s="5">
+        <v>60</v>
+      </c>
       <c r="CY13" s="5"/>
       <c r="CZ13" s="5"/>
       <c r="DA13" s="5"/>
@@ -11661,7 +11688,9 @@
       <c r="CW14" s="5">
         <v>39.85</v>
       </c>
-      <c r="CX14" s="5"/>
+      <c r="CX14" s="5">
+        <v>40.35</v>
+      </c>
       <c r="CY14" s="5"/>
       <c r="CZ14" s="5"/>
       <c r="DA14" s="5"/>
@@ -11961,7 +11990,9 @@
       <c r="CW15" s="5">
         <v>27.65</v>
       </c>
-      <c r="CX15" s="5"/>
+      <c r="CX15" s="5">
+        <v>27.5</v>
+      </c>
       <c r="CY15" s="5"/>
       <c r="CZ15" s="5"/>
       <c r="DA15" s="5"/>
@@ -12269,7 +12300,9 @@
       <c r="CW16" s="5">
         <v>771.65</v>
       </c>
-      <c r="CX16" s="5"/>
+      <c r="CX16" s="5">
+        <v>769</v>
+      </c>
       <c r="CY16" s="5"/>
       <c r="CZ16" s="5"/>
       <c r="DA16" s="5"/>
@@ -12577,7 +12610,9 @@
       <c r="CW17" s="5">
         <v>524</v>
       </c>
-      <c r="CX17" s="5"/>
+      <c r="CX17" s="5">
+        <v>529.4</v>
+      </c>
       <c r="CY17" s="5"/>
       <c r="CZ17" s="5"/>
       <c r="DA17" s="5"/>
@@ -12885,7 +12920,9 @@
       <c r="CW18" s="5">
         <v>270.55</v>
       </c>
-      <c r="CX18" s="5"/>
+      <c r="CX18" s="5">
+        <v>272.10000000000002</v>
+      </c>
       <c r="CY18" s="5"/>
       <c r="CZ18" s="5"/>
       <c r="DA18" s="5"/>
@@ -13193,7 +13230,9 @@
       <c r="CW19" s="5">
         <v>425.95</v>
       </c>
-      <c r="CX19" s="5"/>
+      <c r="CX19" s="5">
+        <v>448</v>
+      </c>
       <c r="CY19" s="5"/>
       <c r="CZ19" s="5"/>
       <c r="DA19" s="5"/>
@@ -13501,7 +13540,9 @@
       <c r="CW20" s="5">
         <v>678.8</v>
       </c>
-      <c r="CX20" s="5"/>
+      <c r="CX20" s="5">
+        <v>674.9</v>
+      </c>
       <c r="CY20" s="5"/>
       <c r="CZ20" s="5"/>
       <c r="DA20" s="5"/>
@@ -13809,7 +13850,9 @@
       <c r="CW21" s="5">
         <v>520.1</v>
       </c>
-      <c r="CX21" s="5"/>
+      <c r="CX21" s="5">
+        <v>515.9</v>
+      </c>
       <c r="CY21" s="5"/>
       <c r="CZ21" s="5"/>
       <c r="DA21" s="5"/>
@@ -14063,7 +14106,9 @@
       <c r="CW22" s="5">
         <v>415.9</v>
       </c>
-      <c r="CX22" s="5"/>
+      <c r="CX22" s="5">
+        <v>414.65</v>
+      </c>
       <c r="CY22" s="5"/>
       <c r="CZ22" s="5"/>
       <c r="DA22" s="5"/>
@@ -14363,7 +14408,9 @@
       <c r="CW23" s="5">
         <v>64.900000000000006</v>
       </c>
-      <c r="CX23" s="5"/>
+      <c r="CX23" s="5">
+        <v>64.5</v>
+      </c>
       <c r="CY23" s="5"/>
       <c r="CZ23" s="5"/>
       <c r="DA23" s="5"/>
@@ -14659,7 +14706,9 @@
       <c r="CW24" s="5">
         <v>254.05</v>
       </c>
-      <c r="CX24" s="5"/>
+      <c r="CX24" s="5">
+        <v>254.1</v>
+      </c>
       <c r="CY24" s="5"/>
       <c r="CZ24" s="5"/>
       <c r="DA24" s="5"/>
@@ -14671,11 +14720,11 @@
       </c>
       <c r="B25" s="12">
         <f t="shared" si="1"/>
-        <v>1038.05</v>
+        <v>1076.5</v>
       </c>
       <c r="C25" s="12">
         <f t="shared" si="2"/>
-        <v>162.04999999999995</v>
+        <v>200.5</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="46" t="s">
@@ -14937,7 +14986,9 @@
       <c r="CW25" s="5">
         <v>1038.05</v>
       </c>
-      <c r="CX25" s="5"/>
+      <c r="CX25" s="5">
+        <v>1076.5</v>
+      </c>
       <c r="CY25" s="5"/>
       <c r="CZ25" s="5"/>
       <c r="DA25" s="5"/>
@@ -15203,7 +15254,9 @@
       <c r="CW26" s="5">
         <v>110.4</v>
       </c>
-      <c r="CX26" s="5"/>
+      <c r="CX26" s="5">
+        <v>111.4</v>
+      </c>
       <c r="CY26" s="5"/>
       <c r="CZ26" s="5"/>
       <c r="DA26" s="5"/>
@@ -15469,7 +15522,9 @@
       <c r="CW27" s="5">
         <v>41.85</v>
       </c>
-      <c r="CX27" s="5"/>
+      <c r="CX27" s="5">
+        <v>43.7</v>
+      </c>
       <c r="CY27" s="5"/>
       <c r="CZ27" s="5"/>
       <c r="DA27" s="5"/>
@@ -15481,11 +15536,11 @@
       </c>
       <c r="B28" s="12">
         <f t="shared" si="1"/>
-        <v>141.65</v>
+        <v>147.05000000000001</v>
       </c>
       <c r="C28" s="12">
         <f t="shared" si="2"/>
-        <v>29.700000000000003</v>
+        <v>35.100000000000009</v>
       </c>
       <c r="D28" s="12">
         <v>136</v>
@@ -15737,7 +15792,9 @@
       <c r="CW28" s="5">
         <v>140.25</v>
       </c>
-      <c r="CX28" s="5"/>
+      <c r="CX28" s="5">
+        <v>147.05000000000001</v>
+      </c>
       <c r="CY28" s="5"/>
       <c r="CZ28" s="5"/>
       <c r="DA28" s="5"/>
@@ -16005,7 +16062,9 @@
       <c r="CW29" s="5">
         <v>72.3</v>
       </c>
-      <c r="CX29" s="5"/>
+      <c r="CX29" s="5">
+        <v>78.150000000000006</v>
+      </c>
       <c r="CY29" s="5"/>
       <c r="CZ29" s="5"/>
       <c r="DA29" s="5"/>
@@ -16271,7 +16330,9 @@
       <c r="CW30" s="5">
         <v>44.4</v>
       </c>
-      <c r="CX30" s="5"/>
+      <c r="CX30" s="5">
+        <v>48.75</v>
+      </c>
       <c r="CY30" s="5"/>
       <c r="CZ30" s="5"/>
       <c r="DA30" s="5"/>
@@ -16537,7 +16598,9 @@
       <c r="CW31" s="5">
         <v>163.65</v>
       </c>
-      <c r="CX31" s="5"/>
+      <c r="CX31" s="5">
+        <v>149</v>
+      </c>
       <c r="CY31" s="5"/>
       <c r="CZ31" s="5"/>
       <c r="DA31" s="5"/>
@@ -16793,7 +16856,9 @@
       <c r="CW32" s="5">
         <v>105.7</v>
       </c>
-      <c r="CX32" s="5"/>
+      <c r="CX32" s="5">
+        <v>108.2</v>
+      </c>
       <c r="CY32" s="5"/>
       <c r="CZ32" s="5"/>
       <c r="DA32" s="5"/>
@@ -17035,7 +17100,9 @@
       <c r="CW33" s="5">
         <v>74.150000000000006</v>
       </c>
-      <c r="CX33" s="5"/>
+      <c r="CX33" s="5">
+        <v>73.95</v>
+      </c>
       <c r="CY33" s="5"/>
       <c r="CZ33" s="5"/>
       <c r="DA33" s="5"/>
@@ -17271,7 +17338,9 @@
       <c r="CW34" s="5">
         <v>298.8</v>
       </c>
-      <c r="CX34" s="5"/>
+      <c r="CX34" s="5">
+        <v>284.5</v>
+      </c>
       <c r="CY34" s="5"/>
       <c r="CZ34" s="5"/>
       <c r="DA34" s="5"/>
@@ -17485,7 +17554,9 @@
       <c r="CW35" s="5">
         <v>433</v>
       </c>
-      <c r="CX35" s="5"/>
+      <c r="CX35" s="5">
+        <v>428</v>
+      </c>
       <c r="CY35" s="5"/>
       <c r="CZ35" s="5"/>
       <c r="DA35" s="5"/>
@@ -17689,7 +17760,9 @@
       <c r="CW36" s="5">
         <v>465.8</v>
       </c>
-      <c r="CX36" s="5"/>
+      <c r="CX36" s="5">
+        <v>448.25</v>
+      </c>
       <c r="CY36" s="5"/>
       <c r="CZ36" s="5"/>
       <c r="DA36" s="5"/>
@@ -17885,7 +17958,9 @@
       <c r="CW37" s="5">
         <v>85.5</v>
       </c>
-      <c r="CX37" s="5"/>
+      <c r="CX37" s="5">
+        <v>83.65</v>
+      </c>
       <c r="CY37" s="5"/>
       <c r="CZ37" s="5"/>
       <c r="DA37" s="5"/>
@@ -18083,7 +18158,9 @@
       <c r="CW38" s="5">
         <v>427.85</v>
       </c>
-      <c r="CX38" s="5"/>
+      <c r="CX38" s="5">
+        <v>440</v>
+      </c>
       <c r="CY38" s="5"/>
       <c r="CZ38" s="5"/>
       <c r="DA38" s="5"/>
@@ -18275,7 +18352,9 @@
       <c r="CW39" s="5">
         <v>212.25</v>
       </c>
-      <c r="CX39" s="5"/>
+      <c r="CX39" s="5">
+        <v>218.25</v>
+      </c>
       <c r="CY39" s="5"/>
       <c r="CZ39" s="5"/>
       <c r="DA39" s="5"/>
@@ -18463,7 +18542,9 @@
       <c r="CW40" s="5">
         <v>43</v>
       </c>
-      <c r="CX40" s="5"/>
+      <c r="CX40" s="5">
+        <v>41.95</v>
+      </c>
       <c r="CY40" s="5"/>
       <c r="CZ40" s="5"/>
       <c r="DA40" s="5"/>
@@ -18649,7 +18730,9 @@
       <c r="CW41" s="5">
         <v>866.3</v>
       </c>
-      <c r="CX41" s="5"/>
+      <c r="CX41" s="5">
+        <v>843</v>
+      </c>
       <c r="CY41" s="5"/>
       <c r="CZ41" s="5"/>
       <c r="DA41" s="5"/>
@@ -18661,11 +18744,11 @@
       </c>
       <c r="B42" s="12">
         <f t="shared" si="1"/>
-        <v>922.55</v>
+        <v>928.7</v>
       </c>
       <c r="C42" s="12">
         <f t="shared" si="2"/>
-        <v>111.94999999999993</v>
+        <v>118.10000000000002</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="45" t="s">
@@ -18835,7 +18918,9 @@
       <c r="CW42" s="5">
         <v>922.55</v>
       </c>
-      <c r="CX42" s="5"/>
+      <c r="CX42" s="5">
+        <v>928.7</v>
+      </c>
       <c r="CY42" s="5"/>
       <c r="CZ42" s="5"/>
       <c r="DA42" s="5"/>
@@ -18847,11 +18932,11 @@
       </c>
       <c r="B43" s="12">
         <f t="shared" si="1"/>
-        <v>154.25</v>
+        <v>158.69999999999999</v>
       </c>
       <c r="C43" s="12">
         <f t="shared" si="2"/>
-        <v>20.25</v>
+        <v>24.699999999999989</v>
       </c>
       <c r="D43" s="12">
         <v>153</v>
@@ -19021,7 +19106,9 @@
       <c r="CW43" s="5">
         <v>153.65</v>
       </c>
-      <c r="CX43" s="5"/>
+      <c r="CX43" s="5">
+        <v>158.69999999999999</v>
+      </c>
       <c r="CY43" s="5"/>
       <c r="CZ43" s="5"/>
       <c r="DA43" s="5"/>
@@ -19201,7 +19288,9 @@
       <c r="CW44" s="5">
         <v>626.25</v>
       </c>
-      <c r="CX44" s="5"/>
+      <c r="CX44" s="5">
+        <v>628.70000000000005</v>
+      </c>
       <c r="CY44" s="5"/>
       <c r="CZ44" s="5"/>
       <c r="DA44" s="5"/>
@@ -19371,7 +19460,9 @@
       <c r="CW45" s="5">
         <v>120.35</v>
       </c>
-      <c r="CX45" s="5"/>
+      <c r="CX45" s="5">
+        <v>120.5</v>
+      </c>
       <c r="CY45" s="5"/>
       <c r="CZ45" s="5"/>
       <c r="DA45" s="5"/>
@@ -19383,11 +19474,11 @@
       </c>
       <c r="B46" s="12">
         <f t="shared" si="1"/>
-        <v>145</v>
+        <v>146.55000000000001</v>
       </c>
       <c r="C46" s="12">
         <f t="shared" si="2"/>
-        <v>12.800000000000011</v>
+        <v>14.350000000000023</v>
       </c>
       <c r="D46" s="12">
         <v>145</v>
@@ -19529,7 +19620,9 @@
       <c r="CW46" s="5">
         <v>137.15</v>
       </c>
-      <c r="CX46" s="5"/>
+      <c r="CX46" s="5">
+        <v>146.55000000000001</v>
+      </c>
       <c r="CY46" s="5"/>
       <c r="CZ46" s="5"/>
       <c r="DA46" s="5"/>
@@ -19667,7 +19760,9 @@
       <c r="CW47" s="5">
         <v>95.9</v>
       </c>
-      <c r="CX47" s="5"/>
+      <c r="CX47" s="5">
+        <v>96.35</v>
+      </c>
       <c r="CY47" s="5"/>
       <c r="CZ47" s="5"/>
       <c r="DA47" s="5"/>
@@ -19795,7 +19890,9 @@
       <c r="CW48" s="5">
         <v>108</v>
       </c>
-      <c r="CX48" s="5"/>
+      <c r="CX48" s="5">
+        <v>103.5</v>
+      </c>
       <c r="CY48" s="5"/>
       <c r="CZ48" s="5"/>
       <c r="DA48" s="5"/>

</xml_diff>

<commit_message>
Updated pom.xml and home.xls
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="344">
   <si>
     <t>Date</t>
   </si>
@@ -1054,6 +1054,9 @@
   </si>
   <si>
     <t>Tendulkar@123</t>
+  </si>
+  <si>
+    <t>21/1/2018</t>
   </si>
 </sst>
 </file>
@@ -7308,8 +7311,8 @@
   <dimension ref="A1:DA48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="CO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CX1" sqref="CX1"/>
+      <pane xSplit="5" topLeftCell="CQ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7370,6 +7373,7 @@
     <col min="95" max="96" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="97" max="101" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="12" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:105" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7679,7 +7683,9 @@
       <c r="CX1" s="11">
         <v>43405</v>
       </c>
-      <c r="CY1" s="27"/>
+      <c r="CY1" s="49" t="s">
+        <v>343</v>
+      </c>
       <c r="CZ1" s="27"/>
       <c r="DA1" s="27"/>
     </row>
@@ -7983,7 +7989,9 @@
       <c r="CX2" s="5">
         <v>302.14999999999998</v>
       </c>
-      <c r="CY2" s="5"/>
+      <c r="CY2" s="5">
+        <v>302.10000000000002</v>
+      </c>
       <c r="CZ2" s="5"/>
       <c r="DA2" s="5"/>
     </row>
@@ -8287,7 +8295,9 @@
       <c r="CX3" s="5">
         <v>308.85000000000002</v>
       </c>
-      <c r="CY3" s="5"/>
+      <c r="CY3" s="5">
+        <v>314.55</v>
+      </c>
       <c r="CZ3" s="5"/>
       <c r="DA3" s="5"/>
     </row>
@@ -8599,7 +8609,9 @@
       <c r="CX4" s="5">
         <v>269.95</v>
       </c>
-      <c r="CY4" s="5"/>
+      <c r="CY4" s="5">
+        <v>267.05</v>
+      </c>
       <c r="CZ4" s="5"/>
       <c r="DA4" s="5"/>
     </row>
@@ -8909,7 +8921,9 @@
       <c r="CX5" s="5">
         <v>936.9</v>
       </c>
-      <c r="CY5" s="5"/>
+      <c r="CY5" s="5">
+        <v>946.85</v>
+      </c>
       <c r="CZ5" s="5"/>
       <c r="DA5" s="5"/>
     </row>
@@ -8920,11 +8934,11 @@
       </c>
       <c r="B6" s="12">
         <f t="shared" si="1"/>
-        <v>308.14999999999998</v>
+        <v>308.8</v>
       </c>
       <c r="C6" s="12">
         <f t="shared" si="2"/>
-        <v>71.699999999999989</v>
+        <v>72.350000000000023</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="45" t="s">
@@ -9219,7 +9233,9 @@
       <c r="CX6" s="5">
         <v>308.14999999999998</v>
       </c>
-      <c r="CY6" s="5"/>
+      <c r="CY6" s="5">
+        <v>308.8</v>
+      </c>
       <c r="CZ6" s="5"/>
       <c r="DA6" s="5"/>
     </row>
@@ -9529,7 +9545,9 @@
       <c r="CX7" s="5">
         <v>21.65</v>
       </c>
-      <c r="CY7" s="5"/>
+      <c r="CY7" s="5">
+        <v>21.2</v>
+      </c>
       <c r="CZ7" s="5"/>
       <c r="DA7" s="5"/>
     </row>
@@ -9839,7 +9857,9 @@
       <c r="CX8" s="5">
         <v>98.4</v>
       </c>
-      <c r="CY8" s="5"/>
+      <c r="CY8" s="5">
+        <v>98.5</v>
+      </c>
       <c r="CZ8" s="5"/>
       <c r="DA8" s="5"/>
     </row>
@@ -10141,7 +10161,9 @@
       <c r="CX9" s="28">
         <v>68.25</v>
       </c>
-      <c r="CY9" s="28"/>
+      <c r="CY9" s="28">
+        <v>67.3</v>
+      </c>
       <c r="CZ9" s="28"/>
       <c r="DA9" s="28"/>
     </row>
@@ -10451,7 +10473,9 @@
       <c r="CX10" s="5">
         <v>55.55</v>
       </c>
-      <c r="CY10" s="5"/>
+      <c r="CY10" s="5">
+        <v>55.05</v>
+      </c>
       <c r="CZ10" s="5"/>
       <c r="DA10" s="5"/>
     </row>
@@ -10761,7 +10785,9 @@
       <c r="CX11" s="5">
         <v>107.15</v>
       </c>
-      <c r="CY11" s="5"/>
+      <c r="CY11" s="5">
+        <v>104.3</v>
+      </c>
       <c r="CZ11" s="5"/>
       <c r="DA11" s="5"/>
     </row>
@@ -11071,7 +11097,9 @@
       <c r="CX12" s="5">
         <v>103.55</v>
       </c>
-      <c r="CY12" s="5"/>
+      <c r="CY12" s="5">
+        <v>102.9</v>
+      </c>
       <c r="CZ12" s="5"/>
       <c r="DA12" s="5"/>
     </row>
@@ -11082,11 +11110,11 @@
       </c>
       <c r="B13" s="12">
         <f t="shared" si="1"/>
-        <v>60.8</v>
+        <v>61.4</v>
       </c>
       <c r="C13" s="12">
         <f t="shared" si="2"/>
-        <v>16.699999999999996</v>
+        <v>17.299999999999997</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="45" t="s">
@@ -11381,7 +11409,9 @@
       <c r="CX13" s="5">
         <v>60</v>
       </c>
-      <c r="CY13" s="5"/>
+      <c r="CY13" s="5">
+        <v>61.4</v>
+      </c>
       <c r="CZ13" s="5"/>
       <c r="DA13" s="5"/>
     </row>
@@ -11691,7 +11721,9 @@
       <c r="CX14" s="5">
         <v>40.35</v>
       </c>
-      <c r="CY14" s="5"/>
+      <c r="CY14" s="5">
+        <v>40.450000000000003</v>
+      </c>
       <c r="CZ14" s="5"/>
       <c r="DA14" s="5"/>
     </row>
@@ -11993,7 +12025,9 @@
       <c r="CX15" s="5">
         <v>27.5</v>
       </c>
-      <c r="CY15" s="5"/>
+      <c r="CY15" s="5">
+        <v>26.85</v>
+      </c>
       <c r="CZ15" s="5"/>
       <c r="DA15" s="5"/>
     </row>
@@ -12303,7 +12337,9 @@
       <c r="CX16" s="5">
         <v>769</v>
       </c>
-      <c r="CY16" s="5"/>
+      <c r="CY16" s="5">
+        <v>767.45</v>
+      </c>
       <c r="CZ16" s="5"/>
       <c r="DA16" s="5"/>
     </row>
@@ -12320,7 +12356,9 @@
         <f t="shared" si="2"/>
         <v>237</v>
       </c>
-      <c r="D17" s="12"/>
+      <c r="D17" s="12">
+        <v>670</v>
+      </c>
       <c r="E17" s="44" t="s">
         <v>26</v>
       </c>
@@ -12613,7 +12651,9 @@
       <c r="CX17" s="5">
         <v>529.4</v>
       </c>
-      <c r="CY17" s="5"/>
+      <c r="CY17" s="5">
+        <v>521.5</v>
+      </c>
       <c r="CZ17" s="5"/>
       <c r="DA17" s="5"/>
     </row>
@@ -12923,7 +12963,9 @@
       <c r="CX18" s="5">
         <v>272.10000000000002</v>
       </c>
-      <c r="CY18" s="5"/>
+      <c r="CY18" s="5">
+        <v>276.60000000000002</v>
+      </c>
       <c r="CZ18" s="5"/>
       <c r="DA18" s="5"/>
     </row>
@@ -13233,7 +13275,9 @@
       <c r="CX19" s="5">
         <v>448</v>
       </c>
-      <c r="CY19" s="5"/>
+      <c r="CY19" s="5">
+        <v>446.6</v>
+      </c>
       <c r="CZ19" s="5"/>
       <c r="DA19" s="5"/>
     </row>
@@ -13543,7 +13587,9 @@
       <c r="CX20" s="5">
         <v>674.9</v>
       </c>
-      <c r="CY20" s="5"/>
+      <c r="CY20" s="5">
+        <v>669.9</v>
+      </c>
       <c r="CZ20" s="5"/>
       <c r="DA20" s="5"/>
     </row>
@@ -13853,7 +13899,9 @@
       <c r="CX21" s="5">
         <v>515.9</v>
       </c>
-      <c r="CY21" s="5"/>
+      <c r="CY21" s="5">
+        <v>507.7</v>
+      </c>
       <c r="CZ21" s="5"/>
       <c r="DA21" s="5"/>
     </row>
@@ -14109,7 +14157,9 @@
       <c r="CX22" s="5">
         <v>414.65</v>
       </c>
-      <c r="CY22" s="5"/>
+      <c r="CY22" s="5">
+        <v>410.8</v>
+      </c>
       <c r="CZ22" s="5"/>
       <c r="DA22" s="5"/>
     </row>
@@ -14126,7 +14176,9 @@
         <f t="shared" si="2"/>
         <v>34.800000000000004</v>
       </c>
-      <c r="D23" s="12"/>
+      <c r="D23" s="12">
+        <v>66</v>
+      </c>
       <c r="E23" s="45" t="s">
         <v>127</v>
       </c>
@@ -14411,7 +14463,9 @@
       <c r="CX23" s="5">
         <v>64.5</v>
       </c>
-      <c r="CY23" s="5"/>
+      <c r="CY23" s="5">
+        <v>63.7</v>
+      </c>
       <c r="CZ23" s="5"/>
       <c r="DA23" s="5"/>
     </row>
@@ -14709,7 +14763,9 @@
       <c r="CX24" s="5">
         <v>254.1</v>
       </c>
-      <c r="CY24" s="5"/>
+      <c r="CY24" s="5">
+        <v>252</v>
+      </c>
       <c r="CZ24" s="5"/>
       <c r="DA24" s="5"/>
     </row>
@@ -14720,11 +14776,11 @@
       </c>
       <c r="B25" s="12">
         <f t="shared" si="1"/>
-        <v>1076.5</v>
+        <v>1079.3499999999999</v>
       </c>
       <c r="C25" s="12">
         <f t="shared" si="2"/>
-        <v>200.5</v>
+        <v>203.34999999999991</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="46" t="s">
@@ -14989,7 +15045,9 @@
       <c r="CX25" s="5">
         <v>1076.5</v>
       </c>
-      <c r="CY25" s="5"/>
+      <c r="CY25" s="5">
+        <v>1079.3499999999999</v>
+      </c>
       <c r="CZ25" s="5"/>
       <c r="DA25" s="5"/>
     </row>
@@ -15000,11 +15058,11 @@
       </c>
       <c r="B26" s="12">
         <f t="shared" si="1"/>
-        <v>115.5</v>
+        <v>123.2</v>
       </c>
       <c r="C26" s="12">
         <f t="shared" si="2"/>
-        <v>32.400000000000006</v>
+        <v>40.100000000000009</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="45" t="s">
@@ -15257,7 +15315,9 @@
       <c r="CX26" s="5">
         <v>111.4</v>
       </c>
-      <c r="CY26" s="5"/>
+      <c r="CY26" s="5">
+        <v>123.2</v>
+      </c>
       <c r="CZ26" s="5"/>
       <c r="DA26" s="5"/>
     </row>
@@ -15268,11 +15328,11 @@
       </c>
       <c r="B27" s="12">
         <f t="shared" si="1"/>
-        <v>44.75</v>
+        <v>46.25</v>
       </c>
       <c r="C27" s="12">
         <f t="shared" si="2"/>
-        <v>8.5499999999999972</v>
+        <v>10.049999999999997</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="45" t="s">
@@ -15525,7 +15585,9 @@
       <c r="CX27" s="5">
         <v>43.7</v>
       </c>
-      <c r="CY27" s="5"/>
+      <c r="CY27" s="5">
+        <v>46.25</v>
+      </c>
       <c r="CZ27" s="5"/>
       <c r="DA27" s="5"/>
     </row>
@@ -15542,9 +15604,7 @@
         <f t="shared" si="2"/>
         <v>35.100000000000009</v>
       </c>
-      <c r="D28" s="12">
-        <v>136</v>
-      </c>
+      <c r="D28" s="12"/>
       <c r="E28" s="45" t="s">
         <v>254</v>
       </c>
@@ -15795,7 +15855,9 @@
       <c r="CX28" s="5">
         <v>147.05000000000001</v>
       </c>
-      <c r="CY28" s="5"/>
+      <c r="CY28" s="5">
+        <v>144.15</v>
+      </c>
       <c r="CZ28" s="5"/>
       <c r="DA28" s="5"/>
     </row>
@@ -15812,9 +15874,7 @@
         <f t="shared" si="2"/>
         <v>16.549999999999997</v>
       </c>
-      <c r="D29" s="12">
-        <v>73</v>
-      </c>
+      <c r="D29" s="12"/>
       <c r="E29" s="45" t="s">
         <v>255</v>
       </c>
@@ -16065,7 +16125,9 @@
       <c r="CX29" s="5">
         <v>78.150000000000006</v>
       </c>
-      <c r="CY29" s="5"/>
+      <c r="CY29" s="5">
+        <v>78.05</v>
+      </c>
       <c r="CZ29" s="5"/>
       <c r="DA29" s="5"/>
     </row>
@@ -16333,7 +16395,9 @@
       <c r="CX30" s="5">
         <v>48.75</v>
       </c>
-      <c r="CY30" s="5"/>
+      <c r="CY30" s="5">
+        <v>47.1</v>
+      </c>
       <c r="CZ30" s="5"/>
       <c r="DA30" s="5"/>
     </row>
@@ -16601,7 +16665,9 @@
       <c r="CX31" s="5">
         <v>149</v>
       </c>
-      <c r="CY31" s="5"/>
+      <c r="CY31" s="5">
+        <v>146.5</v>
+      </c>
       <c r="CZ31" s="5"/>
       <c r="DA31" s="5"/>
     </row>
@@ -16859,7 +16925,9 @@
       <c r="CX32" s="5">
         <v>108.2</v>
       </c>
-      <c r="CY32" s="5"/>
+      <c r="CY32" s="5">
+        <v>107.35</v>
+      </c>
       <c r="CZ32" s="5"/>
       <c r="DA32" s="5"/>
     </row>
@@ -17103,7 +17171,9 @@
       <c r="CX33" s="5">
         <v>73.95</v>
       </c>
-      <c r="CY33" s="5"/>
+      <c r="CY33" s="5">
+        <v>73.25</v>
+      </c>
       <c r="CZ33" s="5"/>
       <c r="DA33" s="5"/>
     </row>
@@ -17341,7 +17411,9 @@
       <c r="CX34" s="5">
         <v>284.5</v>
       </c>
-      <c r="CY34" s="5"/>
+      <c r="CY34" s="5">
+        <v>283</v>
+      </c>
       <c r="CZ34" s="5"/>
       <c r="DA34" s="5"/>
     </row>
@@ -17557,7 +17629,9 @@
       <c r="CX35" s="5">
         <v>428</v>
       </c>
-      <c r="CY35" s="5"/>
+      <c r="CY35" s="5">
+        <v>426</v>
+      </c>
       <c r="CZ35" s="5"/>
       <c r="DA35" s="5"/>
     </row>
@@ -17763,7 +17837,9 @@
       <c r="CX36" s="5">
         <v>448.25</v>
       </c>
-      <c r="CY36" s="5"/>
+      <c r="CY36" s="5">
+        <v>444.9</v>
+      </c>
       <c r="CZ36" s="5"/>
       <c r="DA36" s="5"/>
     </row>
@@ -17780,7 +17856,9 @@
         <f t="shared" si="2"/>
         <v>10.299999999999997</v>
       </c>
-      <c r="D37" s="12"/>
+      <c r="D37" s="12">
+        <v>80</v>
+      </c>
       <c r="E37" s="45" t="s">
         <v>303</v>
       </c>
@@ -17961,7 +18039,9 @@
       <c r="CX37" s="5">
         <v>83.65</v>
       </c>
-      <c r="CY37" s="5"/>
+      <c r="CY37" s="5">
+        <v>78.8</v>
+      </c>
       <c r="CZ37" s="5"/>
       <c r="DA37" s="5"/>
     </row>
@@ -18161,7 +18241,9 @@
       <c r="CX38" s="5">
         <v>440</v>
       </c>
-      <c r="CY38" s="5"/>
+      <c r="CY38" s="5">
+        <v>443.65</v>
+      </c>
       <c r="CZ38" s="5"/>
       <c r="DA38" s="5"/>
     </row>
@@ -18355,7 +18437,9 @@
       <c r="CX39" s="5">
         <v>218.25</v>
       </c>
-      <c r="CY39" s="5"/>
+      <c r="CY39" s="5">
+        <v>221.8</v>
+      </c>
       <c r="CZ39" s="5"/>
       <c r="DA39" s="5"/>
     </row>
@@ -18545,7 +18629,9 @@
       <c r="CX40" s="5">
         <v>41.95</v>
       </c>
-      <c r="CY40" s="5"/>
+      <c r="CY40" s="5">
+        <v>42.65</v>
+      </c>
       <c r="CZ40" s="5"/>
       <c r="DA40" s="5"/>
     </row>
@@ -18733,7 +18819,9 @@
       <c r="CX41" s="5">
         <v>843</v>
       </c>
-      <c r="CY41" s="5"/>
+      <c r="CY41" s="5">
+        <v>848.6</v>
+      </c>
       <c r="CZ41" s="5"/>
       <c r="DA41" s="5"/>
     </row>
@@ -18921,7 +19009,9 @@
       <c r="CX42" s="5">
         <v>928.7</v>
       </c>
-      <c r="CY42" s="5"/>
+      <c r="CY42" s="5">
+        <v>918.75</v>
+      </c>
       <c r="CZ42" s="5"/>
       <c r="DA42" s="5"/>
     </row>
@@ -18938,9 +19028,7 @@
         <f t="shared" si="2"/>
         <v>24.699999999999989</v>
       </c>
-      <c r="D43" s="12">
-        <v>153</v>
-      </c>
+      <c r="D43" s="12"/>
       <c r="E43" s="45" t="s">
         <v>309</v>
       </c>
@@ -19109,7 +19197,9 @@
       <c r="CX43" s="5">
         <v>158.69999999999999</v>
       </c>
-      <c r="CY43" s="5"/>
+      <c r="CY43" s="5">
+        <v>157.30000000000001</v>
+      </c>
       <c r="CZ43" s="5"/>
       <c r="DA43" s="5"/>
     </row>
@@ -19291,7 +19381,9 @@
       <c r="CX44" s="5">
         <v>628.70000000000005</v>
       </c>
-      <c r="CY44" s="5"/>
+      <c r="CY44" s="5">
+        <v>623.9</v>
+      </c>
       <c r="CZ44" s="5"/>
       <c r="DA44" s="5"/>
     </row>
@@ -19463,7 +19555,9 @@
       <c r="CX45" s="5">
         <v>120.5</v>
       </c>
-      <c r="CY45" s="5"/>
+      <c r="CY45" s="5">
+        <v>119.35</v>
+      </c>
       <c r="CZ45" s="5"/>
       <c r="DA45" s="5"/>
     </row>
@@ -19474,15 +19568,13 @@
       </c>
       <c r="B46" s="12">
         <f t="shared" si="1"/>
-        <v>146.55000000000001</v>
+        <v>161.85</v>
       </c>
       <c r="C46" s="12">
         <f t="shared" si="2"/>
-        <v>14.350000000000023</v>
-      </c>
-      <c r="D46" s="12">
-        <v>145</v>
-      </c>
+        <v>29.650000000000006</v>
+      </c>
+      <c r="D46" s="12"/>
       <c r="E46" s="45" t="s">
         <v>324</v>
       </c>
@@ -19623,7 +19715,9 @@
       <c r="CX46" s="5">
         <v>146.55000000000001</v>
       </c>
-      <c r="CY46" s="5"/>
+      <c r="CY46" s="5">
+        <v>161.85</v>
+      </c>
       <c r="CZ46" s="5"/>
       <c r="DA46" s="5"/>
     </row>
@@ -19763,7 +19857,9 @@
       <c r="CX47" s="5">
         <v>96.35</v>
       </c>
-      <c r="CY47" s="5"/>
+      <c r="CY47" s="5">
+        <v>95.55</v>
+      </c>
       <c r="CZ47" s="5"/>
       <c r="DA47" s="5"/>
     </row>
@@ -19893,7 +19989,9 @@
       <c r="CX48" s="5">
         <v>103.5</v>
       </c>
-      <c r="CY48" s="5"/>
+      <c r="CY48" s="5">
+        <v>102.4</v>
+      </c>
       <c r="CZ48" s="5"/>
       <c r="DA48" s="5"/>
     </row>

</xml_diff>

<commit_message>
Added stock data for 19/1/2018
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="354">
   <si>
     <t>Date</t>
   </si>
@@ -1072,6 +1072,21 @@
   </si>
   <si>
     <t>18/1/2018</t>
+  </si>
+  <si>
+    <t>19/1/2018</t>
+  </si>
+  <si>
+    <t>22/1/2018</t>
+  </si>
+  <si>
+    <t>23/1/2018</t>
+  </si>
+  <si>
+    <t>24/1/2018</t>
+  </si>
+  <si>
+    <t>25/1/2018</t>
   </si>
 </sst>
 </file>
@@ -7331,11 +7346,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DB48"/>
+  <dimension ref="A1:DG48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="DA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DB48" sqref="DB48"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="DC1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DN21" sqref="DN21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7398,10 +7413,12 @@
     <col min="102" max="102" width="12" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="104" max="104" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="105" max="106" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="105" max="107" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="13" customWidth="1"/>
+    <col min="109" max="111" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:106" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:111" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>249</v>
       </c>
@@ -7720,8 +7737,23 @@
       <c r="DB1" s="49" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="2" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC1" s="49" t="s">
+        <v>349</v>
+      </c>
+      <c r="DD1" s="49" t="s">
+        <v>350</v>
+      </c>
+      <c r="DE1" s="49" t="s">
+        <v>351</v>
+      </c>
+      <c r="DF1" s="49" t="s">
+        <v>352</v>
+      </c>
+      <c r="DG1" s="49" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="2" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <f t="shared" ref="A2:A46" si="0">MIN(F2:ZR2)</f>
         <v>243.6</v>
@@ -8033,19 +8065,26 @@
       <c r="DB2" s="5">
         <v>304.8</v>
       </c>
-    </row>
-    <row r="3" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC2" s="5">
+        <v>308.8</v>
+      </c>
+      <c r="DD2" s="5"/>
+      <c r="DE2" s="5"/>
+      <c r="DF2" s="5"/>
+      <c r="DG2" s="5"/>
+    </row>
+    <row r="3" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <f t="shared" si="0"/>
         <v>262.7</v>
       </c>
       <c r="B3" s="12">
         <f t="shared" si="1"/>
-        <v>346</v>
+        <v>354.15</v>
       </c>
       <c r="C3" s="12">
         <f t="shared" si="2"/>
-        <v>83.300000000000011</v>
+        <v>91.449999999999989</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="44" t="s">
@@ -8346,8 +8385,15 @@
       <c r="DB3" s="5">
         <v>346</v>
       </c>
-    </row>
-    <row r="4" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC3" s="5">
+        <v>354.15</v>
+      </c>
+      <c r="DD3" s="5"/>
+      <c r="DE3" s="5"/>
+      <c r="DF3" s="5"/>
+      <c r="DG3" s="5"/>
+    </row>
+    <row r="4" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <f t="shared" si="0"/>
         <v>251.25</v>
@@ -8667,8 +8713,15 @@
       <c r="DB4" s="5">
         <v>274</v>
       </c>
-    </row>
-    <row r="5" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC4" s="5">
+        <v>274</v>
+      </c>
+      <c r="DD4" s="5"/>
+      <c r="DE4" s="5"/>
+      <c r="DF4" s="5"/>
+      <c r="DG4" s="5"/>
+    </row>
+    <row r="5" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <f t="shared" si="0"/>
         <v>786.25</v>
@@ -8986,8 +9039,15 @@
       <c r="DB5" s="5">
         <v>922</v>
       </c>
-    </row>
-    <row r="6" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC5" s="5">
+        <v>934.2</v>
+      </c>
+      <c r="DD5" s="5"/>
+      <c r="DE5" s="5"/>
+      <c r="DF5" s="5"/>
+      <c r="DG5" s="5"/>
+    </row>
+    <row r="6" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <f t="shared" si="0"/>
         <v>236.45</v>
@@ -9305,8 +9365,15 @@
       <c r="DB6" s="5">
         <v>284.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC6" s="5">
+        <v>284.35000000000002</v>
+      </c>
+      <c r="DD6" s="5"/>
+      <c r="DE6" s="5"/>
+      <c r="DF6" s="5"/>
+      <c r="DG6" s="5"/>
+    </row>
+    <row r="7" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <f t="shared" si="0"/>
         <v>15.6</v>
@@ -9624,8 +9691,15 @@
       <c r="DB7" s="5">
         <v>22.65</v>
       </c>
-    </row>
-    <row r="8" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC7" s="5">
+        <v>22.6</v>
+      </c>
+      <c r="DD7" s="5"/>
+      <c r="DE7" s="5"/>
+      <c r="DF7" s="5"/>
+      <c r="DG7" s="5"/>
+    </row>
+    <row r="8" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <f t="shared" si="0"/>
         <v>53.4</v>
@@ -9943,8 +10017,15 @@
       <c r="DB8" s="5">
         <v>92.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:106" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="DC8" s="5">
+        <v>93.25</v>
+      </c>
+      <c r="DD8" s="5"/>
+      <c r="DE8" s="5"/>
+      <c r="DF8" s="5"/>
+      <c r="DG8" s="5"/>
+    </row>
+    <row r="9" spans="1:111" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <f t="shared" si="0"/>
         <v>51.55</v>
@@ -10254,8 +10335,15 @@
       <c r="DB9" s="28">
         <v>58.95</v>
       </c>
-    </row>
-    <row r="10" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC9" s="28">
+        <v>58.8</v>
+      </c>
+      <c r="DD9" s="28"/>
+      <c r="DE9" s="28"/>
+      <c r="DF9" s="28"/>
+      <c r="DG9" s="28"/>
+    </row>
+    <row r="10" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <f t="shared" si="0"/>
         <v>35.15</v>
@@ -10573,8 +10661,15 @@
       <c r="DB10" s="5">
         <v>48.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC10" s="5">
+        <v>48.75</v>
+      </c>
+      <c r="DD10" s="5"/>
+      <c r="DE10" s="5"/>
+      <c r="DF10" s="5"/>
+      <c r="DG10" s="5"/>
+    </row>
+    <row r="11" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <f t="shared" si="0"/>
         <v>72.650000000000006</v>
@@ -10892,8 +10987,15 @@
       <c r="DB11" s="5">
         <v>100.85</v>
       </c>
-    </row>
-    <row r="12" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC11" s="5">
+        <v>102</v>
+      </c>
+      <c r="DD11" s="5"/>
+      <c r="DE11" s="5"/>
+      <c r="DF11" s="5"/>
+      <c r="DG11" s="5"/>
+    </row>
+    <row r="12" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
         <v>82.65</v>
@@ -11211,8 +11313,15 @@
       <c r="DB12" s="5">
         <v>97.55</v>
       </c>
-    </row>
-    <row r="13" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC12" s="5">
+        <v>97.35</v>
+      </c>
+      <c r="DD12" s="5"/>
+      <c r="DE12" s="5"/>
+      <c r="DF12" s="5"/>
+      <c r="DG12" s="5"/>
+    </row>
+    <row r="13" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <f t="shared" si="0"/>
         <v>44.1</v>
@@ -11530,8 +11639,15 @@
       <c r="DB13" s="5">
         <v>54.85</v>
       </c>
-    </row>
-    <row r="14" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC13" s="5">
+        <v>54.6</v>
+      </c>
+      <c r="DD13" s="5"/>
+      <c r="DE13" s="5"/>
+      <c r="DF13" s="5"/>
+      <c r="DG13" s="5"/>
+    </row>
+    <row r="14" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <f t="shared" si="0"/>
         <v>29.75</v>
@@ -11849,8 +11965,15 @@
       <c r="DB14" s="5">
         <v>41.8</v>
       </c>
-    </row>
-    <row r="15" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC14" s="5">
+        <v>42.1</v>
+      </c>
+      <c r="DD14" s="5"/>
+      <c r="DE14" s="5"/>
+      <c r="DF14" s="5"/>
+      <c r="DG14" s="5"/>
+    </row>
+    <row r="15" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <f t="shared" si="0"/>
         <v>21.35</v>
@@ -12160,8 +12283,15 @@
       <c r="DB15" s="5">
         <v>23.95</v>
       </c>
-    </row>
-    <row r="16" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC15" s="5">
+        <v>24.25</v>
+      </c>
+      <c r="DD15" s="5"/>
+      <c r="DE15" s="5"/>
+      <c r="DF15" s="5"/>
+      <c r="DG15" s="5"/>
+    </row>
+    <row r="16" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <f t="shared" si="0"/>
         <v>552</v>
@@ -12479,8 +12609,15 @@
       <c r="DB16" s="5">
         <v>750.35</v>
       </c>
-    </row>
-    <row r="17" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC16" s="5">
+        <v>753</v>
+      </c>
+      <c r="DD16" s="5"/>
+      <c r="DE16" s="5"/>
+      <c r="DF16" s="5"/>
+      <c r="DG16" s="5"/>
+    </row>
+    <row r="17" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <f t="shared" si="0"/>
         <v>433</v>
@@ -12800,8 +12937,15 @@
       <c r="DB17" s="5">
         <v>490</v>
       </c>
-    </row>
-    <row r="18" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC17" s="5">
+        <v>489</v>
+      </c>
+      <c r="DD17" s="5"/>
+      <c r="DE17" s="5"/>
+      <c r="DF17" s="5"/>
+      <c r="DG17" s="5"/>
+    </row>
+    <row r="18" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <f t="shared" si="0"/>
         <v>178.8</v>
@@ -13119,8 +13263,15 @@
       <c r="DB18" s="5">
         <v>265.35000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC18" s="5">
+        <v>275.5</v>
+      </c>
+      <c r="DD18" s="5"/>
+      <c r="DE18" s="5"/>
+      <c r="DF18" s="5"/>
+      <c r="DG18" s="5"/>
+    </row>
+    <row r="19" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <f t="shared" si="0"/>
         <v>395.5</v>
@@ -13438,8 +13589,15 @@
       <c r="DB19" s="5">
         <v>436</v>
       </c>
-    </row>
-    <row r="20" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC19" s="5">
+        <v>448.95</v>
+      </c>
+      <c r="DD19" s="5"/>
+      <c r="DE19" s="5"/>
+      <c r="DF19" s="5"/>
+      <c r="DG19" s="5"/>
+    </row>
+    <row r="20" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <f t="shared" si="0"/>
         <v>642.6</v>
@@ -13757,8 +13915,15 @@
       <c r="DB20" s="5">
         <v>644.65</v>
       </c>
-    </row>
-    <row r="21" spans="1:106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="DC20" s="5">
+        <v>644.15</v>
+      </c>
+      <c r="DD20" s="5"/>
+      <c r="DE20" s="5"/>
+      <c r="DF20" s="5"/>
+      <c r="DG20" s="5"/>
+    </row>
+    <row r="21" spans="1:111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <f t="shared" si="0"/>
         <v>376.7</v>
@@ -14076,8 +14241,15 @@
       <c r="DB21" s="5">
         <v>494</v>
       </c>
-    </row>
-    <row r="22" spans="1:106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="DC21" s="5">
+        <v>498.05</v>
+      </c>
+      <c r="DD21" s="5"/>
+      <c r="DE21" s="5"/>
+      <c r="DF21" s="5"/>
+      <c r="DG21" s="5"/>
+    </row>
+    <row r="22" spans="1:111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <f t="shared" si="0"/>
         <v>315.2</v>
@@ -14341,8 +14513,15 @@
       <c r="DB22" s="5">
         <v>394.8</v>
       </c>
-    </row>
-    <row r="23" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC22" s="5">
+        <v>409.25</v>
+      </c>
+      <c r="DD22" s="5"/>
+      <c r="DE22" s="5"/>
+      <c r="DF22" s="5"/>
+      <c r="DG22" s="5"/>
+    </row>
+    <row r="23" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <f t="shared" si="0"/>
         <v>50.85</v>
@@ -14654,8 +14833,15 @@
       <c r="DB23" s="5">
         <v>61.45</v>
       </c>
-    </row>
-    <row r="24" spans="1:106" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="DC23" s="5">
+        <v>60.95</v>
+      </c>
+      <c r="DD23" s="5"/>
+      <c r="DE23" s="5"/>
+      <c r="DF23" s="5"/>
+      <c r="DG23" s="5"/>
+    </row>
+    <row r="24" spans="1:111" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <f t="shared" si="0"/>
         <v>210.65</v>
@@ -14961,8 +15147,15 @@
       <c r="DB24" s="5">
         <v>241.95</v>
       </c>
-    </row>
-    <row r="25" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC24" s="5">
+        <v>242.75</v>
+      </c>
+      <c r="DD24" s="5"/>
+      <c r="DE24" s="5"/>
+      <c r="DF24" s="5"/>
+      <c r="DG24" s="5"/>
+    </row>
+    <row r="25" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <f t="shared" si="0"/>
         <v>876</v>
@@ -15250,8 +15443,15 @@
       <c r="DB25" s="5">
         <v>1152</v>
       </c>
-    </row>
-    <row r="26" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC25" s="5">
+        <v>1145.9000000000001</v>
+      </c>
+      <c r="DD25" s="5"/>
+      <c r="DE25" s="5"/>
+      <c r="DF25" s="5"/>
+      <c r="DG25" s="5"/>
+    </row>
+    <row r="26" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <f t="shared" si="0"/>
         <v>83.1</v>
@@ -15527,8 +15727,15 @@
       <c r="DB26" s="5">
         <v>122.7</v>
       </c>
-    </row>
-    <row r="27" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC26" s="5">
+        <v>121.5</v>
+      </c>
+      <c r="DD26" s="5"/>
+      <c r="DE26" s="5"/>
+      <c r="DF26" s="5"/>
+      <c r="DG26" s="5"/>
+    </row>
+    <row r="27" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <f t="shared" si="0"/>
         <v>36.200000000000003</v>
@@ -15804,8 +16011,15 @@
       <c r="DB27" s="5">
         <v>44.55</v>
       </c>
-    </row>
-    <row r="28" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC27" s="5">
+        <v>44.6</v>
+      </c>
+      <c r="DD27" s="5"/>
+      <c r="DE27" s="5"/>
+      <c r="DF27" s="5"/>
+      <c r="DG27" s="5"/>
+    </row>
+    <row r="28" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <f t="shared" si="0"/>
         <v>111.95</v>
@@ -16081,8 +16295,15 @@
       <c r="DB28" s="5">
         <v>135.69999999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC28" s="5">
+        <v>135.69999999999999</v>
+      </c>
+      <c r="DD28" s="5"/>
+      <c r="DE28" s="5"/>
+      <c r="DF28" s="5"/>
+      <c r="DG28" s="5"/>
+    </row>
+    <row r="29" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <f t="shared" si="0"/>
         <v>62.3</v>
@@ -16358,8 +16579,15 @@
       <c r="DB29" s="5">
         <v>72.55</v>
       </c>
-    </row>
-    <row r="30" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC29" s="5">
+        <v>73.150000000000006</v>
+      </c>
+      <c r="DD29" s="5"/>
+      <c r="DE29" s="5"/>
+      <c r="DF29" s="5"/>
+      <c r="DG29" s="5"/>
+    </row>
+    <row r="30" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <f t="shared" si="0"/>
         <v>34.450000000000003</v>
@@ -16635,8 +16863,15 @@
       <c r="DB30" s="5">
         <v>43.9</v>
       </c>
-    </row>
-    <row r="31" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC30" s="5">
+        <v>44.5</v>
+      </c>
+      <c r="DD30" s="5"/>
+      <c r="DE30" s="5"/>
+      <c r="DF30" s="5"/>
+      <c r="DG30" s="5"/>
+    </row>
+    <row r="31" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <f t="shared" si="0"/>
         <v>125.3</v>
@@ -16912,8 +17147,15 @@
       <c r="DB31" s="5">
         <v>145.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC31" s="5">
+        <v>145.30000000000001</v>
+      </c>
+      <c r="DD31" s="5"/>
+      <c r="DE31" s="5"/>
+      <c r="DF31" s="5"/>
+      <c r="DG31" s="5"/>
+    </row>
+    <row r="32" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <f t="shared" si="0"/>
         <v>94.7</v>
@@ -17179,8 +17421,15 @@
       <c r="DB32" s="5">
         <v>99.6</v>
       </c>
-    </row>
-    <row r="33" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC32" s="5">
+        <v>100.15</v>
+      </c>
+      <c r="DD32" s="5"/>
+      <c r="DE32" s="5"/>
+      <c r="DF32" s="5"/>
+      <c r="DG32" s="5"/>
+    </row>
+    <row r="33" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <f t="shared" si="0"/>
         <v>56.75</v>
@@ -17432,8 +17681,15 @@
       <c r="DB33" s="5">
         <v>67.3</v>
       </c>
-    </row>
-    <row r="34" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC33" s="5">
+        <v>68.2</v>
+      </c>
+      <c r="DD33" s="5"/>
+      <c r="DE33" s="5"/>
+      <c r="DF33" s="5"/>
+      <c r="DG33" s="5"/>
+    </row>
+    <row r="34" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <f t="shared" si="0"/>
         <v>167.9</v>
@@ -17679,8 +17935,15 @@
       <c r="DB34" s="5">
         <v>249</v>
       </c>
-    </row>
-    <row r="35" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC34" s="5">
+        <v>256.8</v>
+      </c>
+      <c r="DD34" s="5"/>
+      <c r="DE34" s="5"/>
+      <c r="DF34" s="5"/>
+      <c r="DG34" s="5"/>
+    </row>
+    <row r="35" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <f t="shared" si="0"/>
         <v>388</v>
@@ -17904,8 +18167,15 @@
       <c r="DB35" s="5">
         <v>405.65</v>
       </c>
-    </row>
-    <row r="36" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC35" s="5">
+        <v>400</v>
+      </c>
+      <c r="DD35" s="5"/>
+      <c r="DE35" s="5"/>
+      <c r="DF35" s="5"/>
+      <c r="DG35" s="5"/>
+    </row>
+    <row r="36" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <f t="shared" si="0"/>
         <v>226</v>
@@ -18119,8 +18389,15 @@
       <c r="DB36" s="5">
         <v>419.25</v>
       </c>
-    </row>
-    <row r="37" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC36" s="5">
+        <v>431.95</v>
+      </c>
+      <c r="DD36" s="5"/>
+      <c r="DE36" s="5"/>
+      <c r="DF36" s="5"/>
+      <c r="DG36" s="5"/>
+    </row>
+    <row r="37" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <f t="shared" si="0"/>
         <v>72.2</v>
@@ -18328,8 +18605,15 @@
       <c r="DB37" s="5">
         <v>72.599999999999994</v>
       </c>
-    </row>
-    <row r="38" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC37" s="5">
+        <v>72.650000000000006</v>
+      </c>
+      <c r="DD37" s="5"/>
+      <c r="DE37" s="5"/>
+      <c r="DF37" s="5"/>
+      <c r="DG37" s="5"/>
+    </row>
+    <row r="38" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <f t="shared" si="0"/>
         <v>407.05</v>
@@ -18537,8 +18821,15 @@
       <c r="DB38" s="5">
         <v>437.6</v>
       </c>
-    </row>
-    <row r="39" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC38" s="5">
+        <v>451</v>
+      </c>
+      <c r="DD38" s="5"/>
+      <c r="DE38" s="5"/>
+      <c r="DF38" s="5"/>
+      <c r="DG38" s="5"/>
+    </row>
+    <row r="39" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <f t="shared" si="0"/>
         <v>175.2</v>
@@ -18740,8 +19031,15 @@
       <c r="DB39" s="5">
         <v>226</v>
       </c>
-    </row>
-    <row r="40" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC39" s="5">
+        <v>228.1</v>
+      </c>
+      <c r="DD39" s="5"/>
+      <c r="DE39" s="5"/>
+      <c r="DF39" s="5"/>
+      <c r="DG39" s="5"/>
+    </row>
+    <row r="40" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <f t="shared" si="0"/>
         <v>34.5</v>
@@ -18939,8 +19237,15 @@
       <c r="DB40" s="5">
         <v>36.6</v>
       </c>
-    </row>
-    <row r="41" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC40" s="5">
+        <v>37</v>
+      </c>
+      <c r="DD40" s="5"/>
+      <c r="DE40" s="5"/>
+      <c r="DF40" s="5"/>
+      <c r="DG40" s="5"/>
+    </row>
+    <row r="41" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <f t="shared" si="0"/>
         <v>552.04999999999995</v>
@@ -19136,8 +19441,15 @@
       <c r="DB41" s="5">
         <v>754</v>
       </c>
-    </row>
-    <row r="42" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC41" s="5">
+        <v>779.2</v>
+      </c>
+      <c r="DD41" s="5"/>
+      <c r="DE41" s="5"/>
+      <c r="DF41" s="5"/>
+      <c r="DG41" s="5"/>
+    </row>
+    <row r="42" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <f t="shared" si="0"/>
         <v>810.6</v>
@@ -19333,8 +19645,15 @@
       <c r="DB42" s="5">
         <v>921</v>
       </c>
-    </row>
-    <row r="43" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC42" s="5">
+        <v>923</v>
+      </c>
+      <c r="DD42" s="5"/>
+      <c r="DE42" s="5"/>
+      <c r="DF42" s="5"/>
+      <c r="DG42" s="5"/>
+    </row>
+    <row r="43" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <f t="shared" si="0"/>
         <v>134</v>
@@ -19528,8 +19847,15 @@
       <c r="DB43" s="5">
         <v>150</v>
       </c>
-    </row>
-    <row r="44" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC43" s="5">
+        <v>152.55000000000001</v>
+      </c>
+      <c r="DD43" s="5"/>
+      <c r="DE43" s="5"/>
+      <c r="DF43" s="5"/>
+      <c r="DG43" s="5"/>
+    </row>
+    <row r="44" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <f t="shared" si="0"/>
         <v>538.4</v>
@@ -19719,8 +20045,15 @@
       <c r="DB44" s="5">
         <v>608.9</v>
       </c>
-    </row>
-    <row r="45" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC44" s="5">
+        <v>607.9</v>
+      </c>
+      <c r="DD44" s="5"/>
+      <c r="DE44" s="5"/>
+      <c r="DF44" s="5"/>
+      <c r="DG44" s="5"/>
+    </row>
+    <row r="45" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <f t="shared" si="0"/>
         <v>101.4</v>
@@ -19900,8 +20233,15 @@
       <c r="DB45" s="5">
         <v>106.05</v>
       </c>
-    </row>
-    <row r="46" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC45" s="5">
+        <v>109.85</v>
+      </c>
+      <c r="DD45" s="5"/>
+      <c r="DE45" s="5"/>
+      <c r="DF45" s="5"/>
+      <c r="DG45" s="5"/>
+    </row>
+    <row r="46" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <f t="shared" si="0"/>
         <v>132.19999999999999</v>
@@ -20067,11 +20407,18 @@
       <c r="DB46" s="5">
         <v>152.4</v>
       </c>
-    </row>
-    <row r="47" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC46" s="5">
+        <v>153.5</v>
+      </c>
+      <c r="DD46" s="5"/>
+      <c r="DE46" s="5"/>
+      <c r="DF46" s="5"/>
+      <c r="DG46" s="5"/>
+    </row>
+    <row r="47" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <f t="shared" ref="A47" si="3">MIN(F47:ZR47)</f>
-        <v>90.7</v>
+        <v>89</v>
       </c>
       <c r="B47" s="12">
         <f t="shared" ref="B47" si="4">MAX(F47:ZR47)</f>
@@ -20079,7 +20426,7 @@
       </c>
       <c r="C47" s="12">
         <f t="shared" si="2"/>
-        <v>6.0999999999999943</v>
+        <v>7.7999999999999972</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="45" t="s">
@@ -20216,8 +20563,15 @@
       <c r="DB47" s="5">
         <v>90.7</v>
       </c>
-    </row>
-    <row r="48" spans="1:106" x14ac:dyDescent="0.25">
+      <c r="DC47" s="5">
+        <v>89</v>
+      </c>
+      <c r="DD47" s="5"/>
+      <c r="DE47" s="5"/>
+      <c r="DF47" s="5"/>
+      <c r="DG47" s="5"/>
+    </row>
+    <row r="48" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <f t="shared" ref="A48" si="5">MIN(F48:ZR48)</f>
         <v>90.9</v>
@@ -20355,6 +20709,13 @@
       <c r="DB48" s="5">
         <v>90.9</v>
       </c>
+      <c r="DC48" s="5">
+        <v>92.95</v>
+      </c>
+      <c r="DD48" s="5"/>
+      <c r="DE48" s="5"/>
+      <c r="DF48" s="5"/>
+      <c r="DG48" s="5"/>
     </row>
   </sheetData>
   <sortState ref="M1:M37">

</xml_diff>

<commit_message>
Added Apache MQ implementation
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -7350,7 +7350,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="5" topLeftCell="DC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DN21" sqref="DN21"/>
+      <selection pane="topRight" activeCell="DD2" sqref="DD2:DD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8068,7 +8068,9 @@
       <c r="DC2" s="5">
         <v>308.8</v>
       </c>
-      <c r="DD2" s="5"/>
+      <c r="DD2" s="5">
+        <v>306.3</v>
+      </c>
       <c r="DE2" s="5"/>
       <c r="DF2" s="5"/>
       <c r="DG2" s="5"/>
@@ -8388,7 +8390,9 @@
       <c r="DC3" s="5">
         <v>354.15</v>
       </c>
-      <c r="DD3" s="5"/>
+      <c r="DD3" s="5">
+        <v>350.25</v>
+      </c>
       <c r="DE3" s="5"/>
       <c r="DF3" s="5"/>
       <c r="DG3" s="5"/>
@@ -8716,7 +8720,9 @@
       <c r="DC4" s="5">
         <v>274</v>
       </c>
-      <c r="DD4" s="5"/>
+      <c r="DD4" s="5">
+        <v>272.7</v>
+      </c>
       <c r="DE4" s="5"/>
       <c r="DF4" s="5"/>
       <c r="DG4" s="5"/>
@@ -8728,11 +8734,11 @@
       </c>
       <c r="B5" s="12">
         <f t="shared" si="1"/>
-        <v>951.25</v>
+        <v>970.2</v>
       </c>
       <c r="C5" s="12">
         <f t="shared" si="2"/>
-        <v>165</v>
+        <v>183.95000000000005</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="44" t="s">
@@ -9042,7 +9048,9 @@
       <c r="DC5" s="5">
         <v>934.2</v>
       </c>
-      <c r="DD5" s="5"/>
+      <c r="DD5" s="5">
+        <v>970.2</v>
+      </c>
       <c r="DE5" s="5"/>
       <c r="DF5" s="5"/>
       <c r="DG5" s="5"/>
@@ -9368,7 +9376,9 @@
       <c r="DC6" s="5">
         <v>284.35000000000002</v>
       </c>
-      <c r="DD6" s="5"/>
+      <c r="DD6" s="5">
+        <v>285</v>
+      </c>
       <c r="DE6" s="5"/>
       <c r="DF6" s="5"/>
       <c r="DG6" s="5"/>
@@ -9694,7 +9704,9 @@
       <c r="DC7" s="5">
         <v>22.6</v>
       </c>
-      <c r="DD7" s="5"/>
+      <c r="DD7" s="5">
+        <v>22.9</v>
+      </c>
       <c r="DE7" s="5"/>
       <c r="DF7" s="5"/>
       <c r="DG7" s="5"/>
@@ -10020,7 +10032,9 @@
       <c r="DC8" s="5">
         <v>93.25</v>
       </c>
-      <c r="DD8" s="5"/>
+      <c r="DD8" s="5">
+        <v>93</v>
+      </c>
       <c r="DE8" s="5"/>
       <c r="DF8" s="5"/>
       <c r="DG8" s="5"/>
@@ -10338,7 +10352,9 @@
       <c r="DC9" s="28">
         <v>58.8</v>
       </c>
-      <c r="DD9" s="28"/>
+      <c r="DD9" s="28">
+        <v>59.35</v>
+      </c>
       <c r="DE9" s="28"/>
       <c r="DF9" s="28"/>
       <c r="DG9" s="28"/>
@@ -10664,7 +10680,9 @@
       <c r="DC10" s="5">
         <v>48.75</v>
       </c>
-      <c r="DD10" s="5"/>
+      <c r="DD10" s="5">
+        <v>47.7</v>
+      </c>
       <c r="DE10" s="5"/>
       <c r="DF10" s="5"/>
       <c r="DG10" s="5"/>
@@ -10990,7 +11008,9 @@
       <c r="DC11" s="5">
         <v>102</v>
       </c>
-      <c r="DD11" s="5"/>
+      <c r="DD11" s="5">
+        <v>99.45</v>
+      </c>
       <c r="DE11" s="5"/>
       <c r="DF11" s="5"/>
       <c r="DG11" s="5"/>
@@ -11002,11 +11022,11 @@
       </c>
       <c r="B12" s="12">
         <f t="shared" si="1"/>
-        <v>103.55</v>
+        <v>105.1</v>
       </c>
       <c r="C12" s="12">
         <f t="shared" si="2"/>
-        <v>20.899999999999991</v>
+        <v>22.449999999999989</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="45" t="s">
@@ -11316,7 +11336,9 @@
       <c r="DC12" s="5">
         <v>97.35</v>
       </c>
-      <c r="DD12" s="5"/>
+      <c r="DD12" s="5">
+        <v>105.1</v>
+      </c>
       <c r="DE12" s="5"/>
       <c r="DF12" s="5"/>
       <c r="DG12" s="5"/>
@@ -11642,7 +11664,9 @@
       <c r="DC13" s="5">
         <v>54.6</v>
       </c>
-      <c r="DD13" s="5"/>
+      <c r="DD13" s="5">
+        <v>55.7</v>
+      </c>
       <c r="DE13" s="5"/>
       <c r="DF13" s="5"/>
       <c r="DG13" s="5"/>
@@ -11968,7 +11992,9 @@
       <c r="DC14" s="5">
         <v>42.1</v>
       </c>
-      <c r="DD14" s="5"/>
+      <c r="DD14" s="5">
+        <v>42.3</v>
+      </c>
       <c r="DE14" s="5"/>
       <c r="DF14" s="5"/>
       <c r="DG14" s="5"/>
@@ -12286,7 +12312,9 @@
       <c r="DC15" s="5">
         <v>24.25</v>
       </c>
-      <c r="DD15" s="5"/>
+      <c r="DD15" s="5">
+        <v>23.95</v>
+      </c>
       <c r="DE15" s="5"/>
       <c r="DF15" s="5"/>
       <c r="DG15" s="5"/>
@@ -12612,7 +12640,9 @@
       <c r="DC16" s="5">
         <v>753</v>
       </c>
-      <c r="DD16" s="5"/>
+      <c r="DD16" s="5">
+        <v>753.55</v>
+      </c>
       <c r="DE16" s="5"/>
       <c r="DF16" s="5"/>
       <c r="DG16" s="5"/>
@@ -12940,7 +12970,9 @@
       <c r="DC17" s="5">
         <v>489</v>
       </c>
-      <c r="DD17" s="5"/>
+      <c r="DD17" s="5">
+        <v>484.5</v>
+      </c>
       <c r="DE17" s="5"/>
       <c r="DF17" s="5"/>
       <c r="DG17" s="5"/>
@@ -13266,7 +13298,9 @@
       <c r="DC18" s="5">
         <v>275.5</v>
       </c>
-      <c r="DD18" s="5"/>
+      <c r="DD18" s="5">
+        <v>282.10000000000002</v>
+      </c>
       <c r="DE18" s="5"/>
       <c r="DF18" s="5"/>
       <c r="DG18" s="5"/>
@@ -13592,7 +13626,9 @@
       <c r="DC19" s="5">
         <v>448.95</v>
       </c>
-      <c r="DD19" s="5"/>
+      <c r="DD19" s="5">
+        <v>473.7</v>
+      </c>
       <c r="DE19" s="5"/>
       <c r="DF19" s="5"/>
       <c r="DG19" s="5"/>
@@ -13600,7 +13636,7 @@
     <row r="20" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <f t="shared" si="0"/>
-        <v>642.6</v>
+        <v>642</v>
       </c>
       <c r="B20" s="12">
         <f t="shared" si="1"/>
@@ -13608,7 +13644,7 @@
       </c>
       <c r="C20" s="12">
         <f t="shared" si="2"/>
-        <v>153.35000000000002</v>
+        <v>153.95000000000005</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="44" t="s">
@@ -13918,7 +13954,9 @@
       <c r="DC20" s="5">
         <v>644.15</v>
       </c>
-      <c r="DD20" s="5"/>
+      <c r="DD20" s="5">
+        <v>642</v>
+      </c>
       <c r="DE20" s="5"/>
       <c r="DF20" s="5"/>
       <c r="DG20" s="5"/>
@@ -14244,7 +14282,9 @@
       <c r="DC21" s="5">
         <v>498.05</v>
       </c>
-      <c r="DD21" s="5"/>
+      <c r="DD21" s="5">
+        <v>491</v>
+      </c>
       <c r="DE21" s="5"/>
       <c r="DF21" s="5"/>
       <c r="DG21" s="5"/>
@@ -14516,7 +14556,9 @@
       <c r="DC22" s="5">
         <v>409.25</v>
       </c>
-      <c r="DD22" s="5"/>
+      <c r="DD22" s="5">
+        <v>410</v>
+      </c>
       <c r="DE22" s="5"/>
       <c r="DF22" s="5"/>
       <c r="DG22" s="5"/>
@@ -14836,7 +14878,9 @@
       <c r="DC23" s="5">
         <v>60.95</v>
       </c>
-      <c r="DD23" s="5"/>
+      <c r="DD23" s="5">
+        <v>61.75</v>
+      </c>
       <c r="DE23" s="5"/>
       <c r="DF23" s="5"/>
       <c r="DG23" s="5"/>
@@ -15150,7 +15194,9 @@
       <c r="DC24" s="5">
         <v>242.75</v>
       </c>
-      <c r="DD24" s="5"/>
+      <c r="DD24" s="5">
+        <v>237.9</v>
+      </c>
       <c r="DE24" s="5"/>
       <c r="DF24" s="5"/>
       <c r="DG24" s="5"/>
@@ -15446,7 +15492,9 @@
       <c r="DC25" s="5">
         <v>1145.9000000000001</v>
       </c>
-      <c r="DD25" s="5"/>
+      <c r="DD25" s="5">
+        <v>1148.0999999999999</v>
+      </c>
       <c r="DE25" s="5"/>
       <c r="DF25" s="5"/>
       <c r="DG25" s="5"/>
@@ -15730,7 +15778,9 @@
       <c r="DC26" s="5">
         <v>121.5</v>
       </c>
-      <c r="DD26" s="5"/>
+      <c r="DD26" s="5">
+        <v>121.55</v>
+      </c>
       <c r="DE26" s="5"/>
       <c r="DF26" s="5"/>
       <c r="DG26" s="5"/>
@@ -16014,7 +16064,9 @@
       <c r="DC27" s="5">
         <v>44.6</v>
       </c>
-      <c r="DD27" s="5"/>
+      <c r="DD27" s="5">
+        <v>43.75</v>
+      </c>
       <c r="DE27" s="5"/>
       <c r="DF27" s="5"/>
       <c r="DG27" s="5"/>
@@ -16298,7 +16350,9 @@
       <c r="DC28" s="5">
         <v>135.69999999999999</v>
       </c>
-      <c r="DD28" s="5"/>
+      <c r="DD28" s="5">
+        <v>139</v>
+      </c>
       <c r="DE28" s="5"/>
       <c r="DF28" s="5"/>
       <c r="DG28" s="5"/>
@@ -16582,7 +16636,9 @@
       <c r="DC29" s="5">
         <v>73.150000000000006</v>
       </c>
-      <c r="DD29" s="5"/>
+      <c r="DD29" s="5">
+        <v>72.650000000000006</v>
+      </c>
       <c r="DE29" s="5"/>
       <c r="DF29" s="5"/>
       <c r="DG29" s="5"/>
@@ -16866,7 +16922,9 @@
       <c r="DC30" s="5">
         <v>44.5</v>
       </c>
-      <c r="DD30" s="5"/>
+      <c r="DD30" s="5">
+        <v>44</v>
+      </c>
       <c r="DE30" s="5"/>
       <c r="DF30" s="5"/>
       <c r="DG30" s="5"/>
@@ -17150,7 +17208,9 @@
       <c r="DC31" s="5">
         <v>145.30000000000001</v>
       </c>
-      <c r="DD31" s="5"/>
+      <c r="DD31" s="5">
+        <v>146.85</v>
+      </c>
       <c r="DE31" s="5"/>
       <c r="DF31" s="5"/>
       <c r="DG31" s="5"/>
@@ -17424,7 +17484,9 @@
       <c r="DC32" s="5">
         <v>100.15</v>
       </c>
-      <c r="DD32" s="5"/>
+      <c r="DD32" s="5">
+        <v>100.7</v>
+      </c>
       <c r="DE32" s="5"/>
       <c r="DF32" s="5"/>
       <c r="DG32" s="5"/>
@@ -17684,7 +17746,9 @@
       <c r="DC33" s="5">
         <v>68.2</v>
       </c>
-      <c r="DD33" s="5"/>
+      <c r="DD33" s="5">
+        <v>68.55</v>
+      </c>
       <c r="DE33" s="5"/>
       <c r="DF33" s="5"/>
       <c r="DG33" s="5"/>
@@ -17938,7 +18002,9 @@
       <c r="DC34" s="5">
         <v>256.8</v>
       </c>
-      <c r="DD34" s="5"/>
+      <c r="DD34" s="5">
+        <v>257</v>
+      </c>
       <c r="DE34" s="5"/>
       <c r="DF34" s="5"/>
       <c r="DG34" s="5"/>
@@ -18170,7 +18236,9 @@
       <c r="DC35" s="5">
         <v>400</v>
       </c>
-      <c r="DD35" s="5"/>
+      <c r="DD35" s="5">
+        <v>419.75</v>
+      </c>
       <c r="DE35" s="5"/>
       <c r="DF35" s="5"/>
       <c r="DG35" s="5"/>
@@ -18392,7 +18460,9 @@
       <c r="DC36" s="5">
         <v>431.95</v>
       </c>
-      <c r="DD36" s="5"/>
+      <c r="DD36" s="5">
+        <v>430.35</v>
+      </c>
       <c r="DE36" s="5"/>
       <c r="DF36" s="5"/>
       <c r="DG36" s="5"/>
@@ -18400,7 +18470,7 @@
     <row r="37" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <f t="shared" si="0"/>
-        <v>72.2</v>
+        <v>71.25</v>
       </c>
       <c r="B37" s="12">
         <f t="shared" si="1"/>
@@ -18408,7 +18478,7 @@
       </c>
       <c r="C37" s="12">
         <f t="shared" si="2"/>
-        <v>13.299999999999997</v>
+        <v>14.25</v>
       </c>
       <c r="D37" s="12">
         <v>80</v>
@@ -18608,7 +18678,9 @@
       <c r="DC37" s="5">
         <v>72.650000000000006</v>
       </c>
-      <c r="DD37" s="5"/>
+      <c r="DD37" s="5">
+        <v>71.25</v>
+      </c>
       <c r="DE37" s="5"/>
       <c r="DF37" s="5"/>
       <c r="DG37" s="5"/>
@@ -18824,7 +18896,9 @@
       <c r="DC38" s="5">
         <v>451</v>
       </c>
-      <c r="DD38" s="5"/>
+      <c r="DD38" s="5">
+        <v>427.5</v>
+      </c>
       <c r="DE38" s="5"/>
       <c r="DF38" s="5"/>
       <c r="DG38" s="5"/>
@@ -19034,7 +19108,9 @@
       <c r="DC39" s="5">
         <v>228.1</v>
       </c>
-      <c r="DD39" s="5"/>
+      <c r="DD39" s="5">
+        <v>227</v>
+      </c>
       <c r="DE39" s="5"/>
       <c r="DF39" s="5"/>
       <c r="DG39" s="5"/>
@@ -19240,7 +19316,9 @@
       <c r="DC40" s="5">
         <v>37</v>
       </c>
-      <c r="DD40" s="5"/>
+      <c r="DD40" s="5">
+        <v>38.200000000000003</v>
+      </c>
       <c r="DE40" s="5"/>
       <c r="DF40" s="5"/>
       <c r="DG40" s="5"/>
@@ -19444,7 +19522,9 @@
       <c r="DC41" s="5">
         <v>779.2</v>
       </c>
-      <c r="DD41" s="5"/>
+      <c r="DD41" s="5">
+        <v>805.5</v>
+      </c>
       <c r="DE41" s="5"/>
       <c r="DF41" s="5"/>
       <c r="DG41" s="5"/>
@@ -19456,11 +19536,11 @@
       </c>
       <c r="B42" s="12">
         <f t="shared" si="1"/>
-        <v>928.7</v>
+        <v>930</v>
       </c>
       <c r="C42" s="12">
         <f t="shared" si="2"/>
-        <v>118.10000000000002</v>
+        <v>119.39999999999998</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="45" t="s">
@@ -19648,7 +19728,9 @@
       <c r="DC42" s="5">
         <v>923</v>
       </c>
-      <c r="DD42" s="5"/>
+      <c r="DD42" s="5">
+        <v>930</v>
+      </c>
       <c r="DE42" s="5"/>
       <c r="DF42" s="5"/>
       <c r="DG42" s="5"/>
@@ -19850,7 +19932,9 @@
       <c r="DC43" s="5">
         <v>152.55000000000001</v>
       </c>
-      <c r="DD43" s="5"/>
+      <c r="DD43" s="5">
+        <v>155.25</v>
+      </c>
       <c r="DE43" s="5"/>
       <c r="DF43" s="5"/>
       <c r="DG43" s="5"/>
@@ -20048,7 +20132,9 @@
       <c r="DC44" s="5">
         <v>607.9</v>
       </c>
-      <c r="DD44" s="5"/>
+      <c r="DD44" s="5">
+        <v>617.5</v>
+      </c>
       <c r="DE44" s="5"/>
       <c r="DF44" s="5"/>
       <c r="DG44" s="5"/>
@@ -20236,7 +20322,9 @@
       <c r="DC45" s="5">
         <v>109.85</v>
       </c>
-      <c r="DD45" s="5"/>
+      <c r="DD45" s="5">
+        <v>118.25</v>
+      </c>
       <c r="DE45" s="5"/>
       <c r="DF45" s="5"/>
       <c r="DG45" s="5"/>
@@ -20410,7 +20498,9 @@
       <c r="DC46" s="5">
         <v>153.5</v>
       </c>
-      <c r="DD46" s="5"/>
+      <c r="DD46" s="5">
+        <v>151.5</v>
+      </c>
       <c r="DE46" s="5"/>
       <c r="DF46" s="5"/>
       <c r="DG46" s="5"/>
@@ -20566,7 +20656,9 @@
       <c r="DC47" s="5">
         <v>89</v>
       </c>
-      <c r="DD47" s="5"/>
+      <c r="DD47" s="5">
+        <v>90.1</v>
+      </c>
       <c r="DE47" s="5"/>
       <c r="DF47" s="5"/>
       <c r="DG47" s="5"/>
@@ -20712,7 +20804,9 @@
       <c r="DC48" s="5">
         <v>92.95</v>
       </c>
-      <c r="DD48" s="5"/>
+      <c r="DD48" s="5">
+        <v>93.1</v>
+      </c>
       <c r="DE48" s="5"/>
       <c r="DF48" s="5"/>
       <c r="DG48" s="5"/>

</xml_diff>

<commit_message>
Native and SSL documentation
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14205" yWindow="1035" windowWidth="13530" windowHeight="5625" activeTab="1"/>
+    <workbookView xWindow="14205" yWindow="1035" windowWidth="13530" windowHeight="5625" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="PaidTillDate" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="360">
   <si>
     <t>Date</t>
   </si>
@@ -1099,6 +1099,12 @@
   </si>
   <si>
     <t>2017</t>
+  </si>
+  <si>
+    <t>Kitchen items</t>
+  </si>
+  <si>
+    <t>7th May</t>
   </si>
 </sst>
 </file>
@@ -1289,7 +1295,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1358,12 +1364,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -1371,6 +1371,13 @@
     <xf numFmtId="15" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -6347,7 +6354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DR50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="6" topLeftCell="DJ1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="DU23" sqref="DU23"/>
     </sheetView>
@@ -21547,12 +21554,12 @@
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="2" spans="2:7" ht="15" customHeight="1">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
     </row>
     <row r="3" spans="2:7" ht="15" customHeight="1">
       <c r="B3" s="6" t="s">
@@ -21698,7 +21705,7 @@
       <c r="B15" s="27"/>
       <c r="C15" s="12"/>
       <c r="D15" s="11"/>
-      <c r="E15" s="56" t="s">
+      <c r="E15" s="54" t="s">
         <v>330</v>
       </c>
       <c r="F15" s="44"/>
@@ -21805,7 +21812,7 @@
       <c r="D21" s="53" t="s">
         <v>322</v>
       </c>
-      <c r="E21" s="56" t="s">
+      <c r="E21" s="54" t="s">
         <v>335</v>
       </c>
       <c r="F21" s="27">
@@ -21819,7 +21826,7 @@
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
-      <c r="E22" s="56" t="s">
+      <c r="E22" s="54" t="s">
         <v>336</v>
       </c>
       <c r="F22" s="27" t="s">
@@ -21963,10 +21970,10 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="55"/>
+      <c r="B8" s="62"/>
       <c r="D8" s="9" t="s">
         <v>9</v>
       </c>
@@ -22376,10 +22383,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30:K36"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22424,7 +22431,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(B2:B200)</f>
-        <v>1323793</v>
+        <v>1363793</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -22442,7 +22449,7 @@
       </c>
       <c r="F3" s="5">
         <f>F1-F2</f>
-        <v>151596</v>
+        <v>111596</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -23163,6 +23170,17 @@
       </c>
       <c r="C53" s="23">
         <v>43221</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="42" t="s">
+        <v>358</v>
+      </c>
+      <c r="B54" s="18">
+        <v>40000</v>
+      </c>
+      <c r="C54" s="63" t="s">
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -23182,7 +23200,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" style="58" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" style="56" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
@@ -23201,10 +23219,10 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="55" t="s">
         <v>346</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="57" t="s">
         <v>356</v>
       </c>
       <c r="C2">
@@ -23223,7 +23241,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="55" t="s">
         <v>347</v>
       </c>
       <c r="C3">
@@ -23242,7 +23260,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="55" t="s">
         <v>348</v>
       </c>
       <c r="C4">
@@ -23254,7 +23272,7 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="55" t="s">
         <v>349</v>
       </c>
       <c r="C5">
@@ -23272,7 +23290,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="55" t="s">
         <v>350</v>
       </c>
       <c r="C6">
@@ -23290,7 +23308,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="55" t="s">
         <v>351</v>
       </c>
       <c r="C7">
@@ -23309,7 +23327,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="55" t="s">
         <v>352</v>
       </c>
       <c r="C8">
@@ -23328,10 +23346,10 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="55" t="s">
         <v>343</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="57" t="s">
         <v>357</v>
       </c>
       <c r="C9">
@@ -23349,7 +23367,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="55" t="s">
         <v>344</v>
       </c>
       <c r="C10">
@@ -23361,7 +23379,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="55" t="s">
         <v>324</v>
       </c>
       <c r="C11">
@@ -23373,7 +23391,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="55" t="s">
         <v>325</v>
       </c>
       <c r="C12">
@@ -23385,7 +23403,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="55" t="s">
         <v>345</v>
       </c>
       <c r="C13">
@@ -23397,7 +23415,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="55" t="s">
         <v>346</v>
       </c>
       <c r="C14">
@@ -23409,7 +23427,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="55" t="s">
         <v>347</v>
       </c>
       <c r="C15">
@@ -23422,7 +23440,7 @@
       <c r="F15" s="26"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="55" t="s">
         <v>348</v>
       </c>
       <c r="C16">
@@ -23434,7 +23452,7 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="55" t="s">
         <v>349</v>
       </c>
       <c r="C17">
@@ -23446,7 +23464,7 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="55" t="s">
         <v>350</v>
       </c>
       <c r="C18">
@@ -23458,7 +23476,7 @@
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="55" t="s">
         <v>351</v>
       </c>
       <c r="C19">
@@ -23470,7 +23488,7 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="55" t="s">
         <v>352</v>
       </c>
       <c r="C20">
@@ -23482,10 +23500,10 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="57" t="s">
+      <c r="A21" s="55" t="s">
         <v>343</v>
       </c>
-      <c r="B21" s="59">
+      <c r="B21" s="57">
         <v>2018</v>
       </c>
       <c r="C21">
@@ -23497,10 +23515,10 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="57" t="s">
+      <c r="A22" s="55" t="s">
         <v>344</v>
       </c>
-      <c r="B22" s="59"/>
+      <c r="B22" s="57"/>
       <c r="C22">
         <v>5800</v>
       </c>
@@ -23510,10 +23528,10 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="57" t="s">
+      <c r="A23" s="55" t="s">
         <v>324</v>
       </c>
-      <c r="B23" s="59"/>
+      <c r="B23" s="57"/>
       <c r="C23">
         <v>5800</v>
       </c>
@@ -23522,24 +23540,24 @@
         <v>127600</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="62" customFormat="1">
-      <c r="A24" s="60" t="s">
+    <row r="24" spans="1:4" s="60" customFormat="1">
+      <c r="A24" s="58" t="s">
         <v>325</v>
       </c>
-      <c r="B24" s="61"/>
-      <c r="C24" s="62">
+      <c r="B24" s="59"/>
+      <c r="C24" s="60">
         <v>5800</v>
       </c>
-      <c r="D24" s="62">
+      <c r="D24" s="60">
         <f t="shared" si="0"/>
         <v>133400</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="55" t="s">
         <v>345</v>
       </c>
-      <c r="B25" s="59"/>
+      <c r="B25" s="57"/>
       <c r="C25">
         <v>5800</v>
       </c>
@@ -23549,10 +23567,10 @@
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="57" t="s">
+      <c r="A26" s="55" t="s">
         <v>346</v>
       </c>
-      <c r="B26" s="59"/>
+      <c r="B26" s="57"/>
       <c r="C26">
         <v>5800</v>
       </c>
@@ -23562,10 +23580,10 @@
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="57" t="s">
+      <c r="A27" s="55" t="s">
         <v>347</v>
       </c>
-      <c r="B27" s="59"/>
+      <c r="B27" s="57"/>
       <c r="C27">
         <v>5800</v>
       </c>
@@ -23575,10 +23593,10 @@
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="57" t="s">
+      <c r="A28" s="55" t="s">
         <v>348</v>
       </c>
-      <c r="B28" s="59"/>
+      <c r="B28" s="57"/>
       <c r="C28">
         <v>5800</v>
       </c>
@@ -23588,10 +23606,10 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="57" t="s">
+      <c r="A29" s="55" t="s">
         <v>349</v>
       </c>
-      <c r="B29" s="59"/>
+      <c r="B29" s="57"/>
       <c r="C29">
         <v>5800</v>
       </c>
@@ -23601,10 +23619,10 @@
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="57" t="s">
+      <c r="A30" s="55" t="s">
         <v>350</v>
       </c>
-      <c r="B30" s="59"/>
+      <c r="B30" s="57"/>
       <c r="C30">
         <v>5800</v>
       </c>
@@ -23614,10 +23632,10 @@
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="57" t="s">
+      <c r="A31" s="55" t="s">
         <v>351</v>
       </c>
-      <c r="B31" s="59"/>
+      <c r="B31" s="57"/>
       <c r="C31">
         <v>5800</v>
       </c>
@@ -23627,10 +23645,10 @@
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="57" t="s">
+      <c r="A32" s="55" t="s">
         <v>352</v>
       </c>
-      <c r="B32" s="59"/>
+      <c r="B32" s="57"/>
       <c r="C32">
         <v>5800</v>
       </c>
@@ -23640,10 +23658,10 @@
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="57" t="s">
+      <c r="A33" s="55" t="s">
         <v>343</v>
       </c>
-      <c r="B33" s="59" t="s">
+      <c r="B33" s="57" t="s">
         <v>353</v>
       </c>
       <c r="C33">
@@ -23655,7 +23673,7 @@
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="57" t="s">
+      <c r="A34" s="55" t="s">
         <v>344</v>
       </c>
       <c r="C34">
@@ -23667,7 +23685,7 @@
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="57" t="s">
+      <c r="A35" s="55" t="s">
         <v>324</v>
       </c>
       <c r="C35">
@@ -23679,7 +23697,7 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="55" t="s">
         <v>325</v>
       </c>
       <c r="C36">
@@ -23691,7 +23709,7 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="57" t="s">
+      <c r="A37" s="55" t="s">
         <v>345</v>
       </c>
       <c r="C37">
@@ -23703,7 +23721,7 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="57" t="s">
+      <c r="A38" s="55" t="s">
         <v>346</v>
       </c>
       <c r="C38">
@@ -23715,7 +23733,7 @@
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="57" t="s">
+      <c r="A39" s="55" t="s">
         <v>347</v>
       </c>
       <c r="C39">
@@ -23727,7 +23745,7 @@
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="57" t="s">
+      <c r="A40" s="55" t="s">
         <v>348</v>
       </c>
       <c r="C40">
@@ -23739,7 +23757,7 @@
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="57" t="s">
+      <c r="A41" s="55" t="s">
         <v>349</v>
       </c>
       <c r="C41">
@@ -23751,7 +23769,7 @@
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="57" t="s">
+      <c r="A42" s="55" t="s">
         <v>350</v>
       </c>
       <c r="C42">
@@ -23763,7 +23781,7 @@
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="57" t="s">
+      <c r="A43" s="55" t="s">
         <v>351</v>
       </c>
       <c r="C43">
@@ -23775,7 +23793,7 @@
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="57" t="s">
+      <c r="A44" s="55" t="s">
         <v>352</v>
       </c>
       <c r="C44">
@@ -23787,10 +23805,10 @@
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="57" t="s">
+      <c r="A45" s="55" t="s">
         <v>343</v>
       </c>
-      <c r="B45" s="59" t="s">
+      <c r="B45" s="57" t="s">
         <v>355</v>
       </c>
       <c r="C45">
@@ -23802,7 +23820,7 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="55" t="s">
         <v>344</v>
       </c>
       <c r="C46">
@@ -23814,7 +23832,7 @@
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="57" t="s">
+      <c r="A47" s="55" t="s">
         <v>324</v>
       </c>
       <c r="C47">
@@ -23826,7 +23844,7 @@
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="57" t="s">
+      <c r="A48" s="55" t="s">
         <v>325</v>
       </c>
       <c r="C48">
@@ -23838,7 +23856,7 @@
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="57" t="s">
+      <c r="A49" s="55" t="s">
         <v>345</v>
       </c>
       <c r="C49">
@@ -23850,7 +23868,7 @@
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="57" t="s">
+      <c r="A50" s="55" t="s">
         <v>346</v>
       </c>
       <c r="C50">
@@ -23862,7 +23880,7 @@
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="57" t="s">
+      <c r="A51" s="55" t="s">
         <v>347</v>
       </c>
       <c r="C51">
@@ -23874,7 +23892,7 @@
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="57" t="s">
+      <c r="A52" s="55" t="s">
         <v>348</v>
       </c>
       <c r="C52">
@@ -23886,7 +23904,7 @@
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="57" t="s">
+      <c r="A53" s="55" t="s">
         <v>349</v>
       </c>
       <c r="C53">
@@ -23898,7 +23916,7 @@
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="57" t="s">
+      <c r="A54" s="55" t="s">
         <v>350</v>
       </c>
       <c r="C54">
@@ -23910,7 +23928,7 @@
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="57" t="s">
+      <c r="A55" s="55" t="s">
         <v>351</v>
       </c>
       <c r="C55">
@@ -23922,7 +23940,7 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="57" t="s">
+      <c r="A56" s="55" t="s">
         <v>352</v>
       </c>
       <c r="C56">
@@ -23934,10 +23952,10 @@
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="57" t="s">
+      <c r="A57" s="55" t="s">
         <v>343</v>
       </c>
-      <c r="B57" s="59" t="s">
+      <c r="B57" s="57" t="s">
         <v>354</v>
       </c>
       <c r="C57">
@@ -23949,7 +23967,7 @@
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="57" t="s">
+      <c r="A58" s="55" t="s">
         <v>344</v>
       </c>
       <c r="C58">
@@ -23961,7 +23979,7 @@
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="57" t="s">
+      <c r="A59" s="55" t="s">
         <v>324</v>
       </c>
       <c r="C59">
@@ -23973,7 +23991,7 @@
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="57" t="s">
+      <c r="A60" s="55" t="s">
         <v>325</v>
       </c>
       <c r="C60">
@@ -23985,7 +24003,7 @@
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="57" t="s">
+      <c r="A61" s="55" t="s">
         <v>345</v>
       </c>
       <c r="C61">

</xml_diff>

<commit_message>
Added few more learning
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14210" yWindow="1040" windowWidth="13530" windowHeight="5630"/>
+    <workbookView xWindow="14210" yWindow="1040" windowWidth="13530" windowHeight="5630" firstSheet="4" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="PaidTillDate" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="377">
   <si>
     <t>Date</t>
   </si>
@@ -991,9 +991,6 @@
     <t>myfriendwa</t>
   </si>
   <si>
-    <t>myfriend</t>
-  </si>
-  <si>
     <t>{{normal}}</t>
   </si>
   <si>
@@ -1136,6 +1133,30 @@
   </si>
   <si>
     <t>6- July, 2019</t>
+  </si>
+  <si>
+    <t>8-August, 2019</t>
+  </si>
+  <si>
+    <t>India Post</t>
+  </si>
+  <si>
+    <t>anshulsood</t>
+  </si>
+  <si>
+    <t>FirstNamenormalLast</t>
+  </si>
+  <si>
+    <t>Epost</t>
+  </si>
+  <si>
+    <t>anshulsood2006</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>5-Sept, 2019</t>
   </si>
 </sst>
 </file>
@@ -1718,8 +1739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F29" activeCellId="1" sqref="E6 F29"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1"/>
@@ -1780,7 +1801,7 @@
       </c>
       <c r="E2" s="4">
         <f>E1-B34</f>
-        <v>-34010</v>
+        <v>-44010</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -2015,7 +2036,7 @@
     </row>
     <row r="28" spans="1:24">
       <c r="A28" s="63" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B28" s="17">
         <v>10000</v>
@@ -2023,7 +2044,7 @@
     </row>
     <row r="29" spans="1:24">
       <c r="A29" s="64" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B29" s="17">
         <v>5000</v>
@@ -2031,19 +2052,27 @@
     </row>
     <row r="30" spans="1:24">
       <c r="A30" s="64" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B30" s="17">
         <v>5000</v>
       </c>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="64"/>
-      <c r="B31" s="17"/>
+      <c r="A31" s="64" t="s">
+        <v>369</v>
+      </c>
+      <c r="B31" s="17">
+        <v>5000</v>
+      </c>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" s="64"/>
-      <c r="B32" s="17"/>
+      <c r="A32" s="64" t="s">
+        <v>376</v>
+      </c>
+      <c r="B32" s="17">
+        <v>5000</v>
+      </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="64"/>
@@ -2054,8 +2083,8 @@
         <v>2</v>
       </c>
       <c r="B34" s="13">
-        <f>SUM(B2:B30)</f>
-        <v>592500</v>
+        <f>SUM(B2:B32)</f>
+        <v>602500</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -6433,10 +6462,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6451,35 +6480,35 @@
     <col min="11" max="16384" width="8.7265625" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="C1" s="44" t="s">
+        <v>361</v>
+      </c>
+      <c r="D1" s="44" t="s">
         <v>362</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="E1" s="44" t="s">
         <v>363</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="F1" s="44" t="s">
         <v>364</v>
-      </c>
-      <c r="F1" s="44" t="s">
-        <v>365</v>
       </c>
       <c r="G1" s="44" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="44" t="s">
+        <v>365</v>
+      </c>
+      <c r="I1" s="44" t="s">
         <v>366</v>
       </c>
-      <c r="I1" s="44" t="s">
+      <c r="J1" s="44" t="s">
         <v>367</v>
       </c>
-      <c r="J1" s="44" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="44" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B2" s="44">
         <v>2019</v>
@@ -6506,24 +6535,24 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="44" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B3" s="44">
         <v>2019</v>
       </c>
       <c r="C3" s="44">
-        <v>38425</v>
+        <v>0</v>
       </c>
       <c r="D3" s="44">
-        <v>15000</v>
+        <v>0</v>
       </c>
       <c r="E3" s="44">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="F3" s="44">
-        <v>5800</v>
+        <v>0</v>
       </c>
       <c r="G3" s="44">
         <v>12000</v>
@@ -6535,24 +6564,24 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" s="44" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B4" s="44">
         <v>2019</v>
       </c>
       <c r="C4" s="44">
-        <v>38425</v>
+        <v>0</v>
       </c>
       <c r="D4" s="44">
-        <v>15000</v>
+        <v>0</v>
       </c>
       <c r="E4" s="44">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="F4" s="44">
-        <v>5800</v>
+        <v>0</v>
       </c>
       <c r="G4" s="44">
         <v>12000</v>
@@ -6564,24 +6593,24 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" s="44" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B5" s="44">
         <v>2019</v>
       </c>
       <c r="C5" s="44">
-        <v>38425</v>
+        <v>0</v>
       </c>
       <c r="D5" s="44">
-        <v>15000</v>
+        <v>0</v>
       </c>
       <c r="E5" s="44">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="F5" s="44">
-        <v>5800</v>
+        <v>0</v>
       </c>
       <c r="G5" s="44">
         <v>12000</v>
@@ -6592,10 +6621,13 @@
       <c r="I5" s="44">
         <v>2000</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5" s="44">
+        <v>61000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="44" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B6" s="44">
         <v>2019</v>
@@ -6621,10 +6653,14 @@
       <c r="I6" s="44">
         <v>2000</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6" s="44">
+        <f>K5-5100</f>
+        <v>55900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="44" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B7" s="44">
         <v>2019</v>
@@ -6650,10 +6686,14 @@
       <c r="I7" s="44">
         <v>2000</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7" s="44">
+        <f t="shared" ref="K7:K16" si="0">K6-5100</f>
+        <v>50800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="44" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B8" s="44">
         <v>2019</v>
@@ -6679,10 +6719,14 @@
       <c r="I8" s="44">
         <v>2000</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="44">
+        <f t="shared" si="0"/>
+        <v>45700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="44" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B9" s="44">
         <v>2020</v>
@@ -6708,10 +6752,14 @@
       <c r="I9" s="44">
         <v>2000</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" s="44">
+        <f t="shared" si="0"/>
+        <v>40600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="44" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B10" s="44">
         <v>2020</v>
@@ -6737,10 +6785,14 @@
       <c r="I10" s="44">
         <v>2000</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" s="44">
+        <f t="shared" si="0"/>
+        <v>35500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="44" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B11" s="44">
         <v>2020</v>
@@ -6766,10 +6818,14 @@
       <c r="I11" s="44">
         <v>2000</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" s="44">
+        <f t="shared" si="0"/>
+        <v>30400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="44" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B12" s="44">
         <v>2020</v>
@@ -6795,10 +6851,14 @@
       <c r="I12" s="44">
         <v>2000</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12" s="44">
+        <f t="shared" si="0"/>
+        <v>25300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="44" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B13" s="44">
         <v>2020</v>
@@ -6824,10 +6884,14 @@
       <c r="I13" s="44">
         <v>2000</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13" s="44">
+        <f t="shared" si="0"/>
+        <v>20200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="44" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B14" s="44">
         <v>2020</v>
@@ -6853,10 +6917,14 @@
       <c r="I14" s="44">
         <v>2000</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14" s="44">
+        <f t="shared" si="0"/>
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="44" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B15" s="44">
         <v>2020</v>
@@ -6882,10 +6950,14 @@
       <c r="I15" s="44">
         <v>2000</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15" s="44">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="44" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B16" s="44">
         <v>2020</v>
@@ -6908,10 +6980,14 @@
       <c r="I16" s="44">
         <v>7000</v>
       </c>
+      <c r="K16" s="44">
+        <f t="shared" si="0"/>
+        <v>4900</v>
+      </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="44" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B17" s="44">
         <v>2020</v>
@@ -6937,7 +7013,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="44" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B18" s="44">
         <v>2020</v>
@@ -6963,7 +7039,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="44" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B19" s="44">
         <v>2020</v>
@@ -6989,7 +7065,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="44" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B20" s="44">
         <v>2020</v>
@@ -7015,7 +7091,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="44" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B21" s="44">
         <v>2021</v>
@@ -7041,7 +7117,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="44" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B22" s="44">
         <v>2021</v>
@@ -7067,7 +7143,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="44" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B23" s="44">
         <v>2021</v>
@@ -7093,7 +7169,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="44" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B24" s="44">
         <v>2021</v>
@@ -7119,7 +7195,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="44" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B25" s="44">
         <v>2021</v>
@@ -7145,7 +7221,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="44" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B26" s="44">
         <v>2021</v>
@@ -7171,7 +7247,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="44" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B27" s="44">
         <v>2021</v>
@@ -7197,7 +7273,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="44" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B28" s="44">
         <v>2021</v>
@@ -7224,30 +7300,30 @@
     <row r="29" spans="1:9">
       <c r="C29" s="44">
         <f>SUM(C2:C28)</f>
-        <v>999050</v>
+        <v>883775</v>
       </c>
       <c r="D29" s="44">
         <f>SUM(D2:D28)</f>
-        <v>390000</v>
+        <v>345000</v>
       </c>
       <c r="E29" s="44">
         <f>SUM(E2:E28)</f>
-        <v>1040000</v>
+        <v>920000</v>
       </c>
       <c r="F29" s="44">
-        <f t="shared" ref="F29:I29" si="0">SUM(F2:F28)</f>
-        <v>75400</v>
+        <f t="shared" ref="F29:I29" si="1">SUM(F2:F28)</f>
+        <v>58000</v>
       </c>
       <c r="G29" s="44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>324000</v>
       </c>
       <c r="H29" s="44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>148000</v>
       </c>
       <c r="I29" s="44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>119000</v>
       </c>
     </row>
@@ -22453,15 +22529,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:F19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
   </cols>
@@ -22606,7 +22682,7 @@
     </row>
     <row r="14" spans="2:7" ht="15" customHeight="1">
       <c r="B14" s="39" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="11"/>
@@ -22619,7 +22695,7 @@
       <c r="C15" s="12"/>
       <c r="D15" s="11"/>
       <c r="E15" s="54" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F15" s="44"/>
       <c r="G15" s="11"/>
@@ -22635,7 +22711,7 @@
         <v>298</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F16" s="27">
         <v>86269</v>
@@ -22653,7 +22729,7 @@
         <v>297</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F17" s="27">
         <v>21600</v>
@@ -22689,7 +22765,7 @@
         <v>309</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F19" s="27">
         <v>36000</v>
@@ -22707,7 +22783,7 @@
         <v>318</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F20" s="27">
         <f>SUM(F16:F19)</f>
@@ -22720,39 +22796,51 @@
         <v>320</v>
       </c>
       <c r="C21" s="52" t="s">
+        <v>320</v>
+      </c>
+      <c r="D21" s="53" t="s">
         <v>321</v>
       </c>
-      <c r="D21" s="53" t="s">
-        <v>322</v>
-      </c>
       <c r="E21" s="54" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F21" s="27">
         <v>75000</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="15" customHeight="1">
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
+      <c r="B22" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="D22" s="53" t="s">
+        <v>372</v>
+      </c>
       <c r="E22" s="54" t="s">
+        <v>335</v>
+      </c>
+      <c r="F22" s="27" t="s">
         <v>336</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="2:7" ht="15" customHeight="1">
+      <c r="B23" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="C23" s="43" t="s">
+        <v>374</v>
+      </c>
+      <c r="D23" s="53" t="s">
+        <v>375</v>
+      </c>
+      <c r="E23" s="27" t="s">
         <v>337</v>
-      </c>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="2:7" ht="15" customHeight="1">
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="27" t="s">
-        <v>338</v>
       </c>
       <c r="F23" s="27">
         <v>14978</v>
@@ -22768,9 +22856,10 @@
     <hyperlink ref="D18" r:id="rId2"/>
     <hyperlink ref="D19" r:id="rId3"/>
     <hyperlink ref="C17" r:id="rId4"/>
+    <hyperlink ref="C22" r:id="rId5" display="anshulsood/Name786@"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -22810,7 +22899,7 @@
         <v>5000</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E2" s="5">
         <v>17500</v>
@@ -22839,7 +22928,7 @@
         <v>500</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E4" s="5">
         <v>15000</v>
@@ -22854,7 +22943,7 @@
         <v>1250000</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E5" s="10">
         <v>20000</v>
@@ -22945,7 +23034,7 @@
         <v>700</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E12" s="10">
         <v>4000</v>
@@ -22959,7 +23048,7 @@
         <v>400</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E13" s="10">
         <v>5000</v>
@@ -24044,35 +24133,35 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="28" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B50" s="10">
         <v>10000</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="28" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B51" s="10">
         <v>10000</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="28" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B52" s="10">
         <v>30000</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -24088,13 +24177,13 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="42" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B54" s="18">
         <v>40000</v>
       </c>
       <c r="C54" s="61" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -24107,8 +24196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38:C55"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -24134,10 +24223,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="55" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B2" s="57" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C2">
         <v>5800</v>
@@ -24156,7 +24245,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="55" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C3">
         <v>5800</v>
@@ -24175,7 +24264,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="55" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C4">
         <v>5800</v>
@@ -24187,7 +24276,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="55" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C5">
         <v>5800</v>
@@ -24205,7 +24294,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="55" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C6">
         <v>5800</v>
@@ -24223,7 +24312,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="55" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C7">
         <v>5800</v>
@@ -24242,7 +24331,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="55" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C8">
         <v>5800</v>
@@ -24261,10 +24350,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="55" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C9">
         <v>5800</v>
@@ -24282,7 +24371,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="55" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C10">
         <v>5800</v>
@@ -24294,7 +24383,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="55" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C11">
         <v>5800</v>
@@ -24306,7 +24395,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="55" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C12">
         <v>5800</v>
@@ -24318,7 +24407,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="55" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C13">
         <v>5800</v>
@@ -24330,7 +24419,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="55" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C14">
         <v>5800</v>
@@ -24342,7 +24431,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="55" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C15">
         <v>5800</v>
@@ -24355,7 +24444,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="55" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C16">
         <v>5800</v>
@@ -24367,7 +24456,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="55" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C17">
         <v>5800</v>
@@ -24379,7 +24468,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="55" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C18">
         <v>5800</v>
@@ -24391,7 +24480,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="55" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C19">
         <v>5800</v>
@@ -24403,7 +24492,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="55" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C20">
         <v>5800</v>
@@ -24415,7 +24504,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="55" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B21" s="57">
         <v>2018</v>
@@ -24430,7 +24519,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="55" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B22" s="57"/>
       <c r="C22">
@@ -24443,7 +24532,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="55" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B23" s="57"/>
       <c r="C23">
@@ -24456,7 +24545,7 @@
     </row>
     <row r="24" spans="1:4" s="67" customFormat="1">
       <c r="A24" s="65" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B24" s="66"/>
       <c r="C24" s="67">
@@ -24469,7 +24558,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="55" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B25" s="57"/>
       <c r="C25">
@@ -24482,7 +24571,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="55" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B26" s="57"/>
       <c r="C26">
@@ -24495,7 +24584,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="55" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B27" s="57"/>
       <c r="C27">
@@ -24508,7 +24597,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="55" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B28" s="57"/>
       <c r="C28">
@@ -24521,7 +24610,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="55" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B29" s="57"/>
       <c r="C29">
@@ -24534,7 +24623,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="55" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B30" s="57"/>
       <c r="C30">
@@ -24547,7 +24636,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="55" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B31" s="57"/>
       <c r="C31">
@@ -24560,7 +24649,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="55" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B32" s="57"/>
       <c r="C32">
@@ -24573,10 +24662,10 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="55" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B33" s="57" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C33">
         <v>5800</v>
@@ -24588,7 +24677,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="55" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C34">
         <v>5800</v>
@@ -24600,7 +24689,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="55" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C35">
         <v>5800</v>
@@ -24612,7 +24701,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="55" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C36">
         <v>5800</v>
@@ -24622,22 +24711,22 @@
         <v>203000</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="60" customFormat="1">
-      <c r="A37" s="58" t="s">
-        <v>345</v>
-      </c>
-      <c r="B37" s="59"/>
-      <c r="C37" s="60">
+    <row r="37" spans="1:4" s="67" customFormat="1">
+      <c r="A37" s="65" t="s">
+        <v>344</v>
+      </c>
+      <c r="B37" s="66"/>
+      <c r="C37" s="67">
         <v>5800</v>
       </c>
-      <c r="D37" s="60">
+      <c r="D37" s="67">
         <f t="shared" si="0"/>
         <v>208800</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="55" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C38">
         <v>5800</v>
@@ -24649,7 +24738,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="55" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C39">
         <v>5800</v>
@@ -24659,21 +24748,22 @@
         <v>220400</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="55" t="s">
-        <v>348</v>
-      </c>
-      <c r="C40">
+    <row r="40" spans="1:4" s="60" customFormat="1">
+      <c r="A40" s="58" t="s">
+        <v>347</v>
+      </c>
+      <c r="B40" s="59"/>
+      <c r="C40" s="60">
         <v>5800</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="60">
         <f t="shared" si="0"/>
         <v>226200</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="55" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C41">
         <v>5800</v>
@@ -24685,7 +24775,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="55" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C42">
         <v>5800</v>
@@ -24697,7 +24787,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="55" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C43">
         <v>5800</v>
@@ -24709,7 +24799,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="55" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C44">
         <v>5800</v>
@@ -24721,10 +24811,10 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="55" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B45" s="57" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C45">
         <v>5800</v>
@@ -24736,7 +24826,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="55" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C46">
         <v>5800</v>
@@ -24748,7 +24838,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="55" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C47">
         <v>5800</v>
@@ -24760,7 +24850,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="55" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C48">
         <v>5800</v>
@@ -24772,7 +24862,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="55" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C49">
         <v>5800</v>
@@ -24784,7 +24874,7 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="55" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C50">
         <v>5800</v>
@@ -24796,7 +24886,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="55" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C51">
         <v>5800</v>
@@ -24808,7 +24898,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="55" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C52">
         <v>5800</v>
@@ -24820,7 +24910,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="55" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C53">
         <v>5800</v>
@@ -24832,7 +24922,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="55" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C54">
         <v>5800</v>
@@ -24844,7 +24934,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="55" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C55">
         <v>5800</v>
@@ -24856,7 +24946,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="55" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C56">
         <v>5800</v>
@@ -24868,10 +24958,10 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="55" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B57" s="57" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C57">
         <v>5800</v>
@@ -24883,7 +24973,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="55" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C58">
         <v>5800</v>
@@ -24895,7 +24985,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="55" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C59">
         <v>5800</v>
@@ -24907,7 +24997,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="55" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C60">
         <v>5800</v>
@@ -24919,7 +25009,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="55" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C61">
         <v>5800</v>

</xml_diff>

<commit_message>
Started with micro services
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="380">
   <si>
     <t>Date</t>
   </si>
@@ -1162,6 +1162,15 @@
   </si>
   <si>
     <t>5-Sept, 2019</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>PlLLLLl</t>
+  </si>
+  <si>
+    <t>;</t>
   </si>
 </sst>
 </file>
@@ -1352,7 +1361,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1441,6 +1450,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -6472,10 +6482,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:F15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6490,7 +6500,7 @@
     <col min="11" max="16384" width="8.7265625" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C1" s="44" t="s">
         <v>361</v>
       </c>
@@ -6516,227 +6526,209 @@
         <v>367</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="44" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B2" s="44">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C2" s="44">
-        <v>0</v>
+        <v>38425</v>
       </c>
       <c r="D2" s="44">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="E2" s="44">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="F2" s="44">
-        <v>0</v>
+        <v>5800</v>
       </c>
       <c r="G2" s="44">
         <v>12000</v>
       </c>
       <c r="H2" s="44">
-        <v>2500</v>
+        <v>6000</v>
       </c>
       <c r="I2" s="44">
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B3" s="44">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C3" s="44">
-        <v>0</v>
+        <v>38425</v>
       </c>
       <c r="D3" s="44">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="E3" s="44">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="F3" s="44">
-        <v>0</v>
+        <v>5800</v>
       </c>
       <c r="G3" s="44">
         <v>12000</v>
       </c>
       <c r="H3" s="44">
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="I3" s="44">
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="44" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="B4" s="44">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C4" s="44">
-        <v>0</v>
+        <v>38425</v>
       </c>
       <c r="D4" s="44">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="E4" s="44">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="F4" s="44">
-        <v>0</v>
+        <v>5800</v>
       </c>
       <c r="G4" s="44">
         <v>12000</v>
       </c>
       <c r="H4" s="44">
-        <v>3500</v>
+        <v>6000</v>
       </c>
       <c r="I4" s="44">
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="44" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="B5" s="44">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C5" s="44">
-        <v>0</v>
+        <v>38425</v>
       </c>
       <c r="D5" s="44">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="E5" s="44">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="F5" s="44">
-        <v>0</v>
+        <v>5800</v>
       </c>
       <c r="G5" s="44">
         <v>12000</v>
       </c>
       <c r="H5" s="44">
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="I5" s="44">
         <v>2000</v>
       </c>
-      <c r="K5" s="44">
-        <v>37200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="44" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B6" s="44">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C6" s="44">
-        <v>0</v>
+        <v>38425</v>
       </c>
       <c r="D6" s="44">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="E6" s="44">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="F6" s="44">
-        <v>0</v>
+        <v>5800</v>
       </c>
       <c r="G6" s="44">
         <v>12000</v>
       </c>
       <c r="H6" s="44">
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="I6" s="44">
         <v>2000</v>
       </c>
-      <c r="K6" s="44">
-        <f>K5-5800</f>
-        <v>31400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="44" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="B7" s="44">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C7" s="44">
-        <v>0</v>
+        <v>38425</v>
       </c>
       <c r="D7" s="44">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="E7" s="44">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="F7" s="44">
-        <v>0</v>
+        <v>5800</v>
       </c>
       <c r="G7" s="44">
         <v>12000</v>
       </c>
       <c r="H7" s="44">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="I7" s="44">
         <v>2000</v>
       </c>
-      <c r="K7" s="44">
-        <f>K6-5800</f>
-        <v>25600</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="44" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B8" s="44">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C8" s="44">
-        <v>0</v>
+        <v>38425</v>
       </c>
       <c r="D8" s="44">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="E8" s="44">
-        <v>0</v>
-      </c>
-      <c r="F8" s="44">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="G8" s="44">
         <v>12000</v>
       </c>
       <c r="H8" s="44">
-        <v>5500</v>
+        <v>6000</v>
       </c>
       <c r="I8" s="44">
-        <v>2000</v>
-      </c>
-      <c r="K8" s="44">
-        <f t="shared" ref="K8:K12" si="0">K7-5800</f>
-        <v>19800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="44" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="B9" s="44">
         <v>2020</v>
@@ -6757,16 +6749,12 @@
         <v>6000</v>
       </c>
       <c r="I9" s="44">
-        <v>2000</v>
-      </c>
-      <c r="K9" s="44">
-        <f t="shared" si="0"/>
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="44" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="B10" s="44">
         <v>2020</v>
@@ -6780,9 +6768,6 @@
       <c r="E10" s="44">
         <v>40000</v>
       </c>
-      <c r="F10" s="44">
-        <v>5800</v>
-      </c>
       <c r="G10" s="44">
         <v>12000</v>
       </c>
@@ -6790,16 +6775,12 @@
         <v>6000</v>
       </c>
       <c r="I10" s="44">
-        <v>2000</v>
-      </c>
-      <c r="K10" s="44">
-        <f t="shared" si="0"/>
-        <v>8200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="44" t="s">
-        <v>323</v>
+        <v>349</v>
       </c>
       <c r="B11" s="44">
         <v>2020</v>
@@ -6813,9 +6794,6 @@
       <c r="E11" s="44">
         <v>40000</v>
       </c>
-      <c r="F11" s="44">
-        <v>5800</v>
-      </c>
       <c r="G11" s="44">
         <v>12000</v>
       </c>
@@ -6823,16 +6801,12 @@
         <v>6000</v>
       </c>
       <c r="I11" s="44">
-        <v>2000</v>
-      </c>
-      <c r="K11" s="44">
-        <f t="shared" si="0"/>
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="44" t="s">
-        <v>324</v>
+        <v>350</v>
       </c>
       <c r="B12" s="44">
         <v>2020</v>
@@ -6846,9 +6820,6 @@
       <c r="E12" s="44">
         <v>40000</v>
       </c>
-      <c r="F12" s="44">
-        <v>5800</v>
-      </c>
       <c r="G12" s="44">
         <v>12000</v>
       </c>
@@ -6856,16 +6827,12 @@
         <v>6000</v>
       </c>
       <c r="I12" s="44">
-        <v>2000</v>
-      </c>
-      <c r="K12" s="44">
-        <f t="shared" si="0"/>
-        <v>-3400</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="44" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="B13" s="44">
         <v>2020</v>
@@ -6879,9 +6846,6 @@
       <c r="E13" s="44">
         <v>40000</v>
       </c>
-      <c r="F13" s="44">
-        <v>5800</v>
-      </c>
       <c r="G13" s="44">
         <v>12000</v>
       </c>
@@ -6892,12 +6856,12 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="44" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B14" s="44">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C14" s="44">
         <v>38425</v>
@@ -6908,9 +6872,6 @@
       <c r="E14" s="44">
         <v>40000</v>
       </c>
-      <c r="F14" s="44">
-        <v>5800</v>
-      </c>
       <c r="G14" s="44">
         <v>12000</v>
       </c>
@@ -6921,12 +6882,12 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B15" s="44">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C15" s="44">
         <v>38425</v>
@@ -6937,9 +6898,6 @@
       <c r="E15" s="44">
         <v>40000</v>
       </c>
-      <c r="F15" s="44">
-        <v>5800</v>
-      </c>
       <c r="G15" s="44">
         <v>12000</v>
       </c>
@@ -6950,12 +6908,12 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="44" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="B16" s="44">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C16" s="44">
         <v>38425</v>
@@ -6976,12 +6934,12 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="44" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="B17" s="44">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C17" s="44">
         <v>38425</v>
@@ -7002,12 +6960,12 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="44" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B18" s="44">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C18" s="44">
         <v>38425</v>
@@ -7028,12 +6986,12 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="44" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="B19" s="44">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C19" s="44">
         <v>38425</v>
@@ -7054,12 +7012,12 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="44" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B20" s="44">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C20" s="44">
         <v>38425</v>
@@ -7080,9 +7038,9 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="44" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="B21" s="44">
         <v>2021</v>
@@ -7106,219 +7064,55 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="44" t="s">
-        <v>343</v>
-      </c>
-      <c r="B22" s="44">
-        <v>2021</v>
-      </c>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C22" s="44">
-        <v>38425</v>
+        <f>SUM(C2:C21)</f>
+        <v>768500</v>
       </c>
       <c r="D22" s="44">
-        <v>15000</v>
+        <f>SUM(D2:D21)</f>
+        <v>300000</v>
       </c>
       <c r="E22" s="44">
-        <v>40000</v>
+        <f>SUM(E2:E21)</f>
+        <v>800000</v>
+      </c>
+      <c r="F22" s="44">
+        <f>SUM(F2:F21)</f>
+        <v>34800</v>
       </c>
       <c r="G22" s="44">
-        <v>12000</v>
+        <f>SUM(G2:G21)</f>
+        <v>240000</v>
       </c>
       <c r="H22" s="44">
-        <v>6000</v>
+        <f>SUM(H2:H21)</f>
+        <v>120000</v>
       </c>
       <c r="I22" s="44">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="44" t="s">
-        <v>323</v>
-      </c>
-      <c r="B23" s="44">
-        <v>2021</v>
-      </c>
-      <c r="C23" s="44">
-        <v>38425</v>
-      </c>
-      <c r="D23" s="44">
-        <v>15000</v>
-      </c>
-      <c r="E23" s="44">
-        <v>40000</v>
-      </c>
-      <c r="G23" s="44">
-        <v>12000</v>
-      </c>
-      <c r="H23" s="44">
-        <v>6000</v>
-      </c>
-      <c r="I23" s="44">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="44" t="s">
-        <v>324</v>
-      </c>
-      <c r="B24" s="44">
-        <v>2021</v>
-      </c>
-      <c r="C24" s="44">
-        <v>38425</v>
-      </c>
-      <c r="D24" s="44">
-        <v>15000</v>
-      </c>
-      <c r="E24" s="44">
-        <v>40000</v>
-      </c>
-      <c r="G24" s="44">
-        <v>12000</v>
-      </c>
-      <c r="H24" s="44">
-        <v>6000</v>
-      </c>
-      <c r="I24" s="44">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="44" t="s">
-        <v>344</v>
-      </c>
-      <c r="B25" s="44">
-        <v>2021</v>
-      </c>
-      <c r="C25" s="44">
-        <v>38425</v>
-      </c>
-      <c r="D25" s="44">
-        <v>15000</v>
-      </c>
-      <c r="E25" s="44">
-        <v>40000</v>
-      </c>
-      <c r="G25" s="44">
-        <v>12000</v>
-      </c>
-      <c r="H25" s="44">
-        <v>6000</v>
-      </c>
-      <c r="I25" s="44">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="44" t="s">
-        <v>345</v>
-      </c>
-      <c r="B26" s="44">
-        <v>2021</v>
-      </c>
-      <c r="C26" s="44">
-        <v>38425</v>
-      </c>
-      <c r="D26" s="44">
-        <v>15000</v>
-      </c>
-      <c r="E26" s="44">
-        <v>40000</v>
-      </c>
-      <c r="G26" s="44">
-        <v>12000</v>
-      </c>
-      <c r="H26" s="44">
-        <v>6000</v>
-      </c>
-      <c r="I26" s="44">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="44" t="s">
-        <v>346</v>
-      </c>
-      <c r="B27" s="44">
-        <v>2021</v>
-      </c>
-      <c r="C27" s="44">
-        <v>38425</v>
-      </c>
-      <c r="D27" s="44">
-        <v>15000</v>
-      </c>
-      <c r="E27" s="44">
-        <v>40000</v>
-      </c>
-      <c r="G27" s="44">
-        <v>12000</v>
-      </c>
-      <c r="H27" s="44">
-        <v>6000</v>
-      </c>
-      <c r="I27" s="44">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="B28" s="44">
-        <v>2021</v>
-      </c>
-      <c r="C28" s="44">
-        <v>38425</v>
-      </c>
-      <c r="D28" s="44">
-        <v>15000</v>
-      </c>
-      <c r="E28" s="44">
-        <v>40000</v>
-      </c>
-      <c r="G28" s="44">
-        <v>12000</v>
-      </c>
-      <c r="H28" s="44">
-        <v>6000</v>
-      </c>
-      <c r="I28" s="44">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C29" s="44">
-        <f>SUM(C2:C28)</f>
-        <v>768500</v>
-      </c>
-      <c r="D29" s="44">
-        <f>SUM(D2:D28)</f>
-        <v>300000</v>
-      </c>
-      <c r="E29" s="44">
-        <f>SUM(E2:E28)</f>
-        <v>800000</v>
-      </c>
-      <c r="F29" s="44">
-        <f t="shared" ref="F29:I29" si="1">SUM(F2:F28)</f>
-        <v>34800</v>
-      </c>
-      <c r="G29" s="44">
-        <f t="shared" si="1"/>
-        <v>324000</v>
-      </c>
-      <c r="H29" s="44">
-        <f t="shared" si="1"/>
-        <v>148000</v>
-      </c>
-      <c r="I29" s="44">
-        <f t="shared" si="1"/>
-        <v>134000</v>
+        <f>SUM(I2:I21)</f>
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L24" s="44" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L25" s="44" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="46" spans="12:12" x14ac:dyDescent="0.35">
+      <c r="L46" s="70" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L46" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Changed database to mysql
</commit_message>
<xml_diff>
--- a/documents/Home.xlsx
+++ b/documents/Home.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14210" yWindow="1040" windowWidth="13530" windowHeight="5630" firstSheet="4" activeTab="12"/>
+    <workbookView xWindow="14210" yWindow="1040" windowWidth="13530" windowHeight="5630" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PaidTillDate" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="381">
   <si>
     <t>Date</t>
   </si>
@@ -1171,6 +1171,9 @@
   </si>
   <si>
     <t>;</t>
+  </si>
+  <si>
+    <t>49480503/loansupport@hdfcbank.com</t>
   </si>
 </sst>
 </file>
@@ -1444,13 +1447,13 @@
     <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -6484,8 +6487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6533,18 +6536,6 @@
       <c r="B2" s="44">
         <v>2020</v>
       </c>
-      <c r="C2" s="44">
-        <v>38425</v>
-      </c>
-      <c r="D2" s="44">
-        <v>15000</v>
-      </c>
-      <c r="E2" s="44">
-        <v>40000</v>
-      </c>
-      <c r="F2" s="44">
-        <v>5800</v>
-      </c>
       <c r="G2" s="44">
         <v>12000</v>
       </c>
@@ -7066,31 +7057,31 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C22" s="44">
-        <f>SUM(C2:C21)</f>
-        <v>768500</v>
+        <f t="shared" ref="C22:I22" si="0">SUM(C2:C21)</f>
+        <v>730075</v>
       </c>
       <c r="D22" s="44">
-        <f>SUM(D2:D21)</f>
-        <v>300000</v>
+        <f t="shared" si="0"/>
+        <v>285000</v>
       </c>
       <c r="E22" s="44">
-        <f>SUM(E2:E21)</f>
-        <v>800000</v>
+        <f t="shared" si="0"/>
+        <v>760000</v>
       </c>
       <c r="F22" s="44">
-        <f>SUM(F2:F21)</f>
-        <v>34800</v>
+        <f t="shared" si="0"/>
+        <v>29000</v>
       </c>
       <c r="G22" s="44">
-        <f>SUM(G2:G21)</f>
+        <f t="shared" si="0"/>
         <v>240000</v>
       </c>
       <c r="H22" s="44">
-        <f>SUM(H2:H21)</f>
+        <f t="shared" si="0"/>
         <v>120000</v>
       </c>
       <c r="I22" s="44">
-        <f>SUM(I2:I21)</f>
+        <f t="shared" si="0"/>
         <v>110000</v>
       </c>
     </row>
@@ -7105,7 +7096,7 @@
       </c>
     </row>
     <row r="46" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L46" s="70" t="s">
+      <c r="L46" s="68" t="s">
         <v>378</v>
       </c>
     </row>
@@ -22312,10 +22303,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G23"/>
+  <dimension ref="A2:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:D23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -22328,12 +22319,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
     </row>
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
@@ -22503,7 +22494,7 @@
       </c>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="27" t="s">
         <v>296</v>
       </c>
@@ -22521,7 +22512,10 @@
       </c>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="68" t="s">
+        <v>380</v>
+      </c>
       <c r="B18" s="27" t="s">
         <v>299</v>
       </c>
@@ -22539,7 +22533,7 @@
       </c>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="27" t="s">
         <v>310</v>
       </c>
@@ -22557,7 +22551,7 @@
       </c>
       <c r="G19" s="11"/>
     </row>
-    <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="12" t="s">
         <v>319</v>
       </c>
@@ -22576,7 +22570,7 @@
       </c>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="12" t="s">
         <v>320</v>
       </c>
@@ -22596,7 +22590,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="12" t="s">
         <v>370</v>
       </c>
@@ -22614,7 +22608,7 @@
       </c>
       <c r="G22" s="11"/>
     </row>
-    <row r="23" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="12" t="s">
         <v>373</v>
       </c>
@@ -22642,9 +22636,10 @@
     <hyperlink ref="D19" r:id="rId3"/>
     <hyperlink ref="C17" r:id="rId4"/>
     <hyperlink ref="C22" r:id="rId5" display="anshulsood/Name786@"/>
+    <hyperlink ref="A18" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -22758,10 +22753,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="69"/>
+      <c r="B8" s="70"/>
       <c r="D8" s="9" t="s">
         <v>9</v>
       </c>

</xml_diff>